<commit_message>
Atualização automática 2026-02-18 09:21:16.205630
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -601,7 +601,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>2026-02-13T15:22:52</t>
+          <t>2026-02-18T06:54:54</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -672,7 +672,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>2026-02-13T15:04:46</t>
+          <t>2026-02-18T07:19:17</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -743,7 +743,7 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>2026-02-13T14:49:04</t>
+          <t>2026-02-13T16:36:42</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
@@ -814,7 +814,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>2026-02-13T15:31:59</t>
+          <t>2026-02-18T07:31:13</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -1144,7 +1144,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>2026-02-13T15:19:42</t>
+          <t>2026-02-18T07:19:27</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -1474,7 +1474,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>2026-02-13T15:41:51</t>
+          <t>2026-02-18T07:15:48</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
@@ -1540,7 +1540,7 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>2026-02-13T14:20:13</t>
+          <t>2026-02-13T17:06:18</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
@@ -1606,7 +1606,7 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>2026-02-13T15:18:32</t>
+          <t>2026-02-18T07:30:01</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
@@ -6885,7 +6885,7 @@
       </c>
       <c r="N95" t="inlineStr">
         <is>
-          <t>2026-02-13T15:08:56</t>
+          <t>2026-02-18T07:30:24</t>
         </is>
       </c>
       <c r="O95" t="inlineStr">
@@ -6956,7 +6956,7 @@
       </c>
       <c r="N96" t="inlineStr">
         <is>
-          <t>2026-02-13T15:33:19</t>
+          <t>2026-02-14T14:45:18</t>
         </is>
       </c>
       <c r="O96" t="inlineStr">
@@ -6976,6 +6976,11 @@
           <t>COORDENACAO</t>
         </is>
       </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>10.69.3.93</t>
+        </is>
+      </c>
       <c r="D97" t="n">
         <v>2025</v>
       </c>
@@ -7022,7 +7027,7 @@
       </c>
       <c r="N97" t="inlineStr">
         <is>
-          <t>2026-02-13T14:50:09</t>
+          <t>2026-02-18T07:32:46</t>
         </is>
       </c>
       <c r="O97" t="inlineStr">
@@ -7088,7 +7093,7 @@
       </c>
       <c r="N98" t="inlineStr">
         <is>
-          <t>2026-02-13T15:24:18</t>
+          <t>2026-02-13T19:08:47</t>
         </is>
       </c>
       <c r="O98" t="inlineStr">
@@ -7159,7 +7164,7 @@
       </c>
       <c r="N99" t="inlineStr">
         <is>
-          <t>2026-02-13T15:36:50</t>
+          <t>2026-02-13T16:35:51</t>
         </is>
       </c>
       <c r="O99" t="inlineStr">
@@ -7230,7 +7235,7 @@
       </c>
       <c r="N100" t="inlineStr">
         <is>
-          <t>2026-02-13T14:44:47</t>
+          <t>2026-02-18T07:02:20</t>
         </is>
       </c>
       <c r="O100" t="inlineStr">
@@ -7301,7 +7306,7 @@
       </c>
       <c r="N101" t="inlineStr">
         <is>
-          <t>2026-02-13T15:30:49</t>
+          <t>2026-02-14T00:05:14</t>
         </is>
       </c>
       <c r="O101" t="inlineStr">
@@ -7443,7 +7448,7 @@
       </c>
       <c r="N103" t="inlineStr">
         <is>
-          <t>2026-02-13T15:01:11</t>
+          <t>2026-02-18T07:11:47</t>
         </is>
       </c>
       <c r="O103" t="inlineStr">
@@ -7708,7 +7713,7 @@
       </c>
       <c r="N107" t="inlineStr">
         <is>
-          <t>2026-02-13T14:56:29</t>
+          <t>2026-02-13T15:49:28</t>
         </is>
       </c>
       <c r="O107" t="inlineStr">
@@ -7850,7 +7855,7 @@
       </c>
       <c r="N109" t="inlineStr">
         <is>
-          <t>2026-02-13T15:14:54</t>
+          <t>2026-02-18T07:02:25</t>
         </is>
       </c>
       <c r="O109" t="inlineStr">
@@ -7921,7 +7926,7 @@
       </c>
       <c r="N110" t="inlineStr">
         <is>
-          <t>2026-02-13T15:29:28</t>
+          <t>2026-02-18T07:12:07</t>
         </is>
       </c>
       <c r="O110" t="inlineStr">
@@ -7992,7 +7997,7 @@
       </c>
       <c r="N111" t="inlineStr">
         <is>
-          <t>2026-02-13T15:37:08</t>
+          <t>2026-02-13T18:48:54</t>
         </is>
       </c>
       <c r="O111" t="inlineStr">
@@ -8063,7 +8068,7 @@
       </c>
       <c r="N112" t="inlineStr">
         <is>
-          <t>2026-02-13T15:06:53</t>
+          <t>2026-02-13T16:05:46</t>
         </is>
       </c>
       <c r="O112" t="inlineStr">
@@ -8134,7 +8139,7 @@
       </c>
       <c r="N113" t="inlineStr">
         <is>
-          <t>2026-02-13T15:12:41</t>
+          <t>2026-02-18T06:50:03</t>
         </is>
       </c>
       <c r="O113" t="inlineStr">
@@ -8205,7 +8210,7 @@
       </c>
       <c r="N114" t="inlineStr">
         <is>
-          <t>2026-02-13T15:26:19</t>
+          <t>2026-02-18T06:45:27</t>
         </is>
       </c>
       <c r="O114" t="inlineStr">
@@ -8273,7 +8278,7 @@
       </c>
       <c r="N115" t="inlineStr">
         <is>
-          <t>2026-02-13T15:18:22</t>
+          <t>2026-02-18T07:21:57</t>
         </is>
       </c>
       <c r="O115" t="inlineStr">
@@ -8344,7 +8349,7 @@
       </c>
       <c r="N116" t="inlineStr">
         <is>
-          <t>2026-02-13T15:19:06</t>
+          <t>2026-02-18T07:07:25</t>
         </is>
       </c>
       <c r="O116" t="inlineStr">
@@ -8415,7 +8420,7 @@
       </c>
       <c r="N117" t="inlineStr">
         <is>
-          <t>2026-02-13T15:19:34</t>
+          <t>2026-02-18T07:02:02</t>
         </is>
       </c>
       <c r="O117" t="inlineStr">
@@ -8696,7 +8701,7 @@
       </c>
       <c r="N121" t="inlineStr">
         <is>
-          <t>2026-02-13T14:49:34</t>
+          <t>2026-02-13T18:41:48</t>
         </is>
       </c>
       <c r="O121" t="inlineStr">
@@ -8764,7 +8769,7 @@
       </c>
       <c r="N122" t="inlineStr">
         <is>
-          <t>2026-02-13T14:56:36</t>
+          <t>2026-02-18T07:02:44</t>
         </is>
       </c>
       <c r="O122" t="inlineStr">
@@ -8835,7 +8840,7 @@
       </c>
       <c r="N123" t="inlineStr">
         <is>
-          <t>2026-02-13T15:02:06</t>
+          <t>2026-02-14T14:12:35</t>
         </is>
       </c>
       <c r="O123" t="inlineStr">
@@ -8906,7 +8911,7 @@
       </c>
       <c r="N124" t="inlineStr">
         <is>
-          <t>2026-02-13T15:34:26</t>
+          <t>2026-02-18T07:04:48</t>
         </is>
       </c>
       <c r="O124" t="inlineStr">
@@ -8977,7 +8982,7 @@
       </c>
       <c r="N125" t="inlineStr">
         <is>
-          <t>2026-02-13T15:28:24</t>
+          <t>2026-02-13T16:26:01</t>
         </is>
       </c>
       <c r="O125" t="inlineStr">
@@ -9048,7 +9053,7 @@
       </c>
       <c r="N126" t="inlineStr">
         <is>
-          <t>2026-02-13T14:55:47</t>
+          <t>2026-02-13T15:55:40</t>
         </is>
       </c>
       <c r="O126" t="inlineStr">
@@ -9119,7 +9124,7 @@
       </c>
       <c r="N127" t="inlineStr">
         <is>
-          <t>2026-02-13T15:20:07</t>
+          <t>2026-02-18T07:27:15</t>
         </is>
       </c>
       <c r="O127" t="inlineStr">
@@ -9190,7 +9195,7 @@
       </c>
       <c r="N128" t="inlineStr">
         <is>
-          <t>2026-02-13T15:32:20</t>
+          <t>2026-02-13T16:31:50</t>
         </is>
       </c>
       <c r="O128" t="inlineStr">
@@ -9261,7 +9266,7 @@
       </c>
       <c r="N129" t="inlineStr">
         <is>
-          <t>2026-02-13T15:05:05</t>
+          <t>2026-02-14T13:26:31</t>
         </is>
       </c>
       <c r="O129" t="inlineStr">
@@ -9332,7 +9337,7 @@
       </c>
       <c r="N130" t="inlineStr">
         <is>
-          <t>2026-02-13T15:02:30</t>
+          <t>2026-02-13T15:53:21</t>
         </is>
       </c>
       <c r="O130" t="inlineStr">
@@ -9352,11 +9357,6 @@
           <t>ADM/FIN</t>
         </is>
       </c>
-      <c r="C131" t="inlineStr">
-        <is>
-          <t>10.69.3.93</t>
-        </is>
-      </c>
       <c r="D131" t="n">
         <v>2025</v>
       </c>
@@ -9403,7 +9403,7 @@
       </c>
       <c r="N131" t="inlineStr">
         <is>
-          <t>2026-02-13T15:41:49</t>
+          <t>2026-02-13T16:36:29</t>
         </is>
       </c>
       <c r="O131" t="inlineStr">
@@ -9540,7 +9540,7 @@
       </c>
       <c r="N133" t="inlineStr">
         <is>
-          <t>2026-02-13T15:13:14</t>
+          <t>2026-02-18T07:13:15</t>
         </is>
       </c>
       <c r="O133" t="inlineStr">
@@ -9606,7 +9606,7 @@
       </c>
       <c r="N134" t="inlineStr">
         <is>
-          <t>2026-02-13T15:27:36</t>
+          <t>2026-02-18T07:11:10</t>
         </is>
       </c>
       <c r="O134" t="inlineStr">
@@ -9672,7 +9672,7 @@
       </c>
       <c r="N135" t="inlineStr">
         <is>
-          <t>2026-02-13T14:54:47</t>
+          <t>2026-02-18T07:10:55</t>
         </is>
       </c>
       <c r="O135" t="inlineStr">
@@ -9738,7 +9738,7 @@
       </c>
       <c r="N136" t="inlineStr">
         <is>
-          <t>2026-02-13T15:28:50</t>
+          <t>2026-02-13T19:18:26</t>
         </is>
       </c>
       <c r="O136" t="inlineStr">
@@ -9869,7 +9869,7 @@
       </c>
       <c r="N138" t="inlineStr">
         <is>
-          <t>2026-02-13T15:39:44</t>
+          <t>2026-02-18T07:11:27</t>
         </is>
       </c>
       <c r="O138" t="inlineStr">
@@ -9935,7 +9935,7 @@
       </c>
       <c r="N139" t="inlineStr">
         <is>
-          <t>2026-02-13T14:52:26</t>
+          <t>2026-02-14T13:18:18</t>
         </is>
       </c>
       <c r="O139" t="inlineStr">
@@ -10001,7 +10001,7 @@
       </c>
       <c r="N140" t="inlineStr">
         <is>
-          <t>2026-02-13T15:21:46</t>
+          <t>2026-02-14T14:17:34</t>
         </is>
       </c>
       <c r="O140" t="inlineStr">
@@ -10067,7 +10067,7 @@
       </c>
       <c r="N141" t="inlineStr">
         <is>
-          <t>2026-02-13T14:57:15</t>
+          <t>2026-02-18T07:11:46</t>
         </is>
       </c>
       <c r="O141" t="inlineStr">
@@ -10133,7 +10133,7 @@
       </c>
       <c r="N142" t="inlineStr">
         <is>
-          <t>2026-02-13T15:14:47</t>
+          <t>2026-02-14T14:03:13</t>
         </is>
       </c>
       <c r="O142" t="inlineStr">
@@ -10199,7 +10199,7 @@
       </c>
       <c r="N143" t="inlineStr">
         <is>
-          <t>2026-02-13T14:55:49</t>
+          <t>2026-02-14T14:18:29</t>
         </is>
       </c>
       <c r="O143" t="inlineStr">
@@ -10265,7 +10265,7 @@
       </c>
       <c r="N144" t="inlineStr">
         <is>
-          <t>2026-02-13T15:04:29</t>
+          <t>2026-02-14T14:05:23</t>
         </is>
       </c>
       <c r="O144" t="inlineStr">
@@ -10331,7 +10331,7 @@
       </c>
       <c r="N145" t="inlineStr">
         <is>
-          <t>2026-02-13T15:30:02</t>
+          <t>2026-02-14T14:15:55</t>
         </is>
       </c>
       <c r="O145" t="inlineStr">
@@ -10397,7 +10397,7 @@
       </c>
       <c r="N146" t="inlineStr">
         <is>
-          <t>2026-02-13T14:59:04</t>
+          <t>2026-02-14T14:45:21</t>
         </is>
       </c>
       <c r="O146" t="inlineStr">
@@ -10463,7 +10463,7 @@
       </c>
       <c r="N147" t="inlineStr">
         <is>
-          <t>2026-02-13T15:25:50</t>
+          <t>2026-02-14T14:48:06</t>
         </is>
       </c>
       <c r="O147" t="inlineStr">
@@ -10529,7 +10529,7 @@
       </c>
       <c r="N148" t="inlineStr">
         <is>
-          <t>2026-02-13T15:20:10</t>
+          <t>2026-02-18T07:37:36</t>
         </is>
       </c>
       <c r="O148" t="inlineStr">
@@ -10595,7 +10595,7 @@
       </c>
       <c r="N149" t="inlineStr">
         <is>
-          <t>2026-02-13T15:06:16</t>
+          <t>2026-02-14T14:17:34</t>
         </is>
       </c>
       <c r="O149" t="inlineStr">
@@ -10661,7 +10661,7 @@
       </c>
       <c r="N150" t="inlineStr">
         <is>
-          <t>2026-02-13T13:42:40</t>
+          <t>2026-02-14T20:54:17</t>
         </is>
       </c>
       <c r="O150" t="inlineStr">
@@ -10727,7 +10727,7 @@
       </c>
       <c r="N151" t="inlineStr">
         <is>
-          <t>2026-02-13T15:34:10</t>
+          <t>2026-02-14T20:14:15</t>
         </is>
       </c>
       <c r="O151" t="inlineStr">
@@ -10793,7 +10793,7 @@
       </c>
       <c r="N152" t="inlineStr">
         <is>
-          <t>2026-02-13T14:54:02</t>
+          <t>2026-02-14T14:38:15</t>
         </is>
       </c>
       <c r="O152" t="inlineStr">
@@ -10854,7 +10854,7 @@
       </c>
       <c r="N153" t="inlineStr">
         <is>
-          <t>2026-02-13T14:57:48</t>
+          <t>2026-02-14T20:13:45</t>
         </is>
       </c>
       <c r="O153" t="inlineStr">
@@ -10920,7 +10920,7 @@
       </c>
       <c r="N154" t="inlineStr">
         <is>
-          <t>2026-02-13T14:59:41</t>
+          <t>2026-02-18T07:33:43</t>
         </is>
       </c>
       <c r="O154" t="inlineStr">
@@ -10986,7 +10986,7 @@
       </c>
       <c r="N155" t="inlineStr">
         <is>
-          <t>2026-02-13T14:52:54</t>
+          <t>2026-02-14T20:25:23</t>
         </is>
       </c>
       <c r="O155" t="inlineStr">
@@ -11052,7 +11052,7 @@
       </c>
       <c r="N156" t="inlineStr">
         <is>
-          <t>2026-02-13T13:51:56</t>
+          <t>2026-02-14T14:09:57</t>
         </is>
       </c>
       <c r="O156" t="inlineStr">
@@ -11118,7 +11118,7 @@
       </c>
       <c r="N157" t="inlineStr">
         <is>
-          <t>2026-02-13T15:31:18</t>
+          <t>2026-02-14T20:37:37</t>
         </is>
       </c>
       <c r="O157" t="inlineStr">
@@ -11184,7 +11184,7 @@
       </c>
       <c r="N158" t="inlineStr">
         <is>
-          <t>2026-02-13T13:09:55</t>
+          <t>2026-02-14T14:38:41</t>
         </is>
       </c>
       <c r="O158" t="inlineStr">
@@ -11250,7 +11250,7 @@
       </c>
       <c r="N159" t="inlineStr">
         <is>
-          <t>2026-02-13T14:51:18</t>
+          <t>2026-02-14T14:04:41</t>
         </is>
       </c>
       <c r="O159" t="inlineStr">
@@ -11316,7 +11316,7 @@
       </c>
       <c r="N160" t="inlineStr">
         <is>
-          <t>2026-02-13T13:10:28</t>
+          <t>2026-02-18T07:26:41</t>
         </is>
       </c>
       <c r="O160" t="inlineStr">
@@ -11382,7 +11382,7 @@
       </c>
       <c r="N161" t="inlineStr">
         <is>
-          <t>2026-02-13T13:14:41</t>
+          <t>2026-02-14T14:42:15</t>
         </is>
       </c>
       <c r="O161" t="inlineStr">
@@ -11448,7 +11448,7 @@
       </c>
       <c r="N162" t="inlineStr">
         <is>
-          <t>2026-02-13T15:01:13</t>
+          <t>2026-02-14T13:54:50</t>
         </is>
       </c>
       <c r="O162" t="inlineStr">
@@ -11576,11 +11576,11 @@
         </is>
       </c>
       <c r="M164" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N164" t="inlineStr">
         <is>
-          <t>2026-02-13T15:27:15</t>
+          <t>2026-02-18T07:10:17</t>
         </is>
       </c>
       <c r="O164" t="inlineStr">
@@ -11642,11 +11642,11 @@
         </is>
       </c>
       <c r="M165" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N165" t="inlineStr">
         <is>
-          <t>2026-02-13T15:28:25</t>
+          <t>2026-02-18T06:53:30</t>
         </is>
       </c>
       <c r="O165" t="inlineStr">
@@ -11708,11 +11708,11 @@
         </is>
       </c>
       <c r="M166" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N166" t="inlineStr">
         <is>
-          <t>2026-02-13T14:55:55</t>
+          <t>2026-02-18T07:12:42</t>
         </is>
       </c>
       <c r="O166" t="inlineStr">
@@ -11774,11 +11774,11 @@
         </is>
       </c>
       <c r="M167" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N167" t="inlineStr">
         <is>
-          <t>2026-02-13T14:10:02</t>
+          <t>2026-02-18T07:06:33</t>
         </is>
       </c>
       <c r="O167" t="inlineStr">
@@ -11840,11 +11840,11 @@
         </is>
       </c>
       <c r="M168" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N168" t="inlineStr">
         <is>
-          <t>2026-02-13T13:14:06</t>
+          <t>2026-02-18T07:19:35</t>
         </is>
       </c>
       <c r="O168" t="inlineStr">
@@ -11910,7 +11910,7 @@
       </c>
       <c r="N169" t="inlineStr">
         <is>
-          <t>2026-02-13T15:18:40</t>
+          <t>2026-02-18T07:10:15</t>
         </is>
       </c>
       <c r="O169" t="inlineStr">
@@ -11976,7 +11976,7 @@
       </c>
       <c r="N170" t="inlineStr">
         <is>
-          <t>2026-02-13T15:28:57</t>
+          <t>2026-02-14T14:36:54</t>
         </is>
       </c>
       <c r="O170" t="inlineStr">
@@ -12038,11 +12038,11 @@
         </is>
       </c>
       <c r="M171" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N171" t="inlineStr">
         <is>
-          <t>2026-02-13T13:30:27</t>
+          <t>2026-02-14T09:16:10</t>
         </is>
       </c>
       <c r="O171" t="inlineStr">
@@ -12108,7 +12108,7 @@
       </c>
       <c r="N172" t="inlineStr">
         <is>
-          <t>2026-02-13T15:00:49</t>
+          <t>2026-02-14T12:31:07</t>
         </is>
       </c>
       <c r="O172" t="inlineStr">
@@ -12174,7 +12174,7 @@
       </c>
       <c r="N173" t="inlineStr">
         <is>
-          <t>2026-02-13T15:31:22</t>
+          <t>2026-02-18T06:55:30</t>
         </is>
       </c>
       <c r="O173" t="inlineStr">
@@ -12240,7 +12240,7 @@
       </c>
       <c r="N174" t="inlineStr">
         <is>
-          <t>2026-02-13T13:13:54</t>
+          <t>2026-02-14T20:54:51</t>
         </is>
       </c>
       <c r="O174" t="inlineStr">
@@ -12306,7 +12306,7 @@
       </c>
       <c r="N175" t="inlineStr">
         <is>
-          <t>2026-02-13T15:12:02</t>
+          <t>2026-02-18T07:10:03</t>
         </is>
       </c>
       <c r="O175" t="inlineStr">
@@ -12372,7 +12372,7 @@
       </c>
       <c r="N176" t="inlineStr">
         <is>
-          <t>2026-02-13T15:27:57</t>
+          <t>2026-02-14T09:18:53</t>
         </is>
       </c>
       <c r="O176" t="inlineStr">
@@ -12438,7 +12438,7 @@
       </c>
       <c r="N177" t="inlineStr">
         <is>
-          <t>2026-02-13T15:12:03</t>
+          <t>2026-02-14T12:30:54</t>
         </is>
       </c>
       <c r="O177" t="inlineStr">
@@ -12504,7 +12504,7 @@
       </c>
       <c r="N178" t="inlineStr">
         <is>
-          <t>2026-02-13T15:24:18</t>
+          <t>2026-02-18T06:49:37</t>
         </is>
       </c>
       <c r="O178" t="inlineStr">
@@ -12570,7 +12570,7 @@
       </c>
       <c r="N179" t="inlineStr">
         <is>
-          <t>2026-02-13T15:03:36</t>
+          <t>2026-02-18T07:21:34</t>
         </is>
       </c>
       <c r="O179" t="inlineStr">
@@ -12636,7 +12636,7 @@
       </c>
       <c r="N180" t="inlineStr">
         <is>
-          <t>2026-02-13T14:50:31</t>
+          <t>2026-02-18T07:21:59</t>
         </is>
       </c>
       <c r="O180" t="inlineStr">
@@ -12702,7 +12702,7 @@
       </c>
       <c r="N181" t="inlineStr">
         <is>
-          <t>2026-02-13T13:35:55</t>
+          <t>2026-02-14T20:08:28</t>
         </is>
       </c>
       <c r="O181" t="inlineStr">
@@ -12768,7 +12768,7 @@
       </c>
       <c r="N182" t="inlineStr">
         <is>
-          <t>2026-02-13T15:13:14</t>
+          <t>2026-02-13T20:56:42</t>
         </is>
       </c>
       <c r="O182" t="inlineStr">
@@ -12834,7 +12834,7 @@
       </c>
       <c r="N183" t="inlineStr">
         <is>
-          <t>2026-02-13T13:43:04</t>
+          <t>2026-02-18T07:33:50</t>
         </is>
       </c>
       <c r="O183" t="inlineStr">
@@ -13037,7 +13037,7 @@
       </c>
       <c r="N186" t="inlineStr">
         <is>
-          <t>2026-02-13T14:33:42</t>
+          <t>2026-02-18T07:10:56</t>
         </is>
       </c>
       <c r="O186" t="inlineStr">
@@ -13103,7 +13103,7 @@
       </c>
       <c r="N187" t="inlineStr">
         <is>
-          <t>2026-02-13T15:40:27</t>
+          <t>2026-02-14T20:03:48</t>
         </is>
       </c>
       <c r="O187" t="inlineStr">
@@ -13301,7 +13301,7 @@
       </c>
       <c r="N190" t="inlineStr">
         <is>
-          <t>2026-02-13T14:55:23</t>
+          <t>2026-02-18T07:33:26</t>
         </is>
       </c>
       <c r="O190" t="inlineStr">
@@ -13367,7 +13367,7 @@
       </c>
       <c r="N191" t="inlineStr">
         <is>
-          <t>2026-02-13T13:46:56</t>
+          <t>2026-02-14T14:50:48</t>
         </is>
       </c>
       <c r="O191" t="inlineStr">
@@ -13433,7 +13433,7 @@
       </c>
       <c r="N192" t="inlineStr">
         <is>
-          <t>2026-02-13T14:57:04</t>
+          <t>2026-02-14T14:36:40</t>
         </is>
       </c>
       <c r="O192" t="inlineStr">
@@ -13562,7 +13562,7 @@
       </c>
       <c r="N194" t="inlineStr">
         <is>
-          <t>2026-02-13T14:49:58</t>
+          <t>2026-02-18T06:10:40</t>
         </is>
       </c>
       <c r="O194" t="inlineStr">
@@ -13628,7 +13628,7 @@
       </c>
       <c r="N195" t="inlineStr">
         <is>
-          <t>2026-02-13T15:07:36</t>
+          <t>2026-02-14T14:03:42</t>
         </is>
       </c>
       <c r="O195" t="inlineStr">
@@ -13694,7 +13694,7 @@
       </c>
       <c r="N196" t="inlineStr">
         <is>
-          <t>2026-02-13T14:57:14</t>
+          <t>2026-02-13T19:54:14</t>
         </is>
       </c>
       <c r="O196" t="inlineStr">
@@ -13892,7 +13892,7 @@
       </c>
       <c r="N199" t="inlineStr">
         <is>
-          <t>2026-02-13T15:17:57</t>
+          <t>2026-02-13T19:10:31</t>
         </is>
       </c>
       <c r="O199" t="inlineStr">
@@ -13958,7 +13958,7 @@
       </c>
       <c r="N200" t="inlineStr">
         <is>
-          <t>2026-02-13T15:06:23</t>
+          <t>2026-02-13T19:44:19</t>
         </is>
       </c>
       <c r="O200" t="inlineStr">
@@ -14021,7 +14021,7 @@
       </c>
       <c r="N201" t="inlineStr">
         <is>
-          <t>2026-02-13T15:40:58</t>
+          <t>2026-02-13T19:21:01</t>
         </is>
       </c>
       <c r="O201" t="inlineStr">
@@ -14087,7 +14087,7 @@
       </c>
       <c r="N202" t="inlineStr">
         <is>
-          <t>2026-02-13T15:08:22</t>
+          <t>2026-02-14T14:51:05</t>
         </is>
       </c>
       <c r="O202" t="inlineStr">
@@ -14153,7 +14153,7 @@
       </c>
       <c r="N203" t="inlineStr">
         <is>
-          <t>2026-02-13T14:54:30</t>
+          <t>2026-02-14T14:51:03</t>
         </is>
       </c>
       <c r="O203" t="inlineStr">
@@ -14219,7 +14219,7 @@
       </c>
       <c r="N204" t="inlineStr">
         <is>
-          <t>2026-02-13T15:13:20</t>
+          <t>2026-02-13T19:50:13</t>
         </is>
       </c>
       <c r="O204" t="inlineStr">
@@ -14285,7 +14285,7 @@
       </c>
       <c r="N205" t="inlineStr">
         <is>
-          <t>2026-02-13T15:33:52</t>
+          <t>2026-02-13T19:23:30</t>
         </is>
       </c>
       <c r="O205" t="inlineStr">
@@ -14351,7 +14351,7 @@
       </c>
       <c r="N206" t="inlineStr">
         <is>
-          <t>2026-02-13T15:31:51</t>
+          <t>2026-02-18T06:58:59</t>
         </is>
       </c>
       <c r="O206" t="inlineStr">
@@ -14417,7 +14417,7 @@
       </c>
       <c r="N207" t="inlineStr">
         <is>
-          <t>2026-02-13T14:56:50</t>
+          <t>2026-02-13T19:30:21</t>
         </is>
       </c>
       <c r="O207" t="inlineStr">
@@ -14483,7 +14483,7 @@
       </c>
       <c r="N208" t="inlineStr">
         <is>
-          <t>2026-02-13T15:15:17</t>
+          <t>2026-02-14T14:41:01</t>
         </is>
       </c>
       <c r="O208" t="inlineStr">
@@ -14549,7 +14549,7 @@
       </c>
       <c r="N209" t="inlineStr">
         <is>
-          <t>2026-02-13T15:32:46</t>
+          <t>2026-02-13T20:27:36</t>
         </is>
       </c>
       <c r="O209" t="inlineStr">
@@ -14615,7 +14615,7 @@
       </c>
       <c r="N210" t="inlineStr">
         <is>
-          <t>2026-02-13T14:56:00</t>
+          <t>2026-02-14T20:30:39</t>
         </is>
       </c>
       <c r="O210" t="inlineStr">
@@ -14681,7 +14681,7 @@
       </c>
       <c r="N211" t="inlineStr">
         <is>
-          <t>2026-02-13T14:53:04</t>
+          <t>2026-02-18T07:20:48</t>
         </is>
       </c>
       <c r="O211" t="inlineStr">
@@ -14747,7 +14747,7 @@
       </c>
       <c r="N212" t="inlineStr">
         <is>
-          <t>2026-02-13T15:09:19</t>
+          <t>2026-02-18T07:19:58</t>
         </is>
       </c>
       <c r="O212" t="inlineStr">
@@ -14813,7 +14813,7 @@
       </c>
       <c r="N213" t="inlineStr">
         <is>
-          <t>2026-02-13T15:12:39</t>
+          <t>2026-02-14T14:25:02</t>
         </is>
       </c>
       <c r="O213" t="inlineStr">
@@ -14879,7 +14879,7 @@
       </c>
       <c r="N214" t="inlineStr">
         <is>
-          <t>2026-02-13T15:27:07</t>
+          <t>2026-02-14T09:03:27</t>
         </is>
       </c>
       <c r="O214" t="inlineStr">
@@ -14945,7 +14945,7 @@
       </c>
       <c r="N215" t="inlineStr">
         <is>
-          <t>2026-02-13T15:27:16</t>
+          <t>2026-02-18T07:20:26</t>
         </is>
       </c>
       <c r="O215" t="inlineStr">
@@ -15011,7 +15011,7 @@
       </c>
       <c r="N216" t="inlineStr">
         <is>
-          <t>2026-02-13T15:24:42</t>
+          <t>2026-02-18T07:20:25</t>
         </is>
       </c>
       <c r="O216" t="inlineStr">
@@ -15077,7 +15077,7 @@
       </c>
       <c r="N217" t="inlineStr">
         <is>
-          <t>2026-02-13T15:26:44</t>
+          <t>2026-02-18T07:20:28</t>
         </is>
       </c>
       <c r="O217" t="inlineStr">
@@ -15143,7 +15143,7 @@
       </c>
       <c r="N218" t="inlineStr">
         <is>
-          <t>2026-02-13T15:31:26</t>
+          <t>2026-02-14T14:31:04</t>
         </is>
       </c>
       <c r="O218" t="inlineStr">
@@ -15209,7 +15209,7 @@
       </c>
       <c r="N219" t="inlineStr">
         <is>
-          <t>2026-02-13T15:21:37</t>
+          <t>2026-02-18T07:20:59</t>
         </is>
       </c>
       <c r="O219" t="inlineStr">
@@ -15280,7 +15280,7 @@
       </c>
       <c r="N220" t="inlineStr">
         <is>
-          <t>2026-02-13T15:07:01</t>
+          <t>2026-02-18T07:36:57</t>
         </is>
       </c>
       <c r="O220" t="inlineStr">
@@ -15346,7 +15346,7 @@
       </c>
       <c r="N221" t="inlineStr">
         <is>
-          <t>2026-02-13T14:58:03</t>
+          <t>2026-02-14T14:27:04</t>
         </is>
       </c>
       <c r="O221" t="inlineStr">
@@ -15412,7 +15412,7 @@
       </c>
       <c r="N222" t="inlineStr">
         <is>
-          <t>2026-02-13T15:05:17</t>
+          <t>2026-02-13T19:36:24</t>
         </is>
       </c>
       <c r="O222" t="inlineStr">
@@ -15478,7 +15478,7 @@
       </c>
       <c r="N223" t="inlineStr">
         <is>
-          <t>2026-02-13T15:38:03</t>
+          <t>2026-02-13T19:24:57</t>
         </is>
       </c>
       <c r="O223" t="inlineStr">
@@ -15544,7 +15544,7 @@
       </c>
       <c r="N224" t="inlineStr">
         <is>
-          <t>2026-02-13T15:39:38</t>
+          <t>2026-02-14T14:42:15</t>
         </is>
       </c>
       <c r="O224" t="inlineStr">
@@ -15610,7 +15610,7 @@
       </c>
       <c r="N225" t="inlineStr">
         <is>
-          <t>2026-02-13T15:09:44</t>
+          <t>2026-02-18T07:24:03</t>
         </is>
       </c>
       <c r="O225" t="inlineStr">
@@ -15676,7 +15676,7 @@
       </c>
       <c r="N226" t="inlineStr">
         <is>
-          <t>2026-02-13T14:59:18</t>
+          <t>2026-02-14T14:55:20</t>
         </is>
       </c>
       <c r="O226" t="inlineStr">
@@ -15742,7 +15742,7 @@
       </c>
       <c r="N227" t="inlineStr">
         <is>
-          <t>2026-02-13T15:35:44</t>
+          <t>2026-02-14T14:16:07</t>
         </is>
       </c>
       <c r="O227" t="inlineStr">
@@ -15808,7 +15808,7 @@
       </c>
       <c r="N228" t="inlineStr">
         <is>
-          <t>2026-02-13T15:23:10</t>
+          <t>2026-02-14T14:14:29</t>
         </is>
       </c>
       <c r="O228" t="inlineStr">
@@ -15874,7 +15874,7 @@
       </c>
       <c r="N229" t="inlineStr">
         <is>
-          <t>2026-02-13T15:39:29</t>
+          <t>2026-02-14T14:37:04</t>
         </is>
       </c>
       <c r="O229" t="inlineStr">
@@ -15940,7 +15940,7 @@
       </c>
       <c r="N230" t="inlineStr">
         <is>
-          <t>2026-02-13T15:13:26</t>
+          <t>2026-02-18T07:27:09</t>
         </is>
       </c>
       <c r="O230" t="inlineStr">
@@ -16006,7 +16006,7 @@
       </c>
       <c r="N231" t="inlineStr">
         <is>
-          <t>2026-02-13T15:29:38</t>
+          <t>2026-02-13T19:10:03</t>
         </is>
       </c>
       <c r="O231" t="inlineStr">
@@ -16072,7 +16072,7 @@
       </c>
       <c r="N232" t="inlineStr">
         <is>
-          <t>2026-02-13T14:55:14</t>
+          <t>2026-02-14T13:38:44</t>
         </is>
       </c>
       <c r="O232" t="inlineStr">
@@ -16138,7 +16138,7 @@
       </c>
       <c r="N233" t="inlineStr">
         <is>
-          <t>2026-02-13T15:36:58</t>
+          <t>2026-02-13T19:14:47</t>
         </is>
       </c>
       <c r="O233" t="inlineStr">
@@ -16204,7 +16204,7 @@
       </c>
       <c r="N234" t="inlineStr">
         <is>
-          <t>2026-02-13T15:21:19</t>
+          <t>2026-02-13T19:09:29</t>
         </is>
       </c>
       <c r="O234" t="inlineStr">
@@ -16270,7 +16270,7 @@
       </c>
       <c r="N235" t="inlineStr">
         <is>
-          <t>2026-02-13T15:15:07</t>
+          <t>2026-02-13T19:02:52</t>
         </is>
       </c>
       <c r="O235" t="inlineStr">
@@ -16336,7 +16336,7 @@
       </c>
       <c r="N236" t="inlineStr">
         <is>
-          <t>2026-02-13T15:13:40</t>
+          <t>2026-02-13T19:50:39</t>
         </is>
       </c>
       <c r="O236" t="inlineStr">
@@ -16402,7 +16402,7 @@
       </c>
       <c r="N237" t="inlineStr">
         <is>
-          <t>2026-02-13T15:39:58</t>
+          <t>2026-02-13T19:19:08</t>
         </is>
       </c>
       <c r="O237" t="inlineStr">
@@ -16468,7 +16468,7 @@
       </c>
       <c r="N238" t="inlineStr">
         <is>
-          <t>2026-02-13T15:23:07</t>
+          <t>2026-02-13T19:08:06</t>
         </is>
       </c>
       <c r="O238" t="inlineStr">
@@ -16534,7 +16534,7 @@
       </c>
       <c r="N239" t="inlineStr">
         <is>
-          <t>2026-02-13T15:00:04</t>
+          <t>2026-02-14T14:33:49</t>
         </is>
       </c>
       <c r="O239" t="inlineStr">
@@ -16600,7 +16600,7 @@
       </c>
       <c r="N240" t="inlineStr">
         <is>
-          <t>2026-02-13T15:05:19</t>
+          <t>2026-02-14T09:04:41</t>
         </is>
       </c>
       <c r="O240" t="inlineStr">
@@ -16666,7 +16666,7 @@
       </c>
       <c r="N241" t="inlineStr">
         <is>
-          <t>2026-02-13T15:14:00</t>
+          <t>2026-02-18T07:32:40</t>
         </is>
       </c>
       <c r="O241" t="inlineStr">
@@ -16732,7 +16732,7 @@
       </c>
       <c r="N242" t="inlineStr">
         <is>
-          <t>2026-02-13T15:03:38</t>
+          <t>2026-02-18T07:32:41</t>
         </is>
       </c>
       <c r="O242" t="inlineStr">
@@ -16798,7 +16798,7 @@
       </c>
       <c r="N243" t="inlineStr">
         <is>
-          <t>2026-02-13T15:34:10</t>
+          <t>2026-02-18T06:57:10</t>
         </is>
       </c>
       <c r="O243" t="inlineStr">
@@ -16864,7 +16864,7 @@
       </c>
       <c r="N244" t="inlineStr">
         <is>
-          <t>2026-02-13T14:47:51</t>
+          <t>2026-02-13T19:30:26</t>
         </is>
       </c>
       <c r="O244" t="inlineStr">
@@ -16930,7 +16930,7 @@
       </c>
       <c r="N245" t="inlineStr">
         <is>
-          <t>2026-02-13T15:05:12</t>
+          <t>2026-02-18T07:22:06</t>
         </is>
       </c>
       <c r="O245" t="inlineStr">
@@ -16996,7 +16996,7 @@
       </c>
       <c r="N246" t="inlineStr">
         <is>
-          <t>2026-02-13T15:09:05</t>
+          <t>2026-02-18T07:22:19</t>
         </is>
       </c>
       <c r="O246" t="inlineStr">
@@ -17062,7 +17062,7 @@
       </c>
       <c r="N247" t="inlineStr">
         <is>
-          <t>2026-02-13T15:11:46</t>
+          <t>2026-02-18T07:21:36</t>
         </is>
       </c>
       <c r="O247" t="inlineStr">
@@ -17128,7 +17128,7 @@
       </c>
       <c r="N248" t="inlineStr">
         <is>
-          <t>2026-02-13T13:39:27</t>
+          <t>2026-02-18T07:21:19</t>
         </is>
       </c>
       <c r="O248" t="inlineStr">
@@ -17194,7 +17194,7 @@
       </c>
       <c r="N249" t="inlineStr">
         <is>
-          <t>2026-02-13T15:25:11</t>
+          <t>2026-02-18T07:21:36</t>
         </is>
       </c>
       <c r="O249" t="inlineStr">
@@ -17214,11 +17214,6 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
-      <c r="C250" t="inlineStr">
-        <is>
-          <t>10.69.5.118</t>
-        </is>
-      </c>
       <c r="D250" t="n">
         <v>2017</v>
       </c>
@@ -17260,7 +17255,7 @@
       </c>
       <c r="N250" t="inlineStr">
         <is>
-          <t>2026-02-13T15:38:25</t>
+          <t>2026-02-18T07:22:04</t>
         </is>
       </c>
       <c r="O250" t="inlineStr">
@@ -17326,7 +17321,7 @@
       </c>
       <c r="N251" t="inlineStr">
         <is>
-          <t>2026-02-13T15:09:25</t>
+          <t>2026-02-18T07:21:57</t>
         </is>
       </c>
       <c r="O251" t="inlineStr">
@@ -17392,7 +17387,7 @@
       </c>
       <c r="N252" t="inlineStr">
         <is>
-          <t>2026-02-13T14:07:44</t>
+          <t>2026-02-18T07:21:46</t>
         </is>
       </c>
       <c r="O252" t="inlineStr">
@@ -17458,7 +17453,7 @@
       </c>
       <c r="N253" t="inlineStr">
         <is>
-          <t>2026-02-13T14:59:23</t>
+          <t>2026-02-18T07:25:59</t>
         </is>
       </c>
       <c r="O253" t="inlineStr">
@@ -17518,7 +17513,7 @@
       </c>
       <c r="N254" t="inlineStr">
         <is>
-          <t>2026-02-13T14:53:24</t>
+          <t>2026-02-18T07:27:59</t>
         </is>
       </c>
       <c r="O254" t="inlineStr">
@@ -17584,7 +17579,7 @@
       </c>
       <c r="N255" t="inlineStr">
         <is>
-          <t>2026-02-13T15:13:08</t>
+          <t>2026-02-14T11:45:08</t>
         </is>
       </c>
       <c r="O255" t="inlineStr">
@@ -17650,7 +17645,7 @@
       </c>
       <c r="N256" t="inlineStr">
         <is>
-          <t>2026-02-13T15:41:59</t>
+          <t>2026-02-18T07:35:49</t>
         </is>
       </c>
       <c r="O256" t="inlineStr">
@@ -17716,7 +17711,7 @@
       </c>
       <c r="N257" t="inlineStr">
         <is>
-          <t>2026-02-13T15:21:55</t>
+          <t>2026-02-14T13:15:29</t>
         </is>
       </c>
       <c r="O257" t="inlineStr">
@@ -17782,7 +17777,7 @@
       </c>
       <c r="N258" t="inlineStr">
         <is>
-          <t>2026-02-13T15:01:40</t>
+          <t>2026-02-14T14:07:10</t>
         </is>
       </c>
       <c r="O258" t="inlineStr">
@@ -17848,7 +17843,7 @@
       </c>
       <c r="N259" t="inlineStr">
         <is>
-          <t>2026-02-13T15:39:39</t>
+          <t>2026-02-18T07:26:39</t>
         </is>
       </c>
       <c r="O259" t="inlineStr">
@@ -17914,7 +17909,7 @@
       </c>
       <c r="N260" t="inlineStr">
         <is>
-          <t>2026-02-13T14:31:54</t>
+          <t>2026-02-18T07:36:34</t>
         </is>
       </c>
       <c r="O260" t="inlineStr">
@@ -17980,7 +17975,7 @@
       </c>
       <c r="N261" t="inlineStr">
         <is>
-          <t>2026-02-13T14:20:49</t>
+          <t>2026-02-14T14:08:25</t>
         </is>
       </c>
       <c r="O261" t="inlineStr">
@@ -18046,7 +18041,7 @@
       </c>
       <c r="N262" t="inlineStr">
         <is>
-          <t>2026-02-13T14:58:11</t>
+          <t>2026-02-14T11:16:15</t>
         </is>
       </c>
       <c r="O262" t="inlineStr">
@@ -18112,7 +18107,7 @@
       </c>
       <c r="N263" t="inlineStr">
         <is>
-          <t>2026-02-13T14:58:08</t>
+          <t>2026-02-14T14:13:29</t>
         </is>
       </c>
       <c r="O263" t="inlineStr">
@@ -18178,7 +18173,7 @@
       </c>
       <c r="N264" t="inlineStr">
         <is>
-          <t>2026-02-13T15:26:38</t>
+          <t>2026-02-18T07:37:49</t>
         </is>
       </c>
       <c r="O264" t="inlineStr">
@@ -18244,7 +18239,7 @@
       </c>
       <c r="N265" t="inlineStr">
         <is>
-          <t>2026-02-13T13:37:07</t>
+          <t>2026-02-14T14:08:33</t>
         </is>
       </c>
       <c r="O265" t="inlineStr">
@@ -18310,7 +18305,7 @@
       </c>
       <c r="N266" t="inlineStr">
         <is>
-          <t>2026-02-13T15:36:05</t>
+          <t>2026-02-14T14:12:12</t>
         </is>
       </c>
       <c r="O266" t="inlineStr">
@@ -18376,7 +18371,7 @@
       </c>
       <c r="N267" t="inlineStr">
         <is>
-          <t>2026-02-13T14:49:35</t>
+          <t>2026-02-14T14:20:14</t>
         </is>
       </c>
       <c r="O267" t="inlineStr">
@@ -18442,7 +18437,7 @@
       </c>
       <c r="N268" t="inlineStr">
         <is>
-          <t>2026-02-13T14:56:39</t>
+          <t>2026-02-14T20:18:54</t>
         </is>
       </c>
       <c r="O268" t="inlineStr">
@@ -18508,7 +18503,7 @@
       </c>
       <c r="N269" t="inlineStr">
         <is>
-          <t>2026-02-13T15:28:40</t>
+          <t>2026-02-14T11:16:09</t>
         </is>
       </c>
       <c r="O269" t="inlineStr">
@@ -18571,7 +18566,7 @@
       </c>
       <c r="N270" t="inlineStr">
         <is>
-          <t>2026-02-13T15:30:26</t>
+          <t>2026-02-18T07:02:07</t>
         </is>
       </c>
       <c r="O270" t="inlineStr">
@@ -18637,7 +18632,7 @@
       </c>
       <c r="N271" t="inlineStr">
         <is>
-          <t>2026-02-13T08:33:47</t>
+          <t>2026-02-18T04:51:20</t>
         </is>
       </c>
       <c r="O271" t="inlineStr">
@@ -18703,7 +18698,7 @@
       </c>
       <c r="N272" t="inlineStr">
         <is>
-          <t>2026-02-13T13:36:45</t>
+          <t>2026-02-14T14:52:39</t>
         </is>
       </c>
       <c r="O272" t="inlineStr">
@@ -18769,7 +18764,7 @@
       </c>
       <c r="N273" t="inlineStr">
         <is>
-          <t>2026-02-13T13:33:46</t>
+          <t>2026-02-14T12:58:08</t>
         </is>
       </c>
       <c r="O273" t="inlineStr">
@@ -19033,7 +19028,7 @@
       </c>
       <c r="N277" t="inlineStr">
         <is>
-          <t>2026-02-07T20:16:23</t>
+          <t>2026-02-14T20:37:11</t>
         </is>
       </c>
       <c r="O277" t="inlineStr">
@@ -19099,7 +19094,7 @@
       </c>
       <c r="N278" t="inlineStr">
         <is>
-          <t>2026-02-12T19:28:42</t>
+          <t>2026-02-18T07:23:35</t>
         </is>
       </c>
       <c r="O278" t="inlineStr">
@@ -19165,7 +19160,7 @@
       </c>
       <c r="N279" t="inlineStr">
         <is>
-          <t>2026-02-12T19:35:18</t>
+          <t>2026-02-14T20:39:39</t>
         </is>
       </c>
       <c r="O279" t="inlineStr">
@@ -19231,7 +19226,7 @@
       </c>
       <c r="N280" t="inlineStr">
         <is>
-          <t>2026-02-13T06:27:39</t>
+          <t>2026-02-14T09:59:02</t>
         </is>
       </c>
       <c r="O280" t="inlineStr">
@@ -19297,7 +19292,7 @@
       </c>
       <c r="N281" t="inlineStr">
         <is>
-          <t>2026-02-12T20:18:17</t>
+          <t>2026-02-14T20:42:36</t>
         </is>
       </c>
       <c r="O281" t="inlineStr">
@@ -19317,6 +19312,11 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>10.69.5.151</t>
+        </is>
+      </c>
       <c r="D282" t="n">
         <v>2017</v>
       </c>
@@ -19358,7 +19358,7 @@
       </c>
       <c r="N282" t="inlineStr">
         <is>
-          <t>2026-02-13T15:03:41</t>
+          <t>2026-02-18T07:32:04</t>
         </is>
       </c>
       <c r="O282" t="inlineStr">
@@ -19424,7 +19424,7 @@
       </c>
       <c r="N283" t="inlineStr">
         <is>
-          <t>2026-02-13T15:02:31</t>
+          <t>2026-02-14T14:00:49</t>
         </is>
       </c>
       <c r="O283" t="inlineStr">
@@ -19490,7 +19490,7 @@
       </c>
       <c r="N284" t="inlineStr">
         <is>
-          <t>2026-02-13T13:39:18</t>
+          <t>2026-02-14T14:36:32</t>
         </is>
       </c>
       <c r="O284" t="inlineStr">
@@ -19556,7 +19556,7 @@
       </c>
       <c r="N285" t="inlineStr">
         <is>
-          <t>2026-02-13T13:10:34</t>
+          <t>2026-02-14T14:16:15</t>
         </is>
       </c>
       <c r="O285" t="inlineStr">
@@ -19683,7 +19683,7 @@
       </c>
       <c r="N287" t="inlineStr">
         <is>
-          <t>2026-02-13T14:27:13</t>
+          <t>2026-02-18T07:26:11</t>
         </is>
       </c>
       <c r="O287" t="inlineStr">
@@ -19749,7 +19749,7 @@
       </c>
       <c r="N288" t="inlineStr">
         <is>
-          <t>2026-02-13T13:39:21</t>
+          <t>2026-02-18T07:15:10</t>
         </is>
       </c>
       <c r="O288" t="inlineStr">
@@ -19815,7 +19815,7 @@
       </c>
       <c r="N289" t="inlineStr">
         <is>
-          <t>2026-02-13T14:59:23</t>
+          <t>2026-02-13T20:45:49</t>
         </is>
       </c>
       <c r="O289" t="inlineStr">
@@ -20635,7 +20635,7 @@
       </c>
       <c r="N302" t="inlineStr">
         <is>
-          <t>2026-02-13T15:01:56</t>
+          <t>2026-02-18T07:26:46</t>
         </is>
       </c>
       <c r="O302" t="inlineStr">
@@ -21400,7 +21400,7 @@
       </c>
       <c r="N314" t="inlineStr">
         <is>
-          <t>2026-02-07T01:03:41</t>
+          <t>2026-02-18T06:42:42</t>
         </is>
       </c>
       <c r="O314" t="inlineStr">
@@ -21787,7 +21787,7 @@
       </c>
       <c r="N320" t="inlineStr">
         <is>
-          <t>2026-02-13T15:10:13</t>
+          <t>2026-02-18T07:06:15</t>
         </is>
       </c>
       <c r="O320" t="inlineStr">
@@ -22536,7 +22536,7 @@
       </c>
       <c r="N332" t="inlineStr">
         <is>
-          <t>2026-02-13T14:52:37</t>
+          <t>2026-02-14T06:42:20</t>
         </is>
       </c>
       <c r="O332" t="inlineStr">
@@ -22602,7 +22602,7 @@
       </c>
       <c r="N333" t="inlineStr">
         <is>
-          <t>2026-02-13T15:17:00</t>
+          <t>2026-02-18T07:37:40</t>
         </is>
       </c>
       <c r="O333" t="inlineStr">
@@ -22668,7 +22668,7 @@
       </c>
       <c r="N334" t="inlineStr">
         <is>
-          <t>2026-02-13T15:34:10</t>
+          <t>2026-02-18T07:41:22</t>
         </is>
       </c>
       <c r="O334" t="inlineStr">
@@ -22734,7 +22734,7 @@
       </c>
       <c r="N335" t="inlineStr">
         <is>
-          <t>2026-02-13T15:14:19</t>
+          <t>2026-02-18T06:46:01</t>
         </is>
       </c>
       <c r="O335" t="inlineStr">
@@ -22800,7 +22800,7 @@
       </c>
       <c r="N336" t="inlineStr">
         <is>
-          <t>2026-02-13T15:16:32</t>
+          <t>2026-02-18T06:45:20</t>
         </is>
       </c>
       <c r="O336" t="inlineStr">
@@ -22866,7 +22866,7 @@
       </c>
       <c r="N337" t="inlineStr">
         <is>
-          <t>2026-02-13T15:19:42</t>
+          <t>2026-02-18T06:47:09</t>
         </is>
       </c>
       <c r="O337" t="inlineStr">
@@ -22932,7 +22932,7 @@
       </c>
       <c r="N338" t="inlineStr">
         <is>
-          <t>2026-02-13T15:01:08</t>
+          <t>2026-02-18T07:38:05</t>
         </is>
       </c>
       <c r="O338" t="inlineStr">
@@ -22998,7 +22998,7 @@
       </c>
       <c r="N339" t="inlineStr">
         <is>
-          <t>2026-02-13T14:59:41</t>
+          <t>2026-02-18T07:07:14</t>
         </is>
       </c>
       <c r="O339" t="inlineStr">
@@ -23064,7 +23064,7 @@
       </c>
       <c r="N340" t="inlineStr">
         <is>
-          <t>2026-02-13T13:17:29</t>
+          <t>2026-02-14T07:33:11</t>
         </is>
       </c>
       <c r="O340" t="inlineStr">
@@ -23130,7 +23130,7 @@
       </c>
       <c r="N341" t="inlineStr">
         <is>
-          <t>2026-02-13T14:09:05</t>
+          <t>2026-02-14T12:17:42</t>
         </is>
       </c>
       <c r="O341" t="inlineStr">
@@ -23192,11 +23192,11 @@
         </is>
       </c>
       <c r="M342" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N342" t="inlineStr">
         <is>
-          <t>2026-02-13T15:07:36</t>
+          <t>2026-02-14T12:00:44</t>
         </is>
       </c>
       <c r="O342" t="inlineStr">
@@ -23259,7 +23259,7 @@
       </c>
       <c r="N343" t="inlineStr">
         <is>
-          <t>2026-02-13T14:49:43</t>
+          <t>2026-02-13T17:35:51</t>
         </is>
       </c>
       <c r="O343" t="inlineStr">
@@ -23848,7 +23848,7 @@
       </c>
       <c r="N352" t="inlineStr">
         <is>
-          <t>2026-02-13T15:10:25</t>
+          <t>2026-02-18T06:47:01</t>
         </is>
       </c>
       <c r="O352" t="inlineStr">
@@ -24688,7 +24688,7 @@
       </c>
       <c r="N365" t="inlineStr">
         <is>
-          <t>2026-02-13T15:36:59</t>
+          <t>2026-02-18T07:39:40</t>
         </is>
       </c>
       <c r="O365" t="inlineStr">
@@ -24756,7 +24756,7 @@
       </c>
       <c r="N366" t="inlineStr">
         <is>
-          <t>2026-02-13T15:35:31</t>
+          <t>2026-02-18T06:53:25</t>
         </is>
       </c>
       <c r="O366" t="inlineStr">
@@ -24886,7 +24886,7 @@
       </c>
       <c r="N368" t="inlineStr">
         <is>
-          <t>2026-02-13T15:03:44</t>
+          <t>2026-02-13T15:54:38</t>
         </is>
       </c>
       <c r="O368" t="inlineStr">
@@ -24949,7 +24949,7 @@
       </c>
       <c r="N369" t="inlineStr">
         <is>
-          <t>2026-02-13T14:57:01</t>
+          <t>2026-02-13T15:49:56</t>
         </is>
       </c>
       <c r="O369" t="inlineStr">
@@ -25372,7 +25372,7 @@
       </c>
       <c r="N375" t="inlineStr">
         <is>
-          <t>2026-02-13T15:23:30</t>
+          <t>2026-02-18T07:20:31</t>
         </is>
       </c>
       <c r="O375" t="inlineStr">
@@ -25438,7 +25438,7 @@
       </c>
       <c r="N376" t="inlineStr">
         <is>
-          <t>2026-02-13T14:55:15</t>
+          <t>2026-02-16T20:21:03</t>
         </is>
       </c>
       <c r="O376" t="inlineStr">
@@ -25509,7 +25509,7 @@
       </c>
       <c r="N377" t="inlineStr">
         <is>
-          <t>2026-02-13T15:33:07</t>
+          <t>2026-02-13T16:30:25</t>
         </is>
       </c>
       <c r="O377" t="inlineStr">
@@ -25580,7 +25580,7 @@
       </c>
       <c r="N378" t="inlineStr">
         <is>
-          <t>2026-02-13T14:58:42</t>
+          <t>2026-02-18T06:44:05</t>
         </is>
       </c>
       <c r="O378" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática 2026-02-18 09:53:03.952172
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -601,7 +601,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>2026-02-18T06:54:54</t>
+          <t>2026-02-18T09:40:28</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -672,7 +672,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>2026-02-18T07:19:17</t>
+          <t>2026-02-18T09:06:32</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -814,7 +814,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>2026-02-18T07:31:13</t>
+          <t>2026-02-18T09:22:14</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -1144,7 +1144,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>2026-02-18T07:19:27</t>
+          <t>2026-02-18T09:14:46</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -1474,7 +1474,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>2026-02-18T07:15:48</t>
+          <t>2026-02-18T09:12:12</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
@@ -1606,7 +1606,7 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>2026-02-18T07:30:01</t>
+          <t>2026-02-18T09:20:11</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
@@ -6885,7 +6885,7 @@
       </c>
       <c r="N95" t="inlineStr">
         <is>
-          <t>2026-02-18T07:30:24</t>
+          <t>2026-02-18T09:18:41</t>
         </is>
       </c>
       <c r="O95" t="inlineStr">
@@ -6976,11 +6976,6 @@
           <t>COORDENACAO</t>
         </is>
       </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>10.69.3.93</t>
-        </is>
-      </c>
       <c r="D97" t="n">
         <v>2025</v>
       </c>
@@ -7027,7 +7022,7 @@
       </c>
       <c r="N97" t="inlineStr">
         <is>
-          <t>2026-02-18T07:32:46</t>
+          <t>2026-02-18T09:27:14</t>
         </is>
       </c>
       <c r="O97" t="inlineStr">
@@ -7093,7 +7088,7 @@
       </c>
       <c r="N98" t="inlineStr">
         <is>
-          <t>2026-02-13T19:08:47</t>
+          <t>2026-02-18T08:50:00</t>
         </is>
       </c>
       <c r="O98" t="inlineStr">
@@ -7164,7 +7159,7 @@
       </c>
       <c r="N99" t="inlineStr">
         <is>
-          <t>2026-02-13T16:35:51</t>
+          <t>2026-02-18T09:34:45</t>
         </is>
       </c>
       <c r="O99" t="inlineStr">
@@ -7235,7 +7230,7 @@
       </c>
       <c r="N100" t="inlineStr">
         <is>
-          <t>2026-02-18T07:02:20</t>
+          <t>2026-02-18T08:55:59</t>
         </is>
       </c>
       <c r="O100" t="inlineStr">
@@ -7306,7 +7301,7 @@
       </c>
       <c r="N101" t="inlineStr">
         <is>
-          <t>2026-02-14T00:05:14</t>
+          <t>2026-02-18T08:59:04</t>
         </is>
       </c>
       <c r="O101" t="inlineStr">
@@ -7448,7 +7443,7 @@
       </c>
       <c r="N103" t="inlineStr">
         <is>
-          <t>2026-02-18T07:11:47</t>
+          <t>2026-02-18T09:00:43</t>
         </is>
       </c>
       <c r="O103" t="inlineStr">
@@ -7713,7 +7708,7 @@
       </c>
       <c r="N107" t="inlineStr">
         <is>
-          <t>2026-02-13T15:49:28</t>
+          <t>2026-02-18T09:18:18</t>
         </is>
       </c>
       <c r="O107" t="inlineStr">
@@ -7855,7 +7850,7 @@
       </c>
       <c r="N109" t="inlineStr">
         <is>
-          <t>2026-02-18T07:02:25</t>
+          <t>2026-02-18T08:54:16</t>
         </is>
       </c>
       <c r="O109" t="inlineStr">
@@ -7926,7 +7921,7 @@
       </c>
       <c r="N110" t="inlineStr">
         <is>
-          <t>2026-02-18T07:12:07</t>
+          <t>2026-02-18T08:59:35</t>
         </is>
       </c>
       <c r="O110" t="inlineStr">
@@ -7997,7 +7992,7 @@
       </c>
       <c r="N111" t="inlineStr">
         <is>
-          <t>2026-02-13T18:48:54</t>
+          <t>2026-02-18T08:53:23</t>
         </is>
       </c>
       <c r="O111" t="inlineStr">
@@ -8068,7 +8063,7 @@
       </c>
       <c r="N112" t="inlineStr">
         <is>
-          <t>2026-02-13T16:05:46</t>
+          <t>2026-02-18T09:42:23</t>
         </is>
       </c>
       <c r="O112" t="inlineStr">
@@ -8139,7 +8134,7 @@
       </c>
       <c r="N113" t="inlineStr">
         <is>
-          <t>2026-02-18T06:50:03</t>
+          <t>2026-02-18T09:39:03</t>
         </is>
       </c>
       <c r="O113" t="inlineStr">
@@ -8210,7 +8205,7 @@
       </c>
       <c r="N114" t="inlineStr">
         <is>
-          <t>2026-02-18T06:45:27</t>
+          <t>2026-02-18T09:38:21</t>
         </is>
       </c>
       <c r="O114" t="inlineStr">
@@ -8278,7 +8273,7 @@
       </c>
       <c r="N115" t="inlineStr">
         <is>
-          <t>2026-02-18T07:21:57</t>
+          <t>2026-02-18T09:09:03</t>
         </is>
       </c>
       <c r="O115" t="inlineStr">
@@ -8349,7 +8344,7 @@
       </c>
       <c r="N116" t="inlineStr">
         <is>
-          <t>2026-02-18T07:07:25</t>
+          <t>2026-02-18T09:02:37</t>
         </is>
       </c>
       <c r="O116" t="inlineStr">
@@ -8369,11 +8364,6 @@
           <t>DP</t>
         </is>
       </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>10.69.3.23</t>
-        </is>
-      </c>
       <c r="D117" t="n">
         <v>2025</v>
       </c>
@@ -8420,7 +8410,7 @@
       </c>
       <c r="N117" t="inlineStr">
         <is>
-          <t>2026-02-18T07:02:02</t>
+          <t>2026-02-18T08:50:54</t>
         </is>
       </c>
       <c r="O117" t="inlineStr">
@@ -8630,7 +8620,7 @@
       </c>
       <c r="N120" t="inlineStr">
         <is>
-          <t>2026-02-13T14:45:48</t>
+          <t>2026-02-18T09:41:44</t>
         </is>
       </c>
       <c r="O120" t="inlineStr">
@@ -8769,7 +8759,7 @@
       </c>
       <c r="N122" t="inlineStr">
         <is>
-          <t>2026-02-18T07:02:44</t>
+          <t>2026-02-18T08:52:16</t>
         </is>
       </c>
       <c r="O122" t="inlineStr">
@@ -8911,7 +8901,7 @@
       </c>
       <c r="N124" t="inlineStr">
         <is>
-          <t>2026-02-18T07:04:48</t>
+          <t>2026-02-18T09:00:43</t>
         </is>
       </c>
       <c r="O124" t="inlineStr">
@@ -8982,7 +8972,7 @@
       </c>
       <c r="N125" t="inlineStr">
         <is>
-          <t>2026-02-13T16:26:01</t>
+          <t>2026-02-18T08:50:29</t>
         </is>
       </c>
       <c r="O125" t="inlineStr">
@@ -9053,7 +9043,7 @@
       </c>
       <c r="N126" t="inlineStr">
         <is>
-          <t>2026-02-13T15:55:40</t>
+          <t>2026-02-18T09:05:31</t>
         </is>
       </c>
       <c r="O126" t="inlineStr">
@@ -9124,7 +9114,7 @@
       </c>
       <c r="N127" t="inlineStr">
         <is>
-          <t>2026-02-18T07:27:15</t>
+          <t>2026-02-18T09:26:15</t>
         </is>
       </c>
       <c r="O127" t="inlineStr">
@@ -9195,7 +9185,7 @@
       </c>
       <c r="N128" t="inlineStr">
         <is>
-          <t>2026-02-13T16:31:50</t>
+          <t>2026-02-18T09:01:38</t>
         </is>
       </c>
       <c r="O128" t="inlineStr">
@@ -9337,7 +9327,7 @@
       </c>
       <c r="N130" t="inlineStr">
         <is>
-          <t>2026-02-13T15:53:21</t>
+          <t>2026-02-18T08:59:04</t>
         </is>
       </c>
       <c r="O130" t="inlineStr">
@@ -9357,6 +9347,11 @@
           <t>ADM/FIN</t>
         </is>
       </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>10.69.3.6</t>
+        </is>
+      </c>
       <c r="D131" t="n">
         <v>2025</v>
       </c>
@@ -9403,7 +9398,7 @@
       </c>
       <c r="N131" t="inlineStr">
         <is>
-          <t>2026-02-13T16:36:29</t>
+          <t>2026-02-18T09:41:12</t>
         </is>
       </c>
       <c r="O131" t="inlineStr">
@@ -9540,7 +9535,7 @@
       </c>
       <c r="N133" t="inlineStr">
         <is>
-          <t>2026-02-18T07:13:15</t>
+          <t>2026-02-18T09:09:57</t>
         </is>
       </c>
       <c r="O133" t="inlineStr">
@@ -9606,7 +9601,7 @@
       </c>
       <c r="N134" t="inlineStr">
         <is>
-          <t>2026-02-18T07:11:10</t>
+          <t>2026-02-18T09:24:40</t>
         </is>
       </c>
       <c r="O134" t="inlineStr">
@@ -9672,7 +9667,7 @@
       </c>
       <c r="N135" t="inlineStr">
         <is>
-          <t>2026-02-18T07:10:55</t>
+          <t>2026-02-18T09:07:13</t>
         </is>
       </c>
       <c r="O135" t="inlineStr">
@@ -9869,7 +9864,7 @@
       </c>
       <c r="N138" t="inlineStr">
         <is>
-          <t>2026-02-18T07:11:27</t>
+          <t>2026-02-18T08:58:13</t>
         </is>
       </c>
       <c r="O138" t="inlineStr">
@@ -9935,7 +9930,7 @@
       </c>
       <c r="N139" t="inlineStr">
         <is>
-          <t>2026-02-14T13:18:18</t>
+          <t>2026-02-18T08:53:39</t>
         </is>
       </c>
       <c r="O139" t="inlineStr">
@@ -10001,7 +9996,7 @@
       </c>
       <c r="N140" t="inlineStr">
         <is>
-          <t>2026-02-14T14:17:34</t>
+          <t>2026-02-18T09:25:28</t>
         </is>
       </c>
       <c r="O140" t="inlineStr">
@@ -10067,7 +10062,7 @@
       </c>
       <c r="N141" t="inlineStr">
         <is>
-          <t>2026-02-18T07:11:46</t>
+          <t>2026-02-18T09:00:29</t>
         </is>
       </c>
       <c r="O141" t="inlineStr">
@@ -10397,7 +10392,7 @@
       </c>
       <c r="N146" t="inlineStr">
         <is>
-          <t>2026-02-14T14:45:21</t>
+          <t>2026-02-18T08:53:02</t>
         </is>
       </c>
       <c r="O146" t="inlineStr">
@@ -10463,7 +10458,7 @@
       </c>
       <c r="N147" t="inlineStr">
         <is>
-          <t>2026-02-14T14:48:06</t>
+          <t>2026-02-18T08:58:13</t>
         </is>
       </c>
       <c r="O147" t="inlineStr">
@@ -10529,7 +10524,7 @@
       </c>
       <c r="N148" t="inlineStr">
         <is>
-          <t>2026-02-18T07:37:36</t>
+          <t>2026-02-18T09:27:43</t>
         </is>
       </c>
       <c r="O148" t="inlineStr">
@@ -10727,7 +10722,7 @@
       </c>
       <c r="N151" t="inlineStr">
         <is>
-          <t>2026-02-14T20:14:15</t>
+          <t>2026-02-18T09:38:27</t>
         </is>
       </c>
       <c r="O151" t="inlineStr">
@@ -10793,7 +10788,7 @@
       </c>
       <c r="N152" t="inlineStr">
         <is>
-          <t>2026-02-14T14:38:15</t>
+          <t>2026-02-18T09:08:34</t>
         </is>
       </c>
       <c r="O152" t="inlineStr">
@@ -10854,7 +10849,7 @@
       </c>
       <c r="N153" t="inlineStr">
         <is>
-          <t>2026-02-14T20:13:45</t>
+          <t>2026-02-18T09:06:39</t>
         </is>
       </c>
       <c r="O153" t="inlineStr">
@@ -10920,7 +10915,7 @@
       </c>
       <c r="N154" t="inlineStr">
         <is>
-          <t>2026-02-18T07:33:43</t>
+          <t>2026-02-18T09:31:04</t>
         </is>
       </c>
       <c r="O154" t="inlineStr">
@@ -10986,7 +10981,7 @@
       </c>
       <c r="N155" t="inlineStr">
         <is>
-          <t>2026-02-14T20:25:23</t>
+          <t>2026-02-18T09:07:15</t>
         </is>
       </c>
       <c r="O155" t="inlineStr">
@@ -11052,7 +11047,7 @@
       </c>
       <c r="N156" t="inlineStr">
         <is>
-          <t>2026-02-14T14:09:57</t>
+          <t>2026-02-18T09:01:01</t>
         </is>
       </c>
       <c r="O156" t="inlineStr">
@@ -11118,7 +11113,7 @@
       </c>
       <c r="N157" t="inlineStr">
         <is>
-          <t>2026-02-14T20:37:37</t>
+          <t>2026-02-18T08:59:07</t>
         </is>
       </c>
       <c r="O157" t="inlineStr">
@@ -11184,7 +11179,7 @@
       </c>
       <c r="N158" t="inlineStr">
         <is>
-          <t>2026-02-14T14:38:41</t>
+          <t>2026-02-18T08:39:38</t>
         </is>
       </c>
       <c r="O158" t="inlineStr">
@@ -11250,7 +11245,7 @@
       </c>
       <c r="N159" t="inlineStr">
         <is>
-          <t>2026-02-14T14:04:41</t>
+          <t>2026-02-18T09:35:52</t>
         </is>
       </c>
       <c r="O159" t="inlineStr">
@@ -11316,7 +11311,7 @@
       </c>
       <c r="N160" t="inlineStr">
         <is>
-          <t>2026-02-18T07:26:41</t>
+          <t>2026-02-18T09:21:05</t>
         </is>
       </c>
       <c r="O160" t="inlineStr">
@@ -11382,7 +11377,7 @@
       </c>
       <c r="N161" t="inlineStr">
         <is>
-          <t>2026-02-14T14:42:15</t>
+          <t>2026-02-18T08:53:46</t>
         </is>
       </c>
       <c r="O161" t="inlineStr">
@@ -11448,7 +11443,7 @@
       </c>
       <c r="N162" t="inlineStr">
         <is>
-          <t>2026-02-14T13:54:50</t>
+          <t>2026-02-18T09:23:40</t>
         </is>
       </c>
       <c r="O162" t="inlineStr">
@@ -11576,11 +11571,11 @@
         </is>
       </c>
       <c r="M164" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N164" t="inlineStr">
         <is>
-          <t>2026-02-18T07:10:17</t>
+          <t>2026-02-18T08:56:56</t>
         </is>
       </c>
       <c r="O164" t="inlineStr">
@@ -11642,11 +11637,11 @@
         </is>
       </c>
       <c r="M165" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N165" t="inlineStr">
         <is>
-          <t>2026-02-18T06:53:30</t>
+          <t>2026-02-18T09:42:04</t>
         </is>
       </c>
       <c r="O165" t="inlineStr">
@@ -11708,11 +11703,11 @@
         </is>
       </c>
       <c r="M166" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N166" t="inlineStr">
         <is>
-          <t>2026-02-18T07:12:42</t>
+          <t>2026-02-18T09:06:38</t>
         </is>
       </c>
       <c r="O166" t="inlineStr">
@@ -11778,7 +11773,7 @@
       </c>
       <c r="N167" t="inlineStr">
         <is>
-          <t>2026-02-18T07:06:33</t>
+          <t>2026-02-18T09:42:22</t>
         </is>
       </c>
       <c r="O167" t="inlineStr">
@@ -11840,11 +11835,11 @@
         </is>
       </c>
       <c r="M168" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N168" t="inlineStr">
         <is>
-          <t>2026-02-18T07:19:35</t>
+          <t>2026-02-18T09:10:50</t>
         </is>
       </c>
       <c r="O168" t="inlineStr">
@@ -11910,7 +11905,7 @@
       </c>
       <c r="N169" t="inlineStr">
         <is>
-          <t>2026-02-18T07:10:15</t>
+          <t>2026-02-18T09:06:17</t>
         </is>
       </c>
       <c r="O169" t="inlineStr">
@@ -11976,7 +11971,7 @@
       </c>
       <c r="N170" t="inlineStr">
         <is>
-          <t>2026-02-14T14:36:54</t>
+          <t>2026-02-18T08:58:09</t>
         </is>
       </c>
       <c r="O170" t="inlineStr">
@@ -12170,11 +12165,11 @@
         </is>
       </c>
       <c r="M173" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N173" t="inlineStr">
         <is>
-          <t>2026-02-18T06:55:30</t>
+          <t>2026-02-18T09:40:21</t>
         </is>
       </c>
       <c r="O173" t="inlineStr">
@@ -12240,7 +12235,7 @@
       </c>
       <c r="N174" t="inlineStr">
         <is>
-          <t>2026-02-14T20:54:51</t>
+          <t>2026-02-18T08:45:13</t>
         </is>
       </c>
       <c r="O174" t="inlineStr">
@@ -12306,7 +12301,7 @@
       </c>
       <c r="N175" t="inlineStr">
         <is>
-          <t>2026-02-18T07:10:03</t>
+          <t>2026-02-18T09:03:49</t>
         </is>
       </c>
       <c r="O175" t="inlineStr">
@@ -12372,7 +12367,7 @@
       </c>
       <c r="N176" t="inlineStr">
         <is>
-          <t>2026-02-14T09:18:53</t>
+          <t>2026-02-18T09:37:18</t>
         </is>
       </c>
       <c r="O176" t="inlineStr">
@@ -12438,7 +12433,7 @@
       </c>
       <c r="N177" t="inlineStr">
         <is>
-          <t>2026-02-14T12:30:54</t>
+          <t>2026-02-18T09:42:29</t>
         </is>
       </c>
       <c r="O177" t="inlineStr">
@@ -12504,7 +12499,7 @@
       </c>
       <c r="N178" t="inlineStr">
         <is>
-          <t>2026-02-18T06:49:37</t>
+          <t>2026-02-18T09:42:04</t>
         </is>
       </c>
       <c r="O178" t="inlineStr">
@@ -12570,7 +12565,7 @@
       </c>
       <c r="N179" t="inlineStr">
         <is>
-          <t>2026-02-18T07:21:34</t>
+          <t>2026-02-18T09:11:30</t>
         </is>
       </c>
       <c r="O179" t="inlineStr">
@@ -12636,7 +12631,7 @@
       </c>
       <c r="N180" t="inlineStr">
         <is>
-          <t>2026-02-18T07:21:59</t>
+          <t>2026-02-18T09:12:21</t>
         </is>
       </c>
       <c r="O180" t="inlineStr">
@@ -12834,7 +12829,7 @@
       </c>
       <c r="N183" t="inlineStr">
         <is>
-          <t>2026-02-18T07:33:50</t>
+          <t>2026-02-18T09:20:04</t>
         </is>
       </c>
       <c r="O183" t="inlineStr">
@@ -13037,7 +13032,7 @@
       </c>
       <c r="N186" t="inlineStr">
         <is>
-          <t>2026-02-18T07:10:56</t>
+          <t>2026-02-18T08:55:35</t>
         </is>
       </c>
       <c r="O186" t="inlineStr">
@@ -13103,7 +13098,7 @@
       </c>
       <c r="N187" t="inlineStr">
         <is>
-          <t>2026-02-14T20:03:48</t>
+          <t>2026-02-18T09:42:04</t>
         </is>
       </c>
       <c r="O187" t="inlineStr">
@@ -13169,7 +13164,7 @@
       </c>
       <c r="N188" t="inlineStr">
         <is>
-          <t>2026-02-13T13:39:59</t>
+          <t>2026-02-18T08:55:46</t>
         </is>
       </c>
       <c r="O188" t="inlineStr">
@@ -13301,7 +13296,7 @@
       </c>
       <c r="N190" t="inlineStr">
         <is>
-          <t>2026-02-18T07:33:26</t>
+          <t>2026-02-18T09:31:58</t>
         </is>
       </c>
       <c r="O190" t="inlineStr">
@@ -13562,7 +13557,7 @@
       </c>
       <c r="N194" t="inlineStr">
         <is>
-          <t>2026-02-18T06:10:40</t>
+          <t>2026-02-18T07:57:11</t>
         </is>
       </c>
       <c r="O194" t="inlineStr">
@@ -13628,7 +13623,7 @@
       </c>
       <c r="N195" t="inlineStr">
         <is>
-          <t>2026-02-14T14:03:42</t>
+          <t>2026-02-18T08:55:37</t>
         </is>
       </c>
       <c r="O195" t="inlineStr">
@@ -13694,7 +13689,7 @@
       </c>
       <c r="N196" t="inlineStr">
         <is>
-          <t>2026-02-13T19:54:14</t>
+          <t>2026-02-18T08:57:19</t>
         </is>
       </c>
       <c r="O196" t="inlineStr">
@@ -13760,7 +13755,7 @@
       </c>
       <c r="N197" t="inlineStr">
         <is>
-          <t>2026-02-13T10:04:52</t>
+          <t>2026-02-18T08:47:42</t>
         </is>
       </c>
       <c r="O197" t="inlineStr">
@@ -13826,7 +13821,7 @@
       </c>
       <c r="N198" t="inlineStr">
         <is>
-          <t>2026-02-10T19:55:07</t>
+          <t>2026-02-18T09:02:04</t>
         </is>
       </c>
       <c r="O198" t="inlineStr">
@@ -14087,7 +14082,7 @@
       </c>
       <c r="N202" t="inlineStr">
         <is>
-          <t>2026-02-14T14:51:05</t>
+          <t>2026-02-18T08:58:37</t>
         </is>
       </c>
       <c r="O202" t="inlineStr">
@@ -14153,7 +14148,7 @@
       </c>
       <c r="N203" t="inlineStr">
         <is>
-          <t>2026-02-14T14:51:03</t>
+          <t>2026-02-18T09:39:30</t>
         </is>
       </c>
       <c r="O203" t="inlineStr">
@@ -14219,7 +14214,7 @@
       </c>
       <c r="N204" t="inlineStr">
         <is>
-          <t>2026-02-13T19:50:13</t>
+          <t>2026-02-18T09:28:18</t>
         </is>
       </c>
       <c r="O204" t="inlineStr">
@@ -14285,7 +14280,7 @@
       </c>
       <c r="N205" t="inlineStr">
         <is>
-          <t>2026-02-13T19:23:30</t>
+          <t>2026-02-18T09:00:33</t>
         </is>
       </c>
       <c r="O205" t="inlineStr">
@@ -14351,7 +14346,7 @@
       </c>
       <c r="N206" t="inlineStr">
         <is>
-          <t>2026-02-18T06:58:59</t>
+          <t>2026-02-18T08:53:59</t>
         </is>
       </c>
       <c r="O206" t="inlineStr">
@@ -14417,7 +14412,7 @@
       </c>
       <c r="N207" t="inlineStr">
         <is>
-          <t>2026-02-13T19:30:21</t>
+          <t>2026-02-18T09:40:37</t>
         </is>
       </c>
       <c r="O207" t="inlineStr">
@@ -14483,7 +14478,7 @@
       </c>
       <c r="N208" t="inlineStr">
         <is>
-          <t>2026-02-14T14:41:01</t>
+          <t>2026-02-18T09:34:55</t>
         </is>
       </c>
       <c r="O208" t="inlineStr">
@@ -14549,7 +14544,7 @@
       </c>
       <c r="N209" t="inlineStr">
         <is>
-          <t>2026-02-13T20:27:36</t>
+          <t>2026-02-18T08:50:06</t>
         </is>
       </c>
       <c r="O209" t="inlineStr">
@@ -14615,7 +14610,7 @@
       </c>
       <c r="N210" t="inlineStr">
         <is>
-          <t>2026-02-14T20:30:39</t>
+          <t>2026-02-18T08:56:14</t>
         </is>
       </c>
       <c r="O210" t="inlineStr">
@@ -14681,7 +14676,7 @@
       </c>
       <c r="N211" t="inlineStr">
         <is>
-          <t>2026-02-18T07:20:48</t>
+          <t>2026-02-18T09:19:29</t>
         </is>
       </c>
       <c r="O211" t="inlineStr">
@@ -14747,7 +14742,7 @@
       </c>
       <c r="N212" t="inlineStr">
         <is>
-          <t>2026-02-18T07:19:58</t>
+          <t>2026-02-18T09:12:27</t>
         </is>
       </c>
       <c r="O212" t="inlineStr">
@@ -14813,7 +14808,7 @@
       </c>
       <c r="N213" t="inlineStr">
         <is>
-          <t>2026-02-14T14:25:02</t>
+          <t>2026-02-18T08:59:45</t>
         </is>
       </c>
       <c r="O213" t="inlineStr">
@@ -14945,7 +14940,7 @@
       </c>
       <c r="N215" t="inlineStr">
         <is>
-          <t>2026-02-18T07:20:26</t>
+          <t>2026-02-18T09:02:03</t>
         </is>
       </c>
       <c r="O215" t="inlineStr">
@@ -15011,7 +15006,7 @@
       </c>
       <c r="N216" t="inlineStr">
         <is>
-          <t>2026-02-18T07:20:25</t>
+          <t>2026-02-18T09:14:36</t>
         </is>
       </c>
       <c r="O216" t="inlineStr">
@@ -15077,7 +15072,7 @@
       </c>
       <c r="N217" t="inlineStr">
         <is>
-          <t>2026-02-18T07:20:28</t>
+          <t>2026-02-18T09:15:19</t>
         </is>
       </c>
       <c r="O217" t="inlineStr">
@@ -15143,7 +15138,7 @@
       </c>
       <c r="N218" t="inlineStr">
         <is>
-          <t>2026-02-14T14:31:04</t>
+          <t>2026-02-18T09:01:14</t>
         </is>
       </c>
       <c r="O218" t="inlineStr">
@@ -15209,7 +15204,7 @@
       </c>
       <c r="N219" t="inlineStr">
         <is>
-          <t>2026-02-18T07:20:59</t>
+          <t>2026-02-18T09:19:58</t>
         </is>
       </c>
       <c r="O219" t="inlineStr">
@@ -15280,7 +15275,7 @@
       </c>
       <c r="N220" t="inlineStr">
         <is>
-          <t>2026-02-18T07:36:57</t>
+          <t>2026-02-18T09:06:20</t>
         </is>
       </c>
       <c r="O220" t="inlineStr">
@@ -15478,7 +15473,7 @@
       </c>
       <c r="N223" t="inlineStr">
         <is>
-          <t>2026-02-13T19:24:57</t>
+          <t>2026-02-18T09:14:22</t>
         </is>
       </c>
       <c r="O223" t="inlineStr">
@@ -15610,7 +15605,7 @@
       </c>
       <c r="N225" t="inlineStr">
         <is>
-          <t>2026-02-18T07:24:03</t>
+          <t>2026-02-18T09:14:27</t>
         </is>
       </c>
       <c r="O225" t="inlineStr">
@@ -15676,7 +15671,7 @@
       </c>
       <c r="N226" t="inlineStr">
         <is>
-          <t>2026-02-14T14:55:20</t>
+          <t>2026-02-18T08:52:41</t>
         </is>
       </c>
       <c r="O226" t="inlineStr">
@@ -15742,7 +15737,7 @@
       </c>
       <c r="N227" t="inlineStr">
         <is>
-          <t>2026-02-14T14:16:07</t>
+          <t>2026-02-18T08:56:27</t>
         </is>
       </c>
       <c r="O227" t="inlineStr">
@@ -15940,7 +15935,7 @@
       </c>
       <c r="N230" t="inlineStr">
         <is>
-          <t>2026-02-18T07:27:09</t>
+          <t>2026-02-18T09:17:05</t>
         </is>
       </c>
       <c r="O230" t="inlineStr">
@@ -16006,7 +16001,7 @@
       </c>
       <c r="N231" t="inlineStr">
         <is>
-          <t>2026-02-13T19:10:03</t>
+          <t>2026-02-18T09:41:33</t>
         </is>
       </c>
       <c r="O231" t="inlineStr">
@@ -16072,7 +16067,7 @@
       </c>
       <c r="N232" t="inlineStr">
         <is>
-          <t>2026-02-14T13:38:44</t>
+          <t>2026-02-18T08:54:22</t>
         </is>
       </c>
       <c r="O232" t="inlineStr">
@@ -16138,7 +16133,7 @@
       </c>
       <c r="N233" t="inlineStr">
         <is>
-          <t>2026-02-13T19:14:47</t>
+          <t>2026-02-18T09:21:09</t>
         </is>
       </c>
       <c r="O233" t="inlineStr">
@@ -16468,7 +16463,7 @@
       </c>
       <c r="N238" t="inlineStr">
         <is>
-          <t>2026-02-13T19:08:06</t>
+          <t>2026-02-18T08:59:51</t>
         </is>
       </c>
       <c r="O238" t="inlineStr">
@@ -16534,7 +16529,7 @@
       </c>
       <c r="N239" t="inlineStr">
         <is>
-          <t>2026-02-14T14:33:49</t>
+          <t>2026-02-18T09:21:57</t>
         </is>
       </c>
       <c r="O239" t="inlineStr">
@@ -16600,7 +16595,7 @@
       </c>
       <c r="N240" t="inlineStr">
         <is>
-          <t>2026-02-14T09:04:41</t>
+          <t>2026-02-18T09:20:14</t>
         </is>
       </c>
       <c r="O240" t="inlineStr">
@@ -16666,7 +16661,7 @@
       </c>
       <c r="N241" t="inlineStr">
         <is>
-          <t>2026-02-18T07:32:40</t>
+          <t>2026-02-18T09:23:56</t>
         </is>
       </c>
       <c r="O241" t="inlineStr">
@@ -16732,7 +16727,7 @@
       </c>
       <c r="N242" t="inlineStr">
         <is>
-          <t>2026-02-18T07:32:41</t>
+          <t>2026-02-18T09:26:38</t>
         </is>
       </c>
       <c r="O242" t="inlineStr">
@@ -16798,7 +16793,7 @@
       </c>
       <c r="N243" t="inlineStr">
         <is>
-          <t>2026-02-18T06:57:10</t>
+          <t>2026-02-18T09:39:50</t>
         </is>
       </c>
       <c r="O243" t="inlineStr">
@@ -16818,11 +16813,6 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
-      <c r="C244" t="inlineStr">
-        <is>
-          <t>10.69.5.112</t>
-        </is>
-      </c>
       <c r="D244" t="n">
         <v>2019</v>
       </c>
@@ -16930,7 +16920,7 @@
       </c>
       <c r="N245" t="inlineStr">
         <is>
-          <t>2026-02-18T07:22:06</t>
+          <t>2026-02-18T09:16:17</t>
         </is>
       </c>
       <c r="O245" t="inlineStr">
@@ -16996,7 +16986,7 @@
       </c>
       <c r="N246" t="inlineStr">
         <is>
-          <t>2026-02-18T07:22:19</t>
+          <t>2026-02-18T09:10:32</t>
         </is>
       </c>
       <c r="O246" t="inlineStr">
@@ -17062,7 +17052,7 @@
       </c>
       <c r="N247" t="inlineStr">
         <is>
-          <t>2026-02-18T07:21:36</t>
+          <t>2026-02-18T09:16:55</t>
         </is>
       </c>
       <c r="O247" t="inlineStr">
@@ -17128,7 +17118,7 @@
       </c>
       <c r="N248" t="inlineStr">
         <is>
-          <t>2026-02-18T07:21:19</t>
+          <t>2026-02-18T09:14:38</t>
         </is>
       </c>
       <c r="O248" t="inlineStr">
@@ -17194,7 +17184,7 @@
       </c>
       <c r="N249" t="inlineStr">
         <is>
-          <t>2026-02-18T07:21:36</t>
+          <t>2026-02-18T09:11:04</t>
         </is>
       </c>
       <c r="O249" t="inlineStr">
@@ -17255,7 +17245,7 @@
       </c>
       <c r="N250" t="inlineStr">
         <is>
-          <t>2026-02-18T07:22:04</t>
+          <t>2026-02-18T09:08:30</t>
         </is>
       </c>
       <c r="O250" t="inlineStr">
@@ -17321,7 +17311,7 @@
       </c>
       <c r="N251" t="inlineStr">
         <is>
-          <t>2026-02-18T07:21:57</t>
+          <t>2026-02-18T08:10:50</t>
         </is>
       </c>
       <c r="O251" t="inlineStr">
@@ -17387,7 +17377,7 @@
       </c>
       <c r="N252" t="inlineStr">
         <is>
-          <t>2026-02-18T07:21:46</t>
+          <t>2026-02-18T09:19:14</t>
         </is>
       </c>
       <c r="O252" t="inlineStr">
@@ -17453,7 +17443,7 @@
       </c>
       <c r="N253" t="inlineStr">
         <is>
-          <t>2026-02-18T07:25:59</t>
+          <t>2026-02-18T09:19:49</t>
         </is>
       </c>
       <c r="O253" t="inlineStr">
@@ -17513,7 +17503,7 @@
       </c>
       <c r="N254" t="inlineStr">
         <is>
-          <t>2026-02-18T07:27:59</t>
+          <t>2026-02-18T09:17:22</t>
         </is>
       </c>
       <c r="O254" t="inlineStr">
@@ -17579,7 +17569,7 @@
       </c>
       <c r="N255" t="inlineStr">
         <is>
-          <t>2026-02-14T11:45:08</t>
+          <t>2026-02-18T09:22:00</t>
         </is>
       </c>
       <c r="O255" t="inlineStr">
@@ -17645,7 +17635,7 @@
       </c>
       <c r="N256" t="inlineStr">
         <is>
-          <t>2026-02-18T07:35:49</t>
+          <t>2026-02-18T09:33:27</t>
         </is>
       </c>
       <c r="O256" t="inlineStr">
@@ -17777,7 +17767,7 @@
       </c>
       <c r="N258" t="inlineStr">
         <is>
-          <t>2026-02-14T14:07:10</t>
+          <t>2026-02-18T09:03:13</t>
         </is>
       </c>
       <c r="O258" t="inlineStr">
@@ -17843,7 +17833,7 @@
       </c>
       <c r="N259" t="inlineStr">
         <is>
-          <t>2026-02-18T07:26:39</t>
+          <t>2026-02-18T09:11:02</t>
         </is>
       </c>
       <c r="O259" t="inlineStr">
@@ -17909,7 +17899,7 @@
       </c>
       <c r="N260" t="inlineStr">
         <is>
-          <t>2026-02-18T07:36:34</t>
+          <t>2026-02-18T09:23:35</t>
         </is>
       </c>
       <c r="O260" t="inlineStr">
@@ -17975,7 +17965,7 @@
       </c>
       <c r="N261" t="inlineStr">
         <is>
-          <t>2026-02-14T14:08:25</t>
+          <t>2026-02-18T08:54:43</t>
         </is>
       </c>
       <c r="O261" t="inlineStr">
@@ -18041,7 +18031,7 @@
       </c>
       <c r="N262" t="inlineStr">
         <is>
-          <t>2026-02-14T11:16:15</t>
+          <t>2026-02-18T08:48:30</t>
         </is>
       </c>
       <c r="O262" t="inlineStr">
@@ -18107,7 +18097,7 @@
       </c>
       <c r="N263" t="inlineStr">
         <is>
-          <t>2026-02-14T14:13:29</t>
+          <t>2026-02-18T08:55:15</t>
         </is>
       </c>
       <c r="O263" t="inlineStr">
@@ -18173,7 +18163,7 @@
       </c>
       <c r="N264" t="inlineStr">
         <is>
-          <t>2026-02-18T07:37:49</t>
+          <t>2026-02-18T09:36:43</t>
         </is>
       </c>
       <c r="O264" t="inlineStr">
@@ -18239,7 +18229,7 @@
       </c>
       <c r="N265" t="inlineStr">
         <is>
-          <t>2026-02-14T14:08:33</t>
+          <t>2026-02-18T09:37:09</t>
         </is>
       </c>
       <c r="O265" t="inlineStr">
@@ -18305,7 +18295,7 @@
       </c>
       <c r="N266" t="inlineStr">
         <is>
-          <t>2026-02-14T14:12:12</t>
+          <t>2026-02-18T09:05:19</t>
         </is>
       </c>
       <c r="O266" t="inlineStr">
@@ -18371,7 +18361,7 @@
       </c>
       <c r="N267" t="inlineStr">
         <is>
-          <t>2026-02-14T14:20:14</t>
+          <t>2026-02-18T09:00:45</t>
         </is>
       </c>
       <c r="O267" t="inlineStr">
@@ -18437,7 +18427,7 @@
       </c>
       <c r="N268" t="inlineStr">
         <is>
-          <t>2026-02-14T20:18:54</t>
+          <t>2026-02-18T08:59:23</t>
         </is>
       </c>
       <c r="O268" t="inlineStr">
@@ -18503,7 +18493,7 @@
       </c>
       <c r="N269" t="inlineStr">
         <is>
-          <t>2026-02-14T11:16:09</t>
+          <t>2026-02-18T09:30:15</t>
         </is>
       </c>
       <c r="O269" t="inlineStr">
@@ -18566,7 +18556,7 @@
       </c>
       <c r="N270" t="inlineStr">
         <is>
-          <t>2026-02-18T07:02:07</t>
+          <t>2026-02-18T08:56:37</t>
         </is>
       </c>
       <c r="O270" t="inlineStr">
@@ -18698,7 +18688,7 @@
       </c>
       <c r="N272" t="inlineStr">
         <is>
-          <t>2026-02-14T14:52:39</t>
+          <t>2026-02-18T09:01:35</t>
         </is>
       </c>
       <c r="O272" t="inlineStr">
@@ -18764,7 +18754,7 @@
       </c>
       <c r="N273" t="inlineStr">
         <is>
-          <t>2026-02-14T12:58:08</t>
+          <t>2026-02-18T09:18:40</t>
         </is>
       </c>
       <c r="O273" t="inlineStr">
@@ -19094,7 +19084,7 @@
       </c>
       <c r="N278" t="inlineStr">
         <is>
-          <t>2026-02-18T07:23:35</t>
+          <t>2026-02-18T09:17:21</t>
         </is>
       </c>
       <c r="O278" t="inlineStr">
@@ -19226,7 +19216,7 @@
       </c>
       <c r="N280" t="inlineStr">
         <is>
-          <t>2026-02-14T09:59:02</t>
+          <t>2026-02-18T09:30:30</t>
         </is>
       </c>
       <c r="O280" t="inlineStr">
@@ -19312,11 +19302,6 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
-      <c r="C282" t="inlineStr">
-        <is>
-          <t>10.69.5.151</t>
-        </is>
-      </c>
       <c r="D282" t="n">
         <v>2017</v>
       </c>
@@ -19358,7 +19343,7 @@
       </c>
       <c r="N282" t="inlineStr">
         <is>
-          <t>2026-02-18T07:32:04</t>
+          <t>2026-02-18T09:16:28</t>
         </is>
       </c>
       <c r="O282" t="inlineStr">
@@ -19424,7 +19409,7 @@
       </c>
       <c r="N283" t="inlineStr">
         <is>
-          <t>2026-02-14T14:00:49</t>
+          <t>2026-02-18T09:05:23</t>
         </is>
       </c>
       <c r="O283" t="inlineStr">
@@ -19490,7 +19475,7 @@
       </c>
       <c r="N284" t="inlineStr">
         <is>
-          <t>2026-02-14T14:36:32</t>
+          <t>2026-02-18T09:40:15</t>
         </is>
       </c>
       <c r="O284" t="inlineStr">
@@ -19556,7 +19541,7 @@
       </c>
       <c r="N285" t="inlineStr">
         <is>
-          <t>2026-02-14T14:16:15</t>
+          <t>2026-02-18T09:37:06</t>
         </is>
       </c>
       <c r="O285" t="inlineStr">
@@ -19576,6 +19561,11 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>10.69.5.155</t>
+        </is>
+      </c>
       <c r="D286" t="n">
         <v>2019</v>
       </c>
@@ -19617,7 +19607,7 @@
       </c>
       <c r="N286" t="inlineStr">
         <is>
-          <t>2026-02-13T08:34:30</t>
+          <t>2026-02-18T08:56:50</t>
         </is>
       </c>
       <c r="O286" t="inlineStr">
@@ -19683,7 +19673,7 @@
       </c>
       <c r="N287" t="inlineStr">
         <is>
-          <t>2026-02-18T07:26:11</t>
+          <t>2026-02-18T09:16:58</t>
         </is>
       </c>
       <c r="O287" t="inlineStr">
@@ -19749,7 +19739,7 @@
       </c>
       <c r="N288" t="inlineStr">
         <is>
-          <t>2026-02-18T07:15:10</t>
+          <t>2026-02-18T09:06:02</t>
         </is>
       </c>
       <c r="O288" t="inlineStr">
@@ -19815,7 +19805,7 @@
       </c>
       <c r="N289" t="inlineStr">
         <is>
-          <t>2026-02-13T20:45:49</t>
+          <t>2026-02-18T09:31:32</t>
         </is>
       </c>
       <c r="O289" t="inlineStr">
@@ -20635,7 +20625,7 @@
       </c>
       <c r="N302" t="inlineStr">
         <is>
-          <t>2026-02-18T07:26:46</t>
+          <t>2026-02-18T09:19:23</t>
         </is>
       </c>
       <c r="O302" t="inlineStr">
@@ -21400,7 +21390,7 @@
       </c>
       <c r="N314" t="inlineStr">
         <is>
-          <t>2026-02-18T06:42:42</t>
+          <t>2026-02-18T09:37:59</t>
         </is>
       </c>
       <c r="O314" t="inlineStr">
@@ -21787,7 +21777,7 @@
       </c>
       <c r="N320" t="inlineStr">
         <is>
-          <t>2026-02-18T07:06:15</t>
+          <t>2026-02-18T09:02:48</t>
         </is>
       </c>
       <c r="O320" t="inlineStr">
@@ -22536,7 +22526,7 @@
       </c>
       <c r="N332" t="inlineStr">
         <is>
-          <t>2026-02-14T06:42:20</t>
+          <t>2026-02-18T08:59:45</t>
         </is>
       </c>
       <c r="O332" t="inlineStr">
@@ -22602,7 +22592,7 @@
       </c>
       <c r="N333" t="inlineStr">
         <is>
-          <t>2026-02-18T07:37:40</t>
+          <t>2026-02-18T09:26:02</t>
         </is>
       </c>
       <c r="O333" t="inlineStr">
@@ -22668,7 +22658,7 @@
       </c>
       <c r="N334" t="inlineStr">
         <is>
-          <t>2026-02-18T07:41:22</t>
+          <t>2026-02-18T09:39:31</t>
         </is>
       </c>
       <c r="O334" t="inlineStr">
@@ -22734,7 +22724,7 @@
       </c>
       <c r="N335" t="inlineStr">
         <is>
-          <t>2026-02-18T06:46:01</t>
+          <t>2026-02-18T09:28:53</t>
         </is>
       </c>
       <c r="O335" t="inlineStr">
@@ -22800,7 +22790,7 @@
       </c>
       <c r="N336" t="inlineStr">
         <is>
-          <t>2026-02-18T06:45:20</t>
+          <t>2026-02-18T09:39:55</t>
         </is>
       </c>
       <c r="O336" t="inlineStr">
@@ -22866,7 +22856,7 @@
       </c>
       <c r="N337" t="inlineStr">
         <is>
-          <t>2026-02-18T06:47:09</t>
+          <t>2026-02-18T09:36:16</t>
         </is>
       </c>
       <c r="O337" t="inlineStr">
@@ -22932,7 +22922,7 @@
       </c>
       <c r="N338" t="inlineStr">
         <is>
-          <t>2026-02-18T07:38:05</t>
+          <t>2026-02-18T09:29:08</t>
         </is>
       </c>
       <c r="O338" t="inlineStr">
@@ -22998,7 +22988,7 @@
       </c>
       <c r="N339" t="inlineStr">
         <is>
-          <t>2026-02-18T07:07:14</t>
+          <t>2026-02-18T09:05:39</t>
         </is>
       </c>
       <c r="O339" t="inlineStr">
@@ -23130,7 +23120,7 @@
       </c>
       <c r="N341" t="inlineStr">
         <is>
-          <t>2026-02-14T12:17:42</t>
+          <t>2026-02-18T09:02:01</t>
         </is>
       </c>
       <c r="O341" t="inlineStr">
@@ -23196,7 +23186,7 @@
       </c>
       <c r="N342" t="inlineStr">
         <is>
-          <t>2026-02-14T12:00:44</t>
+          <t>2026-02-18T09:42:25</t>
         </is>
       </c>
       <c r="O342" t="inlineStr">
@@ -23216,6 +23206,11 @@
           <t>OPERACAO 9.1</t>
         </is>
       </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>10.69.5.237</t>
+        </is>
+      </c>
       <c r="D343" t="n">
         <v>2017</v>
       </c>
@@ -23259,7 +23254,7 @@
       </c>
       <c r="N343" t="inlineStr">
         <is>
-          <t>2026-02-13T17:35:51</t>
+          <t>2026-02-18T09:24:31</t>
         </is>
       </c>
       <c r="O343" t="inlineStr">
@@ -23848,7 +23843,7 @@
       </c>
       <c r="N352" t="inlineStr">
         <is>
-          <t>2026-02-18T06:47:01</t>
+          <t>2026-02-18T09:38:01</t>
         </is>
       </c>
       <c r="O352" t="inlineStr">
@@ -24688,7 +24683,7 @@
       </c>
       <c r="N365" t="inlineStr">
         <is>
-          <t>2026-02-18T07:39:40</t>
+          <t>2026-02-18T09:28:27</t>
         </is>
       </c>
       <c r="O365" t="inlineStr">
@@ -24756,7 +24751,7 @@
       </c>
       <c r="N366" t="inlineStr">
         <is>
-          <t>2026-02-18T06:53:25</t>
+          <t>2026-02-18T09:35:24</t>
         </is>
       </c>
       <c r="O366" t="inlineStr">
@@ -24886,7 +24881,7 @@
       </c>
       <c r="N368" t="inlineStr">
         <is>
-          <t>2026-02-13T15:54:38</t>
+          <t>2026-02-18T08:52:28</t>
         </is>
       </c>
       <c r="O368" t="inlineStr">
@@ -24906,6 +24901,11 @@
           <t>RH</t>
         </is>
       </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>10.69.3.13</t>
+        </is>
+      </c>
       <c r="D369" t="n">
         <v>2025</v>
       </c>
@@ -24949,7 +24949,7 @@
       </c>
       <c r="N369" t="inlineStr">
         <is>
-          <t>2026-02-13T15:49:56</t>
+          <t>2026-02-18T09:27:24</t>
         </is>
       </c>
       <c r="O369" t="inlineStr">
@@ -25020,7 +25020,7 @@
       </c>
       <c r="N370" t="inlineStr">
         <is>
-          <t>2026-02-13T15:41:54</t>
+          <t>2026-02-18T09:18:19</t>
         </is>
       </c>
       <c r="O370" t="inlineStr">
@@ -25162,7 +25162,7 @@
       </c>
       <c r="N372" t="inlineStr">
         <is>
-          <t>2026-02-13T15:42:20</t>
+          <t>2026-02-18T08:56:33</t>
         </is>
       </c>
       <c r="O372" t="inlineStr">
@@ -25372,7 +25372,7 @@
       </c>
       <c r="N375" t="inlineStr">
         <is>
-          <t>2026-02-18T07:20:31</t>
+          <t>2026-02-18T09:14:58</t>
         </is>
       </c>
       <c r="O375" t="inlineStr">
@@ -25509,7 +25509,7 @@
       </c>
       <c r="N377" t="inlineStr">
         <is>
-          <t>2026-02-13T16:30:25</t>
+          <t>2026-02-18T09:37:52</t>
         </is>
       </c>
       <c r="O377" t="inlineStr">
@@ -25580,7 +25580,7 @@
       </c>
       <c r="N378" t="inlineStr">
         <is>
-          <t>2026-02-18T06:44:05</t>
+          <t>2026-02-18T09:39:46</t>
         </is>
       </c>
       <c r="O378" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática 2026-02-18 11:52:08.301265
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -601,7 +601,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>2026-02-18T09:40:28</t>
+          <t>2026-02-18T11:25:09</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -672,7 +672,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>2026-02-18T09:06:32</t>
+          <t>2026-02-18T10:54:27</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -814,7 +814,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>2026-02-18T09:22:14</t>
+          <t>2026-02-18T11:03:05</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -1144,7 +1144,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>2026-02-18T09:14:46</t>
+          <t>2026-02-18T11:04:18</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -1474,7 +1474,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>2026-02-18T09:12:12</t>
+          <t>2026-02-18T11:03:40</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
@@ -1606,7 +1606,7 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>2026-02-18T09:20:11</t>
+          <t>2026-02-18T11:16:53</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
@@ -6885,7 +6885,7 @@
       </c>
       <c r="N95" t="inlineStr">
         <is>
-          <t>2026-02-18T09:18:41</t>
+          <t>2026-02-18T11:04:18</t>
         </is>
       </c>
       <c r="O95" t="inlineStr">
@@ -6956,7 +6956,7 @@
       </c>
       <c r="N96" t="inlineStr">
         <is>
-          <t>2026-02-14T14:45:18</t>
+          <t>2026-02-18T10:54:46</t>
         </is>
       </c>
       <c r="O96" t="inlineStr">
@@ -7022,7 +7022,7 @@
       </c>
       <c r="N97" t="inlineStr">
         <is>
-          <t>2026-02-18T09:27:14</t>
+          <t>2026-02-18T11:11:12</t>
         </is>
       </c>
       <c r="O97" t="inlineStr">
@@ -7088,7 +7088,7 @@
       </c>
       <c r="N98" t="inlineStr">
         <is>
-          <t>2026-02-18T08:50:00</t>
+          <t>2026-02-18T11:35:10</t>
         </is>
       </c>
       <c r="O98" t="inlineStr">
@@ -7159,7 +7159,7 @@
       </c>
       <c r="N99" t="inlineStr">
         <is>
-          <t>2026-02-18T09:34:45</t>
+          <t>2026-02-18T11:26:48</t>
         </is>
       </c>
       <c r="O99" t="inlineStr">
@@ -7230,7 +7230,7 @@
       </c>
       <c r="N100" t="inlineStr">
         <is>
-          <t>2026-02-18T08:55:59</t>
+          <t>2026-02-18T10:55:24</t>
         </is>
       </c>
       <c r="O100" t="inlineStr">
@@ -7301,7 +7301,7 @@
       </c>
       <c r="N101" t="inlineStr">
         <is>
-          <t>2026-02-18T08:59:04</t>
+          <t>2026-02-18T11:34:08</t>
         </is>
       </c>
       <c r="O101" t="inlineStr">
@@ -7443,7 +7443,7 @@
       </c>
       <c r="N103" t="inlineStr">
         <is>
-          <t>2026-02-18T09:00:43</t>
+          <t>2026-02-18T10:52:02</t>
         </is>
       </c>
       <c r="O103" t="inlineStr">
@@ -7708,7 +7708,7 @@
       </c>
       <c r="N107" t="inlineStr">
         <is>
-          <t>2026-02-18T09:18:18</t>
+          <t>2026-02-18T11:17:18</t>
         </is>
       </c>
       <c r="O107" t="inlineStr">
@@ -7850,7 +7850,7 @@
       </c>
       <c r="N109" t="inlineStr">
         <is>
-          <t>2026-02-18T08:54:16</t>
+          <t>2026-02-18T10:51:52</t>
         </is>
       </c>
       <c r="O109" t="inlineStr">
@@ -7921,7 +7921,7 @@
       </c>
       <c r="N110" t="inlineStr">
         <is>
-          <t>2026-02-18T08:59:35</t>
+          <t>2026-02-18T10:51:58</t>
         </is>
       </c>
       <c r="O110" t="inlineStr">
@@ -7992,7 +7992,7 @@
       </c>
       <c r="N111" t="inlineStr">
         <is>
-          <t>2026-02-18T08:53:23</t>
+          <t>2026-02-18T10:45:41</t>
         </is>
       </c>
       <c r="O111" t="inlineStr">
@@ -8063,7 +8063,7 @@
       </c>
       <c r="N112" t="inlineStr">
         <is>
-          <t>2026-02-18T09:42:23</t>
+          <t>2026-02-18T11:27:19</t>
         </is>
       </c>
       <c r="O112" t="inlineStr">
@@ -8134,7 +8134,7 @@
       </c>
       <c r="N113" t="inlineStr">
         <is>
-          <t>2026-02-18T09:39:03</t>
+          <t>2026-02-18T11:31:32</t>
         </is>
       </c>
       <c r="O113" t="inlineStr">
@@ -8205,7 +8205,7 @@
       </c>
       <c r="N114" t="inlineStr">
         <is>
-          <t>2026-02-18T09:38:21</t>
+          <t>2026-02-18T11:35:02</t>
         </is>
       </c>
       <c r="O114" t="inlineStr">
@@ -8273,7 +8273,7 @@
       </c>
       <c r="N115" t="inlineStr">
         <is>
-          <t>2026-02-18T09:09:03</t>
+          <t>2026-02-18T11:01:40</t>
         </is>
       </c>
       <c r="O115" t="inlineStr">
@@ -8344,7 +8344,7 @@
       </c>
       <c r="N116" t="inlineStr">
         <is>
-          <t>2026-02-18T09:02:37</t>
+          <t>2026-02-18T11:40:58</t>
         </is>
       </c>
       <c r="O116" t="inlineStr">
@@ -8364,6 +8364,11 @@
           <t>DP</t>
         </is>
       </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>10.69.3.23</t>
+        </is>
+      </c>
       <c r="D117" t="n">
         <v>2025</v>
       </c>
@@ -8410,7 +8415,7 @@
       </c>
       <c r="N117" t="inlineStr">
         <is>
-          <t>2026-02-18T08:50:54</t>
+          <t>2026-02-18T11:35:14</t>
         </is>
       </c>
       <c r="O117" t="inlineStr">
@@ -8620,7 +8625,7 @@
       </c>
       <c r="N120" t="inlineStr">
         <is>
-          <t>2026-02-18T09:41:44</t>
+          <t>2026-02-18T10:41:55</t>
         </is>
       </c>
       <c r="O120" t="inlineStr">
@@ -8691,7 +8696,7 @@
       </c>
       <c r="N121" t="inlineStr">
         <is>
-          <t>2026-02-13T18:41:48</t>
+          <t>2026-02-18T11:25:30</t>
         </is>
       </c>
       <c r="O121" t="inlineStr">
@@ -8759,7 +8764,7 @@
       </c>
       <c r="N122" t="inlineStr">
         <is>
-          <t>2026-02-18T08:52:16</t>
+          <t>2026-02-18T11:34:26</t>
         </is>
       </c>
       <c r="O122" t="inlineStr">
@@ -8901,7 +8906,7 @@
       </c>
       <c r="N124" t="inlineStr">
         <is>
-          <t>2026-02-18T09:00:43</t>
+          <t>2026-02-18T10:52:24</t>
         </is>
       </c>
       <c r="O124" t="inlineStr">
@@ -8972,7 +8977,7 @@
       </c>
       <c r="N125" t="inlineStr">
         <is>
-          <t>2026-02-18T08:50:29</t>
+          <t>2026-02-18T11:31:38</t>
         </is>
       </c>
       <c r="O125" t="inlineStr">
@@ -9043,7 +9048,7 @@
       </c>
       <c r="N126" t="inlineStr">
         <is>
-          <t>2026-02-18T09:05:31</t>
+          <t>2026-02-18T11:00:36</t>
         </is>
       </c>
       <c r="O126" t="inlineStr">
@@ -9114,7 +9119,7 @@
       </c>
       <c r="N127" t="inlineStr">
         <is>
-          <t>2026-02-18T09:26:15</t>
+          <t>2026-02-18T11:12:07</t>
         </is>
       </c>
       <c r="O127" t="inlineStr">
@@ -9185,7 +9190,7 @@
       </c>
       <c r="N128" t="inlineStr">
         <is>
-          <t>2026-02-18T09:01:38</t>
+          <t>2026-02-18T10:50:35</t>
         </is>
       </c>
       <c r="O128" t="inlineStr">
@@ -9256,7 +9261,7 @@
       </c>
       <c r="N129" t="inlineStr">
         <is>
-          <t>2026-02-14T13:26:31</t>
+          <t>2026-02-18T11:10:05</t>
         </is>
       </c>
       <c r="O129" t="inlineStr">
@@ -9327,7 +9332,7 @@
       </c>
       <c r="N130" t="inlineStr">
         <is>
-          <t>2026-02-18T08:59:04</t>
+          <t>2026-02-18T10:51:04</t>
         </is>
       </c>
       <c r="O130" t="inlineStr">
@@ -9398,7 +9403,7 @@
       </c>
       <c r="N131" t="inlineStr">
         <is>
-          <t>2026-02-18T09:41:12</t>
+          <t>2026-02-18T11:41:03</t>
         </is>
       </c>
       <c r="O131" t="inlineStr">
@@ -9535,7 +9540,7 @@
       </c>
       <c r="N133" t="inlineStr">
         <is>
-          <t>2026-02-18T09:09:57</t>
+          <t>2026-02-18T11:01:22</t>
         </is>
       </c>
       <c r="O133" t="inlineStr">
@@ -9601,7 +9606,7 @@
       </c>
       <c r="N134" t="inlineStr">
         <is>
-          <t>2026-02-18T09:24:40</t>
+          <t>2026-02-18T11:12:30</t>
         </is>
       </c>
       <c r="O134" t="inlineStr">
@@ -9667,7 +9672,7 @@
       </c>
       <c r="N135" t="inlineStr">
         <is>
-          <t>2026-02-18T09:07:13</t>
+          <t>2026-02-18T10:54:58</t>
         </is>
       </c>
       <c r="O135" t="inlineStr">
@@ -9864,7 +9869,7 @@
       </c>
       <c r="N138" t="inlineStr">
         <is>
-          <t>2026-02-18T08:58:13</t>
+          <t>2026-02-18T11:39:34</t>
         </is>
       </c>
       <c r="O138" t="inlineStr">
@@ -9930,7 +9935,7 @@
       </c>
       <c r="N139" t="inlineStr">
         <is>
-          <t>2026-02-18T08:53:39</t>
+          <t>2026-02-18T11:35:08</t>
         </is>
       </c>
       <c r="O139" t="inlineStr">
@@ -9996,7 +10001,7 @@
       </c>
       <c r="N140" t="inlineStr">
         <is>
-          <t>2026-02-18T09:25:28</t>
+          <t>2026-02-18T11:20:56</t>
         </is>
       </c>
       <c r="O140" t="inlineStr">
@@ -10062,7 +10067,7 @@
       </c>
       <c r="N141" t="inlineStr">
         <is>
-          <t>2026-02-18T09:00:29</t>
+          <t>2026-02-18T10:53:16</t>
         </is>
       </c>
       <c r="O141" t="inlineStr">
@@ -10260,7 +10265,7 @@
       </c>
       <c r="N144" t="inlineStr">
         <is>
-          <t>2026-02-14T14:05:23</t>
+          <t>2026-02-18T11:15:05</t>
         </is>
       </c>
       <c r="O144" t="inlineStr">
@@ -10326,7 +10331,7 @@
       </c>
       <c r="N145" t="inlineStr">
         <is>
-          <t>2026-02-14T14:15:55</t>
+          <t>2026-02-18T11:12:32</t>
         </is>
       </c>
       <c r="O145" t="inlineStr">
@@ -10392,7 +10397,7 @@
       </c>
       <c r="N146" t="inlineStr">
         <is>
-          <t>2026-02-18T08:53:02</t>
+          <t>2026-02-18T10:53:58</t>
         </is>
       </c>
       <c r="O146" t="inlineStr">
@@ -10458,7 +10463,7 @@
       </c>
       <c r="N147" t="inlineStr">
         <is>
-          <t>2026-02-18T08:58:13</t>
+          <t>2026-02-18T11:38:30</t>
         </is>
       </c>
       <c r="O147" t="inlineStr">
@@ -10524,7 +10529,7 @@
       </c>
       <c r="N148" t="inlineStr">
         <is>
-          <t>2026-02-18T09:27:43</t>
+          <t>2026-02-18T11:18:29</t>
         </is>
       </c>
       <c r="O148" t="inlineStr">
@@ -10722,7 +10727,7 @@
       </c>
       <c r="N151" t="inlineStr">
         <is>
-          <t>2026-02-18T09:38:27</t>
+          <t>2026-02-18T11:32:33</t>
         </is>
       </c>
       <c r="O151" t="inlineStr">
@@ -10788,7 +10793,7 @@
       </c>
       <c r="N152" t="inlineStr">
         <is>
-          <t>2026-02-18T09:08:34</t>
+          <t>2026-02-18T11:00:30</t>
         </is>
       </c>
       <c r="O152" t="inlineStr">
@@ -10849,7 +10854,7 @@
       </c>
       <c r="N153" t="inlineStr">
         <is>
-          <t>2026-02-18T09:06:39</t>
+          <t>2026-02-18T10:57:06</t>
         </is>
       </c>
       <c r="O153" t="inlineStr">
@@ -10915,7 +10920,7 @@
       </c>
       <c r="N154" t="inlineStr">
         <is>
-          <t>2026-02-18T09:31:04</t>
+          <t>2026-02-18T11:18:06</t>
         </is>
       </c>
       <c r="O154" t="inlineStr">
@@ -10981,7 +10986,7 @@
       </c>
       <c r="N155" t="inlineStr">
         <is>
-          <t>2026-02-18T09:07:15</t>
+          <t>2026-02-18T10:57:00</t>
         </is>
       </c>
       <c r="O155" t="inlineStr">
@@ -11113,7 +11118,7 @@
       </c>
       <c r="N157" t="inlineStr">
         <is>
-          <t>2026-02-18T08:59:07</t>
+          <t>2026-02-18T10:53:52</t>
         </is>
       </c>
       <c r="O157" t="inlineStr">
@@ -11146,7 +11151,7 @@
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>Microsoft Windows 8.1 Pro</t>
+          <t>Windows</t>
         </is>
       </c>
       <c r="G158" t="inlineStr">
@@ -11179,7 +11184,7 @@
       </c>
       <c r="N158" t="inlineStr">
         <is>
-          <t>2026-02-18T08:39:38</t>
+          <t>2026-02-18T10:51:43</t>
         </is>
       </c>
       <c r="O158" t="inlineStr">
@@ -11245,7 +11250,7 @@
       </c>
       <c r="N159" t="inlineStr">
         <is>
-          <t>2026-02-18T09:35:52</t>
+          <t>2026-02-18T11:27:29</t>
         </is>
       </c>
       <c r="O159" t="inlineStr">
@@ -11311,7 +11316,7 @@
       </c>
       <c r="N160" t="inlineStr">
         <is>
-          <t>2026-02-18T09:21:05</t>
+          <t>2026-02-18T11:04:56</t>
         </is>
       </c>
       <c r="O160" t="inlineStr">
@@ -11377,7 +11382,7 @@
       </c>
       <c r="N161" t="inlineStr">
         <is>
-          <t>2026-02-18T08:53:46</t>
+          <t>2026-02-18T11:42:01</t>
         </is>
       </c>
       <c r="O161" t="inlineStr">
@@ -11443,7 +11448,7 @@
       </c>
       <c r="N162" t="inlineStr">
         <is>
-          <t>2026-02-18T09:23:40</t>
+          <t>2026-02-18T11:16:44</t>
         </is>
       </c>
       <c r="O162" t="inlineStr">
@@ -11575,7 +11580,7 @@
       </c>
       <c r="N164" t="inlineStr">
         <is>
-          <t>2026-02-18T08:56:56</t>
+          <t>2026-02-18T10:50:07</t>
         </is>
       </c>
       <c r="O164" t="inlineStr">
@@ -11641,7 +11646,7 @@
       </c>
       <c r="N165" t="inlineStr">
         <is>
-          <t>2026-02-18T09:42:04</t>
+          <t>2026-02-18T11:34:08</t>
         </is>
       </c>
       <c r="O165" t="inlineStr">
@@ -11707,7 +11712,7 @@
       </c>
       <c r="N166" t="inlineStr">
         <is>
-          <t>2026-02-18T09:06:38</t>
+          <t>2026-02-18T11:04:50</t>
         </is>
       </c>
       <c r="O166" t="inlineStr">
@@ -11773,7 +11778,7 @@
       </c>
       <c r="N167" t="inlineStr">
         <is>
-          <t>2026-02-18T09:42:22</t>
+          <t>2026-02-18T11:30:38</t>
         </is>
       </c>
       <c r="O167" t="inlineStr">
@@ -11839,7 +11844,7 @@
       </c>
       <c r="N168" t="inlineStr">
         <is>
-          <t>2026-02-18T09:10:50</t>
+          <t>2026-02-18T11:04:30</t>
         </is>
       </c>
       <c r="O168" t="inlineStr">
@@ -11905,7 +11910,7 @@
       </c>
       <c r="N169" t="inlineStr">
         <is>
-          <t>2026-02-18T09:06:17</t>
+          <t>2026-02-18T10:56:41</t>
         </is>
       </c>
       <c r="O169" t="inlineStr">
@@ -11971,7 +11976,7 @@
       </c>
       <c r="N170" t="inlineStr">
         <is>
-          <t>2026-02-18T08:58:09</t>
+          <t>2026-02-18T10:43:25</t>
         </is>
       </c>
       <c r="O170" t="inlineStr">
@@ -12037,7 +12042,7 @@
       </c>
       <c r="N171" t="inlineStr">
         <is>
-          <t>2026-02-14T09:16:10</t>
+          <t>2026-02-18T11:35:21</t>
         </is>
       </c>
       <c r="O171" t="inlineStr">
@@ -12103,7 +12108,7 @@
       </c>
       <c r="N172" t="inlineStr">
         <is>
-          <t>2026-02-14T12:31:07</t>
+          <t>2026-02-18T11:10:19</t>
         </is>
       </c>
       <c r="O172" t="inlineStr">
@@ -12169,7 +12174,7 @@
       </c>
       <c r="N173" t="inlineStr">
         <is>
-          <t>2026-02-18T09:40:21</t>
+          <t>2026-02-18T11:29:39</t>
         </is>
       </c>
       <c r="O173" t="inlineStr">
@@ -12235,7 +12240,7 @@
       </c>
       <c r="N174" t="inlineStr">
         <is>
-          <t>2026-02-18T08:45:13</t>
+          <t>2026-02-18T10:49:42</t>
         </is>
       </c>
       <c r="O174" t="inlineStr">
@@ -12301,7 +12306,7 @@
       </c>
       <c r="N175" t="inlineStr">
         <is>
-          <t>2026-02-18T09:03:49</t>
+          <t>2026-02-18T10:54:17</t>
         </is>
       </c>
       <c r="O175" t="inlineStr">
@@ -12367,7 +12372,7 @@
       </c>
       <c r="N176" t="inlineStr">
         <is>
-          <t>2026-02-18T09:37:18</t>
+          <t>2026-02-18T11:24:14</t>
         </is>
       </c>
       <c r="O176" t="inlineStr">
@@ -12433,7 +12438,7 @@
       </c>
       <c r="N177" t="inlineStr">
         <is>
-          <t>2026-02-18T09:42:29</t>
+          <t>2026-02-18T11:37:00</t>
         </is>
       </c>
       <c r="O177" t="inlineStr">
@@ -12499,7 +12504,7 @@
       </c>
       <c r="N178" t="inlineStr">
         <is>
-          <t>2026-02-18T09:42:04</t>
+          <t>2026-02-18T11:32:54</t>
         </is>
       </c>
       <c r="O178" t="inlineStr">
@@ -12565,7 +12570,7 @@
       </c>
       <c r="N179" t="inlineStr">
         <is>
-          <t>2026-02-18T09:11:30</t>
+          <t>2026-02-18T10:56:45</t>
         </is>
       </c>
       <c r="O179" t="inlineStr">
@@ -12631,7 +12636,7 @@
       </c>
       <c r="N180" t="inlineStr">
         <is>
-          <t>2026-02-18T09:12:21</t>
+          <t>2026-02-18T11:04:25</t>
         </is>
       </c>
       <c r="O180" t="inlineStr">
@@ -12829,7 +12834,7 @@
       </c>
       <c r="N183" t="inlineStr">
         <is>
-          <t>2026-02-18T09:20:04</t>
+          <t>2026-02-18T11:16:28</t>
         </is>
       </c>
       <c r="O183" t="inlineStr">
@@ -13032,7 +13037,7 @@
       </c>
       <c r="N186" t="inlineStr">
         <is>
-          <t>2026-02-18T08:55:35</t>
+          <t>2026-02-18T11:41:26</t>
         </is>
       </c>
       <c r="O186" t="inlineStr">
@@ -13098,7 +13103,7 @@
       </c>
       <c r="N187" t="inlineStr">
         <is>
-          <t>2026-02-18T09:42:04</t>
+          <t>2026-02-18T11:34:13</t>
         </is>
       </c>
       <c r="O187" t="inlineStr">
@@ -13164,7 +13169,7 @@
       </c>
       <c r="N188" t="inlineStr">
         <is>
-          <t>2026-02-18T08:55:46</t>
+          <t>2026-02-18T11:41:08</t>
         </is>
       </c>
       <c r="O188" t="inlineStr">
@@ -13296,7 +13301,7 @@
       </c>
       <c r="N190" t="inlineStr">
         <is>
-          <t>2026-02-18T09:31:58</t>
+          <t>2026-02-18T11:15:53</t>
         </is>
       </c>
       <c r="O190" t="inlineStr">
@@ -13623,7 +13628,7 @@
       </c>
       <c r="N195" t="inlineStr">
         <is>
-          <t>2026-02-18T08:55:37</t>
+          <t>2026-02-18T10:50:14</t>
         </is>
       </c>
       <c r="O195" t="inlineStr">
@@ -13689,7 +13694,7 @@
       </c>
       <c r="N196" t="inlineStr">
         <is>
-          <t>2026-02-18T08:57:19</t>
+          <t>2026-02-18T10:47:05</t>
         </is>
       </c>
       <c r="O196" t="inlineStr">
@@ -13755,7 +13760,7 @@
       </c>
       <c r="N197" t="inlineStr">
         <is>
-          <t>2026-02-18T08:47:42</t>
+          <t>2026-02-18T11:29:44</t>
         </is>
       </c>
       <c r="O197" t="inlineStr">
@@ -13821,7 +13826,7 @@
       </c>
       <c r="N198" t="inlineStr">
         <is>
-          <t>2026-02-18T09:02:04</t>
+          <t>2026-02-18T10:49:38</t>
         </is>
       </c>
       <c r="O198" t="inlineStr">
@@ -14082,7 +14087,7 @@
       </c>
       <c r="N202" t="inlineStr">
         <is>
-          <t>2026-02-18T08:58:37</t>
+          <t>2026-02-18T10:52:57</t>
         </is>
       </c>
       <c r="O202" t="inlineStr">
@@ -14148,7 +14153,7 @@
       </c>
       <c r="N203" t="inlineStr">
         <is>
-          <t>2026-02-18T09:39:30</t>
+          <t>2026-02-18T11:24:24</t>
         </is>
       </c>
       <c r="O203" t="inlineStr">
@@ -14214,7 +14219,7 @@
       </c>
       <c r="N204" t="inlineStr">
         <is>
-          <t>2026-02-18T09:28:18</t>
+          <t>2026-02-18T11:18:09</t>
         </is>
       </c>
       <c r="O204" t="inlineStr">
@@ -14280,7 +14285,7 @@
       </c>
       <c r="N205" t="inlineStr">
         <is>
-          <t>2026-02-18T09:00:33</t>
+          <t>2026-02-18T10:53:00</t>
         </is>
       </c>
       <c r="O205" t="inlineStr">
@@ -14346,7 +14351,7 @@
       </c>
       <c r="N206" t="inlineStr">
         <is>
-          <t>2026-02-18T08:53:59</t>
+          <t>2026-02-18T11:37:33</t>
         </is>
       </c>
       <c r="O206" t="inlineStr">
@@ -14412,7 +14417,7 @@
       </c>
       <c r="N207" t="inlineStr">
         <is>
-          <t>2026-02-18T09:40:37</t>
+          <t>2026-02-18T11:35:06</t>
         </is>
       </c>
       <c r="O207" t="inlineStr">
@@ -14478,7 +14483,7 @@
       </c>
       <c r="N208" t="inlineStr">
         <is>
-          <t>2026-02-18T09:34:55</t>
+          <t>2026-02-18T11:31:02</t>
         </is>
       </c>
       <c r="O208" t="inlineStr">
@@ -14544,7 +14549,7 @@
       </c>
       <c r="N209" t="inlineStr">
         <is>
-          <t>2026-02-18T08:50:06</t>
+          <t>2026-02-18T10:44:22</t>
         </is>
       </c>
       <c r="O209" t="inlineStr">
@@ -14610,7 +14615,7 @@
       </c>
       <c r="N210" t="inlineStr">
         <is>
-          <t>2026-02-18T08:56:14</t>
+          <t>2026-02-18T11:40:28</t>
         </is>
       </c>
       <c r="O210" t="inlineStr">
@@ -14676,7 +14681,7 @@
       </c>
       <c r="N211" t="inlineStr">
         <is>
-          <t>2026-02-18T09:19:29</t>
+          <t>2026-02-18T11:09:38</t>
         </is>
       </c>
       <c r="O211" t="inlineStr">
@@ -14742,7 +14747,7 @@
       </c>
       <c r="N212" t="inlineStr">
         <is>
-          <t>2026-02-18T09:12:27</t>
+          <t>2026-02-18T11:12:28</t>
         </is>
       </c>
       <c r="O212" t="inlineStr">
@@ -14808,7 +14813,7 @@
       </c>
       <c r="N213" t="inlineStr">
         <is>
-          <t>2026-02-18T08:59:45</t>
+          <t>2026-02-18T10:49:59</t>
         </is>
       </c>
       <c r="O213" t="inlineStr">
@@ -14940,7 +14945,7 @@
       </c>
       <c r="N215" t="inlineStr">
         <is>
-          <t>2026-02-18T09:02:03</t>
+          <t>2026-02-18T10:57:57</t>
         </is>
       </c>
       <c r="O215" t="inlineStr">
@@ -15006,7 +15011,7 @@
       </c>
       <c r="N216" t="inlineStr">
         <is>
-          <t>2026-02-18T09:14:36</t>
+          <t>2026-02-18T11:06:29</t>
         </is>
       </c>
       <c r="O216" t="inlineStr">
@@ -15072,7 +15077,7 @@
       </c>
       <c r="N217" t="inlineStr">
         <is>
-          <t>2026-02-18T09:15:19</t>
+          <t>2026-02-18T10:57:55</t>
         </is>
       </c>
       <c r="O217" t="inlineStr">
@@ -15138,7 +15143,7 @@
       </c>
       <c r="N218" t="inlineStr">
         <is>
-          <t>2026-02-18T09:01:14</t>
+          <t>2026-02-18T10:49:53</t>
         </is>
       </c>
       <c r="O218" t="inlineStr">
@@ -15204,7 +15209,7 @@
       </c>
       <c r="N219" t="inlineStr">
         <is>
-          <t>2026-02-18T09:19:58</t>
+          <t>2026-02-18T11:15:56</t>
         </is>
       </c>
       <c r="O219" t="inlineStr">
@@ -15275,7 +15280,7 @@
       </c>
       <c r="N220" t="inlineStr">
         <is>
-          <t>2026-02-18T09:06:20</t>
+          <t>2026-02-18T10:55:58</t>
         </is>
       </c>
       <c r="O220" t="inlineStr">
@@ -15473,7 +15478,7 @@
       </c>
       <c r="N223" t="inlineStr">
         <is>
-          <t>2026-02-18T09:14:22</t>
+          <t>2026-02-18T11:13:45</t>
         </is>
       </c>
       <c r="O223" t="inlineStr">
@@ -15605,7 +15610,7 @@
       </c>
       <c r="N225" t="inlineStr">
         <is>
-          <t>2026-02-18T09:14:27</t>
+          <t>2026-02-18T11:10:39</t>
         </is>
       </c>
       <c r="O225" t="inlineStr">
@@ -15671,7 +15676,7 @@
       </c>
       <c r="N226" t="inlineStr">
         <is>
-          <t>2026-02-18T08:52:41</t>
+          <t>2026-02-18T10:49:51</t>
         </is>
       </c>
       <c r="O226" t="inlineStr">
@@ -15737,7 +15742,7 @@
       </c>
       <c r="N227" t="inlineStr">
         <is>
-          <t>2026-02-18T08:56:27</t>
+          <t>2026-02-18T11:39:17</t>
         </is>
       </c>
       <c r="O227" t="inlineStr">
@@ -15935,7 +15940,7 @@
       </c>
       <c r="N230" t="inlineStr">
         <is>
-          <t>2026-02-18T09:17:05</t>
+          <t>2026-02-18T11:04:17</t>
         </is>
       </c>
       <c r="O230" t="inlineStr">
@@ -16001,7 +16006,7 @@
       </c>
       <c r="N231" t="inlineStr">
         <is>
-          <t>2026-02-18T09:41:33</t>
+          <t>2026-02-18T11:32:42</t>
         </is>
       </c>
       <c r="O231" t="inlineStr">
@@ -16067,7 +16072,7 @@
       </c>
       <c r="N232" t="inlineStr">
         <is>
-          <t>2026-02-18T08:54:22</t>
+          <t>2026-02-18T11:35:19</t>
         </is>
       </c>
       <c r="O232" t="inlineStr">
@@ -16133,7 +16138,7 @@
       </c>
       <c r="N233" t="inlineStr">
         <is>
-          <t>2026-02-18T09:21:09</t>
+          <t>2026-02-18T11:17:25</t>
         </is>
       </c>
       <c r="O233" t="inlineStr">
@@ -16463,7 +16468,7 @@
       </c>
       <c r="N238" t="inlineStr">
         <is>
-          <t>2026-02-18T08:59:51</t>
+          <t>2026-02-18T11:40:11</t>
         </is>
       </c>
       <c r="O238" t="inlineStr">
@@ -16529,7 +16534,7 @@
       </c>
       <c r="N239" t="inlineStr">
         <is>
-          <t>2026-02-18T09:21:57</t>
+          <t>2026-02-18T11:15:02</t>
         </is>
       </c>
       <c r="O239" t="inlineStr">
@@ -16595,7 +16600,7 @@
       </c>
       <c r="N240" t="inlineStr">
         <is>
-          <t>2026-02-18T09:20:14</t>
+          <t>2026-02-18T11:17:26</t>
         </is>
       </c>
       <c r="O240" t="inlineStr">
@@ -16661,7 +16666,7 @@
       </c>
       <c r="N241" t="inlineStr">
         <is>
-          <t>2026-02-18T09:23:56</t>
+          <t>2026-02-18T11:20:13</t>
         </is>
       </c>
       <c r="O241" t="inlineStr">
@@ -16727,7 +16732,7 @@
       </c>
       <c r="N242" t="inlineStr">
         <is>
-          <t>2026-02-18T09:26:38</t>
+          <t>2026-02-18T11:21:58</t>
         </is>
       </c>
       <c r="O242" t="inlineStr">
@@ -16793,7 +16798,7 @@
       </c>
       <c r="N243" t="inlineStr">
         <is>
-          <t>2026-02-18T09:39:50</t>
+          <t>2026-02-18T11:27:49</t>
         </is>
       </c>
       <c r="O243" t="inlineStr">
@@ -16920,7 +16925,7 @@
       </c>
       <c r="N245" t="inlineStr">
         <is>
-          <t>2026-02-18T09:16:17</t>
+          <t>2026-02-18T11:08:06</t>
         </is>
       </c>
       <c r="O245" t="inlineStr">
@@ -16986,7 +16991,7 @@
       </c>
       <c r="N246" t="inlineStr">
         <is>
-          <t>2026-02-18T09:10:32</t>
+          <t>2026-02-18T11:00:58</t>
         </is>
       </c>
       <c r="O246" t="inlineStr">
@@ -17052,7 +17057,7 @@
       </c>
       <c r="N247" t="inlineStr">
         <is>
-          <t>2026-02-18T09:16:55</t>
+          <t>2026-02-18T11:14:26</t>
         </is>
       </c>
       <c r="O247" t="inlineStr">
@@ -17118,7 +17123,7 @@
       </c>
       <c r="N248" t="inlineStr">
         <is>
-          <t>2026-02-18T09:14:38</t>
+          <t>2026-02-18T11:04:24</t>
         </is>
       </c>
       <c r="O248" t="inlineStr">
@@ -17184,7 +17189,7 @@
       </c>
       <c r="N249" t="inlineStr">
         <is>
-          <t>2026-02-18T09:11:04</t>
+          <t>2026-02-18T11:01:53</t>
         </is>
       </c>
       <c r="O249" t="inlineStr">
@@ -17245,7 +17250,7 @@
       </c>
       <c r="N250" t="inlineStr">
         <is>
-          <t>2026-02-18T09:08:30</t>
+          <t>2026-02-18T11:07:41</t>
         </is>
       </c>
       <c r="O250" t="inlineStr">
@@ -17311,7 +17316,7 @@
       </c>
       <c r="N251" t="inlineStr">
         <is>
-          <t>2026-02-18T08:10:50</t>
+          <t>2026-02-18T11:37:02</t>
         </is>
       </c>
       <c r="O251" t="inlineStr">
@@ -17377,7 +17382,7 @@
       </c>
       <c r="N252" t="inlineStr">
         <is>
-          <t>2026-02-18T09:19:14</t>
+          <t>2026-02-18T11:11:55</t>
         </is>
       </c>
       <c r="O252" t="inlineStr">
@@ -17443,7 +17448,7 @@
       </c>
       <c r="N253" t="inlineStr">
         <is>
-          <t>2026-02-18T09:19:49</t>
+          <t>2026-02-18T11:19:22</t>
         </is>
       </c>
       <c r="O253" t="inlineStr">
@@ -17503,7 +17508,7 @@
       </c>
       <c r="N254" t="inlineStr">
         <is>
-          <t>2026-02-18T09:17:22</t>
+          <t>2026-02-18T11:05:46</t>
         </is>
       </c>
       <c r="O254" t="inlineStr">
@@ -17569,7 +17574,7 @@
       </c>
       <c r="N255" t="inlineStr">
         <is>
-          <t>2026-02-18T09:22:00</t>
+          <t>2026-02-18T11:05:13</t>
         </is>
       </c>
       <c r="O255" t="inlineStr">
@@ -17635,7 +17640,7 @@
       </c>
       <c r="N256" t="inlineStr">
         <is>
-          <t>2026-02-18T09:33:27</t>
+          <t>2026-02-18T11:30:43</t>
         </is>
       </c>
       <c r="O256" t="inlineStr">
@@ -17767,7 +17772,7 @@
       </c>
       <c r="N258" t="inlineStr">
         <is>
-          <t>2026-02-18T09:03:13</t>
+          <t>2026-02-18T10:56:36</t>
         </is>
       </c>
       <c r="O258" t="inlineStr">
@@ -17833,7 +17838,7 @@
       </c>
       <c r="N259" t="inlineStr">
         <is>
-          <t>2026-02-18T09:11:02</t>
+          <t>2026-02-18T11:09:54</t>
         </is>
       </c>
       <c r="O259" t="inlineStr">
@@ -17899,7 +17904,7 @@
       </c>
       <c r="N260" t="inlineStr">
         <is>
-          <t>2026-02-18T09:23:35</t>
+          <t>2026-02-18T11:13:51</t>
         </is>
       </c>
       <c r="O260" t="inlineStr">
@@ -17965,7 +17970,7 @@
       </c>
       <c r="N261" t="inlineStr">
         <is>
-          <t>2026-02-18T08:54:43</t>
+          <t>2026-02-18T10:52:46</t>
         </is>
       </c>
       <c r="O261" t="inlineStr">
@@ -18031,7 +18036,7 @@
       </c>
       <c r="N262" t="inlineStr">
         <is>
-          <t>2026-02-18T08:48:30</t>
+          <t>2026-02-18T11:35:55</t>
         </is>
       </c>
       <c r="O262" t="inlineStr">
@@ -18097,7 +18102,7 @@
       </c>
       <c r="N263" t="inlineStr">
         <is>
-          <t>2026-02-18T08:55:15</t>
+          <t>2026-02-18T11:33:39</t>
         </is>
       </c>
       <c r="O263" t="inlineStr">
@@ -18163,7 +18168,7 @@
       </c>
       <c r="N264" t="inlineStr">
         <is>
-          <t>2026-02-18T09:36:43</t>
+          <t>2026-02-18T11:28:51</t>
         </is>
       </c>
       <c r="O264" t="inlineStr">
@@ -18229,7 +18234,7 @@
       </c>
       <c r="N265" t="inlineStr">
         <is>
-          <t>2026-02-18T09:37:09</t>
+          <t>2026-02-18T11:33:32</t>
         </is>
       </c>
       <c r="O265" t="inlineStr">
@@ -18295,7 +18300,7 @@
       </c>
       <c r="N266" t="inlineStr">
         <is>
-          <t>2026-02-18T09:05:19</t>
+          <t>2026-02-18T11:02:06</t>
         </is>
       </c>
       <c r="O266" t="inlineStr">
@@ -18361,7 +18366,7 @@
       </c>
       <c r="N267" t="inlineStr">
         <is>
-          <t>2026-02-18T09:00:45</t>
+          <t>2026-02-18T10:58:39</t>
         </is>
       </c>
       <c r="O267" t="inlineStr">
@@ -18427,7 +18432,7 @@
       </c>
       <c r="N268" t="inlineStr">
         <is>
-          <t>2026-02-18T08:59:23</t>
+          <t>2026-02-18T10:55:14</t>
         </is>
       </c>
       <c r="O268" t="inlineStr">
@@ -18493,7 +18498,7 @@
       </c>
       <c r="N269" t="inlineStr">
         <is>
-          <t>2026-02-18T09:30:15</t>
+          <t>2026-02-18T11:21:47</t>
         </is>
       </c>
       <c r="O269" t="inlineStr">
@@ -18556,7 +18561,7 @@
       </c>
       <c r="N270" t="inlineStr">
         <is>
-          <t>2026-02-18T08:56:37</t>
+          <t>2026-02-18T10:47:22</t>
         </is>
       </c>
       <c r="O270" t="inlineStr">
@@ -18688,7 +18693,7 @@
       </c>
       <c r="N272" t="inlineStr">
         <is>
-          <t>2026-02-18T09:01:35</t>
+          <t>2026-02-18T11:39:15</t>
         </is>
       </c>
       <c r="O272" t="inlineStr">
@@ -18754,7 +18759,7 @@
       </c>
       <c r="N273" t="inlineStr">
         <is>
-          <t>2026-02-18T09:18:40</t>
+          <t>2026-02-18T11:06:35</t>
         </is>
       </c>
       <c r="O273" t="inlineStr">
@@ -19084,7 +19089,7 @@
       </c>
       <c r="N278" t="inlineStr">
         <is>
-          <t>2026-02-18T09:17:21</t>
+          <t>2026-02-18T11:04:10</t>
         </is>
       </c>
       <c r="O278" t="inlineStr">
@@ -19216,7 +19221,7 @@
       </c>
       <c r="N280" t="inlineStr">
         <is>
-          <t>2026-02-18T09:30:30</t>
+          <t>2026-02-18T11:25:37</t>
         </is>
       </c>
       <c r="O280" t="inlineStr">
@@ -19343,7 +19348,7 @@
       </c>
       <c r="N282" t="inlineStr">
         <is>
-          <t>2026-02-18T09:16:28</t>
+          <t>2026-02-18T11:15:38</t>
         </is>
       </c>
       <c r="O282" t="inlineStr">
@@ -19409,7 +19414,7 @@
       </c>
       <c r="N283" t="inlineStr">
         <is>
-          <t>2026-02-18T09:05:23</t>
+          <t>2026-02-18T11:41:32</t>
         </is>
       </c>
       <c r="O283" t="inlineStr">
@@ -19475,7 +19480,7 @@
       </c>
       <c r="N284" t="inlineStr">
         <is>
-          <t>2026-02-18T09:40:15</t>
+          <t>2026-02-18T11:36:23</t>
         </is>
       </c>
       <c r="O284" t="inlineStr">
@@ -19541,7 +19546,7 @@
       </c>
       <c r="N285" t="inlineStr">
         <is>
-          <t>2026-02-18T09:37:06</t>
+          <t>2026-02-18T11:31:41</t>
         </is>
       </c>
       <c r="O285" t="inlineStr">
@@ -19607,7 +19612,7 @@
       </c>
       <c r="N286" t="inlineStr">
         <is>
-          <t>2026-02-18T08:56:50</t>
+          <t>2026-02-18T11:00:12</t>
         </is>
       </c>
       <c r="O286" t="inlineStr">
@@ -19673,7 +19678,7 @@
       </c>
       <c r="N287" t="inlineStr">
         <is>
-          <t>2026-02-18T09:16:58</t>
+          <t>2026-02-18T11:10:35</t>
         </is>
       </c>
       <c r="O287" t="inlineStr">
@@ -19739,7 +19744,7 @@
       </c>
       <c r="N288" t="inlineStr">
         <is>
-          <t>2026-02-18T09:06:02</t>
+          <t>2026-02-18T11:05:53</t>
         </is>
       </c>
       <c r="O288" t="inlineStr">
@@ -19805,7 +19810,7 @@
       </c>
       <c r="N289" t="inlineStr">
         <is>
-          <t>2026-02-18T09:31:32</t>
+          <t>2026-02-18T11:20:47</t>
         </is>
       </c>
       <c r="O289" t="inlineStr">
@@ -20625,7 +20630,7 @@
       </c>
       <c r="N302" t="inlineStr">
         <is>
-          <t>2026-02-18T09:19:23</t>
+          <t>2026-02-18T11:13:08</t>
         </is>
       </c>
       <c r="O302" t="inlineStr">
@@ -21390,7 +21395,7 @@
       </c>
       <c r="N314" t="inlineStr">
         <is>
-          <t>2026-02-18T09:37:59</t>
+          <t>2026-02-18T11:30:00</t>
         </is>
       </c>
       <c r="O314" t="inlineStr">
@@ -21777,7 +21782,7 @@
       </c>
       <c r="N320" t="inlineStr">
         <is>
-          <t>2026-02-18T09:02:48</t>
+          <t>2026-02-18T10:51:11</t>
         </is>
       </c>
       <c r="O320" t="inlineStr">
@@ -22526,7 +22531,7 @@
       </c>
       <c r="N332" t="inlineStr">
         <is>
-          <t>2026-02-18T08:59:45</t>
+          <t>2026-02-18T10:50:31</t>
         </is>
       </c>
       <c r="O332" t="inlineStr">
@@ -22592,7 +22597,7 @@
       </c>
       <c r="N333" t="inlineStr">
         <is>
-          <t>2026-02-18T09:26:02</t>
+          <t>2026-02-18T11:18:36</t>
         </is>
       </c>
       <c r="O333" t="inlineStr">
@@ -22658,7 +22663,7 @@
       </c>
       <c r="N334" t="inlineStr">
         <is>
-          <t>2026-02-18T09:39:31</t>
+          <t>2026-02-18T11:29:02</t>
         </is>
       </c>
       <c r="O334" t="inlineStr">
@@ -22724,7 +22729,7 @@
       </c>
       <c r="N335" t="inlineStr">
         <is>
-          <t>2026-02-18T09:28:53</t>
+          <t>2026-02-18T11:20:00</t>
         </is>
       </c>
       <c r="O335" t="inlineStr">
@@ -22790,7 +22795,7 @@
       </c>
       <c r="N336" t="inlineStr">
         <is>
-          <t>2026-02-18T09:39:55</t>
+          <t>2026-02-18T11:33:00</t>
         </is>
       </c>
       <c r="O336" t="inlineStr">
@@ -22856,7 +22861,7 @@
       </c>
       <c r="N337" t="inlineStr">
         <is>
-          <t>2026-02-18T09:36:16</t>
+          <t>2026-02-18T11:28:03</t>
         </is>
       </c>
       <c r="O337" t="inlineStr">
@@ -22922,7 +22927,7 @@
       </c>
       <c r="N338" t="inlineStr">
         <is>
-          <t>2026-02-18T09:29:08</t>
+          <t>2026-02-18T11:22:02</t>
         </is>
       </c>
       <c r="O338" t="inlineStr">
@@ -22988,7 +22993,7 @@
       </c>
       <c r="N339" t="inlineStr">
         <is>
-          <t>2026-02-18T09:05:39</t>
+          <t>2026-02-18T10:55:36</t>
         </is>
       </c>
       <c r="O339" t="inlineStr">
@@ -23120,7 +23125,7 @@
       </c>
       <c r="N341" t="inlineStr">
         <is>
-          <t>2026-02-18T09:02:01</t>
+          <t>2026-02-18T10:56:22</t>
         </is>
       </c>
       <c r="O341" t="inlineStr">
@@ -23186,7 +23191,7 @@
       </c>
       <c r="N342" t="inlineStr">
         <is>
-          <t>2026-02-18T09:42:25</t>
+          <t>2026-02-18T11:31:18</t>
         </is>
       </c>
       <c r="O342" t="inlineStr">
@@ -23254,7 +23259,7 @@
       </c>
       <c r="N343" t="inlineStr">
         <is>
-          <t>2026-02-18T09:24:31</t>
+          <t>2026-02-18T11:17:34</t>
         </is>
       </c>
       <c r="O343" t="inlineStr">
@@ -23843,7 +23848,7 @@
       </c>
       <c r="N352" t="inlineStr">
         <is>
-          <t>2026-02-18T09:38:01</t>
+          <t>2026-02-18T11:33:56</t>
         </is>
       </c>
       <c r="O352" t="inlineStr">
@@ -24683,7 +24688,7 @@
       </c>
       <c r="N365" t="inlineStr">
         <is>
-          <t>2026-02-18T09:28:27</t>
+          <t>2026-02-18T11:22:09</t>
         </is>
       </c>
       <c r="O365" t="inlineStr">
@@ -24751,7 +24756,7 @@
       </c>
       <c r="N366" t="inlineStr">
         <is>
-          <t>2026-02-18T09:35:24</t>
+          <t>2026-02-18T11:32:12</t>
         </is>
       </c>
       <c r="O366" t="inlineStr">
@@ -24881,7 +24886,7 @@
       </c>
       <c r="N368" t="inlineStr">
         <is>
-          <t>2026-02-18T08:52:28</t>
+          <t>2026-02-18T11:34:53</t>
         </is>
       </c>
       <c r="O368" t="inlineStr">
@@ -24901,11 +24906,6 @@
           <t>RH</t>
         </is>
       </c>
-      <c r="C369" t="inlineStr">
-        <is>
-          <t>10.69.3.13</t>
-        </is>
-      </c>
       <c r="D369" t="n">
         <v>2025</v>
       </c>
@@ -24949,7 +24949,7 @@
       </c>
       <c r="N369" t="inlineStr">
         <is>
-          <t>2026-02-18T09:27:24</t>
+          <t>2026-02-18T11:24:35</t>
         </is>
       </c>
       <c r="O369" t="inlineStr">
@@ -25020,7 +25020,7 @@
       </c>
       <c r="N370" t="inlineStr">
         <is>
-          <t>2026-02-18T09:18:19</t>
+          <t>2026-02-18T11:12:07</t>
         </is>
       </c>
       <c r="O370" t="inlineStr">
@@ -25162,7 +25162,7 @@
       </c>
       <c r="N372" t="inlineStr">
         <is>
-          <t>2026-02-18T08:56:33</t>
+          <t>2026-02-18T10:52:54</t>
         </is>
       </c>
       <c r="O372" t="inlineStr">
@@ -25372,7 +25372,7 @@
       </c>
       <c r="N375" t="inlineStr">
         <is>
-          <t>2026-02-18T09:14:58</t>
+          <t>2026-02-18T11:06:45</t>
         </is>
       </c>
       <c r="O375" t="inlineStr">
@@ -25509,7 +25509,7 @@
       </c>
       <c r="N377" t="inlineStr">
         <is>
-          <t>2026-02-18T09:37:52</t>
+          <t>2026-02-18T11:25:58</t>
         </is>
       </c>
       <c r="O377" t="inlineStr">
@@ -25580,7 +25580,7 @@
       </c>
       <c r="N378" t="inlineStr">
         <is>
-          <t>2026-02-18T09:39:46</t>
+          <t>2026-02-18T11:36:42</t>
         </is>
       </c>
       <c r="O378" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática 2026-02-18 13:52:04.742617
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -601,7 +601,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>2026-02-18T11:25:09</t>
+          <t>2026-02-18T13:22:51</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -672,7 +672,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>2026-02-18T10:54:27</t>
+          <t>2026-02-18T13:38:30</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -814,7 +814,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>2026-02-18T11:03:05</t>
+          <t>2026-02-18T12:52:29</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -1144,7 +1144,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>2026-02-18T11:04:18</t>
+          <t>2026-02-18T12:57:52</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -1474,7 +1474,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>2026-02-18T11:03:40</t>
+          <t>2026-02-18T12:53:49</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
@@ -1606,7 +1606,7 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>2026-02-18T11:16:53</t>
+          <t>2026-02-18T13:11:43</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
@@ -6885,7 +6885,7 @@
       </c>
       <c r="N95" t="inlineStr">
         <is>
-          <t>2026-02-18T11:04:18</t>
+          <t>2026-02-18T12:59:00</t>
         </is>
       </c>
       <c r="O95" t="inlineStr">
@@ -6956,7 +6956,7 @@
       </c>
       <c r="N96" t="inlineStr">
         <is>
-          <t>2026-02-18T10:54:46</t>
+          <t>2026-02-18T12:48:12</t>
         </is>
       </c>
       <c r="O96" t="inlineStr">
@@ -7022,7 +7022,7 @@
       </c>
       <c r="N97" t="inlineStr">
         <is>
-          <t>2026-02-18T11:11:12</t>
+          <t>2026-02-18T13:04:08</t>
         </is>
       </c>
       <c r="O97" t="inlineStr">
@@ -7088,7 +7088,7 @@
       </c>
       <c r="N98" t="inlineStr">
         <is>
-          <t>2026-02-18T11:35:10</t>
+          <t>2026-02-18T13:24:00</t>
         </is>
       </c>
       <c r="O98" t="inlineStr">
@@ -7159,7 +7159,7 @@
       </c>
       <c r="N99" t="inlineStr">
         <is>
-          <t>2026-02-18T11:26:48</t>
+          <t>2026-02-18T13:19:13</t>
         </is>
       </c>
       <c r="O99" t="inlineStr">
@@ -7230,7 +7230,7 @@
       </c>
       <c r="N100" t="inlineStr">
         <is>
-          <t>2026-02-18T10:55:24</t>
+          <t>2026-02-18T12:49:10</t>
         </is>
       </c>
       <c r="O100" t="inlineStr">
@@ -7301,7 +7301,7 @@
       </c>
       <c r="N101" t="inlineStr">
         <is>
-          <t>2026-02-18T11:34:08</t>
+          <t>2026-02-18T13:31:53</t>
         </is>
       </c>
       <c r="O101" t="inlineStr">
@@ -7443,7 +7443,7 @@
       </c>
       <c r="N103" t="inlineStr">
         <is>
-          <t>2026-02-18T10:52:02</t>
+          <t>2026-02-18T13:37:43</t>
         </is>
       </c>
       <c r="O103" t="inlineStr">
@@ -7708,7 +7708,7 @@
       </c>
       <c r="N107" t="inlineStr">
         <is>
-          <t>2026-02-18T11:17:18</t>
+          <t>2026-02-18T13:07:46</t>
         </is>
       </c>
       <c r="O107" t="inlineStr">
@@ -7850,7 +7850,7 @@
       </c>
       <c r="N109" t="inlineStr">
         <is>
-          <t>2026-02-18T10:51:52</t>
+          <t>2026-02-18T12:46:57</t>
         </is>
       </c>
       <c r="O109" t="inlineStr">
@@ -7921,7 +7921,7 @@
       </c>
       <c r="N110" t="inlineStr">
         <is>
-          <t>2026-02-18T10:51:58</t>
+          <t>2026-02-18T12:47:01</t>
         </is>
       </c>
       <c r="O110" t="inlineStr">
@@ -7992,7 +7992,7 @@
       </c>
       <c r="N111" t="inlineStr">
         <is>
-          <t>2026-02-18T10:45:41</t>
+          <t>2026-02-18T13:29:16</t>
         </is>
       </c>
       <c r="O111" t="inlineStr">
@@ -8063,7 +8063,7 @@
       </c>
       <c r="N112" t="inlineStr">
         <is>
-          <t>2026-02-18T11:27:19</t>
+          <t>2026-02-18T13:20:08</t>
         </is>
       </c>
       <c r="O112" t="inlineStr">
@@ -8134,7 +8134,7 @@
       </c>
       <c r="N113" t="inlineStr">
         <is>
-          <t>2026-02-18T11:31:32</t>
+          <t>2026-02-18T13:32:04</t>
         </is>
       </c>
       <c r="O113" t="inlineStr">
@@ -8205,7 +8205,7 @@
       </c>
       <c r="N114" t="inlineStr">
         <is>
-          <t>2026-02-18T11:35:02</t>
+          <t>2026-02-18T13:26:36</t>
         </is>
       </c>
       <c r="O114" t="inlineStr">
@@ -8273,7 +8273,7 @@
       </c>
       <c r="N115" t="inlineStr">
         <is>
-          <t>2026-02-18T11:01:40</t>
+          <t>2026-02-18T12:47:57</t>
         </is>
       </c>
       <c r="O115" t="inlineStr">
@@ -8344,7 +8344,7 @@
       </c>
       <c r="N116" t="inlineStr">
         <is>
-          <t>2026-02-18T11:40:58</t>
+          <t>2026-02-18T13:33:09</t>
         </is>
       </c>
       <c r="O116" t="inlineStr">
@@ -8364,11 +8364,6 @@
           <t>DP</t>
         </is>
       </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>10.69.3.23</t>
-        </is>
-      </c>
       <c r="D117" t="n">
         <v>2025</v>
       </c>
@@ -8415,7 +8410,7 @@
       </c>
       <c r="N117" t="inlineStr">
         <is>
-          <t>2026-02-18T11:35:14</t>
+          <t>2026-02-18T13:19:15</t>
         </is>
       </c>
       <c r="O117" t="inlineStr">
@@ -8625,7 +8620,7 @@
       </c>
       <c r="N120" t="inlineStr">
         <is>
-          <t>2026-02-18T10:41:55</t>
+          <t>2026-02-18T13:31:59</t>
         </is>
       </c>
       <c r="O120" t="inlineStr">
@@ -8696,7 +8691,7 @@
       </c>
       <c r="N121" t="inlineStr">
         <is>
-          <t>2026-02-18T11:25:30</t>
+          <t>2026-02-18T13:11:20</t>
         </is>
       </c>
       <c r="O121" t="inlineStr">
@@ -8764,7 +8759,7 @@
       </c>
       <c r="N122" t="inlineStr">
         <is>
-          <t>2026-02-18T11:34:26</t>
+          <t>2026-02-18T13:25:39</t>
         </is>
       </c>
       <c r="O122" t="inlineStr">
@@ -8906,7 +8901,7 @@
       </c>
       <c r="N124" t="inlineStr">
         <is>
-          <t>2026-02-18T10:52:24</t>
+          <t>2026-02-18T13:37:51</t>
         </is>
       </c>
       <c r="O124" t="inlineStr">
@@ -8977,7 +8972,7 @@
       </c>
       <c r="N125" t="inlineStr">
         <is>
-          <t>2026-02-18T11:31:38</t>
+          <t>2026-02-18T13:28:12</t>
         </is>
       </c>
       <c r="O125" t="inlineStr">
@@ -9048,7 +9043,7 @@
       </c>
       <c r="N126" t="inlineStr">
         <is>
-          <t>2026-02-18T11:00:36</t>
+          <t>2026-02-18T12:44:25</t>
         </is>
       </c>
       <c r="O126" t="inlineStr">
@@ -9119,7 +9114,7 @@
       </c>
       <c r="N127" t="inlineStr">
         <is>
-          <t>2026-02-18T11:12:07</t>
+          <t>2026-02-18T13:05:01</t>
         </is>
       </c>
       <c r="O127" t="inlineStr">
@@ -9190,7 +9185,7 @@
       </c>
       <c r="N128" t="inlineStr">
         <is>
-          <t>2026-02-18T10:50:35</t>
+          <t>2026-02-18T13:36:39</t>
         </is>
       </c>
       <c r="O128" t="inlineStr">
@@ -9261,7 +9256,7 @@
       </c>
       <c r="N129" t="inlineStr">
         <is>
-          <t>2026-02-18T11:10:05</t>
+          <t>2026-02-18T13:00:52</t>
         </is>
       </c>
       <c r="O129" t="inlineStr">
@@ -9332,7 +9327,7 @@
       </c>
       <c r="N130" t="inlineStr">
         <is>
-          <t>2026-02-18T10:51:04</t>
+          <t>2026-02-18T13:37:15</t>
         </is>
       </c>
       <c r="O130" t="inlineStr">
@@ -9403,7 +9398,7 @@
       </c>
       <c r="N131" t="inlineStr">
         <is>
-          <t>2026-02-18T11:41:03</t>
+          <t>2026-02-18T13:36:15</t>
         </is>
       </c>
       <c r="O131" t="inlineStr">
@@ -9540,7 +9535,7 @@
       </c>
       <c r="N133" t="inlineStr">
         <is>
-          <t>2026-02-18T11:01:22</t>
+          <t>2026-02-18T12:53:18</t>
         </is>
       </c>
       <c r="O133" t="inlineStr">
@@ -9606,7 +9601,7 @@
       </c>
       <c r="N134" t="inlineStr">
         <is>
-          <t>2026-02-18T11:12:30</t>
+          <t>2026-02-18T13:04:49</t>
         </is>
       </c>
       <c r="O134" t="inlineStr">
@@ -9672,7 +9667,7 @@
       </c>
       <c r="N135" t="inlineStr">
         <is>
-          <t>2026-02-18T10:54:58</t>
+          <t>2026-02-18T12:52:19</t>
         </is>
       </c>
       <c r="O135" t="inlineStr">
@@ -9869,7 +9864,7 @@
       </c>
       <c r="N138" t="inlineStr">
         <is>
-          <t>2026-02-18T11:39:34</t>
+          <t>2026-02-18T13:30:55</t>
         </is>
       </c>
       <c r="O138" t="inlineStr">
@@ -9935,7 +9930,7 @@
       </c>
       <c r="N139" t="inlineStr">
         <is>
-          <t>2026-02-18T11:35:08</t>
+          <t>2026-02-18T13:26:01</t>
         </is>
       </c>
       <c r="O139" t="inlineStr">
@@ -10001,7 +9996,7 @@
       </c>
       <c r="N140" t="inlineStr">
         <is>
-          <t>2026-02-18T11:20:56</t>
+          <t>2026-02-18T13:16:22</t>
         </is>
       </c>
       <c r="O140" t="inlineStr">
@@ -10067,7 +10062,7 @@
       </c>
       <c r="N141" t="inlineStr">
         <is>
-          <t>2026-02-18T10:53:16</t>
+          <t>2026-02-18T13:37:28</t>
         </is>
       </c>
       <c r="O141" t="inlineStr">
@@ -10265,7 +10260,7 @@
       </c>
       <c r="N144" t="inlineStr">
         <is>
-          <t>2026-02-18T11:15:05</t>
+          <t>2026-02-18T13:06:37</t>
         </is>
       </c>
       <c r="O144" t="inlineStr">
@@ -10331,7 +10326,7 @@
       </c>
       <c r="N145" t="inlineStr">
         <is>
-          <t>2026-02-18T11:12:32</t>
+          <t>2026-02-18T13:09:12</t>
         </is>
       </c>
       <c r="O145" t="inlineStr">
@@ -10397,7 +10392,7 @@
       </c>
       <c r="N146" t="inlineStr">
         <is>
-          <t>2026-02-18T10:53:58</t>
+          <t>2026-02-18T12:48:33</t>
         </is>
       </c>
       <c r="O146" t="inlineStr">
@@ -10463,7 +10458,7 @@
       </c>
       <c r="N147" t="inlineStr">
         <is>
-          <t>2026-02-18T11:38:30</t>
+          <t>2026-02-18T13:36:33</t>
         </is>
       </c>
       <c r="O147" t="inlineStr">
@@ -10529,7 +10524,7 @@
       </c>
       <c r="N148" t="inlineStr">
         <is>
-          <t>2026-02-18T11:18:29</t>
+          <t>2026-02-18T13:10:49</t>
         </is>
       </c>
       <c r="O148" t="inlineStr">
@@ -10727,7 +10722,7 @@
       </c>
       <c r="N151" t="inlineStr">
         <is>
-          <t>2026-02-18T11:32:33</t>
+          <t>2026-02-18T13:22:30</t>
         </is>
       </c>
       <c r="O151" t="inlineStr">
@@ -10793,7 +10788,7 @@
       </c>
       <c r="N152" t="inlineStr">
         <is>
-          <t>2026-02-18T11:00:30</t>
+          <t>2026-02-18T12:50:06</t>
         </is>
       </c>
       <c r="O152" t="inlineStr">
@@ -10854,7 +10849,7 @@
       </c>
       <c r="N153" t="inlineStr">
         <is>
-          <t>2026-02-18T10:57:06</t>
+          <t>2026-02-18T12:51:51</t>
         </is>
       </c>
       <c r="O153" t="inlineStr">
@@ -10920,7 +10915,7 @@
       </c>
       <c r="N154" t="inlineStr">
         <is>
-          <t>2026-02-18T11:18:06</t>
+          <t>2026-02-18T13:03:11</t>
         </is>
       </c>
       <c r="O154" t="inlineStr">
@@ -10986,7 +10981,7 @@
       </c>
       <c r="N155" t="inlineStr">
         <is>
-          <t>2026-02-18T10:57:00</t>
+          <t>2026-02-18T13:34:33</t>
         </is>
       </c>
       <c r="O155" t="inlineStr">
@@ -11118,7 +11113,7 @@
       </c>
       <c r="N157" t="inlineStr">
         <is>
-          <t>2026-02-18T10:53:52</t>
+          <t>2026-02-18T13:39:45</t>
         </is>
       </c>
       <c r="O157" t="inlineStr">
@@ -11151,7 +11146,7 @@
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>Windows</t>
+          <t>Microsoft Windows 8.1 Pro</t>
         </is>
       </c>
       <c r="G158" t="inlineStr">
@@ -11184,7 +11179,7 @@
       </c>
       <c r="N158" t="inlineStr">
         <is>
-          <t>2026-02-18T10:51:43</t>
+          <t>2026-02-18T13:10:35</t>
         </is>
       </c>
       <c r="O158" t="inlineStr">
@@ -11250,7 +11245,7 @@
       </c>
       <c r="N159" t="inlineStr">
         <is>
-          <t>2026-02-18T11:27:29</t>
+          <t>2026-02-18T13:23:28</t>
         </is>
       </c>
       <c r="O159" t="inlineStr">
@@ -11316,7 +11311,7 @@
       </c>
       <c r="N160" t="inlineStr">
         <is>
-          <t>2026-02-18T11:04:56</t>
+          <t>2026-02-18T12:58:18</t>
         </is>
       </c>
       <c r="O160" t="inlineStr">
@@ -11382,7 +11377,7 @@
       </c>
       <c r="N161" t="inlineStr">
         <is>
-          <t>2026-02-18T11:42:01</t>
+          <t>2026-02-18T13:33:50</t>
         </is>
       </c>
       <c r="O161" t="inlineStr">
@@ -11448,7 +11443,7 @@
       </c>
       <c r="N162" t="inlineStr">
         <is>
-          <t>2026-02-18T11:16:44</t>
+          <t>2026-02-18T12:59:23</t>
         </is>
       </c>
       <c r="O162" t="inlineStr">
@@ -11580,7 +11575,7 @@
       </c>
       <c r="N164" t="inlineStr">
         <is>
-          <t>2026-02-18T10:50:07</t>
+          <t>2026-02-18T13:38:07</t>
         </is>
       </c>
       <c r="O164" t="inlineStr">
@@ -11646,7 +11641,7 @@
       </c>
       <c r="N165" t="inlineStr">
         <is>
-          <t>2026-02-18T11:34:08</t>
+          <t>2026-02-18T12:31:47</t>
         </is>
       </c>
       <c r="O165" t="inlineStr">
@@ -11712,7 +11707,7 @@
       </c>
       <c r="N166" t="inlineStr">
         <is>
-          <t>2026-02-18T11:04:50</t>
+          <t>2026-02-18T12:56:43</t>
         </is>
       </c>
       <c r="O166" t="inlineStr">
@@ -11774,11 +11769,11 @@
         </is>
       </c>
       <c r="M167" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N167" t="inlineStr">
         <is>
-          <t>2026-02-18T11:30:38</t>
+          <t>2026-02-18T13:20:12</t>
         </is>
       </c>
       <c r="O167" t="inlineStr">
@@ -11844,7 +11839,7 @@
       </c>
       <c r="N168" t="inlineStr">
         <is>
-          <t>2026-02-18T11:04:30</t>
+          <t>2026-02-18T13:00:17</t>
         </is>
       </c>
       <c r="O168" t="inlineStr">
@@ -11910,7 +11905,7 @@
       </c>
       <c r="N169" t="inlineStr">
         <is>
-          <t>2026-02-18T10:56:41</t>
+          <t>2026-02-18T12:47:20</t>
         </is>
       </c>
       <c r="O169" t="inlineStr">
@@ -11976,7 +11971,7 @@
       </c>
       <c r="N170" t="inlineStr">
         <is>
-          <t>2026-02-18T10:43:25</t>
+          <t>2026-02-18T13:32:42</t>
         </is>
       </c>
       <c r="O170" t="inlineStr">
@@ -12038,11 +12033,11 @@
         </is>
       </c>
       <c r="M171" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N171" t="inlineStr">
         <is>
-          <t>2026-02-18T11:35:21</t>
+          <t>2026-02-18T13:21:47</t>
         </is>
       </c>
       <c r="O171" t="inlineStr">
@@ -12108,7 +12103,7 @@
       </c>
       <c r="N172" t="inlineStr">
         <is>
-          <t>2026-02-18T11:10:19</t>
+          <t>2026-02-18T13:07:33</t>
         </is>
       </c>
       <c r="O172" t="inlineStr">
@@ -12170,11 +12165,11 @@
         </is>
       </c>
       <c r="M173" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N173" t="inlineStr">
         <is>
-          <t>2026-02-18T11:29:39</t>
+          <t>2026-02-18T13:18:03</t>
         </is>
       </c>
       <c r="O173" t="inlineStr">
@@ -12240,7 +12235,7 @@
       </c>
       <c r="N174" t="inlineStr">
         <is>
-          <t>2026-02-18T10:49:42</t>
+          <t>2026-02-18T12:51:42</t>
         </is>
       </c>
       <c r="O174" t="inlineStr">
@@ -12306,7 +12301,7 @@
       </c>
       <c r="N175" t="inlineStr">
         <is>
-          <t>2026-02-18T10:54:17</t>
+          <t>2026-02-18T13:38:34</t>
         </is>
       </c>
       <c r="O175" t="inlineStr">
@@ -12372,7 +12367,7 @@
       </c>
       <c r="N176" t="inlineStr">
         <is>
-          <t>2026-02-18T11:24:14</t>
+          <t>2026-02-18T13:12:42</t>
         </is>
       </c>
       <c r="O176" t="inlineStr">
@@ -12438,7 +12433,7 @@
       </c>
       <c r="N177" t="inlineStr">
         <is>
-          <t>2026-02-18T11:37:00</t>
+          <t>2026-02-18T13:30:34</t>
         </is>
       </c>
       <c r="O177" t="inlineStr">
@@ -12504,7 +12499,7 @@
       </c>
       <c r="N178" t="inlineStr">
         <is>
-          <t>2026-02-18T11:32:54</t>
+          <t>2026-02-18T13:25:19</t>
         </is>
       </c>
       <c r="O178" t="inlineStr">
@@ -12570,7 +12565,7 @@
       </c>
       <c r="N179" t="inlineStr">
         <is>
-          <t>2026-02-18T10:56:45</t>
+          <t>2026-02-18T13:37:18</t>
         </is>
       </c>
       <c r="O179" t="inlineStr">
@@ -12636,7 +12631,7 @@
       </c>
       <c r="N180" t="inlineStr">
         <is>
-          <t>2026-02-18T11:04:25</t>
+          <t>2026-02-18T13:03:35</t>
         </is>
       </c>
       <c r="O180" t="inlineStr">
@@ -12834,7 +12829,7 @@
       </c>
       <c r="N183" t="inlineStr">
         <is>
-          <t>2026-02-18T11:16:28</t>
+          <t>2026-02-18T13:14:07</t>
         </is>
       </c>
       <c r="O183" t="inlineStr">
@@ -13037,7 +13032,7 @@
       </c>
       <c r="N186" t="inlineStr">
         <is>
-          <t>2026-02-18T11:41:26</t>
+          <t>2026-02-18T13:30:19</t>
         </is>
       </c>
       <c r="O186" t="inlineStr">
@@ -13103,7 +13098,7 @@
       </c>
       <c r="N187" t="inlineStr">
         <is>
-          <t>2026-02-18T11:34:13</t>
+          <t>2026-02-18T13:29:32</t>
         </is>
       </c>
       <c r="O187" t="inlineStr">
@@ -13169,7 +13164,7 @@
       </c>
       <c r="N188" t="inlineStr">
         <is>
-          <t>2026-02-18T11:41:08</t>
+          <t>2026-02-18T13:24:22</t>
         </is>
       </c>
       <c r="O188" t="inlineStr">
@@ -13301,7 +13296,7 @@
       </c>
       <c r="N190" t="inlineStr">
         <is>
-          <t>2026-02-18T11:15:53</t>
+          <t>2026-02-18T13:03:08</t>
         </is>
       </c>
       <c r="O190" t="inlineStr">
@@ -13628,7 +13623,7 @@
       </c>
       <c r="N195" t="inlineStr">
         <is>
-          <t>2026-02-18T10:50:14</t>
+          <t>2026-02-18T12:47:54</t>
         </is>
       </c>
       <c r="O195" t="inlineStr">
@@ -13694,7 +13689,7 @@
       </c>
       <c r="N196" t="inlineStr">
         <is>
-          <t>2026-02-18T10:47:05</t>
+          <t>2026-02-18T13:37:18</t>
         </is>
       </c>
       <c r="O196" t="inlineStr">
@@ -13760,7 +13755,7 @@
       </c>
       <c r="N197" t="inlineStr">
         <is>
-          <t>2026-02-18T11:29:44</t>
+          <t>2026-02-18T13:22:28</t>
         </is>
       </c>
       <c r="O197" t="inlineStr">
@@ -13826,7 +13821,7 @@
       </c>
       <c r="N198" t="inlineStr">
         <is>
-          <t>2026-02-18T10:49:38</t>
+          <t>2026-02-18T13:37:52</t>
         </is>
       </c>
       <c r="O198" t="inlineStr">
@@ -14087,7 +14082,7 @@
       </c>
       <c r="N202" t="inlineStr">
         <is>
-          <t>2026-02-18T10:52:57</t>
+          <t>2026-02-18T13:27:58</t>
         </is>
       </c>
       <c r="O202" t="inlineStr">
@@ -14153,7 +14148,7 @@
       </c>
       <c r="N203" t="inlineStr">
         <is>
-          <t>2026-02-18T11:24:24</t>
+          <t>2026-02-18T13:21:40</t>
         </is>
       </c>
       <c r="O203" t="inlineStr">
@@ -14219,7 +14214,7 @@
       </c>
       <c r="N204" t="inlineStr">
         <is>
-          <t>2026-02-18T11:18:09</t>
+          <t>2026-02-18T13:15:41</t>
         </is>
       </c>
       <c r="O204" t="inlineStr">
@@ -14285,7 +14280,7 @@
       </c>
       <c r="N205" t="inlineStr">
         <is>
-          <t>2026-02-18T10:53:00</t>
+          <t>2026-02-18T12:51:10</t>
         </is>
       </c>
       <c r="O205" t="inlineStr">
@@ -14351,7 +14346,7 @@
       </c>
       <c r="N206" t="inlineStr">
         <is>
-          <t>2026-02-18T11:37:33</t>
+          <t>2026-02-18T13:33:08</t>
         </is>
       </c>
       <c r="O206" t="inlineStr">
@@ -14417,7 +14412,7 @@
       </c>
       <c r="N207" t="inlineStr">
         <is>
-          <t>2026-02-18T11:35:06</t>
+          <t>2026-02-18T13:36:24</t>
         </is>
       </c>
       <c r="O207" t="inlineStr">
@@ -14483,7 +14478,7 @@
       </c>
       <c r="N208" t="inlineStr">
         <is>
-          <t>2026-02-18T11:31:02</t>
+          <t>2026-02-18T13:30:28</t>
         </is>
       </c>
       <c r="O208" t="inlineStr">
@@ -14549,7 +14544,7 @@
       </c>
       <c r="N209" t="inlineStr">
         <is>
-          <t>2026-02-18T10:44:22</t>
+          <t>2026-02-18T13:38:38</t>
         </is>
       </c>
       <c r="O209" t="inlineStr">
@@ -14615,7 +14610,7 @@
       </c>
       <c r="N210" t="inlineStr">
         <is>
-          <t>2026-02-18T11:40:28</t>
+          <t>2026-02-18T13:30:56</t>
         </is>
       </c>
       <c r="O210" t="inlineStr">
@@ -14681,7 +14676,7 @@
       </c>
       <c r="N211" t="inlineStr">
         <is>
-          <t>2026-02-18T11:09:38</t>
+          <t>2026-02-18T12:59:21</t>
         </is>
       </c>
       <c r="O211" t="inlineStr">
@@ -14747,7 +14742,7 @@
       </c>
       <c r="N212" t="inlineStr">
         <is>
-          <t>2026-02-18T11:12:28</t>
+          <t>2026-02-18T13:05:14</t>
         </is>
       </c>
       <c r="O212" t="inlineStr">
@@ -14813,7 +14808,7 @@
       </c>
       <c r="N213" t="inlineStr">
         <is>
-          <t>2026-02-18T10:49:59</t>
+          <t>2026-02-18T13:37:59</t>
         </is>
       </c>
       <c r="O213" t="inlineStr">
@@ -14945,7 +14940,7 @@
       </c>
       <c r="N215" t="inlineStr">
         <is>
-          <t>2026-02-18T10:57:57</t>
+          <t>2026-02-18T13:38:49</t>
         </is>
       </c>
       <c r="O215" t="inlineStr">
@@ -15011,7 +15006,7 @@
       </c>
       <c r="N216" t="inlineStr">
         <is>
-          <t>2026-02-18T11:06:29</t>
+          <t>2026-02-18T13:15:35</t>
         </is>
       </c>
       <c r="O216" t="inlineStr">
@@ -15077,7 +15072,7 @@
       </c>
       <c r="N217" t="inlineStr">
         <is>
-          <t>2026-02-18T10:57:55</t>
+          <t>2026-02-18T13:37:26</t>
         </is>
       </c>
       <c r="O217" t="inlineStr">
@@ -15143,7 +15138,7 @@
       </c>
       <c r="N218" t="inlineStr">
         <is>
-          <t>2026-02-18T10:49:53</t>
+          <t>2026-02-18T13:34:28</t>
         </is>
       </c>
       <c r="O218" t="inlineStr">
@@ -15209,7 +15204,7 @@
       </c>
       <c r="N219" t="inlineStr">
         <is>
-          <t>2026-02-18T11:15:56</t>
+          <t>2026-02-18T13:07:19</t>
         </is>
       </c>
       <c r="O219" t="inlineStr">
@@ -15280,7 +15275,7 @@
       </c>
       <c r="N220" t="inlineStr">
         <is>
-          <t>2026-02-18T10:55:58</t>
+          <t>2026-02-18T12:47:34</t>
         </is>
       </c>
       <c r="O220" t="inlineStr">
@@ -15478,7 +15473,7 @@
       </c>
       <c r="N223" t="inlineStr">
         <is>
-          <t>2026-02-18T11:13:45</t>
+          <t>2026-02-18T13:04:46</t>
         </is>
       </c>
       <c r="O223" t="inlineStr">
@@ -15610,7 +15605,7 @@
       </c>
       <c r="N225" t="inlineStr">
         <is>
-          <t>2026-02-18T11:10:39</t>
+          <t>2026-02-18T13:03:51</t>
         </is>
       </c>
       <c r="O225" t="inlineStr">
@@ -15676,7 +15671,7 @@
       </c>
       <c r="N226" t="inlineStr">
         <is>
-          <t>2026-02-18T10:49:51</t>
+          <t>2026-02-18T13:35:33</t>
         </is>
       </c>
       <c r="O226" t="inlineStr">
@@ -15742,7 +15737,7 @@
       </c>
       <c r="N227" t="inlineStr">
         <is>
-          <t>2026-02-18T11:39:17</t>
+          <t>2026-02-18T13:36:29</t>
         </is>
       </c>
       <c r="O227" t="inlineStr">
@@ -15940,7 +15935,7 @@
       </c>
       <c r="N230" t="inlineStr">
         <is>
-          <t>2026-02-18T11:04:17</t>
+          <t>2026-02-18T12:52:42</t>
         </is>
       </c>
       <c r="O230" t="inlineStr">
@@ -16006,7 +16001,7 @@
       </c>
       <c r="N231" t="inlineStr">
         <is>
-          <t>2026-02-18T11:32:42</t>
+          <t>2026-02-18T13:24:05</t>
         </is>
       </c>
       <c r="O231" t="inlineStr">
@@ -16072,7 +16067,7 @@
       </c>
       <c r="N232" t="inlineStr">
         <is>
-          <t>2026-02-18T11:35:19</t>
+          <t>2026-02-18T13:25:06</t>
         </is>
       </c>
       <c r="O232" t="inlineStr">
@@ -16138,7 +16133,7 @@
       </c>
       <c r="N233" t="inlineStr">
         <is>
-          <t>2026-02-18T11:17:25</t>
+          <t>2026-02-18T13:01:40</t>
         </is>
       </c>
       <c r="O233" t="inlineStr">
@@ -16468,7 +16463,7 @@
       </c>
       <c r="N238" t="inlineStr">
         <is>
-          <t>2026-02-18T11:40:11</t>
+          <t>2026-02-18T13:26:37</t>
         </is>
       </c>
       <c r="O238" t="inlineStr">
@@ -16534,7 +16529,7 @@
       </c>
       <c r="N239" t="inlineStr">
         <is>
-          <t>2026-02-18T11:15:02</t>
+          <t>2026-02-18T13:10:08</t>
         </is>
       </c>
       <c r="O239" t="inlineStr">
@@ -16600,7 +16595,7 @@
       </c>
       <c r="N240" t="inlineStr">
         <is>
-          <t>2026-02-18T11:17:26</t>
+          <t>2026-02-18T13:08:13</t>
         </is>
       </c>
       <c r="O240" t="inlineStr">
@@ -16666,7 +16661,7 @@
       </c>
       <c r="N241" t="inlineStr">
         <is>
-          <t>2026-02-18T11:20:13</t>
+          <t>2026-02-18T13:14:05</t>
         </is>
       </c>
       <c r="O241" t="inlineStr">
@@ -16732,7 +16727,7 @@
       </c>
       <c r="N242" t="inlineStr">
         <is>
-          <t>2026-02-18T11:21:58</t>
+          <t>2026-02-18T13:13:44</t>
         </is>
       </c>
       <c r="O242" t="inlineStr">
@@ -16798,7 +16793,7 @@
       </c>
       <c r="N243" t="inlineStr">
         <is>
-          <t>2026-02-18T11:27:49</t>
+          <t>2026-02-18T13:17:31</t>
         </is>
       </c>
       <c r="O243" t="inlineStr">
@@ -16925,7 +16920,7 @@
       </c>
       <c r="N245" t="inlineStr">
         <is>
-          <t>2026-02-18T11:08:06</t>
+          <t>2026-02-18T12:59:41</t>
         </is>
       </c>
       <c r="O245" t="inlineStr">
@@ -16991,7 +16986,7 @@
       </c>
       <c r="N246" t="inlineStr">
         <is>
-          <t>2026-02-18T11:00:58</t>
+          <t>2026-02-18T12:53:55</t>
         </is>
       </c>
       <c r="O246" t="inlineStr">
@@ -17057,7 +17052,7 @@
       </c>
       <c r="N247" t="inlineStr">
         <is>
-          <t>2026-02-18T11:14:26</t>
+          <t>2026-02-18T13:03:12</t>
         </is>
       </c>
       <c r="O247" t="inlineStr">
@@ -17123,7 +17118,7 @@
       </c>
       <c r="N248" t="inlineStr">
         <is>
-          <t>2026-02-18T11:04:24</t>
+          <t>2026-02-18T12:53:59</t>
         </is>
       </c>
       <c r="O248" t="inlineStr">
@@ -17189,7 +17184,7 @@
       </c>
       <c r="N249" t="inlineStr">
         <is>
-          <t>2026-02-18T11:01:53</t>
+          <t>2026-02-18T13:42:11</t>
         </is>
       </c>
       <c r="O249" t="inlineStr">
@@ -17250,7 +17245,7 @@
       </c>
       <c r="N250" t="inlineStr">
         <is>
-          <t>2026-02-18T11:07:41</t>
+          <t>2026-02-18T13:00:54</t>
         </is>
       </c>
       <c r="O250" t="inlineStr">
@@ -17316,7 +17311,7 @@
       </c>
       <c r="N251" t="inlineStr">
         <is>
-          <t>2026-02-18T11:37:02</t>
+          <t>2026-02-18T13:28:29</t>
         </is>
       </c>
       <c r="O251" t="inlineStr">
@@ -17382,7 +17377,7 @@
       </c>
       <c r="N252" t="inlineStr">
         <is>
-          <t>2026-02-18T11:11:55</t>
+          <t>2026-02-18T13:05:54</t>
         </is>
       </c>
       <c r="O252" t="inlineStr">
@@ -17448,7 +17443,7 @@
       </c>
       <c r="N253" t="inlineStr">
         <is>
-          <t>2026-02-18T11:19:22</t>
+          <t>2026-02-18T13:11:27</t>
         </is>
       </c>
       <c r="O253" t="inlineStr">
@@ -17508,7 +17503,7 @@
       </c>
       <c r="N254" t="inlineStr">
         <is>
-          <t>2026-02-18T11:05:46</t>
+          <t>2026-02-18T12:56:36</t>
         </is>
       </c>
       <c r="O254" t="inlineStr">
@@ -17574,7 +17569,7 @@
       </c>
       <c r="N255" t="inlineStr">
         <is>
-          <t>2026-02-18T11:05:13</t>
+          <t>2026-02-18T12:50:06</t>
         </is>
       </c>
       <c r="O255" t="inlineStr">
@@ -17640,7 +17635,7 @@
       </c>
       <c r="N256" t="inlineStr">
         <is>
-          <t>2026-02-18T11:30:43</t>
+          <t>2026-02-18T13:32:43</t>
         </is>
       </c>
       <c r="O256" t="inlineStr">
@@ -17772,7 +17767,7 @@
       </c>
       <c r="N258" t="inlineStr">
         <is>
-          <t>2026-02-18T10:56:36</t>
+          <t>2026-02-18T12:48:43</t>
         </is>
       </c>
       <c r="O258" t="inlineStr">
@@ -17838,7 +17833,7 @@
       </c>
       <c r="N259" t="inlineStr">
         <is>
-          <t>2026-02-18T11:09:54</t>
+          <t>2026-02-18T12:59:18</t>
         </is>
       </c>
       <c r="O259" t="inlineStr">
@@ -17904,7 +17899,7 @@
       </c>
       <c r="N260" t="inlineStr">
         <is>
-          <t>2026-02-18T11:13:51</t>
+          <t>2026-02-18T13:02:43</t>
         </is>
       </c>
       <c r="O260" t="inlineStr">
@@ -17970,7 +17965,7 @@
       </c>
       <c r="N261" t="inlineStr">
         <is>
-          <t>2026-02-18T10:52:46</t>
+          <t>2026-02-18T13:36:16</t>
         </is>
       </c>
       <c r="O261" t="inlineStr">
@@ -18036,7 +18031,7 @@
       </c>
       <c r="N262" t="inlineStr">
         <is>
-          <t>2026-02-18T11:35:55</t>
+          <t>2026-02-18T13:32:14</t>
         </is>
       </c>
       <c r="O262" t="inlineStr">
@@ -18102,7 +18097,7 @@
       </c>
       <c r="N263" t="inlineStr">
         <is>
-          <t>2026-02-18T11:33:39</t>
+          <t>2026-02-18T13:26:21</t>
         </is>
       </c>
       <c r="O263" t="inlineStr">
@@ -18168,7 +18163,7 @@
       </c>
       <c r="N264" t="inlineStr">
         <is>
-          <t>2026-02-18T11:28:51</t>
+          <t>2026-02-18T13:19:28</t>
         </is>
       </c>
       <c r="O264" t="inlineStr">
@@ -18234,7 +18229,7 @@
       </c>
       <c r="N265" t="inlineStr">
         <is>
-          <t>2026-02-18T11:33:32</t>
+          <t>2026-02-18T13:24:38</t>
         </is>
       </c>
       <c r="O265" t="inlineStr">
@@ -18300,7 +18295,7 @@
       </c>
       <c r="N266" t="inlineStr">
         <is>
-          <t>2026-02-18T11:02:06</t>
+          <t>2026-02-18T12:53:03</t>
         </is>
       </c>
       <c r="O266" t="inlineStr">
@@ -18366,7 +18361,7 @@
       </c>
       <c r="N267" t="inlineStr">
         <is>
-          <t>2026-02-18T10:58:39</t>
+          <t>2026-02-18T12:48:00</t>
         </is>
       </c>
       <c r="O267" t="inlineStr">
@@ -18432,7 +18427,7 @@
       </c>
       <c r="N268" t="inlineStr">
         <is>
-          <t>2026-02-18T10:55:14</t>
+          <t>2026-02-18T13:38:59</t>
         </is>
       </c>
       <c r="O268" t="inlineStr">
@@ -18498,7 +18493,7 @@
       </c>
       <c r="N269" t="inlineStr">
         <is>
-          <t>2026-02-18T11:21:47</t>
+          <t>2026-02-18T13:12:23</t>
         </is>
       </c>
       <c r="O269" t="inlineStr">
@@ -18561,7 +18556,7 @@
       </c>
       <c r="N270" t="inlineStr">
         <is>
-          <t>2026-02-18T10:47:22</t>
+          <t>2026-02-18T12:47:49</t>
         </is>
       </c>
       <c r="O270" t="inlineStr">
@@ -18627,7 +18622,7 @@
       </c>
       <c r="N271" t="inlineStr">
         <is>
-          <t>2026-02-18T04:51:20</t>
+          <t>2026-02-18T12:00:02</t>
         </is>
       </c>
       <c r="O271" t="inlineStr">
@@ -18693,7 +18688,7 @@
       </c>
       <c r="N272" t="inlineStr">
         <is>
-          <t>2026-02-18T11:39:15</t>
+          <t>2026-02-18T13:31:35</t>
         </is>
       </c>
       <c r="O272" t="inlineStr">
@@ -18759,7 +18754,7 @@
       </c>
       <c r="N273" t="inlineStr">
         <is>
-          <t>2026-02-18T11:06:35</t>
+          <t>2026-02-18T13:02:50</t>
         </is>
       </c>
       <c r="O273" t="inlineStr">
@@ -19089,7 +19084,7 @@
       </c>
       <c r="N278" t="inlineStr">
         <is>
-          <t>2026-02-18T11:04:10</t>
+          <t>2026-02-18T12:46:40</t>
         </is>
       </c>
       <c r="O278" t="inlineStr">
@@ -19221,7 +19216,7 @@
       </c>
       <c r="N280" t="inlineStr">
         <is>
-          <t>2026-02-18T11:25:37</t>
+          <t>2026-02-18T13:15:21</t>
         </is>
       </c>
       <c r="O280" t="inlineStr">
@@ -19348,7 +19343,7 @@
       </c>
       <c r="N282" t="inlineStr">
         <is>
-          <t>2026-02-18T11:15:38</t>
+          <t>2026-02-18T13:02:01</t>
         </is>
       </c>
       <c r="O282" t="inlineStr">
@@ -19414,7 +19409,7 @@
       </c>
       <c r="N283" t="inlineStr">
         <is>
-          <t>2026-02-18T11:41:32</t>
+          <t>2026-02-18T13:31:37</t>
         </is>
       </c>
       <c r="O283" t="inlineStr">
@@ -19480,7 +19475,7 @@
       </c>
       <c r="N284" t="inlineStr">
         <is>
-          <t>2026-02-18T11:36:23</t>
+          <t>2026-02-18T13:35:00</t>
         </is>
       </c>
       <c r="O284" t="inlineStr">
@@ -19546,7 +19541,7 @@
       </c>
       <c r="N285" t="inlineStr">
         <is>
-          <t>2026-02-18T11:31:41</t>
+          <t>2026-02-18T13:18:17</t>
         </is>
       </c>
       <c r="O285" t="inlineStr">
@@ -19612,7 +19607,7 @@
       </c>
       <c r="N286" t="inlineStr">
         <is>
-          <t>2026-02-18T11:00:12</t>
+          <t>2026-02-18T12:49:06</t>
         </is>
       </c>
       <c r="O286" t="inlineStr">
@@ -19678,7 +19673,7 @@
       </c>
       <c r="N287" t="inlineStr">
         <is>
-          <t>2026-02-18T11:10:35</t>
+          <t>2026-02-18T12:57:58</t>
         </is>
       </c>
       <c r="O287" t="inlineStr">
@@ -19744,7 +19739,7 @@
       </c>
       <c r="N288" t="inlineStr">
         <is>
-          <t>2026-02-18T11:05:53</t>
+          <t>2026-02-18T13:01:10</t>
         </is>
       </c>
       <c r="O288" t="inlineStr">
@@ -19810,7 +19805,7 @@
       </c>
       <c r="N289" t="inlineStr">
         <is>
-          <t>2026-02-18T11:20:47</t>
+          <t>2026-02-18T13:16:06</t>
         </is>
       </c>
       <c r="O289" t="inlineStr">
@@ -20630,7 +20625,7 @@
       </c>
       <c r="N302" t="inlineStr">
         <is>
-          <t>2026-02-18T11:13:08</t>
+          <t>2026-02-18T12:58:56</t>
         </is>
       </c>
       <c r="O302" t="inlineStr">
@@ -21395,7 +21390,7 @@
       </c>
       <c r="N314" t="inlineStr">
         <is>
-          <t>2026-02-18T11:30:00</t>
+          <t>2026-02-18T13:16:35</t>
         </is>
       </c>
       <c r="O314" t="inlineStr">
@@ -21782,7 +21777,7 @@
       </c>
       <c r="N320" t="inlineStr">
         <is>
-          <t>2026-02-18T10:51:11</t>
+          <t>2026-02-18T13:38:31</t>
         </is>
       </c>
       <c r="O320" t="inlineStr">
@@ -22531,7 +22526,7 @@
       </c>
       <c r="N332" t="inlineStr">
         <is>
-          <t>2026-02-18T10:50:31</t>
+          <t>2026-02-18T13:34:17</t>
         </is>
       </c>
       <c r="O332" t="inlineStr">
@@ -22597,7 +22592,7 @@
       </c>
       <c r="N333" t="inlineStr">
         <is>
-          <t>2026-02-18T11:18:36</t>
+          <t>2026-02-18T13:08:23</t>
         </is>
       </c>
       <c r="O333" t="inlineStr">
@@ -22663,7 +22658,7 @@
       </c>
       <c r="N334" t="inlineStr">
         <is>
-          <t>2026-02-18T11:29:02</t>
+          <t>2026-02-18T13:29:33</t>
         </is>
       </c>
       <c r="O334" t="inlineStr">
@@ -22729,7 +22724,7 @@
       </c>
       <c r="N335" t="inlineStr">
         <is>
-          <t>2026-02-18T11:20:00</t>
+          <t>2026-02-18T13:05:03</t>
         </is>
       </c>
       <c r="O335" t="inlineStr">
@@ -22795,7 +22790,7 @@
       </c>
       <c r="N336" t="inlineStr">
         <is>
-          <t>2026-02-18T11:33:00</t>
+          <t>2026-02-18T13:24:49</t>
         </is>
       </c>
       <c r="O336" t="inlineStr">
@@ -22861,7 +22856,7 @@
       </c>
       <c r="N337" t="inlineStr">
         <is>
-          <t>2026-02-18T11:28:03</t>
+          <t>2026-02-18T13:24:48</t>
         </is>
       </c>
       <c r="O337" t="inlineStr">
@@ -22927,7 +22922,7 @@
       </c>
       <c r="N338" t="inlineStr">
         <is>
-          <t>2026-02-18T11:22:02</t>
+          <t>2026-02-18T13:05:19</t>
         </is>
       </c>
       <c r="O338" t="inlineStr">
@@ -22993,7 +22988,7 @@
       </c>
       <c r="N339" t="inlineStr">
         <is>
-          <t>2026-02-18T10:55:36</t>
+          <t>2026-02-18T12:50:25</t>
         </is>
       </c>
       <c r="O339" t="inlineStr">
@@ -23125,7 +23120,7 @@
       </c>
       <c r="N341" t="inlineStr">
         <is>
-          <t>2026-02-18T10:56:22</t>
+          <t>2026-02-18T13:38:02</t>
         </is>
       </c>
       <c r="O341" t="inlineStr">
@@ -23191,7 +23186,7 @@
       </c>
       <c r="N342" t="inlineStr">
         <is>
-          <t>2026-02-18T11:31:18</t>
+          <t>2026-02-18T13:17:29</t>
         </is>
       </c>
       <c r="O342" t="inlineStr">
@@ -23259,7 +23254,7 @@
       </c>
       <c r="N343" t="inlineStr">
         <is>
-          <t>2026-02-18T11:17:34</t>
+          <t>2026-02-18T13:07:22</t>
         </is>
       </c>
       <c r="O343" t="inlineStr">
@@ -23848,7 +23843,7 @@
       </c>
       <c r="N352" t="inlineStr">
         <is>
-          <t>2026-02-18T11:33:56</t>
+          <t>2026-02-18T13:19:48</t>
         </is>
       </c>
       <c r="O352" t="inlineStr">
@@ -24688,7 +24683,7 @@
       </c>
       <c r="N365" t="inlineStr">
         <is>
-          <t>2026-02-18T11:22:09</t>
+          <t>2026-02-18T13:11:27</t>
         </is>
       </c>
       <c r="O365" t="inlineStr">
@@ -24756,7 +24751,7 @@
       </c>
       <c r="N366" t="inlineStr">
         <is>
-          <t>2026-02-18T11:32:12</t>
+          <t>2026-02-18T13:30:21</t>
         </is>
       </c>
       <c r="O366" t="inlineStr">
@@ -24886,7 +24881,7 @@
       </c>
       <c r="N368" t="inlineStr">
         <is>
-          <t>2026-02-18T11:34:53</t>
+          <t>2026-02-18T13:20:42</t>
         </is>
       </c>
       <c r="O368" t="inlineStr">
@@ -24906,6 +24901,11 @@
           <t>RH</t>
         </is>
       </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>10.69.3.13</t>
+        </is>
+      </c>
       <c r="D369" t="n">
         <v>2025</v>
       </c>
@@ -24949,7 +24949,7 @@
       </c>
       <c r="N369" t="inlineStr">
         <is>
-          <t>2026-02-18T11:24:35</t>
+          <t>2026-02-18T13:35:23</t>
         </is>
       </c>
       <c r="O369" t="inlineStr">
@@ -25020,7 +25020,7 @@
       </c>
       <c r="N370" t="inlineStr">
         <is>
-          <t>2026-02-18T11:12:07</t>
+          <t>2026-02-18T13:07:05</t>
         </is>
       </c>
       <c r="O370" t="inlineStr">
@@ -25162,7 +25162,7 @@
       </c>
       <c r="N372" t="inlineStr">
         <is>
-          <t>2026-02-18T10:52:54</t>
+          <t>2026-02-18T11:53:23</t>
         </is>
       </c>
       <c r="O372" t="inlineStr">
@@ -25372,7 +25372,7 @@
       </c>
       <c r="N375" t="inlineStr">
         <is>
-          <t>2026-02-18T11:06:45</t>
+          <t>2026-02-18T12:57:57</t>
         </is>
       </c>
       <c r="O375" t="inlineStr">
@@ -25509,7 +25509,7 @@
       </c>
       <c r="N377" t="inlineStr">
         <is>
-          <t>2026-02-18T11:25:58</t>
+          <t>2026-02-18T13:13:30</t>
         </is>
       </c>
       <c r="O377" t="inlineStr">
@@ -25580,7 +25580,7 @@
       </c>
       <c r="N378" t="inlineStr">
         <is>
-          <t>2026-02-18T11:36:42</t>
+          <t>2026-02-18T13:21:58</t>
         </is>
       </c>
       <c r="O378" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática 2026-02-18 15:52:03.478280
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -601,7 +601,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>2026-02-18T13:22:51</t>
+          <t>2026-02-18T15:17:53</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -672,7 +672,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>2026-02-18T13:38:30</t>
+          <t>2026-02-18T15:29:32</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -814,7 +814,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>2026-02-18T12:52:29</t>
+          <t>2026-02-18T15:39:45</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -1103,6 +1103,11 @@
           <t>AUDITORIO</t>
         </is>
       </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>10.69.3.160</t>
+        </is>
+      </c>
       <c r="D10" t="n">
         <v>2017</v>
       </c>
@@ -1144,7 +1149,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>2026-02-18T12:57:52</t>
+          <t>2026-02-18T15:41:57</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -1474,7 +1479,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>2026-02-18T12:53:49</t>
+          <t>2026-02-18T15:39:25</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
@@ -1606,7 +1611,7 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>2026-02-18T13:11:43</t>
+          <t>2026-02-18T15:06:03</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
@@ -6885,7 +6890,7 @@
       </c>
       <c r="N95" t="inlineStr">
         <is>
-          <t>2026-02-18T12:59:00</t>
+          <t>2026-02-18T14:51:46</t>
         </is>
       </c>
       <c r="O95" t="inlineStr">
@@ -6956,7 +6961,7 @@
       </c>
       <c r="N96" t="inlineStr">
         <is>
-          <t>2026-02-18T12:48:12</t>
+          <t>2026-02-18T14:44:14</t>
         </is>
       </c>
       <c r="O96" t="inlineStr">
@@ -7022,7 +7027,7 @@
       </c>
       <c r="N97" t="inlineStr">
         <is>
-          <t>2026-02-18T13:04:08</t>
+          <t>2026-02-18T14:56:12</t>
         </is>
       </c>
       <c r="O97" t="inlineStr">
@@ -7088,7 +7093,7 @@
       </c>
       <c r="N98" t="inlineStr">
         <is>
-          <t>2026-02-18T13:24:00</t>
+          <t>2026-02-18T15:12:03</t>
         </is>
       </c>
       <c r="O98" t="inlineStr">
@@ -7159,7 +7164,7 @@
       </c>
       <c r="N99" t="inlineStr">
         <is>
-          <t>2026-02-18T13:19:13</t>
+          <t>2026-02-18T15:08:07</t>
         </is>
       </c>
       <c r="O99" t="inlineStr">
@@ -7230,7 +7235,7 @@
       </c>
       <c r="N100" t="inlineStr">
         <is>
-          <t>2026-02-18T12:49:10</t>
+          <t>2026-02-18T15:41:48</t>
         </is>
       </c>
       <c r="O100" t="inlineStr">
@@ -7301,7 +7306,7 @@
       </c>
       <c r="N101" t="inlineStr">
         <is>
-          <t>2026-02-18T13:31:53</t>
+          <t>2026-02-18T15:17:31</t>
         </is>
       </c>
       <c r="O101" t="inlineStr">
@@ -7443,7 +7448,7 @@
       </c>
       <c r="N103" t="inlineStr">
         <is>
-          <t>2026-02-18T13:37:43</t>
+          <t>2026-02-18T15:27:31</t>
         </is>
       </c>
       <c r="O103" t="inlineStr">
@@ -7708,7 +7713,7 @@
       </c>
       <c r="N107" t="inlineStr">
         <is>
-          <t>2026-02-18T13:07:46</t>
+          <t>2026-02-18T15:02:23</t>
         </is>
       </c>
       <c r="O107" t="inlineStr">
@@ -7850,7 +7855,7 @@
       </c>
       <c r="N109" t="inlineStr">
         <is>
-          <t>2026-02-18T12:46:57</t>
+          <t>2026-02-18T14:42:06</t>
         </is>
       </c>
       <c r="O109" t="inlineStr">
@@ -7921,7 +7926,7 @@
       </c>
       <c r="N110" t="inlineStr">
         <is>
-          <t>2026-02-18T12:47:01</t>
+          <t>2026-02-18T15:38:34</t>
         </is>
       </c>
       <c r="O110" t="inlineStr">
@@ -7992,7 +7997,7 @@
       </c>
       <c r="N111" t="inlineStr">
         <is>
-          <t>2026-02-18T13:29:16</t>
+          <t>2026-02-18T15:28:04</t>
         </is>
       </c>
       <c r="O111" t="inlineStr">
@@ -8063,7 +8068,7 @@
       </c>
       <c r="N112" t="inlineStr">
         <is>
-          <t>2026-02-18T13:20:08</t>
+          <t>2026-02-18T15:15:31</t>
         </is>
       </c>
       <c r="O112" t="inlineStr">
@@ -8134,7 +8139,7 @@
       </c>
       <c r="N113" t="inlineStr">
         <is>
-          <t>2026-02-18T13:32:04</t>
+          <t>2026-02-18T15:27:28</t>
         </is>
       </c>
       <c r="O113" t="inlineStr">
@@ -8205,7 +8210,7 @@
       </c>
       <c r="N114" t="inlineStr">
         <is>
-          <t>2026-02-18T13:26:36</t>
+          <t>2026-02-18T15:20:10</t>
         </is>
       </c>
       <c r="O114" t="inlineStr">
@@ -8273,7 +8278,7 @@
       </c>
       <c r="N115" t="inlineStr">
         <is>
-          <t>2026-02-18T12:47:57</t>
+          <t>2026-02-18T15:40:50</t>
         </is>
       </c>
       <c r="O115" t="inlineStr">
@@ -8344,7 +8349,7 @@
       </c>
       <c r="N116" t="inlineStr">
         <is>
-          <t>2026-02-18T13:33:09</t>
+          <t>2026-02-18T15:27:24</t>
         </is>
       </c>
       <c r="O116" t="inlineStr">
@@ -8364,6 +8369,11 @@
           <t>DP</t>
         </is>
       </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>10.69.3.23</t>
+        </is>
+      </c>
       <c r="D117" t="n">
         <v>2025</v>
       </c>
@@ -8410,7 +8420,7 @@
       </c>
       <c r="N117" t="inlineStr">
         <is>
-          <t>2026-02-18T13:19:15</t>
+          <t>2026-02-18T15:32:21</t>
         </is>
       </c>
       <c r="O117" t="inlineStr">
@@ -8620,7 +8630,7 @@
       </c>
       <c r="N120" t="inlineStr">
         <is>
-          <t>2026-02-18T13:31:59</t>
+          <t>2026-02-18T15:09:17</t>
         </is>
       </c>
       <c r="O120" t="inlineStr">
@@ -8691,7 +8701,7 @@
       </c>
       <c r="N121" t="inlineStr">
         <is>
-          <t>2026-02-18T13:11:20</t>
+          <t>2026-02-18T14:59:06</t>
         </is>
       </c>
       <c r="O121" t="inlineStr">
@@ -8759,7 +8769,7 @@
       </c>
       <c r="N122" t="inlineStr">
         <is>
-          <t>2026-02-18T13:25:39</t>
+          <t>2026-02-18T15:19:04</t>
         </is>
       </c>
       <c r="O122" t="inlineStr">
@@ -8901,7 +8911,7 @@
       </c>
       <c r="N124" t="inlineStr">
         <is>
-          <t>2026-02-18T13:37:51</t>
+          <t>2026-02-18T15:27:57</t>
         </is>
       </c>
       <c r="O124" t="inlineStr">
@@ -8972,7 +8982,7 @@
       </c>
       <c r="N125" t="inlineStr">
         <is>
-          <t>2026-02-18T13:28:12</t>
+          <t>2026-02-18T15:23:19</t>
         </is>
       </c>
       <c r="O125" t="inlineStr">
@@ -9043,7 +9053,7 @@
       </c>
       <c r="N126" t="inlineStr">
         <is>
-          <t>2026-02-18T12:44:25</t>
+          <t>2026-02-18T15:37:05</t>
         </is>
       </c>
       <c r="O126" t="inlineStr">
@@ -9114,7 +9124,7 @@
       </c>
       <c r="N127" t="inlineStr">
         <is>
-          <t>2026-02-18T13:05:01</t>
+          <t>2026-02-18T15:41:15</t>
         </is>
       </c>
       <c r="O127" t="inlineStr">
@@ -9185,7 +9195,7 @@
       </c>
       <c r="N128" t="inlineStr">
         <is>
-          <t>2026-02-18T13:36:39</t>
+          <t>2026-02-18T15:23:04</t>
         </is>
       </c>
       <c r="O128" t="inlineStr">
@@ -9256,7 +9266,7 @@
       </c>
       <c r="N129" t="inlineStr">
         <is>
-          <t>2026-02-18T13:00:52</t>
+          <t>2026-02-18T14:53:50</t>
         </is>
       </c>
       <c r="O129" t="inlineStr">
@@ -9327,7 +9337,7 @@
       </c>
       <c r="N130" t="inlineStr">
         <is>
-          <t>2026-02-18T13:37:15</t>
+          <t>2026-02-18T15:23:55</t>
         </is>
       </c>
       <c r="O130" t="inlineStr">
@@ -9398,7 +9408,7 @@
       </c>
       <c r="N131" t="inlineStr">
         <is>
-          <t>2026-02-18T13:36:15</t>
+          <t>2026-02-18T15:29:29</t>
         </is>
       </c>
       <c r="O131" t="inlineStr">
@@ -9535,7 +9545,7 @@
       </c>
       <c r="N133" t="inlineStr">
         <is>
-          <t>2026-02-18T12:53:18</t>
+          <t>2026-02-18T15:39:39</t>
         </is>
       </c>
       <c r="O133" t="inlineStr">
@@ -9601,7 +9611,7 @@
       </c>
       <c r="N134" t="inlineStr">
         <is>
-          <t>2026-02-18T13:04:49</t>
+          <t>2026-02-18T14:57:57</t>
         </is>
       </c>
       <c r="O134" t="inlineStr">
@@ -9667,7 +9677,7 @@
       </c>
       <c r="N135" t="inlineStr">
         <is>
-          <t>2026-02-18T12:52:19</t>
+          <t>2026-02-18T15:39:47</t>
         </is>
       </c>
       <c r="O135" t="inlineStr">
@@ -9864,7 +9874,7 @@
       </c>
       <c r="N138" t="inlineStr">
         <is>
-          <t>2026-02-18T13:30:55</t>
+          <t>2026-02-18T15:20:52</t>
         </is>
       </c>
       <c r="O138" t="inlineStr">
@@ -9930,7 +9940,7 @@
       </c>
       <c r="N139" t="inlineStr">
         <is>
-          <t>2026-02-18T13:26:01</t>
+          <t>2026-02-18T14:57:49</t>
         </is>
       </c>
       <c r="O139" t="inlineStr">
@@ -9996,7 +10006,7 @@
       </c>
       <c r="N140" t="inlineStr">
         <is>
-          <t>2026-02-18T13:16:22</t>
+          <t>2026-02-18T15:05:14</t>
         </is>
       </c>
       <c r="O140" t="inlineStr">
@@ -10062,7 +10072,7 @@
       </c>
       <c r="N141" t="inlineStr">
         <is>
-          <t>2026-02-18T13:37:28</t>
+          <t>2026-02-18T15:26:18</t>
         </is>
       </c>
       <c r="O141" t="inlineStr">
@@ -10128,7 +10138,7 @@
       </c>
       <c r="N142" t="inlineStr">
         <is>
-          <t>2026-02-14T14:03:13</t>
+          <t>2026-02-18T14:58:28</t>
         </is>
       </c>
       <c r="O142" t="inlineStr">
@@ -10194,7 +10204,7 @@
       </c>
       <c r="N143" t="inlineStr">
         <is>
-          <t>2026-02-14T14:18:29</t>
+          <t>2026-02-18T14:56:50</t>
         </is>
       </c>
       <c r="O143" t="inlineStr">
@@ -10260,7 +10270,7 @@
       </c>
       <c r="N144" t="inlineStr">
         <is>
-          <t>2026-02-18T13:06:37</t>
+          <t>2026-02-18T14:53:35</t>
         </is>
       </c>
       <c r="O144" t="inlineStr">
@@ -10326,7 +10336,7 @@
       </c>
       <c r="N145" t="inlineStr">
         <is>
-          <t>2026-02-18T13:09:12</t>
+          <t>2026-02-18T15:00:33</t>
         </is>
       </c>
       <c r="O145" t="inlineStr">
@@ -10392,7 +10402,7 @@
       </c>
       <c r="N146" t="inlineStr">
         <is>
-          <t>2026-02-18T12:48:33</t>
+          <t>2026-02-18T15:00:07</t>
         </is>
       </c>
       <c r="O146" t="inlineStr">
@@ -10458,7 +10468,7 @@
       </c>
       <c r="N147" t="inlineStr">
         <is>
-          <t>2026-02-18T13:36:33</t>
+          <t>2026-02-18T15:31:11</t>
         </is>
       </c>
       <c r="O147" t="inlineStr">
@@ -10524,7 +10534,7 @@
       </c>
       <c r="N148" t="inlineStr">
         <is>
-          <t>2026-02-18T13:10:49</t>
+          <t>2026-02-18T14:57:55</t>
         </is>
       </c>
       <c r="O148" t="inlineStr">
@@ -10590,7 +10600,7 @@
       </c>
       <c r="N149" t="inlineStr">
         <is>
-          <t>2026-02-14T14:17:34</t>
+          <t>2026-02-18T15:38:56</t>
         </is>
       </c>
       <c r="O149" t="inlineStr">
@@ -10722,7 +10732,7 @@
       </c>
       <c r="N151" t="inlineStr">
         <is>
-          <t>2026-02-18T13:22:30</t>
+          <t>2026-02-18T15:15:21</t>
         </is>
       </c>
       <c r="O151" t="inlineStr">
@@ -10788,7 +10798,7 @@
       </c>
       <c r="N152" t="inlineStr">
         <is>
-          <t>2026-02-18T12:50:06</t>
+          <t>2026-02-18T15:41:23</t>
         </is>
       </c>
       <c r="O152" t="inlineStr">
@@ -10849,7 +10859,7 @@
       </c>
       <c r="N153" t="inlineStr">
         <is>
-          <t>2026-02-18T12:51:51</t>
+          <t>2026-02-18T15:01:57</t>
         </is>
       </c>
       <c r="O153" t="inlineStr">
@@ -10915,7 +10925,7 @@
       </c>
       <c r="N154" t="inlineStr">
         <is>
-          <t>2026-02-18T13:03:11</t>
+          <t>2026-02-18T14:52:40</t>
         </is>
       </c>
       <c r="O154" t="inlineStr">
@@ -10981,7 +10991,7 @@
       </c>
       <c r="N155" t="inlineStr">
         <is>
-          <t>2026-02-18T13:34:33</t>
+          <t>2026-02-18T15:26:08</t>
         </is>
       </c>
       <c r="O155" t="inlineStr">
@@ -11113,7 +11123,7 @@
       </c>
       <c r="N157" t="inlineStr">
         <is>
-          <t>2026-02-18T13:39:45</t>
+          <t>2026-02-18T14:57:57</t>
         </is>
       </c>
       <c r="O157" t="inlineStr">
@@ -11245,7 +11255,7 @@
       </c>
       <c r="N159" t="inlineStr">
         <is>
-          <t>2026-02-18T13:23:28</t>
+          <t>2026-02-18T14:58:12</t>
         </is>
       </c>
       <c r="O159" t="inlineStr">
@@ -11443,7 +11453,7 @@
       </c>
       <c r="N162" t="inlineStr">
         <is>
-          <t>2026-02-18T12:59:23</t>
+          <t>2026-02-18T15:33:13</t>
         </is>
       </c>
       <c r="O162" t="inlineStr">
@@ -11575,7 +11585,7 @@
       </c>
       <c r="N164" t="inlineStr">
         <is>
-          <t>2026-02-18T13:38:07</t>
+          <t>2026-02-18T15:33:10</t>
         </is>
       </c>
       <c r="O164" t="inlineStr">
@@ -11707,7 +11717,7 @@
       </c>
       <c r="N166" t="inlineStr">
         <is>
-          <t>2026-02-18T12:56:43</t>
+          <t>2026-02-18T14:55:47</t>
         </is>
       </c>
       <c r="O166" t="inlineStr">
@@ -11773,7 +11783,7 @@
       </c>
       <c r="N167" t="inlineStr">
         <is>
-          <t>2026-02-18T13:20:12</t>
+          <t>2026-02-18T15:05:49</t>
         </is>
       </c>
       <c r="O167" t="inlineStr">
@@ -11839,7 +11849,7 @@
       </c>
       <c r="N168" t="inlineStr">
         <is>
-          <t>2026-02-18T13:00:17</t>
+          <t>2026-02-18T13:51:25</t>
         </is>
       </c>
       <c r="O168" t="inlineStr">
@@ -11905,7 +11915,7 @@
       </c>
       <c r="N169" t="inlineStr">
         <is>
-          <t>2026-02-18T12:47:20</t>
+          <t>2026-02-18T15:34:27</t>
         </is>
       </c>
       <c r="O169" t="inlineStr">
@@ -11971,7 +11981,7 @@
       </c>
       <c r="N170" t="inlineStr">
         <is>
-          <t>2026-02-18T13:32:42</t>
+          <t>2026-02-18T15:21:33</t>
         </is>
       </c>
       <c r="O170" t="inlineStr">
@@ -12033,11 +12043,11 @@
         </is>
       </c>
       <c r="M171" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N171" t="inlineStr">
         <is>
-          <t>2026-02-18T13:21:47</t>
+          <t>2026-02-18T15:14:28</t>
         </is>
       </c>
       <c r="O171" t="inlineStr">
@@ -12165,11 +12175,11 @@
         </is>
       </c>
       <c r="M173" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N173" t="inlineStr">
         <is>
-          <t>2026-02-18T13:18:03</t>
+          <t>2026-02-18T15:08:20</t>
         </is>
       </c>
       <c r="O173" t="inlineStr">
@@ -12235,7 +12245,7 @@
       </c>
       <c r="N174" t="inlineStr">
         <is>
-          <t>2026-02-18T12:51:42</t>
+          <t>2026-02-18T15:26:13</t>
         </is>
       </c>
       <c r="O174" t="inlineStr">
@@ -12301,7 +12311,7 @@
       </c>
       <c r="N175" t="inlineStr">
         <is>
-          <t>2026-02-18T13:38:34</t>
+          <t>2026-02-18T15:24:34</t>
         </is>
       </c>
       <c r="O175" t="inlineStr">
@@ -12367,7 +12377,7 @@
       </c>
       <c r="N176" t="inlineStr">
         <is>
-          <t>2026-02-18T13:12:42</t>
+          <t>2026-02-18T14:58:01</t>
         </is>
       </c>
       <c r="O176" t="inlineStr">
@@ -12433,7 +12443,7 @@
       </c>
       <c r="N177" t="inlineStr">
         <is>
-          <t>2026-02-18T13:30:34</t>
+          <t>2026-02-18T15:25:39</t>
         </is>
       </c>
       <c r="O177" t="inlineStr">
@@ -12499,7 +12509,7 @@
       </c>
       <c r="N178" t="inlineStr">
         <is>
-          <t>2026-02-18T13:25:19</t>
+          <t>2026-02-18T15:18:32</t>
         </is>
       </c>
       <c r="O178" t="inlineStr">
@@ -12631,7 +12641,7 @@
       </c>
       <c r="N180" t="inlineStr">
         <is>
-          <t>2026-02-18T13:03:35</t>
+          <t>2026-02-18T15:13:58</t>
         </is>
       </c>
       <c r="O180" t="inlineStr">
@@ -12697,7 +12707,7 @@
       </c>
       <c r="N181" t="inlineStr">
         <is>
-          <t>2026-02-14T20:08:28</t>
+          <t>2026-02-18T15:36:04</t>
         </is>
       </c>
       <c r="O181" t="inlineStr">
@@ -13032,7 +13042,7 @@
       </c>
       <c r="N186" t="inlineStr">
         <is>
-          <t>2026-02-18T13:30:19</t>
+          <t>2026-02-18T14:26:49</t>
         </is>
       </c>
       <c r="O186" t="inlineStr">
@@ -13098,7 +13108,7 @@
       </c>
       <c r="N187" t="inlineStr">
         <is>
-          <t>2026-02-18T13:29:32</t>
+          <t>2026-02-18T15:23:32</t>
         </is>
       </c>
       <c r="O187" t="inlineStr">
@@ -13164,7 +13174,7 @@
       </c>
       <c r="N188" t="inlineStr">
         <is>
-          <t>2026-02-18T13:24:22</t>
+          <t>2026-02-18T14:44:01</t>
         </is>
       </c>
       <c r="O188" t="inlineStr">
@@ -13296,7 +13306,7 @@
       </c>
       <c r="N190" t="inlineStr">
         <is>
-          <t>2026-02-18T13:03:08</t>
+          <t>2026-02-18T14:50:15</t>
         </is>
       </c>
       <c r="O190" t="inlineStr">
@@ -13362,7 +13372,7 @@
       </c>
       <c r="N191" t="inlineStr">
         <is>
-          <t>2026-02-14T14:50:48</t>
+          <t>2026-02-18T14:59:25</t>
         </is>
       </c>
       <c r="O191" t="inlineStr">
@@ -13428,7 +13438,7 @@
       </c>
       <c r="N192" t="inlineStr">
         <is>
-          <t>2026-02-14T14:36:40</t>
+          <t>2026-02-18T15:24:26</t>
         </is>
       </c>
       <c r="O192" t="inlineStr">
@@ -13557,7 +13567,7 @@
       </c>
       <c r="N194" t="inlineStr">
         <is>
-          <t>2026-02-18T07:57:11</t>
+          <t>2026-02-18T14:36:06</t>
         </is>
       </c>
       <c r="O194" t="inlineStr">
@@ -13623,7 +13633,7 @@
       </c>
       <c r="N195" t="inlineStr">
         <is>
-          <t>2026-02-18T12:47:54</t>
+          <t>2026-02-18T15:37:55</t>
         </is>
       </c>
       <c r="O195" t="inlineStr">
@@ -13689,7 +13699,7 @@
       </c>
       <c r="N196" t="inlineStr">
         <is>
-          <t>2026-02-18T13:37:18</t>
+          <t>2026-02-18T15:05:44</t>
         </is>
       </c>
       <c r="O196" t="inlineStr">
@@ -13755,7 +13765,7 @@
       </c>
       <c r="N197" t="inlineStr">
         <is>
-          <t>2026-02-18T13:22:28</t>
+          <t>2026-02-18T14:50:27</t>
         </is>
       </c>
       <c r="O197" t="inlineStr">
@@ -13821,7 +13831,7 @@
       </c>
       <c r="N198" t="inlineStr">
         <is>
-          <t>2026-02-18T13:37:52</t>
+          <t>2026-02-18T15:30:22</t>
         </is>
       </c>
       <c r="O198" t="inlineStr">
@@ -13887,7 +13897,7 @@
       </c>
       <c r="N199" t="inlineStr">
         <is>
-          <t>2026-02-13T19:10:31</t>
+          <t>2026-02-18T15:02:56</t>
         </is>
       </c>
       <c r="O199" t="inlineStr">
@@ -13953,7 +13963,7 @@
       </c>
       <c r="N200" t="inlineStr">
         <is>
-          <t>2026-02-13T19:44:19</t>
+          <t>2026-02-18T15:00:50</t>
         </is>
       </c>
       <c r="O200" t="inlineStr">
@@ -14082,7 +14092,7 @@
       </c>
       <c r="N202" t="inlineStr">
         <is>
-          <t>2026-02-18T13:27:58</t>
+          <t>2026-02-18T15:05:28</t>
         </is>
       </c>
       <c r="O202" t="inlineStr">
@@ -14148,7 +14158,7 @@
       </c>
       <c r="N203" t="inlineStr">
         <is>
-          <t>2026-02-18T13:21:40</t>
+          <t>2026-02-18T15:01:09</t>
         </is>
       </c>
       <c r="O203" t="inlineStr">
@@ -14214,7 +14224,7 @@
       </c>
       <c r="N204" t="inlineStr">
         <is>
-          <t>2026-02-18T13:15:41</t>
+          <t>2026-02-18T15:07:46</t>
         </is>
       </c>
       <c r="O204" t="inlineStr">
@@ -14280,7 +14290,7 @@
       </c>
       <c r="N205" t="inlineStr">
         <is>
-          <t>2026-02-18T12:51:10</t>
+          <t>2026-02-18T15:40:57</t>
         </is>
       </c>
       <c r="O205" t="inlineStr">
@@ -14346,7 +14356,7 @@
       </c>
       <c r="N206" t="inlineStr">
         <is>
-          <t>2026-02-18T13:33:08</t>
+          <t>2026-02-18T15:30:07</t>
         </is>
       </c>
       <c r="O206" t="inlineStr">
@@ -14412,7 +14422,7 @@
       </c>
       <c r="N207" t="inlineStr">
         <is>
-          <t>2026-02-18T13:36:24</t>
+          <t>2026-02-18T15:35:02</t>
         </is>
       </c>
       <c r="O207" t="inlineStr">
@@ -14544,7 +14554,7 @@
       </c>
       <c r="N209" t="inlineStr">
         <is>
-          <t>2026-02-18T13:38:38</t>
+          <t>2026-02-18T15:26:12</t>
         </is>
       </c>
       <c r="O209" t="inlineStr">
@@ -14610,7 +14620,7 @@
       </c>
       <c r="N210" t="inlineStr">
         <is>
-          <t>2026-02-18T13:30:56</t>
+          <t>2026-02-18T15:27:40</t>
         </is>
       </c>
       <c r="O210" t="inlineStr">
@@ -14676,7 +14686,7 @@
       </c>
       <c r="N211" t="inlineStr">
         <is>
-          <t>2026-02-18T12:59:21</t>
+          <t>2026-02-18T14:53:10</t>
         </is>
       </c>
       <c r="O211" t="inlineStr">
@@ -14742,7 +14752,7 @@
       </c>
       <c r="N212" t="inlineStr">
         <is>
-          <t>2026-02-18T13:05:14</t>
+          <t>2026-02-18T15:01:42</t>
         </is>
       </c>
       <c r="O212" t="inlineStr">
@@ -14808,7 +14818,7 @@
       </c>
       <c r="N213" t="inlineStr">
         <is>
-          <t>2026-02-18T13:37:59</t>
+          <t>2026-02-18T14:58:03</t>
         </is>
       </c>
       <c r="O213" t="inlineStr">
@@ -14874,7 +14884,7 @@
       </c>
       <c r="N214" t="inlineStr">
         <is>
-          <t>2026-02-14T09:03:27</t>
+          <t>2026-02-18T14:56:30</t>
         </is>
       </c>
       <c r="O214" t="inlineStr">
@@ -14940,7 +14950,7 @@
       </c>
       <c r="N215" t="inlineStr">
         <is>
-          <t>2026-02-18T13:38:49</t>
+          <t>2026-02-18T14:56:47</t>
         </is>
       </c>
       <c r="O215" t="inlineStr">
@@ -15006,7 +15016,7 @@
       </c>
       <c r="N216" t="inlineStr">
         <is>
-          <t>2026-02-18T13:15:35</t>
+          <t>2026-02-18T15:08:46</t>
         </is>
       </c>
       <c r="O216" t="inlineStr">
@@ -15072,7 +15082,7 @@
       </c>
       <c r="N217" t="inlineStr">
         <is>
-          <t>2026-02-18T13:37:26</t>
+          <t>2026-02-18T15:30:04</t>
         </is>
       </c>
       <c r="O217" t="inlineStr">
@@ -15138,7 +15148,7 @@
       </c>
       <c r="N218" t="inlineStr">
         <is>
-          <t>2026-02-18T13:34:28</t>
+          <t>2026-02-18T15:29:06</t>
         </is>
       </c>
       <c r="O218" t="inlineStr">
@@ -15204,7 +15214,7 @@
       </c>
       <c r="N219" t="inlineStr">
         <is>
-          <t>2026-02-18T13:07:19</t>
+          <t>2026-02-18T14:03:58</t>
         </is>
       </c>
       <c r="O219" t="inlineStr">
@@ -15275,7 +15285,7 @@
       </c>
       <c r="N220" t="inlineStr">
         <is>
-          <t>2026-02-18T12:47:34</t>
+          <t>2026-02-18T14:46:20</t>
         </is>
       </c>
       <c r="O220" t="inlineStr">
@@ -15341,7 +15351,7 @@
       </c>
       <c r="N221" t="inlineStr">
         <is>
-          <t>2026-02-14T14:27:04</t>
+          <t>2026-02-18T15:03:25</t>
         </is>
       </c>
       <c r="O221" t="inlineStr">
@@ -15407,7 +15417,7 @@
       </c>
       <c r="N222" t="inlineStr">
         <is>
-          <t>2026-02-13T19:36:24</t>
+          <t>2026-02-18T15:38:27</t>
         </is>
       </c>
       <c r="O222" t="inlineStr">
@@ -15473,7 +15483,7 @@
       </c>
       <c r="N223" t="inlineStr">
         <is>
-          <t>2026-02-18T13:04:46</t>
+          <t>2026-02-18T15:11:43</t>
         </is>
       </c>
       <c r="O223" t="inlineStr">
@@ -15539,7 +15549,7 @@
       </c>
       <c r="N224" t="inlineStr">
         <is>
-          <t>2026-02-14T14:42:15</t>
+          <t>2026-02-18T15:04:51</t>
         </is>
       </c>
       <c r="O224" t="inlineStr">
@@ -15605,7 +15615,7 @@
       </c>
       <c r="N225" t="inlineStr">
         <is>
-          <t>2026-02-18T13:03:51</t>
+          <t>2026-02-18T14:57:26</t>
         </is>
       </c>
       <c r="O225" t="inlineStr">
@@ -15671,7 +15681,7 @@
       </c>
       <c r="N226" t="inlineStr">
         <is>
-          <t>2026-02-18T13:35:33</t>
+          <t>2026-02-18T14:56:14</t>
         </is>
       </c>
       <c r="O226" t="inlineStr">
@@ -15737,7 +15747,7 @@
       </c>
       <c r="N227" t="inlineStr">
         <is>
-          <t>2026-02-18T13:36:29</t>
+          <t>2026-02-18T15:30:13</t>
         </is>
       </c>
       <c r="O227" t="inlineStr">
@@ -15803,7 +15813,7 @@
       </c>
       <c r="N228" t="inlineStr">
         <is>
-          <t>2026-02-14T14:14:29</t>
+          <t>2026-02-18T15:02:30</t>
         </is>
       </c>
       <c r="O228" t="inlineStr">
@@ -15935,7 +15945,7 @@
       </c>
       <c r="N230" t="inlineStr">
         <is>
-          <t>2026-02-18T12:52:42</t>
+          <t>2026-02-18T15:12:23</t>
         </is>
       </c>
       <c r="O230" t="inlineStr">
@@ -16001,7 +16011,7 @@
       </c>
       <c r="N231" t="inlineStr">
         <is>
-          <t>2026-02-18T13:24:05</t>
+          <t>2026-02-18T15:10:57</t>
         </is>
       </c>
       <c r="O231" t="inlineStr">
@@ -16067,7 +16077,7 @@
       </c>
       <c r="N232" t="inlineStr">
         <is>
-          <t>2026-02-18T13:25:06</t>
+          <t>2026-02-18T15:20:33</t>
         </is>
       </c>
       <c r="O232" t="inlineStr">
@@ -16133,7 +16143,7 @@
       </c>
       <c r="N233" t="inlineStr">
         <is>
-          <t>2026-02-18T13:01:40</t>
+          <t>2026-02-18T14:55:35</t>
         </is>
       </c>
       <c r="O233" t="inlineStr">
@@ -16199,7 +16209,7 @@
       </c>
       <c r="N234" t="inlineStr">
         <is>
-          <t>2026-02-13T19:09:29</t>
+          <t>2026-02-18T15:18:09</t>
         </is>
       </c>
       <c r="O234" t="inlineStr">
@@ -16265,7 +16275,7 @@
       </c>
       <c r="N235" t="inlineStr">
         <is>
-          <t>2026-02-13T19:02:52</t>
+          <t>2026-02-18T15:00:46</t>
         </is>
       </c>
       <c r="O235" t="inlineStr">
@@ -16331,7 +16341,7 @@
       </c>
       <c r="N236" t="inlineStr">
         <is>
-          <t>2026-02-13T19:50:39</t>
+          <t>2026-02-18T14:59:00</t>
         </is>
       </c>
       <c r="O236" t="inlineStr">
@@ -16397,7 +16407,7 @@
       </c>
       <c r="N237" t="inlineStr">
         <is>
-          <t>2026-02-13T19:19:08</t>
+          <t>2026-02-18T15:02:40</t>
         </is>
       </c>
       <c r="O237" t="inlineStr">
@@ -16463,7 +16473,7 @@
       </c>
       <c r="N238" t="inlineStr">
         <is>
-          <t>2026-02-18T13:26:37</t>
+          <t>2026-02-18T15:16:28</t>
         </is>
       </c>
       <c r="O238" t="inlineStr">
@@ -16529,7 +16539,7 @@
       </c>
       <c r="N239" t="inlineStr">
         <is>
-          <t>2026-02-18T13:10:08</t>
+          <t>2026-02-18T15:06:28</t>
         </is>
       </c>
       <c r="O239" t="inlineStr">
@@ -16595,7 +16605,7 @@
       </c>
       <c r="N240" t="inlineStr">
         <is>
-          <t>2026-02-18T13:08:13</t>
+          <t>2026-02-18T15:02:37</t>
         </is>
       </c>
       <c r="O240" t="inlineStr">
@@ -16661,7 +16671,7 @@
       </c>
       <c r="N241" t="inlineStr">
         <is>
-          <t>2026-02-18T13:14:05</t>
+          <t>2026-02-18T14:14:05</t>
         </is>
       </c>
       <c r="O241" t="inlineStr">
@@ -16727,7 +16737,7 @@
       </c>
       <c r="N242" t="inlineStr">
         <is>
-          <t>2026-02-18T13:13:44</t>
+          <t>2026-02-18T15:05:08</t>
         </is>
       </c>
       <c r="O242" t="inlineStr">
@@ -16793,7 +16803,7 @@
       </c>
       <c r="N243" t="inlineStr">
         <is>
-          <t>2026-02-18T13:17:31</t>
+          <t>2026-02-18T15:05:40</t>
         </is>
       </c>
       <c r="O243" t="inlineStr">
@@ -16854,7 +16864,7 @@
       </c>
       <c r="N244" t="inlineStr">
         <is>
-          <t>2026-02-13T19:30:26</t>
+          <t>2026-02-18T14:58:25</t>
         </is>
       </c>
       <c r="O244" t="inlineStr">
@@ -16920,7 +16930,7 @@
       </c>
       <c r="N245" t="inlineStr">
         <is>
-          <t>2026-02-18T12:59:41</t>
+          <t>2026-02-18T14:51:43</t>
         </is>
       </c>
       <c r="O245" t="inlineStr">
@@ -16986,7 +16996,7 @@
       </c>
       <c r="N246" t="inlineStr">
         <is>
-          <t>2026-02-18T12:53:55</t>
+          <t>2026-02-18T15:35:29</t>
         </is>
       </c>
       <c r="O246" t="inlineStr">
@@ -17052,7 +17062,7 @@
       </c>
       <c r="N247" t="inlineStr">
         <is>
-          <t>2026-02-18T13:03:12</t>
+          <t>2026-02-18T14:57:37</t>
         </is>
       </c>
       <c r="O247" t="inlineStr">
@@ -17118,7 +17128,7 @@
       </c>
       <c r="N248" t="inlineStr">
         <is>
-          <t>2026-02-18T12:53:59</t>
+          <t>2026-02-18T15:40:44</t>
         </is>
       </c>
       <c r="O248" t="inlineStr">
@@ -17184,7 +17194,7 @@
       </c>
       <c r="N249" t="inlineStr">
         <is>
-          <t>2026-02-18T13:42:11</t>
+          <t>2026-02-18T15:26:23</t>
         </is>
       </c>
       <c r="O249" t="inlineStr">
@@ -17245,7 +17255,7 @@
       </c>
       <c r="N250" t="inlineStr">
         <is>
-          <t>2026-02-18T13:00:54</t>
+          <t>2026-02-18T14:50:59</t>
         </is>
       </c>
       <c r="O250" t="inlineStr">
@@ -17311,7 +17321,7 @@
       </c>
       <c r="N251" t="inlineStr">
         <is>
-          <t>2026-02-18T13:28:29</t>
+          <t>2026-02-18T15:21:51</t>
         </is>
       </c>
       <c r="O251" t="inlineStr">
@@ -17377,7 +17387,7 @@
       </c>
       <c r="N252" t="inlineStr">
         <is>
-          <t>2026-02-18T13:05:54</t>
+          <t>2026-02-18T15:38:58</t>
         </is>
       </c>
       <c r="O252" t="inlineStr">
@@ -17443,7 +17453,7 @@
       </c>
       <c r="N253" t="inlineStr">
         <is>
-          <t>2026-02-18T13:11:27</t>
+          <t>2026-02-18T14:54:29</t>
         </is>
       </c>
       <c r="O253" t="inlineStr">
@@ -17503,7 +17513,7 @@
       </c>
       <c r="N254" t="inlineStr">
         <is>
-          <t>2026-02-18T12:56:36</t>
+          <t>2026-02-18T15:13:50</t>
         </is>
       </c>
       <c r="O254" t="inlineStr">
@@ -17569,7 +17579,7 @@
       </c>
       <c r="N255" t="inlineStr">
         <is>
-          <t>2026-02-18T12:50:06</t>
+          <t>2026-02-18T15:40:00</t>
         </is>
       </c>
       <c r="O255" t="inlineStr">
@@ -17635,7 +17645,7 @@
       </c>
       <c r="N256" t="inlineStr">
         <is>
-          <t>2026-02-18T13:32:43</t>
+          <t>2026-02-18T15:27:41</t>
         </is>
       </c>
       <c r="O256" t="inlineStr">
@@ -17701,7 +17711,7 @@
       </c>
       <c r="N257" t="inlineStr">
         <is>
-          <t>2026-02-14T13:15:29</t>
+          <t>2026-02-18T15:11:00</t>
         </is>
       </c>
       <c r="O257" t="inlineStr">
@@ -17767,7 +17777,7 @@
       </c>
       <c r="N258" t="inlineStr">
         <is>
-          <t>2026-02-18T12:48:43</t>
+          <t>2026-02-18T15:37:38</t>
         </is>
       </c>
       <c r="O258" t="inlineStr">
@@ -17833,7 +17843,7 @@
       </c>
       <c r="N259" t="inlineStr">
         <is>
-          <t>2026-02-18T12:59:18</t>
+          <t>2026-02-18T15:35:19</t>
         </is>
       </c>
       <c r="O259" t="inlineStr">
@@ -17899,7 +17909,7 @@
       </c>
       <c r="N260" t="inlineStr">
         <is>
-          <t>2026-02-18T13:02:43</t>
+          <t>2026-02-18T14:01:31</t>
         </is>
       </c>
       <c r="O260" t="inlineStr">
@@ -18031,7 +18041,7 @@
       </c>
       <c r="N262" t="inlineStr">
         <is>
-          <t>2026-02-18T13:32:14</t>
+          <t>2026-02-18T15:28:52</t>
         </is>
       </c>
       <c r="O262" t="inlineStr">
@@ -18097,7 +18107,7 @@
       </c>
       <c r="N263" t="inlineStr">
         <is>
-          <t>2026-02-18T13:26:21</t>
+          <t>2026-02-18T14:59:48</t>
         </is>
       </c>
       <c r="O263" t="inlineStr">
@@ -18163,7 +18173,7 @@
       </c>
       <c r="N264" t="inlineStr">
         <is>
-          <t>2026-02-18T13:19:28</t>
+          <t>2026-02-18T15:11:47</t>
         </is>
       </c>
       <c r="O264" t="inlineStr">
@@ -18229,7 +18239,7 @@
       </c>
       <c r="N265" t="inlineStr">
         <is>
-          <t>2026-02-18T13:24:38</t>
+          <t>2026-02-18T15:02:29</t>
         </is>
       </c>
       <c r="O265" t="inlineStr">
@@ -18295,7 +18305,7 @@
       </c>
       <c r="N266" t="inlineStr">
         <is>
-          <t>2026-02-18T12:53:03</t>
+          <t>2026-02-18T14:43:33</t>
         </is>
       </c>
       <c r="O266" t="inlineStr">
@@ -18361,7 +18371,7 @@
       </c>
       <c r="N267" t="inlineStr">
         <is>
-          <t>2026-02-18T12:48:00</t>
+          <t>2026-02-18T15:36:35</t>
         </is>
       </c>
       <c r="O267" t="inlineStr">
@@ -18427,7 +18437,7 @@
       </c>
       <c r="N268" t="inlineStr">
         <is>
-          <t>2026-02-18T13:38:59</t>
+          <t>2026-02-18T15:35:04</t>
         </is>
       </c>
       <c r="O268" t="inlineStr">
@@ -18493,7 +18503,7 @@
       </c>
       <c r="N269" t="inlineStr">
         <is>
-          <t>2026-02-18T13:12:23</t>
+          <t>2026-02-18T15:01:28</t>
         </is>
       </c>
       <c r="O269" t="inlineStr">
@@ -18556,7 +18566,7 @@
       </c>
       <c r="N270" t="inlineStr">
         <is>
-          <t>2026-02-18T12:47:49</t>
+          <t>2026-02-18T15:38:30</t>
         </is>
       </c>
       <c r="O270" t="inlineStr">
@@ -18688,7 +18698,7 @@
       </c>
       <c r="N272" t="inlineStr">
         <is>
-          <t>2026-02-18T13:31:35</t>
+          <t>2026-02-18T14:53:50</t>
         </is>
       </c>
       <c r="O272" t="inlineStr">
@@ -18754,7 +18764,7 @@
       </c>
       <c r="N273" t="inlineStr">
         <is>
-          <t>2026-02-18T13:02:50</t>
+          <t>2026-02-18T15:04:10</t>
         </is>
       </c>
       <c r="O273" t="inlineStr">
@@ -19084,7 +19094,7 @@
       </c>
       <c r="N278" t="inlineStr">
         <is>
-          <t>2026-02-18T12:46:40</t>
+          <t>2026-02-18T15:29:02</t>
         </is>
       </c>
       <c r="O278" t="inlineStr">
@@ -19216,7 +19226,7 @@
       </c>
       <c r="N280" t="inlineStr">
         <is>
-          <t>2026-02-18T13:15:21</t>
+          <t>2026-02-18T15:06:27</t>
         </is>
       </c>
       <c r="O280" t="inlineStr">
@@ -19343,7 +19353,7 @@
       </c>
       <c r="N282" t="inlineStr">
         <is>
-          <t>2026-02-18T13:02:01</t>
+          <t>2026-02-18T14:50:29</t>
         </is>
       </c>
       <c r="O282" t="inlineStr">
@@ -19409,7 +19419,7 @@
       </c>
       <c r="N283" t="inlineStr">
         <is>
-          <t>2026-02-18T13:31:37</t>
+          <t>2026-02-18T15:19:00</t>
         </is>
       </c>
       <c r="O283" t="inlineStr">
@@ -19475,7 +19485,7 @@
       </c>
       <c r="N284" t="inlineStr">
         <is>
-          <t>2026-02-18T13:35:00</t>
+          <t>2026-02-18T15:23:20</t>
         </is>
       </c>
       <c r="O284" t="inlineStr">
@@ -19607,7 +19617,7 @@
       </c>
       <c r="N286" t="inlineStr">
         <is>
-          <t>2026-02-18T12:49:06</t>
+          <t>2026-02-18T15:38:12</t>
         </is>
       </c>
       <c r="O286" t="inlineStr">
@@ -19673,7 +19683,7 @@
       </c>
       <c r="N287" t="inlineStr">
         <is>
-          <t>2026-02-18T12:57:58</t>
+          <t>2026-02-18T13:52:20</t>
         </is>
       </c>
       <c r="O287" t="inlineStr">
@@ -19805,7 +19815,7 @@
       </c>
       <c r="N289" t="inlineStr">
         <is>
-          <t>2026-02-18T13:16:06</t>
+          <t>2026-02-18T15:10:26</t>
         </is>
       </c>
       <c r="O289" t="inlineStr">
@@ -20625,7 +20635,7 @@
       </c>
       <c r="N302" t="inlineStr">
         <is>
-          <t>2026-02-18T12:58:56</t>
+          <t>2026-02-18T14:49:31</t>
         </is>
       </c>
       <c r="O302" t="inlineStr">
@@ -21390,7 +21400,7 @@
       </c>
       <c r="N314" t="inlineStr">
         <is>
-          <t>2026-02-18T13:16:35</t>
+          <t>2026-02-18T15:11:26</t>
         </is>
       </c>
       <c r="O314" t="inlineStr">
@@ -21777,7 +21787,7 @@
       </c>
       <c r="N320" t="inlineStr">
         <is>
-          <t>2026-02-18T13:38:31</t>
+          <t>2026-02-18T15:35:54</t>
         </is>
       </c>
       <c r="O320" t="inlineStr">
@@ -22526,7 +22536,7 @@
       </c>
       <c r="N332" t="inlineStr">
         <is>
-          <t>2026-02-18T13:34:17</t>
+          <t>2026-02-18T15:28:28</t>
         </is>
       </c>
       <c r="O332" t="inlineStr">
@@ -22592,7 +22602,7 @@
       </c>
       <c r="N333" t="inlineStr">
         <is>
-          <t>2026-02-18T13:08:23</t>
+          <t>2026-02-18T14:58:13</t>
         </is>
       </c>
       <c r="O333" t="inlineStr">
@@ -22658,7 +22668,7 @@
       </c>
       <c r="N334" t="inlineStr">
         <is>
-          <t>2026-02-18T13:29:33</t>
+          <t>2026-02-18T15:21:32</t>
         </is>
       </c>
       <c r="O334" t="inlineStr">
@@ -22724,7 +22734,7 @@
       </c>
       <c r="N335" t="inlineStr">
         <is>
-          <t>2026-02-18T13:05:03</t>
+          <t>2026-02-18T14:56:14</t>
         </is>
       </c>
       <c r="O335" t="inlineStr">
@@ -22856,7 +22866,7 @@
       </c>
       <c r="N337" t="inlineStr">
         <is>
-          <t>2026-02-18T13:24:48</t>
+          <t>2026-02-18T15:25:30</t>
         </is>
       </c>
       <c r="O337" t="inlineStr">
@@ -22922,7 +22932,7 @@
       </c>
       <c r="N338" t="inlineStr">
         <is>
-          <t>2026-02-18T13:05:19</t>
+          <t>2026-02-18T14:59:46</t>
         </is>
       </c>
       <c r="O338" t="inlineStr">
@@ -22988,7 +22998,7 @@
       </c>
       <c r="N339" t="inlineStr">
         <is>
-          <t>2026-02-18T12:50:25</t>
+          <t>2026-02-18T15:34:17</t>
         </is>
       </c>
       <c r="O339" t="inlineStr">
@@ -23206,11 +23216,6 @@
           <t>OPERACAO 9.1</t>
         </is>
       </c>
-      <c r="C343" t="inlineStr">
-        <is>
-          <t>10.69.5.237</t>
-        </is>
-      </c>
       <c r="D343" t="n">
         <v>2017</v>
       </c>
@@ -23254,7 +23259,7 @@
       </c>
       <c r="N343" t="inlineStr">
         <is>
-          <t>2026-02-18T13:07:22</t>
+          <t>2026-02-18T14:57:20</t>
         </is>
       </c>
       <c r="O343" t="inlineStr">
@@ -23843,7 +23848,7 @@
       </c>
       <c r="N352" t="inlineStr">
         <is>
-          <t>2026-02-18T13:19:48</t>
+          <t>2026-02-18T15:06:20</t>
         </is>
       </c>
       <c r="O352" t="inlineStr">
@@ -24683,7 +24688,7 @@
       </c>
       <c r="N365" t="inlineStr">
         <is>
-          <t>2026-02-18T13:11:27</t>
+          <t>2026-02-18T14:58:27</t>
         </is>
       </c>
       <c r="O365" t="inlineStr">
@@ -24751,7 +24756,7 @@
       </c>
       <c r="N366" t="inlineStr">
         <is>
-          <t>2026-02-18T13:30:21</t>
+          <t>2026-02-18T15:25:21</t>
         </is>
       </c>
       <c r="O366" t="inlineStr">
@@ -24881,7 +24886,7 @@
       </c>
       <c r="N368" t="inlineStr">
         <is>
-          <t>2026-02-18T13:20:42</t>
+          <t>2026-02-18T15:09:01</t>
         </is>
       </c>
       <c r="O368" t="inlineStr">
@@ -24901,11 +24906,6 @@
           <t>RH</t>
         </is>
       </c>
-      <c r="C369" t="inlineStr">
-        <is>
-          <t>10.69.3.13</t>
-        </is>
-      </c>
       <c r="D369" t="n">
         <v>2025</v>
       </c>
@@ -24949,7 +24949,7 @@
       </c>
       <c r="N369" t="inlineStr">
         <is>
-          <t>2026-02-18T13:35:23</t>
+          <t>2026-02-18T15:29:46</t>
         </is>
       </c>
       <c r="O369" t="inlineStr">
@@ -25020,7 +25020,7 @@
       </c>
       <c r="N370" t="inlineStr">
         <is>
-          <t>2026-02-18T13:07:05</t>
+          <t>2026-02-18T14:59:08</t>
         </is>
       </c>
       <c r="O370" t="inlineStr">
@@ -25372,7 +25372,7 @@
       </c>
       <c r="N375" t="inlineStr">
         <is>
-          <t>2026-02-18T12:57:57</t>
+          <t>2026-02-18T14:52:49</t>
         </is>
       </c>
       <c r="O375" t="inlineStr">
@@ -25509,7 +25509,7 @@
       </c>
       <c r="N377" t="inlineStr">
         <is>
-          <t>2026-02-18T13:13:30</t>
+          <t>2026-02-18T14:57:13</t>
         </is>
       </c>
       <c r="O377" t="inlineStr">
@@ -25580,7 +25580,7 @@
       </c>
       <c r="N378" t="inlineStr">
         <is>
-          <t>2026-02-18T13:21:58</t>
+          <t>2026-02-18T15:05:11</t>
         </is>
       </c>
       <c r="O378" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática 2026-02-18 17:52:04.932024
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -601,7 +601,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>2026-02-18T15:17:53</t>
+          <t>2026-02-18T17:09:20</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -672,7 +672,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>2026-02-18T15:29:32</t>
+          <t>2026-02-18T17:26:05</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -814,7 +814,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>2026-02-18T15:39:45</t>
+          <t>2026-02-18T16:32:07</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -1103,11 +1103,6 @@
           <t>AUDITORIO</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>10.69.3.160</t>
-        </is>
-      </c>
       <c r="D10" t="n">
         <v>2017</v>
       </c>
@@ -1149,7 +1144,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>2026-02-18T15:41:57</t>
+          <t>2026-02-18T17:32:20</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -1479,7 +1474,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>2026-02-18T15:39:25</t>
+          <t>2026-02-18T17:38:22</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
@@ -1611,7 +1606,7 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>2026-02-18T15:06:03</t>
+          <t>2026-02-18T17:05:12</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
@@ -6890,7 +6885,7 @@
       </c>
       <c r="N95" t="inlineStr">
         <is>
-          <t>2026-02-18T14:51:46</t>
+          <t>2026-02-18T16:44:03</t>
         </is>
       </c>
       <c r="O95" t="inlineStr">
@@ -6961,7 +6956,7 @@
       </c>
       <c r="N96" t="inlineStr">
         <is>
-          <t>2026-02-18T14:44:14</t>
+          <t>2026-02-18T17:36:05</t>
         </is>
       </c>
       <c r="O96" t="inlineStr">
@@ -6981,6 +6976,11 @@
           <t>COORDENACAO</t>
         </is>
       </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>10.69.3.93</t>
+        </is>
+      </c>
       <c r="D97" t="n">
         <v>2025</v>
       </c>
@@ -7027,7 +7027,7 @@
       </c>
       <c r="N97" t="inlineStr">
         <is>
-          <t>2026-02-18T14:56:12</t>
+          <t>2026-02-18T17:40:29</t>
         </is>
       </c>
       <c r="O97" t="inlineStr">
@@ -7093,7 +7093,7 @@
       </c>
       <c r="N98" t="inlineStr">
         <is>
-          <t>2026-02-18T15:12:03</t>
+          <t>2026-02-18T16:04:16</t>
         </is>
       </c>
       <c r="O98" t="inlineStr">
@@ -7164,7 +7164,7 @@
       </c>
       <c r="N99" t="inlineStr">
         <is>
-          <t>2026-02-18T15:08:07</t>
+          <t>2026-02-18T15:59:14</t>
         </is>
       </c>
       <c r="O99" t="inlineStr">
@@ -7235,7 +7235,7 @@
       </c>
       <c r="N100" t="inlineStr">
         <is>
-          <t>2026-02-18T15:41:48</t>
+          <t>2026-02-18T17:32:28</t>
         </is>
       </c>
       <c r="O100" t="inlineStr">
@@ -7306,7 +7306,7 @@
       </c>
       <c r="N101" t="inlineStr">
         <is>
-          <t>2026-02-18T15:17:31</t>
+          <t>2026-02-18T17:05:22</t>
         </is>
       </c>
       <c r="O101" t="inlineStr">
@@ -7448,7 +7448,7 @@
       </c>
       <c r="N103" t="inlineStr">
         <is>
-          <t>2026-02-18T15:27:31</t>
+          <t>2026-02-18T17:18:30</t>
         </is>
       </c>
       <c r="O103" t="inlineStr">
@@ -7713,7 +7713,7 @@
       </c>
       <c r="N107" t="inlineStr">
         <is>
-          <t>2026-02-18T15:02:23</t>
+          <t>2026-02-18T16:55:29</t>
         </is>
       </c>
       <c r="O107" t="inlineStr">
@@ -7855,7 +7855,7 @@
       </c>
       <c r="N109" t="inlineStr">
         <is>
-          <t>2026-02-18T14:42:06</t>
+          <t>2026-02-18T17:30:47</t>
         </is>
       </c>
       <c r="O109" t="inlineStr">
@@ -7926,7 +7926,7 @@
       </c>
       <c r="N110" t="inlineStr">
         <is>
-          <t>2026-02-18T15:38:34</t>
+          <t>2026-02-18T17:31:17</t>
         </is>
       </c>
       <c r="O110" t="inlineStr">
@@ -7997,7 +7997,7 @@
       </c>
       <c r="N111" t="inlineStr">
         <is>
-          <t>2026-02-18T15:28:04</t>
+          <t>2026-02-18T16:23:15</t>
         </is>
       </c>
       <c r="O111" t="inlineStr">
@@ -8068,7 +8068,7 @@
       </c>
       <c r="N112" t="inlineStr">
         <is>
-          <t>2026-02-18T15:15:31</t>
+          <t>2026-02-18T17:08:38</t>
         </is>
       </c>
       <c r="O112" t="inlineStr">
@@ -8139,7 +8139,7 @@
       </c>
       <c r="N113" t="inlineStr">
         <is>
-          <t>2026-02-18T15:27:28</t>
+          <t>2026-02-18T17:28:40</t>
         </is>
       </c>
       <c r="O113" t="inlineStr">
@@ -8210,7 +8210,7 @@
       </c>
       <c r="N114" t="inlineStr">
         <is>
-          <t>2026-02-18T15:20:10</t>
+          <t>2026-02-18T17:19:37</t>
         </is>
       </c>
       <c r="O114" t="inlineStr">
@@ -8278,7 +8278,7 @@
       </c>
       <c r="N115" t="inlineStr">
         <is>
-          <t>2026-02-18T15:40:50</t>
+          <t>2026-02-18T17:33:06</t>
         </is>
       </c>
       <c r="O115" t="inlineStr">
@@ -8349,7 +8349,7 @@
       </c>
       <c r="N116" t="inlineStr">
         <is>
-          <t>2026-02-18T15:27:24</t>
+          <t>2026-02-18T16:19:54</t>
         </is>
       </c>
       <c r="O116" t="inlineStr">
@@ -8369,11 +8369,6 @@
           <t>DP</t>
         </is>
       </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>10.69.3.23</t>
-        </is>
-      </c>
       <c r="D117" t="n">
         <v>2025</v>
       </c>
@@ -8420,7 +8415,7 @@
       </c>
       <c r="N117" t="inlineStr">
         <is>
-          <t>2026-02-18T15:32:21</t>
+          <t>2026-02-18T16:29:23</t>
         </is>
       </c>
       <c r="O117" t="inlineStr">
@@ -8630,7 +8625,7 @@
       </c>
       <c r="N120" t="inlineStr">
         <is>
-          <t>2026-02-18T15:09:17</t>
+          <t>2026-02-18T17:09:29</t>
         </is>
       </c>
       <c r="O120" t="inlineStr">
@@ -8701,7 +8696,7 @@
       </c>
       <c r="N121" t="inlineStr">
         <is>
-          <t>2026-02-18T14:59:06</t>
+          <t>2026-02-18T16:43:55</t>
         </is>
       </c>
       <c r="O121" t="inlineStr">
@@ -8769,7 +8764,7 @@
       </c>
       <c r="N122" t="inlineStr">
         <is>
-          <t>2026-02-18T15:19:04</t>
+          <t>2026-02-18T17:37:19</t>
         </is>
       </c>
       <c r="O122" t="inlineStr">
@@ -8911,7 +8906,7 @@
       </c>
       <c r="N124" t="inlineStr">
         <is>
-          <t>2026-02-18T15:27:57</t>
+          <t>2026-02-18T17:14:39</t>
         </is>
       </c>
       <c r="O124" t="inlineStr">
@@ -8982,7 +8977,7 @@
       </c>
       <c r="N125" t="inlineStr">
         <is>
-          <t>2026-02-18T15:23:19</t>
+          <t>2026-02-18T16:19:15</t>
         </is>
       </c>
       <c r="O125" t="inlineStr">
@@ -9124,7 +9119,7 @@
       </c>
       <c r="N127" t="inlineStr">
         <is>
-          <t>2026-02-18T15:41:15</t>
+          <t>2026-02-18T16:36:34</t>
         </is>
       </c>
       <c r="O127" t="inlineStr">
@@ -9195,7 +9190,7 @@
       </c>
       <c r="N128" t="inlineStr">
         <is>
-          <t>2026-02-18T15:23:04</t>
+          <t>2026-02-18T16:23:18</t>
         </is>
       </c>
       <c r="O128" t="inlineStr">
@@ -9266,7 +9261,7 @@
       </c>
       <c r="N129" t="inlineStr">
         <is>
-          <t>2026-02-18T14:53:50</t>
+          <t>2026-02-18T17:37:42</t>
         </is>
       </c>
       <c r="O129" t="inlineStr">
@@ -9337,7 +9332,7 @@
       </c>
       <c r="N130" t="inlineStr">
         <is>
-          <t>2026-02-18T15:23:55</t>
+          <t>2026-02-18T17:22:31</t>
         </is>
       </c>
       <c r="O130" t="inlineStr">
@@ -9357,11 +9352,6 @@
           <t>ADM/FIN</t>
         </is>
       </c>
-      <c r="C131" t="inlineStr">
-        <is>
-          <t>10.69.3.6</t>
-        </is>
-      </c>
       <c r="D131" t="n">
         <v>2025</v>
       </c>
@@ -9408,7 +9398,7 @@
       </c>
       <c r="N131" t="inlineStr">
         <is>
-          <t>2026-02-18T15:29:29</t>
+          <t>2026-02-18T17:21:39</t>
         </is>
       </c>
       <c r="O131" t="inlineStr">
@@ -9545,7 +9535,7 @@
       </c>
       <c r="N133" t="inlineStr">
         <is>
-          <t>2026-02-18T15:39:39</t>
+          <t>2026-02-18T17:25:11</t>
         </is>
       </c>
       <c r="O133" t="inlineStr">
@@ -9611,7 +9601,7 @@
       </c>
       <c r="N134" t="inlineStr">
         <is>
-          <t>2026-02-18T14:57:57</t>
+          <t>2026-02-18T17:37:39</t>
         </is>
       </c>
       <c r="O134" t="inlineStr">
@@ -9677,7 +9667,7 @@
       </c>
       <c r="N135" t="inlineStr">
         <is>
-          <t>2026-02-18T15:39:47</t>
+          <t>2026-02-18T17:31:33</t>
         </is>
       </c>
       <c r="O135" t="inlineStr">
@@ -9874,7 +9864,7 @@
       </c>
       <c r="N138" t="inlineStr">
         <is>
-          <t>2026-02-18T15:20:52</t>
+          <t>2026-02-18T17:06:50</t>
         </is>
       </c>
       <c r="O138" t="inlineStr">
@@ -9940,7 +9930,7 @@
       </c>
       <c r="N139" t="inlineStr">
         <is>
-          <t>2026-02-18T14:57:49</t>
+          <t>2026-02-18T17:40:19</t>
         </is>
       </c>
       <c r="O139" t="inlineStr">
@@ -10006,7 +9996,7 @@
       </c>
       <c r="N140" t="inlineStr">
         <is>
-          <t>2026-02-18T15:05:14</t>
+          <t>2026-02-18T17:02:12</t>
         </is>
       </c>
       <c r="O140" t="inlineStr">
@@ -10072,7 +10062,7 @@
       </c>
       <c r="N141" t="inlineStr">
         <is>
-          <t>2026-02-18T15:26:18</t>
+          <t>2026-02-18T17:24:16</t>
         </is>
       </c>
       <c r="O141" t="inlineStr">
@@ -10138,7 +10128,7 @@
       </c>
       <c r="N142" t="inlineStr">
         <is>
-          <t>2026-02-18T14:58:28</t>
+          <t>2026-02-18T16:45:36</t>
         </is>
       </c>
       <c r="O142" t="inlineStr">
@@ -10204,7 +10194,7 @@
       </c>
       <c r="N143" t="inlineStr">
         <is>
-          <t>2026-02-18T14:56:50</t>
+          <t>2026-02-18T16:52:00</t>
         </is>
       </c>
       <c r="O143" t="inlineStr">
@@ -10270,7 +10260,7 @@
       </c>
       <c r="N144" t="inlineStr">
         <is>
-          <t>2026-02-18T14:53:35</t>
+          <t>2026-02-18T16:52:29</t>
         </is>
       </c>
       <c r="O144" t="inlineStr">
@@ -10336,7 +10326,7 @@
       </c>
       <c r="N145" t="inlineStr">
         <is>
-          <t>2026-02-18T15:00:33</t>
+          <t>2026-02-18T16:58:53</t>
         </is>
       </c>
       <c r="O145" t="inlineStr">
@@ -10402,7 +10392,7 @@
       </c>
       <c r="N146" t="inlineStr">
         <is>
-          <t>2026-02-18T15:00:07</t>
+          <t>2026-02-18T16:55:41</t>
         </is>
       </c>
       <c r="O146" t="inlineStr">
@@ -10468,7 +10458,7 @@
       </c>
       <c r="N147" t="inlineStr">
         <is>
-          <t>2026-02-18T15:31:11</t>
+          <t>2026-02-18T17:24:03</t>
         </is>
       </c>
       <c r="O147" t="inlineStr">
@@ -10534,7 +10524,7 @@
       </c>
       <c r="N148" t="inlineStr">
         <is>
-          <t>2026-02-18T14:57:55</t>
+          <t>2026-02-18T16:51:02</t>
         </is>
       </c>
       <c r="O148" t="inlineStr">
@@ -10600,7 +10590,7 @@
       </c>
       <c r="N149" t="inlineStr">
         <is>
-          <t>2026-02-18T15:38:56</t>
+          <t>2026-02-18T17:34:18</t>
         </is>
       </c>
       <c r="O149" t="inlineStr">
@@ -10732,7 +10722,7 @@
       </c>
       <c r="N151" t="inlineStr">
         <is>
-          <t>2026-02-18T15:15:21</t>
+          <t>2026-02-18T17:08:40</t>
         </is>
       </c>
       <c r="O151" t="inlineStr">
@@ -10798,7 +10788,7 @@
       </c>
       <c r="N152" t="inlineStr">
         <is>
-          <t>2026-02-18T15:41:23</t>
+          <t>2026-02-18T17:39:53</t>
         </is>
       </c>
       <c r="O152" t="inlineStr">
@@ -10859,7 +10849,7 @@
       </c>
       <c r="N153" t="inlineStr">
         <is>
-          <t>2026-02-18T15:01:57</t>
+          <t>2026-02-18T16:54:53</t>
         </is>
       </c>
       <c r="O153" t="inlineStr">
@@ -10925,7 +10915,7 @@
       </c>
       <c r="N154" t="inlineStr">
         <is>
-          <t>2026-02-18T14:52:40</t>
+          <t>2026-02-18T17:38:16</t>
         </is>
       </c>
       <c r="O154" t="inlineStr">
@@ -10991,7 +10981,7 @@
       </c>
       <c r="N155" t="inlineStr">
         <is>
-          <t>2026-02-18T15:26:08</t>
+          <t>2026-02-18T17:18:50</t>
         </is>
       </c>
       <c r="O155" t="inlineStr">
@@ -11123,7 +11113,7 @@
       </c>
       <c r="N157" t="inlineStr">
         <is>
-          <t>2026-02-18T14:57:57</t>
+          <t>2026-02-18T16:59:20</t>
         </is>
       </c>
       <c r="O157" t="inlineStr">
@@ -11255,7 +11245,7 @@
       </c>
       <c r="N159" t="inlineStr">
         <is>
-          <t>2026-02-18T14:58:12</t>
+          <t>2026-02-18T16:53:41</t>
         </is>
       </c>
       <c r="O159" t="inlineStr">
@@ -11453,7 +11443,7 @@
       </c>
       <c r="N162" t="inlineStr">
         <is>
-          <t>2026-02-18T15:33:13</t>
+          <t>2026-02-18T17:21:48</t>
         </is>
       </c>
       <c r="O162" t="inlineStr">
@@ -11585,7 +11575,7 @@
       </c>
       <c r="N164" t="inlineStr">
         <is>
-          <t>2026-02-18T15:33:10</t>
+          <t>2026-02-18T17:21:32</t>
         </is>
       </c>
       <c r="O164" t="inlineStr">
@@ -11783,7 +11773,7 @@
       </c>
       <c r="N167" t="inlineStr">
         <is>
-          <t>2026-02-18T15:05:49</t>
+          <t>2026-02-18T16:54:08</t>
         </is>
       </c>
       <c r="O167" t="inlineStr">
@@ -11915,7 +11905,7 @@
       </c>
       <c r="N169" t="inlineStr">
         <is>
-          <t>2026-02-18T15:34:27</t>
+          <t>2026-02-18T17:21:33</t>
         </is>
       </c>
       <c r="O169" t="inlineStr">
@@ -11981,7 +11971,7 @@
       </c>
       <c r="N170" t="inlineStr">
         <is>
-          <t>2026-02-18T15:21:33</t>
+          <t>2026-02-18T16:14:14</t>
         </is>
       </c>
       <c r="O170" t="inlineStr">
@@ -12047,7 +12037,7 @@
       </c>
       <c r="N171" t="inlineStr">
         <is>
-          <t>2026-02-18T15:14:28</t>
+          <t>2026-02-18T16:59:42</t>
         </is>
       </c>
       <c r="O171" t="inlineStr">
@@ -12179,7 +12169,7 @@
       </c>
       <c r="N173" t="inlineStr">
         <is>
-          <t>2026-02-18T15:08:20</t>
+          <t>2026-02-18T17:00:58</t>
         </is>
       </c>
       <c r="O173" t="inlineStr">
@@ -12245,7 +12235,7 @@
       </c>
       <c r="N174" t="inlineStr">
         <is>
-          <t>2026-02-18T15:26:13</t>
+          <t>2026-02-18T17:09:23</t>
         </is>
       </c>
       <c r="O174" t="inlineStr">
@@ -12311,7 +12301,7 @@
       </c>
       <c r="N175" t="inlineStr">
         <is>
-          <t>2026-02-18T15:24:34</t>
+          <t>2026-02-18T17:11:14</t>
         </is>
       </c>
       <c r="O175" t="inlineStr">
@@ -12377,7 +12367,7 @@
       </c>
       <c r="N176" t="inlineStr">
         <is>
-          <t>2026-02-18T14:58:01</t>
+          <t>2026-02-18T15:55:07</t>
         </is>
       </c>
       <c r="O176" t="inlineStr">
@@ -12443,7 +12433,7 @@
       </c>
       <c r="N177" t="inlineStr">
         <is>
-          <t>2026-02-18T15:25:39</t>
+          <t>2026-02-18T16:22:09</t>
         </is>
       </c>
       <c r="O177" t="inlineStr">
@@ -12509,7 +12499,7 @@
       </c>
       <c r="N178" t="inlineStr">
         <is>
-          <t>2026-02-18T15:18:32</t>
+          <t>2026-02-18T17:08:22</t>
         </is>
       </c>
       <c r="O178" t="inlineStr">
@@ -12641,7 +12631,7 @@
       </c>
       <c r="N180" t="inlineStr">
         <is>
-          <t>2026-02-18T15:13:58</t>
+          <t>2026-02-18T17:06:16</t>
         </is>
       </c>
       <c r="O180" t="inlineStr">
@@ -12707,7 +12697,7 @@
       </c>
       <c r="N181" t="inlineStr">
         <is>
-          <t>2026-02-18T15:36:04</t>
+          <t>2026-02-18T17:22:45</t>
         </is>
       </c>
       <c r="O181" t="inlineStr">
@@ -13108,7 +13098,7 @@
       </c>
       <c r="N187" t="inlineStr">
         <is>
-          <t>2026-02-18T15:23:32</t>
+          <t>2026-02-18T17:16:40</t>
         </is>
       </c>
       <c r="O187" t="inlineStr">
@@ -13174,7 +13164,7 @@
       </c>
       <c r="N188" t="inlineStr">
         <is>
-          <t>2026-02-18T14:44:01</t>
+          <t>2026-02-18T17:37:07</t>
         </is>
       </c>
       <c r="O188" t="inlineStr">
@@ -13306,7 +13296,7 @@
       </c>
       <c r="N190" t="inlineStr">
         <is>
-          <t>2026-02-18T14:50:15</t>
+          <t>2026-02-18T17:35:42</t>
         </is>
       </c>
       <c r="O190" t="inlineStr">
@@ -13372,7 +13362,7 @@
       </c>
       <c r="N191" t="inlineStr">
         <is>
-          <t>2026-02-18T14:59:25</t>
+          <t>2026-02-18T16:50:27</t>
         </is>
       </c>
       <c r="O191" t="inlineStr">
@@ -13438,7 +13428,7 @@
       </c>
       <c r="N192" t="inlineStr">
         <is>
-          <t>2026-02-18T15:24:26</t>
+          <t>2026-02-18T17:16:48</t>
         </is>
       </c>
       <c r="O192" t="inlineStr">
@@ -13633,7 +13623,7 @@
       </c>
       <c r="N195" t="inlineStr">
         <is>
-          <t>2026-02-18T15:37:55</t>
+          <t>2026-02-18T17:32:12</t>
         </is>
       </c>
       <c r="O195" t="inlineStr">
@@ -13699,7 +13689,7 @@
       </c>
       <c r="N196" t="inlineStr">
         <is>
-          <t>2026-02-18T15:05:44</t>
+          <t>2026-02-18T17:04:07</t>
         </is>
       </c>
       <c r="O196" t="inlineStr">
@@ -13765,7 +13755,7 @@
       </c>
       <c r="N197" t="inlineStr">
         <is>
-          <t>2026-02-18T14:50:27</t>
+          <t>2026-02-18T17:40:31</t>
         </is>
       </c>
       <c r="O197" t="inlineStr">
@@ -13831,7 +13821,7 @@
       </c>
       <c r="N198" t="inlineStr">
         <is>
-          <t>2026-02-18T15:30:22</t>
+          <t>2026-02-18T16:27:54</t>
         </is>
       </c>
       <c r="O198" t="inlineStr">
@@ -13897,7 +13887,7 @@
       </c>
       <c r="N199" t="inlineStr">
         <is>
-          <t>2026-02-18T15:02:56</t>
+          <t>2026-02-18T17:38:22</t>
         </is>
       </c>
       <c r="O199" t="inlineStr">
@@ -13963,7 +13953,7 @@
       </c>
       <c r="N200" t="inlineStr">
         <is>
-          <t>2026-02-18T15:00:50</t>
+          <t>2026-02-18T16:50:49</t>
         </is>
       </c>
       <c r="O200" t="inlineStr">
@@ -14026,7 +14016,7 @@
       </c>
       <c r="N201" t="inlineStr">
         <is>
-          <t>2026-02-13T19:21:01</t>
+          <t>2026-02-18T16:54:00</t>
         </is>
       </c>
       <c r="O201" t="inlineStr">
@@ -14092,7 +14082,7 @@
       </c>
       <c r="N202" t="inlineStr">
         <is>
-          <t>2026-02-18T15:05:28</t>
+          <t>2026-02-18T16:59:53</t>
         </is>
       </c>
       <c r="O202" t="inlineStr">
@@ -14158,7 +14148,7 @@
       </c>
       <c r="N203" t="inlineStr">
         <is>
-          <t>2026-02-18T15:01:09</t>
+          <t>2026-02-18T17:40:52</t>
         </is>
       </c>
       <c r="O203" t="inlineStr">
@@ -14224,7 +14214,7 @@
       </c>
       <c r="N204" t="inlineStr">
         <is>
-          <t>2026-02-18T15:07:46</t>
+          <t>2026-02-18T17:04:20</t>
         </is>
       </c>
       <c r="O204" t="inlineStr">
@@ -14290,7 +14280,7 @@
       </c>
       <c r="N205" t="inlineStr">
         <is>
-          <t>2026-02-18T15:40:57</t>
+          <t>2026-02-18T17:40:04</t>
         </is>
       </c>
       <c r="O205" t="inlineStr">
@@ -14356,7 +14346,7 @@
       </c>
       <c r="N206" t="inlineStr">
         <is>
-          <t>2026-02-18T15:30:07</t>
+          <t>2026-02-18T17:30:15</t>
         </is>
       </c>
       <c r="O206" t="inlineStr">
@@ -14422,7 +14412,7 @@
       </c>
       <c r="N207" t="inlineStr">
         <is>
-          <t>2026-02-18T15:35:02</t>
+          <t>2026-02-18T17:24:14</t>
         </is>
       </c>
       <c r="O207" t="inlineStr">
@@ -14554,7 +14544,7 @@
       </c>
       <c r="N209" t="inlineStr">
         <is>
-          <t>2026-02-18T15:26:12</t>
+          <t>2026-02-18T17:20:46</t>
         </is>
       </c>
       <c r="O209" t="inlineStr">
@@ -14620,7 +14610,7 @@
       </c>
       <c r="N210" t="inlineStr">
         <is>
-          <t>2026-02-18T15:27:40</t>
+          <t>2026-02-18T17:19:23</t>
         </is>
       </c>
       <c r="O210" t="inlineStr">
@@ -14686,7 +14676,7 @@
       </c>
       <c r="N211" t="inlineStr">
         <is>
-          <t>2026-02-18T14:53:10</t>
+          <t>2026-02-18T16:47:45</t>
         </is>
       </c>
       <c r="O211" t="inlineStr">
@@ -14752,7 +14742,7 @@
       </c>
       <c r="N212" t="inlineStr">
         <is>
-          <t>2026-02-18T15:01:42</t>
+          <t>2026-02-18T16:50:50</t>
         </is>
       </c>
       <c r="O212" t="inlineStr">
@@ -14818,7 +14808,7 @@
       </c>
       <c r="N213" t="inlineStr">
         <is>
-          <t>2026-02-18T14:58:03</t>
+          <t>2026-02-18T16:54:46</t>
         </is>
       </c>
       <c r="O213" t="inlineStr">
@@ -14884,7 +14874,7 @@
       </c>
       <c r="N214" t="inlineStr">
         <is>
-          <t>2026-02-18T14:56:30</t>
+          <t>2026-02-18T16:47:28</t>
         </is>
       </c>
       <c r="O214" t="inlineStr">
@@ -14950,7 +14940,7 @@
       </c>
       <c r="N215" t="inlineStr">
         <is>
-          <t>2026-02-18T14:56:47</t>
+          <t>2026-02-18T16:53:28</t>
         </is>
       </c>
       <c r="O215" t="inlineStr">
@@ -15016,7 +15006,7 @@
       </c>
       <c r="N216" t="inlineStr">
         <is>
-          <t>2026-02-18T15:08:46</t>
+          <t>2026-02-18T16:53:18</t>
         </is>
       </c>
       <c r="O216" t="inlineStr">
@@ -15082,7 +15072,7 @@
       </c>
       <c r="N217" t="inlineStr">
         <is>
-          <t>2026-02-18T15:30:04</t>
+          <t>2026-02-18T17:13:28</t>
         </is>
       </c>
       <c r="O217" t="inlineStr">
@@ -15148,7 +15138,7 @@
       </c>
       <c r="N218" t="inlineStr">
         <is>
-          <t>2026-02-18T15:29:06</t>
+          <t>2026-02-18T17:19:30</t>
         </is>
       </c>
       <c r="O218" t="inlineStr">
@@ -15214,7 +15204,7 @@
       </c>
       <c r="N219" t="inlineStr">
         <is>
-          <t>2026-02-18T14:03:58</t>
+          <t>2026-02-18T15:54:46</t>
         </is>
       </c>
       <c r="O219" t="inlineStr">
@@ -15285,7 +15275,7 @@
       </c>
       <c r="N220" t="inlineStr">
         <is>
-          <t>2026-02-18T14:46:20</t>
+          <t>2026-02-18T17:36:53</t>
         </is>
       </c>
       <c r="O220" t="inlineStr">
@@ -15351,7 +15341,7 @@
       </c>
       <c r="N221" t="inlineStr">
         <is>
-          <t>2026-02-18T15:03:25</t>
+          <t>2026-02-18T16:53:46</t>
         </is>
       </c>
       <c r="O221" t="inlineStr">
@@ -15417,7 +15407,7 @@
       </c>
       <c r="N222" t="inlineStr">
         <is>
-          <t>2026-02-18T15:38:27</t>
+          <t>2026-02-18T17:33:26</t>
         </is>
       </c>
       <c r="O222" t="inlineStr">
@@ -15483,7 +15473,7 @@
       </c>
       <c r="N223" t="inlineStr">
         <is>
-          <t>2026-02-18T15:11:43</t>
+          <t>2026-02-18T17:03:30</t>
         </is>
       </c>
       <c r="O223" t="inlineStr">
@@ -15549,7 +15539,7 @@
       </c>
       <c r="N224" t="inlineStr">
         <is>
-          <t>2026-02-18T15:04:51</t>
+          <t>2026-02-18T16:56:13</t>
         </is>
       </c>
       <c r="O224" t="inlineStr">
@@ -15615,7 +15605,7 @@
       </c>
       <c r="N225" t="inlineStr">
         <is>
-          <t>2026-02-18T14:57:26</t>
+          <t>2026-02-18T16:53:20</t>
         </is>
       </c>
       <c r="O225" t="inlineStr">
@@ -15681,7 +15671,7 @@
       </c>
       <c r="N226" t="inlineStr">
         <is>
-          <t>2026-02-18T14:56:14</t>
+          <t>2026-02-18T16:44:37</t>
         </is>
       </c>
       <c r="O226" t="inlineStr">
@@ -15747,7 +15737,7 @@
       </c>
       <c r="N227" t="inlineStr">
         <is>
-          <t>2026-02-18T15:30:13</t>
+          <t>2026-02-18T17:13:39</t>
         </is>
       </c>
       <c r="O227" t="inlineStr">
@@ -15813,7 +15803,7 @@
       </c>
       <c r="N228" t="inlineStr">
         <is>
-          <t>2026-02-18T15:02:30</t>
+          <t>2026-02-18T16:52:40</t>
         </is>
       </c>
       <c r="O228" t="inlineStr">
@@ -15945,7 +15935,7 @@
       </c>
       <c r="N230" t="inlineStr">
         <is>
-          <t>2026-02-18T15:12:23</t>
+          <t>2026-02-18T17:11:01</t>
         </is>
       </c>
       <c r="O230" t="inlineStr">
@@ -16011,7 +16001,7 @@
       </c>
       <c r="N231" t="inlineStr">
         <is>
-          <t>2026-02-18T15:10:57</t>
+          <t>2026-02-18T16:49:00</t>
         </is>
       </c>
       <c r="O231" t="inlineStr">
@@ -16077,7 +16067,7 @@
       </c>
       <c r="N232" t="inlineStr">
         <is>
-          <t>2026-02-18T15:20:33</t>
+          <t>2026-02-18T17:16:06</t>
         </is>
       </c>
       <c r="O232" t="inlineStr">
@@ -16143,7 +16133,7 @@
       </c>
       <c r="N233" t="inlineStr">
         <is>
-          <t>2026-02-18T14:55:35</t>
+          <t>2026-02-18T16:45:20</t>
         </is>
       </c>
       <c r="O233" t="inlineStr">
@@ -16209,7 +16199,7 @@
       </c>
       <c r="N234" t="inlineStr">
         <is>
-          <t>2026-02-18T15:18:09</t>
+          <t>2026-02-18T17:14:23</t>
         </is>
       </c>
       <c r="O234" t="inlineStr">
@@ -16275,7 +16265,7 @@
       </c>
       <c r="N235" t="inlineStr">
         <is>
-          <t>2026-02-18T15:00:46</t>
+          <t>2026-02-18T16:55:05</t>
         </is>
       </c>
       <c r="O235" t="inlineStr">
@@ -16341,7 +16331,7 @@
       </c>
       <c r="N236" t="inlineStr">
         <is>
-          <t>2026-02-18T14:59:00</t>
+          <t>2026-02-18T16:55:56</t>
         </is>
       </c>
       <c r="O236" t="inlineStr">
@@ -16407,7 +16397,7 @@
       </c>
       <c r="N237" t="inlineStr">
         <is>
-          <t>2026-02-18T15:02:40</t>
+          <t>2026-02-18T17:01:17</t>
         </is>
       </c>
       <c r="O237" t="inlineStr">
@@ -16473,7 +16463,7 @@
       </c>
       <c r="N238" t="inlineStr">
         <is>
-          <t>2026-02-18T15:16:28</t>
+          <t>2026-02-18T17:04:53</t>
         </is>
       </c>
       <c r="O238" t="inlineStr">
@@ -16539,7 +16529,7 @@
       </c>
       <c r="N239" t="inlineStr">
         <is>
-          <t>2026-02-18T15:06:28</t>
+          <t>2026-02-18T16:54:23</t>
         </is>
       </c>
       <c r="O239" t="inlineStr">
@@ -16605,7 +16595,7 @@
       </c>
       <c r="N240" t="inlineStr">
         <is>
-          <t>2026-02-18T15:02:37</t>
+          <t>2026-02-18T16:55:35</t>
         </is>
       </c>
       <c r="O240" t="inlineStr">
@@ -16737,7 +16727,7 @@
       </c>
       <c r="N242" t="inlineStr">
         <is>
-          <t>2026-02-18T15:05:08</t>
+          <t>2026-02-18T16:54:07</t>
         </is>
       </c>
       <c r="O242" t="inlineStr">
@@ -16803,7 +16793,7 @@
       </c>
       <c r="N243" t="inlineStr">
         <is>
-          <t>2026-02-18T15:05:40</t>
+          <t>2026-02-18T17:06:10</t>
         </is>
       </c>
       <c r="O243" t="inlineStr">
@@ -16864,7 +16854,7 @@
       </c>
       <c r="N244" t="inlineStr">
         <is>
-          <t>2026-02-18T14:58:25</t>
+          <t>2026-02-18T17:01:32</t>
         </is>
       </c>
       <c r="O244" t="inlineStr">
@@ -16930,7 +16920,7 @@
       </c>
       <c r="N245" t="inlineStr">
         <is>
-          <t>2026-02-18T14:51:43</t>
+          <t>2026-02-18T17:40:46</t>
         </is>
       </c>
       <c r="O245" t="inlineStr">
@@ -16996,7 +16986,7 @@
       </c>
       <c r="N246" t="inlineStr">
         <is>
-          <t>2026-02-18T15:35:29</t>
+          <t>2026-02-18T17:28:28</t>
         </is>
       </c>
       <c r="O246" t="inlineStr">
@@ -17062,7 +17052,7 @@
       </c>
       <c r="N247" t="inlineStr">
         <is>
-          <t>2026-02-18T14:57:37</t>
+          <t>2026-02-18T17:41:36</t>
         </is>
       </c>
       <c r="O247" t="inlineStr">
@@ -17128,7 +17118,7 @@
       </c>
       <c r="N248" t="inlineStr">
         <is>
-          <t>2026-02-18T15:40:44</t>
+          <t>2026-02-18T17:21:00</t>
         </is>
       </c>
       <c r="O248" t="inlineStr">
@@ -17194,7 +17184,7 @@
       </c>
       <c r="N249" t="inlineStr">
         <is>
-          <t>2026-02-18T15:26:23</t>
+          <t>2026-02-18T17:16:33</t>
         </is>
       </c>
       <c r="O249" t="inlineStr">
@@ -17255,7 +17245,7 @@
       </c>
       <c r="N250" t="inlineStr">
         <is>
-          <t>2026-02-18T14:50:59</t>
+          <t>2026-02-18T17:37:20</t>
         </is>
       </c>
       <c r="O250" t="inlineStr">
@@ -17321,7 +17311,7 @@
       </c>
       <c r="N251" t="inlineStr">
         <is>
-          <t>2026-02-18T15:21:51</t>
+          <t>2026-02-18T17:12:06</t>
         </is>
       </c>
       <c r="O251" t="inlineStr">
@@ -17387,7 +17377,7 @@
       </c>
       <c r="N252" t="inlineStr">
         <is>
-          <t>2026-02-18T15:38:58</t>
+          <t>2026-02-18T17:30:50</t>
         </is>
       </c>
       <c r="O252" t="inlineStr">
@@ -17453,7 +17443,7 @@
       </c>
       <c r="N253" t="inlineStr">
         <is>
-          <t>2026-02-18T14:54:29</t>
+          <t>2026-02-18T16:52:46</t>
         </is>
       </c>
       <c r="O253" t="inlineStr">
@@ -17513,7 +17503,7 @@
       </c>
       <c r="N254" t="inlineStr">
         <is>
-          <t>2026-02-18T15:13:50</t>
+          <t>2026-02-18T17:05:28</t>
         </is>
       </c>
       <c r="O254" t="inlineStr">
@@ -17579,7 +17569,7 @@
       </c>
       <c r="N255" t="inlineStr">
         <is>
-          <t>2026-02-18T15:40:00</t>
+          <t>2026-02-18T17:33:45</t>
         </is>
       </c>
       <c r="O255" t="inlineStr">
@@ -17645,7 +17635,7 @@
       </c>
       <c r="N256" t="inlineStr">
         <is>
-          <t>2026-02-18T15:27:41</t>
+          <t>2026-02-18T17:25:25</t>
         </is>
       </c>
       <c r="O256" t="inlineStr">
@@ -17711,7 +17701,7 @@
       </c>
       <c r="N257" t="inlineStr">
         <is>
-          <t>2026-02-18T15:11:00</t>
+          <t>2026-02-18T17:09:23</t>
         </is>
       </c>
       <c r="O257" t="inlineStr">
@@ -17777,7 +17767,7 @@
       </c>
       <c r="N258" t="inlineStr">
         <is>
-          <t>2026-02-18T15:37:38</t>
+          <t>2026-02-18T17:26:26</t>
         </is>
       </c>
       <c r="O258" t="inlineStr">
@@ -17843,7 +17833,7 @@
       </c>
       <c r="N259" t="inlineStr">
         <is>
-          <t>2026-02-18T15:35:19</t>
+          <t>2026-02-18T17:25:55</t>
         </is>
       </c>
       <c r="O259" t="inlineStr">
@@ -17975,7 +17965,7 @@
       </c>
       <c r="N261" t="inlineStr">
         <is>
-          <t>2026-02-18T13:36:16</t>
+          <t>2026-02-18T15:52:16</t>
         </is>
       </c>
       <c r="O261" t="inlineStr">
@@ -18041,7 +18031,7 @@
       </c>
       <c r="N262" t="inlineStr">
         <is>
-          <t>2026-02-18T15:28:52</t>
+          <t>2026-02-18T16:21:43</t>
         </is>
       </c>
       <c r="O262" t="inlineStr">
@@ -18107,7 +18097,7 @@
       </c>
       <c r="N263" t="inlineStr">
         <is>
-          <t>2026-02-18T14:59:48</t>
+          <t>2026-02-18T16:48:42</t>
         </is>
       </c>
       <c r="O263" t="inlineStr">
@@ -18173,7 +18163,7 @@
       </c>
       <c r="N264" t="inlineStr">
         <is>
-          <t>2026-02-18T15:11:47</t>
+          <t>2026-02-18T17:01:22</t>
         </is>
       </c>
       <c r="O264" t="inlineStr">
@@ -18239,7 +18229,7 @@
       </c>
       <c r="N265" t="inlineStr">
         <is>
-          <t>2026-02-18T15:02:29</t>
+          <t>2026-02-18T16:59:43</t>
         </is>
       </c>
       <c r="O265" t="inlineStr">
@@ -18305,7 +18295,7 @@
       </c>
       <c r="N266" t="inlineStr">
         <is>
-          <t>2026-02-18T14:43:33</t>
+          <t>2026-02-18T17:31:06</t>
         </is>
       </c>
       <c r="O266" t="inlineStr">
@@ -18371,7 +18361,7 @@
       </c>
       <c r="N267" t="inlineStr">
         <is>
-          <t>2026-02-18T15:36:35</t>
+          <t>2026-02-18T17:30:00</t>
         </is>
       </c>
       <c r="O267" t="inlineStr">
@@ -18437,7 +18427,7 @@
       </c>
       <c r="N268" t="inlineStr">
         <is>
-          <t>2026-02-18T15:35:04</t>
+          <t>2026-02-18T17:29:11</t>
         </is>
       </c>
       <c r="O268" t="inlineStr">
@@ -18503,7 +18493,7 @@
       </c>
       <c r="N269" t="inlineStr">
         <is>
-          <t>2026-02-18T15:01:28</t>
+          <t>2026-02-18T17:24:14</t>
         </is>
       </c>
       <c r="O269" t="inlineStr">
@@ -18566,7 +18556,7 @@
       </c>
       <c r="N270" t="inlineStr">
         <is>
-          <t>2026-02-18T15:38:30</t>
+          <t>2026-02-18T17:27:07</t>
         </is>
       </c>
       <c r="O270" t="inlineStr">
@@ -18698,7 +18688,7 @@
       </c>
       <c r="N272" t="inlineStr">
         <is>
-          <t>2026-02-18T14:53:50</t>
+          <t>2026-02-18T17:00:27</t>
         </is>
       </c>
       <c r="O272" t="inlineStr">
@@ -18764,7 +18754,7 @@
       </c>
       <c r="N273" t="inlineStr">
         <is>
-          <t>2026-02-18T15:04:10</t>
+          <t>2026-02-18T17:38:43</t>
         </is>
       </c>
       <c r="O273" t="inlineStr">
@@ -19094,7 +19084,7 @@
       </c>
       <c r="N278" t="inlineStr">
         <is>
-          <t>2026-02-18T15:29:02</t>
+          <t>2026-02-18T17:30:08</t>
         </is>
       </c>
       <c r="O278" t="inlineStr">
@@ -19226,7 +19216,7 @@
       </c>
       <c r="N280" t="inlineStr">
         <is>
-          <t>2026-02-18T15:06:27</t>
+          <t>2026-02-18T16:51:56</t>
         </is>
       </c>
       <c r="O280" t="inlineStr">
@@ -19353,7 +19343,7 @@
       </c>
       <c r="N282" t="inlineStr">
         <is>
-          <t>2026-02-18T14:50:29</t>
+          <t>2026-02-18T16:49:07</t>
         </is>
       </c>
       <c r="O282" t="inlineStr">
@@ -19419,7 +19409,7 @@
       </c>
       <c r="N283" t="inlineStr">
         <is>
-          <t>2026-02-18T15:19:00</t>
+          <t>2026-02-18T17:08:43</t>
         </is>
       </c>
       <c r="O283" t="inlineStr">
@@ -19485,7 +19475,7 @@
       </c>
       <c r="N284" t="inlineStr">
         <is>
-          <t>2026-02-18T15:23:20</t>
+          <t>2026-02-18T17:14:32</t>
         </is>
       </c>
       <c r="O284" t="inlineStr">
@@ -19617,7 +19607,7 @@
       </c>
       <c r="N286" t="inlineStr">
         <is>
-          <t>2026-02-18T15:38:12</t>
+          <t>2026-02-18T17:25:12</t>
         </is>
       </c>
       <c r="O286" t="inlineStr">
@@ -19815,7 +19805,7 @@
       </c>
       <c r="N289" t="inlineStr">
         <is>
-          <t>2026-02-18T15:10:26</t>
+          <t>2026-02-18T16:58:08</t>
         </is>
       </c>
       <c r="O289" t="inlineStr">
@@ -20635,7 +20625,7 @@
       </c>
       <c r="N302" t="inlineStr">
         <is>
-          <t>2026-02-18T14:49:31</t>
+          <t>2026-02-18T17:40:41</t>
         </is>
       </c>
       <c r="O302" t="inlineStr">
@@ -21400,7 +21390,7 @@
       </c>
       <c r="N314" t="inlineStr">
         <is>
-          <t>2026-02-18T15:11:26</t>
+          <t>2026-02-18T17:04:13</t>
         </is>
       </c>
       <c r="O314" t="inlineStr">
@@ -21787,7 +21777,7 @@
       </c>
       <c r="N320" t="inlineStr">
         <is>
-          <t>2026-02-18T15:35:54</t>
+          <t>2026-02-18T17:19:16</t>
         </is>
       </c>
       <c r="O320" t="inlineStr">
@@ -22536,7 +22526,7 @@
       </c>
       <c r="N332" t="inlineStr">
         <is>
-          <t>2026-02-18T15:28:28</t>
+          <t>2026-02-18T17:26:39</t>
         </is>
       </c>
       <c r="O332" t="inlineStr">
@@ -22602,7 +22592,7 @@
       </c>
       <c r="N333" t="inlineStr">
         <is>
-          <t>2026-02-18T14:58:13</t>
+          <t>2026-02-18T16:46:54</t>
         </is>
       </c>
       <c r="O333" t="inlineStr">
@@ -22668,7 +22658,7 @@
       </c>
       <c r="N334" t="inlineStr">
         <is>
-          <t>2026-02-18T15:21:32</t>
+          <t>2026-02-18T17:23:00</t>
         </is>
       </c>
       <c r="O334" t="inlineStr">
@@ -22734,7 +22724,7 @@
       </c>
       <c r="N335" t="inlineStr">
         <is>
-          <t>2026-02-18T14:56:14</t>
+          <t>2026-02-18T16:50:16</t>
         </is>
       </c>
       <c r="O335" t="inlineStr">
@@ -22866,7 +22856,7 @@
       </c>
       <c r="N337" t="inlineStr">
         <is>
-          <t>2026-02-18T15:25:30</t>
+          <t>2026-02-18T17:14:52</t>
         </is>
       </c>
       <c r="O337" t="inlineStr">
@@ -22932,7 +22922,7 @@
       </c>
       <c r="N338" t="inlineStr">
         <is>
-          <t>2026-02-18T14:59:46</t>
+          <t>2026-02-18T16:54:05</t>
         </is>
       </c>
       <c r="O338" t="inlineStr">
@@ -22998,7 +22988,7 @@
       </c>
       <c r="N339" t="inlineStr">
         <is>
-          <t>2026-02-18T15:34:17</t>
+          <t>2026-02-18T17:22:45</t>
         </is>
       </c>
       <c r="O339" t="inlineStr">
@@ -23216,6 +23206,11 @@
           <t>OPERACAO 9.1</t>
         </is>
       </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>10.69.5.151</t>
+        </is>
+      </c>
       <c r="D343" t="n">
         <v>2017</v>
       </c>
@@ -23259,7 +23254,7 @@
       </c>
       <c r="N343" t="inlineStr">
         <is>
-          <t>2026-02-18T14:57:20</t>
+          <t>2026-02-18T17:40:27</t>
         </is>
       </c>
       <c r="O343" t="inlineStr">
@@ -23848,7 +23843,7 @@
       </c>
       <c r="N352" t="inlineStr">
         <is>
-          <t>2026-02-18T15:06:20</t>
+          <t>2026-02-18T16:50:58</t>
         </is>
       </c>
       <c r="O352" t="inlineStr">
@@ -24688,7 +24683,7 @@
       </c>
       <c r="N365" t="inlineStr">
         <is>
-          <t>2026-02-18T14:58:27</t>
+          <t>2026-02-18T16:53:17</t>
         </is>
       </c>
       <c r="O365" t="inlineStr">
@@ -24756,7 +24751,7 @@
       </c>
       <c r="N366" t="inlineStr">
         <is>
-          <t>2026-02-18T15:25:21</t>
+          <t>2026-02-18T17:11:28</t>
         </is>
       </c>
       <c r="O366" t="inlineStr">
@@ -24886,7 +24881,7 @@
       </c>
       <c r="N368" t="inlineStr">
         <is>
-          <t>2026-02-18T15:09:01</t>
+          <t>2026-02-18T17:07:56</t>
         </is>
       </c>
       <c r="O368" t="inlineStr">
@@ -24906,6 +24901,11 @@
           <t>RH</t>
         </is>
       </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>10.69.3.13</t>
+        </is>
+      </c>
       <c r="D369" t="n">
         <v>2025</v>
       </c>
@@ -24949,7 +24949,7 @@
       </c>
       <c r="N369" t="inlineStr">
         <is>
-          <t>2026-02-18T15:29:46</t>
+          <t>2026-02-18T16:29:40</t>
         </is>
       </c>
       <c r="O369" t="inlineStr">
@@ -25020,7 +25020,7 @@
       </c>
       <c r="N370" t="inlineStr">
         <is>
-          <t>2026-02-18T14:59:08</t>
+          <t>2026-02-18T16:50:17</t>
         </is>
       </c>
       <c r="O370" t="inlineStr">
@@ -25372,7 +25372,7 @@
       </c>
       <c r="N375" t="inlineStr">
         <is>
-          <t>2026-02-18T14:52:49</t>
+          <t>2026-02-18T17:39:13</t>
         </is>
       </c>
       <c r="O375" t="inlineStr">
@@ -25509,7 +25509,7 @@
       </c>
       <c r="N377" t="inlineStr">
         <is>
-          <t>2026-02-18T14:57:13</t>
+          <t>2026-02-18T15:50:46</t>
         </is>
       </c>
       <c r="O377" t="inlineStr">
@@ -25580,7 +25580,7 @@
       </c>
       <c r="N378" t="inlineStr">
         <is>
-          <t>2026-02-18T15:05:11</t>
+          <t>2026-02-18T16:54:42</t>
         </is>
       </c>
       <c r="O378" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática 2026-02-19 07:52:03.729091
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -601,7 +601,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>2026-02-18T17:09:20</t>
+          <t>2026-02-19T06:59:15</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -672,7 +672,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>2026-02-18T17:26:05</t>
+          <t>2026-02-19T07:31:28</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -1144,7 +1144,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>2026-02-18T17:32:20</t>
+          <t>2026-02-19T07:21:02</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -1474,7 +1474,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>2026-02-18T17:38:22</t>
+          <t>2026-02-19T07:30:58</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
@@ -1606,7 +1606,7 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>2026-02-18T17:05:12</t>
+          <t>2026-02-19T06:54:17</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
@@ -6956,7 +6956,7 @@
       </c>
       <c r="N96" t="inlineStr">
         <is>
-          <t>2026-02-18T17:36:05</t>
+          <t>2026-02-18T19:26:26</t>
         </is>
       </c>
       <c r="O96" t="inlineStr">
@@ -7027,7 +7027,7 @@
       </c>
       <c r="N97" t="inlineStr">
         <is>
-          <t>2026-02-18T17:40:29</t>
+          <t>2026-02-19T06:53:59</t>
         </is>
       </c>
       <c r="O97" t="inlineStr">
@@ -7235,7 +7235,7 @@
       </c>
       <c r="N100" t="inlineStr">
         <is>
-          <t>2026-02-18T17:32:28</t>
+          <t>2026-02-19T07:36:36</t>
         </is>
       </c>
       <c r="O100" t="inlineStr">
@@ -7306,7 +7306,7 @@
       </c>
       <c r="N101" t="inlineStr">
         <is>
-          <t>2026-02-18T17:05:22</t>
+          <t>2026-02-19T07:04:34</t>
         </is>
       </c>
       <c r="O101" t="inlineStr">
@@ -7448,7 +7448,7 @@
       </c>
       <c r="N103" t="inlineStr">
         <is>
-          <t>2026-02-18T17:18:30</t>
+          <t>2026-02-19T07:12:50</t>
         </is>
       </c>
       <c r="O103" t="inlineStr">
@@ -7855,7 +7855,7 @@
       </c>
       <c r="N109" t="inlineStr">
         <is>
-          <t>2026-02-18T17:30:47</t>
+          <t>2026-02-19T07:33:21</t>
         </is>
       </c>
       <c r="O109" t="inlineStr">
@@ -7926,7 +7926,7 @@
       </c>
       <c r="N110" t="inlineStr">
         <is>
-          <t>2026-02-18T17:31:17</t>
+          <t>2026-02-19T06:52:44</t>
         </is>
       </c>
       <c r="O110" t="inlineStr">
@@ -8068,7 +8068,7 @@
       </c>
       <c r="N112" t="inlineStr">
         <is>
-          <t>2026-02-18T17:08:38</t>
+          <t>2026-02-19T07:11:13</t>
         </is>
       </c>
       <c r="O112" t="inlineStr">
@@ -8139,7 +8139,7 @@
       </c>
       <c r="N113" t="inlineStr">
         <is>
-          <t>2026-02-18T17:28:40</t>
+          <t>2026-02-19T07:16:30</t>
         </is>
       </c>
       <c r="O113" t="inlineStr">
@@ -8210,7 +8210,7 @@
       </c>
       <c r="N114" t="inlineStr">
         <is>
-          <t>2026-02-18T17:19:37</t>
+          <t>2026-02-19T07:26:38</t>
         </is>
       </c>
       <c r="O114" t="inlineStr">
@@ -8278,7 +8278,7 @@
       </c>
       <c r="N115" t="inlineStr">
         <is>
-          <t>2026-02-18T17:33:06</t>
+          <t>2026-02-19T07:30:21</t>
         </is>
       </c>
       <c r="O115" t="inlineStr">
@@ -8696,7 +8696,7 @@
       </c>
       <c r="N121" t="inlineStr">
         <is>
-          <t>2026-02-18T16:43:55</t>
+          <t>2026-02-18T19:35:51</t>
         </is>
       </c>
       <c r="O121" t="inlineStr">
@@ -8764,7 +8764,7 @@
       </c>
       <c r="N122" t="inlineStr">
         <is>
-          <t>2026-02-18T17:37:19</t>
+          <t>2026-02-19T07:30:03</t>
         </is>
       </c>
       <c r="O122" t="inlineStr">
@@ -8906,7 +8906,7 @@
       </c>
       <c r="N124" t="inlineStr">
         <is>
-          <t>2026-02-18T17:14:39</t>
+          <t>2026-02-19T07:30:26</t>
         </is>
       </c>
       <c r="O124" t="inlineStr">
@@ -9119,7 +9119,7 @@
       </c>
       <c r="N127" t="inlineStr">
         <is>
-          <t>2026-02-18T16:36:34</t>
+          <t>2026-02-19T06:20:47</t>
         </is>
       </c>
       <c r="O127" t="inlineStr">
@@ -9261,7 +9261,7 @@
       </c>
       <c r="N129" t="inlineStr">
         <is>
-          <t>2026-02-18T17:37:42</t>
+          <t>2026-02-18T18:38:17</t>
         </is>
       </c>
       <c r="O129" t="inlineStr">
@@ -9332,7 +9332,7 @@
       </c>
       <c r="N130" t="inlineStr">
         <is>
-          <t>2026-02-18T17:22:31</t>
+          <t>2026-02-18T18:20:49</t>
         </is>
       </c>
       <c r="O130" t="inlineStr">
@@ -9535,7 +9535,7 @@
       </c>
       <c r="N133" t="inlineStr">
         <is>
-          <t>2026-02-18T17:25:11</t>
+          <t>2026-02-18T19:13:46</t>
         </is>
       </c>
       <c r="O133" t="inlineStr">
@@ -9601,7 +9601,7 @@
       </c>
       <c r="N134" t="inlineStr">
         <is>
-          <t>2026-02-18T17:37:39</t>
+          <t>2026-02-18T20:13:50</t>
         </is>
       </c>
       <c r="O134" t="inlineStr">
@@ -9667,7 +9667,7 @@
       </c>
       <c r="N135" t="inlineStr">
         <is>
-          <t>2026-02-18T17:31:33</t>
+          <t>2026-02-18T19:25:18</t>
         </is>
       </c>
       <c r="O135" t="inlineStr">
@@ -9864,7 +9864,7 @@
       </c>
       <c r="N138" t="inlineStr">
         <is>
-          <t>2026-02-18T17:06:50</t>
+          <t>2026-02-18T19:05:19</t>
         </is>
       </c>
       <c r="O138" t="inlineStr">
@@ -9930,7 +9930,7 @@
       </c>
       <c r="N139" t="inlineStr">
         <is>
-          <t>2026-02-18T17:40:19</t>
+          <t>2026-02-18T19:32:20</t>
         </is>
       </c>
       <c r="O139" t="inlineStr">
@@ -9996,7 +9996,7 @@
       </c>
       <c r="N140" t="inlineStr">
         <is>
-          <t>2026-02-18T17:02:12</t>
+          <t>2026-02-18T19:47:43</t>
         </is>
       </c>
       <c r="O140" t="inlineStr">
@@ -10062,7 +10062,7 @@
       </c>
       <c r="N141" t="inlineStr">
         <is>
-          <t>2026-02-18T17:24:16</t>
+          <t>2026-02-18T19:09:39</t>
         </is>
       </c>
       <c r="O141" t="inlineStr">
@@ -10128,7 +10128,7 @@
       </c>
       <c r="N142" t="inlineStr">
         <is>
-          <t>2026-02-18T16:45:36</t>
+          <t>2026-02-19T07:31:55</t>
         </is>
       </c>
       <c r="O142" t="inlineStr">
@@ -10194,7 +10194,7 @@
       </c>
       <c r="N143" t="inlineStr">
         <is>
-          <t>2026-02-18T16:52:00</t>
+          <t>2026-02-19T07:32:21</t>
         </is>
       </c>
       <c r="O143" t="inlineStr">
@@ -10260,7 +10260,7 @@
       </c>
       <c r="N144" t="inlineStr">
         <is>
-          <t>2026-02-18T16:52:29</t>
+          <t>2026-02-18T19:36:56</t>
         </is>
       </c>
       <c r="O144" t="inlineStr">
@@ -10326,7 +10326,7 @@
       </c>
       <c r="N145" t="inlineStr">
         <is>
-          <t>2026-02-18T16:58:53</t>
+          <t>2026-02-19T07:32:22</t>
         </is>
       </c>
       <c r="O145" t="inlineStr">
@@ -10392,7 +10392,7 @@
       </c>
       <c r="N146" t="inlineStr">
         <is>
-          <t>2026-02-18T16:55:41</t>
+          <t>2026-02-19T07:33:39</t>
         </is>
       </c>
       <c r="O146" t="inlineStr">
@@ -10458,7 +10458,7 @@
       </c>
       <c r="N147" t="inlineStr">
         <is>
-          <t>2026-02-18T17:24:03</t>
+          <t>2026-02-19T07:32:46</t>
         </is>
       </c>
       <c r="O147" t="inlineStr">
@@ -10524,7 +10524,7 @@
       </c>
       <c r="N148" t="inlineStr">
         <is>
-          <t>2026-02-18T16:51:02</t>
+          <t>2026-02-19T07:32:17</t>
         </is>
       </c>
       <c r="O148" t="inlineStr">
@@ -10590,7 +10590,7 @@
       </c>
       <c r="N149" t="inlineStr">
         <is>
-          <t>2026-02-18T17:34:18</t>
+          <t>2026-02-19T07:31:57</t>
         </is>
       </c>
       <c r="O149" t="inlineStr">
@@ -10656,7 +10656,7 @@
       </c>
       <c r="N150" t="inlineStr">
         <is>
-          <t>2026-02-14T20:54:17</t>
+          <t>2026-02-19T07:31:47</t>
         </is>
       </c>
       <c r="O150" t="inlineStr">
@@ -10722,7 +10722,7 @@
       </c>
       <c r="N151" t="inlineStr">
         <is>
-          <t>2026-02-18T17:08:40</t>
+          <t>2026-02-18T18:58:56</t>
         </is>
       </c>
       <c r="O151" t="inlineStr">
@@ -10788,7 +10788,7 @@
       </c>
       <c r="N152" t="inlineStr">
         <is>
-          <t>2026-02-18T17:39:53</t>
+          <t>2026-02-18T19:32:04</t>
         </is>
       </c>
       <c r="O152" t="inlineStr">
@@ -10849,7 +10849,7 @@
       </c>
       <c r="N153" t="inlineStr">
         <is>
-          <t>2026-02-18T16:54:53</t>
+          <t>2026-02-18T19:39:55</t>
         </is>
       </c>
       <c r="O153" t="inlineStr">
@@ -10915,7 +10915,7 @@
       </c>
       <c r="N154" t="inlineStr">
         <is>
-          <t>2026-02-18T17:38:16</t>
+          <t>2026-02-19T07:40:48</t>
         </is>
       </c>
       <c r="O154" t="inlineStr">
@@ -10981,7 +10981,7 @@
       </c>
       <c r="N155" t="inlineStr">
         <is>
-          <t>2026-02-18T17:18:50</t>
+          <t>2026-02-18T20:00:10</t>
         </is>
       </c>
       <c r="O155" t="inlineStr">
@@ -11113,7 +11113,7 @@
       </c>
       <c r="N157" t="inlineStr">
         <is>
-          <t>2026-02-18T16:59:20</t>
+          <t>2026-02-18T19:51:39</t>
         </is>
       </c>
       <c r="O157" t="inlineStr">
@@ -11245,7 +11245,7 @@
       </c>
       <c r="N159" t="inlineStr">
         <is>
-          <t>2026-02-18T16:53:41</t>
+          <t>2026-02-18T19:46:47</t>
         </is>
       </c>
       <c r="O159" t="inlineStr">
@@ -11311,7 +11311,7 @@
       </c>
       <c r="N160" t="inlineStr">
         <is>
-          <t>2026-02-18T12:58:18</t>
+          <t>2026-02-19T07:01:37</t>
         </is>
       </c>
       <c r="O160" t="inlineStr">
@@ -11377,7 +11377,7 @@
       </c>
       <c r="N161" t="inlineStr">
         <is>
-          <t>2026-02-18T13:33:50</t>
+          <t>2026-02-19T07:13:00</t>
         </is>
       </c>
       <c r="O161" t="inlineStr">
@@ -11443,7 +11443,7 @@
       </c>
       <c r="N162" t="inlineStr">
         <is>
-          <t>2026-02-18T17:21:48</t>
+          <t>2026-02-18T19:11:35</t>
         </is>
       </c>
       <c r="O162" t="inlineStr">
@@ -11571,11 +11571,11 @@
         </is>
       </c>
       <c r="M164" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N164" t="inlineStr">
         <is>
-          <t>2026-02-18T17:21:32</t>
+          <t>2026-02-19T06:51:08</t>
         </is>
       </c>
       <c r="O164" t="inlineStr">
@@ -11637,11 +11637,11 @@
         </is>
       </c>
       <c r="M165" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N165" t="inlineStr">
         <is>
-          <t>2026-02-18T12:31:47</t>
+          <t>2026-02-19T06:53:58</t>
         </is>
       </c>
       <c r="O165" t="inlineStr">
@@ -11773,7 +11773,7 @@
       </c>
       <c r="N167" t="inlineStr">
         <is>
-          <t>2026-02-18T16:54:08</t>
+          <t>2026-02-18T18:45:29</t>
         </is>
       </c>
       <c r="O167" t="inlineStr">
@@ -11905,7 +11905,7 @@
       </c>
       <c r="N169" t="inlineStr">
         <is>
-          <t>2026-02-18T17:21:33</t>
+          <t>2026-02-19T06:50:57</t>
         </is>
       </c>
       <c r="O169" t="inlineStr">
@@ -12037,7 +12037,7 @@
       </c>
       <c r="N171" t="inlineStr">
         <is>
-          <t>2026-02-18T16:59:42</t>
+          <t>2026-02-18T18:48:28</t>
         </is>
       </c>
       <c r="O171" t="inlineStr">
@@ -12169,7 +12169,7 @@
       </c>
       <c r="N173" t="inlineStr">
         <is>
-          <t>2026-02-18T17:00:58</t>
+          <t>2026-02-18T18:53:36</t>
         </is>
       </c>
       <c r="O173" t="inlineStr">
@@ -12235,7 +12235,7 @@
       </c>
       <c r="N174" t="inlineStr">
         <is>
-          <t>2026-02-18T17:09:23</t>
+          <t>2026-02-19T07:38:05</t>
         </is>
       </c>
       <c r="O174" t="inlineStr">
@@ -12301,7 +12301,7 @@
       </c>
       <c r="N175" t="inlineStr">
         <is>
-          <t>2026-02-18T17:11:14</t>
+          <t>2026-02-19T06:58:04</t>
         </is>
       </c>
       <c r="O175" t="inlineStr">
@@ -12499,7 +12499,7 @@
       </c>
       <c r="N178" t="inlineStr">
         <is>
-          <t>2026-02-18T17:08:22</t>
+          <t>2026-02-19T06:54:25</t>
         </is>
       </c>
       <c r="O178" t="inlineStr">
@@ -12631,7 +12631,7 @@
       </c>
       <c r="N180" t="inlineStr">
         <is>
-          <t>2026-02-18T17:06:16</t>
+          <t>2026-02-19T07:33:46</t>
         </is>
       </c>
       <c r="O180" t="inlineStr">
@@ -12697,7 +12697,7 @@
       </c>
       <c r="N181" t="inlineStr">
         <is>
-          <t>2026-02-18T17:22:45</t>
+          <t>2026-02-18T19:15:55</t>
         </is>
       </c>
       <c r="O181" t="inlineStr">
@@ -13098,7 +13098,7 @@
       </c>
       <c r="N187" t="inlineStr">
         <is>
-          <t>2026-02-18T17:16:40</t>
+          <t>2026-02-18T20:10:45</t>
         </is>
       </c>
       <c r="O187" t="inlineStr">
@@ -13164,7 +13164,7 @@
       </c>
       <c r="N188" t="inlineStr">
         <is>
-          <t>2026-02-18T17:37:07</t>
+          <t>2026-02-19T07:30:52</t>
         </is>
       </c>
       <c r="O188" t="inlineStr">
@@ -13296,7 +13296,7 @@
       </c>
       <c r="N190" t="inlineStr">
         <is>
-          <t>2026-02-18T17:35:42</t>
+          <t>2026-02-18T19:29:22</t>
         </is>
       </c>
       <c r="O190" t="inlineStr">
@@ -13362,7 +13362,7 @@
       </c>
       <c r="N191" t="inlineStr">
         <is>
-          <t>2026-02-18T16:50:27</t>
+          <t>2026-02-18T19:28:57</t>
         </is>
       </c>
       <c r="O191" t="inlineStr">
@@ -13428,7 +13428,7 @@
       </c>
       <c r="N192" t="inlineStr">
         <is>
-          <t>2026-02-18T17:16:48</t>
+          <t>2026-02-18T19:08:08</t>
         </is>
       </c>
       <c r="O192" t="inlineStr">
@@ -13557,7 +13557,7 @@
       </c>
       <c r="N194" t="inlineStr">
         <is>
-          <t>2026-02-18T14:36:06</t>
+          <t>2026-02-19T07:29:35</t>
         </is>
       </c>
       <c r="O194" t="inlineStr">
@@ -13623,7 +13623,7 @@
       </c>
       <c r="N195" t="inlineStr">
         <is>
-          <t>2026-02-18T17:32:12</t>
+          <t>2026-02-18T19:27:05</t>
         </is>
       </c>
       <c r="O195" t="inlineStr">
@@ -13689,7 +13689,7 @@
       </c>
       <c r="N196" t="inlineStr">
         <is>
-          <t>2026-02-18T17:04:07</t>
+          <t>2026-02-18T19:49:26</t>
         </is>
       </c>
       <c r="O196" t="inlineStr">
@@ -13755,7 +13755,7 @@
       </c>
       <c r="N197" t="inlineStr">
         <is>
-          <t>2026-02-18T17:40:31</t>
+          <t>2026-02-18T19:32:09</t>
         </is>
       </c>
       <c r="O197" t="inlineStr">
@@ -13887,7 +13887,7 @@
       </c>
       <c r="N199" t="inlineStr">
         <is>
-          <t>2026-02-18T17:38:22</t>
+          <t>2026-02-18T19:23:54</t>
         </is>
       </c>
       <c r="O199" t="inlineStr">
@@ -13953,7 +13953,7 @@
       </c>
       <c r="N200" t="inlineStr">
         <is>
-          <t>2026-02-18T16:50:49</t>
+          <t>2026-02-18T19:35:54</t>
         </is>
       </c>
       <c r="O200" t="inlineStr">
@@ -14016,7 +14016,7 @@
       </c>
       <c r="N201" t="inlineStr">
         <is>
-          <t>2026-02-18T16:54:00</t>
+          <t>2026-02-18T19:45:11</t>
         </is>
       </c>
       <c r="O201" t="inlineStr">
@@ -14082,7 +14082,7 @@
       </c>
       <c r="N202" t="inlineStr">
         <is>
-          <t>2026-02-18T16:59:53</t>
+          <t>2026-02-18T19:47:36</t>
         </is>
       </c>
       <c r="O202" t="inlineStr">
@@ -14148,7 +14148,7 @@
       </c>
       <c r="N203" t="inlineStr">
         <is>
-          <t>2026-02-18T17:40:52</t>
+          <t>2026-02-19T07:17:12</t>
         </is>
       </c>
       <c r="O203" t="inlineStr">
@@ -14214,7 +14214,7 @@
       </c>
       <c r="N204" t="inlineStr">
         <is>
-          <t>2026-02-18T17:04:20</t>
+          <t>2026-02-18T19:48:14</t>
         </is>
       </c>
       <c r="O204" t="inlineStr">
@@ -14280,7 +14280,7 @@
       </c>
       <c r="N205" t="inlineStr">
         <is>
-          <t>2026-02-18T17:40:04</t>
+          <t>2026-02-18T19:27:06</t>
         </is>
       </c>
       <c r="O205" t="inlineStr">
@@ -14346,7 +14346,7 @@
       </c>
       <c r="N206" t="inlineStr">
         <is>
-          <t>2026-02-18T17:30:15</t>
+          <t>2026-02-18T19:26:40</t>
         </is>
       </c>
       <c r="O206" t="inlineStr">
@@ -14412,7 +14412,7 @@
       </c>
       <c r="N207" t="inlineStr">
         <is>
-          <t>2026-02-18T17:24:14</t>
+          <t>2026-02-19T07:31:21</t>
         </is>
       </c>
       <c r="O207" t="inlineStr">
@@ -14478,7 +14478,7 @@
       </c>
       <c r="N208" t="inlineStr">
         <is>
-          <t>2026-02-18T13:30:28</t>
+          <t>2026-02-19T07:32:14</t>
         </is>
       </c>
       <c r="O208" t="inlineStr">
@@ -14544,7 +14544,7 @@
       </c>
       <c r="N209" t="inlineStr">
         <is>
-          <t>2026-02-18T17:20:46</t>
+          <t>2026-02-19T07:38:04</t>
         </is>
       </c>
       <c r="O209" t="inlineStr">
@@ -14610,7 +14610,7 @@
       </c>
       <c r="N210" t="inlineStr">
         <is>
-          <t>2026-02-18T17:19:23</t>
+          <t>2026-02-18T20:54:14</t>
         </is>
       </c>
       <c r="O210" t="inlineStr">
@@ -14676,7 +14676,7 @@
       </c>
       <c r="N211" t="inlineStr">
         <is>
-          <t>2026-02-18T16:47:45</t>
+          <t>2026-02-18T19:36:41</t>
         </is>
       </c>
       <c r="O211" t="inlineStr">
@@ -14742,7 +14742,7 @@
       </c>
       <c r="N212" t="inlineStr">
         <is>
-          <t>2026-02-18T16:50:50</t>
+          <t>2026-02-19T07:40:44</t>
         </is>
       </c>
       <c r="O212" t="inlineStr">
@@ -14808,7 +14808,7 @@
       </c>
       <c r="N213" t="inlineStr">
         <is>
-          <t>2026-02-18T16:54:46</t>
+          <t>2026-02-19T07:41:14</t>
         </is>
       </c>
       <c r="O213" t="inlineStr">
@@ -14874,7 +14874,7 @@
       </c>
       <c r="N214" t="inlineStr">
         <is>
-          <t>2026-02-18T16:47:28</t>
+          <t>2026-02-18T19:33:47</t>
         </is>
       </c>
       <c r="O214" t="inlineStr">
@@ -14940,7 +14940,7 @@
       </c>
       <c r="N215" t="inlineStr">
         <is>
-          <t>2026-02-18T16:53:28</t>
+          <t>2026-02-19T07:38:27</t>
         </is>
       </c>
       <c r="O215" t="inlineStr">
@@ -15006,7 +15006,7 @@
       </c>
       <c r="N216" t="inlineStr">
         <is>
-          <t>2026-02-18T16:53:18</t>
+          <t>2026-02-19T07:40:21</t>
         </is>
       </c>
       <c r="O216" t="inlineStr">
@@ -15072,7 +15072,7 @@
       </c>
       <c r="N217" t="inlineStr">
         <is>
-          <t>2026-02-18T17:13:28</t>
+          <t>2026-02-19T07:41:20</t>
         </is>
       </c>
       <c r="O217" t="inlineStr">
@@ -15138,7 +15138,7 @@
       </c>
       <c r="N218" t="inlineStr">
         <is>
-          <t>2026-02-18T17:19:30</t>
+          <t>2026-02-19T07:13:35</t>
         </is>
       </c>
       <c r="O218" t="inlineStr">
@@ -15204,7 +15204,7 @@
       </c>
       <c r="N219" t="inlineStr">
         <is>
-          <t>2026-02-18T15:54:46</t>
+          <t>2026-02-19T07:08:36</t>
         </is>
       </c>
       <c r="O219" t="inlineStr">
@@ -15275,7 +15275,7 @@
       </c>
       <c r="N220" t="inlineStr">
         <is>
-          <t>2026-02-18T17:36:53</t>
+          <t>2026-02-19T07:41:39</t>
         </is>
       </c>
       <c r="O220" t="inlineStr">
@@ -15341,7 +15341,7 @@
       </c>
       <c r="N221" t="inlineStr">
         <is>
-          <t>2026-02-18T16:53:46</t>
+          <t>2026-02-18T19:41:13</t>
         </is>
       </c>
       <c r="O221" t="inlineStr">
@@ -15407,7 +15407,7 @@
       </c>
       <c r="N222" t="inlineStr">
         <is>
-          <t>2026-02-18T17:33:26</t>
+          <t>2026-02-18T19:30:24</t>
         </is>
       </c>
       <c r="O222" t="inlineStr">
@@ -15473,7 +15473,7 @@
       </c>
       <c r="N223" t="inlineStr">
         <is>
-          <t>2026-02-18T17:03:30</t>
+          <t>2026-02-18T19:01:52</t>
         </is>
       </c>
       <c r="O223" t="inlineStr">
@@ -15539,7 +15539,7 @@
       </c>
       <c r="N224" t="inlineStr">
         <is>
-          <t>2026-02-18T16:56:13</t>
+          <t>2026-02-18T19:51:33</t>
         </is>
       </c>
       <c r="O224" t="inlineStr">
@@ -15605,7 +15605,7 @@
       </c>
       <c r="N225" t="inlineStr">
         <is>
-          <t>2026-02-18T16:53:20</t>
+          <t>2026-02-18T19:39:17</t>
         </is>
       </c>
       <c r="O225" t="inlineStr">
@@ -15671,7 +15671,7 @@
       </c>
       <c r="N226" t="inlineStr">
         <is>
-          <t>2026-02-18T16:44:37</t>
+          <t>2026-02-18T19:41:17</t>
         </is>
       </c>
       <c r="O226" t="inlineStr">
@@ -15737,7 +15737,7 @@
       </c>
       <c r="N227" t="inlineStr">
         <is>
-          <t>2026-02-18T17:13:39</t>
+          <t>2026-02-18T19:10:33</t>
         </is>
       </c>
       <c r="O227" t="inlineStr">
@@ -15803,7 +15803,7 @@
       </c>
       <c r="N228" t="inlineStr">
         <is>
-          <t>2026-02-18T16:52:40</t>
+          <t>2026-02-18T19:43:16</t>
         </is>
       </c>
       <c r="O228" t="inlineStr">
@@ -15935,7 +15935,7 @@
       </c>
       <c r="N230" t="inlineStr">
         <is>
-          <t>2026-02-18T17:11:01</t>
+          <t>2026-02-19T07:40:58</t>
         </is>
       </c>
       <c r="O230" t="inlineStr">
@@ -16001,7 +16001,7 @@
       </c>
       <c r="N231" t="inlineStr">
         <is>
-          <t>2026-02-18T16:49:00</t>
+          <t>2026-02-18T19:41:13</t>
         </is>
       </c>
       <c r="O231" t="inlineStr">
@@ -16067,7 +16067,7 @@
       </c>
       <c r="N232" t="inlineStr">
         <is>
-          <t>2026-02-18T17:16:06</t>
+          <t>2026-02-18T19:09:51</t>
         </is>
       </c>
       <c r="O232" t="inlineStr">
@@ -16133,7 +16133,7 @@
       </c>
       <c r="N233" t="inlineStr">
         <is>
-          <t>2026-02-18T16:45:20</t>
+          <t>2026-02-19T07:37:56</t>
         </is>
       </c>
       <c r="O233" t="inlineStr">
@@ -16199,7 +16199,7 @@
       </c>
       <c r="N234" t="inlineStr">
         <is>
-          <t>2026-02-18T17:14:23</t>
+          <t>2026-02-19T07:26:07</t>
         </is>
       </c>
       <c r="O234" t="inlineStr">
@@ -16265,7 +16265,7 @@
       </c>
       <c r="N235" t="inlineStr">
         <is>
-          <t>2026-02-18T16:55:05</t>
+          <t>2026-02-18T19:54:27</t>
         </is>
       </c>
       <c r="O235" t="inlineStr">
@@ -16331,7 +16331,7 @@
       </c>
       <c r="N236" t="inlineStr">
         <is>
-          <t>2026-02-18T16:55:56</t>
+          <t>2026-02-18T19:49:00</t>
         </is>
       </c>
       <c r="O236" t="inlineStr">
@@ -16397,7 +16397,7 @@
       </c>
       <c r="N237" t="inlineStr">
         <is>
-          <t>2026-02-18T17:01:17</t>
+          <t>2026-02-18T19:50:35</t>
         </is>
       </c>
       <c r="O237" t="inlineStr">
@@ -16463,7 +16463,7 @@
       </c>
       <c r="N238" t="inlineStr">
         <is>
-          <t>2026-02-18T17:04:53</t>
+          <t>2026-02-18T19:48:57</t>
         </is>
       </c>
       <c r="O238" t="inlineStr">
@@ -16529,7 +16529,7 @@
       </c>
       <c r="N239" t="inlineStr">
         <is>
-          <t>2026-02-18T16:54:23</t>
+          <t>2026-02-18T19:39:45</t>
         </is>
       </c>
       <c r="O239" t="inlineStr">
@@ -16595,7 +16595,7 @@
       </c>
       <c r="N240" t="inlineStr">
         <is>
-          <t>2026-02-18T16:55:35</t>
+          <t>2026-02-18T20:40:21</t>
         </is>
       </c>
       <c r="O240" t="inlineStr">
@@ -16727,7 +16727,7 @@
       </c>
       <c r="N242" t="inlineStr">
         <is>
-          <t>2026-02-18T16:54:07</t>
+          <t>2026-02-18T19:33:59</t>
         </is>
       </c>
       <c r="O242" t="inlineStr">
@@ -16793,7 +16793,7 @@
       </c>
       <c r="N243" t="inlineStr">
         <is>
-          <t>2026-02-18T17:06:10</t>
+          <t>2026-02-18T19:54:00</t>
         </is>
       </c>
       <c r="O243" t="inlineStr">
@@ -16854,7 +16854,7 @@
       </c>
       <c r="N244" t="inlineStr">
         <is>
-          <t>2026-02-18T17:01:32</t>
+          <t>2026-02-18T19:43:39</t>
         </is>
       </c>
       <c r="O244" t="inlineStr">
@@ -16920,7 +16920,7 @@
       </c>
       <c r="N245" t="inlineStr">
         <is>
-          <t>2026-02-18T17:40:46</t>
+          <t>2026-02-18T19:33:45</t>
         </is>
       </c>
       <c r="O245" t="inlineStr">
@@ -16986,7 +16986,7 @@
       </c>
       <c r="N246" t="inlineStr">
         <is>
-          <t>2026-02-18T17:28:28</t>
+          <t>2026-02-18T20:18:58</t>
         </is>
       </c>
       <c r="O246" t="inlineStr">
@@ -17052,7 +17052,7 @@
       </c>
       <c r="N247" t="inlineStr">
         <is>
-          <t>2026-02-18T17:41:36</t>
+          <t>2026-02-18T19:42:20</t>
         </is>
       </c>
       <c r="O247" t="inlineStr">
@@ -17118,7 +17118,7 @@
       </c>
       <c r="N248" t="inlineStr">
         <is>
-          <t>2026-02-18T17:21:00</t>
+          <t>2026-02-18T19:17:38</t>
         </is>
       </c>
       <c r="O248" t="inlineStr">
@@ -17184,7 +17184,7 @@
       </c>
       <c r="N249" t="inlineStr">
         <is>
-          <t>2026-02-18T17:16:33</t>
+          <t>2026-02-18T19:52:10</t>
         </is>
       </c>
       <c r="O249" t="inlineStr">
@@ -17245,7 +17245,7 @@
       </c>
       <c r="N250" t="inlineStr">
         <is>
-          <t>2026-02-18T17:37:20</t>
+          <t>2026-02-18T19:23:55</t>
         </is>
       </c>
       <c r="O250" t="inlineStr">
@@ -17311,7 +17311,7 @@
       </c>
       <c r="N251" t="inlineStr">
         <is>
-          <t>2026-02-18T17:12:06</t>
+          <t>2026-02-18T20:49:40</t>
         </is>
       </c>
       <c r="O251" t="inlineStr">
@@ -17377,7 +17377,7 @@
       </c>
       <c r="N252" t="inlineStr">
         <is>
-          <t>2026-02-18T17:30:50</t>
+          <t>2026-02-18T19:27:22</t>
         </is>
       </c>
       <c r="O252" t="inlineStr">
@@ -17443,7 +17443,7 @@
       </c>
       <c r="N253" t="inlineStr">
         <is>
-          <t>2026-02-18T16:52:46</t>
+          <t>2026-02-18T19:38:50</t>
         </is>
       </c>
       <c r="O253" t="inlineStr">
@@ -17503,7 +17503,7 @@
       </c>
       <c r="N254" t="inlineStr">
         <is>
-          <t>2026-02-18T17:05:28</t>
+          <t>2026-02-19T07:39:39</t>
         </is>
       </c>
       <c r="O254" t="inlineStr">
@@ -17569,7 +17569,7 @@
       </c>
       <c r="N255" t="inlineStr">
         <is>
-          <t>2026-02-18T17:33:45</t>
+          <t>2026-02-18T19:22:19</t>
         </is>
       </c>
       <c r="O255" t="inlineStr">
@@ -17635,7 +17635,7 @@
       </c>
       <c r="N256" t="inlineStr">
         <is>
-          <t>2026-02-18T17:25:25</t>
+          <t>2026-02-18T19:45:15</t>
         </is>
       </c>
       <c r="O256" t="inlineStr">
@@ -17701,7 +17701,7 @@
       </c>
       <c r="N257" t="inlineStr">
         <is>
-          <t>2026-02-18T17:09:23</t>
+          <t>2026-02-18T19:27:49</t>
         </is>
       </c>
       <c r="O257" t="inlineStr">
@@ -17767,7 +17767,7 @@
       </c>
       <c r="N258" t="inlineStr">
         <is>
-          <t>2026-02-18T17:26:26</t>
+          <t>2026-02-18T19:15:19</t>
         </is>
       </c>
       <c r="O258" t="inlineStr">
@@ -17833,7 +17833,7 @@
       </c>
       <c r="N259" t="inlineStr">
         <is>
-          <t>2026-02-18T17:25:55</t>
+          <t>2026-02-18T19:25:01</t>
         </is>
       </c>
       <c r="O259" t="inlineStr">
@@ -18097,7 +18097,7 @@
       </c>
       <c r="N263" t="inlineStr">
         <is>
-          <t>2026-02-18T16:48:42</t>
+          <t>2026-02-18T19:35:04</t>
         </is>
       </c>
       <c r="O263" t="inlineStr">
@@ -18163,7 +18163,7 @@
       </c>
       <c r="N264" t="inlineStr">
         <is>
-          <t>2026-02-18T17:01:22</t>
+          <t>2026-02-18T19:44:39</t>
         </is>
       </c>
       <c r="O264" t="inlineStr">
@@ -18229,7 +18229,7 @@
       </c>
       <c r="N265" t="inlineStr">
         <is>
-          <t>2026-02-18T16:59:43</t>
+          <t>2026-02-18T20:38:19</t>
         </is>
       </c>
       <c r="O265" t="inlineStr">
@@ -18295,7 +18295,7 @@
       </c>
       <c r="N266" t="inlineStr">
         <is>
-          <t>2026-02-18T17:31:06</t>
+          <t>2026-02-18T20:21:13</t>
         </is>
       </c>
       <c r="O266" t="inlineStr">
@@ -18361,7 +18361,7 @@
       </c>
       <c r="N267" t="inlineStr">
         <is>
-          <t>2026-02-18T17:30:00</t>
+          <t>2026-02-18T19:23:48</t>
         </is>
       </c>
       <c r="O267" t="inlineStr">
@@ -18427,7 +18427,7 @@
       </c>
       <c r="N268" t="inlineStr">
         <is>
-          <t>2026-02-18T17:29:11</t>
+          <t>2026-02-18T19:18:54</t>
         </is>
       </c>
       <c r="O268" t="inlineStr">
@@ -18493,7 +18493,7 @@
       </c>
       <c r="N269" t="inlineStr">
         <is>
-          <t>2026-02-18T17:24:14</t>
+          <t>2026-02-18T19:12:27</t>
         </is>
       </c>
       <c r="O269" t="inlineStr">
@@ -18556,7 +18556,7 @@
       </c>
       <c r="N270" t="inlineStr">
         <is>
-          <t>2026-02-18T17:27:07</t>
+          <t>2026-02-19T07:39:48</t>
         </is>
       </c>
       <c r="O270" t="inlineStr">
@@ -18688,7 +18688,7 @@
       </c>
       <c r="N272" t="inlineStr">
         <is>
-          <t>2026-02-18T17:00:27</t>
+          <t>2026-02-18T19:53:13</t>
         </is>
       </c>
       <c r="O272" t="inlineStr">
@@ -18754,7 +18754,7 @@
       </c>
       <c r="N273" t="inlineStr">
         <is>
-          <t>2026-02-18T17:38:43</t>
+          <t>2026-02-19T07:17:05</t>
         </is>
       </c>
       <c r="O273" t="inlineStr">
@@ -19084,7 +19084,7 @@
       </c>
       <c r="N278" t="inlineStr">
         <is>
-          <t>2026-02-18T17:30:08</t>
+          <t>2026-02-19T07:26:08</t>
         </is>
       </c>
       <c r="O278" t="inlineStr">
@@ -19150,7 +19150,7 @@
       </c>
       <c r="N279" t="inlineStr">
         <is>
-          <t>2026-02-14T20:39:39</t>
+          <t>2026-02-19T07:17:54</t>
         </is>
       </c>
       <c r="O279" t="inlineStr">
@@ -19216,7 +19216,7 @@
       </c>
       <c r="N280" t="inlineStr">
         <is>
-          <t>2026-02-18T16:51:56</t>
+          <t>2026-02-19T06:55:26</t>
         </is>
       </c>
       <c r="O280" t="inlineStr">
@@ -19282,7 +19282,7 @@
       </c>
       <c r="N281" t="inlineStr">
         <is>
-          <t>2026-02-14T20:42:36</t>
+          <t>2026-02-19T07:36:32</t>
         </is>
       </c>
       <c r="O281" t="inlineStr">
@@ -19302,6 +19302,11 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>10.69.5.151</t>
+        </is>
+      </c>
       <c r="D282" t="n">
         <v>2017</v>
       </c>
@@ -19343,7 +19348,7 @@
       </c>
       <c r="N282" t="inlineStr">
         <is>
-          <t>2026-02-18T16:49:07</t>
+          <t>2026-02-19T07:35:36</t>
         </is>
       </c>
       <c r="O282" t="inlineStr">
@@ -19409,7 +19414,7 @@
       </c>
       <c r="N283" t="inlineStr">
         <is>
-          <t>2026-02-18T17:08:43</t>
+          <t>2026-02-18T19:51:45</t>
         </is>
       </c>
       <c r="O283" t="inlineStr">
@@ -19475,7 +19480,7 @@
       </c>
       <c r="N284" t="inlineStr">
         <is>
-          <t>2026-02-18T17:14:32</t>
+          <t>2026-02-18T20:55:53</t>
         </is>
       </c>
       <c r="O284" t="inlineStr">
@@ -19607,7 +19612,7 @@
       </c>
       <c r="N286" t="inlineStr">
         <is>
-          <t>2026-02-18T17:25:12</t>
+          <t>2026-02-19T05:47:01</t>
         </is>
       </c>
       <c r="O286" t="inlineStr">
@@ -19673,7 +19678,7 @@
       </c>
       <c r="N287" t="inlineStr">
         <is>
-          <t>2026-02-18T13:52:20</t>
+          <t>2026-02-19T04:14:19</t>
         </is>
       </c>
       <c r="O287" t="inlineStr">
@@ -19739,7 +19744,7 @@
       </c>
       <c r="N288" t="inlineStr">
         <is>
-          <t>2026-02-18T13:01:10</t>
+          <t>2026-02-19T07:35:27</t>
         </is>
       </c>
       <c r="O288" t="inlineStr">
@@ -19805,7 +19810,7 @@
       </c>
       <c r="N289" t="inlineStr">
         <is>
-          <t>2026-02-18T16:58:08</t>
+          <t>2026-02-18T20:44:20</t>
         </is>
       </c>
       <c r="O289" t="inlineStr">
@@ -20625,7 +20630,7 @@
       </c>
       <c r="N302" t="inlineStr">
         <is>
-          <t>2026-02-18T17:40:41</t>
+          <t>2026-02-19T07:38:59</t>
         </is>
       </c>
       <c r="O302" t="inlineStr">
@@ -21390,7 +21395,7 @@
       </c>
       <c r="N314" t="inlineStr">
         <is>
-          <t>2026-02-18T17:04:13</t>
+          <t>2026-02-18T18:58:06</t>
         </is>
       </c>
       <c r="O314" t="inlineStr">
@@ -21777,7 +21782,7 @@
       </c>
       <c r="N320" t="inlineStr">
         <is>
-          <t>2026-02-18T17:19:16</t>
+          <t>2026-02-19T07:27:06</t>
         </is>
       </c>
       <c r="O320" t="inlineStr">
@@ -22526,7 +22531,7 @@
       </c>
       <c r="N332" t="inlineStr">
         <is>
-          <t>2026-02-18T17:26:39</t>
+          <t>2026-02-18T18:25:12</t>
         </is>
       </c>
       <c r="O332" t="inlineStr">
@@ -22592,7 +22597,7 @@
       </c>
       <c r="N333" t="inlineStr">
         <is>
-          <t>2026-02-18T16:46:54</t>
+          <t>2026-02-19T06:46:13</t>
         </is>
       </c>
       <c r="O333" t="inlineStr">
@@ -22658,7 +22663,7 @@
       </c>
       <c r="N334" t="inlineStr">
         <is>
-          <t>2026-02-18T17:23:00</t>
+          <t>2026-02-19T06:47:03</t>
         </is>
       </c>
       <c r="O334" t="inlineStr">
@@ -22724,7 +22729,7 @@
       </c>
       <c r="N335" t="inlineStr">
         <is>
-          <t>2026-02-18T16:50:16</t>
+          <t>2026-02-19T06:46:26</t>
         </is>
       </c>
       <c r="O335" t="inlineStr">
@@ -22790,7 +22795,7 @@
       </c>
       <c r="N336" t="inlineStr">
         <is>
-          <t>2026-02-18T13:24:49</t>
+          <t>2026-02-19T06:46:36</t>
         </is>
       </c>
       <c r="O336" t="inlineStr">
@@ -22856,7 +22861,7 @@
       </c>
       <c r="N337" t="inlineStr">
         <is>
-          <t>2026-02-18T17:14:52</t>
+          <t>2026-02-19T06:46:38</t>
         </is>
       </c>
       <c r="O337" t="inlineStr">
@@ -22922,7 +22927,7 @@
       </c>
       <c r="N338" t="inlineStr">
         <is>
-          <t>2026-02-18T16:54:05</t>
+          <t>2026-02-19T07:22:06</t>
         </is>
       </c>
       <c r="O338" t="inlineStr">
@@ -22988,7 +22993,7 @@
       </c>
       <c r="N339" t="inlineStr">
         <is>
-          <t>2026-02-18T17:22:45</t>
+          <t>2026-02-19T07:27:31</t>
         </is>
       </c>
       <c r="O339" t="inlineStr">
@@ -23182,11 +23187,11 @@
         </is>
       </c>
       <c r="M342" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N342" t="inlineStr">
         <is>
-          <t>2026-02-18T13:17:29</t>
+          <t>2026-02-19T06:54:22</t>
         </is>
       </c>
       <c r="O342" t="inlineStr">
@@ -23206,11 +23211,6 @@
           <t>OPERACAO 9.1</t>
         </is>
       </c>
-      <c r="C343" t="inlineStr">
-        <is>
-          <t>10.69.5.151</t>
-        </is>
-      </c>
       <c r="D343" t="n">
         <v>2017</v>
       </c>
@@ -23843,7 +23843,7 @@
       </c>
       <c r="N352" t="inlineStr">
         <is>
-          <t>2026-02-18T16:50:58</t>
+          <t>2026-02-19T07:02:28</t>
         </is>
       </c>
       <c r="O352" t="inlineStr">
@@ -24751,7 +24751,7 @@
       </c>
       <c r="N366" t="inlineStr">
         <is>
-          <t>2026-02-18T17:11:28</t>
+          <t>2026-02-19T07:09:16</t>
         </is>
       </c>
       <c r="O366" t="inlineStr">
@@ -24881,7 +24881,7 @@
       </c>
       <c r="N368" t="inlineStr">
         <is>
-          <t>2026-02-18T17:07:56</t>
+          <t>2026-02-19T07:06:07</t>
         </is>
       </c>
       <c r="O368" t="inlineStr">
@@ -25372,7 +25372,7 @@
       </c>
       <c r="N375" t="inlineStr">
         <is>
-          <t>2026-02-18T17:39:13</t>
+          <t>2026-02-19T07:00:30</t>
         </is>
       </c>
       <c r="O375" t="inlineStr">
@@ -25580,7 +25580,7 @@
       </c>
       <c r="N378" t="inlineStr">
         <is>
-          <t>2026-02-18T16:54:42</t>
+          <t>2026-02-19T06:57:16</t>
         </is>
       </c>
       <c r="O378" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática 2026-02-19 09:52:05.261238
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -601,7 +601,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>2026-02-19T06:59:15</t>
+          <t>2026-02-19T08:53:36</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -672,7 +672,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>2026-02-19T07:31:28</t>
+          <t>2026-02-19T09:21:13</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -743,7 +743,7 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>2026-02-13T16:36:42</t>
+          <t>2026-02-19T09:16:54</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
@@ -814,7 +814,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>2026-02-18T16:32:07</t>
+          <t>2026-02-19T08:50:48</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -1144,7 +1144,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>2026-02-19T07:21:02</t>
+          <t>2026-02-19T09:12:37</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -1474,7 +1474,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>2026-02-19T07:30:58</t>
+          <t>2026-02-19T09:15:09</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
@@ -1606,7 +1606,7 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>2026-02-19T06:54:17</t>
+          <t>2026-02-19T09:41:44</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
@@ -7027,7 +7027,7 @@
       </c>
       <c r="N97" t="inlineStr">
         <is>
-          <t>2026-02-19T06:53:59</t>
+          <t>2026-02-19T09:38:35</t>
         </is>
       </c>
       <c r="O97" t="inlineStr">
@@ -7093,7 +7093,7 @@
       </c>
       <c r="N98" t="inlineStr">
         <is>
-          <t>2026-02-18T16:04:16</t>
+          <t>2026-02-19T09:04:45</t>
         </is>
       </c>
       <c r="O98" t="inlineStr">
@@ -7235,7 +7235,7 @@
       </c>
       <c r="N100" t="inlineStr">
         <is>
-          <t>2026-02-19T07:36:36</t>
+          <t>2026-02-19T09:24:56</t>
         </is>
       </c>
       <c r="O100" t="inlineStr">
@@ -7306,7 +7306,7 @@
       </c>
       <c r="N101" t="inlineStr">
         <is>
-          <t>2026-02-19T07:04:34</t>
+          <t>2026-02-19T08:57:57</t>
         </is>
       </c>
       <c r="O101" t="inlineStr">
@@ -7448,7 +7448,7 @@
       </c>
       <c r="N103" t="inlineStr">
         <is>
-          <t>2026-02-19T07:12:50</t>
+          <t>2026-02-19T09:06:24</t>
         </is>
       </c>
       <c r="O103" t="inlineStr">
@@ -7713,7 +7713,7 @@
       </c>
       <c r="N107" t="inlineStr">
         <is>
-          <t>2026-02-18T16:55:29</t>
+          <t>2026-02-19T09:16:49</t>
         </is>
       </c>
       <c r="O107" t="inlineStr">
@@ -7855,7 +7855,7 @@
       </c>
       <c r="N109" t="inlineStr">
         <is>
-          <t>2026-02-19T07:33:21</t>
+          <t>2026-02-19T09:17:05</t>
         </is>
       </c>
       <c r="O109" t="inlineStr">
@@ -7926,7 +7926,7 @@
       </c>
       <c r="N110" t="inlineStr">
         <is>
-          <t>2026-02-19T06:52:44</t>
+          <t>2026-02-19T09:41:22</t>
         </is>
       </c>
       <c r="O110" t="inlineStr">
@@ -7997,7 +7997,7 @@
       </c>
       <c r="N111" t="inlineStr">
         <is>
-          <t>2026-02-18T16:23:15</t>
+          <t>2026-02-19T08:45:07</t>
         </is>
       </c>
       <c r="O111" t="inlineStr">
@@ -8068,7 +8068,7 @@
       </c>
       <c r="N112" t="inlineStr">
         <is>
-          <t>2026-02-19T07:11:13</t>
+          <t>2026-02-19T09:11:47</t>
         </is>
       </c>
       <c r="O112" t="inlineStr">
@@ -8139,7 +8139,7 @@
       </c>
       <c r="N113" t="inlineStr">
         <is>
-          <t>2026-02-19T07:16:30</t>
+          <t>2026-02-19T09:12:42</t>
         </is>
       </c>
       <c r="O113" t="inlineStr">
@@ -8210,7 +8210,7 @@
       </c>
       <c r="N114" t="inlineStr">
         <is>
-          <t>2026-02-19T07:26:38</t>
+          <t>2026-02-19T09:25:12</t>
         </is>
       </c>
       <c r="O114" t="inlineStr">
@@ -8278,7 +8278,7 @@
       </c>
       <c r="N115" t="inlineStr">
         <is>
-          <t>2026-02-19T07:30:21</t>
+          <t>2026-02-19T09:18:11</t>
         </is>
       </c>
       <c r="O115" t="inlineStr">
@@ -8349,7 +8349,7 @@
       </c>
       <c r="N116" t="inlineStr">
         <is>
-          <t>2026-02-18T16:19:54</t>
+          <t>2026-02-19T09:24:48</t>
         </is>
       </c>
       <c r="O116" t="inlineStr">
@@ -8369,6 +8369,11 @@
           <t>DP</t>
         </is>
       </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>10.69.3.23</t>
+        </is>
+      </c>
       <c r="D117" t="n">
         <v>2025</v>
       </c>
@@ -8415,7 +8420,7 @@
       </c>
       <c r="N117" t="inlineStr">
         <is>
-          <t>2026-02-18T16:29:23</t>
+          <t>2026-02-19T09:37:12</t>
         </is>
       </c>
       <c r="O117" t="inlineStr">
@@ -8625,7 +8630,7 @@
       </c>
       <c r="N120" t="inlineStr">
         <is>
-          <t>2026-02-18T17:09:29</t>
+          <t>2026-02-19T09:01:58</t>
         </is>
       </c>
       <c r="O120" t="inlineStr">
@@ -8764,7 +8769,7 @@
       </c>
       <c r="N122" t="inlineStr">
         <is>
-          <t>2026-02-19T07:30:03</t>
+          <t>2026-02-19T09:17:43</t>
         </is>
       </c>
       <c r="O122" t="inlineStr">
@@ -8906,7 +8911,7 @@
       </c>
       <c r="N124" t="inlineStr">
         <is>
-          <t>2026-02-19T07:30:26</t>
+          <t>2026-02-19T09:21:27</t>
         </is>
       </c>
       <c r="O124" t="inlineStr">
@@ -8977,7 +8982,7 @@
       </c>
       <c r="N125" t="inlineStr">
         <is>
-          <t>2026-02-18T16:19:15</t>
+          <t>2026-02-19T09:04:27</t>
         </is>
       </c>
       <c r="O125" t="inlineStr">
@@ -9048,7 +9053,7 @@
       </c>
       <c r="N126" t="inlineStr">
         <is>
-          <t>2026-02-18T15:37:05</t>
+          <t>2026-02-19T08:58:58</t>
         </is>
       </c>
       <c r="O126" t="inlineStr">
@@ -9119,7 +9124,7 @@
       </c>
       <c r="N127" t="inlineStr">
         <is>
-          <t>2026-02-19T06:20:47</t>
+          <t>2026-02-19T09:00:43</t>
         </is>
       </c>
       <c r="O127" t="inlineStr">
@@ -9190,7 +9195,7 @@
       </c>
       <c r="N128" t="inlineStr">
         <is>
-          <t>2026-02-18T16:23:18</t>
+          <t>2026-02-19T08:55:02</t>
         </is>
       </c>
       <c r="O128" t="inlineStr">
@@ -9332,7 +9337,7 @@
       </c>
       <c r="N130" t="inlineStr">
         <is>
-          <t>2026-02-18T18:20:49</t>
+          <t>2026-02-19T09:06:55</t>
         </is>
       </c>
       <c r="O130" t="inlineStr">
@@ -9398,7 +9403,7 @@
       </c>
       <c r="N131" t="inlineStr">
         <is>
-          <t>2026-02-18T17:21:39</t>
+          <t>2026-02-19T08:48:08</t>
         </is>
       </c>
       <c r="O131" t="inlineStr">
@@ -9535,7 +9540,7 @@
       </c>
       <c r="N133" t="inlineStr">
         <is>
-          <t>2026-02-18T19:13:46</t>
+          <t>2026-02-19T08:57:23</t>
         </is>
       </c>
       <c r="O133" t="inlineStr">
@@ -9667,7 +9672,7 @@
       </c>
       <c r="N135" t="inlineStr">
         <is>
-          <t>2026-02-18T19:25:18</t>
+          <t>2026-02-19T08:59:06</t>
         </is>
       </c>
       <c r="O135" t="inlineStr">
@@ -9864,7 +9869,7 @@
       </c>
       <c r="N138" t="inlineStr">
         <is>
-          <t>2026-02-18T19:05:19</t>
+          <t>2026-02-19T08:57:53</t>
         </is>
       </c>
       <c r="O138" t="inlineStr">
@@ -9930,7 +9935,7 @@
       </c>
       <c r="N139" t="inlineStr">
         <is>
-          <t>2026-02-18T19:32:20</t>
+          <t>2026-02-19T08:46:11</t>
         </is>
       </c>
       <c r="O139" t="inlineStr">
@@ -9996,7 +10001,7 @@
       </c>
       <c r="N140" t="inlineStr">
         <is>
-          <t>2026-02-18T19:47:43</t>
+          <t>2026-02-19T09:00:42</t>
         </is>
       </c>
       <c r="O140" t="inlineStr">
@@ -10128,7 +10133,7 @@
       </c>
       <c r="N142" t="inlineStr">
         <is>
-          <t>2026-02-19T07:31:55</t>
+          <t>2026-02-19T09:23:01</t>
         </is>
       </c>
       <c r="O142" t="inlineStr">
@@ -10194,7 +10199,7 @@
       </c>
       <c r="N143" t="inlineStr">
         <is>
-          <t>2026-02-19T07:32:21</t>
+          <t>2026-02-19T09:21:49</t>
         </is>
       </c>
       <c r="O143" t="inlineStr">
@@ -10260,7 +10265,7 @@
       </c>
       <c r="N144" t="inlineStr">
         <is>
-          <t>2026-02-18T19:36:56</t>
+          <t>2026-02-19T09:30:39</t>
         </is>
       </c>
       <c r="O144" t="inlineStr">
@@ -10326,7 +10331,7 @@
       </c>
       <c r="N145" t="inlineStr">
         <is>
-          <t>2026-02-19T07:32:22</t>
+          <t>2026-02-19T09:26:35</t>
         </is>
       </c>
       <c r="O145" t="inlineStr">
@@ -10392,7 +10397,7 @@
       </c>
       <c r="N146" t="inlineStr">
         <is>
-          <t>2026-02-19T07:33:39</t>
+          <t>2026-02-19T09:28:44</t>
         </is>
       </c>
       <c r="O146" t="inlineStr">
@@ -10458,7 +10463,7 @@
       </c>
       <c r="N147" t="inlineStr">
         <is>
-          <t>2026-02-19T07:32:46</t>
+          <t>2026-02-19T09:21:36</t>
         </is>
       </c>
       <c r="O147" t="inlineStr">
@@ -10524,7 +10529,7 @@
       </c>
       <c r="N148" t="inlineStr">
         <is>
-          <t>2026-02-19T07:32:17</t>
+          <t>2026-02-19T09:22:44</t>
         </is>
       </c>
       <c r="O148" t="inlineStr">
@@ -10590,7 +10595,7 @@
       </c>
       <c r="N149" t="inlineStr">
         <is>
-          <t>2026-02-19T07:31:57</t>
+          <t>2026-02-19T09:22:59</t>
         </is>
       </c>
       <c r="O149" t="inlineStr">
@@ -10656,7 +10661,7 @@
       </c>
       <c r="N150" t="inlineStr">
         <is>
-          <t>2026-02-19T07:31:47</t>
+          <t>2026-02-19T09:27:55</t>
         </is>
       </c>
       <c r="O150" t="inlineStr">
@@ -10722,7 +10727,7 @@
       </c>
       <c r="N151" t="inlineStr">
         <is>
-          <t>2026-02-18T18:58:56</t>
+          <t>2026-02-19T09:20:40</t>
         </is>
       </c>
       <c r="O151" t="inlineStr">
@@ -10788,7 +10793,7 @@
       </c>
       <c r="N152" t="inlineStr">
         <is>
-          <t>2026-02-18T19:32:04</t>
+          <t>2026-02-19T09:22:29</t>
         </is>
       </c>
       <c r="O152" t="inlineStr">
@@ -10915,7 +10920,7 @@
       </c>
       <c r="N154" t="inlineStr">
         <is>
-          <t>2026-02-19T07:40:48</t>
+          <t>2026-02-19T09:28:36</t>
         </is>
       </c>
       <c r="O154" t="inlineStr">
@@ -10981,7 +10986,7 @@
       </c>
       <c r="N155" t="inlineStr">
         <is>
-          <t>2026-02-18T20:00:10</t>
+          <t>2026-02-19T09:09:08</t>
         </is>
       </c>
       <c r="O155" t="inlineStr">
@@ -11047,7 +11052,7 @@
       </c>
       <c r="N156" t="inlineStr">
         <is>
-          <t>2026-02-18T09:01:01</t>
+          <t>2026-02-19T08:56:45</t>
         </is>
       </c>
       <c r="O156" t="inlineStr">
@@ -11113,7 +11118,7 @@
       </c>
       <c r="N157" t="inlineStr">
         <is>
-          <t>2026-02-18T19:51:39</t>
+          <t>2026-02-19T09:09:20</t>
         </is>
       </c>
       <c r="O157" t="inlineStr">
@@ -11146,7 +11151,7 @@
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>Microsoft Windows 8.1 Pro</t>
+          <t>Windows</t>
         </is>
       </c>
       <c r="G158" t="inlineStr">
@@ -11179,7 +11184,7 @@
       </c>
       <c r="N158" t="inlineStr">
         <is>
-          <t>2026-02-18T13:10:35</t>
+          <t>2026-02-19T08:46:52</t>
         </is>
       </c>
       <c r="O158" t="inlineStr">
@@ -11245,7 +11250,7 @@
       </c>
       <c r="N159" t="inlineStr">
         <is>
-          <t>2026-02-18T19:46:47</t>
+          <t>2026-02-19T09:35:50</t>
         </is>
       </c>
       <c r="O159" t="inlineStr">
@@ -11311,7 +11316,7 @@
       </c>
       <c r="N160" t="inlineStr">
         <is>
-          <t>2026-02-19T07:01:37</t>
+          <t>2026-02-19T09:38:15</t>
         </is>
       </c>
       <c r="O160" t="inlineStr">
@@ -11377,7 +11382,7 @@
       </c>
       <c r="N161" t="inlineStr">
         <is>
-          <t>2026-02-19T07:13:00</t>
+          <t>2026-02-19T09:05:09</t>
         </is>
       </c>
       <c r="O161" t="inlineStr">
@@ -11443,7 +11448,7 @@
       </c>
       <c r="N162" t="inlineStr">
         <is>
-          <t>2026-02-18T19:11:35</t>
+          <t>2026-02-19T09:29:23</t>
         </is>
       </c>
       <c r="O162" t="inlineStr">
@@ -11571,11 +11576,11 @@
         </is>
       </c>
       <c r="M164" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N164" t="inlineStr">
         <is>
-          <t>2026-02-19T06:51:08</t>
+          <t>2026-02-19T09:34:23</t>
         </is>
       </c>
       <c r="O164" t="inlineStr">
@@ -11637,11 +11642,11 @@
         </is>
       </c>
       <c r="M165" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N165" t="inlineStr">
         <is>
-          <t>2026-02-19T06:53:58</t>
+          <t>2026-02-19T08:44:27</t>
         </is>
       </c>
       <c r="O165" t="inlineStr">
@@ -11707,7 +11712,7 @@
       </c>
       <c r="N166" t="inlineStr">
         <is>
-          <t>2026-02-18T14:55:47</t>
+          <t>2026-02-19T09:26:59</t>
         </is>
       </c>
       <c r="O166" t="inlineStr">
@@ -11773,7 +11778,7 @@
       </c>
       <c r="N167" t="inlineStr">
         <is>
-          <t>2026-02-18T18:45:29</t>
+          <t>2026-02-19T08:57:07</t>
         </is>
       </c>
       <c r="O167" t="inlineStr">
@@ -11839,7 +11844,7 @@
       </c>
       <c r="N168" t="inlineStr">
         <is>
-          <t>2026-02-18T13:51:25</t>
+          <t>2026-02-19T09:03:30</t>
         </is>
       </c>
       <c r="O168" t="inlineStr">
@@ -11905,7 +11910,7 @@
       </c>
       <c r="N169" t="inlineStr">
         <is>
-          <t>2026-02-19T06:50:57</t>
+          <t>2026-02-19T09:36:15</t>
         </is>
       </c>
       <c r="O169" t="inlineStr">
@@ -11971,7 +11976,7 @@
       </c>
       <c r="N170" t="inlineStr">
         <is>
-          <t>2026-02-18T16:14:14</t>
+          <t>2026-02-19T08:56:13</t>
         </is>
       </c>
       <c r="O170" t="inlineStr">
@@ -12033,11 +12038,11 @@
         </is>
       </c>
       <c r="M171" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N171" t="inlineStr">
         <is>
-          <t>2026-02-18T18:48:28</t>
+          <t>2026-02-19T08:53:35</t>
         </is>
       </c>
       <c r="O171" t="inlineStr">
@@ -12165,7 +12170,7 @@
         </is>
       </c>
       <c r="M173" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N173" t="inlineStr">
         <is>
@@ -12235,7 +12240,7 @@
       </c>
       <c r="N174" t="inlineStr">
         <is>
-          <t>2026-02-19T07:38:05</t>
+          <t>2026-02-19T09:29:51</t>
         </is>
       </c>
       <c r="O174" t="inlineStr">
@@ -12301,7 +12306,7 @@
       </c>
       <c r="N175" t="inlineStr">
         <is>
-          <t>2026-02-19T06:58:04</t>
+          <t>2026-02-19T09:38:02</t>
         </is>
       </c>
       <c r="O175" t="inlineStr">
@@ -12499,7 +12504,7 @@
       </c>
       <c r="N178" t="inlineStr">
         <is>
-          <t>2026-02-19T06:54:25</t>
+          <t>2026-02-19T09:30:22</t>
         </is>
       </c>
       <c r="O178" t="inlineStr">
@@ -12565,7 +12570,7 @@
       </c>
       <c r="N179" t="inlineStr">
         <is>
-          <t>2026-02-18T13:37:18</t>
+          <t>2026-02-19T09:31:44</t>
         </is>
       </c>
       <c r="O179" t="inlineStr">
@@ -12631,7 +12636,7 @@
       </c>
       <c r="N180" t="inlineStr">
         <is>
-          <t>2026-02-19T07:33:46</t>
+          <t>2026-02-19T09:30:48</t>
         </is>
       </c>
       <c r="O180" t="inlineStr">
@@ -12697,7 +12702,7 @@
       </c>
       <c r="N181" t="inlineStr">
         <is>
-          <t>2026-02-18T19:15:55</t>
+          <t>2026-02-19T09:35:46</t>
         </is>
       </c>
       <c r="O181" t="inlineStr">
@@ -12966,7 +12971,7 @@
       </c>
       <c r="N185" t="inlineStr">
         <is>
-          <t>2026-02-13T13:32:01</t>
+          <t>2026-02-19T09:36:00</t>
         </is>
       </c>
       <c r="O185" t="inlineStr">
@@ -13032,7 +13037,7 @@
       </c>
       <c r="N186" t="inlineStr">
         <is>
-          <t>2026-02-18T14:26:49</t>
+          <t>2026-02-19T09:33:00</t>
         </is>
       </c>
       <c r="O186" t="inlineStr">
@@ -13098,7 +13103,7 @@
       </c>
       <c r="N187" t="inlineStr">
         <is>
-          <t>2026-02-18T20:10:45</t>
+          <t>2026-02-19T09:28:50</t>
         </is>
       </c>
       <c r="O187" t="inlineStr">
@@ -13164,7 +13169,7 @@
       </c>
       <c r="N188" t="inlineStr">
         <is>
-          <t>2026-02-19T07:30:52</t>
+          <t>2026-02-19T09:38:44</t>
         </is>
       </c>
       <c r="O188" t="inlineStr">
@@ -13296,7 +13301,7 @@
       </c>
       <c r="N190" t="inlineStr">
         <is>
-          <t>2026-02-18T19:29:22</t>
+          <t>2026-02-19T09:29:11</t>
         </is>
       </c>
       <c r="O190" t="inlineStr">
@@ -13428,7 +13433,7 @@
       </c>
       <c r="N192" t="inlineStr">
         <is>
-          <t>2026-02-18T19:08:08</t>
+          <t>2026-02-19T09:40:57</t>
         </is>
       </c>
       <c r="O192" t="inlineStr">
@@ -13557,7 +13562,7 @@
       </c>
       <c r="N194" t="inlineStr">
         <is>
-          <t>2026-02-19T07:29:35</t>
+          <t>2026-02-19T09:36:01</t>
         </is>
       </c>
       <c r="O194" t="inlineStr">
@@ -13623,7 +13628,7 @@
       </c>
       <c r="N195" t="inlineStr">
         <is>
-          <t>2026-02-18T19:27:05</t>
+          <t>2026-02-19T09:26:20</t>
         </is>
       </c>
       <c r="O195" t="inlineStr">
@@ -13689,7 +13694,7 @@
       </c>
       <c r="N196" t="inlineStr">
         <is>
-          <t>2026-02-18T19:49:26</t>
+          <t>2026-02-19T09:04:56</t>
         </is>
       </c>
       <c r="O196" t="inlineStr">
@@ -13755,7 +13760,7 @@
       </c>
       <c r="N197" t="inlineStr">
         <is>
-          <t>2026-02-18T19:32:09</t>
+          <t>2026-02-19T09:10:08</t>
         </is>
       </c>
       <c r="O197" t="inlineStr">
@@ -13821,7 +13826,7 @@
       </c>
       <c r="N198" t="inlineStr">
         <is>
-          <t>2026-02-18T16:27:54</t>
+          <t>2026-02-19T08:12:26</t>
         </is>
       </c>
       <c r="O198" t="inlineStr">
@@ -13887,7 +13892,7 @@
       </c>
       <c r="N199" t="inlineStr">
         <is>
-          <t>2026-02-18T19:23:54</t>
+          <t>2026-02-19T09:11:07</t>
         </is>
       </c>
       <c r="O199" t="inlineStr">
@@ -14016,7 +14021,7 @@
       </c>
       <c r="N201" t="inlineStr">
         <is>
-          <t>2026-02-18T19:45:11</t>
+          <t>2026-02-19T09:02:55</t>
         </is>
       </c>
       <c r="O201" t="inlineStr">
@@ -14082,7 +14087,7 @@
       </c>
       <c r="N202" t="inlineStr">
         <is>
-          <t>2026-02-18T19:47:36</t>
+          <t>2026-02-19T09:08:22</t>
         </is>
       </c>
       <c r="O202" t="inlineStr">
@@ -14148,7 +14153,7 @@
       </c>
       <c r="N203" t="inlineStr">
         <is>
-          <t>2026-02-19T07:17:12</t>
+          <t>2026-02-19T09:03:56</t>
         </is>
       </c>
       <c r="O203" t="inlineStr">
@@ -14214,7 +14219,7 @@
       </c>
       <c r="N204" t="inlineStr">
         <is>
-          <t>2026-02-18T19:48:14</t>
+          <t>2026-02-19T09:04:07</t>
         </is>
       </c>
       <c r="O204" t="inlineStr">
@@ -14280,7 +14285,7 @@
       </c>
       <c r="N205" t="inlineStr">
         <is>
-          <t>2026-02-18T19:27:06</t>
+          <t>2026-02-19T08:44:17</t>
         </is>
       </c>
       <c r="O205" t="inlineStr">
@@ -14346,7 +14351,7 @@
       </c>
       <c r="N206" t="inlineStr">
         <is>
-          <t>2026-02-18T19:26:40</t>
+          <t>2026-02-19T09:13:20</t>
         </is>
       </c>
       <c r="O206" t="inlineStr">
@@ -14412,7 +14417,7 @@
       </c>
       <c r="N207" t="inlineStr">
         <is>
-          <t>2026-02-19T07:31:21</t>
+          <t>2026-02-19T09:15:50</t>
         </is>
       </c>
       <c r="O207" t="inlineStr">
@@ -14478,7 +14483,7 @@
       </c>
       <c r="N208" t="inlineStr">
         <is>
-          <t>2026-02-19T07:32:14</t>
+          <t>2026-02-19T09:30:34</t>
         </is>
       </c>
       <c r="O208" t="inlineStr">
@@ -14544,7 +14549,7 @@
       </c>
       <c r="N209" t="inlineStr">
         <is>
-          <t>2026-02-19T07:38:04</t>
+          <t>2026-02-19T09:26:37</t>
         </is>
       </c>
       <c r="O209" t="inlineStr">
@@ -14610,7 +14615,7 @@
       </c>
       <c r="N210" t="inlineStr">
         <is>
-          <t>2026-02-18T20:54:14</t>
+          <t>2026-02-19T09:28:19</t>
         </is>
       </c>
       <c r="O210" t="inlineStr">
@@ -14676,7 +14681,7 @@
       </c>
       <c r="N211" t="inlineStr">
         <is>
-          <t>2026-02-18T19:36:41</t>
+          <t>2026-02-19T09:37:45</t>
         </is>
       </c>
       <c r="O211" t="inlineStr">
@@ -14742,7 +14747,7 @@
       </c>
       <c r="N212" t="inlineStr">
         <is>
-          <t>2026-02-19T07:40:44</t>
+          <t>2026-02-19T09:27:28</t>
         </is>
       </c>
       <c r="O212" t="inlineStr">
@@ -14808,7 +14813,7 @@
       </c>
       <c r="N213" t="inlineStr">
         <is>
-          <t>2026-02-19T07:41:14</t>
+          <t>2026-02-19T09:26:31</t>
         </is>
       </c>
       <c r="O213" t="inlineStr">
@@ -14940,7 +14945,7 @@
       </c>
       <c r="N215" t="inlineStr">
         <is>
-          <t>2026-02-19T07:38:27</t>
+          <t>2026-02-19T09:32:43</t>
         </is>
       </c>
       <c r="O215" t="inlineStr">
@@ -15006,7 +15011,7 @@
       </c>
       <c r="N216" t="inlineStr">
         <is>
-          <t>2026-02-19T07:40:21</t>
+          <t>2026-02-19T09:38:14</t>
         </is>
       </c>
       <c r="O216" t="inlineStr">
@@ -15072,7 +15077,7 @@
       </c>
       <c r="N217" t="inlineStr">
         <is>
-          <t>2026-02-19T07:41:20</t>
+          <t>2026-02-19T09:35:12</t>
         </is>
       </c>
       <c r="O217" t="inlineStr">
@@ -15204,7 +15209,7 @@
       </c>
       <c r="N219" t="inlineStr">
         <is>
-          <t>2026-02-19T07:08:36</t>
+          <t>2026-02-19T09:01:09</t>
         </is>
       </c>
       <c r="O219" t="inlineStr">
@@ -15275,7 +15280,7 @@
       </c>
       <c r="N220" t="inlineStr">
         <is>
-          <t>2026-02-19T07:41:39</t>
+          <t>2026-02-19T09:40:37</t>
         </is>
       </c>
       <c r="O220" t="inlineStr">
@@ -15341,7 +15346,7 @@
       </c>
       <c r="N221" t="inlineStr">
         <is>
-          <t>2026-02-18T19:41:13</t>
+          <t>2026-02-19T09:03:58</t>
         </is>
       </c>
       <c r="O221" t="inlineStr">
@@ -15473,7 +15478,7 @@
       </c>
       <c r="N223" t="inlineStr">
         <is>
-          <t>2026-02-18T19:01:52</t>
+          <t>2026-02-19T09:10:31</t>
         </is>
       </c>
       <c r="O223" t="inlineStr">
@@ -15605,7 +15610,7 @@
       </c>
       <c r="N225" t="inlineStr">
         <is>
-          <t>2026-02-18T19:39:17</t>
+          <t>2026-02-19T09:31:17</t>
         </is>
       </c>
       <c r="O225" t="inlineStr">
@@ -15671,7 +15676,7 @@
       </c>
       <c r="N226" t="inlineStr">
         <is>
-          <t>2026-02-18T19:41:17</t>
+          <t>2026-02-19T09:34:36</t>
         </is>
       </c>
       <c r="O226" t="inlineStr">
@@ -15737,7 +15742,7 @@
       </c>
       <c r="N227" t="inlineStr">
         <is>
-          <t>2026-02-18T19:10:33</t>
+          <t>2026-02-19T09:02:27</t>
         </is>
       </c>
       <c r="O227" t="inlineStr">
@@ -15803,7 +15808,7 @@
       </c>
       <c r="N228" t="inlineStr">
         <is>
-          <t>2026-02-18T19:43:16</t>
+          <t>2026-02-19T08:50:11</t>
         </is>
       </c>
       <c r="O228" t="inlineStr">
@@ -15869,7 +15874,7 @@
       </c>
       <c r="N229" t="inlineStr">
         <is>
-          <t>2026-02-14T14:37:04</t>
+          <t>2026-02-19T09:14:33</t>
         </is>
       </c>
       <c r="O229" t="inlineStr">
@@ -15935,7 +15940,7 @@
       </c>
       <c r="N230" t="inlineStr">
         <is>
-          <t>2026-02-19T07:40:58</t>
+          <t>2026-02-19T09:01:00</t>
         </is>
       </c>
       <c r="O230" t="inlineStr">
@@ -16001,7 +16006,7 @@
       </c>
       <c r="N231" t="inlineStr">
         <is>
-          <t>2026-02-18T19:41:13</t>
+          <t>2026-02-19T08:57:57</t>
         </is>
       </c>
       <c r="O231" t="inlineStr">
@@ -16067,7 +16072,7 @@
       </c>
       <c r="N232" t="inlineStr">
         <is>
-          <t>2026-02-18T19:09:51</t>
+          <t>2026-02-19T08:45:57</t>
         </is>
       </c>
       <c r="O232" t="inlineStr">
@@ -16133,7 +16138,7 @@
       </c>
       <c r="N233" t="inlineStr">
         <is>
-          <t>2026-02-19T07:37:56</t>
+          <t>2026-02-19T09:03:08</t>
         </is>
       </c>
       <c r="O233" t="inlineStr">
@@ -16199,7 +16204,7 @@
       </c>
       <c r="N234" t="inlineStr">
         <is>
-          <t>2026-02-19T07:26:07</t>
+          <t>2026-02-19T09:11:06</t>
         </is>
       </c>
       <c r="O234" t="inlineStr">
@@ -16463,7 +16468,7 @@
       </c>
       <c r="N238" t="inlineStr">
         <is>
-          <t>2026-02-18T19:48:57</t>
+          <t>2026-02-19T09:35:24</t>
         </is>
       </c>
       <c r="O238" t="inlineStr">
@@ -16529,7 +16534,7 @@
       </c>
       <c r="N239" t="inlineStr">
         <is>
-          <t>2026-02-18T19:39:45</t>
+          <t>2026-02-19T09:40:45</t>
         </is>
       </c>
       <c r="O239" t="inlineStr">
@@ -16595,7 +16600,7 @@
       </c>
       <c r="N240" t="inlineStr">
         <is>
-          <t>2026-02-18T20:40:21</t>
+          <t>2026-02-19T08:54:35</t>
         </is>
       </c>
       <c r="O240" t="inlineStr">
@@ -16661,7 +16666,7 @@
       </c>
       <c r="N241" t="inlineStr">
         <is>
-          <t>2026-02-18T14:14:05</t>
+          <t>2026-02-19T09:00:20</t>
         </is>
       </c>
       <c r="O241" t="inlineStr">
@@ -16727,7 +16732,7 @@
       </c>
       <c r="N242" t="inlineStr">
         <is>
-          <t>2026-02-18T19:33:59</t>
+          <t>2026-02-19T09:01:53</t>
         </is>
       </c>
       <c r="O242" t="inlineStr">
@@ -16793,7 +16798,7 @@
       </c>
       <c r="N243" t="inlineStr">
         <is>
-          <t>2026-02-18T19:54:00</t>
+          <t>2026-02-19T09:36:37</t>
         </is>
       </c>
       <c r="O243" t="inlineStr">
@@ -16920,7 +16925,7 @@
       </c>
       <c r="N245" t="inlineStr">
         <is>
-          <t>2026-02-18T19:33:45</t>
+          <t>2026-02-19T09:36:49</t>
         </is>
       </c>
       <c r="O245" t="inlineStr">
@@ -16986,7 +16991,7 @@
       </c>
       <c r="N246" t="inlineStr">
         <is>
-          <t>2026-02-18T20:18:58</t>
+          <t>2026-02-19T09:13:40</t>
         </is>
       </c>
       <c r="O246" t="inlineStr">
@@ -17052,7 +17057,7 @@
       </c>
       <c r="N247" t="inlineStr">
         <is>
-          <t>2026-02-18T19:42:20</t>
+          <t>2026-02-19T08:46:03</t>
         </is>
       </c>
       <c r="O247" t="inlineStr">
@@ -17118,7 +17123,7 @@
       </c>
       <c r="N248" t="inlineStr">
         <is>
-          <t>2026-02-18T19:17:38</t>
+          <t>2026-02-19T08:46:47</t>
         </is>
       </c>
       <c r="O248" t="inlineStr">
@@ -17184,7 +17189,7 @@
       </c>
       <c r="N249" t="inlineStr">
         <is>
-          <t>2026-02-18T19:52:10</t>
+          <t>2026-02-19T09:33:55</t>
         </is>
       </c>
       <c r="O249" t="inlineStr">
@@ -17245,7 +17250,7 @@
       </c>
       <c r="N250" t="inlineStr">
         <is>
-          <t>2026-02-18T19:23:55</t>
+          <t>2026-02-19T08:48:06</t>
         </is>
       </c>
       <c r="O250" t="inlineStr">
@@ -17311,7 +17316,7 @@
       </c>
       <c r="N251" t="inlineStr">
         <is>
-          <t>2026-02-18T20:49:40</t>
+          <t>2026-02-19T09:35:54</t>
         </is>
       </c>
       <c r="O251" t="inlineStr">
@@ -17377,7 +17382,7 @@
       </c>
       <c r="N252" t="inlineStr">
         <is>
-          <t>2026-02-18T19:27:22</t>
+          <t>2026-02-19T09:38:10</t>
         </is>
       </c>
       <c r="O252" t="inlineStr">
@@ -17443,7 +17448,7 @@
       </c>
       <c r="N253" t="inlineStr">
         <is>
-          <t>2026-02-18T19:38:50</t>
+          <t>2026-02-19T08:47:25</t>
         </is>
       </c>
       <c r="O253" t="inlineStr">
@@ -17503,7 +17508,7 @@
       </c>
       <c r="N254" t="inlineStr">
         <is>
-          <t>2026-02-19T07:39:39</t>
+          <t>2026-02-19T09:24:12</t>
         </is>
       </c>
       <c r="O254" t="inlineStr">
@@ -17569,7 +17574,7 @@
       </c>
       <c r="N255" t="inlineStr">
         <is>
-          <t>2026-02-18T19:22:19</t>
+          <t>2026-02-19T08:46:21</t>
         </is>
       </c>
       <c r="O255" t="inlineStr">
@@ -17635,7 +17640,7 @@
       </c>
       <c r="N256" t="inlineStr">
         <is>
-          <t>2026-02-18T19:45:15</t>
+          <t>2026-02-19T08:49:01</t>
         </is>
       </c>
       <c r="O256" t="inlineStr">
@@ -17701,7 +17706,7 @@
       </c>
       <c r="N257" t="inlineStr">
         <is>
-          <t>2026-02-18T19:27:49</t>
+          <t>2026-02-19T09:27:54</t>
         </is>
       </c>
       <c r="O257" t="inlineStr">
@@ -17767,7 +17772,7 @@
       </c>
       <c r="N258" t="inlineStr">
         <is>
-          <t>2026-02-18T19:15:19</t>
+          <t>2026-02-19T09:00:22</t>
         </is>
       </c>
       <c r="O258" t="inlineStr">
@@ -17833,7 +17838,7 @@
       </c>
       <c r="N259" t="inlineStr">
         <is>
-          <t>2026-02-18T19:25:01</t>
+          <t>2026-02-19T09:13:07</t>
         </is>
       </c>
       <c r="O259" t="inlineStr">
@@ -17899,7 +17904,7 @@
       </c>
       <c r="N260" t="inlineStr">
         <is>
-          <t>2026-02-18T14:01:31</t>
+          <t>2026-02-19T09:23:16</t>
         </is>
       </c>
       <c r="O260" t="inlineStr">
@@ -17965,7 +17970,7 @@
       </c>
       <c r="N261" t="inlineStr">
         <is>
-          <t>2026-02-18T15:52:16</t>
+          <t>2026-02-19T08:54:09</t>
         </is>
       </c>
       <c r="O261" t="inlineStr">
@@ -18031,7 +18036,7 @@
       </c>
       <c r="N262" t="inlineStr">
         <is>
-          <t>2026-02-18T16:21:43</t>
+          <t>2026-02-19T09:34:27</t>
         </is>
       </c>
       <c r="O262" t="inlineStr">
@@ -18097,7 +18102,7 @@
       </c>
       <c r="N263" t="inlineStr">
         <is>
-          <t>2026-02-18T19:35:04</t>
+          <t>2026-02-19T09:02:33</t>
         </is>
       </c>
       <c r="O263" t="inlineStr">
@@ -18163,7 +18168,7 @@
       </c>
       <c r="N264" t="inlineStr">
         <is>
-          <t>2026-02-18T19:44:39</t>
+          <t>2026-02-19T09:32:52</t>
         </is>
       </c>
       <c r="O264" t="inlineStr">
@@ -18229,7 +18234,7 @@
       </c>
       <c r="N265" t="inlineStr">
         <is>
-          <t>2026-02-18T20:38:19</t>
+          <t>2026-02-19T09:36:57</t>
         </is>
       </c>
       <c r="O265" t="inlineStr">
@@ -18295,7 +18300,7 @@
       </c>
       <c r="N266" t="inlineStr">
         <is>
-          <t>2026-02-18T20:21:13</t>
+          <t>2026-02-19T09:25:26</t>
         </is>
       </c>
       <c r="O266" t="inlineStr">
@@ -18361,7 +18366,7 @@
       </c>
       <c r="N267" t="inlineStr">
         <is>
-          <t>2026-02-18T19:23:48</t>
+          <t>2026-02-19T08:59:44</t>
         </is>
       </c>
       <c r="O267" t="inlineStr">
@@ -18427,7 +18432,7 @@
       </c>
       <c r="N268" t="inlineStr">
         <is>
-          <t>2026-02-18T19:18:54</t>
+          <t>2026-02-19T09:08:20</t>
         </is>
       </c>
       <c r="O268" t="inlineStr">
@@ -18556,7 +18561,7 @@
       </c>
       <c r="N270" t="inlineStr">
         <is>
-          <t>2026-02-19T07:39:48</t>
+          <t>2026-02-19T09:39:54</t>
         </is>
       </c>
       <c r="O270" t="inlineStr">
@@ -18688,7 +18693,7 @@
       </c>
       <c r="N272" t="inlineStr">
         <is>
-          <t>2026-02-18T19:53:13</t>
+          <t>2026-02-19T08:56:31</t>
         </is>
       </c>
       <c r="O272" t="inlineStr">
@@ -18754,7 +18759,7 @@
       </c>
       <c r="N273" t="inlineStr">
         <is>
-          <t>2026-02-19T07:17:05</t>
+          <t>2026-02-19T09:05:46</t>
         </is>
       </c>
       <c r="O273" t="inlineStr">
@@ -19084,7 +19089,7 @@
       </c>
       <c r="N278" t="inlineStr">
         <is>
-          <t>2026-02-19T07:26:08</t>
+          <t>2026-02-19T09:15:43</t>
         </is>
       </c>
       <c r="O278" t="inlineStr">
@@ -19150,7 +19155,7 @@
       </c>
       <c r="N279" t="inlineStr">
         <is>
-          <t>2026-02-19T07:17:54</t>
+          <t>2026-02-19T09:20:29</t>
         </is>
       </c>
       <c r="O279" t="inlineStr">
@@ -19216,7 +19221,7 @@
       </c>
       <c r="N280" t="inlineStr">
         <is>
-          <t>2026-02-19T06:55:26</t>
+          <t>2026-02-19T09:03:40</t>
         </is>
       </c>
       <c r="O280" t="inlineStr">
@@ -19282,7 +19287,7 @@
       </c>
       <c r="N281" t="inlineStr">
         <is>
-          <t>2026-02-19T07:36:32</t>
+          <t>2026-02-19T09:25:00</t>
         </is>
       </c>
       <c r="O281" t="inlineStr">
@@ -19348,7 +19353,7 @@
       </c>
       <c r="N282" t="inlineStr">
         <is>
-          <t>2026-02-19T07:35:36</t>
+          <t>2026-02-19T09:31:54</t>
         </is>
       </c>
       <c r="O282" t="inlineStr">
@@ -19414,7 +19419,7 @@
       </c>
       <c r="N283" t="inlineStr">
         <is>
-          <t>2026-02-18T19:51:45</t>
+          <t>2026-02-19T09:16:09</t>
         </is>
       </c>
       <c r="O283" t="inlineStr">
@@ -19480,7 +19485,7 @@
       </c>
       <c r="N284" t="inlineStr">
         <is>
-          <t>2026-02-18T20:55:53</t>
+          <t>2026-02-19T08:58:02</t>
         </is>
       </c>
       <c r="O284" t="inlineStr">
@@ -19546,7 +19551,7 @@
       </c>
       <c r="N285" t="inlineStr">
         <is>
-          <t>2026-02-18T13:18:17</t>
+          <t>2026-02-19T09:32:44</t>
         </is>
       </c>
       <c r="O285" t="inlineStr">
@@ -19612,7 +19617,7 @@
       </c>
       <c r="N286" t="inlineStr">
         <is>
-          <t>2026-02-19T05:47:01</t>
+          <t>2026-02-19T08:20:24</t>
         </is>
       </c>
       <c r="O286" t="inlineStr">
@@ -19678,7 +19683,7 @@
       </c>
       <c r="N287" t="inlineStr">
         <is>
-          <t>2026-02-19T04:14:19</t>
+          <t>2026-02-19T08:56:53</t>
         </is>
       </c>
       <c r="O287" t="inlineStr">
@@ -19744,7 +19749,7 @@
       </c>
       <c r="N288" t="inlineStr">
         <is>
-          <t>2026-02-19T07:35:27</t>
+          <t>2026-02-19T09:28:49</t>
         </is>
       </c>
       <c r="O288" t="inlineStr">
@@ -20630,7 +20635,7 @@
       </c>
       <c r="N302" t="inlineStr">
         <is>
-          <t>2026-02-19T07:38:59</t>
+          <t>2026-02-19T09:26:30</t>
         </is>
       </c>
       <c r="O302" t="inlineStr">
@@ -21782,7 +21787,7 @@
       </c>
       <c r="N320" t="inlineStr">
         <is>
-          <t>2026-02-19T07:27:06</t>
+          <t>2026-02-19T09:16:22</t>
         </is>
       </c>
       <c r="O320" t="inlineStr">
@@ -22531,7 +22536,7 @@
       </c>
       <c r="N332" t="inlineStr">
         <is>
-          <t>2026-02-18T18:25:12</t>
+          <t>2026-02-19T09:03:06</t>
         </is>
       </c>
       <c r="O332" t="inlineStr">
@@ -22597,7 +22602,7 @@
       </c>
       <c r="N333" t="inlineStr">
         <is>
-          <t>2026-02-19T06:46:13</t>
+          <t>2026-02-19T09:34:14</t>
         </is>
       </c>
       <c r="O333" t="inlineStr">
@@ -22663,7 +22668,7 @@
       </c>
       <c r="N334" t="inlineStr">
         <is>
-          <t>2026-02-19T06:47:03</t>
+          <t>2026-02-19T09:31:42</t>
         </is>
       </c>
       <c r="O334" t="inlineStr">
@@ -22729,7 +22734,7 @@
       </c>
       <c r="N335" t="inlineStr">
         <is>
-          <t>2026-02-19T06:46:26</t>
+          <t>2026-02-19T09:33:21</t>
         </is>
       </c>
       <c r="O335" t="inlineStr">
@@ -22795,7 +22800,7 @@
       </c>
       <c r="N336" t="inlineStr">
         <is>
-          <t>2026-02-19T06:46:36</t>
+          <t>2026-02-19T09:40:14</t>
         </is>
       </c>
       <c r="O336" t="inlineStr">
@@ -22861,7 +22866,7 @@
       </c>
       <c r="N337" t="inlineStr">
         <is>
-          <t>2026-02-19T06:46:38</t>
+          <t>2026-02-19T09:35:07</t>
         </is>
       </c>
       <c r="O337" t="inlineStr">
@@ -22927,7 +22932,7 @@
       </c>
       <c r="N338" t="inlineStr">
         <is>
-          <t>2026-02-19T07:22:06</t>
+          <t>2026-02-19T09:12:56</t>
         </is>
       </c>
       <c r="O338" t="inlineStr">
@@ -22993,7 +22998,7 @@
       </c>
       <c r="N339" t="inlineStr">
         <is>
-          <t>2026-02-19T07:27:31</t>
+          <t>2026-02-19T09:39:30</t>
         </is>
       </c>
       <c r="O339" t="inlineStr">
@@ -23125,7 +23130,7 @@
       </c>
       <c r="N341" t="inlineStr">
         <is>
-          <t>2026-02-18T13:38:02</t>
+          <t>2026-02-19T08:58:09</t>
         </is>
       </c>
       <c r="O341" t="inlineStr">
@@ -23191,7 +23196,7 @@
       </c>
       <c r="N342" t="inlineStr">
         <is>
-          <t>2026-02-19T06:54:22</t>
+          <t>2026-02-19T09:31:39</t>
         </is>
       </c>
       <c r="O342" t="inlineStr">
@@ -23254,7 +23259,7 @@
       </c>
       <c r="N343" t="inlineStr">
         <is>
-          <t>2026-02-18T17:40:27</t>
+          <t>2026-02-19T09:20:26</t>
         </is>
       </c>
       <c r="O343" t="inlineStr">
@@ -23518,7 +23523,7 @@
       </c>
       <c r="N347" t="inlineStr">
         <is>
-          <t>2026-02-12T16:32:39</t>
+          <t>2026-02-19T08:45:39</t>
         </is>
       </c>
       <c r="O347" t="inlineStr">
@@ -23584,7 +23589,7 @@
       </c>
       <c r="N348" t="inlineStr">
         <is>
-          <t>2026-02-12T20:31:39</t>
+          <t>2026-02-19T08:45:46</t>
         </is>
       </c>
       <c r="O348" t="inlineStr">
@@ -23650,7 +23655,7 @@
       </c>
       <c r="N349" t="inlineStr">
         <is>
-          <t>2026-02-12T16:33:36</t>
+          <t>2026-02-19T09:39:12</t>
         </is>
       </c>
       <c r="O349" t="inlineStr">
@@ -23711,7 +23716,7 @@
       </c>
       <c r="N350" t="inlineStr">
         <is>
-          <t>2026-02-12T16:10:32</t>
+          <t>2026-02-19T09:21:34</t>
         </is>
       </c>
       <c r="O350" t="inlineStr">
@@ -23777,7 +23782,7 @@
       </c>
       <c r="N351" t="inlineStr">
         <is>
-          <t>2026-02-12T16:40:02</t>
+          <t>2026-02-19T08:46:21</t>
         </is>
       </c>
       <c r="O351" t="inlineStr">
@@ -23843,7 +23848,7 @@
       </c>
       <c r="N352" t="inlineStr">
         <is>
-          <t>2026-02-19T07:02:28</t>
+          <t>2026-02-19T08:54:24</t>
         </is>
       </c>
       <c r="O352" t="inlineStr">
@@ -23906,7 +23911,7 @@
       </c>
       <c r="N353" t="inlineStr">
         <is>
-          <t>2026-02-12T16:35:49</t>
+          <t>2026-02-19T08:45:22</t>
         </is>
       </c>
       <c r="O353" t="inlineStr">
@@ -23969,7 +23974,7 @@
       </c>
       <c r="N354" t="inlineStr">
         <is>
-          <t>2026-02-12T16:34:55</t>
+          <t>2026-02-19T08:45:32</t>
         </is>
       </c>
       <c r="O354" t="inlineStr">
@@ -24035,7 +24040,7 @@
       </c>
       <c r="N355" t="inlineStr">
         <is>
-          <t>2026-02-12T16:41:56</t>
+          <t>2026-02-19T09:37:02</t>
         </is>
       </c>
       <c r="O355" t="inlineStr">
@@ -24101,7 +24106,7 @@
       </c>
       <c r="N356" t="inlineStr">
         <is>
-          <t>2026-02-11T20:44:03</t>
+          <t>2026-02-19T09:40:47</t>
         </is>
       </c>
       <c r="O356" t="inlineStr">
@@ -24167,7 +24172,7 @@
       </c>
       <c r="N357" t="inlineStr">
         <is>
-          <t>2026-02-12T16:40:31</t>
+          <t>2026-02-19T08:44:53</t>
         </is>
       </c>
       <c r="O357" t="inlineStr">
@@ -24228,7 +24233,7 @@
       </c>
       <c r="N358" t="inlineStr">
         <is>
-          <t>2026-02-12T16:37:14</t>
+          <t>2026-02-19T08:48:37</t>
         </is>
       </c>
       <c r="O358" t="inlineStr">
@@ -24294,7 +24299,7 @@
       </c>
       <c r="N359" t="inlineStr">
         <is>
-          <t>2026-02-12T16:35:52</t>
+          <t>2026-02-19T09:37:14</t>
         </is>
       </c>
       <c r="O359" t="inlineStr">
@@ -24360,7 +24365,7 @@
       </c>
       <c r="N360" t="inlineStr">
         <is>
-          <t>2026-02-12T16:48:22</t>
+          <t>2026-02-19T08:46:41</t>
         </is>
       </c>
       <c r="O360" t="inlineStr">
@@ -24426,7 +24431,7 @@
       </c>
       <c r="N361" t="inlineStr">
         <is>
-          <t>2026-02-13T11:16:06</t>
+          <t>2026-02-19T08:45:27</t>
         </is>
       </c>
       <c r="O361" t="inlineStr">
@@ -24489,7 +24494,7 @@
       </c>
       <c r="N362" t="inlineStr">
         <is>
-          <t>2026-02-12T13:30:33</t>
+          <t>2026-02-19T09:26:52</t>
         </is>
       </c>
       <c r="O362" t="inlineStr">
@@ -24618,7 +24623,7 @@
       </c>
       <c r="N364" t="inlineStr">
         <is>
-          <t>2026-02-09T20:46:41</t>
+          <t>2026-02-19T09:30:19</t>
         </is>
       </c>
       <c r="O364" t="inlineStr">
@@ -24683,7 +24688,7 @@
       </c>
       <c r="N365" t="inlineStr">
         <is>
-          <t>2026-02-18T16:53:17</t>
+          <t>2026-02-19T08:53:56</t>
         </is>
       </c>
       <c r="O365" t="inlineStr">
@@ -24751,7 +24756,7 @@
       </c>
       <c r="N366" t="inlineStr">
         <is>
-          <t>2026-02-19T07:09:16</t>
+          <t>2026-02-19T08:52:38</t>
         </is>
       </c>
       <c r="O366" t="inlineStr">
@@ -24881,7 +24886,7 @@
       </c>
       <c r="N368" t="inlineStr">
         <is>
-          <t>2026-02-19T07:06:07</t>
+          <t>2026-02-19T08:59:30</t>
         </is>
       </c>
       <c r="O368" t="inlineStr">
@@ -24901,11 +24906,6 @@
           <t>RH</t>
         </is>
       </c>
-      <c r="C369" t="inlineStr">
-        <is>
-          <t>10.69.3.13</t>
-        </is>
-      </c>
       <c r="D369" t="n">
         <v>2025</v>
       </c>
@@ -24949,7 +24949,7 @@
       </c>
       <c r="N369" t="inlineStr">
         <is>
-          <t>2026-02-18T16:29:40</t>
+          <t>2026-02-19T09:00:50</t>
         </is>
       </c>
       <c r="O369" t="inlineStr">
@@ -25020,7 +25020,7 @@
       </c>
       <c r="N370" t="inlineStr">
         <is>
-          <t>2026-02-18T16:50:17</t>
+          <t>2026-02-19T09:38:08</t>
         </is>
       </c>
       <c r="O370" t="inlineStr">
@@ -25233,7 +25233,7 @@
       </c>
       <c r="N373" t="inlineStr">
         <is>
-          <t>2026-02-12T13:53:49</t>
+          <t>2026-02-19T09:26:51</t>
         </is>
       </c>
       <c r="O373" t="inlineStr">
@@ -25304,7 +25304,7 @@
       </c>
       <c r="N374" t="inlineStr">
         <is>
-          <t>2026-01-30T16:55:32</t>
+          <t>2026-02-19T09:02:59</t>
         </is>
       </c>
       <c r="O374" t="inlineStr">
@@ -25372,7 +25372,7 @@
       </c>
       <c r="N375" t="inlineStr">
         <is>
-          <t>2026-02-19T07:00:30</t>
+          <t>2026-02-19T08:53:24</t>
         </is>
       </c>
       <c r="O375" t="inlineStr">
@@ -25509,7 +25509,7 @@
       </c>
       <c r="N377" t="inlineStr">
         <is>
-          <t>2026-02-18T15:50:46</t>
+          <t>2026-02-19T08:47:57</t>
         </is>
       </c>
       <c r="O377" t="inlineStr">
@@ -25580,7 +25580,7 @@
       </c>
       <c r="N378" t="inlineStr">
         <is>
-          <t>2026-02-19T06:57:16</t>
+          <t>2026-02-19T08:55:00</t>
         </is>
       </c>
       <c r="O378" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática 2026-02-19 11:52:03.839235
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -601,7 +601,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>2026-02-19T08:53:36</t>
+          <t>2026-02-19T11:42:02</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -672,7 +672,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>2026-02-19T09:21:13</t>
+          <t>2026-02-19T11:07:11</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -743,7 +743,7 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>2026-02-19T09:16:54</t>
+          <t>2026-02-19T11:14:10</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
@@ -814,7 +814,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>2026-02-19T08:50:48</t>
+          <t>2026-02-19T11:38:57</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -1144,7 +1144,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>2026-02-19T09:12:37</t>
+          <t>2026-02-19T11:11:35</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -1474,7 +1474,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>2026-02-19T09:15:09</t>
+          <t>2026-02-19T11:05:10</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
@@ -1606,7 +1606,7 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>2026-02-19T09:41:44</t>
+          <t>2026-02-19T11:25:46</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>2026-02-13T13:54:25</t>
+          <t>2026-02-19T11:29:08</t>
         </is>
       </c>
       <c r="O28" t="inlineStr">
@@ -6885,7 +6885,7 @@
       </c>
       <c r="N95" t="inlineStr">
         <is>
-          <t>2026-02-18T16:44:03</t>
+          <t>2026-02-19T11:40:22</t>
         </is>
       </c>
       <c r="O95" t="inlineStr">
@@ -6976,11 +6976,6 @@
           <t>COORDENACAO</t>
         </is>
       </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>10.69.3.93</t>
-        </is>
-      </c>
       <c r="D97" t="n">
         <v>2025</v>
       </c>
@@ -7027,7 +7022,7 @@
       </c>
       <c r="N97" t="inlineStr">
         <is>
-          <t>2026-02-19T09:38:35</t>
+          <t>2026-02-19T11:25:36</t>
         </is>
       </c>
       <c r="O97" t="inlineStr">
@@ -7093,7 +7088,7 @@
       </c>
       <c r="N98" t="inlineStr">
         <is>
-          <t>2026-02-19T09:04:45</t>
+          <t>2026-02-19T10:57:40</t>
         </is>
       </c>
       <c r="O98" t="inlineStr">
@@ -7164,7 +7159,7 @@
       </c>
       <c r="N99" t="inlineStr">
         <is>
-          <t>2026-02-18T15:59:14</t>
+          <t>2026-02-19T11:38:59</t>
         </is>
       </c>
       <c r="O99" t="inlineStr">
@@ -7235,7 +7230,7 @@
       </c>
       <c r="N100" t="inlineStr">
         <is>
-          <t>2026-02-19T09:24:56</t>
+          <t>2026-02-19T11:20:07</t>
         </is>
       </c>
       <c r="O100" t="inlineStr">
@@ -7306,7 +7301,7 @@
       </c>
       <c r="N101" t="inlineStr">
         <is>
-          <t>2026-02-19T08:57:57</t>
+          <t>2026-02-19T10:56:52</t>
         </is>
       </c>
       <c r="O101" t="inlineStr">
@@ -7448,7 +7443,7 @@
       </c>
       <c r="N103" t="inlineStr">
         <is>
-          <t>2026-02-19T09:06:24</t>
+          <t>2026-02-19T10:56:24</t>
         </is>
       </c>
       <c r="O103" t="inlineStr">
@@ -7713,7 +7708,7 @@
       </c>
       <c r="N107" t="inlineStr">
         <is>
-          <t>2026-02-19T09:16:49</t>
+          <t>2026-02-19T11:05:18</t>
         </is>
       </c>
       <c r="O107" t="inlineStr">
@@ -7855,7 +7850,7 @@
       </c>
       <c r="N109" t="inlineStr">
         <is>
-          <t>2026-02-19T09:17:05</t>
+          <t>2026-02-19T11:12:12</t>
         </is>
       </c>
       <c r="O109" t="inlineStr">
@@ -7926,7 +7921,7 @@
       </c>
       <c r="N110" t="inlineStr">
         <is>
-          <t>2026-02-19T09:41:22</t>
+          <t>2026-02-19T11:28:33</t>
         </is>
       </c>
       <c r="O110" t="inlineStr">
@@ -7997,7 +7992,7 @@
       </c>
       <c r="N111" t="inlineStr">
         <is>
-          <t>2026-02-19T08:45:07</t>
+          <t>2026-02-19T11:40:05</t>
         </is>
       </c>
       <c r="O111" t="inlineStr">
@@ -8068,7 +8063,7 @@
       </c>
       <c r="N112" t="inlineStr">
         <is>
-          <t>2026-02-19T09:11:47</t>
+          <t>2026-02-19T11:10:01</t>
         </is>
       </c>
       <c r="O112" t="inlineStr">
@@ -8139,7 +8134,7 @@
       </c>
       <c r="N113" t="inlineStr">
         <is>
-          <t>2026-02-19T09:12:42</t>
+          <t>2026-02-19T10:57:43</t>
         </is>
       </c>
       <c r="O113" t="inlineStr">
@@ -8210,7 +8205,7 @@
       </c>
       <c r="N114" t="inlineStr">
         <is>
-          <t>2026-02-19T09:25:12</t>
+          <t>2026-02-19T11:12:39</t>
         </is>
       </c>
       <c r="O114" t="inlineStr">
@@ -8278,7 +8273,7 @@
       </c>
       <c r="N115" t="inlineStr">
         <is>
-          <t>2026-02-19T09:18:11</t>
+          <t>2026-02-19T11:08:28</t>
         </is>
       </c>
       <c r="O115" t="inlineStr">
@@ -8349,7 +8344,7 @@
       </c>
       <c r="N116" t="inlineStr">
         <is>
-          <t>2026-02-19T09:24:48</t>
+          <t>2026-02-19T11:10:02</t>
         </is>
       </c>
       <c r="O116" t="inlineStr">
@@ -8420,7 +8415,7 @@
       </c>
       <c r="N117" t="inlineStr">
         <is>
-          <t>2026-02-19T09:37:12</t>
+          <t>2026-02-19T11:30:45</t>
         </is>
       </c>
       <c r="O117" t="inlineStr">
@@ -8630,7 +8625,7 @@
       </c>
       <c r="N120" t="inlineStr">
         <is>
-          <t>2026-02-19T09:01:58</t>
+          <t>2026-02-19T10:59:49</t>
         </is>
       </c>
       <c r="O120" t="inlineStr">
@@ -8701,7 +8696,7 @@
       </c>
       <c r="N121" t="inlineStr">
         <is>
-          <t>2026-02-18T19:35:51</t>
+          <t>2026-02-19T11:34:47</t>
         </is>
       </c>
       <c r="O121" t="inlineStr">
@@ -8769,7 +8764,7 @@
       </c>
       <c r="N122" t="inlineStr">
         <is>
-          <t>2026-02-19T09:17:43</t>
+          <t>2026-02-19T11:16:48</t>
         </is>
       </c>
       <c r="O122" t="inlineStr">
@@ -8840,7 +8835,7 @@
       </c>
       <c r="N123" t="inlineStr">
         <is>
-          <t>2026-02-14T14:12:35</t>
+          <t>2026-02-19T10:49:27</t>
         </is>
       </c>
       <c r="O123" t="inlineStr">
@@ -8911,7 +8906,7 @@
       </c>
       <c r="N124" t="inlineStr">
         <is>
-          <t>2026-02-19T09:21:27</t>
+          <t>2026-02-19T11:18:20</t>
         </is>
       </c>
       <c r="O124" t="inlineStr">
@@ -8982,7 +8977,7 @@
       </c>
       <c r="N125" t="inlineStr">
         <is>
-          <t>2026-02-19T09:04:27</t>
+          <t>2026-02-19T10:58:40</t>
         </is>
       </c>
       <c r="O125" t="inlineStr">
@@ -9053,7 +9048,7 @@
       </c>
       <c r="N126" t="inlineStr">
         <is>
-          <t>2026-02-19T08:58:58</t>
+          <t>2026-02-19T10:54:18</t>
         </is>
       </c>
       <c r="O126" t="inlineStr">
@@ -9124,7 +9119,7 @@
       </c>
       <c r="N127" t="inlineStr">
         <is>
-          <t>2026-02-19T09:00:43</t>
+          <t>2026-02-19T10:53:00</t>
         </is>
       </c>
       <c r="O127" t="inlineStr">
@@ -9195,7 +9190,7 @@
       </c>
       <c r="N128" t="inlineStr">
         <is>
-          <t>2026-02-19T08:55:02</t>
+          <t>2026-02-19T11:41:47</t>
         </is>
       </c>
       <c r="O128" t="inlineStr">
@@ -9266,7 +9261,7 @@
       </c>
       <c r="N129" t="inlineStr">
         <is>
-          <t>2026-02-18T18:38:17</t>
+          <t>2026-02-19T11:12:12</t>
         </is>
       </c>
       <c r="O129" t="inlineStr">
@@ -9337,7 +9332,7 @@
       </c>
       <c r="N130" t="inlineStr">
         <is>
-          <t>2026-02-19T09:06:55</t>
+          <t>2026-02-19T11:00:45</t>
         </is>
       </c>
       <c r="O130" t="inlineStr">
@@ -9357,6 +9352,11 @@
           <t>ADM/FIN</t>
         </is>
       </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>10.69.3.6</t>
+        </is>
+      </c>
       <c r="D131" t="n">
         <v>2025</v>
       </c>
@@ -9403,7 +9403,7 @@
       </c>
       <c r="N131" t="inlineStr">
         <is>
-          <t>2026-02-19T08:48:08</t>
+          <t>2026-02-19T11:35:12</t>
         </is>
       </c>
       <c r="O131" t="inlineStr">
@@ -9540,7 +9540,7 @@
       </c>
       <c r="N133" t="inlineStr">
         <is>
-          <t>2026-02-19T08:57:23</t>
+          <t>2026-02-19T10:47:19</t>
         </is>
       </c>
       <c r="O133" t="inlineStr">
@@ -9672,7 +9672,7 @@
       </c>
       <c r="N135" t="inlineStr">
         <is>
-          <t>2026-02-19T08:59:06</t>
+          <t>2026-02-19T10:52:11</t>
         </is>
       </c>
       <c r="O135" t="inlineStr">
@@ -9869,7 +9869,7 @@
       </c>
       <c r="N138" t="inlineStr">
         <is>
-          <t>2026-02-19T08:57:53</t>
+          <t>2026-02-19T10:44:58</t>
         </is>
       </c>
       <c r="O138" t="inlineStr">
@@ -9935,7 +9935,7 @@
       </c>
       <c r="N139" t="inlineStr">
         <is>
-          <t>2026-02-19T08:46:11</t>
+          <t>2026-02-19T11:39:23</t>
         </is>
       </c>
       <c r="O139" t="inlineStr">
@@ -10001,7 +10001,7 @@
       </c>
       <c r="N140" t="inlineStr">
         <is>
-          <t>2026-02-19T09:00:42</t>
+          <t>2026-02-19T10:52:52</t>
         </is>
       </c>
       <c r="O140" t="inlineStr">
@@ -10133,7 +10133,7 @@
       </c>
       <c r="N142" t="inlineStr">
         <is>
-          <t>2026-02-19T09:23:01</t>
+          <t>2026-02-19T11:11:01</t>
         </is>
       </c>
       <c r="O142" t="inlineStr">
@@ -10199,7 +10199,7 @@
       </c>
       <c r="N143" t="inlineStr">
         <is>
-          <t>2026-02-19T09:21:49</t>
+          <t>2026-02-19T11:21:02</t>
         </is>
       </c>
       <c r="O143" t="inlineStr">
@@ -10265,7 +10265,7 @@
       </c>
       <c r="N144" t="inlineStr">
         <is>
-          <t>2026-02-19T09:30:39</t>
+          <t>2026-02-19T11:13:16</t>
         </is>
       </c>
       <c r="O144" t="inlineStr">
@@ -10331,7 +10331,7 @@
       </c>
       <c r="N145" t="inlineStr">
         <is>
-          <t>2026-02-19T09:26:35</t>
+          <t>2026-02-19T11:22:44</t>
         </is>
       </c>
       <c r="O145" t="inlineStr">
@@ -10397,7 +10397,7 @@
       </c>
       <c r="N146" t="inlineStr">
         <is>
-          <t>2026-02-19T09:28:44</t>
+          <t>2026-02-19T11:22:30</t>
         </is>
       </c>
       <c r="O146" t="inlineStr">
@@ -10463,7 +10463,7 @@
       </c>
       <c r="N147" t="inlineStr">
         <is>
-          <t>2026-02-19T09:21:36</t>
+          <t>2026-02-19T11:14:54</t>
         </is>
       </c>
       <c r="O147" t="inlineStr">
@@ -10529,7 +10529,7 @@
       </c>
       <c r="N148" t="inlineStr">
         <is>
-          <t>2026-02-19T09:22:44</t>
+          <t>2026-02-19T11:13:43</t>
         </is>
       </c>
       <c r="O148" t="inlineStr">
@@ -10595,7 +10595,7 @@
       </c>
       <c r="N149" t="inlineStr">
         <is>
-          <t>2026-02-19T09:22:59</t>
+          <t>2026-02-19T11:11:37</t>
         </is>
       </c>
       <c r="O149" t="inlineStr">
@@ -10661,7 +10661,7 @@
       </c>
       <c r="N150" t="inlineStr">
         <is>
-          <t>2026-02-19T09:27:55</t>
+          <t>2026-02-19T11:14:47</t>
         </is>
       </c>
       <c r="O150" t="inlineStr">
@@ -10727,7 +10727,7 @@
       </c>
       <c r="N151" t="inlineStr">
         <is>
-          <t>2026-02-19T09:20:40</t>
+          <t>2026-02-19T11:05:46</t>
         </is>
       </c>
       <c r="O151" t="inlineStr">
@@ -10793,7 +10793,7 @@
       </c>
       <c r="N152" t="inlineStr">
         <is>
-          <t>2026-02-19T09:22:29</t>
+          <t>2026-02-19T11:09:51</t>
         </is>
       </c>
       <c r="O152" t="inlineStr">
@@ -10920,7 +10920,7 @@
       </c>
       <c r="N154" t="inlineStr">
         <is>
-          <t>2026-02-19T09:28:36</t>
+          <t>2026-02-19T11:20:49</t>
         </is>
       </c>
       <c r="O154" t="inlineStr">
@@ -10986,7 +10986,7 @@
       </c>
       <c r="N155" t="inlineStr">
         <is>
-          <t>2026-02-19T09:09:08</t>
+          <t>2026-02-19T10:56:48</t>
         </is>
       </c>
       <c r="O155" t="inlineStr">
@@ -11052,7 +11052,7 @@
       </c>
       <c r="N156" t="inlineStr">
         <is>
-          <t>2026-02-19T08:56:45</t>
+          <t>2026-02-19T11:41:31</t>
         </is>
       </c>
       <c r="O156" t="inlineStr">
@@ -11118,7 +11118,7 @@
       </c>
       <c r="N157" t="inlineStr">
         <is>
-          <t>2026-02-19T09:09:20</t>
+          <t>2026-02-19T11:03:32</t>
         </is>
       </c>
       <c r="O157" t="inlineStr">
@@ -11151,7 +11151,7 @@
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>Windows</t>
+          <t>Microsoft Windows 8.1 Pro</t>
         </is>
       </c>
       <c r="G158" t="inlineStr">
@@ -11184,7 +11184,7 @@
       </c>
       <c r="N158" t="inlineStr">
         <is>
-          <t>2026-02-19T08:46:52</t>
+          <t>2026-02-19T10:00:02</t>
         </is>
       </c>
       <c r="O158" t="inlineStr">
@@ -11250,7 +11250,7 @@
       </c>
       <c r="N159" t="inlineStr">
         <is>
-          <t>2026-02-19T09:35:50</t>
+          <t>2026-02-19T11:25:49</t>
         </is>
       </c>
       <c r="O159" t="inlineStr">
@@ -11316,7 +11316,7 @@
       </c>
       <c r="N160" t="inlineStr">
         <is>
-          <t>2026-02-19T09:38:15</t>
+          <t>2026-02-19T11:27:37</t>
         </is>
       </c>
       <c r="O160" t="inlineStr">
@@ -11382,7 +11382,7 @@
       </c>
       <c r="N161" t="inlineStr">
         <is>
-          <t>2026-02-19T09:05:09</t>
+          <t>2026-02-19T11:02:27</t>
         </is>
       </c>
       <c r="O161" t="inlineStr">
@@ -11448,7 +11448,7 @@
       </c>
       <c r="N162" t="inlineStr">
         <is>
-          <t>2026-02-19T09:29:23</t>
+          <t>2026-02-19T11:23:50</t>
         </is>
       </c>
       <c r="O162" t="inlineStr">
@@ -11580,7 +11580,7 @@
       </c>
       <c r="N164" t="inlineStr">
         <is>
-          <t>2026-02-19T09:34:23</t>
+          <t>2026-02-19T11:30:08</t>
         </is>
       </c>
       <c r="O164" t="inlineStr">
@@ -11646,7 +11646,7 @@
       </c>
       <c r="N165" t="inlineStr">
         <is>
-          <t>2026-02-19T08:44:27</t>
+          <t>2026-02-19T11:29:00</t>
         </is>
       </c>
       <c r="O165" t="inlineStr">
@@ -11712,7 +11712,7 @@
       </c>
       <c r="N166" t="inlineStr">
         <is>
-          <t>2026-02-19T09:26:59</t>
+          <t>2026-02-19T11:20:24</t>
         </is>
       </c>
       <c r="O166" t="inlineStr">
@@ -11778,7 +11778,7 @@
       </c>
       <c r="N167" t="inlineStr">
         <is>
-          <t>2026-02-19T08:57:07</t>
+          <t>2026-02-19T10:53:56</t>
         </is>
       </c>
       <c r="O167" t="inlineStr">
@@ -11844,7 +11844,7 @@
       </c>
       <c r="N168" t="inlineStr">
         <is>
-          <t>2026-02-19T09:03:30</t>
+          <t>2026-02-19T11:40:54</t>
         </is>
       </c>
       <c r="O168" t="inlineStr">
@@ -11910,7 +11910,7 @@
       </c>
       <c r="N169" t="inlineStr">
         <is>
-          <t>2026-02-19T09:36:15</t>
+          <t>2026-02-19T11:35:49</t>
         </is>
       </c>
       <c r="O169" t="inlineStr">
@@ -11976,7 +11976,7 @@
       </c>
       <c r="N170" t="inlineStr">
         <is>
-          <t>2026-02-19T08:56:13</t>
+          <t>2026-02-19T11:39:53</t>
         </is>
       </c>
       <c r="O170" t="inlineStr">
@@ -12042,7 +12042,7 @@
       </c>
       <c r="N171" t="inlineStr">
         <is>
-          <t>2026-02-19T08:53:35</t>
+          <t>2026-02-19T10:49:43</t>
         </is>
       </c>
       <c r="O171" t="inlineStr">
@@ -12240,7 +12240,7 @@
       </c>
       <c r="N174" t="inlineStr">
         <is>
-          <t>2026-02-19T09:29:51</t>
+          <t>2026-02-19T11:19:15</t>
         </is>
       </c>
       <c r="O174" t="inlineStr">
@@ -12306,7 +12306,7 @@
       </c>
       <c r="N175" t="inlineStr">
         <is>
-          <t>2026-02-19T09:38:02</t>
+          <t>2026-02-19T11:31:28</t>
         </is>
       </c>
       <c r="O175" t="inlineStr">
@@ -12372,7 +12372,7 @@
       </c>
       <c r="N176" t="inlineStr">
         <is>
-          <t>2026-02-18T15:55:07</t>
+          <t>2026-02-19T11:03:57</t>
         </is>
       </c>
       <c r="O176" t="inlineStr">
@@ -12438,7 +12438,7 @@
       </c>
       <c r="N177" t="inlineStr">
         <is>
-          <t>2026-02-18T16:22:09</t>
+          <t>2026-02-19T11:03:58</t>
         </is>
       </c>
       <c r="O177" t="inlineStr">
@@ -12504,7 +12504,7 @@
       </c>
       <c r="N178" t="inlineStr">
         <is>
-          <t>2026-02-19T09:30:22</t>
+          <t>2026-02-19T11:13:30</t>
         </is>
       </c>
       <c r="O178" t="inlineStr">
@@ -12570,7 +12570,7 @@
       </c>
       <c r="N179" t="inlineStr">
         <is>
-          <t>2026-02-19T09:31:44</t>
+          <t>2026-02-19T11:26:05</t>
         </is>
       </c>
       <c r="O179" t="inlineStr">
@@ -12636,7 +12636,7 @@
       </c>
       <c r="N180" t="inlineStr">
         <is>
-          <t>2026-02-19T09:30:48</t>
+          <t>2026-02-19T11:20:54</t>
         </is>
       </c>
       <c r="O180" t="inlineStr">
@@ -12702,7 +12702,7 @@
       </c>
       <c r="N181" t="inlineStr">
         <is>
-          <t>2026-02-19T09:35:46</t>
+          <t>2026-02-19T11:32:21</t>
         </is>
       </c>
       <c r="O181" t="inlineStr">
@@ -12971,7 +12971,7 @@
       </c>
       <c r="N185" t="inlineStr">
         <is>
-          <t>2026-02-19T09:36:00</t>
+          <t>2026-02-19T11:23:23</t>
         </is>
       </c>
       <c r="O185" t="inlineStr">
@@ -13037,7 +13037,7 @@
       </c>
       <c r="N186" t="inlineStr">
         <is>
-          <t>2026-02-19T09:33:00</t>
+          <t>2026-02-19T11:25:44</t>
         </is>
       </c>
       <c r="O186" t="inlineStr">
@@ -13103,7 +13103,7 @@
       </c>
       <c r="N187" t="inlineStr">
         <is>
-          <t>2026-02-19T09:28:50</t>
+          <t>2026-02-19T11:16:42</t>
         </is>
       </c>
       <c r="O187" t="inlineStr">
@@ -13169,7 +13169,7 @@
       </c>
       <c r="N188" t="inlineStr">
         <is>
-          <t>2026-02-19T09:38:44</t>
+          <t>2026-02-19T11:26:04</t>
         </is>
       </c>
       <c r="O188" t="inlineStr">
@@ -13301,7 +13301,7 @@
       </c>
       <c r="N190" t="inlineStr">
         <is>
-          <t>2026-02-19T09:29:11</t>
+          <t>2026-02-19T11:14:52</t>
         </is>
       </c>
       <c r="O190" t="inlineStr">
@@ -13433,7 +13433,7 @@
       </c>
       <c r="N192" t="inlineStr">
         <is>
-          <t>2026-02-19T09:40:57</t>
+          <t>2026-02-19T11:30:46</t>
         </is>
       </c>
       <c r="O192" t="inlineStr">
@@ -13562,7 +13562,7 @@
       </c>
       <c r="N194" t="inlineStr">
         <is>
-          <t>2026-02-19T09:36:01</t>
+          <t>2026-02-19T11:32:48</t>
         </is>
       </c>
       <c r="O194" t="inlineStr">
@@ -13628,7 +13628,7 @@
       </c>
       <c r="N195" t="inlineStr">
         <is>
-          <t>2026-02-19T09:26:20</t>
+          <t>2026-02-19T11:20:34</t>
         </is>
       </c>
       <c r="O195" t="inlineStr">
@@ -13694,7 +13694,7 @@
       </c>
       <c r="N196" t="inlineStr">
         <is>
-          <t>2026-02-19T09:04:56</t>
+          <t>2026-02-19T10:50:52</t>
         </is>
       </c>
       <c r="O196" t="inlineStr">
@@ -13760,7 +13760,7 @@
       </c>
       <c r="N197" t="inlineStr">
         <is>
-          <t>2026-02-19T09:10:08</t>
+          <t>2026-02-19T11:19:46</t>
         </is>
       </c>
       <c r="O197" t="inlineStr">
@@ -13892,7 +13892,7 @@
       </c>
       <c r="N199" t="inlineStr">
         <is>
-          <t>2026-02-19T09:11:07</t>
+          <t>2026-02-19T11:07:23</t>
         </is>
       </c>
       <c r="O199" t="inlineStr">
@@ -14021,7 +14021,7 @@
       </c>
       <c r="N201" t="inlineStr">
         <is>
-          <t>2026-02-19T09:02:55</t>
+          <t>2026-02-19T10:53:23</t>
         </is>
       </c>
       <c r="O201" t="inlineStr">
@@ -14087,7 +14087,7 @@
       </c>
       <c r="N202" t="inlineStr">
         <is>
-          <t>2026-02-19T09:08:22</t>
+          <t>2026-02-19T10:53:14</t>
         </is>
       </c>
       <c r="O202" t="inlineStr">
@@ -14153,7 +14153,7 @@
       </c>
       <c r="N203" t="inlineStr">
         <is>
-          <t>2026-02-19T09:03:56</t>
+          <t>2026-02-19T11:01:31</t>
         </is>
       </c>
       <c r="O203" t="inlineStr">
@@ -14219,7 +14219,7 @@
       </c>
       <c r="N204" t="inlineStr">
         <is>
-          <t>2026-02-19T09:04:07</t>
+          <t>2026-02-19T10:58:36</t>
         </is>
       </c>
       <c r="O204" t="inlineStr">
@@ -14285,7 +14285,7 @@
       </c>
       <c r="N205" t="inlineStr">
         <is>
-          <t>2026-02-19T08:44:17</t>
+          <t>2026-02-19T11:32:36</t>
         </is>
       </c>
       <c r="O205" t="inlineStr">
@@ -14351,7 +14351,7 @@
       </c>
       <c r="N206" t="inlineStr">
         <is>
-          <t>2026-02-19T09:13:20</t>
+          <t>2026-02-19T11:07:58</t>
         </is>
       </c>
       <c r="O206" t="inlineStr">
@@ -14417,7 +14417,7 @@
       </c>
       <c r="N207" t="inlineStr">
         <is>
-          <t>2026-02-19T09:15:50</t>
+          <t>2026-02-19T11:12:59</t>
         </is>
       </c>
       <c r="O207" t="inlineStr">
@@ -14483,7 +14483,7 @@
       </c>
       <c r="N208" t="inlineStr">
         <is>
-          <t>2026-02-19T09:30:34</t>
+          <t>2026-02-19T11:18:35</t>
         </is>
       </c>
       <c r="O208" t="inlineStr">
@@ -14549,7 +14549,7 @@
       </c>
       <c r="N209" t="inlineStr">
         <is>
-          <t>2026-02-19T09:26:37</t>
+          <t>2026-02-19T11:13:43</t>
         </is>
       </c>
       <c r="O209" t="inlineStr">
@@ -14615,7 +14615,7 @@
       </c>
       <c r="N210" t="inlineStr">
         <is>
-          <t>2026-02-19T09:28:19</t>
+          <t>2026-02-19T11:22:20</t>
         </is>
       </c>
       <c r="O210" t="inlineStr">
@@ -14681,7 +14681,7 @@
       </c>
       <c r="N211" t="inlineStr">
         <is>
-          <t>2026-02-19T09:37:45</t>
+          <t>2026-02-19T11:25:57</t>
         </is>
       </c>
       <c r="O211" t="inlineStr">
@@ -14747,7 +14747,7 @@
       </c>
       <c r="N212" t="inlineStr">
         <is>
-          <t>2026-02-19T09:27:28</t>
+          <t>2026-02-19T11:21:35</t>
         </is>
       </c>
       <c r="O212" t="inlineStr">
@@ -14813,7 +14813,7 @@
       </c>
       <c r="N213" t="inlineStr">
         <is>
-          <t>2026-02-19T09:26:31</t>
+          <t>2026-02-19T11:24:18</t>
         </is>
       </c>
       <c r="O213" t="inlineStr">
@@ -14945,7 +14945,7 @@
       </c>
       <c r="N215" t="inlineStr">
         <is>
-          <t>2026-02-19T09:32:43</t>
+          <t>2026-02-19T11:20:27</t>
         </is>
       </c>
       <c r="O215" t="inlineStr">
@@ -15011,7 +15011,7 @@
       </c>
       <c r="N216" t="inlineStr">
         <is>
-          <t>2026-02-19T09:38:14</t>
+          <t>2026-02-19T11:32:42</t>
         </is>
       </c>
       <c r="O216" t="inlineStr">
@@ -15077,7 +15077,7 @@
       </c>
       <c r="N217" t="inlineStr">
         <is>
-          <t>2026-02-19T09:35:12</t>
+          <t>2026-02-19T11:22:18</t>
         </is>
       </c>
       <c r="O217" t="inlineStr">
@@ -15209,7 +15209,7 @@
       </c>
       <c r="N219" t="inlineStr">
         <is>
-          <t>2026-02-19T09:01:09</t>
+          <t>2026-02-19T10:56:11</t>
         </is>
       </c>
       <c r="O219" t="inlineStr">
@@ -15280,7 +15280,7 @@
       </c>
       <c r="N220" t="inlineStr">
         <is>
-          <t>2026-02-19T09:40:37</t>
+          <t>2026-02-19T11:36:16</t>
         </is>
       </c>
       <c r="O220" t="inlineStr">
@@ -15346,7 +15346,7 @@
       </c>
       <c r="N221" t="inlineStr">
         <is>
-          <t>2026-02-19T09:03:58</t>
+          <t>2026-02-19T10:54:05</t>
         </is>
       </c>
       <c r="O221" t="inlineStr">
@@ -15478,7 +15478,7 @@
       </c>
       <c r="N223" t="inlineStr">
         <is>
-          <t>2026-02-19T09:10:31</t>
+          <t>2026-02-19T10:56:55</t>
         </is>
       </c>
       <c r="O223" t="inlineStr">
@@ -15610,7 +15610,7 @@
       </c>
       <c r="N225" t="inlineStr">
         <is>
-          <t>2026-02-19T09:31:17</t>
+          <t>2026-02-19T11:27:26</t>
         </is>
       </c>
       <c r="O225" t="inlineStr">
@@ -15676,7 +15676,7 @@
       </c>
       <c r="N226" t="inlineStr">
         <is>
-          <t>2026-02-19T09:34:36</t>
+          <t>2026-02-19T11:25:10</t>
         </is>
       </c>
       <c r="O226" t="inlineStr">
@@ -15742,7 +15742,7 @@
       </c>
       <c r="N227" t="inlineStr">
         <is>
-          <t>2026-02-19T09:02:27</t>
+          <t>2026-02-19T10:54:35</t>
         </is>
       </c>
       <c r="O227" t="inlineStr">
@@ -15808,7 +15808,7 @@
       </c>
       <c r="N228" t="inlineStr">
         <is>
-          <t>2026-02-19T08:50:11</t>
+          <t>2026-02-19T11:36:00</t>
         </is>
       </c>
       <c r="O228" t="inlineStr">
@@ -15874,7 +15874,7 @@
       </c>
       <c r="N229" t="inlineStr">
         <is>
-          <t>2026-02-19T09:14:33</t>
+          <t>2026-02-19T11:08:39</t>
         </is>
       </c>
       <c r="O229" t="inlineStr">
@@ -15940,7 +15940,7 @@
       </c>
       <c r="N230" t="inlineStr">
         <is>
-          <t>2026-02-19T09:01:00</t>
+          <t>2026-02-19T10:56:08</t>
         </is>
       </c>
       <c r="O230" t="inlineStr">
@@ -16006,7 +16006,7 @@
       </c>
       <c r="N231" t="inlineStr">
         <is>
-          <t>2026-02-19T08:57:57</t>
+          <t>2026-02-19T10:48:43</t>
         </is>
       </c>
       <c r="O231" t="inlineStr">
@@ -16072,7 +16072,7 @@
       </c>
       <c r="N232" t="inlineStr">
         <is>
-          <t>2026-02-19T08:45:57</t>
+          <t>2026-02-19T11:33:11</t>
         </is>
       </c>
       <c r="O232" t="inlineStr">
@@ -16138,7 +16138,7 @@
       </c>
       <c r="N233" t="inlineStr">
         <is>
-          <t>2026-02-19T09:03:08</t>
+          <t>2026-02-19T10:54:40</t>
         </is>
       </c>
       <c r="O233" t="inlineStr">
@@ -16204,7 +16204,7 @@
       </c>
       <c r="N234" t="inlineStr">
         <is>
-          <t>2026-02-19T09:11:06</t>
+          <t>2026-02-19T11:07:03</t>
         </is>
       </c>
       <c r="O234" t="inlineStr">
@@ -16468,7 +16468,7 @@
       </c>
       <c r="N238" t="inlineStr">
         <is>
-          <t>2026-02-19T09:35:24</t>
+          <t>2026-02-19T11:29:53</t>
         </is>
       </c>
       <c r="O238" t="inlineStr">
@@ -16534,7 +16534,7 @@
       </c>
       <c r="N239" t="inlineStr">
         <is>
-          <t>2026-02-19T09:40:45</t>
+          <t>2026-02-19T11:30:19</t>
         </is>
       </c>
       <c r="O239" t="inlineStr">
@@ -16600,7 +16600,7 @@
       </c>
       <c r="N240" t="inlineStr">
         <is>
-          <t>2026-02-19T08:54:35</t>
+          <t>2026-02-19T10:50:06</t>
         </is>
       </c>
       <c r="O240" t="inlineStr">
@@ -16666,7 +16666,7 @@
       </c>
       <c r="N241" t="inlineStr">
         <is>
-          <t>2026-02-19T09:00:20</t>
+          <t>2026-02-19T11:39:52</t>
         </is>
       </c>
       <c r="O241" t="inlineStr">
@@ -16732,7 +16732,7 @@
       </c>
       <c r="N242" t="inlineStr">
         <is>
-          <t>2026-02-19T09:01:53</t>
+          <t>2026-02-19T10:51:01</t>
         </is>
       </c>
       <c r="O242" t="inlineStr">
@@ -16798,7 +16798,7 @@
       </c>
       <c r="N243" t="inlineStr">
         <is>
-          <t>2026-02-19T09:36:37</t>
+          <t>2026-02-19T11:21:12</t>
         </is>
       </c>
       <c r="O243" t="inlineStr">
@@ -16925,7 +16925,7 @@
       </c>
       <c r="N245" t="inlineStr">
         <is>
-          <t>2026-02-19T09:36:49</t>
+          <t>2026-02-19T11:30:24</t>
         </is>
       </c>
       <c r="O245" t="inlineStr">
@@ -16991,7 +16991,7 @@
       </c>
       <c r="N246" t="inlineStr">
         <is>
-          <t>2026-02-19T09:13:40</t>
+          <t>2026-02-19T11:06:05</t>
         </is>
       </c>
       <c r="O246" t="inlineStr">
@@ -17057,7 +17057,7 @@
       </c>
       <c r="N247" t="inlineStr">
         <is>
-          <t>2026-02-19T08:46:03</t>
+          <t>2026-02-19T11:30:21</t>
         </is>
       </c>
       <c r="O247" t="inlineStr">
@@ -17123,7 +17123,7 @@
       </c>
       <c r="N248" t="inlineStr">
         <is>
-          <t>2026-02-19T08:46:47</t>
+          <t>2026-02-19T10:47:17</t>
         </is>
       </c>
       <c r="O248" t="inlineStr">
@@ -17189,7 +17189,7 @@
       </c>
       <c r="N249" t="inlineStr">
         <is>
-          <t>2026-02-19T09:33:55</t>
+          <t>2026-02-19T11:23:49</t>
         </is>
       </c>
       <c r="O249" t="inlineStr">
@@ -17209,6 +17209,11 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>10.69.5.118</t>
+        </is>
+      </c>
       <c r="D250" t="n">
         <v>2017</v>
       </c>
@@ -17250,7 +17255,7 @@
       </c>
       <c r="N250" t="inlineStr">
         <is>
-          <t>2026-02-19T08:48:06</t>
+          <t>2026-02-19T11:30:09</t>
         </is>
       </c>
       <c r="O250" t="inlineStr">
@@ -17316,7 +17321,7 @@
       </c>
       <c r="N251" t="inlineStr">
         <is>
-          <t>2026-02-19T09:35:54</t>
+          <t>2026-02-19T11:30:15</t>
         </is>
       </c>
       <c r="O251" t="inlineStr">
@@ -17382,7 +17387,7 @@
       </c>
       <c r="N252" t="inlineStr">
         <is>
-          <t>2026-02-19T09:38:10</t>
+          <t>2026-02-19T11:33:54</t>
         </is>
       </c>
       <c r="O252" t="inlineStr">
@@ -17448,7 +17453,7 @@
       </c>
       <c r="N253" t="inlineStr">
         <is>
-          <t>2026-02-19T08:47:25</t>
+          <t>2026-02-19T11:35:42</t>
         </is>
       </c>
       <c r="O253" t="inlineStr">
@@ -17508,7 +17513,7 @@
       </c>
       <c r="N254" t="inlineStr">
         <is>
-          <t>2026-02-19T09:24:12</t>
+          <t>2026-02-19T11:14:13</t>
         </is>
       </c>
       <c r="O254" t="inlineStr">
@@ -17574,7 +17579,7 @@
       </c>
       <c r="N255" t="inlineStr">
         <is>
-          <t>2026-02-19T08:46:21</t>
+          <t>2026-02-19T11:36:45</t>
         </is>
       </c>
       <c r="O255" t="inlineStr">
@@ -17640,7 +17645,7 @@
       </c>
       <c r="N256" t="inlineStr">
         <is>
-          <t>2026-02-19T08:49:01</t>
+          <t>2026-02-19T10:44:16</t>
         </is>
       </c>
       <c r="O256" t="inlineStr">
@@ -17706,7 +17711,7 @@
       </c>
       <c r="N257" t="inlineStr">
         <is>
-          <t>2026-02-19T09:27:54</t>
+          <t>2026-02-19T11:14:02</t>
         </is>
       </c>
       <c r="O257" t="inlineStr">
@@ -17772,7 +17777,7 @@
       </c>
       <c r="N258" t="inlineStr">
         <is>
-          <t>2026-02-19T09:00:22</t>
+          <t>2026-02-19T10:51:47</t>
         </is>
       </c>
       <c r="O258" t="inlineStr">
@@ -17838,7 +17843,7 @@
       </c>
       <c r="N259" t="inlineStr">
         <is>
-          <t>2026-02-19T09:13:07</t>
+          <t>2026-02-19T11:06:23</t>
         </is>
       </c>
       <c r="O259" t="inlineStr">
@@ -17904,7 +17909,7 @@
       </c>
       <c r="N260" t="inlineStr">
         <is>
-          <t>2026-02-19T09:23:16</t>
+          <t>2026-02-19T11:14:08</t>
         </is>
       </c>
       <c r="O260" t="inlineStr">
@@ -17970,7 +17975,7 @@
       </c>
       <c r="N261" t="inlineStr">
         <is>
-          <t>2026-02-19T08:54:09</t>
+          <t>2026-02-19T11:37:19</t>
         </is>
       </c>
       <c r="O261" t="inlineStr">
@@ -18036,7 +18041,7 @@
       </c>
       <c r="N262" t="inlineStr">
         <is>
-          <t>2026-02-19T09:34:27</t>
+          <t>2026-02-19T11:26:58</t>
         </is>
       </c>
       <c r="O262" t="inlineStr">
@@ -18102,7 +18107,7 @@
       </c>
       <c r="N263" t="inlineStr">
         <is>
-          <t>2026-02-19T09:02:33</t>
+          <t>2026-02-19T11:38:30</t>
         </is>
       </c>
       <c r="O263" t="inlineStr">
@@ -18168,7 +18173,7 @@
       </c>
       <c r="N264" t="inlineStr">
         <is>
-          <t>2026-02-19T09:32:52</t>
+          <t>2026-02-19T11:22:34</t>
         </is>
       </c>
       <c r="O264" t="inlineStr">
@@ -18234,7 +18239,7 @@
       </c>
       <c r="N265" t="inlineStr">
         <is>
-          <t>2026-02-19T09:36:57</t>
+          <t>2026-02-19T11:22:55</t>
         </is>
       </c>
       <c r="O265" t="inlineStr">
@@ -18300,7 +18305,7 @@
       </c>
       <c r="N266" t="inlineStr">
         <is>
-          <t>2026-02-19T09:25:26</t>
+          <t>2026-02-19T11:17:48</t>
         </is>
       </c>
       <c r="O266" t="inlineStr">
@@ -18366,7 +18371,7 @@
       </c>
       <c r="N267" t="inlineStr">
         <is>
-          <t>2026-02-19T08:59:44</t>
+          <t>2026-02-19T10:56:31</t>
         </is>
       </c>
       <c r="O267" t="inlineStr">
@@ -18432,7 +18437,7 @@
       </c>
       <c r="N268" t="inlineStr">
         <is>
-          <t>2026-02-19T09:08:20</t>
+          <t>2026-02-19T11:04:28</t>
         </is>
       </c>
       <c r="O268" t="inlineStr">
@@ -18498,7 +18503,7 @@
       </c>
       <c r="N269" t="inlineStr">
         <is>
-          <t>2026-02-18T19:12:27</t>
+          <t>2026-02-19T11:07:49</t>
         </is>
       </c>
       <c r="O269" t="inlineStr">
@@ -18561,7 +18566,7 @@
       </c>
       <c r="N270" t="inlineStr">
         <is>
-          <t>2026-02-19T09:39:54</t>
+          <t>2026-02-19T11:26:37</t>
         </is>
       </c>
       <c r="O270" t="inlineStr">
@@ -18693,7 +18698,7 @@
       </c>
       <c r="N272" t="inlineStr">
         <is>
-          <t>2026-02-19T08:56:31</t>
+          <t>2026-02-19T11:37:55</t>
         </is>
       </c>
       <c r="O272" t="inlineStr">
@@ -18759,7 +18764,7 @@
       </c>
       <c r="N273" t="inlineStr">
         <is>
-          <t>2026-02-19T09:05:46</t>
+          <t>2026-02-19T11:26:00</t>
         </is>
       </c>
       <c r="O273" t="inlineStr">
@@ -19089,7 +19094,7 @@
       </c>
       <c r="N278" t="inlineStr">
         <is>
-          <t>2026-02-19T09:15:43</t>
+          <t>2026-02-19T11:41:15</t>
         </is>
       </c>
       <c r="O278" t="inlineStr">
@@ -19155,7 +19160,7 @@
       </c>
       <c r="N279" t="inlineStr">
         <is>
-          <t>2026-02-19T09:20:29</t>
+          <t>2026-02-19T11:05:30</t>
         </is>
       </c>
       <c r="O279" t="inlineStr">
@@ -19221,7 +19226,7 @@
       </c>
       <c r="N280" t="inlineStr">
         <is>
-          <t>2026-02-19T09:03:40</t>
+          <t>2026-02-19T10:58:47</t>
         </is>
       </c>
       <c r="O280" t="inlineStr">
@@ -19287,7 +19292,7 @@
       </c>
       <c r="N281" t="inlineStr">
         <is>
-          <t>2026-02-19T09:25:00</t>
+          <t>2026-02-19T11:10:21</t>
         </is>
       </c>
       <c r="O281" t="inlineStr">
@@ -19307,11 +19312,6 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
-      <c r="C282" t="inlineStr">
-        <is>
-          <t>10.69.5.151</t>
-        </is>
-      </c>
       <c r="D282" t="n">
         <v>2017</v>
       </c>
@@ -19353,7 +19353,7 @@
       </c>
       <c r="N282" t="inlineStr">
         <is>
-          <t>2026-02-19T09:31:54</t>
+          <t>2026-02-19T11:19:04</t>
         </is>
       </c>
       <c r="O282" t="inlineStr">
@@ -19419,7 +19419,7 @@
       </c>
       <c r="N283" t="inlineStr">
         <is>
-          <t>2026-02-19T09:16:09</t>
+          <t>2026-02-19T11:08:47</t>
         </is>
       </c>
       <c r="O283" t="inlineStr">
@@ -19485,7 +19485,7 @@
       </c>
       <c r="N284" t="inlineStr">
         <is>
-          <t>2026-02-19T08:58:02</t>
+          <t>2026-02-19T10:54:08</t>
         </is>
       </c>
       <c r="O284" t="inlineStr">
@@ -19551,7 +19551,7 @@
       </c>
       <c r="N285" t="inlineStr">
         <is>
-          <t>2026-02-19T09:32:44</t>
+          <t>2026-02-19T11:24:10</t>
         </is>
       </c>
       <c r="O285" t="inlineStr">
@@ -19683,7 +19683,7 @@
       </c>
       <c r="N287" t="inlineStr">
         <is>
-          <t>2026-02-19T08:56:53</t>
+          <t>2026-02-19T10:50:05</t>
         </is>
       </c>
       <c r="O287" t="inlineStr">
@@ -19749,7 +19749,7 @@
       </c>
       <c r="N288" t="inlineStr">
         <is>
-          <t>2026-02-19T09:28:49</t>
+          <t>2026-02-19T11:17:18</t>
         </is>
       </c>
       <c r="O288" t="inlineStr">
@@ -19815,7 +19815,7 @@
       </c>
       <c r="N289" t="inlineStr">
         <is>
-          <t>2026-02-18T20:44:20</t>
+          <t>2026-02-19T11:03:51</t>
         </is>
       </c>
       <c r="O289" t="inlineStr">
@@ -20635,7 +20635,7 @@
       </c>
       <c r="N302" t="inlineStr">
         <is>
-          <t>2026-02-19T09:26:30</t>
+          <t>2026-02-19T11:26:10</t>
         </is>
       </c>
       <c r="O302" t="inlineStr">
@@ -21787,7 +21787,7 @@
       </c>
       <c r="N320" t="inlineStr">
         <is>
-          <t>2026-02-19T09:16:22</t>
+          <t>2026-02-19T11:10:14</t>
         </is>
       </c>
       <c r="O320" t="inlineStr">
@@ -22536,7 +22536,7 @@
       </c>
       <c r="N332" t="inlineStr">
         <is>
-          <t>2026-02-19T09:03:06</t>
+          <t>2026-02-19T10:48:25</t>
         </is>
       </c>
       <c r="O332" t="inlineStr">
@@ -22602,7 +22602,7 @@
       </c>
       <c r="N333" t="inlineStr">
         <is>
-          <t>2026-02-19T09:34:14</t>
+          <t>2026-02-19T11:25:42</t>
         </is>
       </c>
       <c r="O333" t="inlineStr">
@@ -22668,7 +22668,7 @@
       </c>
       <c r="N334" t="inlineStr">
         <is>
-          <t>2026-02-19T09:31:42</t>
+          <t>2026-02-19T11:19:31</t>
         </is>
       </c>
       <c r="O334" t="inlineStr">
@@ -22734,7 +22734,7 @@
       </c>
       <c r="N335" t="inlineStr">
         <is>
-          <t>2026-02-19T09:33:21</t>
+          <t>2026-02-19T11:16:35</t>
         </is>
       </c>
       <c r="O335" t="inlineStr">
@@ -22800,7 +22800,7 @@
       </c>
       <c r="N336" t="inlineStr">
         <is>
-          <t>2026-02-19T09:40:14</t>
+          <t>2026-02-19T11:34:08</t>
         </is>
       </c>
       <c r="O336" t="inlineStr">
@@ -22866,7 +22866,7 @@
       </c>
       <c r="N337" t="inlineStr">
         <is>
-          <t>2026-02-19T09:35:07</t>
+          <t>2026-02-19T11:33:00</t>
         </is>
       </c>
       <c r="O337" t="inlineStr">
@@ -22932,7 +22932,7 @@
       </c>
       <c r="N338" t="inlineStr">
         <is>
-          <t>2026-02-19T09:12:56</t>
+          <t>2026-02-19T11:02:44</t>
         </is>
       </c>
       <c r="O338" t="inlineStr">
@@ -22998,7 +22998,7 @@
       </c>
       <c r="N339" t="inlineStr">
         <is>
-          <t>2026-02-19T09:39:30</t>
+          <t>2026-02-19T11:26:54</t>
         </is>
       </c>
       <c r="O339" t="inlineStr">
@@ -23130,7 +23130,7 @@
       </c>
       <c r="N341" t="inlineStr">
         <is>
-          <t>2026-02-19T08:58:09</t>
+          <t>2026-02-19T10:51:27</t>
         </is>
       </c>
       <c r="O341" t="inlineStr">
@@ -23196,7 +23196,7 @@
       </c>
       <c r="N342" t="inlineStr">
         <is>
-          <t>2026-02-19T09:31:39</t>
+          <t>2026-02-19T11:23:54</t>
         </is>
       </c>
       <c r="O342" t="inlineStr">
@@ -23259,7 +23259,7 @@
       </c>
       <c r="N343" t="inlineStr">
         <is>
-          <t>2026-02-19T09:20:26</t>
+          <t>2026-02-19T11:18:15</t>
         </is>
       </c>
       <c r="O343" t="inlineStr">
@@ -23523,7 +23523,7 @@
       </c>
       <c r="N347" t="inlineStr">
         <is>
-          <t>2026-02-19T08:45:39</t>
+          <t>2026-02-19T11:39:21</t>
         </is>
       </c>
       <c r="O347" t="inlineStr">
@@ -23589,7 +23589,7 @@
       </c>
       <c r="N348" t="inlineStr">
         <is>
-          <t>2026-02-19T08:45:46</t>
+          <t>2026-02-19T09:42:14</t>
         </is>
       </c>
       <c r="O348" t="inlineStr">
@@ -23782,7 +23782,7 @@
       </c>
       <c r="N351" t="inlineStr">
         <is>
-          <t>2026-02-19T08:46:21</t>
+          <t>2026-02-19T09:45:14</t>
         </is>
       </c>
       <c r="O351" t="inlineStr">
@@ -23848,7 +23848,7 @@
       </c>
       <c r="N352" t="inlineStr">
         <is>
-          <t>2026-02-19T08:54:24</t>
+          <t>2026-02-19T09:48:02</t>
         </is>
       </c>
       <c r="O352" t="inlineStr">
@@ -23974,7 +23974,7 @@
       </c>
       <c r="N354" t="inlineStr">
         <is>
-          <t>2026-02-19T08:45:32</t>
+          <t>2026-02-19T11:40:26</t>
         </is>
       </c>
       <c r="O354" t="inlineStr">
@@ -24040,7 +24040,7 @@
       </c>
       <c r="N355" t="inlineStr">
         <is>
-          <t>2026-02-19T09:37:02</t>
+          <t>2026-02-19T11:28:19</t>
         </is>
       </c>
       <c r="O355" t="inlineStr">
@@ -24106,7 +24106,7 @@
       </c>
       <c r="N356" t="inlineStr">
         <is>
-          <t>2026-02-19T09:40:47</t>
+          <t>2026-02-19T11:33:15</t>
         </is>
       </c>
       <c r="O356" t="inlineStr">
@@ -24172,7 +24172,7 @@
       </c>
       <c r="N357" t="inlineStr">
         <is>
-          <t>2026-02-19T08:44:53</t>
+          <t>2026-02-19T11:39:43</t>
         </is>
       </c>
       <c r="O357" t="inlineStr">
@@ -24233,7 +24233,7 @@
       </c>
       <c r="N358" t="inlineStr">
         <is>
-          <t>2026-02-19T08:48:37</t>
+          <t>2026-02-19T09:46:11</t>
         </is>
       </c>
       <c r="O358" t="inlineStr">
@@ -24299,7 +24299,7 @@
       </c>
       <c r="N359" t="inlineStr">
         <is>
-          <t>2026-02-19T09:37:14</t>
+          <t>2026-02-19T11:28:48</t>
         </is>
       </c>
       <c r="O359" t="inlineStr">
@@ -24365,7 +24365,7 @@
       </c>
       <c r="N360" t="inlineStr">
         <is>
-          <t>2026-02-19T08:46:41</t>
+          <t>2026-02-19T11:41:39</t>
         </is>
       </c>
       <c r="O360" t="inlineStr">
@@ -24431,7 +24431,7 @@
       </c>
       <c r="N361" t="inlineStr">
         <is>
-          <t>2026-02-19T08:45:27</t>
+          <t>2026-02-19T10:53:27</t>
         </is>
       </c>
       <c r="O361" t="inlineStr">
@@ -24494,7 +24494,7 @@
       </c>
       <c r="N362" t="inlineStr">
         <is>
-          <t>2026-02-19T09:26:52</t>
+          <t>2026-02-19T11:11:46</t>
         </is>
       </c>
       <c r="O362" t="inlineStr">
@@ -24688,7 +24688,7 @@
       </c>
       <c r="N365" t="inlineStr">
         <is>
-          <t>2026-02-19T08:53:56</t>
+          <t>2026-02-19T11:42:17</t>
         </is>
       </c>
       <c r="O365" t="inlineStr">
@@ -24756,7 +24756,7 @@
       </c>
       <c r="N366" t="inlineStr">
         <is>
-          <t>2026-02-19T08:52:38</t>
+          <t>2026-02-19T11:38:41</t>
         </is>
       </c>
       <c r="O366" t="inlineStr">
@@ -24886,7 +24886,7 @@
       </c>
       <c r="N368" t="inlineStr">
         <is>
-          <t>2026-02-19T08:59:30</t>
+          <t>2026-02-19T10:52:16</t>
         </is>
       </c>
       <c r="O368" t="inlineStr">
@@ -24949,7 +24949,7 @@
       </c>
       <c r="N369" t="inlineStr">
         <is>
-          <t>2026-02-19T09:00:50</t>
+          <t>2026-02-19T10:48:26</t>
         </is>
       </c>
       <c r="O369" t="inlineStr">
@@ -25020,7 +25020,7 @@
       </c>
       <c r="N370" t="inlineStr">
         <is>
-          <t>2026-02-19T09:38:08</t>
+          <t>2026-02-19T11:33:04</t>
         </is>
       </c>
       <c r="O370" t="inlineStr">
@@ -25091,7 +25091,7 @@
       </c>
       <c r="N371" t="inlineStr">
         <is>
-          <t>2026-02-13T14:00:43</t>
+          <t>2026-02-19T11:11:53</t>
         </is>
       </c>
       <c r="O371" t="inlineStr">
@@ -25233,7 +25233,7 @@
       </c>
       <c r="N373" t="inlineStr">
         <is>
-          <t>2026-02-19T09:26:51</t>
+          <t>2026-02-19T10:20:32</t>
         </is>
       </c>
       <c r="O373" t="inlineStr">
@@ -25304,7 +25304,7 @@
       </c>
       <c r="N374" t="inlineStr">
         <is>
-          <t>2026-02-19T09:02:59</t>
+          <t>2026-02-19T11:00:02</t>
         </is>
       </c>
       <c r="O374" t="inlineStr">
@@ -25372,7 +25372,7 @@
       </c>
       <c r="N375" t="inlineStr">
         <is>
-          <t>2026-02-19T08:53:24</t>
+          <t>2026-02-19T11:35:38</t>
         </is>
       </c>
       <c r="O375" t="inlineStr">
@@ -25438,7 +25438,7 @@
       </c>
       <c r="N376" t="inlineStr">
         <is>
-          <t>2026-02-16T20:21:03</t>
+          <t>2026-02-19T11:10:47</t>
         </is>
       </c>
       <c r="O376" t="inlineStr">
@@ -25509,7 +25509,7 @@
       </c>
       <c r="N377" t="inlineStr">
         <is>
-          <t>2026-02-19T08:47:57</t>
+          <t>2026-02-19T11:34:55</t>
         </is>
       </c>
       <c r="O377" t="inlineStr">
@@ -25580,7 +25580,7 @@
       </c>
       <c r="N378" t="inlineStr">
         <is>
-          <t>2026-02-19T08:55:00</t>
+          <t>2026-02-19T11:40:48</t>
         </is>
       </c>
       <c r="O378" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática 2026-02-19 13:52:03.292233
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -601,7 +601,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>2026-02-19T11:42:02</t>
+          <t>2026-02-19T13:26:04</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -672,7 +672,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>2026-02-19T11:07:11</t>
+          <t>2026-02-19T12:58:58</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -743,7 +743,7 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>2026-02-19T11:14:10</t>
+          <t>2026-02-19T12:59:54</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
@@ -814,7 +814,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>2026-02-19T11:38:57</t>
+          <t>2026-02-19T13:29:25</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -1144,7 +1144,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>2026-02-19T11:11:35</t>
+          <t>2026-02-19T13:06:40</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -1474,7 +1474,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>2026-02-19T11:05:10</t>
+          <t>2026-02-19T13:02:45</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
@@ -1606,7 +1606,7 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>2026-02-19T11:25:46</t>
+          <t>2026-02-19T13:17:40</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>2026-02-19T11:29:08</t>
+          <t>2026-02-19T13:13:28</t>
         </is>
       </c>
       <c r="O28" t="inlineStr">
@@ -6885,7 +6885,7 @@
       </c>
       <c r="N95" t="inlineStr">
         <is>
-          <t>2026-02-19T11:40:22</t>
+          <t>2026-02-19T13:29:43</t>
         </is>
       </c>
       <c r="O95" t="inlineStr">
@@ -6956,7 +6956,7 @@
       </c>
       <c r="N96" t="inlineStr">
         <is>
-          <t>2026-02-18T19:26:26</t>
+          <t>2026-02-19T13:31:03</t>
         </is>
       </c>
       <c r="O96" t="inlineStr">
@@ -7022,7 +7022,7 @@
       </c>
       <c r="N97" t="inlineStr">
         <is>
-          <t>2026-02-19T11:25:36</t>
+          <t>2026-02-19T13:14:50</t>
         </is>
       </c>
       <c r="O97" t="inlineStr">
@@ -7042,6 +7042,11 @@
           <t>COORDENACAO</t>
         </is>
       </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>10.69.3.94</t>
+        </is>
+      </c>
       <c r="D98" t="n">
         <v>2025</v>
       </c>
@@ -7088,7 +7093,7 @@
       </c>
       <c r="N98" t="inlineStr">
         <is>
-          <t>2026-02-19T10:57:40</t>
+          <t>2026-02-19T13:42:04</t>
         </is>
       </c>
       <c r="O98" t="inlineStr">
@@ -7159,7 +7164,7 @@
       </c>
       <c r="N99" t="inlineStr">
         <is>
-          <t>2026-02-19T11:38:59</t>
+          <t>2026-02-19T13:28:27</t>
         </is>
       </c>
       <c r="O99" t="inlineStr">
@@ -7230,7 +7235,7 @@
       </c>
       <c r="N100" t="inlineStr">
         <is>
-          <t>2026-02-19T11:20:07</t>
+          <t>2026-02-19T13:11:36</t>
         </is>
       </c>
       <c r="O100" t="inlineStr">
@@ -7301,7 +7306,7 @@
       </c>
       <c r="N101" t="inlineStr">
         <is>
-          <t>2026-02-19T10:56:52</t>
+          <t>2026-02-19T12:53:30</t>
         </is>
       </c>
       <c r="O101" t="inlineStr">
@@ -7443,7 +7448,7 @@
       </c>
       <c r="N103" t="inlineStr">
         <is>
-          <t>2026-02-19T10:56:24</t>
+          <t>2026-02-19T12:49:25</t>
         </is>
       </c>
       <c r="O103" t="inlineStr">
@@ -7708,7 +7713,7 @@
       </c>
       <c r="N107" t="inlineStr">
         <is>
-          <t>2026-02-19T11:05:18</t>
+          <t>2026-02-19T12:51:46</t>
         </is>
       </c>
       <c r="O107" t="inlineStr">
@@ -7850,7 +7855,7 @@
       </c>
       <c r="N109" t="inlineStr">
         <is>
-          <t>2026-02-19T11:12:12</t>
+          <t>2026-02-19T13:01:00</t>
         </is>
       </c>
       <c r="O109" t="inlineStr">
@@ -7921,7 +7926,7 @@
       </c>
       <c r="N110" t="inlineStr">
         <is>
-          <t>2026-02-19T11:28:33</t>
+          <t>2026-02-19T13:29:01</t>
         </is>
       </c>
       <c r="O110" t="inlineStr">
@@ -7992,7 +7997,7 @@
       </c>
       <c r="N111" t="inlineStr">
         <is>
-          <t>2026-02-19T11:40:05</t>
+          <t>2026-02-19T13:24:43</t>
         </is>
       </c>
       <c r="O111" t="inlineStr">
@@ -8063,7 +8068,7 @@
       </c>
       <c r="N112" t="inlineStr">
         <is>
-          <t>2026-02-19T11:10:01</t>
+          <t>2026-02-19T13:04:53</t>
         </is>
       </c>
       <c r="O112" t="inlineStr">
@@ -8134,7 +8139,7 @@
       </c>
       <c r="N113" t="inlineStr">
         <is>
-          <t>2026-02-19T10:57:43</t>
+          <t>2026-02-19T12:50:32</t>
         </is>
       </c>
       <c r="O113" t="inlineStr">
@@ -8205,7 +8210,7 @@
       </c>
       <c r="N114" t="inlineStr">
         <is>
-          <t>2026-02-19T11:12:39</t>
+          <t>2026-02-19T12:57:08</t>
         </is>
       </c>
       <c r="O114" t="inlineStr">
@@ -8273,7 +8278,7 @@
       </c>
       <c r="N115" t="inlineStr">
         <is>
-          <t>2026-02-19T11:08:28</t>
+          <t>2026-02-19T12:55:35</t>
         </is>
       </c>
       <c r="O115" t="inlineStr">
@@ -8344,7 +8349,7 @@
       </c>
       <c r="N116" t="inlineStr">
         <is>
-          <t>2026-02-19T11:10:02</t>
+          <t>2026-02-19T13:07:09</t>
         </is>
       </c>
       <c r="O116" t="inlineStr">
@@ -8364,11 +8369,6 @@
           <t>DP</t>
         </is>
       </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>10.69.3.23</t>
-        </is>
-      </c>
       <c r="D117" t="n">
         <v>2025</v>
       </c>
@@ -8415,7 +8415,7 @@
       </c>
       <c r="N117" t="inlineStr">
         <is>
-          <t>2026-02-19T11:30:45</t>
+          <t>2026-02-19T13:18:09</t>
         </is>
       </c>
       <c r="O117" t="inlineStr">
@@ -8625,7 +8625,7 @@
       </c>
       <c r="N120" t="inlineStr">
         <is>
-          <t>2026-02-19T10:59:49</t>
+          <t>2026-02-19T12:56:25</t>
         </is>
       </c>
       <c r="O120" t="inlineStr">
@@ -8696,7 +8696,7 @@
       </c>
       <c r="N121" t="inlineStr">
         <is>
-          <t>2026-02-19T11:34:47</t>
+          <t>2026-02-19T12:29:28</t>
         </is>
       </c>
       <c r="O121" t="inlineStr">
@@ -8764,7 +8764,7 @@
       </c>
       <c r="N122" t="inlineStr">
         <is>
-          <t>2026-02-19T11:16:48</t>
+          <t>2026-02-19T13:12:24</t>
         </is>
       </c>
       <c r="O122" t="inlineStr">
@@ -8835,7 +8835,7 @@
       </c>
       <c r="N123" t="inlineStr">
         <is>
-          <t>2026-02-19T10:49:27</t>
+          <t>2026-02-19T13:29:41</t>
         </is>
       </c>
       <c r="O123" t="inlineStr">
@@ -8906,7 +8906,7 @@
       </c>
       <c r="N124" t="inlineStr">
         <is>
-          <t>2026-02-19T11:18:20</t>
+          <t>2026-02-19T13:07:19</t>
         </is>
       </c>
       <c r="O124" t="inlineStr">
@@ -8977,7 +8977,7 @@
       </c>
       <c r="N125" t="inlineStr">
         <is>
-          <t>2026-02-19T10:58:40</t>
+          <t>2026-02-19T12:55:54</t>
         </is>
       </c>
       <c r="O125" t="inlineStr">
@@ -9048,7 +9048,7 @@
       </c>
       <c r="N126" t="inlineStr">
         <is>
-          <t>2026-02-19T10:54:18</t>
+          <t>2026-02-19T12:50:08</t>
         </is>
       </c>
       <c r="O126" t="inlineStr">
@@ -9119,7 +9119,7 @@
       </c>
       <c r="N127" t="inlineStr">
         <is>
-          <t>2026-02-19T10:53:00</t>
+          <t>2026-02-19T13:32:56</t>
         </is>
       </c>
       <c r="O127" t="inlineStr">
@@ -9190,7 +9190,7 @@
       </c>
       <c r="N128" t="inlineStr">
         <is>
-          <t>2026-02-19T11:41:47</t>
+          <t>2026-02-19T13:29:39</t>
         </is>
       </c>
       <c r="O128" t="inlineStr">
@@ -9261,7 +9261,7 @@
       </c>
       <c r="N129" t="inlineStr">
         <is>
-          <t>2026-02-19T11:12:12</t>
+          <t>2026-02-19T13:05:46</t>
         </is>
       </c>
       <c r="O129" t="inlineStr">
@@ -9332,7 +9332,7 @@
       </c>
       <c r="N130" t="inlineStr">
         <is>
-          <t>2026-02-19T11:00:45</t>
+          <t>2026-02-19T12:54:11</t>
         </is>
       </c>
       <c r="O130" t="inlineStr">
@@ -9352,11 +9352,6 @@
           <t>ADM/FIN</t>
         </is>
       </c>
-      <c r="C131" t="inlineStr">
-        <is>
-          <t>10.69.3.6</t>
-        </is>
-      </c>
       <c r="D131" t="n">
         <v>2025</v>
       </c>
@@ -9403,7 +9398,7 @@
       </c>
       <c r="N131" t="inlineStr">
         <is>
-          <t>2026-02-19T11:35:12</t>
+          <t>2026-02-19T13:21:31</t>
         </is>
       </c>
       <c r="O131" t="inlineStr">
@@ -9540,7 +9535,7 @@
       </c>
       <c r="N133" t="inlineStr">
         <is>
-          <t>2026-02-19T10:47:19</t>
+          <t>2026-02-19T13:33:23</t>
         </is>
       </c>
       <c r="O133" t="inlineStr">
@@ -9672,7 +9667,7 @@
       </c>
       <c r="N135" t="inlineStr">
         <is>
-          <t>2026-02-19T10:52:11</t>
+          <t>2026-02-19T13:35:21</t>
         </is>
       </c>
       <c r="O135" t="inlineStr">
@@ -9869,7 +9864,7 @@
       </c>
       <c r="N138" t="inlineStr">
         <is>
-          <t>2026-02-19T10:44:58</t>
+          <t>2026-02-19T13:41:13</t>
         </is>
       </c>
       <c r="O138" t="inlineStr">
@@ -9935,7 +9930,7 @@
       </c>
       <c r="N139" t="inlineStr">
         <is>
-          <t>2026-02-19T11:39:23</t>
+          <t>2026-02-19T13:30:54</t>
         </is>
       </c>
       <c r="O139" t="inlineStr">
@@ -10001,7 +9996,7 @@
       </c>
       <c r="N140" t="inlineStr">
         <is>
-          <t>2026-02-19T10:52:52</t>
+          <t>2026-02-19T13:38:08</t>
         </is>
       </c>
       <c r="O140" t="inlineStr">
@@ -10133,7 +10128,7 @@
       </c>
       <c r="N142" t="inlineStr">
         <is>
-          <t>2026-02-19T11:11:01</t>
+          <t>2026-02-19T13:01:12</t>
         </is>
       </c>
       <c r="O142" t="inlineStr">
@@ -10199,7 +10194,7 @@
       </c>
       <c r="N143" t="inlineStr">
         <is>
-          <t>2026-02-19T11:21:02</t>
+          <t>2026-02-19T13:19:28</t>
         </is>
       </c>
       <c r="O143" t="inlineStr">
@@ -10265,7 +10260,7 @@
       </c>
       <c r="N144" t="inlineStr">
         <is>
-          <t>2026-02-19T11:13:16</t>
+          <t>2026-02-19T12:58:56</t>
         </is>
       </c>
       <c r="O144" t="inlineStr">
@@ -10331,7 +10326,7 @@
       </c>
       <c r="N145" t="inlineStr">
         <is>
-          <t>2026-02-19T11:22:44</t>
+          <t>2026-02-19T13:13:25</t>
         </is>
       </c>
       <c r="O145" t="inlineStr">
@@ -10397,7 +10392,7 @@
       </c>
       <c r="N146" t="inlineStr">
         <is>
-          <t>2026-02-19T11:22:30</t>
+          <t>2026-02-19T13:17:23</t>
         </is>
       </c>
       <c r="O146" t="inlineStr">
@@ -10463,7 +10458,7 @@
       </c>
       <c r="N147" t="inlineStr">
         <is>
-          <t>2026-02-19T11:14:54</t>
+          <t>2026-02-19T13:07:26</t>
         </is>
       </c>
       <c r="O147" t="inlineStr">
@@ -10529,7 +10524,7 @@
       </c>
       <c r="N148" t="inlineStr">
         <is>
-          <t>2026-02-19T11:13:43</t>
+          <t>2026-02-19T13:05:57</t>
         </is>
       </c>
       <c r="O148" t="inlineStr">
@@ -10595,7 +10590,7 @@
       </c>
       <c r="N149" t="inlineStr">
         <is>
-          <t>2026-02-19T11:11:37</t>
+          <t>2026-02-19T13:08:27</t>
         </is>
       </c>
       <c r="O149" t="inlineStr">
@@ -10661,7 +10656,7 @@
       </c>
       <c r="N150" t="inlineStr">
         <is>
-          <t>2026-02-19T11:14:47</t>
+          <t>2026-02-19T13:05:48</t>
         </is>
       </c>
       <c r="O150" t="inlineStr">
@@ -10727,7 +10722,7 @@
       </c>
       <c r="N151" t="inlineStr">
         <is>
-          <t>2026-02-19T11:05:46</t>
+          <t>2026-02-19T13:00:28</t>
         </is>
       </c>
       <c r="O151" t="inlineStr">
@@ -10793,7 +10788,7 @@
       </c>
       <c r="N152" t="inlineStr">
         <is>
-          <t>2026-02-19T11:09:51</t>
+          <t>2026-02-19T12:57:35</t>
         </is>
       </c>
       <c r="O152" t="inlineStr">
@@ -10920,7 +10915,7 @@
       </c>
       <c r="N154" t="inlineStr">
         <is>
-          <t>2026-02-19T11:20:49</t>
+          <t>2026-02-19T13:13:16</t>
         </is>
       </c>
       <c r="O154" t="inlineStr">
@@ -10986,7 +10981,7 @@
       </c>
       <c r="N155" t="inlineStr">
         <is>
-          <t>2026-02-19T10:56:48</t>
+          <t>2026-02-19T12:55:07</t>
         </is>
       </c>
       <c r="O155" t="inlineStr">
@@ -11052,7 +11047,7 @@
       </c>
       <c r="N156" t="inlineStr">
         <is>
-          <t>2026-02-19T11:41:31</t>
+          <t>2026-02-19T13:23:49</t>
         </is>
       </c>
       <c r="O156" t="inlineStr">
@@ -11118,7 +11113,7 @@
       </c>
       <c r="N157" t="inlineStr">
         <is>
-          <t>2026-02-19T11:03:32</t>
+          <t>2026-02-19T12:57:26</t>
         </is>
       </c>
       <c r="O157" t="inlineStr">
@@ -11184,7 +11179,7 @@
       </c>
       <c r="N158" t="inlineStr">
         <is>
-          <t>2026-02-19T10:00:02</t>
+          <t>2026-02-19T12:59:01</t>
         </is>
       </c>
       <c r="O158" t="inlineStr">
@@ -11250,7 +11245,7 @@
       </c>
       <c r="N159" t="inlineStr">
         <is>
-          <t>2026-02-19T11:25:49</t>
+          <t>2026-02-19T13:16:44</t>
         </is>
       </c>
       <c r="O159" t="inlineStr">
@@ -11316,7 +11311,7 @@
       </c>
       <c r="N160" t="inlineStr">
         <is>
-          <t>2026-02-19T11:27:37</t>
+          <t>2026-02-19T13:20:37</t>
         </is>
       </c>
       <c r="O160" t="inlineStr">
@@ -11382,7 +11377,7 @@
       </c>
       <c r="N161" t="inlineStr">
         <is>
-          <t>2026-02-19T11:02:27</t>
+          <t>2026-02-19T12:55:37</t>
         </is>
       </c>
       <c r="O161" t="inlineStr">
@@ -11448,7 +11443,7 @@
       </c>
       <c r="N162" t="inlineStr">
         <is>
-          <t>2026-02-19T11:23:50</t>
+          <t>2026-02-19T13:15:07</t>
         </is>
       </c>
       <c r="O162" t="inlineStr">
@@ -11580,7 +11575,7 @@
       </c>
       <c r="N164" t="inlineStr">
         <is>
-          <t>2026-02-19T11:30:08</t>
+          <t>2026-02-19T13:28:11</t>
         </is>
       </c>
       <c r="O164" t="inlineStr">
@@ -11646,7 +11641,7 @@
       </c>
       <c r="N165" t="inlineStr">
         <is>
-          <t>2026-02-19T11:29:00</t>
+          <t>2026-02-19T13:18:48</t>
         </is>
       </c>
       <c r="O165" t="inlineStr">
@@ -11712,7 +11707,7 @@
       </c>
       <c r="N166" t="inlineStr">
         <is>
-          <t>2026-02-19T11:20:24</t>
+          <t>2026-02-19T13:10:57</t>
         </is>
       </c>
       <c r="O166" t="inlineStr">
@@ -11778,7 +11773,7 @@
       </c>
       <c r="N167" t="inlineStr">
         <is>
-          <t>2026-02-19T10:53:56</t>
+          <t>2026-02-19T13:34:14</t>
         </is>
       </c>
       <c r="O167" t="inlineStr">
@@ -11844,7 +11839,7 @@
       </c>
       <c r="N168" t="inlineStr">
         <is>
-          <t>2026-02-19T11:40:54</t>
+          <t>2026-02-19T13:33:36</t>
         </is>
       </c>
       <c r="O168" t="inlineStr">
@@ -11910,7 +11905,7 @@
       </c>
       <c r="N169" t="inlineStr">
         <is>
-          <t>2026-02-19T11:35:49</t>
+          <t>2026-02-19T13:22:21</t>
         </is>
       </c>
       <c r="O169" t="inlineStr">
@@ -11976,7 +11971,7 @@
       </c>
       <c r="N170" t="inlineStr">
         <is>
-          <t>2026-02-19T11:39:53</t>
+          <t>2026-02-19T13:28:36</t>
         </is>
       </c>
       <c r="O170" t="inlineStr">
@@ -12042,7 +12037,7 @@
       </c>
       <c r="N171" t="inlineStr">
         <is>
-          <t>2026-02-19T10:49:43</t>
+          <t>2026-02-19T13:37:35</t>
         </is>
       </c>
       <c r="O171" t="inlineStr">
@@ -12108,7 +12103,7 @@
       </c>
       <c r="N172" t="inlineStr">
         <is>
-          <t>2026-02-18T13:07:33</t>
+          <t>2026-02-19T13:00:25</t>
         </is>
       </c>
       <c r="O172" t="inlineStr">
@@ -12174,7 +12169,7 @@
       </c>
       <c r="N173" t="inlineStr">
         <is>
-          <t>2026-02-18T18:53:36</t>
+          <t>2026-02-19T13:10:20</t>
         </is>
       </c>
       <c r="O173" t="inlineStr">
@@ -12240,7 +12235,7 @@
       </c>
       <c r="N174" t="inlineStr">
         <is>
-          <t>2026-02-19T11:19:15</t>
+          <t>2026-02-19T13:11:47</t>
         </is>
       </c>
       <c r="O174" t="inlineStr">
@@ -12306,7 +12301,7 @@
       </c>
       <c r="N175" t="inlineStr">
         <is>
-          <t>2026-02-19T11:31:28</t>
+          <t>2026-02-19T13:24:12</t>
         </is>
       </c>
       <c r="O175" t="inlineStr">
@@ -12372,7 +12367,7 @@
       </c>
       <c r="N176" t="inlineStr">
         <is>
-          <t>2026-02-19T11:03:57</t>
+          <t>2026-02-19T12:53:20</t>
         </is>
       </c>
       <c r="O176" t="inlineStr">
@@ -12438,7 +12433,7 @@
       </c>
       <c r="N177" t="inlineStr">
         <is>
-          <t>2026-02-19T11:03:58</t>
+          <t>2026-02-19T12:57:48</t>
         </is>
       </c>
       <c r="O177" t="inlineStr">
@@ -12504,7 +12499,7 @@
       </c>
       <c r="N178" t="inlineStr">
         <is>
-          <t>2026-02-19T11:13:30</t>
+          <t>2026-02-19T13:11:12</t>
         </is>
       </c>
       <c r="O178" t="inlineStr">
@@ -12570,7 +12565,7 @@
       </c>
       <c r="N179" t="inlineStr">
         <is>
-          <t>2026-02-19T11:26:05</t>
+          <t>2026-02-19T13:26:19</t>
         </is>
       </c>
       <c r="O179" t="inlineStr">
@@ -12636,7 +12631,7 @@
       </c>
       <c r="N180" t="inlineStr">
         <is>
-          <t>2026-02-19T11:20:54</t>
+          <t>2026-02-19T13:16:23</t>
         </is>
       </c>
       <c r="O180" t="inlineStr">
@@ -12702,7 +12697,7 @@
       </c>
       <c r="N181" t="inlineStr">
         <is>
-          <t>2026-02-19T11:32:21</t>
+          <t>2026-02-19T13:23:13</t>
         </is>
       </c>
       <c r="O181" t="inlineStr">
@@ -12971,7 +12966,7 @@
       </c>
       <c r="N185" t="inlineStr">
         <is>
-          <t>2026-02-19T11:23:23</t>
+          <t>2026-02-19T13:13:13</t>
         </is>
       </c>
       <c r="O185" t="inlineStr">
@@ -13037,7 +13032,7 @@
       </c>
       <c r="N186" t="inlineStr">
         <is>
-          <t>2026-02-19T11:25:44</t>
+          <t>2026-02-19T13:15:47</t>
         </is>
       </c>
       <c r="O186" t="inlineStr">
@@ -13103,7 +13098,7 @@
       </c>
       <c r="N187" t="inlineStr">
         <is>
-          <t>2026-02-19T11:16:42</t>
+          <t>2026-02-19T12:49:59</t>
         </is>
       </c>
       <c r="O187" t="inlineStr">
@@ -13169,7 +13164,7 @@
       </c>
       <c r="N188" t="inlineStr">
         <is>
-          <t>2026-02-19T11:26:04</t>
+          <t>2026-02-19T12:53:05</t>
         </is>
       </c>
       <c r="O188" t="inlineStr">
@@ -13301,7 +13296,7 @@
       </c>
       <c r="N190" t="inlineStr">
         <is>
-          <t>2026-02-19T11:14:52</t>
+          <t>2026-02-19T13:06:22</t>
         </is>
       </c>
       <c r="O190" t="inlineStr">
@@ -13433,7 +13428,7 @@
       </c>
       <c r="N192" t="inlineStr">
         <is>
-          <t>2026-02-19T11:30:46</t>
+          <t>2026-02-19T13:18:34</t>
         </is>
       </c>
       <c r="O192" t="inlineStr">
@@ -13562,7 +13557,7 @@
       </c>
       <c r="N194" t="inlineStr">
         <is>
-          <t>2026-02-19T11:32:48</t>
+          <t>2026-02-19T13:20:03</t>
         </is>
       </c>
       <c r="O194" t="inlineStr">
@@ -13628,7 +13623,7 @@
       </c>
       <c r="N195" t="inlineStr">
         <is>
-          <t>2026-02-19T11:20:34</t>
+          <t>2026-02-19T13:08:01</t>
         </is>
       </c>
       <c r="O195" t="inlineStr">
@@ -13694,7 +13689,7 @@
       </c>
       <c r="N196" t="inlineStr">
         <is>
-          <t>2026-02-19T10:50:52</t>
+          <t>2026-02-19T13:37:14</t>
         </is>
       </c>
       <c r="O196" t="inlineStr">
@@ -13760,7 +13755,7 @@
       </c>
       <c r="N197" t="inlineStr">
         <is>
-          <t>2026-02-19T11:19:46</t>
+          <t>2026-02-19T13:24:42</t>
         </is>
       </c>
       <c r="O197" t="inlineStr">
@@ -13892,7 +13887,7 @@
       </c>
       <c r="N199" t="inlineStr">
         <is>
-          <t>2026-02-19T11:07:23</t>
+          <t>2026-02-19T12:59:41</t>
         </is>
       </c>
       <c r="O199" t="inlineStr">
@@ -13958,7 +13953,7 @@
       </c>
       <c r="N200" t="inlineStr">
         <is>
-          <t>2026-02-18T19:35:54</t>
+          <t>2026-02-19T13:21:30</t>
         </is>
       </c>
       <c r="O200" t="inlineStr">
@@ -14021,7 +14016,7 @@
       </c>
       <c r="N201" t="inlineStr">
         <is>
-          <t>2026-02-19T10:53:23</t>
+          <t>2026-02-19T12:50:06</t>
         </is>
       </c>
       <c r="O201" t="inlineStr">
@@ -14087,7 +14082,7 @@
       </c>
       <c r="N202" t="inlineStr">
         <is>
-          <t>2026-02-19T10:53:14</t>
+          <t>2026-02-19T12:44:07</t>
         </is>
       </c>
       <c r="O202" t="inlineStr">
@@ -14153,7 +14148,7 @@
       </c>
       <c r="N203" t="inlineStr">
         <is>
-          <t>2026-02-19T11:01:31</t>
+          <t>2026-02-19T12:51:39</t>
         </is>
       </c>
       <c r="O203" t="inlineStr">
@@ -14219,7 +14214,7 @@
       </c>
       <c r="N204" t="inlineStr">
         <is>
-          <t>2026-02-19T10:58:36</t>
+          <t>2026-02-19T12:52:08</t>
         </is>
       </c>
       <c r="O204" t="inlineStr">
@@ -14285,7 +14280,7 @@
       </c>
       <c r="N205" t="inlineStr">
         <is>
-          <t>2026-02-19T11:32:36</t>
+          <t>2026-02-19T13:24:03</t>
         </is>
       </c>
       <c r="O205" t="inlineStr">
@@ -14351,7 +14346,7 @@
       </c>
       <c r="N206" t="inlineStr">
         <is>
-          <t>2026-02-19T11:07:58</t>
+          <t>2026-02-19T13:04:45</t>
         </is>
       </c>
       <c r="O206" t="inlineStr">
@@ -14417,7 +14412,7 @@
       </c>
       <c r="N207" t="inlineStr">
         <is>
-          <t>2026-02-19T11:12:59</t>
+          <t>2026-02-19T12:59:00</t>
         </is>
       </c>
       <c r="O207" t="inlineStr">
@@ -14483,7 +14478,7 @@
       </c>
       <c r="N208" t="inlineStr">
         <is>
-          <t>2026-02-19T11:18:35</t>
+          <t>2026-02-19T13:05:20</t>
         </is>
       </c>
       <c r="O208" t="inlineStr">
@@ -14549,7 +14544,7 @@
       </c>
       <c r="N209" t="inlineStr">
         <is>
-          <t>2026-02-19T11:13:43</t>
+          <t>2026-02-19T13:02:37</t>
         </is>
       </c>
       <c r="O209" t="inlineStr">
@@ -14615,7 +14610,7 @@
       </c>
       <c r="N210" t="inlineStr">
         <is>
-          <t>2026-02-19T11:22:20</t>
+          <t>2026-02-19T13:09:24</t>
         </is>
       </c>
       <c r="O210" t="inlineStr">
@@ -14681,7 +14676,7 @@
       </c>
       <c r="N211" t="inlineStr">
         <is>
-          <t>2026-02-19T11:25:57</t>
+          <t>2026-02-19T13:22:37</t>
         </is>
       </c>
       <c r="O211" t="inlineStr">
@@ -14747,7 +14742,7 @@
       </c>
       <c r="N212" t="inlineStr">
         <is>
-          <t>2026-02-19T11:21:35</t>
+          <t>2026-02-19T13:10:53</t>
         </is>
       </c>
       <c r="O212" t="inlineStr">
@@ -14813,7 +14808,7 @@
       </c>
       <c r="N213" t="inlineStr">
         <is>
-          <t>2026-02-19T11:24:18</t>
+          <t>2026-02-19T13:19:40</t>
         </is>
       </c>
       <c r="O213" t="inlineStr">
@@ -14879,7 +14874,7 @@
       </c>
       <c r="N214" t="inlineStr">
         <is>
-          <t>2026-02-18T19:33:47</t>
+          <t>2026-02-19T13:11:41</t>
         </is>
       </c>
       <c r="O214" t="inlineStr">
@@ -14945,7 +14940,7 @@
       </c>
       <c r="N215" t="inlineStr">
         <is>
-          <t>2026-02-19T11:20:27</t>
+          <t>2026-02-19T13:12:48</t>
         </is>
       </c>
       <c r="O215" t="inlineStr">
@@ -15011,7 +15006,7 @@
       </c>
       <c r="N216" t="inlineStr">
         <is>
-          <t>2026-02-19T11:32:42</t>
+          <t>2026-02-19T13:28:18</t>
         </is>
       </c>
       <c r="O216" t="inlineStr">
@@ -15077,7 +15072,7 @@
       </c>
       <c r="N217" t="inlineStr">
         <is>
-          <t>2026-02-19T11:22:18</t>
+          <t>2026-02-19T13:17:06</t>
         </is>
       </c>
       <c r="O217" t="inlineStr">
@@ -15143,7 +15138,7 @@
       </c>
       <c r="N218" t="inlineStr">
         <is>
-          <t>2026-02-19T07:13:35</t>
+          <t>2026-02-19T13:01:50</t>
         </is>
       </c>
       <c r="O218" t="inlineStr">
@@ -15209,7 +15204,7 @@
       </c>
       <c r="N219" t="inlineStr">
         <is>
-          <t>2026-02-19T10:56:11</t>
+          <t>2026-02-19T12:48:07</t>
         </is>
       </c>
       <c r="O219" t="inlineStr">
@@ -15280,7 +15275,7 @@
       </c>
       <c r="N220" t="inlineStr">
         <is>
-          <t>2026-02-19T11:36:16</t>
+          <t>2026-02-19T13:25:26</t>
         </is>
       </c>
       <c r="O220" t="inlineStr">
@@ -15346,7 +15341,7 @@
       </c>
       <c r="N221" t="inlineStr">
         <is>
-          <t>2026-02-19T10:54:05</t>
+          <t>2026-02-19T13:37:19</t>
         </is>
       </c>
       <c r="O221" t="inlineStr">
@@ -15412,7 +15407,7 @@
       </c>
       <c r="N222" t="inlineStr">
         <is>
-          <t>2026-02-18T19:30:24</t>
+          <t>2026-02-19T13:03:41</t>
         </is>
       </c>
       <c r="O222" t="inlineStr">
@@ -15478,7 +15473,7 @@
       </c>
       <c r="N223" t="inlineStr">
         <is>
-          <t>2026-02-19T10:56:55</t>
+          <t>2026-02-19T13:39:57</t>
         </is>
       </c>
       <c r="O223" t="inlineStr">
@@ -15544,7 +15539,7 @@
       </c>
       <c r="N224" t="inlineStr">
         <is>
-          <t>2026-02-18T19:51:33</t>
+          <t>2026-02-19T13:06:43</t>
         </is>
       </c>
       <c r="O224" t="inlineStr">
@@ -15610,7 +15605,7 @@
       </c>
       <c r="N225" t="inlineStr">
         <is>
-          <t>2026-02-19T11:27:26</t>
+          <t>2026-02-19T13:18:53</t>
         </is>
       </c>
       <c r="O225" t="inlineStr">
@@ -15676,7 +15671,7 @@
       </c>
       <c r="N226" t="inlineStr">
         <is>
-          <t>2026-02-19T11:25:10</t>
+          <t>2026-02-19T13:13:33</t>
         </is>
       </c>
       <c r="O226" t="inlineStr">
@@ -15742,7 +15737,7 @@
       </c>
       <c r="N227" t="inlineStr">
         <is>
-          <t>2026-02-19T10:54:35</t>
+          <t>2026-02-19T12:46:57</t>
         </is>
       </c>
       <c r="O227" t="inlineStr">
@@ -15808,7 +15803,7 @@
       </c>
       <c r="N228" t="inlineStr">
         <is>
-          <t>2026-02-19T11:36:00</t>
+          <t>2026-02-19T13:28:11</t>
         </is>
       </c>
       <c r="O228" t="inlineStr">
@@ -15874,7 +15869,7 @@
       </c>
       <c r="N229" t="inlineStr">
         <is>
-          <t>2026-02-19T11:08:39</t>
+          <t>2026-02-19T13:02:52</t>
         </is>
       </c>
       <c r="O229" t="inlineStr">
@@ -15940,7 +15935,7 @@
       </c>
       <c r="N230" t="inlineStr">
         <is>
-          <t>2026-02-19T10:56:08</t>
+          <t>2026-02-19T12:43:53</t>
         </is>
       </c>
       <c r="O230" t="inlineStr">
@@ -16006,7 +16001,7 @@
       </c>
       <c r="N231" t="inlineStr">
         <is>
-          <t>2026-02-19T10:48:43</t>
+          <t>2026-02-19T13:36:39</t>
         </is>
       </c>
       <c r="O231" t="inlineStr">
@@ -16072,7 +16067,7 @@
       </c>
       <c r="N232" t="inlineStr">
         <is>
-          <t>2026-02-19T11:33:11</t>
+          <t>2026-02-19T13:21:10</t>
         </is>
       </c>
       <c r="O232" t="inlineStr">
@@ -16138,7 +16133,7 @@
       </c>
       <c r="N233" t="inlineStr">
         <is>
-          <t>2026-02-19T10:54:40</t>
+          <t>2026-02-19T12:47:09</t>
         </is>
       </c>
       <c r="O233" t="inlineStr">
@@ -16204,7 +16199,7 @@
       </c>
       <c r="N234" t="inlineStr">
         <is>
-          <t>2026-02-19T11:07:03</t>
+          <t>2026-02-19T13:02:14</t>
         </is>
       </c>
       <c r="O234" t="inlineStr">
@@ -16270,7 +16265,7 @@
       </c>
       <c r="N235" t="inlineStr">
         <is>
-          <t>2026-02-18T19:54:27</t>
+          <t>2026-02-19T12:59:54</t>
         </is>
       </c>
       <c r="O235" t="inlineStr">
@@ -16336,7 +16331,7 @@
       </c>
       <c r="N236" t="inlineStr">
         <is>
-          <t>2026-02-18T19:49:00</t>
+          <t>2026-02-19T12:58:19</t>
         </is>
       </c>
       <c r="O236" t="inlineStr">
@@ -16402,7 +16397,7 @@
       </c>
       <c r="N237" t="inlineStr">
         <is>
-          <t>2026-02-18T19:50:35</t>
+          <t>2026-02-19T13:01:09</t>
         </is>
       </c>
       <c r="O237" t="inlineStr">
@@ -16468,7 +16463,7 @@
       </c>
       <c r="N238" t="inlineStr">
         <is>
-          <t>2026-02-19T11:29:53</t>
+          <t>2026-02-19T13:21:42</t>
         </is>
       </c>
       <c r="O238" t="inlineStr">
@@ -16534,7 +16529,7 @@
       </c>
       <c r="N239" t="inlineStr">
         <is>
-          <t>2026-02-19T11:30:19</t>
+          <t>2026-02-19T13:25:40</t>
         </is>
       </c>
       <c r="O239" t="inlineStr">
@@ -16600,7 +16595,7 @@
       </c>
       <c r="N240" t="inlineStr">
         <is>
-          <t>2026-02-19T10:50:06</t>
+          <t>2026-02-19T13:41:13</t>
         </is>
       </c>
       <c r="O240" t="inlineStr">
@@ -16666,7 +16661,7 @@
       </c>
       <c r="N241" t="inlineStr">
         <is>
-          <t>2026-02-19T11:39:52</t>
+          <t>2026-02-19T13:27:57</t>
         </is>
       </c>
       <c r="O241" t="inlineStr">
@@ -16732,7 +16727,7 @@
       </c>
       <c r="N242" t="inlineStr">
         <is>
-          <t>2026-02-19T10:51:01</t>
+          <t>2026-02-19T13:40:29</t>
         </is>
       </c>
       <c r="O242" t="inlineStr">
@@ -16798,7 +16793,7 @@
       </c>
       <c r="N243" t="inlineStr">
         <is>
-          <t>2026-02-19T11:21:12</t>
+          <t>2026-02-19T13:11:15</t>
         </is>
       </c>
       <c r="O243" t="inlineStr">
@@ -16818,6 +16813,11 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>10.69.5.112</t>
+        </is>
+      </c>
       <c r="D244" t="n">
         <v>2019</v>
       </c>
@@ -16859,7 +16859,7 @@
       </c>
       <c r="N244" t="inlineStr">
         <is>
-          <t>2026-02-18T19:43:39</t>
+          <t>2026-02-19T13:17:03</t>
         </is>
       </c>
       <c r="O244" t="inlineStr">
@@ -16925,7 +16925,7 @@
       </c>
       <c r="N245" t="inlineStr">
         <is>
-          <t>2026-02-19T11:30:24</t>
+          <t>2026-02-19T13:24:58</t>
         </is>
       </c>
       <c r="O245" t="inlineStr">
@@ -16991,7 +16991,7 @@
       </c>
       <c r="N246" t="inlineStr">
         <is>
-          <t>2026-02-19T11:06:05</t>
+          <t>2026-02-19T13:04:09</t>
         </is>
       </c>
       <c r="O246" t="inlineStr">
@@ -17057,7 +17057,7 @@
       </c>
       <c r="N247" t="inlineStr">
         <is>
-          <t>2026-02-19T11:30:21</t>
+          <t>2026-02-19T13:22:49</t>
         </is>
       </c>
       <c r="O247" t="inlineStr">
@@ -17123,7 +17123,7 @@
       </c>
       <c r="N248" t="inlineStr">
         <is>
-          <t>2026-02-19T10:47:17</t>
+          <t>2026-02-19T13:35:52</t>
         </is>
       </c>
       <c r="O248" t="inlineStr">
@@ -17189,7 +17189,7 @@
       </c>
       <c r="N249" t="inlineStr">
         <is>
-          <t>2026-02-19T11:23:49</t>
+          <t>2026-02-19T13:16:54</t>
         </is>
       </c>
       <c r="O249" t="inlineStr">
@@ -17255,7 +17255,7 @@
       </c>
       <c r="N250" t="inlineStr">
         <is>
-          <t>2026-02-19T11:30:09</t>
+          <t>2026-02-19T13:21:56</t>
         </is>
       </c>
       <c r="O250" t="inlineStr">
@@ -17321,7 +17321,7 @@
       </c>
       <c r="N251" t="inlineStr">
         <is>
-          <t>2026-02-19T11:30:15</t>
+          <t>2026-02-19T13:28:26</t>
         </is>
       </c>
       <c r="O251" t="inlineStr">
@@ -17387,7 +17387,7 @@
       </c>
       <c r="N252" t="inlineStr">
         <is>
-          <t>2026-02-19T11:33:54</t>
+          <t>2026-02-19T13:24:51</t>
         </is>
       </c>
       <c r="O252" t="inlineStr">
@@ -17453,7 +17453,7 @@
       </c>
       <c r="N253" t="inlineStr">
         <is>
-          <t>2026-02-19T11:35:42</t>
+          <t>2026-02-19T13:27:13</t>
         </is>
       </c>
       <c r="O253" t="inlineStr">
@@ -17513,7 +17513,7 @@
       </c>
       <c r="N254" t="inlineStr">
         <is>
-          <t>2026-02-19T11:14:13</t>
+          <t>2026-02-19T13:01:44</t>
         </is>
       </c>
       <c r="O254" t="inlineStr">
@@ -17579,7 +17579,7 @@
       </c>
       <c r="N255" t="inlineStr">
         <is>
-          <t>2026-02-19T11:36:45</t>
+          <t>2026-02-19T13:31:51</t>
         </is>
       </c>
       <c r="O255" t="inlineStr">
@@ -17645,7 +17645,7 @@
       </c>
       <c r="N256" t="inlineStr">
         <is>
-          <t>2026-02-19T10:44:16</t>
+          <t>2026-02-19T12:42:23</t>
         </is>
       </c>
       <c r="O256" t="inlineStr">
@@ -17711,7 +17711,7 @@
       </c>
       <c r="N257" t="inlineStr">
         <is>
-          <t>2026-02-19T11:14:02</t>
+          <t>2026-02-19T13:06:49</t>
         </is>
       </c>
       <c r="O257" t="inlineStr">
@@ -17777,7 +17777,7 @@
       </c>
       <c r="N258" t="inlineStr">
         <is>
-          <t>2026-02-19T10:51:47</t>
+          <t>2026-02-19T12:47:58</t>
         </is>
       </c>
       <c r="O258" t="inlineStr">
@@ -17843,7 +17843,7 @@
       </c>
       <c r="N259" t="inlineStr">
         <is>
-          <t>2026-02-19T11:06:23</t>
+          <t>2026-02-19T12:57:14</t>
         </is>
       </c>
       <c r="O259" t="inlineStr">
@@ -17909,7 +17909,7 @@
       </c>
       <c r="N260" t="inlineStr">
         <is>
-          <t>2026-02-19T11:14:08</t>
+          <t>2026-02-19T13:07:02</t>
         </is>
       </c>
       <c r="O260" t="inlineStr">
@@ -17975,7 +17975,7 @@
       </c>
       <c r="N261" t="inlineStr">
         <is>
-          <t>2026-02-19T11:37:19</t>
+          <t>2026-02-19T13:30:11</t>
         </is>
       </c>
       <c r="O261" t="inlineStr">
@@ -18041,7 +18041,7 @@
       </c>
       <c r="N262" t="inlineStr">
         <is>
-          <t>2026-02-19T11:26:58</t>
+          <t>2026-02-19T13:16:27</t>
         </is>
       </c>
       <c r="O262" t="inlineStr">
@@ -18107,7 +18107,7 @@
       </c>
       <c r="N263" t="inlineStr">
         <is>
-          <t>2026-02-19T11:38:30</t>
+          <t>2026-02-19T13:31:14</t>
         </is>
       </c>
       <c r="O263" t="inlineStr">
@@ -18173,7 +18173,7 @@
       </c>
       <c r="N264" t="inlineStr">
         <is>
-          <t>2026-02-19T11:22:34</t>
+          <t>2026-02-19T13:16:50</t>
         </is>
       </c>
       <c r="O264" t="inlineStr">
@@ -18239,7 +18239,7 @@
       </c>
       <c r="N265" t="inlineStr">
         <is>
-          <t>2026-02-19T11:22:55</t>
+          <t>2026-02-19T13:14:11</t>
         </is>
       </c>
       <c r="O265" t="inlineStr">
@@ -18305,7 +18305,7 @@
       </c>
       <c r="N266" t="inlineStr">
         <is>
-          <t>2026-02-19T11:17:48</t>
+          <t>2026-02-19T13:08:49</t>
         </is>
       </c>
       <c r="O266" t="inlineStr">
@@ -18371,7 +18371,7 @@
       </c>
       <c r="N267" t="inlineStr">
         <is>
-          <t>2026-02-19T10:56:31</t>
+          <t>2026-02-19T12:51:39</t>
         </is>
       </c>
       <c r="O267" t="inlineStr">
@@ -18437,7 +18437,7 @@
       </c>
       <c r="N268" t="inlineStr">
         <is>
-          <t>2026-02-19T11:04:28</t>
+          <t>2026-02-19T12:51:45</t>
         </is>
       </c>
       <c r="O268" t="inlineStr">
@@ -18503,7 +18503,7 @@
       </c>
       <c r="N269" t="inlineStr">
         <is>
-          <t>2026-02-19T11:07:49</t>
+          <t>2026-02-19T13:05:26</t>
         </is>
       </c>
       <c r="O269" t="inlineStr">
@@ -18566,7 +18566,7 @@
       </c>
       <c r="N270" t="inlineStr">
         <is>
-          <t>2026-02-19T11:26:37</t>
+          <t>2026-02-19T13:18:29</t>
         </is>
       </c>
       <c r="O270" t="inlineStr">
@@ -18698,7 +18698,7 @@
       </c>
       <c r="N272" t="inlineStr">
         <is>
-          <t>2026-02-19T11:37:55</t>
+          <t>2026-02-19T13:29:07</t>
         </is>
       </c>
       <c r="O272" t="inlineStr">
@@ -18764,7 +18764,7 @@
       </c>
       <c r="N273" t="inlineStr">
         <is>
-          <t>2026-02-19T11:26:00</t>
+          <t>2026-02-19T13:19:47</t>
         </is>
       </c>
       <c r="O273" t="inlineStr">
@@ -19094,7 +19094,7 @@
       </c>
       <c r="N278" t="inlineStr">
         <is>
-          <t>2026-02-19T11:41:15</t>
+          <t>2026-02-19T13:32:17</t>
         </is>
       </c>
       <c r="O278" t="inlineStr">
@@ -19160,7 +19160,7 @@
       </c>
       <c r="N279" t="inlineStr">
         <is>
-          <t>2026-02-19T11:05:30</t>
+          <t>2026-02-19T12:58:30</t>
         </is>
       </c>
       <c r="O279" t="inlineStr">
@@ -19226,7 +19226,7 @@
       </c>
       <c r="N280" t="inlineStr">
         <is>
-          <t>2026-02-19T10:58:47</t>
+          <t>2026-02-19T12:49:12</t>
         </is>
       </c>
       <c r="O280" t="inlineStr">
@@ -19292,7 +19292,7 @@
       </c>
       <c r="N281" t="inlineStr">
         <is>
-          <t>2026-02-19T11:10:21</t>
+          <t>2026-02-19T13:05:15</t>
         </is>
       </c>
       <c r="O281" t="inlineStr">
@@ -19353,7 +19353,7 @@
       </c>
       <c r="N282" t="inlineStr">
         <is>
-          <t>2026-02-19T11:19:04</t>
+          <t>2026-02-19T13:06:05</t>
         </is>
       </c>
       <c r="O282" t="inlineStr">
@@ -19419,7 +19419,7 @@
       </c>
       <c r="N283" t="inlineStr">
         <is>
-          <t>2026-02-19T11:08:47</t>
+          <t>2026-02-19T13:06:39</t>
         </is>
       </c>
       <c r="O283" t="inlineStr">
@@ -19485,7 +19485,7 @@
       </c>
       <c r="N284" t="inlineStr">
         <is>
-          <t>2026-02-19T10:54:08</t>
+          <t>2026-02-19T13:31:47</t>
         </is>
       </c>
       <c r="O284" t="inlineStr">
@@ -19551,7 +19551,7 @@
       </c>
       <c r="N285" t="inlineStr">
         <is>
-          <t>2026-02-19T11:24:10</t>
+          <t>2026-02-19T13:16:19</t>
         </is>
       </c>
       <c r="O285" t="inlineStr">
@@ -19571,11 +19571,6 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
-      <c r="C286" t="inlineStr">
-        <is>
-          <t>10.69.5.155</t>
-        </is>
-      </c>
       <c r="D286" t="n">
         <v>2019</v>
       </c>
@@ -19683,7 +19678,7 @@
       </c>
       <c r="N287" t="inlineStr">
         <is>
-          <t>2026-02-19T10:50:05</t>
+          <t>2026-02-19T13:36:29</t>
         </is>
       </c>
       <c r="O287" t="inlineStr">
@@ -19749,7 +19744,7 @@
       </c>
       <c r="N288" t="inlineStr">
         <is>
-          <t>2026-02-19T11:17:18</t>
+          <t>2026-02-19T13:09:41</t>
         </is>
       </c>
       <c r="O288" t="inlineStr">
@@ -19815,7 +19810,7 @@
       </c>
       <c r="N289" t="inlineStr">
         <is>
-          <t>2026-02-19T11:03:51</t>
+          <t>2026-02-19T12:58:03</t>
         </is>
       </c>
       <c r="O289" t="inlineStr">
@@ -20635,7 +20630,7 @@
       </c>
       <c r="N302" t="inlineStr">
         <is>
-          <t>2026-02-19T11:26:10</t>
+          <t>2026-02-19T13:12:48</t>
         </is>
       </c>
       <c r="O302" t="inlineStr">
@@ -21787,7 +21782,7 @@
       </c>
       <c r="N320" t="inlineStr">
         <is>
-          <t>2026-02-19T11:10:14</t>
+          <t>2026-02-19T13:08:39</t>
         </is>
       </c>
       <c r="O320" t="inlineStr">
@@ -22536,7 +22531,7 @@
       </c>
       <c r="N332" t="inlineStr">
         <is>
-          <t>2026-02-19T10:48:25</t>
+          <t>2026-02-19T13:34:26</t>
         </is>
       </c>
       <c r="O332" t="inlineStr">
@@ -22602,7 +22597,7 @@
       </c>
       <c r="N333" t="inlineStr">
         <is>
-          <t>2026-02-19T11:25:42</t>
+          <t>2026-02-19T13:21:35</t>
         </is>
       </c>
       <c r="O333" t="inlineStr">
@@ -22668,7 +22663,7 @@
       </c>
       <c r="N334" t="inlineStr">
         <is>
-          <t>2026-02-19T11:19:31</t>
+          <t>2026-02-19T13:11:45</t>
         </is>
       </c>
       <c r="O334" t="inlineStr">
@@ -22734,7 +22729,7 @@
       </c>
       <c r="N335" t="inlineStr">
         <is>
-          <t>2026-02-19T11:16:35</t>
+          <t>2026-02-19T13:10:47</t>
         </is>
       </c>
       <c r="O335" t="inlineStr">
@@ -22800,7 +22795,7 @@
       </c>
       <c r="N336" t="inlineStr">
         <is>
-          <t>2026-02-19T11:34:08</t>
+          <t>2026-02-19T13:23:24</t>
         </is>
       </c>
       <c r="O336" t="inlineStr">
@@ -22866,7 +22861,7 @@
       </c>
       <c r="N337" t="inlineStr">
         <is>
-          <t>2026-02-19T11:33:00</t>
+          <t>2026-02-19T13:32:24</t>
         </is>
       </c>
       <c r="O337" t="inlineStr">
@@ -22932,7 +22927,7 @@
       </c>
       <c r="N338" t="inlineStr">
         <is>
-          <t>2026-02-19T11:02:44</t>
+          <t>2026-02-19T12:58:14</t>
         </is>
       </c>
       <c r="O338" t="inlineStr">
@@ -22998,7 +22993,7 @@
       </c>
       <c r="N339" t="inlineStr">
         <is>
-          <t>2026-02-19T11:26:54</t>
+          <t>2026-02-19T13:15:34</t>
         </is>
       </c>
       <c r="O339" t="inlineStr">
@@ -23130,7 +23125,7 @@
       </c>
       <c r="N341" t="inlineStr">
         <is>
-          <t>2026-02-19T10:51:27</t>
+          <t>2026-02-19T12:47:27</t>
         </is>
       </c>
       <c r="O341" t="inlineStr">
@@ -23196,7 +23191,7 @@
       </c>
       <c r="N342" t="inlineStr">
         <is>
-          <t>2026-02-19T11:23:54</t>
+          <t>2026-02-19T13:18:58</t>
         </is>
       </c>
       <c r="O342" t="inlineStr">
@@ -23259,7 +23254,7 @@
       </c>
       <c r="N343" t="inlineStr">
         <is>
-          <t>2026-02-19T11:18:15</t>
+          <t>2026-02-19T13:12:11</t>
         </is>
       </c>
       <c r="O343" t="inlineStr">
@@ -23523,7 +23518,7 @@
       </c>
       <c r="N347" t="inlineStr">
         <is>
-          <t>2026-02-19T11:39:21</t>
+          <t>2026-02-19T13:36:54</t>
         </is>
       </c>
       <c r="O347" t="inlineStr">
@@ -23974,7 +23969,7 @@
       </c>
       <c r="N354" t="inlineStr">
         <is>
-          <t>2026-02-19T11:40:26</t>
+          <t>2026-02-19T13:25:54</t>
         </is>
       </c>
       <c r="O354" t="inlineStr">
@@ -24040,7 +24035,7 @@
       </c>
       <c r="N355" t="inlineStr">
         <is>
-          <t>2026-02-19T11:28:19</t>
+          <t>2026-02-19T13:22:33</t>
         </is>
       </c>
       <c r="O355" t="inlineStr">
@@ -24172,7 +24167,7 @@
       </c>
       <c r="N357" t="inlineStr">
         <is>
-          <t>2026-02-19T11:39:43</t>
+          <t>2026-02-19T13:31:37</t>
         </is>
       </c>
       <c r="O357" t="inlineStr">
@@ -24365,7 +24360,7 @@
       </c>
       <c r="N360" t="inlineStr">
         <is>
-          <t>2026-02-19T11:41:39</t>
+          <t>2026-02-19T13:28:22</t>
         </is>
       </c>
       <c r="O360" t="inlineStr">
@@ -24431,7 +24426,7 @@
       </c>
       <c r="N361" t="inlineStr">
         <is>
-          <t>2026-02-19T10:53:27</t>
+          <t>2026-02-19T13:37:04</t>
         </is>
       </c>
       <c r="O361" t="inlineStr">
@@ -24494,7 +24489,7 @@
       </c>
       <c r="N362" t="inlineStr">
         <is>
-          <t>2026-02-19T11:11:46</t>
+          <t>2026-02-19T13:10:34</t>
         </is>
       </c>
       <c r="O362" t="inlineStr">
@@ -24688,7 +24683,7 @@
       </c>
       <c r="N365" t="inlineStr">
         <is>
-          <t>2026-02-19T11:42:17</t>
+          <t>2026-02-19T13:29:52</t>
         </is>
       </c>
       <c r="O365" t="inlineStr">
@@ -24756,7 +24751,7 @@
       </c>
       <c r="N366" t="inlineStr">
         <is>
-          <t>2026-02-19T11:38:41</t>
+          <t>2026-02-19T13:26:38</t>
         </is>
       </c>
       <c r="O366" t="inlineStr">
@@ -24886,7 +24881,7 @@
       </c>
       <c r="N368" t="inlineStr">
         <is>
-          <t>2026-02-19T10:52:16</t>
+          <t>2026-02-19T12:44:31</t>
         </is>
       </c>
       <c r="O368" t="inlineStr">
@@ -24906,6 +24901,11 @@
           <t>RH</t>
         </is>
       </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>10.69.3.13</t>
+        </is>
+      </c>
       <c r="D369" t="n">
         <v>2025</v>
       </c>
@@ -24949,7 +24949,7 @@
       </c>
       <c r="N369" t="inlineStr">
         <is>
-          <t>2026-02-19T10:48:26</t>
+          <t>2026-02-19T13:33:12</t>
         </is>
       </c>
       <c r="O369" t="inlineStr">
@@ -25020,7 +25020,7 @@
       </c>
       <c r="N370" t="inlineStr">
         <is>
-          <t>2026-02-19T11:33:04</t>
+          <t>2026-02-19T13:20:02</t>
         </is>
       </c>
       <c r="O370" t="inlineStr">
@@ -25091,7 +25091,7 @@
       </c>
       <c r="N371" t="inlineStr">
         <is>
-          <t>2026-02-19T11:11:53</t>
+          <t>2026-02-19T13:09:20</t>
         </is>
       </c>
       <c r="O371" t="inlineStr">
@@ -25304,7 +25304,7 @@
       </c>
       <c r="N374" t="inlineStr">
         <is>
-          <t>2026-02-19T11:00:02</t>
+          <t>2026-02-19T12:54:20</t>
         </is>
       </c>
       <c r="O374" t="inlineStr">
@@ -25372,7 +25372,7 @@
       </c>
       <c r="N375" t="inlineStr">
         <is>
-          <t>2026-02-19T11:35:38</t>
+          <t>2026-02-19T13:33:42</t>
         </is>
       </c>
       <c r="O375" t="inlineStr">
@@ -25438,7 +25438,7 @@
       </c>
       <c r="N376" t="inlineStr">
         <is>
-          <t>2026-02-19T11:10:47</t>
+          <t>2026-02-19T13:01:51</t>
         </is>
       </c>
       <c r="O376" t="inlineStr">
@@ -25509,7 +25509,7 @@
       </c>
       <c r="N377" t="inlineStr">
         <is>
-          <t>2026-02-19T11:34:55</t>
+          <t>2026-02-19T13:18:44</t>
         </is>
       </c>
       <c r="O377" t="inlineStr">
@@ -25580,7 +25580,7 @@
       </c>
       <c r="N378" t="inlineStr">
         <is>
-          <t>2026-02-19T11:40:48</t>
+          <t>2026-02-19T13:29:32</t>
         </is>
       </c>
       <c r="O378" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática 2026-02-19 15:52:03.153001
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -601,7 +601,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>2026-02-19T13:26:04</t>
+          <t>2026-02-19T15:17:48</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -672,7 +672,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>2026-02-19T12:58:58</t>
+          <t>2026-02-19T14:55:02</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -743,7 +743,7 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>2026-02-19T12:59:54</t>
+          <t>2026-02-19T14:55:19</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
@@ -814,7 +814,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>2026-02-19T13:29:25</t>
+          <t>2026-02-19T15:18:44</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -1103,6 +1103,11 @@
           <t>AUDITORIO</t>
         </is>
       </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>10.69.3.160</t>
+        </is>
+      </c>
       <c r="D10" t="n">
         <v>2017</v>
       </c>
@@ -1144,7 +1149,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>2026-02-19T13:06:40</t>
+          <t>2026-02-19T14:59:44</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -1474,7 +1479,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>2026-02-19T13:02:45</t>
+          <t>2026-02-19T14:50:13</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
@@ -1540,7 +1545,7 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>2026-02-13T17:06:18</t>
+          <t>2026-02-19T15:02:24</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
@@ -1606,7 +1611,7 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>2026-02-19T13:17:40</t>
+          <t>2026-02-19T14:17:55</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
@@ -2293,7 +2298,7 @@
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>2026-02-19T13:13:28</t>
+          <t>2026-02-19T14:59:58</t>
         </is>
       </c>
       <c r="O28" t="inlineStr">
@@ -6885,7 +6890,7 @@
       </c>
       <c r="N95" t="inlineStr">
         <is>
-          <t>2026-02-19T13:29:43</t>
+          <t>2026-02-19T15:20:49</t>
         </is>
       </c>
       <c r="O95" t="inlineStr">
@@ -6956,7 +6961,7 @@
       </c>
       <c r="N96" t="inlineStr">
         <is>
-          <t>2026-02-19T13:31:03</t>
+          <t>2026-02-19T15:27:06</t>
         </is>
       </c>
       <c r="O96" t="inlineStr">
@@ -7022,7 +7027,7 @@
       </c>
       <c r="N97" t="inlineStr">
         <is>
-          <t>2026-02-19T13:14:50</t>
+          <t>2026-02-19T15:06:42</t>
         </is>
       </c>
       <c r="O97" t="inlineStr">
@@ -7093,7 +7098,7 @@
       </c>
       <c r="N98" t="inlineStr">
         <is>
-          <t>2026-02-19T13:42:04</t>
+          <t>2026-02-19T15:27:38</t>
         </is>
       </c>
       <c r="O98" t="inlineStr">
@@ -7164,7 +7169,7 @@
       </c>
       <c r="N99" t="inlineStr">
         <is>
-          <t>2026-02-19T13:28:27</t>
+          <t>2026-02-19T15:21:19</t>
         </is>
       </c>
       <c r="O99" t="inlineStr">
@@ -7235,7 +7240,7 @@
       </c>
       <c r="N100" t="inlineStr">
         <is>
-          <t>2026-02-19T13:11:36</t>
+          <t>2026-02-19T14:55:21</t>
         </is>
       </c>
       <c r="O100" t="inlineStr">
@@ -7306,7 +7311,7 @@
       </c>
       <c r="N101" t="inlineStr">
         <is>
-          <t>2026-02-19T12:53:30</t>
+          <t>2026-02-19T15:41:57</t>
         </is>
       </c>
       <c r="O101" t="inlineStr">
@@ -7448,7 +7453,7 @@
       </c>
       <c r="N103" t="inlineStr">
         <is>
-          <t>2026-02-19T12:49:25</t>
+          <t>2026-02-19T15:33:18</t>
         </is>
       </c>
       <c r="O103" t="inlineStr">
@@ -7713,7 +7718,7 @@
       </c>
       <c r="N107" t="inlineStr">
         <is>
-          <t>2026-02-19T12:51:46</t>
+          <t>2026-02-19T15:37:21</t>
         </is>
       </c>
       <c r="O107" t="inlineStr">
@@ -7855,7 +7860,7 @@
       </c>
       <c r="N109" t="inlineStr">
         <is>
-          <t>2026-02-19T13:01:00</t>
+          <t>2026-02-19T14:50:12</t>
         </is>
       </c>
       <c r="O109" t="inlineStr">
@@ -7926,7 +7931,7 @@
       </c>
       <c r="N110" t="inlineStr">
         <is>
-          <t>2026-02-19T13:29:01</t>
+          <t>2026-02-19T15:22:19</t>
         </is>
       </c>
       <c r="O110" t="inlineStr">
@@ -7997,7 +8002,7 @@
       </c>
       <c r="N111" t="inlineStr">
         <is>
-          <t>2026-02-19T13:24:43</t>
+          <t>2026-02-19T15:17:27</t>
         </is>
       </c>
       <c r="O111" t="inlineStr">
@@ -8068,7 +8073,7 @@
       </c>
       <c r="N112" t="inlineStr">
         <is>
-          <t>2026-02-19T13:04:53</t>
+          <t>2026-02-19T15:05:45</t>
         </is>
       </c>
       <c r="O112" t="inlineStr">
@@ -8139,7 +8144,7 @@
       </c>
       <c r="N113" t="inlineStr">
         <is>
-          <t>2026-02-19T12:50:32</t>
+          <t>2026-02-19T14:48:43</t>
         </is>
       </c>
       <c r="O113" t="inlineStr">
@@ -8210,7 +8215,7 @@
       </c>
       <c r="N114" t="inlineStr">
         <is>
-          <t>2026-02-19T12:57:08</t>
+          <t>2026-02-19T14:52:15</t>
         </is>
       </c>
       <c r="O114" t="inlineStr">
@@ -8278,7 +8283,7 @@
       </c>
       <c r="N115" t="inlineStr">
         <is>
-          <t>2026-02-19T12:55:35</t>
+          <t>2026-02-19T14:49:28</t>
         </is>
       </c>
       <c r="O115" t="inlineStr">
@@ -8349,7 +8354,7 @@
       </c>
       <c r="N116" t="inlineStr">
         <is>
-          <t>2026-02-19T13:07:09</t>
+          <t>2026-02-19T14:54:52</t>
         </is>
       </c>
       <c r="O116" t="inlineStr">
@@ -8415,7 +8420,7 @@
       </c>
       <c r="N117" t="inlineStr">
         <is>
-          <t>2026-02-19T13:18:09</t>
+          <t>2026-02-19T15:07:23</t>
         </is>
       </c>
       <c r="O117" t="inlineStr">
@@ -8625,7 +8630,7 @@
       </c>
       <c r="N120" t="inlineStr">
         <is>
-          <t>2026-02-19T12:56:25</t>
+          <t>2026-02-19T15:34:56</t>
         </is>
       </c>
       <c r="O120" t="inlineStr">
@@ -8696,7 +8701,7 @@
       </c>
       <c r="N121" t="inlineStr">
         <is>
-          <t>2026-02-19T12:29:28</t>
+          <t>2026-02-19T14:59:22</t>
         </is>
       </c>
       <c r="O121" t="inlineStr">
@@ -8764,7 +8769,7 @@
       </c>
       <c r="N122" t="inlineStr">
         <is>
-          <t>2026-02-19T13:12:24</t>
+          <t>2026-02-19T15:03:28</t>
         </is>
       </c>
       <c r="O122" t="inlineStr">
@@ -8835,7 +8840,7 @@
       </c>
       <c r="N123" t="inlineStr">
         <is>
-          <t>2026-02-19T13:29:41</t>
+          <t>2026-02-19T15:27:26</t>
         </is>
       </c>
       <c r="O123" t="inlineStr">
@@ -8906,7 +8911,7 @@
       </c>
       <c r="N124" t="inlineStr">
         <is>
-          <t>2026-02-19T13:07:19</t>
+          <t>2026-02-19T15:01:58</t>
         </is>
       </c>
       <c r="O124" t="inlineStr">
@@ -8977,7 +8982,7 @@
       </c>
       <c r="N125" t="inlineStr">
         <is>
-          <t>2026-02-19T12:55:54</t>
+          <t>2026-02-19T15:40:19</t>
         </is>
       </c>
       <c r="O125" t="inlineStr">
@@ -9048,7 +9053,7 @@
       </c>
       <c r="N126" t="inlineStr">
         <is>
-          <t>2026-02-19T12:50:08</t>
+          <t>2026-02-19T15:33:10</t>
         </is>
       </c>
       <c r="O126" t="inlineStr">
@@ -9119,7 +9124,7 @@
       </c>
       <c r="N127" t="inlineStr">
         <is>
-          <t>2026-02-19T13:32:56</t>
+          <t>2026-02-19T14:51:08</t>
         </is>
       </c>
       <c r="O127" t="inlineStr">
@@ -9190,7 +9195,7 @@
       </c>
       <c r="N128" t="inlineStr">
         <is>
-          <t>2026-02-19T13:29:39</t>
+          <t>2026-02-19T15:20:22</t>
         </is>
       </c>
       <c r="O128" t="inlineStr">
@@ -9261,7 +9266,7 @@
       </c>
       <c r="N129" t="inlineStr">
         <is>
-          <t>2026-02-19T13:05:46</t>
+          <t>2026-02-19T14:57:45</t>
         </is>
       </c>
       <c r="O129" t="inlineStr">
@@ -9332,7 +9337,7 @@
       </c>
       <c r="N130" t="inlineStr">
         <is>
-          <t>2026-02-19T12:54:11</t>
+          <t>2026-02-19T14:46:01</t>
         </is>
       </c>
       <c r="O130" t="inlineStr">
@@ -9398,7 +9403,7 @@
       </c>
       <c r="N131" t="inlineStr">
         <is>
-          <t>2026-02-19T13:21:31</t>
+          <t>2026-02-19T15:10:50</t>
         </is>
       </c>
       <c r="O131" t="inlineStr">
@@ -9535,7 +9540,7 @@
       </c>
       <c r="N133" t="inlineStr">
         <is>
-          <t>2026-02-19T13:33:23</t>
+          <t>2026-02-19T15:26:40</t>
         </is>
       </c>
       <c r="O133" t="inlineStr">
@@ -9601,7 +9606,7 @@
       </c>
       <c r="N134" t="inlineStr">
         <is>
-          <t>2026-02-18T20:13:50</t>
+          <t>2026-02-19T14:58:24</t>
         </is>
       </c>
       <c r="O134" t="inlineStr">
@@ -9667,7 +9672,7 @@
       </c>
       <c r="N135" t="inlineStr">
         <is>
-          <t>2026-02-19T13:35:21</t>
+          <t>2026-02-19T15:24:59</t>
         </is>
       </c>
       <c r="O135" t="inlineStr">
@@ -9864,7 +9869,7 @@
       </c>
       <c r="N138" t="inlineStr">
         <is>
-          <t>2026-02-19T13:41:13</t>
+          <t>2026-02-19T15:25:19</t>
         </is>
       </c>
       <c r="O138" t="inlineStr">
@@ -9930,7 +9935,7 @@
       </c>
       <c r="N139" t="inlineStr">
         <is>
-          <t>2026-02-19T13:30:54</t>
+          <t>2026-02-19T14:53:54</t>
         </is>
       </c>
       <c r="O139" t="inlineStr">
@@ -9996,7 +10001,7 @@
       </c>
       <c r="N140" t="inlineStr">
         <is>
-          <t>2026-02-19T13:38:08</t>
+          <t>2026-02-19T15:32:08</t>
         </is>
       </c>
       <c r="O140" t="inlineStr">
@@ -10062,7 +10067,7 @@
       </c>
       <c r="N141" t="inlineStr">
         <is>
-          <t>2026-02-18T19:09:39</t>
+          <t>2026-02-19T14:53:30</t>
         </is>
       </c>
       <c r="O141" t="inlineStr">
@@ -10128,7 +10133,7 @@
       </c>
       <c r="N142" t="inlineStr">
         <is>
-          <t>2026-02-19T13:01:12</t>
+          <t>2026-02-19T15:36:31</t>
         </is>
       </c>
       <c r="O142" t="inlineStr">
@@ -10194,7 +10199,7 @@
       </c>
       <c r="N143" t="inlineStr">
         <is>
-          <t>2026-02-19T13:19:28</t>
+          <t>2026-02-19T15:14:30</t>
         </is>
       </c>
       <c r="O143" t="inlineStr">
@@ -10260,7 +10265,7 @@
       </c>
       <c r="N144" t="inlineStr">
         <is>
-          <t>2026-02-19T12:58:56</t>
+          <t>2026-02-19T14:55:29</t>
         </is>
       </c>
       <c r="O144" t="inlineStr">
@@ -10326,7 +10331,7 @@
       </c>
       <c r="N145" t="inlineStr">
         <is>
-          <t>2026-02-19T13:13:25</t>
+          <t>2026-02-19T14:56:36</t>
         </is>
       </c>
       <c r="O145" t="inlineStr">
@@ -10392,7 +10397,7 @@
       </c>
       <c r="N146" t="inlineStr">
         <is>
-          <t>2026-02-19T13:17:23</t>
+          <t>2026-02-19T14:59:09</t>
         </is>
       </c>
       <c r="O146" t="inlineStr">
@@ -10458,7 +10463,7 @@
       </c>
       <c r="N147" t="inlineStr">
         <is>
-          <t>2026-02-19T13:07:26</t>
+          <t>2026-02-19T14:59:16</t>
         </is>
       </c>
       <c r="O147" t="inlineStr">
@@ -10524,7 +10529,7 @@
       </c>
       <c r="N148" t="inlineStr">
         <is>
-          <t>2026-02-19T13:05:57</t>
+          <t>2026-02-19T14:58:21</t>
         </is>
       </c>
       <c r="O148" t="inlineStr">
@@ -10590,7 +10595,7 @@
       </c>
       <c r="N149" t="inlineStr">
         <is>
-          <t>2026-02-19T13:08:27</t>
+          <t>2026-02-19T14:56:48</t>
         </is>
       </c>
       <c r="O149" t="inlineStr">
@@ -10656,7 +10661,7 @@
       </c>
       <c r="N150" t="inlineStr">
         <is>
-          <t>2026-02-19T13:05:48</t>
+          <t>2026-02-19T14:48:28</t>
         </is>
       </c>
       <c r="O150" t="inlineStr">
@@ -10722,7 +10727,7 @@
       </c>
       <c r="N151" t="inlineStr">
         <is>
-          <t>2026-02-19T13:00:28</t>
+          <t>2026-02-19T15:38:57</t>
         </is>
       </c>
       <c r="O151" t="inlineStr">
@@ -10788,7 +10793,7 @@
       </c>
       <c r="N152" t="inlineStr">
         <is>
-          <t>2026-02-19T12:57:35</t>
+          <t>2026-02-19T14:55:01</t>
         </is>
       </c>
       <c r="O152" t="inlineStr">
@@ -10849,7 +10854,7 @@
       </c>
       <c r="N153" t="inlineStr">
         <is>
-          <t>2026-02-18T19:39:55</t>
+          <t>2026-02-19T14:55:45</t>
         </is>
       </c>
       <c r="O153" t="inlineStr">
@@ -10915,7 +10920,7 @@
       </c>
       <c r="N154" t="inlineStr">
         <is>
-          <t>2026-02-19T13:13:16</t>
+          <t>2026-02-19T14:53:15</t>
         </is>
       </c>
       <c r="O154" t="inlineStr">
@@ -10981,7 +10986,7 @@
       </c>
       <c r="N155" t="inlineStr">
         <is>
-          <t>2026-02-19T12:55:07</t>
+          <t>2026-02-19T14:56:25</t>
         </is>
       </c>
       <c r="O155" t="inlineStr">
@@ -11113,7 +11118,7 @@
       </c>
       <c r="N157" t="inlineStr">
         <is>
-          <t>2026-02-19T12:57:26</t>
+          <t>2026-02-19T14:55:42</t>
         </is>
       </c>
       <c r="O157" t="inlineStr">
@@ -11245,7 +11250,7 @@
       </c>
       <c r="N159" t="inlineStr">
         <is>
-          <t>2026-02-19T13:16:44</t>
+          <t>2026-02-19T15:02:27</t>
         </is>
       </c>
       <c r="O159" t="inlineStr">
@@ -11443,7 +11448,7 @@
       </c>
       <c r="N162" t="inlineStr">
         <is>
-          <t>2026-02-19T13:15:07</t>
+          <t>2026-02-19T15:18:44</t>
         </is>
       </c>
       <c r="O162" t="inlineStr">
@@ -11575,7 +11580,7 @@
       </c>
       <c r="N164" t="inlineStr">
         <is>
-          <t>2026-02-19T13:28:11</t>
+          <t>2026-02-19T15:21:04</t>
         </is>
       </c>
       <c r="O164" t="inlineStr">
@@ -11641,7 +11646,7 @@
       </c>
       <c r="N165" t="inlineStr">
         <is>
-          <t>2026-02-19T13:18:48</t>
+          <t>2026-02-19T15:13:31</t>
         </is>
       </c>
       <c r="O165" t="inlineStr">
@@ -11707,7 +11712,7 @@
       </c>
       <c r="N166" t="inlineStr">
         <is>
-          <t>2026-02-19T13:10:57</t>
+          <t>2026-02-19T14:08:50</t>
         </is>
       </c>
       <c r="O166" t="inlineStr">
@@ -11773,7 +11778,7 @@
       </c>
       <c r="N167" t="inlineStr">
         <is>
-          <t>2026-02-19T13:34:14</t>
+          <t>2026-02-19T14:33:47</t>
         </is>
       </c>
       <c r="O167" t="inlineStr">
@@ -11905,7 +11910,7 @@
       </c>
       <c r="N169" t="inlineStr">
         <is>
-          <t>2026-02-19T13:22:21</t>
+          <t>2026-02-19T15:18:41</t>
         </is>
       </c>
       <c r="O169" t="inlineStr">
@@ -11971,7 +11976,7 @@
       </c>
       <c r="N170" t="inlineStr">
         <is>
-          <t>2026-02-19T13:28:36</t>
+          <t>2026-02-19T15:19:00</t>
         </is>
       </c>
       <c r="O170" t="inlineStr">
@@ -12033,7 +12038,7 @@
         </is>
       </c>
       <c r="M171" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N171" t="inlineStr">
         <is>
@@ -12103,7 +12108,7 @@
       </c>
       <c r="N172" t="inlineStr">
         <is>
-          <t>2026-02-19T13:00:25</t>
+          <t>2026-02-19T14:53:23</t>
         </is>
       </c>
       <c r="O172" t="inlineStr">
@@ -12165,11 +12170,11 @@
         </is>
       </c>
       <c r="M173" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N173" t="inlineStr">
         <is>
-          <t>2026-02-19T13:10:20</t>
+          <t>2026-02-19T14:58:15</t>
         </is>
       </c>
       <c r="O173" t="inlineStr">
@@ -12301,7 +12306,7 @@
       </c>
       <c r="N175" t="inlineStr">
         <is>
-          <t>2026-02-19T13:24:12</t>
+          <t>2026-02-19T15:13:45</t>
         </is>
       </c>
       <c r="O175" t="inlineStr">
@@ -12367,7 +12372,7 @@
       </c>
       <c r="N176" t="inlineStr">
         <is>
-          <t>2026-02-19T12:53:20</t>
+          <t>2026-02-19T15:35:28</t>
         </is>
       </c>
       <c r="O176" t="inlineStr">
@@ -12433,7 +12438,7 @@
       </c>
       <c r="N177" t="inlineStr">
         <is>
-          <t>2026-02-19T12:57:48</t>
+          <t>2026-02-19T14:52:06</t>
         </is>
       </c>
       <c r="O177" t="inlineStr">
@@ -12499,7 +12504,7 @@
       </c>
       <c r="N178" t="inlineStr">
         <is>
-          <t>2026-02-19T13:11:12</t>
+          <t>2026-02-19T14:58:56</t>
         </is>
       </c>
       <c r="O178" t="inlineStr">
@@ -12565,7 +12570,7 @@
       </c>
       <c r="N179" t="inlineStr">
         <is>
-          <t>2026-02-19T13:26:19</t>
+          <t>2026-02-19T15:13:50</t>
         </is>
       </c>
       <c r="O179" t="inlineStr">
@@ -12631,7 +12636,7 @@
       </c>
       <c r="N180" t="inlineStr">
         <is>
-          <t>2026-02-19T13:16:23</t>
+          <t>2026-02-19T14:54:46</t>
         </is>
       </c>
       <c r="O180" t="inlineStr">
@@ -12697,7 +12702,7 @@
       </c>
       <c r="N181" t="inlineStr">
         <is>
-          <t>2026-02-19T13:23:13</t>
+          <t>2026-02-19T15:16:36</t>
         </is>
       </c>
       <c r="O181" t="inlineStr">
@@ -12966,7 +12971,7 @@
       </c>
       <c r="N185" t="inlineStr">
         <is>
-          <t>2026-02-19T13:13:13</t>
+          <t>2026-02-19T15:00:06</t>
         </is>
       </c>
       <c r="O185" t="inlineStr">
@@ -13032,7 +13037,7 @@
       </c>
       <c r="N186" t="inlineStr">
         <is>
-          <t>2026-02-19T13:15:47</t>
+          <t>2026-02-19T14:11:55</t>
         </is>
       </c>
       <c r="O186" t="inlineStr">
@@ -13098,7 +13103,7 @@
       </c>
       <c r="N187" t="inlineStr">
         <is>
-          <t>2026-02-19T12:49:59</t>
+          <t>2026-02-19T15:27:07</t>
         </is>
       </c>
       <c r="O187" t="inlineStr">
@@ -13164,7 +13169,7 @@
       </c>
       <c r="N188" t="inlineStr">
         <is>
-          <t>2026-02-19T12:53:05</t>
+          <t>2026-02-19T14:50:42</t>
         </is>
       </c>
       <c r="O188" t="inlineStr">
@@ -13296,7 +13301,7 @@
       </c>
       <c r="N190" t="inlineStr">
         <is>
-          <t>2026-02-19T13:06:22</t>
+          <t>2026-02-19T14:57:39</t>
         </is>
       </c>
       <c r="O190" t="inlineStr">
@@ -13362,7 +13367,7 @@
       </c>
       <c r="N191" t="inlineStr">
         <is>
-          <t>2026-02-18T19:28:57</t>
+          <t>2026-02-19T15:19:03</t>
         </is>
       </c>
       <c r="O191" t="inlineStr">
@@ -13428,7 +13433,7 @@
       </c>
       <c r="N192" t="inlineStr">
         <is>
-          <t>2026-02-19T13:18:34</t>
+          <t>2026-02-19T15:10:39</t>
         </is>
       </c>
       <c r="O192" t="inlineStr">
@@ -13557,7 +13562,7 @@
       </c>
       <c r="N194" t="inlineStr">
         <is>
-          <t>2026-02-19T13:20:03</t>
+          <t>2026-02-19T15:12:09</t>
         </is>
       </c>
       <c r="O194" t="inlineStr">
@@ -13623,7 +13628,7 @@
       </c>
       <c r="N195" t="inlineStr">
         <is>
-          <t>2026-02-19T13:08:01</t>
+          <t>2026-02-19T15:02:43</t>
         </is>
       </c>
       <c r="O195" t="inlineStr">
@@ -13689,7 +13694,7 @@
       </c>
       <c r="N196" t="inlineStr">
         <is>
-          <t>2026-02-19T13:37:14</t>
+          <t>2026-02-19T14:56:14</t>
         </is>
       </c>
       <c r="O196" t="inlineStr">
@@ -13755,7 +13760,7 @@
       </c>
       <c r="N197" t="inlineStr">
         <is>
-          <t>2026-02-19T13:24:42</t>
+          <t>2026-02-19T15:01:06</t>
         </is>
       </c>
       <c r="O197" t="inlineStr">
@@ -13821,7 +13826,7 @@
       </c>
       <c r="N198" t="inlineStr">
         <is>
-          <t>2026-02-19T08:12:26</t>
+          <t>2026-02-19T15:35:20</t>
         </is>
       </c>
       <c r="O198" t="inlineStr">
@@ -13887,7 +13892,7 @@
       </c>
       <c r="N199" t="inlineStr">
         <is>
-          <t>2026-02-19T12:59:41</t>
+          <t>2026-02-19T14:54:07</t>
         </is>
       </c>
       <c r="O199" t="inlineStr">
@@ -13953,7 +13958,7 @@
       </c>
       <c r="N200" t="inlineStr">
         <is>
-          <t>2026-02-19T13:21:30</t>
+          <t>2026-02-19T15:09:50</t>
         </is>
       </c>
       <c r="O200" t="inlineStr">
@@ -14016,7 +14021,7 @@
       </c>
       <c r="N201" t="inlineStr">
         <is>
-          <t>2026-02-19T12:50:06</t>
+          <t>2026-02-19T15:37:25</t>
         </is>
       </c>
       <c r="O201" t="inlineStr">
@@ -14082,7 +14087,7 @@
       </c>
       <c r="N202" t="inlineStr">
         <is>
-          <t>2026-02-19T12:44:07</t>
+          <t>2026-02-19T15:07:40</t>
         </is>
       </c>
       <c r="O202" t="inlineStr">
@@ -14148,7 +14153,7 @@
       </c>
       <c r="N203" t="inlineStr">
         <is>
-          <t>2026-02-19T12:51:39</t>
+          <t>2026-02-19T15:14:20</t>
         </is>
       </c>
       <c r="O203" t="inlineStr">
@@ -14214,7 +14219,7 @@
       </c>
       <c r="N204" t="inlineStr">
         <is>
-          <t>2026-02-19T12:52:08</t>
+          <t>2026-02-19T15:36:08</t>
         </is>
       </c>
       <c r="O204" t="inlineStr">
@@ -14280,7 +14285,7 @@
       </c>
       <c r="N205" t="inlineStr">
         <is>
-          <t>2026-02-19T13:24:03</t>
+          <t>2026-02-19T15:16:37</t>
         </is>
       </c>
       <c r="O205" t="inlineStr">
@@ -14346,7 +14351,7 @@
       </c>
       <c r="N206" t="inlineStr">
         <is>
-          <t>2026-02-19T13:04:45</t>
+          <t>2026-02-19T14:54:47</t>
         </is>
       </c>
       <c r="O206" t="inlineStr">
@@ -14412,7 +14417,7 @@
       </c>
       <c r="N207" t="inlineStr">
         <is>
-          <t>2026-02-19T12:59:00</t>
+          <t>2026-02-19T15:40:01</t>
         </is>
       </c>
       <c r="O207" t="inlineStr">
@@ -14478,7 +14483,7 @@
       </c>
       <c r="N208" t="inlineStr">
         <is>
-          <t>2026-02-19T13:05:20</t>
+          <t>2026-02-19T15:37:58</t>
         </is>
       </c>
       <c r="O208" t="inlineStr">
@@ -14544,7 +14549,7 @@
       </c>
       <c r="N209" t="inlineStr">
         <is>
-          <t>2026-02-19T13:02:37</t>
+          <t>2026-02-19T14:53:32</t>
         </is>
       </c>
       <c r="O209" t="inlineStr">
@@ -14610,7 +14615,7 @@
       </c>
       <c r="N210" t="inlineStr">
         <is>
-          <t>2026-02-19T13:09:24</t>
+          <t>2026-02-19T15:02:01</t>
         </is>
       </c>
       <c r="O210" t="inlineStr">
@@ -14676,7 +14681,7 @@
       </c>
       <c r="N211" t="inlineStr">
         <is>
-          <t>2026-02-19T13:22:37</t>
+          <t>2026-02-19T14:51:38</t>
         </is>
       </c>
       <c r="O211" t="inlineStr">
@@ -14742,7 +14747,7 @@
       </c>
       <c r="N212" t="inlineStr">
         <is>
-          <t>2026-02-19T13:10:53</t>
+          <t>2026-02-19T15:10:19</t>
         </is>
       </c>
       <c r="O212" t="inlineStr">
@@ -14808,7 +14813,7 @@
       </c>
       <c r="N213" t="inlineStr">
         <is>
-          <t>2026-02-19T13:19:40</t>
+          <t>2026-02-19T14:53:20</t>
         </is>
       </c>
       <c r="O213" t="inlineStr">
@@ -14874,7 +14879,7 @@
       </c>
       <c r="N214" t="inlineStr">
         <is>
-          <t>2026-02-19T13:11:41</t>
+          <t>2026-02-19T15:05:36</t>
         </is>
       </c>
       <c r="O214" t="inlineStr">
@@ -14940,7 +14945,7 @@
       </c>
       <c r="N215" t="inlineStr">
         <is>
-          <t>2026-02-19T13:12:48</t>
+          <t>2026-02-19T14:58:46</t>
         </is>
       </c>
       <c r="O215" t="inlineStr">
@@ -15006,7 +15011,7 @@
       </c>
       <c r="N216" t="inlineStr">
         <is>
-          <t>2026-02-19T13:28:18</t>
+          <t>2026-02-19T15:23:43</t>
         </is>
       </c>
       <c r="O216" t="inlineStr">
@@ -15072,7 +15077,7 @@
       </c>
       <c r="N217" t="inlineStr">
         <is>
-          <t>2026-02-19T13:17:06</t>
+          <t>2026-02-19T15:10:05</t>
         </is>
       </c>
       <c r="O217" t="inlineStr">
@@ -15138,7 +15143,7 @@
       </c>
       <c r="N218" t="inlineStr">
         <is>
-          <t>2026-02-19T13:01:50</t>
+          <t>2026-02-19T14:53:35</t>
         </is>
       </c>
       <c r="O218" t="inlineStr">
@@ -15204,7 +15209,7 @@
       </c>
       <c r="N219" t="inlineStr">
         <is>
-          <t>2026-02-19T12:48:07</t>
+          <t>2026-02-19T15:31:28</t>
         </is>
       </c>
       <c r="O219" t="inlineStr">
@@ -15275,7 +15280,7 @@
       </c>
       <c r="N220" t="inlineStr">
         <is>
-          <t>2026-02-19T13:25:26</t>
+          <t>2026-02-19T15:19:58</t>
         </is>
       </c>
       <c r="O220" t="inlineStr">
@@ -15341,7 +15346,7 @@
       </c>
       <c r="N221" t="inlineStr">
         <is>
-          <t>2026-02-19T13:37:19</t>
+          <t>2026-02-19T15:31:48</t>
         </is>
       </c>
       <c r="O221" t="inlineStr">
@@ -15407,7 +15412,7 @@
       </c>
       <c r="N222" t="inlineStr">
         <is>
-          <t>2026-02-19T13:03:41</t>
+          <t>2026-02-19T14:55:44</t>
         </is>
       </c>
       <c r="O222" t="inlineStr">
@@ -15473,7 +15478,7 @@
       </c>
       <c r="N223" t="inlineStr">
         <is>
-          <t>2026-02-19T13:39:57</t>
+          <t>2026-02-19T14:59:57</t>
         </is>
       </c>
       <c r="O223" t="inlineStr">
@@ -15539,7 +15544,7 @@
       </c>
       <c r="N224" t="inlineStr">
         <is>
-          <t>2026-02-19T13:06:43</t>
+          <t>2026-02-19T14:59:17</t>
         </is>
       </c>
       <c r="O224" t="inlineStr">
@@ -15605,7 +15610,7 @@
       </c>
       <c r="N225" t="inlineStr">
         <is>
-          <t>2026-02-19T13:18:53</t>
+          <t>2026-02-19T14:59:17</t>
         </is>
       </c>
       <c r="O225" t="inlineStr">
@@ -15671,7 +15676,7 @@
       </c>
       <c r="N226" t="inlineStr">
         <is>
-          <t>2026-02-19T13:13:33</t>
+          <t>2026-02-19T14:58:19</t>
         </is>
       </c>
       <c r="O226" t="inlineStr">
@@ -15737,7 +15742,7 @@
       </c>
       <c r="N227" t="inlineStr">
         <is>
-          <t>2026-02-19T12:46:57</t>
+          <t>2026-02-19T15:34:31</t>
         </is>
       </c>
       <c r="O227" t="inlineStr">
@@ -15803,7 +15808,7 @@
       </c>
       <c r="N228" t="inlineStr">
         <is>
-          <t>2026-02-19T13:28:11</t>
+          <t>2026-02-19T15:18:28</t>
         </is>
       </c>
       <c r="O228" t="inlineStr">
@@ -15869,7 +15874,7 @@
       </c>
       <c r="N229" t="inlineStr">
         <is>
-          <t>2026-02-19T13:02:52</t>
+          <t>2026-02-19T14:56:39</t>
         </is>
       </c>
       <c r="O229" t="inlineStr">
@@ -15935,7 +15940,7 @@
       </c>
       <c r="N230" t="inlineStr">
         <is>
-          <t>2026-02-19T12:43:53</t>
+          <t>2026-02-19T15:00:32</t>
         </is>
       </c>
       <c r="O230" t="inlineStr">
@@ -16001,7 +16006,7 @@
       </c>
       <c r="N231" t="inlineStr">
         <is>
-          <t>2026-02-19T13:36:39</t>
+          <t>2026-02-19T15:33:35</t>
         </is>
       </c>
       <c r="O231" t="inlineStr">
@@ -16067,7 +16072,7 @@
       </c>
       <c r="N232" t="inlineStr">
         <is>
-          <t>2026-02-19T13:21:10</t>
+          <t>2026-02-19T15:12:30</t>
         </is>
       </c>
       <c r="O232" t="inlineStr">
@@ -16133,7 +16138,7 @@
       </c>
       <c r="N233" t="inlineStr">
         <is>
-          <t>2026-02-19T12:47:09</t>
+          <t>2026-02-19T15:35:26</t>
         </is>
       </c>
       <c r="O233" t="inlineStr">
@@ -16199,7 +16204,7 @@
       </c>
       <c r="N234" t="inlineStr">
         <is>
-          <t>2026-02-19T13:02:14</t>
+          <t>2026-02-19T15:01:22</t>
         </is>
       </c>
       <c r="O234" t="inlineStr">
@@ -16265,7 +16270,7 @@
       </c>
       <c r="N235" t="inlineStr">
         <is>
-          <t>2026-02-19T12:59:54</t>
+          <t>2026-02-19T14:59:11</t>
         </is>
       </c>
       <c r="O235" t="inlineStr">
@@ -16331,7 +16336,7 @@
       </c>
       <c r="N236" t="inlineStr">
         <is>
-          <t>2026-02-19T12:58:19</t>
+          <t>2026-02-19T14:51:34</t>
         </is>
       </c>
       <c r="O236" t="inlineStr">
@@ -16397,7 +16402,7 @@
       </c>
       <c r="N237" t="inlineStr">
         <is>
-          <t>2026-02-19T13:01:09</t>
+          <t>2026-02-19T14:57:16</t>
         </is>
       </c>
       <c r="O237" t="inlineStr">
@@ -16463,7 +16468,7 @@
       </c>
       <c r="N238" t="inlineStr">
         <is>
-          <t>2026-02-19T13:21:42</t>
+          <t>2026-02-19T15:13:26</t>
         </is>
       </c>
       <c r="O238" t="inlineStr">
@@ -16595,7 +16600,7 @@
       </c>
       <c r="N240" t="inlineStr">
         <is>
-          <t>2026-02-19T13:41:13</t>
+          <t>2026-02-19T15:00:52</t>
         </is>
       </c>
       <c r="O240" t="inlineStr">
@@ -16661,7 +16666,7 @@
       </c>
       <c r="N241" t="inlineStr">
         <is>
-          <t>2026-02-19T13:27:57</t>
+          <t>2026-02-19T15:31:31</t>
         </is>
       </c>
       <c r="O241" t="inlineStr">
@@ -16727,7 +16732,7 @@
       </c>
       <c r="N242" t="inlineStr">
         <is>
-          <t>2026-02-19T13:40:29</t>
+          <t>2026-02-19T15:32:46</t>
         </is>
       </c>
       <c r="O242" t="inlineStr">
@@ -16793,7 +16798,7 @@
       </c>
       <c r="N243" t="inlineStr">
         <is>
-          <t>2026-02-19T13:11:15</t>
+          <t>2026-02-19T15:07:00</t>
         </is>
       </c>
       <c r="O243" t="inlineStr">
@@ -16859,7 +16864,7 @@
       </c>
       <c r="N244" t="inlineStr">
         <is>
-          <t>2026-02-19T13:17:03</t>
+          <t>2026-02-19T15:30:57</t>
         </is>
       </c>
       <c r="O244" t="inlineStr">
@@ -16925,7 +16930,7 @@
       </c>
       <c r="N245" t="inlineStr">
         <is>
-          <t>2026-02-19T13:24:58</t>
+          <t>2026-02-19T15:23:15</t>
         </is>
       </c>
       <c r="O245" t="inlineStr">
@@ -16991,7 +16996,7 @@
       </c>
       <c r="N246" t="inlineStr">
         <is>
-          <t>2026-02-19T13:04:09</t>
+          <t>2026-02-19T15:41:57</t>
         </is>
       </c>
       <c r="O246" t="inlineStr">
@@ -17057,7 +17062,7 @@
       </c>
       <c r="N247" t="inlineStr">
         <is>
-          <t>2026-02-19T13:22:49</t>
+          <t>2026-02-19T15:03:24</t>
         </is>
       </c>
       <c r="O247" t="inlineStr">
@@ -17123,7 +17128,7 @@
       </c>
       <c r="N248" t="inlineStr">
         <is>
-          <t>2026-02-19T13:35:52</t>
+          <t>2026-02-19T15:31:37</t>
         </is>
       </c>
       <c r="O248" t="inlineStr">
@@ -17189,7 +17194,7 @@
       </c>
       <c r="N249" t="inlineStr">
         <is>
-          <t>2026-02-19T13:16:54</t>
+          <t>2026-02-19T14:08:04</t>
         </is>
       </c>
       <c r="O249" t="inlineStr">
@@ -17209,11 +17214,6 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
-      <c r="C250" t="inlineStr">
-        <is>
-          <t>10.69.5.118</t>
-        </is>
-      </c>
       <c r="D250" t="n">
         <v>2017</v>
       </c>
@@ -17255,7 +17255,7 @@
       </c>
       <c r="N250" t="inlineStr">
         <is>
-          <t>2026-02-19T13:21:56</t>
+          <t>2026-02-19T14:28:42</t>
         </is>
       </c>
       <c r="O250" t="inlineStr">
@@ -17321,7 +17321,7 @@
       </c>
       <c r="N251" t="inlineStr">
         <is>
-          <t>2026-02-19T13:28:26</t>
+          <t>2026-02-19T15:20:26</t>
         </is>
       </c>
       <c r="O251" t="inlineStr">
@@ -17387,7 +17387,7 @@
       </c>
       <c r="N252" t="inlineStr">
         <is>
-          <t>2026-02-19T13:24:51</t>
+          <t>2026-02-19T15:18:14</t>
         </is>
       </c>
       <c r="O252" t="inlineStr">
@@ -17453,7 +17453,7 @@
       </c>
       <c r="N253" t="inlineStr">
         <is>
-          <t>2026-02-19T13:27:13</t>
+          <t>2026-02-19T15:01:34</t>
         </is>
       </c>
       <c r="O253" t="inlineStr">
@@ -17513,7 +17513,7 @@
       </c>
       <c r="N254" t="inlineStr">
         <is>
-          <t>2026-02-19T13:01:44</t>
+          <t>2026-02-19T14:51:25</t>
         </is>
       </c>
       <c r="O254" t="inlineStr">
@@ -17579,7 +17579,7 @@
       </c>
       <c r="N255" t="inlineStr">
         <is>
-          <t>2026-02-19T13:31:51</t>
+          <t>2026-02-19T15:32:28</t>
         </is>
       </c>
       <c r="O255" t="inlineStr">
@@ -17645,7 +17645,7 @@
       </c>
       <c r="N256" t="inlineStr">
         <is>
-          <t>2026-02-19T12:42:23</t>
+          <t>2026-02-19T15:35:31</t>
         </is>
       </c>
       <c r="O256" t="inlineStr">
@@ -17711,7 +17711,7 @@
       </c>
       <c r="N257" t="inlineStr">
         <is>
-          <t>2026-02-19T13:06:49</t>
+          <t>2026-02-19T14:55:48</t>
         </is>
       </c>
       <c r="O257" t="inlineStr">
@@ -17777,7 +17777,7 @@
       </c>
       <c r="N258" t="inlineStr">
         <is>
-          <t>2026-02-19T12:47:58</t>
+          <t>2026-02-19T15:31:57</t>
         </is>
       </c>
       <c r="O258" t="inlineStr">
@@ -17843,7 +17843,7 @@
       </c>
       <c r="N259" t="inlineStr">
         <is>
-          <t>2026-02-19T12:57:14</t>
+          <t>2026-02-19T14:47:38</t>
         </is>
       </c>
       <c r="O259" t="inlineStr">
@@ -17909,7 +17909,7 @@
       </c>
       <c r="N260" t="inlineStr">
         <is>
-          <t>2026-02-19T13:07:02</t>
+          <t>2026-02-19T15:06:02</t>
         </is>
       </c>
       <c r="O260" t="inlineStr">
@@ -18041,7 +18041,7 @@
       </c>
       <c r="N262" t="inlineStr">
         <is>
-          <t>2026-02-19T13:16:27</t>
+          <t>2026-02-19T15:01:04</t>
         </is>
       </c>
       <c r="O262" t="inlineStr">
@@ -18107,7 +18107,7 @@
       </c>
       <c r="N263" t="inlineStr">
         <is>
-          <t>2026-02-19T13:31:14</t>
+          <t>2026-02-19T15:30:12</t>
         </is>
       </c>
       <c r="O263" t="inlineStr">
@@ -18173,7 +18173,7 @@
       </c>
       <c r="N264" t="inlineStr">
         <is>
-          <t>2026-02-19T13:16:50</t>
+          <t>2026-02-19T15:03:29</t>
         </is>
       </c>
       <c r="O264" t="inlineStr">
@@ -18239,7 +18239,7 @@
       </c>
       <c r="N265" t="inlineStr">
         <is>
-          <t>2026-02-19T13:14:11</t>
+          <t>2026-02-19T15:40:23</t>
         </is>
       </c>
       <c r="O265" t="inlineStr">
@@ -18305,7 +18305,7 @@
       </c>
       <c r="N266" t="inlineStr">
         <is>
-          <t>2026-02-19T13:08:49</t>
+          <t>2026-02-19T14:56:30</t>
         </is>
       </c>
       <c r="O266" t="inlineStr">
@@ -18371,7 +18371,7 @@
       </c>
       <c r="N267" t="inlineStr">
         <is>
-          <t>2026-02-19T12:51:39</t>
+          <t>2026-02-19T14:46:47</t>
         </is>
       </c>
       <c r="O267" t="inlineStr">
@@ -18437,7 +18437,7 @@
       </c>
       <c r="N268" t="inlineStr">
         <is>
-          <t>2026-02-19T12:51:45</t>
+          <t>2026-02-19T15:38:57</t>
         </is>
       </c>
       <c r="O268" t="inlineStr">
@@ -18503,7 +18503,7 @@
       </c>
       <c r="N269" t="inlineStr">
         <is>
-          <t>2026-02-19T13:05:26</t>
+          <t>2026-02-19T14:53:44</t>
         </is>
       </c>
       <c r="O269" t="inlineStr">
@@ -18566,7 +18566,7 @@
       </c>
       <c r="N270" t="inlineStr">
         <is>
-          <t>2026-02-19T13:18:29</t>
+          <t>2026-02-19T15:13:16</t>
         </is>
       </c>
       <c r="O270" t="inlineStr">
@@ -18698,7 +18698,7 @@
       </c>
       <c r="N272" t="inlineStr">
         <is>
-          <t>2026-02-19T13:29:07</t>
+          <t>2026-02-19T14:58:33</t>
         </is>
       </c>
       <c r="O272" t="inlineStr">
@@ -18764,7 +18764,7 @@
       </c>
       <c r="N273" t="inlineStr">
         <is>
-          <t>2026-02-19T13:19:47</t>
+          <t>2026-02-19T15:11:30</t>
         </is>
       </c>
       <c r="O273" t="inlineStr">
@@ -19094,7 +19094,7 @@
       </c>
       <c r="N278" t="inlineStr">
         <is>
-          <t>2026-02-19T13:32:17</t>
+          <t>2026-02-19T14:56:22</t>
         </is>
       </c>
       <c r="O278" t="inlineStr">
@@ -19160,7 +19160,7 @@
       </c>
       <c r="N279" t="inlineStr">
         <is>
-          <t>2026-02-19T12:58:30</t>
+          <t>2026-02-19T13:55:42</t>
         </is>
       </c>
       <c r="O279" t="inlineStr">
@@ -19226,7 +19226,7 @@
       </c>
       <c r="N280" t="inlineStr">
         <is>
-          <t>2026-02-19T12:49:12</t>
+          <t>2026-02-19T14:42:35</t>
         </is>
       </c>
       <c r="O280" t="inlineStr">
@@ -19292,7 +19292,7 @@
       </c>
       <c r="N281" t="inlineStr">
         <is>
-          <t>2026-02-19T13:05:15</t>
+          <t>2026-02-19T14:49:10</t>
         </is>
       </c>
       <c r="O281" t="inlineStr">
@@ -19353,7 +19353,7 @@
       </c>
       <c r="N282" t="inlineStr">
         <is>
-          <t>2026-02-19T13:06:05</t>
+          <t>2026-02-19T14:59:10</t>
         </is>
       </c>
       <c r="O282" t="inlineStr">
@@ -19419,7 +19419,7 @@
       </c>
       <c r="N283" t="inlineStr">
         <is>
-          <t>2026-02-19T13:06:39</t>
+          <t>2026-02-19T14:54:18</t>
         </is>
       </c>
       <c r="O283" t="inlineStr">
@@ -19485,7 +19485,7 @@
       </c>
       <c r="N284" t="inlineStr">
         <is>
-          <t>2026-02-19T13:31:47</t>
+          <t>2026-02-19T15:30:00</t>
         </is>
       </c>
       <c r="O284" t="inlineStr">
@@ -19551,7 +19551,7 @@
       </c>
       <c r="N285" t="inlineStr">
         <is>
-          <t>2026-02-19T13:16:19</t>
+          <t>2026-02-19T15:08:24</t>
         </is>
       </c>
       <c r="O285" t="inlineStr">
@@ -19612,7 +19612,7 @@
       </c>
       <c r="N286" t="inlineStr">
         <is>
-          <t>2026-02-19T08:20:24</t>
+          <t>2026-02-19T14:59:26</t>
         </is>
       </c>
       <c r="O286" t="inlineStr">
@@ -19678,7 +19678,7 @@
       </c>
       <c r="N287" t="inlineStr">
         <is>
-          <t>2026-02-19T13:36:29</t>
+          <t>2026-02-19T15:29:46</t>
         </is>
       </c>
       <c r="O287" t="inlineStr">
@@ -19810,7 +19810,7 @@
       </c>
       <c r="N289" t="inlineStr">
         <is>
-          <t>2026-02-19T12:58:03</t>
+          <t>2026-02-19T15:38:57</t>
         </is>
       </c>
       <c r="O289" t="inlineStr">
@@ -20630,7 +20630,7 @@
       </c>
       <c r="N302" t="inlineStr">
         <is>
-          <t>2026-02-19T13:12:48</t>
+          <t>2026-02-19T15:02:04</t>
         </is>
       </c>
       <c r="O302" t="inlineStr">
@@ -21782,7 +21782,7 @@
       </c>
       <c r="N320" t="inlineStr">
         <is>
-          <t>2026-02-19T13:08:39</t>
+          <t>2026-02-19T15:02:12</t>
         </is>
       </c>
       <c r="O320" t="inlineStr">
@@ -22531,7 +22531,7 @@
       </c>
       <c r="N332" t="inlineStr">
         <is>
-          <t>2026-02-19T13:34:26</t>
+          <t>2026-02-19T15:24:08</t>
         </is>
       </c>
       <c r="O332" t="inlineStr">
@@ -22597,7 +22597,7 @@
       </c>
       <c r="N333" t="inlineStr">
         <is>
-          <t>2026-02-19T13:21:35</t>
+          <t>2026-02-19T15:11:44</t>
         </is>
       </c>
       <c r="O333" t="inlineStr">
@@ -22663,7 +22663,7 @@
       </c>
       <c r="N334" t="inlineStr">
         <is>
-          <t>2026-02-19T13:11:45</t>
+          <t>2026-02-19T15:10:54</t>
         </is>
       </c>
       <c r="O334" t="inlineStr">
@@ -22729,7 +22729,7 @@
       </c>
       <c r="N335" t="inlineStr">
         <is>
-          <t>2026-02-19T13:10:47</t>
+          <t>2026-02-19T14:58:02</t>
         </is>
       </c>
       <c r="O335" t="inlineStr">
@@ -22861,7 +22861,7 @@
       </c>
       <c r="N337" t="inlineStr">
         <is>
-          <t>2026-02-19T13:32:24</t>
+          <t>2026-02-19T15:29:40</t>
         </is>
       </c>
       <c r="O337" t="inlineStr">
@@ -22927,7 +22927,7 @@
       </c>
       <c r="N338" t="inlineStr">
         <is>
-          <t>2026-02-19T12:58:14</t>
+          <t>2026-02-19T14:50:58</t>
         </is>
       </c>
       <c r="O338" t="inlineStr">
@@ -22993,7 +22993,7 @@
       </c>
       <c r="N339" t="inlineStr">
         <is>
-          <t>2026-02-19T13:15:34</t>
+          <t>2026-02-19T15:00:07</t>
         </is>
       </c>
       <c r="O339" t="inlineStr">
@@ -23125,7 +23125,7 @@
       </c>
       <c r="N341" t="inlineStr">
         <is>
-          <t>2026-02-19T12:47:27</t>
+          <t>2026-02-19T13:43:55</t>
         </is>
       </c>
       <c r="O341" t="inlineStr">
@@ -23254,7 +23254,7 @@
       </c>
       <c r="N343" t="inlineStr">
         <is>
-          <t>2026-02-19T13:12:11</t>
+          <t>2026-02-19T14:58:11</t>
         </is>
       </c>
       <c r="O343" t="inlineStr">
@@ -23518,7 +23518,7 @@
       </c>
       <c r="N347" t="inlineStr">
         <is>
-          <t>2026-02-19T13:36:54</t>
+          <t>2026-02-19T14:33:25</t>
         </is>
       </c>
       <c r="O347" t="inlineStr">
@@ -23969,7 +23969,7 @@
       </c>
       <c r="N354" t="inlineStr">
         <is>
-          <t>2026-02-19T13:25:54</t>
+          <t>2026-02-19T14:20:10</t>
         </is>
       </c>
       <c r="O354" t="inlineStr">
@@ -24035,7 +24035,7 @@
       </c>
       <c r="N355" t="inlineStr">
         <is>
-          <t>2026-02-19T13:22:33</t>
+          <t>2026-02-19T14:13:47</t>
         </is>
       </c>
       <c r="O355" t="inlineStr">
@@ -24167,7 +24167,7 @@
       </c>
       <c r="N357" t="inlineStr">
         <is>
-          <t>2026-02-19T13:31:37</t>
+          <t>2026-02-19T14:30:06</t>
         </is>
       </c>
       <c r="O357" t="inlineStr">
@@ -24360,7 +24360,7 @@
       </c>
       <c r="N360" t="inlineStr">
         <is>
-          <t>2026-02-19T13:28:22</t>
+          <t>2026-02-19T14:19:32</t>
         </is>
       </c>
       <c r="O360" t="inlineStr">
@@ -24426,7 +24426,7 @@
       </c>
       <c r="N361" t="inlineStr">
         <is>
-          <t>2026-02-19T13:37:04</t>
+          <t>2026-02-19T14:30:38</t>
         </is>
       </c>
       <c r="O361" t="inlineStr">
@@ -24489,7 +24489,7 @@
       </c>
       <c r="N362" t="inlineStr">
         <is>
-          <t>2026-02-19T13:10:34</t>
+          <t>2026-02-19T14:07:42</t>
         </is>
       </c>
       <c r="O362" t="inlineStr">
@@ -24683,7 +24683,7 @@
       </c>
       <c r="N365" t="inlineStr">
         <is>
-          <t>2026-02-19T13:29:52</t>
+          <t>2026-02-19T15:19:39</t>
         </is>
       </c>
       <c r="O365" t="inlineStr">
@@ -24751,7 +24751,7 @@
       </c>
       <c r="N366" t="inlineStr">
         <is>
-          <t>2026-02-19T13:26:38</t>
+          <t>2026-02-19T15:13:08</t>
         </is>
       </c>
       <c r="O366" t="inlineStr">
@@ -24881,7 +24881,7 @@
       </c>
       <c r="N368" t="inlineStr">
         <is>
-          <t>2026-02-19T12:44:31</t>
+          <t>2026-02-19T15:34:46</t>
         </is>
       </c>
       <c r="O368" t="inlineStr">
@@ -24949,7 +24949,7 @@
       </c>
       <c r="N369" t="inlineStr">
         <is>
-          <t>2026-02-19T13:33:12</t>
+          <t>2026-02-19T15:31:00</t>
         </is>
       </c>
       <c r="O369" t="inlineStr">
@@ -25020,7 +25020,7 @@
       </c>
       <c r="N370" t="inlineStr">
         <is>
-          <t>2026-02-19T13:20:02</t>
+          <t>2026-02-19T15:19:36</t>
         </is>
       </c>
       <c r="O370" t="inlineStr">
@@ -25091,7 +25091,7 @@
       </c>
       <c r="N371" t="inlineStr">
         <is>
-          <t>2026-02-19T13:09:20</t>
+          <t>2026-02-19T15:01:10</t>
         </is>
       </c>
       <c r="O371" t="inlineStr">
@@ -25124,7 +25124,7 @@
       </c>
       <c r="F372" t="inlineStr">
         <is>
-          <t>Microsoft Windows 11 Pro</t>
+          <t>Windows</t>
         </is>
       </c>
       <c r="G372" t="inlineStr">
@@ -25162,7 +25162,7 @@
       </c>
       <c r="N372" t="inlineStr">
         <is>
-          <t>2026-02-18T11:53:23</t>
+          <t>2026-02-19T15:30:46</t>
         </is>
       </c>
       <c r="O372" t="inlineStr">
@@ -25233,7 +25233,7 @@
       </c>
       <c r="N373" t="inlineStr">
         <is>
-          <t>2026-02-19T10:20:32</t>
+          <t>2026-02-19T15:26:51</t>
         </is>
       </c>
       <c r="O373" t="inlineStr">
@@ -25304,7 +25304,7 @@
       </c>
       <c r="N374" t="inlineStr">
         <is>
-          <t>2026-02-19T12:54:20</t>
+          <t>2026-02-19T14:46:38</t>
         </is>
       </c>
       <c r="O374" t="inlineStr">
@@ -25372,7 +25372,7 @@
       </c>
       <c r="N375" t="inlineStr">
         <is>
-          <t>2026-02-19T13:33:42</t>
+          <t>2026-02-19T15:27:29</t>
         </is>
       </c>
       <c r="O375" t="inlineStr">
@@ -25438,7 +25438,7 @@
       </c>
       <c r="N376" t="inlineStr">
         <is>
-          <t>2026-02-19T13:01:51</t>
+          <t>2026-02-19T15:01:08</t>
         </is>
       </c>
       <c r="O376" t="inlineStr">
@@ -25509,7 +25509,7 @@
       </c>
       <c r="N377" t="inlineStr">
         <is>
-          <t>2026-02-19T13:18:44</t>
+          <t>2026-02-19T15:08:43</t>
         </is>
       </c>
       <c r="O377" t="inlineStr">
@@ -25580,7 +25580,7 @@
       </c>
       <c r="N378" t="inlineStr">
         <is>
-          <t>2026-02-19T13:29:32</t>
+          <t>2026-02-19T15:20:17</t>
         </is>
       </c>
       <c r="O378" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática 2026-02-19 17:52:02.989723
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -601,7 +601,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>2026-02-19T15:17:48</t>
+          <t>2026-02-19T17:07:23</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -672,7 +672,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>2026-02-19T14:55:02</t>
+          <t>2026-02-19T17:36:44</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -743,7 +743,7 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>2026-02-19T14:55:19</t>
+          <t>2026-02-19T16:45:24</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
@@ -814,7 +814,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>2026-02-19T15:18:44</t>
+          <t>2026-02-19T16:15:27</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -1103,11 +1103,6 @@
           <t>AUDITORIO</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>10.69.3.160</t>
-        </is>
-      </c>
       <c r="D10" t="n">
         <v>2017</v>
       </c>
@@ -1149,7 +1144,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>2026-02-19T14:59:44</t>
+          <t>2026-02-19T17:40:00</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -1479,7 +1474,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>2026-02-19T14:50:13</t>
+          <t>2026-02-19T16:50:29</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
@@ -1545,7 +1540,7 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>2026-02-19T15:02:24</t>
+          <t>2026-02-19T16:45:34</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
@@ -2298,7 +2293,7 @@
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>2026-02-19T14:59:58</t>
+          <t>2026-02-19T16:54:18</t>
         </is>
       </c>
       <c r="O28" t="inlineStr">
@@ -6890,7 +6885,7 @@
       </c>
       <c r="N95" t="inlineStr">
         <is>
-          <t>2026-02-19T15:20:49</t>
+          <t>2026-02-19T17:08:33</t>
         </is>
       </c>
       <c r="O95" t="inlineStr">
@@ -6961,7 +6956,7 @@
       </c>
       <c r="N96" t="inlineStr">
         <is>
-          <t>2026-02-19T15:27:06</t>
+          <t>2026-02-19T17:14:44</t>
         </is>
       </c>
       <c r="O96" t="inlineStr">
@@ -7027,7 +7022,7 @@
       </c>
       <c r="N97" t="inlineStr">
         <is>
-          <t>2026-02-19T15:06:42</t>
+          <t>2026-02-19T15:58:02</t>
         </is>
       </c>
       <c r="O97" t="inlineStr">
@@ -7047,11 +7042,6 @@
           <t>COORDENACAO</t>
         </is>
       </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>10.69.3.94</t>
-        </is>
-      </c>
       <c r="D98" t="n">
         <v>2025</v>
       </c>
@@ -7098,7 +7088,7 @@
       </c>
       <c r="N98" t="inlineStr">
         <is>
-          <t>2026-02-19T15:27:38</t>
+          <t>2026-02-19T16:26:36</t>
         </is>
       </c>
       <c r="O98" t="inlineStr">
@@ -7169,7 +7159,7 @@
       </c>
       <c r="N99" t="inlineStr">
         <is>
-          <t>2026-02-19T15:21:19</t>
+          <t>2026-02-19T17:15:22</t>
         </is>
       </c>
       <c r="O99" t="inlineStr">
@@ -7240,7 +7230,7 @@
       </c>
       <c r="N100" t="inlineStr">
         <is>
-          <t>2026-02-19T14:55:21</t>
+          <t>2026-02-19T16:48:48</t>
         </is>
       </c>
       <c r="O100" t="inlineStr">
@@ -7311,7 +7301,7 @@
       </c>
       <c r="N101" t="inlineStr">
         <is>
-          <t>2026-02-19T15:41:57</t>
+          <t>2026-02-19T17:36:00</t>
         </is>
       </c>
       <c r="O101" t="inlineStr">
@@ -7453,7 +7443,7 @@
       </c>
       <c r="N103" t="inlineStr">
         <is>
-          <t>2026-02-19T15:33:18</t>
+          <t>2026-02-19T17:22:18</t>
         </is>
       </c>
       <c r="O103" t="inlineStr">
@@ -7718,7 +7708,7 @@
       </c>
       <c r="N107" t="inlineStr">
         <is>
-          <t>2026-02-19T15:37:21</t>
+          <t>2026-02-19T16:33:37</t>
         </is>
       </c>
       <c r="O107" t="inlineStr">
@@ -7860,7 +7850,7 @@
       </c>
       <c r="N109" t="inlineStr">
         <is>
-          <t>2026-02-19T14:50:12</t>
+          <t>2026-02-19T16:48:07</t>
         </is>
       </c>
       <c r="O109" t="inlineStr">
@@ -7931,7 +7921,7 @@
       </c>
       <c r="N110" t="inlineStr">
         <is>
-          <t>2026-02-19T15:22:19</t>
+          <t>2026-02-19T17:16:15</t>
         </is>
       </c>
       <c r="O110" t="inlineStr">
@@ -8002,7 +7992,7 @@
       </c>
       <c r="N111" t="inlineStr">
         <is>
-          <t>2026-02-19T15:17:27</t>
+          <t>2026-02-19T17:06:28</t>
         </is>
       </c>
       <c r="O111" t="inlineStr">
@@ -8073,7 +8063,7 @@
       </c>
       <c r="N112" t="inlineStr">
         <is>
-          <t>2026-02-19T15:05:45</t>
+          <t>2026-02-19T16:56:57</t>
         </is>
       </c>
       <c r="O112" t="inlineStr">
@@ -8144,7 +8134,7 @@
       </c>
       <c r="N113" t="inlineStr">
         <is>
-          <t>2026-02-19T14:48:43</t>
+          <t>2026-02-19T16:49:11</t>
         </is>
       </c>
       <c r="O113" t="inlineStr">
@@ -8215,7 +8205,7 @@
       </c>
       <c r="N114" t="inlineStr">
         <is>
-          <t>2026-02-19T14:52:15</t>
+          <t>2026-02-19T16:49:36</t>
         </is>
       </c>
       <c r="O114" t="inlineStr">
@@ -8283,7 +8273,7 @@
       </c>
       <c r="N115" t="inlineStr">
         <is>
-          <t>2026-02-19T14:49:28</t>
+          <t>2026-02-19T16:42:31</t>
         </is>
       </c>
       <c r="O115" t="inlineStr">
@@ -8354,7 +8344,7 @@
       </c>
       <c r="N116" t="inlineStr">
         <is>
-          <t>2026-02-19T14:54:52</t>
+          <t>2026-02-19T16:40:55</t>
         </is>
       </c>
       <c r="O116" t="inlineStr">
@@ -8420,7 +8410,7 @@
       </c>
       <c r="N117" t="inlineStr">
         <is>
-          <t>2026-02-19T15:07:23</t>
+          <t>2026-02-19T16:54:41</t>
         </is>
       </c>
       <c r="O117" t="inlineStr">
@@ -8630,7 +8620,7 @@
       </c>
       <c r="N120" t="inlineStr">
         <is>
-          <t>2026-02-19T15:34:56</t>
+          <t>2026-02-19T17:26:58</t>
         </is>
       </c>
       <c r="O120" t="inlineStr">
@@ -8701,7 +8691,7 @@
       </c>
       <c r="N121" t="inlineStr">
         <is>
-          <t>2026-02-19T14:59:22</t>
+          <t>2026-02-19T16:51:14</t>
         </is>
       </c>
       <c r="O121" t="inlineStr">
@@ -8769,7 +8759,7 @@
       </c>
       <c r="N122" t="inlineStr">
         <is>
-          <t>2026-02-19T15:03:28</t>
+          <t>2026-02-19T16:57:37</t>
         </is>
       </c>
       <c r="O122" t="inlineStr">
@@ -8840,7 +8830,7 @@
       </c>
       <c r="N123" t="inlineStr">
         <is>
-          <t>2026-02-19T15:27:26</t>
+          <t>2026-02-19T17:07:09</t>
         </is>
       </c>
       <c r="O123" t="inlineStr">
@@ -8911,7 +8901,7 @@
       </c>
       <c r="N124" t="inlineStr">
         <is>
-          <t>2026-02-19T15:01:58</t>
+          <t>2026-02-19T16:57:18</t>
         </is>
       </c>
       <c r="O124" t="inlineStr">
@@ -9053,7 +9043,7 @@
       </c>
       <c r="N126" t="inlineStr">
         <is>
-          <t>2026-02-19T15:33:10</t>
+          <t>2026-02-19T17:27:00</t>
         </is>
       </c>
       <c r="O126" t="inlineStr">
@@ -9124,7 +9114,7 @@
       </c>
       <c r="N127" t="inlineStr">
         <is>
-          <t>2026-02-19T14:51:08</t>
+          <t>2026-02-19T16:43:56</t>
         </is>
       </c>
       <c r="O127" t="inlineStr">
@@ -9195,7 +9185,7 @@
       </c>
       <c r="N128" t="inlineStr">
         <is>
-          <t>2026-02-19T15:20:22</t>
+          <t>2026-02-19T17:07:51</t>
         </is>
       </c>
       <c r="O128" t="inlineStr">
@@ -9266,7 +9256,7 @@
       </c>
       <c r="N129" t="inlineStr">
         <is>
-          <t>2026-02-19T14:57:45</t>
+          <t>2026-02-19T17:38:35</t>
         </is>
       </c>
       <c r="O129" t="inlineStr">
@@ -9337,7 +9327,7 @@
       </c>
       <c r="N130" t="inlineStr">
         <is>
-          <t>2026-02-19T14:46:01</t>
+          <t>2026-02-19T16:41:45</t>
         </is>
       </c>
       <c r="O130" t="inlineStr">
@@ -9403,7 +9393,7 @@
       </c>
       <c r="N131" t="inlineStr">
         <is>
-          <t>2026-02-19T15:10:50</t>
+          <t>2026-02-19T16:10:36</t>
         </is>
       </c>
       <c r="O131" t="inlineStr">
@@ -9540,7 +9530,7 @@
       </c>
       <c r="N133" t="inlineStr">
         <is>
-          <t>2026-02-19T15:26:40</t>
+          <t>2026-02-19T17:22:45</t>
         </is>
       </c>
       <c r="O133" t="inlineStr">
@@ -9606,7 +9596,7 @@
       </c>
       <c r="N134" t="inlineStr">
         <is>
-          <t>2026-02-19T14:58:24</t>
+          <t>2026-02-19T16:57:03</t>
         </is>
       </c>
       <c r="O134" t="inlineStr">
@@ -9672,7 +9662,7 @@
       </c>
       <c r="N135" t="inlineStr">
         <is>
-          <t>2026-02-19T15:24:59</t>
+          <t>2026-02-19T17:13:22</t>
         </is>
       </c>
       <c r="O135" t="inlineStr">
@@ -9869,7 +9859,7 @@
       </c>
       <c r="N138" t="inlineStr">
         <is>
-          <t>2026-02-19T15:25:19</t>
+          <t>2026-02-19T17:15:15</t>
         </is>
       </c>
       <c r="O138" t="inlineStr">
@@ -9935,7 +9925,7 @@
       </c>
       <c r="N139" t="inlineStr">
         <is>
-          <t>2026-02-19T14:53:54</t>
+          <t>2026-02-19T16:44:19</t>
         </is>
       </c>
       <c r="O139" t="inlineStr">
@@ -10001,7 +9991,7 @@
       </c>
       <c r="N140" t="inlineStr">
         <is>
-          <t>2026-02-19T15:32:08</t>
+          <t>2026-02-19T17:20:26</t>
         </is>
       </c>
       <c r="O140" t="inlineStr">
@@ -10067,7 +10057,7 @@
       </c>
       <c r="N141" t="inlineStr">
         <is>
-          <t>2026-02-19T14:53:30</t>
+          <t>2026-02-19T17:39:07</t>
         </is>
       </c>
       <c r="O141" t="inlineStr">
@@ -10133,7 +10123,7 @@
       </c>
       <c r="N142" t="inlineStr">
         <is>
-          <t>2026-02-19T15:36:31</t>
+          <t>2026-02-19T17:22:31</t>
         </is>
       </c>
       <c r="O142" t="inlineStr">
@@ -10199,7 +10189,7 @@
       </c>
       <c r="N143" t="inlineStr">
         <is>
-          <t>2026-02-19T15:14:30</t>
+          <t>2026-02-19T17:02:54</t>
         </is>
       </c>
       <c r="O143" t="inlineStr">
@@ -10265,7 +10255,7 @@
       </c>
       <c r="N144" t="inlineStr">
         <is>
-          <t>2026-02-19T14:55:29</t>
+          <t>2026-02-19T17:41:45</t>
         </is>
       </c>
       <c r="O144" t="inlineStr">
@@ -10331,7 +10321,7 @@
       </c>
       <c r="N145" t="inlineStr">
         <is>
-          <t>2026-02-19T14:56:36</t>
+          <t>2026-02-19T17:41:33</t>
         </is>
       </c>
       <c r="O145" t="inlineStr">
@@ -10397,7 +10387,7 @@
       </c>
       <c r="N146" t="inlineStr">
         <is>
-          <t>2026-02-19T14:59:09</t>
+          <t>2026-02-19T16:53:53</t>
         </is>
       </c>
       <c r="O146" t="inlineStr">
@@ -10463,7 +10453,7 @@
       </c>
       <c r="N147" t="inlineStr">
         <is>
-          <t>2026-02-19T14:59:16</t>
+          <t>2026-02-19T16:48:45</t>
         </is>
       </c>
       <c r="O147" t="inlineStr">
@@ -10529,7 +10519,7 @@
       </c>
       <c r="N148" t="inlineStr">
         <is>
-          <t>2026-02-19T14:58:21</t>
+          <t>2026-02-19T16:47:13</t>
         </is>
       </c>
       <c r="O148" t="inlineStr">
@@ -10595,7 +10585,7 @@
       </c>
       <c r="N149" t="inlineStr">
         <is>
-          <t>2026-02-19T14:56:48</t>
+          <t>2026-02-19T17:38:20</t>
         </is>
       </c>
       <c r="O149" t="inlineStr">
@@ -10661,7 +10651,7 @@
       </c>
       <c r="N150" t="inlineStr">
         <is>
-          <t>2026-02-19T14:48:28</t>
+          <t>2026-02-19T17:36:49</t>
         </is>
       </c>
       <c r="O150" t="inlineStr">
@@ -10727,7 +10717,7 @@
       </c>
       <c r="N151" t="inlineStr">
         <is>
-          <t>2026-02-19T15:38:57</t>
+          <t>2026-02-19T17:30:52</t>
         </is>
       </c>
       <c r="O151" t="inlineStr">
@@ -10793,7 +10783,7 @@
       </c>
       <c r="N152" t="inlineStr">
         <is>
-          <t>2026-02-19T14:55:01</t>
+          <t>2026-02-19T16:48:36</t>
         </is>
       </c>
       <c r="O152" t="inlineStr">
@@ -10854,7 +10844,7 @@
       </c>
       <c r="N153" t="inlineStr">
         <is>
-          <t>2026-02-19T14:55:45</t>
+          <t>2026-02-19T16:44:22</t>
         </is>
       </c>
       <c r="O153" t="inlineStr">
@@ -10920,7 +10910,7 @@
       </c>
       <c r="N154" t="inlineStr">
         <is>
-          <t>2026-02-19T14:53:15</t>
+          <t>2026-02-19T17:39:15</t>
         </is>
       </c>
       <c r="O154" t="inlineStr">
@@ -10986,7 +10976,7 @@
       </c>
       <c r="N155" t="inlineStr">
         <is>
-          <t>2026-02-19T14:56:25</t>
+          <t>2026-02-19T17:36:35</t>
         </is>
       </c>
       <c r="O155" t="inlineStr">
@@ -11118,7 +11108,7 @@
       </c>
       <c r="N157" t="inlineStr">
         <is>
-          <t>2026-02-19T14:55:42</t>
+          <t>2026-02-19T17:41:46</t>
         </is>
       </c>
       <c r="O157" t="inlineStr">
@@ -11250,7 +11240,7 @@
       </c>
       <c r="N159" t="inlineStr">
         <is>
-          <t>2026-02-19T15:02:27</t>
+          <t>2026-02-19T16:54:52</t>
         </is>
       </c>
       <c r="O159" t="inlineStr">
@@ -11448,7 +11438,7 @@
       </c>
       <c r="N162" t="inlineStr">
         <is>
-          <t>2026-02-19T15:18:44</t>
+          <t>2026-02-19T17:08:08</t>
         </is>
       </c>
       <c r="O162" t="inlineStr">
@@ -11580,7 +11570,7 @@
       </c>
       <c r="N164" t="inlineStr">
         <is>
-          <t>2026-02-19T15:21:04</t>
+          <t>2026-02-19T17:13:00</t>
         </is>
       </c>
       <c r="O164" t="inlineStr">
@@ -11646,7 +11636,7 @@
       </c>
       <c r="N165" t="inlineStr">
         <is>
-          <t>2026-02-19T15:13:31</t>
+          <t>2026-02-19T16:10:37</t>
         </is>
       </c>
       <c r="O165" t="inlineStr">
@@ -11910,7 +11900,7 @@
       </c>
       <c r="N169" t="inlineStr">
         <is>
-          <t>2026-02-19T15:18:41</t>
+          <t>2026-02-19T17:17:23</t>
         </is>
       </c>
       <c r="O169" t="inlineStr">
@@ -11976,7 +11966,7 @@
       </c>
       <c r="N170" t="inlineStr">
         <is>
-          <t>2026-02-19T15:19:00</t>
+          <t>2026-02-19T17:08:46</t>
         </is>
       </c>
       <c r="O170" t="inlineStr">
@@ -12108,7 +12098,7 @@
       </c>
       <c r="N172" t="inlineStr">
         <is>
-          <t>2026-02-19T14:53:23</t>
+          <t>2026-02-19T17:39:40</t>
         </is>
       </c>
       <c r="O172" t="inlineStr">
@@ -12174,7 +12164,7 @@
       </c>
       <c r="N173" t="inlineStr">
         <is>
-          <t>2026-02-19T14:58:15</t>
+          <t>2026-02-19T16:56:31</t>
         </is>
       </c>
       <c r="O173" t="inlineStr">
@@ -12306,7 +12296,7 @@
       </c>
       <c r="N175" t="inlineStr">
         <is>
-          <t>2026-02-19T15:13:45</t>
+          <t>2026-02-19T17:05:11</t>
         </is>
       </c>
       <c r="O175" t="inlineStr">
@@ -12438,7 +12428,7 @@
       </c>
       <c r="N177" t="inlineStr">
         <is>
-          <t>2026-02-19T14:52:06</t>
+          <t>2026-02-19T16:38:03</t>
         </is>
       </c>
       <c r="O177" t="inlineStr">
@@ -12504,7 +12494,7 @@
       </c>
       <c r="N178" t="inlineStr">
         <is>
-          <t>2026-02-19T14:58:56</t>
+          <t>2026-02-19T17:40:05</t>
         </is>
       </c>
       <c r="O178" t="inlineStr">
@@ -12570,7 +12560,7 @@
       </c>
       <c r="N179" t="inlineStr">
         <is>
-          <t>2026-02-19T15:13:50</t>
+          <t>2026-02-19T17:03:26</t>
         </is>
       </c>
       <c r="O179" t="inlineStr">
@@ -12636,7 +12626,7 @@
       </c>
       <c r="N180" t="inlineStr">
         <is>
-          <t>2026-02-19T14:54:46</t>
+          <t>2026-02-19T16:49:57</t>
         </is>
       </c>
       <c r="O180" t="inlineStr">
@@ -12702,7 +12692,7 @@
       </c>
       <c r="N181" t="inlineStr">
         <is>
-          <t>2026-02-19T15:16:36</t>
+          <t>2026-02-19T17:05:16</t>
         </is>
       </c>
       <c r="O181" t="inlineStr">
@@ -12905,7 +12895,7 @@
       </c>
       <c r="N184" t="inlineStr">
         <is>
-          <t>2026-02-13T13:41:42</t>
+          <t>2026-02-19T17:38:48</t>
         </is>
       </c>
       <c r="O184" t="inlineStr">
@@ -12971,7 +12961,7 @@
       </c>
       <c r="N185" t="inlineStr">
         <is>
-          <t>2026-02-19T15:00:06</t>
+          <t>2026-02-19T17:38:31</t>
         </is>
       </c>
       <c r="O185" t="inlineStr">
@@ -13037,7 +13027,7 @@
       </c>
       <c r="N186" t="inlineStr">
         <is>
-          <t>2026-02-19T14:11:55</t>
+          <t>2026-02-19T15:57:20</t>
         </is>
       </c>
       <c r="O186" t="inlineStr">
@@ -13103,7 +13093,7 @@
       </c>
       <c r="N187" t="inlineStr">
         <is>
-          <t>2026-02-19T15:27:07</t>
+          <t>2026-02-19T17:38:31</t>
         </is>
       </c>
       <c r="O187" t="inlineStr">
@@ -13169,7 +13159,7 @@
       </c>
       <c r="N188" t="inlineStr">
         <is>
-          <t>2026-02-19T14:50:42</t>
+          <t>2026-02-19T15:48:14</t>
         </is>
       </c>
       <c r="O188" t="inlineStr">
@@ -13301,7 +13291,7 @@
       </c>
       <c r="N190" t="inlineStr">
         <is>
-          <t>2026-02-19T14:57:39</t>
+          <t>2026-02-19T16:53:32</t>
         </is>
       </c>
       <c r="O190" t="inlineStr">
@@ -13367,7 +13357,7 @@
       </c>
       <c r="N191" t="inlineStr">
         <is>
-          <t>2026-02-19T15:19:03</t>
+          <t>2026-02-19T17:11:09</t>
         </is>
       </c>
       <c r="O191" t="inlineStr">
@@ -13433,7 +13423,7 @@
       </c>
       <c r="N192" t="inlineStr">
         <is>
-          <t>2026-02-19T15:10:39</t>
+          <t>2026-02-19T16:57:24</t>
         </is>
       </c>
       <c r="O192" t="inlineStr">
@@ -13562,7 +13552,7 @@
       </c>
       <c r="N194" t="inlineStr">
         <is>
-          <t>2026-02-19T15:12:09</t>
+          <t>2026-02-19T16:58:09</t>
         </is>
       </c>
       <c r="O194" t="inlineStr">
@@ -13628,7 +13618,7 @@
       </c>
       <c r="N195" t="inlineStr">
         <is>
-          <t>2026-02-19T15:02:43</t>
+          <t>2026-02-19T16:55:45</t>
         </is>
       </c>
       <c r="O195" t="inlineStr">
@@ -13694,7 +13684,7 @@
       </c>
       <c r="N196" t="inlineStr">
         <is>
-          <t>2026-02-19T14:56:14</t>
+          <t>2026-02-19T17:42:07</t>
         </is>
       </c>
       <c r="O196" t="inlineStr">
@@ -13760,7 +13750,7 @@
       </c>
       <c r="N197" t="inlineStr">
         <is>
-          <t>2026-02-19T15:01:06</t>
+          <t>2026-02-19T16:51:06</t>
         </is>
       </c>
       <c r="O197" t="inlineStr">
@@ -13826,7 +13816,7 @@
       </c>
       <c r="N198" t="inlineStr">
         <is>
-          <t>2026-02-19T15:35:20</t>
+          <t>2026-02-19T17:24:10</t>
         </is>
       </c>
       <c r="O198" t="inlineStr">
@@ -13892,7 +13882,7 @@
       </c>
       <c r="N199" t="inlineStr">
         <is>
-          <t>2026-02-19T14:54:07</t>
+          <t>2026-02-19T17:40:10</t>
         </is>
       </c>
       <c r="O199" t="inlineStr">
@@ -13958,7 +13948,7 @@
       </c>
       <c r="N200" t="inlineStr">
         <is>
-          <t>2026-02-19T15:09:50</t>
+          <t>2026-02-19T16:55:07</t>
         </is>
       </c>
       <c r="O200" t="inlineStr">
@@ -14021,7 +14011,7 @@
       </c>
       <c r="N201" t="inlineStr">
         <is>
-          <t>2026-02-19T15:37:25</t>
+          <t>2026-02-19T17:25:54</t>
         </is>
       </c>
       <c r="O201" t="inlineStr">
@@ -14087,7 +14077,7 @@
       </c>
       <c r="N202" t="inlineStr">
         <is>
-          <t>2026-02-19T15:07:40</t>
+          <t>2026-02-19T16:54:10</t>
         </is>
       </c>
       <c r="O202" t="inlineStr">
@@ -14153,7 +14143,7 @@
       </c>
       <c r="N203" t="inlineStr">
         <is>
-          <t>2026-02-19T15:14:20</t>
+          <t>2026-02-19T17:03:01</t>
         </is>
       </c>
       <c r="O203" t="inlineStr">
@@ -14219,7 +14209,7 @@
       </c>
       <c r="N204" t="inlineStr">
         <is>
-          <t>2026-02-19T15:36:08</t>
+          <t>2026-02-19T17:24:46</t>
         </is>
       </c>
       <c r="O204" t="inlineStr">
@@ -14285,7 +14275,7 @@
       </c>
       <c r="N205" t="inlineStr">
         <is>
-          <t>2026-02-19T15:16:37</t>
+          <t>2026-02-19T17:13:52</t>
         </is>
       </c>
       <c r="O205" t="inlineStr">
@@ -14351,7 +14341,7 @@
       </c>
       <c r="N206" t="inlineStr">
         <is>
-          <t>2026-02-19T14:54:47</t>
+          <t>2026-02-19T16:53:03</t>
         </is>
       </c>
       <c r="O206" t="inlineStr">
@@ -14417,7 +14407,7 @@
       </c>
       <c r="N207" t="inlineStr">
         <is>
-          <t>2026-02-19T15:40:01</t>
+          <t>2026-02-19T17:30:13</t>
         </is>
       </c>
       <c r="O207" t="inlineStr">
@@ -14483,7 +14473,7 @@
       </c>
       <c r="N208" t="inlineStr">
         <is>
-          <t>2026-02-19T15:37:58</t>
+          <t>2026-02-19T17:34:14</t>
         </is>
       </c>
       <c r="O208" t="inlineStr">
@@ -14549,7 +14539,7 @@
       </c>
       <c r="N209" t="inlineStr">
         <is>
-          <t>2026-02-19T14:53:32</t>
+          <t>2026-02-19T17:36:45</t>
         </is>
       </c>
       <c r="O209" t="inlineStr">
@@ -14615,7 +14605,7 @@
       </c>
       <c r="N210" t="inlineStr">
         <is>
-          <t>2026-02-19T15:02:01</t>
+          <t>2026-02-19T16:56:09</t>
         </is>
       </c>
       <c r="O210" t="inlineStr">
@@ -14681,7 +14671,7 @@
       </c>
       <c r="N211" t="inlineStr">
         <is>
-          <t>2026-02-19T14:51:38</t>
+          <t>2026-02-19T16:51:26</t>
         </is>
       </c>
       <c r="O211" t="inlineStr">
@@ -14747,7 +14737,7 @@
       </c>
       <c r="N212" t="inlineStr">
         <is>
-          <t>2026-02-19T15:10:19</t>
+          <t>2026-02-19T16:58:05</t>
         </is>
       </c>
       <c r="O212" t="inlineStr">
@@ -14813,7 +14803,7 @@
       </c>
       <c r="N213" t="inlineStr">
         <is>
-          <t>2026-02-19T14:53:20</t>
+          <t>2026-02-19T16:50:10</t>
         </is>
       </c>
       <c r="O213" t="inlineStr">
@@ -14879,7 +14869,7 @@
       </c>
       <c r="N214" t="inlineStr">
         <is>
-          <t>2026-02-19T15:05:36</t>
+          <t>2026-02-19T16:59:19</t>
         </is>
       </c>
       <c r="O214" t="inlineStr">
@@ -14945,7 +14935,7 @@
       </c>
       <c r="N215" t="inlineStr">
         <is>
-          <t>2026-02-19T14:58:46</t>
+          <t>2026-02-19T16:46:10</t>
         </is>
       </c>
       <c r="O215" t="inlineStr">
@@ -15011,7 +15001,7 @@
       </c>
       <c r="N216" t="inlineStr">
         <is>
-          <t>2026-02-19T15:23:43</t>
+          <t>2026-02-19T17:16:15</t>
         </is>
       </c>
       <c r="O216" t="inlineStr">
@@ -15077,7 +15067,7 @@
       </c>
       <c r="N217" t="inlineStr">
         <is>
-          <t>2026-02-19T15:10:05</t>
+          <t>2026-02-19T17:06:09</t>
         </is>
       </c>
       <c r="O217" t="inlineStr">
@@ -15143,7 +15133,7 @@
       </c>
       <c r="N218" t="inlineStr">
         <is>
-          <t>2026-02-19T14:53:35</t>
+          <t>2026-02-19T17:39:52</t>
         </is>
       </c>
       <c r="O218" t="inlineStr">
@@ -15209,7 +15199,7 @@
       </c>
       <c r="N219" t="inlineStr">
         <is>
-          <t>2026-02-19T15:31:28</t>
+          <t>2026-02-19T17:27:36</t>
         </is>
       </c>
       <c r="O219" t="inlineStr">
@@ -15280,7 +15270,7 @@
       </c>
       <c r="N220" t="inlineStr">
         <is>
-          <t>2026-02-19T15:19:58</t>
+          <t>2026-02-19T17:07:31</t>
         </is>
       </c>
       <c r="O220" t="inlineStr">
@@ -15412,7 +15402,7 @@
       </c>
       <c r="N222" t="inlineStr">
         <is>
-          <t>2026-02-19T14:55:44</t>
+          <t>2026-02-19T17:01:00</t>
         </is>
       </c>
       <c r="O222" t="inlineStr">
@@ -15478,7 +15468,7 @@
       </c>
       <c r="N223" t="inlineStr">
         <is>
-          <t>2026-02-19T14:59:57</t>
+          <t>2026-02-19T16:56:54</t>
         </is>
       </c>
       <c r="O223" t="inlineStr">
@@ -15544,7 +15534,7 @@
       </c>
       <c r="N224" t="inlineStr">
         <is>
-          <t>2026-02-19T14:59:17</t>
+          <t>2026-02-19T17:07:57</t>
         </is>
       </c>
       <c r="O224" t="inlineStr">
@@ -15610,7 +15600,7 @@
       </c>
       <c r="N225" t="inlineStr">
         <is>
-          <t>2026-02-19T14:59:17</t>
+          <t>2026-02-19T17:29:36</t>
         </is>
       </c>
       <c r="O225" t="inlineStr">
@@ -15676,7 +15666,7 @@
       </c>
       <c r="N226" t="inlineStr">
         <is>
-          <t>2026-02-19T14:58:19</t>
+          <t>2026-02-19T16:53:18</t>
         </is>
       </c>
       <c r="O226" t="inlineStr">
@@ -15742,7 +15732,7 @@
       </c>
       <c r="N227" t="inlineStr">
         <is>
-          <t>2026-02-19T15:34:31</t>
+          <t>2026-02-19T17:18:12</t>
         </is>
       </c>
       <c r="O227" t="inlineStr">
@@ -15808,7 +15798,7 @@
       </c>
       <c r="N228" t="inlineStr">
         <is>
-          <t>2026-02-19T15:18:28</t>
+          <t>2026-02-19T17:14:57</t>
         </is>
       </c>
       <c r="O228" t="inlineStr">
@@ -15874,7 +15864,7 @@
       </c>
       <c r="N229" t="inlineStr">
         <is>
-          <t>2026-02-19T14:56:39</t>
+          <t>2026-02-19T17:39:24</t>
         </is>
       </c>
       <c r="O229" t="inlineStr">
@@ -15940,7 +15930,7 @@
       </c>
       <c r="N230" t="inlineStr">
         <is>
-          <t>2026-02-19T15:00:32</t>
+          <t>2026-02-19T16:58:18</t>
         </is>
       </c>
       <c r="O230" t="inlineStr">
@@ -16006,7 +15996,7 @@
       </c>
       <c r="N231" t="inlineStr">
         <is>
-          <t>2026-02-19T15:33:35</t>
+          <t>2026-02-19T17:23:54</t>
         </is>
       </c>
       <c r="O231" t="inlineStr">
@@ -16072,7 +16062,7 @@
       </c>
       <c r="N232" t="inlineStr">
         <is>
-          <t>2026-02-19T15:12:30</t>
+          <t>2026-02-19T17:09:30</t>
         </is>
       </c>
       <c r="O232" t="inlineStr">
@@ -16138,7 +16128,7 @@
       </c>
       <c r="N233" t="inlineStr">
         <is>
-          <t>2026-02-19T15:35:26</t>
+          <t>2026-02-19T17:30:20</t>
         </is>
       </c>
       <c r="O233" t="inlineStr">
@@ -16204,7 +16194,7 @@
       </c>
       <c r="N234" t="inlineStr">
         <is>
-          <t>2026-02-19T15:01:22</t>
+          <t>2026-02-19T16:49:00</t>
         </is>
       </c>
       <c r="O234" t="inlineStr">
@@ -16270,7 +16260,7 @@
       </c>
       <c r="N235" t="inlineStr">
         <is>
-          <t>2026-02-19T14:59:11</t>
+          <t>2026-02-19T16:49:21</t>
         </is>
       </c>
       <c r="O235" t="inlineStr">
@@ -16336,7 +16326,7 @@
       </c>
       <c r="N236" t="inlineStr">
         <is>
-          <t>2026-02-19T14:51:34</t>
+          <t>2026-02-19T17:40:31</t>
         </is>
       </c>
       <c r="O236" t="inlineStr">
@@ -16402,7 +16392,7 @@
       </c>
       <c r="N237" t="inlineStr">
         <is>
-          <t>2026-02-19T14:57:16</t>
+          <t>2026-02-19T16:51:27</t>
         </is>
       </c>
       <c r="O237" t="inlineStr">
@@ -16468,7 +16458,7 @@
       </c>
       <c r="N238" t="inlineStr">
         <is>
-          <t>2026-02-19T15:13:26</t>
+          <t>2026-02-19T16:56:25</t>
         </is>
       </c>
       <c r="O238" t="inlineStr">
@@ -16534,7 +16524,7 @@
       </c>
       <c r="N239" t="inlineStr">
         <is>
-          <t>2026-02-19T13:25:40</t>
+          <t>2026-02-19T17:17:12</t>
         </is>
       </c>
       <c r="O239" t="inlineStr">
@@ -16600,7 +16590,7 @@
       </c>
       <c r="N240" t="inlineStr">
         <is>
-          <t>2026-02-19T15:00:52</t>
+          <t>2026-02-19T16:55:47</t>
         </is>
       </c>
       <c r="O240" t="inlineStr">
@@ -16666,7 +16656,7 @@
       </c>
       <c r="N241" t="inlineStr">
         <is>
-          <t>2026-02-19T15:31:31</t>
+          <t>2026-02-19T17:29:38</t>
         </is>
       </c>
       <c r="O241" t="inlineStr">
@@ -16732,7 +16722,7 @@
       </c>
       <c r="N242" t="inlineStr">
         <is>
-          <t>2026-02-19T15:32:46</t>
+          <t>2026-02-19T17:27:01</t>
         </is>
       </c>
       <c r="O242" t="inlineStr">
@@ -16798,7 +16788,7 @@
       </c>
       <c r="N243" t="inlineStr">
         <is>
-          <t>2026-02-19T15:07:00</t>
+          <t>2026-02-19T16:58:33</t>
         </is>
       </c>
       <c r="O243" t="inlineStr">
@@ -16864,7 +16854,7 @@
       </c>
       <c r="N244" t="inlineStr">
         <is>
-          <t>2026-02-19T15:30:57</t>
+          <t>2026-02-19T17:20:58</t>
         </is>
       </c>
       <c r="O244" t="inlineStr">
@@ -16930,7 +16920,7 @@
       </c>
       <c r="N245" t="inlineStr">
         <is>
-          <t>2026-02-19T15:23:15</t>
+          <t>2026-02-19T17:10:09</t>
         </is>
       </c>
       <c r="O245" t="inlineStr">
@@ -16996,7 +16986,7 @@
       </c>
       <c r="N246" t="inlineStr">
         <is>
-          <t>2026-02-19T15:41:57</t>
+          <t>2026-02-19T17:31:54</t>
         </is>
       </c>
       <c r="O246" t="inlineStr">
@@ -17062,7 +17052,7 @@
       </c>
       <c r="N247" t="inlineStr">
         <is>
-          <t>2026-02-19T15:03:24</t>
+          <t>2026-02-19T16:54:41</t>
         </is>
       </c>
       <c r="O247" t="inlineStr">
@@ -17128,7 +17118,7 @@
       </c>
       <c r="N248" t="inlineStr">
         <is>
-          <t>2026-02-19T15:31:37</t>
+          <t>2026-02-19T17:27:40</t>
         </is>
       </c>
       <c r="O248" t="inlineStr">
@@ -17321,7 +17311,7 @@
       </c>
       <c r="N251" t="inlineStr">
         <is>
-          <t>2026-02-19T15:20:26</t>
+          <t>2026-02-19T17:12:31</t>
         </is>
       </c>
       <c r="O251" t="inlineStr">
@@ -17387,7 +17377,7 @@
       </c>
       <c r="N252" t="inlineStr">
         <is>
-          <t>2026-02-19T15:18:14</t>
+          <t>2026-02-19T17:12:02</t>
         </is>
       </c>
       <c r="O252" t="inlineStr">
@@ -17453,7 +17443,7 @@
       </c>
       <c r="N253" t="inlineStr">
         <is>
-          <t>2026-02-19T15:01:34</t>
+          <t>2026-02-19T16:58:06</t>
         </is>
       </c>
       <c r="O253" t="inlineStr">
@@ -17513,7 +17503,7 @@
       </c>
       <c r="N254" t="inlineStr">
         <is>
-          <t>2026-02-19T14:51:25</t>
+          <t>2026-02-19T16:48:35</t>
         </is>
       </c>
       <c r="O254" t="inlineStr">
@@ -17579,7 +17569,7 @@
       </c>
       <c r="N255" t="inlineStr">
         <is>
-          <t>2026-02-19T15:32:28</t>
+          <t>2026-02-19T17:23:05</t>
         </is>
       </c>
       <c r="O255" t="inlineStr">
@@ -17645,7 +17635,7 @@
       </c>
       <c r="N256" t="inlineStr">
         <is>
-          <t>2026-02-19T15:35:31</t>
+          <t>2026-02-19T17:28:04</t>
         </is>
       </c>
       <c r="O256" t="inlineStr">
@@ -17711,7 +17701,7 @@
       </c>
       <c r="N257" t="inlineStr">
         <is>
-          <t>2026-02-19T14:55:48</t>
+          <t>2026-02-19T16:45:59</t>
         </is>
       </c>
       <c r="O257" t="inlineStr">
@@ -17777,7 +17767,7 @@
       </c>
       <c r="N258" t="inlineStr">
         <is>
-          <t>2026-02-19T15:31:57</t>
+          <t>2026-02-19T17:36:31</t>
         </is>
       </c>
       <c r="O258" t="inlineStr">
@@ -17843,7 +17833,7 @@
       </c>
       <c r="N259" t="inlineStr">
         <is>
-          <t>2026-02-19T14:47:38</t>
+          <t>2026-02-19T17:33:44</t>
         </is>
       </c>
       <c r="O259" t="inlineStr">
@@ -17909,7 +17899,7 @@
       </c>
       <c r="N260" t="inlineStr">
         <is>
-          <t>2026-02-19T15:06:02</t>
+          <t>2026-02-19T16:54:54</t>
         </is>
       </c>
       <c r="O260" t="inlineStr">
@@ -18041,7 +18031,7 @@
       </c>
       <c r="N262" t="inlineStr">
         <is>
-          <t>2026-02-19T15:01:04</t>
+          <t>2026-02-19T16:55:04</t>
         </is>
       </c>
       <c r="O262" t="inlineStr">
@@ -18107,7 +18097,7 @@
       </c>
       <c r="N263" t="inlineStr">
         <is>
-          <t>2026-02-19T15:30:12</t>
+          <t>2026-02-19T17:25:30</t>
         </is>
       </c>
       <c r="O263" t="inlineStr">
@@ -18173,7 +18163,7 @@
       </c>
       <c r="N264" t="inlineStr">
         <is>
-          <t>2026-02-19T15:03:29</t>
+          <t>2026-02-19T17:42:08</t>
         </is>
       </c>
       <c r="O264" t="inlineStr">
@@ -18239,7 +18229,7 @@
       </c>
       <c r="N265" t="inlineStr">
         <is>
-          <t>2026-02-19T15:40:23</t>
+          <t>2026-02-19T17:33:39</t>
         </is>
       </c>
       <c r="O265" t="inlineStr">
@@ -18305,7 +18295,7 @@
       </c>
       <c r="N266" t="inlineStr">
         <is>
-          <t>2026-02-19T14:56:30</t>
+          <t>2026-02-19T16:49:26</t>
         </is>
       </c>
       <c r="O266" t="inlineStr">
@@ -18371,7 +18361,7 @@
       </c>
       <c r="N267" t="inlineStr">
         <is>
-          <t>2026-02-19T14:46:47</t>
+          <t>2026-02-19T16:44:52</t>
         </is>
       </c>
       <c r="O267" t="inlineStr">
@@ -18437,7 +18427,7 @@
       </c>
       <c r="N268" t="inlineStr">
         <is>
-          <t>2026-02-19T15:38:57</t>
+          <t>2026-02-19T17:35:14</t>
         </is>
       </c>
       <c r="O268" t="inlineStr">
@@ -18503,7 +18493,7 @@
       </c>
       <c r="N269" t="inlineStr">
         <is>
-          <t>2026-02-19T14:53:44</t>
+          <t>2026-02-19T17:39:27</t>
         </is>
       </c>
       <c r="O269" t="inlineStr">
@@ -18566,7 +18556,7 @@
       </c>
       <c r="N270" t="inlineStr">
         <is>
-          <t>2026-02-19T15:13:16</t>
+          <t>2026-02-19T17:16:19</t>
         </is>
       </c>
       <c r="O270" t="inlineStr">
@@ -18698,7 +18688,7 @@
       </c>
       <c r="N272" t="inlineStr">
         <is>
-          <t>2026-02-19T14:58:33</t>
+          <t>2026-02-19T16:53:50</t>
         </is>
       </c>
       <c r="O272" t="inlineStr">
@@ -18764,7 +18754,7 @@
       </c>
       <c r="N273" t="inlineStr">
         <is>
-          <t>2026-02-19T15:11:30</t>
+          <t>2026-02-19T17:03:27</t>
         </is>
       </c>
       <c r="O273" t="inlineStr">
@@ -19226,7 +19216,7 @@
       </c>
       <c r="N280" t="inlineStr">
         <is>
-          <t>2026-02-19T14:42:35</t>
+          <t>2026-02-19T17:38:02</t>
         </is>
       </c>
       <c r="O280" t="inlineStr">
@@ -19292,7 +19282,7 @@
       </c>
       <c r="N281" t="inlineStr">
         <is>
-          <t>2026-02-19T14:49:10</t>
+          <t>2026-02-19T17:31:54</t>
         </is>
       </c>
       <c r="O281" t="inlineStr">
@@ -19312,6 +19302,11 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>10.69.5.151</t>
+        </is>
+      </c>
       <c r="D282" t="n">
         <v>2017</v>
       </c>
@@ -19353,7 +19348,7 @@
       </c>
       <c r="N282" t="inlineStr">
         <is>
-          <t>2026-02-19T14:59:10</t>
+          <t>2026-02-19T17:40:29</t>
         </is>
       </c>
       <c r="O282" t="inlineStr">
@@ -19419,7 +19414,7 @@
       </c>
       <c r="N283" t="inlineStr">
         <is>
-          <t>2026-02-19T14:54:18</t>
+          <t>2026-02-19T17:41:09</t>
         </is>
       </c>
       <c r="O283" t="inlineStr">
@@ -19485,7 +19480,7 @@
       </c>
       <c r="N284" t="inlineStr">
         <is>
-          <t>2026-02-19T15:30:00</t>
+          <t>2026-02-19T17:21:39</t>
         </is>
       </c>
       <c r="O284" t="inlineStr">
@@ -19551,7 +19546,7 @@
       </c>
       <c r="N285" t="inlineStr">
         <is>
-          <t>2026-02-19T15:08:24</t>
+          <t>2026-02-19T17:03:01</t>
         </is>
       </c>
       <c r="O285" t="inlineStr">
@@ -19678,7 +19673,7 @@
       </c>
       <c r="N287" t="inlineStr">
         <is>
-          <t>2026-02-19T15:29:46</t>
+          <t>2026-02-19T17:24:36</t>
         </is>
       </c>
       <c r="O287" t="inlineStr">
@@ -19810,7 +19805,7 @@
       </c>
       <c r="N289" t="inlineStr">
         <is>
-          <t>2026-02-19T15:38:57</t>
+          <t>2026-02-19T17:30:18</t>
         </is>
       </c>
       <c r="O289" t="inlineStr">
@@ -20630,7 +20625,7 @@
       </c>
       <c r="N302" t="inlineStr">
         <is>
-          <t>2026-02-19T15:02:04</t>
+          <t>2026-02-19T16:53:43</t>
         </is>
       </c>
       <c r="O302" t="inlineStr">
@@ -21782,7 +21777,7 @@
       </c>
       <c r="N320" t="inlineStr">
         <is>
-          <t>2026-02-19T15:02:12</t>
+          <t>2026-02-19T16:49:02</t>
         </is>
       </c>
       <c r="O320" t="inlineStr">
@@ -22531,7 +22526,7 @@
       </c>
       <c r="N332" t="inlineStr">
         <is>
-          <t>2026-02-19T15:24:08</t>
+          <t>2026-02-19T17:14:37</t>
         </is>
       </c>
       <c r="O332" t="inlineStr">
@@ -22597,7 +22592,7 @@
       </c>
       <c r="N333" t="inlineStr">
         <is>
-          <t>2026-02-19T15:11:44</t>
+          <t>2026-02-19T17:03:50</t>
         </is>
       </c>
       <c r="O333" t="inlineStr">
@@ -22663,7 +22658,7 @@
       </c>
       <c r="N334" t="inlineStr">
         <is>
-          <t>2026-02-19T15:10:54</t>
+          <t>2026-02-19T17:07:01</t>
         </is>
       </c>
       <c r="O334" t="inlineStr">
@@ -22729,7 +22724,7 @@
       </c>
       <c r="N335" t="inlineStr">
         <is>
-          <t>2026-02-19T14:58:02</t>
+          <t>2026-02-19T17:37:16</t>
         </is>
       </c>
       <c r="O335" t="inlineStr">
@@ -22861,7 +22856,7 @@
       </c>
       <c r="N337" t="inlineStr">
         <is>
-          <t>2026-02-19T15:29:40</t>
+          <t>2026-02-19T17:25:25</t>
         </is>
       </c>
       <c r="O337" t="inlineStr">
@@ -22927,7 +22922,7 @@
       </c>
       <c r="N338" t="inlineStr">
         <is>
-          <t>2026-02-19T14:50:58</t>
+          <t>2026-02-19T16:49:06</t>
         </is>
       </c>
       <c r="O338" t="inlineStr">
@@ -22993,7 +22988,7 @@
       </c>
       <c r="N339" t="inlineStr">
         <is>
-          <t>2026-02-19T15:00:07</t>
+          <t>2026-02-19T16:53:03</t>
         </is>
       </c>
       <c r="O339" t="inlineStr">
@@ -23254,7 +23249,7 @@
       </c>
       <c r="N343" t="inlineStr">
         <is>
-          <t>2026-02-19T14:58:11</t>
+          <t>2026-02-19T16:50:10</t>
         </is>
       </c>
       <c r="O343" t="inlineStr">
@@ -24683,7 +24678,7 @@
       </c>
       <c r="N365" t="inlineStr">
         <is>
-          <t>2026-02-19T15:19:39</t>
+          <t>2026-02-19T16:12:43</t>
         </is>
       </c>
       <c r="O365" t="inlineStr">
@@ -24751,7 +24746,7 @@
       </c>
       <c r="N366" t="inlineStr">
         <is>
-          <t>2026-02-19T15:13:08</t>
+          <t>2026-02-19T17:00:11</t>
         </is>
       </c>
       <c r="O366" t="inlineStr">
@@ -24881,7 +24876,7 @@
       </c>
       <c r="N368" t="inlineStr">
         <is>
-          <t>2026-02-19T15:34:46</t>
+          <t>2026-02-19T16:34:57</t>
         </is>
       </c>
       <c r="O368" t="inlineStr">
@@ -24949,7 +24944,7 @@
       </c>
       <c r="N369" t="inlineStr">
         <is>
-          <t>2026-02-19T15:31:00</t>
+          <t>2026-02-19T17:25:53</t>
         </is>
       </c>
       <c r="O369" t="inlineStr">
@@ -25020,7 +25015,7 @@
       </c>
       <c r="N370" t="inlineStr">
         <is>
-          <t>2026-02-19T15:19:36</t>
+          <t>2026-02-19T17:03:52</t>
         </is>
       </c>
       <c r="O370" t="inlineStr">
@@ -25091,7 +25086,7 @@
       </c>
       <c r="N371" t="inlineStr">
         <is>
-          <t>2026-02-19T15:01:10</t>
+          <t>2026-02-19T16:44:51</t>
         </is>
       </c>
       <c r="O371" t="inlineStr">
@@ -25304,7 +25299,7 @@
       </c>
       <c r="N374" t="inlineStr">
         <is>
-          <t>2026-02-19T14:46:38</t>
+          <t>2026-02-19T16:51:38</t>
         </is>
       </c>
       <c r="O374" t="inlineStr">
@@ -25372,7 +25367,7 @@
       </c>
       <c r="N375" t="inlineStr">
         <is>
-          <t>2026-02-19T15:27:29</t>
+          <t>2026-02-19T17:13:16</t>
         </is>
       </c>
       <c r="O375" t="inlineStr">
@@ -25392,6 +25387,11 @@
           <t>COORDENACAO</t>
         </is>
       </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>10.69.3.72</t>
+        </is>
+      </c>
       <c r="D376" t="n">
         <v>2025</v>
       </c>
@@ -25438,7 +25438,7 @@
       </c>
       <c r="N376" t="inlineStr">
         <is>
-          <t>2026-02-19T15:01:08</t>
+          <t>2026-02-19T16:51:56</t>
         </is>
       </c>
       <c r="O376" t="inlineStr">
@@ -25509,7 +25509,7 @@
       </c>
       <c r="N377" t="inlineStr">
         <is>
-          <t>2026-02-19T15:08:43</t>
+          <t>2026-02-19T17:01:02</t>
         </is>
       </c>
       <c r="O377" t="inlineStr">
@@ -25580,7 +25580,7 @@
       </c>
       <c r="N378" t="inlineStr">
         <is>
-          <t>2026-02-19T15:20:17</t>
+          <t>2026-02-19T17:12:29</t>
         </is>
       </c>
       <c r="O378" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática 2026-02-20 07:52:02.898775
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -601,7 +601,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>2026-02-19T17:07:23</t>
+          <t>2026-02-20T06:50:28</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -672,7 +672,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>2026-02-19T17:36:44</t>
+          <t>2026-02-20T07:21:34</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -1144,7 +1144,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>2026-02-19T17:40:00</t>
+          <t>2026-02-20T07:32:35</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -1474,7 +1474,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>2026-02-19T16:50:29</t>
+          <t>2026-02-20T07:05:44</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
@@ -1540,7 +1540,7 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>2026-02-19T16:45:34</t>
+          <t>2026-02-20T07:39:16</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>2026-02-19T16:54:18</t>
+          <t>2026-02-19T17:47:47</t>
         </is>
       </c>
       <c r="O28" t="inlineStr">
@@ -6885,7 +6885,7 @@
       </c>
       <c r="N95" t="inlineStr">
         <is>
-          <t>2026-02-19T17:08:33</t>
+          <t>2026-02-20T07:32:59</t>
         </is>
       </c>
       <c r="O95" t="inlineStr">
@@ -6956,7 +6956,7 @@
       </c>
       <c r="N96" t="inlineStr">
         <is>
-          <t>2026-02-19T17:14:44</t>
+          <t>2026-02-19T19:14:16</t>
         </is>
       </c>
       <c r="O96" t="inlineStr">
@@ -7159,7 +7159,7 @@
       </c>
       <c r="N99" t="inlineStr">
         <is>
-          <t>2026-02-19T17:15:22</t>
+          <t>2026-02-19T19:01:34</t>
         </is>
       </c>
       <c r="O99" t="inlineStr">
@@ -7230,7 +7230,7 @@
       </c>
       <c r="N100" t="inlineStr">
         <is>
-          <t>2026-02-19T16:48:48</t>
+          <t>2026-02-20T07:07:53</t>
         </is>
       </c>
       <c r="O100" t="inlineStr">
@@ -7301,7 +7301,7 @@
       </c>
       <c r="N101" t="inlineStr">
         <is>
-          <t>2026-02-19T17:36:00</t>
+          <t>2026-02-20T07:28:00</t>
         </is>
       </c>
       <c r="O101" t="inlineStr">
@@ -7443,7 +7443,7 @@
       </c>
       <c r="N103" t="inlineStr">
         <is>
-          <t>2026-02-19T17:22:18</t>
+          <t>2026-02-20T07:36:38</t>
         </is>
       </c>
       <c r="O103" t="inlineStr">
@@ -7850,7 +7850,7 @@
       </c>
       <c r="N109" t="inlineStr">
         <is>
-          <t>2026-02-19T16:48:07</t>
+          <t>2026-02-20T06:49:55</t>
         </is>
       </c>
       <c r="O109" t="inlineStr">
@@ -7921,7 +7921,7 @@
       </c>
       <c r="N110" t="inlineStr">
         <is>
-          <t>2026-02-19T17:16:15</t>
+          <t>2026-02-20T07:35:03</t>
         </is>
       </c>
       <c r="O110" t="inlineStr">
@@ -8063,7 +8063,7 @@
       </c>
       <c r="N112" t="inlineStr">
         <is>
-          <t>2026-02-19T16:56:57</t>
+          <t>2026-02-20T07:01:38</t>
         </is>
       </c>
       <c r="O112" t="inlineStr">
@@ -8134,7 +8134,7 @@
       </c>
       <c r="N113" t="inlineStr">
         <is>
-          <t>2026-02-19T16:49:11</t>
+          <t>2026-02-20T06:48:26</t>
         </is>
       </c>
       <c r="O113" t="inlineStr">
@@ -8205,7 +8205,7 @@
       </c>
       <c r="N114" t="inlineStr">
         <is>
-          <t>2026-02-19T16:49:36</t>
+          <t>2026-02-20T07:35:07</t>
         </is>
       </c>
       <c r="O114" t="inlineStr">
@@ -8344,7 +8344,7 @@
       </c>
       <c r="N116" t="inlineStr">
         <is>
-          <t>2026-02-19T16:40:55</t>
+          <t>2026-02-20T07:34:52</t>
         </is>
       </c>
       <c r="O116" t="inlineStr">
@@ -8364,6 +8364,11 @@
           <t>DP</t>
         </is>
       </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>10.69.3.23</t>
+        </is>
+      </c>
       <c r="D117" t="n">
         <v>2025</v>
       </c>
@@ -8410,7 +8415,7 @@
       </c>
       <c r="N117" t="inlineStr">
         <is>
-          <t>2026-02-19T16:54:41</t>
+          <t>2026-02-19T17:54:15</t>
         </is>
       </c>
       <c r="O117" t="inlineStr">
@@ -8691,7 +8696,7 @@
       </c>
       <c r="N121" t="inlineStr">
         <is>
-          <t>2026-02-19T16:51:14</t>
+          <t>2026-02-19T19:45:28</t>
         </is>
       </c>
       <c r="O121" t="inlineStr">
@@ -8830,7 +8835,7 @@
       </c>
       <c r="N123" t="inlineStr">
         <is>
-          <t>2026-02-19T17:07:09</t>
+          <t>2026-02-20T07:08:51</t>
         </is>
       </c>
       <c r="O123" t="inlineStr">
@@ -8901,7 +8906,7 @@
       </c>
       <c r="N124" t="inlineStr">
         <is>
-          <t>2026-02-19T16:57:18</t>
+          <t>2026-02-20T07:22:30</t>
         </is>
       </c>
       <c r="O124" t="inlineStr">
@@ -9114,7 +9119,7 @@
       </c>
       <c r="N127" t="inlineStr">
         <is>
-          <t>2026-02-19T16:43:56</t>
+          <t>2026-02-19T19:13:10</t>
         </is>
       </c>
       <c r="O127" t="inlineStr">
@@ -9256,7 +9261,7 @@
       </c>
       <c r="N129" t="inlineStr">
         <is>
-          <t>2026-02-19T17:38:35</t>
+          <t>2026-02-19T19:26:40</t>
         </is>
       </c>
       <c r="O129" t="inlineStr">
@@ -9530,7 +9535,7 @@
       </c>
       <c r="N133" t="inlineStr">
         <is>
-          <t>2026-02-19T17:22:45</t>
+          <t>2026-02-20T07:14:55</t>
         </is>
       </c>
       <c r="O133" t="inlineStr">
@@ -9596,7 +9601,7 @@
       </c>
       <c r="N134" t="inlineStr">
         <is>
-          <t>2026-02-19T16:57:03</t>
+          <t>2026-02-20T07:14:19</t>
         </is>
       </c>
       <c r="O134" t="inlineStr">
@@ -9662,7 +9667,7 @@
       </c>
       <c r="N135" t="inlineStr">
         <is>
-          <t>2026-02-19T17:13:22</t>
+          <t>2026-02-20T07:13:48</t>
         </is>
       </c>
       <c r="O135" t="inlineStr">
@@ -9859,7 +9864,7 @@
       </c>
       <c r="N138" t="inlineStr">
         <is>
-          <t>2026-02-19T17:15:15</t>
+          <t>2026-02-20T07:13:45</t>
         </is>
       </c>
       <c r="O138" t="inlineStr">
@@ -9925,7 +9930,7 @@
       </c>
       <c r="N139" t="inlineStr">
         <is>
-          <t>2026-02-19T16:44:19</t>
+          <t>2026-02-19T19:33:52</t>
         </is>
       </c>
       <c r="O139" t="inlineStr">
@@ -9991,7 +9996,7 @@
       </c>
       <c r="N140" t="inlineStr">
         <is>
-          <t>2026-02-19T17:20:26</t>
+          <t>2026-02-20T07:13:48</t>
         </is>
       </c>
       <c r="O140" t="inlineStr">
@@ -10057,7 +10062,7 @@
       </c>
       <c r="N141" t="inlineStr">
         <is>
-          <t>2026-02-19T17:39:07</t>
+          <t>2026-02-20T07:14:33</t>
         </is>
       </c>
       <c r="O141" t="inlineStr">
@@ -10123,7 +10128,7 @@
       </c>
       <c r="N142" t="inlineStr">
         <is>
-          <t>2026-02-19T17:22:31</t>
+          <t>2026-02-19T20:13:53</t>
         </is>
       </c>
       <c r="O142" t="inlineStr">
@@ -10189,7 +10194,7 @@
       </c>
       <c r="N143" t="inlineStr">
         <is>
-          <t>2026-02-19T17:02:54</t>
+          <t>2026-02-19T19:37:51</t>
         </is>
       </c>
       <c r="O143" t="inlineStr">
@@ -10255,7 +10260,7 @@
       </c>
       <c r="N144" t="inlineStr">
         <is>
-          <t>2026-02-19T17:41:45</t>
+          <t>2026-02-19T19:40:14</t>
         </is>
       </c>
       <c r="O144" t="inlineStr">
@@ -10321,7 +10326,7 @@
       </c>
       <c r="N145" t="inlineStr">
         <is>
-          <t>2026-02-19T17:41:33</t>
+          <t>2026-02-19T19:34:15</t>
         </is>
       </c>
       <c r="O145" t="inlineStr">
@@ -10387,7 +10392,7 @@
       </c>
       <c r="N146" t="inlineStr">
         <is>
-          <t>2026-02-19T16:53:53</t>
+          <t>2026-02-19T19:49:59</t>
         </is>
       </c>
       <c r="O146" t="inlineStr">
@@ -10453,7 +10458,7 @@
       </c>
       <c r="N147" t="inlineStr">
         <is>
-          <t>2026-02-19T16:48:45</t>
+          <t>2026-02-19T19:38:13</t>
         </is>
       </c>
       <c r="O147" t="inlineStr">
@@ -10519,7 +10524,7 @@
       </c>
       <c r="N148" t="inlineStr">
         <is>
-          <t>2026-02-19T16:47:13</t>
+          <t>2026-02-19T19:30:11</t>
         </is>
       </c>
       <c r="O148" t="inlineStr">
@@ -10585,7 +10590,7 @@
       </c>
       <c r="N149" t="inlineStr">
         <is>
-          <t>2026-02-19T17:38:20</t>
+          <t>2026-02-19T20:27:05</t>
         </is>
       </c>
       <c r="O149" t="inlineStr">
@@ -10651,7 +10656,7 @@
       </c>
       <c r="N150" t="inlineStr">
         <is>
-          <t>2026-02-19T17:36:49</t>
+          <t>2026-02-19T19:20:32</t>
         </is>
       </c>
       <c r="O150" t="inlineStr">
@@ -10783,7 +10788,7 @@
       </c>
       <c r="N152" t="inlineStr">
         <is>
-          <t>2026-02-19T16:48:36</t>
+          <t>2026-02-19T19:33:34</t>
         </is>
       </c>
       <c r="O152" t="inlineStr">
@@ -10844,7 +10849,7 @@
       </c>
       <c r="N153" t="inlineStr">
         <is>
-          <t>2026-02-19T16:44:22</t>
+          <t>2026-02-19T19:36:53</t>
         </is>
       </c>
       <c r="O153" t="inlineStr">
@@ -10910,7 +10915,7 @@
       </c>
       <c r="N154" t="inlineStr">
         <is>
-          <t>2026-02-19T17:39:15</t>
+          <t>2026-02-20T07:28:01</t>
         </is>
       </c>
       <c r="O154" t="inlineStr">
@@ -10976,7 +10981,7 @@
       </c>
       <c r="N155" t="inlineStr">
         <is>
-          <t>2026-02-19T17:36:35</t>
+          <t>2026-02-19T19:30:33</t>
         </is>
       </c>
       <c r="O155" t="inlineStr">
@@ -11108,7 +11113,7 @@
       </c>
       <c r="N157" t="inlineStr">
         <is>
-          <t>2026-02-19T17:41:46</t>
+          <t>2026-02-19T19:51:11</t>
         </is>
       </c>
       <c r="O157" t="inlineStr">
@@ -11240,7 +11245,7 @@
       </c>
       <c r="N159" t="inlineStr">
         <is>
-          <t>2026-02-19T16:54:52</t>
+          <t>2026-02-19T19:45:44</t>
         </is>
       </c>
       <c r="O159" t="inlineStr">
@@ -11306,7 +11311,7 @@
       </c>
       <c r="N160" t="inlineStr">
         <is>
-          <t>2026-02-19T13:20:37</t>
+          <t>2026-02-20T07:10:56</t>
         </is>
       </c>
       <c r="O160" t="inlineStr">
@@ -11438,7 +11443,7 @@
       </c>
       <c r="N162" t="inlineStr">
         <is>
-          <t>2026-02-19T17:08:08</t>
+          <t>2026-02-19T18:59:54</t>
         </is>
       </c>
       <c r="O162" t="inlineStr">
@@ -11570,7 +11575,7 @@
       </c>
       <c r="N164" t="inlineStr">
         <is>
-          <t>2026-02-19T17:13:00</t>
+          <t>2026-02-20T07:41:46</t>
         </is>
       </c>
       <c r="O164" t="inlineStr">
@@ -11632,11 +11637,11 @@
         </is>
       </c>
       <c r="M165" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N165" t="inlineStr">
         <is>
-          <t>2026-02-19T16:10:37</t>
+          <t>2026-02-20T06:53:59</t>
         </is>
       </c>
       <c r="O165" t="inlineStr">
@@ -11896,11 +11901,11 @@
         </is>
       </c>
       <c r="M169" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N169" t="inlineStr">
         <is>
-          <t>2026-02-19T17:17:23</t>
+          <t>2026-02-20T06:56:54</t>
         </is>
       </c>
       <c r="O169" t="inlineStr">
@@ -11966,7 +11971,7 @@
       </c>
       <c r="N170" t="inlineStr">
         <is>
-          <t>2026-02-19T17:08:46</t>
+          <t>2026-02-19T18:05:53</t>
         </is>
       </c>
       <c r="O170" t="inlineStr">
@@ -12028,11 +12033,11 @@
         </is>
       </c>
       <c r="M171" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N171" t="inlineStr">
         <is>
-          <t>2026-02-19T13:37:35</t>
+          <t>2026-02-20T07:15:02</t>
         </is>
       </c>
       <c r="O171" t="inlineStr">
@@ -12098,7 +12103,7 @@
       </c>
       <c r="N172" t="inlineStr">
         <is>
-          <t>2026-02-19T17:39:40</t>
+          <t>2026-02-19T18:38:10</t>
         </is>
       </c>
       <c r="O172" t="inlineStr">
@@ -12160,11 +12165,11 @@
         </is>
       </c>
       <c r="M173" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N173" t="inlineStr">
         <is>
-          <t>2026-02-19T16:56:31</t>
+          <t>2026-02-19T18:48:15</t>
         </is>
       </c>
       <c r="O173" t="inlineStr">
@@ -12230,7 +12235,7 @@
       </c>
       <c r="N174" t="inlineStr">
         <is>
-          <t>2026-02-19T13:11:47</t>
+          <t>2026-02-19T20:45:09</t>
         </is>
       </c>
       <c r="O174" t="inlineStr">
@@ -12296,7 +12301,7 @@
       </c>
       <c r="N175" t="inlineStr">
         <is>
-          <t>2026-02-19T17:05:11</t>
+          <t>2026-02-20T07:18:46</t>
         </is>
       </c>
       <c r="O175" t="inlineStr">
@@ -12494,7 +12499,7 @@
       </c>
       <c r="N178" t="inlineStr">
         <is>
-          <t>2026-02-19T17:40:05</t>
+          <t>2026-02-20T06:52:22</t>
         </is>
       </c>
       <c r="O178" t="inlineStr">
@@ -12560,7 +12565,7 @@
       </c>
       <c r="N179" t="inlineStr">
         <is>
-          <t>2026-02-19T17:03:26</t>
+          <t>2026-02-20T07:38:54</t>
         </is>
       </c>
       <c r="O179" t="inlineStr">
@@ -12626,7 +12631,7 @@
       </c>
       <c r="N180" t="inlineStr">
         <is>
-          <t>2026-02-19T16:49:57</t>
+          <t>2026-02-20T07:37:45</t>
         </is>
       </c>
       <c r="O180" t="inlineStr">
@@ -12692,7 +12697,7 @@
       </c>
       <c r="N181" t="inlineStr">
         <is>
-          <t>2026-02-19T17:05:16</t>
+          <t>2026-02-19T20:50:42</t>
         </is>
       </c>
       <c r="O181" t="inlineStr">
@@ -12895,7 +12900,7 @@
       </c>
       <c r="N184" t="inlineStr">
         <is>
-          <t>2026-02-19T17:38:48</t>
+          <t>2026-02-19T19:31:03</t>
         </is>
       </c>
       <c r="O184" t="inlineStr">
@@ -12961,7 +12966,7 @@
       </c>
       <c r="N185" t="inlineStr">
         <is>
-          <t>2026-02-19T17:38:31</t>
+          <t>2026-02-19T19:26:50</t>
         </is>
       </c>
       <c r="O185" t="inlineStr">
@@ -13027,7 +13032,7 @@
       </c>
       <c r="N186" t="inlineStr">
         <is>
-          <t>2026-02-19T15:57:20</t>
+          <t>2026-02-20T07:34:20</t>
         </is>
       </c>
       <c r="O186" t="inlineStr">
@@ -13093,7 +13098,7 @@
       </c>
       <c r="N187" t="inlineStr">
         <is>
-          <t>2026-02-19T17:38:31</t>
+          <t>2026-02-19T19:28:52</t>
         </is>
       </c>
       <c r="O187" t="inlineStr">
@@ -13291,7 +13296,7 @@
       </c>
       <c r="N190" t="inlineStr">
         <is>
-          <t>2026-02-19T16:53:32</t>
+          <t>2026-02-19T19:43:04</t>
         </is>
       </c>
       <c r="O190" t="inlineStr">
@@ -13357,7 +13362,7 @@
       </c>
       <c r="N191" t="inlineStr">
         <is>
-          <t>2026-02-19T17:11:09</t>
+          <t>2026-02-19T18:59:34</t>
         </is>
       </c>
       <c r="O191" t="inlineStr">
@@ -13423,7 +13428,7 @@
       </c>
       <c r="N192" t="inlineStr">
         <is>
-          <t>2026-02-19T16:57:24</t>
+          <t>2026-02-19T19:48:25</t>
         </is>
       </c>
       <c r="O192" t="inlineStr">
@@ -13552,7 +13557,7 @@
       </c>
       <c r="N194" t="inlineStr">
         <is>
-          <t>2026-02-19T16:58:09</t>
+          <t>2026-02-19T18:55:51</t>
         </is>
       </c>
       <c r="O194" t="inlineStr">
@@ -13618,7 +13623,7 @@
       </c>
       <c r="N195" t="inlineStr">
         <is>
-          <t>2026-02-19T16:55:45</t>
+          <t>2026-02-19T20:36:09</t>
         </is>
       </c>
       <c r="O195" t="inlineStr">
@@ -13684,7 +13689,7 @@
       </c>
       <c r="N196" t="inlineStr">
         <is>
-          <t>2026-02-19T17:42:07</t>
+          <t>2026-02-19T19:31:47</t>
         </is>
       </c>
       <c r="O196" t="inlineStr">
@@ -13750,7 +13755,7 @@
       </c>
       <c r="N197" t="inlineStr">
         <is>
-          <t>2026-02-19T16:51:06</t>
+          <t>2026-02-19T19:35:40</t>
         </is>
       </c>
       <c r="O197" t="inlineStr">
@@ -13816,7 +13821,7 @@
       </c>
       <c r="N198" t="inlineStr">
         <is>
-          <t>2026-02-19T17:24:10</t>
+          <t>2026-02-19T19:19:35</t>
         </is>
       </c>
       <c r="O198" t="inlineStr">
@@ -13882,7 +13887,7 @@
       </c>
       <c r="N199" t="inlineStr">
         <is>
-          <t>2026-02-19T17:40:10</t>
+          <t>2026-02-19T19:31:15</t>
         </is>
       </c>
       <c r="O199" t="inlineStr">
@@ -13948,7 +13953,7 @@
       </c>
       <c r="N200" t="inlineStr">
         <is>
-          <t>2026-02-19T16:55:07</t>
+          <t>2026-02-19T19:34:56</t>
         </is>
       </c>
       <c r="O200" t="inlineStr">
@@ -14011,7 +14016,7 @@
       </c>
       <c r="N201" t="inlineStr">
         <is>
-          <t>2026-02-19T17:25:54</t>
+          <t>2026-02-19T19:19:50</t>
         </is>
       </c>
       <c r="O201" t="inlineStr">
@@ -14077,7 +14082,7 @@
       </c>
       <c r="N202" t="inlineStr">
         <is>
-          <t>2026-02-19T16:54:10</t>
+          <t>2026-02-20T07:33:21</t>
         </is>
       </c>
       <c r="O202" t="inlineStr">
@@ -14143,7 +14148,7 @@
       </c>
       <c r="N203" t="inlineStr">
         <is>
-          <t>2026-02-19T17:03:01</t>
+          <t>2026-02-19T19:48:23</t>
         </is>
       </c>
       <c r="O203" t="inlineStr">
@@ -14209,7 +14214,7 @@
       </c>
       <c r="N204" t="inlineStr">
         <is>
-          <t>2026-02-19T17:24:46</t>
+          <t>2026-02-19T19:22:45</t>
         </is>
       </c>
       <c r="O204" t="inlineStr">
@@ -14275,7 +14280,7 @@
       </c>
       <c r="N205" t="inlineStr">
         <is>
-          <t>2026-02-19T17:13:52</t>
+          <t>2026-02-19T19:09:50</t>
         </is>
       </c>
       <c r="O205" t="inlineStr">
@@ -14341,7 +14346,7 @@
       </c>
       <c r="N206" t="inlineStr">
         <is>
-          <t>2026-02-19T16:53:03</t>
+          <t>2026-02-19T19:47:24</t>
         </is>
       </c>
       <c r="O206" t="inlineStr">
@@ -14407,7 +14412,7 @@
       </c>
       <c r="N207" t="inlineStr">
         <is>
-          <t>2026-02-19T17:30:13</t>
+          <t>2026-02-20T07:18:16</t>
         </is>
       </c>
       <c r="O207" t="inlineStr">
@@ -14473,7 +14478,7 @@
       </c>
       <c r="N208" t="inlineStr">
         <is>
-          <t>2026-02-19T17:34:14</t>
+          <t>2026-02-20T07:20:49</t>
         </is>
       </c>
       <c r="O208" t="inlineStr">
@@ -14539,7 +14544,7 @@
       </c>
       <c r="N209" t="inlineStr">
         <is>
-          <t>2026-02-19T17:36:45</t>
+          <t>2026-02-19T19:33:47</t>
         </is>
       </c>
       <c r="O209" t="inlineStr">
@@ -14605,7 +14610,7 @@
       </c>
       <c r="N210" t="inlineStr">
         <is>
-          <t>2026-02-19T16:56:09</t>
+          <t>2026-02-19T19:37:24</t>
         </is>
       </c>
       <c r="O210" t="inlineStr">
@@ -14671,7 +14676,7 @@
       </c>
       <c r="N211" t="inlineStr">
         <is>
-          <t>2026-02-19T16:51:26</t>
+          <t>2026-02-20T07:07:49</t>
         </is>
       </c>
       <c r="O211" t="inlineStr">
@@ -14737,7 +14742,7 @@
       </c>
       <c r="N212" t="inlineStr">
         <is>
-          <t>2026-02-19T16:58:05</t>
+          <t>2026-02-20T07:35:49</t>
         </is>
       </c>
       <c r="O212" t="inlineStr">
@@ -14803,7 +14808,7 @@
       </c>
       <c r="N213" t="inlineStr">
         <is>
-          <t>2026-02-19T16:50:10</t>
+          <t>2026-02-19T19:45:10</t>
         </is>
       </c>
       <c r="O213" t="inlineStr">
@@ -14869,7 +14874,7 @@
       </c>
       <c r="N214" t="inlineStr">
         <is>
-          <t>2026-02-19T16:59:19</t>
+          <t>2026-02-19T19:52:01</t>
         </is>
       </c>
       <c r="O214" t="inlineStr">
@@ -14935,7 +14940,7 @@
       </c>
       <c r="N215" t="inlineStr">
         <is>
-          <t>2026-02-19T16:46:10</t>
+          <t>2026-02-20T07:35:45</t>
         </is>
       </c>
       <c r="O215" t="inlineStr">
@@ -15001,7 +15006,7 @@
       </c>
       <c r="N216" t="inlineStr">
         <is>
-          <t>2026-02-19T17:16:15</t>
+          <t>2026-02-20T07:35:34</t>
         </is>
       </c>
       <c r="O216" t="inlineStr">
@@ -15067,7 +15072,7 @@
       </c>
       <c r="N217" t="inlineStr">
         <is>
-          <t>2026-02-19T17:06:09</t>
+          <t>2026-02-20T07:36:03</t>
         </is>
       </c>
       <c r="O217" t="inlineStr">
@@ -15133,7 +15138,7 @@
       </c>
       <c r="N218" t="inlineStr">
         <is>
-          <t>2026-02-19T17:39:52</t>
+          <t>2026-02-19T19:21:41</t>
         </is>
       </c>
       <c r="O218" t="inlineStr">
@@ -15199,7 +15204,7 @@
       </c>
       <c r="N219" t="inlineStr">
         <is>
-          <t>2026-02-19T17:27:36</t>
+          <t>2026-02-20T07:35:54</t>
         </is>
       </c>
       <c r="O219" t="inlineStr">
@@ -15270,7 +15275,7 @@
       </c>
       <c r="N220" t="inlineStr">
         <is>
-          <t>2026-02-19T17:07:31</t>
+          <t>2026-02-20T07:37:21</t>
         </is>
       </c>
       <c r="O220" t="inlineStr">
@@ -15402,7 +15407,7 @@
       </c>
       <c r="N222" t="inlineStr">
         <is>
-          <t>2026-02-19T17:01:00</t>
+          <t>2026-02-19T19:50:42</t>
         </is>
       </c>
       <c r="O222" t="inlineStr">
@@ -15468,7 +15473,7 @@
       </c>
       <c r="N223" t="inlineStr">
         <is>
-          <t>2026-02-19T16:56:54</t>
+          <t>2026-02-19T19:39:58</t>
         </is>
       </c>
       <c r="O223" t="inlineStr">
@@ -15534,7 +15539,7 @@
       </c>
       <c r="N224" t="inlineStr">
         <is>
-          <t>2026-02-19T17:07:57</t>
+          <t>2026-02-19T18:05:41</t>
         </is>
       </c>
       <c r="O224" t="inlineStr">
@@ -15600,7 +15605,7 @@
       </c>
       <c r="N225" t="inlineStr">
         <is>
-          <t>2026-02-19T17:29:36</t>
+          <t>2026-02-19T19:20:14</t>
         </is>
       </c>
       <c r="O225" t="inlineStr">
@@ -15666,7 +15671,7 @@
       </c>
       <c r="N226" t="inlineStr">
         <is>
-          <t>2026-02-19T16:53:18</t>
+          <t>2026-02-20T07:31:30</t>
         </is>
       </c>
       <c r="O226" t="inlineStr">
@@ -15732,7 +15737,7 @@
       </c>
       <c r="N227" t="inlineStr">
         <is>
-          <t>2026-02-19T17:18:12</t>
+          <t>2026-02-19T19:11:26</t>
         </is>
       </c>
       <c r="O227" t="inlineStr">
@@ -15798,7 +15803,7 @@
       </c>
       <c r="N228" t="inlineStr">
         <is>
-          <t>2026-02-19T17:14:57</t>
+          <t>2026-02-19T19:12:33</t>
         </is>
       </c>
       <c r="O228" t="inlineStr">
@@ -15864,7 +15869,7 @@
       </c>
       <c r="N229" t="inlineStr">
         <is>
-          <t>2026-02-19T17:39:24</t>
+          <t>2026-02-19T19:28:20</t>
         </is>
       </c>
       <c r="O229" t="inlineStr">
@@ -15930,7 +15935,7 @@
       </c>
       <c r="N230" t="inlineStr">
         <is>
-          <t>2026-02-19T16:58:18</t>
+          <t>2026-02-20T07:33:32</t>
         </is>
       </c>
       <c r="O230" t="inlineStr">
@@ -15996,7 +16001,7 @@
       </c>
       <c r="N231" t="inlineStr">
         <is>
-          <t>2026-02-19T17:23:54</t>
+          <t>2026-02-19T19:12:20</t>
         </is>
       </c>
       <c r="O231" t="inlineStr">
@@ -16062,7 +16067,7 @@
       </c>
       <c r="N232" t="inlineStr">
         <is>
-          <t>2026-02-19T17:09:30</t>
+          <t>2026-02-19T19:01:06</t>
         </is>
       </c>
       <c r="O232" t="inlineStr">
@@ -16128,7 +16133,7 @@
       </c>
       <c r="N233" t="inlineStr">
         <is>
-          <t>2026-02-19T17:30:20</t>
+          <t>2026-02-19T19:20:43</t>
         </is>
       </c>
       <c r="O233" t="inlineStr">
@@ -16194,7 +16199,7 @@
       </c>
       <c r="N234" t="inlineStr">
         <is>
-          <t>2026-02-19T16:49:00</t>
+          <t>2026-02-19T19:39:27</t>
         </is>
       </c>
       <c r="O234" t="inlineStr">
@@ -16260,7 +16265,7 @@
       </c>
       <c r="N235" t="inlineStr">
         <is>
-          <t>2026-02-19T16:49:21</t>
+          <t>2026-02-19T19:42:32</t>
         </is>
       </c>
       <c r="O235" t="inlineStr">
@@ -16326,7 +16331,7 @@
       </c>
       <c r="N236" t="inlineStr">
         <is>
-          <t>2026-02-19T17:40:31</t>
+          <t>2026-02-19T19:22:52</t>
         </is>
       </c>
       <c r="O236" t="inlineStr">
@@ -16392,7 +16397,7 @@
       </c>
       <c r="N237" t="inlineStr">
         <is>
-          <t>2026-02-19T16:51:27</t>
+          <t>2026-02-19T19:38:36</t>
         </is>
       </c>
       <c r="O237" t="inlineStr">
@@ -16458,7 +16463,7 @@
       </c>
       <c r="N238" t="inlineStr">
         <is>
-          <t>2026-02-19T16:56:25</t>
+          <t>2026-02-19T19:41:44</t>
         </is>
       </c>
       <c r="O238" t="inlineStr">
@@ -16524,7 +16529,7 @@
       </c>
       <c r="N239" t="inlineStr">
         <is>
-          <t>2026-02-19T17:17:12</t>
+          <t>2026-02-19T19:14:21</t>
         </is>
       </c>
       <c r="O239" t="inlineStr">
@@ -16590,7 +16595,7 @@
       </c>
       <c r="N240" t="inlineStr">
         <is>
-          <t>2026-02-19T16:55:47</t>
+          <t>2026-02-19T19:41:18</t>
         </is>
       </c>
       <c r="O240" t="inlineStr">
@@ -16656,7 +16661,7 @@
       </c>
       <c r="N241" t="inlineStr">
         <is>
-          <t>2026-02-19T17:29:38</t>
+          <t>2026-02-20T07:32:24</t>
         </is>
       </c>
       <c r="O241" t="inlineStr">
@@ -16722,7 +16727,7 @@
       </c>
       <c r="N242" t="inlineStr">
         <is>
-          <t>2026-02-19T17:27:01</t>
+          <t>2026-02-20T07:33:29</t>
         </is>
       </c>
       <c r="O242" t="inlineStr">
@@ -16788,7 +16793,7 @@
       </c>
       <c r="N243" t="inlineStr">
         <is>
-          <t>2026-02-19T16:58:33</t>
+          <t>2026-02-20T07:32:10</t>
         </is>
       </c>
       <c r="O243" t="inlineStr">
@@ -16808,11 +16813,6 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
-      <c r="C244" t="inlineStr">
-        <is>
-          <t>10.69.5.112</t>
-        </is>
-      </c>
       <c r="D244" t="n">
         <v>2019</v>
       </c>
@@ -16854,7 +16854,7 @@
       </c>
       <c r="N244" t="inlineStr">
         <is>
-          <t>2026-02-19T17:20:58</t>
+          <t>2026-02-19T19:05:10</t>
         </is>
       </c>
       <c r="O244" t="inlineStr">
@@ -16920,7 +16920,7 @@
       </c>
       <c r="N245" t="inlineStr">
         <is>
-          <t>2026-02-19T17:10:09</t>
+          <t>2026-02-20T07:35:19</t>
         </is>
       </c>
       <c r="O245" t="inlineStr">
@@ -16986,7 +16986,7 @@
       </c>
       <c r="N246" t="inlineStr">
         <is>
-          <t>2026-02-19T17:31:54</t>
+          <t>2026-02-20T07:35:12</t>
         </is>
       </c>
       <c r="O246" t="inlineStr">
@@ -17052,7 +17052,7 @@
       </c>
       <c r="N247" t="inlineStr">
         <is>
-          <t>2026-02-19T16:54:41</t>
+          <t>2026-02-20T07:34:14</t>
         </is>
       </c>
       <c r="O247" t="inlineStr">
@@ -17118,7 +17118,7 @@
       </c>
       <c r="N248" t="inlineStr">
         <is>
-          <t>2026-02-19T17:27:40</t>
+          <t>2026-02-20T07:34:23</t>
         </is>
       </c>
       <c r="O248" t="inlineStr">
@@ -17204,6 +17204,11 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>10.69.5.118</t>
+        </is>
+      </c>
       <c r="D250" t="n">
         <v>2017</v>
       </c>
@@ -17245,7 +17250,7 @@
       </c>
       <c r="N250" t="inlineStr">
         <is>
-          <t>2026-02-19T14:28:42</t>
+          <t>2026-02-20T07:35:01</t>
         </is>
       </c>
       <c r="O250" t="inlineStr">
@@ -17311,7 +17316,7 @@
       </c>
       <c r="N251" t="inlineStr">
         <is>
-          <t>2026-02-19T17:12:31</t>
+          <t>2026-02-20T07:34:23</t>
         </is>
       </c>
       <c r="O251" t="inlineStr">
@@ -17377,7 +17382,7 @@
       </c>
       <c r="N252" t="inlineStr">
         <is>
-          <t>2026-02-19T17:12:02</t>
+          <t>2026-02-20T07:34:50</t>
         </is>
       </c>
       <c r="O252" t="inlineStr">
@@ -17443,7 +17448,7 @@
       </c>
       <c r="N253" t="inlineStr">
         <is>
-          <t>2026-02-19T16:58:06</t>
+          <t>2026-02-20T07:38:22</t>
         </is>
       </c>
       <c r="O253" t="inlineStr">
@@ -17503,7 +17508,7 @@
       </c>
       <c r="N254" t="inlineStr">
         <is>
-          <t>2026-02-19T16:48:35</t>
+          <t>2026-02-20T07:35:54</t>
         </is>
       </c>
       <c r="O254" t="inlineStr">
@@ -17569,7 +17574,7 @@
       </c>
       <c r="N255" t="inlineStr">
         <is>
-          <t>2026-02-19T17:23:05</t>
+          <t>2026-02-20T07:21:00</t>
         </is>
       </c>
       <c r="O255" t="inlineStr">
@@ -17635,7 +17640,7 @@
       </c>
       <c r="N256" t="inlineStr">
         <is>
-          <t>2026-02-19T17:28:04</t>
+          <t>2026-02-19T19:20:02</t>
         </is>
       </c>
       <c r="O256" t="inlineStr">
@@ -17701,7 +17706,7 @@
       </c>
       <c r="N257" t="inlineStr">
         <is>
-          <t>2026-02-19T16:45:59</t>
+          <t>2026-02-19T19:38:46</t>
         </is>
       </c>
       <c r="O257" t="inlineStr">
@@ -17767,7 +17772,7 @@
       </c>
       <c r="N258" t="inlineStr">
         <is>
-          <t>2026-02-19T17:36:31</t>
+          <t>2026-02-19T19:31:53</t>
         </is>
       </c>
       <c r="O258" t="inlineStr">
@@ -17833,7 +17838,7 @@
       </c>
       <c r="N259" t="inlineStr">
         <is>
-          <t>2026-02-19T17:33:44</t>
+          <t>2026-02-19T19:04:55</t>
         </is>
       </c>
       <c r="O259" t="inlineStr">
@@ -17899,7 +17904,7 @@
       </c>
       <c r="N260" t="inlineStr">
         <is>
-          <t>2026-02-19T16:54:54</t>
+          <t>2026-02-19T19:46:46</t>
         </is>
       </c>
       <c r="O260" t="inlineStr">
@@ -18031,7 +18036,7 @@
       </c>
       <c r="N262" t="inlineStr">
         <is>
-          <t>2026-02-19T16:55:04</t>
+          <t>2026-02-19T19:44:11</t>
         </is>
       </c>
       <c r="O262" t="inlineStr">
@@ -18097,7 +18102,7 @@
       </c>
       <c r="N263" t="inlineStr">
         <is>
-          <t>2026-02-19T17:25:30</t>
+          <t>2026-02-19T19:13:29</t>
         </is>
       </c>
       <c r="O263" t="inlineStr">
@@ -18163,7 +18168,7 @@
       </c>
       <c r="N264" t="inlineStr">
         <is>
-          <t>2026-02-19T17:42:08</t>
+          <t>2026-02-19T19:31:20</t>
         </is>
       </c>
       <c r="O264" t="inlineStr">
@@ -18229,7 +18234,7 @@
       </c>
       <c r="N265" t="inlineStr">
         <is>
-          <t>2026-02-19T17:33:39</t>
+          <t>2026-02-19T19:25:26</t>
         </is>
       </c>
       <c r="O265" t="inlineStr">
@@ -18295,7 +18300,7 @@
       </c>
       <c r="N266" t="inlineStr">
         <is>
-          <t>2026-02-19T16:49:26</t>
+          <t>2026-02-19T20:41:39</t>
         </is>
       </c>
       <c r="O266" t="inlineStr">
@@ -18361,7 +18366,7 @@
       </c>
       <c r="N267" t="inlineStr">
         <is>
-          <t>2026-02-19T16:44:52</t>
+          <t>2026-02-19T19:38:55</t>
         </is>
       </c>
       <c r="O267" t="inlineStr">
@@ -18427,7 +18432,7 @@
       </c>
       <c r="N268" t="inlineStr">
         <is>
-          <t>2026-02-19T17:35:14</t>
+          <t>2026-02-19T19:23:25</t>
         </is>
       </c>
       <c r="O268" t="inlineStr">
@@ -18493,7 +18498,7 @@
       </c>
       <c r="N269" t="inlineStr">
         <is>
-          <t>2026-02-19T17:39:27</t>
+          <t>2026-02-19T19:33:57</t>
         </is>
       </c>
       <c r="O269" t="inlineStr">
@@ -18556,7 +18561,7 @@
       </c>
       <c r="N270" t="inlineStr">
         <is>
-          <t>2026-02-19T17:16:19</t>
+          <t>2026-02-20T07:30:12</t>
         </is>
       </c>
       <c r="O270" t="inlineStr">
@@ -18622,7 +18627,7 @@
       </c>
       <c r="N271" t="inlineStr">
         <is>
-          <t>2026-02-18T12:00:02</t>
+          <t>2026-02-19T22:07:44</t>
         </is>
       </c>
       <c r="O271" t="inlineStr">
@@ -18688,7 +18693,7 @@
       </c>
       <c r="N272" t="inlineStr">
         <is>
-          <t>2026-02-19T16:53:50</t>
+          <t>2026-02-19T20:25:25</t>
         </is>
       </c>
       <c r="O272" t="inlineStr">
@@ -18754,7 +18759,7 @@
       </c>
       <c r="N273" t="inlineStr">
         <is>
-          <t>2026-02-19T17:03:27</t>
+          <t>2026-02-20T07:09:48</t>
         </is>
       </c>
       <c r="O273" t="inlineStr">
@@ -19150,7 +19155,7 @@
       </c>
       <c r="N279" t="inlineStr">
         <is>
-          <t>2026-02-19T13:55:42</t>
+          <t>2026-02-20T07:09:37</t>
         </is>
       </c>
       <c r="O279" t="inlineStr">
@@ -19216,7 +19221,7 @@
       </c>
       <c r="N280" t="inlineStr">
         <is>
-          <t>2026-02-19T17:38:02</t>
+          <t>2026-02-20T06:48:19</t>
         </is>
       </c>
       <c r="O280" t="inlineStr">
@@ -19282,7 +19287,7 @@
       </c>
       <c r="N281" t="inlineStr">
         <is>
-          <t>2026-02-19T17:31:54</t>
+          <t>2026-02-20T07:35:34</t>
         </is>
       </c>
       <c r="O281" t="inlineStr">
@@ -19302,11 +19307,6 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
-      <c r="C282" t="inlineStr">
-        <is>
-          <t>10.69.5.151</t>
-        </is>
-      </c>
       <c r="D282" t="n">
         <v>2017</v>
       </c>
@@ -19348,7 +19348,7 @@
       </c>
       <c r="N282" t="inlineStr">
         <is>
-          <t>2026-02-19T17:40:29</t>
+          <t>2026-02-20T07:33:59</t>
         </is>
       </c>
       <c r="O282" t="inlineStr">
@@ -19414,7 +19414,7 @@
       </c>
       <c r="N283" t="inlineStr">
         <is>
-          <t>2026-02-19T17:41:09</t>
+          <t>2026-02-19T19:34:48</t>
         </is>
       </c>
       <c r="O283" t="inlineStr">
@@ -19480,7 +19480,7 @@
       </c>
       <c r="N284" t="inlineStr">
         <is>
-          <t>2026-02-19T17:21:39</t>
+          <t>2026-02-19T19:12:37</t>
         </is>
       </c>
       <c r="O284" t="inlineStr">
@@ -19546,7 +19546,7 @@
       </c>
       <c r="N285" t="inlineStr">
         <is>
-          <t>2026-02-19T17:03:01</t>
+          <t>2026-02-19T18:55:19</t>
         </is>
       </c>
       <c r="O285" t="inlineStr">
@@ -19566,6 +19566,11 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>10.69.5.155</t>
+        </is>
+      </c>
       <c r="D286" t="n">
         <v>2019</v>
       </c>
@@ -19607,7 +19612,7 @@
       </c>
       <c r="N286" t="inlineStr">
         <is>
-          <t>2026-02-19T14:59:26</t>
+          <t>2026-02-20T02:10:20</t>
         </is>
       </c>
       <c r="O286" t="inlineStr">
@@ -19673,7 +19678,7 @@
       </c>
       <c r="N287" t="inlineStr">
         <is>
-          <t>2026-02-19T17:24:36</t>
+          <t>2026-02-20T07:37:52</t>
         </is>
       </c>
       <c r="O287" t="inlineStr">
@@ -19739,7 +19744,7 @@
       </c>
       <c r="N288" t="inlineStr">
         <is>
-          <t>2026-02-19T13:09:41</t>
+          <t>2026-02-20T07:33:51</t>
         </is>
       </c>
       <c r="O288" t="inlineStr">
@@ -19805,7 +19810,7 @@
       </c>
       <c r="N289" t="inlineStr">
         <is>
-          <t>2026-02-19T17:30:18</t>
+          <t>2026-02-19T20:24:29</t>
         </is>
       </c>
       <c r="O289" t="inlineStr">
@@ -20625,7 +20630,7 @@
       </c>
       <c r="N302" t="inlineStr">
         <is>
-          <t>2026-02-19T16:53:43</t>
+          <t>2026-02-20T07:38:44</t>
         </is>
       </c>
       <c r="O302" t="inlineStr">
@@ -21777,7 +21782,7 @@
       </c>
       <c r="N320" t="inlineStr">
         <is>
-          <t>2026-02-19T16:49:02</t>
+          <t>2026-02-20T06:54:40</t>
         </is>
       </c>
       <c r="O320" t="inlineStr">
@@ -22526,7 +22531,7 @@
       </c>
       <c r="N332" t="inlineStr">
         <is>
-          <t>2026-02-19T17:14:37</t>
+          <t>2026-02-20T07:38:58</t>
         </is>
       </c>
       <c r="O332" t="inlineStr">
@@ -22592,7 +22597,7 @@
       </c>
       <c r="N333" t="inlineStr">
         <is>
-          <t>2026-02-19T17:03:50</t>
+          <t>2026-02-20T07:35:55</t>
         </is>
       </c>
       <c r="O333" t="inlineStr">
@@ -22658,7 +22663,7 @@
       </c>
       <c r="N334" t="inlineStr">
         <is>
-          <t>2026-02-19T17:07:01</t>
+          <t>2026-02-20T07:41:51</t>
         </is>
       </c>
       <c r="O334" t="inlineStr">
@@ -22724,7 +22729,7 @@
       </c>
       <c r="N335" t="inlineStr">
         <is>
-          <t>2026-02-19T17:37:16</t>
+          <t>2026-02-20T07:41:51</t>
         </is>
       </c>
       <c r="O335" t="inlineStr">
@@ -22790,7 +22795,7 @@
       </c>
       <c r="N336" t="inlineStr">
         <is>
-          <t>2026-02-19T13:23:24</t>
+          <t>2026-02-20T07:37:38</t>
         </is>
       </c>
       <c r="O336" t="inlineStr">
@@ -22856,7 +22861,7 @@
       </c>
       <c r="N337" t="inlineStr">
         <is>
-          <t>2026-02-19T17:25:25</t>
+          <t>2026-02-20T07:39:14</t>
         </is>
       </c>
       <c r="O337" t="inlineStr">
@@ -22922,7 +22927,7 @@
       </c>
       <c r="N338" t="inlineStr">
         <is>
-          <t>2026-02-19T16:49:06</t>
+          <t>2026-02-20T07:39:32</t>
         </is>
       </c>
       <c r="O338" t="inlineStr">
@@ -22988,7 +22993,7 @@
       </c>
       <c r="N339" t="inlineStr">
         <is>
-          <t>2026-02-19T16:53:03</t>
+          <t>2026-02-20T06:47:47</t>
         </is>
       </c>
       <c r="O339" t="inlineStr">
@@ -24746,7 +24751,7 @@
       </c>
       <c r="N366" t="inlineStr">
         <is>
-          <t>2026-02-19T17:00:11</t>
+          <t>2026-02-20T06:59:16</t>
         </is>
       </c>
       <c r="O366" t="inlineStr">
@@ -24896,11 +24901,6 @@
           <t>RH</t>
         </is>
       </c>
-      <c r="C369" t="inlineStr">
-        <is>
-          <t>10.69.3.13</t>
-        </is>
-      </c>
       <c r="D369" t="n">
         <v>2025</v>
       </c>
@@ -25015,7 +25015,7 @@
       </c>
       <c r="N370" t="inlineStr">
         <is>
-          <t>2026-02-19T17:03:52</t>
+          <t>2026-02-19T18:01:11</t>
         </is>
       </c>
       <c r="O370" t="inlineStr">
@@ -25299,7 +25299,7 @@
       </c>
       <c r="N374" t="inlineStr">
         <is>
-          <t>2026-02-19T16:51:38</t>
+          <t>2026-02-19T18:25:58</t>
         </is>
       </c>
       <c r="O374" t="inlineStr">
@@ -25367,7 +25367,7 @@
       </c>
       <c r="N375" t="inlineStr">
         <is>
-          <t>2026-02-19T17:13:16</t>
+          <t>2026-02-20T07:08:29</t>
         </is>
       </c>
       <c r="O375" t="inlineStr">
@@ -25438,7 +25438,7 @@
       </c>
       <c r="N376" t="inlineStr">
         <is>
-          <t>2026-02-19T16:51:56</t>
+          <t>2026-02-20T06:56:45</t>
         </is>
       </c>
       <c r="O376" t="inlineStr">
@@ -25580,7 +25580,7 @@
       </c>
       <c r="N378" t="inlineStr">
         <is>
-          <t>2026-02-19T17:12:29</t>
+          <t>2026-02-20T07:00:08</t>
         </is>
       </c>
       <c r="O378" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática 2026-02-20 09:52:04.758777
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -601,7 +601,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>2026-02-20T06:50:28</t>
+          <t>2026-02-20T09:34:42</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -672,7 +672,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>2026-02-20T07:21:34</t>
+          <t>2026-02-20T09:09:33</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -743,7 +743,7 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>2026-02-19T16:45:24</t>
+          <t>2026-02-20T09:04:45</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
@@ -814,7 +814,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>2026-02-19T16:15:27</t>
+          <t>2026-02-20T09:01:58</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -1144,7 +1144,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>2026-02-20T07:32:35</t>
+          <t>2026-02-20T09:25:04</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -1474,7 +1474,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>2026-02-20T07:05:44</t>
+          <t>2026-02-20T09:01:43</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
@@ -1540,7 +1540,7 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>2026-02-20T07:39:16</t>
+          <t>2026-02-20T09:32:52</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
@@ -6885,7 +6885,7 @@
       </c>
       <c r="N95" t="inlineStr">
         <is>
-          <t>2026-02-20T07:32:59</t>
+          <t>2026-02-20T09:19:36</t>
         </is>
       </c>
       <c r="O95" t="inlineStr">
@@ -6976,6 +6976,11 @@
           <t>COORDENACAO</t>
         </is>
       </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>10.69.3.93</t>
+        </is>
+      </c>
       <c r="D97" t="n">
         <v>2025</v>
       </c>
@@ -7022,7 +7027,7 @@
       </c>
       <c r="N97" t="inlineStr">
         <is>
-          <t>2026-02-19T15:58:02</t>
+          <t>2026-02-20T09:41:17</t>
         </is>
       </c>
       <c r="O97" t="inlineStr">
@@ -7230,7 +7235,7 @@
       </c>
       <c r="N100" t="inlineStr">
         <is>
-          <t>2026-02-20T07:07:53</t>
+          <t>2026-02-20T08:56:50</t>
         </is>
       </c>
       <c r="O100" t="inlineStr">
@@ -7301,7 +7306,7 @@
       </c>
       <c r="N101" t="inlineStr">
         <is>
-          <t>2026-02-20T07:28:00</t>
+          <t>2026-02-20T09:15:58</t>
         </is>
       </c>
       <c r="O101" t="inlineStr">
@@ -7443,7 +7448,7 @@
       </c>
       <c r="N103" t="inlineStr">
         <is>
-          <t>2026-02-20T07:36:38</t>
+          <t>2026-02-20T09:31:00</t>
         </is>
       </c>
       <c r="O103" t="inlineStr">
@@ -7708,7 +7713,7 @@
       </c>
       <c r="N107" t="inlineStr">
         <is>
-          <t>2026-02-19T16:33:37</t>
+          <t>2026-02-20T09:21:38</t>
         </is>
       </c>
       <c r="O107" t="inlineStr">
@@ -7850,7 +7855,7 @@
       </c>
       <c r="N109" t="inlineStr">
         <is>
-          <t>2026-02-20T06:49:55</t>
+          <t>2026-02-20T09:40:13</t>
         </is>
       </c>
       <c r="O109" t="inlineStr">
@@ -7921,7 +7926,7 @@
       </c>
       <c r="N110" t="inlineStr">
         <is>
-          <t>2026-02-20T07:35:03</t>
+          <t>2026-02-20T09:25:48</t>
         </is>
       </c>
       <c r="O110" t="inlineStr">
@@ -7992,7 +7997,7 @@
       </c>
       <c r="N111" t="inlineStr">
         <is>
-          <t>2026-02-19T17:06:28</t>
+          <t>2026-02-20T09:14:08</t>
         </is>
       </c>
       <c r="O111" t="inlineStr">
@@ -8063,7 +8068,7 @@
       </c>
       <c r="N112" t="inlineStr">
         <is>
-          <t>2026-02-20T07:01:38</t>
+          <t>2026-02-20T08:59:22</t>
         </is>
       </c>
       <c r="O112" t="inlineStr">
@@ -8134,7 +8139,7 @@
       </c>
       <c r="N113" t="inlineStr">
         <is>
-          <t>2026-02-20T06:48:26</t>
+          <t>2026-02-20T09:35:25</t>
         </is>
       </c>
       <c r="O113" t="inlineStr">
@@ -8205,7 +8210,7 @@
       </c>
       <c r="N114" t="inlineStr">
         <is>
-          <t>2026-02-20T07:35:07</t>
+          <t>2026-02-20T09:28:36</t>
         </is>
       </c>
       <c r="O114" t="inlineStr">
@@ -8273,7 +8278,7 @@
       </c>
       <c r="N115" t="inlineStr">
         <is>
-          <t>2026-02-19T16:42:31</t>
+          <t>2026-02-20T09:01:29</t>
         </is>
       </c>
       <c r="O115" t="inlineStr">
@@ -8344,7 +8349,7 @@
       </c>
       <c r="N116" t="inlineStr">
         <is>
-          <t>2026-02-20T07:34:52</t>
+          <t>2026-02-20T09:26:38</t>
         </is>
       </c>
       <c r="O116" t="inlineStr">
@@ -8364,11 +8369,6 @@
           <t>DP</t>
         </is>
       </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>10.69.3.23</t>
-        </is>
-      </c>
       <c r="D117" t="n">
         <v>2025</v>
       </c>
@@ -8415,7 +8415,7 @@
       </c>
       <c r="N117" t="inlineStr">
         <is>
-          <t>2026-02-19T17:54:15</t>
+          <t>2026-02-20T09:32:14</t>
         </is>
       </c>
       <c r="O117" t="inlineStr">
@@ -8625,7 +8625,7 @@
       </c>
       <c r="N120" t="inlineStr">
         <is>
-          <t>2026-02-19T17:26:58</t>
+          <t>2026-02-20T09:36:32</t>
         </is>
       </c>
       <c r="O120" t="inlineStr">
@@ -8764,7 +8764,7 @@
       </c>
       <c r="N122" t="inlineStr">
         <is>
-          <t>2026-02-19T16:57:37</t>
+          <t>2026-02-20T09:29:43</t>
         </is>
       </c>
       <c r="O122" t="inlineStr">
@@ -8906,7 +8906,7 @@
       </c>
       <c r="N124" t="inlineStr">
         <is>
-          <t>2026-02-20T07:22:30</t>
+          <t>2026-02-20T09:13:32</t>
         </is>
       </c>
       <c r="O124" t="inlineStr">
@@ -8977,7 +8977,7 @@
       </c>
       <c r="N125" t="inlineStr">
         <is>
-          <t>2026-02-19T15:40:19</t>
+          <t>2026-02-20T09:38:13</t>
         </is>
       </c>
       <c r="O125" t="inlineStr">
@@ -9044,11 +9044,11 @@
         </is>
       </c>
       <c r="M126" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N126" t="inlineStr">
         <is>
-          <t>2026-02-19T17:27:00</t>
+          <t>2026-02-20T09:25:53</t>
         </is>
       </c>
       <c r="O126" t="inlineStr">
@@ -9119,7 +9119,7 @@
       </c>
       <c r="N127" t="inlineStr">
         <is>
-          <t>2026-02-19T19:13:10</t>
+          <t>2026-02-20T09:38:45</t>
         </is>
       </c>
       <c r="O127" t="inlineStr">
@@ -9190,7 +9190,7 @@
       </c>
       <c r="N128" t="inlineStr">
         <is>
-          <t>2026-02-19T17:07:51</t>
+          <t>2026-02-20T08:55:11</t>
         </is>
       </c>
       <c r="O128" t="inlineStr">
@@ -9261,7 +9261,7 @@
       </c>
       <c r="N129" t="inlineStr">
         <is>
-          <t>2026-02-19T19:26:40</t>
+          <t>2026-02-20T09:26:43</t>
         </is>
       </c>
       <c r="O129" t="inlineStr">
@@ -9332,7 +9332,7 @@
       </c>
       <c r="N130" t="inlineStr">
         <is>
-          <t>2026-02-19T16:41:45</t>
+          <t>2026-02-20T09:41:31</t>
         </is>
       </c>
       <c r="O130" t="inlineStr">
@@ -9398,7 +9398,7 @@
       </c>
       <c r="N131" t="inlineStr">
         <is>
-          <t>2026-02-19T16:10:36</t>
+          <t>2026-02-20T09:34:56</t>
         </is>
       </c>
       <c r="O131" t="inlineStr">
@@ -9535,7 +9535,7 @@
       </c>
       <c r="N133" t="inlineStr">
         <is>
-          <t>2026-02-20T07:14:55</t>
+          <t>2026-02-20T09:02:48</t>
         </is>
       </c>
       <c r="O133" t="inlineStr">
@@ -9601,7 +9601,7 @@
       </c>
       <c r="N134" t="inlineStr">
         <is>
-          <t>2026-02-20T07:14:19</t>
+          <t>2026-02-20T09:12:16</t>
         </is>
       </c>
       <c r="O134" t="inlineStr">
@@ -9667,7 +9667,7 @@
       </c>
       <c r="N135" t="inlineStr">
         <is>
-          <t>2026-02-20T07:13:48</t>
+          <t>2026-02-20T09:07:35</t>
         </is>
       </c>
       <c r="O135" t="inlineStr">
@@ -9864,7 +9864,7 @@
       </c>
       <c r="N138" t="inlineStr">
         <is>
-          <t>2026-02-20T07:13:45</t>
+          <t>2026-02-20T09:05:35</t>
         </is>
       </c>
       <c r="O138" t="inlineStr">
@@ -9930,7 +9930,7 @@
       </c>
       <c r="N139" t="inlineStr">
         <is>
-          <t>2026-02-19T19:33:52</t>
+          <t>2026-02-20T09:34:29</t>
         </is>
       </c>
       <c r="O139" t="inlineStr">
@@ -9996,7 +9996,7 @@
       </c>
       <c r="N140" t="inlineStr">
         <is>
-          <t>2026-02-20T07:13:48</t>
+          <t>2026-02-20T09:03:48</t>
         </is>
       </c>
       <c r="O140" t="inlineStr">
@@ -10062,7 +10062,7 @@
       </c>
       <c r="N141" t="inlineStr">
         <is>
-          <t>2026-02-20T07:14:33</t>
+          <t>2026-02-20T08:58:04</t>
         </is>
       </c>
       <c r="O141" t="inlineStr">
@@ -10128,7 +10128,7 @@
       </c>
       <c r="N142" t="inlineStr">
         <is>
-          <t>2026-02-19T20:13:53</t>
+          <t>2026-02-20T08:50:05</t>
         </is>
       </c>
       <c r="O142" t="inlineStr">
@@ -10194,7 +10194,7 @@
       </c>
       <c r="N143" t="inlineStr">
         <is>
-          <t>2026-02-19T19:37:51</t>
+          <t>2026-02-20T08:47:47</t>
         </is>
       </c>
       <c r="O143" t="inlineStr">
@@ -10260,7 +10260,7 @@
       </c>
       <c r="N144" t="inlineStr">
         <is>
-          <t>2026-02-19T19:40:14</t>
+          <t>2026-02-20T09:25:21</t>
         </is>
       </c>
       <c r="O144" t="inlineStr">
@@ -10326,7 +10326,7 @@
       </c>
       <c r="N145" t="inlineStr">
         <is>
-          <t>2026-02-19T19:34:15</t>
+          <t>2026-02-20T08:54:21</t>
         </is>
       </c>
       <c r="O145" t="inlineStr">
@@ -10392,7 +10392,7 @@
       </c>
       <c r="N146" t="inlineStr">
         <is>
-          <t>2026-02-19T19:49:59</t>
+          <t>2026-02-20T09:39:23</t>
         </is>
       </c>
       <c r="O146" t="inlineStr">
@@ -10458,7 +10458,7 @@
       </c>
       <c r="N147" t="inlineStr">
         <is>
-          <t>2026-02-19T19:38:13</t>
+          <t>2026-02-20T08:48:52</t>
         </is>
       </c>
       <c r="O147" t="inlineStr">
@@ -10524,7 +10524,7 @@
       </c>
       <c r="N148" t="inlineStr">
         <is>
-          <t>2026-02-19T19:30:11</t>
+          <t>2026-02-20T09:41:47</t>
         </is>
       </c>
       <c r="O148" t="inlineStr">
@@ -10590,7 +10590,7 @@
       </c>
       <c r="N149" t="inlineStr">
         <is>
-          <t>2026-02-19T20:27:05</t>
+          <t>2026-02-20T08:47:49</t>
         </is>
       </c>
       <c r="O149" t="inlineStr">
@@ -10656,7 +10656,7 @@
       </c>
       <c r="N150" t="inlineStr">
         <is>
-          <t>2026-02-19T19:20:32</t>
+          <t>2026-02-20T08:50:27</t>
         </is>
       </c>
       <c r="O150" t="inlineStr">
@@ -10722,7 +10722,7 @@
       </c>
       <c r="N151" t="inlineStr">
         <is>
-          <t>2026-02-19T17:30:52</t>
+          <t>2026-02-20T08:49:58</t>
         </is>
       </c>
       <c r="O151" t="inlineStr">
@@ -10788,7 +10788,7 @@
       </c>
       <c r="N152" t="inlineStr">
         <is>
-          <t>2026-02-19T19:33:34</t>
+          <t>2026-02-20T08:54:48</t>
         </is>
       </c>
       <c r="O152" t="inlineStr">
@@ -10849,7 +10849,7 @@
       </c>
       <c r="N153" t="inlineStr">
         <is>
-          <t>2026-02-19T19:36:53</t>
+          <t>2026-02-20T08:55:10</t>
         </is>
       </c>
       <c r="O153" t="inlineStr">
@@ -10915,7 +10915,7 @@
       </c>
       <c r="N154" t="inlineStr">
         <is>
-          <t>2026-02-20T07:28:01</t>
+          <t>2026-02-20T09:21:14</t>
         </is>
       </c>
       <c r="O154" t="inlineStr">
@@ -10981,7 +10981,7 @@
       </c>
       <c r="N155" t="inlineStr">
         <is>
-          <t>2026-02-19T19:30:33</t>
+          <t>2026-02-20T08:49:53</t>
         </is>
       </c>
       <c r="O155" t="inlineStr">
@@ -11047,7 +11047,7 @@
       </c>
       <c r="N156" t="inlineStr">
         <is>
-          <t>2026-02-19T13:23:49</t>
+          <t>2026-02-20T08:54:06</t>
         </is>
       </c>
       <c r="O156" t="inlineStr">
@@ -11113,7 +11113,7 @@
       </c>
       <c r="N157" t="inlineStr">
         <is>
-          <t>2026-02-19T19:51:11</t>
+          <t>2026-02-20T08:56:24</t>
         </is>
       </c>
       <c r="O157" t="inlineStr">
@@ -11146,7 +11146,7 @@
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>Microsoft Windows 8.1 Pro</t>
+          <t>Windows</t>
         </is>
       </c>
       <c r="G158" t="inlineStr">
@@ -11179,7 +11179,7 @@
       </c>
       <c r="N158" t="inlineStr">
         <is>
-          <t>2026-02-19T12:59:01</t>
+          <t>2026-02-20T09:04:58</t>
         </is>
       </c>
       <c r="O158" t="inlineStr">
@@ -11245,7 +11245,7 @@
       </c>
       <c r="N159" t="inlineStr">
         <is>
-          <t>2026-02-19T19:45:44</t>
+          <t>2026-02-20T08:57:23</t>
         </is>
       </c>
       <c r="O159" t="inlineStr">
@@ -11311,7 +11311,7 @@
       </c>
       <c r="N160" t="inlineStr">
         <is>
-          <t>2026-02-20T07:10:56</t>
+          <t>2026-02-20T09:03:31</t>
         </is>
       </c>
       <c r="O160" t="inlineStr">
@@ -11377,7 +11377,7 @@
       </c>
       <c r="N161" t="inlineStr">
         <is>
-          <t>2026-02-19T12:55:37</t>
+          <t>2026-02-20T08:57:39</t>
         </is>
       </c>
       <c r="O161" t="inlineStr">
@@ -11443,7 +11443,7 @@
       </c>
       <c r="N162" t="inlineStr">
         <is>
-          <t>2026-02-19T18:59:54</t>
+          <t>2026-02-20T09:37:42</t>
         </is>
       </c>
       <c r="O162" t="inlineStr">
@@ -11575,7 +11575,7 @@
       </c>
       <c r="N164" t="inlineStr">
         <is>
-          <t>2026-02-20T07:41:46</t>
+          <t>2026-02-20T09:32:19</t>
         </is>
       </c>
       <c r="O164" t="inlineStr">
@@ -11637,11 +11637,11 @@
         </is>
       </c>
       <c r="M165" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N165" t="inlineStr">
         <is>
-          <t>2026-02-20T06:53:59</t>
+          <t>2026-02-20T09:37:41</t>
         </is>
       </c>
       <c r="O165" t="inlineStr">
@@ -11707,7 +11707,7 @@
       </c>
       <c r="N166" t="inlineStr">
         <is>
-          <t>2026-02-19T14:08:50</t>
+          <t>2026-02-20T08:57:19</t>
         </is>
       </c>
       <c r="O166" t="inlineStr">
@@ -11769,11 +11769,11 @@
         </is>
       </c>
       <c r="M167" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N167" t="inlineStr">
         <is>
-          <t>2026-02-19T14:33:47</t>
+          <t>2026-02-20T08:48:52</t>
         </is>
       </c>
       <c r="O167" t="inlineStr">
@@ -11839,7 +11839,7 @@
       </c>
       <c r="N168" t="inlineStr">
         <is>
-          <t>2026-02-19T13:33:36</t>
+          <t>2026-02-20T08:53:23</t>
         </is>
       </c>
       <c r="O168" t="inlineStr">
@@ -11901,11 +11901,11 @@
         </is>
       </c>
       <c r="M169" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N169" t="inlineStr">
         <is>
-          <t>2026-02-20T06:56:54</t>
+          <t>2026-02-20T09:39:29</t>
         </is>
       </c>
       <c r="O169" t="inlineStr">
@@ -11971,7 +11971,7 @@
       </c>
       <c r="N170" t="inlineStr">
         <is>
-          <t>2026-02-19T18:05:53</t>
+          <t>2026-02-20T09:02:29</t>
         </is>
       </c>
       <c r="O170" t="inlineStr">
@@ -12037,7 +12037,7 @@
       </c>
       <c r="N171" t="inlineStr">
         <is>
-          <t>2026-02-20T07:15:02</t>
+          <t>2026-02-20T09:06:17</t>
         </is>
       </c>
       <c r="O171" t="inlineStr">
@@ -12235,7 +12235,7 @@
       </c>
       <c r="N174" t="inlineStr">
         <is>
-          <t>2026-02-19T20:45:09</t>
+          <t>2026-02-20T08:53:48</t>
         </is>
       </c>
       <c r="O174" t="inlineStr">
@@ -12301,7 +12301,7 @@
       </c>
       <c r="N175" t="inlineStr">
         <is>
-          <t>2026-02-20T07:18:46</t>
+          <t>2026-02-20T09:10:23</t>
         </is>
       </c>
       <c r="O175" t="inlineStr">
@@ -12499,7 +12499,7 @@
       </c>
       <c r="N178" t="inlineStr">
         <is>
-          <t>2026-02-20T06:52:22</t>
+          <t>2026-02-20T09:42:22</t>
         </is>
       </c>
       <c r="O178" t="inlineStr">
@@ -12565,7 +12565,7 @@
       </c>
       <c r="N179" t="inlineStr">
         <is>
-          <t>2026-02-20T07:38:54</t>
+          <t>2026-02-20T09:33:36</t>
         </is>
       </c>
       <c r="O179" t="inlineStr">
@@ -12631,7 +12631,7 @@
       </c>
       <c r="N180" t="inlineStr">
         <is>
-          <t>2026-02-20T07:37:45</t>
+          <t>2026-02-20T09:25:59</t>
         </is>
       </c>
       <c r="O180" t="inlineStr">
@@ -12697,7 +12697,7 @@
       </c>
       <c r="N181" t="inlineStr">
         <is>
-          <t>2026-02-19T20:50:42</t>
+          <t>2026-02-20T08:45:11</t>
         </is>
       </c>
       <c r="O181" t="inlineStr">
@@ -12966,7 +12966,7 @@
       </c>
       <c r="N185" t="inlineStr">
         <is>
-          <t>2026-02-19T19:26:50</t>
+          <t>2026-02-20T09:39:38</t>
         </is>
       </c>
       <c r="O185" t="inlineStr">
@@ -13032,7 +13032,7 @@
       </c>
       <c r="N186" t="inlineStr">
         <is>
-          <t>2026-02-20T07:34:20</t>
+          <t>2026-02-20T09:23:55</t>
         </is>
       </c>
       <c r="O186" t="inlineStr">
@@ -13098,7 +13098,7 @@
       </c>
       <c r="N187" t="inlineStr">
         <is>
-          <t>2026-02-19T19:28:52</t>
+          <t>2026-02-20T09:07:49</t>
         </is>
       </c>
       <c r="O187" t="inlineStr">
@@ -13164,7 +13164,7 @@
       </c>
       <c r="N188" t="inlineStr">
         <is>
-          <t>2026-02-19T15:48:14</t>
+          <t>2026-02-20T09:08:03</t>
         </is>
       </c>
       <c r="O188" t="inlineStr">
@@ -13296,7 +13296,7 @@
       </c>
       <c r="N190" t="inlineStr">
         <is>
-          <t>2026-02-19T19:43:04</t>
+          <t>2026-02-20T09:31:36</t>
         </is>
       </c>
       <c r="O190" t="inlineStr">
@@ -13428,7 +13428,7 @@
       </c>
       <c r="N192" t="inlineStr">
         <is>
-          <t>2026-02-19T19:48:25</t>
+          <t>2026-02-20T09:23:47</t>
         </is>
       </c>
       <c r="O192" t="inlineStr">
@@ -13557,7 +13557,7 @@
       </c>
       <c r="N194" t="inlineStr">
         <is>
-          <t>2026-02-19T18:55:51</t>
+          <t>2026-02-20T08:56:37</t>
         </is>
       </c>
       <c r="O194" t="inlineStr">
@@ -13623,7 +13623,7 @@
       </c>
       <c r="N195" t="inlineStr">
         <is>
-          <t>2026-02-19T20:36:09</t>
+          <t>2026-02-20T09:17:00</t>
         </is>
       </c>
       <c r="O195" t="inlineStr">
@@ -13689,7 +13689,7 @@
       </c>
       <c r="N196" t="inlineStr">
         <is>
-          <t>2026-02-19T19:31:47</t>
+          <t>2026-02-20T09:03:35</t>
         </is>
       </c>
       <c r="O196" t="inlineStr">
@@ -13755,7 +13755,7 @@
       </c>
       <c r="N197" t="inlineStr">
         <is>
-          <t>2026-02-19T19:35:40</t>
+          <t>2026-02-20T09:14:07</t>
         </is>
       </c>
       <c r="O197" t="inlineStr">
@@ -13821,7 +13821,7 @@
       </c>
       <c r="N198" t="inlineStr">
         <is>
-          <t>2026-02-19T19:19:35</t>
+          <t>2026-02-20T09:16:08</t>
         </is>
       </c>
       <c r="O198" t="inlineStr">
@@ -13887,7 +13887,7 @@
       </c>
       <c r="N199" t="inlineStr">
         <is>
-          <t>2026-02-19T19:31:15</t>
+          <t>2026-02-20T09:15:24</t>
         </is>
       </c>
       <c r="O199" t="inlineStr">
@@ -13953,7 +13953,7 @@
       </c>
       <c r="N200" t="inlineStr">
         <is>
-          <t>2026-02-19T19:34:56</t>
+          <t>2026-02-20T09:20:15</t>
         </is>
       </c>
       <c r="O200" t="inlineStr">
@@ -14016,7 +14016,7 @@
       </c>
       <c r="N201" t="inlineStr">
         <is>
-          <t>2026-02-19T19:19:50</t>
+          <t>2026-02-20T08:59:59</t>
         </is>
       </c>
       <c r="O201" t="inlineStr">
@@ -14082,7 +14082,7 @@
       </c>
       <c r="N202" t="inlineStr">
         <is>
-          <t>2026-02-20T07:33:21</t>
+          <t>2026-02-20T09:05:24</t>
         </is>
       </c>
       <c r="O202" t="inlineStr">
@@ -14148,7 +14148,7 @@
       </c>
       <c r="N203" t="inlineStr">
         <is>
-          <t>2026-02-19T19:48:23</t>
+          <t>2026-02-20T09:37:01</t>
         </is>
       </c>
       <c r="O203" t="inlineStr">
@@ -14214,7 +14214,7 @@
       </c>
       <c r="N204" t="inlineStr">
         <is>
-          <t>2026-02-19T19:22:45</t>
+          <t>2026-02-20T09:02:13</t>
         </is>
       </c>
       <c r="O204" t="inlineStr">
@@ -14280,7 +14280,7 @@
       </c>
       <c r="N205" t="inlineStr">
         <is>
-          <t>2026-02-19T19:09:50</t>
+          <t>2026-02-20T09:40:26</t>
         </is>
       </c>
       <c r="O205" t="inlineStr">
@@ -14346,7 +14346,7 @@
       </c>
       <c r="N206" t="inlineStr">
         <is>
-          <t>2026-02-19T19:47:24</t>
+          <t>2026-02-20T09:03:39</t>
         </is>
       </c>
       <c r="O206" t="inlineStr">
@@ -14412,7 +14412,7 @@
       </c>
       <c r="N207" t="inlineStr">
         <is>
-          <t>2026-02-20T07:18:16</t>
+          <t>2026-02-20T09:15:30</t>
         </is>
       </c>
       <c r="O207" t="inlineStr">
@@ -14478,7 +14478,7 @@
       </c>
       <c r="N208" t="inlineStr">
         <is>
-          <t>2026-02-20T07:20:49</t>
+          <t>2026-02-20T09:12:53</t>
         </is>
       </c>
       <c r="O208" t="inlineStr">
@@ -14544,7 +14544,7 @@
       </c>
       <c r="N209" t="inlineStr">
         <is>
-          <t>2026-02-19T19:33:47</t>
+          <t>2026-02-20T09:36:03</t>
         </is>
       </c>
       <c r="O209" t="inlineStr">
@@ -14610,7 +14610,7 @@
       </c>
       <c r="N210" t="inlineStr">
         <is>
-          <t>2026-02-19T19:37:24</t>
+          <t>2026-02-20T08:50:57</t>
         </is>
       </c>
       <c r="O210" t="inlineStr">
@@ -14676,7 +14676,7 @@
       </c>
       <c r="N211" t="inlineStr">
         <is>
-          <t>2026-02-20T07:07:49</t>
+          <t>2026-02-20T09:02:21</t>
         </is>
       </c>
       <c r="O211" t="inlineStr">
@@ -14742,7 +14742,7 @@
       </c>
       <c r="N212" t="inlineStr">
         <is>
-          <t>2026-02-20T07:35:49</t>
+          <t>2026-02-20T09:26:41</t>
         </is>
       </c>
       <c r="O212" t="inlineStr">
@@ -14808,7 +14808,7 @@
       </c>
       <c r="N213" t="inlineStr">
         <is>
-          <t>2026-02-19T19:45:10</t>
+          <t>2026-02-20T09:08:36</t>
         </is>
       </c>
       <c r="O213" t="inlineStr">
@@ -14874,7 +14874,7 @@
       </c>
       <c r="N214" t="inlineStr">
         <is>
-          <t>2026-02-19T19:52:01</t>
+          <t>2026-02-20T09:37:37</t>
         </is>
       </c>
       <c r="O214" t="inlineStr">
@@ -14940,7 +14940,7 @@
       </c>
       <c r="N215" t="inlineStr">
         <is>
-          <t>2026-02-20T07:35:45</t>
+          <t>2026-02-20T09:19:17</t>
         </is>
       </c>
       <c r="O215" t="inlineStr">
@@ -15006,7 +15006,7 @@
       </c>
       <c r="N216" t="inlineStr">
         <is>
-          <t>2026-02-20T07:35:34</t>
+          <t>2026-02-20T09:32:21</t>
         </is>
       </c>
       <c r="O216" t="inlineStr">
@@ -15072,7 +15072,7 @@
       </c>
       <c r="N217" t="inlineStr">
         <is>
-          <t>2026-02-20T07:36:03</t>
+          <t>2026-02-20T09:25:43</t>
         </is>
       </c>
       <c r="O217" t="inlineStr">
@@ -15138,7 +15138,7 @@
       </c>
       <c r="N218" t="inlineStr">
         <is>
-          <t>2026-02-19T19:21:41</t>
+          <t>2026-02-20T09:08:04</t>
         </is>
       </c>
       <c r="O218" t="inlineStr">
@@ -15204,7 +15204,7 @@
       </c>
       <c r="N219" t="inlineStr">
         <is>
-          <t>2026-02-20T07:35:54</t>
+          <t>2026-02-20T08:29:39</t>
         </is>
       </c>
       <c r="O219" t="inlineStr">
@@ -15275,7 +15275,7 @@
       </c>
       <c r="N220" t="inlineStr">
         <is>
-          <t>2026-02-20T07:37:21</t>
+          <t>2026-02-20T09:29:29</t>
         </is>
       </c>
       <c r="O220" t="inlineStr">
@@ -15341,7 +15341,7 @@
       </c>
       <c r="N221" t="inlineStr">
         <is>
-          <t>2026-02-19T15:31:48</t>
+          <t>2026-02-20T08:58:37</t>
         </is>
       </c>
       <c r="O221" t="inlineStr">
@@ -15407,7 +15407,7 @@
       </c>
       <c r="N222" t="inlineStr">
         <is>
-          <t>2026-02-19T19:50:42</t>
+          <t>2026-02-20T09:01:16</t>
         </is>
       </c>
       <c r="O222" t="inlineStr">
@@ -15671,7 +15671,7 @@
       </c>
       <c r="N226" t="inlineStr">
         <is>
-          <t>2026-02-20T07:31:30</t>
+          <t>2026-02-20T09:17:02</t>
         </is>
       </c>
       <c r="O226" t="inlineStr">
@@ -15737,7 +15737,7 @@
       </c>
       <c r="N227" t="inlineStr">
         <is>
-          <t>2026-02-19T19:11:26</t>
+          <t>2026-02-20T08:54:09</t>
         </is>
       </c>
       <c r="O227" t="inlineStr">
@@ -15869,7 +15869,7 @@
       </c>
       <c r="N229" t="inlineStr">
         <is>
-          <t>2026-02-19T19:28:20</t>
+          <t>2026-02-20T09:00:53</t>
         </is>
       </c>
       <c r="O229" t="inlineStr">
@@ -15935,7 +15935,7 @@
       </c>
       <c r="N230" t="inlineStr">
         <is>
-          <t>2026-02-20T07:33:32</t>
+          <t>2026-02-20T09:23:07</t>
         </is>
       </c>
       <c r="O230" t="inlineStr">
@@ -16001,7 +16001,7 @@
       </c>
       <c r="N231" t="inlineStr">
         <is>
-          <t>2026-02-19T19:12:20</t>
+          <t>2026-02-20T09:08:46</t>
         </is>
       </c>
       <c r="O231" t="inlineStr">
@@ -16067,7 +16067,7 @@
       </c>
       <c r="N232" t="inlineStr">
         <is>
-          <t>2026-02-19T19:01:06</t>
+          <t>2026-02-20T08:55:05</t>
         </is>
       </c>
       <c r="O232" t="inlineStr">
@@ -16133,7 +16133,7 @@
       </c>
       <c r="N233" t="inlineStr">
         <is>
-          <t>2026-02-19T19:20:43</t>
+          <t>2026-02-20T08:57:35</t>
         </is>
       </c>
       <c r="O233" t="inlineStr">
@@ -16199,7 +16199,7 @@
       </c>
       <c r="N234" t="inlineStr">
         <is>
-          <t>2026-02-19T19:39:27</t>
+          <t>2026-02-20T09:12:54</t>
         </is>
       </c>
       <c r="O234" t="inlineStr">
@@ -16463,7 +16463,7 @@
       </c>
       <c r="N238" t="inlineStr">
         <is>
-          <t>2026-02-19T19:41:44</t>
+          <t>2026-02-20T08:51:34</t>
         </is>
       </c>
       <c r="O238" t="inlineStr">
@@ -16529,7 +16529,7 @@
       </c>
       <c r="N239" t="inlineStr">
         <is>
-          <t>2026-02-19T19:14:21</t>
+          <t>2026-02-20T09:27:01</t>
         </is>
       </c>
       <c r="O239" t="inlineStr">
@@ -16595,7 +16595,7 @@
       </c>
       <c r="N240" t="inlineStr">
         <is>
-          <t>2026-02-19T19:41:18</t>
+          <t>2026-02-20T08:47:53</t>
         </is>
       </c>
       <c r="O240" t="inlineStr">
@@ -16661,7 +16661,7 @@
       </c>
       <c r="N241" t="inlineStr">
         <is>
-          <t>2026-02-20T07:32:24</t>
+          <t>2026-02-20T09:17:19</t>
         </is>
       </c>
       <c r="O241" t="inlineStr">
@@ -16727,7 +16727,7 @@
       </c>
       <c r="N242" t="inlineStr">
         <is>
-          <t>2026-02-20T07:33:29</t>
+          <t>2026-02-20T09:28:11</t>
         </is>
       </c>
       <c r="O242" t="inlineStr">
@@ -16793,7 +16793,7 @@
       </c>
       <c r="N243" t="inlineStr">
         <is>
-          <t>2026-02-20T07:32:10</t>
+          <t>2026-02-20T09:19:06</t>
         </is>
       </c>
       <c r="O243" t="inlineStr">
@@ -16813,6 +16813,11 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>10.69.5.112</t>
+        </is>
+      </c>
       <c r="D244" t="n">
         <v>2019</v>
       </c>
@@ -16854,7 +16859,7 @@
       </c>
       <c r="N244" t="inlineStr">
         <is>
-          <t>2026-02-19T19:05:10</t>
+          <t>2026-02-20T08:55:35</t>
         </is>
       </c>
       <c r="O244" t="inlineStr">
@@ -16920,7 +16925,7 @@
       </c>
       <c r="N245" t="inlineStr">
         <is>
-          <t>2026-02-20T07:35:19</t>
+          <t>2026-02-20T09:19:49</t>
         </is>
       </c>
       <c r="O245" t="inlineStr">
@@ -16986,7 +16991,7 @@
       </c>
       <c r="N246" t="inlineStr">
         <is>
-          <t>2026-02-20T07:35:12</t>
+          <t>2026-02-20T09:26:36</t>
         </is>
       </c>
       <c r="O246" t="inlineStr">
@@ -17052,7 +17057,7 @@
       </c>
       <c r="N247" t="inlineStr">
         <is>
-          <t>2026-02-20T07:34:14</t>
+          <t>2026-02-20T09:25:27</t>
         </is>
       </c>
       <c r="O247" t="inlineStr">
@@ -17118,7 +17123,7 @@
       </c>
       <c r="N248" t="inlineStr">
         <is>
-          <t>2026-02-20T07:34:23</t>
+          <t>2026-02-20T09:26:44</t>
         </is>
       </c>
       <c r="O248" t="inlineStr">
@@ -17184,7 +17189,7 @@
       </c>
       <c r="N249" t="inlineStr">
         <is>
-          <t>2026-02-19T14:08:04</t>
+          <t>2026-02-20T09:00:50</t>
         </is>
       </c>
       <c r="O249" t="inlineStr">
@@ -17204,11 +17209,6 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
-      <c r="C250" t="inlineStr">
-        <is>
-          <t>10.69.5.118</t>
-        </is>
-      </c>
       <c r="D250" t="n">
         <v>2017</v>
       </c>
@@ -17250,7 +17250,7 @@
       </c>
       <c r="N250" t="inlineStr">
         <is>
-          <t>2026-02-20T07:35:01</t>
+          <t>2026-02-20T09:32:36</t>
         </is>
       </c>
       <c r="O250" t="inlineStr">
@@ -17316,7 +17316,7 @@
       </c>
       <c r="N251" t="inlineStr">
         <is>
-          <t>2026-02-20T07:34:23</t>
+          <t>2026-02-20T09:19:27</t>
         </is>
       </c>
       <c r="O251" t="inlineStr">
@@ -17382,7 +17382,7 @@
       </c>
       <c r="N252" t="inlineStr">
         <is>
-          <t>2026-02-20T07:34:50</t>
+          <t>2026-02-20T09:34:06</t>
         </is>
       </c>
       <c r="O252" t="inlineStr">
@@ -17448,7 +17448,7 @@
       </c>
       <c r="N253" t="inlineStr">
         <is>
-          <t>2026-02-20T07:38:22</t>
+          <t>2026-02-20T09:33:01</t>
         </is>
       </c>
       <c r="O253" t="inlineStr">
@@ -17508,7 +17508,7 @@
       </c>
       <c r="N254" t="inlineStr">
         <is>
-          <t>2026-02-20T07:35:54</t>
+          <t>2026-02-20T09:32:01</t>
         </is>
       </c>
       <c r="O254" t="inlineStr">
@@ -17574,7 +17574,7 @@
       </c>
       <c r="N255" t="inlineStr">
         <is>
-          <t>2026-02-20T07:21:00</t>
+          <t>2026-02-20T09:11:56</t>
         </is>
       </c>
       <c r="O255" t="inlineStr">
@@ -17640,7 +17640,7 @@
       </c>
       <c r="N256" t="inlineStr">
         <is>
-          <t>2026-02-19T19:20:02</t>
+          <t>2026-02-20T08:43:59</t>
         </is>
       </c>
       <c r="O256" t="inlineStr">
@@ -17706,7 +17706,7 @@
       </c>
       <c r="N257" t="inlineStr">
         <is>
-          <t>2026-02-19T19:38:46</t>
+          <t>2026-02-20T09:08:19</t>
         </is>
       </c>
       <c r="O257" t="inlineStr">
@@ -17772,7 +17772,7 @@
       </c>
       <c r="N258" t="inlineStr">
         <is>
-          <t>2026-02-19T19:31:53</t>
+          <t>2026-02-20T08:59:24</t>
         </is>
       </c>
       <c r="O258" t="inlineStr">
@@ -17838,7 +17838,7 @@
       </c>
       <c r="N259" t="inlineStr">
         <is>
-          <t>2026-02-19T19:04:55</t>
+          <t>2026-02-20T08:56:40</t>
         </is>
       </c>
       <c r="O259" t="inlineStr">
@@ -17904,7 +17904,7 @@
       </c>
       <c r="N260" t="inlineStr">
         <is>
-          <t>2026-02-19T19:46:46</t>
+          <t>2026-02-20T09:38:10</t>
         </is>
       </c>
       <c r="O260" t="inlineStr">
@@ -17970,7 +17970,7 @@
       </c>
       <c r="N261" t="inlineStr">
         <is>
-          <t>2026-02-19T13:30:11</t>
+          <t>2026-02-20T08:55:28</t>
         </is>
       </c>
       <c r="O261" t="inlineStr">
@@ -18036,7 +18036,7 @@
       </c>
       <c r="N262" t="inlineStr">
         <is>
-          <t>2026-02-19T19:44:11</t>
+          <t>2026-02-20T09:09:41</t>
         </is>
       </c>
       <c r="O262" t="inlineStr">
@@ -18102,7 +18102,7 @@
       </c>
       <c r="N263" t="inlineStr">
         <is>
-          <t>2026-02-19T19:13:29</t>
+          <t>2026-02-20T08:51:18</t>
         </is>
       </c>
       <c r="O263" t="inlineStr">
@@ -18168,7 +18168,7 @@
       </c>
       <c r="N264" t="inlineStr">
         <is>
-          <t>2026-02-19T19:31:20</t>
+          <t>2026-02-20T09:00:46</t>
         </is>
       </c>
       <c r="O264" t="inlineStr">
@@ -18234,7 +18234,7 @@
       </c>
       <c r="N265" t="inlineStr">
         <is>
-          <t>2026-02-19T19:25:26</t>
+          <t>2026-02-20T09:30:21</t>
         </is>
       </c>
       <c r="O265" t="inlineStr">
@@ -18300,7 +18300,7 @@
       </c>
       <c r="N266" t="inlineStr">
         <is>
-          <t>2026-02-19T20:41:39</t>
+          <t>2026-02-20T09:11:29</t>
         </is>
       </c>
       <c r="O266" t="inlineStr">
@@ -18366,7 +18366,7 @@
       </c>
       <c r="N267" t="inlineStr">
         <is>
-          <t>2026-02-19T19:38:55</t>
+          <t>2026-02-20T08:50:43</t>
         </is>
       </c>
       <c r="O267" t="inlineStr">
@@ -18432,7 +18432,7 @@
       </c>
       <c r="N268" t="inlineStr">
         <is>
-          <t>2026-02-19T19:23:25</t>
+          <t>2026-02-20T08:54:39</t>
         </is>
       </c>
       <c r="O268" t="inlineStr">
@@ -18561,7 +18561,7 @@
       </c>
       <c r="N270" t="inlineStr">
         <is>
-          <t>2026-02-20T07:30:12</t>
+          <t>2026-02-20T09:25:16</t>
         </is>
       </c>
       <c r="O270" t="inlineStr">
@@ -18693,7 +18693,7 @@
       </c>
       <c r="N272" t="inlineStr">
         <is>
-          <t>2026-02-19T20:25:25</t>
+          <t>2026-02-20T09:33:06</t>
         </is>
       </c>
       <c r="O272" t="inlineStr">
@@ -18759,7 +18759,7 @@
       </c>
       <c r="N273" t="inlineStr">
         <is>
-          <t>2026-02-20T07:09:48</t>
+          <t>2026-02-20T08:56:28</t>
         </is>
       </c>
       <c r="O273" t="inlineStr">
@@ -19089,7 +19089,7 @@
       </c>
       <c r="N278" t="inlineStr">
         <is>
-          <t>2026-02-19T14:56:22</t>
+          <t>2026-02-20T09:04:24</t>
         </is>
       </c>
       <c r="O278" t="inlineStr">
@@ -19155,7 +19155,7 @@
       </c>
       <c r="N279" t="inlineStr">
         <is>
-          <t>2026-02-20T07:09:37</t>
+          <t>2026-02-20T09:11:07</t>
         </is>
       </c>
       <c r="O279" t="inlineStr">
@@ -19221,7 +19221,7 @@
       </c>
       <c r="N280" t="inlineStr">
         <is>
-          <t>2026-02-20T06:48:19</t>
+          <t>2026-02-20T09:40:05</t>
         </is>
       </c>
       <c r="O280" t="inlineStr">
@@ -19287,7 +19287,7 @@
       </c>
       <c r="N281" t="inlineStr">
         <is>
-          <t>2026-02-20T07:35:34</t>
+          <t>2026-02-20T09:35:16</t>
         </is>
       </c>
       <c r="O281" t="inlineStr">
@@ -19348,7 +19348,7 @@
       </c>
       <c r="N282" t="inlineStr">
         <is>
-          <t>2026-02-20T07:33:59</t>
+          <t>2026-02-20T09:27:20</t>
         </is>
       </c>
       <c r="O282" t="inlineStr">
@@ -19414,7 +19414,7 @@
       </c>
       <c r="N283" t="inlineStr">
         <is>
-          <t>2026-02-19T19:34:48</t>
+          <t>2026-02-20T08:58:20</t>
         </is>
       </c>
       <c r="O283" t="inlineStr">
@@ -19480,7 +19480,7 @@
       </c>
       <c r="N284" t="inlineStr">
         <is>
-          <t>2026-02-19T19:12:37</t>
+          <t>2026-02-20T08:56:49</t>
         </is>
       </c>
       <c r="O284" t="inlineStr">
@@ -19546,7 +19546,7 @@
       </c>
       <c r="N285" t="inlineStr">
         <is>
-          <t>2026-02-19T18:55:19</t>
+          <t>2026-02-20T09:37:45</t>
         </is>
       </c>
       <c r="O285" t="inlineStr">
@@ -19566,11 +19566,6 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
-      <c r="C286" t="inlineStr">
-        <is>
-          <t>10.69.5.155</t>
-        </is>
-      </c>
       <c r="D286" t="n">
         <v>2019</v>
       </c>
@@ -19612,7 +19607,7 @@
       </c>
       <c r="N286" t="inlineStr">
         <is>
-          <t>2026-02-20T02:10:20</t>
+          <t>2026-02-20T07:51:40</t>
         </is>
       </c>
       <c r="O286" t="inlineStr">
@@ -19678,7 +19673,7 @@
       </c>
       <c r="N287" t="inlineStr">
         <is>
-          <t>2026-02-20T07:37:52</t>
+          <t>2026-02-20T09:25:47</t>
         </is>
       </c>
       <c r="O287" t="inlineStr">
@@ -19744,7 +19739,7 @@
       </c>
       <c r="N288" t="inlineStr">
         <is>
-          <t>2026-02-20T07:33:51</t>
+          <t>2026-02-20T09:24:25</t>
         </is>
       </c>
       <c r="O288" t="inlineStr">
@@ -20630,7 +20625,7 @@
       </c>
       <c r="N302" t="inlineStr">
         <is>
-          <t>2026-02-20T07:38:44</t>
+          <t>2026-02-20T09:28:22</t>
         </is>
       </c>
       <c r="O302" t="inlineStr">
@@ -21782,7 +21777,7 @@
       </c>
       <c r="N320" t="inlineStr">
         <is>
-          <t>2026-02-20T06:54:40</t>
+          <t>2026-02-20T09:31:42</t>
         </is>
       </c>
       <c r="O320" t="inlineStr">
@@ -22531,7 +22526,7 @@
       </c>
       <c r="N332" t="inlineStr">
         <is>
-          <t>2026-02-20T07:38:58</t>
+          <t>2026-02-20T09:24:53</t>
         </is>
       </c>
       <c r="O332" t="inlineStr">
@@ -22597,7 +22592,7 @@
       </c>
       <c r="N333" t="inlineStr">
         <is>
-          <t>2026-02-20T07:35:55</t>
+          <t>2026-02-20T09:21:28</t>
         </is>
       </c>
       <c r="O333" t="inlineStr">
@@ -22663,7 +22658,7 @@
       </c>
       <c r="N334" t="inlineStr">
         <is>
-          <t>2026-02-20T07:41:51</t>
+          <t>2026-02-20T09:35:04</t>
         </is>
       </c>
       <c r="O334" t="inlineStr">
@@ -22729,7 +22724,7 @@
       </c>
       <c r="N335" t="inlineStr">
         <is>
-          <t>2026-02-20T07:41:51</t>
+          <t>2026-02-20T09:37:34</t>
         </is>
       </c>
       <c r="O335" t="inlineStr">
@@ -22795,7 +22790,7 @@
       </c>
       <c r="N336" t="inlineStr">
         <is>
-          <t>2026-02-20T07:37:38</t>
+          <t>2026-02-20T09:19:36</t>
         </is>
       </c>
       <c r="O336" t="inlineStr">
@@ -22861,7 +22856,7 @@
       </c>
       <c r="N337" t="inlineStr">
         <is>
-          <t>2026-02-20T07:39:14</t>
+          <t>2026-02-20T09:36:47</t>
         </is>
       </c>
       <c r="O337" t="inlineStr">
@@ -22927,7 +22922,7 @@
       </c>
       <c r="N338" t="inlineStr">
         <is>
-          <t>2026-02-20T07:39:32</t>
+          <t>2026-02-20T09:26:24</t>
         </is>
       </c>
       <c r="O338" t="inlineStr">
@@ -22993,7 +22988,7 @@
       </c>
       <c r="N339" t="inlineStr">
         <is>
-          <t>2026-02-20T06:47:47</t>
+          <t>2026-02-20T09:32:15</t>
         </is>
       </c>
       <c r="O339" t="inlineStr">
@@ -23015,7 +23010,7 @@
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>10.69.5.234</t>
+          <t>10.69.2.194</t>
         </is>
       </c>
       <c r="D340" t="n">
@@ -23059,7 +23054,7 @@
       </c>
       <c r="N340" t="inlineStr">
         <is>
-          <t>2026-02-14T07:33:11</t>
+          <t>2026-02-20T08:54:23</t>
         </is>
       </c>
       <c r="O340" t="inlineStr">
@@ -23125,7 +23120,7 @@
       </c>
       <c r="N341" t="inlineStr">
         <is>
-          <t>2026-02-19T13:43:55</t>
+          <t>2026-02-20T09:04:08</t>
         </is>
       </c>
       <c r="O341" t="inlineStr">
@@ -23191,7 +23186,7 @@
       </c>
       <c r="N342" t="inlineStr">
         <is>
-          <t>2026-02-19T13:18:58</t>
+          <t>2026-02-20T09:10:35</t>
         </is>
       </c>
       <c r="O342" t="inlineStr">
@@ -23211,6 +23206,11 @@
           <t>OPERACAO 9.1</t>
         </is>
       </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>10.69.5.237</t>
+        </is>
+      </c>
       <c r="D343" t="n">
         <v>2017</v>
       </c>
@@ -23254,7 +23254,7 @@
       </c>
       <c r="N343" t="inlineStr">
         <is>
-          <t>2026-02-19T16:50:10</t>
+          <t>2026-02-20T09:33:05</t>
         </is>
       </c>
       <c r="O343" t="inlineStr">
@@ -23518,7 +23518,7 @@
       </c>
       <c r="N347" t="inlineStr">
         <is>
-          <t>2026-02-19T14:33:25</t>
+          <t>2026-02-20T09:07:34</t>
         </is>
       </c>
       <c r="O347" t="inlineStr">
@@ -23584,7 +23584,7 @@
       </c>
       <c r="N348" t="inlineStr">
         <is>
-          <t>2026-02-19T09:42:14</t>
+          <t>2026-02-20T09:08:42</t>
         </is>
       </c>
       <c r="O348" t="inlineStr">
@@ -23650,7 +23650,7 @@
       </c>
       <c r="N349" t="inlineStr">
         <is>
-          <t>2026-02-19T09:39:12</t>
+          <t>2026-02-20T09:08:26</t>
         </is>
       </c>
       <c r="O349" t="inlineStr">
@@ -23777,7 +23777,7 @@
       </c>
       <c r="N351" t="inlineStr">
         <is>
-          <t>2026-02-19T09:45:14</t>
+          <t>2026-02-20T09:10:04</t>
         </is>
       </c>
       <c r="O351" t="inlineStr">
@@ -23843,7 +23843,7 @@
       </c>
       <c r="N352" t="inlineStr">
         <is>
-          <t>2026-02-19T09:48:02</t>
+          <t>2026-02-20T09:11:59</t>
         </is>
       </c>
       <c r="O352" t="inlineStr">
@@ -23906,7 +23906,7 @@
       </c>
       <c r="N353" t="inlineStr">
         <is>
-          <t>2026-02-19T08:45:22</t>
+          <t>2026-02-20T09:07:45</t>
         </is>
       </c>
       <c r="O353" t="inlineStr">
@@ -23969,7 +23969,7 @@
       </c>
       <c r="N354" t="inlineStr">
         <is>
-          <t>2026-02-19T14:20:10</t>
+          <t>2026-02-20T09:07:09</t>
         </is>
       </c>
       <c r="O354" t="inlineStr">
@@ -24035,7 +24035,7 @@
       </c>
       <c r="N355" t="inlineStr">
         <is>
-          <t>2026-02-19T14:13:47</t>
+          <t>2026-02-20T09:06:17</t>
         </is>
       </c>
       <c r="O355" t="inlineStr">
@@ -24101,7 +24101,7 @@
       </c>
       <c r="N356" t="inlineStr">
         <is>
-          <t>2026-02-19T11:33:15</t>
+          <t>2026-02-20T09:07:00</t>
         </is>
       </c>
       <c r="O356" t="inlineStr">
@@ -24294,7 +24294,7 @@
       </c>
       <c r="N359" t="inlineStr">
         <is>
-          <t>2026-02-19T11:28:48</t>
+          <t>2026-02-20T09:07:48</t>
         </is>
       </c>
       <c r="O359" t="inlineStr">
@@ -24360,7 +24360,7 @@
       </c>
       <c r="N360" t="inlineStr">
         <is>
-          <t>2026-02-19T14:19:32</t>
+          <t>2026-02-20T09:07:35</t>
         </is>
       </c>
       <c r="O360" t="inlineStr">
@@ -24426,7 +24426,7 @@
       </c>
       <c r="N361" t="inlineStr">
         <is>
-          <t>2026-02-19T14:30:38</t>
+          <t>2026-02-20T09:06:41</t>
         </is>
       </c>
       <c r="O361" t="inlineStr">
@@ -24489,7 +24489,7 @@
       </c>
       <c r="N362" t="inlineStr">
         <is>
-          <t>2026-02-19T14:07:42</t>
+          <t>2026-02-20T09:08:24</t>
         </is>
       </c>
       <c r="O362" t="inlineStr">
@@ -24683,7 +24683,7 @@
       </c>
       <c r="N365" t="inlineStr">
         <is>
-          <t>2026-02-19T16:12:43</t>
+          <t>2026-02-20T08:58:19</t>
         </is>
       </c>
       <c r="O365" t="inlineStr">
@@ -24751,7 +24751,7 @@
       </c>
       <c r="N366" t="inlineStr">
         <is>
-          <t>2026-02-20T06:59:16</t>
+          <t>2026-02-20T08:50:43</t>
         </is>
       </c>
       <c r="O366" t="inlineStr">
@@ -24881,7 +24881,7 @@
       </c>
       <c r="N368" t="inlineStr">
         <is>
-          <t>2026-02-19T16:34:57</t>
+          <t>2026-02-20T09:35:51</t>
         </is>
       </c>
       <c r="O368" t="inlineStr">
@@ -24901,6 +24901,11 @@
           <t>RH</t>
         </is>
       </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>10.69.3.13</t>
+        </is>
+      </c>
       <c r="D369" t="n">
         <v>2025</v>
       </c>
@@ -24944,7 +24949,7 @@
       </c>
       <c r="N369" t="inlineStr">
         <is>
-          <t>2026-02-19T17:25:53</t>
+          <t>2026-02-20T09:33:29</t>
         </is>
       </c>
       <c r="O369" t="inlineStr">
@@ -25015,7 +25020,7 @@
       </c>
       <c r="N370" t="inlineStr">
         <is>
-          <t>2026-02-19T18:01:11</t>
+          <t>2026-02-20T09:25:13</t>
         </is>
       </c>
       <c r="O370" t="inlineStr">
@@ -25299,7 +25304,7 @@
       </c>
       <c r="N374" t="inlineStr">
         <is>
-          <t>2026-02-19T18:25:58</t>
+          <t>2026-02-20T09:20:35</t>
         </is>
       </c>
       <c r="O374" t="inlineStr">
@@ -25367,7 +25372,7 @@
       </c>
       <c r="N375" t="inlineStr">
         <is>
-          <t>2026-02-20T07:08:29</t>
+          <t>2026-02-20T09:01:41</t>
         </is>
       </c>
       <c r="O375" t="inlineStr">
@@ -25387,11 +25392,6 @@
           <t>COORDENACAO</t>
         </is>
       </c>
-      <c r="C376" t="inlineStr">
-        <is>
-          <t>10.69.3.72</t>
-        </is>
-      </c>
       <c r="D376" t="n">
         <v>2025</v>
       </c>
@@ -25438,7 +25438,7 @@
       </c>
       <c r="N376" t="inlineStr">
         <is>
-          <t>2026-02-20T06:56:45</t>
+          <t>2026-02-20T08:50:43</t>
         </is>
       </c>
       <c r="O376" t="inlineStr">
@@ -25509,7 +25509,7 @@
       </c>
       <c r="N377" t="inlineStr">
         <is>
-          <t>2026-02-19T17:01:02</t>
+          <t>2026-02-20T09:19:15</t>
         </is>
       </c>
       <c r="O377" t="inlineStr">
@@ -25580,7 +25580,7 @@
       </c>
       <c r="N378" t="inlineStr">
         <is>
-          <t>2026-02-20T07:00:08</t>
+          <t>2026-02-20T08:57:28</t>
         </is>
       </c>
       <c r="O378" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática 2026-02-20 11:52:03.787432
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -19,13 +19,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -36,7 +39,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -44,12 +47,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
@@ -445,87 +457,87 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Nome do computador</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Setor</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>IP</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Ano de compra</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>NF</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Sistema operacional instalado</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Serial</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Office instalado</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Processador</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Total Memória RAM</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Fabricante</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Modelo</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Monitores conectados</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Última Atualização</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Observação</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Data baixa</t>
         </is>
@@ -591,8 +603,8 @@
       <c r="M2" t="n">
         <v>1</v>
       </c>
-      <c r="N2" s="2" t="n">
-        <v>46073.39909722222</v>
+      <c r="N2" s="3" t="n">
+        <v>46073.47710648148</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -660,8 +672,8 @@
       <c r="M3" t="n">
         <v>1</v>
       </c>
-      <c r="N3" s="2" t="n">
-        <v>46073.38163194444</v>
+      <c r="N3" s="3" t="n">
+        <v>46073.46390046296</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -729,8 +741,8 @@
       <c r="M4" t="n">
         <v>2</v>
       </c>
-      <c r="N4" s="2" t="n">
-        <v>46073.37829861111</v>
+      <c r="N4" s="3" t="n">
+        <v>46073.4574537037</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -798,8 +810,8 @@
       <c r="M5" t="n">
         <v>1</v>
       </c>
-      <c r="N5" s="2" t="n">
-        <v>46073.37636574074</v>
+      <c r="N5" s="3" t="n">
+        <v>46073.45621527778</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -862,7 +874,7 @@
       <c r="M6" t="n">
         <v>1</v>
       </c>
-      <c r="N6" s="2" t="n">
+      <c r="N6" s="3" t="n">
         <v>46064.4572800926</v>
       </c>
       <c r="O6" t="inlineStr">
@@ -931,7 +943,7 @@
       <c r="M7" t="n">
         <v>1</v>
       </c>
-      <c r="N7" s="2" t="n">
+      <c r="N7" s="3" t="n">
         <v>46064.42020833334</v>
       </c>
       <c r="O7" t="inlineStr">
@@ -995,7 +1007,7 @@
       <c r="M8" t="n">
         <v>1</v>
       </c>
-      <c r="N8" s="2" t="n">
+      <c r="N8" s="3" t="n">
         <v>46064.45694444444</v>
       </c>
       <c r="O8" t="inlineStr">
@@ -1059,7 +1071,7 @@
       <c r="M9" t="n">
         <v>1</v>
       </c>
-      <c r="N9" s="2" t="n">
+      <c r="N9" s="3" t="n">
         <v>46066.60008101852</v>
       </c>
       <c r="O9" t="inlineStr">
@@ -1118,8 +1130,8 @@
       <c r="M10" t="n">
         <v>1</v>
       </c>
-      <c r="N10" s="2" t="n">
-        <v>46073.39240740741</v>
+      <c r="N10" s="3" t="n">
+        <v>46073.47350694444</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1182,7 +1194,7 @@
       <c r="M11" t="n">
         <v>1</v>
       </c>
-      <c r="N11" s="2" t="n">
+      <c r="N11" s="3" t="n">
         <v>46062.63414351852</v>
       </c>
       <c r="O11" t="inlineStr">
@@ -1246,7 +1258,7 @@
       <c r="M12" t="n">
         <v>1</v>
       </c>
-      <c r="N12" s="2" t="n">
+      <c r="N12" s="3" t="n">
         <v>46064.45525462963</v>
       </c>
       <c r="O12" t="inlineStr">
@@ -1310,7 +1322,7 @@
       <c r="M13" t="n">
         <v>1</v>
       </c>
-      <c r="N13" s="2" t="n">
+      <c r="N13" s="3" t="n">
         <v>46064.46146990741</v>
       </c>
       <c r="O13" t="inlineStr">
@@ -1374,7 +1386,7 @@
       <c r="M14" t="n">
         <v>2</v>
       </c>
-      <c r="N14" s="2" t="n">
+      <c r="N14" s="3" t="n">
         <v>46064.45708333333</v>
       </c>
       <c r="O14" t="inlineStr">
@@ -1438,8 +1450,8 @@
       <c r="M15" t="n">
         <v>1</v>
       </c>
-      <c r="N15" s="2" t="n">
-        <v>46073.37619212963</v>
+      <c r="N15" s="3" t="n">
+        <v>46073.45480324074</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1502,8 +1514,8 @@
       <c r="M16" t="n">
         <v>2</v>
       </c>
-      <c r="N16" s="2" t="n">
-        <v>46073.39782407408</v>
+      <c r="N16" s="3" t="n">
+        <v>46073.47081018519</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1566,7 +1578,7 @@
       <c r="M17" t="n">
         <v>1</v>
       </c>
-      <c r="N17" s="2" t="n">
+      <c r="N17" s="3" t="n">
         <v>46072.59577546296</v>
       </c>
       <c r="O17" t="inlineStr">
@@ -1630,7 +1642,7 @@
       <c r="M18" t="n">
         <v>2</v>
       </c>
-      <c r="N18" s="2" t="n">
+      <c r="N18" s="3" t="n">
         <v>46066.59618055556</v>
       </c>
       <c r="O18" t="inlineStr">
@@ -1691,7 +1703,7 @@
           <t>HP ProDesk 400 G4 SFF</t>
         </is>
       </c>
-      <c r="N19" s="2" t="n">
+      <c r="N19" s="3" t="n">
         <v>45995.65027777778</v>
       </c>
       <c r="O19" t="inlineStr">
@@ -1755,7 +1767,7 @@
       <c r="M20" t="n">
         <v>1</v>
       </c>
-      <c r="N20" s="2" t="n">
+      <c r="N20" s="3" t="n">
         <v>46066.59634259259</v>
       </c>
       <c r="O20" t="inlineStr">
@@ -1819,7 +1831,7 @@
       <c r="M21" t="n">
         <v>1</v>
       </c>
-      <c r="N21" s="2" t="n">
+      <c r="N21" s="3" t="n">
         <v>46064.47733796296</v>
       </c>
       <c r="O21" t="inlineStr">
@@ -1878,7 +1890,7 @@
       <c r="M22" t="n">
         <v>1</v>
       </c>
-      <c r="N22" s="2" t="n">
+      <c r="N22" s="3" t="n">
         <v>46066.61251157407</v>
       </c>
       <c r="O22" t="inlineStr">
@@ -1937,7 +1949,7 @@
       <c r="M23" t="n">
         <v>1</v>
       </c>
-      <c r="N23" s="2" t="n">
+      <c r="N23" s="3" t="n">
         <v>46064.41899305556</v>
       </c>
       <c r="O23" t="inlineStr">
@@ -1996,7 +2008,7 @@
       <c r="M24" t="n">
         <v>1</v>
       </c>
-      <c r="N24" s="2" t="n">
+      <c r="N24" s="3" t="n">
         <v>46058.21155092592</v>
       </c>
       <c r="O24" t="inlineStr">
@@ -2052,7 +2064,7 @@
           <t>HP 402 G1 SFF Business PC</t>
         </is>
       </c>
-      <c r="N25" s="2" t="n">
+      <c r="N25" s="3" t="n">
         <v>46063.72092592593</v>
       </c>
       <c r="O25" t="inlineStr">
@@ -2111,7 +2123,7 @@
       <c r="M26" t="n">
         <v>1</v>
       </c>
-      <c r="N26" s="2" t="n">
+      <c r="N26" s="3" t="n">
         <v>46064.45631944444</v>
       </c>
       <c r="O26" t="inlineStr">
@@ -2170,7 +2182,7 @@
       <c r="M27" t="n">
         <v>1</v>
       </c>
-      <c r="N27" s="2" t="n">
+      <c r="N27" s="3" t="n">
         <v>46064.45870370371</v>
       </c>
       <c r="O27" t="inlineStr">
@@ -2231,7 +2243,7 @@
           <t>HP ProDesk 400 G4 SFF</t>
         </is>
       </c>
-      <c r="N28" s="2" t="n">
+      <c r="N28" s="3" t="n">
         <v>46072.74151620371</v>
       </c>
       <c r="O28" t="inlineStr">
@@ -2287,7 +2299,7 @@
           <t>HP Compaq Pro 4300 SFF Brazil PC</t>
         </is>
       </c>
-      <c r="N29" s="2" t="n">
+      <c r="N29" s="3" t="n">
         <v>45758.33916666666</v>
       </c>
       <c r="O29" t="inlineStr">
@@ -2295,7 +2307,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q29" s="2" t="n">
+      <c r="Q29" s="3" t="n">
         <v>45758</v>
       </c>
     </row>
@@ -2346,7 +2358,7 @@
           <t>HP Compaq Pro 4300 SFF Brazil PC</t>
         </is>
       </c>
-      <c r="N30" s="2" t="n">
+      <c r="N30" s="3" t="n">
         <v>45758.34476851852</v>
       </c>
       <c r="O30" t="inlineStr">
@@ -2354,7 +2366,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q30" s="2" t="n">
+      <c r="Q30" s="3" t="n">
         <v>45520</v>
       </c>
     </row>
@@ -2405,7 +2417,7 @@
           <t>HP Compaq 6005 Pro SFF PC</t>
         </is>
       </c>
-      <c r="N31" s="2" t="n">
+      <c r="N31" s="3" t="n">
         <v>45758.34480324074</v>
       </c>
       <c r="O31" t="inlineStr">
@@ -2413,7 +2425,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q31" s="2" t="n">
+      <c r="Q31" s="3" t="n">
         <v>45520</v>
       </c>
     </row>
@@ -2464,7 +2476,7 @@
           <t>HP 402 G1 SFF Business PC</t>
         </is>
       </c>
-      <c r="N32" s="2" t="n">
+      <c r="N32" s="3" t="n">
         <v>45758.34482638889</v>
       </c>
       <c r="O32" t="inlineStr">
@@ -2472,7 +2484,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q32" s="2" t="n">
+      <c r="Q32" s="3" t="n">
         <v>45520</v>
       </c>
     </row>
@@ -2523,7 +2535,7 @@
           <t>OptiPlex 745</t>
         </is>
       </c>
-      <c r="N33" s="2" t="n">
+      <c r="N33" s="3" t="n">
         <v>45758.34486111111</v>
       </c>
       <c r="O33" t="inlineStr">
@@ -2531,7 +2543,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q33" s="2" t="n">
+      <c r="Q33" s="3" t="n">
         <v>45520</v>
       </c>
     </row>
@@ -2582,7 +2594,7 @@
           <t>HP Pro 3410 Series</t>
         </is>
       </c>
-      <c r="N34" s="2" t="n">
+      <c r="N34" s="3" t="n">
         <v>45758.34511574074</v>
       </c>
       <c r="O34" t="inlineStr">
@@ -2590,7 +2602,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q34" s="2" t="n">
+      <c r="Q34" s="3" t="n">
         <v>45520</v>
       </c>
     </row>
@@ -2641,7 +2653,7 @@
           <t>HP Compaq Pro 4300 SFF Brazil PC</t>
         </is>
       </c>
-      <c r="N35" s="2" t="n">
+      <c r="N35" s="3" t="n">
         <v>45758.34513888889</v>
       </c>
       <c r="O35" t="inlineStr">
@@ -2649,7 +2661,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q35" s="2" t="n">
+      <c r="Q35" s="3" t="n">
         <v>45520</v>
       </c>
     </row>
@@ -2700,7 +2712,7 @@
           <t>ThinkCentre A55</t>
         </is>
       </c>
-      <c r="N36" s="2" t="n">
+      <c r="N36" s="3" t="n">
         <v>45758.34517361111</v>
       </c>
       <c r="O36" t="inlineStr">
@@ -2708,7 +2720,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q36" s="2" t="n">
+      <c r="Q36" s="3" t="n">
         <v>44960</v>
       </c>
     </row>
@@ -2759,7 +2771,7 @@
           <t>KE642AA-AC4 dx2295MT</t>
         </is>
       </c>
-      <c r="N37" s="2" t="n">
+      <c r="N37" s="3" t="n">
         <v>45758.34525462963</v>
       </c>
       <c r="O37" t="inlineStr">
@@ -2767,7 +2779,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q37" s="2" t="n">
+      <c r="Q37" s="3" t="n">
         <v>44945</v>
       </c>
     </row>
@@ -2818,7 +2830,7 @@
           <t>HP Compaq Pro 4300 SFF Brazil PC</t>
         </is>
       </c>
-      <c r="N38" s="2" t="n">
+      <c r="N38" s="3" t="n">
         <v>45758.34527777778</v>
       </c>
       <c r="O38" t="inlineStr">
@@ -2826,7 +2838,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q38" s="2" t="n">
+      <c r="Q38" s="3" t="n">
         <v>44937</v>
       </c>
     </row>
@@ -2877,7 +2889,7 @@
           <t>HP Compaq Pro 4300 SFF Brazil PC</t>
         </is>
       </c>
-      <c r="N39" s="2" t="n">
+      <c r="N39" s="3" t="n">
         <v>45758.34528935186</v>
       </c>
       <c r="O39" t="inlineStr">
@@ -2885,7 +2897,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q39" s="2" t="n">
+      <c r="Q39" s="3" t="n">
         <v>44937</v>
       </c>
     </row>
@@ -2936,7 +2948,7 @@
           <t>OptiPlex 755</t>
         </is>
       </c>
-      <c r="N40" s="2" t="n">
+      <c r="N40" s="3" t="n">
         <v>45758.3453125</v>
       </c>
       <c r="O40" t="inlineStr">
@@ -2944,7 +2956,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q40" s="2" t="n">
+      <c r="Q40" s="3" t="n">
         <v>44937</v>
       </c>
     </row>
@@ -2995,7 +3007,7 @@
           <t>OptiPlex 755</t>
         </is>
       </c>
-      <c r="N41" s="2" t="n">
+      <c r="N41" s="3" t="n">
         <v>45758.34533564815</v>
       </c>
       <c r="O41" t="inlineStr">
@@ -3003,7 +3015,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q41" s="2" t="n">
+      <c r="Q41" s="3" t="n">
         <v>44742</v>
       </c>
     </row>
@@ -3054,7 +3066,7 @@
           <t>OptiPlex 755</t>
         </is>
       </c>
-      <c r="N42" s="2" t="n">
+      <c r="N42" s="3" t="n">
         <v>45758.34538194445</v>
       </c>
       <c r="O42" t="inlineStr">
@@ -3062,7 +3074,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q42" s="2" t="n">
+      <c r="Q42" s="3" t="n">
         <v>44742</v>
       </c>
     </row>
@@ -3113,7 +3125,7 @@
           <t>OptiPlex 755</t>
         </is>
       </c>
-      <c r="N43" s="2" t="n">
+      <c r="N43" s="3" t="n">
         <v>45758.34565972222</v>
       </c>
       <c r="O43" t="inlineStr">
@@ -3121,7 +3133,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q43" s="2" t="n">
+      <c r="Q43" s="3" t="n">
         <v>44742</v>
       </c>
     </row>
@@ -3172,7 +3184,7 @@
           <t>KE642AA-AC4 dx2295MT</t>
         </is>
       </c>
-      <c r="N44" s="2" t="n">
+      <c r="N44" s="3" t="n">
         <v>45758.34570601852</v>
       </c>
       <c r="O44" t="inlineStr">
@@ -3180,7 +3192,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q44" s="2" t="n">
+      <c r="Q44" s="3" t="n">
         <v>44742</v>
       </c>
     </row>
@@ -3231,7 +3243,7 @@
           <t>HP Compaq dc5750 Small Form Factor</t>
         </is>
       </c>
-      <c r="N45" s="2" t="n">
+      <c r="N45" s="3" t="n">
         <v>45758.34572916666</v>
       </c>
       <c r="O45" t="inlineStr">
@@ -3239,7 +3251,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q45" s="2" t="n">
+      <c r="Q45" s="3" t="n">
         <v>44742</v>
       </c>
     </row>
@@ -3290,7 +3302,7 @@
           <t>KE642AA-AC4 dx2295MT</t>
         </is>
       </c>
-      <c r="N46" s="2" t="n">
+      <c r="N46" s="3" t="n">
         <v>45758.34574074074</v>
       </c>
       <c r="O46" t="inlineStr">
@@ -3298,7 +3310,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q46" s="2" t="n">
+      <c r="Q46" s="3" t="n">
         <v>44742</v>
       </c>
     </row>
@@ -3349,7 +3361,7 @@
           <t>KE642AA-AC4 dx2295MT</t>
         </is>
       </c>
-      <c r="N47" s="2" t="n">
+      <c r="N47" s="3" t="n">
         <v>45758.34576388889</v>
       </c>
       <c r="O47" t="inlineStr">
@@ -3357,7 +3369,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q47" s="2" t="n">
+      <c r="Q47" s="3" t="n">
         <v>44742</v>
       </c>
     </row>
@@ -3408,7 +3420,7 @@
           <t>KE642AA-AC4 dx2295MT</t>
         </is>
       </c>
-      <c r="N48" s="2" t="n">
+      <c r="N48" s="3" t="n">
         <v>45758.34578703704</v>
       </c>
       <c r="O48" t="inlineStr">
@@ -3416,7 +3428,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q48" s="2" t="n">
+      <c r="Q48" s="3" t="n">
         <v>44742</v>
       </c>
     </row>
@@ -3467,7 +3479,7 @@
           <t>KE642AA-AC4 dx2295MT</t>
         </is>
       </c>
-      <c r="N49" s="2" t="n">
+      <c r="N49" s="3" t="n">
         <v>45758.34582175926</v>
       </c>
       <c r="O49" t="inlineStr">
@@ -3475,7 +3487,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q49" s="2" t="n">
+      <c r="Q49" s="3" t="n">
         <v>44742</v>
       </c>
     </row>
@@ -3526,7 +3538,7 @@
           <t>KE642AA-AC4 dx2295MT</t>
         </is>
       </c>
-      <c r="N50" s="2" t="n">
+      <c r="N50" s="3" t="n">
         <v>45758.34586805556</v>
       </c>
       <c r="O50" t="inlineStr">
@@ -3534,7 +3546,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q50" s="2" t="n">
+      <c r="Q50" s="3" t="n">
         <v>44742</v>
       </c>
     </row>
@@ -3585,7 +3597,7 @@
           <t>HP Compaq dc5750 Small Form Factor</t>
         </is>
       </c>
-      <c r="N51" s="2" t="n">
+      <c r="N51" s="3" t="n">
         <v>45758.3458912037</v>
       </c>
       <c r="O51" t="inlineStr">
@@ -3593,7 +3605,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q51" s="2" t="n">
+      <c r="Q51" s="3" t="n">
         <v>44742</v>
       </c>
     </row>
@@ -3644,7 +3656,7 @@
           <t>HP Compaq dc5750 Small Form Factor</t>
         </is>
       </c>
-      <c r="N52" s="2" t="n">
+      <c r="N52" s="3" t="n">
         <v>45758.34607638889</v>
       </c>
       <c r="O52" t="inlineStr">
@@ -3652,7 +3664,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q52" s="2" t="n">
+      <c r="Q52" s="3" t="n">
         <v>44742</v>
       </c>
     </row>
@@ -3703,7 +3715,7 @@
           <t>KE642AA-AC4 dx2295MT</t>
         </is>
       </c>
-      <c r="N53" s="2" t="n">
+      <c r="N53" s="3" t="n">
         <v>45758.34609953704</v>
       </c>
       <c r="O53" t="inlineStr">
@@ -3711,7 +3723,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q53" s="2" t="n">
+      <c r="Q53" s="3" t="n">
         <v>44742</v>
       </c>
     </row>
@@ -3762,7 +3774,7 @@
           <t>HP Compaq dc5700 Microtower</t>
         </is>
       </c>
-      <c r="N54" s="2" t="n">
+      <c r="N54" s="3" t="n">
         <v>45758.34611111111</v>
       </c>
       <c r="O54" t="inlineStr">
@@ -3770,7 +3782,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q54" s="2" t="n">
+      <c r="Q54" s="3" t="n">
         <v>44742</v>
       </c>
     </row>
@@ -3821,7 +3833,7 @@
           <t>KE642AA-AC4 dx2295MT</t>
         </is>
       </c>
-      <c r="N55" s="2" t="n">
+      <c r="N55" s="3" t="n">
         <v>45758.34614583333</v>
       </c>
       <c r="O55" t="inlineStr">
@@ -3829,7 +3841,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q55" s="2" t="n">
+      <c r="Q55" s="3" t="n">
         <v>44742</v>
       </c>
     </row>
@@ -3880,7 +3892,7 @@
           <t>HP Compaq dc5700 Microtower</t>
         </is>
       </c>
-      <c r="N56" s="2" t="n">
+      <c r="N56" s="3" t="n">
         <v>45758.34618055556</v>
       </c>
       <c r="O56" t="inlineStr">
@@ -3888,7 +3900,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q56" s="2" t="n">
+      <c r="Q56" s="3" t="n">
         <v>44742</v>
       </c>
     </row>
@@ -3939,7 +3951,7 @@
           <t>HP Compaq dc5750 Small Form Factor</t>
         </is>
       </c>
-      <c r="N57" s="2" t="n">
+      <c r="N57" s="3" t="n">
         <v>45758.3462037037</v>
       </c>
       <c r="O57" t="inlineStr">
@@ -3947,7 +3959,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q57" s="2" t="n">
+      <c r="Q57" s="3" t="n">
         <v>44742</v>
       </c>
     </row>
@@ -3998,7 +4010,7 @@
           <t>HP Compaq dc5750 Small Form Factor</t>
         </is>
       </c>
-      <c r="N58" s="2" t="n">
+      <c r="N58" s="3" t="n">
         <v>45758.34622685185</v>
       </c>
       <c r="O58" t="inlineStr">
@@ -4006,7 +4018,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q58" s="2" t="n">
+      <c r="Q58" s="3" t="n">
         <v>44742</v>
       </c>
     </row>
@@ -4057,7 +4069,7 @@
           <t>HP Compaq dc5750 Small Form Factor</t>
         </is>
       </c>
-      <c r="N59" s="2" t="n">
+      <c r="N59" s="3" t="n">
         <v>45758.34642361111</v>
       </c>
       <c r="O59" t="inlineStr">
@@ -4065,7 +4077,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q59" s="2" t="n">
+      <c r="Q59" s="3" t="n">
         <v>44742</v>
       </c>
     </row>
@@ -4116,7 +4128,7 @@
           <t>KE642AA-AC4 dx2295MT</t>
         </is>
       </c>
-      <c r="N60" s="2" t="n">
+      <c r="N60" s="3" t="n">
         <v>45758.34646990741</v>
       </c>
       <c r="O60" t="inlineStr">
@@ -4124,7 +4136,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q60" s="2" t="n">
+      <c r="Q60" s="3" t="n">
         <v>44742</v>
       </c>
     </row>
@@ -4175,7 +4187,7 @@
           <t>KE642AA-AC4 dx2295MT</t>
         </is>
       </c>
-      <c r="N61" s="2" t="n">
+      <c r="N61" s="3" t="n">
         <v>45758.34652777778</v>
       </c>
       <c r="O61" t="inlineStr">
@@ -4183,7 +4195,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q61" s="2" t="n">
+      <c r="Q61" s="3" t="n">
         <v>44742</v>
       </c>
     </row>
@@ -4234,7 +4246,7 @@
           <t>KE642AA-AC4 dx2295MT</t>
         </is>
       </c>
-      <c r="N62" s="2" t="n">
+      <c r="N62" s="3" t="n">
         <v>45758.3465625</v>
       </c>
       <c r="O62" t="inlineStr">
@@ -4242,7 +4254,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q62" s="2" t="n">
+      <c r="Q62" s="3" t="n">
         <v>44742</v>
       </c>
     </row>
@@ -4293,7 +4305,7 @@
           <t>KE642AA-AC4 dx2295MT</t>
         </is>
       </c>
-      <c r="N63" s="2" t="n">
+      <c r="N63" s="3" t="n">
         <v>45758.3469675926</v>
       </c>
       <c r="O63" t="inlineStr">
@@ -4301,7 +4313,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q63" s="2" t="n">
+      <c r="Q63" s="3" t="n">
         <v>44742</v>
       </c>
     </row>
@@ -4352,7 +4364,7 @@
           <t>OptiPlex 755</t>
         </is>
       </c>
-      <c r="N64" s="2" t="n">
+      <c r="N64" s="3" t="n">
         <v>45758.34694444444</v>
       </c>
       <c r="O64" t="inlineStr">
@@ -4360,7 +4372,7 @@
           <t>Descarte</t>
         </is>
       </c>
-      <c r="Q64" s="2" t="n">
+      <c r="Q64" s="3" t="n">
         <v>44742</v>
       </c>
     </row>
@@ -4416,7 +4428,7 @@
           <t>OptiPlex 360</t>
         </is>
       </c>
-      <c r="N65" s="2" t="n">
+      <c r="N65" s="3" t="n">
         <v>45824.70222222222</v>
       </c>
       <c r="O65" t="inlineStr">
@@ -4431,7 +4443,7 @@
 DATA DESCARTE 16-06-2025</t>
         </is>
       </c>
-      <c r="Q65" s="2" t="n">
+      <c r="Q65" s="3" t="n">
         <v>45824</v>
       </c>
     </row>
@@ -4487,7 +4499,7 @@
           <t>OptiPlex 745</t>
         </is>
       </c>
-      <c r="N66" s="2" t="n">
+      <c r="N66" s="3" t="n">
         <v>45824.70469907407</v>
       </c>
       <c r="O66" t="inlineStr">
@@ -4502,7 +4514,7 @@
 DATA DESCARTE 16-06-2025</t>
         </is>
       </c>
-      <c r="Q66" s="2" t="n">
+      <c r="Q66" s="3" t="n">
         <v>45824</v>
       </c>
     </row>
@@ -4558,7 +4570,7 @@
           <t>OptiPlex 745</t>
         </is>
       </c>
-      <c r="N67" s="2" t="n">
+      <c r="N67" s="3" t="n">
         <v>45824.70399305555</v>
       </c>
       <c r="O67" t="inlineStr">
@@ -4573,7 +4585,7 @@
 DATA DESCARTE 16-06-2025</t>
         </is>
       </c>
-      <c r="Q67" s="2" t="n">
+      <c r="Q67" s="3" t="n">
         <v>45824</v>
       </c>
     </row>
@@ -4629,7 +4641,7 @@
           <t>OptiPlex 360</t>
         </is>
       </c>
-      <c r="N68" s="2" t="n">
+      <c r="N68" s="3" t="n">
         <v>45835.61572916667</v>
       </c>
       <c r="O68" t="inlineStr">
@@ -4644,7 +4656,7 @@
 27/06/2025</t>
         </is>
       </c>
-      <c r="Q68" s="2" t="n">
+      <c r="Q68" s="3" t="n">
         <v>45835</v>
       </c>
     </row>
@@ -4700,7 +4712,7 @@
           <t>HP Compaq Pro 4300 SFF Brazil PC</t>
         </is>
       </c>
-      <c r="N69" s="2" t="n">
+      <c r="N69" s="3" t="n">
         <v>45835.62068287037</v>
       </c>
       <c r="O69" t="inlineStr">
@@ -4715,7 +4727,7 @@
 27/06/2025</t>
         </is>
       </c>
-      <c r="Q69" s="2" t="n">
+      <c r="Q69" s="3" t="n">
         <v>45835</v>
       </c>
     </row>
@@ -4776,7 +4788,7 @@
           <t>HP 402 G1 SFF Business PC</t>
         </is>
       </c>
-      <c r="N70" s="2" t="n">
+      <c r="N70" s="3" t="n">
         <v>45835.62427083333</v>
       </c>
       <c r="O70" t="inlineStr">
@@ -4791,7 +4803,7 @@
 27/06/2025</t>
         </is>
       </c>
-      <c r="Q70" s="2" t="n">
+      <c r="Q70" s="3" t="n">
         <v>45835</v>
       </c>
     </row>
@@ -4847,7 +4859,7 @@
           <t>HP Compaq Pro 4300 SFF Brazil PC</t>
         </is>
       </c>
-      <c r="N71" s="2" t="n">
+      <c r="N71" s="3" t="n">
         <v>45835.62575231482</v>
       </c>
       <c r="O71" t="inlineStr">
@@ -4862,7 +4874,7 @@
 27/06/2025</t>
         </is>
       </c>
-      <c r="Q71" s="2" t="n">
+      <c r="Q71" s="3" t="n">
         <v>45835</v>
       </c>
     </row>
@@ -4918,7 +4930,7 @@
           <t>HP Compaq dc7800p Convertible Minitower</t>
         </is>
       </c>
-      <c r="N72" s="2" t="n">
+      <c r="N72" s="3" t="n">
         <v>45838.58099537037</v>
       </c>
       <c r="O72" t="inlineStr">
@@ -4933,7 +4945,7 @@
 ANTIGA PA_074</t>
         </is>
       </c>
-      <c r="Q72" s="2" t="n">
+      <c r="Q72" s="3" t="n">
         <v>45838</v>
       </c>
     </row>
@@ -4989,7 +5001,7 @@
           <t>OptiPlex 745</t>
         </is>
       </c>
-      <c r="N73" s="2" t="n">
+      <c r="N73" s="3" t="n">
         <v>45838.61657407408</v>
       </c>
       <c r="O73" t="inlineStr">
@@ -5004,7 +5016,7 @@
 30/06/2025</t>
         </is>
       </c>
-      <c r="Q73" s="2" t="n">
+      <c r="Q73" s="3" t="n">
         <v>45838</v>
       </c>
     </row>
@@ -5060,7 +5072,7 @@
           <t>ThinkCentre M55e</t>
         </is>
       </c>
-      <c r="N74" s="2" t="n">
+      <c r="N74" s="3" t="n">
         <v>45841.49379629629</v>
       </c>
       <c r="O74" t="inlineStr">
@@ -5075,7 +5087,7 @@
 03/07/2025</t>
         </is>
       </c>
-      <c r="Q74" s="2" t="n">
+      <c r="Q74" s="3" t="n">
         <v>45841</v>
       </c>
     </row>
@@ -5131,7 +5143,7 @@
           <t>OptiPlex 745</t>
         </is>
       </c>
-      <c r="N75" s="2" t="n">
+      <c r="N75" s="3" t="n">
         <v>45841.49898148148</v>
       </c>
       <c r="O75" t="inlineStr">
@@ -5146,7 +5158,7 @@
 ANTIGA PA_207</t>
         </is>
       </c>
-      <c r="Q75" s="2" t="n">
+      <c r="Q75" s="3" t="n">
         <v>45841</v>
       </c>
     </row>
@@ -5202,7 +5214,7 @@
           <t>ThinkCentre XXXX</t>
         </is>
       </c>
-      <c r="N76" s="2" t="n">
+      <c r="N76" s="3" t="n">
         <v>45841.50194444445</v>
       </c>
       <c r="O76" t="inlineStr">
@@ -5217,7 +5229,7 @@
 ANTIGA PA_210</t>
         </is>
       </c>
-      <c r="Q76" s="2" t="n">
+      <c r="Q76" s="3" t="n">
         <v>45841</v>
       </c>
     </row>
@@ -5273,7 +5285,7 @@
           <t>ThinkCentre M55e</t>
         </is>
       </c>
-      <c r="N77" s="2" t="n">
+      <c r="N77" s="3" t="n">
         <v>45846.49549768519</v>
       </c>
       <c r="O77" t="inlineStr">
@@ -5288,7 +5300,7 @@
 ANTIGA PA_201</t>
         </is>
       </c>
-      <c r="Q77" s="2" t="n">
+      <c r="Q77" s="3" t="n">
         <v>45841</v>
       </c>
     </row>
@@ -5344,7 +5356,7 @@
           <t>ThinkCentre A55</t>
         </is>
       </c>
-      <c r="N78" s="2" t="n">
+      <c r="N78" s="3" t="n">
         <v>45841.51126157407</v>
       </c>
       <c r="O78" t="inlineStr">
@@ -5359,7 +5371,7 @@
 ANTIGA PA_195</t>
         </is>
       </c>
-      <c r="Q78" s="2" t="n">
+      <c r="Q78" s="3" t="n">
         <v>45841</v>
       </c>
     </row>
@@ -5415,7 +5427,7 @@
           <t>ThinkCentre A55</t>
         </is>
       </c>
-      <c r="N79" s="2" t="n">
+      <c r="N79" s="3" t="n">
         <v>45842.60928240741</v>
       </c>
       <c r="O79" t="inlineStr">
@@ -5430,7 +5442,7 @@
 ANTIGA PA_184</t>
         </is>
       </c>
-      <c r="Q79" s="2" t="n">
+      <c r="Q79" s="3" t="n">
         <v>45842</v>
       </c>
     </row>
@@ -5481,7 +5493,7 @@
           <t>ThinkCentre XXXX</t>
         </is>
       </c>
-      <c r="N80" s="2" t="n">
+      <c r="N80" s="3" t="n">
         <v>45846.49222222222</v>
       </c>
       <c r="O80" t="inlineStr">
@@ -5495,7 +5507,7 @@
 31/01/2025</t>
         </is>
       </c>
-      <c r="Q80" s="2" t="n">
+      <c r="Q80" s="3" t="n">
         <v>45688</v>
       </c>
     </row>
@@ -5551,7 +5563,7 @@
           <t>ThinkCentre XXXX</t>
         </is>
       </c>
-      <c r="N81" s="2" t="n">
+      <c r="N81" s="3" t="n">
         <v>45846.47541666667</v>
       </c>
       <c r="O81" t="inlineStr">
@@ -5566,7 +5578,7 @@
 ANTIGA PA_181</t>
         </is>
       </c>
-      <c r="Q81" s="2" t="n">
+      <c r="Q81" s="3" t="n">
         <v>45842</v>
       </c>
     </row>
@@ -5622,7 +5634,7 @@
           <t>ThinkCentre A55</t>
         </is>
       </c>
-      <c r="N82" s="2" t="n">
+      <c r="N82" s="3" t="n">
         <v>45842.62258101852</v>
       </c>
       <c r="O82" t="inlineStr">
@@ -5637,7 +5649,7 @@
 ANTIGA PA_170</t>
         </is>
       </c>
-      <c r="Q82" s="2" t="n">
+      <c r="Q82" s="3" t="n">
         <v>45842</v>
       </c>
     </row>
@@ -5693,7 +5705,7 @@
           <t>OptiPlex 745</t>
         </is>
       </c>
-      <c r="N83" s="2" t="n">
+      <c r="N83" s="3" t="n">
         <v>45842.6375462963</v>
       </c>
       <c r="O83" t="inlineStr">
@@ -5708,7 +5720,7 @@
 ANTIGA PA_196</t>
         </is>
       </c>
-      <c r="Q83" s="2" t="n">
+      <c r="Q83" s="3" t="n">
         <v>45842</v>
       </c>
     </row>
@@ -5764,7 +5776,7 @@
           <t>OptiPlex 745</t>
         </is>
       </c>
-      <c r="N84" s="2" t="n">
+      <c r="N84" s="3" t="n">
         <v>45846.5080787037</v>
       </c>
       <c r="O84" t="inlineStr">
@@ -5779,7 +5791,7 @@
 ANTIGA PA_182</t>
         </is>
       </c>
-      <c r="Q84" s="2" t="n">
+      <c r="Q84" s="3" t="n">
         <v>45842</v>
       </c>
     </row>
@@ -5835,7 +5847,7 @@
           <t>OptiPlex 755</t>
         </is>
       </c>
-      <c r="N85" s="2" t="n">
+      <c r="N85" s="3" t="n">
         <v>46038.39550925926</v>
       </c>
       <c r="O85" t="inlineStr">
@@ -5849,7 +5861,7 @@
 ANTIGA PA_183</t>
         </is>
       </c>
-      <c r="Q85" s="2" t="n">
+      <c r="Q85" s="3" t="n">
         <v>46038</v>
       </c>
     </row>
@@ -5905,7 +5917,7 @@
           <t>ThinkCentre A55</t>
         </is>
       </c>
-      <c r="N86" s="2" t="n">
+      <c r="N86" s="3" t="n">
         <v>46038.37561342592</v>
       </c>
       <c r="O86" t="inlineStr">
@@ -5920,7 +5932,7 @@
 ANTIGA PA_214</t>
         </is>
       </c>
-      <c r="Q86" s="2" t="n">
+      <c r="Q86" s="3" t="n">
         <v>46038</v>
       </c>
     </row>
@@ -5976,7 +5988,7 @@
           <t>ThinkCentre A55</t>
         </is>
       </c>
-      <c r="N87" s="2" t="n">
+      <c r="N87" s="3" t="n">
         <v>46038.37711805556</v>
       </c>
       <c r="O87" t="inlineStr">
@@ -5991,7 +6003,7 @@
 ANTIGA PA_212</t>
         </is>
       </c>
-      <c r="Q87" s="2" t="n">
+      <c r="Q87" s="3" t="n">
         <v>46038</v>
       </c>
     </row>
@@ -6047,7 +6059,7 @@
           <t>ThinkCentre A55</t>
         </is>
       </c>
-      <c r="N88" s="2" t="n">
+      <c r="N88" s="3" t="n">
         <v>46038.37935185185</v>
       </c>
       <c r="O88" t="inlineStr">
@@ -6062,7 +6074,7 @@
 ANTIGA PA_204</t>
         </is>
       </c>
-      <c r="Q88" s="2" t="n">
+      <c r="Q88" s="3" t="n">
         <v>46038</v>
       </c>
     </row>
@@ -6118,7 +6130,7 @@
           <t>ThinkCentre M55e</t>
         </is>
       </c>
-      <c r="N89" s="2" t="n">
+      <c r="N89" s="3" t="n">
         <v>46038.38335648148</v>
       </c>
       <c r="O89" t="inlineStr">
@@ -6134,7 +6146,7 @@
 ANTIGA PA_203</t>
         </is>
       </c>
-      <c r="Q89" s="2" t="n">
+      <c r="Q89" s="3" t="n">
         <v>46038</v>
       </c>
     </row>
@@ -6190,7 +6202,7 @@
           <t>ThinkCentre A55</t>
         </is>
       </c>
-      <c r="N90" s="2" t="n">
+      <c r="N90" s="3" t="n">
         <v>46038.38379629629</v>
       </c>
       <c r="O90" t="inlineStr">
@@ -6205,7 +6217,7 @@
 ANTIGA PA_200</t>
         </is>
       </c>
-      <c r="Q90" s="2" t="n">
+      <c r="Q90" s="3" t="n">
         <v>46038</v>
       </c>
     </row>
@@ -6261,7 +6273,7 @@
           <t>ThinkCentre A55</t>
         </is>
       </c>
-      <c r="N91" s="2" t="n">
+      <c r="N91" s="3" t="n">
         <v>46038.38583333333</v>
       </c>
       <c r="O91" t="inlineStr">
@@ -6276,7 +6288,7 @@
 ANTIGA PA_194</t>
         </is>
       </c>
-      <c r="Q91" s="2" t="n">
+      <c r="Q91" s="3" t="n">
         <v>46038</v>
       </c>
     </row>
@@ -6335,7 +6347,7 @@
       <c r="M92" t="n">
         <v>1</v>
       </c>
-      <c r="N92" s="2" t="n">
+      <c r="N92" s="3" t="n">
         <v>46038.38940972222</v>
       </c>
       <c r="O92" t="inlineStr">
@@ -6350,7 +6362,7 @@
 ANTIGA PA_197</t>
         </is>
       </c>
-      <c r="Q92" s="2" t="n">
+      <c r="Q92" s="3" t="n">
         <v>46038</v>
       </c>
     </row>
@@ -6406,7 +6418,7 @@
           <t>ThinkCentre A55</t>
         </is>
       </c>
-      <c r="N93" s="2" t="n">
+      <c r="N93" s="3" t="n">
         <v>46038.39097222222</v>
       </c>
       <c r="O93" t="inlineStr">
@@ -6421,7 +6433,7 @@
 ANTIGA PA_192</t>
         </is>
       </c>
-      <c r="Q93" s="2" t="n">
+      <c r="Q93" s="3" t="n">
         <v>46038</v>
       </c>
     </row>
@@ -6477,7 +6489,7 @@
           <t>HP 402 G1 SFF Business PC</t>
         </is>
       </c>
-      <c r="N94" s="2" t="n">
+      <c r="N94" s="3" t="n">
         <v>46038.39429398148</v>
       </c>
       <c r="O94" t="inlineStr">
@@ -6493,7 +6505,7 @@
 16/01/2026</t>
         </is>
       </c>
-      <c r="Q94" s="2" t="n">
+      <c r="Q94" s="3" t="n">
         <v>46038</v>
       </c>
     </row>
@@ -6557,8 +6569,8 @@
       <c r="M95" t="n">
         <v>1</v>
       </c>
-      <c r="N95" s="2" t="n">
-        <v>46073.38861111111</v>
+      <c r="N95" s="3" t="n">
+        <v>46073.46717592593</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -6626,8 +6638,8 @@
       <c r="M96" t="n">
         <v>1</v>
       </c>
-      <c r="N96" s="2" t="n">
-        <v>46072.80157407407</v>
+      <c r="N96" s="3" t="n">
+        <v>46073.47141203703</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
@@ -6646,11 +6658,6 @@
           <t>COORDENACAO</t>
         </is>
       </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>10.69.3.93</t>
-        </is>
-      </c>
       <c r="D97" t="n">
         <v>2025</v>
       </c>
@@ -6695,8 +6702,8 @@
       <c r="M97" t="n">
         <v>1</v>
       </c>
-      <c r="N97" s="2" t="n">
-        <v>46073.40366898148</v>
+      <c r="N97" s="3" t="n">
+        <v>46073.48112268518</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -6759,7 +6766,7 @@
       <c r="M98" t="n">
         <v>1</v>
       </c>
-      <c r="N98" s="2" t="n">
+      <c r="N98" s="3" t="n">
         <v>46072.68513888889</v>
       </c>
       <c r="O98" t="inlineStr">
@@ -6828,7 +6835,7 @@
       <c r="M99" t="n">
         <v>1</v>
       </c>
-      <c r="N99" s="2" t="n">
+      <c r="N99" s="3" t="n">
         <v>46072.79275462963</v>
       </c>
       <c r="O99" t="inlineStr">
@@ -6897,8 +6904,8 @@
       <c r="M100" t="n">
         <v>2</v>
       </c>
-      <c r="N100" s="2" t="n">
-        <v>46073.37280092593</v>
+      <c r="N100" s="3" t="n">
+        <v>46073.4875462963</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6966,8 +6973,8 @@
       <c r="M101" t="n">
         <v>1</v>
       </c>
-      <c r="N101" s="2" t="n">
-        <v>46073.38608796296</v>
+      <c r="N101" s="3" t="n">
+        <v>46073.46143518519</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -7035,7 +7042,7 @@
       <c r="M102" t="n">
         <v>1</v>
       </c>
-      <c r="N102" s="2" t="n">
+      <c r="N102" s="3" t="n">
         <v>46065.69311342593</v>
       </c>
       <c r="O102" t="inlineStr">
@@ -7104,8 +7111,8 @@
       <c r="M103" t="n">
         <v>2</v>
       </c>
-      <c r="N103" s="2" t="n">
-        <v>46073.39652777778</v>
+      <c r="N103" s="3" t="n">
+        <v>46073.47716435185</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7165,7 +7172,7 @@
           <t>HP 240 G5 Notebook PC</t>
         </is>
       </c>
-      <c r="N104" s="2" t="n">
+      <c r="N104" s="3" t="n">
         <v>45527.46174768519</v>
       </c>
       <c r="O104" t="inlineStr">
@@ -7231,7 +7238,7 @@
           <t>HP ProBook 440 14 inch G9 Notebook PC</t>
         </is>
       </c>
-      <c r="N105" s="2" t="n">
+      <c r="N105" s="3" t="n">
         <v>46051.74359953704</v>
       </c>
       <c r="O105" t="inlineStr">
@@ -7292,7 +7299,7 @@
           <t>HP ProBook 440 G1</t>
         </is>
       </c>
-      <c r="N106" s="2" t="n">
+      <c r="N106" s="3" t="n">
         <v>46031.66342592592</v>
       </c>
       <c r="O106" t="inlineStr">
@@ -7361,8 +7368,8 @@
       <c r="M107" t="n">
         <v>1</v>
       </c>
-      <c r="N107" s="2" t="n">
-        <v>46073.39002314815</v>
+      <c r="N107" s="3" t="n">
+        <v>46073.46638888889</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -7430,7 +7437,7 @@
       <c r="M108" t="n">
         <v>1</v>
       </c>
-      <c r="N108" s="2" t="n">
+      <c r="N108" s="3" t="n">
         <v>45903.39740740741</v>
       </c>
       <c r="O108" t="inlineStr">
@@ -7499,8 +7506,8 @@
       <c r="M109" t="n">
         <v>1</v>
       </c>
-      <c r="N109" s="2" t="n">
-        <v>46073.40292824074</v>
+      <c r="N109" s="3" t="n">
+        <v>46073.48663194444</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7568,8 +7575,8 @@
       <c r="M110" t="n">
         <v>2</v>
       </c>
-      <c r="N110" s="2" t="n">
-        <v>46073.39291666666</v>
+      <c r="N110" s="3" t="n">
+        <v>46073.47532407408</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7637,8 +7644,8 @@
       <c r="M111" t="n">
         <v>2</v>
       </c>
-      <c r="N111" s="2" t="n">
-        <v>46073.38481481482</v>
+      <c r="N111" s="3" t="n">
+        <v>46073.46740740741</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
@@ -7706,8 +7713,8 @@
       <c r="M112" t="n">
         <v>2</v>
       </c>
-      <c r="N112" s="2" t="n">
-        <v>46073.37456018518</v>
+      <c r="N112" s="3" t="n">
+        <v>46073.48740740741</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7775,8 +7782,8 @@
       <c r="M113" t="n">
         <v>1</v>
       </c>
-      <c r="N113" s="2" t="n">
-        <v>46073.39959490741</v>
+      <c r="N113" s="3" t="n">
+        <v>46073.4728125</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7844,8 +7851,8 @@
       <c r="M114" t="n">
         <v>1</v>
       </c>
-      <c r="N114" s="2" t="n">
-        <v>46073.39486111111</v>
+      <c r="N114" s="3" t="n">
+        <v>46073.47325231481</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -7910,8 +7917,8 @@
           <t>HP ProDesk 400 G5 SFF (Brazil)</t>
         </is>
       </c>
-      <c r="N115" s="2" t="n">
-        <v>46073.37603009259</v>
+      <c r="N115" s="3" t="n">
+        <v>46073.48346064815</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -7979,8 +7986,8 @@
       <c r="M116" t="n">
         <v>1</v>
       </c>
-      <c r="N116" s="2" t="n">
-        <v>46073.39349537037</v>
+      <c r="N116" s="3" t="n">
+        <v>46073.47070601852</v>
       </c>
       <c r="O116" t="inlineStr">
         <is>
@@ -7999,6 +8006,11 @@
           <t>DP</t>
         </is>
       </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>10.69.3.23</t>
+        </is>
+      </c>
       <c r="D117" t="n">
         <v>2025</v>
       </c>
@@ -8043,8 +8055,8 @@
       <c r="M117" t="n">
         <v>1</v>
       </c>
-      <c r="N117" s="2" t="n">
-        <v>46073.39738425926</v>
+      <c r="N117" s="3" t="n">
+        <v>46073.47856481482</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -8109,7 +8121,7 @@
           <t>HP ProDesk 400 G5 SFF</t>
         </is>
       </c>
-      <c r="N118" s="2" t="n">
+      <c r="N118" s="3" t="n">
         <v>46059.69064814815</v>
       </c>
       <c r="O118" t="inlineStr">
@@ -8178,7 +8190,7 @@
       <c r="M119" t="n">
         <v>1</v>
       </c>
-      <c r="N119" s="2" t="n">
+      <c r="N119" s="3" t="n">
         <v>46036.58722222222</v>
       </c>
       <c r="O119" t="inlineStr">
@@ -8247,8 +8259,8 @@
       <c r="M120" t="n">
         <v>1</v>
       </c>
-      <c r="N120" s="2" t="n">
-        <v>46073.40037037037</v>
+      <c r="N120" s="3" t="n">
+        <v>46073.47305555556</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -8316,8 +8328,8 @@
       <c r="M121" t="n">
         <v>1</v>
       </c>
-      <c r="N121" s="2" t="n">
-        <v>46072.82324074074</v>
+      <c r="N121" s="3" t="n">
+        <v>46073.47019675926</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -8382,8 +8394,8 @@
           <t>OptiPlex 3070</t>
         </is>
       </c>
-      <c r="N122" s="2" t="n">
-        <v>46073.39563657407</v>
+      <c r="N122" s="3" t="n">
+        <v>46073.47486111111</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -8451,8 +8463,8 @@
       <c r="M123" t="n">
         <v>2</v>
       </c>
-      <c r="N123" s="2" t="n">
-        <v>46073.2978125</v>
+      <c r="N123" s="3" t="n">
+        <v>46073.47032407407</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -8520,8 +8532,8 @@
       <c r="M124" t="n">
         <v>1</v>
       </c>
-      <c r="N124" s="2" t="n">
-        <v>46073.38439814815</v>
+      <c r="N124" s="3" t="n">
+        <v>46073.46333333333</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -8589,8 +8601,8 @@
       <c r="M125" t="n">
         <v>1</v>
       </c>
-      <c r="N125" s="2" t="n">
-        <v>46073.40153935185</v>
+      <c r="N125" s="3" t="n">
+        <v>46073.4784375</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -8658,8 +8670,8 @@
       <c r="M126" t="n">
         <v>1</v>
       </c>
-      <c r="N126" s="2" t="n">
-        <v>46073.39297453704</v>
+      <c r="N126" s="3" t="n">
+        <v>46073.46949074074</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -8727,8 +8739,8 @@
       <c r="M127" t="n">
         <v>2</v>
       </c>
-      <c r="N127" s="2" t="n">
-        <v>46073.40190972222</v>
+      <c r="N127" s="3" t="n">
+        <v>46073.47959490741</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -8796,8 +8808,8 @@
       <c r="M128" t="n">
         <v>1</v>
       </c>
-      <c r="N128" s="2" t="n">
-        <v>46073.37165509259</v>
+      <c r="N128" s="3" t="n">
+        <v>46073.44976851852</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -8865,8 +8877,8 @@
       <c r="M129" t="n">
         <v>1</v>
       </c>
-      <c r="N129" s="2" t="n">
-        <v>46073.39355324074</v>
+      <c r="N129" s="3" t="n">
+        <v>46073.47447916667</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -8934,8 +8946,8 @@
       <c r="M130" t="n">
         <v>1</v>
       </c>
-      <c r="N130" s="2" t="n">
-        <v>46073.40383101852</v>
+      <c r="N130" s="3" t="n">
+        <v>46073.48274305555</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -8998,8 +9010,8 @@
       <c r="M131" t="n">
         <v>1</v>
       </c>
-      <c r="N131" s="2" t="n">
-        <v>46073.39925925926</v>
+      <c r="N131" s="3" t="n">
+        <v>46073.47479166667</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -9067,7 +9079,7 @@
       <c r="M132" t="n">
         <v>1</v>
       </c>
-      <c r="N132" s="2" t="n">
+      <c r="N132" s="3" t="n">
         <v>45938.56157407408</v>
       </c>
       <c r="O132" t="inlineStr">
@@ -9131,8 +9143,8 @@
       <c r="M133" t="n">
         <v>1</v>
       </c>
-      <c r="N133" s="2" t="n">
-        <v>46073.37694444445</v>
+      <c r="N133" s="3" t="n">
+        <v>46073.45274305555</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -9195,8 +9207,8 @@
       <c r="M134" t="n">
         <v>1</v>
       </c>
-      <c r="N134" s="2" t="n">
-        <v>46073.38351851852</v>
+      <c r="N134" s="3" t="n">
+        <v>46073.46253472222</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -9259,8 +9271,8 @@
       <c r="M135" t="n">
         <v>1</v>
       </c>
-      <c r="N135" s="2" t="n">
-        <v>46073.38026620371</v>
+      <c r="N135" s="3" t="n">
+        <v>46073.45353009259</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -9323,7 +9335,7 @@
       <c r="M136" t="n">
         <v>1</v>
       </c>
-      <c r="N136" s="2" t="n">
+      <c r="N136" s="3" t="n">
         <v>46066.80446759259</v>
       </c>
       <c r="O136" t="inlineStr">
@@ -9379,7 +9391,7 @@
           <t>HP Compaq Pro 4300 SFF Brazil PC</t>
         </is>
       </c>
-      <c r="N137" s="2" t="n">
+      <c r="N137" s="3" t="n">
         <v>46020.45556712963</v>
       </c>
       <c r="O137" t="inlineStr">
@@ -9450,8 +9462,8 @@
       <c r="M138" t="n">
         <v>1</v>
       </c>
-      <c r="N138" s="2" t="n">
-        <v>46073.37887731481</v>
+      <c r="N138" s="3" t="n">
+        <v>46073.46060185185</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9514,8 +9526,8 @@
       <c r="M139" t="n">
         <v>1</v>
       </c>
-      <c r="N139" s="2" t="n">
-        <v>46073.39894675926</v>
+      <c r="N139" s="3" t="n">
+        <v>46073.47848379629</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9578,8 +9590,8 @@
       <c r="M140" t="n">
         <v>1</v>
       </c>
-      <c r="N140" s="2" t="n">
-        <v>46073.37763888889</v>
+      <c r="N140" s="3" t="n">
+        <v>46073.45166666667</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9642,8 +9654,8 @@
       <c r="M141" t="n">
         <v>1</v>
       </c>
-      <c r="N141" s="2" t="n">
-        <v>46073.37365740741</v>
+      <c r="N141" s="3" t="n">
+        <v>46073.44671296296</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9706,8 +9718,8 @@
       <c r="M142" t="n">
         <v>1</v>
       </c>
-      <c r="N142" s="2" t="n">
-        <v>46073.36811342592</v>
+      <c r="N142" s="3" t="n">
+        <v>46073.47739583333</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9770,8 +9782,8 @@
       <c r="M143" t="n">
         <v>1</v>
       </c>
-      <c r="N143" s="2" t="n">
-        <v>46073.36651620371</v>
+      <c r="N143" s="3" t="n">
+        <v>46073.47967592593</v>
       </c>
       <c r="O143" t="inlineStr">
         <is>
@@ -9834,8 +9846,8 @@
       <c r="M144" t="n">
         <v>1</v>
       </c>
-      <c r="N144" s="2" t="n">
-        <v>46073.39260416666</v>
+      <c r="N144" s="3" t="n">
+        <v>46073.47019675926</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9898,8 +9910,8 @@
       <c r="M145" t="n">
         <v>1</v>
       </c>
-      <c r="N145" s="2" t="n">
-        <v>46073.37107638889</v>
+      <c r="N145" s="3" t="n">
+        <v>46073.45063657407</v>
       </c>
       <c r="O145" t="inlineStr">
         <is>
@@ -9962,8 +9974,8 @@
       <c r="M146" t="n">
         <v>1</v>
       </c>
-      <c r="N146" s="2" t="n">
-        <v>46073.40234953703</v>
+      <c r="N146" s="3" t="n">
+        <v>46073.48275462963</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10026,8 +10038,8 @@
       <c r="M147" t="n">
         <v>1</v>
       </c>
-      <c r="N147" s="2" t="n">
-        <v>46073.36726851852</v>
+      <c r="N147" s="3" t="n">
+        <v>46073.48597222222</v>
       </c>
       <c r="O147" t="inlineStr">
         <is>
@@ -10090,8 +10102,8 @@
       <c r="M148" t="n">
         <v>1</v>
       </c>
-      <c r="N148" s="2" t="n">
-        <v>46073.40401620371</v>
+      <c r="N148" s="3" t="n">
+        <v>46073.48334490741</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10154,8 +10166,8 @@
       <c r="M149" t="n">
         <v>1</v>
       </c>
-      <c r="N149" s="2" t="n">
-        <v>46073.36653935185</v>
+      <c r="N149" s="3" t="n">
+        <v>46073.48458333333</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -10218,8 +10230,8 @@
       <c r="M150" t="n">
         <v>1</v>
       </c>
-      <c r="N150" s="2" t="n">
-        <v>46073.36836805556</v>
+      <c r="N150" s="3" t="n">
+        <v>46073.40594907408</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -10282,8 +10294,8 @@
       <c r="M151" t="n">
         <v>1</v>
       </c>
-      <c r="N151" s="2" t="n">
-        <v>46073.36803240741</v>
+      <c r="N151" s="3" t="n">
+        <v>46073.48521990741</v>
       </c>
       <c r="O151" t="inlineStr">
         <is>
@@ -10346,8 +10358,8 @@
       <c r="M152" t="n">
         <v>1</v>
       </c>
-      <c r="N152" s="2" t="n">
-        <v>46073.37138888889</v>
+      <c r="N152" s="3" t="n">
+        <v>46073.48601851852</v>
       </c>
       <c r="O152" t="inlineStr">
         <is>
@@ -10405,8 +10417,8 @@
       <c r="M153" t="n">
         <v>1</v>
       </c>
-      <c r="N153" s="2" t="n">
-        <v>46073.37164351852</v>
+      <c r="N153" s="3" t="n">
+        <v>46073.45131944444</v>
       </c>
       <c r="O153" t="inlineStr">
         <is>
@@ -10469,8 +10481,8 @@
       <c r="M154" t="n">
         <v>1</v>
       </c>
-      <c r="N154" s="2" t="n">
-        <v>46073.38974537037</v>
+      <c r="N154" s="3" t="n">
+        <v>46073.46508101852</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10533,8 +10545,8 @@
       <c r="M155" t="n">
         <v>1</v>
       </c>
-      <c r="N155" s="2" t="n">
-        <v>46073.36797453704</v>
+      <c r="N155" s="3" t="n">
+        <v>46073.48293981481</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10597,8 +10609,8 @@
       <c r="M156" t="n">
         <v>1</v>
       </c>
-      <c r="N156" s="2" t="n">
-        <v>46073.37090277778</v>
+      <c r="N156" s="3" t="n">
+        <v>46073.44761574074</v>
       </c>
       <c r="O156" t="inlineStr">
         <is>
@@ -10661,8 +10673,8 @@
       <c r="M157" t="n">
         <v>1</v>
       </c>
-      <c r="N157" s="2" t="n">
-        <v>46073.3725</v>
+      <c r="N157" s="3" t="n">
+        <v>46073.45150462963</v>
       </c>
       <c r="O157" t="inlineStr">
         <is>
@@ -10725,8 +10737,8 @@
       <c r="M158" t="n">
         <v>1</v>
       </c>
-      <c r="N158" s="2" t="n">
-        <v>46073.37844907407</v>
+      <c r="N158" s="3" t="n">
+        <v>46073.4716550926</v>
       </c>
       <c r="O158" t="inlineStr">
         <is>
@@ -10789,8 +10801,8 @@
       <c r="M159" t="n">
         <v>1</v>
       </c>
-      <c r="N159" s="2" t="n">
-        <v>46073.37318287037</v>
+      <c r="N159" s="3" t="n">
+        <v>46073.44952546297</v>
       </c>
       <c r="O159" t="inlineStr">
         <is>
@@ -10853,8 +10865,8 @@
       <c r="M160" t="n">
         <v>1</v>
       </c>
-      <c r="N160" s="2" t="n">
-        <v>46073.37744212963</v>
+      <c r="N160" s="3" t="n">
+        <v>46073.45673611111</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
@@ -10917,8 +10929,8 @@
       <c r="M161" t="n">
         <v>1</v>
       </c>
-      <c r="N161" s="2" t="n">
-        <v>46073.37336805555</v>
+      <c r="N161" s="3" t="n">
+        <v>46073.44894675926</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -10981,8 +10993,8 @@
       <c r="M162" t="n">
         <v>1</v>
       </c>
-      <c r="N162" s="2" t="n">
-        <v>46073.40118055556</v>
+      <c r="N162" s="3" t="n">
+        <v>46073.47883101852</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11045,7 +11057,7 @@
       <c r="M163" t="n">
         <v>1</v>
       </c>
-      <c r="N163" s="2" t="n">
+      <c r="N163" s="3" t="n">
         <v>46051.66149305556</v>
       </c>
       <c r="O163" t="inlineStr">
@@ -11109,8 +11121,8 @@
       <c r="M164" t="n">
         <v>2</v>
       </c>
-      <c r="N164" s="2" t="n">
-        <v>46073.39744212963</v>
+      <c r="N164" s="3" t="n">
+        <v>46073.47771990741</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11173,8 +11185,8 @@
       <c r="M165" t="n">
         <v>2</v>
       </c>
-      <c r="N165" s="2" t="n">
-        <v>46073.40116898148</v>
+      <c r="N165" s="3" t="n">
+        <v>46073.47859953704</v>
       </c>
       <c r="O165" t="inlineStr">
         <is>
@@ -11237,8 +11249,8 @@
       <c r="M166" t="n">
         <v>2</v>
       </c>
-      <c r="N166" s="2" t="n">
-        <v>46073.37313657408</v>
+      <c r="N166" s="3" t="n">
+        <v>46073.45508101852</v>
       </c>
       <c r="O166" t="inlineStr">
         <is>
@@ -11299,10 +11311,10 @@
         </is>
       </c>
       <c r="M167" t="n">
-        <v>1</v>
-      </c>
-      <c r="N167" s="2" t="n">
-        <v>46073.36726851852</v>
+        <v>2</v>
+      </c>
+      <c r="N167" s="3" t="n">
+        <v>46073.48695601852</v>
       </c>
       <c r="O167" t="inlineStr">
         <is>
@@ -11365,8 +11377,8 @@
       <c r="M168" t="n">
         <v>2</v>
       </c>
-      <c r="N168" s="2" t="n">
-        <v>46073.3704050926</v>
+      <c r="N168" s="3" t="n">
+        <v>46073.48403935185</v>
       </c>
       <c r="O168" t="inlineStr">
         <is>
@@ -11429,8 +11441,8 @@
       <c r="M169" t="n">
         <v>2</v>
       </c>
-      <c r="N169" s="2" t="n">
-        <v>46073.40241898148</v>
+      <c r="N169" s="3" t="n">
+        <v>46073.47859953704</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -11493,8 +11505,8 @@
       <c r="M170" t="n">
         <v>2</v>
       </c>
-      <c r="N170" s="2" t="n">
-        <v>46073.37672453704</v>
+      <c r="N170" s="3" t="n">
+        <v>46073.45587962963</v>
       </c>
       <c r="O170" t="inlineStr">
         <is>
@@ -11557,8 +11569,8 @@
       <c r="M171" t="n">
         <v>2</v>
       </c>
-      <c r="N171" s="2" t="n">
-        <v>46073.37936342593</v>
+      <c r="N171" s="3" t="n">
+        <v>46073.4597337963</v>
       </c>
       <c r="O171" t="inlineStr">
         <is>
@@ -11621,7 +11633,7 @@
       <c r="M172" t="n">
         <v>2</v>
       </c>
-      <c r="N172" s="2" t="n">
+      <c r="N172" s="3" t="n">
         <v>46072.77650462963</v>
       </c>
       <c r="O172" t="inlineStr">
@@ -11685,7 +11697,7 @@
       <c r="M173" t="n">
         <v>1</v>
       </c>
-      <c r="N173" s="2" t="n">
+      <c r="N173" s="3" t="n">
         <v>46072.78350694444</v>
       </c>
       <c r="O173" t="inlineStr">
@@ -11749,8 +11761,8 @@
       <c r="M174" t="n">
         <v>2</v>
       </c>
-      <c r="N174" s="2" t="n">
-        <v>46073.37069444444</v>
+      <c r="N174" s="3" t="n">
+        <v>46073.44805555556</v>
       </c>
       <c r="O174" t="inlineStr">
         <is>
@@ -11813,8 +11825,8 @@
       <c r="M175" t="n">
         <v>2</v>
       </c>
-      <c r="N175" s="2" t="n">
-        <v>46073.38221064815</v>
+      <c r="N175" s="3" t="n">
+        <v>46073.46365740741</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -11877,8 +11889,8 @@
       <c r="M176" t="n">
         <v>2</v>
       </c>
-      <c r="N176" s="2" t="n">
-        <v>46072.64962962963</v>
+      <c r="N176" s="3" t="n">
+        <v>46073.45179398148</v>
       </c>
       <c r="O176" t="inlineStr">
         <is>
@@ -11941,8 +11953,8 @@
       <c r="M177" t="n">
         <v>2</v>
       </c>
-      <c r="N177" s="2" t="n">
-        <v>46072.69309027777</v>
+      <c r="N177" s="3" t="n">
+        <v>46073.45920138889</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
@@ -12005,8 +12017,8 @@
       <c r="M178" t="n">
         <v>2</v>
       </c>
-      <c r="N178" s="2" t="n">
-        <v>46073.4044212963</v>
+      <c r="N178" s="3" t="n">
+        <v>46073.47934027778</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12069,8 +12081,8 @@
       <c r="M179" t="n">
         <v>1</v>
       </c>
-      <c r="N179" s="2" t="n">
-        <v>46073.39833333333</v>
+      <c r="N179" s="3" t="n">
+        <v>46073.471875</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12133,8 +12145,8 @@
       <c r="M180" t="n">
         <v>1</v>
       </c>
-      <c r="N180" s="2" t="n">
-        <v>46073.39304398148</v>
+      <c r="N180" s="3" t="n">
+        <v>46073.46824074074</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12197,8 +12209,8 @@
       <c r="M181" t="n">
         <v>1</v>
       </c>
-      <c r="N181" s="2" t="n">
-        <v>46073.36471064815</v>
+      <c r="N181" s="3" t="n">
+        <v>46073.44728009259</v>
       </c>
       <c r="O181" t="inlineStr">
         <is>
@@ -12261,7 +12273,7 @@
       <c r="M182" t="n">
         <v>1</v>
       </c>
-      <c r="N182" s="2" t="n">
+      <c r="N182" s="3" t="n">
         <v>46066.87270833334</v>
       </c>
       <c r="O182" t="inlineStr">
@@ -12325,7 +12337,7 @@
       <c r="M183" t="n">
         <v>1</v>
       </c>
-      <c r="N183" s="2" t="n">
+      <c r="N183" s="3" t="n">
         <v>46071.5514699074</v>
       </c>
       <c r="O183" t="inlineStr">
@@ -12394,7 +12406,7 @@
       <c r="M184" t="n">
         <v>2</v>
       </c>
-      <c r="N184" s="2" t="n">
+      <c r="N184" s="3" t="n">
         <v>46072.81322916667</v>
       </c>
       <c r="O184" t="inlineStr">
@@ -12458,8 +12470,8 @@
       <c r="M185" t="n">
         <v>1</v>
       </c>
-      <c r="N185" s="2" t="n">
-        <v>46073.40252314815</v>
+      <c r="N185" s="3" t="n">
+        <v>46073.43803240741</v>
       </c>
       <c r="O185" t="inlineStr">
         <is>
@@ -12522,8 +12534,8 @@
       <c r="M186" t="n">
         <v>1</v>
       </c>
-      <c r="N186" s="2" t="n">
-        <v>46073.39160879629</v>
+      <c r="N186" s="3" t="n">
+        <v>46073.46666666667</v>
       </c>
       <c r="O186" t="inlineStr">
         <is>
@@ -12586,8 +12598,8 @@
       <c r="M187" t="n">
         <v>1</v>
       </c>
-      <c r="N187" s="2" t="n">
-        <v>46073.38042824074</v>
+      <c r="N187" s="3" t="n">
+        <v>46073.45883101852</v>
       </c>
       <c r="O187" t="inlineStr">
         <is>
@@ -12650,8 +12662,8 @@
       <c r="M188" t="n">
         <v>1</v>
       </c>
-      <c r="N188" s="2" t="n">
-        <v>46073.38059027777</v>
+      <c r="N188" s="3" t="n">
+        <v>46073.46096064815</v>
       </c>
       <c r="O188" t="inlineStr">
         <is>
@@ -12711,7 +12723,7 @@
           <t>HP 402 G1 SFF Business PC</t>
         </is>
       </c>
-      <c r="N189" s="2" t="n">
+      <c r="N189" s="3" t="n">
         <v>46043.66105324074</v>
       </c>
       <c r="O189" t="inlineStr">
@@ -12737,11 +12749,6 @@
           <t>OPERACAO 8.1</t>
         </is>
       </c>
-      <c r="C190" t="inlineStr">
-        <is>
-          <t>10.69.5.59</t>
-        </is>
-      </c>
       <c r="D190" t="n">
         <v>2015</v>
       </c>
@@ -12778,8 +12785,8 @@
           <t>HP Compaq 6000 Pro SFF PC</t>
         </is>
       </c>
-      <c r="N190" s="2" t="n">
-        <v>46073.39694444444</v>
+      <c r="N190" s="3" t="n">
+        <v>46073.47305555556</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12842,7 +12849,7 @@
       <c r="M191" t="n">
         <v>1</v>
       </c>
-      <c r="N191" s="2" t="n">
+      <c r="N191" s="3" t="n">
         <v>46072.79136574074</v>
       </c>
       <c r="O191" t="inlineStr">
@@ -12906,8 +12913,8 @@
       <c r="M192" t="n">
         <v>1</v>
       </c>
-      <c r="N192" s="2" t="n">
-        <v>46073.3915162037</v>
+      <c r="N192" s="3" t="n">
+        <v>46073.4681712963</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -12962,7 +12969,7 @@
           <t>HP Compaq Pro 4300 SFF Brazil PC</t>
         </is>
       </c>
-      <c r="N193" s="2" t="n">
+      <c r="N193" s="3" t="n">
         <v>46045.38947916667</v>
       </c>
       <c r="O193" t="inlineStr">
@@ -13031,8 +13038,8 @@
       <c r="M194" t="n">
         <v>2</v>
       </c>
-      <c r="N194" s="2" t="n">
-        <v>46073.37265046296</v>
+      <c r="N194" s="3" t="n">
+        <v>46073.4858912037</v>
       </c>
       <c r="O194" t="inlineStr">
         <is>
@@ -13095,8 +13102,8 @@
       <c r="M195" t="n">
         <v>1</v>
       </c>
-      <c r="N195" s="2" t="n">
-        <v>46073.38680555556</v>
+      <c r="N195" s="3" t="n">
+        <v>46073.46298611111</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13159,8 +13166,8 @@
       <c r="M196" t="n">
         <v>1</v>
       </c>
-      <c r="N196" s="2" t="n">
-        <v>46073.37748842593</v>
+      <c r="N196" s="3" t="n">
+        <v>46073.4596875</v>
       </c>
       <c r="O196" t="inlineStr">
         <is>
@@ -13223,8 +13230,8 @@
       <c r="M197" t="n">
         <v>1</v>
       </c>
-      <c r="N197" s="2" t="n">
-        <v>46073.38480324074</v>
+      <c r="N197" s="3" t="n">
+        <v>46073.463125</v>
       </c>
       <c r="O197" t="inlineStr">
         <is>
@@ -13287,8 +13294,8 @@
       <c r="M198" t="n">
         <v>1</v>
       </c>
-      <c r="N198" s="2" t="n">
-        <v>46073.3862037037</v>
+      <c r="N198" s="3" t="n">
+        <v>46073.45938657408</v>
       </c>
       <c r="O198" t="inlineStr">
         <is>
@@ -13351,8 +13358,8 @@
       <c r="M199" t="n">
         <v>1</v>
       </c>
-      <c r="N199" s="2" t="n">
-        <v>46073.38569444444</v>
+      <c r="N199" s="3" t="n">
+        <v>46073.46548611111</v>
       </c>
       <c r="O199" t="inlineStr">
         <is>
@@ -13415,8 +13422,8 @@
       <c r="M200" t="n">
         <v>1</v>
       </c>
-      <c r="N200" s="2" t="n">
-        <v>46073.3890625</v>
+      <c r="N200" s="3" t="n">
+        <v>46073.46606481481</v>
       </c>
       <c r="O200" t="inlineStr">
         <is>
@@ -13476,8 +13483,8 @@
           <t>HP Compaq Pro 4300 SFF Brazil PC</t>
         </is>
       </c>
-      <c r="N201" s="2" t="n">
-        <v>46073.37498842592</v>
+      <c r="N201" s="3" t="n">
+        <v>46073.48575231482</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -13540,8 +13547,8 @@
       <c r="M202" t="n">
         <v>1</v>
       </c>
-      <c r="N202" s="2" t="n">
-        <v>46073.37875</v>
+      <c r="N202" s="3" t="n">
+        <v>46073.45861111111</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13604,8 +13611,8 @@
       <c r="M203" t="n">
         <v>1</v>
       </c>
-      <c r="N203" s="2" t="n">
-        <v>46073.40070601852</v>
+      <c r="N203" s="3" t="n">
+        <v>46073.47737268519</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13668,8 +13675,8 @@
       <c r="M204" t="n">
         <v>1</v>
       </c>
-      <c r="N204" s="2" t="n">
-        <v>46073.37653935186</v>
+      <c r="N204" s="3" t="n">
+        <v>46073.45255787037</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13732,8 +13739,8 @@
       <c r="M205" t="n">
         <v>1</v>
       </c>
-      <c r="N205" s="2" t="n">
-        <v>46073.4030787037</v>
+      <c r="N205" s="3" t="n">
+        <v>46073.47725694445</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13796,8 +13803,8 @@
       <c r="M206" t="n">
         <v>1</v>
       </c>
-      <c r="N206" s="2" t="n">
-        <v>46073.37753472223</v>
+      <c r="N206" s="3" t="n">
+        <v>46073.45590277778</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -13860,8 +13867,8 @@
       <c r="M207" t="n">
         <v>1</v>
       </c>
-      <c r="N207" s="2" t="n">
-        <v>46073.38576388889</v>
+      <c r="N207" s="3" t="n">
+        <v>46073.46252314815</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -13924,8 +13931,8 @@
       <c r="M208" t="n">
         <v>1</v>
       </c>
-      <c r="N208" s="2" t="n">
-        <v>46073.38394675926</v>
+      <c r="N208" s="3" t="n">
+        <v>46073.46030092592</v>
       </c>
       <c r="O208" t="inlineStr">
         <is>
@@ -13988,8 +13995,8 @@
       <c r="M209" t="n">
         <v>1</v>
       </c>
-      <c r="N209" s="2" t="n">
-        <v>46073.40003472222</v>
+      <c r="N209" s="3" t="n">
+        <v>46073.47914351852</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14052,8 +14059,8 @@
       <c r="M210" t="n">
         <v>1</v>
       </c>
-      <c r="N210" s="2" t="n">
-        <v>46073.36871527778</v>
+      <c r="N210" s="3" t="n">
+        <v>46073.44820601852</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14116,8 +14123,8 @@
       <c r="M211" t="n">
         <v>1</v>
       </c>
-      <c r="N211" s="2" t="n">
-        <v>46073.37663194445</v>
+      <c r="N211" s="3" t="n">
+        <v>46073.48612268519</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -14180,8 +14187,8 @@
       <c r="M212" t="n">
         <v>1</v>
       </c>
-      <c r="N212" s="2" t="n">
-        <v>46073.3935300926</v>
+      <c r="N212" s="3" t="n">
+        <v>46073.47035879629</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -14244,8 +14251,8 @@
       <c r="M213" t="n">
         <v>1</v>
       </c>
-      <c r="N213" s="2" t="n">
-        <v>46073.38097222222</v>
+      <c r="N213" s="3" t="n">
+        <v>46073.46407407407</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
@@ -14308,8 +14315,8 @@
       <c r="M214" t="n">
         <v>1</v>
       </c>
-      <c r="N214" s="2" t="n">
-        <v>46073.40112268519</v>
+      <c r="N214" s="3" t="n">
+        <v>46073.48288194444</v>
       </c>
       <c r="O214" t="inlineStr">
         <is>
@@ -14372,8 +14379,8 @@
       <c r="M215" t="n">
         <v>1</v>
       </c>
-      <c r="N215" s="2" t="n">
-        <v>46073.38839120371</v>
+      <c r="N215" s="3" t="n">
+        <v>46073.46247685186</v>
       </c>
       <c r="O215" t="inlineStr">
         <is>
@@ -14436,8 +14443,8 @@
       <c r="M216" t="n">
         <v>1</v>
       </c>
-      <c r="N216" s="2" t="n">
-        <v>46073.39746527778</v>
+      <c r="N216" s="3" t="n">
+        <v>46073.47142361111</v>
       </c>
       <c r="O216" t="inlineStr">
         <is>
@@ -14500,8 +14507,8 @@
       <c r="M217" t="n">
         <v>1</v>
       </c>
-      <c r="N217" s="2" t="n">
-        <v>46073.39285879629</v>
+      <c r="N217" s="3" t="n">
+        <v>46073.46559027778</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14564,8 +14571,8 @@
       <c r="M218" t="n">
         <v>1</v>
       </c>
-      <c r="N218" s="2" t="n">
-        <v>46073.38060185185</v>
+      <c r="N218" s="3" t="n">
+        <v>46073.45606481482</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14628,7 +14635,7 @@
       <c r="M219" t="n">
         <v>1</v>
       </c>
-      <c r="N219" s="2" t="n">
+      <c r="N219" s="3" t="n">
         <v>46073.35392361111</v>
       </c>
       <c r="O219" t="inlineStr">
@@ -14697,8 +14704,8 @@
       <c r="M220" t="n">
         <v>1</v>
       </c>
-      <c r="N220" s="2" t="n">
-        <v>46073.39547453704</v>
+      <c r="N220" s="3" t="n">
+        <v>46073.46936342592</v>
       </c>
       <c r="O220" t="inlineStr">
         <is>
@@ -14761,8 +14768,8 @@
       <c r="M221" t="n">
         <v>1</v>
       </c>
-      <c r="N221" s="2" t="n">
-        <v>46073.37403935185</v>
+      <c r="N221" s="3" t="n">
+        <v>46073.45256944445</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14825,8 +14832,8 @@
       <c r="M222" t="n">
         <v>1</v>
       </c>
-      <c r="N222" s="2" t="n">
-        <v>46073.37587962963</v>
+      <c r="N222" s="3" t="n">
+        <v>46073.44792824074</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -14889,7 +14896,7 @@
       <c r="M223" t="n">
         <v>1</v>
       </c>
-      <c r="N223" s="2" t="n">
+      <c r="N223" s="3" t="n">
         <v>46072.8194212963</v>
       </c>
       <c r="O223" t="inlineStr">
@@ -14953,7 +14960,7 @@
       <c r="M224" t="n">
         <v>1</v>
       </c>
-      <c r="N224" s="2" t="n">
+      <c r="N224" s="3" t="n">
         <v>46072.75394675926</v>
       </c>
       <c r="O224" t="inlineStr">
@@ -15017,7 +15024,7 @@
       <c r="M225" t="n">
         <v>1</v>
       </c>
-      <c r="N225" s="2" t="n">
+      <c r="N225" s="3" t="n">
         <v>46072.80571759259</v>
       </c>
       <c r="O225" t="inlineStr">
@@ -15081,8 +15088,8 @@
       <c r="M226" t="n">
         <v>1</v>
       </c>
-      <c r="N226" s="2" t="n">
-        <v>46073.3868287037</v>
+      <c r="N226" s="3" t="n">
+        <v>46073.46082175926</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15145,8 +15152,8 @@
       <c r="M227" t="n">
         <v>1</v>
       </c>
-      <c r="N227" s="2" t="n">
-        <v>46073.3709375</v>
+      <c r="N227" s="3" t="n">
+        <v>46073.4477662037</v>
       </c>
       <c r="O227" t="inlineStr">
         <is>
@@ -15209,7 +15216,7 @@
       <c r="M228" t="n">
         <v>1</v>
       </c>
-      <c r="N228" s="2" t="n">
+      <c r="N228" s="3" t="n">
         <v>46072.80038194444</v>
       </c>
       <c r="O228" t="inlineStr">
@@ -15273,8 +15280,8 @@
       <c r="M229" t="n">
         <v>1</v>
       </c>
-      <c r="N229" s="2" t="n">
-        <v>46073.37561342592</v>
+      <c r="N229" s="3" t="n">
+        <v>46073.45429398148</v>
       </c>
       <c r="O229" t="inlineStr">
         <is>
@@ -15337,8 +15344,8 @@
       <c r="M230" t="n">
         <v>1</v>
       </c>
-      <c r="N230" s="2" t="n">
-        <v>46073.39105324074</v>
+      <c r="N230" s="3" t="n">
+        <v>46073.46483796297</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15401,8 +15408,8 @@
       <c r="M231" t="n">
         <v>1</v>
       </c>
-      <c r="N231" s="2" t="n">
-        <v>46073.38108796296</v>
+      <c r="N231" s="3" t="n">
+        <v>46073.45997685185</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15465,8 +15472,8 @@
       <c r="M232" t="n">
         <v>1</v>
       </c>
-      <c r="N232" s="2" t="n">
-        <v>46073.37158564815</v>
+      <c r="N232" s="3" t="n">
+        <v>46073.4774537037</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -15529,8 +15536,8 @@
       <c r="M233" t="n">
         <v>1</v>
       </c>
-      <c r="N233" s="2" t="n">
-        <v>46073.37332175926</v>
+      <c r="N233" s="3" t="n">
+        <v>46073.45591435185</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15593,8 +15600,8 @@
       <c r="M234" t="n">
         <v>1</v>
       </c>
-      <c r="N234" s="2" t="n">
-        <v>46073.38395833333</v>
+      <c r="N234" s="3" t="n">
+        <v>46073.48069444444</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -15657,7 +15664,7 @@
       <c r="M235" t="n">
         <v>1</v>
       </c>
-      <c r="N235" s="2" t="n">
+      <c r="N235" s="3" t="n">
         <v>46072.8212037037</v>
       </c>
       <c r="O235" t="inlineStr">
@@ -15721,7 +15728,7 @@
       <c r="M236" t="n">
         <v>1</v>
       </c>
-      <c r="N236" s="2" t="n">
+      <c r="N236" s="3" t="n">
         <v>46072.8075462963</v>
       </c>
       <c r="O236" t="inlineStr">
@@ -15785,7 +15792,7 @@
       <c r="M237" t="n">
         <v>1</v>
       </c>
-      <c r="N237" s="2" t="n">
+      <c r="N237" s="3" t="n">
         <v>46072.81847222222</v>
       </c>
       <c r="O237" t="inlineStr">
@@ -15849,8 +15856,8 @@
       <c r="M238" t="n">
         <v>1</v>
       </c>
-      <c r="N238" s="2" t="n">
-        <v>46073.36914351852</v>
+      <c r="N238" s="3" t="n">
+        <v>46073.48479166667</v>
       </c>
       <c r="O238" t="inlineStr">
         <is>
@@ -15913,8 +15920,8 @@
       <c r="M239" t="n">
         <v>1</v>
       </c>
-      <c r="N239" s="2" t="n">
-        <v>46073.39376157407</v>
+      <c r="N239" s="3" t="n">
+        <v>46073.47472222222</v>
       </c>
       <c r="O239" t="inlineStr">
         <is>
@@ -15977,8 +15984,8 @@
       <c r="M240" t="n">
         <v>1</v>
       </c>
-      <c r="N240" s="2" t="n">
-        <v>46073.36658564815</v>
+      <c r="N240" s="3" t="n">
+        <v>46073.48271990741</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16041,8 +16048,8 @@
       <c r="M241" t="n">
         <v>1</v>
       </c>
-      <c r="N241" s="2" t="n">
-        <v>46073.38702546297</v>
+      <c r="N241" s="3" t="n">
+        <v>46073.46646990741</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16105,8 +16112,8 @@
       <c r="M242" t="n">
         <v>1</v>
       </c>
-      <c r="N242" s="2" t="n">
-        <v>46073.39457175926</v>
+      <c r="N242" s="3" t="n">
+        <v>46073.47324074074</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16169,8 +16176,8 @@
       <c r="M243" t="n">
         <v>1</v>
       </c>
-      <c r="N243" s="2" t="n">
-        <v>46073.38826388889</v>
+      <c r="N243" s="3" t="n">
+        <v>46073.4615625</v>
       </c>
       <c r="O243" t="inlineStr">
         <is>
@@ -16189,11 +16196,6 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
-      <c r="C244" t="inlineStr">
-        <is>
-          <t>10.69.5.112</t>
-        </is>
-      </c>
       <c r="D244" t="n">
         <v>2019</v>
       </c>
@@ -16233,8 +16235,8 @@
       <c r="M244" t="n">
         <v>1</v>
       </c>
-      <c r="N244" s="2" t="n">
-        <v>46073.37193287037</v>
+      <c r="N244" s="3" t="n">
+        <v>46073.40925925926</v>
       </c>
       <c r="O244" t="inlineStr">
         <is>
@@ -16297,8 +16299,8 @@
       <c r="M245" t="n">
         <v>1</v>
       </c>
-      <c r="N245" s="2" t="n">
-        <v>46073.38876157408</v>
+      <c r="N245" s="3" t="n">
+        <v>46073.46831018518</v>
       </c>
       <c r="O245" t="inlineStr">
         <is>
@@ -16361,8 +16363,8 @@
       <c r="M246" t="n">
         <v>1</v>
       </c>
-      <c r="N246" s="2" t="n">
-        <v>46073.39347222223</v>
+      <c r="N246" s="3" t="n">
+        <v>46073.47136574074</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16425,8 +16427,8 @@
       <c r="M247" t="n">
         <v>1</v>
       </c>
-      <c r="N247" s="2" t="n">
-        <v>46073.39267361111</v>
+      <c r="N247" s="3" t="n">
+        <v>46073.47594907408</v>
       </c>
       <c r="O247" t="inlineStr">
         <is>
@@ -16489,8 +16491,8 @@
       <c r="M248" t="n">
         <v>1</v>
       </c>
-      <c r="N248" s="2" t="n">
-        <v>46073.39356481482</v>
+      <c r="N248" s="3" t="n">
+        <v>46073.46679398148</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16553,8 +16555,8 @@
       <c r="M249" t="n">
         <v>1</v>
       </c>
-      <c r="N249" s="2" t="n">
-        <v>46073.3755787037</v>
+      <c r="N249" s="3" t="n">
+        <v>46073.48023148148</v>
       </c>
       <c r="O249" t="inlineStr">
         <is>
@@ -16573,6 +16575,11 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>10.69.5.118</t>
+        </is>
+      </c>
       <c r="D250" t="n">
         <v>2017</v>
       </c>
@@ -16612,8 +16619,8 @@
       <c r="M250" t="n">
         <v>1</v>
       </c>
-      <c r="N250" s="2" t="n">
-        <v>46073.39763888889</v>
+      <c r="N250" s="3" t="n">
+        <v>46073.47754629629</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16676,8 +16683,8 @@
       <c r="M251" t="n">
         <v>1</v>
       </c>
-      <c r="N251" s="2" t="n">
-        <v>46073.38850694444</v>
+      <c r="N251" s="3" t="n">
+        <v>46073.46884259259</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16740,8 +16747,8 @@
       <c r="M252" t="n">
         <v>1</v>
       </c>
-      <c r="N252" s="2" t="n">
-        <v>46073.39868055555</v>
+      <c r="N252" s="3" t="n">
+        <v>46073.47478009259</v>
       </c>
       <c r="O252" t="inlineStr">
         <is>
@@ -16804,8 +16811,8 @@
       <c r="M253" t="n">
         <v>1</v>
       </c>
-      <c r="N253" s="2" t="n">
-        <v>46073.39792824074</v>
+      <c r="N253" s="3" t="n">
+        <v>46073.47702546296</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16862,8 +16869,8 @@
       <c r="M254" t="n">
         <v>1</v>
       </c>
-      <c r="N254" s="2" t="n">
-        <v>46073.3972337963</v>
+      <c r="N254" s="3" t="n">
+        <v>46073.47385416667</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -16926,8 +16933,8 @@
       <c r="M255" t="n">
         <v>1</v>
       </c>
-      <c r="N255" s="2" t="n">
-        <v>46073.38328703704</v>
+      <c r="N255" s="3" t="n">
+        <v>46073.46239583333</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -16990,8 +16997,8 @@
       <c r="M256" t="n">
         <v>1</v>
       </c>
-      <c r="N256" s="2" t="n">
-        <v>46073.36387731481</v>
+      <c r="N256" s="3" t="n">
+        <v>46073.48295138889</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17054,8 +17061,8 @@
       <c r="M257" t="n">
         <v>1</v>
       </c>
-      <c r="N257" s="2" t="n">
-        <v>46073.38077546296</v>
+      <c r="N257" s="3" t="n">
+        <v>46073.45731481481</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17118,8 +17125,8 @@
       <c r="M258" t="n">
         <v>1</v>
       </c>
-      <c r="N258" s="2" t="n">
-        <v>46073.37458333333</v>
+      <c r="N258" s="3" t="n">
+        <v>46073.44947916667</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
@@ -17182,8 +17189,8 @@
       <c r="M259" t="n">
         <v>1</v>
       </c>
-      <c r="N259" s="2" t="n">
-        <v>46073.37268518518</v>
+      <c r="N259" s="3" t="n">
+        <v>46073.44798611111</v>
       </c>
       <c r="O259" t="inlineStr">
         <is>
@@ -17246,8 +17253,8 @@
       <c r="M260" t="n">
         <v>1</v>
       </c>
-      <c r="N260" s="2" t="n">
-        <v>46073.40150462963</v>
+      <c r="N260" s="3" t="n">
+        <v>46073.48180555556</v>
       </c>
       <c r="O260" t="inlineStr">
         <is>
@@ -17310,8 +17317,8 @@
       <c r="M261" t="n">
         <v>1</v>
       </c>
-      <c r="N261" s="2" t="n">
-        <v>46073.37185185185</v>
+      <c r="N261" s="3" t="n">
+        <v>46073.45108796296</v>
       </c>
       <c r="O261" t="inlineStr">
         <is>
@@ -17374,8 +17381,8 @@
       <c r="M262" t="n">
         <v>1</v>
       </c>
-      <c r="N262" s="2" t="n">
-        <v>46073.38172453704</v>
+      <c r="N262" s="3" t="n">
+        <v>46073.45975694444</v>
       </c>
       <c r="O262" t="inlineStr">
         <is>
@@ -17438,8 +17445,8 @@
       <c r="M263" t="n">
         <v>1</v>
       </c>
-      <c r="N263" s="2" t="n">
-        <v>46073.36895833333</v>
+      <c r="N263" s="3" t="n">
+        <v>46073.48707175926</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17502,8 +17509,8 @@
       <c r="M264" t="n">
         <v>1</v>
       </c>
-      <c r="N264" s="2" t="n">
-        <v>46073.37553240741</v>
+      <c r="N264" s="3" t="n">
+        <v>46073.45393518519</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17566,8 +17573,8 @@
       <c r="M265" t="n">
         <v>1</v>
       </c>
-      <c r="N265" s="2" t="n">
-        <v>46073.39607638889</v>
+      <c r="N265" s="3" t="n">
+        <v>46073.45158564814</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17630,8 +17637,8 @@
       <c r="M266" t="n">
         <v>1</v>
       </c>
-      <c r="N266" s="2" t="n">
-        <v>46073.38297453704</v>
+      <c r="N266" s="3" t="n">
+        <v>46073.45802083334</v>
       </c>
       <c r="O266" t="inlineStr">
         <is>
@@ -17694,8 +17701,8 @@
       <c r="M267" t="n">
         <v>1</v>
       </c>
-      <c r="N267" s="2" t="n">
-        <v>46073.36855324074</v>
+      <c r="N267" s="3" t="n">
+        <v>46073.47905092593</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17758,8 +17765,8 @@
       <c r="M268" t="n">
         <v>1</v>
       </c>
-      <c r="N268" s="2" t="n">
-        <v>46073.37128472222</v>
+      <c r="N268" s="3" t="n">
+        <v>46073.450625</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17822,8 +17829,8 @@
       <c r="M269" t="n">
         <v>1</v>
       </c>
-      <c r="N269" s="2" t="n">
-        <v>46072.81524305556</v>
+      <c r="N269" s="3" t="n">
+        <v>46073.45212962963</v>
       </c>
       <c r="O269" t="inlineStr">
         <is>
@@ -17883,8 +17890,8 @@
           <t>HP Compaq 6005 Pro SFF PC</t>
         </is>
       </c>
-      <c r="N270" s="2" t="n">
-        <v>46073.39254629629</v>
+      <c r="N270" s="3" t="n">
+        <v>46073.4730324074</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -17947,8 +17954,8 @@
       <c r="M271" t="n">
         <v>1</v>
       </c>
-      <c r="N271" s="2" t="n">
-        <v>46072.92203703704</v>
+      <c r="N271" s="3" t="n">
+        <v>46073.45253472222</v>
       </c>
       <c r="O271" t="inlineStr">
         <is>
@@ -18011,8 +18018,8 @@
       <c r="M272" t="n">
         <v>1</v>
       </c>
-      <c r="N272" s="2" t="n">
-        <v>46073.39798611111</v>
+      <c r="N272" s="3" t="n">
+        <v>46073.47112268519</v>
       </c>
       <c r="O272" t="inlineStr">
         <is>
@@ -18075,8 +18082,8 @@
       <c r="M273" t="n">
         <v>2</v>
       </c>
-      <c r="N273" s="2" t="n">
-        <v>46073.3725462963</v>
+      <c r="N273" s="3" t="n">
+        <v>46073.46599537037</v>
       </c>
       <c r="O273" t="inlineStr">
         <is>
@@ -18139,7 +18146,7 @@
       <c r="M274" t="n">
         <v>1</v>
       </c>
-      <c r="N274" s="2" t="n">
+      <c r="N274" s="3" t="n">
         <v>46032.86671296296</v>
       </c>
       <c r="O274" t="inlineStr">
@@ -18203,7 +18210,7 @@
       <c r="M275" t="n">
         <v>1</v>
       </c>
-      <c r="N275" s="2" t="n">
+      <c r="N275" s="3" t="n">
         <v>46057.48512731482</v>
       </c>
       <c r="O275" t="inlineStr">
@@ -18267,7 +18274,7 @@
       <c r="M276" t="n">
         <v>1</v>
       </c>
-      <c r="N276" s="2" t="n">
+      <c r="N276" s="3" t="n">
         <v>46060.84670138889</v>
       </c>
       <c r="O276" t="inlineStr">
@@ -18331,7 +18338,7 @@
       <c r="M277" t="n">
         <v>1</v>
       </c>
-      <c r="N277" s="2" t="n">
+      <c r="N277" s="3" t="n">
         <v>46067.85915509259</v>
       </c>
       <c r="O277" t="inlineStr">
@@ -18395,8 +18402,8 @@
       <c r="M278" t="n">
         <v>1</v>
       </c>
-      <c r="N278" s="2" t="n">
-        <v>46073.37805555556</v>
+      <c r="N278" s="3" t="n">
+        <v>46073.45769675926</v>
       </c>
       <c r="O278" t="inlineStr">
         <is>
@@ -18459,8 +18466,8 @@
       <c r="M279" t="n">
         <v>1</v>
       </c>
-      <c r="N279" s="2" t="n">
-        <v>46073.38271990741</v>
+      <c r="N279" s="3" t="n">
+        <v>46073.46763888889</v>
       </c>
       <c r="O279" t="inlineStr">
         <is>
@@ -18523,8 +18530,8 @@
       <c r="M280" t="n">
         <v>1</v>
       </c>
-      <c r="N280" s="2" t="n">
-        <v>46073.40283564815</v>
+      <c r="N280" s="3" t="n">
+        <v>46073.47653935185</v>
       </c>
       <c r="O280" t="inlineStr">
         <is>
@@ -18587,8 +18594,8 @@
       <c r="M281" t="n">
         <v>1</v>
       </c>
-      <c r="N281" s="2" t="n">
-        <v>46073.39949074074</v>
+      <c r="N281" s="3" t="n">
+        <v>46073.4733912037</v>
       </c>
       <c r="O281" t="inlineStr">
         <is>
@@ -18646,8 +18653,8 @@
       <c r="M282" t="n">
         <v>1</v>
       </c>
-      <c r="N282" s="2" t="n">
-        <v>46073.39398148148</v>
+      <c r="N282" s="3" t="n">
+        <v>46073.47054398148</v>
       </c>
       <c r="O282" t="inlineStr">
         <is>
@@ -18710,8 +18717,8 @@
       <c r="M283" t="n">
         <v>1</v>
       </c>
-      <c r="N283" s="2" t="n">
-        <v>46073.37384259259</v>
+      <c r="N283" s="3" t="n">
+        <v>46073.4495949074</v>
       </c>
       <c r="O283" t="inlineStr">
         <is>
@@ -18774,8 +18781,8 @@
       <c r="M284" t="n">
         <v>1</v>
       </c>
-      <c r="N284" s="2" t="n">
-        <v>46073.37278935185</v>
+      <c r="N284" s="3" t="n">
+        <v>46073.45428240741</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18838,8 +18845,8 @@
       <c r="M285" t="n">
         <v>1</v>
       </c>
-      <c r="N285" s="2" t="n">
-        <v>46073.40121527778</v>
+      <c r="N285" s="3" t="n">
+        <v>46073.47928240741</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -18858,6 +18865,11 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>10.69.5.155</t>
+        </is>
+      </c>
       <c r="D286" t="n">
         <v>2019</v>
       </c>
@@ -18897,8 +18909,8 @@
       <c r="M286" t="n">
         <v>1</v>
       </c>
-      <c r="N286" s="2" t="n">
-        <v>46073.3275462963</v>
+      <c r="N286" s="3" t="n">
+        <v>46073.46982638889</v>
       </c>
       <c r="O286" t="inlineStr">
         <is>
@@ -18961,8 +18973,8 @@
       <c r="M287" t="n">
         <v>1</v>
       </c>
-      <c r="N287" s="2" t="n">
-        <v>46073.39290509259</v>
+      <c r="N287" s="3" t="n">
+        <v>46073.4709375</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
@@ -19025,8 +19037,8 @@
       <c r="M288" t="n">
         <v>1</v>
       </c>
-      <c r="N288" s="2" t="n">
-        <v>46073.39195601852</v>
+      <c r="N288" s="3" t="n">
+        <v>46073.46717592593</v>
       </c>
       <c r="O288" t="inlineStr">
         <is>
@@ -19089,8 +19101,8 @@
       <c r="M289" t="n">
         <v>1</v>
       </c>
-      <c r="N289" s="2" t="n">
-        <v>46072.85033564815</v>
+      <c r="N289" s="3" t="n">
+        <v>46073.45945601852</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -19145,7 +19157,7 @@
           <t>ThinkCentre A55</t>
         </is>
       </c>
-      <c r="N290" s="2" t="n">
+      <c r="N290" s="3" t="n">
         <v>45944.86892361111</v>
       </c>
       <c r="O290" t="inlineStr">
@@ -19206,7 +19218,7 @@
           <t>OptiPlex 360</t>
         </is>
       </c>
-      <c r="N291" s="2" t="n">
+      <c r="N291" s="3" t="n">
         <v>45932.79061342592</v>
       </c>
       <c r="O291" t="inlineStr">
@@ -19267,7 +19279,7 @@
           <t>HP 402 G1 SFF Business PC</t>
         </is>
       </c>
-      <c r="N292" s="2" t="n">
+      <c r="N292" s="3" t="n">
         <v>45937.38847222222</v>
       </c>
       <c r="O292" t="inlineStr">
@@ -19328,7 +19340,7 @@
           <t>OptiPlex 360</t>
         </is>
       </c>
-      <c r="N293" s="2" t="n">
+      <c r="N293" s="3" t="n">
         <v>45932.74287037037</v>
       </c>
       <c r="O293" t="inlineStr">
@@ -19389,7 +19401,7 @@
           <t>OptiPlex 360</t>
         </is>
       </c>
-      <c r="N294" s="2" t="n">
+      <c r="N294" s="3" t="n">
         <v>45826.57208333333</v>
       </c>
       <c r="O294" t="inlineStr">
@@ -19450,7 +19462,7 @@
           <t>ThinkCentre A55</t>
         </is>
       </c>
-      <c r="N295" s="2" t="n">
+      <c r="N295" s="3" t="n">
         <v>45901.85885416667</v>
       </c>
       <c r="O295" t="inlineStr">
@@ -19511,7 +19523,7 @@
           <t>OptiPlex 360</t>
         </is>
       </c>
-      <c r="N296" s="2" t="n">
+      <c r="N296" s="3" t="n">
         <v>45932.7109375</v>
       </c>
       <c r="O296" t="inlineStr">
@@ -19572,7 +19584,7 @@
           <t>ThinkCentre M58e</t>
         </is>
       </c>
-      <c r="N297" s="2" t="n">
+      <c r="N297" s="3" t="n">
         <v>45908.87260416667</v>
       </c>
       <c r="O297" t="inlineStr">
@@ -19633,7 +19645,7 @@
           <t>OptiPlex 755</t>
         </is>
       </c>
-      <c r="N298" s="2" t="n">
+      <c r="N298" s="3" t="n">
         <v>45937.37885416667</v>
       </c>
       <c r="O298" t="inlineStr">
@@ -19694,7 +19706,7 @@
           <t>OptiPlex 360</t>
         </is>
       </c>
-      <c r="N299" s="2" t="n">
+      <c r="N299" s="3" t="n">
         <v>45932.63596064815</v>
       </c>
       <c r="O299" t="inlineStr">
@@ -19758,7 +19770,7 @@
       <c r="M300" t="n">
         <v>1</v>
       </c>
-      <c r="N300" s="2" t="n">
+      <c r="N300" s="3" t="n">
         <v>45895.86393518518</v>
       </c>
       <c r="O300" t="inlineStr">
@@ -19819,7 +19831,7 @@
           <t>OptiPlex 745</t>
         </is>
       </c>
-      <c r="N301" s="2" t="n">
+      <c r="N301" s="3" t="n">
         <v>45932.62702546296</v>
       </c>
       <c r="O301" t="inlineStr">
@@ -19883,8 +19895,8 @@
       <c r="M302" t="n">
         <v>1</v>
       </c>
-      <c r="N302" s="2" t="n">
-        <v>46073.39469907407</v>
+      <c r="N302" s="3" t="n">
+        <v>46073.46896990741</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -19944,7 +19956,7 @@
           <t>OptiPlex 755</t>
         </is>
       </c>
-      <c r="N303" s="2" t="n">
+      <c r="N303" s="3" t="n">
         <v>45932.6643287037</v>
       </c>
       <c r="O303" t="inlineStr">
@@ -20005,7 +20017,7 @@
           <t>ThinkCentre A55</t>
         </is>
       </c>
-      <c r="N304" s="2" t="n">
+      <c r="N304" s="3" t="n">
         <v>46066.15606481482</v>
       </c>
       <c r="O304" t="inlineStr">
@@ -20069,7 +20081,7 @@
       <c r="M305" t="n">
         <v>1</v>
       </c>
-      <c r="N305" s="2" t="n">
+      <c r="N305" s="3" t="n">
         <v>46036.83804398148</v>
       </c>
       <c r="O305" t="inlineStr">
@@ -20130,7 +20142,7 @@
           <t>ThinkCentre A55</t>
         </is>
       </c>
-      <c r="N306" s="2" t="n">
+      <c r="N306" s="3" t="n">
         <v>46022.85438657407</v>
       </c>
       <c r="O306" t="inlineStr">
@@ -20194,7 +20206,7 @@
       <c r="M307" t="n">
         <v>1</v>
       </c>
-      <c r="N307" s="2" t="n">
+      <c r="N307" s="3" t="n">
         <v>46043.58903935185</v>
       </c>
       <c r="O307" t="inlineStr">
@@ -20255,7 +20267,7 @@
           <t>OptiPlex 360</t>
         </is>
       </c>
-      <c r="N308" s="2" t="n">
+      <c r="N308" s="3" t="n">
         <v>45903.47273148148</v>
       </c>
       <c r="O308" t="inlineStr">
@@ -20316,7 +20328,7 @@
           <t>OptiPlex 745</t>
         </is>
       </c>
-      <c r="N309" s="2" t="n">
+      <c r="N309" s="3" t="n">
         <v>45971.67914351852</v>
       </c>
       <c r="O309" t="inlineStr">
@@ -20377,7 +20389,7 @@
           <t>OptiPlex 755</t>
         </is>
       </c>
-      <c r="N310" s="2" t="n">
+      <c r="N310" s="3" t="n">
         <v>46046.92365740741</v>
       </c>
       <c r="O310" t="inlineStr">
@@ -20441,7 +20453,7 @@
       <c r="M311" t="n">
         <v>2</v>
       </c>
-      <c r="N311" s="2" t="n">
+      <c r="N311" s="3" t="n">
         <v>46055.8405324074</v>
       </c>
       <c r="O311" t="inlineStr">
@@ -20502,7 +20514,7 @@
           <t>OptiPlex 745</t>
         </is>
       </c>
-      <c r="N312" s="2" t="n">
+      <c r="N312" s="3" t="n">
         <v>46056.50774305555</v>
       </c>
       <c r="O312" t="inlineStr">
@@ -20563,7 +20575,7 @@
           <t>OptiPlex 360</t>
         </is>
       </c>
-      <c r="N313" s="2" t="n">
+      <c r="N313" s="3" t="n">
         <v>46057.83956018519</v>
       </c>
       <c r="O313" t="inlineStr">
@@ -20624,7 +20636,7 @@
           <t>HP Compaq dx7400 Brazil SFF PC.</t>
         </is>
       </c>
-      <c r="N314" s="2" t="n">
+      <c r="N314" s="3" t="n">
         <v>46071.79034722222</v>
       </c>
       <c r="O314" t="inlineStr">
@@ -20688,7 +20700,7 @@
       <c r="M315" t="n">
         <v>1</v>
       </c>
-      <c r="N315" s="2" t="n">
+      <c r="N315" s="3" t="n">
         <v>46055.61493055556</v>
       </c>
       <c r="O315" t="inlineStr">
@@ -20749,7 +20761,7 @@
           <t>OptiPlex 745</t>
         </is>
       </c>
-      <c r="N316" s="2" t="n">
+      <c r="N316" s="3" t="n">
         <v>46056.8555324074</v>
       </c>
       <c r="O316" t="inlineStr">
@@ -20813,7 +20825,7 @@
       <c r="M317" t="n">
         <v>1</v>
       </c>
-      <c r="N317" s="2" t="n">
+      <c r="N317" s="3" t="n">
         <v>46056.84979166667</v>
       </c>
       <c r="O317" t="inlineStr">
@@ -20877,7 +20889,7 @@
       <c r="M318" t="n">
         <v>1</v>
       </c>
-      <c r="N318" s="2" t="n">
+      <c r="N318" s="3" t="n">
         <v>46055.84016203704</v>
       </c>
       <c r="O318" t="inlineStr">
@@ -20938,7 +20950,7 @@
           <t>OptiPlex 745</t>
         </is>
       </c>
-      <c r="N319" s="2" t="n">
+      <c r="N319" s="3" t="n">
         <v>46055.83638888889</v>
       </c>
       <c r="O319" t="inlineStr">
@@ -20999,8 +21011,8 @@
           <t>OptiPlex 755</t>
         </is>
       </c>
-      <c r="N320" s="2" t="n">
-        <v>46073.39701388889</v>
+      <c r="N320" s="3" t="n">
+        <v>46073.47508101852</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21060,7 +21072,7 @@
           <t>OptiPlex 360</t>
         </is>
       </c>
-      <c r="N321" s="2" t="n">
+      <c r="N321" s="3" t="n">
         <v>46022.84603009259</v>
       </c>
       <c r="O321" t="inlineStr">
@@ -21124,7 +21136,7 @@
       <c r="M322" t="n">
         <v>1</v>
       </c>
-      <c r="N322" s="2" t="n">
+      <c r="N322" s="3" t="n">
         <v>46055.86734953704</v>
       </c>
       <c r="O322" t="inlineStr">
@@ -21188,7 +21200,7 @@
       <c r="M323" t="n">
         <v>1</v>
       </c>
-      <c r="N323" s="2" t="n">
+      <c r="N323" s="3" t="n">
         <v>46055.8446412037</v>
       </c>
       <c r="O323" t="inlineStr">
@@ -21252,7 +21264,7 @@
       <c r="M324" t="n">
         <v>1</v>
       </c>
-      <c r="N324" s="2" t="n">
+      <c r="N324" s="3" t="n">
         <v>46043.49694444444</v>
       </c>
       <c r="O324" t="inlineStr">
@@ -21316,7 +21328,7 @@
       <c r="M325" t="n">
         <v>1</v>
       </c>
-      <c r="N325" s="2" t="n">
+      <c r="N325" s="3" t="n">
         <v>46052.84412037037</v>
       </c>
       <c r="O325" t="inlineStr">
@@ -21377,7 +21389,7 @@
           <t>ThinkCentre A55</t>
         </is>
       </c>
-      <c r="N326" s="2" t="n">
+      <c r="N326" s="3" t="n">
         <v>46052.87260416667</v>
       </c>
       <c r="O326" t="inlineStr">
@@ -21438,7 +21450,7 @@
           <t>OptiPlex 745</t>
         </is>
       </c>
-      <c r="N327" s="2" t="n">
+      <c r="N327" s="3" t="n">
         <v>46058.66199074074</v>
       </c>
       <c r="O327" t="inlineStr">
@@ -21471,7 +21483,7 @@
       <c r="M328" t="n">
         <v>2</v>
       </c>
-      <c r="N328" s="2" t="n">
+      <c r="N328" s="3" t="n">
         <v>46055.55023148148</v>
       </c>
       <c r="O328" t="inlineStr">
@@ -21535,7 +21547,7 @@
       <c r="M329" t="n">
         <v>1</v>
       </c>
-      <c r="N329" s="2" t="n">
+      <c r="N329" s="3" t="n">
         <v>46064.39572916667</v>
       </c>
       <c r="O329" t="inlineStr">
@@ -21596,7 +21608,7 @@
           <t>OptiPlex 755</t>
         </is>
       </c>
-      <c r="N330" s="2" t="n">
+      <c r="N330" s="3" t="n">
         <v>46055.858125</v>
       </c>
       <c r="O330" t="inlineStr">
@@ -21660,7 +21672,7 @@
       <c r="M331" t="n">
         <v>1</v>
       </c>
-      <c r="N331" s="2" t="n">
+      <c r="N331" s="3" t="n">
         <v>46051.86351851852</v>
       </c>
       <c r="O331" t="inlineStr">
@@ -21724,8 +21736,8 @@
       <c r="M332" t="n">
         <v>1</v>
       </c>
-      <c r="N332" s="2" t="n">
-        <v>46073.39228009259</v>
+      <c r="N332" s="3" t="n">
+        <v>46073.46829861111</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21788,8 +21800,8 @@
       <c r="M333" t="n">
         <v>2</v>
       </c>
-      <c r="N333" s="2" t="n">
-        <v>46073.38990740741</v>
+      <c r="N333" s="3" t="n">
+        <v>46073.4690162037</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21852,8 +21864,8 @@
       <c r="M334" t="n">
         <v>2</v>
       </c>
-      <c r="N334" s="2" t="n">
-        <v>46073.39935185185</v>
+      <c r="N334" s="3" t="n">
+        <v>46073.47671296296</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21916,8 +21928,8 @@
       <c r="M335" t="n">
         <v>2</v>
       </c>
-      <c r="N335" s="2" t="n">
-        <v>46073.40108796296</v>
+      <c r="N335" s="3" t="n">
+        <v>46073.47715277778</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -21980,8 +21992,8 @@
       <c r="M336" t="n">
         <v>1</v>
       </c>
-      <c r="N336" s="2" t="n">
-        <v>46073.38861111111</v>
+      <c r="N336" s="3" t="n">
+        <v>46073.46670138889</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22044,8 +22056,8 @@
       <c r="M337" t="n">
         <v>1</v>
       </c>
-      <c r="N337" s="2" t="n">
-        <v>46073.40054398148</v>
+      <c r="N337" s="3" t="n">
+        <v>46073.48015046296</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22108,8 +22120,8 @@
       <c r="M338" t="n">
         <v>2</v>
       </c>
-      <c r="N338" s="2" t="n">
-        <v>46073.39333333333</v>
+      <c r="N338" s="3" t="n">
+        <v>46073.47547453704</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -22172,8 +22184,8 @@
       <c r="M339" t="n">
         <v>2</v>
       </c>
-      <c r="N339" s="2" t="n">
-        <v>46073.39739583333</v>
+      <c r="N339" s="3" t="n">
+        <v>46073.47252314815</v>
       </c>
       <c r="O339" t="inlineStr">
         <is>
@@ -22234,10 +22246,10 @@
         </is>
       </c>
       <c r="M340" t="n">
-        <v>2</v>
-      </c>
-      <c r="N340" s="2" t="n">
-        <v>46073.37109953703</v>
+        <v>1</v>
+      </c>
+      <c r="N340" s="3" t="n">
+        <v>46073.4329050926</v>
       </c>
       <c r="O340" t="inlineStr">
         <is>
@@ -22300,8 +22312,8 @@
       <c r="M341" t="n">
         <v>2</v>
       </c>
-      <c r="N341" s="2" t="n">
-        <v>46073.37787037037</v>
+      <c r="N341" s="3" t="n">
+        <v>46073.45701388889</v>
       </c>
       <c r="O341" t="inlineStr">
         <is>
@@ -22364,8 +22376,8 @@
       <c r="M342" t="n">
         <v>2</v>
       </c>
-      <c r="N342" s="2" t="n">
-        <v>46073.38234953704</v>
+      <c r="N342" s="3" t="n">
+        <v>46073.45991898148</v>
       </c>
       <c r="O342" t="inlineStr">
         <is>
@@ -22384,11 +22396,6 @@
           <t>OPERACAO 9.1</t>
         </is>
       </c>
-      <c r="C343" t="inlineStr">
-        <is>
-          <t>10.69.5.237</t>
-        </is>
-      </c>
       <c r="D343" t="n">
         <v>2017</v>
       </c>
@@ -22430,8 +22437,8 @@
           <t>HP Compaq Pro 4300 SFF Brazil PC</t>
         </is>
       </c>
-      <c r="N343" s="2" t="n">
-        <v>46073.39797453704</v>
+      <c r="N343" s="3" t="n">
+        <v>46073.47489583334</v>
       </c>
       <c r="O343" t="inlineStr">
         <is>
@@ -22499,7 +22506,7 @@
       <c r="M344" t="n">
         <v>1</v>
       </c>
-      <c r="N344" s="2" t="n">
+      <c r="N344" s="3" t="n">
         <v>46057.41765046296</v>
       </c>
       <c r="O344" t="inlineStr">
@@ -22558,7 +22565,7 @@
       <c r="M345" t="n">
         <v>1</v>
       </c>
-      <c r="N345" s="2" t="n">
+      <c r="N345" s="3" t="n">
         <v>46057.4218287037</v>
       </c>
       <c r="O345" t="inlineStr">
@@ -22622,7 +22629,7 @@
       <c r="M346" t="n">
         <v>2</v>
       </c>
-      <c r="N346" s="2" t="n">
+      <c r="N346" s="3" t="n">
         <v>46045.4404050926</v>
       </c>
       <c r="O346" t="inlineStr">
@@ -22686,8 +22693,8 @@
       <c r="M347" t="n">
         <v>1</v>
       </c>
-      <c r="N347" s="2" t="n">
-        <v>46073.38025462963</v>
+      <c r="N347" s="3" t="n">
+        <v>46073.4621412037</v>
       </c>
       <c r="O347" t="inlineStr">
         <is>
@@ -22748,10 +22755,10 @@
         </is>
       </c>
       <c r="M348" t="n">
-        <v>1</v>
-      </c>
-      <c r="N348" s="2" t="n">
-        <v>46073.38104166667</v>
+        <v>2</v>
+      </c>
+      <c r="N348" s="3" t="n">
+        <v>46073.45680555556</v>
       </c>
       <c r="O348" t="inlineStr">
         <is>
@@ -22814,8 +22821,8 @@
       <c r="M349" t="n">
         <v>1</v>
       </c>
-      <c r="N349" s="2" t="n">
-        <v>46073.38085648148</v>
+      <c r="N349" s="3" t="n">
+        <v>46073.45896990741</v>
       </c>
       <c r="O349" t="inlineStr">
         <is>
@@ -22834,6 +22841,11 @@
           <t>OPERACAO 9.1</t>
         </is>
       </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>10.69.5.244</t>
+        </is>
+      </c>
       <c r="D350" t="n">
         <v>2014</v>
       </c>
@@ -22873,8 +22885,8 @@
       <c r="M350" t="n">
         <v>1</v>
       </c>
-      <c r="N350" s="2" t="n">
-        <v>46072.38997685185</v>
+      <c r="N350" s="3" t="n">
+        <v>46073.4872337963</v>
       </c>
       <c r="O350" t="inlineStr">
         <is>
@@ -22937,8 +22949,8 @@
       <c r="M351" t="n">
         <v>1</v>
       </c>
-      <c r="N351" s="2" t="n">
-        <v>46073.38199074074</v>
+      <c r="N351" s="3" t="n">
+        <v>46073.46149305555</v>
       </c>
       <c r="O351" t="inlineStr">
         <is>
@@ -23001,8 +23013,8 @@
       <c r="M352" t="n">
         <v>1</v>
       </c>
-      <c r="N352" s="2" t="n">
-        <v>46073.38332175926</v>
+      <c r="N352" s="3" t="n">
+        <v>46073.46563657407</v>
       </c>
       <c r="O352" t="inlineStr">
         <is>
@@ -23062,8 +23074,8 @@
           <t>HP 402 G1 SFF Business PC</t>
         </is>
       </c>
-      <c r="N353" s="2" t="n">
-        <v>46073.38038194444</v>
+      <c r="N353" s="3" t="n">
+        <v>46073.46053240741</v>
       </c>
       <c r="O353" t="inlineStr">
         <is>
@@ -23123,8 +23135,8 @@
           <t>HP 402 G1 SFF Business PC</t>
         </is>
       </c>
-      <c r="N354" s="2" t="n">
-        <v>46073.37996527777</v>
+      <c r="N354" s="3" t="n">
+        <v>46073.45943287037</v>
       </c>
       <c r="O354" t="inlineStr">
         <is>
@@ -23187,8 +23199,8 @@
       <c r="M355" t="n">
         <v>1</v>
       </c>
-      <c r="N355" s="2" t="n">
-        <v>46073.37936342593</v>
+      <c r="N355" s="3" t="n">
+        <v>46073.45901620371</v>
       </c>
       <c r="O355" t="inlineStr">
         <is>
@@ -23251,8 +23263,8 @@
       <c r="M356" t="n">
         <v>1</v>
       </c>
-      <c r="N356" s="2" t="n">
-        <v>46073.37986111111</v>
+      <c r="N356" s="3" t="n">
+        <v>46073.45615740741</v>
       </c>
       <c r="O356" t="inlineStr">
         <is>
@@ -23315,8 +23327,8 @@
       <c r="M357" t="n">
         <v>1</v>
       </c>
-      <c r="N357" s="2" t="n">
-        <v>46072.60423611111</v>
+      <c r="N357" s="3" t="n">
+        <v>46073.45711805556</v>
       </c>
       <c r="O357" t="inlineStr">
         <is>
@@ -23374,7 +23386,7 @@
       <c r="M358" t="n">
         <v>1</v>
       </c>
-      <c r="N358" s="2" t="n">
+      <c r="N358" s="3" t="n">
         <v>46072.40707175926</v>
       </c>
       <c r="O358" t="inlineStr">
@@ -23438,7 +23450,7 @@
       <c r="M359" t="n">
         <v>2</v>
       </c>
-      <c r="N359" s="2" t="n">
+      <c r="N359" s="3" t="n">
         <v>46073.38041666667</v>
       </c>
       <c r="O359" t="inlineStr">
@@ -23502,8 +23514,8 @@
       <c r="M360" t="n">
         <v>2</v>
       </c>
-      <c r="N360" s="2" t="n">
-        <v>46073.38026620371</v>
+      <c r="N360" s="3" t="n">
+        <v>46073.454375</v>
       </c>
       <c r="O360" t="inlineStr">
         <is>
@@ -23566,8 +23578,8 @@
       <c r="M361" t="n">
         <v>1</v>
       </c>
-      <c r="N361" s="2" t="n">
-        <v>46073.3796412037</v>
+      <c r="N361" s="3" t="n">
+        <v>46073.46128472222</v>
       </c>
       <c r="O361" t="inlineStr">
         <is>
@@ -23627,8 +23639,8 @@
           <t>OptiPlex 360</t>
         </is>
       </c>
-      <c r="N362" s="2" t="n">
-        <v>46073.38083333334</v>
+      <c r="N362" s="3" t="n">
+        <v>46073.46034722222</v>
       </c>
       <c r="O362" t="inlineStr">
         <is>
@@ -23688,7 +23700,7 @@
           <t>OptiPlex 755</t>
         </is>
       </c>
-      <c r="N363" s="2" t="n">
+      <c r="N363" s="3" t="n">
         <v>46049.60199074074</v>
       </c>
       <c r="O363" t="inlineStr">
@@ -23752,7 +23764,7 @@
       <c r="M364" t="n">
         <v>2</v>
       </c>
-      <c r="N364" s="2" t="n">
+      <c r="N364" s="3" t="n">
         <v>46072.39605324074</v>
       </c>
       <c r="O364" t="inlineStr">
@@ -23815,8 +23827,8 @@
       <c r="M365" t="n">
         <v>1</v>
       </c>
-      <c r="N365" s="2" t="n">
-        <v>46073.37383101852</v>
+      <c r="N365" s="3" t="n">
+        <v>46073.45385416667</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
@@ -23881,8 +23893,8 @@
           <t>OptiPlex 3070</t>
         </is>
       </c>
-      <c r="N366" s="2" t="n">
-        <v>46073.36855324074</v>
+      <c r="N366" s="3" t="n">
+        <v>46073.47943287037</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -23936,7 +23948,7 @@
           <t>HP 420</t>
         </is>
       </c>
-      <c r="N367" s="2" t="n">
+      <c r="N367" s="3" t="n">
         <v>46002.58769675926</v>
       </c>
       <c r="O367" t="inlineStr">
@@ -24007,8 +24019,8 @@
           <t>HP ProDesk 400 G5 SFF</t>
         </is>
       </c>
-      <c r="N368" s="2" t="n">
-        <v>46073.39989583333</v>
+      <c r="N368" s="3" t="n">
+        <v>46073.47994212963</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -24027,11 +24039,6 @@
           <t>RH</t>
         </is>
       </c>
-      <c r="C369" t="inlineStr">
-        <is>
-          <t>10.69.3.13</t>
-        </is>
-      </c>
       <c r="D369" t="n">
         <v>2025</v>
       </c>
@@ -24073,8 +24080,8 @@
           <t>HP ProDesk 400 G5 SFF</t>
         </is>
       </c>
-      <c r="N369" s="2" t="n">
-        <v>46073.39825231482</v>
+      <c r="N369" s="3" t="n">
+        <v>46073.47359953704</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
@@ -24142,8 +24149,8 @@
       <c r="M370" t="n">
         <v>1</v>
       </c>
-      <c r="N370" s="2" t="n">
-        <v>46073.39251157407</v>
+      <c r="N370" s="3" t="n">
+        <v>46073.47099537037</v>
       </c>
       <c r="O370" t="inlineStr">
         <is>
@@ -24211,7 +24218,7 @@
       <c r="M371" t="n">
         <v>1</v>
       </c>
-      <c r="N371" s="2" t="n">
+      <c r="N371" s="3" t="n">
         <v>46072.6978125</v>
       </c>
       <c r="O371" t="inlineStr">
@@ -24280,7 +24287,7 @@
       <c r="M372" t="n">
         <v>1</v>
       </c>
-      <c r="N372" s="2" t="n">
+      <c r="N372" s="3" t="n">
         <v>46072.64636574074</v>
       </c>
       <c r="O372" t="inlineStr">
@@ -24349,7 +24356,7 @@
       <c r="M373" t="n">
         <v>1</v>
       </c>
-      <c r="N373" s="2" t="n">
+      <c r="N373" s="3" t="n">
         <v>46072.64364583333</v>
       </c>
       <c r="O373" t="inlineStr">
@@ -24418,8 +24425,8 @@
       <c r="M374" t="n">
         <v>1</v>
       </c>
-      <c r="N374" s="2" t="n">
-        <v>46073.38929398148</v>
+      <c r="N374" s="3" t="n">
+        <v>46073.46418981482</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24484,8 +24491,8 @@
           <t>OptiPlex 3070</t>
         </is>
       </c>
-      <c r="N375" s="2" t="n">
-        <v>46073.37616898148</v>
+      <c r="N375" s="3" t="n">
+        <v>46073.45827546297</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
@@ -24504,6 +24511,11 @@
           <t>COORDENACAO</t>
         </is>
       </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>10.69.3.72</t>
+        </is>
+      </c>
       <c r="D376" t="n">
         <v>2025</v>
       </c>
@@ -24548,8 +24560,8 @@
       <c r="M376" t="n">
         <v>1</v>
       </c>
-      <c r="N376" s="2" t="n">
-        <v>46073.36855324074</v>
+      <c r="N376" s="3" t="n">
+        <v>46073.48287037037</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -24617,8 +24629,8 @@
       <c r="M377" t="n">
         <v>2</v>
       </c>
-      <c r="N377" s="2" t="n">
-        <v>46073.38836805556</v>
+      <c r="N377" s="3" t="n">
+        <v>46073.46291666666</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -24686,8 +24698,8 @@
       <c r="M378" t="n">
         <v>2</v>
       </c>
-      <c r="N378" s="2" t="n">
-        <v>46073.37324074074</v>
+      <c r="N378" s="3" t="n">
+        <v>46073.45381944445</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização automática 2026-02-20 13:52:03.909019
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>46073.47710648148</v>
+        <v>46073.55310185185</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>46073.46390046296</v>
+        <v>46073.54446759259</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
         <v>2</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>46073.4574537037</v>
+        <v>46073.53719907408</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>46073.45621527778</v>
+        <v>46073.53348379629</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -1131,7 +1131,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="3" t="n">
-        <v>46073.47350694444</v>
+        <v>46073.54879629629</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1451,7 +1451,7 @@
         <v>1</v>
       </c>
       <c r="N15" s="3" t="n">
-        <v>46073.45480324074</v>
+        <v>46073.56809027777</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1515,7 +1515,7 @@
         <v>2</v>
       </c>
       <c r="N16" s="3" t="n">
-        <v>46073.47081018519</v>
+        <v>46073.55006944444</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -2244,7 +2244,7 @@
         </is>
       </c>
       <c r="N28" s="3" t="n">
-        <v>46072.74151620371</v>
+        <v>46073.54253472222</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -6570,7 +6570,7 @@
         <v>1</v>
       </c>
       <c r="N95" s="3" t="n">
-        <v>46073.46717592593</v>
+        <v>46073.54114583333</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -6639,7 +6639,7 @@
         <v>1</v>
       </c>
       <c r="N96" s="3" t="n">
-        <v>46073.47141203703</v>
+        <v>46073.55028935185</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
@@ -6658,6 +6658,11 @@
           <t>COORDENACAO</t>
         </is>
       </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>10.69.3.93</t>
+        </is>
+      </c>
       <c r="D97" t="n">
         <v>2025</v>
       </c>
@@ -6703,7 +6708,7 @@
         <v>1</v>
       </c>
       <c r="N97" s="3" t="n">
-        <v>46073.48112268518</v>
+        <v>46073.56362268519</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -6767,7 +6772,7 @@
         <v>1</v>
       </c>
       <c r="N98" s="3" t="n">
-        <v>46072.68513888889</v>
+        <v>46073.53438657407</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -6905,7 +6910,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>46073.4875462963</v>
+        <v>46073.56778935185</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6974,7 +6979,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="3" t="n">
-        <v>46073.46143518519</v>
+        <v>46073.53777777778</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -7112,7 +7117,7 @@
         <v>2</v>
       </c>
       <c r="N103" s="3" t="n">
-        <v>46073.47716435185</v>
+        <v>46073.55546296296</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7369,7 +7374,7 @@
         <v>1</v>
       </c>
       <c r="N107" s="3" t="n">
-        <v>46073.46638888889</v>
+        <v>46073.54255787037</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -7507,7 +7512,7 @@
         <v>1</v>
       </c>
       <c r="N109" s="3" t="n">
-        <v>46073.48663194444</v>
+        <v>46073.56684027778</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7576,7 +7581,7 @@
         <v>2</v>
       </c>
       <c r="N110" s="3" t="n">
-        <v>46073.47532407408</v>
+        <v>46073.55362268518</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7645,7 +7650,7 @@
         <v>2</v>
       </c>
       <c r="N111" s="3" t="n">
-        <v>46073.46740740741</v>
+        <v>46073.56353009259</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
@@ -7714,7 +7719,7 @@
         <v>2</v>
       </c>
       <c r="N112" s="3" t="n">
-        <v>46073.48740740741</v>
+        <v>46073.5662962963</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7783,7 +7788,7 @@
         <v>1</v>
       </c>
       <c r="N113" s="3" t="n">
-        <v>46073.4728125</v>
+        <v>46073.55079861111</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7852,7 +7857,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>46073.47325231481</v>
+        <v>46073.55560185185</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -7918,7 +7923,7 @@
         </is>
       </c>
       <c r="N115" s="3" t="n">
-        <v>46073.48346064815</v>
+        <v>46073.56305555555</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -7987,7 +7992,7 @@
         <v>1</v>
       </c>
       <c r="N116" s="3" t="n">
-        <v>46073.47070601852</v>
+        <v>46073.55271990741</v>
       </c>
       <c r="O116" t="inlineStr">
         <is>
@@ -8006,11 +8011,6 @@
           <t>DP</t>
         </is>
       </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>10.69.3.23</t>
-        </is>
-      </c>
       <c r="D117" t="n">
         <v>2025</v>
       </c>
@@ -8056,7 +8056,7 @@
         <v>1</v>
       </c>
       <c r="N117" s="3" t="n">
-        <v>46073.47856481482</v>
+        <v>46073.51700231482</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -8260,7 +8260,7 @@
         <v>1</v>
       </c>
       <c r="N120" s="3" t="n">
-        <v>46073.47305555556</v>
+        <v>46073.54914351852</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -8329,7 +8329,7 @@
         <v>1</v>
       </c>
       <c r="N121" s="3" t="n">
-        <v>46073.47019675926</v>
+        <v>46073.54833333333</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -8395,7 +8395,7 @@
         </is>
       </c>
       <c r="N122" s="3" t="n">
-        <v>46073.47486111111</v>
+        <v>46073.55076388889</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -8464,7 +8464,7 @@
         <v>2</v>
       </c>
       <c r="N123" s="3" t="n">
-        <v>46073.47032407407</v>
+        <v>46073.54980324074</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -8533,7 +8533,7 @@
         <v>1</v>
       </c>
       <c r="N124" s="3" t="n">
-        <v>46073.46333333333</v>
+        <v>46073.5353587963</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -8602,7 +8602,7 @@
         <v>1</v>
       </c>
       <c r="N125" s="3" t="n">
-        <v>46073.4784375</v>
+        <v>46073.55802083333</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -8671,7 +8671,7 @@
         <v>1</v>
       </c>
       <c r="N126" s="3" t="n">
-        <v>46073.46949074074</v>
+        <v>46073.54555555555</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -8740,7 +8740,7 @@
         <v>2</v>
       </c>
       <c r="N127" s="3" t="n">
-        <v>46073.47959490741</v>
+        <v>46073.55962962963</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -8809,7 +8809,7 @@
         <v>1</v>
       </c>
       <c r="N128" s="3" t="n">
-        <v>46073.44976851852</v>
+        <v>46073.56907407408</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -8878,7 +8878,7 @@
         <v>1</v>
       </c>
       <c r="N129" s="3" t="n">
-        <v>46073.47447916667</v>
+        <v>46073.55243055556</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -8947,7 +8947,7 @@
         <v>1</v>
       </c>
       <c r="N130" s="3" t="n">
-        <v>46073.48274305555</v>
+        <v>46073.55601851852</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -9011,7 +9011,7 @@
         <v>1</v>
       </c>
       <c r="N131" s="3" t="n">
-        <v>46073.47479166667</v>
+        <v>46073.55613425926</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -9144,7 +9144,7 @@
         <v>1</v>
       </c>
       <c r="N133" s="3" t="n">
-        <v>46073.45274305555</v>
+        <v>46073.56487268519</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -9208,7 +9208,7 @@
         <v>1</v>
       </c>
       <c r="N134" s="3" t="n">
-        <v>46073.46253472222</v>
+        <v>46073.54048611111</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -9272,7 +9272,7 @@
         <v>1</v>
       </c>
       <c r="N135" s="3" t="n">
-        <v>46073.45353009259</v>
+        <v>46073.56689814815</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -9463,7 +9463,7 @@
         <v>1</v>
       </c>
       <c r="N138" s="3" t="n">
-        <v>46073.46060185185</v>
+        <v>46073.54357638889</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9527,7 +9527,7 @@
         <v>1</v>
       </c>
       <c r="N139" s="3" t="n">
-        <v>46073.47848379629</v>
+        <v>46073.55971064815</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9591,7 +9591,7 @@
         <v>1</v>
       </c>
       <c r="N140" s="3" t="n">
-        <v>46073.45166666667</v>
+        <v>46073.53268518519</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9655,7 +9655,7 @@
         <v>1</v>
       </c>
       <c r="N141" s="3" t="n">
-        <v>46073.44671296296</v>
+        <v>46073.56403935186</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9719,7 +9719,7 @@
         <v>1</v>
       </c>
       <c r="N142" s="3" t="n">
-        <v>46073.47739583333</v>
+        <v>46073.55744212963</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9783,7 +9783,7 @@
         <v>1</v>
       </c>
       <c r="N143" s="3" t="n">
-        <v>46073.47967592593</v>
+        <v>46073.55893518519</v>
       </c>
       <c r="O143" t="inlineStr">
         <is>
@@ -9847,7 +9847,7 @@
         <v>1</v>
       </c>
       <c r="N144" s="3" t="n">
-        <v>46073.47019675926</v>
+        <v>46073.54737268519</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9911,7 +9911,7 @@
         <v>1</v>
       </c>
       <c r="N145" s="3" t="n">
-        <v>46073.45063657407</v>
+        <v>46073.48858796297</v>
       </c>
       <c r="O145" t="inlineStr">
         <is>
@@ -9975,7 +9975,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="3" t="n">
-        <v>46073.48275462963</v>
+        <v>46073.5646875</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10039,7 +10039,7 @@
         <v>1</v>
       </c>
       <c r="N147" s="3" t="n">
-        <v>46073.48597222222</v>
+        <v>46073.56480324074</v>
       </c>
       <c r="O147" t="inlineStr">
         <is>
@@ -10103,7 +10103,7 @@
         <v>1</v>
       </c>
       <c r="N148" s="3" t="n">
-        <v>46073.48334490741</v>
+        <v>46073.56519675926</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10167,7 +10167,7 @@
         <v>1</v>
       </c>
       <c r="N149" s="3" t="n">
-        <v>46073.48458333333</v>
+        <v>46073.56355324074</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -10295,7 +10295,7 @@
         <v>1</v>
       </c>
       <c r="N151" s="3" t="n">
-        <v>46073.48521990741</v>
+        <v>46073.55965277777</v>
       </c>
       <c r="O151" t="inlineStr">
         <is>
@@ -10359,7 +10359,7 @@
         <v>1</v>
       </c>
       <c r="N152" s="3" t="n">
-        <v>46073.48601851852</v>
+        <v>46073.56111111111</v>
       </c>
       <c r="O152" t="inlineStr">
         <is>
@@ -10378,6 +10378,11 @@
           <t>OPERACAO 7.1</t>
         </is>
       </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>10.69.5.21</t>
+        </is>
+      </c>
       <c r="D153" t="n">
         <v>2018</v>
       </c>
@@ -10418,7 +10423,7 @@
         <v>1</v>
       </c>
       <c r="N153" s="3" t="n">
-        <v>46073.45131944444</v>
+        <v>46073.56908564815</v>
       </c>
       <c r="O153" t="inlineStr">
         <is>
@@ -10482,7 +10487,7 @@
         <v>1</v>
       </c>
       <c r="N154" s="3" t="n">
-        <v>46073.46508101852</v>
+        <v>46073.53877314815</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10546,7 +10551,7 @@
         <v>1</v>
       </c>
       <c r="N155" s="3" t="n">
-        <v>46073.48293981481</v>
+        <v>46073.55679398148</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10610,7 +10615,7 @@
         <v>1</v>
       </c>
       <c r="N156" s="3" t="n">
-        <v>46073.44761574074</v>
+        <v>46073.56585648148</v>
       </c>
       <c r="O156" t="inlineStr">
         <is>
@@ -10674,7 +10679,7 @@
         <v>1</v>
       </c>
       <c r="N157" s="3" t="n">
-        <v>46073.45150462963</v>
+        <v>46073.56768518518</v>
       </c>
       <c r="O157" t="inlineStr">
         <is>
@@ -10706,7 +10711,7 @@
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>Windows</t>
+          <t>Microsoft Windows 8.1 Pro</t>
         </is>
       </c>
       <c r="G158" t="inlineStr">
@@ -10738,7 +10743,7 @@
         <v>1</v>
       </c>
       <c r="N158" s="3" t="n">
-        <v>46073.4716550926</v>
+        <v>46073.53177083333</v>
       </c>
       <c r="O158" t="inlineStr">
         <is>
@@ -10802,7 +10807,7 @@
         <v>1</v>
       </c>
       <c r="N159" s="3" t="n">
-        <v>46073.44952546297</v>
+        <v>46073.56733796297</v>
       </c>
       <c r="O159" t="inlineStr">
         <is>
@@ -10866,7 +10871,7 @@
         <v>1</v>
       </c>
       <c r="N160" s="3" t="n">
-        <v>46073.45673611111</v>
+        <v>46073.53212962963</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
@@ -10930,7 +10935,7 @@
         <v>1</v>
       </c>
       <c r="N161" s="3" t="n">
-        <v>46073.44894675926</v>
+        <v>46073.57064814815</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -10994,7 +10999,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="3" t="n">
-        <v>46073.47883101852</v>
+        <v>46073.55766203703</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11122,7 +11127,7 @@
         <v>2</v>
       </c>
       <c r="N164" s="3" t="n">
-        <v>46073.47771990741</v>
+        <v>46073.5514699074</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11186,7 +11191,7 @@
         <v>2</v>
       </c>
       <c r="N165" s="3" t="n">
-        <v>46073.47859953704</v>
+        <v>46073.55263888889</v>
       </c>
       <c r="O165" t="inlineStr">
         <is>
@@ -11250,7 +11255,7 @@
         <v>2</v>
       </c>
       <c r="N166" s="3" t="n">
-        <v>46073.45508101852</v>
+        <v>46073.57071759259</v>
       </c>
       <c r="O166" t="inlineStr">
         <is>
@@ -11314,7 +11319,7 @@
         <v>2</v>
       </c>
       <c r="N167" s="3" t="n">
-        <v>46073.48695601852</v>
+        <v>46073.56596064815</v>
       </c>
       <c r="O167" t="inlineStr">
         <is>
@@ -11378,7 +11383,7 @@
         <v>2</v>
       </c>
       <c r="N168" s="3" t="n">
-        <v>46073.48403935185</v>
+        <v>46073.56337962963</v>
       </c>
       <c r="O168" t="inlineStr">
         <is>
@@ -11442,7 +11447,7 @@
         <v>2</v>
       </c>
       <c r="N169" s="3" t="n">
-        <v>46073.47859953704</v>
+        <v>46073.55767361111</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -11506,7 +11511,7 @@
         <v>2</v>
       </c>
       <c r="N170" s="3" t="n">
-        <v>46073.45587962963</v>
+        <v>46073.56878472222</v>
       </c>
       <c r="O170" t="inlineStr">
         <is>
@@ -11570,7 +11575,7 @@
         <v>2</v>
       </c>
       <c r="N171" s="3" t="n">
-        <v>46073.4597337963</v>
+        <v>46073.53583333334</v>
       </c>
       <c r="O171" t="inlineStr">
         <is>
@@ -11634,7 +11639,7 @@
         <v>2</v>
       </c>
       <c r="N172" s="3" t="n">
-        <v>46072.77650462963</v>
+        <v>46073.54311342593</v>
       </c>
       <c r="O172" t="inlineStr">
         <is>
@@ -11698,7 +11703,7 @@
         <v>1</v>
       </c>
       <c r="N173" s="3" t="n">
-        <v>46072.78350694444</v>
+        <v>46073.54113425926</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -11762,7 +11767,7 @@
         <v>2</v>
       </c>
       <c r="N174" s="3" t="n">
-        <v>46073.44805555556</v>
+        <v>46073.53026620371</v>
       </c>
       <c r="O174" t="inlineStr">
         <is>
@@ -11826,7 +11831,7 @@
         <v>2</v>
       </c>
       <c r="N175" s="3" t="n">
-        <v>46073.46365740741</v>
+        <v>46073.54202546296</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -11890,7 +11895,7 @@
         <v>2</v>
       </c>
       <c r="N176" s="3" t="n">
-        <v>46073.45179398148</v>
+        <v>46073.53175925926</v>
       </c>
       <c r="O176" t="inlineStr">
         <is>
@@ -11954,7 +11959,7 @@
         <v>2</v>
       </c>
       <c r="N177" s="3" t="n">
-        <v>46073.45920138889</v>
+        <v>46073.53711805555</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
@@ -12018,7 +12023,7 @@
         <v>2</v>
       </c>
       <c r="N178" s="3" t="n">
-        <v>46073.47934027778</v>
+        <v>46073.55306712963</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12082,7 +12087,7 @@
         <v>1</v>
       </c>
       <c r="N179" s="3" t="n">
-        <v>46073.471875</v>
+        <v>46073.54638888889</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12146,7 +12151,7 @@
         <v>1</v>
       </c>
       <c r="N180" s="3" t="n">
-        <v>46073.46824074074</v>
+        <v>46073.5459837963</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12210,7 +12215,7 @@
         <v>1</v>
       </c>
       <c r="N181" s="3" t="n">
-        <v>46073.44728009259</v>
+        <v>46073.56762731481</v>
       </c>
       <c r="O181" t="inlineStr">
         <is>
@@ -12535,7 +12540,7 @@
         <v>1</v>
       </c>
       <c r="N186" s="3" t="n">
-        <v>46073.46666666667</v>
+        <v>46073.54069444445</v>
       </c>
       <c r="O186" t="inlineStr">
         <is>
@@ -12599,7 +12604,7 @@
         <v>1</v>
       </c>
       <c r="N187" s="3" t="n">
-        <v>46073.45883101852</v>
+        <v>46073.53917824074</v>
       </c>
       <c r="O187" t="inlineStr">
         <is>
@@ -12663,7 +12668,7 @@
         <v>1</v>
       </c>
       <c r="N188" s="3" t="n">
-        <v>46073.46096064815</v>
+        <v>46073.57087962963</v>
       </c>
       <c r="O188" t="inlineStr">
         <is>
@@ -12786,7 +12791,7 @@
         </is>
       </c>
       <c r="N190" s="3" t="n">
-        <v>46073.47305555556</v>
+        <v>46073.55572916667</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12914,7 +12919,7 @@
         <v>1</v>
       </c>
       <c r="N192" s="3" t="n">
-        <v>46073.4681712963</v>
+        <v>46073.55200231481</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -13039,7 +13044,7 @@
         <v>2</v>
       </c>
       <c r="N194" s="3" t="n">
-        <v>46073.4858912037</v>
+        <v>46073.56954861111</v>
       </c>
       <c r="O194" t="inlineStr">
         <is>
@@ -13103,7 +13108,7 @@
         <v>1</v>
       </c>
       <c r="N195" s="3" t="n">
-        <v>46073.46298611111</v>
+        <v>46073.54185185185</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13167,7 +13172,7 @@
         <v>1</v>
       </c>
       <c r="N196" s="3" t="n">
-        <v>46073.4596875</v>
+        <v>46073.53695601852</v>
       </c>
       <c r="O196" t="inlineStr">
         <is>
@@ -13231,7 +13236,7 @@
         <v>1</v>
       </c>
       <c r="N197" s="3" t="n">
-        <v>46073.463125</v>
+        <v>46073.54310185185</v>
       </c>
       <c r="O197" t="inlineStr">
         <is>
@@ -13295,7 +13300,7 @@
         <v>1</v>
       </c>
       <c r="N198" s="3" t="n">
-        <v>46073.45938657408</v>
+        <v>46073.53648148148</v>
       </c>
       <c r="O198" t="inlineStr">
         <is>
@@ -13359,7 +13364,7 @@
         <v>1</v>
       </c>
       <c r="N199" s="3" t="n">
-        <v>46073.46548611111</v>
+        <v>46073.54251157407</v>
       </c>
       <c r="O199" t="inlineStr">
         <is>
@@ -13423,7 +13428,7 @@
         <v>1</v>
       </c>
       <c r="N200" s="3" t="n">
-        <v>46073.46606481481</v>
+        <v>46073.54153935185</v>
       </c>
       <c r="O200" t="inlineStr">
         <is>
@@ -13484,7 +13489,7 @@
         </is>
       </c>
       <c r="N201" s="3" t="n">
-        <v>46073.48575231482</v>
+        <v>46073.56107638889</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -13548,7 +13553,7 @@
         <v>1</v>
       </c>
       <c r="N202" s="3" t="n">
-        <v>46073.45861111111</v>
+        <v>46073.56702546297</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13612,7 +13617,7 @@
         <v>1</v>
       </c>
       <c r="N203" s="3" t="n">
-        <v>46073.47737268519</v>
+        <v>46073.55559027778</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13676,7 +13681,7 @@
         <v>1</v>
       </c>
       <c r="N204" s="3" t="n">
-        <v>46073.45255787037</v>
+        <v>46073.56278935185</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13740,7 +13745,7 @@
         <v>1</v>
       </c>
       <c r="N205" s="3" t="n">
-        <v>46073.47725694445</v>
+        <v>46073.55740740741</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13804,7 +13809,7 @@
         <v>1</v>
       </c>
       <c r="N206" s="3" t="n">
-        <v>46073.45590277778</v>
+        <v>46073.53266203704</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -13868,7 +13873,7 @@
         <v>1</v>
       </c>
       <c r="N207" s="3" t="n">
-        <v>46073.46252314815</v>
+        <v>46073.54226851852</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -13932,7 +13937,7 @@
         <v>1</v>
       </c>
       <c r="N208" s="3" t="n">
-        <v>46073.46030092592</v>
+        <v>46073.54111111111</v>
       </c>
       <c r="O208" t="inlineStr">
         <is>
@@ -13996,7 +14001,7 @@
         <v>1</v>
       </c>
       <c r="N209" s="3" t="n">
-        <v>46073.47914351852</v>
+        <v>46073.55202546297</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14060,7 +14065,7 @@
         <v>1</v>
       </c>
       <c r="N210" s="3" t="n">
-        <v>46073.44820601852</v>
+        <v>46073.56570601852</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14124,7 +14129,7 @@
         <v>1</v>
       </c>
       <c r="N211" s="3" t="n">
-        <v>46073.48612268519</v>
+        <v>46073.56815972222</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -14188,7 +14193,7 @@
         <v>1</v>
       </c>
       <c r="N212" s="3" t="n">
-        <v>46073.47035879629</v>
+        <v>46073.54825231482</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -14252,7 +14257,7 @@
         <v>1</v>
       </c>
       <c r="N213" s="3" t="n">
-        <v>46073.46407407407</v>
+        <v>46073.54178240741</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
@@ -14316,7 +14321,7 @@
         <v>1</v>
       </c>
       <c r="N214" s="3" t="n">
-        <v>46073.48288194444</v>
+        <v>46073.56028935185</v>
       </c>
       <c r="O214" t="inlineStr">
         <is>
@@ -14380,7 +14385,7 @@
         <v>1</v>
       </c>
       <c r="N215" s="3" t="n">
-        <v>46073.46247685186</v>
+        <v>46073.54199074074</v>
       </c>
       <c r="O215" t="inlineStr">
         <is>
@@ -14444,7 +14449,7 @@
         <v>1</v>
       </c>
       <c r="N216" s="3" t="n">
-        <v>46073.47142361111</v>
+        <v>46073.55170138889</v>
       </c>
       <c r="O216" t="inlineStr">
         <is>
@@ -14463,11 +14468,6 @@
           <t>OPERACAO 8.1</t>
         </is>
       </c>
-      <c r="C217" t="inlineStr">
-        <is>
-          <t>10.69.5.85</t>
-        </is>
-      </c>
       <c r="D217" t="n">
         <v>2017</v>
       </c>
@@ -14508,7 +14508,7 @@
         <v>1</v>
       </c>
       <c r="N217" s="3" t="n">
-        <v>46073.46559027778</v>
+        <v>46073.54594907408</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14572,7 +14572,7 @@
         <v>1</v>
       </c>
       <c r="N218" s="3" t="n">
-        <v>46073.45606481482</v>
+        <v>46073.56548611111</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14636,7 +14636,7 @@
         <v>1</v>
       </c>
       <c r="N219" s="3" t="n">
-        <v>46073.35392361111</v>
+        <v>46073.48967592593</v>
       </c>
       <c r="O219" t="inlineStr">
         <is>
@@ -14705,7 +14705,7 @@
         <v>1</v>
       </c>
       <c r="N220" s="3" t="n">
-        <v>46073.46936342592</v>
+        <v>46073.50677083333</v>
       </c>
       <c r="O220" t="inlineStr">
         <is>
@@ -14769,7 +14769,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="3" t="n">
-        <v>46073.45256944445</v>
+        <v>46073.56626157407</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14833,7 +14833,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="3" t="n">
-        <v>46073.44792824074</v>
+        <v>46073.56379629629</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -15089,7 +15089,7 @@
         <v>1</v>
       </c>
       <c r="N226" s="3" t="n">
-        <v>46073.46082175926</v>
+        <v>46073.5393287037</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15153,7 +15153,7 @@
         <v>1</v>
       </c>
       <c r="N227" s="3" t="n">
-        <v>46073.4477662037</v>
+        <v>46073.56765046297</v>
       </c>
       <c r="O227" t="inlineStr">
         <is>
@@ -15281,7 +15281,7 @@
         <v>1</v>
       </c>
       <c r="N229" s="3" t="n">
-        <v>46073.45429398148</v>
+        <v>46073.5625462963</v>
       </c>
       <c r="O229" t="inlineStr">
         <is>
@@ -15345,7 +15345,7 @@
         <v>1</v>
       </c>
       <c r="N230" s="3" t="n">
-        <v>46073.46483796297</v>
+        <v>46073.53916666667</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15409,7 +15409,7 @@
         <v>1</v>
       </c>
       <c r="N231" s="3" t="n">
-        <v>46073.45997685185</v>
+        <v>46073.53674768518</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15473,7 +15473,7 @@
         <v>1</v>
       </c>
       <c r="N232" s="3" t="n">
-        <v>46073.4774537037</v>
+        <v>46073.55577546296</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -15537,7 +15537,7 @@
         <v>1</v>
       </c>
       <c r="N233" s="3" t="n">
-        <v>46073.45591435185</v>
+        <v>46073.53484953703</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15601,7 +15601,7 @@
         <v>1</v>
       </c>
       <c r="N234" s="3" t="n">
-        <v>46073.48069444444</v>
+        <v>46073.55782407407</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -15857,7 +15857,7 @@
         <v>1</v>
       </c>
       <c r="N238" s="3" t="n">
-        <v>46073.48479166667</v>
+        <v>46073.56349537037</v>
       </c>
       <c r="O238" t="inlineStr">
         <is>
@@ -15921,7 +15921,7 @@
         <v>1</v>
       </c>
       <c r="N239" s="3" t="n">
-        <v>46073.47472222222</v>
+        <v>46073.54677083333</v>
       </c>
       <c r="O239" t="inlineStr">
         <is>
@@ -15985,7 +15985,7 @@
         <v>1</v>
       </c>
       <c r="N240" s="3" t="n">
-        <v>46073.48271990741</v>
+        <v>46073.55864583333</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16049,7 +16049,7 @@
         <v>1</v>
       </c>
       <c r="N241" s="3" t="n">
-        <v>46073.46646990741</v>
+        <v>46073.54549768518</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16113,7 +16113,7 @@
         <v>1</v>
       </c>
       <c r="N242" s="3" t="n">
-        <v>46073.47324074074</v>
+        <v>46073.55013888889</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16177,7 +16177,7 @@
         <v>1</v>
       </c>
       <c r="N243" s="3" t="n">
-        <v>46073.4615625</v>
+        <v>46073.53672453704</v>
       </c>
       <c r="O243" t="inlineStr">
         <is>
@@ -16300,7 +16300,7 @@
         <v>1</v>
       </c>
       <c r="N245" s="3" t="n">
-        <v>46073.46831018518</v>
+        <v>46073.54495370371</v>
       </c>
       <c r="O245" t="inlineStr">
         <is>
@@ -16364,7 +16364,7 @@
         <v>1</v>
       </c>
       <c r="N246" s="3" t="n">
-        <v>46073.47136574074</v>
+        <v>46073.54415509259</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16428,7 +16428,7 @@
         <v>1</v>
       </c>
       <c r="N247" s="3" t="n">
-        <v>46073.47594907408</v>
+        <v>46073.55517361111</v>
       </c>
       <c r="O247" t="inlineStr">
         <is>
@@ -16492,7 +16492,7 @@
         <v>1</v>
       </c>
       <c r="N248" s="3" t="n">
-        <v>46073.46679398148</v>
+        <v>46073.53924768518</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16556,7 +16556,7 @@
         <v>1</v>
       </c>
       <c r="N249" s="3" t="n">
-        <v>46073.48023148148</v>
+        <v>46073.55804398148</v>
       </c>
       <c r="O249" t="inlineStr">
         <is>
@@ -16620,7 +16620,7 @@
         <v>1</v>
       </c>
       <c r="N250" s="3" t="n">
-        <v>46073.47754629629</v>
+        <v>46073.5575462963</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16684,7 +16684,7 @@
         <v>1</v>
       </c>
       <c r="N251" s="3" t="n">
-        <v>46073.46884259259</v>
+        <v>46073.54226851852</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16748,7 +16748,7 @@
         <v>1</v>
       </c>
       <c r="N252" s="3" t="n">
-        <v>46073.47478009259</v>
+        <v>46073.54922453704</v>
       </c>
       <c r="O252" t="inlineStr">
         <is>
@@ -16812,7 +16812,7 @@
         <v>1</v>
       </c>
       <c r="N253" s="3" t="n">
-        <v>46073.47702546296</v>
+        <v>46073.56105324074</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16870,7 +16870,7 @@
         <v>1</v>
       </c>
       <c r="N254" s="3" t="n">
-        <v>46073.47385416667</v>
+        <v>46073.54986111111</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -16934,7 +16934,7 @@
         <v>1</v>
       </c>
       <c r="N255" s="3" t="n">
-        <v>46073.46239583333</v>
+        <v>46073.5439699074</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -16998,7 +16998,7 @@
         <v>1</v>
       </c>
       <c r="N256" s="3" t="n">
-        <v>46073.48295138889</v>
+        <v>46073.55956018518</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17062,7 +17062,7 @@
         <v>1</v>
       </c>
       <c r="N257" s="3" t="n">
-        <v>46073.45731481481</v>
+        <v>46073.53170138889</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17126,7 +17126,7 @@
         <v>1</v>
       </c>
       <c r="N258" s="3" t="n">
-        <v>46073.44947916667</v>
+        <v>46073.56494212963</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
@@ -17190,7 +17190,7 @@
         <v>1</v>
       </c>
       <c r="N259" s="3" t="n">
-        <v>46073.44798611111</v>
+        <v>46073.56711805556</v>
       </c>
       <c r="O259" t="inlineStr">
         <is>
@@ -17254,7 +17254,7 @@
         <v>1</v>
       </c>
       <c r="N260" s="3" t="n">
-        <v>46073.48180555556</v>
+        <v>46073.56116898148</v>
       </c>
       <c r="O260" t="inlineStr">
         <is>
@@ -17318,7 +17318,7 @@
         <v>1</v>
       </c>
       <c r="N261" s="3" t="n">
-        <v>46073.45108796296</v>
+        <v>46073.56637731481</v>
       </c>
       <c r="O261" t="inlineStr">
         <is>
@@ -17382,7 +17382,7 @@
         <v>1</v>
       </c>
       <c r="N262" s="3" t="n">
-        <v>46073.45975694444</v>
+        <v>46073.54030092592</v>
       </c>
       <c r="O262" t="inlineStr">
         <is>
@@ -17446,7 +17446,7 @@
         <v>1</v>
       </c>
       <c r="N263" s="3" t="n">
-        <v>46073.48707175926</v>
+        <v>46073.56549768519</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17510,7 +17510,7 @@
         <v>1</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>46073.45393518519</v>
+        <v>46073.57115740741</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17574,7 +17574,7 @@
         <v>1</v>
       </c>
       <c r="N265" s="3" t="n">
-        <v>46073.45158564814</v>
+        <v>46073.53457175926</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17638,7 +17638,7 @@
         <v>1</v>
       </c>
       <c r="N266" s="3" t="n">
-        <v>46073.45802083334</v>
+        <v>46073.53493055556</v>
       </c>
       <c r="O266" t="inlineStr">
         <is>
@@ -17702,7 +17702,7 @@
         <v>1</v>
       </c>
       <c r="N267" s="3" t="n">
-        <v>46073.47905092593</v>
+        <v>46073.55527777778</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17766,7 +17766,7 @@
         <v>1</v>
       </c>
       <c r="N268" s="3" t="n">
-        <v>46073.450625</v>
+        <v>46073.53055555555</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17830,7 +17830,7 @@
         <v>1</v>
       </c>
       <c r="N269" s="3" t="n">
-        <v>46073.45212962963</v>
+        <v>46073.57077546296</v>
       </c>
       <c r="O269" t="inlineStr">
         <is>
@@ -17891,7 +17891,7 @@
         </is>
       </c>
       <c r="N270" s="3" t="n">
-        <v>46073.4730324074</v>
+        <v>46073.54967592593</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -18019,7 +18019,7 @@
         <v>1</v>
       </c>
       <c r="N272" s="3" t="n">
-        <v>46073.47112268519</v>
+        <v>46073.54831018519</v>
       </c>
       <c r="O272" t="inlineStr">
         <is>
@@ -18083,7 +18083,7 @@
         <v>2</v>
       </c>
       <c r="N273" s="3" t="n">
-        <v>46073.46599537037</v>
+        <v>46073.54390046297</v>
       </c>
       <c r="O273" t="inlineStr">
         <is>
@@ -18403,7 +18403,7 @@
         <v>1</v>
       </c>
       <c r="N278" s="3" t="n">
-        <v>46073.45769675926</v>
+        <v>46073.56991898148</v>
       </c>
       <c r="O278" t="inlineStr">
         <is>
@@ -18467,7 +18467,7 @@
         <v>1</v>
       </c>
       <c r="N279" s="3" t="n">
-        <v>46073.46763888889</v>
+        <v>46073.54751157408</v>
       </c>
       <c r="O279" t="inlineStr">
         <is>
@@ -18531,7 +18531,7 @@
         <v>1</v>
       </c>
       <c r="N280" s="3" t="n">
-        <v>46073.47653935185</v>
+        <v>46073.55460648148</v>
       </c>
       <c r="O280" t="inlineStr">
         <is>
@@ -18595,7 +18595,7 @@
         <v>1</v>
       </c>
       <c r="N281" s="3" t="n">
-        <v>46073.4733912037</v>
+        <v>46073.55024305556</v>
       </c>
       <c r="O281" t="inlineStr">
         <is>
@@ -18654,7 +18654,7 @@
         <v>1</v>
       </c>
       <c r="N282" s="3" t="n">
-        <v>46073.47054398148</v>
+        <v>46073.55273148148</v>
       </c>
       <c r="O282" t="inlineStr">
         <is>
@@ -18718,7 +18718,7 @@
         <v>1</v>
       </c>
       <c r="N283" s="3" t="n">
-        <v>46073.4495949074</v>
+        <v>46073.53045138889</v>
       </c>
       <c r="O283" t="inlineStr">
         <is>
@@ -18782,7 +18782,7 @@
         <v>1</v>
       </c>
       <c r="N284" s="3" t="n">
-        <v>46073.45428240741</v>
+        <v>46073.56300925926</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18846,7 +18846,7 @@
         <v>1</v>
       </c>
       <c r="N285" s="3" t="n">
-        <v>46073.47928240741</v>
+        <v>46073.55717592593</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -18910,7 +18910,7 @@
         <v>1</v>
       </c>
       <c r="N286" s="3" t="n">
-        <v>46073.46982638889</v>
+        <v>46073.50994212963</v>
       </c>
       <c r="O286" t="inlineStr">
         <is>
@@ -18974,7 +18974,7 @@
         <v>1</v>
       </c>
       <c r="N287" s="3" t="n">
-        <v>46073.4709375</v>
+        <v>46073.54762731482</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
@@ -19038,7 +19038,7 @@
         <v>1</v>
       </c>
       <c r="N288" s="3" t="n">
-        <v>46073.46717592593</v>
+        <v>46073.5425</v>
       </c>
       <c r="O288" t="inlineStr">
         <is>
@@ -19102,7 +19102,7 @@
         <v>1</v>
       </c>
       <c r="N289" s="3" t="n">
-        <v>46073.45945601852</v>
+        <v>46073.53822916667</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -19896,7 +19896,7 @@
         <v>1</v>
       </c>
       <c r="N302" s="3" t="n">
-        <v>46073.46896990741</v>
+        <v>46073.54935185185</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -21012,7 +21012,7 @@
         </is>
       </c>
       <c r="N320" s="3" t="n">
-        <v>46073.47508101852</v>
+        <v>46073.55310185185</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21737,7 +21737,7 @@
         <v>1</v>
       </c>
       <c r="N332" s="3" t="n">
-        <v>46073.46829861111</v>
+        <v>46073.543125</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21801,7 +21801,7 @@
         <v>2</v>
       </c>
       <c r="N333" s="3" t="n">
-        <v>46073.4690162037</v>
+        <v>46073.54233796296</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21865,7 +21865,7 @@
         <v>2</v>
       </c>
       <c r="N334" s="3" t="n">
-        <v>46073.47671296296</v>
+        <v>46073.54971064815</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21929,7 +21929,7 @@
         <v>2</v>
       </c>
       <c r="N335" s="3" t="n">
-        <v>46073.47715277778</v>
+        <v>46073.55378472222</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -21993,7 +21993,7 @@
         <v>1</v>
       </c>
       <c r="N336" s="3" t="n">
-        <v>46073.46670138889</v>
+        <v>46073.54052083333</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22057,7 +22057,7 @@
         <v>1</v>
       </c>
       <c r="N337" s="3" t="n">
-        <v>46073.48015046296</v>
+        <v>46073.55474537037</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22121,7 +22121,7 @@
         <v>2</v>
       </c>
       <c r="N338" s="3" t="n">
-        <v>46073.47547453704</v>
+        <v>46073.55574074074</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -22185,7 +22185,7 @@
         <v>2</v>
       </c>
       <c r="N339" s="3" t="n">
-        <v>46073.47252314815</v>
+        <v>46073.55048611111</v>
       </c>
       <c r="O339" t="inlineStr">
         <is>
@@ -22313,7 +22313,7 @@
         <v>2</v>
       </c>
       <c r="N341" s="3" t="n">
-        <v>46073.45701388889</v>
+        <v>46073.57005787037</v>
       </c>
       <c r="O341" t="inlineStr">
         <is>
@@ -22374,10 +22374,10 @@
         </is>
       </c>
       <c r="M342" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N342" s="3" t="n">
-        <v>46073.45991898148</v>
+        <v>46073.53517361111</v>
       </c>
       <c r="O342" t="inlineStr">
         <is>
@@ -22438,7 +22438,7 @@
         </is>
       </c>
       <c r="N343" s="3" t="n">
-        <v>46073.47489583334</v>
+        <v>46073.54935185185</v>
       </c>
       <c r="O343" t="inlineStr">
         <is>
@@ -22694,7 +22694,7 @@
         <v>1</v>
       </c>
       <c r="N347" s="3" t="n">
-        <v>46073.4621412037</v>
+        <v>46073.54513888889</v>
       </c>
       <c r="O347" t="inlineStr">
         <is>
@@ -22758,7 +22758,7 @@
         <v>2</v>
       </c>
       <c r="N348" s="3" t="n">
-        <v>46073.45680555556</v>
+        <v>46073.53108796296</v>
       </c>
       <c r="O348" t="inlineStr">
         <is>
@@ -22822,7 +22822,7 @@
         <v>1</v>
       </c>
       <c r="N349" s="3" t="n">
-        <v>46073.45896990741</v>
+        <v>46073.53733796296</v>
       </c>
       <c r="O349" t="inlineStr">
         <is>
@@ -22886,7 +22886,7 @@
         <v>1</v>
       </c>
       <c r="N350" s="3" t="n">
-        <v>46073.4872337963</v>
+        <v>46073.56927083333</v>
       </c>
       <c r="O350" t="inlineStr">
         <is>
@@ -22950,7 +22950,7 @@
         <v>1</v>
       </c>
       <c r="N351" s="3" t="n">
-        <v>46073.46149305555</v>
+        <v>46073.54331018519</v>
       </c>
       <c r="O351" t="inlineStr">
         <is>
@@ -23014,7 +23014,7 @@
         <v>1</v>
       </c>
       <c r="N352" s="3" t="n">
-        <v>46073.46563657407</v>
+        <v>46073.53935185185</v>
       </c>
       <c r="O352" t="inlineStr">
         <is>
@@ -23075,7 +23075,7 @@
         </is>
       </c>
       <c r="N353" s="3" t="n">
-        <v>46073.46053240741</v>
+        <v>46073.53971064815</v>
       </c>
       <c r="O353" t="inlineStr">
         <is>
@@ -23136,7 +23136,7 @@
         </is>
       </c>
       <c r="N354" s="3" t="n">
-        <v>46073.45943287037</v>
+        <v>46073.53892361111</v>
       </c>
       <c r="O354" t="inlineStr">
         <is>
@@ -23200,7 +23200,7 @@
         <v>1</v>
       </c>
       <c r="N355" s="3" t="n">
-        <v>46073.45901620371</v>
+        <v>46073.53895833333</v>
       </c>
       <c r="O355" t="inlineStr">
         <is>
@@ -23264,7 +23264,7 @@
         <v>1</v>
       </c>
       <c r="N356" s="3" t="n">
-        <v>46073.45615740741</v>
+        <v>46073.53622685185</v>
       </c>
       <c r="O356" t="inlineStr">
         <is>
@@ -23328,7 +23328,7 @@
         <v>1</v>
       </c>
       <c r="N357" s="3" t="n">
-        <v>46073.45711805556</v>
+        <v>46073.53700231481</v>
       </c>
       <c r="O357" t="inlineStr">
         <is>
@@ -23515,7 +23515,7 @@
         <v>2</v>
       </c>
       <c r="N360" s="3" t="n">
-        <v>46073.454375</v>
+        <v>46073.53261574074</v>
       </c>
       <c r="O360" t="inlineStr">
         <is>
@@ -23579,7 +23579,7 @@
         <v>1</v>
       </c>
       <c r="N361" s="3" t="n">
-        <v>46073.46128472222</v>
+        <v>46073.54159722223</v>
       </c>
       <c r="O361" t="inlineStr">
         <is>
@@ -23640,7 +23640,7 @@
         </is>
       </c>
       <c r="N362" s="3" t="n">
-        <v>46073.46034722222</v>
+        <v>46073.53834490741</v>
       </c>
       <c r="O362" t="inlineStr">
         <is>
@@ -23828,7 +23828,7 @@
         <v>1</v>
       </c>
       <c r="N365" s="3" t="n">
-        <v>46073.45385416667</v>
+        <v>46073.53197916667</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
@@ -23894,7 +23894,7 @@
         </is>
       </c>
       <c r="N366" s="3" t="n">
-        <v>46073.47943287037</v>
+        <v>46073.56184027778</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -24020,7 +24020,7 @@
         </is>
       </c>
       <c r="N368" s="3" t="n">
-        <v>46073.47994212963</v>
+        <v>46073.55369212963</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -24039,6 +24039,11 @@
           <t>RH</t>
         </is>
       </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>10.69.3.13</t>
+        </is>
+      </c>
       <c r="D369" t="n">
         <v>2025</v>
       </c>
@@ -24081,7 +24086,7 @@
         </is>
       </c>
       <c r="N369" s="3" t="n">
-        <v>46073.47359953704</v>
+        <v>46073.55615740741</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
@@ -24150,7 +24155,7 @@
         <v>1</v>
       </c>
       <c r="N370" s="3" t="n">
-        <v>46073.47099537037</v>
+        <v>46073.55251157407</v>
       </c>
       <c r="O370" t="inlineStr">
         <is>
@@ -24426,7 +24431,7 @@
         <v>1</v>
       </c>
       <c r="N374" s="3" t="n">
-        <v>46073.46418981482</v>
+        <v>46073.53827546296</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24492,7 +24497,7 @@
         </is>
       </c>
       <c r="N375" s="3" t="n">
-        <v>46073.45827546297</v>
+        <v>46073.57018518518</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
@@ -24511,11 +24516,6 @@
           <t>COORDENACAO</t>
         </is>
       </c>
-      <c r="C376" t="inlineStr">
-        <is>
-          <t>10.69.3.72</t>
-        </is>
-      </c>
       <c r="D376" t="n">
         <v>2025</v>
       </c>
@@ -24561,7 +24561,7 @@
         <v>1</v>
       </c>
       <c r="N376" s="3" t="n">
-        <v>46073.48287037037</v>
+        <v>46073.56222222222</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -24630,7 +24630,7 @@
         <v>2</v>
       </c>
       <c r="N377" s="3" t="n">
-        <v>46073.46291666666</v>
+        <v>46073.53771990741</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -24699,7 +24699,7 @@
         <v>2</v>
       </c>
       <c r="N378" s="3" t="n">
-        <v>46073.45381944445</v>
+        <v>46073.53424768519</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização automática 2026-02-20 15:52:03.946281
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>46073.55310185185</v>
+        <v>46073.62866898148</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>46073.54446759259</v>
+        <v>46073.61938657407</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
         <v>2</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>46073.53719907408</v>
+        <v>46073.65064814815</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>46073.53348379629</v>
+        <v>46073.65215277778</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -1131,7 +1131,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="3" t="n">
-        <v>46073.54879629629</v>
+        <v>46073.62952546297</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1451,7 +1451,7 @@
         <v>1</v>
       </c>
       <c r="N15" s="3" t="n">
-        <v>46073.56809027777</v>
+        <v>46073.65078703704</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1515,7 +1515,7 @@
         <v>2</v>
       </c>
       <c r="N16" s="3" t="n">
-        <v>46073.55006944444</v>
+        <v>46073.62695601852</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -2244,7 +2244,7 @@
         </is>
       </c>
       <c r="N28" s="3" t="n">
-        <v>46073.54253472222</v>
+        <v>46073.61810185185</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -6570,7 +6570,7 @@
         <v>1</v>
       </c>
       <c r="N95" s="3" t="n">
-        <v>46073.54114583333</v>
+        <v>46073.61950231482</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -6639,7 +6639,7 @@
         <v>1</v>
       </c>
       <c r="N96" s="3" t="n">
-        <v>46073.55028935185</v>
+        <v>46073.62659722222</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
@@ -6658,11 +6658,6 @@
           <t>COORDENACAO</t>
         </is>
       </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>10.69.3.93</t>
-        </is>
-      </c>
       <c r="D97" t="n">
         <v>2025</v>
       </c>
@@ -6708,7 +6703,7 @@
         <v>1</v>
       </c>
       <c r="N97" s="3" t="n">
-        <v>46073.56362268519</v>
+        <v>46073.64060185185</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -6727,6 +6722,11 @@
           <t>COORDENACAO</t>
         </is>
       </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>10.69.3.94</t>
+        </is>
+      </c>
       <c r="D98" t="n">
         <v>2025</v>
       </c>
@@ -6772,7 +6772,7 @@
         <v>1</v>
       </c>
       <c r="N98" s="3" t="n">
-        <v>46073.53438657407</v>
+        <v>46073.64871527778</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -6910,7 +6910,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>46073.56778935185</v>
+        <v>46073.64547453704</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6979,7 +6979,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="3" t="n">
-        <v>46073.53777777778</v>
+        <v>46073.61675925926</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -7117,7 +7117,7 @@
         <v>2</v>
       </c>
       <c r="N103" s="3" t="n">
-        <v>46073.55546296296</v>
+        <v>46073.63006944444</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7374,7 +7374,7 @@
         <v>1</v>
       </c>
       <c r="N107" s="3" t="n">
-        <v>46073.54255787037</v>
+        <v>46073.6183912037</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -7512,7 +7512,7 @@
         <v>1</v>
       </c>
       <c r="N109" s="3" t="n">
-        <v>46073.56684027778</v>
+        <v>46073.64761574074</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7581,7 +7581,7 @@
         <v>2</v>
       </c>
       <c r="N110" s="3" t="n">
-        <v>46073.55362268518</v>
+        <v>46073.63528935185</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7650,7 +7650,7 @@
         <v>2</v>
       </c>
       <c r="N111" s="3" t="n">
-        <v>46073.56353009259</v>
+        <v>46073.64070601852</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
@@ -7719,7 +7719,7 @@
         <v>2</v>
       </c>
       <c r="N112" s="3" t="n">
-        <v>46073.5662962963</v>
+        <v>46073.64163194445</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7788,7 +7788,7 @@
         <v>1</v>
       </c>
       <c r="N113" s="3" t="n">
-        <v>46073.55079861111</v>
+        <v>46073.62608796296</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7857,7 +7857,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>46073.55560185185</v>
+        <v>46073.63515046296</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -7923,7 +7923,7 @@
         </is>
       </c>
       <c r="N115" s="3" t="n">
-        <v>46073.56305555555</v>
+        <v>46073.64040509259</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -7992,7 +7992,7 @@
         <v>1</v>
       </c>
       <c r="N116" s="3" t="n">
-        <v>46073.55271990741</v>
+        <v>46073.63271990741</v>
       </c>
       <c r="O116" t="inlineStr">
         <is>
@@ -8011,6 +8011,11 @@
           <t>DP</t>
         </is>
       </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>10.69.3.23</t>
+        </is>
+      </c>
       <c r="D117" t="n">
         <v>2025</v>
       </c>
@@ -8056,7 +8061,7 @@
         <v>1</v>
       </c>
       <c r="N117" s="3" t="n">
-        <v>46073.51700231482</v>
+        <v>46073.65416666667</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -8260,7 +8265,7 @@
         <v>1</v>
       </c>
       <c r="N120" s="3" t="n">
-        <v>46073.54914351852</v>
+        <v>46073.6265625</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -8329,7 +8334,7 @@
         <v>1</v>
       </c>
       <c r="N121" s="3" t="n">
-        <v>46073.54833333333</v>
+        <v>46073.6299074074</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -8395,7 +8400,7 @@
         </is>
       </c>
       <c r="N122" s="3" t="n">
-        <v>46073.55076388889</v>
+        <v>46073.62711805556</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -8464,7 +8469,7 @@
         <v>2</v>
       </c>
       <c r="N123" s="3" t="n">
-        <v>46073.54980324074</v>
+        <v>46073.62328703704</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -8533,7 +8538,7 @@
         <v>1</v>
       </c>
       <c r="N124" s="3" t="n">
-        <v>46073.5353587963</v>
+        <v>46073.6493287037</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -8602,7 +8607,7 @@
         <v>1</v>
       </c>
       <c r="N125" s="3" t="n">
-        <v>46073.55802083333</v>
+        <v>46073.63644675926</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -8671,7 +8676,7 @@
         <v>1</v>
       </c>
       <c r="N126" s="3" t="n">
-        <v>46073.54555555555</v>
+        <v>46073.62375</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -8740,7 +8745,7 @@
         <v>2</v>
       </c>
       <c r="N127" s="3" t="n">
-        <v>46073.55962962963</v>
+        <v>46073.63575231482</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -8809,7 +8814,7 @@
         <v>1</v>
       </c>
       <c r="N128" s="3" t="n">
-        <v>46073.56907407408</v>
+        <v>46073.64767361111</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -8878,7 +8883,7 @@
         <v>1</v>
       </c>
       <c r="N129" s="3" t="n">
-        <v>46073.55243055556</v>
+        <v>46073.62746527778</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -8947,7 +8952,7 @@
         <v>1</v>
       </c>
       <c r="N130" s="3" t="n">
-        <v>46073.55601851852</v>
+        <v>46073.63625</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -9011,7 +9016,7 @@
         <v>1</v>
       </c>
       <c r="N131" s="3" t="n">
-        <v>46073.55613425926</v>
+        <v>46073.6333912037</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -9144,7 +9149,7 @@
         <v>1</v>
       </c>
       <c r="N133" s="3" t="n">
-        <v>46073.56487268519</v>
+        <v>46073.63890046296</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -9208,7 +9213,7 @@
         <v>1</v>
       </c>
       <c r="N134" s="3" t="n">
-        <v>46073.54048611111</v>
+        <v>46073.61700231482</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -9272,7 +9277,7 @@
         <v>1</v>
       </c>
       <c r="N135" s="3" t="n">
-        <v>46073.56689814815</v>
+        <v>46073.64847222222</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -9463,7 +9468,7 @@
         <v>1</v>
       </c>
       <c r="N138" s="3" t="n">
-        <v>46073.54357638889</v>
+        <v>46073.62471064815</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9527,7 +9532,7 @@
         <v>1</v>
       </c>
       <c r="N139" s="3" t="n">
-        <v>46073.55971064815</v>
+        <v>46073.62226851852</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9591,7 +9596,7 @@
         <v>1</v>
       </c>
       <c r="N140" s="3" t="n">
-        <v>46073.53268518519</v>
+        <v>46073.65045138889</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9655,7 +9660,7 @@
         <v>1</v>
       </c>
       <c r="N141" s="3" t="n">
-        <v>46073.56403935186</v>
+        <v>46073.62081018519</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9719,7 +9724,7 @@
         <v>1</v>
       </c>
       <c r="N142" s="3" t="n">
-        <v>46073.55744212963</v>
+        <v>46073.63635416667</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9783,7 +9788,7 @@
         <v>1</v>
       </c>
       <c r="N143" s="3" t="n">
-        <v>46073.55893518519</v>
+        <v>46073.62324074074</v>
       </c>
       <c r="O143" t="inlineStr">
         <is>
@@ -9847,7 +9852,7 @@
         <v>1</v>
       </c>
       <c r="N144" s="3" t="n">
-        <v>46073.54737268519</v>
+        <v>46073.62424768518</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9911,7 +9916,7 @@
         <v>1</v>
       </c>
       <c r="N145" s="3" t="n">
-        <v>46073.48858796297</v>
+        <v>46073.62175925926</v>
       </c>
       <c r="O145" t="inlineStr">
         <is>
@@ -9975,7 +9980,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="3" t="n">
-        <v>46073.5646875</v>
+        <v>46073.61898148148</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10039,7 +10044,7 @@
         <v>1</v>
       </c>
       <c r="N147" s="3" t="n">
-        <v>46073.56480324074</v>
+        <v>46073.64524305556</v>
       </c>
       <c r="O147" t="inlineStr">
         <is>
@@ -10103,7 +10108,7 @@
         <v>1</v>
       </c>
       <c r="N148" s="3" t="n">
-        <v>46073.56519675926</v>
+        <v>46073.64549768518</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10167,7 +10172,7 @@
         <v>1</v>
       </c>
       <c r="N149" s="3" t="n">
-        <v>46073.56355324074</v>
+        <v>46073.64280092593</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -10295,7 +10300,7 @@
         <v>1</v>
       </c>
       <c r="N151" s="3" t="n">
-        <v>46073.55965277777</v>
+        <v>46073.63704861111</v>
       </c>
       <c r="O151" t="inlineStr">
         <is>
@@ -10359,7 +10364,7 @@
         <v>1</v>
       </c>
       <c r="N152" s="3" t="n">
-        <v>46073.56111111111</v>
+        <v>46073.62025462963</v>
       </c>
       <c r="O152" t="inlineStr">
         <is>
@@ -10423,7 +10428,7 @@
         <v>1</v>
       </c>
       <c r="N153" s="3" t="n">
-        <v>46073.56908564815</v>
+        <v>46073.64875</v>
       </c>
       <c r="O153" t="inlineStr">
         <is>
@@ -10487,7 +10492,7 @@
         <v>1</v>
       </c>
       <c r="N154" s="3" t="n">
-        <v>46073.53877314815</v>
+        <v>46073.62189814815</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10551,7 +10556,7 @@
         <v>1</v>
       </c>
       <c r="N155" s="3" t="n">
-        <v>46073.55679398148</v>
+        <v>46073.62208333334</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10679,7 +10684,7 @@
         <v>1</v>
       </c>
       <c r="N157" s="3" t="n">
-        <v>46073.56768518518</v>
+        <v>46073.62059027778</v>
       </c>
       <c r="O157" t="inlineStr">
         <is>
@@ -10743,7 +10748,7 @@
         <v>1</v>
       </c>
       <c r="N158" s="3" t="n">
-        <v>46073.53177083333</v>
+        <v>46073.57555555556</v>
       </c>
       <c r="O158" t="inlineStr">
         <is>
@@ -10807,7 +10812,7 @@
         <v>1</v>
       </c>
       <c r="N159" s="3" t="n">
-        <v>46073.56733796297</v>
+        <v>46073.64628472222</v>
       </c>
       <c r="O159" t="inlineStr">
         <is>
@@ -10871,7 +10876,7 @@
         <v>1</v>
       </c>
       <c r="N160" s="3" t="n">
-        <v>46073.53212962963</v>
+        <v>46073.57277777778</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
@@ -10999,7 +11004,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="3" t="n">
-        <v>46073.55766203703</v>
+        <v>46073.63545138889</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11127,7 +11132,7 @@
         <v>2</v>
       </c>
       <c r="N164" s="3" t="n">
-        <v>46073.5514699074</v>
+        <v>46073.6303587963</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11191,7 +11196,7 @@
         <v>2</v>
       </c>
       <c r="N165" s="3" t="n">
-        <v>46073.55263888889</v>
+        <v>46073.62736111111</v>
       </c>
       <c r="O165" t="inlineStr">
         <is>
@@ -11255,7 +11260,7 @@
         <v>2</v>
       </c>
       <c r="N166" s="3" t="n">
-        <v>46073.57071759259</v>
+        <v>46073.61207175926</v>
       </c>
       <c r="O166" t="inlineStr">
         <is>
@@ -11319,7 +11324,7 @@
         <v>2</v>
       </c>
       <c r="N167" s="3" t="n">
-        <v>46073.56596064815</v>
+        <v>46073.60625</v>
       </c>
       <c r="O167" t="inlineStr">
         <is>
@@ -11447,7 +11452,7 @@
         <v>2</v>
       </c>
       <c r="N169" s="3" t="n">
-        <v>46073.55767361111</v>
+        <v>46073.63478009259</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -11511,7 +11516,7 @@
         <v>2</v>
       </c>
       <c r="N170" s="3" t="n">
-        <v>46073.56878472222</v>
+        <v>46073.64931712963</v>
       </c>
       <c r="O170" t="inlineStr">
         <is>
@@ -11572,7 +11577,7 @@
         </is>
       </c>
       <c r="M171" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N171" s="3" t="n">
         <v>46073.53583333334</v>
@@ -11639,7 +11644,7 @@
         <v>2</v>
       </c>
       <c r="N172" s="3" t="n">
-        <v>46073.54311342593</v>
+        <v>46073.61986111111</v>
       </c>
       <c r="O172" t="inlineStr">
         <is>
@@ -11700,10 +11705,10 @@
         </is>
       </c>
       <c r="M173" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N173" s="3" t="n">
-        <v>46073.54113425926</v>
+        <v>46073.62208333334</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -11767,7 +11772,7 @@
         <v>2</v>
       </c>
       <c r="N174" s="3" t="n">
-        <v>46073.53026620371</v>
+        <v>46073.57134259259</v>
       </c>
       <c r="O174" t="inlineStr">
         <is>
@@ -11831,7 +11836,7 @@
         <v>2</v>
       </c>
       <c r="N175" s="3" t="n">
-        <v>46073.54202546296</v>
+        <v>46073.61971064815</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -11895,7 +11900,7 @@
         <v>2</v>
       </c>
       <c r="N176" s="3" t="n">
-        <v>46073.53175925926</v>
+        <v>46073.64792824074</v>
       </c>
       <c r="O176" t="inlineStr">
         <is>
@@ -11959,7 +11964,7 @@
         <v>2</v>
       </c>
       <c r="N177" s="3" t="n">
-        <v>46073.53711805555</v>
+        <v>46073.61417824074</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
@@ -12023,7 +12028,7 @@
         <v>2</v>
       </c>
       <c r="N178" s="3" t="n">
-        <v>46073.55306712963</v>
+        <v>46073.62996527777</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12087,7 +12092,7 @@
         <v>1</v>
       </c>
       <c r="N179" s="3" t="n">
-        <v>46073.54638888889</v>
+        <v>46073.63991898148</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12151,7 +12156,7 @@
         <v>1</v>
       </c>
       <c r="N180" s="3" t="n">
-        <v>46073.5459837963</v>
+        <v>46073.62032407407</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12215,7 +12220,7 @@
         <v>1</v>
       </c>
       <c r="N181" s="3" t="n">
-        <v>46073.56762731481</v>
+        <v>46073.64716435185</v>
       </c>
       <c r="O181" t="inlineStr">
         <is>
@@ -12540,7 +12545,7 @@
         <v>1</v>
       </c>
       <c r="N186" s="3" t="n">
-        <v>46073.54069444445</v>
+        <v>46073.57961805556</v>
       </c>
       <c r="O186" t="inlineStr">
         <is>
@@ -12604,7 +12609,7 @@
         <v>1</v>
       </c>
       <c r="N187" s="3" t="n">
-        <v>46073.53917824074</v>
+        <v>46073.62079861111</v>
       </c>
       <c r="O187" t="inlineStr">
         <is>
@@ -12754,6 +12759,11 @@
           <t>OPERACAO 8.1</t>
         </is>
       </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>10.69.5.59</t>
+        </is>
+      </c>
       <c r="D190" t="n">
         <v>2015</v>
       </c>
@@ -12791,7 +12801,7 @@
         </is>
       </c>
       <c r="N190" s="3" t="n">
-        <v>46073.55572916667</v>
+        <v>46073.62104166667</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12855,7 +12865,7 @@
         <v>1</v>
       </c>
       <c r="N191" s="3" t="n">
-        <v>46072.79136574074</v>
+        <v>46073.61459490741</v>
       </c>
       <c r="O191" t="inlineStr">
         <is>
@@ -12919,7 +12929,7 @@
         <v>1</v>
       </c>
       <c r="N192" s="3" t="n">
-        <v>46073.55200231481</v>
+        <v>46073.63047453704</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -13044,7 +13054,7 @@
         <v>2</v>
       </c>
       <c r="N194" s="3" t="n">
-        <v>46073.56954861111</v>
+        <v>46073.61572916667</v>
       </c>
       <c r="O194" t="inlineStr">
         <is>
@@ -13108,7 +13118,7 @@
         <v>1</v>
       </c>
       <c r="N195" s="3" t="n">
-        <v>46073.54185185185</v>
+        <v>46073.61953703704</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13172,7 +13182,7 @@
         <v>1</v>
       </c>
       <c r="N196" s="3" t="n">
-        <v>46073.53695601852</v>
+        <v>46073.62190972222</v>
       </c>
       <c r="O196" t="inlineStr">
         <is>
@@ -13236,7 +13246,7 @@
         <v>1</v>
       </c>
       <c r="N197" s="3" t="n">
-        <v>46073.54310185185</v>
+        <v>46073.61754629629</v>
       </c>
       <c r="O197" t="inlineStr">
         <is>
@@ -13300,7 +13310,7 @@
         <v>1</v>
       </c>
       <c r="N198" s="3" t="n">
-        <v>46073.53648148148</v>
+        <v>46073.65328703704</v>
       </c>
       <c r="O198" t="inlineStr">
         <is>
@@ -13364,7 +13374,7 @@
         <v>1</v>
       </c>
       <c r="N199" s="3" t="n">
-        <v>46073.54251157407</v>
+        <v>46073.62240740741</v>
       </c>
       <c r="O199" t="inlineStr">
         <is>
@@ -13428,7 +13438,7 @@
         <v>1</v>
       </c>
       <c r="N200" s="3" t="n">
-        <v>46073.54153935185</v>
+        <v>46073.6434375</v>
       </c>
       <c r="O200" t="inlineStr">
         <is>
@@ -13489,7 +13499,7 @@
         </is>
       </c>
       <c r="N201" s="3" t="n">
-        <v>46073.56107638889</v>
+        <v>46073.63636574074</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -13553,7 +13563,7 @@
         <v>1</v>
       </c>
       <c r="N202" s="3" t="n">
-        <v>46073.56702546297</v>
+        <v>46073.62311342593</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13617,7 +13627,7 @@
         <v>1</v>
       </c>
       <c r="N203" s="3" t="n">
-        <v>46073.55559027778</v>
+        <v>46073.63091435185</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13681,7 +13691,7 @@
         <v>1</v>
       </c>
       <c r="N204" s="3" t="n">
-        <v>46073.56278935185</v>
+        <v>46073.64045138889</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13745,7 +13755,7 @@
         <v>1</v>
       </c>
       <c r="N205" s="3" t="n">
-        <v>46073.55740740741</v>
+        <v>46073.63332175926</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13809,7 +13819,7 @@
         <v>1</v>
       </c>
       <c r="N206" s="3" t="n">
-        <v>46073.53266203704</v>
+        <v>46073.65171296296</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -13873,7 +13883,7 @@
         <v>1</v>
       </c>
       <c r="N207" s="3" t="n">
-        <v>46073.54226851852</v>
+        <v>46073.61866898148</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -14001,7 +14011,7 @@
         <v>1</v>
       </c>
       <c r="N209" s="3" t="n">
-        <v>46073.55202546297</v>
+        <v>46073.62671296296</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14065,7 +14075,7 @@
         <v>1</v>
       </c>
       <c r="N210" s="3" t="n">
-        <v>46073.56570601852</v>
+        <v>46073.64670138889</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14129,7 +14139,7 @@
         <v>1</v>
       </c>
       <c r="N211" s="3" t="n">
-        <v>46073.56815972222</v>
+        <v>46073.62670138889</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -14193,7 +14203,7 @@
         <v>1</v>
       </c>
       <c r="N212" s="3" t="n">
-        <v>46073.54825231482</v>
+        <v>46073.62702546296</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -14257,7 +14267,7 @@
         <v>1</v>
       </c>
       <c r="N213" s="3" t="n">
-        <v>46073.54178240741</v>
+        <v>46073.65414351852</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
@@ -14321,7 +14331,7 @@
         <v>1</v>
       </c>
       <c r="N214" s="3" t="n">
-        <v>46073.56028935185</v>
+        <v>46073.63657407407</v>
       </c>
       <c r="O214" t="inlineStr">
         <is>
@@ -14385,7 +14395,7 @@
         <v>1</v>
       </c>
       <c r="N215" s="3" t="n">
-        <v>46073.54199074074</v>
+        <v>46073.62081018519</v>
       </c>
       <c r="O215" t="inlineStr">
         <is>
@@ -14449,7 +14459,7 @@
         <v>1</v>
       </c>
       <c r="N216" s="3" t="n">
-        <v>46073.55170138889</v>
+        <v>46073.6334375</v>
       </c>
       <c r="O216" t="inlineStr">
         <is>
@@ -14508,7 +14518,7 @@
         <v>1</v>
       </c>
       <c r="N217" s="3" t="n">
-        <v>46073.54594907408</v>
+        <v>46073.62578703704</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14572,7 +14582,7 @@
         <v>1</v>
       </c>
       <c r="N218" s="3" t="n">
-        <v>46073.56548611111</v>
+        <v>46073.64834490741</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14636,7 +14646,7 @@
         <v>1</v>
       </c>
       <c r="N219" s="3" t="n">
-        <v>46073.48967592593</v>
+        <v>46073.62157407407</v>
       </c>
       <c r="O219" t="inlineStr">
         <is>
@@ -14705,7 +14715,7 @@
         <v>1</v>
       </c>
       <c r="N220" s="3" t="n">
-        <v>46073.50677083333</v>
+        <v>46073.62635416666</v>
       </c>
       <c r="O220" t="inlineStr">
         <is>
@@ -14769,7 +14779,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="3" t="n">
-        <v>46073.56626157407</v>
+        <v>46073.63777777777</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14833,7 +14843,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="3" t="n">
-        <v>46073.56379629629</v>
+        <v>46073.64078703704</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -14897,7 +14907,7 @@
         <v>1</v>
       </c>
       <c r="N223" s="3" t="n">
-        <v>46072.8194212963</v>
+        <v>46073.62372685185</v>
       </c>
       <c r="O223" t="inlineStr">
         <is>
@@ -14961,7 +14971,7 @@
         <v>1</v>
       </c>
       <c r="N224" s="3" t="n">
-        <v>46072.75394675926</v>
+        <v>46073.64930555555</v>
       </c>
       <c r="O224" t="inlineStr">
         <is>
@@ -15025,7 +15035,7 @@
         <v>1</v>
       </c>
       <c r="N225" s="3" t="n">
-        <v>46072.80571759259</v>
+        <v>46073.63091435185</v>
       </c>
       <c r="O225" t="inlineStr">
         <is>
@@ -15089,7 +15099,7 @@
         <v>1</v>
       </c>
       <c r="N226" s="3" t="n">
-        <v>46073.5393287037</v>
+        <v>46073.62082175926</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15153,7 +15163,7 @@
         <v>1</v>
       </c>
       <c r="N227" s="3" t="n">
-        <v>46073.56765046297</v>
+        <v>46073.64791666667</v>
       </c>
       <c r="O227" t="inlineStr">
         <is>
@@ -15217,7 +15227,7 @@
         <v>1</v>
       </c>
       <c r="N228" s="3" t="n">
-        <v>46072.80038194444</v>
+        <v>46073.63697916667</v>
       </c>
       <c r="O228" t="inlineStr">
         <is>
@@ -15281,7 +15291,7 @@
         <v>1</v>
       </c>
       <c r="N229" s="3" t="n">
-        <v>46073.5625462963</v>
+        <v>46073.6359837963</v>
       </c>
       <c r="O229" t="inlineStr">
         <is>
@@ -15345,7 +15355,7 @@
         <v>1</v>
       </c>
       <c r="N230" s="3" t="n">
-        <v>46073.53916666667</v>
+        <v>46073.6215162037</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15409,7 +15419,7 @@
         <v>1</v>
       </c>
       <c r="N231" s="3" t="n">
-        <v>46073.53674768518</v>
+        <v>46073.63783564815</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15473,7 +15483,7 @@
         <v>1</v>
       </c>
       <c r="N232" s="3" t="n">
-        <v>46073.55577546296</v>
+        <v>46073.58748842592</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -15537,7 +15547,7 @@
         <v>1</v>
       </c>
       <c r="N233" s="3" t="n">
-        <v>46073.53484953703</v>
+        <v>46073.61719907408</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15601,7 +15611,7 @@
         <v>1</v>
       </c>
       <c r="N234" s="3" t="n">
-        <v>46073.55782407407</v>
+        <v>46073.62560185185</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -15665,7 +15675,7 @@
         <v>1</v>
       </c>
       <c r="N235" s="3" t="n">
-        <v>46072.8212037037</v>
+        <v>46073.62003472223</v>
       </c>
       <c r="O235" t="inlineStr">
         <is>
@@ -15729,7 +15739,7 @@
         <v>1</v>
       </c>
       <c r="N236" s="3" t="n">
-        <v>46072.8075462963</v>
+        <v>46073.63353009259</v>
       </c>
       <c r="O236" t="inlineStr">
         <is>
@@ -15793,7 +15803,7 @@
         <v>1</v>
       </c>
       <c r="N237" s="3" t="n">
-        <v>46072.81847222222</v>
+        <v>46073.62128472222</v>
       </c>
       <c r="O237" t="inlineStr">
         <is>
@@ -15857,7 +15867,7 @@
         <v>1</v>
       </c>
       <c r="N238" s="3" t="n">
-        <v>46073.56349537037</v>
+        <v>46073.64494212963</v>
       </c>
       <c r="O238" t="inlineStr">
         <is>
@@ -15921,7 +15931,7 @@
         <v>1</v>
       </c>
       <c r="N239" s="3" t="n">
-        <v>46073.54677083333</v>
+        <v>46073.62712962963</v>
       </c>
       <c r="O239" t="inlineStr">
         <is>
@@ -15985,7 +15995,7 @@
         <v>1</v>
       </c>
       <c r="N240" s="3" t="n">
-        <v>46073.55864583333</v>
+        <v>46073.6215162037</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16049,7 +16059,7 @@
         <v>1</v>
       </c>
       <c r="N241" s="3" t="n">
-        <v>46073.54549768518</v>
+        <v>46073.63231481481</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16113,7 +16123,7 @@
         <v>1</v>
       </c>
       <c r="N242" s="3" t="n">
-        <v>46073.55013888889</v>
+        <v>46073.62728009259</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16177,7 +16187,7 @@
         <v>1</v>
       </c>
       <c r="N243" s="3" t="n">
-        <v>46073.53672453704</v>
+        <v>46073.65077546296</v>
       </c>
       <c r="O243" t="inlineStr">
         <is>
@@ -16300,7 +16310,7 @@
         <v>1</v>
       </c>
       <c r="N245" s="3" t="n">
-        <v>46073.54495370371</v>
+        <v>46073.62739583333</v>
       </c>
       <c r="O245" t="inlineStr">
         <is>
@@ -16364,7 +16374,7 @@
         <v>1</v>
       </c>
       <c r="N246" s="3" t="n">
-        <v>46073.54415509259</v>
+        <v>46073.61859953704</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16492,7 +16502,7 @@
         <v>1</v>
       </c>
       <c r="N248" s="3" t="n">
-        <v>46073.53924768518</v>
+        <v>46073.63318287037</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16556,7 +16566,7 @@
         <v>1</v>
       </c>
       <c r="N249" s="3" t="n">
-        <v>46073.55804398148</v>
+        <v>46073.62756944444</v>
       </c>
       <c r="O249" t="inlineStr">
         <is>
@@ -16620,7 +16630,7 @@
         <v>1</v>
       </c>
       <c r="N250" s="3" t="n">
-        <v>46073.5575462963</v>
+        <v>46073.63877314814</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16684,7 +16694,7 @@
         <v>1</v>
       </c>
       <c r="N251" s="3" t="n">
-        <v>46073.54226851852</v>
+        <v>46073.6252662037</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16748,7 +16758,7 @@
         <v>1</v>
       </c>
       <c r="N252" s="3" t="n">
-        <v>46073.54922453704</v>
+        <v>46073.62761574074</v>
       </c>
       <c r="O252" t="inlineStr">
         <is>
@@ -16812,7 +16822,7 @@
         <v>1</v>
       </c>
       <c r="N253" s="3" t="n">
-        <v>46073.56105324074</v>
+        <v>46073.62152777778</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16870,7 +16880,7 @@
         <v>1</v>
       </c>
       <c r="N254" s="3" t="n">
-        <v>46073.54986111111</v>
+        <v>46073.63644675926</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -16934,7 +16944,7 @@
         <v>1</v>
       </c>
       <c r="N255" s="3" t="n">
-        <v>46073.5439699074</v>
+        <v>46073.62748842593</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -16998,7 +17008,7 @@
         <v>1</v>
       </c>
       <c r="N256" s="3" t="n">
-        <v>46073.55956018518</v>
+        <v>46073.63689814815</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17062,7 +17072,7 @@
         <v>1</v>
       </c>
       <c r="N257" s="3" t="n">
-        <v>46073.53170138889</v>
+        <v>46073.64961805556</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17126,7 +17136,7 @@
         <v>1</v>
       </c>
       <c r="N258" s="3" t="n">
-        <v>46073.56494212963</v>
+        <v>46073.64681712963</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
@@ -17190,7 +17200,7 @@
         <v>1</v>
       </c>
       <c r="N259" s="3" t="n">
-        <v>46073.56711805556</v>
+        <v>46073.64939814815</v>
       </c>
       <c r="O259" t="inlineStr">
         <is>
@@ -17254,7 +17264,7 @@
         <v>1</v>
       </c>
       <c r="N260" s="3" t="n">
-        <v>46073.56116898148</v>
+        <v>46073.62822916666</v>
       </c>
       <c r="O260" t="inlineStr">
         <is>
@@ -17446,7 +17456,7 @@
         <v>1</v>
       </c>
       <c r="N263" s="3" t="n">
-        <v>46073.56549768519</v>
+        <v>46073.63923611111</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17510,7 +17520,7 @@
         <v>1</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>46073.57115740741</v>
+        <v>46073.6484375</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17574,7 +17584,7 @@
         <v>1</v>
       </c>
       <c r="N265" s="3" t="n">
-        <v>46073.53457175926</v>
+        <v>46073.62402777778</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17638,7 +17648,7 @@
         <v>1</v>
       </c>
       <c r="N266" s="3" t="n">
-        <v>46073.53493055556</v>
+        <v>46073.65109953703</v>
       </c>
       <c r="O266" t="inlineStr">
         <is>
@@ -17702,7 +17712,7 @@
         <v>1</v>
       </c>
       <c r="N267" s="3" t="n">
-        <v>46073.55527777778</v>
+        <v>46073.62888888889</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17766,7 +17776,7 @@
         <v>1</v>
       </c>
       <c r="N268" s="3" t="n">
-        <v>46073.53055555555</v>
+        <v>46073.65125</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17830,7 +17840,7 @@
         <v>1</v>
       </c>
       <c r="N269" s="3" t="n">
-        <v>46073.57077546296</v>
+        <v>46073.64725694444</v>
       </c>
       <c r="O269" t="inlineStr">
         <is>
@@ -17891,7 +17901,7 @@
         </is>
       </c>
       <c r="N270" s="3" t="n">
-        <v>46073.54967592593</v>
+        <v>46073.63393518519</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -18019,7 +18029,7 @@
         <v>1</v>
       </c>
       <c r="N272" s="3" t="n">
-        <v>46073.54831018519</v>
+        <v>46073.6199537037</v>
       </c>
       <c r="O272" t="inlineStr">
         <is>
@@ -18083,7 +18093,7 @@
         <v>2</v>
       </c>
       <c r="N273" s="3" t="n">
-        <v>46073.54390046297</v>
+        <v>46073.62356481481</v>
       </c>
       <c r="O273" t="inlineStr">
         <is>
@@ -18403,7 +18413,7 @@
         <v>1</v>
       </c>
       <c r="N278" s="3" t="n">
-        <v>46073.56991898148</v>
+        <v>46073.64618055556</v>
       </c>
       <c r="O278" t="inlineStr">
         <is>
@@ -18531,7 +18541,7 @@
         <v>1</v>
       </c>
       <c r="N280" s="3" t="n">
-        <v>46073.55460648148</v>
+        <v>46073.63097222222</v>
       </c>
       <c r="O280" t="inlineStr">
         <is>
@@ -18595,7 +18605,7 @@
         <v>1</v>
       </c>
       <c r="N281" s="3" t="n">
-        <v>46073.55024305556</v>
+        <v>46073.63325231482</v>
       </c>
       <c r="O281" t="inlineStr">
         <is>
@@ -18718,7 +18728,7 @@
         <v>1</v>
       </c>
       <c r="N283" s="3" t="n">
-        <v>46073.53045138889</v>
+        <v>46073.62880787037</v>
       </c>
       <c r="O283" t="inlineStr">
         <is>
@@ -18782,7 +18792,7 @@
         <v>1</v>
       </c>
       <c r="N284" s="3" t="n">
-        <v>46073.56300925926</v>
+        <v>46073.64150462963</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18846,7 +18856,7 @@
         <v>1</v>
       </c>
       <c r="N285" s="3" t="n">
-        <v>46073.55717592593</v>
+        <v>46073.63177083333</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -18974,7 +18984,7 @@
         <v>1</v>
       </c>
       <c r="N287" s="3" t="n">
-        <v>46073.54762731482</v>
+        <v>46073.62616898148</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
@@ -19102,7 +19112,7 @@
         <v>1</v>
       </c>
       <c r="N289" s="3" t="n">
-        <v>46073.53822916667</v>
+        <v>46073.6203125</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -19896,7 +19906,7 @@
         <v>1</v>
       </c>
       <c r="N302" s="3" t="n">
-        <v>46073.54935185185</v>
+        <v>46073.62912037037</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -21012,7 +21022,7 @@
         </is>
       </c>
       <c r="N320" s="3" t="n">
-        <v>46073.55310185185</v>
+        <v>46073.63309027778</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21737,7 +21747,7 @@
         <v>1</v>
       </c>
       <c r="N332" s="3" t="n">
-        <v>46073.543125</v>
+        <v>46073.62159722222</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21801,7 +21811,7 @@
         <v>2</v>
       </c>
       <c r="N333" s="3" t="n">
-        <v>46073.54233796296</v>
+        <v>46073.62229166667</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21865,7 +21875,7 @@
         <v>2</v>
       </c>
       <c r="N334" s="3" t="n">
-        <v>46073.54971064815</v>
+        <v>46073.62203703704</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21929,7 +21939,7 @@
         <v>2</v>
       </c>
       <c r="N335" s="3" t="n">
-        <v>46073.55378472222</v>
+        <v>46073.62872685185</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -21993,7 +22003,7 @@
         <v>1</v>
       </c>
       <c r="N336" s="3" t="n">
-        <v>46073.54052083333</v>
+        <v>46073.61796296296</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22057,7 +22067,7 @@
         <v>1</v>
       </c>
       <c r="N337" s="3" t="n">
-        <v>46073.55474537037</v>
+        <v>46073.63467592592</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22121,7 +22131,7 @@
         <v>2</v>
       </c>
       <c r="N338" s="3" t="n">
-        <v>46073.55574074074</v>
+        <v>46073.6306712963</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -22377,7 +22387,7 @@
         <v>1</v>
       </c>
       <c r="N342" s="3" t="n">
-        <v>46073.53517361111</v>
+        <v>46073.57138888889</v>
       </c>
       <c r="O342" t="inlineStr">
         <is>
@@ -22438,7 +22448,7 @@
         </is>
       </c>
       <c r="N343" s="3" t="n">
-        <v>46073.54935185185</v>
+        <v>46073.62903935185</v>
       </c>
       <c r="O343" t="inlineStr">
         <is>
@@ -22694,7 +22704,7 @@
         <v>1</v>
       </c>
       <c r="N347" s="3" t="n">
-        <v>46073.54513888889</v>
+        <v>46073.58310185185</v>
       </c>
       <c r="O347" t="inlineStr">
         <is>
@@ -22758,7 +22768,7 @@
         <v>2</v>
       </c>
       <c r="N348" s="3" t="n">
-        <v>46073.53108796296</v>
+        <v>46073.57166666666</v>
       </c>
       <c r="O348" t="inlineStr">
         <is>
@@ -22822,7 +22832,7 @@
         <v>1</v>
       </c>
       <c r="N349" s="3" t="n">
-        <v>46073.53733796296</v>
+        <v>46073.57833333333</v>
       </c>
       <c r="O349" t="inlineStr">
         <is>
@@ -22841,11 +22851,6 @@
           <t>OPERACAO 9.1</t>
         </is>
       </c>
-      <c r="C350" t="inlineStr">
-        <is>
-          <t>10.69.5.244</t>
-        </is>
-      </c>
       <c r="D350" t="n">
         <v>2014</v>
       </c>
@@ -22950,7 +22955,7 @@
         <v>1</v>
       </c>
       <c r="N351" s="3" t="n">
-        <v>46073.54331018519</v>
+        <v>46073.58429398148</v>
       </c>
       <c r="O351" t="inlineStr">
         <is>
@@ -23014,7 +23019,7 @@
         <v>1</v>
       </c>
       <c r="N352" s="3" t="n">
-        <v>46073.53935185185</v>
+        <v>46073.57822916667</v>
       </c>
       <c r="O352" t="inlineStr">
         <is>
@@ -23075,7 +23080,7 @@
         </is>
       </c>
       <c r="N353" s="3" t="n">
-        <v>46073.53971064815</v>
+        <v>46073.57987268519</v>
       </c>
       <c r="O353" t="inlineStr">
         <is>
@@ -23136,7 +23141,7 @@
         </is>
       </c>
       <c r="N354" s="3" t="n">
-        <v>46073.53892361111</v>
+        <v>46073.57917824074</v>
       </c>
       <c r="O354" t="inlineStr">
         <is>
@@ -23200,7 +23205,7 @@
         <v>1</v>
       </c>
       <c r="N355" s="3" t="n">
-        <v>46073.53895833333</v>
+        <v>46073.58078703703</v>
       </c>
       <c r="O355" t="inlineStr">
         <is>
@@ -23264,7 +23269,7 @@
         <v>1</v>
       </c>
       <c r="N356" s="3" t="n">
-        <v>46073.53622685185</v>
+        <v>46073.5746412037</v>
       </c>
       <c r="O356" t="inlineStr">
         <is>
@@ -23328,7 +23333,7 @@
         <v>1</v>
       </c>
       <c r="N357" s="3" t="n">
-        <v>46073.53700231481</v>
+        <v>46073.57524305556</v>
       </c>
       <c r="O357" t="inlineStr">
         <is>
@@ -23515,7 +23520,7 @@
         <v>2</v>
       </c>
       <c r="N360" s="3" t="n">
-        <v>46073.53261574074</v>
+        <v>46073.57143518519</v>
       </c>
       <c r="O360" t="inlineStr">
         <is>
@@ -23579,7 +23584,7 @@
         <v>1</v>
       </c>
       <c r="N361" s="3" t="n">
-        <v>46073.54159722223</v>
+        <v>46073.64043981482</v>
       </c>
       <c r="O361" t="inlineStr">
         <is>
@@ -23640,7 +23645,7 @@
         </is>
       </c>
       <c r="N362" s="3" t="n">
-        <v>46073.53834490741</v>
+        <v>46073.5766087963</v>
       </c>
       <c r="O362" t="inlineStr">
         <is>
@@ -23828,7 +23833,7 @@
         <v>1</v>
       </c>
       <c r="N365" s="3" t="n">
-        <v>46073.53197916667</v>
+        <v>46073.64759259259</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
@@ -23894,7 +23899,7 @@
         </is>
       </c>
       <c r="N366" s="3" t="n">
-        <v>46073.56184027778</v>
+        <v>46073.64391203703</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -24020,7 +24025,7 @@
         </is>
       </c>
       <c r="N368" s="3" t="n">
-        <v>46073.55369212963</v>
+        <v>46073.63209490741</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -24039,11 +24044,6 @@
           <t>RH</t>
         </is>
       </c>
-      <c r="C369" t="inlineStr">
-        <is>
-          <t>10.69.3.13</t>
-        </is>
-      </c>
       <c r="D369" t="n">
         <v>2025</v>
       </c>
@@ -24086,7 +24086,7 @@
         </is>
       </c>
       <c r="N369" s="3" t="n">
-        <v>46073.55615740741</v>
+        <v>46073.63134259259</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
@@ -24155,7 +24155,7 @@
         <v>1</v>
       </c>
       <c r="N370" s="3" t="n">
-        <v>46073.55251157407</v>
+        <v>46073.63275462963</v>
       </c>
       <c r="O370" t="inlineStr">
         <is>
@@ -24293,7 +24293,7 @@
         <v>1</v>
       </c>
       <c r="N372" s="3" t="n">
-        <v>46072.64636574074</v>
+        <v>46073.62052083333</v>
       </c>
       <c r="O372" t="inlineStr">
         <is>
@@ -24314,7 +24314,7 @@
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>10.69.2.194</t>
+          <t>10.69.2.197</t>
         </is>
       </c>
       <c r="D373" t="n">
@@ -24362,7 +24362,7 @@
         <v>1</v>
       </c>
       <c r="N373" s="3" t="n">
-        <v>46072.64364583333</v>
+        <v>46073.62837962963</v>
       </c>
       <c r="O373" t="inlineStr">
         <is>
@@ -24431,7 +24431,7 @@
         <v>1</v>
       </c>
       <c r="N374" s="3" t="n">
-        <v>46073.53827546296</v>
+        <v>46073.65376157407</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24497,7 +24497,7 @@
         </is>
       </c>
       <c r="N375" s="3" t="n">
-        <v>46073.57018518518</v>
+        <v>46073.64290509259</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
@@ -24561,7 +24561,7 @@
         <v>1</v>
       </c>
       <c r="N376" s="3" t="n">
-        <v>46073.56222222222</v>
+        <v>46073.64045138889</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -24630,7 +24630,7 @@
         <v>2</v>
       </c>
       <c r="N377" s="3" t="n">
-        <v>46073.53771990741</v>
+        <v>46073.65453703704</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -24699,7 +24699,7 @@
         <v>2</v>
       </c>
       <c r="N378" s="3" t="n">
-        <v>46073.53424768519</v>
+        <v>46073.65006944445</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização automática 2026-02-20 17:52:04.287881
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>46073.62866898148</v>
+        <v>46073.70947916667</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>46073.61938657407</v>
+        <v>46073.73753472222</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
         <v>2</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>46073.65064814815</v>
+        <v>46073.6917824074</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>46073.65215277778</v>
+        <v>46073.73434027778</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -1131,7 +1131,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="3" t="n">
-        <v>46073.62952546297</v>
+        <v>46073.70746527778</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1451,7 +1451,7 @@
         <v>1</v>
       </c>
       <c r="N15" s="3" t="n">
-        <v>46073.65078703704</v>
+        <v>46073.72855324074</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1515,7 +1515,7 @@
         <v>2</v>
       </c>
       <c r="N16" s="3" t="n">
-        <v>46073.62695601852</v>
+        <v>46073.70487268519</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -2244,7 +2244,7 @@
         </is>
       </c>
       <c r="N28" s="3" t="n">
-        <v>46073.61810185185</v>
+        <v>46073.73467592592</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -6570,7 +6570,7 @@
         <v>1</v>
       </c>
       <c r="N95" s="3" t="n">
-        <v>46073.61950231482</v>
+        <v>46073.69754629629</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -6639,7 +6639,7 @@
         <v>1</v>
       </c>
       <c r="N96" s="3" t="n">
-        <v>46073.62659722222</v>
+        <v>46073.69917824074</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
@@ -6703,7 +6703,7 @@
         <v>1</v>
       </c>
       <c r="N97" s="3" t="n">
-        <v>46073.64060185185</v>
+        <v>46073.71755787037</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -6772,7 +6772,7 @@
         <v>1</v>
       </c>
       <c r="N98" s="3" t="n">
-        <v>46073.64871527778</v>
+        <v>46073.72436342593</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -6910,7 +6910,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>46073.64547453704</v>
+        <v>46073.719375</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6979,7 +6979,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="3" t="n">
-        <v>46073.61675925926</v>
+        <v>46073.69701388889</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -7117,7 +7117,7 @@
         <v>2</v>
       </c>
       <c r="N103" s="3" t="n">
-        <v>46073.63006944444</v>
+        <v>46073.70494212963</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7374,7 +7374,7 @@
         <v>1</v>
       </c>
       <c r="N107" s="3" t="n">
-        <v>46073.6183912037</v>
+        <v>46073.69743055556</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -7512,7 +7512,7 @@
         <v>1</v>
       </c>
       <c r="N109" s="3" t="n">
-        <v>46073.64761574074</v>
+        <v>46073.73207175926</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7581,7 +7581,7 @@
         <v>2</v>
       </c>
       <c r="N110" s="3" t="n">
-        <v>46073.63528935185</v>
+        <v>46073.70979166667</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7650,7 +7650,7 @@
         <v>2</v>
       </c>
       <c r="N111" s="3" t="n">
-        <v>46073.64070601852</v>
+        <v>46073.71922453704</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
@@ -7719,7 +7719,7 @@
         <v>2</v>
       </c>
       <c r="N112" s="3" t="n">
-        <v>46073.64163194445</v>
+        <v>46073.72145833333</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7788,7 +7788,7 @@
         <v>1</v>
       </c>
       <c r="N113" s="3" t="n">
-        <v>46073.62608796296</v>
+        <v>46073.70430555556</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7857,7 +7857,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>46073.63515046296</v>
+        <v>46073.71875</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -7923,7 +7923,7 @@
         </is>
       </c>
       <c r="N115" s="3" t="n">
-        <v>46073.64040509259</v>
+        <v>46073.71651620371</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -7992,7 +7992,7 @@
         <v>1</v>
       </c>
       <c r="N116" s="3" t="n">
-        <v>46073.63271990741</v>
+        <v>46073.70998842592</v>
       </c>
       <c r="O116" t="inlineStr">
         <is>
@@ -8011,11 +8011,6 @@
           <t>DP</t>
         </is>
       </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>10.69.3.23</t>
-        </is>
-      </c>
       <c r="D117" t="n">
         <v>2025</v>
       </c>
@@ -8061,7 +8056,7 @@
         <v>1</v>
       </c>
       <c r="N117" s="3" t="n">
-        <v>46073.65416666667</v>
+        <v>46073.69517361111</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -8265,7 +8260,7 @@
         <v>1</v>
       </c>
       <c r="N120" s="3" t="n">
-        <v>46073.6265625</v>
+        <v>46073.73755787037</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -8334,7 +8329,7 @@
         <v>1</v>
       </c>
       <c r="N121" s="3" t="n">
-        <v>46073.6299074074</v>
+        <v>46073.70646990741</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -8400,7 +8395,7 @@
         </is>
       </c>
       <c r="N122" s="3" t="n">
-        <v>46073.62711805556</v>
+        <v>46073.72890046296</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -8469,7 +8464,7 @@
         <v>2</v>
       </c>
       <c r="N123" s="3" t="n">
-        <v>46073.62328703704</v>
+        <v>46073.69956018519</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -8538,7 +8533,7 @@
         <v>1</v>
       </c>
       <c r="N124" s="3" t="n">
-        <v>46073.6493287037</v>
+        <v>46073.72692129629</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -8607,7 +8602,7 @@
         <v>1</v>
       </c>
       <c r="N125" s="3" t="n">
-        <v>46073.63644675926</v>
+        <v>46073.71335648148</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -8676,7 +8671,7 @@
         <v>1</v>
       </c>
       <c r="N126" s="3" t="n">
-        <v>46073.62375</v>
+        <v>46073.70068287037</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -8745,7 +8740,7 @@
         <v>2</v>
       </c>
       <c r="N127" s="3" t="n">
-        <v>46073.63575231482</v>
+        <v>46073.71240740741</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -8814,7 +8809,7 @@
         <v>1</v>
       </c>
       <c r="N128" s="3" t="n">
-        <v>46073.64767361111</v>
+        <v>46073.68280092593</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -8883,7 +8878,7 @@
         <v>1</v>
       </c>
       <c r="N129" s="3" t="n">
-        <v>46073.62746527778</v>
+        <v>46073.70827546297</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -8952,7 +8947,7 @@
         <v>1</v>
       </c>
       <c r="N130" s="3" t="n">
-        <v>46073.63625</v>
+        <v>46073.67806712963</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -9016,7 +9011,7 @@
         <v>1</v>
       </c>
       <c r="N131" s="3" t="n">
-        <v>46073.6333912037</v>
+        <v>46073.71293981482</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -9149,7 +9144,7 @@
         <v>1</v>
       </c>
       <c r="N133" s="3" t="n">
-        <v>46073.63890046296</v>
+        <v>46073.71950231482</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -9213,7 +9208,7 @@
         <v>1</v>
       </c>
       <c r="N134" s="3" t="n">
-        <v>46073.61700231482</v>
+        <v>46073.72908564815</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -9277,7 +9272,7 @@
         <v>1</v>
       </c>
       <c r="N135" s="3" t="n">
-        <v>46073.64847222222</v>
+        <v>46073.72878472223</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -9468,7 +9463,7 @@
         <v>1</v>
       </c>
       <c r="N138" s="3" t="n">
-        <v>46073.62471064815</v>
+        <v>46073.70126157408</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9532,7 +9527,7 @@
         <v>1</v>
       </c>
       <c r="N139" s="3" t="n">
-        <v>46073.62226851852</v>
+        <v>46073.73770833333</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9596,7 +9591,7 @@
         <v>1</v>
       </c>
       <c r="N140" s="3" t="n">
-        <v>46073.65045138889</v>
+        <v>46073.7246875</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9660,7 +9655,7 @@
         <v>1</v>
       </c>
       <c r="N141" s="3" t="n">
-        <v>46073.62081018519</v>
+        <v>46073.70212962963</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9724,7 +9719,7 @@
         <v>1</v>
       </c>
       <c r="N142" s="3" t="n">
-        <v>46073.63635416667</v>
+        <v>46073.71393518519</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9788,7 +9783,7 @@
         <v>1</v>
       </c>
       <c r="N143" s="3" t="n">
-        <v>46073.62324074074</v>
+        <v>46073.7059837963</v>
       </c>
       <c r="O143" t="inlineStr">
         <is>
@@ -9852,7 +9847,7 @@
         <v>1</v>
       </c>
       <c r="N144" s="3" t="n">
-        <v>46073.62424768518</v>
+        <v>46073.70085648148</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9916,7 +9911,7 @@
         <v>1</v>
       </c>
       <c r="N145" s="3" t="n">
-        <v>46073.62175925926</v>
+        <v>46073.70071759259</v>
       </c>
       <c r="O145" t="inlineStr">
         <is>
@@ -9980,7 +9975,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="3" t="n">
-        <v>46073.61898148148</v>
+        <v>46073.73335648148</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10044,7 +10039,7 @@
         <v>1</v>
       </c>
       <c r="N147" s="3" t="n">
-        <v>46073.64524305556</v>
+        <v>46073.71831018518</v>
       </c>
       <c r="O147" t="inlineStr">
         <is>
@@ -10108,7 +10103,7 @@
         <v>1</v>
       </c>
       <c r="N148" s="3" t="n">
-        <v>46073.64549768518</v>
+        <v>46073.72137731482</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10172,7 +10167,7 @@
         <v>1</v>
       </c>
       <c r="N149" s="3" t="n">
-        <v>46073.64280092593</v>
+        <v>46073.72304398148</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -10300,7 +10295,7 @@
         <v>1</v>
       </c>
       <c r="N151" s="3" t="n">
-        <v>46073.63704861111</v>
+        <v>46073.71430555556</v>
       </c>
       <c r="O151" t="inlineStr">
         <is>
@@ -10364,7 +10359,7 @@
         <v>1</v>
       </c>
       <c r="N152" s="3" t="n">
-        <v>46073.62025462963</v>
+        <v>46073.69875</v>
       </c>
       <c r="O152" t="inlineStr">
         <is>
@@ -10428,7 +10423,7 @@
         <v>1</v>
       </c>
       <c r="N153" s="3" t="n">
-        <v>46073.64875</v>
+        <v>46073.72969907407</v>
       </c>
       <c r="O153" t="inlineStr">
         <is>
@@ -10492,7 +10487,7 @@
         <v>1</v>
       </c>
       <c r="N154" s="3" t="n">
-        <v>46073.62189814815</v>
+        <v>46073.70202546296</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10556,7 +10551,7 @@
         <v>1</v>
       </c>
       <c r="N155" s="3" t="n">
-        <v>46073.62208333334</v>
+        <v>46073.69869212963</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10684,7 +10679,7 @@
         <v>1</v>
       </c>
       <c r="N157" s="3" t="n">
-        <v>46073.62059027778</v>
+        <v>46073.73583333333</v>
       </c>
       <c r="O157" t="inlineStr">
         <is>
@@ -10812,7 +10807,7 @@
         <v>1</v>
       </c>
       <c r="N159" s="3" t="n">
-        <v>46073.64628472222</v>
+        <v>46073.72405092593</v>
       </c>
       <c r="O159" t="inlineStr">
         <is>
@@ -11004,7 +10999,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="3" t="n">
-        <v>46073.63545138889</v>
+        <v>46073.71219907407</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11132,7 +11127,7 @@
         <v>2</v>
       </c>
       <c r="N164" s="3" t="n">
-        <v>46073.6303587963</v>
+        <v>46073.70666666667</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11196,7 +11191,7 @@
         <v>2</v>
       </c>
       <c r="N165" s="3" t="n">
-        <v>46073.62736111111</v>
+        <v>46073.70420138889</v>
       </c>
       <c r="O165" t="inlineStr">
         <is>
@@ -11452,7 +11447,7 @@
         <v>2</v>
       </c>
       <c r="N169" s="3" t="n">
-        <v>46073.63478009259</v>
+        <v>46073.71071759259</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -11516,7 +11511,7 @@
         <v>2</v>
       </c>
       <c r="N170" s="3" t="n">
-        <v>46073.64931712963</v>
+        <v>46073.72961805556</v>
       </c>
       <c r="O170" t="inlineStr">
         <is>
@@ -11644,7 +11639,7 @@
         <v>2</v>
       </c>
       <c r="N172" s="3" t="n">
-        <v>46073.61986111111</v>
+        <v>46073.73344907408</v>
       </c>
       <c r="O172" t="inlineStr">
         <is>
@@ -11708,7 +11703,7 @@
         <v>2</v>
       </c>
       <c r="N173" s="3" t="n">
-        <v>46073.62208333334</v>
+        <v>46073.70238425926</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -11836,7 +11831,7 @@
         <v>2</v>
       </c>
       <c r="N175" s="3" t="n">
-        <v>46073.61971064815</v>
+        <v>46073.70326388889</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -11964,7 +11959,7 @@
         <v>2</v>
       </c>
       <c r="N177" s="3" t="n">
-        <v>46073.61417824074</v>
+        <v>46073.69657407407</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
@@ -12028,7 +12023,7 @@
         <v>2</v>
       </c>
       <c r="N178" s="3" t="n">
-        <v>46073.62996527777</v>
+        <v>46073.70726851852</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12092,7 +12087,7 @@
         <v>1</v>
       </c>
       <c r="N179" s="3" t="n">
-        <v>46073.63991898148</v>
+        <v>46073.72288194444</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12156,7 +12151,7 @@
         <v>1</v>
       </c>
       <c r="N180" s="3" t="n">
-        <v>46073.62032407407</v>
+        <v>46073.73020833333</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12220,7 +12215,7 @@
         <v>1</v>
       </c>
       <c r="N181" s="3" t="n">
-        <v>46073.64716435185</v>
+        <v>46073.7256712963</v>
       </c>
       <c r="O181" t="inlineStr">
         <is>
@@ -12609,7 +12604,7 @@
         <v>1</v>
       </c>
       <c r="N187" s="3" t="n">
-        <v>46073.62079861111</v>
+        <v>46073.70072916667</v>
       </c>
       <c r="O187" t="inlineStr">
         <is>
@@ -12759,11 +12754,6 @@
           <t>OPERACAO 8.1</t>
         </is>
       </c>
-      <c r="C190" t="inlineStr">
-        <is>
-          <t>10.69.5.59</t>
-        </is>
-      </c>
       <c r="D190" t="n">
         <v>2015</v>
       </c>
@@ -12801,7 +12791,7 @@
         </is>
       </c>
       <c r="N190" s="3" t="n">
-        <v>46073.62104166667</v>
+        <v>46073.7015625</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12865,7 +12855,7 @@
         <v>1</v>
       </c>
       <c r="N191" s="3" t="n">
-        <v>46073.61459490741</v>
+        <v>46073.7328125</v>
       </c>
       <c r="O191" t="inlineStr">
         <is>
@@ -12929,7 +12919,7 @@
         <v>1</v>
       </c>
       <c r="N192" s="3" t="n">
-        <v>46073.63047453704</v>
+        <v>46073.70230324074</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -13054,7 +13044,7 @@
         <v>2</v>
       </c>
       <c r="N194" s="3" t="n">
-        <v>46073.61572916667</v>
+        <v>46073.69778935185</v>
       </c>
       <c r="O194" t="inlineStr">
         <is>
@@ -13118,7 +13108,7 @@
         <v>1</v>
       </c>
       <c r="N195" s="3" t="n">
-        <v>46073.61953703704</v>
+        <v>46073.69761574074</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13182,7 +13172,7 @@
         <v>1</v>
       </c>
       <c r="N196" s="3" t="n">
-        <v>46073.62190972222</v>
+        <v>46073.70025462963</v>
       </c>
       <c r="O196" t="inlineStr">
         <is>
@@ -13246,7 +13236,7 @@
         <v>1</v>
       </c>
       <c r="N197" s="3" t="n">
-        <v>46073.61754629629</v>
+        <v>46073.73730324074</v>
       </c>
       <c r="O197" t="inlineStr">
         <is>
@@ -13310,7 +13300,7 @@
         <v>1</v>
       </c>
       <c r="N198" s="3" t="n">
-        <v>46073.65328703704</v>
+        <v>46073.73479166667</v>
       </c>
       <c r="O198" t="inlineStr">
         <is>
@@ -13374,7 +13364,7 @@
         <v>1</v>
       </c>
       <c r="N199" s="3" t="n">
-        <v>46073.62240740741</v>
+        <v>46073.70560185185</v>
       </c>
       <c r="O199" t="inlineStr">
         <is>
@@ -13438,7 +13428,7 @@
         <v>1</v>
       </c>
       <c r="N200" s="3" t="n">
-        <v>46073.6434375</v>
+        <v>46073.7127662037</v>
       </c>
       <c r="O200" t="inlineStr">
         <is>
@@ -13499,7 +13489,7 @@
         </is>
       </c>
       <c r="N201" s="3" t="n">
-        <v>46073.63636574074</v>
+        <v>46073.71769675926</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -13563,7 +13553,7 @@
         <v>1</v>
       </c>
       <c r="N202" s="3" t="n">
-        <v>46073.62311342593</v>
+        <v>46073.70153935185</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13627,7 +13617,7 @@
         <v>1</v>
       </c>
       <c r="N203" s="3" t="n">
-        <v>46073.63091435185</v>
+        <v>46073.72726851852</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13691,7 +13681,7 @@
         <v>1</v>
       </c>
       <c r="N204" s="3" t="n">
-        <v>46073.64045138889</v>
+        <v>46073.71761574074</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13755,7 +13745,7 @@
         <v>1</v>
       </c>
       <c r="N205" s="3" t="n">
-        <v>46073.63332175926</v>
+        <v>46073.71144675926</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13819,7 +13809,7 @@
         <v>1</v>
       </c>
       <c r="N206" s="3" t="n">
-        <v>46073.65171296296</v>
+        <v>46073.72695601852</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -13883,7 +13873,7 @@
         <v>1</v>
       </c>
       <c r="N207" s="3" t="n">
-        <v>46073.61866898148</v>
+        <v>46073.67253472222</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -14011,7 +14001,7 @@
         <v>1</v>
       </c>
       <c r="N209" s="3" t="n">
-        <v>46073.62671296296</v>
+        <v>46073.73738425926</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14075,7 +14065,7 @@
         <v>1</v>
       </c>
       <c r="N210" s="3" t="n">
-        <v>46073.64670138889</v>
+        <v>46073.72759259259</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14139,7 +14129,7 @@
         <v>1</v>
       </c>
       <c r="N211" s="3" t="n">
-        <v>46073.62670138889</v>
+        <v>46073.70135416667</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -14203,7 +14193,7 @@
         <v>1</v>
       </c>
       <c r="N212" s="3" t="n">
-        <v>46073.62702546296</v>
+        <v>46073.70181712963</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -14267,7 +14257,7 @@
         <v>1</v>
       </c>
       <c r="N213" s="3" t="n">
-        <v>46073.65414351852</v>
+        <v>46073.73081018519</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
@@ -14331,7 +14321,7 @@
         <v>1</v>
       </c>
       <c r="N214" s="3" t="n">
-        <v>46073.63657407407</v>
+        <v>46073.71372685185</v>
       </c>
       <c r="O214" t="inlineStr">
         <is>
@@ -14395,7 +14385,7 @@
         <v>1</v>
       </c>
       <c r="N215" s="3" t="n">
-        <v>46073.62081018519</v>
+        <v>46073.70395833333</v>
       </c>
       <c r="O215" t="inlineStr">
         <is>
@@ -14459,7 +14449,7 @@
         <v>1</v>
       </c>
       <c r="N216" s="3" t="n">
-        <v>46073.6334375</v>
+        <v>46073.71153935185</v>
       </c>
       <c r="O216" t="inlineStr">
         <is>
@@ -14518,7 +14508,7 @@
         <v>1</v>
       </c>
       <c r="N217" s="3" t="n">
-        <v>46073.62578703704</v>
+        <v>46073.70238425926</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14582,7 +14572,7 @@
         <v>1</v>
       </c>
       <c r="N218" s="3" t="n">
-        <v>46073.64834490741</v>
+        <v>46073.72780092592</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14646,7 +14636,7 @@
         <v>1</v>
       </c>
       <c r="N219" s="3" t="n">
-        <v>46073.62157407407</v>
+        <v>46073.67429398148</v>
       </c>
       <c r="O219" t="inlineStr">
         <is>
@@ -14715,7 +14705,7 @@
         <v>1</v>
       </c>
       <c r="N220" s="3" t="n">
-        <v>46073.62635416666</v>
+        <v>46073.70287037037</v>
       </c>
       <c r="O220" t="inlineStr">
         <is>
@@ -14779,7 +14769,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="3" t="n">
-        <v>46073.63777777777</v>
+        <v>46073.71880787037</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14843,7 +14833,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="3" t="n">
-        <v>46073.64078703704</v>
+        <v>46073.71142361111</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -14907,7 +14897,7 @@
         <v>1</v>
       </c>
       <c r="N223" s="3" t="n">
-        <v>46073.62372685185</v>
+        <v>46073.73364583333</v>
       </c>
       <c r="O223" t="inlineStr">
         <is>
@@ -14971,7 +14961,7 @@
         <v>1</v>
       </c>
       <c r="N224" s="3" t="n">
-        <v>46073.64930555555</v>
+        <v>46073.71427083333</v>
       </c>
       <c r="O224" t="inlineStr">
         <is>
@@ -15035,7 +15025,7 @@
         <v>1</v>
       </c>
       <c r="N225" s="3" t="n">
-        <v>46073.63091435185</v>
+        <v>46073.70865740741</v>
       </c>
       <c r="O225" t="inlineStr">
         <is>
@@ -15099,7 +15089,7 @@
         <v>1</v>
       </c>
       <c r="N226" s="3" t="n">
-        <v>46073.62082175926</v>
+        <v>46073.69674768519</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15163,7 +15153,7 @@
         <v>1</v>
       </c>
       <c r="N227" s="3" t="n">
-        <v>46073.64791666667</v>
+        <v>46073.7265625</v>
       </c>
       <c r="O227" t="inlineStr">
         <is>
@@ -15227,7 +15217,7 @@
         <v>1</v>
       </c>
       <c r="N228" s="3" t="n">
-        <v>46073.63697916667</v>
+        <v>46073.71868055555</v>
       </c>
       <c r="O228" t="inlineStr">
         <is>
@@ -15291,7 +15281,7 @@
         <v>1</v>
       </c>
       <c r="N229" s="3" t="n">
-        <v>46073.6359837963</v>
+        <v>46073.71759259259</v>
       </c>
       <c r="O229" t="inlineStr">
         <is>
@@ -15355,7 +15345,7 @@
         <v>1</v>
       </c>
       <c r="N230" s="3" t="n">
-        <v>46073.6215162037</v>
+        <v>46073.70017361111</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15419,7 +15409,7 @@
         <v>1</v>
       </c>
       <c r="N231" s="3" t="n">
-        <v>46073.63783564815</v>
+        <v>46073.7196875</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15483,7 +15473,7 @@
         <v>1</v>
       </c>
       <c r="N232" s="3" t="n">
-        <v>46073.58748842592</v>
+        <v>46073.69118055556</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -15547,7 +15537,7 @@
         <v>1</v>
       </c>
       <c r="N233" s="3" t="n">
-        <v>46073.61719907408</v>
+        <v>46073.73660879629</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15611,7 +15601,7 @@
         <v>1</v>
       </c>
       <c r="N234" s="3" t="n">
-        <v>46073.62560185185</v>
+        <v>46073.69894675926</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -15675,7 +15665,7 @@
         <v>1</v>
       </c>
       <c r="N235" s="3" t="n">
-        <v>46073.62003472223</v>
+        <v>46073.70006944444</v>
       </c>
       <c r="O235" t="inlineStr">
         <is>
@@ -15739,7 +15729,7 @@
         <v>1</v>
       </c>
       <c r="N236" s="3" t="n">
-        <v>46073.63353009259</v>
+        <v>46073.71017361111</v>
       </c>
       <c r="O236" t="inlineStr">
         <is>
@@ -15803,7 +15793,7 @@
         <v>1</v>
       </c>
       <c r="N237" s="3" t="n">
-        <v>46073.62128472222</v>
+        <v>46073.69726851852</v>
       </c>
       <c r="O237" t="inlineStr">
         <is>
@@ -15867,7 +15857,7 @@
         <v>1</v>
       </c>
       <c r="N238" s="3" t="n">
-        <v>46073.64494212963</v>
+        <v>46073.73618055556</v>
       </c>
       <c r="O238" t="inlineStr">
         <is>
@@ -15931,7 +15921,7 @@
         <v>1</v>
       </c>
       <c r="N239" s="3" t="n">
-        <v>46073.62712962963</v>
+        <v>46073.70643518519</v>
       </c>
       <c r="O239" t="inlineStr">
         <is>
@@ -15995,7 +15985,7 @@
         <v>1</v>
       </c>
       <c r="N240" s="3" t="n">
-        <v>46073.6215162037</v>
+        <v>46073.70074074074</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16059,7 +16049,7 @@
         <v>1</v>
       </c>
       <c r="N241" s="3" t="n">
-        <v>46073.63231481481</v>
+        <v>46073.70967592593</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16123,7 +16113,7 @@
         <v>1</v>
       </c>
       <c r="N242" s="3" t="n">
-        <v>46073.62728009259</v>
+        <v>46073.70518518519</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16187,7 +16177,7 @@
         <v>1</v>
       </c>
       <c r="N243" s="3" t="n">
-        <v>46073.65077546296</v>
+        <v>46073.73145833334</v>
       </c>
       <c r="O243" t="inlineStr">
         <is>
@@ -16310,7 +16300,7 @@
         <v>1</v>
       </c>
       <c r="N245" s="3" t="n">
-        <v>46073.62739583333</v>
+        <v>46073.70581018519</v>
       </c>
       <c r="O245" t="inlineStr">
         <is>
@@ -16374,7 +16364,7 @@
         <v>1</v>
       </c>
       <c r="N246" s="3" t="n">
-        <v>46073.61859953704</v>
+        <v>46073.7302662037</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16502,7 +16492,7 @@
         <v>1</v>
       </c>
       <c r="N248" s="3" t="n">
-        <v>46073.63318287037</v>
+        <v>46073.70858796296</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16566,7 +16556,7 @@
         <v>1</v>
       </c>
       <c r="N249" s="3" t="n">
-        <v>46073.62756944444</v>
+        <v>46073.70457175926</v>
       </c>
       <c r="O249" t="inlineStr">
         <is>
@@ -16630,7 +16620,7 @@
         <v>1</v>
       </c>
       <c r="N250" s="3" t="n">
-        <v>46073.63877314814</v>
+        <v>46073.71510416667</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16694,7 +16684,7 @@
         <v>1</v>
       </c>
       <c r="N251" s="3" t="n">
-        <v>46073.6252662037</v>
+        <v>46073.70314814815</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16758,7 +16748,7 @@
         <v>1</v>
       </c>
       <c r="N252" s="3" t="n">
-        <v>46073.62761574074</v>
+        <v>46073.71115740741</v>
       </c>
       <c r="O252" t="inlineStr">
         <is>
@@ -16822,7 +16812,7 @@
         <v>1</v>
       </c>
       <c r="N253" s="3" t="n">
-        <v>46073.62152777778</v>
+        <v>46073.70133101852</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16880,7 +16870,7 @@
         <v>1</v>
       </c>
       <c r="N254" s="3" t="n">
-        <v>46073.63644675926</v>
+        <v>46073.70997685185</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -16944,7 +16934,7 @@
         <v>1</v>
       </c>
       <c r="N255" s="3" t="n">
-        <v>46073.62748842593</v>
+        <v>46073.70814814815</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -17008,7 +16998,7 @@
         <v>1</v>
       </c>
       <c r="N256" s="3" t="n">
-        <v>46073.63689814815</v>
+        <v>46073.71556712963</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17072,7 +17062,7 @@
         <v>1</v>
       </c>
       <c r="N257" s="3" t="n">
-        <v>46073.64961805556</v>
+        <v>46073.72362268518</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17136,7 +17126,7 @@
         <v>1</v>
       </c>
       <c r="N258" s="3" t="n">
-        <v>46073.64681712963</v>
+        <v>46073.72253472222</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
@@ -17200,7 +17190,7 @@
         <v>1</v>
       </c>
       <c r="N259" s="3" t="n">
-        <v>46073.64939814815</v>
+        <v>46073.72872685185</v>
       </c>
       <c r="O259" t="inlineStr">
         <is>
@@ -17264,7 +17254,7 @@
         <v>1</v>
       </c>
       <c r="N260" s="3" t="n">
-        <v>46073.62822916666</v>
+        <v>46073.70597222223</v>
       </c>
       <c r="O260" t="inlineStr">
         <is>
@@ -17456,7 +17446,7 @@
         <v>1</v>
       </c>
       <c r="N263" s="3" t="n">
-        <v>46073.63923611111</v>
+        <v>46073.71864583333</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17520,7 +17510,7 @@
         <v>1</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>46073.6484375</v>
+        <v>46073.72684027778</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17584,7 +17574,7 @@
         <v>1</v>
       </c>
       <c r="N265" s="3" t="n">
-        <v>46073.62402777778</v>
+        <v>46073.73547453704</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17648,7 +17638,7 @@
         <v>1</v>
       </c>
       <c r="N266" s="3" t="n">
-        <v>46073.65109953703</v>
+        <v>46073.73516203704</v>
       </c>
       <c r="O266" t="inlineStr">
         <is>
@@ -17712,7 +17702,7 @@
         <v>1</v>
       </c>
       <c r="N267" s="3" t="n">
-        <v>46073.62888888889</v>
+        <v>46073.71178240741</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17776,7 +17766,7 @@
         <v>1</v>
       </c>
       <c r="N268" s="3" t="n">
-        <v>46073.65125</v>
+        <v>46073.72796296296</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17840,7 +17830,7 @@
         <v>1</v>
       </c>
       <c r="N269" s="3" t="n">
-        <v>46073.64725694444</v>
+        <v>46073.72123842593</v>
       </c>
       <c r="O269" t="inlineStr">
         <is>
@@ -17901,7 +17891,7 @@
         </is>
       </c>
       <c r="N270" s="3" t="n">
-        <v>46073.63393518519</v>
+        <v>46073.71422453703</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -18029,7 +18019,7 @@
         <v>1</v>
       </c>
       <c r="N272" s="3" t="n">
-        <v>46073.6199537037</v>
+        <v>46073.6574537037</v>
       </c>
       <c r="O272" t="inlineStr">
         <is>
@@ -18093,7 +18083,7 @@
         <v>2</v>
       </c>
       <c r="N273" s="3" t="n">
-        <v>46073.62356481481</v>
+        <v>46073.66003472222</v>
       </c>
       <c r="O273" t="inlineStr">
         <is>
@@ -18413,7 +18403,7 @@
         <v>1</v>
       </c>
       <c r="N278" s="3" t="n">
-        <v>46073.64618055556</v>
+        <v>46073.72538194444</v>
       </c>
       <c r="O278" t="inlineStr">
         <is>
@@ -18541,7 +18531,7 @@
         <v>1</v>
       </c>
       <c r="N280" s="3" t="n">
-        <v>46073.63097222222</v>
+        <v>46073.70400462963</v>
       </c>
       <c r="O280" t="inlineStr">
         <is>
@@ -18605,7 +18595,7 @@
         <v>1</v>
       </c>
       <c r="N281" s="3" t="n">
-        <v>46073.63325231482</v>
+        <v>46073.71434027778</v>
       </c>
       <c r="O281" t="inlineStr">
         <is>
@@ -18728,7 +18718,7 @@
         <v>1</v>
       </c>
       <c r="N283" s="3" t="n">
-        <v>46073.62880787037</v>
+        <v>46073.70460648148</v>
       </c>
       <c r="O283" t="inlineStr">
         <is>
@@ -18792,7 +18782,7 @@
         <v>1</v>
       </c>
       <c r="N284" s="3" t="n">
-        <v>46073.64150462963</v>
+        <v>46073.71934027778</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18856,7 +18846,7 @@
         <v>1</v>
       </c>
       <c r="N285" s="3" t="n">
-        <v>46073.63177083333</v>
+        <v>46073.70583333333</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -18984,7 +18974,7 @@
         <v>1</v>
       </c>
       <c r="N287" s="3" t="n">
-        <v>46073.62616898148</v>
+        <v>46073.704375</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
@@ -19112,7 +19102,7 @@
         <v>1</v>
       </c>
       <c r="N289" s="3" t="n">
-        <v>46073.6203125</v>
+        <v>46073.73370370371</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -19906,7 +19896,7 @@
         <v>1</v>
       </c>
       <c r="N302" s="3" t="n">
-        <v>46073.62912037037</v>
+        <v>46073.7112037037</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -21022,7 +21012,7 @@
         </is>
       </c>
       <c r="N320" s="3" t="n">
-        <v>46073.63309027778</v>
+        <v>46073.71248842592</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21747,7 +21737,7 @@
         <v>1</v>
       </c>
       <c r="N332" s="3" t="n">
-        <v>46073.62159722222</v>
+        <v>46073.73409722222</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21811,7 +21801,7 @@
         <v>2</v>
       </c>
       <c r="N333" s="3" t="n">
-        <v>46073.62229166667</v>
+        <v>46073.69988425926</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21875,7 +21865,7 @@
         <v>2</v>
       </c>
       <c r="N334" s="3" t="n">
-        <v>46073.62203703704</v>
+        <v>46073.73532407408</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21939,7 +21929,7 @@
         <v>2</v>
       </c>
       <c r="N335" s="3" t="n">
-        <v>46073.62872685185</v>
+        <v>46073.70690972222</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -22003,7 +21993,7 @@
         <v>1</v>
       </c>
       <c r="N336" s="3" t="n">
-        <v>46073.61796296296</v>
+        <v>46073.73548611111</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22067,7 +22057,7 @@
         <v>1</v>
       </c>
       <c r="N337" s="3" t="n">
-        <v>46073.63467592592</v>
+        <v>46073.71641203704</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22131,7 +22121,7 @@
         <v>2</v>
       </c>
       <c r="N338" s="3" t="n">
-        <v>46073.6306712963</v>
+        <v>46073.70998842592</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -22216,7 +22206,7 @@
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>10.69.2.194</t>
+          <t>10.69.5.234</t>
         </is>
       </c>
       <c r="D340" t="n">
@@ -22259,7 +22249,7 @@
         <v>1</v>
       </c>
       <c r="N340" s="3" t="n">
-        <v>46073.4329050926</v>
+        <v>46073.71038194445</v>
       </c>
       <c r="O340" t="inlineStr">
         <is>
@@ -22448,7 +22438,7 @@
         </is>
       </c>
       <c r="N343" s="3" t="n">
-        <v>46073.62903935185</v>
+        <v>46073.70519675926</v>
       </c>
       <c r="O343" t="inlineStr">
         <is>
@@ -22851,6 +22841,11 @@
           <t>OPERACAO 9.1</t>
         </is>
       </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>10.69.5.244</t>
+        </is>
+      </c>
       <c r="D350" t="n">
         <v>2014</v>
       </c>
@@ -22891,7 +22886,7 @@
         <v>1</v>
       </c>
       <c r="N350" s="3" t="n">
-        <v>46073.56927083333</v>
+        <v>46073.70173611111</v>
       </c>
       <c r="O350" t="inlineStr">
         <is>
@@ -23584,7 +23579,7 @@
         <v>1</v>
       </c>
       <c r="N361" s="3" t="n">
-        <v>46073.64043981482</v>
+        <v>46073.67961805555</v>
       </c>
       <c r="O361" t="inlineStr">
         <is>
@@ -23833,7 +23828,7 @@
         <v>1</v>
       </c>
       <c r="N365" s="3" t="n">
-        <v>46073.64759259259</v>
+        <v>46073.68641203704</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
@@ -23899,7 +23894,7 @@
         </is>
       </c>
       <c r="N366" s="3" t="n">
-        <v>46073.64391203703</v>
+        <v>46073.72146990741</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -24025,7 +24020,7 @@
         </is>
       </c>
       <c r="N368" s="3" t="n">
-        <v>46073.63209490741</v>
+        <v>46073.71178240741</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -24044,6 +24039,11 @@
           <t>RH</t>
         </is>
       </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>10.69.3.13</t>
+        </is>
+      </c>
       <c r="D369" t="n">
         <v>2025</v>
       </c>
@@ -24086,7 +24086,7 @@
         </is>
       </c>
       <c r="N369" s="3" t="n">
-        <v>46073.63134259259</v>
+        <v>46073.71048611111</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
@@ -24155,7 +24155,7 @@
         <v>1</v>
       </c>
       <c r="N370" s="3" t="n">
-        <v>46073.63275462963</v>
+        <v>46073.70724537037</v>
       </c>
       <c r="O370" t="inlineStr">
         <is>
@@ -24431,7 +24431,7 @@
         <v>1</v>
       </c>
       <c r="N374" s="3" t="n">
-        <v>46073.65376157407</v>
+        <v>46073.72709490741</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24497,7 +24497,7 @@
         </is>
       </c>
       <c r="N375" s="3" t="n">
-        <v>46073.64290509259</v>
+        <v>46073.72311342593</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
@@ -24561,7 +24561,7 @@
         <v>1</v>
       </c>
       <c r="N376" s="3" t="n">
-        <v>46073.64045138889</v>
+        <v>46073.71952546296</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -24630,7 +24630,7 @@
         <v>2</v>
       </c>
       <c r="N377" s="3" t="n">
-        <v>46073.65453703704</v>
+        <v>46073.69086805556</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -24699,7 +24699,7 @@
         <v>2</v>
       </c>
       <c r="N378" s="3" t="n">
-        <v>46073.65006944445</v>
+        <v>46073.73082175926</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização automática 2026-02-23 07:52:05.462339
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>46073.70947916667</v>
+        <v>46076.30568287037</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>46073.73753472222</v>
+        <v>46076.30667824074</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -1131,7 +1131,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="3" t="n">
-        <v>46073.70746527778</v>
+        <v>46076.2999537037</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1451,7 +1451,7 @@
         <v>1</v>
       </c>
       <c r="N15" s="3" t="n">
-        <v>46073.72855324074</v>
+        <v>46076.30304398148</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1515,7 +1515,7 @@
         <v>2</v>
       </c>
       <c r="N16" s="3" t="n">
-        <v>46073.70487268519</v>
+        <v>46076.30726851852</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -6639,7 +6639,7 @@
         <v>1</v>
       </c>
       <c r="N96" s="3" t="n">
-        <v>46073.69917824074</v>
+        <v>46073.82103009259</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
@@ -6658,6 +6658,11 @@
           <t>COORDENACAO</t>
         </is>
       </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>10.69.3.93</t>
+        </is>
+      </c>
       <c r="D97" t="n">
         <v>2025</v>
       </c>
@@ -6703,7 +6708,7 @@
         <v>1</v>
       </c>
       <c r="N97" s="3" t="n">
-        <v>46073.71755787037</v>
+        <v>46074.6058912037</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -6722,11 +6727,6 @@
           <t>COORDENACAO</t>
         </is>
       </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>10.69.3.94</t>
-        </is>
-      </c>
       <c r="D98" t="n">
         <v>2025</v>
       </c>
@@ -6772,7 +6772,7 @@
         <v>1</v>
       </c>
       <c r="N98" s="3" t="n">
-        <v>46073.72436342593</v>
+        <v>46074.55390046296</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -6910,7 +6910,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>46073.719375</v>
+        <v>46076.29877314815</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6979,7 +6979,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="3" t="n">
-        <v>46073.69701388889</v>
+        <v>46075.06710648148</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -7117,7 +7117,7 @@
         <v>2</v>
       </c>
       <c r="N103" s="3" t="n">
-        <v>46073.70494212963</v>
+        <v>46076.30193287037</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7512,7 +7512,7 @@
         <v>1</v>
       </c>
       <c r="N109" s="3" t="n">
-        <v>46073.73207175926</v>
+        <v>46076.30444444445</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7581,7 +7581,7 @@
         <v>2</v>
       </c>
       <c r="N110" s="3" t="n">
-        <v>46073.70979166667</v>
+        <v>46076.30501157408</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7719,7 +7719,7 @@
         <v>2</v>
       </c>
       <c r="N112" s="3" t="n">
-        <v>46073.72145833333</v>
+        <v>46076.31232638889</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7788,7 +7788,7 @@
         <v>1</v>
       </c>
       <c r="N113" s="3" t="n">
-        <v>46073.70430555556</v>
+        <v>46076.30126157407</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7857,7 +7857,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>46073.71875</v>
+        <v>46076.30136574074</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -7923,7 +7923,7 @@
         </is>
       </c>
       <c r="N115" s="3" t="n">
-        <v>46073.71651620371</v>
+        <v>46073.75619212963</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -8011,6 +8011,11 @@
           <t>DP</t>
         </is>
       </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>10.69.3.23</t>
+        </is>
+      </c>
       <c r="D117" t="n">
         <v>2025</v>
       </c>
@@ -8056,7 +8061,7 @@
         <v>1</v>
       </c>
       <c r="N117" s="3" t="n">
-        <v>46073.69517361111</v>
+        <v>46076.31689814815</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -8329,7 +8334,7 @@
         <v>1</v>
       </c>
       <c r="N121" s="3" t="n">
-        <v>46073.70646990741</v>
+        <v>46074.62326388889</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -8395,7 +8400,7 @@
         </is>
       </c>
       <c r="N122" s="3" t="n">
-        <v>46073.72890046296</v>
+        <v>46074.56532407407</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -8464,7 +8469,7 @@
         <v>2</v>
       </c>
       <c r="N123" s="3" t="n">
-        <v>46073.69956018519</v>
+        <v>46073.81395833333</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -8602,7 +8607,7 @@
         <v>1</v>
       </c>
       <c r="N125" s="3" t="n">
-        <v>46073.71335648148</v>
+        <v>46073.75414351852</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -8740,7 +8745,7 @@
         <v>2</v>
       </c>
       <c r="N127" s="3" t="n">
-        <v>46073.71240740741</v>
+        <v>46074.35770833334</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -9144,7 +9149,7 @@
         <v>1</v>
       </c>
       <c r="N133" s="3" t="n">
-        <v>46073.71950231482</v>
+        <v>46074.60693287037</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -9208,7 +9213,7 @@
         <v>1</v>
       </c>
       <c r="N134" s="3" t="n">
-        <v>46073.72908564815</v>
+        <v>46074.61475694444</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -9272,7 +9277,7 @@
         <v>1</v>
       </c>
       <c r="N135" s="3" t="n">
-        <v>46073.72878472223</v>
+        <v>46074.60179398148</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -9463,7 +9468,7 @@
         <v>1</v>
       </c>
       <c r="N138" s="3" t="n">
-        <v>46073.70126157408</v>
+        <v>46074.59217592593</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9527,7 +9532,7 @@
         <v>1</v>
       </c>
       <c r="N139" s="3" t="n">
-        <v>46073.73770833333</v>
+        <v>46074.59896990741</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9591,7 +9596,7 @@
         <v>1</v>
       </c>
       <c r="N140" s="3" t="n">
-        <v>46073.7246875</v>
+        <v>46074.60511574074</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9655,7 +9660,7 @@
         <v>1</v>
       </c>
       <c r="N141" s="3" t="n">
-        <v>46073.70212962963</v>
+        <v>46074.61393518518</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9719,7 +9724,7 @@
         <v>1</v>
       </c>
       <c r="N142" s="3" t="n">
-        <v>46073.71393518519</v>
+        <v>46074.60136574074</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9783,7 +9788,7 @@
         <v>1</v>
       </c>
       <c r="N143" s="3" t="n">
-        <v>46073.7059837963</v>
+        <v>46074.60040509259</v>
       </c>
       <c r="O143" t="inlineStr">
         <is>
@@ -9847,7 +9852,7 @@
         <v>1</v>
       </c>
       <c r="N144" s="3" t="n">
-        <v>46073.70085648148</v>
+        <v>46074.60400462963</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9911,7 +9916,7 @@
         <v>1</v>
       </c>
       <c r="N145" s="3" t="n">
-        <v>46073.70071759259</v>
+        <v>46074.59888888889</v>
       </c>
       <c r="O145" t="inlineStr">
         <is>
@@ -9975,7 +9980,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="3" t="n">
-        <v>46073.73335648148</v>
+        <v>46074.59736111111</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10039,7 +10044,7 @@
         <v>1</v>
       </c>
       <c r="N147" s="3" t="n">
-        <v>46073.71831018518</v>
+        <v>46074.59951388889</v>
       </c>
       <c r="O147" t="inlineStr">
         <is>
@@ -10103,7 +10108,7 @@
         <v>1</v>
       </c>
       <c r="N148" s="3" t="n">
-        <v>46073.72137731482</v>
+        <v>46074.5902662037</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10167,7 +10172,7 @@
         <v>1</v>
       </c>
       <c r="N149" s="3" t="n">
-        <v>46073.72304398148</v>
+        <v>46074.59215277778</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -10231,7 +10236,7 @@
         <v>1</v>
       </c>
       <c r="N150" s="3" t="n">
-        <v>46073.40594907408</v>
+        <v>46074.61709490741</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -10295,7 +10300,7 @@
         <v>1</v>
       </c>
       <c r="N151" s="3" t="n">
-        <v>46073.71430555556</v>
+        <v>46074.61783564815</v>
       </c>
       <c r="O151" t="inlineStr">
         <is>
@@ -10359,7 +10364,7 @@
         <v>1</v>
       </c>
       <c r="N152" s="3" t="n">
-        <v>46073.69875</v>
+        <v>46074.60386574074</v>
       </c>
       <c r="O152" t="inlineStr">
         <is>
@@ -10378,11 +10383,6 @@
           <t>OPERACAO 7.1</t>
         </is>
       </c>
-      <c r="C153" t="inlineStr">
-        <is>
-          <t>10.69.5.21</t>
-        </is>
-      </c>
       <c r="D153" t="n">
         <v>2018</v>
       </c>
@@ -10423,7 +10423,7 @@
         <v>1</v>
       </c>
       <c r="N153" s="3" t="n">
-        <v>46073.72969907407</v>
+        <v>46074.5840625</v>
       </c>
       <c r="O153" t="inlineStr">
         <is>
@@ -10487,7 +10487,7 @@
         <v>1</v>
       </c>
       <c r="N154" s="3" t="n">
-        <v>46073.70202546296</v>
+        <v>46076.31998842592</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10551,7 +10551,7 @@
         <v>1</v>
       </c>
       <c r="N155" s="3" t="n">
-        <v>46073.69869212963</v>
+        <v>46074.56212962963</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10615,7 +10615,7 @@
         <v>1</v>
       </c>
       <c r="N156" s="3" t="n">
-        <v>46073.56585648148</v>
+        <v>46074.41208333334</v>
       </c>
       <c r="O156" t="inlineStr">
         <is>
@@ -10679,7 +10679,7 @@
         <v>1</v>
       </c>
       <c r="N157" s="3" t="n">
-        <v>46073.73583333333</v>
+        <v>46074.59215277778</v>
       </c>
       <c r="O157" t="inlineStr">
         <is>
@@ -10743,7 +10743,7 @@
         <v>1</v>
       </c>
       <c r="N158" s="3" t="n">
-        <v>46073.57555555556</v>
+        <v>46074.61853009259</v>
       </c>
       <c r="O158" t="inlineStr">
         <is>
@@ -10807,7 +10807,7 @@
         <v>1</v>
       </c>
       <c r="N159" s="3" t="n">
-        <v>46073.72405092593</v>
+        <v>46074.37443287037</v>
       </c>
       <c r="O159" t="inlineStr">
         <is>
@@ -10871,7 +10871,7 @@
         <v>1</v>
       </c>
       <c r="N160" s="3" t="n">
-        <v>46073.57277777778</v>
+        <v>46074.5880787037</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
@@ -10935,7 +10935,7 @@
         <v>1</v>
       </c>
       <c r="N161" s="3" t="n">
-        <v>46073.57064814815</v>
+        <v>46074.84267361111</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -10999,7 +10999,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="3" t="n">
-        <v>46073.71219907407</v>
+        <v>46074.59388888889</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11124,10 +11124,10 @@
         </is>
       </c>
       <c r="M164" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N164" s="3" t="n">
-        <v>46073.70666666667</v>
+        <v>46076.28990740741</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11188,10 +11188,10 @@
         </is>
       </c>
       <c r="M165" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N165" s="3" t="n">
-        <v>46073.70420138889</v>
+        <v>46076.29327546297</v>
       </c>
       <c r="O165" t="inlineStr">
         <is>
@@ -11447,7 +11447,7 @@
         <v>2</v>
       </c>
       <c r="N169" s="3" t="n">
-        <v>46073.71071759259</v>
+        <v>46076.31556712963</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -11511,7 +11511,7 @@
         <v>2</v>
       </c>
       <c r="N170" s="3" t="n">
-        <v>46073.72961805556</v>
+        <v>46073.76934027778</v>
       </c>
       <c r="O170" t="inlineStr">
         <is>
@@ -11575,7 +11575,7 @@
         <v>1</v>
       </c>
       <c r="N171" s="3" t="n">
-        <v>46073.53583333334</v>
+        <v>46074.52553240741</v>
       </c>
       <c r="O171" t="inlineStr">
         <is>
@@ -11639,7 +11639,7 @@
         <v>2</v>
       </c>
       <c r="N172" s="3" t="n">
-        <v>46073.73344907408</v>
+        <v>46073.7734837963</v>
       </c>
       <c r="O172" t="inlineStr">
         <is>
@@ -11703,7 +11703,7 @@
         <v>2</v>
       </c>
       <c r="N173" s="3" t="n">
-        <v>46073.70238425926</v>
+        <v>46076.31501157407</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -11831,7 +11831,7 @@
         <v>2</v>
       </c>
       <c r="N175" s="3" t="n">
-        <v>46073.70326388889</v>
+        <v>46076.3034375</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -11895,7 +11895,7 @@
         <v>2</v>
       </c>
       <c r="N176" s="3" t="n">
-        <v>46073.64792824074</v>
+        <v>46074.52883101852</v>
       </c>
       <c r="O176" t="inlineStr">
         <is>
@@ -12023,7 +12023,7 @@
         <v>2</v>
       </c>
       <c r="N178" s="3" t="n">
-        <v>46073.70726851852</v>
+        <v>46076.28716435185</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12087,7 +12087,7 @@
         <v>1</v>
       </c>
       <c r="N179" s="3" t="n">
-        <v>46073.72288194444</v>
+        <v>46076.31368055556</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12151,7 +12151,7 @@
         <v>1</v>
       </c>
       <c r="N180" s="3" t="n">
-        <v>46073.73020833333</v>
+        <v>46076.30809027778</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12215,7 +12215,7 @@
         <v>1</v>
       </c>
       <c r="N181" s="3" t="n">
-        <v>46073.7256712963</v>
+        <v>46074.61596064815</v>
       </c>
       <c r="O181" t="inlineStr">
         <is>
@@ -12343,7 +12343,7 @@
         <v>1</v>
       </c>
       <c r="N183" s="3" t="n">
-        <v>46071.5514699074</v>
+        <v>46074.60883101852</v>
       </c>
       <c r="O183" t="inlineStr">
         <is>
@@ -12540,7 +12540,7 @@
         <v>1</v>
       </c>
       <c r="N186" s="3" t="n">
-        <v>46073.57961805556</v>
+        <v>46074.58528935185</v>
       </c>
       <c r="O186" t="inlineStr">
         <is>
@@ -12604,7 +12604,7 @@
         <v>1</v>
       </c>
       <c r="N187" s="3" t="n">
-        <v>46073.70072916667</v>
+        <v>46074.87423611111</v>
       </c>
       <c r="O187" t="inlineStr">
         <is>
@@ -12668,7 +12668,7 @@
         <v>1</v>
       </c>
       <c r="N188" s="3" t="n">
-        <v>46073.57087962963</v>
+        <v>46074.61282407407</v>
       </c>
       <c r="O188" t="inlineStr">
         <is>
@@ -12754,6 +12754,11 @@
           <t>OPERACAO 8.1</t>
         </is>
       </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>10.69.5.59</t>
+        </is>
+      </c>
       <c r="D190" t="n">
         <v>2015</v>
       </c>
@@ -12791,7 +12796,7 @@
         </is>
       </c>
       <c r="N190" s="3" t="n">
-        <v>46073.7015625</v>
+        <v>46074.60863425926</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12855,7 +12860,7 @@
         <v>1</v>
       </c>
       <c r="N191" s="3" t="n">
-        <v>46073.7328125</v>
+        <v>46074.61650462963</v>
       </c>
       <c r="O191" t="inlineStr">
         <is>
@@ -12919,7 +12924,7 @@
         <v>1</v>
       </c>
       <c r="N192" s="3" t="n">
-        <v>46073.70230324074</v>
+        <v>46074.60201388889</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -13044,7 +13049,7 @@
         <v>2</v>
       </c>
       <c r="N194" s="3" t="n">
-        <v>46073.69778935185</v>
+        <v>46076.20421296296</v>
       </c>
       <c r="O194" t="inlineStr">
         <is>
@@ -13108,7 +13113,7 @@
         <v>1</v>
       </c>
       <c r="N195" s="3" t="n">
-        <v>46073.69761574074</v>
+        <v>46074.61150462963</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13172,7 +13177,7 @@
         <v>1</v>
       </c>
       <c r="N196" s="3" t="n">
-        <v>46073.70025462963</v>
+        <v>46074.60332175926</v>
       </c>
       <c r="O196" t="inlineStr">
         <is>
@@ -13236,7 +13241,7 @@
         <v>1</v>
       </c>
       <c r="N197" s="3" t="n">
-        <v>46073.73730324074</v>
+        <v>46074.36774305555</v>
       </c>
       <c r="O197" t="inlineStr">
         <is>
@@ -13300,7 +13305,7 @@
         <v>1</v>
       </c>
       <c r="N198" s="3" t="n">
-        <v>46073.73479166667</v>
+        <v>46074.85094907408</v>
       </c>
       <c r="O198" t="inlineStr">
         <is>
@@ -13364,7 +13369,7 @@
         <v>1</v>
       </c>
       <c r="N199" s="3" t="n">
-        <v>46073.70560185185</v>
+        <v>46073.81803240741</v>
       </c>
       <c r="O199" t="inlineStr">
         <is>
@@ -13428,7 +13433,7 @@
         <v>1</v>
       </c>
       <c r="N200" s="3" t="n">
-        <v>46073.7127662037</v>
+        <v>46073.82743055555</v>
       </c>
       <c r="O200" t="inlineStr">
         <is>
@@ -13489,7 +13494,7 @@
         </is>
       </c>
       <c r="N201" s="3" t="n">
-        <v>46073.71769675926</v>
+        <v>46073.82716435185</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -13553,7 +13558,7 @@
         <v>1</v>
       </c>
       <c r="N202" s="3" t="n">
-        <v>46073.70153935185</v>
+        <v>46076.31222222222</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13617,7 +13622,7 @@
         <v>1</v>
       </c>
       <c r="N203" s="3" t="n">
-        <v>46073.72726851852</v>
+        <v>46076.29096064815</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13681,7 +13686,7 @@
         <v>1</v>
       </c>
       <c r="N204" s="3" t="n">
-        <v>46073.71761574074</v>
+        <v>46073.79753472222</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13745,7 +13750,7 @@
         <v>1</v>
       </c>
       <c r="N205" s="3" t="n">
-        <v>46073.71144675926</v>
+        <v>46074.61515046296</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13809,7 +13814,7 @@
         <v>1</v>
       </c>
       <c r="N206" s="3" t="n">
-        <v>46073.72695601852</v>
+        <v>46074.61296296296</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -13873,7 +13878,7 @@
         <v>1</v>
       </c>
       <c r="N207" s="3" t="n">
-        <v>46073.67253472222</v>
+        <v>46076.31108796296</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -13937,7 +13942,7 @@
         <v>1</v>
       </c>
       <c r="N208" s="3" t="n">
-        <v>46073.54111111111</v>
+        <v>46074.59482638889</v>
       </c>
       <c r="O208" t="inlineStr">
         <is>
@@ -14001,7 +14006,7 @@
         <v>1</v>
       </c>
       <c r="N209" s="3" t="n">
-        <v>46073.73738425926</v>
+        <v>46074.60290509259</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14065,7 +14070,7 @@
         <v>1</v>
       </c>
       <c r="N210" s="3" t="n">
-        <v>46073.72759259259</v>
+        <v>46074.8603125</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14129,7 +14134,7 @@
         <v>1</v>
       </c>
       <c r="N211" s="3" t="n">
-        <v>46073.70135416667</v>
+        <v>46074.58298611111</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -14193,7 +14198,7 @@
         <v>1</v>
       </c>
       <c r="N212" s="3" t="n">
-        <v>46073.70181712963</v>
+        <v>46074.59787037037</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -14257,7 +14262,7 @@
         <v>1</v>
       </c>
       <c r="N213" s="3" t="n">
-        <v>46073.73081018519</v>
+        <v>46074.59224537037</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
@@ -14321,7 +14326,7 @@
         <v>1</v>
       </c>
       <c r="N214" s="3" t="n">
-        <v>46073.71372685185</v>
+        <v>46074.58793981482</v>
       </c>
       <c r="O214" t="inlineStr">
         <is>
@@ -14385,7 +14390,7 @@
         <v>1</v>
       </c>
       <c r="N215" s="3" t="n">
-        <v>46073.70395833333</v>
+        <v>46074.59216435185</v>
       </c>
       <c r="O215" t="inlineStr">
         <is>
@@ -14449,7 +14454,7 @@
         <v>1</v>
       </c>
       <c r="N216" s="3" t="n">
-        <v>46073.71153935185</v>
+        <v>46074.59849537037</v>
       </c>
       <c r="O216" t="inlineStr">
         <is>
@@ -14468,6 +14473,11 @@
           <t>OPERACAO 8.1</t>
         </is>
       </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>10.69.5.85</t>
+        </is>
+      </c>
       <c r="D217" t="n">
         <v>2017</v>
       </c>
@@ -14508,7 +14518,7 @@
         <v>1</v>
       </c>
       <c r="N217" s="3" t="n">
-        <v>46073.70238425926</v>
+        <v>46074.59806712963</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14572,7 +14582,7 @@
         <v>1</v>
       </c>
       <c r="N218" s="3" t="n">
-        <v>46073.72780092592</v>
+        <v>46074.58684027778</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14636,7 +14646,7 @@
         <v>1</v>
       </c>
       <c r="N219" s="3" t="n">
-        <v>46073.67429398148</v>
+        <v>46074.61226851852</v>
       </c>
       <c r="O219" t="inlineStr">
         <is>
@@ -14705,7 +14715,7 @@
         <v>1</v>
       </c>
       <c r="N220" s="3" t="n">
-        <v>46073.70287037037</v>
+        <v>46074.62039351852</v>
       </c>
       <c r="O220" t="inlineStr">
         <is>
@@ -14769,7 +14779,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="3" t="n">
-        <v>46073.71880787037</v>
+        <v>46074.5980787037</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14833,7 +14843,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="3" t="n">
-        <v>46073.71142361111</v>
+        <v>46074.87258101852</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -14897,7 +14907,7 @@
         <v>1</v>
       </c>
       <c r="N223" s="3" t="n">
-        <v>46073.73364583333</v>
+        <v>46074.59097222222</v>
       </c>
       <c r="O223" t="inlineStr">
         <is>
@@ -14961,7 +14971,7 @@
         <v>1</v>
       </c>
       <c r="N224" s="3" t="n">
-        <v>46073.71427083333</v>
+        <v>46074.45204861111</v>
       </c>
       <c r="O224" t="inlineStr">
         <is>
@@ -15025,7 +15035,7 @@
         <v>1</v>
       </c>
       <c r="N225" s="3" t="n">
-        <v>46073.70865740741</v>
+        <v>46074.60195601852</v>
       </c>
       <c r="O225" t="inlineStr">
         <is>
@@ -15089,7 +15099,7 @@
         <v>1</v>
       </c>
       <c r="N226" s="3" t="n">
-        <v>46073.69674768519</v>
+        <v>46074.59061342593</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15153,7 +15163,7 @@
         <v>1</v>
       </c>
       <c r="N227" s="3" t="n">
-        <v>46073.7265625</v>
+        <v>46074.61186342593</v>
       </c>
       <c r="O227" t="inlineStr">
         <is>
@@ -15217,7 +15227,7 @@
         <v>1</v>
       </c>
       <c r="N228" s="3" t="n">
-        <v>46073.71868055555</v>
+        <v>46074.60641203704</v>
       </c>
       <c r="O228" t="inlineStr">
         <is>
@@ -15281,7 +15291,7 @@
         <v>1</v>
       </c>
       <c r="N229" s="3" t="n">
-        <v>46073.71759259259</v>
+        <v>46074.50202546296</v>
       </c>
       <c r="O229" t="inlineStr">
         <is>
@@ -15345,7 +15355,7 @@
         <v>1</v>
       </c>
       <c r="N230" s="3" t="n">
-        <v>46073.70017361111</v>
+        <v>46074.5630787037</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15409,7 +15419,7 @@
         <v>1</v>
       </c>
       <c r="N231" s="3" t="n">
-        <v>46073.7196875</v>
+        <v>46074.83606481482</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15473,7 +15483,7 @@
         <v>1</v>
       </c>
       <c r="N232" s="3" t="n">
-        <v>46073.69118055556</v>
+        <v>46074.36681712963</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -15537,7 +15547,7 @@
         <v>1</v>
       </c>
       <c r="N233" s="3" t="n">
-        <v>46073.73660879629</v>
+        <v>46074.48827546297</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15601,7 +15611,7 @@
         <v>1</v>
       </c>
       <c r="N234" s="3" t="n">
-        <v>46073.69894675926</v>
+        <v>46074.62008101852</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -15665,7 +15675,7 @@
         <v>1</v>
       </c>
       <c r="N235" s="3" t="n">
-        <v>46073.70006944444</v>
+        <v>46074.61873842592</v>
       </c>
       <c r="O235" t="inlineStr">
         <is>
@@ -15729,7 +15739,7 @@
         <v>1</v>
       </c>
       <c r="N236" s="3" t="n">
-        <v>46073.71017361111</v>
+        <v>46074.56008101852</v>
       </c>
       <c r="O236" t="inlineStr">
         <is>
@@ -15793,7 +15803,7 @@
         <v>1</v>
       </c>
       <c r="N237" s="3" t="n">
-        <v>46073.69726851852</v>
+        <v>46074.59880787037</v>
       </c>
       <c r="O237" t="inlineStr">
         <is>
@@ -15857,7 +15867,7 @@
         <v>1</v>
       </c>
       <c r="N238" s="3" t="n">
-        <v>46073.73618055556</v>
+        <v>46074.59366898148</v>
       </c>
       <c r="O238" t="inlineStr">
         <is>
@@ -15921,7 +15931,7 @@
         <v>1</v>
       </c>
       <c r="N239" s="3" t="n">
-        <v>46073.70643518519</v>
+        <v>46074.57987268519</v>
       </c>
       <c r="O239" t="inlineStr">
         <is>
@@ -15985,7 +15995,7 @@
         <v>1</v>
       </c>
       <c r="N240" s="3" t="n">
-        <v>46073.70074074074</v>
+        <v>46074.56337962963</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16049,7 +16059,7 @@
         <v>1</v>
       </c>
       <c r="N241" s="3" t="n">
-        <v>46073.70967592593</v>
+        <v>46073.7858449074</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16113,7 +16123,7 @@
         <v>1</v>
       </c>
       <c r="N242" s="3" t="n">
-        <v>46073.70518518519</v>
+        <v>46074.55965277777</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16177,7 +16187,7 @@
         <v>1</v>
       </c>
       <c r="N243" s="3" t="n">
-        <v>46073.73145833334</v>
+        <v>46073.81146990741</v>
       </c>
       <c r="O243" t="inlineStr">
         <is>
@@ -16236,7 +16246,7 @@
         <v>1</v>
       </c>
       <c r="N244" s="3" t="n">
-        <v>46073.40925925926</v>
+        <v>46076.20893518518</v>
       </c>
       <c r="O244" t="inlineStr">
         <is>
@@ -16300,7 +16310,7 @@
         <v>1</v>
       </c>
       <c r="N245" s="3" t="n">
-        <v>46073.70581018519</v>
+        <v>46076.31284722222</v>
       </c>
       <c r="O245" t="inlineStr">
         <is>
@@ -16364,7 +16374,7 @@
         <v>1</v>
       </c>
       <c r="N246" s="3" t="n">
-        <v>46073.7302662037</v>
+        <v>46076.31244212963</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16428,7 +16438,7 @@
         <v>1</v>
       </c>
       <c r="N247" s="3" t="n">
-        <v>46073.55517361111</v>
+        <v>46076.31219907408</v>
       </c>
       <c r="O247" t="inlineStr">
         <is>
@@ -16492,7 +16502,7 @@
         <v>1</v>
       </c>
       <c r="N248" s="3" t="n">
-        <v>46073.70858796296</v>
+        <v>46076.3121875</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16556,7 +16566,7 @@
         <v>1</v>
       </c>
       <c r="N249" s="3" t="n">
-        <v>46073.70457175926</v>
+        <v>46076.31995370371</v>
       </c>
       <c r="O249" t="inlineStr">
         <is>
@@ -16620,7 +16630,7 @@
         <v>1</v>
       </c>
       <c r="N250" s="3" t="n">
-        <v>46073.71510416667</v>
+        <v>46076.31877314814</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16684,7 +16694,7 @@
         <v>1</v>
       </c>
       <c r="N251" s="3" t="n">
-        <v>46073.70314814815</v>
+        <v>46076.31210648148</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16748,7 +16758,7 @@
         <v>1</v>
       </c>
       <c r="N252" s="3" t="n">
-        <v>46073.71115740741</v>
+        <v>46076.31225694445</v>
       </c>
       <c r="O252" t="inlineStr">
         <is>
@@ -16812,7 +16822,7 @@
         <v>1</v>
       </c>
       <c r="N253" s="3" t="n">
-        <v>46073.70133101852</v>
+        <v>46074.58370370371</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16870,7 +16880,7 @@
         <v>1</v>
       </c>
       <c r="N254" s="3" t="n">
-        <v>46073.70997685185</v>
+        <v>46074.61710648148</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -16934,7 +16944,7 @@
         <v>1</v>
       </c>
       <c r="N255" s="3" t="n">
-        <v>46073.70814814815</v>
+        <v>46074.61524305555</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -16998,7 +17008,7 @@
         <v>1</v>
       </c>
       <c r="N256" s="3" t="n">
-        <v>46073.71556712963</v>
+        <v>46074.59122685185</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17062,7 +17072,7 @@
         <v>1</v>
       </c>
       <c r="N257" s="3" t="n">
-        <v>46073.72362268518</v>
+        <v>46074.59708333333</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17126,7 +17136,7 @@
         <v>1</v>
       </c>
       <c r="N258" s="3" t="n">
-        <v>46073.72253472222</v>
+        <v>46074.60739583334</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
@@ -17190,7 +17200,7 @@
         <v>1</v>
       </c>
       <c r="N259" s="3" t="n">
-        <v>46073.72872685185</v>
+        <v>46074.45996527778</v>
       </c>
       <c r="O259" t="inlineStr">
         <is>
@@ -17254,7 +17264,7 @@
         <v>1</v>
       </c>
       <c r="N260" s="3" t="n">
-        <v>46073.70597222223</v>
+        <v>46076.28324074074</v>
       </c>
       <c r="O260" t="inlineStr">
         <is>
@@ -17318,7 +17328,7 @@
         <v>1</v>
       </c>
       <c r="N261" s="3" t="n">
-        <v>46073.56637731481</v>
+        <v>46074.6368287037</v>
       </c>
       <c r="O261" t="inlineStr">
         <is>
@@ -17382,7 +17392,7 @@
         <v>1</v>
       </c>
       <c r="N262" s="3" t="n">
-        <v>46073.54030092592</v>
+        <v>46074.59364583333</v>
       </c>
       <c r="O262" t="inlineStr">
         <is>
@@ -17446,7 +17456,7 @@
         <v>1</v>
       </c>
       <c r="N263" s="3" t="n">
-        <v>46073.71864583333</v>
+        <v>46076.31122685185</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17510,7 +17520,7 @@
         <v>1</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>46073.72684027778</v>
+        <v>46074.51443287037</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17574,7 +17584,7 @@
         <v>1</v>
       </c>
       <c r="N265" s="3" t="n">
-        <v>46073.73547453704</v>
+        <v>46074.58900462963</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17638,7 +17648,7 @@
         <v>1</v>
       </c>
       <c r="N266" s="3" t="n">
-        <v>46073.73516203704</v>
+        <v>46074.3731712963</v>
       </c>
       <c r="O266" t="inlineStr">
         <is>
@@ -17702,7 +17712,7 @@
         <v>1</v>
       </c>
       <c r="N267" s="3" t="n">
-        <v>46073.71178240741</v>
+        <v>46074.60369212963</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17766,7 +17776,7 @@
         <v>1</v>
       </c>
       <c r="N268" s="3" t="n">
-        <v>46073.72796296296</v>
+        <v>46074.57481481481</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17830,7 +17840,7 @@
         <v>1</v>
       </c>
       <c r="N269" s="3" t="n">
-        <v>46073.72123842593</v>
+        <v>46074.58395833334</v>
       </c>
       <c r="O269" t="inlineStr">
         <is>
@@ -17891,7 +17901,7 @@
         </is>
       </c>
       <c r="N270" s="3" t="n">
-        <v>46073.71422453703</v>
+        <v>46076.30293981481</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -17955,7 +17965,7 @@
         <v>1</v>
       </c>
       <c r="N271" s="3" t="n">
-        <v>46073.45253472222</v>
+        <v>46074.45915509259</v>
       </c>
       <c r="O271" t="inlineStr">
         <is>
@@ -18019,7 +18029,7 @@
         <v>1</v>
       </c>
       <c r="N272" s="3" t="n">
-        <v>46073.6574537037</v>
+        <v>46074.60545138889</v>
       </c>
       <c r="O272" t="inlineStr">
         <is>
@@ -18083,7 +18093,7 @@
         <v>2</v>
       </c>
       <c r="N273" s="3" t="n">
-        <v>46073.66003472222</v>
+        <v>46076.29390046297</v>
       </c>
       <c r="O273" t="inlineStr">
         <is>
@@ -18403,7 +18413,7 @@
         <v>1</v>
       </c>
       <c r="N278" s="3" t="n">
-        <v>46073.72538194444</v>
+        <v>46074.52625</v>
       </c>
       <c r="O278" t="inlineStr">
         <is>
@@ -18467,7 +18477,7 @@
         <v>1</v>
       </c>
       <c r="N279" s="3" t="n">
-        <v>46073.54751157408</v>
+        <v>46076.31510416666</v>
       </c>
       <c r="O279" t="inlineStr">
         <is>
@@ -18531,7 +18541,7 @@
         <v>1</v>
       </c>
       <c r="N280" s="3" t="n">
-        <v>46073.70400462963</v>
+        <v>46074.59521990741</v>
       </c>
       <c r="O280" t="inlineStr">
         <is>
@@ -18595,7 +18605,7 @@
         <v>1</v>
       </c>
       <c r="N281" s="3" t="n">
-        <v>46073.71434027778</v>
+        <v>46076.31453703704</v>
       </c>
       <c r="O281" t="inlineStr">
         <is>
@@ -18654,7 +18664,7 @@
         <v>1</v>
       </c>
       <c r="N282" s="3" t="n">
-        <v>46073.55273148148</v>
+        <v>46074.43244212963</v>
       </c>
       <c r="O282" t="inlineStr">
         <is>
@@ -18718,7 +18728,7 @@
         <v>1</v>
       </c>
       <c r="N283" s="3" t="n">
-        <v>46073.70460648148</v>
+        <v>46073.82201388889</v>
       </c>
       <c r="O283" t="inlineStr">
         <is>
@@ -18782,7 +18792,7 @@
         <v>1</v>
       </c>
       <c r="N284" s="3" t="n">
-        <v>46073.71934027778</v>
+        <v>46074.45539351852</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18846,7 +18856,7 @@
         <v>1</v>
       </c>
       <c r="N285" s="3" t="n">
-        <v>46073.70583333333</v>
+        <v>46074.45655092593</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -18910,7 +18920,7 @@
         <v>1</v>
       </c>
       <c r="N286" s="3" t="n">
-        <v>46073.50994212963</v>
+        <v>46076.29733796296</v>
       </c>
       <c r="O286" t="inlineStr">
         <is>
@@ -18974,7 +18984,7 @@
         <v>1</v>
       </c>
       <c r="N287" s="3" t="n">
-        <v>46073.704375</v>
+        <v>46074.46532407407</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
@@ -19038,7 +19048,7 @@
         <v>1</v>
       </c>
       <c r="N288" s="3" t="n">
-        <v>46073.5425</v>
+        <v>46076.31679398148</v>
       </c>
       <c r="O288" t="inlineStr">
         <is>
@@ -19102,7 +19112,7 @@
         <v>1</v>
       </c>
       <c r="N289" s="3" t="n">
-        <v>46073.73370370371</v>
+        <v>46076.30862268519</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -19896,7 +19906,7 @@
         <v>1</v>
       </c>
       <c r="N302" s="3" t="n">
-        <v>46073.7112037037</v>
+        <v>46076.31034722222</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -21012,7 +21022,7 @@
         </is>
       </c>
       <c r="N320" s="3" t="n">
-        <v>46073.71248842592</v>
+        <v>46076.30619212963</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21737,7 +21747,7 @@
         <v>1</v>
       </c>
       <c r="N332" s="3" t="n">
-        <v>46073.73409722222</v>
+        <v>46074.53166666667</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21801,7 +21811,7 @@
         <v>2</v>
       </c>
       <c r="N333" s="3" t="n">
-        <v>46073.69988425926</v>
+        <v>46076.28776620371</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21865,7 +21875,7 @@
         <v>2</v>
       </c>
       <c r="N334" s="3" t="n">
-        <v>46073.73532407408</v>
+        <v>46076.28846064815</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21929,7 +21939,7 @@
         <v>2</v>
       </c>
       <c r="N335" s="3" t="n">
-        <v>46073.70690972222</v>
+        <v>46076.28802083333</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -21993,7 +22003,7 @@
         <v>1</v>
       </c>
       <c r="N336" s="3" t="n">
-        <v>46073.73548611111</v>
+        <v>46076.3095949074</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22057,7 +22067,7 @@
         <v>1</v>
       </c>
       <c r="N337" s="3" t="n">
-        <v>46073.71641203704</v>
+        <v>46076.2881712963</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22121,7 +22131,7 @@
         <v>2</v>
       </c>
       <c r="N338" s="3" t="n">
-        <v>46073.70998842592</v>
+        <v>46074.50121527778</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -22249,7 +22259,7 @@
         <v>1</v>
       </c>
       <c r="N340" s="3" t="n">
-        <v>46073.71038194445</v>
+        <v>46073.83497685185</v>
       </c>
       <c r="O340" t="inlineStr">
         <is>
@@ -22841,11 +22851,6 @@
           <t>OPERACAO 9.1</t>
         </is>
       </c>
-      <c r="C350" t="inlineStr">
-        <is>
-          <t>10.69.5.244</t>
-        </is>
-      </c>
       <c r="D350" t="n">
         <v>2014</v>
       </c>
@@ -22886,7 +22891,7 @@
         <v>1</v>
       </c>
       <c r="N350" s="3" t="n">
-        <v>46073.70173611111</v>
+        <v>46073.8572337963</v>
       </c>
       <c r="O350" t="inlineStr">
         <is>
@@ -23894,7 +23899,7 @@
         </is>
       </c>
       <c r="N366" s="3" t="n">
-        <v>46073.72146990741</v>
+        <v>46076.29938657407</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -24039,11 +24044,6 @@
           <t>RH</t>
         </is>
       </c>
-      <c r="C369" t="inlineStr">
-        <is>
-          <t>10.69.3.13</t>
-        </is>
-      </c>
       <c r="D369" t="n">
         <v>2025</v>
       </c>
@@ -24155,7 +24155,7 @@
         <v>1</v>
       </c>
       <c r="N370" s="3" t="n">
-        <v>46073.70724537037</v>
+        <v>46073.74658564815</v>
       </c>
       <c r="O370" t="inlineStr">
         <is>
@@ -24431,7 +24431,7 @@
         <v>1</v>
       </c>
       <c r="N374" s="3" t="n">
-        <v>46073.72709490741</v>
+        <v>46073.76869212963</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24497,7 +24497,7 @@
         </is>
       </c>
       <c r="N375" s="3" t="n">
-        <v>46073.72311342593</v>
+        <v>46076.28959490741</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
@@ -24561,7 +24561,7 @@
         <v>1</v>
       </c>
       <c r="N376" s="3" t="n">
-        <v>46073.71952546296</v>
+        <v>46074.36466435185</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -24630,7 +24630,7 @@
         <v>2</v>
       </c>
       <c r="N377" s="3" t="n">
-        <v>46073.69086805556</v>
+        <v>46074.47112268519</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -24699,7 +24699,7 @@
         <v>2</v>
       </c>
       <c r="N378" s="3" t="n">
-        <v>46073.73082175926</v>
+        <v>46076.28778935185</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização automática 2026-02-23 09:52:04.850511
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>46076.30568287037</v>
+        <v>46076.38034722222</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>46076.30667824074</v>
+        <v>46076.37806712963</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -739,10 +739,10 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>46073.6917824074</v>
+        <v>46076.39019675926</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>46073.73434027778</v>
+        <v>46076.38290509259</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -1131,7 +1131,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="3" t="n">
-        <v>46076.2999537037</v>
+        <v>46076.38372685185</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1451,7 +1451,7 @@
         <v>1</v>
       </c>
       <c r="N15" s="3" t="n">
-        <v>46076.30304398148</v>
+        <v>46076.38152777778</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1515,7 +1515,7 @@
         <v>2</v>
       </c>
       <c r="N16" s="3" t="n">
-        <v>46076.30726851852</v>
+        <v>46076.38643518519</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -6570,7 +6570,7 @@
         <v>1</v>
       </c>
       <c r="N95" s="3" t="n">
-        <v>46073.69754629629</v>
+        <v>46076.40098379629</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -6708,7 +6708,7 @@
         <v>1</v>
       </c>
       <c r="N97" s="3" t="n">
-        <v>46074.6058912037</v>
+        <v>46076.40021990741</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -6910,7 +6910,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>46076.29877314815</v>
+        <v>46076.38107638889</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6979,7 +6979,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="3" t="n">
-        <v>46075.06710648148</v>
+        <v>46076.37842592593</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -7117,7 +7117,7 @@
         <v>2</v>
       </c>
       <c r="N103" s="3" t="n">
-        <v>46076.30193287037</v>
+        <v>46076.38101851852</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7512,7 +7512,7 @@
         <v>1</v>
       </c>
       <c r="N109" s="3" t="n">
-        <v>46076.30444444445</v>
+        <v>46076.38048611111</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7581,7 +7581,7 @@
         <v>2</v>
       </c>
       <c r="N110" s="3" t="n">
-        <v>46076.30501157408</v>
+        <v>46076.38604166666</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7650,7 +7650,7 @@
         <v>2</v>
       </c>
       <c r="N111" s="3" t="n">
-        <v>46073.71922453704</v>
+        <v>46076.3693287037</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
@@ -7719,7 +7719,7 @@
         <v>2</v>
       </c>
       <c r="N112" s="3" t="n">
-        <v>46076.31232638889</v>
+        <v>46076.39040509259</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7788,7 +7788,7 @@
         <v>1</v>
       </c>
       <c r="N113" s="3" t="n">
-        <v>46076.30126157407</v>
+        <v>46076.3799537037</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7857,7 +7857,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>46076.30136574074</v>
+        <v>46076.38144675926</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -7923,7 +7923,7 @@
         </is>
       </c>
       <c r="N115" s="3" t="n">
-        <v>46073.75619212963</v>
+        <v>46076.3722337963</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -7992,7 +7992,7 @@
         <v>1</v>
       </c>
       <c r="N116" s="3" t="n">
-        <v>46073.70998842592</v>
+        <v>46076.37649305556</v>
       </c>
       <c r="O116" t="inlineStr">
         <is>
@@ -8061,7 +8061,7 @@
         <v>1</v>
       </c>
       <c r="N117" s="3" t="n">
-        <v>46076.31689814815</v>
+        <v>46076.39670138889</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -8265,7 +8265,7 @@
         <v>1</v>
       </c>
       <c r="N120" s="3" t="n">
-        <v>46073.73755787037</v>
+        <v>46076.39</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -8400,7 +8400,7 @@
         </is>
       </c>
       <c r="N122" s="3" t="n">
-        <v>46074.56532407407</v>
+        <v>46076.36479166667</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -8469,7 +8469,7 @@
         <v>2</v>
       </c>
       <c r="N123" s="3" t="n">
-        <v>46073.81395833333</v>
+        <v>46076.36074074074</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -8538,7 +8538,7 @@
         <v>1</v>
       </c>
       <c r="N124" s="3" t="n">
-        <v>46073.72692129629</v>
+        <v>46076.3865625</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -8607,7 +8607,7 @@
         <v>1</v>
       </c>
       <c r="N125" s="3" t="n">
-        <v>46073.75414351852</v>
+        <v>46076.36550925926</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -8745,7 +8745,7 @@
         <v>2</v>
       </c>
       <c r="N127" s="3" t="n">
-        <v>46074.35770833334</v>
+        <v>46076.40200231481</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -8814,7 +8814,7 @@
         <v>1</v>
       </c>
       <c r="N128" s="3" t="n">
-        <v>46073.68280092593</v>
+        <v>46076.36589120371</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -8883,7 +8883,7 @@
         <v>1</v>
       </c>
       <c r="N129" s="3" t="n">
-        <v>46073.70827546297</v>
+        <v>46076.39400462963</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -8952,7 +8952,7 @@
         <v>1</v>
       </c>
       <c r="N130" s="3" t="n">
-        <v>46073.67806712963</v>
+        <v>46076.37075231481</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -9016,7 +9016,7 @@
         <v>1</v>
       </c>
       <c r="N131" s="3" t="n">
-        <v>46073.71293981482</v>
+        <v>46076.38774305556</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -9149,7 +9149,7 @@
         <v>1</v>
       </c>
       <c r="N133" s="3" t="n">
-        <v>46074.60693287037</v>
+        <v>46076.38026620371</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -9213,7 +9213,7 @@
         <v>1</v>
       </c>
       <c r="N134" s="3" t="n">
-        <v>46074.61475694444</v>
+        <v>46076.37180555556</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -9277,7 +9277,7 @@
         <v>1</v>
       </c>
       <c r="N135" s="3" t="n">
-        <v>46074.60179398148</v>
+        <v>46076.36795138889</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -9468,7 +9468,7 @@
         <v>1</v>
       </c>
       <c r="N138" s="3" t="n">
-        <v>46074.59217592593</v>
+        <v>46076.38017361111</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9532,7 +9532,7 @@
         <v>1</v>
       </c>
       <c r="N139" s="3" t="n">
-        <v>46074.59896990741</v>
+        <v>46076.39362268519</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9596,7 +9596,7 @@
         <v>1</v>
       </c>
       <c r="N140" s="3" t="n">
-        <v>46074.60511574074</v>
+        <v>46076.38131944444</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9660,7 +9660,7 @@
         <v>1</v>
       </c>
       <c r="N141" s="3" t="n">
-        <v>46074.61393518518</v>
+        <v>46076.38077546296</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9724,7 +9724,7 @@
         <v>1</v>
       </c>
       <c r="N142" s="3" t="n">
-        <v>46074.60136574074</v>
+        <v>46076.3705787037</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9788,7 +9788,7 @@
         <v>1</v>
       </c>
       <c r="N143" s="3" t="n">
-        <v>46074.60040509259</v>
+        <v>46076.37773148148</v>
       </c>
       <c r="O143" t="inlineStr">
         <is>
@@ -9852,7 +9852,7 @@
         <v>1</v>
       </c>
       <c r="N144" s="3" t="n">
-        <v>46074.60400462963</v>
+        <v>46076.38502314815</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9980,7 +9980,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="3" t="n">
-        <v>46074.59736111111</v>
+        <v>46076.37024305556</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10044,7 +10044,7 @@
         <v>1</v>
       </c>
       <c r="N147" s="3" t="n">
-        <v>46074.59951388889</v>
+        <v>46076.36665509259</v>
       </c>
       <c r="O147" t="inlineStr">
         <is>
@@ -10108,7 +10108,7 @@
         <v>1</v>
       </c>
       <c r="N148" s="3" t="n">
-        <v>46074.5902662037</v>
+        <v>46076.37935185185</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10172,7 +10172,7 @@
         <v>1</v>
       </c>
       <c r="N149" s="3" t="n">
-        <v>46074.59215277778</v>
+        <v>46076.40175925926</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -10236,7 +10236,7 @@
         <v>1</v>
       </c>
       <c r="N150" s="3" t="n">
-        <v>46074.61709490741</v>
+        <v>46076.37167824074</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -10364,7 +10364,7 @@
         <v>1</v>
       </c>
       <c r="N152" s="3" t="n">
-        <v>46074.60386574074</v>
+        <v>46076.39314814815</v>
       </c>
       <c r="O152" t="inlineStr">
         <is>
@@ -10383,6 +10383,11 @@
           <t>OPERACAO 7.1</t>
         </is>
       </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>10.69.5.21</t>
+        </is>
+      </c>
       <c r="D153" t="n">
         <v>2018</v>
       </c>
@@ -10423,7 +10428,7 @@
         <v>1</v>
       </c>
       <c r="N153" s="3" t="n">
-        <v>46074.5840625</v>
+        <v>46076.37305555555</v>
       </c>
       <c r="O153" t="inlineStr">
         <is>
@@ -10487,7 +10492,7 @@
         <v>1</v>
       </c>
       <c r="N154" s="3" t="n">
-        <v>46076.31998842592</v>
+        <v>46076.40310185185</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10551,7 +10556,7 @@
         <v>1</v>
       </c>
       <c r="N155" s="3" t="n">
-        <v>46074.56212962963</v>
+        <v>46076.39966435185</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10679,7 +10684,7 @@
         <v>1</v>
       </c>
       <c r="N157" s="3" t="n">
-        <v>46074.59215277778</v>
+        <v>46076.38680555556</v>
       </c>
       <c r="O157" t="inlineStr">
         <is>
@@ -10743,7 +10748,7 @@
         <v>1</v>
       </c>
       <c r="N158" s="3" t="n">
-        <v>46074.61853009259</v>
+        <v>46076.39215277778</v>
       </c>
       <c r="O158" t="inlineStr">
         <is>
@@ -10807,7 +10812,7 @@
         <v>1</v>
       </c>
       <c r="N159" s="3" t="n">
-        <v>46074.37443287037</v>
+        <v>46076.36890046296</v>
       </c>
       <c r="O159" t="inlineStr">
         <is>
@@ -10871,7 +10876,7 @@
         <v>1</v>
       </c>
       <c r="N160" s="3" t="n">
-        <v>46074.5880787037</v>
+        <v>46076.37993055556</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
@@ -10935,7 +10940,7 @@
         <v>1</v>
       </c>
       <c r="N161" s="3" t="n">
-        <v>46074.84267361111</v>
+        <v>46076.3659837963</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -10999,7 +11004,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="3" t="n">
-        <v>46074.59388888889</v>
+        <v>46076.36725694445</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11124,10 +11129,10 @@
         </is>
       </c>
       <c r="M164" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N164" s="3" t="n">
-        <v>46076.28990740741</v>
+        <v>46076.37123842593</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11188,10 +11193,10 @@
         </is>
       </c>
       <c r="M165" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N165" s="3" t="n">
-        <v>46076.29327546297</v>
+        <v>46076.36981481482</v>
       </c>
       <c r="O165" t="inlineStr">
         <is>
@@ -11255,7 +11260,7 @@
         <v>2</v>
       </c>
       <c r="N166" s="3" t="n">
-        <v>46073.61207175926</v>
+        <v>46076.3833912037</v>
       </c>
       <c r="O166" t="inlineStr">
         <is>
@@ -11319,7 +11324,7 @@
         <v>2</v>
       </c>
       <c r="N167" s="3" t="n">
-        <v>46073.60625</v>
+        <v>46076.40356481481</v>
       </c>
       <c r="O167" t="inlineStr">
         <is>
@@ -11383,7 +11388,7 @@
         <v>2</v>
       </c>
       <c r="N168" s="3" t="n">
-        <v>46073.56337962963</v>
+        <v>46076.39761574074</v>
       </c>
       <c r="O168" t="inlineStr">
         <is>
@@ -11447,7 +11452,7 @@
         <v>2</v>
       </c>
       <c r="N169" s="3" t="n">
-        <v>46076.31556712963</v>
+        <v>46076.39270833333</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -11511,7 +11516,7 @@
         <v>2</v>
       </c>
       <c r="N170" s="3" t="n">
-        <v>46073.76934027778</v>
+        <v>46076.38333333333</v>
       </c>
       <c r="O170" t="inlineStr">
         <is>
@@ -11575,7 +11580,7 @@
         <v>1</v>
       </c>
       <c r="N171" s="3" t="n">
-        <v>46074.52553240741</v>
+        <v>46076.37311342593</v>
       </c>
       <c r="O171" t="inlineStr">
         <is>
@@ -11703,7 +11708,7 @@
         <v>2</v>
       </c>
       <c r="N173" s="3" t="n">
-        <v>46076.31501157407</v>
+        <v>46076.39061342592</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -11767,7 +11772,7 @@
         <v>2</v>
       </c>
       <c r="N174" s="3" t="n">
-        <v>46073.57134259259</v>
+        <v>46076.37344907408</v>
       </c>
       <c r="O174" t="inlineStr">
         <is>
@@ -11831,7 +11836,7 @@
         <v>2</v>
       </c>
       <c r="N175" s="3" t="n">
-        <v>46076.3034375</v>
+        <v>46076.37965277778</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -12023,7 +12028,7 @@
         <v>2</v>
       </c>
       <c r="N178" s="3" t="n">
-        <v>46076.28716435185</v>
+        <v>46076.40226851852</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12087,7 +12092,7 @@
         <v>1</v>
       </c>
       <c r="N179" s="3" t="n">
-        <v>46076.31368055556</v>
+        <v>46076.39179398148</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12151,7 +12156,7 @@
         <v>1</v>
       </c>
       <c r="N180" s="3" t="n">
-        <v>46076.30809027778</v>
+        <v>46076.38414351852</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12215,7 +12220,7 @@
         <v>1</v>
       </c>
       <c r="N181" s="3" t="n">
-        <v>46074.61596064815</v>
+        <v>46076.3746875</v>
       </c>
       <c r="O181" t="inlineStr">
         <is>
@@ -12412,7 +12417,7 @@
         <v>2</v>
       </c>
       <c r="N184" s="3" t="n">
-        <v>46072.81322916667</v>
+        <v>46076.37796296296</v>
       </c>
       <c r="O184" t="inlineStr">
         <is>
@@ -12540,7 +12545,7 @@
         <v>1</v>
       </c>
       <c r="N186" s="3" t="n">
-        <v>46074.58528935185</v>
+        <v>46076.39076388889</v>
       </c>
       <c r="O186" t="inlineStr">
         <is>
@@ -12604,7 +12609,7 @@
         <v>1</v>
       </c>
       <c r="N187" s="3" t="n">
-        <v>46074.87423611111</v>
+        <v>46076.39106481482</v>
       </c>
       <c r="O187" t="inlineStr">
         <is>
@@ -12668,7 +12673,7 @@
         <v>1</v>
       </c>
       <c r="N188" s="3" t="n">
-        <v>46074.61282407407</v>
+        <v>46076.38618055556</v>
       </c>
       <c r="O188" t="inlineStr">
         <is>
@@ -12796,7 +12801,7 @@
         </is>
       </c>
       <c r="N190" s="3" t="n">
-        <v>46074.60863425926</v>
+        <v>46076.4005787037</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12924,7 +12929,7 @@
         <v>1</v>
       </c>
       <c r="N192" s="3" t="n">
-        <v>46074.60201388889</v>
+        <v>46076.37759259259</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -13049,7 +13054,7 @@
         <v>2</v>
       </c>
       <c r="N194" s="3" t="n">
-        <v>46076.20421296296</v>
+        <v>46076.37033564815</v>
       </c>
       <c r="O194" t="inlineStr">
         <is>
@@ -13113,7 +13118,7 @@
         <v>1</v>
       </c>
       <c r="N195" s="3" t="n">
-        <v>46074.61150462963</v>
+        <v>46076.38150462963</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13177,7 +13182,7 @@
         <v>1</v>
       </c>
       <c r="N196" s="3" t="n">
-        <v>46074.60332175926</v>
+        <v>46076.39996527778</v>
       </c>
       <c r="O196" t="inlineStr">
         <is>
@@ -13241,7 +13246,7 @@
         <v>1</v>
       </c>
       <c r="N197" s="3" t="n">
-        <v>46074.36774305555</v>
+        <v>46076.4031712963</v>
       </c>
       <c r="O197" t="inlineStr">
         <is>
@@ -13369,7 +13374,7 @@
         <v>1</v>
       </c>
       <c r="N199" s="3" t="n">
-        <v>46073.81803240741</v>
+        <v>46076.37359953704</v>
       </c>
       <c r="O199" t="inlineStr">
         <is>
@@ -13494,7 +13499,7 @@
         </is>
       </c>
       <c r="N201" s="3" t="n">
-        <v>46073.82716435185</v>
+        <v>46076.38903935185</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -13558,7 +13563,7 @@
         <v>1</v>
       </c>
       <c r="N202" s="3" t="n">
-        <v>46076.31222222222</v>
+        <v>46076.38815972222</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13622,7 +13627,7 @@
         <v>1</v>
       </c>
       <c r="N203" s="3" t="n">
-        <v>46076.29096064815</v>
+        <v>46076.38886574074</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13686,7 +13691,7 @@
         <v>1</v>
       </c>
       <c r="N204" s="3" t="n">
-        <v>46073.79753472222</v>
+        <v>46076.38868055555</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13750,7 +13755,7 @@
         <v>1</v>
       </c>
       <c r="N205" s="3" t="n">
-        <v>46074.61515046296</v>
+        <v>46076.37418981481</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13814,7 +13819,7 @@
         <v>1</v>
       </c>
       <c r="N206" s="3" t="n">
-        <v>46074.61296296296</v>
+        <v>46076.39998842592</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -13878,7 +13883,7 @@
         <v>1</v>
       </c>
       <c r="N207" s="3" t="n">
-        <v>46076.31108796296</v>
+        <v>46076.37501157408</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -13942,7 +13947,7 @@
         <v>1</v>
       </c>
       <c r="N208" s="3" t="n">
-        <v>46074.59482638889</v>
+        <v>46076.40399305556</v>
       </c>
       <c r="O208" t="inlineStr">
         <is>
@@ -14006,7 +14011,7 @@
         <v>1</v>
       </c>
       <c r="N209" s="3" t="n">
-        <v>46074.60290509259</v>
+        <v>46076.39859953704</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14070,7 +14075,7 @@
         <v>1</v>
       </c>
       <c r="N210" s="3" t="n">
-        <v>46074.8603125</v>
+        <v>46076.37467592592</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14134,7 +14139,7 @@
         <v>1</v>
       </c>
       <c r="N211" s="3" t="n">
-        <v>46074.58298611111</v>
+        <v>46076.39630787037</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -14198,7 +14203,7 @@
         <v>1</v>
       </c>
       <c r="N212" s="3" t="n">
-        <v>46074.59787037037</v>
+        <v>46076.40035879629</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -14262,7 +14267,7 @@
         <v>1</v>
       </c>
       <c r="N213" s="3" t="n">
-        <v>46074.59224537037</v>
+        <v>46076.37253472222</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
@@ -14390,7 +14395,7 @@
         <v>1</v>
       </c>
       <c r="N215" s="3" t="n">
-        <v>46074.59216435185</v>
+        <v>46076.40260416667</v>
       </c>
       <c r="O215" t="inlineStr">
         <is>
@@ -14454,7 +14459,7 @@
         <v>1</v>
       </c>
       <c r="N216" s="3" t="n">
-        <v>46074.59849537037</v>
+        <v>46076.40200231481</v>
       </c>
       <c r="O216" t="inlineStr">
         <is>
@@ -14473,11 +14478,6 @@
           <t>OPERACAO 8.1</t>
         </is>
       </c>
-      <c r="C217" t="inlineStr">
-        <is>
-          <t>10.69.5.85</t>
-        </is>
-      </c>
       <c r="D217" t="n">
         <v>2017</v>
       </c>
@@ -14518,7 +14518,7 @@
         <v>1</v>
       </c>
       <c r="N217" s="3" t="n">
-        <v>46074.59806712963</v>
+        <v>46076.36678240741</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14582,7 +14582,7 @@
         <v>1</v>
       </c>
       <c r="N218" s="3" t="n">
-        <v>46074.58684027778</v>
+        <v>46076.36545138889</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14646,7 +14646,7 @@
         <v>1</v>
       </c>
       <c r="N219" s="3" t="n">
-        <v>46074.61226851852</v>
+        <v>46076.36848379629</v>
       </c>
       <c r="O219" t="inlineStr">
         <is>
@@ -14715,7 +14715,7 @@
         <v>1</v>
       </c>
       <c r="N220" s="3" t="n">
-        <v>46074.62039351852</v>
+        <v>46076.38965277778</v>
       </c>
       <c r="O220" t="inlineStr">
         <is>
@@ -14779,7 +14779,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="3" t="n">
-        <v>46074.5980787037</v>
+        <v>46076.37829861111</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14843,7 +14843,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="3" t="n">
-        <v>46074.87258101852</v>
+        <v>46076.39465277778</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -14907,7 +14907,7 @@
         <v>1</v>
       </c>
       <c r="N223" s="3" t="n">
-        <v>46074.59097222222</v>
+        <v>46076.4025925926</v>
       </c>
       <c r="O223" t="inlineStr">
         <is>
@@ -15099,7 +15099,7 @@
         <v>1</v>
       </c>
       <c r="N226" s="3" t="n">
-        <v>46074.59061342593</v>
+        <v>46076.37190972222</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15163,7 +15163,7 @@
         <v>1</v>
       </c>
       <c r="N227" s="3" t="n">
-        <v>46074.61186342593</v>
+        <v>46076.38277777778</v>
       </c>
       <c r="O227" t="inlineStr">
         <is>
@@ -15291,7 +15291,7 @@
         <v>1</v>
       </c>
       <c r="N229" s="3" t="n">
-        <v>46074.50202546296</v>
+        <v>46076.39912037037</v>
       </c>
       <c r="O229" t="inlineStr">
         <is>
@@ -15355,7 +15355,7 @@
         <v>1</v>
       </c>
       <c r="N230" s="3" t="n">
-        <v>46074.5630787037</v>
+        <v>46076.40269675926</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15419,7 +15419,7 @@
         <v>1</v>
       </c>
       <c r="N231" s="3" t="n">
-        <v>46074.83606481482</v>
+        <v>46076.36929398148</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15483,7 +15483,7 @@
         <v>1</v>
       </c>
       <c r="N232" s="3" t="n">
-        <v>46074.36681712963</v>
+        <v>46076.36325231481</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -15547,7 +15547,7 @@
         <v>1</v>
       </c>
       <c r="N233" s="3" t="n">
-        <v>46074.48827546297</v>
+        <v>46076.37659722222</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15611,7 +15611,7 @@
         <v>1</v>
       </c>
       <c r="N234" s="3" t="n">
-        <v>46074.62008101852</v>
+        <v>46076.3865625</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -15675,7 +15675,7 @@
         <v>1</v>
       </c>
       <c r="N235" s="3" t="n">
-        <v>46074.61873842592</v>
+        <v>46076.38532407407</v>
       </c>
       <c r="O235" t="inlineStr">
         <is>
@@ -15739,7 +15739,7 @@
         <v>1</v>
       </c>
       <c r="N236" s="3" t="n">
-        <v>46074.56008101852</v>
+        <v>46076.38378472222</v>
       </c>
       <c r="O236" t="inlineStr">
         <is>
@@ -15803,7 +15803,7 @@
         <v>1</v>
       </c>
       <c r="N237" s="3" t="n">
-        <v>46074.59880787037</v>
+        <v>46076.38482638889</v>
       </c>
       <c r="O237" t="inlineStr">
         <is>
@@ -15931,7 +15931,7 @@
         <v>1</v>
       </c>
       <c r="N239" s="3" t="n">
-        <v>46074.57987268519</v>
+        <v>46076.37813657407</v>
       </c>
       <c r="O239" t="inlineStr">
         <is>
@@ -15995,7 +15995,7 @@
         <v>1</v>
       </c>
       <c r="N240" s="3" t="n">
-        <v>46074.56337962963</v>
+        <v>46076.4027199074</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16059,7 +16059,7 @@
         <v>1</v>
       </c>
       <c r="N241" s="3" t="n">
-        <v>46073.7858449074</v>
+        <v>46076.40219907407</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16123,7 +16123,7 @@
         <v>1</v>
       </c>
       <c r="N242" s="3" t="n">
-        <v>46074.55965277777</v>
+        <v>46076.40206018519</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16187,7 +16187,7 @@
         <v>1</v>
       </c>
       <c r="N243" s="3" t="n">
-        <v>46073.81146990741</v>
+        <v>46076.40321759259</v>
       </c>
       <c r="O243" t="inlineStr">
         <is>
@@ -16206,6 +16206,11 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>10.69.5.112</t>
+        </is>
+      </c>
       <c r="D244" t="n">
         <v>2019</v>
       </c>
@@ -16246,7 +16251,7 @@
         <v>1</v>
       </c>
       <c r="N244" s="3" t="n">
-        <v>46076.20893518518</v>
+        <v>46076.38189814815</v>
       </c>
       <c r="O244" t="inlineStr">
         <is>
@@ -16310,7 +16315,7 @@
         <v>1</v>
       </c>
       <c r="N245" s="3" t="n">
-        <v>46076.31284722222</v>
+        <v>46076.38400462963</v>
       </c>
       <c r="O245" t="inlineStr">
         <is>
@@ -16374,7 +16379,7 @@
         <v>1</v>
       </c>
       <c r="N246" s="3" t="n">
-        <v>46076.31244212963</v>
+        <v>46076.38959490741</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16438,7 +16443,7 @@
         <v>1</v>
       </c>
       <c r="N247" s="3" t="n">
-        <v>46076.31219907408</v>
+        <v>46076.37039351852</v>
       </c>
       <c r="O247" t="inlineStr">
         <is>
@@ -16502,7 +16507,7 @@
         <v>1</v>
       </c>
       <c r="N248" s="3" t="n">
-        <v>46076.3121875</v>
+        <v>46076.38137731481</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16566,7 +16571,7 @@
         <v>1</v>
       </c>
       <c r="N249" s="3" t="n">
-        <v>46076.31995370371</v>
+        <v>46076.38298611111</v>
       </c>
       <c r="O249" t="inlineStr">
         <is>
@@ -16585,11 +16590,6 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
-      <c r="C250" t="inlineStr">
-        <is>
-          <t>10.69.5.118</t>
-        </is>
-      </c>
       <c r="D250" t="n">
         <v>2017</v>
       </c>
@@ -16630,7 +16630,7 @@
         <v>1</v>
       </c>
       <c r="N250" s="3" t="n">
-        <v>46076.31877314814</v>
+        <v>46076.3749537037</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16694,7 +16694,7 @@
         <v>1</v>
       </c>
       <c r="N251" s="3" t="n">
-        <v>46076.31210648148</v>
+        <v>46076.38310185185</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16758,7 +16758,7 @@
         <v>1</v>
       </c>
       <c r="N252" s="3" t="n">
-        <v>46076.31225694445</v>
+        <v>46076.37841435185</v>
       </c>
       <c r="O252" t="inlineStr">
         <is>
@@ -16822,7 +16822,7 @@
         <v>1</v>
       </c>
       <c r="N253" s="3" t="n">
-        <v>46074.58370370371</v>
+        <v>46076.36815972222</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16880,7 +16880,7 @@
         <v>1</v>
       </c>
       <c r="N254" s="3" t="n">
-        <v>46074.61710648148</v>
+        <v>46076.38028935185</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -16944,7 +16944,7 @@
         <v>1</v>
       </c>
       <c r="N255" s="3" t="n">
-        <v>46074.61524305555</v>
+        <v>46076.37334490741</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -17008,7 +17008,7 @@
         <v>1</v>
       </c>
       <c r="N256" s="3" t="n">
-        <v>46074.59122685185</v>
+        <v>46076.38287037037</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17072,7 +17072,7 @@
         <v>1</v>
       </c>
       <c r="N257" s="3" t="n">
-        <v>46074.59708333333</v>
+        <v>46076.36767361111</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17136,7 +17136,7 @@
         <v>1</v>
       </c>
       <c r="N258" s="3" t="n">
-        <v>46074.60739583334</v>
+        <v>46076.37356481481</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
@@ -17200,7 +17200,7 @@
         <v>1</v>
       </c>
       <c r="N259" s="3" t="n">
-        <v>46074.45996527778</v>
+        <v>46076.37903935185</v>
       </c>
       <c r="O259" t="inlineStr">
         <is>
@@ -17264,7 +17264,7 @@
         <v>1</v>
       </c>
       <c r="N260" s="3" t="n">
-        <v>46076.28324074074</v>
+        <v>46076.3846412037</v>
       </c>
       <c r="O260" t="inlineStr">
         <is>
@@ -17328,7 +17328,7 @@
         <v>1</v>
       </c>
       <c r="N261" s="3" t="n">
-        <v>46074.6368287037</v>
+        <v>46076.36719907408</v>
       </c>
       <c r="O261" t="inlineStr">
         <is>
@@ -17392,7 +17392,7 @@
         <v>1</v>
       </c>
       <c r="N262" s="3" t="n">
-        <v>46074.59364583333</v>
+        <v>46076.37056712963</v>
       </c>
       <c r="O262" t="inlineStr">
         <is>
@@ -17456,7 +17456,7 @@
         <v>1</v>
       </c>
       <c r="N263" s="3" t="n">
-        <v>46076.31122685185</v>
+        <v>46076.37355324074</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17520,7 +17520,7 @@
         <v>1</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>46074.51443287037</v>
+        <v>46076.37523148148</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17584,7 +17584,7 @@
         <v>1</v>
       </c>
       <c r="N265" s="3" t="n">
-        <v>46074.58900462963</v>
+        <v>46076.39047453704</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17648,7 +17648,7 @@
         <v>1</v>
       </c>
       <c r="N266" s="3" t="n">
-        <v>46074.3731712963</v>
+        <v>46076.38361111111</v>
       </c>
       <c r="O266" t="inlineStr">
         <is>
@@ -17712,7 +17712,7 @@
         <v>1</v>
       </c>
       <c r="N267" s="3" t="n">
-        <v>46074.60369212963</v>
+        <v>46076.40107638889</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17776,7 +17776,7 @@
         <v>1</v>
       </c>
       <c r="N268" s="3" t="n">
-        <v>46074.57481481481</v>
+        <v>46076.37640046296</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17901,7 +17901,7 @@
         </is>
       </c>
       <c r="N270" s="3" t="n">
-        <v>46076.30293981481</v>
+        <v>46076.38003472222</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -18029,7 +18029,7 @@
         <v>1</v>
       </c>
       <c r="N272" s="3" t="n">
-        <v>46074.60545138889</v>
+        <v>46076.37087962963</v>
       </c>
       <c r="O272" t="inlineStr">
         <is>
@@ -18093,7 +18093,7 @@
         <v>2</v>
       </c>
       <c r="N273" s="3" t="n">
-        <v>46076.29390046297</v>
+        <v>46076.36805555555</v>
       </c>
       <c r="O273" t="inlineStr">
         <is>
@@ -18413,7 +18413,7 @@
         <v>1</v>
       </c>
       <c r="N278" s="3" t="n">
-        <v>46074.52625</v>
+        <v>46076.35682870371</v>
       </c>
       <c r="O278" t="inlineStr">
         <is>
@@ -18477,7 +18477,7 @@
         <v>1</v>
       </c>
       <c r="N279" s="3" t="n">
-        <v>46076.31510416666</v>
+        <v>46076.38357638889</v>
       </c>
       <c r="O279" t="inlineStr">
         <is>
@@ -18541,7 +18541,7 @@
         <v>1</v>
       </c>
       <c r="N280" s="3" t="n">
-        <v>46074.59521990741</v>
+        <v>46076.36902777778</v>
       </c>
       <c r="O280" t="inlineStr">
         <is>
@@ -18605,7 +18605,7 @@
         <v>1</v>
       </c>
       <c r="N281" s="3" t="n">
-        <v>46076.31453703704</v>
+        <v>46076.39537037037</v>
       </c>
       <c r="O281" t="inlineStr">
         <is>
@@ -18624,6 +18624,11 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>10.69.5.151</t>
+        </is>
+      </c>
       <c r="D282" t="n">
         <v>2017</v>
       </c>
@@ -18664,7 +18669,7 @@
         <v>1</v>
       </c>
       <c r="N282" s="3" t="n">
-        <v>46074.43244212963</v>
+        <v>46076.40094907407</v>
       </c>
       <c r="O282" t="inlineStr">
         <is>
@@ -18792,7 +18797,7 @@
         <v>1</v>
       </c>
       <c r="N284" s="3" t="n">
-        <v>46074.45539351852</v>
+        <v>46076.37582175926</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18856,7 +18861,7 @@
         <v>1</v>
       </c>
       <c r="N285" s="3" t="n">
-        <v>46074.45655092593</v>
+        <v>46076.36704861111</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -18875,11 +18880,6 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
-      <c r="C286" t="inlineStr">
-        <is>
-          <t>10.69.5.155</t>
-        </is>
-      </c>
       <c r="D286" t="n">
         <v>2019</v>
       </c>
@@ -18920,7 +18920,7 @@
         <v>1</v>
       </c>
       <c r="N286" s="3" t="n">
-        <v>46076.29733796296</v>
+        <v>46076.37554398148</v>
       </c>
       <c r="O286" t="inlineStr">
         <is>
@@ -18984,7 +18984,7 @@
         <v>1</v>
       </c>
       <c r="N287" s="3" t="n">
-        <v>46074.46532407407</v>
+        <v>46076.3978587963</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
@@ -19048,7 +19048,7 @@
         <v>1</v>
       </c>
       <c r="N288" s="3" t="n">
-        <v>46076.31679398148</v>
+        <v>46076.39879629629</v>
       </c>
       <c r="O288" t="inlineStr">
         <is>
@@ -19112,7 +19112,7 @@
         <v>1</v>
       </c>
       <c r="N289" s="3" t="n">
-        <v>46076.30862268519</v>
+        <v>46076.38565972223</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -19906,7 +19906,7 @@
         <v>1</v>
       </c>
       <c r="N302" s="3" t="n">
-        <v>46076.31034722222</v>
+        <v>46076.38511574074</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -21022,7 +21022,7 @@
         </is>
       </c>
       <c r="N320" s="3" t="n">
-        <v>46076.30619212963</v>
+        <v>46076.38111111111</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21461,7 +21461,7 @@
         </is>
       </c>
       <c r="N327" s="3" t="n">
-        <v>46058.66199074074</v>
+        <v>46076.38082175926</v>
       </c>
       <c r="O327" t="inlineStr">
         <is>
@@ -21494,7 +21494,7 @@
         <v>2</v>
       </c>
       <c r="N328" s="3" t="n">
-        <v>46055.55023148148</v>
+        <v>46076.38509259259</v>
       </c>
       <c r="O328" t="inlineStr">
         <is>
@@ -21747,7 +21747,7 @@
         <v>1</v>
       </c>
       <c r="N332" s="3" t="n">
-        <v>46074.53166666667</v>
+        <v>46076.37414351852</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21811,7 +21811,7 @@
         <v>2</v>
       </c>
       <c r="N333" s="3" t="n">
-        <v>46076.28776620371</v>
+        <v>46076.40237268519</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21875,7 +21875,7 @@
         <v>2</v>
       </c>
       <c r="N334" s="3" t="n">
-        <v>46076.28846064815</v>
+        <v>46076.40386574074</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21939,7 +21939,7 @@
         <v>2</v>
       </c>
       <c r="N335" s="3" t="n">
-        <v>46076.28802083333</v>
+        <v>46076.36516203704</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -22003,7 +22003,7 @@
         <v>1</v>
       </c>
       <c r="N336" s="3" t="n">
-        <v>46076.3095949074</v>
+        <v>46076.38621527778</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22067,7 +22067,7 @@
         <v>1</v>
       </c>
       <c r="N337" s="3" t="n">
-        <v>46076.2881712963</v>
+        <v>46076.3720949074</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22323,7 +22323,7 @@
         <v>2</v>
       </c>
       <c r="N341" s="3" t="n">
-        <v>46073.57005787037</v>
+        <v>46076.37225694444</v>
       </c>
       <c r="O341" t="inlineStr">
         <is>
@@ -22384,10 +22384,10 @@
         </is>
       </c>
       <c r="M342" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N342" s="3" t="n">
-        <v>46073.57138888889</v>
+        <v>46076.37314814814</v>
       </c>
       <c r="O342" t="inlineStr">
         <is>
@@ -22448,7 +22448,7 @@
         </is>
       </c>
       <c r="N343" s="3" t="n">
-        <v>46073.70519675926</v>
+        <v>46076.37824074074</v>
       </c>
       <c r="O343" t="inlineStr">
         <is>
@@ -22704,7 +22704,7 @@
         <v>1</v>
       </c>
       <c r="N347" s="3" t="n">
-        <v>46073.58310185185</v>
+        <v>46076.39743055555</v>
       </c>
       <c r="O347" t="inlineStr">
         <is>
@@ -22768,7 +22768,7 @@
         <v>2</v>
       </c>
       <c r="N348" s="3" t="n">
-        <v>46073.57166666666</v>
+        <v>46076.39991898148</v>
       </c>
       <c r="O348" t="inlineStr">
         <is>
@@ -22832,7 +22832,7 @@
         <v>1</v>
       </c>
       <c r="N349" s="3" t="n">
-        <v>46073.57833333333</v>
+        <v>46076.39965277778</v>
       </c>
       <c r="O349" t="inlineStr">
         <is>
@@ -22955,7 +22955,7 @@
         <v>1</v>
       </c>
       <c r="N351" s="3" t="n">
-        <v>46073.58429398148</v>
+        <v>46076.39960648148</v>
       </c>
       <c r="O351" t="inlineStr">
         <is>
@@ -23080,7 +23080,7 @@
         </is>
       </c>
       <c r="N353" s="3" t="n">
-        <v>46073.57987268519</v>
+        <v>46076.39851851852</v>
       </c>
       <c r="O353" t="inlineStr">
         <is>
@@ -23141,7 +23141,7 @@
         </is>
       </c>
       <c r="N354" s="3" t="n">
-        <v>46073.57917824074</v>
+        <v>46076.39909722222</v>
       </c>
       <c r="O354" t="inlineStr">
         <is>
@@ -23205,7 +23205,7 @@
         <v>1</v>
       </c>
       <c r="N355" s="3" t="n">
-        <v>46073.58078703703</v>
+        <v>46076.39898148148</v>
       </c>
       <c r="O355" t="inlineStr">
         <is>
@@ -23269,7 +23269,7 @@
         <v>1</v>
       </c>
       <c r="N356" s="3" t="n">
-        <v>46073.5746412037</v>
+        <v>46076.39914351852</v>
       </c>
       <c r="O356" t="inlineStr">
         <is>
@@ -23333,7 +23333,7 @@
         <v>1</v>
       </c>
       <c r="N357" s="3" t="n">
-        <v>46073.57524305556</v>
+        <v>46076.39929398148</v>
       </c>
       <c r="O357" t="inlineStr">
         <is>
@@ -23520,7 +23520,7 @@
         <v>2</v>
       </c>
       <c r="N360" s="3" t="n">
-        <v>46073.57143518519</v>
+        <v>46076.40020833333</v>
       </c>
       <c r="O360" t="inlineStr">
         <is>
@@ -23584,7 +23584,7 @@
         <v>1</v>
       </c>
       <c r="N361" s="3" t="n">
-        <v>46073.67961805555</v>
+        <v>46076.39930555555</v>
       </c>
       <c r="O361" t="inlineStr">
         <is>
@@ -23645,7 +23645,7 @@
         </is>
       </c>
       <c r="N362" s="3" t="n">
-        <v>46073.5766087963</v>
+        <v>46076.40010416666</v>
       </c>
       <c r="O362" t="inlineStr">
         <is>
@@ -23833,7 +23833,7 @@
         <v>1</v>
       </c>
       <c r="N365" s="3" t="n">
-        <v>46073.68641203704</v>
+        <v>46076.38391203704</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
@@ -23899,7 +23899,7 @@
         </is>
       </c>
       <c r="N366" s="3" t="n">
-        <v>46076.29938657407</v>
+        <v>46076.37953703704</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -24025,7 +24025,7 @@
         </is>
       </c>
       <c r="N368" s="3" t="n">
-        <v>46073.71178240741</v>
+        <v>46076.36677083333</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -24086,7 +24086,7 @@
         </is>
       </c>
       <c r="N369" s="3" t="n">
-        <v>46073.71048611111</v>
+        <v>46076.38778935185</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
@@ -24155,7 +24155,7 @@
         <v>1</v>
       </c>
       <c r="N370" s="3" t="n">
-        <v>46073.74658564815</v>
+        <v>46076.36671296296</v>
       </c>
       <c r="O370" t="inlineStr">
         <is>
@@ -24431,7 +24431,7 @@
         <v>1</v>
       </c>
       <c r="N374" s="3" t="n">
-        <v>46073.76869212963</v>
+        <v>46076.40206018519</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24497,7 +24497,7 @@
         </is>
       </c>
       <c r="N375" s="3" t="n">
-        <v>46076.28959490741</v>
+        <v>46076.36747685185</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
@@ -24630,7 +24630,7 @@
         <v>2</v>
       </c>
       <c r="N377" s="3" t="n">
-        <v>46074.47112268519</v>
+        <v>46076.39965277778</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -24699,7 +24699,7 @@
         <v>2</v>
       </c>
       <c r="N378" s="3" t="n">
-        <v>46076.28778935185</v>
+        <v>46076.36771990741</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização automática 2026-02-23 11:52:05.061437
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>46076.38034722222</v>
+        <v>46076.46010416667</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>46076.37806712963</v>
+        <v>46076.45434027778</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
         <v>1</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>46076.39019675926</v>
+        <v>46076.46494212963</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>46076.38290509259</v>
+        <v>46076.45732638889</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -1131,7 +1131,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="3" t="n">
-        <v>46076.38372685185</v>
+        <v>46076.46309027778</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1451,7 +1451,7 @@
         <v>1</v>
       </c>
       <c r="N15" s="3" t="n">
-        <v>46076.38152777778</v>
+        <v>46076.4597337963</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1515,7 +1515,7 @@
         <v>2</v>
       </c>
       <c r="N16" s="3" t="n">
-        <v>46076.38643518519</v>
+        <v>46076.46467592593</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -6570,7 +6570,7 @@
         <v>1</v>
       </c>
       <c r="N95" s="3" t="n">
-        <v>46076.40098379629</v>
+        <v>46076.48091435185</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -6708,7 +6708,7 @@
         <v>1</v>
       </c>
       <c r="N97" s="3" t="n">
-        <v>46076.40021990741</v>
+        <v>46076.47429398148</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -6841,7 +6841,7 @@
         <v>1</v>
       </c>
       <c r="N99" s="3" t="n">
-        <v>46072.79275462963</v>
+        <v>46076.45773148148</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -6910,7 +6910,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>46076.38107638889</v>
+        <v>46076.46229166666</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6979,7 +6979,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="3" t="n">
-        <v>46076.37842592593</v>
+        <v>46076.45460648148</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -7117,7 +7117,7 @@
         <v>2</v>
       </c>
       <c r="N103" s="3" t="n">
-        <v>46076.38101851852</v>
+        <v>46076.46105324074</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7374,7 +7374,7 @@
         <v>1</v>
       </c>
       <c r="N107" s="3" t="n">
-        <v>46073.69743055556</v>
+        <v>46076.47574074074</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -7512,7 +7512,7 @@
         <v>1</v>
       </c>
       <c r="N109" s="3" t="n">
-        <v>46076.38048611111</v>
+        <v>46076.46192129629</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7581,7 +7581,7 @@
         <v>2</v>
       </c>
       <c r="N110" s="3" t="n">
-        <v>46076.38604166666</v>
+        <v>46076.45964120371</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7650,7 +7650,7 @@
         <v>2</v>
       </c>
       <c r="N111" s="3" t="n">
-        <v>46076.3693287037</v>
+        <v>46076.44972222222</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
@@ -7719,7 +7719,7 @@
         <v>2</v>
       </c>
       <c r="N112" s="3" t="n">
-        <v>46076.39040509259</v>
+        <v>46076.46534722222</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7788,7 +7788,7 @@
         <v>1</v>
       </c>
       <c r="N113" s="3" t="n">
-        <v>46076.3799537037</v>
+        <v>46076.45732638889</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7857,7 +7857,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>46076.38144675926</v>
+        <v>46076.46353009259</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -7923,7 +7923,7 @@
         </is>
       </c>
       <c r="N115" s="3" t="n">
-        <v>46076.3722337963</v>
+        <v>46076.48755787037</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -7992,7 +7992,7 @@
         <v>1</v>
       </c>
       <c r="N116" s="3" t="n">
-        <v>46076.37649305556</v>
+        <v>46076.45684027778</v>
       </c>
       <c r="O116" t="inlineStr">
         <is>
@@ -8061,7 +8061,7 @@
         <v>1</v>
       </c>
       <c r="N117" s="3" t="n">
-        <v>46076.39670138889</v>
+        <v>46076.47607638889</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -8265,7 +8265,7 @@
         <v>1</v>
       </c>
       <c r="N120" s="3" t="n">
-        <v>46076.39</v>
+        <v>46076.47248842593</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -8400,7 +8400,7 @@
         </is>
       </c>
       <c r="N122" s="3" t="n">
-        <v>46076.36479166667</v>
+        <v>46076.47775462963</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -8469,7 +8469,7 @@
         <v>2</v>
       </c>
       <c r="N123" s="3" t="n">
-        <v>46076.36074074074</v>
+        <v>46076.46792824074</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -8538,7 +8538,7 @@
         <v>1</v>
       </c>
       <c r="N124" s="3" t="n">
-        <v>46076.3865625</v>
+        <v>46076.46104166667</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -8607,7 +8607,7 @@
         <v>1</v>
       </c>
       <c r="N125" s="3" t="n">
-        <v>46076.36550925926</v>
+        <v>46076.48505787037</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -8673,10 +8673,10 @@
         </is>
       </c>
       <c r="M126" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N126" s="3" t="n">
-        <v>46073.70068287037</v>
+        <v>46076.45584490741</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -8745,7 +8745,7 @@
         <v>2</v>
       </c>
       <c r="N127" s="3" t="n">
-        <v>46076.40200231481</v>
+        <v>46076.47675925926</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -8814,7 +8814,7 @@
         <v>1</v>
       </c>
       <c r="N128" s="3" t="n">
-        <v>46076.36589120371</v>
+        <v>46076.48275462963</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -8883,7 +8883,7 @@
         <v>1</v>
       </c>
       <c r="N129" s="3" t="n">
-        <v>46076.39400462963</v>
+        <v>46076.47201388889</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -8952,7 +8952,7 @@
         <v>1</v>
       </c>
       <c r="N130" s="3" t="n">
-        <v>46076.37075231481</v>
+        <v>46076.44784722223</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -9016,7 +9016,7 @@
         <v>1</v>
       </c>
       <c r="N131" s="3" t="n">
-        <v>46076.38774305556</v>
+        <v>46076.46447916667</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -9149,7 +9149,7 @@
         <v>1</v>
       </c>
       <c r="N133" s="3" t="n">
-        <v>46076.38026620371</v>
+        <v>46076.45585648148</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -9213,7 +9213,7 @@
         <v>1</v>
       </c>
       <c r="N134" s="3" t="n">
-        <v>46076.37180555556</v>
+        <v>46076.48552083333</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -9277,7 +9277,7 @@
         <v>1</v>
       </c>
       <c r="N135" s="3" t="n">
-        <v>46076.36795138889</v>
+        <v>46076.48787037037</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -9468,7 +9468,7 @@
         <v>1</v>
       </c>
       <c r="N138" s="3" t="n">
-        <v>46076.38017361111</v>
+        <v>46076.45984953704</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9532,7 +9532,7 @@
         <v>1</v>
       </c>
       <c r="N139" s="3" t="n">
-        <v>46076.39362268519</v>
+        <v>46076.47604166667</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9596,7 +9596,7 @@
         <v>1</v>
       </c>
       <c r="N140" s="3" t="n">
-        <v>46076.38131944444</v>
+        <v>46076.46150462963</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9660,7 +9660,7 @@
         <v>1</v>
       </c>
       <c r="N141" s="3" t="n">
-        <v>46076.38077546296</v>
+        <v>46076.4637037037</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9724,7 +9724,7 @@
         <v>1</v>
       </c>
       <c r="N142" s="3" t="n">
-        <v>46076.3705787037</v>
+        <v>46076.45929398148</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9788,7 +9788,7 @@
         <v>1</v>
       </c>
       <c r="N143" s="3" t="n">
-        <v>46076.37773148148</v>
+        <v>46076.45752314815</v>
       </c>
       <c r="O143" t="inlineStr">
         <is>
@@ -9852,7 +9852,7 @@
         <v>1</v>
       </c>
       <c r="N144" s="3" t="n">
-        <v>46076.38502314815</v>
+        <v>46076.46630787037</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9980,7 +9980,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="3" t="n">
-        <v>46076.37024305556</v>
+        <v>46076.48663194444</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10044,7 +10044,7 @@
         <v>1</v>
       </c>
       <c r="N147" s="3" t="n">
-        <v>46076.36665509259</v>
+        <v>46076.48748842593</v>
       </c>
       <c r="O147" t="inlineStr">
         <is>
@@ -10108,7 +10108,7 @@
         <v>1</v>
       </c>
       <c r="N148" s="3" t="n">
-        <v>46076.37935185185</v>
+        <v>46076.45989583333</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10172,7 +10172,7 @@
         <v>1</v>
       </c>
       <c r="N149" s="3" t="n">
-        <v>46076.40175925926</v>
+        <v>46076.47861111111</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -10236,7 +10236,7 @@
         <v>1</v>
       </c>
       <c r="N150" s="3" t="n">
-        <v>46076.37167824074</v>
+        <v>46076.44984953704</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -10364,7 +10364,7 @@
         <v>1</v>
       </c>
       <c r="N152" s="3" t="n">
-        <v>46076.39314814815</v>
+        <v>46076.46966435185</v>
       </c>
       <c r="O152" t="inlineStr">
         <is>
@@ -10383,11 +10383,6 @@
           <t>OPERACAO 7.1</t>
         </is>
       </c>
-      <c r="C153" t="inlineStr">
-        <is>
-          <t>10.69.5.21</t>
-        </is>
-      </c>
       <c r="D153" t="n">
         <v>2018</v>
       </c>
@@ -10428,7 +10423,7 @@
         <v>1</v>
       </c>
       <c r="N153" s="3" t="n">
-        <v>46076.37305555555</v>
+        <v>46076.48702546296</v>
       </c>
       <c r="O153" t="inlineStr">
         <is>
@@ -10492,7 +10487,7 @@
         <v>1</v>
       </c>
       <c r="N154" s="3" t="n">
-        <v>46076.40310185185</v>
+        <v>46076.481875</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10556,7 +10551,7 @@
         <v>1</v>
       </c>
       <c r="N155" s="3" t="n">
-        <v>46076.39966435185</v>
+        <v>46076.47659722222</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10684,7 +10679,7 @@
         <v>1</v>
       </c>
       <c r="N157" s="3" t="n">
-        <v>46076.38680555556</v>
+        <v>46076.4662962963</v>
       </c>
       <c r="O157" t="inlineStr">
         <is>
@@ -10748,7 +10743,7 @@
         <v>1</v>
       </c>
       <c r="N158" s="3" t="n">
-        <v>46076.39215277778</v>
+        <v>46076.47024305556</v>
       </c>
       <c r="O158" t="inlineStr">
         <is>
@@ -10812,7 +10807,7 @@
         <v>1</v>
       </c>
       <c r="N159" s="3" t="n">
-        <v>46076.36890046296</v>
+        <v>46076.48664351852</v>
       </c>
       <c r="O159" t="inlineStr">
         <is>
@@ -10876,7 +10871,7 @@
         <v>1</v>
       </c>
       <c r="N160" s="3" t="n">
-        <v>46076.37993055556</v>
+        <v>46076.46152777778</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
@@ -10940,7 +10935,7 @@
         <v>1</v>
       </c>
       <c r="N161" s="3" t="n">
-        <v>46076.3659837963</v>
+        <v>46076.47998842593</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -11004,7 +10999,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="3" t="n">
-        <v>46076.36725694445</v>
+        <v>46076.4809837963</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11132,7 +11127,7 @@
         <v>2</v>
       </c>
       <c r="N164" s="3" t="n">
-        <v>46076.37123842593</v>
+        <v>46076.48307870371</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11196,7 +11191,7 @@
         <v>2</v>
       </c>
       <c r="N165" s="3" t="n">
-        <v>46076.36981481482</v>
+        <v>46076.48239583334</v>
       </c>
       <c r="O165" t="inlineStr">
         <is>
@@ -11260,7 +11255,7 @@
         <v>2</v>
       </c>
       <c r="N166" s="3" t="n">
-        <v>46076.3833912037</v>
+        <v>46076.46049768518</v>
       </c>
       <c r="O166" t="inlineStr">
         <is>
@@ -11324,7 +11319,7 @@
         <v>2</v>
       </c>
       <c r="N167" s="3" t="n">
-        <v>46076.40356481481</v>
+        <v>46076.4811574074</v>
       </c>
       <c r="O167" t="inlineStr">
         <is>
@@ -11388,7 +11383,7 @@
         <v>2</v>
       </c>
       <c r="N168" s="3" t="n">
-        <v>46076.39761574074</v>
+        <v>46076.48085648148</v>
       </c>
       <c r="O168" t="inlineStr">
         <is>
@@ -11452,7 +11447,7 @@
         <v>2</v>
       </c>
       <c r="N169" s="3" t="n">
-        <v>46076.39270833333</v>
+        <v>46076.4712037037</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -11516,7 +11511,7 @@
         <v>2</v>
       </c>
       <c r="N170" s="3" t="n">
-        <v>46076.38333333333</v>
+        <v>46076.46025462963</v>
       </c>
       <c r="O170" t="inlineStr">
         <is>
@@ -11580,7 +11575,7 @@
         <v>1</v>
       </c>
       <c r="N171" s="3" t="n">
-        <v>46076.37311342593</v>
+        <v>46076.45221064815</v>
       </c>
       <c r="O171" t="inlineStr">
         <is>
@@ -11708,7 +11703,7 @@
         <v>2</v>
       </c>
       <c r="N173" s="3" t="n">
-        <v>46076.39061342592</v>
+        <v>46076.46765046296</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -11772,7 +11767,7 @@
         <v>2</v>
       </c>
       <c r="N174" s="3" t="n">
-        <v>46076.37344907408</v>
+        <v>46076.45219907408</v>
       </c>
       <c r="O174" t="inlineStr">
         <is>
@@ -11836,7 +11831,7 @@
         <v>2</v>
       </c>
       <c r="N175" s="3" t="n">
-        <v>46076.37965277778</v>
+        <v>46076.45777777778</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -11900,7 +11895,7 @@
         <v>2</v>
       </c>
       <c r="N176" s="3" t="n">
-        <v>46074.52883101852</v>
+        <v>46076.46116898148</v>
       </c>
       <c r="O176" t="inlineStr">
         <is>
@@ -11961,10 +11956,10 @@
         </is>
       </c>
       <c r="M177" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N177" s="3" t="n">
-        <v>46073.69657407407</v>
+        <v>46076.47340277778</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
@@ -12028,7 +12023,7 @@
         <v>2</v>
       </c>
       <c r="N178" s="3" t="n">
-        <v>46076.40226851852</v>
+        <v>46076.47572916667</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12092,7 +12087,7 @@
         <v>1</v>
       </c>
       <c r="N179" s="3" t="n">
-        <v>46076.39179398148</v>
+        <v>46076.46430555556</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12156,7 +12151,7 @@
         <v>1</v>
       </c>
       <c r="N180" s="3" t="n">
-        <v>46076.38414351852</v>
+        <v>46076.46193287037</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12220,7 +12215,7 @@
         <v>1</v>
       </c>
       <c r="N181" s="3" t="n">
-        <v>46076.3746875</v>
+        <v>46076.45659722222</v>
       </c>
       <c r="O181" t="inlineStr">
         <is>
@@ -12545,7 +12540,7 @@
         <v>1</v>
       </c>
       <c r="N186" s="3" t="n">
-        <v>46076.39076388889</v>
+        <v>46076.47006944445</v>
       </c>
       <c r="O186" t="inlineStr">
         <is>
@@ -12609,7 +12604,7 @@
         <v>1</v>
       </c>
       <c r="N187" s="3" t="n">
-        <v>46076.39106481482</v>
+        <v>46076.46844907408</v>
       </c>
       <c r="O187" t="inlineStr">
         <is>
@@ -12673,7 +12668,7 @@
         <v>1</v>
       </c>
       <c r="N188" s="3" t="n">
-        <v>46076.38618055556</v>
+        <v>46076.46344907407</v>
       </c>
       <c r="O188" t="inlineStr">
         <is>
@@ -12759,11 +12754,6 @@
           <t>OPERACAO 8.1</t>
         </is>
       </c>
-      <c r="C190" t="inlineStr">
-        <is>
-          <t>10.69.5.59</t>
-        </is>
-      </c>
       <c r="D190" t="n">
         <v>2015</v>
       </c>
@@ -12801,7 +12791,7 @@
         </is>
       </c>
       <c r="N190" s="3" t="n">
-        <v>46076.4005787037</v>
+        <v>46076.47620370371</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12929,7 +12919,7 @@
         <v>1</v>
       </c>
       <c r="N192" s="3" t="n">
-        <v>46076.37759259259</v>
+        <v>46076.46136574074</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -13054,7 +13044,7 @@
         <v>2</v>
       </c>
       <c r="N194" s="3" t="n">
-        <v>46076.37033564815</v>
+        <v>46076.46256944445</v>
       </c>
       <c r="O194" t="inlineStr">
         <is>
@@ -13118,7 +13108,7 @@
         <v>1</v>
       </c>
       <c r="N195" s="3" t="n">
-        <v>46076.38150462963</v>
+        <v>46076.46494212963</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13182,7 +13172,7 @@
         <v>1</v>
       </c>
       <c r="N196" s="3" t="n">
-        <v>46076.39996527778</v>
+        <v>46076.46269675926</v>
       </c>
       <c r="O196" t="inlineStr">
         <is>
@@ -13246,7 +13236,7 @@
         <v>1</v>
       </c>
       <c r="N197" s="3" t="n">
-        <v>46076.4031712963</v>
+        <v>46076.48513888889</v>
       </c>
       <c r="O197" t="inlineStr">
         <is>
@@ -13499,7 +13489,7 @@
         </is>
       </c>
       <c r="N201" s="3" t="n">
-        <v>46076.38903935185</v>
+        <v>46076.46524305556</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -13563,7 +13553,7 @@
         <v>1</v>
       </c>
       <c r="N202" s="3" t="n">
-        <v>46076.38815972222</v>
+        <v>46076.46714120371</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13627,7 +13617,7 @@
         <v>1</v>
       </c>
       <c r="N203" s="3" t="n">
-        <v>46076.38886574074</v>
+        <v>46076.46390046296</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13691,7 +13681,7 @@
         <v>1</v>
       </c>
       <c r="N204" s="3" t="n">
-        <v>46076.38868055555</v>
+        <v>46076.46230324074</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13755,7 +13745,7 @@
         <v>1</v>
       </c>
       <c r="N205" s="3" t="n">
-        <v>46076.37418981481</v>
+        <v>46076.45048611111</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13819,7 +13809,7 @@
         <v>1</v>
       </c>
       <c r="N206" s="3" t="n">
-        <v>46076.39998842592</v>
+        <v>46076.47810185186</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -13883,7 +13873,7 @@
         <v>1</v>
       </c>
       <c r="N207" s="3" t="n">
-        <v>46076.37501157408</v>
+        <v>46076.46299768519</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -13947,7 +13937,7 @@
         <v>1</v>
       </c>
       <c r="N208" s="3" t="n">
-        <v>46076.40399305556</v>
+        <v>46076.46706018518</v>
       </c>
       <c r="O208" t="inlineStr">
         <is>
@@ -14011,7 +14001,7 @@
         <v>1</v>
       </c>
       <c r="N209" s="3" t="n">
-        <v>46076.39859953704</v>
+        <v>46076.48099537037</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14075,7 +14065,7 @@
         <v>1</v>
       </c>
       <c r="N210" s="3" t="n">
-        <v>46076.37467592592</v>
+        <v>46076.45245370371</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14139,7 +14129,7 @@
         <v>1</v>
       </c>
       <c r="N211" s="3" t="n">
-        <v>46076.39630787037</v>
+        <v>46076.47528935185</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -14203,7 +14193,7 @@
         <v>1</v>
       </c>
       <c r="N212" s="3" t="n">
-        <v>46076.40035879629</v>
+        <v>46076.48002314815</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -14267,7 +14257,7 @@
         <v>1</v>
       </c>
       <c r="N213" s="3" t="n">
-        <v>46076.37253472222</v>
+        <v>46076.45547453704</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
@@ -14395,7 +14385,7 @@
         <v>1</v>
       </c>
       <c r="N215" s="3" t="n">
-        <v>46076.40260416667</v>
+        <v>46076.4641550926</v>
       </c>
       <c r="O215" t="inlineStr">
         <is>
@@ -14478,6 +14468,11 @@
           <t>OPERACAO 8.1</t>
         </is>
       </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>10.69.5.85</t>
+        </is>
+      </c>
       <c r="D217" t="n">
         <v>2017</v>
       </c>
@@ -14518,7 +14513,7 @@
         <v>1</v>
       </c>
       <c r="N217" s="3" t="n">
-        <v>46076.36678240741</v>
+        <v>46076.48747685185</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14582,7 +14577,7 @@
         <v>1</v>
       </c>
       <c r="N218" s="3" t="n">
-        <v>46076.36545138889</v>
+        <v>46076.48255787037</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14646,7 +14641,7 @@
         <v>1</v>
       </c>
       <c r="N219" s="3" t="n">
-        <v>46076.36848379629</v>
+        <v>46076.48050925926</v>
       </c>
       <c r="O219" t="inlineStr">
         <is>
@@ -14715,7 +14710,7 @@
         <v>1</v>
       </c>
       <c r="N220" s="3" t="n">
-        <v>46076.38965277778</v>
+        <v>46076.46270833333</v>
       </c>
       <c r="O220" t="inlineStr">
         <is>
@@ -14779,7 +14774,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="3" t="n">
-        <v>46076.37829861111</v>
+        <v>46076.45180555555</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14843,7 +14838,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="3" t="n">
-        <v>46076.39465277778</v>
+        <v>46076.46674768518</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -14907,7 +14902,7 @@
         <v>1</v>
       </c>
       <c r="N223" s="3" t="n">
-        <v>46076.4025925926</v>
+        <v>46076.48393518518</v>
       </c>
       <c r="O223" t="inlineStr">
         <is>
@@ -15099,7 +15094,7 @@
         <v>1</v>
       </c>
       <c r="N226" s="3" t="n">
-        <v>46076.37190972222</v>
+        <v>46076.48363425926</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15163,7 +15158,7 @@
         <v>1</v>
       </c>
       <c r="N227" s="3" t="n">
-        <v>46076.38277777778</v>
+        <v>46076.46079861111</v>
       </c>
       <c r="O227" t="inlineStr">
         <is>
@@ -15291,7 +15286,7 @@
         <v>1</v>
       </c>
       <c r="N229" s="3" t="n">
-        <v>46076.39912037037</v>
+        <v>46076.46290509259</v>
       </c>
       <c r="O229" t="inlineStr">
         <is>
@@ -15355,7 +15350,7 @@
         <v>1</v>
       </c>
       <c r="N230" s="3" t="n">
-        <v>46076.40269675926</v>
+        <v>46076.46530092593</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15419,7 +15414,7 @@
         <v>1</v>
       </c>
       <c r="N231" s="3" t="n">
-        <v>46076.36929398148</v>
+        <v>46076.48722222223</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15483,7 +15478,7 @@
         <v>1</v>
       </c>
       <c r="N232" s="3" t="n">
-        <v>46076.36325231481</v>
+        <v>46076.48126157407</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -15547,7 +15542,7 @@
         <v>1</v>
       </c>
       <c r="N233" s="3" t="n">
-        <v>46076.37659722222</v>
+        <v>46076.48508101852</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15611,7 +15606,7 @@
         <v>1</v>
       </c>
       <c r="N234" s="3" t="n">
-        <v>46076.3865625</v>
+        <v>46076.465</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -15675,7 +15670,7 @@
         <v>1</v>
       </c>
       <c r="N235" s="3" t="n">
-        <v>46076.38532407407</v>
+        <v>46076.46431712963</v>
       </c>
       <c r="O235" t="inlineStr">
         <is>
@@ -15739,7 +15734,7 @@
         <v>1</v>
       </c>
       <c r="N236" s="3" t="n">
-        <v>46076.38378472222</v>
+        <v>46076.4627662037</v>
       </c>
       <c r="O236" t="inlineStr">
         <is>
@@ -15867,7 +15862,7 @@
         <v>1</v>
       </c>
       <c r="N238" s="3" t="n">
-        <v>46074.59366898148</v>
+        <v>46076.45822916667</v>
       </c>
       <c r="O238" t="inlineStr">
         <is>
@@ -15931,7 +15926,7 @@
         <v>1</v>
       </c>
       <c r="N239" s="3" t="n">
-        <v>46076.37813657407</v>
+        <v>46076.46243055556</v>
       </c>
       <c r="O239" t="inlineStr">
         <is>
@@ -15995,7 +15990,7 @@
         <v>1</v>
       </c>
       <c r="N240" s="3" t="n">
-        <v>46076.4027199074</v>
+        <v>46076.48121527778</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16059,7 +16054,7 @@
         <v>1</v>
       </c>
       <c r="N241" s="3" t="n">
-        <v>46076.40219907407</v>
+        <v>46076.47552083333</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16123,7 +16118,7 @@
         <v>1</v>
       </c>
       <c r="N242" s="3" t="n">
-        <v>46076.40206018519</v>
+        <v>46076.47951388889</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16187,7 +16182,7 @@
         <v>1</v>
       </c>
       <c r="N243" s="3" t="n">
-        <v>46076.40321759259</v>
+        <v>46076.47988425926</v>
       </c>
       <c r="O243" t="inlineStr">
         <is>
@@ -16251,7 +16246,7 @@
         <v>1</v>
       </c>
       <c r="N244" s="3" t="n">
-        <v>46076.38189814815</v>
+        <v>46076.46063657408</v>
       </c>
       <c r="O244" t="inlineStr">
         <is>
@@ -16315,7 +16310,7 @@
         <v>1</v>
       </c>
       <c r="N245" s="3" t="n">
-        <v>46076.38400462963</v>
+        <v>46076.45903935185</v>
       </c>
       <c r="O245" t="inlineStr">
         <is>
@@ -16379,7 +16374,7 @@
         <v>1</v>
       </c>
       <c r="N246" s="3" t="n">
-        <v>46076.38959490741</v>
+        <v>46076.46957175926</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16443,7 +16438,7 @@
         <v>1</v>
       </c>
       <c r="N247" s="3" t="n">
-        <v>46076.37039351852</v>
+        <v>46076.45015046297</v>
       </c>
       <c r="O247" t="inlineStr">
         <is>
@@ -16507,7 +16502,7 @@
         <v>1</v>
       </c>
       <c r="N248" s="3" t="n">
-        <v>46076.38137731481</v>
+        <v>46076.46511574074</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16571,7 +16566,7 @@
         <v>1</v>
       </c>
       <c r="N249" s="3" t="n">
-        <v>46076.38298611111</v>
+        <v>46076.42236111111</v>
       </c>
       <c r="O249" t="inlineStr">
         <is>
@@ -16630,7 +16625,7 @@
         <v>1</v>
       </c>
       <c r="N250" s="3" t="n">
-        <v>46076.3749537037</v>
+        <v>46076.45559027778</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16694,7 +16689,7 @@
         <v>1</v>
       </c>
       <c r="N251" s="3" t="n">
-        <v>46076.38310185185</v>
+        <v>46076.45133101852</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16758,7 +16753,7 @@
         <v>1</v>
       </c>
       <c r="N252" s="3" t="n">
-        <v>46076.37841435185</v>
+        <v>46076.45633101852</v>
       </c>
       <c r="O252" t="inlineStr">
         <is>
@@ -16822,7 +16817,7 @@
         <v>1</v>
       </c>
       <c r="N253" s="3" t="n">
-        <v>46076.36815972222</v>
+        <v>46076.48674768519</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16880,7 +16875,7 @@
         <v>1</v>
       </c>
       <c r="N254" s="3" t="n">
-        <v>46076.38028935185</v>
+        <v>46076.45946759259</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -16944,7 +16939,7 @@
         <v>1</v>
       </c>
       <c r="N255" s="3" t="n">
-        <v>46076.37334490741</v>
+        <v>46076.48276620371</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -17008,7 +17003,7 @@
         <v>1</v>
       </c>
       <c r="N256" s="3" t="n">
-        <v>46076.38287037037</v>
+        <v>46076.459375</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17072,7 +17067,7 @@
         <v>1</v>
       </c>
       <c r="N257" s="3" t="n">
-        <v>46076.36767361111</v>
+        <v>46076.48186342593</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17136,7 +17131,7 @@
         <v>1</v>
       </c>
       <c r="N258" s="3" t="n">
-        <v>46076.37356481481</v>
+        <v>46076.47885416666</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
@@ -17200,7 +17195,7 @@
         <v>1</v>
       </c>
       <c r="N259" s="3" t="n">
-        <v>46076.37903935185</v>
+        <v>46076.46366898148</v>
       </c>
       <c r="O259" t="inlineStr">
         <is>
@@ -17264,7 +17259,7 @@
         <v>1</v>
       </c>
       <c r="N260" s="3" t="n">
-        <v>46076.3846412037</v>
+        <v>46076.4662962963</v>
       </c>
       <c r="O260" t="inlineStr">
         <is>
@@ -17328,7 +17323,7 @@
         <v>1</v>
       </c>
       <c r="N261" s="3" t="n">
-        <v>46076.36719907408</v>
+        <v>46076.48005787037</v>
       </c>
       <c r="O261" t="inlineStr">
         <is>
@@ -17392,7 +17387,7 @@
         <v>1</v>
       </c>
       <c r="N262" s="3" t="n">
-        <v>46076.37056712963</v>
+        <v>46076.46555555556</v>
       </c>
       <c r="O262" t="inlineStr">
         <is>
@@ -17456,7 +17451,7 @@
         <v>1</v>
       </c>
       <c r="N263" s="3" t="n">
-        <v>46076.37355324074</v>
+        <v>46076.45444444445</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17520,7 +17515,7 @@
         <v>1</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>46076.37523148148</v>
+        <v>46076.46385416666</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17584,7 +17579,7 @@
         <v>1</v>
       </c>
       <c r="N265" s="3" t="n">
-        <v>46076.39047453704</v>
+        <v>46076.46435185185</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17648,7 +17643,7 @@
         <v>1</v>
       </c>
       <c r="N266" s="3" t="n">
-        <v>46076.38361111111</v>
+        <v>46076.4640625</v>
       </c>
       <c r="O266" t="inlineStr">
         <is>
@@ -17712,7 +17707,7 @@
         <v>1</v>
       </c>
       <c r="N267" s="3" t="n">
-        <v>46076.40107638889</v>
+        <v>46076.47778935185</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17776,7 +17771,7 @@
         <v>1</v>
       </c>
       <c r="N268" s="3" t="n">
-        <v>46076.37640046296</v>
+        <v>46076.45261574074</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17840,7 +17835,7 @@
         <v>1</v>
       </c>
       <c r="N269" s="3" t="n">
-        <v>46074.58395833334</v>
+        <v>46076.46399305556</v>
       </c>
       <c r="O269" t="inlineStr">
         <is>
@@ -17901,7 +17896,7 @@
         </is>
       </c>
       <c r="N270" s="3" t="n">
-        <v>46076.38003472222</v>
+        <v>46076.46225694445</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -18029,7 +18024,7 @@
         <v>1</v>
       </c>
       <c r="N272" s="3" t="n">
-        <v>46076.37087962963</v>
+        <v>46076.48097222222</v>
       </c>
       <c r="O272" t="inlineStr">
         <is>
@@ -18093,7 +18088,7 @@
         <v>2</v>
       </c>
       <c r="N273" s="3" t="n">
-        <v>46076.36805555555</v>
+        <v>46076.48440972222</v>
       </c>
       <c r="O273" t="inlineStr">
         <is>
@@ -18317,7 +18312,7 @@
       </c>
       <c r="F277" t="inlineStr">
         <is>
-          <t>Microsoft Windows 7 Professional</t>
+          <t>Windows</t>
         </is>
       </c>
       <c r="G277" t="inlineStr">
@@ -18349,7 +18344,7 @@
         <v>1</v>
       </c>
       <c r="N277" s="3" t="n">
-        <v>46067.85915509259</v>
+        <v>46076.46351851852</v>
       </c>
       <c r="O277" t="inlineStr">
         <is>
@@ -18413,7 +18408,7 @@
         <v>1</v>
       </c>
       <c r="N278" s="3" t="n">
-        <v>46076.35682870371</v>
+        <v>46076.46240740741</v>
       </c>
       <c r="O278" t="inlineStr">
         <is>
@@ -18477,7 +18472,7 @@
         <v>1</v>
       </c>
       <c r="N279" s="3" t="n">
-        <v>46076.38357638889</v>
+        <v>46076.46746527778</v>
       </c>
       <c r="O279" t="inlineStr">
         <is>
@@ -18541,7 +18536,7 @@
         <v>1</v>
       </c>
       <c r="N280" s="3" t="n">
-        <v>46076.36902777778</v>
+        <v>46076.4794212963</v>
       </c>
       <c r="O280" t="inlineStr">
         <is>
@@ -18605,7 +18600,7 @@
         <v>1</v>
       </c>
       <c r="N281" s="3" t="n">
-        <v>46076.39537037037</v>
+        <v>46076.46917824074</v>
       </c>
       <c r="O281" t="inlineStr">
         <is>
@@ -18669,7 +18664,7 @@
         <v>1</v>
       </c>
       <c r="N282" s="3" t="n">
-        <v>46076.40094907407</v>
+        <v>46076.47899305556</v>
       </c>
       <c r="O282" t="inlineStr">
         <is>
@@ -18733,7 +18728,7 @@
         <v>1</v>
       </c>
       <c r="N283" s="3" t="n">
-        <v>46073.82201388889</v>
+        <v>46076.47173611111</v>
       </c>
       <c r="O283" t="inlineStr">
         <is>
@@ -18797,7 +18792,7 @@
         <v>1</v>
       </c>
       <c r="N284" s="3" t="n">
-        <v>46076.37582175926</v>
+        <v>46076.45292824074</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18861,7 +18856,7 @@
         <v>1</v>
       </c>
       <c r="N285" s="3" t="n">
-        <v>46076.36704861111</v>
+        <v>46076.48324074074</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -18920,7 +18915,7 @@
         <v>1</v>
       </c>
       <c r="N286" s="3" t="n">
-        <v>46076.37554398148</v>
+        <v>46076.45392361111</v>
       </c>
       <c r="O286" t="inlineStr">
         <is>
@@ -18984,7 +18979,7 @@
         <v>1</v>
       </c>
       <c r="N287" s="3" t="n">
-        <v>46076.3978587963</v>
+        <v>46076.47704861111</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
@@ -19048,7 +19043,7 @@
         <v>1</v>
       </c>
       <c r="N288" s="3" t="n">
-        <v>46076.39879629629</v>
+        <v>46076.47400462963</v>
       </c>
       <c r="O288" t="inlineStr">
         <is>
@@ -19112,7 +19107,7 @@
         <v>1</v>
       </c>
       <c r="N289" s="3" t="n">
-        <v>46076.38565972223</v>
+        <v>46076.45912037037</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -19906,7 +19901,7 @@
         <v>1</v>
       </c>
       <c r="N302" s="3" t="n">
-        <v>46076.38511574074</v>
+        <v>46076.46077546296</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -21022,7 +21017,7 @@
         </is>
       </c>
       <c r="N320" s="3" t="n">
-        <v>46076.38111111111</v>
+        <v>46076.46228009259</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21494,7 +21489,7 @@
         <v>2</v>
       </c>
       <c r="N328" s="3" t="n">
-        <v>46076.38509259259</v>
+        <v>46076.46356481482</v>
       </c>
       <c r="O328" t="inlineStr">
         <is>
@@ -21747,7 +21742,7 @@
         <v>1</v>
       </c>
       <c r="N332" s="3" t="n">
-        <v>46076.37414351852</v>
+        <v>46076.45525462963</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21811,7 +21806,7 @@
         <v>2</v>
       </c>
       <c r="N333" s="3" t="n">
-        <v>46076.40237268519</v>
+        <v>46076.47871527778</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21875,7 +21870,7 @@
         <v>2</v>
       </c>
       <c r="N334" s="3" t="n">
-        <v>46076.40386574074</v>
+        <v>46076.47754629629</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21939,7 +21934,7 @@
         <v>2</v>
       </c>
       <c r="N335" s="3" t="n">
-        <v>46076.36516203704</v>
+        <v>46076.48334490741</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -22003,7 +21998,7 @@
         <v>1</v>
       </c>
       <c r="N336" s="3" t="n">
-        <v>46076.38621527778</v>
+        <v>46076.46399305556</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22067,7 +22062,7 @@
         <v>1</v>
       </c>
       <c r="N337" s="3" t="n">
-        <v>46076.3720949074</v>
+        <v>46076.45372685185</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22259,7 +22254,7 @@
         <v>1</v>
       </c>
       <c r="N340" s="3" t="n">
-        <v>46073.83497685185</v>
+        <v>46076.47177083333</v>
       </c>
       <c r="O340" t="inlineStr">
         <is>
@@ -22323,7 +22318,7 @@
         <v>2</v>
       </c>
       <c r="N341" s="3" t="n">
-        <v>46076.37225694444</v>
+        <v>46076.45295138889</v>
       </c>
       <c r="O341" t="inlineStr">
         <is>
@@ -22387,7 +22382,7 @@
         <v>2</v>
       </c>
       <c r="N342" s="3" t="n">
-        <v>46076.37314814814</v>
+        <v>46076.44960648148</v>
       </c>
       <c r="O342" t="inlineStr">
         <is>
@@ -22448,7 +22443,7 @@
         </is>
       </c>
       <c r="N343" s="3" t="n">
-        <v>46076.37824074074</v>
+        <v>46076.4519212963</v>
       </c>
       <c r="O343" t="inlineStr">
         <is>
@@ -22704,7 +22699,7 @@
         <v>1</v>
       </c>
       <c r="N347" s="3" t="n">
-        <v>46076.39743055555</v>
+        <v>46076.47495370371</v>
       </c>
       <c r="O347" t="inlineStr">
         <is>
@@ -22768,7 +22763,7 @@
         <v>2</v>
       </c>
       <c r="N348" s="3" t="n">
-        <v>46076.39991898148</v>
+        <v>46076.48173611111</v>
       </c>
       <c r="O348" t="inlineStr">
         <is>
@@ -22832,7 +22827,7 @@
         <v>1</v>
       </c>
       <c r="N349" s="3" t="n">
-        <v>46076.39965277778</v>
+        <v>46076.47814814815</v>
       </c>
       <c r="O349" t="inlineStr">
         <is>
@@ -22851,6 +22846,11 @@
           <t>OPERACAO 9.1</t>
         </is>
       </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>10.69.5.244</t>
+        </is>
+      </c>
       <c r="D350" t="n">
         <v>2014</v>
       </c>
@@ -22891,7 +22891,7 @@
         <v>1</v>
       </c>
       <c r="N350" s="3" t="n">
-        <v>46073.8572337963</v>
+        <v>46076.47680555555</v>
       </c>
       <c r="O350" t="inlineStr">
         <is>
@@ -22955,7 +22955,7 @@
         <v>1</v>
       </c>
       <c r="N351" s="3" t="n">
-        <v>46076.39960648148</v>
+        <v>46076.48005787037</v>
       </c>
       <c r="O351" t="inlineStr">
         <is>
@@ -23080,7 +23080,7 @@
         </is>
       </c>
       <c r="N353" s="3" t="n">
-        <v>46076.39851851852</v>
+        <v>46076.47542824074</v>
       </c>
       <c r="O353" t="inlineStr">
         <is>
@@ -23141,7 +23141,7 @@
         </is>
       </c>
       <c r="N354" s="3" t="n">
-        <v>46076.39909722222</v>
+        <v>46076.47106481482</v>
       </c>
       <c r="O354" t="inlineStr">
         <is>
@@ -23205,7 +23205,7 @@
         <v>1</v>
       </c>
       <c r="N355" s="3" t="n">
-        <v>46076.39898148148</v>
+        <v>46076.4753587963</v>
       </c>
       <c r="O355" t="inlineStr">
         <is>
@@ -23269,7 +23269,7 @@
         <v>1</v>
       </c>
       <c r="N356" s="3" t="n">
-        <v>46076.39914351852</v>
+        <v>46076.47335648148</v>
       </c>
       <c r="O356" t="inlineStr">
         <is>
@@ -23333,7 +23333,7 @@
         <v>1</v>
       </c>
       <c r="N357" s="3" t="n">
-        <v>46076.39929398148</v>
+        <v>46076.47650462963</v>
       </c>
       <c r="O357" t="inlineStr">
         <is>
@@ -23456,7 +23456,7 @@
         <v>2</v>
       </c>
       <c r="N359" s="3" t="n">
-        <v>46073.38041666667</v>
+        <v>46076.47570601852</v>
       </c>
       <c r="O359" t="inlineStr">
         <is>
@@ -23520,7 +23520,7 @@
         <v>2</v>
       </c>
       <c r="N360" s="3" t="n">
-        <v>46076.40020833333</v>
+        <v>46076.47958333333</v>
       </c>
       <c r="O360" t="inlineStr">
         <is>
@@ -23584,7 +23584,7 @@
         <v>1</v>
       </c>
       <c r="N361" s="3" t="n">
-        <v>46076.39930555555</v>
+        <v>46076.47239583333</v>
       </c>
       <c r="O361" t="inlineStr">
         <is>
@@ -23645,7 +23645,7 @@
         </is>
       </c>
       <c r="N362" s="3" t="n">
-        <v>46076.40010416666</v>
+        <v>46076.47976851852</v>
       </c>
       <c r="O362" t="inlineStr">
         <is>
@@ -23833,7 +23833,7 @@
         <v>1</v>
       </c>
       <c r="N365" s="3" t="n">
-        <v>46076.38391203704</v>
+        <v>46076.46259259259</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
@@ -23899,7 +23899,7 @@
         </is>
       </c>
       <c r="N366" s="3" t="n">
-        <v>46076.37953703704</v>
+        <v>46076.45065972222</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -24025,7 +24025,7 @@
         </is>
       </c>
       <c r="N368" s="3" t="n">
-        <v>46076.36677083333</v>
+        <v>46076.4872800926</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -24086,7 +24086,7 @@
         </is>
       </c>
       <c r="N369" s="3" t="n">
-        <v>46076.38778935185</v>
+        <v>46076.46466435185</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
@@ -24155,7 +24155,7 @@
         <v>1</v>
       </c>
       <c r="N370" s="3" t="n">
-        <v>46076.36671296296</v>
+        <v>46076.48554398148</v>
       </c>
       <c r="O370" t="inlineStr">
         <is>
@@ -24431,7 +24431,7 @@
         <v>1</v>
       </c>
       <c r="N374" s="3" t="n">
-        <v>46076.40206018519</v>
+        <v>46076.48096064815</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24497,7 +24497,7 @@
         </is>
       </c>
       <c r="N375" s="3" t="n">
-        <v>46076.36747685185</v>
+        <v>46076.48295138889</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
@@ -24561,7 +24561,7 @@
         <v>1</v>
       </c>
       <c r="N376" s="3" t="n">
-        <v>46074.36466435185</v>
+        <v>46076.45290509259</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -24630,7 +24630,7 @@
         <v>2</v>
       </c>
       <c r="N377" s="3" t="n">
-        <v>46076.39965277778</v>
+        <v>46076.47452546296</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -24699,7 +24699,7 @@
         <v>2</v>
       </c>
       <c r="N378" s="3" t="n">
-        <v>46076.36771990741</v>
+        <v>46076.48484953704</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização automática 2026-02-23 13:52:05.472211
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>46076.46010416667</v>
+        <v>46076.54010416667</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>46076.45434027778</v>
+        <v>46076.53243055556</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
         <v>1</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>46076.46494212963</v>
+        <v>46076.5433912037</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>46076.45732638889</v>
+        <v>46076.53377314815</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -1131,7 +1131,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="3" t="n">
-        <v>46076.46309027778</v>
+        <v>46076.54002314815</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1451,7 +1451,7 @@
         <v>1</v>
       </c>
       <c r="N15" s="3" t="n">
-        <v>46076.4597337963</v>
+        <v>46076.54248842593</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1515,7 +1515,7 @@
         <v>2</v>
       </c>
       <c r="N16" s="3" t="n">
-        <v>46076.46467592593</v>
+        <v>46076.53747685185</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -2244,7 +2244,7 @@
         </is>
       </c>
       <c r="N28" s="3" t="n">
-        <v>46073.73467592592</v>
+        <v>46076.53777777778</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -6570,7 +6570,7 @@
         <v>1</v>
       </c>
       <c r="N95" s="3" t="n">
-        <v>46076.48091435185</v>
+        <v>46076.55744212963</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -6658,11 +6658,6 @@
           <t>COORDENACAO</t>
         </is>
       </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>10.69.3.93</t>
-        </is>
-      </c>
       <c r="D97" t="n">
         <v>2025</v>
       </c>
@@ -6708,7 +6703,7 @@
         <v>1</v>
       </c>
       <c r="N97" s="3" t="n">
-        <v>46076.47429398148</v>
+        <v>46076.5459375</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -6727,6 +6722,11 @@
           <t>COORDENACAO</t>
         </is>
       </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>10.69.3.94</t>
+        </is>
+      </c>
       <c r="D98" t="n">
         <v>2025</v>
       </c>
@@ -6772,7 +6772,7 @@
         <v>1</v>
       </c>
       <c r="N98" s="3" t="n">
-        <v>46074.55390046296</v>
+        <v>46076.54824074074</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -6841,7 +6841,7 @@
         <v>1</v>
       </c>
       <c r="N99" s="3" t="n">
-        <v>46076.45773148148</v>
+        <v>46076.5365625</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -6910,7 +6910,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>46076.46229166666</v>
+        <v>46076.54109953704</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6979,7 +6979,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="3" t="n">
-        <v>46076.45460648148</v>
+        <v>46076.56746527777</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -7117,7 +7117,7 @@
         <v>2</v>
       </c>
       <c r="N103" s="3" t="n">
-        <v>46076.46105324074</v>
+        <v>46076.53806712963</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7374,7 +7374,7 @@
         <v>1</v>
       </c>
       <c r="N107" s="3" t="n">
-        <v>46076.47574074074</v>
+        <v>46076.55649305556</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -7512,7 +7512,7 @@
         <v>1</v>
       </c>
       <c r="N109" s="3" t="n">
-        <v>46076.46192129629</v>
+        <v>46076.5359375</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7581,7 +7581,7 @@
         <v>2</v>
       </c>
       <c r="N110" s="3" t="n">
-        <v>46076.45964120371</v>
+        <v>46076.53818287037</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7650,7 +7650,7 @@
         <v>2</v>
       </c>
       <c r="N111" s="3" t="n">
-        <v>46076.44972222222</v>
+        <v>46076.56568287037</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
@@ -7719,7 +7719,7 @@
         <v>2</v>
       </c>
       <c r="N112" s="3" t="n">
-        <v>46076.46534722222</v>
+        <v>46076.53931712963</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7788,7 +7788,7 @@
         <v>1</v>
       </c>
       <c r="N113" s="3" t="n">
-        <v>46076.45732638889</v>
+        <v>46076.53738425926</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7857,7 +7857,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>46076.46353009259</v>
+        <v>46076.5359837963</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -7923,7 +7923,7 @@
         </is>
       </c>
       <c r="N115" s="3" t="n">
-        <v>46076.48755787037</v>
+        <v>46076.56570601852</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -7992,7 +7992,7 @@
         <v>1</v>
       </c>
       <c r="N116" s="3" t="n">
-        <v>46076.45684027778</v>
+        <v>46076.53216435185</v>
       </c>
       <c r="O116" t="inlineStr">
         <is>
@@ -8011,11 +8011,6 @@
           <t>DP</t>
         </is>
       </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>10.69.3.23</t>
-        </is>
-      </c>
       <c r="D117" t="n">
         <v>2025</v>
       </c>
@@ -8061,7 +8056,7 @@
         <v>1</v>
       </c>
       <c r="N117" s="3" t="n">
-        <v>46076.47607638889</v>
+        <v>46076.55746527778</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -8265,7 +8260,7 @@
         <v>1</v>
       </c>
       <c r="N120" s="3" t="n">
-        <v>46076.47248842593</v>
+        <v>46076.55422453704</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -8334,7 +8329,7 @@
         <v>1</v>
       </c>
       <c r="N121" s="3" t="n">
-        <v>46074.62326388889</v>
+        <v>46076.52967592593</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -8400,7 +8395,7 @@
         </is>
       </c>
       <c r="N122" s="3" t="n">
-        <v>46076.47775462963</v>
+        <v>46076.55475694445</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -8469,7 +8464,7 @@
         <v>2</v>
       </c>
       <c r="N123" s="3" t="n">
-        <v>46076.46792824074</v>
+        <v>46076.54540509259</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -8538,7 +8533,7 @@
         <v>1</v>
       </c>
       <c r="N124" s="3" t="n">
-        <v>46076.46104166667</v>
+        <v>46076.54096064815</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -8607,7 +8602,7 @@
         <v>1</v>
       </c>
       <c r="N125" s="3" t="n">
-        <v>46076.48505787037</v>
+        <v>46076.56039351852</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -8676,7 +8671,7 @@
         <v>2</v>
       </c>
       <c r="N126" s="3" t="n">
-        <v>46076.45584490741</v>
+        <v>46076.53642361111</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -8745,7 +8740,7 @@
         <v>2</v>
       </c>
       <c r="N127" s="3" t="n">
-        <v>46076.47675925926</v>
+        <v>46076.55905092593</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -8814,7 +8809,7 @@
         <v>1</v>
       </c>
       <c r="N128" s="3" t="n">
-        <v>46076.48275462963</v>
+        <v>46076.55893518519</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -8883,7 +8878,7 @@
         <v>1</v>
       </c>
       <c r="N129" s="3" t="n">
-        <v>46076.47201388889</v>
+        <v>46076.54707175926</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -8952,7 +8947,7 @@
         <v>1</v>
       </c>
       <c r="N130" s="3" t="n">
-        <v>46076.44784722223</v>
+        <v>46076.57059027778</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -9016,7 +9011,7 @@
         <v>1</v>
       </c>
       <c r="N131" s="3" t="n">
-        <v>46076.46447916667</v>
+        <v>46076.53847222222</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -9149,7 +9144,7 @@
         <v>1</v>
       </c>
       <c r="N133" s="3" t="n">
-        <v>46076.45585648148</v>
+        <v>46076.56769675926</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -9213,7 +9208,7 @@
         <v>1</v>
       </c>
       <c r="N134" s="3" t="n">
-        <v>46076.48552083333</v>
+        <v>46076.55701388889</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -9277,7 +9272,7 @@
         <v>1</v>
       </c>
       <c r="N135" s="3" t="n">
-        <v>46076.48787037037</v>
+        <v>46076.56230324074</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -9468,7 +9463,7 @@
         <v>1</v>
       </c>
       <c r="N138" s="3" t="n">
-        <v>46076.45984953704</v>
+        <v>46076.5419212963</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9532,7 +9527,7 @@
         <v>1</v>
       </c>
       <c r="N139" s="3" t="n">
-        <v>46076.47604166667</v>
+        <v>46076.55712962963</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9596,7 +9591,7 @@
         <v>1</v>
       </c>
       <c r="N140" s="3" t="n">
-        <v>46076.46150462963</v>
+        <v>46076.54001157408</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9660,7 +9655,7 @@
         <v>1</v>
       </c>
       <c r="N141" s="3" t="n">
-        <v>46076.4637037037</v>
+        <v>46076.53517361111</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9724,7 +9719,7 @@
         <v>1</v>
       </c>
       <c r="N142" s="3" t="n">
-        <v>46076.45929398148</v>
+        <v>46076.57011574074</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9788,7 +9783,7 @@
         <v>1</v>
       </c>
       <c r="N143" s="3" t="n">
-        <v>46076.45752314815</v>
+        <v>46076.53376157407</v>
       </c>
       <c r="O143" t="inlineStr">
         <is>
@@ -9852,7 +9847,7 @@
         <v>1</v>
       </c>
       <c r="N144" s="3" t="n">
-        <v>46076.46630787037</v>
+        <v>46076.50825231482</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9916,7 +9911,7 @@
         <v>1</v>
       </c>
       <c r="N145" s="3" t="n">
-        <v>46074.59888888889</v>
+        <v>46076.53596064815</v>
       </c>
       <c r="O145" t="inlineStr">
         <is>
@@ -9980,7 +9975,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="3" t="n">
-        <v>46076.48663194444</v>
+        <v>46076.56315972222</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10044,7 +10039,7 @@
         <v>1</v>
       </c>
       <c r="N147" s="3" t="n">
-        <v>46076.48748842593</v>
+        <v>46076.57046296296</v>
       </c>
       <c r="O147" t="inlineStr">
         <is>
@@ -10108,7 +10103,7 @@
         <v>1</v>
       </c>
       <c r="N148" s="3" t="n">
-        <v>46076.45989583333</v>
+        <v>46076.53481481481</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10172,7 +10167,7 @@
         <v>1</v>
       </c>
       <c r="N149" s="3" t="n">
-        <v>46076.47861111111</v>
+        <v>46076.55387731481</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -10236,7 +10231,7 @@
         <v>1</v>
       </c>
       <c r="N150" s="3" t="n">
-        <v>46076.44984953704</v>
+        <v>46076.5662962963</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -10364,7 +10359,7 @@
         <v>1</v>
       </c>
       <c r="N152" s="3" t="n">
-        <v>46076.46966435185</v>
+        <v>46076.54638888889</v>
       </c>
       <c r="O152" t="inlineStr">
         <is>
@@ -10423,7 +10418,7 @@
         <v>1</v>
       </c>
       <c r="N153" s="3" t="n">
-        <v>46076.48702546296</v>
+        <v>46076.56631944444</v>
       </c>
       <c r="O153" t="inlineStr">
         <is>
@@ -10487,7 +10482,7 @@
         <v>1</v>
       </c>
       <c r="N154" s="3" t="n">
-        <v>46076.481875</v>
+        <v>46076.55394675926</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10551,7 +10546,7 @@
         <v>1</v>
       </c>
       <c r="N155" s="3" t="n">
-        <v>46076.47659722222</v>
+        <v>46076.55096064815</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10679,7 +10674,7 @@
         <v>1</v>
       </c>
       <c r="N157" s="3" t="n">
-        <v>46076.4662962963</v>
+        <v>46076.54278935185</v>
       </c>
       <c r="O157" t="inlineStr">
         <is>
@@ -10743,7 +10738,7 @@
         <v>1</v>
       </c>
       <c r="N158" s="3" t="n">
-        <v>46076.47024305556</v>
+        <v>46076.54633101852</v>
       </c>
       <c r="O158" t="inlineStr">
         <is>
@@ -10807,7 +10802,7 @@
         <v>1</v>
       </c>
       <c r="N159" s="3" t="n">
-        <v>46076.48664351852</v>
+        <v>46076.56298611111</v>
       </c>
       <c r="O159" t="inlineStr">
         <is>
@@ -10871,7 +10866,7 @@
         <v>1</v>
       </c>
       <c r="N160" s="3" t="n">
-        <v>46076.46152777778</v>
+        <v>46076.54197916666</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
@@ -10935,7 +10930,7 @@
         <v>1</v>
       </c>
       <c r="N161" s="3" t="n">
-        <v>46076.47998842593</v>
+        <v>46076.56197916667</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -10999,7 +10994,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="3" t="n">
-        <v>46076.4809837963</v>
+        <v>46076.55849537037</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11127,7 +11122,7 @@
         <v>2</v>
       </c>
       <c r="N164" s="3" t="n">
-        <v>46076.48307870371</v>
+        <v>46076.5586574074</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11191,7 +11186,7 @@
         <v>2</v>
       </c>
       <c r="N165" s="3" t="n">
-        <v>46076.48239583334</v>
+        <v>46076.5578587963</v>
       </c>
       <c r="O165" t="inlineStr">
         <is>
@@ -11255,7 +11250,7 @@
         <v>2</v>
       </c>
       <c r="N166" s="3" t="n">
-        <v>46076.46049768518</v>
+        <v>46076.54011574074</v>
       </c>
       <c r="O166" t="inlineStr">
         <is>
@@ -11319,7 +11314,7 @@
         <v>2</v>
       </c>
       <c r="N167" s="3" t="n">
-        <v>46076.4811574074</v>
+        <v>46076.5583449074</v>
       </c>
       <c r="O167" t="inlineStr">
         <is>
@@ -11383,7 +11378,7 @@
         <v>2</v>
       </c>
       <c r="N168" s="3" t="n">
-        <v>46076.48085648148</v>
+        <v>46076.55740740741</v>
       </c>
       <c r="O168" t="inlineStr">
         <is>
@@ -11447,7 +11442,7 @@
         <v>2</v>
       </c>
       <c r="N169" s="3" t="n">
-        <v>46076.4712037037</v>
+        <v>46076.55060185185</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -11511,7 +11506,7 @@
         <v>2</v>
       </c>
       <c r="N170" s="3" t="n">
-        <v>46076.46025462963</v>
+        <v>46076.53918981482</v>
       </c>
       <c r="O170" t="inlineStr">
         <is>
@@ -11575,7 +11570,7 @@
         <v>1</v>
       </c>
       <c r="N171" s="3" t="n">
-        <v>46076.45221064815</v>
+        <v>46076.56560185185</v>
       </c>
       <c r="O171" t="inlineStr">
         <is>
@@ -11639,7 +11634,7 @@
         <v>2</v>
       </c>
       <c r="N172" s="3" t="n">
-        <v>46073.7734837963</v>
+        <v>46076.54409722222</v>
       </c>
       <c r="O172" t="inlineStr">
         <is>
@@ -11703,7 +11698,7 @@
         <v>2</v>
       </c>
       <c r="N173" s="3" t="n">
-        <v>46076.46765046296</v>
+        <v>46076.55678240741</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -11767,7 +11762,7 @@
         <v>2</v>
       </c>
       <c r="N174" s="3" t="n">
-        <v>46076.45219907408</v>
+        <v>46076.548125</v>
       </c>
       <c r="O174" t="inlineStr">
         <is>
@@ -11831,7 +11826,7 @@
         <v>2</v>
       </c>
       <c r="N175" s="3" t="n">
-        <v>46076.45777777778</v>
+        <v>46076.57055555555</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -11895,7 +11890,7 @@
         <v>2</v>
       </c>
       <c r="N176" s="3" t="n">
-        <v>46076.46116898148</v>
+        <v>46076.5503587963</v>
       </c>
       <c r="O176" t="inlineStr">
         <is>
@@ -11959,7 +11954,7 @@
         <v>3</v>
       </c>
       <c r="N177" s="3" t="n">
-        <v>46076.47340277778</v>
+        <v>46076.54762731482</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
@@ -12023,7 +12018,7 @@
         <v>2</v>
       </c>
       <c r="N178" s="3" t="n">
-        <v>46076.47572916667</v>
+        <v>46076.55340277778</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12087,7 +12082,7 @@
         <v>1</v>
       </c>
       <c r="N179" s="3" t="n">
-        <v>46076.46430555556</v>
+        <v>46076.53973379629</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12151,7 +12146,7 @@
         <v>1</v>
       </c>
       <c r="N180" s="3" t="n">
-        <v>46076.46193287037</v>
+        <v>46076.53769675926</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12215,7 +12210,7 @@
         <v>1</v>
       </c>
       <c r="N181" s="3" t="n">
-        <v>46076.45659722222</v>
+        <v>46076.5375</v>
       </c>
       <c r="O181" t="inlineStr">
         <is>
@@ -12540,7 +12535,7 @@
         <v>1</v>
       </c>
       <c r="N186" s="3" t="n">
-        <v>46076.47006944445</v>
+        <v>46076.54494212963</v>
       </c>
       <c r="O186" t="inlineStr">
         <is>
@@ -12604,7 +12599,7 @@
         <v>1</v>
       </c>
       <c r="N187" s="3" t="n">
-        <v>46076.46844907408</v>
+        <v>46076.55138888889</v>
       </c>
       <c r="O187" t="inlineStr">
         <is>
@@ -12668,7 +12663,7 @@
         <v>1</v>
       </c>
       <c r="N188" s="3" t="n">
-        <v>46076.46344907407</v>
+        <v>46076.53636574074</v>
       </c>
       <c r="O188" t="inlineStr">
         <is>
@@ -12791,7 +12786,7 @@
         </is>
       </c>
       <c r="N190" s="3" t="n">
-        <v>46076.47620370371</v>
+        <v>46076.54953703703</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12919,7 +12914,7 @@
         <v>1</v>
       </c>
       <c r="N192" s="3" t="n">
-        <v>46076.46136574074</v>
+        <v>46076.54167824074</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -13044,7 +13039,7 @@
         <v>2</v>
       </c>
       <c r="N194" s="3" t="n">
-        <v>46076.46256944445</v>
+        <v>46076.54108796296</v>
       </c>
       <c r="O194" t="inlineStr">
         <is>
@@ -13108,7 +13103,7 @@
         <v>1</v>
       </c>
       <c r="N195" s="3" t="n">
-        <v>46076.46494212963</v>
+        <v>46076.53942129629</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13172,7 +13167,7 @@
         <v>1</v>
       </c>
       <c r="N196" s="3" t="n">
-        <v>46076.46269675926</v>
+        <v>46076.54025462963</v>
       </c>
       <c r="O196" t="inlineStr">
         <is>
@@ -13236,7 +13231,7 @@
         <v>1</v>
       </c>
       <c r="N197" s="3" t="n">
-        <v>46076.48513888889</v>
+        <v>46076.56050925926</v>
       </c>
       <c r="O197" t="inlineStr">
         <is>
@@ -13489,7 +13484,7 @@
         </is>
       </c>
       <c r="N201" s="3" t="n">
-        <v>46076.46524305556</v>
+        <v>46076.54302083333</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -13553,7 +13548,7 @@
         <v>1</v>
       </c>
       <c r="N202" s="3" t="n">
-        <v>46076.46714120371</v>
+        <v>46076.54390046297</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13617,7 +13612,7 @@
         <v>1</v>
       </c>
       <c r="N203" s="3" t="n">
-        <v>46076.46390046296</v>
+        <v>46076.54571759259</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13681,7 +13676,7 @@
         <v>1</v>
       </c>
       <c r="N204" s="3" t="n">
-        <v>46076.46230324074</v>
+        <v>46076.53758101852</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13745,7 +13740,7 @@
         <v>1</v>
       </c>
       <c r="N205" s="3" t="n">
-        <v>46076.45048611111</v>
+        <v>46076.57086805555</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13809,7 +13804,7 @@
         <v>1</v>
       </c>
       <c r="N206" s="3" t="n">
-        <v>46076.47810185186</v>
+        <v>46076.55782407407</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -13873,7 +13868,7 @@
         <v>1</v>
       </c>
       <c r="N207" s="3" t="n">
-        <v>46076.46299768519</v>
+        <v>46076.5431712963</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -13937,7 +13932,7 @@
         <v>1</v>
       </c>
       <c r="N208" s="3" t="n">
-        <v>46076.46706018518</v>
+        <v>46076.55545138889</v>
       </c>
       <c r="O208" t="inlineStr">
         <is>
@@ -14001,7 +13996,7 @@
         <v>1</v>
       </c>
       <c r="N209" s="3" t="n">
-        <v>46076.48099537037</v>
+        <v>46076.55991898148</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14065,7 +14060,7 @@
         <v>1</v>
       </c>
       <c r="N210" s="3" t="n">
-        <v>46076.45245370371</v>
+        <v>46076.53255787037</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14129,7 +14124,7 @@
         <v>1</v>
       </c>
       <c r="N211" s="3" t="n">
-        <v>46076.47528935185</v>
+        <v>46076.54854166666</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -14193,7 +14188,7 @@
         <v>1</v>
       </c>
       <c r="N212" s="3" t="n">
-        <v>46076.48002314815</v>
+        <v>46076.55622685186</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -14257,7 +14252,7 @@
         <v>1</v>
       </c>
       <c r="N213" s="3" t="n">
-        <v>46076.45547453704</v>
+        <v>46076.53355324074</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
@@ -14385,7 +14380,7 @@
         <v>1</v>
       </c>
       <c r="N215" s="3" t="n">
-        <v>46076.4641550926</v>
+        <v>46076.540625</v>
       </c>
       <c r="O215" t="inlineStr">
         <is>
@@ -14513,7 +14508,7 @@
         <v>1</v>
       </c>
       <c r="N217" s="3" t="n">
-        <v>46076.48747685185</v>
+        <v>46076.56797453704</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14577,7 +14572,7 @@
         <v>1</v>
       </c>
       <c r="N218" s="3" t="n">
-        <v>46076.48255787037</v>
+        <v>46076.55722222223</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14641,7 +14636,7 @@
         <v>1</v>
       </c>
       <c r="N219" s="3" t="n">
-        <v>46076.48050925926</v>
+        <v>46076.55634259259</v>
       </c>
       <c r="O219" t="inlineStr">
         <is>
@@ -14710,7 +14705,7 @@
         <v>1</v>
       </c>
       <c r="N220" s="3" t="n">
-        <v>46076.46270833333</v>
+        <v>46076.54538194444</v>
       </c>
       <c r="O220" t="inlineStr">
         <is>
@@ -14774,7 +14769,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="3" t="n">
-        <v>46076.45180555555</v>
+        <v>46076.56872685185</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14838,7 +14833,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="3" t="n">
-        <v>46076.46674768518</v>
+        <v>46076.54741898148</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -14902,7 +14897,7 @@
         <v>1</v>
       </c>
       <c r="N223" s="3" t="n">
-        <v>46076.48393518518</v>
+        <v>46076.55969907407</v>
       </c>
       <c r="O223" t="inlineStr">
         <is>
@@ -15094,7 +15089,7 @@
         <v>1</v>
       </c>
       <c r="N226" s="3" t="n">
-        <v>46076.48363425926</v>
+        <v>46076.56449074074</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15158,7 +15153,7 @@
         <v>1</v>
       </c>
       <c r="N227" s="3" t="n">
-        <v>46076.46079861111</v>
+        <v>46076.53936342592</v>
       </c>
       <c r="O227" t="inlineStr">
         <is>
@@ -15286,7 +15281,7 @@
         <v>1</v>
       </c>
       <c r="N229" s="3" t="n">
-        <v>46076.46290509259</v>
+        <v>46076.53467592593</v>
       </c>
       <c r="O229" t="inlineStr">
         <is>
@@ -15350,7 +15345,7 @@
         <v>1</v>
       </c>
       <c r="N230" s="3" t="n">
-        <v>46076.46530092593</v>
+        <v>46076.54167824074</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15414,7 +15409,7 @@
         <v>1</v>
       </c>
       <c r="N231" s="3" t="n">
-        <v>46076.48722222223</v>
+        <v>46076.56460648148</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15478,7 +15473,7 @@
         <v>1</v>
       </c>
       <c r="N232" s="3" t="n">
-        <v>46076.48126157407</v>
+        <v>46076.56009259259</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -15542,7 +15537,7 @@
         <v>1</v>
       </c>
       <c r="N233" s="3" t="n">
-        <v>46076.48508101852</v>
+        <v>46076.56648148148</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15606,7 +15601,7 @@
         <v>1</v>
       </c>
       <c r="N234" s="3" t="n">
-        <v>46076.465</v>
+        <v>46076.54587962963</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -15670,7 +15665,7 @@
         <v>1</v>
       </c>
       <c r="N235" s="3" t="n">
-        <v>46076.46431712963</v>
+        <v>46076.54016203704</v>
       </c>
       <c r="O235" t="inlineStr">
         <is>
@@ -15734,7 +15729,7 @@
         <v>1</v>
       </c>
       <c r="N236" s="3" t="n">
-        <v>46076.4627662037</v>
+        <v>46076.53983796296</v>
       </c>
       <c r="O236" t="inlineStr">
         <is>
@@ -15862,7 +15857,7 @@
         <v>1</v>
       </c>
       <c r="N238" s="3" t="n">
-        <v>46076.45822916667</v>
+        <v>46076.53502314815</v>
       </c>
       <c r="O238" t="inlineStr">
         <is>
@@ -15926,7 +15921,7 @@
         <v>1</v>
       </c>
       <c r="N239" s="3" t="n">
-        <v>46076.46243055556</v>
+        <v>46076.53592592593</v>
       </c>
       <c r="O239" t="inlineStr">
         <is>
@@ -15990,7 +15985,7 @@
         <v>1</v>
       </c>
       <c r="N240" s="3" t="n">
-        <v>46076.48121527778</v>
+        <v>46076.56091435185</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16054,7 +16049,7 @@
         <v>1</v>
       </c>
       <c r="N241" s="3" t="n">
-        <v>46076.47552083333</v>
+        <v>46076.55634259259</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16118,7 +16113,7 @@
         <v>1</v>
       </c>
       <c r="N242" s="3" t="n">
-        <v>46076.47951388889</v>
+        <v>46076.55287037037</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16182,7 +16177,7 @@
         <v>1</v>
       </c>
       <c r="N243" s="3" t="n">
-        <v>46076.47988425926</v>
+        <v>46076.55689814815</v>
       </c>
       <c r="O243" t="inlineStr">
         <is>
@@ -16201,11 +16196,6 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
-      <c r="C244" t="inlineStr">
-        <is>
-          <t>10.69.5.112</t>
-        </is>
-      </c>
       <c r="D244" t="n">
         <v>2019</v>
       </c>
@@ -16246,7 +16236,7 @@
         <v>1</v>
       </c>
       <c r="N244" s="3" t="n">
-        <v>46076.46063657408</v>
+        <v>46076.49822916667</v>
       </c>
       <c r="O244" t="inlineStr">
         <is>
@@ -16310,7 +16300,7 @@
         <v>1</v>
       </c>
       <c r="N245" s="3" t="n">
-        <v>46076.45903935185</v>
+        <v>46076.54121527778</v>
       </c>
       <c r="O245" t="inlineStr">
         <is>
@@ -16374,7 +16364,7 @@
         <v>1</v>
       </c>
       <c r="N246" s="3" t="n">
-        <v>46076.46957175926</v>
+        <v>46076.5471875</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16438,7 +16428,7 @@
         <v>1</v>
       </c>
       <c r="N247" s="3" t="n">
-        <v>46076.45015046297</v>
+        <v>46076.56905092593</v>
       </c>
       <c r="O247" t="inlineStr">
         <is>
@@ -16502,7 +16492,7 @@
         <v>1</v>
       </c>
       <c r="N248" s="3" t="n">
-        <v>46076.46511574074</v>
+        <v>46076.54268518519</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16566,7 +16556,7 @@
         <v>1</v>
       </c>
       <c r="N249" s="3" t="n">
-        <v>46076.42236111111</v>
+        <v>46076.56515046296</v>
       </c>
       <c r="O249" t="inlineStr">
         <is>
@@ -16585,6 +16575,11 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>10.69.5.118</t>
+        </is>
+      </c>
       <c r="D250" t="n">
         <v>2017</v>
       </c>
@@ -16625,7 +16620,7 @@
         <v>1</v>
       </c>
       <c r="N250" s="3" t="n">
-        <v>46076.45559027778</v>
+        <v>46076.56996527778</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16689,7 +16684,7 @@
         <v>1</v>
       </c>
       <c r="N251" s="3" t="n">
-        <v>46076.45133101852</v>
+        <v>46076.53515046297</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16753,7 +16748,7 @@
         <v>1</v>
       </c>
       <c r="N252" s="3" t="n">
-        <v>46076.45633101852</v>
+        <v>46076.53644675926</v>
       </c>
       <c r="O252" t="inlineStr">
         <is>
@@ -16817,7 +16812,7 @@
         <v>1</v>
       </c>
       <c r="N253" s="3" t="n">
-        <v>46076.48674768519</v>
+        <v>46076.56925925926</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16875,7 +16870,7 @@
         <v>1</v>
       </c>
       <c r="N254" s="3" t="n">
-        <v>46076.45946759259</v>
+        <v>46076.5334375</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -16939,7 +16934,7 @@
         <v>1</v>
       </c>
       <c r="N255" s="3" t="n">
-        <v>46076.48276620371</v>
+        <v>46076.55907407407</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -17003,7 +16998,7 @@
         <v>1</v>
       </c>
       <c r="N256" s="3" t="n">
-        <v>46076.459375</v>
+        <v>46076.57037037037</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17067,7 +17062,7 @@
         <v>1</v>
       </c>
       <c r="N257" s="3" t="n">
-        <v>46076.48186342593</v>
+        <v>46076.55813657407</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17131,7 +17126,7 @@
         <v>1</v>
       </c>
       <c r="N258" s="3" t="n">
-        <v>46076.47885416666</v>
+        <v>46076.55364583333</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
@@ -17195,7 +17190,7 @@
         <v>1</v>
       </c>
       <c r="N259" s="3" t="n">
-        <v>46076.46366898148</v>
+        <v>46076.54112268519</v>
       </c>
       <c r="O259" t="inlineStr">
         <is>
@@ -17259,7 +17254,7 @@
         <v>1</v>
       </c>
       <c r="N260" s="3" t="n">
-        <v>46076.4662962963</v>
+        <v>46076.54555555555</v>
       </c>
       <c r="O260" t="inlineStr">
         <is>
@@ -17323,7 +17318,7 @@
         <v>1</v>
       </c>
       <c r="N261" s="3" t="n">
-        <v>46076.48005787037</v>
+        <v>46076.55996527777</v>
       </c>
       <c r="O261" t="inlineStr">
         <is>
@@ -17387,7 +17382,7 @@
         <v>1</v>
       </c>
       <c r="N262" s="3" t="n">
-        <v>46076.46555555556</v>
+        <v>46076.53973379629</v>
       </c>
       <c r="O262" t="inlineStr">
         <is>
@@ -17451,7 +17446,7 @@
         <v>1</v>
       </c>
       <c r="N263" s="3" t="n">
-        <v>46076.45444444445</v>
+        <v>46076.56770833334</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17515,7 +17510,7 @@
         <v>1</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>46076.46385416666</v>
+        <v>46076.53751157408</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17579,7 +17574,7 @@
         <v>1</v>
       </c>
       <c r="N265" s="3" t="n">
-        <v>46076.46435185185</v>
+        <v>46076.54226851852</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17643,7 +17638,7 @@
         <v>1</v>
       </c>
       <c r="N266" s="3" t="n">
-        <v>46076.4640625</v>
+        <v>46076.54237268519</v>
       </c>
       <c r="O266" t="inlineStr">
         <is>
@@ -17707,7 +17702,7 @@
         <v>1</v>
       </c>
       <c r="N267" s="3" t="n">
-        <v>46076.47778935185</v>
+        <v>46076.55608796296</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17771,7 +17766,7 @@
         <v>1</v>
       </c>
       <c r="N268" s="3" t="n">
-        <v>46076.45261574074</v>
+        <v>46076.53420138889</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17835,7 +17830,7 @@
         <v>1</v>
       </c>
       <c r="N269" s="3" t="n">
-        <v>46076.46399305556</v>
+        <v>46076.54203703703</v>
       </c>
       <c r="O269" t="inlineStr">
         <is>
@@ -17896,7 +17891,7 @@
         </is>
       </c>
       <c r="N270" s="3" t="n">
-        <v>46076.46225694445</v>
+        <v>46076.5418287037</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -18024,7 +18019,7 @@
         <v>1</v>
       </c>
       <c r="N272" s="3" t="n">
-        <v>46076.48097222222</v>
+        <v>46076.55990740741</v>
       </c>
       <c r="O272" t="inlineStr">
         <is>
@@ -18088,7 +18083,7 @@
         <v>2</v>
       </c>
       <c r="N273" s="3" t="n">
-        <v>46076.48440972222</v>
+        <v>46076.56148148148</v>
       </c>
       <c r="O273" t="inlineStr">
         <is>
@@ -18408,7 +18403,7 @@
         <v>1</v>
       </c>
       <c r="N278" s="3" t="n">
-        <v>46076.46240740741</v>
+        <v>46076.54068287037</v>
       </c>
       <c r="O278" t="inlineStr">
         <is>
@@ -18472,7 +18467,7 @@
         <v>1</v>
       </c>
       <c r="N279" s="3" t="n">
-        <v>46076.46746527778</v>
+        <v>46076.55283564814</v>
       </c>
       <c r="O279" t="inlineStr">
         <is>
@@ -18536,7 +18531,7 @@
         <v>1</v>
       </c>
       <c r="N280" s="3" t="n">
-        <v>46076.4794212963</v>
+        <v>46076.56201388889</v>
       </c>
       <c r="O280" t="inlineStr">
         <is>
@@ -18600,7 +18595,7 @@
         <v>1</v>
       </c>
       <c r="N281" s="3" t="n">
-        <v>46076.46917824074</v>
+        <v>46076.56340277778</v>
       </c>
       <c r="O281" t="inlineStr">
         <is>
@@ -18619,11 +18614,6 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
-      <c r="C282" t="inlineStr">
-        <is>
-          <t>10.69.5.151</t>
-        </is>
-      </c>
       <c r="D282" t="n">
         <v>2017</v>
       </c>
@@ -18664,7 +18654,7 @@
         <v>1</v>
       </c>
       <c r="N282" s="3" t="n">
-        <v>46076.47899305556</v>
+        <v>46076.55696759259</v>
       </c>
       <c r="O282" t="inlineStr">
         <is>
@@ -18728,7 +18718,7 @@
         <v>1</v>
       </c>
       <c r="N283" s="3" t="n">
-        <v>46076.47173611111</v>
+        <v>46076.55039351852</v>
       </c>
       <c r="O283" t="inlineStr">
         <is>
@@ -18792,7 +18782,7 @@
         <v>1</v>
       </c>
       <c r="N284" s="3" t="n">
-        <v>46076.45292824074</v>
+        <v>46076.56969907408</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18856,7 +18846,7 @@
         <v>1</v>
       </c>
       <c r="N285" s="3" t="n">
-        <v>46076.48324074074</v>
+        <v>46076.56288194445</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -18875,6 +18865,11 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>10.69.5.155</t>
+        </is>
+      </c>
       <c r="D286" t="n">
         <v>2019</v>
       </c>
@@ -18915,7 +18910,7 @@
         <v>1</v>
       </c>
       <c r="N286" s="3" t="n">
-        <v>46076.45392361111</v>
+        <v>46076.53315972222</v>
       </c>
       <c r="O286" t="inlineStr">
         <is>
@@ -18979,7 +18974,7 @@
         <v>1</v>
       </c>
       <c r="N287" s="3" t="n">
-        <v>46076.47704861111</v>
+        <v>46076.55369212963</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
@@ -19043,7 +19038,7 @@
         <v>1</v>
       </c>
       <c r="N288" s="3" t="n">
-        <v>46076.47400462963</v>
+        <v>46076.55165509259</v>
       </c>
       <c r="O288" t="inlineStr">
         <is>
@@ -19107,7 +19102,7 @@
         <v>1</v>
       </c>
       <c r="N289" s="3" t="n">
-        <v>46076.45912037037</v>
+        <v>46076.53820601852</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -19901,7 +19896,7 @@
         <v>1</v>
       </c>
       <c r="N302" s="3" t="n">
-        <v>46076.46077546296</v>
+        <v>46076.54359953704</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -21017,7 +21012,7 @@
         </is>
       </c>
       <c r="N320" s="3" t="n">
-        <v>46076.46228009259</v>
+        <v>46076.54170138889</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21489,7 +21484,7 @@
         <v>2</v>
       </c>
       <c r="N328" s="3" t="n">
-        <v>46076.46356481482</v>
+        <v>46076.499375</v>
       </c>
       <c r="O328" t="inlineStr">
         <is>
@@ -21742,7 +21737,7 @@
         <v>1</v>
       </c>
       <c r="N332" s="3" t="n">
-        <v>46076.45525462963</v>
+        <v>46076.57072916667</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21806,7 +21801,7 @@
         <v>2</v>
       </c>
       <c r="N333" s="3" t="n">
-        <v>46076.47871527778</v>
+        <v>46076.55429398148</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21870,7 +21865,7 @@
         <v>2</v>
       </c>
       <c r="N334" s="3" t="n">
-        <v>46076.47754629629</v>
+        <v>46076.55660879629</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21934,7 +21929,7 @@
         <v>2</v>
       </c>
       <c r="N335" s="3" t="n">
-        <v>46076.48334490741</v>
+        <v>46076.56253472222</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -21998,7 +21993,7 @@
         <v>1</v>
       </c>
       <c r="N336" s="3" t="n">
-        <v>46076.46399305556</v>
+        <v>46076.54204861111</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22062,7 +22057,7 @@
         <v>1</v>
       </c>
       <c r="N337" s="3" t="n">
-        <v>46076.45372685185</v>
+        <v>46076.53575231481</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22126,7 +22121,7 @@
         <v>2</v>
       </c>
       <c r="N338" s="3" t="n">
-        <v>46074.50121527778</v>
+        <v>46076.54375</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -22254,7 +22249,7 @@
         <v>1</v>
       </c>
       <c r="N340" s="3" t="n">
-        <v>46076.47177083333</v>
+        <v>46076.54915509259</v>
       </c>
       <c r="O340" t="inlineStr">
         <is>
@@ -22318,7 +22313,7 @@
         <v>2</v>
       </c>
       <c r="N341" s="3" t="n">
-        <v>46076.45295138889</v>
+        <v>46076.53319444445</v>
       </c>
       <c r="O341" t="inlineStr">
         <is>
@@ -22382,7 +22377,7 @@
         <v>2</v>
       </c>
       <c r="N342" s="3" t="n">
-        <v>46076.44960648148</v>
+        <v>46076.56592592593</v>
       </c>
       <c r="O342" t="inlineStr">
         <is>
@@ -22443,7 +22438,7 @@
         </is>
       </c>
       <c r="N343" s="3" t="n">
-        <v>46076.4519212963</v>
+        <v>46076.56715277778</v>
       </c>
       <c r="O343" t="inlineStr">
         <is>
@@ -22699,7 +22694,7 @@
         <v>1</v>
       </c>
       <c r="N347" s="3" t="n">
-        <v>46076.47495370371</v>
+        <v>46076.55487268518</v>
       </c>
       <c r="O347" t="inlineStr">
         <is>
@@ -22763,7 +22758,7 @@
         <v>2</v>
       </c>
       <c r="N348" s="3" t="n">
-        <v>46076.48173611111</v>
+        <v>46076.56197916667</v>
       </c>
       <c r="O348" t="inlineStr">
         <is>
@@ -22827,7 +22822,7 @@
         <v>1</v>
       </c>
       <c r="N349" s="3" t="n">
-        <v>46076.47814814815</v>
+        <v>46076.55619212963</v>
       </c>
       <c r="O349" t="inlineStr">
         <is>
@@ -22891,7 +22886,7 @@
         <v>1</v>
       </c>
       <c r="N350" s="3" t="n">
-        <v>46076.47680555555</v>
+        <v>46076.55013888889</v>
       </c>
       <c r="O350" t="inlineStr">
         <is>
@@ -22955,7 +22950,7 @@
         <v>1</v>
       </c>
       <c r="N351" s="3" t="n">
-        <v>46076.48005787037</v>
+        <v>46076.56006944444</v>
       </c>
       <c r="O351" t="inlineStr">
         <is>
@@ -23080,7 +23075,7 @@
         </is>
       </c>
       <c r="N353" s="3" t="n">
-        <v>46076.47542824074</v>
+        <v>46076.55268518518</v>
       </c>
       <c r="O353" t="inlineStr">
         <is>
@@ -23141,7 +23136,7 @@
         </is>
       </c>
       <c r="N354" s="3" t="n">
-        <v>46076.47106481482</v>
+        <v>46076.5525</v>
       </c>
       <c r="O354" t="inlineStr">
         <is>
@@ -23205,7 +23200,7 @@
         <v>1</v>
       </c>
       <c r="N355" s="3" t="n">
-        <v>46076.4753587963</v>
+        <v>46076.55340277778</v>
       </c>
       <c r="O355" t="inlineStr">
         <is>
@@ -23269,7 +23264,7 @@
         <v>1</v>
       </c>
       <c r="N356" s="3" t="n">
-        <v>46076.47335648148</v>
+        <v>46076.54942129629</v>
       </c>
       <c r="O356" t="inlineStr">
         <is>
@@ -23333,7 +23328,7 @@
         <v>1</v>
       </c>
       <c r="N357" s="3" t="n">
-        <v>46076.47650462963</v>
+        <v>46076.5559375</v>
       </c>
       <c r="O357" t="inlineStr">
         <is>
@@ -23456,7 +23451,7 @@
         <v>2</v>
       </c>
       <c r="N359" s="3" t="n">
-        <v>46076.47570601852</v>
+        <v>46076.55167824074</v>
       </c>
       <c r="O359" t="inlineStr">
         <is>
@@ -23520,7 +23515,7 @@
         <v>2</v>
       </c>
       <c r="N360" s="3" t="n">
-        <v>46076.47958333333</v>
+        <v>46076.56289351852</v>
       </c>
       <c r="O360" t="inlineStr">
         <is>
@@ -23584,7 +23579,7 @@
         <v>1</v>
       </c>
       <c r="N361" s="3" t="n">
-        <v>46076.47239583333</v>
+        <v>46076.545</v>
       </c>
       <c r="O361" t="inlineStr">
         <is>
@@ -23645,7 +23640,7 @@
         </is>
       </c>
       <c r="N362" s="3" t="n">
-        <v>46076.47976851852</v>
+        <v>46076.56197916667</v>
       </c>
       <c r="O362" t="inlineStr">
         <is>
@@ -23833,7 +23828,7 @@
         <v>1</v>
       </c>
       <c r="N365" s="3" t="n">
-        <v>46076.46259259259</v>
+        <v>46076.53888888889</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
@@ -23899,7 +23894,7 @@
         </is>
       </c>
       <c r="N366" s="3" t="n">
-        <v>46076.45065972222</v>
+        <v>46076.57091435185</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -24025,7 +24020,7 @@
         </is>
       </c>
       <c r="N368" s="3" t="n">
-        <v>46076.4872800926</v>
+        <v>46076.56447916666</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -24044,6 +24039,11 @@
           <t>RH</t>
         </is>
       </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>10.69.3.13</t>
+        </is>
+      </c>
       <c r="D369" t="n">
         <v>2025</v>
       </c>
@@ -24086,7 +24086,7 @@
         </is>
       </c>
       <c r="N369" s="3" t="n">
-        <v>46076.46466435185</v>
+        <v>46076.56546296296</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
@@ -24155,7 +24155,7 @@
         <v>1</v>
       </c>
       <c r="N370" s="3" t="n">
-        <v>46076.48554398148</v>
+        <v>46076.56341435185</v>
       </c>
       <c r="O370" t="inlineStr">
         <is>
@@ -24224,7 +24224,7 @@
         <v>1</v>
       </c>
       <c r="N371" s="3" t="n">
-        <v>46072.6978125</v>
+        <v>46076.55736111111</v>
       </c>
       <c r="O371" t="inlineStr">
         <is>
@@ -24293,7 +24293,7 @@
         <v>1</v>
       </c>
       <c r="N372" s="3" t="n">
-        <v>46073.62052083333</v>
+        <v>46076.49737268518</v>
       </c>
       <c r="O372" t="inlineStr">
         <is>
@@ -24431,7 +24431,7 @@
         <v>1</v>
       </c>
       <c r="N374" s="3" t="n">
-        <v>46076.48096064815</v>
+        <v>46076.55920138889</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24497,7 +24497,7 @@
         </is>
       </c>
       <c r="N375" s="3" t="n">
-        <v>46076.48295138889</v>
+        <v>46076.5575462963</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
@@ -24561,7 +24561,7 @@
         <v>1</v>
       </c>
       <c r="N376" s="3" t="n">
-        <v>46076.45290509259</v>
+        <v>46076.53585648148</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -24630,7 +24630,7 @@
         <v>2</v>
       </c>
       <c r="N377" s="3" t="n">
-        <v>46076.47452546296</v>
+        <v>46076.54520833334</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -24699,7 +24699,7 @@
         <v>2</v>
       </c>
       <c r="N378" s="3" t="n">
-        <v>46076.48484953704</v>
+        <v>46076.56415509259</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização automática 2026-02-23 15:52:05.099872
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>46076.54010416667</v>
+        <v>46076.62174768518</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>46076.53243055556</v>
+        <v>46076.6159375</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -739,10 +739,10 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>46076.5433912037</v>
+        <v>46076.61898148148</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>46076.53377314815</v>
+        <v>46076.64954861111</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -1131,7 +1131,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="3" t="n">
-        <v>46076.54002314815</v>
+        <v>46076.62016203703</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1451,7 +1451,7 @@
         <v>1</v>
       </c>
       <c r="N15" s="3" t="n">
-        <v>46076.54248842593</v>
+        <v>46076.6172337963</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1515,7 +1515,7 @@
         <v>2</v>
       </c>
       <c r="N16" s="3" t="n">
-        <v>46076.53747685185</v>
+        <v>46076.64849537037</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -2244,7 +2244,7 @@
         </is>
       </c>
       <c r="N28" s="3" t="n">
-        <v>46076.53777777778</v>
+        <v>46076.61978009259</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -6570,7 +6570,7 @@
         <v>1</v>
       </c>
       <c r="N95" s="3" t="n">
-        <v>46076.55744212963</v>
+        <v>46076.63108796296</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -6703,7 +6703,7 @@
         <v>1</v>
       </c>
       <c r="N97" s="3" t="n">
-        <v>46076.5459375</v>
+        <v>46076.62237268518</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -6722,11 +6722,6 @@
           <t>COORDENACAO</t>
         </is>
       </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>10.69.3.94</t>
-        </is>
-      </c>
       <c r="D98" t="n">
         <v>2025</v>
       </c>
@@ -6772,7 +6767,7 @@
         <v>1</v>
       </c>
       <c r="N98" s="3" t="n">
-        <v>46076.54824074074</v>
+        <v>46076.64125</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -6841,7 +6836,7 @@
         <v>1</v>
       </c>
       <c r="N99" s="3" t="n">
-        <v>46076.5365625</v>
+        <v>46076.64931712963</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -6910,7 +6905,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>46076.54109953704</v>
+        <v>46076.62208333334</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6979,7 +6974,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="3" t="n">
-        <v>46076.56746527777</v>
+        <v>46076.64755787037</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -7117,7 +7112,7 @@
         <v>2</v>
       </c>
       <c r="N103" s="3" t="n">
-        <v>46076.53806712963</v>
+        <v>46076.62075231481</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7374,7 +7369,7 @@
         <v>1</v>
       </c>
       <c r="N107" s="3" t="n">
-        <v>46076.55649305556</v>
+        <v>46076.63592592593</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -7512,7 +7507,7 @@
         <v>1</v>
       </c>
       <c r="N109" s="3" t="n">
-        <v>46076.5359375</v>
+        <v>46076.6528587963</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7581,7 +7576,7 @@
         <v>2</v>
       </c>
       <c r="N110" s="3" t="n">
-        <v>46076.53818287037</v>
+        <v>46076.61557870371</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7650,7 +7645,7 @@
         <v>2</v>
       </c>
       <c r="N111" s="3" t="n">
-        <v>46076.56568287037</v>
+        <v>46076.64653935185</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
@@ -7719,7 +7714,7 @@
         <v>2</v>
       </c>
       <c r="N112" s="3" t="n">
-        <v>46076.53931712963</v>
+        <v>46076.62054398148</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7788,7 +7783,7 @@
         <v>1</v>
       </c>
       <c r="N113" s="3" t="n">
-        <v>46076.53738425926</v>
+        <v>46076.61407407407</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7857,7 +7852,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>46076.5359837963</v>
+        <v>46076.61668981481</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -7923,7 +7918,7 @@
         </is>
       </c>
       <c r="N115" s="3" t="n">
-        <v>46076.56570601852</v>
+        <v>46076.64203703704</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -7992,7 +7987,7 @@
         <v>1</v>
       </c>
       <c r="N116" s="3" t="n">
-        <v>46076.53216435185</v>
+        <v>46076.57146990741</v>
       </c>
       <c r="O116" t="inlineStr">
         <is>
@@ -8056,7 +8051,7 @@
         <v>1</v>
       </c>
       <c r="N117" s="3" t="n">
-        <v>46076.55746527778</v>
+        <v>46076.63361111111</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -8260,7 +8255,7 @@
         <v>1</v>
       </c>
       <c r="N120" s="3" t="n">
-        <v>46076.55422453704</v>
+        <v>46076.6290625</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -8329,7 +8324,7 @@
         <v>1</v>
       </c>
       <c r="N121" s="3" t="n">
-        <v>46076.52967592593</v>
+        <v>46076.62424768518</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -8395,7 +8390,7 @@
         </is>
       </c>
       <c r="N122" s="3" t="n">
-        <v>46076.55475694445</v>
+        <v>46076.63138888889</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -8464,7 +8459,7 @@
         <v>2</v>
       </c>
       <c r="N123" s="3" t="n">
-        <v>46076.54540509259</v>
+        <v>46076.6203587963</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -8533,7 +8528,7 @@
         <v>1</v>
       </c>
       <c r="N124" s="3" t="n">
-        <v>46076.54096064815</v>
+        <v>46076.62162037037</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -8602,7 +8597,7 @@
         <v>1</v>
       </c>
       <c r="N125" s="3" t="n">
-        <v>46076.56039351852</v>
+        <v>46076.64115740741</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -8671,7 +8666,7 @@
         <v>2</v>
       </c>
       <c r="N126" s="3" t="n">
-        <v>46076.53642361111</v>
+        <v>46076.65291666667</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -8740,7 +8735,7 @@
         <v>2</v>
       </c>
       <c r="N127" s="3" t="n">
-        <v>46076.55905092593</v>
+        <v>46076.63615740741</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -8809,7 +8804,7 @@
         <v>1</v>
       </c>
       <c r="N128" s="3" t="n">
-        <v>46076.55893518519</v>
+        <v>46076.63902777778</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -8878,7 +8873,7 @@
         <v>1</v>
       </c>
       <c r="N129" s="3" t="n">
-        <v>46076.54707175926</v>
+        <v>46076.62640046296</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -8947,7 +8942,7 @@
         <v>1</v>
       </c>
       <c r="N130" s="3" t="n">
-        <v>46076.57059027778</v>
+        <v>46076.64973379629</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -8966,6 +8961,11 @@
           <t>ADM/FIN</t>
         </is>
       </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>10.69.3.6</t>
+        </is>
+      </c>
       <c r="D131" t="n">
         <v>2025</v>
       </c>
@@ -9011,7 +9011,7 @@
         <v>1</v>
       </c>
       <c r="N131" s="3" t="n">
-        <v>46076.53847222222</v>
+        <v>46076.65296296297</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -9144,7 +9144,7 @@
         <v>1</v>
       </c>
       <c r="N133" s="3" t="n">
-        <v>46076.56769675926</v>
+        <v>46076.64174768519</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -9208,7 +9208,7 @@
         <v>1</v>
       </c>
       <c r="N134" s="3" t="n">
-        <v>46076.55701388889</v>
+        <v>46076.63530092593</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -9272,7 +9272,7 @@
         <v>1</v>
       </c>
       <c r="N135" s="3" t="n">
-        <v>46076.56230324074</v>
+        <v>46076.64398148148</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -9463,7 +9463,7 @@
         <v>1</v>
       </c>
       <c r="N138" s="3" t="n">
-        <v>46076.5419212963</v>
+        <v>46076.61931712963</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9527,7 +9527,7 @@
         <v>1</v>
       </c>
       <c r="N139" s="3" t="n">
-        <v>46076.55712962963</v>
+        <v>46076.62423611111</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9591,7 +9591,7 @@
         <v>1</v>
       </c>
       <c r="N140" s="3" t="n">
-        <v>46076.54001157408</v>
+        <v>46076.61430555556</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9655,7 +9655,7 @@
         <v>1</v>
       </c>
       <c r="N141" s="3" t="n">
-        <v>46076.53517361111</v>
+        <v>46076.64740740741</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9719,7 +9719,7 @@
         <v>1</v>
       </c>
       <c r="N142" s="3" t="n">
-        <v>46076.57011574074</v>
+        <v>46076.64795138889</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9783,7 +9783,7 @@
         <v>1</v>
       </c>
       <c r="N143" s="3" t="n">
-        <v>46076.53376157407</v>
+        <v>46076.64767361111</v>
       </c>
       <c r="O143" t="inlineStr">
         <is>
@@ -9847,7 +9847,7 @@
         <v>1</v>
       </c>
       <c r="N144" s="3" t="n">
-        <v>46076.50825231482</v>
+        <v>46076.65340277777</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9911,7 +9911,7 @@
         <v>1</v>
       </c>
       <c r="N145" s="3" t="n">
-        <v>46076.53596064815</v>
+        <v>46076.61836805556</v>
       </c>
       <c r="O145" t="inlineStr">
         <is>
@@ -9975,7 +9975,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="3" t="n">
-        <v>46076.56315972222</v>
+        <v>46076.62509259259</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10039,7 +10039,7 @@
         <v>1</v>
       </c>
       <c r="N147" s="3" t="n">
-        <v>46076.57046296296</v>
+        <v>46076.62274305556</v>
       </c>
       <c r="O147" t="inlineStr">
         <is>
@@ -10103,7 +10103,7 @@
         <v>1</v>
       </c>
       <c r="N148" s="3" t="n">
-        <v>46076.53481481481</v>
+        <v>46076.64905092592</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10167,7 +10167,7 @@
         <v>1</v>
       </c>
       <c r="N149" s="3" t="n">
-        <v>46076.55387731481</v>
+        <v>46076.63042824074</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -10231,7 +10231,7 @@
         <v>1</v>
       </c>
       <c r="N150" s="3" t="n">
-        <v>46076.5662962963</v>
+        <v>46076.62450231481</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -10295,7 +10295,7 @@
         <v>1</v>
       </c>
       <c r="N151" s="3" t="n">
-        <v>46074.61783564815</v>
+        <v>46076.62344907408</v>
       </c>
       <c r="O151" t="inlineStr">
         <is>
@@ -10359,7 +10359,7 @@
         <v>1</v>
       </c>
       <c r="N152" s="3" t="n">
-        <v>46076.54638888889</v>
+        <v>46076.62681712963</v>
       </c>
       <c r="O152" t="inlineStr">
         <is>
@@ -10418,7 +10418,7 @@
         <v>1</v>
       </c>
       <c r="N153" s="3" t="n">
-        <v>46076.56631944444</v>
+        <v>46076.64209490741</v>
       </c>
       <c r="O153" t="inlineStr">
         <is>
@@ -10482,7 +10482,7 @@
         <v>1</v>
       </c>
       <c r="N154" s="3" t="n">
-        <v>46076.55394675926</v>
+        <v>46076.62351851852</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10546,7 +10546,7 @@
         <v>1</v>
       </c>
       <c r="N155" s="3" t="n">
-        <v>46076.55096064815</v>
+        <v>46076.62349537037</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10610,7 +10610,7 @@
         <v>1</v>
       </c>
       <c r="N156" s="3" t="n">
-        <v>46074.41208333334</v>
+        <v>46076.64444444444</v>
       </c>
       <c r="O156" t="inlineStr">
         <is>
@@ -10674,7 +10674,7 @@
         <v>1</v>
       </c>
       <c r="N157" s="3" t="n">
-        <v>46076.54278935185</v>
+        <v>46076.59125</v>
       </c>
       <c r="O157" t="inlineStr">
         <is>
@@ -10802,7 +10802,7 @@
         <v>1</v>
       </c>
       <c r="N159" s="3" t="n">
-        <v>46076.56298611111</v>
+        <v>46076.58689814815</v>
       </c>
       <c r="O159" t="inlineStr">
         <is>
@@ -10866,7 +10866,7 @@
         <v>1</v>
       </c>
       <c r="N160" s="3" t="n">
-        <v>46076.54197916666</v>
+        <v>46076.62219907407</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
@@ -10930,7 +10930,7 @@
         <v>1</v>
       </c>
       <c r="N161" s="3" t="n">
-        <v>46076.56197916667</v>
+        <v>46076.65434027778</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -10994,7 +10994,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="3" t="n">
-        <v>46076.55849537037</v>
+        <v>46076.63366898148</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11122,7 +11122,7 @@
         <v>2</v>
       </c>
       <c r="N164" s="3" t="n">
-        <v>46076.5586574074</v>
+        <v>46076.63585648148</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11186,7 +11186,7 @@
         <v>2</v>
       </c>
       <c r="N165" s="3" t="n">
-        <v>46076.5578587963</v>
+        <v>46076.63103009259</v>
       </c>
       <c r="O165" t="inlineStr">
         <is>
@@ -11250,7 +11250,7 @@
         <v>2</v>
       </c>
       <c r="N166" s="3" t="n">
-        <v>46076.54011574074</v>
+        <v>46076.61715277778</v>
       </c>
       <c r="O166" t="inlineStr">
         <is>
@@ -11314,7 +11314,7 @@
         <v>2</v>
       </c>
       <c r="N167" s="3" t="n">
-        <v>46076.5583449074</v>
+        <v>46076.60028935185</v>
       </c>
       <c r="O167" t="inlineStr">
         <is>
@@ -11442,7 +11442,7 @@
         <v>2</v>
       </c>
       <c r="N169" s="3" t="n">
-        <v>46076.55060185185</v>
+        <v>46076.63003472222</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -11506,7 +11506,7 @@
         <v>2</v>
       </c>
       <c r="N170" s="3" t="n">
-        <v>46076.53918981482</v>
+        <v>46076.65351851852</v>
       </c>
       <c r="O170" t="inlineStr">
         <is>
@@ -11634,7 +11634,7 @@
         <v>2</v>
       </c>
       <c r="N172" s="3" t="n">
-        <v>46076.54409722222</v>
+        <v>46076.61944444444</v>
       </c>
       <c r="O172" t="inlineStr">
         <is>
@@ -11695,10 +11695,10 @@
         </is>
       </c>
       <c r="M173" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N173" s="3" t="n">
-        <v>46076.55678240741</v>
+        <v>46076.63251157408</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -11826,7 +11826,7 @@
         <v>2</v>
       </c>
       <c r="N175" s="3" t="n">
-        <v>46076.57055555555</v>
+        <v>46076.64849537037</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -11890,7 +11890,7 @@
         <v>2</v>
       </c>
       <c r="N176" s="3" t="n">
-        <v>46076.5503587963</v>
+        <v>46076.62503472222</v>
       </c>
       <c r="O176" t="inlineStr">
         <is>
@@ -11954,7 +11954,7 @@
         <v>3</v>
       </c>
       <c r="N177" s="3" t="n">
-        <v>46076.54762731482</v>
+        <v>46076.62358796296</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
@@ -12018,7 +12018,7 @@
         <v>2</v>
       </c>
       <c r="N178" s="3" t="n">
-        <v>46076.55340277778</v>
+        <v>46076.62872685185</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12082,7 +12082,7 @@
         <v>1</v>
       </c>
       <c r="N179" s="3" t="n">
-        <v>46076.53973379629</v>
+        <v>46076.63115740741</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12146,7 +12146,7 @@
         <v>1</v>
       </c>
       <c r="N180" s="3" t="n">
-        <v>46076.53769675926</v>
+        <v>46076.62260416667</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12210,7 +12210,7 @@
         <v>1</v>
       </c>
       <c r="N181" s="3" t="n">
-        <v>46076.5375</v>
+        <v>46076.62090277778</v>
       </c>
       <c r="O181" t="inlineStr">
         <is>
@@ -12663,7 +12663,7 @@
         <v>1</v>
       </c>
       <c r="N188" s="3" t="n">
-        <v>46076.53636574074</v>
+        <v>46076.57655092593</v>
       </c>
       <c r="O188" t="inlineStr">
         <is>
@@ -12749,6 +12749,11 @@
           <t>OPERACAO 8.1</t>
         </is>
       </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>10.69.5.59</t>
+        </is>
+      </c>
       <c r="D190" t="n">
         <v>2015</v>
       </c>
@@ -12786,7 +12791,7 @@
         </is>
       </c>
       <c r="N190" s="3" t="n">
-        <v>46076.54953703703</v>
+        <v>46076.62475694445</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12850,7 +12855,7 @@
         <v>1</v>
       </c>
       <c r="N191" s="3" t="n">
-        <v>46074.61650462963</v>
+        <v>46076.64664351852</v>
       </c>
       <c r="O191" t="inlineStr">
         <is>
@@ -12914,7 +12919,7 @@
         <v>1</v>
       </c>
       <c r="N192" s="3" t="n">
-        <v>46076.54167824074</v>
+        <v>46076.62076388889</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -13039,7 +13044,7 @@
         <v>2</v>
       </c>
       <c r="N194" s="3" t="n">
-        <v>46076.54108796296</v>
+        <v>46076.62033564815</v>
       </c>
       <c r="O194" t="inlineStr">
         <is>
@@ -13103,7 +13108,7 @@
         <v>1</v>
       </c>
       <c r="N195" s="3" t="n">
-        <v>46076.53942129629</v>
+        <v>46076.6516550926</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13167,7 +13172,7 @@
         <v>1</v>
       </c>
       <c r="N196" s="3" t="n">
-        <v>46076.54025462963</v>
+        <v>46076.62753472223</v>
       </c>
       <c r="O196" t="inlineStr">
         <is>
@@ -13231,7 +13236,7 @@
         <v>1</v>
       </c>
       <c r="N197" s="3" t="n">
-        <v>46076.56050925926</v>
+        <v>46076.63592592593</v>
       </c>
       <c r="O197" t="inlineStr">
         <is>
@@ -13423,7 +13428,7 @@
         <v>1</v>
       </c>
       <c r="N200" s="3" t="n">
-        <v>46073.82743055555</v>
+        <v>46076.63383101852</v>
       </c>
       <c r="O200" t="inlineStr">
         <is>
@@ -13484,7 +13489,7 @@
         </is>
       </c>
       <c r="N201" s="3" t="n">
-        <v>46076.54302083333</v>
+        <v>46076.62509259259</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -13548,7 +13553,7 @@
         <v>1</v>
       </c>
       <c r="N202" s="3" t="n">
-        <v>46076.54390046297</v>
+        <v>46076.62814814815</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13612,7 +13617,7 @@
         <v>1</v>
       </c>
       <c r="N203" s="3" t="n">
-        <v>46076.54571759259</v>
+        <v>46076.62922453704</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13676,7 +13681,7 @@
         <v>1</v>
       </c>
       <c r="N204" s="3" t="n">
-        <v>46076.53758101852</v>
+        <v>46076.65252314815</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13740,7 +13745,7 @@
         <v>1</v>
       </c>
       <c r="N205" s="3" t="n">
-        <v>46076.57086805555</v>
+        <v>46076.65001157407</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13804,7 +13809,7 @@
         <v>1</v>
       </c>
       <c r="N206" s="3" t="n">
-        <v>46076.55782407407</v>
+        <v>46076.63614583333</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -13868,7 +13873,7 @@
         <v>1</v>
       </c>
       <c r="N207" s="3" t="n">
-        <v>46076.5431712963</v>
+        <v>46076.6211574074</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -13932,7 +13937,7 @@
         <v>1</v>
       </c>
       <c r="N208" s="3" t="n">
-        <v>46076.55545138889</v>
+        <v>46076.63375</v>
       </c>
       <c r="O208" t="inlineStr">
         <is>
@@ -13996,7 +14001,7 @@
         <v>1</v>
       </c>
       <c r="N209" s="3" t="n">
-        <v>46076.55991898148</v>
+        <v>46076.65446759259</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14060,7 +14065,7 @@
         <v>1</v>
       </c>
       <c r="N210" s="3" t="n">
-        <v>46076.53255787037</v>
+        <v>46076.64767361111</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14124,7 +14129,7 @@
         <v>1</v>
       </c>
       <c r="N211" s="3" t="n">
-        <v>46076.54854166666</v>
+        <v>46076.62603009259</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -14188,7 +14193,7 @@
         <v>1</v>
       </c>
       <c r="N212" s="3" t="n">
-        <v>46076.55622685186</v>
+        <v>46076.65055555556</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -14252,7 +14257,7 @@
         <v>1</v>
       </c>
       <c r="N213" s="3" t="n">
-        <v>46076.53355324074</v>
+        <v>46076.57293981482</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
@@ -14444,7 +14449,7 @@
         <v>1</v>
       </c>
       <c r="N216" s="3" t="n">
-        <v>46076.40200231481</v>
+        <v>46076.62444444445</v>
       </c>
       <c r="O216" t="inlineStr">
         <is>
@@ -14508,7 +14513,7 @@
         <v>1</v>
       </c>
       <c r="N217" s="3" t="n">
-        <v>46076.56797453704</v>
+        <v>46076.64662037037</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14572,7 +14577,7 @@
         <v>1</v>
       </c>
       <c r="N218" s="3" t="n">
-        <v>46076.55722222223</v>
+        <v>46076.63247685185</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14636,7 +14641,7 @@
         <v>1</v>
       </c>
       <c r="N219" s="3" t="n">
-        <v>46076.55634259259</v>
+        <v>46076.65370370371</v>
       </c>
       <c r="O219" t="inlineStr">
         <is>
@@ -14705,7 +14710,7 @@
         <v>1</v>
       </c>
       <c r="N220" s="3" t="n">
-        <v>46076.54538194444</v>
+        <v>46076.62596064815</v>
       </c>
       <c r="O220" t="inlineStr">
         <is>
@@ -14769,7 +14774,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="3" t="n">
-        <v>46076.56872685185</v>
+        <v>46076.64355324074</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14833,7 +14838,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="3" t="n">
-        <v>46076.54741898148</v>
+        <v>46076.62918981481</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -14897,7 +14902,7 @@
         <v>1</v>
       </c>
       <c r="N223" s="3" t="n">
-        <v>46076.55969907407</v>
+        <v>46076.62484953704</v>
       </c>
       <c r="O223" t="inlineStr">
         <is>
@@ -15025,7 +15030,7 @@
         <v>1</v>
       </c>
       <c r="N225" s="3" t="n">
-        <v>46074.60195601852</v>
+        <v>46076.63336805555</v>
       </c>
       <c r="O225" t="inlineStr">
         <is>
@@ -15089,7 +15094,7 @@
         <v>1</v>
       </c>
       <c r="N226" s="3" t="n">
-        <v>46076.56449074074</v>
+        <v>46076.61984953703</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15153,7 +15158,7 @@
         <v>1</v>
       </c>
       <c r="N227" s="3" t="n">
-        <v>46076.53936342592</v>
+        <v>46076.61541666667</v>
       </c>
       <c r="O227" t="inlineStr">
         <is>
@@ -15217,7 +15222,7 @@
         <v>1</v>
       </c>
       <c r="N228" s="3" t="n">
-        <v>46074.60641203704</v>
+        <v>46076.63694444444</v>
       </c>
       <c r="O228" t="inlineStr">
         <is>
@@ -15281,7 +15286,7 @@
         <v>1</v>
       </c>
       <c r="N229" s="3" t="n">
-        <v>46076.53467592593</v>
+        <v>46076.65481481481</v>
       </c>
       <c r="O229" t="inlineStr">
         <is>
@@ -15345,7 +15350,7 @@
         <v>1</v>
       </c>
       <c r="N230" s="3" t="n">
-        <v>46076.54167824074</v>
+        <v>46076.62137731481</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15409,7 +15414,7 @@
         <v>1</v>
       </c>
       <c r="N231" s="3" t="n">
-        <v>46076.56460648148</v>
+        <v>46076.65460648148</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15473,7 +15478,7 @@
         <v>1</v>
       </c>
       <c r="N232" s="3" t="n">
-        <v>46076.56009259259</v>
+        <v>46076.61415509259</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -15537,7 +15542,7 @@
         <v>1</v>
       </c>
       <c r="N233" s="3" t="n">
-        <v>46076.56648148148</v>
+        <v>46076.65479166667</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15601,7 +15606,7 @@
         <v>1</v>
       </c>
       <c r="N234" s="3" t="n">
-        <v>46076.54587962963</v>
+        <v>46076.62622685185</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -15665,7 +15670,7 @@
         <v>1</v>
       </c>
       <c r="N235" s="3" t="n">
-        <v>46076.54016203704</v>
+        <v>46076.61657407408</v>
       </c>
       <c r="O235" t="inlineStr">
         <is>
@@ -15729,7 +15734,7 @@
         <v>1</v>
       </c>
       <c r="N236" s="3" t="n">
-        <v>46076.53983796296</v>
+        <v>46076.65402777777</v>
       </c>
       <c r="O236" t="inlineStr">
         <is>
@@ -15793,7 +15798,7 @@
         <v>1</v>
       </c>
       <c r="N237" s="3" t="n">
-        <v>46076.38482638889</v>
+        <v>46076.63473379629</v>
       </c>
       <c r="O237" t="inlineStr">
         <is>
@@ -15857,7 +15862,7 @@
         <v>1</v>
       </c>
       <c r="N238" s="3" t="n">
-        <v>46076.53502314815</v>
+        <v>46076.64681712963</v>
       </c>
       <c r="O238" t="inlineStr">
         <is>
@@ -15921,7 +15926,7 @@
         <v>1</v>
       </c>
       <c r="N239" s="3" t="n">
-        <v>46076.53592592593</v>
+        <v>46076.64993055556</v>
       </c>
       <c r="O239" t="inlineStr">
         <is>
@@ -15985,7 +15990,7 @@
         <v>1</v>
       </c>
       <c r="N240" s="3" t="n">
-        <v>46076.56091435185</v>
+        <v>46076.65480324074</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16049,7 +16054,7 @@
         <v>1</v>
       </c>
       <c r="N241" s="3" t="n">
-        <v>46076.55634259259</v>
+        <v>46076.59208333334</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16113,7 +16118,7 @@
         <v>1</v>
       </c>
       <c r="N242" s="3" t="n">
-        <v>46076.55287037037</v>
+        <v>46076.63688657407</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16177,7 +16182,7 @@
         <v>1</v>
       </c>
       <c r="N243" s="3" t="n">
-        <v>46076.55689814815</v>
+        <v>46076.63490740741</v>
       </c>
       <c r="O243" t="inlineStr">
         <is>
@@ -16196,6 +16201,11 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>10.69.5.112</t>
+        </is>
+      </c>
       <c r="D244" t="n">
         <v>2019</v>
       </c>
@@ -16236,7 +16246,7 @@
         <v>1</v>
       </c>
       <c r="N244" s="3" t="n">
-        <v>46076.49822916667</v>
+        <v>46076.65324074074</v>
       </c>
       <c r="O244" t="inlineStr">
         <is>
@@ -16300,7 +16310,7 @@
         <v>1</v>
       </c>
       <c r="N245" s="3" t="n">
-        <v>46076.54121527778</v>
+        <v>46076.62033564815</v>
       </c>
       <c r="O245" t="inlineStr">
         <is>
@@ -16364,7 +16374,7 @@
         <v>1</v>
       </c>
       <c r="N246" s="3" t="n">
-        <v>46076.5471875</v>
+        <v>46076.62333333334</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16428,7 +16438,7 @@
         <v>1</v>
       </c>
       <c r="N247" s="3" t="n">
-        <v>46076.56905092593</v>
+        <v>46076.62175925926</v>
       </c>
       <c r="O247" t="inlineStr">
         <is>
@@ -16492,7 +16502,7 @@
         <v>1</v>
       </c>
       <c r="N248" s="3" t="n">
-        <v>46076.54268518519</v>
+        <v>46076.6221412037</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16556,7 +16566,7 @@
         <v>1</v>
       </c>
       <c r="N249" s="3" t="n">
-        <v>46076.56515046296</v>
+        <v>46076.64736111111</v>
       </c>
       <c r="O249" t="inlineStr">
         <is>
@@ -16575,11 +16585,6 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
-      <c r="C250" t="inlineStr">
-        <is>
-          <t>10.69.5.118</t>
-        </is>
-      </c>
       <c r="D250" t="n">
         <v>2017</v>
       </c>
@@ -16620,7 +16625,7 @@
         <v>1</v>
       </c>
       <c r="N250" s="3" t="n">
-        <v>46076.56996527778</v>
+        <v>46076.64386574074</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16684,7 +16689,7 @@
         <v>1</v>
       </c>
       <c r="N251" s="3" t="n">
-        <v>46076.53515046297</v>
+        <v>46076.615</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16748,7 +16753,7 @@
         <v>1</v>
       </c>
       <c r="N252" s="3" t="n">
-        <v>46076.53644675926</v>
+        <v>46076.61771990741</v>
       </c>
       <c r="O252" t="inlineStr">
         <is>
@@ -16812,7 +16817,7 @@
         <v>1</v>
       </c>
       <c r="N253" s="3" t="n">
-        <v>46076.56925925926</v>
+        <v>46076.6255787037</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16870,7 +16875,7 @@
         <v>1</v>
       </c>
       <c r="N254" s="3" t="n">
-        <v>46076.5334375</v>
+        <v>46076.63055555556</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -16934,7 +16939,7 @@
         <v>1</v>
       </c>
       <c r="N255" s="3" t="n">
-        <v>46076.55907407407</v>
+        <v>46076.64700231481</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -16998,7 +17003,7 @@
         <v>1</v>
       </c>
       <c r="N256" s="3" t="n">
-        <v>46076.57037037037</v>
+        <v>46076.6544212963</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17062,7 +17067,7 @@
         <v>1</v>
       </c>
       <c r="N257" s="3" t="n">
-        <v>46076.55813657407</v>
+        <v>46076.64016203704</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17126,7 +17131,7 @@
         <v>1</v>
       </c>
       <c r="N258" s="3" t="n">
-        <v>46076.55364583333</v>
+        <v>46076.59267361111</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
@@ -17190,7 +17195,7 @@
         <v>1</v>
       </c>
       <c r="N259" s="3" t="n">
-        <v>46076.54112268519</v>
+        <v>46076.65388888889</v>
       </c>
       <c r="O259" t="inlineStr">
         <is>
@@ -17254,7 +17259,7 @@
         <v>1</v>
       </c>
       <c r="N260" s="3" t="n">
-        <v>46076.54555555555</v>
+        <v>46076.62377314815</v>
       </c>
       <c r="O260" t="inlineStr">
         <is>
@@ -17318,7 +17323,7 @@
         <v>1</v>
       </c>
       <c r="N261" s="3" t="n">
-        <v>46076.55996527777</v>
+        <v>46076.63484953704</v>
       </c>
       <c r="O261" t="inlineStr">
         <is>
@@ -17382,7 +17387,7 @@
         <v>1</v>
       </c>
       <c r="N262" s="3" t="n">
-        <v>46076.53973379629</v>
+        <v>46076.62642361111</v>
       </c>
       <c r="O262" t="inlineStr">
         <is>
@@ -17446,7 +17451,7 @@
         <v>1</v>
       </c>
       <c r="N263" s="3" t="n">
-        <v>46076.56770833334</v>
+        <v>46076.64655092593</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17510,7 +17515,7 @@
         <v>1</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>46076.53751157408</v>
+        <v>46076.61476851852</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17574,7 +17579,7 @@
         <v>1</v>
       </c>
       <c r="N265" s="3" t="n">
-        <v>46076.54226851852</v>
+        <v>46076.62787037037</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17638,7 +17643,7 @@
         <v>1</v>
       </c>
       <c r="N266" s="3" t="n">
-        <v>46076.54237268519</v>
+        <v>46076.6219212963</v>
       </c>
       <c r="O266" t="inlineStr">
         <is>
@@ -17702,7 +17707,7 @@
         <v>1</v>
       </c>
       <c r="N267" s="3" t="n">
-        <v>46076.55608796296</v>
+        <v>46076.63737268518</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17766,7 +17771,7 @@
         <v>1</v>
       </c>
       <c r="N268" s="3" t="n">
-        <v>46076.53420138889</v>
+        <v>46076.65416666667</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17830,7 +17835,7 @@
         <v>1</v>
       </c>
       <c r="N269" s="3" t="n">
-        <v>46076.54203703703</v>
+        <v>46076.61458333334</v>
       </c>
       <c r="O269" t="inlineStr">
         <is>
@@ -17891,7 +17896,7 @@
         </is>
       </c>
       <c r="N270" s="3" t="n">
-        <v>46076.5418287037</v>
+        <v>46076.6204050926</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -18019,7 +18024,7 @@
         <v>1</v>
       </c>
       <c r="N272" s="3" t="n">
-        <v>46076.55990740741</v>
+        <v>46076.62418981481</v>
       </c>
       <c r="O272" t="inlineStr">
         <is>
@@ -18083,7 +18088,7 @@
         <v>2</v>
       </c>
       <c r="N273" s="3" t="n">
-        <v>46076.56148148148</v>
+        <v>46076.63957175926</v>
       </c>
       <c r="O273" t="inlineStr">
         <is>
@@ -18403,7 +18408,7 @@
         <v>1</v>
       </c>
       <c r="N278" s="3" t="n">
-        <v>46076.54068287037</v>
+        <v>46076.63667824074</v>
       </c>
       <c r="O278" t="inlineStr">
         <is>
@@ -18467,7 +18472,7 @@
         <v>1</v>
       </c>
       <c r="N279" s="3" t="n">
-        <v>46076.55283564814</v>
+        <v>46076.62613425926</v>
       </c>
       <c r="O279" t="inlineStr">
         <is>
@@ -18531,7 +18536,7 @@
         <v>1</v>
       </c>
       <c r="N280" s="3" t="n">
-        <v>46076.56201388889</v>
+        <v>46076.65061342593</v>
       </c>
       <c r="O280" t="inlineStr">
         <is>
@@ -18595,7 +18600,7 @@
         <v>1</v>
       </c>
       <c r="N281" s="3" t="n">
-        <v>46076.56340277778</v>
+        <v>46076.63337962963</v>
       </c>
       <c r="O281" t="inlineStr">
         <is>
@@ -18654,7 +18659,7 @@
         <v>1</v>
       </c>
       <c r="N282" s="3" t="n">
-        <v>46076.55696759259</v>
+        <v>46076.63214120371</v>
       </c>
       <c r="O282" t="inlineStr">
         <is>
@@ -18718,7 +18723,7 @@
         <v>1</v>
       </c>
       <c r="N283" s="3" t="n">
-        <v>46076.55039351852</v>
+        <v>46076.63303240741</v>
       </c>
       <c r="O283" t="inlineStr">
         <is>
@@ -18782,7 +18787,7 @@
         <v>1</v>
       </c>
       <c r="N284" s="3" t="n">
-        <v>46076.56969907408</v>
+        <v>46076.65143518519</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18846,7 +18851,7 @@
         <v>1</v>
       </c>
       <c r="N285" s="3" t="n">
-        <v>46076.56288194445</v>
+        <v>46076.6374074074</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -18865,11 +18870,6 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
-      <c r="C286" t="inlineStr">
-        <is>
-          <t>10.69.5.155</t>
-        </is>
-      </c>
       <c r="D286" t="n">
         <v>2019</v>
       </c>
@@ -18910,7 +18910,7 @@
         <v>1</v>
       </c>
       <c r="N286" s="3" t="n">
-        <v>46076.53315972222</v>
+        <v>46076.5897800926</v>
       </c>
       <c r="O286" t="inlineStr">
         <is>
@@ -18974,7 +18974,7 @@
         <v>1</v>
       </c>
       <c r="N287" s="3" t="n">
-        <v>46076.55369212963</v>
+        <v>46076.5925</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
@@ -19102,7 +19102,7 @@
         <v>1</v>
       </c>
       <c r="N289" s="3" t="n">
-        <v>46076.53820601852</v>
+        <v>46076.61829861111</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -19896,7 +19896,7 @@
         <v>1</v>
       </c>
       <c r="N302" s="3" t="n">
-        <v>46076.54359953704</v>
+        <v>46076.65280092593</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -21012,7 +21012,7 @@
         </is>
       </c>
       <c r="N320" s="3" t="n">
-        <v>46076.54170138889</v>
+        <v>46076.65418981481</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21737,7 +21737,7 @@
         <v>1</v>
       </c>
       <c r="N332" s="3" t="n">
-        <v>46076.57072916667</v>
+        <v>46076.64337962963</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21801,7 +21801,7 @@
         <v>2</v>
       </c>
       <c r="N333" s="3" t="n">
-        <v>46076.55429398148</v>
+        <v>46076.63384259259</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21865,7 +21865,7 @@
         <v>2</v>
       </c>
       <c r="N334" s="3" t="n">
-        <v>46076.55660879629</v>
+        <v>46076.63517361111</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21929,7 +21929,7 @@
         <v>2</v>
       </c>
       <c r="N335" s="3" t="n">
-        <v>46076.56253472222</v>
+        <v>46076.64192129629</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -21993,7 +21993,7 @@
         <v>1</v>
       </c>
       <c r="N336" s="3" t="n">
-        <v>46076.54204861111</v>
+        <v>46076.6187037037</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22057,7 +22057,7 @@
         <v>1</v>
       </c>
       <c r="N337" s="3" t="n">
-        <v>46076.53575231481</v>
+        <v>46076.65163194444</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22121,7 +22121,7 @@
         <v>2</v>
       </c>
       <c r="N338" s="3" t="n">
-        <v>46076.54375</v>
+        <v>46076.65407407407</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -22313,7 +22313,7 @@
         <v>2</v>
       </c>
       <c r="N341" s="3" t="n">
-        <v>46076.53319444445</v>
+        <v>46076.5753125</v>
       </c>
       <c r="O341" t="inlineStr">
         <is>
@@ -22396,6 +22396,11 @@
           <t>OPERACAO 9.1</t>
         </is>
       </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>10.69.5.237</t>
+        </is>
+      </c>
       <c r="D343" t="n">
         <v>2017</v>
       </c>
@@ -22438,7 +22443,7 @@
         </is>
       </c>
       <c r="N343" s="3" t="n">
-        <v>46076.56715277778</v>
+        <v>46076.64768518518</v>
       </c>
       <c r="O343" t="inlineStr">
         <is>
@@ -22694,7 +22699,7 @@
         <v>1</v>
       </c>
       <c r="N347" s="3" t="n">
-        <v>46076.55487268518</v>
+        <v>46076.5949537037</v>
       </c>
       <c r="O347" t="inlineStr">
         <is>
@@ -22822,7 +22827,7 @@
         <v>1</v>
       </c>
       <c r="N349" s="3" t="n">
-        <v>46076.55619212963</v>
+        <v>46076.5919212963</v>
       </c>
       <c r="O349" t="inlineStr">
         <is>
@@ -22841,11 +22846,6 @@
           <t>OPERACAO 9.1</t>
         </is>
       </c>
-      <c r="C350" t="inlineStr">
-        <is>
-          <t>10.69.5.244</t>
-        </is>
-      </c>
       <c r="D350" t="n">
         <v>2014</v>
       </c>
@@ -22886,7 +22886,7 @@
         <v>1</v>
       </c>
       <c r="N350" s="3" t="n">
-        <v>46076.55013888889</v>
+        <v>46076.58641203704</v>
       </c>
       <c r="O350" t="inlineStr">
         <is>
@@ -23075,7 +23075,7 @@
         </is>
       </c>
       <c r="N353" s="3" t="n">
-        <v>46076.55268518518</v>
+        <v>46076.59017361111</v>
       </c>
       <c r="O353" t="inlineStr">
         <is>
@@ -23136,7 +23136,7 @@
         </is>
       </c>
       <c r="N354" s="3" t="n">
-        <v>46076.5525</v>
+        <v>46076.59353009259</v>
       </c>
       <c r="O354" t="inlineStr">
         <is>
@@ -23200,7 +23200,7 @@
         <v>1</v>
       </c>
       <c r="N355" s="3" t="n">
-        <v>46076.55340277778</v>
+        <v>46076.59435185185</v>
       </c>
       <c r="O355" t="inlineStr">
         <is>
@@ -23264,7 +23264,7 @@
         <v>1</v>
       </c>
       <c r="N356" s="3" t="n">
-        <v>46076.54942129629</v>
+        <v>46076.5891550926</v>
       </c>
       <c r="O356" t="inlineStr">
         <is>
@@ -23328,7 +23328,7 @@
         <v>1</v>
       </c>
       <c r="N357" s="3" t="n">
-        <v>46076.5559375</v>
+        <v>46076.59214120371</v>
       </c>
       <c r="O357" t="inlineStr">
         <is>
@@ -23451,7 +23451,7 @@
         <v>2</v>
       </c>
       <c r="N359" s="3" t="n">
-        <v>46076.55167824074</v>
+        <v>46076.58893518519</v>
       </c>
       <c r="O359" t="inlineStr">
         <is>
@@ -23579,7 +23579,7 @@
         <v>1</v>
       </c>
       <c r="N361" s="3" t="n">
-        <v>46076.545</v>
+        <v>46076.58438657408</v>
       </c>
       <c r="O361" t="inlineStr">
         <is>
@@ -23828,7 +23828,7 @@
         <v>1</v>
       </c>
       <c r="N365" s="3" t="n">
-        <v>46076.53888888889</v>
+        <v>46076.64827546296</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
@@ -23894,7 +23894,7 @@
         </is>
       </c>
       <c r="N366" s="3" t="n">
-        <v>46076.57091435185</v>
+        <v>46076.64618055556</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -24020,7 +24020,7 @@
         </is>
       </c>
       <c r="N368" s="3" t="n">
-        <v>46076.56447916666</v>
+        <v>46076.64303240741</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -24086,7 +24086,7 @@
         </is>
       </c>
       <c r="N369" s="3" t="n">
-        <v>46076.56546296296</v>
+        <v>46076.64309027778</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
@@ -24155,7 +24155,7 @@
         <v>1</v>
       </c>
       <c r="N370" s="3" t="n">
-        <v>46076.56341435185</v>
+        <v>46076.64451388889</v>
       </c>
       <c r="O370" t="inlineStr">
         <is>
@@ -24224,7 +24224,7 @@
         <v>1</v>
       </c>
       <c r="N371" s="3" t="n">
-        <v>46076.55736111111</v>
+        <v>46076.63982638889</v>
       </c>
       <c r="O371" t="inlineStr">
         <is>
@@ -24431,7 +24431,7 @@
         <v>1</v>
       </c>
       <c r="N374" s="3" t="n">
-        <v>46076.55920138889</v>
+        <v>46076.6340625</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24497,7 +24497,7 @@
         </is>
       </c>
       <c r="N375" s="3" t="n">
-        <v>46076.5575462963</v>
+        <v>46076.63052083334</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
@@ -24561,7 +24561,7 @@
         <v>1</v>
       </c>
       <c r="N376" s="3" t="n">
-        <v>46076.53585648148</v>
+        <v>46076.65269675926</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -24630,7 +24630,7 @@
         <v>2</v>
       </c>
       <c r="N377" s="3" t="n">
-        <v>46076.54520833334</v>
+        <v>46076.62857638889</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -24699,7 +24699,7 @@
         <v>2</v>
       </c>
       <c r="N378" s="3" t="n">
-        <v>46076.56415509259</v>
+        <v>46076.64122685185</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização automática 2026-02-23 17:52:04.655497
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>46076.62174768518</v>
+        <v>46076.73453703704</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>46076.6159375</v>
+        <v>46076.73532407408</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -739,10 +739,10 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>46076.61898148148</v>
+        <v>46076.69822916666</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -1091,6 +1091,11 @@
           <t>AUDITORIO</t>
         </is>
       </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>10.69.3.160</t>
+        </is>
+      </c>
       <c r="D10" t="n">
         <v>2017</v>
       </c>
@@ -1131,7 +1136,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="3" t="n">
-        <v>46076.62016203703</v>
+        <v>46076.73760416666</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1451,7 +1456,7 @@
         <v>1</v>
       </c>
       <c r="N15" s="3" t="n">
-        <v>46076.6172337963</v>
+        <v>46076.73608796296</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1515,7 +1520,7 @@
         <v>2</v>
       </c>
       <c r="N16" s="3" t="n">
-        <v>46076.64849537037</v>
+        <v>46076.72787037037</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -2244,7 +2249,7 @@
         </is>
       </c>
       <c r="N28" s="3" t="n">
-        <v>46076.61978009259</v>
+        <v>46076.73538194445</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -6570,7 +6575,7 @@
         <v>1</v>
       </c>
       <c r="N95" s="3" t="n">
-        <v>46076.63108796296</v>
+        <v>46076.70255787037</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -6703,7 +6708,7 @@
         <v>1</v>
       </c>
       <c r="N97" s="3" t="n">
-        <v>46076.62237268518</v>
+        <v>46076.69875</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -6767,7 +6772,7 @@
         <v>1</v>
       </c>
       <c r="N98" s="3" t="n">
-        <v>46076.64125</v>
+        <v>46076.71788194445</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -6836,7 +6841,7 @@
         <v>1</v>
       </c>
       <c r="N99" s="3" t="n">
-        <v>46076.64931712963</v>
+        <v>46076.72723379629</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -6905,7 +6910,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>46076.62208333334</v>
+        <v>46076.73354166667</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6974,7 +6979,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="3" t="n">
-        <v>46076.64755787037</v>
+        <v>46076.72008101852</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -7112,7 +7117,7 @@
         <v>2</v>
       </c>
       <c r="N103" s="3" t="n">
-        <v>46076.62075231481</v>
+        <v>46076.73339120371</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7369,7 +7374,7 @@
         <v>1</v>
       </c>
       <c r="N107" s="3" t="n">
-        <v>46076.63592592593</v>
+        <v>46076.71092592592</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -7507,7 +7512,7 @@
         <v>1</v>
       </c>
       <c r="N109" s="3" t="n">
-        <v>46076.6528587963</v>
+        <v>46076.72520833334</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7576,7 +7581,7 @@
         <v>2</v>
       </c>
       <c r="N110" s="3" t="n">
-        <v>46076.61557870371</v>
+        <v>46076.73584490741</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7645,7 +7650,7 @@
         <v>2</v>
       </c>
       <c r="N111" s="3" t="n">
-        <v>46076.64653935185</v>
+        <v>46076.73309027778</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
@@ -7714,7 +7719,7 @@
         <v>2</v>
       </c>
       <c r="N112" s="3" t="n">
-        <v>46076.62054398148</v>
+        <v>46076.69840277778</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7783,7 +7788,7 @@
         <v>1</v>
       </c>
       <c r="N113" s="3" t="n">
-        <v>46076.61407407407</v>
+        <v>46076.73140046297</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7852,7 +7857,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>46076.61668981481</v>
+        <v>46076.70063657407</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -7918,7 +7923,7 @@
         </is>
       </c>
       <c r="N115" s="3" t="n">
-        <v>46076.64203703704</v>
+        <v>46076.68381944444</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -8051,7 +8056,7 @@
         <v>1</v>
       </c>
       <c r="N117" s="3" t="n">
-        <v>46076.63361111111</v>
+        <v>46076.67082175926</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -8255,7 +8260,7 @@
         <v>1</v>
       </c>
       <c r="N120" s="3" t="n">
-        <v>46076.6290625</v>
+        <v>46076.70918981481</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -8324,7 +8329,7 @@
         <v>1</v>
       </c>
       <c r="N121" s="3" t="n">
-        <v>46076.62424768518</v>
+        <v>46076.70625</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -8390,7 +8395,7 @@
         </is>
       </c>
       <c r="N122" s="3" t="n">
-        <v>46076.63138888889</v>
+        <v>46076.67222222222</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -8459,7 +8464,7 @@
         <v>2</v>
       </c>
       <c r="N123" s="3" t="n">
-        <v>46076.6203587963</v>
+        <v>46076.70427083333</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -8528,7 +8533,7 @@
         <v>1</v>
       </c>
       <c r="N124" s="3" t="n">
-        <v>46076.62162037037</v>
+        <v>46076.73422453704</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -8597,7 +8602,7 @@
         <v>1</v>
       </c>
       <c r="N125" s="3" t="n">
-        <v>46076.64115740741</v>
+        <v>46076.71368055556</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -8666,7 +8671,7 @@
         <v>2</v>
       </c>
       <c r="N126" s="3" t="n">
-        <v>46076.65291666667</v>
+        <v>46076.73329861111</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -8735,7 +8740,7 @@
         <v>2</v>
       </c>
       <c r="N127" s="3" t="n">
-        <v>46076.63615740741</v>
+        <v>46076.71982638889</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -8804,7 +8809,7 @@
         <v>1</v>
       </c>
       <c r="N128" s="3" t="n">
-        <v>46076.63902777778</v>
+        <v>46076.71164351852</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -8873,7 +8878,7 @@
         <v>1</v>
       </c>
       <c r="N129" s="3" t="n">
-        <v>46076.62640046296</v>
+        <v>46076.66789351852</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -8942,7 +8947,7 @@
         <v>1</v>
       </c>
       <c r="N130" s="3" t="n">
-        <v>46076.64973379629</v>
+        <v>46076.729375</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -8961,11 +8966,6 @@
           <t>ADM/FIN</t>
         </is>
       </c>
-      <c r="C131" t="inlineStr">
-        <is>
-          <t>10.69.3.6</t>
-        </is>
-      </c>
       <c r="D131" t="n">
         <v>2025</v>
       </c>
@@ -9011,7 +9011,7 @@
         <v>1</v>
       </c>
       <c r="N131" s="3" t="n">
-        <v>46076.65296296297</v>
+        <v>46076.69158564815</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -9144,7 +9144,7 @@
         <v>1</v>
       </c>
       <c r="N133" s="3" t="n">
-        <v>46076.64174768519</v>
+        <v>46076.72125</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -9208,7 +9208,7 @@
         <v>1</v>
       </c>
       <c r="N134" s="3" t="n">
-        <v>46076.63530092593</v>
+        <v>46076.71251157407</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -9272,7 +9272,7 @@
         <v>1</v>
       </c>
       <c r="N135" s="3" t="n">
-        <v>46076.64398148148</v>
+        <v>46076.7184837963</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -9463,7 +9463,7 @@
         <v>1</v>
       </c>
       <c r="N138" s="3" t="n">
-        <v>46076.61931712963</v>
+        <v>46076.72952546296</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9527,7 +9527,7 @@
         <v>1</v>
       </c>
       <c r="N139" s="3" t="n">
-        <v>46076.62423611111</v>
+        <v>46076.69944444444</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9591,7 +9591,7 @@
         <v>1</v>
       </c>
       <c r="N140" s="3" t="n">
-        <v>46076.61430555556</v>
+        <v>46076.73339120371</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9655,7 +9655,7 @@
         <v>1</v>
       </c>
       <c r="N141" s="3" t="n">
-        <v>46076.64740740741</v>
+        <v>46076.72554398148</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9719,7 +9719,7 @@
         <v>1</v>
       </c>
       <c r="N142" s="3" t="n">
-        <v>46076.64795138889</v>
+        <v>46076.72511574074</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9783,7 +9783,7 @@
         <v>1</v>
       </c>
       <c r="N143" s="3" t="n">
-        <v>46076.64767361111</v>
+        <v>46076.72097222223</v>
       </c>
       <c r="O143" t="inlineStr">
         <is>
@@ -9847,7 +9847,7 @@
         <v>1</v>
       </c>
       <c r="N144" s="3" t="n">
-        <v>46076.65340277777</v>
+        <v>46076.72939814815</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9911,7 +9911,7 @@
         <v>1</v>
       </c>
       <c r="N145" s="3" t="n">
-        <v>46076.61836805556</v>
+        <v>46076.70148148148</v>
       </c>
       <c r="O145" t="inlineStr">
         <is>
@@ -9975,7 +9975,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="3" t="n">
-        <v>46076.62509259259</v>
+        <v>46076.70677083333</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10039,7 +10039,7 @@
         <v>1</v>
       </c>
       <c r="N147" s="3" t="n">
-        <v>46076.62274305556</v>
+        <v>46076.72333333334</v>
       </c>
       <c r="O147" t="inlineStr">
         <is>
@@ -10103,7 +10103,7 @@
         <v>1</v>
       </c>
       <c r="N148" s="3" t="n">
-        <v>46076.64905092592</v>
+        <v>46076.7229050926</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10167,7 +10167,7 @@
         <v>1</v>
       </c>
       <c r="N149" s="3" t="n">
-        <v>46076.63042824074</v>
+        <v>46076.7118287037</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -10231,7 +10231,7 @@
         <v>1</v>
       </c>
       <c r="N150" s="3" t="n">
-        <v>46076.62450231481</v>
+        <v>46076.66200231481</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -10295,7 +10295,7 @@
         <v>1</v>
       </c>
       <c r="N151" s="3" t="n">
-        <v>46076.62344907408</v>
+        <v>46076.69913194444</v>
       </c>
       <c r="O151" t="inlineStr">
         <is>
@@ -10359,7 +10359,7 @@
         <v>1</v>
       </c>
       <c r="N152" s="3" t="n">
-        <v>46076.62681712963</v>
+        <v>46076.70512731482</v>
       </c>
       <c r="O152" t="inlineStr">
         <is>
@@ -10378,6 +10378,11 @@
           <t>OPERACAO 7.1</t>
         </is>
       </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>10.69.5.21</t>
+        </is>
+      </c>
       <c r="D153" t="n">
         <v>2018</v>
       </c>
@@ -10418,7 +10423,7 @@
         <v>1</v>
       </c>
       <c r="N153" s="3" t="n">
-        <v>46076.64209490741</v>
+        <v>46076.71886574074</v>
       </c>
       <c r="O153" t="inlineStr">
         <is>
@@ -10482,7 +10487,7 @@
         <v>1</v>
       </c>
       <c r="N154" s="3" t="n">
-        <v>46076.62351851852</v>
+        <v>46076.70532407407</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10546,7 +10551,7 @@
         <v>1</v>
       </c>
       <c r="N155" s="3" t="n">
-        <v>46076.62349537037</v>
+        <v>46076.73637731482</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10610,7 +10615,7 @@
         <v>1</v>
       </c>
       <c r="N156" s="3" t="n">
-        <v>46076.64444444444</v>
+        <v>46076.72557870371</v>
       </c>
       <c r="O156" t="inlineStr">
         <is>
@@ -10866,7 +10871,7 @@
         <v>1</v>
       </c>
       <c r="N160" s="3" t="n">
-        <v>46076.62219907407</v>
+        <v>46076.73675925926</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
@@ -10930,7 +10935,7 @@
         <v>1</v>
       </c>
       <c r="N161" s="3" t="n">
-        <v>46076.65434027778</v>
+        <v>46076.73771990741</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -10994,7 +10999,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="3" t="n">
-        <v>46076.63366898148</v>
+        <v>46076.7080324074</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11122,7 +11127,7 @@
         <v>2</v>
       </c>
       <c r="N164" s="3" t="n">
-        <v>46076.63585648148</v>
+        <v>46076.71253472222</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11186,7 +11191,7 @@
         <v>2</v>
       </c>
       <c r="N165" s="3" t="n">
-        <v>46076.63103009259</v>
+        <v>46076.67005787037</v>
       </c>
       <c r="O165" t="inlineStr">
         <is>
@@ -11442,7 +11447,7 @@
         <v>2</v>
       </c>
       <c r="N169" s="3" t="n">
-        <v>46076.63003472222</v>
+        <v>46076.71001157408</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -11506,7 +11511,7 @@
         <v>2</v>
       </c>
       <c r="N170" s="3" t="n">
-        <v>46076.65351851852</v>
+        <v>46076.73380787037</v>
       </c>
       <c r="O170" t="inlineStr">
         <is>
@@ -11570,7 +11575,7 @@
         <v>1</v>
       </c>
       <c r="N171" s="3" t="n">
-        <v>46076.56560185185</v>
+        <v>46076.71388888889</v>
       </c>
       <c r="O171" t="inlineStr">
         <is>
@@ -11634,7 +11639,7 @@
         <v>2</v>
       </c>
       <c r="N172" s="3" t="n">
-        <v>46076.61944444444</v>
+        <v>46076.70940972222</v>
       </c>
       <c r="O172" t="inlineStr">
         <is>
@@ -11695,10 +11700,10 @@
         </is>
       </c>
       <c r="M173" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N173" s="3" t="n">
-        <v>46076.63251157408</v>
+        <v>46076.73700231482</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -11826,7 +11831,7 @@
         <v>2</v>
       </c>
       <c r="N175" s="3" t="n">
-        <v>46076.64849537037</v>
+        <v>46076.71513888889</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -11890,7 +11895,7 @@
         <v>2</v>
       </c>
       <c r="N176" s="3" t="n">
-        <v>46076.62503472222</v>
+        <v>46076.66653935185</v>
       </c>
       <c r="O176" t="inlineStr">
         <is>
@@ -11954,7 +11959,7 @@
         <v>3</v>
       </c>
       <c r="N177" s="3" t="n">
-        <v>46076.62358796296</v>
+        <v>46076.70077546296</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
@@ -12018,7 +12023,7 @@
         <v>2</v>
       </c>
       <c r="N178" s="3" t="n">
-        <v>46076.62872685185</v>
+        <v>46076.70798611111</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12082,7 +12087,7 @@
         <v>1</v>
       </c>
       <c r="N179" s="3" t="n">
-        <v>46076.63115740741</v>
+        <v>46076.70289351852</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12146,7 +12151,7 @@
         <v>1</v>
       </c>
       <c r="N180" s="3" t="n">
-        <v>46076.62260416667</v>
+        <v>46076.71085648148</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12210,7 +12215,7 @@
         <v>1</v>
       </c>
       <c r="N181" s="3" t="n">
-        <v>46076.62090277778</v>
+        <v>46076.73451388889</v>
       </c>
       <c r="O181" t="inlineStr">
         <is>
@@ -12791,7 +12796,7 @@
         </is>
       </c>
       <c r="N190" s="3" t="n">
-        <v>46076.62475694445</v>
+        <v>46076.70375</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12855,7 +12860,7 @@
         <v>1</v>
       </c>
       <c r="N191" s="3" t="n">
-        <v>46076.64664351852</v>
+        <v>46076.70166666667</v>
       </c>
       <c r="O191" t="inlineStr">
         <is>
@@ -12919,7 +12924,7 @@
         <v>1</v>
       </c>
       <c r="N192" s="3" t="n">
-        <v>46076.62076388889</v>
+        <v>46076.70276620371</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -13044,7 +13049,7 @@
         <v>2</v>
       </c>
       <c r="N194" s="3" t="n">
-        <v>46076.62033564815</v>
+        <v>46076.71369212963</v>
       </c>
       <c r="O194" t="inlineStr">
         <is>
@@ -13108,7 +13113,7 @@
         <v>1</v>
       </c>
       <c r="N195" s="3" t="n">
-        <v>46076.6516550926</v>
+        <v>46076.73121527778</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13172,7 +13177,7 @@
         <v>1</v>
       </c>
       <c r="N196" s="3" t="n">
-        <v>46076.62753472223</v>
+        <v>46076.70592592593</v>
       </c>
       <c r="O196" t="inlineStr">
         <is>
@@ -13236,7 +13241,7 @@
         <v>1</v>
       </c>
       <c r="N197" s="3" t="n">
-        <v>46076.63592592593</v>
+        <v>46076.70885416667</v>
       </c>
       <c r="O197" t="inlineStr">
         <is>
@@ -13364,7 +13369,7 @@
         <v>1</v>
       </c>
       <c r="N199" s="3" t="n">
-        <v>46076.37359953704</v>
+        <v>46076.70480324074</v>
       </c>
       <c r="O199" t="inlineStr">
         <is>
@@ -13428,7 +13433,7 @@
         <v>1</v>
       </c>
       <c r="N200" s="3" t="n">
-        <v>46076.63383101852</v>
+        <v>46076.70898148148</v>
       </c>
       <c r="O200" t="inlineStr">
         <is>
@@ -13489,7 +13494,7 @@
         </is>
       </c>
       <c r="N201" s="3" t="n">
-        <v>46076.62509259259</v>
+        <v>46076.7049537037</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -13553,7 +13558,7 @@
         <v>1</v>
       </c>
       <c r="N202" s="3" t="n">
-        <v>46076.62814814815</v>
+        <v>46076.70666666667</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13617,7 +13622,7 @@
         <v>1</v>
       </c>
       <c r="N203" s="3" t="n">
-        <v>46076.62922453704</v>
+        <v>46076.70327546296</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13681,7 +13686,7 @@
         <v>1</v>
       </c>
       <c r="N204" s="3" t="n">
-        <v>46076.65252314815</v>
+        <v>46076.72898148148</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13745,7 +13750,7 @@
         <v>1</v>
       </c>
       <c r="N205" s="3" t="n">
-        <v>46076.65001157407</v>
+        <v>46076.73388888889</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13809,7 +13814,7 @@
         <v>1</v>
       </c>
       <c r="N206" s="3" t="n">
-        <v>46076.63614583333</v>
+        <v>46076.71358796296</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -13873,7 +13878,7 @@
         <v>1</v>
       </c>
       <c r="N207" s="3" t="n">
-        <v>46076.6211574074</v>
+        <v>46076.6583912037</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -13937,7 +13942,7 @@
         <v>1</v>
       </c>
       <c r="N208" s="3" t="n">
-        <v>46076.63375</v>
+        <v>46076.71392361111</v>
       </c>
       <c r="O208" t="inlineStr">
         <is>
@@ -14001,7 +14006,7 @@
         <v>1</v>
       </c>
       <c r="N209" s="3" t="n">
-        <v>46076.65446759259</v>
+        <v>46076.72931712963</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14065,7 +14070,7 @@
         <v>1</v>
       </c>
       <c r="N210" s="3" t="n">
-        <v>46076.64767361111</v>
+        <v>46076.72696759259</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14129,7 +14134,7 @@
         <v>1</v>
       </c>
       <c r="N211" s="3" t="n">
-        <v>46076.62603009259</v>
+        <v>46076.70930555555</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -14193,7 +14198,7 @@
         <v>1</v>
       </c>
       <c r="N212" s="3" t="n">
-        <v>46076.65055555556</v>
+        <v>46076.73313657408</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -14257,7 +14262,7 @@
         <v>1</v>
       </c>
       <c r="N213" s="3" t="n">
-        <v>46076.57293981482</v>
+        <v>46076.72825231482</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
@@ -14321,7 +14326,7 @@
         <v>1</v>
       </c>
       <c r="N214" s="3" t="n">
-        <v>46074.58793981482</v>
+        <v>46076.72421296296</v>
       </c>
       <c r="O214" t="inlineStr">
         <is>
@@ -14385,7 +14390,7 @@
         <v>1</v>
       </c>
       <c r="N215" s="3" t="n">
-        <v>46076.540625</v>
+        <v>46076.7216550926</v>
       </c>
       <c r="O215" t="inlineStr">
         <is>
@@ -14449,7 +14454,7 @@
         <v>1</v>
       </c>
       <c r="N216" s="3" t="n">
-        <v>46076.62444444445</v>
+        <v>46076.71829861111</v>
       </c>
       <c r="O216" t="inlineStr">
         <is>
@@ -14468,11 +14473,6 @@
           <t>OPERACAO 8.1</t>
         </is>
       </c>
-      <c r="C217" t="inlineStr">
-        <is>
-          <t>10.69.5.85</t>
-        </is>
-      </c>
       <c r="D217" t="n">
         <v>2017</v>
       </c>
@@ -14513,7 +14513,7 @@
         <v>1</v>
       </c>
       <c r="N217" s="3" t="n">
-        <v>46076.64662037037</v>
+        <v>46076.70379629629</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14577,7 +14577,7 @@
         <v>1</v>
       </c>
       <c r="N218" s="3" t="n">
-        <v>46076.63247685185</v>
+        <v>46076.7124537037</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14641,7 +14641,7 @@
         <v>1</v>
       </c>
       <c r="N219" s="3" t="n">
-        <v>46076.65370370371</v>
+        <v>46076.73715277778</v>
       </c>
       <c r="O219" t="inlineStr">
         <is>
@@ -14774,7 +14774,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="3" t="n">
-        <v>46076.64355324074</v>
+        <v>46076.70457175926</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14838,7 +14838,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="3" t="n">
-        <v>46076.62918981481</v>
+        <v>46076.70340277778</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -14902,7 +14902,7 @@
         <v>1</v>
       </c>
       <c r="N223" s="3" t="n">
-        <v>46076.62484953704</v>
+        <v>46076.71143518519</v>
       </c>
       <c r="O223" t="inlineStr">
         <is>
@@ -14966,7 +14966,7 @@
         <v>1</v>
       </c>
       <c r="N224" s="3" t="n">
-        <v>46074.45204861111</v>
+        <v>46076.72743055555</v>
       </c>
       <c r="O224" t="inlineStr">
         <is>
@@ -15030,7 +15030,7 @@
         <v>1</v>
       </c>
       <c r="N225" s="3" t="n">
-        <v>46076.63336805555</v>
+        <v>46076.69840277778</v>
       </c>
       <c r="O225" t="inlineStr">
         <is>
@@ -15094,7 +15094,7 @@
         <v>1</v>
       </c>
       <c r="N226" s="3" t="n">
-        <v>46076.61984953703</v>
+        <v>46076.70055555556</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15158,7 +15158,7 @@
         <v>1</v>
       </c>
       <c r="N227" s="3" t="n">
-        <v>46076.61541666667</v>
+        <v>46076.73224537037</v>
       </c>
       <c r="O227" t="inlineStr">
         <is>
@@ -15222,7 +15222,7 @@
         <v>1</v>
       </c>
       <c r="N228" s="3" t="n">
-        <v>46076.63694444444</v>
+        <v>46076.71493055556</v>
       </c>
       <c r="O228" t="inlineStr">
         <is>
@@ -15286,7 +15286,7 @@
         <v>1</v>
       </c>
       <c r="N229" s="3" t="n">
-        <v>46076.65481481481</v>
+        <v>46076.73138888889</v>
       </c>
       <c r="O229" t="inlineStr">
         <is>
@@ -15350,7 +15350,7 @@
         <v>1</v>
       </c>
       <c r="N230" s="3" t="n">
-        <v>46076.62137731481</v>
+        <v>46076.700625</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15414,7 +15414,7 @@
         <v>1</v>
       </c>
       <c r="N231" s="3" t="n">
-        <v>46076.65460648148</v>
+        <v>46076.70793981481</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15542,7 +15542,7 @@
         <v>1</v>
       </c>
       <c r="N233" s="3" t="n">
-        <v>46076.65479166667</v>
+        <v>46076.70229166667</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15606,7 +15606,7 @@
         <v>1</v>
       </c>
       <c r="N234" s="3" t="n">
-        <v>46076.62622685185</v>
+        <v>46076.70791666667</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -15670,7 +15670,7 @@
         <v>1</v>
       </c>
       <c r="N235" s="3" t="n">
-        <v>46076.61657407408</v>
+        <v>46076.72476851852</v>
       </c>
       <c r="O235" t="inlineStr">
         <is>
@@ -15734,7 +15734,7 @@
         <v>1</v>
       </c>
       <c r="N236" s="3" t="n">
-        <v>46076.65402777777</v>
+        <v>46076.72701388889</v>
       </c>
       <c r="O236" t="inlineStr">
         <is>
@@ -15798,7 +15798,7 @@
         <v>1</v>
       </c>
       <c r="N237" s="3" t="n">
-        <v>46076.63473379629</v>
+        <v>46076.71039351852</v>
       </c>
       <c r="O237" t="inlineStr">
         <is>
@@ -15862,7 +15862,7 @@
         <v>1</v>
       </c>
       <c r="N238" s="3" t="n">
-        <v>46076.64681712963</v>
+        <v>46076.72914351852</v>
       </c>
       <c r="O238" t="inlineStr">
         <is>
@@ -15926,7 +15926,7 @@
         <v>1</v>
       </c>
       <c r="N239" s="3" t="n">
-        <v>46076.64993055556</v>
+        <v>46076.73451388889</v>
       </c>
       <c r="O239" t="inlineStr">
         <is>
@@ -15990,7 +15990,7 @@
         <v>1</v>
       </c>
       <c r="N240" s="3" t="n">
-        <v>46076.65480324074</v>
+        <v>46076.73399305555</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16054,7 +16054,7 @@
         <v>1</v>
       </c>
       <c r="N241" s="3" t="n">
-        <v>46076.59208333334</v>
+        <v>46076.72371527777</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16118,7 +16118,7 @@
         <v>1</v>
       </c>
       <c r="N242" s="3" t="n">
-        <v>46076.63688657407</v>
+        <v>46076.70850694444</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16182,7 +16182,7 @@
         <v>1</v>
       </c>
       <c r="N243" s="3" t="n">
-        <v>46076.63490740741</v>
+        <v>46076.67247685185</v>
       </c>
       <c r="O243" t="inlineStr">
         <is>
@@ -16310,7 +16310,7 @@
         <v>1</v>
       </c>
       <c r="N245" s="3" t="n">
-        <v>46076.62033564815</v>
+        <v>46076.73438657408</v>
       </c>
       <c r="O245" t="inlineStr">
         <is>
@@ -16374,7 +16374,7 @@
         <v>1</v>
       </c>
       <c r="N246" s="3" t="n">
-        <v>46076.62333333334</v>
+        <v>46076.70545138889</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16438,7 +16438,7 @@
         <v>1</v>
       </c>
       <c r="N247" s="3" t="n">
-        <v>46076.62175925926</v>
+        <v>46076.73392361111</v>
       </c>
       <c r="O247" t="inlineStr">
         <is>
@@ -16502,7 +16502,7 @@
         <v>1</v>
       </c>
       <c r="N248" s="3" t="n">
-        <v>46076.6221412037</v>
+        <v>46076.70577546296</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16625,7 +16625,7 @@
         <v>1</v>
       </c>
       <c r="N250" s="3" t="n">
-        <v>46076.64386574074</v>
+        <v>46076.72375</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16689,7 +16689,7 @@
         <v>1</v>
       </c>
       <c r="N251" s="3" t="n">
-        <v>46076.615</v>
+        <v>46076.73357638889</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16753,7 +16753,7 @@
         <v>1</v>
       </c>
       <c r="N252" s="3" t="n">
-        <v>46076.61771990741</v>
+        <v>46076.7346412037</v>
       </c>
       <c r="O252" t="inlineStr">
         <is>
@@ -16817,7 +16817,7 @@
         <v>1</v>
       </c>
       <c r="N253" s="3" t="n">
-        <v>46076.6255787037</v>
+        <v>46076.70173611111</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16875,7 +16875,7 @@
         <v>1</v>
       </c>
       <c r="N254" s="3" t="n">
-        <v>46076.63055555556</v>
+        <v>46076.70730324074</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -16939,7 +16939,7 @@
         <v>1</v>
       </c>
       <c r="N255" s="3" t="n">
-        <v>46076.64700231481</v>
+        <v>46076.70194444444</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -17003,7 +17003,7 @@
         <v>1</v>
       </c>
       <c r="N256" s="3" t="n">
-        <v>46076.6544212963</v>
+        <v>46076.70689814815</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17067,7 +17067,7 @@
         <v>1</v>
       </c>
       <c r="N257" s="3" t="n">
-        <v>46076.64016203704</v>
+        <v>46076.71556712963</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17195,7 +17195,7 @@
         <v>1</v>
       </c>
       <c r="N259" s="3" t="n">
-        <v>46076.65388888889</v>
+        <v>46076.70084490741</v>
       </c>
       <c r="O259" t="inlineStr">
         <is>
@@ -17387,7 +17387,7 @@
         <v>1</v>
       </c>
       <c r="N262" s="3" t="n">
-        <v>46076.62642361111</v>
+        <v>46076.70920138889</v>
       </c>
       <c r="O262" t="inlineStr">
         <is>
@@ -17451,7 +17451,7 @@
         <v>1</v>
       </c>
       <c r="N263" s="3" t="n">
-        <v>46076.64655092593</v>
+        <v>46076.72741898148</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17515,7 +17515,7 @@
         <v>1</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>46076.61476851852</v>
+        <v>46076.72865740741</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17579,7 +17579,7 @@
         <v>1</v>
       </c>
       <c r="N265" s="3" t="n">
-        <v>46076.62787037037</v>
+        <v>46076.70525462963</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17643,7 +17643,7 @@
         <v>1</v>
       </c>
       <c r="N266" s="3" t="n">
-        <v>46076.6219212963</v>
+        <v>46076.7022337963</v>
       </c>
       <c r="O266" t="inlineStr">
         <is>
@@ -17707,7 +17707,7 @@
         <v>1</v>
       </c>
       <c r="N267" s="3" t="n">
-        <v>46076.63737268518</v>
+        <v>46076.71700231481</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17771,7 +17771,7 @@
         <v>1</v>
       </c>
       <c r="N268" s="3" t="n">
-        <v>46076.65416666667</v>
+        <v>46076.7315625</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17835,7 +17835,7 @@
         <v>1</v>
       </c>
       <c r="N269" s="3" t="n">
-        <v>46076.61458333334</v>
+        <v>46076.69887731481</v>
       </c>
       <c r="O269" t="inlineStr">
         <is>
@@ -17896,7 +17896,7 @@
         </is>
       </c>
       <c r="N270" s="3" t="n">
-        <v>46076.6204050926</v>
+        <v>46076.73762731482</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -17960,7 +17960,7 @@
         <v>1</v>
       </c>
       <c r="N271" s="3" t="n">
-        <v>46074.45915509259</v>
+        <v>46076.65869212963</v>
       </c>
       <c r="O271" t="inlineStr">
         <is>
@@ -18024,7 +18024,7 @@
         <v>1</v>
       </c>
       <c r="N272" s="3" t="n">
-        <v>46076.62418981481</v>
+        <v>46076.66619212963</v>
       </c>
       <c r="O272" t="inlineStr">
         <is>
@@ -18088,7 +18088,7 @@
         <v>2</v>
       </c>
       <c r="N273" s="3" t="n">
-        <v>46076.63957175926</v>
+        <v>46076.71391203703</v>
       </c>
       <c r="O273" t="inlineStr">
         <is>
@@ -18408,7 +18408,7 @@
         <v>1</v>
       </c>
       <c r="N278" s="3" t="n">
-        <v>46076.63667824074</v>
+        <v>46076.71561342593</v>
       </c>
       <c r="O278" t="inlineStr">
         <is>
@@ -18600,7 +18600,7 @@
         <v>1</v>
       </c>
       <c r="N281" s="3" t="n">
-        <v>46076.63337962963</v>
+        <v>46076.706875</v>
       </c>
       <c r="O281" t="inlineStr">
         <is>
@@ -18659,7 +18659,7 @@
         <v>1</v>
       </c>
       <c r="N282" s="3" t="n">
-        <v>46076.63214120371</v>
+        <v>46076.71212962963</v>
       </c>
       <c r="O282" t="inlineStr">
         <is>
@@ -18723,7 +18723,7 @@
         <v>1</v>
       </c>
       <c r="N283" s="3" t="n">
-        <v>46076.63303240741</v>
+        <v>46076.70984953704</v>
       </c>
       <c r="O283" t="inlineStr">
         <is>
@@ -18787,7 +18787,7 @@
         <v>1</v>
       </c>
       <c r="N284" s="3" t="n">
-        <v>46076.65143518519</v>
+        <v>46076.7341087963</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18851,7 +18851,7 @@
         <v>1</v>
       </c>
       <c r="N285" s="3" t="n">
-        <v>46076.6374074074</v>
+        <v>46076.7147337963</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -19102,7 +19102,7 @@
         <v>1</v>
       </c>
       <c r="N289" s="3" t="n">
-        <v>46076.61829861111</v>
+        <v>46076.73748842593</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -19896,7 +19896,7 @@
         <v>1</v>
       </c>
       <c r="N302" s="3" t="n">
-        <v>46076.65280092593</v>
+        <v>46076.73310185185</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -21012,7 +21012,7 @@
         </is>
       </c>
       <c r="N320" s="3" t="n">
-        <v>46076.65418981481</v>
+        <v>46076.73121527778</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21737,7 +21737,7 @@
         <v>1</v>
       </c>
       <c r="N332" s="3" t="n">
-        <v>46076.64337962963</v>
+        <v>46076.71962962963</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21801,7 +21801,7 @@
         <v>2</v>
       </c>
       <c r="N333" s="3" t="n">
-        <v>46076.63384259259</v>
+        <v>46076.71458333333</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21865,7 +21865,7 @@
         <v>2</v>
       </c>
       <c r="N334" s="3" t="n">
-        <v>46076.63517361111</v>
+        <v>46076.71335648148</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21929,7 +21929,7 @@
         <v>2</v>
       </c>
       <c r="N335" s="3" t="n">
-        <v>46076.64192129629</v>
+        <v>46076.71543981481</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -21993,7 +21993,7 @@
         <v>1</v>
       </c>
       <c r="N336" s="3" t="n">
-        <v>46076.6187037037</v>
+        <v>46076.73644675926</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22057,7 +22057,7 @@
         <v>1</v>
       </c>
       <c r="N337" s="3" t="n">
-        <v>46076.65163194444</v>
+        <v>46076.72912037037</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22121,7 +22121,7 @@
         <v>2</v>
       </c>
       <c r="N338" s="3" t="n">
-        <v>46076.65407407407</v>
+        <v>46076.7296412037</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -22396,11 +22396,6 @@
           <t>OPERACAO 9.1</t>
         </is>
       </c>
-      <c r="C343" t="inlineStr">
-        <is>
-          <t>10.69.5.237</t>
-        </is>
-      </c>
       <c r="D343" t="n">
         <v>2017</v>
       </c>
@@ -22443,7 +22438,7 @@
         </is>
       </c>
       <c r="N343" s="3" t="n">
-        <v>46076.64768518518</v>
+        <v>46076.7228125</v>
       </c>
       <c r="O343" t="inlineStr">
         <is>
@@ -23828,7 +23823,7 @@
         <v>1</v>
       </c>
       <c r="N365" s="3" t="n">
-        <v>46076.64827546296</v>
+        <v>46076.6846875</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
@@ -23894,7 +23889,7 @@
         </is>
       </c>
       <c r="N366" s="3" t="n">
-        <v>46076.64618055556</v>
+        <v>46076.72384259259</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -24020,7 +24015,7 @@
         </is>
       </c>
       <c r="N368" s="3" t="n">
-        <v>46076.64303240741</v>
+        <v>46076.71673611111</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -24086,7 +24081,7 @@
         </is>
       </c>
       <c r="N369" s="3" t="n">
-        <v>46076.64309027778</v>
+        <v>46076.72153935185</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
@@ -24155,7 +24150,7 @@
         <v>1</v>
       </c>
       <c r="N370" s="3" t="n">
-        <v>46076.64451388889</v>
+        <v>46076.71877314815</v>
       </c>
       <c r="O370" t="inlineStr">
         <is>
@@ -24224,7 +24219,7 @@
         <v>1</v>
       </c>
       <c r="N371" s="3" t="n">
-        <v>46076.63982638889</v>
+        <v>46076.68086805556</v>
       </c>
       <c r="O371" t="inlineStr">
         <is>
@@ -24431,7 +24426,7 @@
         <v>1</v>
       </c>
       <c r="N374" s="3" t="n">
-        <v>46076.6340625</v>
+        <v>46076.71185185185</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24497,7 +24492,7 @@
         </is>
       </c>
       <c r="N375" s="3" t="n">
-        <v>46076.63052083334</v>
+        <v>46076.71289351852</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
@@ -24516,6 +24511,11 @@
           <t>COORDENACAO</t>
         </is>
       </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>10.69.3.72</t>
+        </is>
+      </c>
       <c r="D376" t="n">
         <v>2025</v>
       </c>
@@ -24561,7 +24561,7 @@
         <v>1</v>
       </c>
       <c r="N376" s="3" t="n">
-        <v>46076.65269675926</v>
+        <v>46076.73079861111</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -24630,7 +24630,7 @@
         <v>2</v>
       </c>
       <c r="N377" s="3" t="n">
-        <v>46076.62857638889</v>
+        <v>46076.66385416667</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -24699,7 +24699,7 @@
         <v>2</v>
       </c>
       <c r="N378" s="3" t="n">
-        <v>46076.64122685185</v>
+        <v>46076.72037037037</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização automática 2026-02-24 07:52:05.101025
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>46076.73453703704</v>
+        <v>46077.29174768519</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>46076.73532407408</v>
+        <v>46077.28112268518</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -1136,7 +1136,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="3" t="n">
-        <v>46076.73760416666</v>
+        <v>46077.31212962963</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1456,7 +1456,7 @@
         <v>1</v>
       </c>
       <c r="N15" s="3" t="n">
-        <v>46076.73608796296</v>
+        <v>46077.30944444444</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1520,7 +1520,7 @@
         <v>2</v>
       </c>
       <c r="N16" s="3" t="n">
-        <v>46076.72787037037</v>
+        <v>46077.3017824074</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -6772,7 +6772,7 @@
         <v>1</v>
       </c>
       <c r="N98" s="3" t="n">
-        <v>46076.71788194445</v>
+        <v>46076.8278125</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -6841,7 +6841,7 @@
         <v>1</v>
       </c>
       <c r="N99" s="3" t="n">
-        <v>46076.72723379629</v>
+        <v>46076.80641203704</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -6910,7 +6910,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>46076.73354166667</v>
+        <v>46077.31611111111</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6979,7 +6979,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="3" t="n">
-        <v>46076.72008101852</v>
+        <v>46076.83690972222</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -7117,7 +7117,7 @@
         <v>2</v>
       </c>
       <c r="N103" s="3" t="n">
-        <v>46076.73339120371</v>
+        <v>46077.31572916666</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7374,7 +7374,7 @@
         <v>1</v>
       </c>
       <c r="N107" s="3" t="n">
-        <v>46076.71092592592</v>
+        <v>46077.31313657408</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -7512,7 +7512,7 @@
         <v>1</v>
       </c>
       <c r="N109" s="3" t="n">
-        <v>46076.72520833334</v>
+        <v>46077.31306712963</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7581,7 +7581,7 @@
         <v>2</v>
       </c>
       <c r="N110" s="3" t="n">
-        <v>46076.73584490741</v>
+        <v>46077.28194444445</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7650,7 +7650,7 @@
         <v>2</v>
       </c>
       <c r="N111" s="3" t="n">
-        <v>46076.73309027778</v>
+        <v>46077.30137731481</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
@@ -7719,7 +7719,7 @@
         <v>2</v>
       </c>
       <c r="N112" s="3" t="n">
-        <v>46076.69840277778</v>
+        <v>46077.28114583333</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7788,7 +7788,7 @@
         <v>1</v>
       </c>
       <c r="N113" s="3" t="n">
-        <v>46076.73140046297</v>
+        <v>46077.31746527777</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7857,7 +7857,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>46076.70063657407</v>
+        <v>46077.28708333334</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -8260,7 +8260,7 @@
         <v>1</v>
       </c>
       <c r="N120" s="3" t="n">
-        <v>46076.70918981481</v>
+        <v>46076.74775462963</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -8329,7 +8329,7 @@
         <v>1</v>
       </c>
       <c r="N121" s="3" t="n">
-        <v>46076.70625</v>
+        <v>46076.82180555556</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -8464,7 +8464,7 @@
         <v>2</v>
       </c>
       <c r="N123" s="3" t="n">
-        <v>46076.70427083333</v>
+        <v>46076.82819444445</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -8533,7 +8533,7 @@
         <v>1</v>
       </c>
       <c r="N124" s="3" t="n">
-        <v>46076.73422453704</v>
+        <v>46077.32006944445</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -8602,7 +8602,7 @@
         <v>1</v>
       </c>
       <c r="N125" s="3" t="n">
-        <v>46076.71368055556</v>
+        <v>46077.2858912037</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -8671,7 +8671,7 @@
         <v>2</v>
       </c>
       <c r="N126" s="3" t="n">
-        <v>46076.73329861111</v>
+        <v>46076.77050925926</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -8740,7 +8740,7 @@
         <v>2</v>
       </c>
       <c r="N127" s="3" t="n">
-        <v>46076.71982638889</v>
+        <v>46077.29306712963</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -9144,7 +9144,7 @@
         <v>1</v>
       </c>
       <c r="N133" s="3" t="n">
-        <v>46076.72125</v>
+        <v>46076.84221064814</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -9208,7 +9208,7 @@
         <v>1</v>
       </c>
       <c r="N134" s="3" t="n">
-        <v>46076.71251157407</v>
+        <v>46076.87162037037</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -9272,7 +9272,7 @@
         <v>1</v>
       </c>
       <c r="N135" s="3" t="n">
-        <v>46076.7184837963</v>
+        <v>46076.79548611111</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -9463,7 +9463,7 @@
         <v>1</v>
       </c>
       <c r="N138" s="3" t="n">
-        <v>46076.72952546296</v>
+        <v>46076.80590277778</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9527,7 +9527,7 @@
         <v>1</v>
       </c>
       <c r="N139" s="3" t="n">
-        <v>46076.69944444444</v>
+        <v>46076.81359953704</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9591,7 +9591,7 @@
         <v>1</v>
       </c>
       <c r="N140" s="3" t="n">
-        <v>46076.73339120371</v>
+        <v>46076.81530092593</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9655,7 +9655,7 @@
         <v>1</v>
       </c>
       <c r="N141" s="3" t="n">
-        <v>46076.72554398148</v>
+        <v>46076.80428240741</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9719,7 +9719,7 @@
         <v>1</v>
       </c>
       <c r="N142" s="3" t="n">
-        <v>46076.72511574074</v>
+        <v>46076.80054398148</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9783,7 +9783,7 @@
         <v>1</v>
       </c>
       <c r="N143" s="3" t="n">
-        <v>46076.72097222223</v>
+        <v>46076.79770833333</v>
       </c>
       <c r="O143" t="inlineStr">
         <is>
@@ -9847,7 +9847,7 @@
         <v>1</v>
       </c>
       <c r="N144" s="3" t="n">
-        <v>46076.72939814815</v>
+        <v>46076.80920138889</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9911,7 +9911,7 @@
         <v>1</v>
       </c>
       <c r="N145" s="3" t="n">
-        <v>46076.70148148148</v>
+        <v>46076.8165162037</v>
       </c>
       <c r="O145" t="inlineStr">
         <is>
@@ -9975,7 +9975,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="3" t="n">
-        <v>46076.70677083333</v>
+        <v>46076.77836805556</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10039,7 +10039,7 @@
         <v>1</v>
       </c>
       <c r="N147" s="3" t="n">
-        <v>46076.72333333334</v>
+        <v>46076.80655092592</v>
       </c>
       <c r="O147" t="inlineStr">
         <is>
@@ -10103,7 +10103,7 @@
         <v>1</v>
       </c>
       <c r="N148" s="3" t="n">
-        <v>46076.7229050926</v>
+        <v>46076.80417824074</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10167,7 +10167,7 @@
         <v>1</v>
       </c>
       <c r="N149" s="3" t="n">
-        <v>46076.7118287037</v>
+        <v>46076.86672453704</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -10359,7 +10359,7 @@
         <v>1</v>
       </c>
       <c r="N152" s="3" t="n">
-        <v>46076.70512731482</v>
+        <v>46076.82327546296</v>
       </c>
       <c r="O152" t="inlineStr">
         <is>
@@ -10378,11 +10378,6 @@
           <t>OPERACAO 7.1</t>
         </is>
       </c>
-      <c r="C153" t="inlineStr">
-        <is>
-          <t>10.69.5.21</t>
-        </is>
-      </c>
       <c r="D153" t="n">
         <v>2018</v>
       </c>
@@ -10423,7 +10418,7 @@
         <v>1</v>
       </c>
       <c r="N153" s="3" t="n">
-        <v>46076.71886574074</v>
+        <v>46076.79827546296</v>
       </c>
       <c r="O153" t="inlineStr">
         <is>
@@ -10487,7 +10482,7 @@
         <v>1</v>
       </c>
       <c r="N154" s="3" t="n">
-        <v>46076.70532407407</v>
+        <v>46076.81946759259</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10551,7 +10546,7 @@
         <v>1</v>
       </c>
       <c r="N155" s="3" t="n">
-        <v>46076.73637731482</v>
+        <v>46076.81880787037</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10615,7 +10610,7 @@
         <v>1</v>
       </c>
       <c r="N156" s="3" t="n">
-        <v>46076.72557870371</v>
+        <v>46076.80028935185</v>
       </c>
       <c r="O156" t="inlineStr">
         <is>
@@ -10871,7 +10866,7 @@
         <v>1</v>
       </c>
       <c r="N160" s="3" t="n">
-        <v>46076.73675925926</v>
+        <v>46076.81438657407</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
@@ -10935,7 +10930,7 @@
         <v>1</v>
       </c>
       <c r="N161" s="3" t="n">
-        <v>46076.73771990741</v>
+        <v>46076.81960648148</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -10999,7 +10994,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="3" t="n">
-        <v>46076.7080324074</v>
+        <v>46076.7890625</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11124,10 +11119,10 @@
         </is>
       </c>
       <c r="M164" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N164" s="3" t="n">
-        <v>46076.71253472222</v>
+        <v>46077.28745370371</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11188,10 +11183,10 @@
         </is>
       </c>
       <c r="M165" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N165" s="3" t="n">
-        <v>46076.67005787037</v>
+        <v>46077.29128472223</v>
       </c>
       <c r="O165" t="inlineStr">
         <is>
@@ -11383,7 +11378,7 @@
         <v>2</v>
       </c>
       <c r="N168" s="3" t="n">
-        <v>46076.55740740741</v>
+        <v>46077.29136574074</v>
       </c>
       <c r="O168" t="inlineStr">
         <is>
@@ -11444,10 +11439,10 @@
         </is>
       </c>
       <c r="M169" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N169" s="3" t="n">
-        <v>46076.71001157408</v>
+        <v>46077.28915509259</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -11511,7 +11506,7 @@
         <v>2</v>
       </c>
       <c r="N170" s="3" t="n">
-        <v>46076.73380787037</v>
+        <v>46076.77549768519</v>
       </c>
       <c r="O170" t="inlineStr">
         <is>
@@ -11575,7 +11570,7 @@
         <v>1</v>
       </c>
       <c r="N171" s="3" t="n">
-        <v>46076.71388888889</v>
+        <v>46076.7529050926</v>
       </c>
       <c r="O171" t="inlineStr">
         <is>
@@ -11639,7 +11634,7 @@
         <v>2</v>
       </c>
       <c r="N172" s="3" t="n">
-        <v>46076.70940972222</v>
+        <v>46076.8602662037</v>
       </c>
       <c r="O172" t="inlineStr">
         <is>
@@ -11703,7 +11698,7 @@
         <v>2</v>
       </c>
       <c r="N173" s="3" t="n">
-        <v>46076.73700231482</v>
+        <v>46077.29851851852</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -11831,7 +11826,7 @@
         <v>2</v>
       </c>
       <c r="N175" s="3" t="n">
-        <v>46076.71513888889</v>
+        <v>46077.2975</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -12023,7 +12018,7 @@
         <v>2</v>
       </c>
       <c r="N178" s="3" t="n">
-        <v>46076.70798611111</v>
+        <v>46077.28731481481</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12087,7 +12082,7 @@
         <v>1</v>
       </c>
       <c r="N179" s="3" t="n">
-        <v>46076.70289351852</v>
+        <v>46076.81600694444</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12151,7 +12146,7 @@
         <v>1</v>
       </c>
       <c r="N180" s="3" t="n">
-        <v>46076.71085648148</v>
+        <v>46076.8238425926</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12215,7 +12210,7 @@
         <v>1</v>
       </c>
       <c r="N181" s="3" t="n">
-        <v>46076.73451388889</v>
+        <v>46076.85011574074</v>
       </c>
       <c r="O181" t="inlineStr">
         <is>
@@ -12796,7 +12791,7 @@
         </is>
       </c>
       <c r="N190" s="3" t="n">
-        <v>46076.70375</v>
+        <v>46076.81680555556</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12860,7 +12855,7 @@
         <v>1</v>
       </c>
       <c r="N191" s="3" t="n">
-        <v>46076.70166666667</v>
+        <v>46076.815625</v>
       </c>
       <c r="O191" t="inlineStr">
         <is>
@@ -12924,7 +12919,7 @@
         <v>1</v>
       </c>
       <c r="N192" s="3" t="n">
-        <v>46076.70276620371</v>
+        <v>46076.81246527778</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -13049,7 +13044,7 @@
         <v>2</v>
       </c>
       <c r="N194" s="3" t="n">
-        <v>46076.71369212963</v>
+        <v>46076.8184837963</v>
       </c>
       <c r="O194" t="inlineStr">
         <is>
@@ -13113,7 +13108,7 @@
         <v>1</v>
       </c>
       <c r="N195" s="3" t="n">
-        <v>46076.73121527778</v>
+        <v>46076.84635416666</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13177,7 +13172,7 @@
         <v>1</v>
       </c>
       <c r="N196" s="3" t="n">
-        <v>46076.70592592593</v>
+        <v>46076.81895833334</v>
       </c>
       <c r="O196" t="inlineStr">
         <is>
@@ -13241,7 +13236,7 @@
         <v>1</v>
       </c>
       <c r="N197" s="3" t="n">
-        <v>46076.70885416667</v>
+        <v>46076.83055555556</v>
       </c>
       <c r="O197" t="inlineStr">
         <is>
@@ -13369,7 +13364,7 @@
         <v>1</v>
       </c>
       <c r="N199" s="3" t="n">
-        <v>46076.70480324074</v>
+        <v>46076.81893518518</v>
       </c>
       <c r="O199" t="inlineStr">
         <is>
@@ -13433,7 +13428,7 @@
         <v>1</v>
       </c>
       <c r="N200" s="3" t="n">
-        <v>46076.70898148148</v>
+        <v>46076.82861111111</v>
       </c>
       <c r="O200" t="inlineStr">
         <is>
@@ -13494,7 +13489,7 @@
         </is>
       </c>
       <c r="N201" s="3" t="n">
-        <v>46076.7049537037</v>
+        <v>46076.81925925926</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -13558,7 +13553,7 @@
         <v>1</v>
       </c>
       <c r="N202" s="3" t="n">
-        <v>46076.70666666667</v>
+        <v>46076.82087962963</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13622,7 +13617,7 @@
         <v>1</v>
       </c>
       <c r="N203" s="3" t="n">
-        <v>46076.70327546296</v>
+        <v>46076.82098379629</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13686,7 +13681,7 @@
         <v>1</v>
       </c>
       <c r="N204" s="3" t="n">
-        <v>46076.72898148148</v>
+        <v>46076.80444444445</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13750,7 +13745,7 @@
         <v>1</v>
       </c>
       <c r="N205" s="3" t="n">
-        <v>46076.73388888889</v>
+        <v>46076.81057870371</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13814,7 +13809,7 @@
         <v>1</v>
       </c>
       <c r="N206" s="3" t="n">
-        <v>46076.71358796296</v>
+        <v>46076.7925462963</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -13942,7 +13937,7 @@
         <v>1</v>
       </c>
       <c r="N208" s="3" t="n">
-        <v>46076.71392361111</v>
+        <v>46076.83181712963</v>
       </c>
       <c r="O208" t="inlineStr">
         <is>
@@ -14006,7 +14001,7 @@
         <v>1</v>
       </c>
       <c r="N209" s="3" t="n">
-        <v>46076.72931712963</v>
+        <v>46076.80087962963</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14070,7 +14065,7 @@
         <v>1</v>
       </c>
       <c r="N210" s="3" t="n">
-        <v>46076.72696759259</v>
+        <v>46076.81162037037</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14134,7 +14129,7 @@
         <v>1</v>
       </c>
       <c r="N211" s="3" t="n">
-        <v>46076.70930555555</v>
+        <v>46076.8244212963</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -14198,7 +14193,7 @@
         <v>1</v>
       </c>
       <c r="N212" s="3" t="n">
-        <v>46076.73313657408</v>
+        <v>46076.80704861111</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -14262,7 +14257,7 @@
         <v>1</v>
       </c>
       <c r="N213" s="3" t="n">
-        <v>46076.72825231482</v>
+        <v>46076.80253472222</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
@@ -14326,7 +14321,7 @@
         <v>1</v>
       </c>
       <c r="N214" s="3" t="n">
-        <v>46076.72421296296</v>
+        <v>46076.80289351852</v>
       </c>
       <c r="O214" t="inlineStr">
         <is>
@@ -14390,7 +14385,7 @@
         <v>1</v>
       </c>
       <c r="N215" s="3" t="n">
-        <v>46076.7216550926</v>
+        <v>46076.79951388889</v>
       </c>
       <c r="O215" t="inlineStr">
         <is>
@@ -14454,7 +14449,7 @@
         <v>1</v>
       </c>
       <c r="N216" s="3" t="n">
-        <v>46076.71829861111</v>
+        <v>46076.79384259259</v>
       </c>
       <c r="O216" t="inlineStr">
         <is>
@@ -14473,6 +14468,11 @@
           <t>OPERACAO 8.1</t>
         </is>
       </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>10.69.5.85</t>
+        </is>
+      </c>
       <c r="D217" t="n">
         <v>2017</v>
       </c>
@@ -14513,7 +14513,7 @@
         <v>1</v>
       </c>
       <c r="N217" s="3" t="n">
-        <v>46076.70379629629</v>
+        <v>46076.81442129629</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14577,7 +14577,7 @@
         <v>1</v>
       </c>
       <c r="N218" s="3" t="n">
-        <v>46076.7124537037</v>
+        <v>46076.78930555555</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14641,7 +14641,7 @@
         <v>1</v>
       </c>
       <c r="N219" s="3" t="n">
-        <v>46076.73715277778</v>
+        <v>46076.81231481482</v>
       </c>
       <c r="O219" t="inlineStr">
         <is>
@@ -14774,7 +14774,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="3" t="n">
-        <v>46076.70457175926</v>
+        <v>46076.81674768519</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14838,7 +14838,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="3" t="n">
-        <v>46076.70340277778</v>
+        <v>46076.818125</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -14902,7 +14902,7 @@
         <v>1</v>
       </c>
       <c r="N223" s="3" t="n">
-        <v>46076.71143518519</v>
+        <v>46076.82512731481</v>
       </c>
       <c r="O223" t="inlineStr">
         <is>
@@ -14966,7 +14966,7 @@
         <v>1</v>
       </c>
       <c r="N224" s="3" t="n">
-        <v>46076.72743055555</v>
+        <v>46076.80793981482</v>
       </c>
       <c r="O224" t="inlineStr">
         <is>
@@ -15030,7 +15030,7 @@
         <v>1</v>
       </c>
       <c r="N225" s="3" t="n">
-        <v>46076.69840277778</v>
+        <v>46076.81807870371</v>
       </c>
       <c r="O225" t="inlineStr">
         <is>
@@ -15094,7 +15094,7 @@
         <v>1</v>
       </c>
       <c r="N226" s="3" t="n">
-        <v>46076.70055555556</v>
+        <v>46076.81930555555</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15158,7 +15158,7 @@
         <v>1</v>
       </c>
       <c r="N227" s="3" t="n">
-        <v>46076.73224537037</v>
+        <v>46076.81046296296</v>
       </c>
       <c r="O227" t="inlineStr">
         <is>
@@ -15222,7 +15222,7 @@
         <v>1</v>
       </c>
       <c r="N228" s="3" t="n">
-        <v>46076.71493055556</v>
+        <v>46076.82831018518</v>
       </c>
       <c r="O228" t="inlineStr">
         <is>
@@ -15286,7 +15286,7 @@
         <v>1</v>
       </c>
       <c r="N229" s="3" t="n">
-        <v>46076.73138888889</v>
+        <v>46076.81256944445</v>
       </c>
       <c r="O229" t="inlineStr">
         <is>
@@ -15350,7 +15350,7 @@
         <v>1</v>
       </c>
       <c r="N230" s="3" t="n">
-        <v>46076.700625</v>
+        <v>46076.81914351852</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15414,7 +15414,7 @@
         <v>1</v>
       </c>
       <c r="N231" s="3" t="n">
-        <v>46076.70793981481</v>
+        <v>46076.82577546296</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15542,7 +15542,7 @@
         <v>1</v>
       </c>
       <c r="N233" s="3" t="n">
-        <v>46076.70229166667</v>
+        <v>46076.81894675926</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15606,7 +15606,7 @@
         <v>1</v>
       </c>
       <c r="N234" s="3" t="n">
-        <v>46076.70791666667</v>
+        <v>46076.8247337963</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -15670,7 +15670,7 @@
         <v>1</v>
       </c>
       <c r="N235" s="3" t="n">
-        <v>46076.72476851852</v>
+        <v>46076.80386574074</v>
       </c>
       <c r="O235" t="inlineStr">
         <is>
@@ -15734,7 +15734,7 @@
         <v>1</v>
       </c>
       <c r="N236" s="3" t="n">
-        <v>46076.72701388889</v>
+        <v>46076.8062037037</v>
       </c>
       <c r="O236" t="inlineStr">
         <is>
@@ -15798,7 +15798,7 @@
         <v>1</v>
       </c>
       <c r="N237" s="3" t="n">
-        <v>46076.71039351852</v>
+        <v>46076.8252662037</v>
       </c>
       <c r="O237" t="inlineStr">
         <is>
@@ -15862,7 +15862,7 @@
         <v>1</v>
       </c>
       <c r="N238" s="3" t="n">
-        <v>46076.72914351852</v>
+        <v>46076.80190972222</v>
       </c>
       <c r="O238" t="inlineStr">
         <is>
@@ -15926,7 +15926,7 @@
         <v>1</v>
       </c>
       <c r="N239" s="3" t="n">
-        <v>46076.73451388889</v>
+        <v>46076.81688657407</v>
       </c>
       <c r="O239" t="inlineStr">
         <is>
@@ -15990,7 +15990,7 @@
         <v>1</v>
       </c>
       <c r="N240" s="3" t="n">
-        <v>46076.73399305555</v>
+        <v>46076.80755787037</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16054,7 +16054,7 @@
         <v>1</v>
       </c>
       <c r="N241" s="3" t="n">
-        <v>46076.72371527777</v>
+        <v>46076.80427083333</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16118,7 +16118,7 @@
         <v>1</v>
       </c>
       <c r="N242" s="3" t="n">
-        <v>46076.70850694444</v>
+        <v>46076.82931712963</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16201,11 +16201,6 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
-      <c r="C244" t="inlineStr">
-        <is>
-          <t>10.69.5.112</t>
-        </is>
-      </c>
       <c r="D244" t="n">
         <v>2019</v>
       </c>
@@ -16310,7 +16305,7 @@
         <v>1</v>
       </c>
       <c r="N245" s="3" t="n">
-        <v>46076.73438657408</v>
+        <v>46076.80967592593</v>
       </c>
       <c r="O245" t="inlineStr">
         <is>
@@ -16374,7 +16369,7 @@
         <v>1</v>
       </c>
       <c r="N246" s="3" t="n">
-        <v>46076.70545138889</v>
+        <v>46076.82318287037</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16438,7 +16433,7 @@
         <v>1</v>
       </c>
       <c r="N247" s="3" t="n">
-        <v>46076.73392361111</v>
+        <v>46076.80577546296</v>
       </c>
       <c r="O247" t="inlineStr">
         <is>
@@ -16502,7 +16497,7 @@
         <v>1</v>
       </c>
       <c r="N248" s="3" t="n">
-        <v>46076.70577546296</v>
+        <v>46076.81885416667</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16625,7 +16620,7 @@
         <v>1</v>
       </c>
       <c r="N250" s="3" t="n">
-        <v>46076.72375</v>
+        <v>46076.79996527778</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16689,7 +16684,7 @@
         <v>1</v>
       </c>
       <c r="N251" s="3" t="n">
-        <v>46076.73357638889</v>
+        <v>46076.84975694444</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16753,7 +16748,7 @@
         <v>1</v>
       </c>
       <c r="N252" s="3" t="n">
-        <v>46076.7346412037</v>
+        <v>46076.81327546296</v>
       </c>
       <c r="O252" t="inlineStr">
         <is>
@@ -16817,7 +16812,7 @@
         <v>1</v>
       </c>
       <c r="N253" s="3" t="n">
-        <v>46076.70173611111</v>
+        <v>46076.82226851852</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16875,7 +16870,7 @@
         <v>1</v>
       </c>
       <c r="N254" s="3" t="n">
-        <v>46076.70730324074</v>
+        <v>46076.81884259259</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -16939,7 +16934,7 @@
         <v>1</v>
       </c>
       <c r="N255" s="3" t="n">
-        <v>46076.70194444444</v>
+        <v>46076.82233796296</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -17003,7 +16998,7 @@
         <v>1</v>
       </c>
       <c r="N256" s="3" t="n">
-        <v>46076.70689814815</v>
+        <v>46076.79159722223</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17067,7 +17062,7 @@
         <v>1</v>
       </c>
       <c r="N257" s="3" t="n">
-        <v>46076.71556712963</v>
+        <v>46076.79739583333</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17195,7 +17190,7 @@
         <v>1</v>
       </c>
       <c r="N259" s="3" t="n">
-        <v>46076.70084490741</v>
+        <v>46076.81821759259</v>
       </c>
       <c r="O259" t="inlineStr">
         <is>
@@ -17387,7 +17382,7 @@
         <v>1</v>
       </c>
       <c r="N262" s="3" t="n">
-        <v>46076.70920138889</v>
+        <v>46076.82581018518</v>
       </c>
       <c r="O262" t="inlineStr">
         <is>
@@ -17451,7 +17446,7 @@
         <v>1</v>
       </c>
       <c r="N263" s="3" t="n">
-        <v>46076.72741898148</v>
+        <v>46076.80466435185</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17515,7 +17510,7 @@
         <v>1</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>46076.72865740741</v>
+        <v>46076.8065162037</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17579,7 +17574,7 @@
         <v>1</v>
       </c>
       <c r="N265" s="3" t="n">
-        <v>46076.70525462963</v>
+        <v>46076.81990740741</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17643,7 +17638,7 @@
         <v>1</v>
       </c>
       <c r="N266" s="3" t="n">
-        <v>46076.7022337963</v>
+        <v>46076.85813657408</v>
       </c>
       <c r="O266" t="inlineStr">
         <is>
@@ -17707,7 +17702,7 @@
         <v>1</v>
       </c>
       <c r="N267" s="3" t="n">
-        <v>46076.71700231481</v>
+        <v>46076.79690972222</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17771,7 +17766,7 @@
         <v>1</v>
       </c>
       <c r="N268" s="3" t="n">
-        <v>46076.7315625</v>
+        <v>46076.80638888889</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17835,7 +17830,7 @@
         <v>1</v>
       </c>
       <c r="N269" s="3" t="n">
-        <v>46076.69887731481</v>
+        <v>46076.81399305556</v>
       </c>
       <c r="O269" t="inlineStr">
         <is>
@@ -17896,7 +17891,7 @@
         </is>
       </c>
       <c r="N270" s="3" t="n">
-        <v>46076.73762731482</v>
+        <v>46077.28304398148</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -17960,7 +17955,7 @@
         <v>1</v>
       </c>
       <c r="N271" s="3" t="n">
-        <v>46076.65869212963</v>
+        <v>46077.05097222222</v>
       </c>
       <c r="O271" t="inlineStr">
         <is>
@@ -18088,7 +18083,7 @@
         <v>2</v>
       </c>
       <c r="N273" s="3" t="n">
-        <v>46076.71391203703</v>
+        <v>46077.28936342592</v>
       </c>
       <c r="O273" t="inlineStr">
         <is>
@@ -18408,7 +18403,7 @@
         <v>1</v>
       </c>
       <c r="N278" s="3" t="n">
-        <v>46076.71561342593</v>
+        <v>46076.79479166667</v>
       </c>
       <c r="O278" t="inlineStr">
         <is>
@@ -18472,7 +18467,7 @@
         <v>1</v>
       </c>
       <c r="N279" s="3" t="n">
-        <v>46076.62613425926</v>
+        <v>46077.30326388889</v>
       </c>
       <c r="O279" t="inlineStr">
         <is>
@@ -18600,7 +18595,7 @@
         <v>1</v>
       </c>
       <c r="N281" s="3" t="n">
-        <v>46076.706875</v>
+        <v>46076.86475694444</v>
       </c>
       <c r="O281" t="inlineStr">
         <is>
@@ -18659,7 +18654,7 @@
         <v>1</v>
       </c>
       <c r="N282" s="3" t="n">
-        <v>46076.71212962963</v>
+        <v>46076.82537037037</v>
       </c>
       <c r="O282" t="inlineStr">
         <is>
@@ -18723,7 +18718,7 @@
         <v>1</v>
       </c>
       <c r="N283" s="3" t="n">
-        <v>46076.70984953704</v>
+        <v>46076.82734953704</v>
       </c>
       <c r="O283" t="inlineStr">
         <is>
@@ -18787,7 +18782,7 @@
         <v>1</v>
       </c>
       <c r="N284" s="3" t="n">
-        <v>46076.7341087963</v>
+        <v>46076.86959490741</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18851,7 +18846,7 @@
         <v>1</v>
       </c>
       <c r="N285" s="3" t="n">
-        <v>46076.7147337963</v>
+        <v>46076.79333333333</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -18870,6 +18865,11 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>10.69.5.155</t>
+        </is>
+      </c>
       <c r="D286" t="n">
         <v>2019</v>
       </c>
@@ -18910,7 +18910,7 @@
         <v>1</v>
       </c>
       <c r="N286" s="3" t="n">
-        <v>46076.5897800926</v>
+        <v>46076.7542824074</v>
       </c>
       <c r="O286" t="inlineStr">
         <is>
@@ -18974,7 +18974,7 @@
         <v>1</v>
       </c>
       <c r="N287" s="3" t="n">
-        <v>46076.5925</v>
+        <v>46077.14640046296</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
@@ -19102,7 +19102,7 @@
         <v>1</v>
       </c>
       <c r="N289" s="3" t="n">
-        <v>46076.73748842593</v>
+        <v>46076.86166666666</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -19896,7 +19896,7 @@
         <v>1</v>
       </c>
       <c r="N302" s="3" t="n">
-        <v>46076.73310185185</v>
+        <v>46077.32010416667</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -21012,7 +21012,7 @@
         </is>
       </c>
       <c r="N320" s="3" t="n">
-        <v>46076.73121527778</v>
+        <v>46077.2959837963</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21737,7 +21737,7 @@
         <v>1</v>
       </c>
       <c r="N332" s="3" t="n">
-        <v>46076.71962962963</v>
+        <v>46077.28819444445</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21801,7 +21801,7 @@
         <v>2</v>
       </c>
       <c r="N333" s="3" t="n">
-        <v>46076.71458333333</v>
+        <v>46077.28802083333</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21865,7 +21865,7 @@
         <v>2</v>
       </c>
       <c r="N334" s="3" t="n">
-        <v>46076.71335648148</v>
+        <v>46077.28866898148</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21929,7 +21929,7 @@
         <v>2</v>
       </c>
       <c r="N335" s="3" t="n">
-        <v>46076.71543981481</v>
+        <v>46077.28825231481</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -21993,7 +21993,7 @@
         <v>1</v>
       </c>
       <c r="N336" s="3" t="n">
-        <v>46076.73644675926</v>
+        <v>46077.29880787037</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22057,7 +22057,7 @@
         <v>1</v>
       </c>
       <c r="N337" s="3" t="n">
-        <v>46076.72912037037</v>
+        <v>46077.28917824074</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22121,7 +22121,7 @@
         <v>2</v>
       </c>
       <c r="N338" s="3" t="n">
-        <v>46076.7296412037</v>
+        <v>46077.28865740741</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -22377,7 +22377,7 @@
         <v>2</v>
       </c>
       <c r="N342" s="3" t="n">
-        <v>46076.56592592593</v>
+        <v>46077.2931712963</v>
       </c>
       <c r="O342" t="inlineStr">
         <is>
@@ -23889,7 +23889,7 @@
         </is>
       </c>
       <c r="N366" s="3" t="n">
-        <v>46076.72384259259</v>
+        <v>46077.30633101852</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -24150,7 +24150,7 @@
         <v>1</v>
       </c>
       <c r="N370" s="3" t="n">
-        <v>46076.71877314815</v>
+        <v>46076.75436342593</v>
       </c>
       <c r="O370" t="inlineStr">
         <is>
@@ -24426,7 +24426,7 @@
         <v>1</v>
       </c>
       <c r="N374" s="3" t="n">
-        <v>46076.71185185185</v>
+        <v>46076.75230324074</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24492,7 +24492,7 @@
         </is>
       </c>
       <c r="N375" s="3" t="n">
-        <v>46076.71289351852</v>
+        <v>46077.30444444445</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
@@ -24561,7 +24561,7 @@
         <v>1</v>
       </c>
       <c r="N376" s="3" t="n">
-        <v>46076.73079861111</v>
+        <v>46077.30716435185</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -24699,7 +24699,7 @@
         <v>2</v>
       </c>
       <c r="N378" s="3" t="n">
-        <v>46076.72037037037</v>
+        <v>46077.29969907407</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização automática 2026-02-24 11:52:06.785706
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>46077.29174768519</v>
+        <v>46077.48548611111</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>46077.28112268518</v>
+        <v>46077.47445601852</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
         <v>1</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>46076.69822916666</v>
+        <v>46077.48221064815</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>46076.64954861111</v>
+        <v>46077.45922453704</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -1091,11 +1091,6 @@
           <t>AUDITORIO</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>10.69.3.160</t>
-        </is>
-      </c>
       <c r="D10" t="n">
         <v>2017</v>
       </c>
@@ -1136,7 +1131,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="3" t="n">
-        <v>46077.31212962963</v>
+        <v>46077.46771990741</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1456,7 +1451,7 @@
         <v>1</v>
       </c>
       <c r="N15" s="3" t="n">
-        <v>46077.30944444444</v>
+        <v>46077.39167824074</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1520,7 +1515,7 @@
         <v>2</v>
       </c>
       <c r="N16" s="3" t="n">
-        <v>46077.3017824074</v>
+        <v>46077.45256944445</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -2249,7 +2244,7 @@
         </is>
       </c>
       <c r="N28" s="3" t="n">
-        <v>46076.73538194445</v>
+        <v>46077.45503472222</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -6575,7 +6570,7 @@
         <v>1</v>
       </c>
       <c r="N95" s="3" t="n">
-        <v>46076.70255787037</v>
+        <v>46077.47164351852</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -6663,6 +6658,11 @@
           <t>COORDENACAO</t>
         </is>
       </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>10.69.3.93</t>
+        </is>
+      </c>
       <c r="D97" t="n">
         <v>2025</v>
       </c>
@@ -6708,7 +6708,7 @@
         <v>1</v>
       </c>
       <c r="N97" s="3" t="n">
-        <v>46076.69875</v>
+        <v>46077.48524305555</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -6772,7 +6772,7 @@
         <v>1</v>
       </c>
       <c r="N98" s="3" t="n">
-        <v>46076.8278125</v>
+        <v>46077.47292824074</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -6841,7 +6841,7 @@
         <v>1</v>
       </c>
       <c r="N99" s="3" t="n">
-        <v>46076.80641203704</v>
+        <v>46077.44916666667</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -6910,7 +6910,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>46077.31611111111</v>
+        <v>46077.4725462963</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -7117,7 +7117,7 @@
         <v>2</v>
       </c>
       <c r="N103" s="3" t="n">
-        <v>46077.31572916666</v>
+        <v>46077.47799768519</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7243,8 +7243,11 @@
           <t>HP ProBook 440 14 inch G9 Notebook PC</t>
         </is>
       </c>
+      <c r="M105" t="n">
+        <v>1</v>
+      </c>
       <c r="N105" s="3" t="n">
-        <v>46051.74359953704</v>
+        <v>46077.46759259259</v>
       </c>
       <c r="O105" t="inlineStr">
         <is>
@@ -7374,7 +7377,7 @@
         <v>1</v>
       </c>
       <c r="N107" s="3" t="n">
-        <v>46077.31313657408</v>
+        <v>46077.46899305555</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -7512,7 +7515,7 @@
         <v>1</v>
       </c>
       <c r="N109" s="3" t="n">
-        <v>46077.31306712963</v>
+        <v>46077.47298611111</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7581,7 +7584,7 @@
         <v>2</v>
       </c>
       <c r="N110" s="3" t="n">
-        <v>46077.28194444445</v>
+        <v>46077.48182870371</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7650,7 +7653,7 @@
         <v>2</v>
       </c>
       <c r="N111" s="3" t="n">
-        <v>46077.30137731481</v>
+        <v>46077.46240740741</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
@@ -7719,7 +7722,7 @@
         <v>2</v>
       </c>
       <c r="N112" s="3" t="n">
-        <v>46077.28114583333</v>
+        <v>46077.45207175926</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7788,7 +7791,7 @@
         <v>1</v>
       </c>
       <c r="N113" s="3" t="n">
-        <v>46077.31746527777</v>
+        <v>46077.48482638889</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7857,7 +7860,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>46077.28708333334</v>
+        <v>46077.48614583333</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -7923,7 +7926,7 @@
         </is>
       </c>
       <c r="N115" s="3" t="n">
-        <v>46076.68381944444</v>
+        <v>46077.46586805556</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -8056,7 +8059,7 @@
         <v>1</v>
       </c>
       <c r="N117" s="3" t="n">
-        <v>46076.67082175926</v>
+        <v>46077.44150462963</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -8122,7 +8125,7 @@
         </is>
       </c>
       <c r="N118" s="3" t="n">
-        <v>46059.69064814815</v>
+        <v>46077.45927083334</v>
       </c>
       <c r="O118" t="inlineStr">
         <is>
@@ -8260,7 +8263,7 @@
         <v>1</v>
       </c>
       <c r="N120" s="3" t="n">
-        <v>46076.74775462963</v>
+        <v>46077.47049768519</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -8329,7 +8332,7 @@
         <v>1</v>
       </c>
       <c r="N121" s="3" t="n">
-        <v>46076.82180555556</v>
+        <v>46077.428125</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -8395,7 +8398,7 @@
         </is>
       </c>
       <c r="N122" s="3" t="n">
-        <v>46076.67222222222</v>
+        <v>46077.48168981481</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -8464,7 +8467,7 @@
         <v>2</v>
       </c>
       <c r="N123" s="3" t="n">
-        <v>46076.82819444445</v>
+        <v>46077.47847222222</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -8533,7 +8536,7 @@
         <v>1</v>
       </c>
       <c r="N124" s="3" t="n">
-        <v>46077.32006944445</v>
+        <v>46077.47162037037</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -8602,7 +8605,7 @@
         <v>1</v>
       </c>
       <c r="N125" s="3" t="n">
-        <v>46077.2858912037</v>
+        <v>46077.48234953704</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -8671,7 +8674,7 @@
         <v>2</v>
       </c>
       <c r="N126" s="3" t="n">
-        <v>46076.77050925926</v>
+        <v>46077.4712037037</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -8740,7 +8743,7 @@
         <v>2</v>
       </c>
       <c r="N127" s="3" t="n">
-        <v>46077.29306712963</v>
+        <v>46077.48553240741</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -8809,7 +8812,7 @@
         <v>1</v>
       </c>
       <c r="N128" s="3" t="n">
-        <v>46076.71164351852</v>
+        <v>46077.45171296296</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -8947,7 +8950,7 @@
         <v>1</v>
       </c>
       <c r="N130" s="3" t="n">
-        <v>46076.729375</v>
+        <v>46077.47740740741</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -9011,7 +9014,7 @@
         <v>1</v>
       </c>
       <c r="N131" s="3" t="n">
-        <v>46076.69158564815</v>
+        <v>46077.4804050926</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -9144,7 +9147,7 @@
         <v>1</v>
       </c>
       <c r="N133" s="3" t="n">
-        <v>46076.84221064814</v>
+        <v>46077.48652777778</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -9463,7 +9466,7 @@
         <v>1</v>
       </c>
       <c r="N138" s="3" t="n">
-        <v>46076.80590277778</v>
+        <v>46077.45543981482</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9527,7 +9530,7 @@
         <v>1</v>
       </c>
       <c r="N139" s="3" t="n">
-        <v>46076.81359953704</v>
+        <v>46077.45866898148</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9591,7 +9594,7 @@
         <v>1</v>
       </c>
       <c r="N140" s="3" t="n">
-        <v>46076.81530092593</v>
+        <v>46077.46556712963</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9655,7 +9658,7 @@
         <v>1</v>
       </c>
       <c r="N141" s="3" t="n">
-        <v>46076.80428240741</v>
+        <v>46077.45891203704</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9719,7 +9722,7 @@
         <v>1</v>
       </c>
       <c r="N142" s="3" t="n">
-        <v>46076.80054398148</v>
+        <v>46077.45677083333</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9783,7 +9786,7 @@
         <v>1</v>
       </c>
       <c r="N143" s="3" t="n">
-        <v>46076.79770833333</v>
+        <v>46077.48805555556</v>
       </c>
       <c r="O143" t="inlineStr">
         <is>
@@ -9847,7 +9850,7 @@
         <v>1</v>
       </c>
       <c r="N144" s="3" t="n">
-        <v>46076.80920138889</v>
+        <v>46077.45958333334</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9975,7 +9978,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="3" t="n">
-        <v>46076.77836805556</v>
+        <v>46077.47035879629</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10039,7 +10042,7 @@
         <v>1</v>
       </c>
       <c r="N147" s="3" t="n">
-        <v>46076.80655092592</v>
+        <v>46077.47700231482</v>
       </c>
       <c r="O147" t="inlineStr">
         <is>
@@ -10103,7 +10106,7 @@
         <v>1</v>
       </c>
       <c r="N148" s="3" t="n">
-        <v>46076.80417824074</v>
+        <v>46077.46990740741</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10167,7 +10170,7 @@
         <v>1</v>
       </c>
       <c r="N149" s="3" t="n">
-        <v>46076.86672453704</v>
+        <v>46077.46895833333</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -10231,7 +10234,7 @@
         <v>1</v>
       </c>
       <c r="N150" s="3" t="n">
-        <v>46076.66200231481</v>
+        <v>46077.48763888889</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -10378,6 +10381,11 @@
           <t>OPERACAO 7.1</t>
         </is>
       </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>10.69.5.21</t>
+        </is>
+      </c>
       <c r="D153" t="n">
         <v>2018</v>
       </c>
@@ -10418,7 +10426,7 @@
         <v>1</v>
       </c>
       <c r="N153" s="3" t="n">
-        <v>46076.79827546296</v>
+        <v>46077.48196759259</v>
       </c>
       <c r="O153" t="inlineStr">
         <is>
@@ -10482,7 +10490,7 @@
         <v>1</v>
       </c>
       <c r="N154" s="3" t="n">
-        <v>46076.81946759259</v>
+        <v>46077.47834490741</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10546,7 +10554,7 @@
         <v>1</v>
       </c>
       <c r="N155" s="3" t="n">
-        <v>46076.81880787037</v>
+        <v>46077.48752314815</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10610,7 +10618,7 @@
         <v>1</v>
       </c>
       <c r="N156" s="3" t="n">
-        <v>46076.80028935185</v>
+        <v>46077.42474537037</v>
       </c>
       <c r="O156" t="inlineStr">
         <is>
@@ -10674,7 +10682,7 @@
         <v>1</v>
       </c>
       <c r="N157" s="3" t="n">
-        <v>46076.59125</v>
+        <v>46077.453125</v>
       </c>
       <c r="O157" t="inlineStr">
         <is>
@@ -10738,7 +10746,7 @@
         <v>1</v>
       </c>
       <c r="N158" s="3" t="n">
-        <v>46076.54633101852</v>
+        <v>46077.46967592592</v>
       </c>
       <c r="O158" t="inlineStr">
         <is>
@@ -10802,7 +10810,7 @@
         <v>1</v>
       </c>
       <c r="N159" s="3" t="n">
-        <v>46076.58689814815</v>
+        <v>46077.47540509259</v>
       </c>
       <c r="O159" t="inlineStr">
         <is>
@@ -10866,7 +10874,7 @@
         <v>1</v>
       </c>
       <c r="N160" s="3" t="n">
-        <v>46076.81438657407</v>
+        <v>46077.45787037037</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
@@ -10930,7 +10938,7 @@
         <v>1</v>
       </c>
       <c r="N161" s="3" t="n">
-        <v>46076.81960648148</v>
+        <v>46077.4540162037</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -10994,7 +11002,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="3" t="n">
-        <v>46076.7890625</v>
+        <v>46077.45111111111</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11119,10 +11127,10 @@
         </is>
       </c>
       <c r="M164" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N164" s="3" t="n">
-        <v>46077.28745370371</v>
+        <v>46077.47741898148</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11183,10 +11191,10 @@
         </is>
       </c>
       <c r="M165" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N165" s="3" t="n">
-        <v>46077.29128472223</v>
+        <v>46077.48633101852</v>
       </c>
       <c r="O165" t="inlineStr">
         <is>
@@ -11314,7 +11322,7 @@
         <v>2</v>
       </c>
       <c r="N167" s="3" t="n">
-        <v>46076.60028935185</v>
+        <v>46077.45063657407</v>
       </c>
       <c r="O167" t="inlineStr">
         <is>
@@ -11378,7 +11386,7 @@
         <v>2</v>
       </c>
       <c r="N168" s="3" t="n">
-        <v>46077.29136574074</v>
+        <v>46077.48010416667</v>
       </c>
       <c r="O168" t="inlineStr">
         <is>
@@ -11439,10 +11447,10 @@
         </is>
       </c>
       <c r="M169" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N169" s="3" t="n">
-        <v>46077.28915509259</v>
+        <v>46077.4815162037</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -11506,7 +11514,7 @@
         <v>2</v>
       </c>
       <c r="N170" s="3" t="n">
-        <v>46076.77549768519</v>
+        <v>46077.47752314815</v>
       </c>
       <c r="O170" t="inlineStr">
         <is>
@@ -11570,7 +11578,7 @@
         <v>1</v>
       </c>
       <c r="N171" s="3" t="n">
-        <v>46076.7529050926</v>
+        <v>46077.48350694445</v>
       </c>
       <c r="O171" t="inlineStr">
         <is>
@@ -11634,7 +11642,7 @@
         <v>2</v>
       </c>
       <c r="N172" s="3" t="n">
-        <v>46076.8602662037</v>
+        <v>46077.48439814815</v>
       </c>
       <c r="O172" t="inlineStr">
         <is>
@@ -11698,7 +11706,7 @@
         <v>2</v>
       </c>
       <c r="N173" s="3" t="n">
-        <v>46077.29851851852</v>
+        <v>46077.48715277778</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -11762,7 +11770,7 @@
         <v>2</v>
       </c>
       <c r="N174" s="3" t="n">
-        <v>46076.548125</v>
+        <v>46077.46326388889</v>
       </c>
       <c r="O174" t="inlineStr">
         <is>
@@ -11826,7 +11834,7 @@
         <v>2</v>
       </c>
       <c r="N175" s="3" t="n">
-        <v>46077.2975</v>
+        <v>46077.45664351852</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -11890,7 +11898,7 @@
         <v>2</v>
       </c>
       <c r="N176" s="3" t="n">
-        <v>46076.66653935185</v>
+        <v>46077.48125</v>
       </c>
       <c r="O176" t="inlineStr">
         <is>
@@ -11954,7 +11962,7 @@
         <v>3</v>
       </c>
       <c r="N177" s="3" t="n">
-        <v>46076.70077546296</v>
+        <v>46077.45925925926</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
@@ -12018,7 +12026,7 @@
         <v>2</v>
       </c>
       <c r="N178" s="3" t="n">
-        <v>46077.28731481481</v>
+        <v>46077.47494212963</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12082,7 +12090,7 @@
         <v>1</v>
       </c>
       <c r="N179" s="3" t="n">
-        <v>46076.81600694444</v>
+        <v>46077.47481481481</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12146,7 +12154,7 @@
         <v>1</v>
       </c>
       <c r="N180" s="3" t="n">
-        <v>46076.8238425926</v>
+        <v>46077.46071759259</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12535,7 +12543,7 @@
         <v>1</v>
       </c>
       <c r="N186" s="3" t="n">
-        <v>46076.54494212963</v>
+        <v>46077.48688657407</v>
       </c>
       <c r="O186" t="inlineStr">
         <is>
@@ -12599,7 +12607,7 @@
         <v>1</v>
       </c>
       <c r="N187" s="3" t="n">
-        <v>46076.55138888889</v>
+        <v>46077.48553240741</v>
       </c>
       <c r="O187" t="inlineStr">
         <is>
@@ -12663,7 +12671,7 @@
         <v>1</v>
       </c>
       <c r="N188" s="3" t="n">
-        <v>46076.57655092593</v>
+        <v>46077.47578703704</v>
       </c>
       <c r="O188" t="inlineStr">
         <is>
@@ -12791,7 +12799,7 @@
         </is>
       </c>
       <c r="N190" s="3" t="n">
-        <v>46076.81680555556</v>
+        <v>46077.47396990741</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12919,7 +12927,7 @@
         <v>1</v>
       </c>
       <c r="N192" s="3" t="n">
-        <v>46076.81246527778</v>
+        <v>46077.48172453704</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -13044,7 +13052,7 @@
         <v>2</v>
       </c>
       <c r="N194" s="3" t="n">
-        <v>46076.8184837963</v>
+        <v>46077.48881944444</v>
       </c>
       <c r="O194" t="inlineStr">
         <is>
@@ -13108,7 +13116,7 @@
         <v>1</v>
       </c>
       <c r="N195" s="3" t="n">
-        <v>46076.84635416666</v>
+        <v>46077.47493055555</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13172,7 +13180,7 @@
         <v>1</v>
       </c>
       <c r="N196" s="3" t="n">
-        <v>46076.81895833334</v>
+        <v>46077.45775462963</v>
       </c>
       <c r="O196" t="inlineStr">
         <is>
@@ -13300,7 +13308,7 @@
         <v>1</v>
       </c>
       <c r="N198" s="3" t="n">
-        <v>46074.85094907408</v>
+        <v>46077.483125</v>
       </c>
       <c r="O198" t="inlineStr">
         <is>
@@ -13489,7 +13497,7 @@
         </is>
       </c>
       <c r="N201" s="3" t="n">
-        <v>46076.81925925926</v>
+        <v>46077.46614583334</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -13553,7 +13561,7 @@
         <v>1</v>
       </c>
       <c r="N202" s="3" t="n">
-        <v>46076.82087962963</v>
+        <v>46077.46539351852</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13617,7 +13625,7 @@
         <v>1</v>
       </c>
       <c r="N203" s="3" t="n">
-        <v>46076.82098379629</v>
+        <v>46077.45571759259</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13681,7 +13689,7 @@
         <v>1</v>
       </c>
       <c r="N204" s="3" t="n">
-        <v>46076.80444444445</v>
+        <v>46077.46771990741</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13745,7 +13753,7 @@
         <v>1</v>
       </c>
       <c r="N205" s="3" t="n">
-        <v>46076.81057870371</v>
+        <v>46077.47450231481</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13809,7 +13817,7 @@
         <v>1</v>
       </c>
       <c r="N206" s="3" t="n">
-        <v>46076.7925462963</v>
+        <v>46077.4650925926</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -13873,7 +13881,7 @@
         <v>1</v>
       </c>
       <c r="N207" s="3" t="n">
-        <v>46076.6583912037</v>
+        <v>46077.46385416666</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -13937,7 +13945,7 @@
         <v>1</v>
       </c>
       <c r="N208" s="3" t="n">
-        <v>46076.83181712963</v>
+        <v>46077.47751157408</v>
       </c>
       <c r="O208" t="inlineStr">
         <is>
@@ -14001,7 +14009,7 @@
         <v>1</v>
       </c>
       <c r="N209" s="3" t="n">
-        <v>46076.80087962963</v>
+        <v>46077.46837962963</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14065,7 +14073,7 @@
         <v>1</v>
       </c>
       <c r="N210" s="3" t="n">
-        <v>46076.81162037037</v>
+        <v>46077.48851851852</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14129,7 +14137,7 @@
         <v>1</v>
       </c>
       <c r="N211" s="3" t="n">
-        <v>46076.8244212963</v>
+        <v>46077.46057870371</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -14193,7 +14201,7 @@
         <v>1</v>
       </c>
       <c r="N212" s="3" t="n">
-        <v>46076.80704861111</v>
+        <v>46077.46108796296</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -14257,7 +14265,7 @@
         <v>1</v>
       </c>
       <c r="N213" s="3" t="n">
-        <v>46076.80253472222</v>
+        <v>46077.46685185185</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
@@ -14321,7 +14329,7 @@
         <v>1</v>
       </c>
       <c r="N214" s="3" t="n">
-        <v>46076.80289351852</v>
+        <v>46077.4608912037</v>
       </c>
       <c r="O214" t="inlineStr">
         <is>
@@ -14385,7 +14393,7 @@
         <v>1</v>
       </c>
       <c r="N215" s="3" t="n">
-        <v>46076.79951388889</v>
+        <v>46077.4581712963</v>
       </c>
       <c r="O215" t="inlineStr">
         <is>
@@ -14449,7 +14457,7 @@
         <v>1</v>
       </c>
       <c r="N216" s="3" t="n">
-        <v>46076.79384259259</v>
+        <v>46077.45829861111</v>
       </c>
       <c r="O216" t="inlineStr">
         <is>
@@ -14468,11 +14476,6 @@
           <t>OPERACAO 8.1</t>
         </is>
       </c>
-      <c r="C217" t="inlineStr">
-        <is>
-          <t>10.69.5.85</t>
-        </is>
-      </c>
       <c r="D217" t="n">
         <v>2017</v>
       </c>
@@ -14513,7 +14516,7 @@
         <v>1</v>
       </c>
       <c r="N217" s="3" t="n">
-        <v>46076.81442129629</v>
+        <v>46077.4572800926</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14577,7 +14580,7 @@
         <v>1</v>
       </c>
       <c r="N218" s="3" t="n">
-        <v>46076.78930555555</v>
+        <v>46077.45650462963</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14641,7 +14644,7 @@
         <v>1</v>
       </c>
       <c r="N219" s="3" t="n">
-        <v>46076.81231481482</v>
+        <v>46077.45829861111</v>
       </c>
       <c r="O219" t="inlineStr">
         <is>
@@ -14710,7 +14713,7 @@
         <v>1</v>
       </c>
       <c r="N220" s="3" t="n">
-        <v>46076.62596064815</v>
+        <v>46077.45881944444</v>
       </c>
       <c r="O220" t="inlineStr">
         <is>
@@ -14774,7 +14777,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="3" t="n">
-        <v>46076.81674768519</v>
+        <v>46077.45365740741</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14838,7 +14841,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="3" t="n">
-        <v>46076.818125</v>
+        <v>46077.45115740741</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -14902,7 +14905,7 @@
         <v>1</v>
       </c>
       <c r="N223" s="3" t="n">
-        <v>46076.82512731481</v>
+        <v>46077.47369212963</v>
       </c>
       <c r="O223" t="inlineStr">
         <is>
@@ -15030,7 +15033,7 @@
         <v>1</v>
       </c>
       <c r="N225" s="3" t="n">
-        <v>46076.81807870371</v>
+        <v>46077.45584490741</v>
       </c>
       <c r="O225" t="inlineStr">
         <is>
@@ -15094,7 +15097,7 @@
         <v>1</v>
       </c>
       <c r="N226" s="3" t="n">
-        <v>46076.81930555555</v>
+        <v>46077.46091435185</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15158,7 +15161,7 @@
         <v>1</v>
       </c>
       <c r="N227" s="3" t="n">
-        <v>46076.81046296296</v>
+        <v>46077.46981481482</v>
       </c>
       <c r="O227" t="inlineStr">
         <is>
@@ -15222,7 +15225,7 @@
         <v>1</v>
       </c>
       <c r="N228" s="3" t="n">
-        <v>46076.82831018518</v>
+        <v>46077.47884259259</v>
       </c>
       <c r="O228" t="inlineStr">
         <is>
@@ -15350,7 +15353,7 @@
         <v>1</v>
       </c>
       <c r="N230" s="3" t="n">
-        <v>46076.81914351852</v>
+        <v>46077.45504629629</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15414,7 +15417,7 @@
         <v>1</v>
       </c>
       <c r="N231" s="3" t="n">
-        <v>46076.82577546296</v>
+        <v>46077.47356481481</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15478,7 +15481,7 @@
         <v>1</v>
       </c>
       <c r="N232" s="3" t="n">
-        <v>46076.61415509259</v>
+        <v>46077.48247685185</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -15542,7 +15545,7 @@
         <v>1</v>
       </c>
       <c r="N233" s="3" t="n">
-        <v>46076.81894675926</v>
+        <v>46077.45417824074</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15606,7 +15609,7 @@
         <v>1</v>
       </c>
       <c r="N234" s="3" t="n">
-        <v>46076.8247337963</v>
+        <v>46077.45644675926</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -15798,7 +15801,7 @@
         <v>1</v>
       </c>
       <c r="N237" s="3" t="n">
-        <v>46076.8252662037</v>
+        <v>46077.38171296296</v>
       </c>
       <c r="O237" t="inlineStr">
         <is>
@@ -15862,7 +15865,7 @@
         <v>1</v>
       </c>
       <c r="N238" s="3" t="n">
-        <v>46076.80190972222</v>
+        <v>46077.48</v>
       </c>
       <c r="O238" t="inlineStr">
         <is>
@@ -15926,7 +15929,7 @@
         <v>1</v>
       </c>
       <c r="N239" s="3" t="n">
-        <v>46076.81688657407</v>
+        <v>46077.45568287037</v>
       </c>
       <c r="O239" t="inlineStr">
         <is>
@@ -15990,7 +15993,7 @@
         <v>1</v>
       </c>
       <c r="N240" s="3" t="n">
-        <v>46076.80755787037</v>
+        <v>46077.4799537037</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16054,7 +16057,7 @@
         <v>1</v>
       </c>
       <c r="N241" s="3" t="n">
-        <v>46076.80427083333</v>
+        <v>46077.469375</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16118,7 +16121,7 @@
         <v>1</v>
       </c>
       <c r="N242" s="3" t="n">
-        <v>46076.82931712963</v>
+        <v>46077.46100694445</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16182,7 +16185,7 @@
         <v>1</v>
       </c>
       <c r="N243" s="3" t="n">
-        <v>46076.67247685185</v>
+        <v>46077.45239583333</v>
       </c>
       <c r="O243" t="inlineStr">
         <is>
@@ -16305,7 +16308,7 @@
         <v>1</v>
       </c>
       <c r="N245" s="3" t="n">
-        <v>46076.80967592593</v>
+        <v>46077.45699074074</v>
       </c>
       <c r="O245" t="inlineStr">
         <is>
@@ -16369,7 +16372,7 @@
         <v>1</v>
       </c>
       <c r="N246" s="3" t="n">
-        <v>46076.82318287037</v>
+        <v>46077.45295138889</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16433,7 +16436,7 @@
         <v>1</v>
       </c>
       <c r="N247" s="3" t="n">
-        <v>46076.80577546296</v>
+        <v>46077.4815162037</v>
       </c>
       <c r="O247" t="inlineStr">
         <is>
@@ -16497,7 +16500,7 @@
         <v>1</v>
       </c>
       <c r="N248" s="3" t="n">
-        <v>46076.81885416667</v>
+        <v>46077.47618055555</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16620,7 +16623,7 @@
         <v>1</v>
       </c>
       <c r="N250" s="3" t="n">
-        <v>46076.79996527778</v>
+        <v>46077.45913194444</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16684,7 +16687,7 @@
         <v>1</v>
       </c>
       <c r="N251" s="3" t="n">
-        <v>46076.84975694444</v>
+        <v>46077.47961805556</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16748,7 +16751,7 @@
         <v>1</v>
       </c>
       <c r="N252" s="3" t="n">
-        <v>46076.81327546296</v>
+        <v>46077.45355324074</v>
       </c>
       <c r="O252" t="inlineStr">
         <is>
@@ -16812,7 +16815,7 @@
         <v>1</v>
       </c>
       <c r="N253" s="3" t="n">
-        <v>46076.82226851852</v>
+        <v>46077.47752314815</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16870,7 +16873,7 @@
         <v>1</v>
       </c>
       <c r="N254" s="3" t="n">
-        <v>46076.81884259259</v>
+        <v>46077.464375</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -16934,7 +16937,7 @@
         <v>1</v>
       </c>
       <c r="N255" s="3" t="n">
-        <v>46076.82233796296</v>
+        <v>46077.48370370371</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -16998,7 +17001,7 @@
         <v>1</v>
       </c>
       <c r="N256" s="3" t="n">
-        <v>46076.79159722223</v>
+        <v>46077.46950231482</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17062,7 +17065,7 @@
         <v>1</v>
       </c>
       <c r="N257" s="3" t="n">
-        <v>46076.79739583333</v>
+        <v>46077.48202546296</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17126,7 +17129,7 @@
         <v>1</v>
       </c>
       <c r="N258" s="3" t="n">
-        <v>46076.59267361111</v>
+        <v>46077.46149305555</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
@@ -17190,7 +17193,7 @@
         <v>1</v>
       </c>
       <c r="N259" s="3" t="n">
-        <v>46076.81821759259</v>
+        <v>46077.46552083334</v>
       </c>
       <c r="O259" t="inlineStr">
         <is>
@@ -17254,7 +17257,7 @@
         <v>1</v>
       </c>
       <c r="N260" s="3" t="n">
-        <v>46076.62377314815</v>
+        <v>46077.46202546296</v>
       </c>
       <c r="O260" t="inlineStr">
         <is>
@@ -17318,7 +17321,7 @@
         <v>1</v>
       </c>
       <c r="N261" s="3" t="n">
-        <v>46076.63484953704</v>
+        <v>46077.46304398148</v>
       </c>
       <c r="O261" t="inlineStr">
         <is>
@@ -17382,7 +17385,7 @@
         <v>1</v>
       </c>
       <c r="N262" s="3" t="n">
-        <v>46076.82581018518</v>
+        <v>46077.47273148148</v>
       </c>
       <c r="O262" t="inlineStr">
         <is>
@@ -17446,7 +17449,7 @@
         <v>1</v>
       </c>
       <c r="N263" s="3" t="n">
-        <v>46076.80466435185</v>
+        <v>46077.47028935186</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17510,7 +17513,7 @@
         <v>1</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>46076.8065162037</v>
+        <v>46077.48652777778</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17574,7 +17577,7 @@
         <v>1</v>
       </c>
       <c r="N265" s="3" t="n">
-        <v>46076.81990740741</v>
+        <v>46077.4733449074</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17638,7 +17641,7 @@
         <v>1</v>
       </c>
       <c r="N266" s="3" t="n">
-        <v>46076.85813657408</v>
+        <v>46077.42767361111</v>
       </c>
       <c r="O266" t="inlineStr">
         <is>
@@ -17702,7 +17705,7 @@
         <v>1</v>
       </c>
       <c r="N267" s="3" t="n">
-        <v>46076.79690972222</v>
+        <v>46077.46946759259</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17766,7 +17769,7 @@
         <v>1</v>
       </c>
       <c r="N268" s="3" t="n">
-        <v>46076.80638888889</v>
+        <v>46077.48538194445</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17830,7 +17833,7 @@
         <v>1</v>
       </c>
       <c r="N269" s="3" t="n">
-        <v>46076.81399305556</v>
+        <v>46077.48490740741</v>
       </c>
       <c r="O269" t="inlineStr">
         <is>
@@ -17891,7 +17894,7 @@
         </is>
       </c>
       <c r="N270" s="3" t="n">
-        <v>46077.28304398148</v>
+        <v>46077.48783564815</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -17955,7 +17958,7 @@
         <v>1</v>
       </c>
       <c r="N271" s="3" t="n">
-        <v>46077.05097222222</v>
+        <v>46077.32462962963</v>
       </c>
       <c r="O271" t="inlineStr">
         <is>
@@ -18019,7 +18022,7 @@
         <v>1</v>
       </c>
       <c r="N272" s="3" t="n">
-        <v>46076.66619212963</v>
+        <v>46077.48277777778</v>
       </c>
       <c r="O272" t="inlineStr">
         <is>
@@ -18083,7 +18086,7 @@
         <v>2</v>
       </c>
       <c r="N273" s="3" t="n">
-        <v>46077.28936342592</v>
+        <v>46077.4455787037</v>
       </c>
       <c r="O273" t="inlineStr">
         <is>
@@ -18467,7 +18470,7 @@
         <v>1</v>
       </c>
       <c r="N279" s="3" t="n">
-        <v>46077.30326388889</v>
+        <v>46077.46458333333</v>
       </c>
       <c r="O279" t="inlineStr">
         <is>
@@ -18531,7 +18534,7 @@
         <v>1</v>
       </c>
       <c r="N280" s="3" t="n">
-        <v>46076.65061342593</v>
+        <v>46077.45995370371</v>
       </c>
       <c r="O280" t="inlineStr">
         <is>
@@ -18595,7 +18598,7 @@
         <v>1</v>
       </c>
       <c r="N281" s="3" t="n">
-        <v>46076.86475694444</v>
+        <v>46077.46506944444</v>
       </c>
       <c r="O281" t="inlineStr">
         <is>
@@ -18654,7 +18657,7 @@
         <v>1</v>
       </c>
       <c r="N282" s="3" t="n">
-        <v>46076.82537037037</v>
+        <v>46077.48318287037</v>
       </c>
       <c r="O282" t="inlineStr">
         <is>
@@ -18718,7 +18721,7 @@
         <v>1</v>
       </c>
       <c r="N283" s="3" t="n">
-        <v>46076.82734953704</v>
+        <v>46077.46971064815</v>
       </c>
       <c r="O283" t="inlineStr">
         <is>
@@ -18782,7 +18785,7 @@
         <v>1</v>
       </c>
       <c r="N284" s="3" t="n">
-        <v>46076.86959490741</v>
+        <v>46077.45681712963</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18846,7 +18849,7 @@
         <v>1</v>
       </c>
       <c r="N285" s="3" t="n">
-        <v>46076.79333333333</v>
+        <v>46077.48165509259</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -18910,7 +18913,7 @@
         <v>1</v>
       </c>
       <c r="N286" s="3" t="n">
-        <v>46076.7542824074</v>
+        <v>46077.48575231482</v>
       </c>
       <c r="O286" t="inlineStr">
         <is>
@@ -18974,7 +18977,7 @@
         <v>1</v>
       </c>
       <c r="N287" s="3" t="n">
-        <v>46077.14640046296</v>
+        <v>46077.45976851852</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
@@ -19038,7 +19041,7 @@
         <v>1</v>
       </c>
       <c r="N288" s="3" t="n">
-        <v>46076.55165509259</v>
+        <v>46077.47457175926</v>
       </c>
       <c r="O288" t="inlineStr">
         <is>
@@ -19102,7 +19105,7 @@
         <v>1</v>
       </c>
       <c r="N289" s="3" t="n">
-        <v>46076.86166666666</v>
+        <v>46077.48542824074</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -19896,7 +19899,7 @@
         <v>1</v>
       </c>
       <c r="N302" s="3" t="n">
-        <v>46077.32010416667</v>
+        <v>46077.47645833333</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -21012,7 +21015,7 @@
         </is>
       </c>
       <c r="N320" s="3" t="n">
-        <v>46077.2959837963</v>
+        <v>46077.48371527778</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21737,7 +21740,7 @@
         <v>1</v>
       </c>
       <c r="N332" s="3" t="n">
-        <v>46077.28819444445</v>
+        <v>46077.48019675926</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21801,7 +21804,7 @@
         <v>2</v>
       </c>
       <c r="N333" s="3" t="n">
-        <v>46077.28802083333</v>
+        <v>46077.45041666667</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21865,7 +21868,7 @@
         <v>2</v>
       </c>
       <c r="N334" s="3" t="n">
-        <v>46077.28866898148</v>
+        <v>46077.48778935185</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21929,7 +21932,7 @@
         <v>2</v>
       </c>
       <c r="N335" s="3" t="n">
-        <v>46077.28825231481</v>
+        <v>46077.48</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -21993,7 +21996,7 @@
         <v>1</v>
       </c>
       <c r="N336" s="3" t="n">
-        <v>46077.29880787037</v>
+        <v>46077.45061342593</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22057,7 +22060,7 @@
         <v>1</v>
       </c>
       <c r="N337" s="3" t="n">
-        <v>46077.28917824074</v>
+        <v>46077.47903935185</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22121,7 +22124,7 @@
         <v>2</v>
       </c>
       <c r="N338" s="3" t="n">
-        <v>46077.28865740741</v>
+        <v>46077.47848379629</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -22313,7 +22316,7 @@
         <v>2</v>
       </c>
       <c r="N341" s="3" t="n">
-        <v>46076.5753125</v>
+        <v>46077.45375</v>
       </c>
       <c r="O341" t="inlineStr">
         <is>
@@ -22377,7 +22380,7 @@
         <v>2</v>
       </c>
       <c r="N342" s="3" t="n">
-        <v>46077.2931712963</v>
+        <v>46077.48434027778</v>
       </c>
       <c r="O342" t="inlineStr">
         <is>
@@ -22396,6 +22399,11 @@
           <t>OPERACAO 9.1</t>
         </is>
       </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>10.69.5.237</t>
+        </is>
+      </c>
       <c r="D343" t="n">
         <v>2017</v>
       </c>
@@ -22438,7 +22446,7 @@
         </is>
       </c>
       <c r="N343" s="3" t="n">
-        <v>46076.7228125</v>
+        <v>46077.4878125</v>
       </c>
       <c r="O343" t="inlineStr">
         <is>
@@ -22694,7 +22702,7 @@
         <v>1</v>
       </c>
       <c r="N347" s="3" t="n">
-        <v>46076.5949537037</v>
+        <v>46077.42240740741</v>
       </c>
       <c r="O347" t="inlineStr">
         <is>
@@ -22758,7 +22766,7 @@
         <v>2</v>
       </c>
       <c r="N348" s="3" t="n">
-        <v>46076.56197916667</v>
+        <v>46077.46237268519</v>
       </c>
       <c r="O348" t="inlineStr">
         <is>
@@ -22822,7 +22830,7 @@
         <v>1</v>
       </c>
       <c r="N349" s="3" t="n">
-        <v>46076.5919212963</v>
+        <v>46077.46165509259</v>
       </c>
       <c r="O349" t="inlineStr">
         <is>
@@ -22881,7 +22889,7 @@
         <v>1</v>
       </c>
       <c r="N350" s="3" t="n">
-        <v>46076.58641203704</v>
+        <v>46077.45594907407</v>
       </c>
       <c r="O350" t="inlineStr">
         <is>
@@ -22945,7 +22953,7 @@
         <v>1</v>
       </c>
       <c r="N351" s="3" t="n">
-        <v>46076.56006944444</v>
+        <v>46077.46319444444</v>
       </c>
       <c r="O351" t="inlineStr">
         <is>
@@ -23009,7 +23017,7 @@
         <v>1</v>
       </c>
       <c r="N352" s="3" t="n">
-        <v>46073.57822916667</v>
+        <v>46077.46219907407</v>
       </c>
       <c r="O352" t="inlineStr">
         <is>
@@ -23070,7 +23078,7 @@
         </is>
       </c>
       <c r="N353" s="3" t="n">
-        <v>46076.59017361111</v>
+        <v>46077.46164351852</v>
       </c>
       <c r="O353" t="inlineStr">
         <is>
@@ -23131,7 +23139,7 @@
         </is>
       </c>
       <c r="N354" s="3" t="n">
-        <v>46076.59353009259</v>
+        <v>46077.4649537037</v>
       </c>
       <c r="O354" t="inlineStr">
         <is>
@@ -23195,7 +23203,7 @@
         <v>1</v>
       </c>
       <c r="N355" s="3" t="n">
-        <v>46076.59435185185</v>
+        <v>46077.45903935185</v>
       </c>
       <c r="O355" t="inlineStr">
         <is>
@@ -23259,7 +23267,7 @@
         <v>1</v>
       </c>
       <c r="N356" s="3" t="n">
-        <v>46076.5891550926</v>
+        <v>46077.45796296297</v>
       </c>
       <c r="O356" t="inlineStr">
         <is>
@@ -23323,7 +23331,7 @@
         <v>1</v>
       </c>
       <c r="N357" s="3" t="n">
-        <v>46076.59214120371</v>
+        <v>46077.45964120371</v>
       </c>
       <c r="O357" t="inlineStr">
         <is>
@@ -23446,7 +23454,7 @@
         <v>2</v>
       </c>
       <c r="N359" s="3" t="n">
-        <v>46076.58893518519</v>
+        <v>46077.46216435185</v>
       </c>
       <c r="O359" t="inlineStr">
         <is>
@@ -23510,7 +23518,7 @@
         <v>2</v>
       </c>
       <c r="N360" s="3" t="n">
-        <v>46076.56289351852</v>
+        <v>46077.46430555556</v>
       </c>
       <c r="O360" t="inlineStr">
         <is>
@@ -23574,7 +23582,7 @@
         <v>1</v>
       </c>
       <c r="N361" s="3" t="n">
-        <v>46076.58438657408</v>
+        <v>46077.42533564815</v>
       </c>
       <c r="O361" t="inlineStr">
         <is>
@@ -23635,7 +23643,7 @@
         </is>
       </c>
       <c r="N362" s="3" t="n">
-        <v>46076.56197916667</v>
+        <v>46077.46253472222</v>
       </c>
       <c r="O362" t="inlineStr">
         <is>
@@ -23823,7 +23831,7 @@
         <v>1</v>
       </c>
       <c r="N365" s="3" t="n">
-        <v>46076.6846875</v>
+        <v>46077.45577546296</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
@@ -23889,7 +23897,7 @@
         </is>
       </c>
       <c r="N366" s="3" t="n">
-        <v>46077.30633101852</v>
+        <v>46077.46357638889</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -24015,7 +24023,7 @@
         </is>
       </c>
       <c r="N368" s="3" t="n">
-        <v>46076.71673611111</v>
+        <v>46077.45134259259</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -24081,7 +24089,7 @@
         </is>
       </c>
       <c r="N369" s="3" t="n">
-        <v>46076.72153935185</v>
+        <v>46077.45008101852</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
@@ -24150,7 +24158,7 @@
         <v>1</v>
       </c>
       <c r="N370" s="3" t="n">
-        <v>46076.75436342593</v>
+        <v>46077.45167824074</v>
       </c>
       <c r="O370" t="inlineStr">
         <is>
@@ -24219,7 +24227,7 @@
         <v>1</v>
       </c>
       <c r="N371" s="3" t="n">
-        <v>46076.68086805556</v>
+        <v>46077.45690972222</v>
       </c>
       <c r="O371" t="inlineStr">
         <is>
@@ -24353,9 +24361,6 @@
           <t>HP ProDesk 400 G5 SFF (Brazil)</t>
         </is>
       </c>
-      <c r="M373" t="n">
-        <v>1</v>
-      </c>
       <c r="N373" s="3" t="n">
         <v>46073.62837962963</v>
       </c>
@@ -24426,7 +24431,7 @@
         <v>1</v>
       </c>
       <c r="N374" s="3" t="n">
-        <v>46076.75230324074</v>
+        <v>46077.47453703704</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24492,7 +24497,7 @@
         </is>
       </c>
       <c r="N375" s="3" t="n">
-        <v>46077.30444444445</v>
+        <v>46077.46145833333</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
@@ -24511,11 +24516,6 @@
           <t>COORDENACAO</t>
         </is>
       </c>
-      <c r="C376" t="inlineStr">
-        <is>
-          <t>10.69.3.72</t>
-        </is>
-      </c>
       <c r="D376" t="n">
         <v>2025</v>
       </c>
@@ -24561,7 +24561,7 @@
         <v>1</v>
       </c>
       <c r="N376" s="3" t="n">
-        <v>46077.30716435185</v>
+        <v>46077.46789351852</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -24630,7 +24630,7 @@
         <v>2</v>
       </c>
       <c r="N377" s="3" t="n">
-        <v>46076.66385416667</v>
+        <v>46077.47815972222</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -24699,7 +24699,7 @@
         <v>2</v>
       </c>
       <c r="N378" s="3" t="n">
-        <v>46077.29969907407</v>
+        <v>46077.45571759259</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização automática 2026-02-24 13:52:08.119830
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>46077.48548611111</v>
+        <v>46077.56351851852</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>46077.47445601852</v>
+        <v>46077.5475</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
         <v>1</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>46077.48221064815</v>
+        <v>46077.55841435185</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>46077.45922453704</v>
+        <v>46077.55815972222</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -1131,7 +1131,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="3" t="n">
-        <v>46077.46771990741</v>
+        <v>46077.54675925926</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1515,7 +1515,7 @@
         <v>2</v>
       </c>
       <c r="N16" s="3" t="n">
-        <v>46077.45256944445</v>
+        <v>46077.56957175926</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -2244,7 +2244,7 @@
         </is>
       </c>
       <c r="N28" s="3" t="n">
-        <v>46077.45503472222</v>
+        <v>46077.56653935185</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -6570,7 +6570,7 @@
         <v>1</v>
       </c>
       <c r="N95" s="3" t="n">
-        <v>46077.47164351852</v>
+        <v>46077.54877314815</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -6708,7 +6708,7 @@
         <v>1</v>
       </c>
       <c r="N97" s="3" t="n">
-        <v>46077.48524305555</v>
+        <v>46077.56730324074</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -6772,7 +6772,7 @@
         <v>1</v>
       </c>
       <c r="N98" s="3" t="n">
-        <v>46077.47292824074</v>
+        <v>46077.55307870371</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -6841,7 +6841,7 @@
         <v>1</v>
       </c>
       <c r="N99" s="3" t="n">
-        <v>46077.44916666667</v>
+        <v>46077.57002314815</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -6910,7 +6910,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>46077.4725462963</v>
+        <v>46077.54787037037</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6979,7 +6979,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="3" t="n">
-        <v>46076.83690972222</v>
+        <v>46077.56800925926</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -7117,7 +7117,7 @@
         <v>2</v>
       </c>
       <c r="N103" s="3" t="n">
-        <v>46077.47799768519</v>
+        <v>46077.55673611111</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7247,7 +7247,7 @@
         <v>1</v>
       </c>
       <c r="N105" s="3" t="n">
-        <v>46077.46759259259</v>
+        <v>46077.50876157408</v>
       </c>
       <c r="O105" t="inlineStr">
         <is>
@@ -7377,7 +7377,7 @@
         <v>1</v>
       </c>
       <c r="N107" s="3" t="n">
-        <v>46077.46899305555</v>
+        <v>46077.5471875</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -7515,7 +7515,7 @@
         <v>1</v>
       </c>
       <c r="N109" s="3" t="n">
-        <v>46077.47298611111</v>
+        <v>46077.55246527777</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7584,7 +7584,7 @@
         <v>2</v>
       </c>
       <c r="N110" s="3" t="n">
-        <v>46077.48182870371</v>
+        <v>46077.56128472222</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7653,7 +7653,7 @@
         <v>2</v>
       </c>
       <c r="N111" s="3" t="n">
-        <v>46077.46240740741</v>
+        <v>46077.53460648148</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
@@ -7722,7 +7722,7 @@
         <v>2</v>
       </c>
       <c r="N112" s="3" t="n">
-        <v>46077.45207175926</v>
+        <v>46077.53197916667</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7791,7 +7791,7 @@
         <v>1</v>
       </c>
       <c r="N113" s="3" t="n">
-        <v>46077.48482638889</v>
+        <v>46077.53549768519</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7860,7 +7860,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>46077.48614583333</v>
+        <v>46077.56331018519</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -7926,7 +7926,7 @@
         </is>
       </c>
       <c r="N115" s="3" t="n">
-        <v>46077.46586805556</v>
+        <v>46077.54061342592</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -8014,6 +8014,11 @@
           <t>DP</t>
         </is>
       </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>10.69.3.23</t>
+        </is>
+      </c>
       <c r="D117" t="n">
         <v>2025</v>
       </c>
@@ -8059,7 +8064,7 @@
         <v>1</v>
       </c>
       <c r="N117" s="3" t="n">
-        <v>46077.44150462963</v>
+        <v>46077.53767361111</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -8125,7 +8130,7 @@
         </is>
       </c>
       <c r="N118" s="3" t="n">
-        <v>46077.45927083334</v>
+        <v>46077.53958333333</v>
       </c>
       <c r="O118" t="inlineStr">
         <is>
@@ -8263,7 +8268,7 @@
         <v>1</v>
       </c>
       <c r="N120" s="3" t="n">
-        <v>46077.47049768519</v>
+        <v>46077.50957175926</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -8332,7 +8337,7 @@
         <v>1</v>
       </c>
       <c r="N121" s="3" t="n">
-        <v>46077.428125</v>
+        <v>46077.54362268518</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -8398,7 +8403,7 @@
         </is>
       </c>
       <c r="N122" s="3" t="n">
-        <v>46077.48168981481</v>
+        <v>46077.55645833333</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -8467,7 +8472,7 @@
         <v>2</v>
       </c>
       <c r="N123" s="3" t="n">
-        <v>46077.47847222222</v>
+        <v>46077.55721064815</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -8536,7 +8541,7 @@
         <v>1</v>
       </c>
       <c r="N124" s="3" t="n">
-        <v>46077.47162037037</v>
+        <v>46077.5512037037</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -8605,7 +8610,7 @@
         <v>1</v>
       </c>
       <c r="N125" s="3" t="n">
-        <v>46077.48234953704</v>
+        <v>46077.56125</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -8674,7 +8679,7 @@
         <v>2</v>
       </c>
       <c r="N126" s="3" t="n">
-        <v>46077.4712037037</v>
+        <v>46077.54775462963</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -8743,7 +8748,7 @@
         <v>2</v>
       </c>
       <c r="N127" s="3" t="n">
-        <v>46077.48553240741</v>
+        <v>46077.56260416667</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -8812,7 +8817,7 @@
         <v>1</v>
       </c>
       <c r="N128" s="3" t="n">
-        <v>46077.45171296296</v>
+        <v>46077.53344907407</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -8881,7 +8886,7 @@
         <v>1</v>
       </c>
       <c r="N129" s="3" t="n">
-        <v>46076.66789351852</v>
+        <v>46077.56211805555</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -8950,7 +8955,7 @@
         <v>1</v>
       </c>
       <c r="N130" s="3" t="n">
-        <v>46077.47740740741</v>
+        <v>46077.55396990741</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -9014,7 +9019,7 @@
         <v>1</v>
       </c>
       <c r="N131" s="3" t="n">
-        <v>46077.4804050926</v>
+        <v>46077.55961805556</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -9147,7 +9152,7 @@
         <v>1</v>
       </c>
       <c r="N133" s="3" t="n">
-        <v>46077.48652777778</v>
+        <v>46077.55888888889</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -9466,7 +9471,7 @@
         <v>1</v>
       </c>
       <c r="N138" s="3" t="n">
-        <v>46077.45543981482</v>
+        <v>46077.57040509259</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9530,7 +9535,7 @@
         <v>1</v>
       </c>
       <c r="N139" s="3" t="n">
-        <v>46077.45866898148</v>
+        <v>46077.53554398148</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9594,7 +9599,7 @@
         <v>1</v>
       </c>
       <c r="N140" s="3" t="n">
-        <v>46077.46556712963</v>
+        <v>46077.54305555556</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9658,7 +9663,7 @@
         <v>1</v>
       </c>
       <c r="N141" s="3" t="n">
-        <v>46077.45891203704</v>
+        <v>46077.53578703704</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9722,7 +9727,7 @@
         <v>1</v>
       </c>
       <c r="N142" s="3" t="n">
-        <v>46077.45677083333</v>
+        <v>46077.56768518518</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9786,7 +9791,7 @@
         <v>1</v>
       </c>
       <c r="N143" s="3" t="n">
-        <v>46077.48805555556</v>
+        <v>46077.56513888889</v>
       </c>
       <c r="O143" t="inlineStr">
         <is>
@@ -9850,7 +9855,7 @@
         <v>1</v>
       </c>
       <c r="N144" s="3" t="n">
-        <v>46077.45958333334</v>
+        <v>46077.53966435185</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9978,7 +9983,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="3" t="n">
-        <v>46077.47035879629</v>
+        <v>46077.55136574074</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10042,7 +10047,7 @@
         <v>1</v>
       </c>
       <c r="N147" s="3" t="n">
-        <v>46077.47700231482</v>
+        <v>46077.54993055556</v>
       </c>
       <c r="O147" t="inlineStr">
         <is>
@@ -10106,7 +10111,7 @@
         <v>1</v>
       </c>
       <c r="N148" s="3" t="n">
-        <v>46077.46990740741</v>
+        <v>46077.54958333333</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10170,7 +10175,7 @@
         <v>1</v>
       </c>
       <c r="N149" s="3" t="n">
-        <v>46077.46895833333</v>
+        <v>46077.54809027778</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -10234,7 +10239,7 @@
         <v>1</v>
       </c>
       <c r="N150" s="3" t="n">
-        <v>46077.48763888889</v>
+        <v>46077.56645833333</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -10426,7 +10431,7 @@
         <v>1</v>
       </c>
       <c r="N153" s="3" t="n">
-        <v>46077.48196759259</v>
+        <v>46077.55393518518</v>
       </c>
       <c r="O153" t="inlineStr">
         <is>
@@ -10490,7 +10495,7 @@
         <v>1</v>
       </c>
       <c r="N154" s="3" t="n">
-        <v>46077.47834490741</v>
+        <v>46077.55486111111</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10554,7 +10559,7 @@
         <v>1</v>
       </c>
       <c r="N155" s="3" t="n">
-        <v>46077.48752314815</v>
+        <v>46077.56861111111</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10682,7 +10687,7 @@
         <v>1</v>
       </c>
       <c r="N157" s="3" t="n">
-        <v>46077.453125</v>
+        <v>46077.53488425926</v>
       </c>
       <c r="O157" t="inlineStr">
         <is>
@@ -10746,7 +10751,7 @@
         <v>1</v>
       </c>
       <c r="N158" s="3" t="n">
-        <v>46077.46967592592</v>
+        <v>46077.54832175926</v>
       </c>
       <c r="O158" t="inlineStr">
         <is>
@@ -10810,7 +10815,7 @@
         <v>1</v>
       </c>
       <c r="N159" s="3" t="n">
-        <v>46077.47540509259</v>
+        <v>46077.55333333334</v>
       </c>
       <c r="O159" t="inlineStr">
         <is>
@@ -10874,7 +10879,7 @@
         <v>1</v>
       </c>
       <c r="N160" s="3" t="n">
-        <v>46077.45787037037</v>
+        <v>46077.53736111111</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
@@ -10938,7 +10943,7 @@
         <v>1</v>
       </c>
       <c r="N161" s="3" t="n">
-        <v>46077.4540162037</v>
+        <v>46077.56988425926</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -11002,7 +11007,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="3" t="n">
-        <v>46077.45111111111</v>
+        <v>46077.56512731482</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11130,7 +11135,7 @@
         <v>2</v>
       </c>
       <c r="N164" s="3" t="n">
-        <v>46077.47741898148</v>
+        <v>46077.55450231482</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11194,7 +11199,7 @@
         <v>2</v>
       </c>
       <c r="N165" s="3" t="n">
-        <v>46077.48633101852</v>
+        <v>46077.52436342592</v>
       </c>
       <c r="O165" t="inlineStr">
         <is>
@@ -11258,7 +11263,7 @@
         <v>2</v>
       </c>
       <c r="N166" s="3" t="n">
-        <v>46076.61715277778</v>
+        <v>46077.54755787037</v>
       </c>
       <c r="O166" t="inlineStr">
         <is>
@@ -11322,7 +11327,7 @@
         <v>2</v>
       </c>
       <c r="N167" s="3" t="n">
-        <v>46077.45063657407</v>
+        <v>46077.56684027778</v>
       </c>
       <c r="O167" t="inlineStr">
         <is>
@@ -11386,7 +11391,7 @@
         <v>2</v>
       </c>
       <c r="N168" s="3" t="n">
-        <v>46077.48010416667</v>
+        <v>46077.55825231481</v>
       </c>
       <c r="O168" t="inlineStr">
         <is>
@@ -11450,7 +11455,7 @@
         <v>2</v>
       </c>
       <c r="N169" s="3" t="n">
-        <v>46077.4815162037</v>
+        <v>46077.55640046296</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -11514,7 +11519,7 @@
         <v>2</v>
       </c>
       <c r="N170" s="3" t="n">
-        <v>46077.47752314815</v>
+        <v>46077.55481481482</v>
       </c>
       <c r="O170" t="inlineStr">
         <is>
@@ -11578,7 +11583,7 @@
         <v>1</v>
       </c>
       <c r="N171" s="3" t="n">
-        <v>46077.48350694445</v>
+        <v>46077.55986111111</v>
       </c>
       <c r="O171" t="inlineStr">
         <is>
@@ -11642,7 +11647,7 @@
         <v>2</v>
       </c>
       <c r="N172" s="3" t="n">
-        <v>46077.48439814815</v>
+        <v>46077.55981481481</v>
       </c>
       <c r="O172" t="inlineStr">
         <is>
@@ -11706,7 +11711,7 @@
         <v>2</v>
       </c>
       <c r="N173" s="3" t="n">
-        <v>46077.48715277778</v>
+        <v>46077.56539351852</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -11770,7 +11775,7 @@
         <v>2</v>
       </c>
       <c r="N174" s="3" t="n">
-        <v>46077.46326388889</v>
+        <v>46077.53944444445</v>
       </c>
       <c r="O174" t="inlineStr">
         <is>
@@ -11834,7 +11839,7 @@
         <v>2</v>
       </c>
       <c r="N175" s="3" t="n">
-        <v>46077.45664351852</v>
+        <v>46077.53288194445</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -11898,7 +11903,7 @@
         <v>2</v>
       </c>
       <c r="N176" s="3" t="n">
-        <v>46077.48125</v>
+        <v>46077.56060185185</v>
       </c>
       <c r="O176" t="inlineStr">
         <is>
@@ -11962,7 +11967,7 @@
         <v>3</v>
       </c>
       <c r="N177" s="3" t="n">
-        <v>46077.45925925926</v>
+        <v>46077.53530092593</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
@@ -12026,7 +12031,7 @@
         <v>2</v>
       </c>
       <c r="N178" s="3" t="n">
-        <v>46077.47494212963</v>
+        <v>46077.55174768518</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12090,7 +12095,7 @@
         <v>1</v>
       </c>
       <c r="N179" s="3" t="n">
-        <v>46077.47481481481</v>
+        <v>46077.55535879629</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12154,7 +12159,7 @@
         <v>1</v>
       </c>
       <c r="N180" s="3" t="n">
-        <v>46077.46071759259</v>
+        <v>46077.53465277778</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12543,7 +12548,7 @@
         <v>1</v>
       </c>
       <c r="N186" s="3" t="n">
-        <v>46077.48688657407</v>
+        <v>46077.49327546296</v>
       </c>
       <c r="O186" t="inlineStr">
         <is>
@@ -12607,7 +12612,7 @@
         <v>1</v>
       </c>
       <c r="N187" s="3" t="n">
-        <v>46077.48553240741</v>
+        <v>46077.56523148148</v>
       </c>
       <c r="O187" t="inlineStr">
         <is>
@@ -12671,7 +12676,7 @@
         <v>1</v>
       </c>
       <c r="N188" s="3" t="n">
-        <v>46077.47578703704</v>
+        <v>46077.55432870371</v>
       </c>
       <c r="O188" t="inlineStr">
         <is>
@@ -12757,11 +12762,6 @@
           <t>OPERACAO 8.1</t>
         </is>
       </c>
-      <c r="C190" t="inlineStr">
-        <is>
-          <t>10.69.5.59</t>
-        </is>
-      </c>
       <c r="D190" t="n">
         <v>2015</v>
       </c>
@@ -12799,7 +12799,7 @@
         </is>
       </c>
       <c r="N190" s="3" t="n">
-        <v>46077.47396990741</v>
+        <v>46077.55202546297</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12927,7 +12927,7 @@
         <v>1</v>
       </c>
       <c r="N192" s="3" t="n">
-        <v>46077.48172453704</v>
+        <v>46077.5352662037</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -13052,7 +13052,7 @@
         <v>2</v>
       </c>
       <c r="N194" s="3" t="n">
-        <v>46077.48881944444</v>
+        <v>46077.5588425926</v>
       </c>
       <c r="O194" t="inlineStr">
         <is>
@@ -13116,7 +13116,7 @@
         <v>1</v>
       </c>
       <c r="N195" s="3" t="n">
-        <v>46077.47493055555</v>
+        <v>46077.55621527778</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13180,7 +13180,7 @@
         <v>1</v>
       </c>
       <c r="N196" s="3" t="n">
-        <v>46077.45775462963</v>
+        <v>46077.53734953704</v>
       </c>
       <c r="O196" t="inlineStr">
         <is>
@@ -13308,7 +13308,7 @@
         <v>1</v>
       </c>
       <c r="N198" s="3" t="n">
-        <v>46077.483125</v>
+        <v>46077.54363425926</v>
       </c>
       <c r="O198" t="inlineStr">
         <is>
@@ -13497,7 +13497,7 @@
         </is>
       </c>
       <c r="N201" s="3" t="n">
-        <v>46077.46614583334</v>
+        <v>46077.54233796296</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -13561,7 +13561,7 @@
         <v>1</v>
       </c>
       <c r="N202" s="3" t="n">
-        <v>46077.46539351852</v>
+        <v>46077.53814814815</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13625,7 +13625,7 @@
         <v>1</v>
       </c>
       <c r="N203" s="3" t="n">
-        <v>46077.45571759259</v>
+        <v>46077.54222222222</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13689,7 +13689,7 @@
         <v>1</v>
       </c>
       <c r="N204" s="3" t="n">
-        <v>46077.46771990741</v>
+        <v>46077.54666666667</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13753,7 +13753,7 @@
         <v>1</v>
       </c>
       <c r="N205" s="3" t="n">
-        <v>46077.47450231481</v>
+        <v>46077.5588425926</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13817,7 +13817,7 @@
         <v>1</v>
       </c>
       <c r="N206" s="3" t="n">
-        <v>46077.4650925926</v>
+        <v>46077.54481481481</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -13881,7 +13881,7 @@
         <v>1</v>
       </c>
       <c r="N207" s="3" t="n">
-        <v>46077.46385416666</v>
+        <v>46077.54293981481</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -13945,7 +13945,7 @@
         <v>1</v>
       </c>
       <c r="N208" s="3" t="n">
-        <v>46077.47751157408</v>
+        <v>46077.54354166667</v>
       </c>
       <c r="O208" t="inlineStr">
         <is>
@@ -14009,7 +14009,7 @@
         <v>1</v>
       </c>
       <c r="N209" s="3" t="n">
-        <v>46077.46837962963</v>
+        <v>46077.54579861111</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14073,7 +14073,7 @@
         <v>1</v>
       </c>
       <c r="N210" s="3" t="n">
-        <v>46077.48851851852</v>
+        <v>46077.56480324074</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14137,7 +14137,7 @@
         <v>1</v>
       </c>
       <c r="N211" s="3" t="n">
-        <v>46077.46057870371</v>
+        <v>46077.53870370371</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -14201,7 +14201,7 @@
         <v>1</v>
       </c>
       <c r="N212" s="3" t="n">
-        <v>46077.46108796296</v>
+        <v>46077.53855324074</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -14265,7 +14265,7 @@
         <v>1</v>
       </c>
       <c r="N213" s="3" t="n">
-        <v>46077.46685185185</v>
+        <v>46077.54153935185</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
@@ -14329,7 +14329,7 @@
         <v>1</v>
       </c>
       <c r="N214" s="3" t="n">
-        <v>46077.4608912037</v>
+        <v>46077.53651620371</v>
       </c>
       <c r="O214" t="inlineStr">
         <is>
@@ -14393,7 +14393,7 @@
         <v>1</v>
       </c>
       <c r="N215" s="3" t="n">
-        <v>46077.4581712963</v>
+        <v>46077.53293981482</v>
       </c>
       <c r="O215" t="inlineStr">
         <is>
@@ -14457,7 +14457,7 @@
         <v>1</v>
       </c>
       <c r="N216" s="3" t="n">
-        <v>46077.45829861111</v>
+        <v>46077.5424537037</v>
       </c>
       <c r="O216" t="inlineStr">
         <is>
@@ -14516,7 +14516,7 @@
         <v>1</v>
       </c>
       <c r="N217" s="3" t="n">
-        <v>46077.4572800926</v>
+        <v>46077.53680555556</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14580,7 +14580,7 @@
         <v>1</v>
       </c>
       <c r="N218" s="3" t="n">
-        <v>46077.45650462963</v>
+        <v>46077.5678587963</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14644,7 +14644,7 @@
         <v>1</v>
       </c>
       <c r="N219" s="3" t="n">
-        <v>46077.45829861111</v>
+        <v>46077.56828703704</v>
       </c>
       <c r="O219" t="inlineStr">
         <is>
@@ -14713,7 +14713,7 @@
         <v>1</v>
       </c>
       <c r="N220" s="3" t="n">
-        <v>46077.45881944444</v>
+        <v>46077.53729166667</v>
       </c>
       <c r="O220" t="inlineStr">
         <is>
@@ -14777,7 +14777,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="3" t="n">
-        <v>46077.45365740741</v>
+        <v>46077.56923611111</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14841,7 +14841,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="3" t="n">
-        <v>46077.45115740741</v>
+        <v>46077.55696759259</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -14905,7 +14905,7 @@
         <v>1</v>
       </c>
       <c r="N223" s="3" t="n">
-        <v>46077.47369212963</v>
+        <v>46077.55006944444</v>
       </c>
       <c r="O223" t="inlineStr">
         <is>
@@ -15033,7 +15033,7 @@
         <v>1</v>
       </c>
       <c r="N225" s="3" t="n">
-        <v>46077.45584490741</v>
+        <v>46077.57085648148</v>
       </c>
       <c r="O225" t="inlineStr">
         <is>
@@ -15097,7 +15097,7 @@
         <v>1</v>
       </c>
       <c r="N226" s="3" t="n">
-        <v>46077.46091435185</v>
+        <v>46077.53865740741</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15161,7 +15161,7 @@
         <v>1</v>
       </c>
       <c r="N227" s="3" t="n">
-        <v>46077.46981481482</v>
+        <v>46077.55577546296</v>
       </c>
       <c r="O227" t="inlineStr">
         <is>
@@ -15225,7 +15225,7 @@
         <v>1</v>
       </c>
       <c r="N228" s="3" t="n">
-        <v>46077.47884259259</v>
+        <v>46077.55684027778</v>
       </c>
       <c r="O228" t="inlineStr">
         <is>
@@ -15353,7 +15353,7 @@
         <v>1</v>
       </c>
       <c r="N230" s="3" t="n">
-        <v>46077.45504629629</v>
+        <v>46077.55793981482</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15417,7 +15417,7 @@
         <v>1</v>
       </c>
       <c r="N231" s="3" t="n">
-        <v>46077.47356481481</v>
+        <v>46077.53283564815</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15481,7 +15481,7 @@
         <v>1</v>
       </c>
       <c r="N232" s="3" t="n">
-        <v>46077.48247685185</v>
+        <v>46077.55876157407</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -15545,7 +15545,7 @@
         <v>1</v>
       </c>
       <c r="N233" s="3" t="n">
-        <v>46077.45417824074</v>
+        <v>46077.5359837963</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15609,7 +15609,7 @@
         <v>1</v>
       </c>
       <c r="N234" s="3" t="n">
-        <v>46077.45644675926</v>
+        <v>46077.53502314815</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -15865,7 +15865,7 @@
         <v>1</v>
       </c>
       <c r="N238" s="3" t="n">
-        <v>46077.48</v>
+        <v>46077.56928240741</v>
       </c>
       <c r="O238" t="inlineStr">
         <is>
@@ -15929,7 +15929,7 @@
         <v>1</v>
       </c>
       <c r="N239" s="3" t="n">
-        <v>46077.45568287037</v>
+        <v>46077.56777777777</v>
       </c>
       <c r="O239" t="inlineStr">
         <is>
@@ -15993,7 +15993,7 @@
         <v>1</v>
       </c>
       <c r="N240" s="3" t="n">
-        <v>46077.4799537037</v>
+        <v>46077.54050925926</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16057,7 +16057,7 @@
         <v>1</v>
       </c>
       <c r="N241" s="3" t="n">
-        <v>46077.469375</v>
+        <v>46077.55635416666</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16121,7 +16121,7 @@
         <v>1</v>
       </c>
       <c r="N242" s="3" t="n">
-        <v>46077.46100694445</v>
+        <v>46077.54076388889</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16185,7 +16185,7 @@
         <v>1</v>
       </c>
       <c r="N243" s="3" t="n">
-        <v>46077.45239583333</v>
+        <v>46077.5712037037</v>
       </c>
       <c r="O243" t="inlineStr">
         <is>
@@ -16308,7 +16308,7 @@
         <v>1</v>
       </c>
       <c r="N245" s="3" t="n">
-        <v>46077.45699074074</v>
+        <v>46077.56820601852</v>
       </c>
       <c r="O245" t="inlineStr">
         <is>
@@ -16372,7 +16372,7 @@
         <v>1</v>
       </c>
       <c r="N246" s="3" t="n">
-        <v>46077.45295138889</v>
+        <v>46077.53314814815</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16436,7 +16436,7 @@
         <v>1</v>
       </c>
       <c r="N247" s="3" t="n">
-        <v>46077.4815162037</v>
+        <v>46077.5581712963</v>
       </c>
       <c r="O247" t="inlineStr">
         <is>
@@ -16500,7 +16500,7 @@
         <v>1</v>
       </c>
       <c r="N248" s="3" t="n">
-        <v>46077.47618055555</v>
+        <v>46077.55504629629</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16623,7 +16623,7 @@
         <v>1</v>
       </c>
       <c r="N250" s="3" t="n">
-        <v>46077.45913194444</v>
+        <v>46077.53300925926</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16687,7 +16687,7 @@
         <v>1</v>
       </c>
       <c r="N251" s="3" t="n">
-        <v>46077.47961805556</v>
+        <v>46077.55798611111</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16751,7 +16751,7 @@
         <v>1</v>
       </c>
       <c r="N252" s="3" t="n">
-        <v>46077.45355324074</v>
+        <v>46077.53541666667</v>
       </c>
       <c r="O252" t="inlineStr">
         <is>
@@ -16815,7 +16815,7 @@
         <v>1</v>
       </c>
       <c r="N253" s="3" t="n">
-        <v>46077.47752314815</v>
+        <v>46077.56190972222</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16873,7 +16873,7 @@
         <v>1</v>
       </c>
       <c r="N254" s="3" t="n">
-        <v>46077.464375</v>
+        <v>46077.54517361111</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -16937,7 +16937,7 @@
         <v>1</v>
       </c>
       <c r="N255" s="3" t="n">
-        <v>46077.48370370371</v>
+        <v>46077.56078703704</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -17001,7 +17001,7 @@
         <v>1</v>
       </c>
       <c r="N256" s="3" t="n">
-        <v>46077.46950231482</v>
+        <v>46077.5459375</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17065,7 +17065,7 @@
         <v>1</v>
       </c>
       <c r="N257" s="3" t="n">
-        <v>46077.48202546296</v>
+        <v>46077.55832175926</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17129,7 +17129,7 @@
         <v>1</v>
       </c>
       <c r="N258" s="3" t="n">
-        <v>46077.46149305555</v>
+        <v>46077.54563657408</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
@@ -17193,7 +17193,7 @@
         <v>1</v>
       </c>
       <c r="N259" s="3" t="n">
-        <v>46077.46552083334</v>
+        <v>46077.5437962963</v>
       </c>
       <c r="O259" t="inlineStr">
         <is>
@@ -17257,7 +17257,7 @@
         <v>1</v>
       </c>
       <c r="N260" s="3" t="n">
-        <v>46077.46202546296</v>
+        <v>46077.54381944444</v>
       </c>
       <c r="O260" t="inlineStr">
         <is>
@@ -17321,7 +17321,7 @@
         <v>1</v>
       </c>
       <c r="N261" s="3" t="n">
-        <v>46077.46304398148</v>
+        <v>46077.54190972223</v>
       </c>
       <c r="O261" t="inlineStr">
         <is>
@@ -17385,7 +17385,7 @@
         <v>1</v>
       </c>
       <c r="N262" s="3" t="n">
-        <v>46077.47273148148</v>
+        <v>46077.5505787037</v>
       </c>
       <c r="O262" t="inlineStr">
         <is>
@@ -17449,7 +17449,7 @@
         <v>1</v>
       </c>
       <c r="N263" s="3" t="n">
-        <v>46077.47028935186</v>
+        <v>46077.56516203703</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17513,7 +17513,7 @@
         <v>1</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>46077.48652777778</v>
+        <v>46077.56608796296</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17577,7 +17577,7 @@
         <v>1</v>
       </c>
       <c r="N265" s="3" t="n">
-        <v>46077.4733449074</v>
+        <v>46077.54358796297</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17705,7 +17705,7 @@
         <v>1</v>
       </c>
       <c r="N267" s="3" t="n">
-        <v>46077.46946759259</v>
+        <v>46077.54399305556</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17769,7 +17769,7 @@
         <v>1</v>
       </c>
       <c r="N268" s="3" t="n">
-        <v>46077.48538194445</v>
+        <v>46077.56178240741</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17833,7 +17833,7 @@
         <v>1</v>
       </c>
       <c r="N269" s="3" t="n">
-        <v>46077.48490740741</v>
+        <v>46077.54743055555</v>
       </c>
       <c r="O269" t="inlineStr">
         <is>
@@ -17894,7 +17894,7 @@
         </is>
       </c>
       <c r="N270" s="3" t="n">
-        <v>46077.48783564815</v>
+        <v>46077.56761574074</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -18022,7 +18022,7 @@
         <v>1</v>
       </c>
       <c r="N272" s="3" t="n">
-        <v>46077.48277777778</v>
+        <v>46077.56184027778</v>
       </c>
       <c r="O272" t="inlineStr">
         <is>
@@ -18406,7 +18406,7 @@
         <v>1</v>
       </c>
       <c r="N278" s="3" t="n">
-        <v>46076.79479166667</v>
+        <v>46077.56746527777</v>
       </c>
       <c r="O278" t="inlineStr">
         <is>
@@ -18470,7 +18470,7 @@
         <v>1</v>
       </c>
       <c r="N279" s="3" t="n">
-        <v>46077.46458333333</v>
+        <v>46077.54202546296</v>
       </c>
       <c r="O279" t="inlineStr">
         <is>
@@ -18534,7 +18534,7 @@
         <v>1</v>
       </c>
       <c r="N280" s="3" t="n">
-        <v>46077.45995370371</v>
+        <v>46077.53841435185</v>
       </c>
       <c r="O280" t="inlineStr">
         <is>
@@ -18598,7 +18598,7 @@
         <v>1</v>
       </c>
       <c r="N281" s="3" t="n">
-        <v>46077.46506944444</v>
+        <v>46077.54679398148</v>
       </c>
       <c r="O281" t="inlineStr">
         <is>
@@ -18617,6 +18617,11 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>10.69.5.151</t>
+        </is>
+      </c>
       <c r="D282" t="n">
         <v>2017</v>
       </c>
@@ -18657,7 +18662,7 @@
         <v>1</v>
       </c>
       <c r="N282" s="3" t="n">
-        <v>46077.48318287037</v>
+        <v>46077.55788194444</v>
       </c>
       <c r="O282" t="inlineStr">
         <is>
@@ -18721,7 +18726,7 @@
         <v>1</v>
       </c>
       <c r="N283" s="3" t="n">
-        <v>46077.46971064815</v>
+        <v>46077.54614583333</v>
       </c>
       <c r="O283" t="inlineStr">
         <is>
@@ -18785,7 +18790,7 @@
         <v>1</v>
       </c>
       <c r="N284" s="3" t="n">
-        <v>46077.45681712963</v>
+        <v>46077.56966435185</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18849,7 +18854,7 @@
         <v>1</v>
       </c>
       <c r="N285" s="3" t="n">
-        <v>46077.48165509259</v>
+        <v>46077.55645833333</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -18913,7 +18918,7 @@
         <v>1</v>
       </c>
       <c r="N286" s="3" t="n">
-        <v>46077.48575231482</v>
+        <v>46077.561875</v>
       </c>
       <c r="O286" t="inlineStr">
         <is>
@@ -18977,7 +18982,7 @@
         <v>1</v>
       </c>
       <c r="N287" s="3" t="n">
-        <v>46077.45976851852</v>
+        <v>46077.53942129629</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
@@ -19041,7 +19046,7 @@
         <v>1</v>
       </c>
       <c r="N288" s="3" t="n">
-        <v>46077.47457175926</v>
+        <v>46077.55445601852</v>
       </c>
       <c r="O288" t="inlineStr">
         <is>
@@ -19105,7 +19110,7 @@
         <v>1</v>
       </c>
       <c r="N289" s="3" t="n">
-        <v>46077.48542824074</v>
+        <v>46077.5654050926</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -19899,7 +19904,7 @@
         <v>1</v>
       </c>
       <c r="N302" s="3" t="n">
-        <v>46077.47645833333</v>
+        <v>46077.55496527778</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -21015,7 +21020,7 @@
         </is>
       </c>
       <c r="N320" s="3" t="n">
-        <v>46077.48371527778</v>
+        <v>46077.56032407407</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21740,7 +21745,7 @@
         <v>1</v>
       </c>
       <c r="N332" s="3" t="n">
-        <v>46077.48019675926</v>
+        <v>46077.55796296296</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21804,7 +21809,7 @@
         <v>2</v>
       </c>
       <c r="N333" s="3" t="n">
-        <v>46077.45041666667</v>
+        <v>46077.50391203703</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21868,7 +21873,7 @@
         <v>2</v>
       </c>
       <c r="N334" s="3" t="n">
-        <v>46077.48778935185</v>
+        <v>46077.56228009259</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21932,7 +21937,7 @@
         <v>2</v>
       </c>
       <c r="N335" s="3" t="n">
-        <v>46077.48</v>
+        <v>46077.5362962963</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -21996,7 +22001,7 @@
         <v>1</v>
       </c>
       <c r="N336" s="3" t="n">
-        <v>46077.45061342593</v>
+        <v>46077.53304398148</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22060,7 +22065,7 @@
         <v>1</v>
       </c>
       <c r="N337" s="3" t="n">
-        <v>46077.47903935185</v>
+        <v>46077.55983796297</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22124,7 +22129,7 @@
         <v>2</v>
       </c>
       <c r="N338" s="3" t="n">
-        <v>46077.47848379629</v>
+        <v>46077.53836805555</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -22252,7 +22257,7 @@
         <v>1</v>
       </c>
       <c r="N340" s="3" t="n">
-        <v>46076.54915509259</v>
+        <v>46077.54107638889</v>
       </c>
       <c r="O340" t="inlineStr">
         <is>
@@ -22316,7 +22321,7 @@
         <v>2</v>
       </c>
       <c r="N341" s="3" t="n">
-        <v>46077.45375</v>
+        <v>46077.53515046297</v>
       </c>
       <c r="O341" t="inlineStr">
         <is>
@@ -22380,7 +22385,7 @@
         <v>2</v>
       </c>
       <c r="N342" s="3" t="n">
-        <v>46077.48434027778</v>
+        <v>46077.56387731482</v>
       </c>
       <c r="O342" t="inlineStr">
         <is>
@@ -22399,11 +22404,6 @@
           <t>OPERACAO 9.1</t>
         </is>
       </c>
-      <c r="C343" t="inlineStr">
-        <is>
-          <t>10.69.5.237</t>
-        </is>
-      </c>
       <c r="D343" t="n">
         <v>2017</v>
       </c>
@@ -22446,7 +22446,7 @@
         </is>
       </c>
       <c r="N343" s="3" t="n">
-        <v>46077.4878125</v>
+        <v>46077.55690972223</v>
       </c>
       <c r="O343" t="inlineStr">
         <is>
@@ -22702,7 +22702,7 @@
         <v>1</v>
       </c>
       <c r="N347" s="3" t="n">
-        <v>46077.42240740741</v>
+        <v>46077.50989583333</v>
       </c>
       <c r="O347" t="inlineStr">
         <is>
@@ -22766,7 +22766,7 @@
         <v>2</v>
       </c>
       <c r="N348" s="3" t="n">
-        <v>46077.46237268519</v>
+        <v>46077.54090277778</v>
       </c>
       <c r="O348" t="inlineStr">
         <is>
@@ -22830,7 +22830,7 @@
         <v>1</v>
       </c>
       <c r="N349" s="3" t="n">
-        <v>46077.46165509259</v>
+        <v>46077.53940972222</v>
       </c>
       <c r="O349" t="inlineStr">
         <is>
@@ -22849,6 +22849,11 @@
           <t>OPERACAO 9.1</t>
         </is>
       </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>10.69.5.244</t>
+        </is>
+      </c>
       <c r="D350" t="n">
         <v>2014</v>
       </c>
@@ -22889,7 +22894,7 @@
         <v>1</v>
       </c>
       <c r="N350" s="3" t="n">
-        <v>46077.45594907407</v>
+        <v>46077.56393518519</v>
       </c>
       <c r="O350" t="inlineStr">
         <is>
@@ -22953,7 +22958,7 @@
         <v>1</v>
       </c>
       <c r="N351" s="3" t="n">
-        <v>46077.46319444444</v>
+        <v>46077.5433449074</v>
       </c>
       <c r="O351" t="inlineStr">
         <is>
@@ -23017,7 +23022,7 @@
         <v>1</v>
       </c>
       <c r="N352" s="3" t="n">
-        <v>46077.46219907407</v>
+        <v>46077.54108796296</v>
       </c>
       <c r="O352" t="inlineStr">
         <is>
@@ -23078,7 +23083,7 @@
         </is>
       </c>
       <c r="N353" s="3" t="n">
-        <v>46077.46164351852</v>
+        <v>46077.53787037037</v>
       </c>
       <c r="O353" t="inlineStr">
         <is>
@@ -23139,7 +23144,7 @@
         </is>
       </c>
       <c r="N354" s="3" t="n">
-        <v>46077.4649537037</v>
+        <v>46077.54251157407</v>
       </c>
       <c r="O354" t="inlineStr">
         <is>
@@ -23203,7 +23208,7 @@
         <v>1</v>
       </c>
       <c r="N355" s="3" t="n">
-        <v>46077.45903935185</v>
+        <v>46077.53454861111</v>
       </c>
       <c r="O355" t="inlineStr">
         <is>
@@ -23267,7 +23272,7 @@
         <v>1</v>
       </c>
       <c r="N356" s="3" t="n">
-        <v>46077.45796296297</v>
+        <v>46077.53331018519</v>
       </c>
       <c r="O356" t="inlineStr">
         <is>
@@ -23331,7 +23336,7 @@
         <v>1</v>
       </c>
       <c r="N357" s="3" t="n">
-        <v>46077.45964120371</v>
+        <v>46077.53469907407</v>
       </c>
       <c r="O357" t="inlineStr">
         <is>
@@ -23454,7 +23459,7 @@
         <v>2</v>
       </c>
       <c r="N359" s="3" t="n">
-        <v>46077.46216435185</v>
+        <v>46077.53886574074</v>
       </c>
       <c r="O359" t="inlineStr">
         <is>
@@ -23518,7 +23523,7 @@
         <v>2</v>
       </c>
       <c r="N360" s="3" t="n">
-        <v>46077.46430555556</v>
+        <v>46077.54126157407</v>
       </c>
       <c r="O360" t="inlineStr">
         <is>
@@ -23582,7 +23587,7 @@
         <v>1</v>
       </c>
       <c r="N361" s="3" t="n">
-        <v>46077.42533564815</v>
+        <v>46077.54055555556</v>
       </c>
       <c r="O361" t="inlineStr">
         <is>
@@ -23643,7 +23648,7 @@
         </is>
       </c>
       <c r="N362" s="3" t="n">
-        <v>46077.46253472222</v>
+        <v>46077.53945601852</v>
       </c>
       <c r="O362" t="inlineStr">
         <is>
@@ -23831,7 +23836,7 @@
         <v>1</v>
       </c>
       <c r="N365" s="3" t="n">
-        <v>46077.45577546296</v>
+        <v>46077.53125</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
@@ -23897,7 +23902,7 @@
         </is>
       </c>
       <c r="N366" s="3" t="n">
-        <v>46077.46357638889</v>
+        <v>46077.54054398148</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -24023,7 +24028,7 @@
         </is>
       </c>
       <c r="N368" s="3" t="n">
-        <v>46077.45134259259</v>
+        <v>46077.53418981482</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -24042,11 +24047,6 @@
           <t>RH</t>
         </is>
       </c>
-      <c r="C369" t="inlineStr">
-        <is>
-          <t>10.69.3.13</t>
-        </is>
-      </c>
       <c r="D369" t="n">
         <v>2025</v>
       </c>
@@ -24089,7 +24089,7 @@
         </is>
       </c>
       <c r="N369" s="3" t="n">
-        <v>46077.45008101852</v>
+        <v>46077.53405092593</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
@@ -24158,7 +24158,7 @@
         <v>1</v>
       </c>
       <c r="N370" s="3" t="n">
-        <v>46077.45167824074</v>
+        <v>46077.56773148148</v>
       </c>
       <c r="O370" t="inlineStr">
         <is>
@@ -24227,7 +24227,7 @@
         <v>1</v>
       </c>
       <c r="N371" s="3" t="n">
-        <v>46077.45690972222</v>
+        <v>46077.5341087963</v>
       </c>
       <c r="O371" t="inlineStr">
         <is>
@@ -24431,7 +24431,7 @@
         <v>1</v>
       </c>
       <c r="N374" s="3" t="n">
-        <v>46077.47453703704</v>
+        <v>46077.55479166667</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24497,7 +24497,7 @@
         </is>
       </c>
       <c r="N375" s="3" t="n">
-        <v>46077.46145833333</v>
+        <v>46077.54384259259</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
@@ -24561,7 +24561,7 @@
         <v>1</v>
       </c>
       <c r="N376" s="3" t="n">
-        <v>46077.46789351852</v>
+        <v>46077.54415509259</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -24630,7 +24630,7 @@
         <v>2</v>
       </c>
       <c r="N377" s="3" t="n">
-        <v>46077.47815972222</v>
+        <v>46077.56071759259</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -24699,7 +24699,7 @@
         <v>2</v>
       </c>
       <c r="N378" s="3" t="n">
-        <v>46077.45571759259</v>
+        <v>46077.56997685185</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização automática 2026-02-24 15:52:09.743239
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>46077.56351851852</v>
+        <v>46077.63839120371</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>46077.5475</v>
+        <v>46077.62663194445</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
         <v>1</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>46077.55841435185</v>
+        <v>46077.63384259259</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>46077.55815972222</v>
+        <v>46077.63504629629</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -1131,7 +1131,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="3" t="n">
-        <v>46077.54675925926</v>
+        <v>46077.62392361111</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1515,7 +1515,7 @@
         <v>2</v>
       </c>
       <c r="N16" s="3" t="n">
-        <v>46077.56957175926</v>
+        <v>46077.65178240741</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -2244,7 +2244,7 @@
         </is>
       </c>
       <c r="N28" s="3" t="n">
-        <v>46077.56653935185</v>
+        <v>46077.64833333333</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -6570,7 +6570,7 @@
         <v>1</v>
       </c>
       <c r="N95" s="3" t="n">
-        <v>46077.54877314815</v>
+        <v>46077.62827546296</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -6708,7 +6708,7 @@
         <v>1</v>
       </c>
       <c r="N97" s="3" t="n">
-        <v>46077.56730324074</v>
+        <v>46077.64597222222</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -6772,7 +6772,7 @@
         <v>1</v>
       </c>
       <c r="N98" s="3" t="n">
-        <v>46077.55307870371</v>
+        <v>46077.62741898148</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -6841,7 +6841,7 @@
         <v>1</v>
       </c>
       <c r="N99" s="3" t="n">
-        <v>46077.57002314815</v>
+        <v>46077.64577546297</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -6910,7 +6910,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>46077.54787037037</v>
+        <v>46077.62858796296</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6979,7 +6979,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="3" t="n">
-        <v>46077.56800925926</v>
+        <v>46077.64050925926</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -7117,7 +7117,7 @@
         <v>2</v>
       </c>
       <c r="N103" s="3" t="n">
-        <v>46077.55673611111</v>
+        <v>46077.63486111111</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7377,7 +7377,7 @@
         <v>1</v>
       </c>
       <c r="N107" s="3" t="n">
-        <v>46077.5471875</v>
+        <v>46077.6244212963</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -7515,7 +7515,7 @@
         <v>1</v>
       </c>
       <c r="N109" s="3" t="n">
-        <v>46077.55246527777</v>
+        <v>46077.63554398148</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7584,7 +7584,7 @@
         <v>2</v>
       </c>
       <c r="N110" s="3" t="n">
-        <v>46077.56128472222</v>
+        <v>46077.64055555555</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7653,7 +7653,7 @@
         <v>2</v>
       </c>
       <c r="N111" s="3" t="n">
-        <v>46077.53460648148</v>
+        <v>46077.65118055556</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
@@ -7722,7 +7722,7 @@
         <v>2</v>
       </c>
       <c r="N112" s="3" t="n">
-        <v>46077.53197916667</v>
+        <v>46077.61469907407</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7791,7 +7791,7 @@
         <v>1</v>
       </c>
       <c r="N113" s="3" t="n">
-        <v>46077.53549768519</v>
+        <v>46077.63082175926</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7860,7 +7860,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>46077.56331018519</v>
+        <v>46077.64034722222</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -7926,7 +7926,7 @@
         </is>
       </c>
       <c r="N115" s="3" t="n">
-        <v>46077.54061342592</v>
+        <v>46077.61847222222</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -8014,11 +8014,6 @@
           <t>DP</t>
         </is>
       </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>10.69.3.23</t>
-        </is>
-      </c>
       <c r="D117" t="n">
         <v>2025</v>
       </c>
@@ -8064,7 +8059,7 @@
         <v>1</v>
       </c>
       <c r="N117" s="3" t="n">
-        <v>46077.53767361111</v>
+        <v>46077.62097222222</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -8130,7 +8125,7 @@
         </is>
       </c>
       <c r="N118" s="3" t="n">
-        <v>46077.53958333333</v>
+        <v>46077.65268518519</v>
       </c>
       <c r="O118" t="inlineStr">
         <is>
@@ -8268,7 +8263,7 @@
         <v>1</v>
       </c>
       <c r="N120" s="3" t="n">
-        <v>46077.50957175926</v>
+        <v>46077.6215625</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -8337,7 +8332,7 @@
         <v>1</v>
       </c>
       <c r="N121" s="3" t="n">
-        <v>46077.54362268518</v>
+        <v>46077.62072916667</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -8403,7 +8398,7 @@
         </is>
       </c>
       <c r="N122" s="3" t="n">
-        <v>46077.55645833333</v>
+        <v>46077.63923611111</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -8472,7 +8467,7 @@
         <v>2</v>
       </c>
       <c r="N123" s="3" t="n">
-        <v>46077.55721064815</v>
+        <v>46077.6355787037</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -8541,7 +8536,7 @@
         <v>1</v>
       </c>
       <c r="N124" s="3" t="n">
-        <v>46077.5512037037</v>
+        <v>46077.63288194445</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -8610,7 +8605,7 @@
         <v>1</v>
       </c>
       <c r="N125" s="3" t="n">
-        <v>46077.56125</v>
+        <v>46077.63804398148</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -8679,7 +8674,7 @@
         <v>2</v>
       </c>
       <c r="N126" s="3" t="n">
-        <v>46077.54775462963</v>
+        <v>46077.62353009259</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -8748,7 +8743,7 @@
         <v>2</v>
       </c>
       <c r="N127" s="3" t="n">
-        <v>46077.56260416667</v>
+        <v>46077.63859953704</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -8817,7 +8812,7 @@
         <v>1</v>
       </c>
       <c r="N128" s="3" t="n">
-        <v>46077.53344907407</v>
+        <v>46077.64770833333</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -8886,7 +8881,7 @@
         <v>1</v>
       </c>
       <c r="N129" s="3" t="n">
-        <v>46077.56211805555</v>
+        <v>46077.63869212963</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -8955,7 +8950,7 @@
         <v>1</v>
       </c>
       <c r="N130" s="3" t="n">
-        <v>46077.55396990741</v>
+        <v>46077.6315625</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -9019,7 +9014,7 @@
         <v>1</v>
       </c>
       <c r="N131" s="3" t="n">
-        <v>46077.55961805556</v>
+        <v>46077.63515046296</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -9152,7 +9147,7 @@
         <v>1</v>
       </c>
       <c r="N133" s="3" t="n">
-        <v>46077.55888888889</v>
+        <v>46077.63475694445</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -9280,7 +9275,7 @@
         <v>1</v>
       </c>
       <c r="N135" s="3" t="n">
-        <v>46076.79548611111</v>
+        <v>46077.62508101852</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -9471,7 +9466,7 @@
         <v>1</v>
       </c>
       <c r="N138" s="3" t="n">
-        <v>46077.57040509259</v>
+        <v>46077.64489583333</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9535,7 +9530,7 @@
         <v>1</v>
       </c>
       <c r="N139" s="3" t="n">
-        <v>46077.53554398148</v>
+        <v>46077.62334490741</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9599,7 +9594,7 @@
         <v>1</v>
       </c>
       <c r="N140" s="3" t="n">
-        <v>46077.54305555556</v>
+        <v>46077.6225462963</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9663,7 +9658,7 @@
         <v>1</v>
       </c>
       <c r="N141" s="3" t="n">
-        <v>46077.53578703704</v>
+        <v>46077.64447916667</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9727,7 +9722,7 @@
         <v>1</v>
       </c>
       <c r="N142" s="3" t="n">
-        <v>46077.56768518518</v>
+        <v>46077.65336805556</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9791,7 +9786,7 @@
         <v>1</v>
       </c>
       <c r="N143" s="3" t="n">
-        <v>46077.56513888889</v>
+        <v>46077.65210648148</v>
       </c>
       <c r="O143" t="inlineStr">
         <is>
@@ -9855,7 +9850,7 @@
         <v>1</v>
       </c>
       <c r="N144" s="3" t="n">
-        <v>46077.53966435185</v>
+        <v>46077.61748842592</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9919,7 +9914,7 @@
         <v>1</v>
       </c>
       <c r="N145" s="3" t="n">
-        <v>46076.8165162037</v>
+        <v>46077.62471064815</v>
       </c>
       <c r="O145" t="inlineStr">
         <is>
@@ -9983,7 +9978,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="3" t="n">
-        <v>46077.55136574074</v>
+        <v>46077.62408564815</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10047,7 +10042,7 @@
         <v>1</v>
       </c>
       <c r="N147" s="3" t="n">
-        <v>46077.54993055556</v>
+        <v>46077.6524074074</v>
       </c>
       <c r="O147" t="inlineStr">
         <is>
@@ -10111,7 +10106,7 @@
         <v>1</v>
       </c>
       <c r="N148" s="3" t="n">
-        <v>46077.54958333333</v>
+        <v>46077.62709490741</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10175,7 +10170,7 @@
         <v>1</v>
       </c>
       <c r="N149" s="3" t="n">
-        <v>46077.54809027778</v>
+        <v>46077.62493055555</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -10239,7 +10234,7 @@
         <v>1</v>
       </c>
       <c r="N150" s="3" t="n">
-        <v>46077.56645833333</v>
+        <v>46077.63912037037</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -10367,7 +10362,7 @@
         <v>1</v>
       </c>
       <c r="N152" s="3" t="n">
-        <v>46076.82327546296</v>
+        <v>46077.62432870371</v>
       </c>
       <c r="O152" t="inlineStr">
         <is>
@@ -10386,11 +10381,6 @@
           <t>OPERACAO 7.1</t>
         </is>
       </c>
-      <c r="C153" t="inlineStr">
-        <is>
-          <t>10.69.5.21</t>
-        </is>
-      </c>
       <c r="D153" t="n">
         <v>2018</v>
       </c>
@@ -10431,7 +10421,7 @@
         <v>1</v>
       </c>
       <c r="N153" s="3" t="n">
-        <v>46077.55393518518</v>
+        <v>46077.63391203704</v>
       </c>
       <c r="O153" t="inlineStr">
         <is>
@@ -10495,7 +10485,7 @@
         <v>1</v>
       </c>
       <c r="N154" s="3" t="n">
-        <v>46077.55486111111</v>
+        <v>46077.61899305556</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10559,7 +10549,7 @@
         <v>1</v>
       </c>
       <c r="N155" s="3" t="n">
-        <v>46077.56861111111</v>
+        <v>46077.63365740741</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10623,7 +10613,7 @@
         <v>1</v>
       </c>
       <c r="N156" s="3" t="n">
-        <v>46077.42474537037</v>
+        <v>46077.64038194445</v>
       </c>
       <c r="O156" t="inlineStr">
         <is>
@@ -10687,7 +10677,7 @@
         <v>1</v>
       </c>
       <c r="N157" s="3" t="n">
-        <v>46077.53488425926</v>
+        <v>46077.57313657407</v>
       </c>
       <c r="O157" t="inlineStr">
         <is>
@@ -10879,7 +10869,7 @@
         <v>1</v>
       </c>
       <c r="N160" s="3" t="n">
-        <v>46077.53736111111</v>
+        <v>46077.61825231482</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
@@ -10943,7 +10933,7 @@
         <v>1</v>
       </c>
       <c r="N161" s="3" t="n">
-        <v>46077.56988425926</v>
+        <v>46077.62640046296</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -11007,7 +10997,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="3" t="n">
-        <v>46077.56512731482</v>
+        <v>46077.64685185185</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11135,7 +11125,7 @@
         <v>2</v>
       </c>
       <c r="N164" s="3" t="n">
-        <v>46077.55450231482</v>
+        <v>46077.62945601852</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11263,7 +11253,7 @@
         <v>2</v>
       </c>
       <c r="N166" s="3" t="n">
-        <v>46077.54755787037</v>
+        <v>46077.62545138889</v>
       </c>
       <c r="O166" t="inlineStr">
         <is>
@@ -11327,7 +11317,7 @@
         <v>2</v>
       </c>
       <c r="N167" s="3" t="n">
-        <v>46077.56684027778</v>
+        <v>46077.60215277778</v>
       </c>
       <c r="O167" t="inlineStr">
         <is>
@@ -11455,7 +11445,7 @@
         <v>2</v>
       </c>
       <c r="N169" s="3" t="n">
-        <v>46077.55640046296</v>
+        <v>46077.63670138889</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -11647,7 +11637,7 @@
         <v>2</v>
       </c>
       <c r="N172" s="3" t="n">
-        <v>46077.55981481481</v>
+        <v>46077.64152777778</v>
       </c>
       <c r="O172" t="inlineStr">
         <is>
@@ -11711,7 +11701,7 @@
         <v>2</v>
       </c>
       <c r="N173" s="3" t="n">
-        <v>46077.56539351852</v>
+        <v>46077.63701388889</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -11839,7 +11829,7 @@
         <v>2</v>
       </c>
       <c r="N175" s="3" t="n">
-        <v>46077.53288194445</v>
+        <v>46077.64855324074</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -11903,7 +11893,7 @@
         <v>2</v>
       </c>
       <c r="N176" s="3" t="n">
-        <v>46077.56060185185</v>
+        <v>46077.64177083333</v>
       </c>
       <c r="O176" t="inlineStr">
         <is>
@@ -11964,10 +11954,10 @@
         </is>
       </c>
       <c r="M177" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N177" s="3" t="n">
-        <v>46077.53530092593</v>
+        <v>46077.65207175926</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
@@ -12031,7 +12021,7 @@
         <v>2</v>
       </c>
       <c r="N178" s="3" t="n">
-        <v>46077.55174768518</v>
+        <v>46077.62881944444</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12095,7 +12085,7 @@
         <v>1</v>
       </c>
       <c r="N179" s="3" t="n">
-        <v>46077.55535879629</v>
+        <v>46077.62793981482</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12159,7 +12149,7 @@
         <v>1</v>
       </c>
       <c r="N180" s="3" t="n">
-        <v>46077.53465277778</v>
+        <v>46077.62267361111</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12612,7 +12602,7 @@
         <v>1</v>
       </c>
       <c r="N187" s="3" t="n">
-        <v>46077.56523148148</v>
+        <v>46077.64548611111</v>
       </c>
       <c r="O187" t="inlineStr">
         <is>
@@ -12676,7 +12666,7 @@
         <v>1</v>
       </c>
       <c r="N188" s="3" t="n">
-        <v>46077.55432870371</v>
+        <v>46077.63094907408</v>
       </c>
       <c r="O188" t="inlineStr">
         <is>
@@ -12762,6 +12752,11 @@
           <t>OPERACAO 8.1</t>
         </is>
       </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>10.69.5.59</t>
+        </is>
+      </c>
       <c r="D190" t="n">
         <v>2015</v>
       </c>
@@ -12799,7 +12794,7 @@
         </is>
       </c>
       <c r="N190" s="3" t="n">
-        <v>46077.55202546297</v>
+        <v>46077.62240740741</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12863,7 +12858,7 @@
         <v>1</v>
       </c>
       <c r="N191" s="3" t="n">
-        <v>46076.815625</v>
+        <v>46077.63354166667</v>
       </c>
       <c r="O191" t="inlineStr">
         <is>
@@ -12927,7 +12922,7 @@
         <v>1</v>
       </c>
       <c r="N192" s="3" t="n">
-        <v>46077.5352662037</v>
+        <v>46077.65400462963</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -13052,7 +13047,7 @@
         <v>2</v>
       </c>
       <c r="N194" s="3" t="n">
-        <v>46077.5588425926</v>
+        <v>46077.61952546296</v>
       </c>
       <c r="O194" t="inlineStr">
         <is>
@@ -13116,7 +13111,7 @@
         <v>1</v>
       </c>
       <c r="N195" s="3" t="n">
-        <v>46077.55621527778</v>
+        <v>46077.63070601852</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13180,7 +13175,7 @@
         <v>1</v>
       </c>
       <c r="N196" s="3" t="n">
-        <v>46077.53734953704</v>
+        <v>46077.62728009259</v>
       </c>
       <c r="O196" t="inlineStr">
         <is>
@@ -13308,7 +13303,7 @@
         <v>1</v>
       </c>
       <c r="N198" s="3" t="n">
-        <v>46077.54363425926</v>
+        <v>46077.62471064815</v>
       </c>
       <c r="O198" t="inlineStr">
         <is>
@@ -13497,7 +13492,7 @@
         </is>
       </c>
       <c r="N201" s="3" t="n">
-        <v>46077.54233796296</v>
+        <v>46077.62520833333</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -13561,7 +13556,7 @@
         <v>1</v>
       </c>
       <c r="N202" s="3" t="n">
-        <v>46077.53814814815</v>
+        <v>46077.62212962963</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13625,7 +13620,7 @@
         <v>1</v>
       </c>
       <c r="N203" s="3" t="n">
-        <v>46077.54222222222</v>
+        <v>46077.63532407407</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13689,7 +13684,7 @@
         <v>1</v>
       </c>
       <c r="N204" s="3" t="n">
-        <v>46077.54666666667</v>
+        <v>46077.62125</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13753,7 +13748,7 @@
         <v>1</v>
       </c>
       <c r="N205" s="3" t="n">
-        <v>46077.5588425926</v>
+        <v>46077.62782407407</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13817,7 +13812,7 @@
         <v>1</v>
       </c>
       <c r="N206" s="3" t="n">
-        <v>46077.54481481481</v>
+        <v>46077.62460648148</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -13881,7 +13876,7 @@
         <v>1</v>
       </c>
       <c r="N207" s="3" t="n">
-        <v>46077.54293981481</v>
+        <v>46077.61884259259</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -13945,7 +13940,7 @@
         <v>1</v>
       </c>
       <c r="N208" s="3" t="n">
-        <v>46077.54354166667</v>
+        <v>46077.57952546296</v>
       </c>
       <c r="O208" t="inlineStr">
         <is>
@@ -14009,7 +14004,7 @@
         <v>1</v>
       </c>
       <c r="N209" s="3" t="n">
-        <v>46077.54579861111</v>
+        <v>46077.62618055556</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14073,7 +14068,7 @@
         <v>1</v>
       </c>
       <c r="N210" s="3" t="n">
-        <v>46077.56480324074</v>
+        <v>46077.64262731482</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14137,7 +14132,7 @@
         <v>1</v>
       </c>
       <c r="N211" s="3" t="n">
-        <v>46077.53870370371</v>
+        <v>46077.58377314815</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -14201,7 +14196,7 @@
         <v>1</v>
       </c>
       <c r="N212" s="3" t="n">
-        <v>46077.53855324074</v>
+        <v>46077.65006944445</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -14265,7 +14260,7 @@
         <v>1</v>
       </c>
       <c r="N213" s="3" t="n">
-        <v>46077.54153935185</v>
+        <v>46077.61665509259</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
@@ -14329,7 +14324,7 @@
         <v>1</v>
       </c>
       <c r="N214" s="3" t="n">
-        <v>46077.53651620371</v>
+        <v>46077.61806712963</v>
       </c>
       <c r="O214" t="inlineStr">
         <is>
@@ -14393,7 +14388,7 @@
         <v>1</v>
       </c>
       <c r="N215" s="3" t="n">
-        <v>46077.53293981482</v>
+        <v>46077.64884259259</v>
       </c>
       <c r="O215" t="inlineStr">
         <is>
@@ -14457,7 +14452,7 @@
         <v>1</v>
       </c>
       <c r="N216" s="3" t="n">
-        <v>46077.5424537037</v>
+        <v>46077.62361111111</v>
       </c>
       <c r="O216" t="inlineStr">
         <is>
@@ -14476,6 +14471,11 @@
           <t>OPERACAO 8.1</t>
         </is>
       </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>10.69.5.85</t>
+        </is>
+      </c>
       <c r="D217" t="n">
         <v>2017</v>
       </c>
@@ -14516,7 +14516,7 @@
         <v>1</v>
       </c>
       <c r="N217" s="3" t="n">
-        <v>46077.53680555556</v>
+        <v>46077.65446759259</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14580,7 +14580,7 @@
         <v>1</v>
       </c>
       <c r="N218" s="3" t="n">
-        <v>46077.5678587963</v>
+        <v>46077.64707175926</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14644,7 +14644,7 @@
         <v>1</v>
       </c>
       <c r="N219" s="3" t="n">
-        <v>46077.56828703704</v>
+        <v>46077.65460648148</v>
       </c>
       <c r="O219" t="inlineStr">
         <is>
@@ -14713,7 +14713,7 @@
         <v>1</v>
       </c>
       <c r="N220" s="3" t="n">
-        <v>46077.53729166667</v>
+        <v>46077.65157407407</v>
       </c>
       <c r="O220" t="inlineStr">
         <is>
@@ -14777,7 +14777,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="3" t="n">
-        <v>46077.56923611111</v>
+        <v>46077.64524305556</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14841,7 +14841,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="3" t="n">
-        <v>46077.55696759259</v>
+        <v>46077.6371412037</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -14905,7 +14905,7 @@
         <v>1</v>
       </c>
       <c r="N223" s="3" t="n">
-        <v>46077.55006944444</v>
+        <v>46077.61907407407</v>
       </c>
       <c r="O223" t="inlineStr">
         <is>
@@ -14969,7 +14969,7 @@
         <v>1</v>
       </c>
       <c r="N224" s="3" t="n">
-        <v>46076.80793981482</v>
+        <v>46077.65172453703</v>
       </c>
       <c r="O224" t="inlineStr">
         <is>
@@ -15033,7 +15033,7 @@
         <v>1</v>
       </c>
       <c r="N225" s="3" t="n">
-        <v>46077.57085648148</v>
+        <v>46077.64261574074</v>
       </c>
       <c r="O225" t="inlineStr">
         <is>
@@ -15097,7 +15097,7 @@
         <v>1</v>
       </c>
       <c r="N226" s="3" t="n">
-        <v>46077.53865740741</v>
+        <v>46077.62444444445</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15161,7 +15161,7 @@
         <v>1</v>
       </c>
       <c r="N227" s="3" t="n">
-        <v>46077.55577546296</v>
+        <v>46077.63923611111</v>
       </c>
       <c r="O227" t="inlineStr">
         <is>
@@ -15225,7 +15225,7 @@
         <v>1</v>
       </c>
       <c r="N228" s="3" t="n">
-        <v>46077.55684027778</v>
+        <v>46077.63497685185</v>
       </c>
       <c r="O228" t="inlineStr">
         <is>
@@ -15289,7 +15289,7 @@
         <v>1</v>
       </c>
       <c r="N229" s="3" t="n">
-        <v>46076.81256944445</v>
+        <v>46077.62744212963</v>
       </c>
       <c r="O229" t="inlineStr">
         <is>
@@ -15353,7 +15353,7 @@
         <v>1</v>
       </c>
       <c r="N230" s="3" t="n">
-        <v>46077.55793981482</v>
+        <v>46077.63831018518</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15417,7 +15417,7 @@
         <v>1</v>
       </c>
       <c r="N231" s="3" t="n">
-        <v>46077.53283564815</v>
+        <v>46077.64783564815</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15481,7 +15481,7 @@
         <v>1</v>
       </c>
       <c r="N232" s="3" t="n">
-        <v>46077.55876157407</v>
+        <v>46077.63295138889</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -15545,7 +15545,7 @@
         <v>1</v>
       </c>
       <c r="N233" s="3" t="n">
-        <v>46077.5359837963</v>
+        <v>46077.62726851852</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15609,7 +15609,7 @@
         <v>1</v>
       </c>
       <c r="N234" s="3" t="n">
-        <v>46077.53502314815</v>
+        <v>46077.64981481482</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -15673,7 +15673,7 @@
         <v>1</v>
       </c>
       <c r="N235" s="3" t="n">
-        <v>46076.80386574074</v>
+        <v>46077.64527777778</v>
       </c>
       <c r="O235" t="inlineStr">
         <is>
@@ -15737,7 +15737,7 @@
         <v>1</v>
       </c>
       <c r="N236" s="3" t="n">
-        <v>46076.8062037037</v>
+        <v>46077.64450231481</v>
       </c>
       <c r="O236" t="inlineStr">
         <is>
@@ -15801,7 +15801,7 @@
         <v>1</v>
       </c>
       <c r="N237" s="3" t="n">
-        <v>46077.38171296296</v>
+        <v>46077.64510416667</v>
       </c>
       <c r="O237" t="inlineStr">
         <is>
@@ -15865,7 +15865,7 @@
         <v>1</v>
       </c>
       <c r="N238" s="3" t="n">
-        <v>46077.56928240741</v>
+        <v>46077.64895833333</v>
       </c>
       <c r="O238" t="inlineStr">
         <is>
@@ -15929,7 +15929,7 @@
         <v>1</v>
       </c>
       <c r="N239" s="3" t="n">
-        <v>46077.56777777777</v>
+        <v>46077.64486111111</v>
       </c>
       <c r="O239" t="inlineStr">
         <is>
@@ -15993,7 +15993,7 @@
         <v>1</v>
       </c>
       <c r="N240" s="3" t="n">
-        <v>46077.54050925926</v>
+        <v>46077.64497685185</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16057,7 +16057,7 @@
         <v>1</v>
       </c>
       <c r="N241" s="3" t="n">
-        <v>46077.55635416666</v>
+        <v>46077.6447800926</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16121,7 +16121,7 @@
         <v>1</v>
       </c>
       <c r="N242" s="3" t="n">
-        <v>46077.54076388889</v>
+        <v>46077.61967592593</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16185,7 +16185,7 @@
         <v>1</v>
       </c>
       <c r="N243" s="3" t="n">
-        <v>46077.5712037037</v>
+        <v>46077.6455787037</v>
       </c>
       <c r="O243" t="inlineStr">
         <is>
@@ -16204,6 +16204,11 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>10.69.5.112</t>
+        </is>
+      </c>
       <c r="D244" t="n">
         <v>2019</v>
       </c>
@@ -16244,7 +16249,7 @@
         <v>1</v>
       </c>
       <c r="N244" s="3" t="n">
-        <v>46076.65324074074</v>
+        <v>46077.62056712963</v>
       </c>
       <c r="O244" t="inlineStr">
         <is>
@@ -16308,7 +16313,7 @@
         <v>1</v>
       </c>
       <c r="N245" s="3" t="n">
-        <v>46077.56820601852</v>
+        <v>46077.64050925926</v>
       </c>
       <c r="O245" t="inlineStr">
         <is>
@@ -16372,7 +16377,7 @@
         <v>1</v>
       </c>
       <c r="N246" s="3" t="n">
-        <v>46077.53314814815</v>
+        <v>46077.65365740741</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16436,7 +16441,7 @@
         <v>1</v>
       </c>
       <c r="N247" s="3" t="n">
-        <v>46077.5581712963</v>
+        <v>46077.62946759259</v>
       </c>
       <c r="O247" t="inlineStr">
         <is>
@@ -16500,7 +16505,7 @@
         <v>1</v>
       </c>
       <c r="N248" s="3" t="n">
-        <v>46077.55504629629</v>
+        <v>46077.63165509259</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16623,7 +16628,7 @@
         <v>1</v>
       </c>
       <c r="N250" s="3" t="n">
-        <v>46077.53300925926</v>
+        <v>46077.62133101852</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16687,7 +16692,7 @@
         <v>1</v>
       </c>
       <c r="N251" s="3" t="n">
-        <v>46077.55798611111</v>
+        <v>46077.59622685185</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16751,7 +16756,7 @@
         <v>1</v>
       </c>
       <c r="N252" s="3" t="n">
-        <v>46077.53541666667</v>
+        <v>46077.65347222222</v>
       </c>
       <c r="O252" t="inlineStr">
         <is>
@@ -16815,7 +16820,7 @@
         <v>1</v>
       </c>
       <c r="N253" s="3" t="n">
-        <v>46077.56190972222</v>
+        <v>46077.62064814815</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16873,7 +16878,7 @@
         <v>1</v>
       </c>
       <c r="N254" s="3" t="n">
-        <v>46077.54517361111</v>
+        <v>46077.63607638889</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -16937,7 +16942,7 @@
         <v>1</v>
       </c>
       <c r="N255" s="3" t="n">
-        <v>46077.56078703704</v>
+        <v>46077.63594907407</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -17001,7 +17006,7 @@
         <v>1</v>
       </c>
       <c r="N256" s="3" t="n">
-        <v>46077.5459375</v>
+        <v>46077.62634259259</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17065,7 +17070,7 @@
         <v>1</v>
       </c>
       <c r="N257" s="3" t="n">
-        <v>46077.55832175926</v>
+        <v>46077.63267361111</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17129,7 +17134,7 @@
         <v>1</v>
       </c>
       <c r="N258" s="3" t="n">
-        <v>46077.54563657408</v>
+        <v>46077.62508101852</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
@@ -17193,7 +17198,7 @@
         <v>1</v>
       </c>
       <c r="N259" s="3" t="n">
-        <v>46077.5437962963</v>
+        <v>46077.61796296296</v>
       </c>
       <c r="O259" t="inlineStr">
         <is>
@@ -17257,7 +17262,7 @@
         <v>1</v>
       </c>
       <c r="N260" s="3" t="n">
-        <v>46077.54381944444</v>
+        <v>46077.61910879629</v>
       </c>
       <c r="O260" t="inlineStr">
         <is>
@@ -17321,7 +17326,7 @@
         <v>1</v>
       </c>
       <c r="N261" s="3" t="n">
-        <v>46077.54190972223</v>
+        <v>46077.62353009259</v>
       </c>
       <c r="O261" t="inlineStr">
         <is>
@@ -17385,7 +17390,7 @@
         <v>1</v>
       </c>
       <c r="N262" s="3" t="n">
-        <v>46077.5505787037</v>
+        <v>46077.62891203703</v>
       </c>
       <c r="O262" t="inlineStr">
         <is>
@@ -17449,7 +17454,7 @@
         <v>1</v>
       </c>
       <c r="N263" s="3" t="n">
-        <v>46077.56516203703</v>
+        <v>46077.64537037037</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17513,7 +17518,7 @@
         <v>1</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>46077.56608796296</v>
+        <v>46077.64123842592</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17577,7 +17582,7 @@
         <v>1</v>
       </c>
       <c r="N265" s="3" t="n">
-        <v>46077.54358796297</v>
+        <v>46077.63707175926</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17641,7 +17646,7 @@
         <v>1</v>
       </c>
       <c r="N266" s="3" t="n">
-        <v>46077.42767361111</v>
+        <v>46077.63783564815</v>
       </c>
       <c r="O266" t="inlineStr">
         <is>
@@ -17705,7 +17710,7 @@
         <v>1</v>
       </c>
       <c r="N267" s="3" t="n">
-        <v>46077.54399305556</v>
+        <v>46077.62315972222</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17769,7 +17774,7 @@
         <v>1</v>
       </c>
       <c r="N268" s="3" t="n">
-        <v>46077.56178240741</v>
+        <v>46077.63834490741</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17833,7 +17838,7 @@
         <v>1</v>
       </c>
       <c r="N269" s="3" t="n">
-        <v>46077.54743055555</v>
+        <v>46077.62708333333</v>
       </c>
       <c r="O269" t="inlineStr">
         <is>
@@ -17894,7 +17899,7 @@
         </is>
       </c>
       <c r="N270" s="3" t="n">
-        <v>46077.56761574074</v>
+        <v>46077.64460648148</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -18022,7 +18027,7 @@
         <v>1</v>
       </c>
       <c r="N272" s="3" t="n">
-        <v>46077.56184027778</v>
+        <v>46077.64484953704</v>
       </c>
       <c r="O272" t="inlineStr">
         <is>
@@ -18086,7 +18091,7 @@
         <v>2</v>
       </c>
       <c r="N273" s="3" t="n">
-        <v>46077.4455787037</v>
+        <v>46077.63230324074</v>
       </c>
       <c r="O273" t="inlineStr">
         <is>
@@ -18406,7 +18411,7 @@
         <v>1</v>
       </c>
       <c r="N278" s="3" t="n">
-        <v>46077.56746527777</v>
+        <v>46077.64924768519</v>
       </c>
       <c r="O278" t="inlineStr">
         <is>
@@ -18470,7 +18475,7 @@
         <v>1</v>
       </c>
       <c r="N279" s="3" t="n">
-        <v>46077.54202546296</v>
+        <v>46077.62165509259</v>
       </c>
       <c r="O279" t="inlineStr">
         <is>
@@ -18534,7 +18539,7 @@
         <v>1</v>
       </c>
       <c r="N280" s="3" t="n">
-        <v>46077.53841435185</v>
+        <v>46077.65201388889</v>
       </c>
       <c r="O280" t="inlineStr">
         <is>
@@ -18617,11 +18622,6 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
-      <c r="C282" t="inlineStr">
-        <is>
-          <t>10.69.5.151</t>
-        </is>
-      </c>
       <c r="D282" t="n">
         <v>2017</v>
       </c>
@@ -18662,7 +18662,7 @@
         <v>1</v>
       </c>
       <c r="N282" s="3" t="n">
-        <v>46077.55788194444</v>
+        <v>46077.63173611111</v>
       </c>
       <c r="O282" t="inlineStr">
         <is>
@@ -18726,7 +18726,7 @@
         <v>1</v>
       </c>
       <c r="N283" s="3" t="n">
-        <v>46077.54614583333</v>
+        <v>46077.62453703704</v>
       </c>
       <c r="O283" t="inlineStr">
         <is>
@@ -18790,7 +18790,7 @@
         <v>1</v>
       </c>
       <c r="N284" s="3" t="n">
-        <v>46077.56966435185</v>
+        <v>46077.65251157407</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18854,7 +18854,7 @@
         <v>1</v>
       </c>
       <c r="N285" s="3" t="n">
-        <v>46077.55645833333</v>
+        <v>46077.63390046296</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -18873,11 +18873,6 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
-      <c r="C286" t="inlineStr">
-        <is>
-          <t>10.69.5.155</t>
-        </is>
-      </c>
       <c r="D286" t="n">
         <v>2019</v>
       </c>
@@ -18918,7 +18913,7 @@
         <v>1</v>
       </c>
       <c r="N286" s="3" t="n">
-        <v>46077.561875</v>
+        <v>46077.60193287037</v>
       </c>
       <c r="O286" t="inlineStr">
         <is>
@@ -18982,7 +18977,7 @@
         <v>1</v>
       </c>
       <c r="N287" s="3" t="n">
-        <v>46077.53942129629</v>
+        <v>46077.61728009259</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
@@ -19046,7 +19041,7 @@
         <v>1</v>
       </c>
       <c r="N288" s="3" t="n">
-        <v>46077.55445601852</v>
+        <v>46077.64530092593</v>
       </c>
       <c r="O288" t="inlineStr">
         <is>
@@ -19110,7 +19105,7 @@
         <v>1</v>
       </c>
       <c r="N289" s="3" t="n">
-        <v>46077.5654050926</v>
+        <v>46077.64225694445</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -19904,7 +19899,7 @@
         <v>1</v>
       </c>
       <c r="N302" s="3" t="n">
-        <v>46077.55496527778</v>
+        <v>46077.63256944445</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -21020,7 +21015,7 @@
         </is>
       </c>
       <c r="N320" s="3" t="n">
-        <v>46077.56032407407</v>
+        <v>46077.63829861111</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21745,7 +21740,7 @@
         <v>1</v>
       </c>
       <c r="N332" s="3" t="n">
-        <v>46077.55796296296</v>
+        <v>46077.63261574074</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21809,7 +21804,7 @@
         <v>2</v>
       </c>
       <c r="N333" s="3" t="n">
-        <v>46077.50391203703</v>
+        <v>46077.62244212963</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21873,7 +21868,7 @@
         <v>2</v>
       </c>
       <c r="N334" s="3" t="n">
-        <v>46077.56228009259</v>
+        <v>46077.6459837963</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21937,7 +21932,7 @@
         <v>2</v>
       </c>
       <c r="N335" s="3" t="n">
-        <v>46077.5362962963</v>
+        <v>46077.65045138889</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -22001,7 +21996,7 @@
         <v>1</v>
       </c>
       <c r="N336" s="3" t="n">
-        <v>46077.53304398148</v>
+        <v>46077.64826388889</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22065,7 +22060,7 @@
         <v>1</v>
       </c>
       <c r="N337" s="3" t="n">
-        <v>46077.55983796297</v>
+        <v>46077.64509259259</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22129,7 +22124,7 @@
         <v>2</v>
       </c>
       <c r="N338" s="3" t="n">
-        <v>46077.53836805555</v>
+        <v>46077.64678240741</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -22257,7 +22252,7 @@
         <v>1</v>
       </c>
       <c r="N340" s="3" t="n">
-        <v>46077.54107638889</v>
+        <v>46077.57763888889</v>
       </c>
       <c r="O340" t="inlineStr">
         <is>
@@ -22321,7 +22316,7 @@
         <v>2</v>
       </c>
       <c r="N341" s="3" t="n">
-        <v>46077.53515046297</v>
+        <v>46077.57143518519</v>
       </c>
       <c r="O341" t="inlineStr">
         <is>
@@ -22404,6 +22399,11 @@
           <t>OPERACAO 9.1</t>
         </is>
       </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>10.69.5.237</t>
+        </is>
+      </c>
       <c r="D343" t="n">
         <v>2017</v>
       </c>
@@ -22446,7 +22446,7 @@
         </is>
       </c>
       <c r="N343" s="3" t="n">
-        <v>46077.55690972223</v>
+        <v>46077.6328587963</v>
       </c>
       <c r="O343" t="inlineStr">
         <is>
@@ -22766,7 +22766,7 @@
         <v>2</v>
       </c>
       <c r="N348" s="3" t="n">
-        <v>46077.54090277778</v>
+        <v>46077.57815972222</v>
       </c>
       <c r="O348" t="inlineStr">
         <is>
@@ -22830,7 +22830,7 @@
         <v>1</v>
       </c>
       <c r="N349" s="3" t="n">
-        <v>46077.53940972222</v>
+        <v>46077.57738425926</v>
       </c>
       <c r="O349" t="inlineStr">
         <is>
@@ -22849,11 +22849,6 @@
           <t>OPERACAO 9.1</t>
         </is>
       </c>
-      <c r="C350" t="inlineStr">
-        <is>
-          <t>10.69.5.244</t>
-        </is>
-      </c>
       <c r="D350" t="n">
         <v>2014</v>
       </c>
@@ -22894,7 +22889,7 @@
         <v>1</v>
       </c>
       <c r="N350" s="3" t="n">
-        <v>46077.56393518519</v>
+        <v>46077.6040625</v>
       </c>
       <c r="O350" t="inlineStr">
         <is>
@@ -22958,7 +22953,7 @@
         <v>1</v>
       </c>
       <c r="N351" s="3" t="n">
-        <v>46077.5433449074</v>
+        <v>46077.58238425926</v>
       </c>
       <c r="O351" t="inlineStr">
         <is>
@@ -23022,7 +23017,7 @@
         <v>1</v>
       </c>
       <c r="N352" s="3" t="n">
-        <v>46077.54108796296</v>
+        <v>46077.58256944444</v>
       </c>
       <c r="O352" t="inlineStr">
         <is>
@@ -23083,7 +23078,7 @@
         </is>
       </c>
       <c r="N353" s="3" t="n">
-        <v>46077.53787037037</v>
+        <v>46077.57596064815</v>
       </c>
       <c r="O353" t="inlineStr">
         <is>
@@ -23144,7 +23139,7 @@
         </is>
       </c>
       <c r="N354" s="3" t="n">
-        <v>46077.54251157407</v>
+        <v>46077.57831018518</v>
       </c>
       <c r="O354" t="inlineStr">
         <is>
@@ -23208,7 +23203,7 @@
         <v>1</v>
       </c>
       <c r="N355" s="3" t="n">
-        <v>46077.53454861111</v>
+        <v>46077.57148148148</v>
       </c>
       <c r="O355" t="inlineStr">
         <is>
@@ -23272,7 +23267,7 @@
         <v>1</v>
       </c>
       <c r="N356" s="3" t="n">
-        <v>46077.53331018519</v>
+        <v>46077.57331018519</v>
       </c>
       <c r="O356" t="inlineStr">
         <is>
@@ -23336,7 +23331,7 @@
         <v>1</v>
       </c>
       <c r="N357" s="3" t="n">
-        <v>46077.53469907407</v>
+        <v>46077.57607638889</v>
       </c>
       <c r="O357" t="inlineStr">
         <is>
@@ -23459,7 +23454,7 @@
         <v>2</v>
       </c>
       <c r="N359" s="3" t="n">
-        <v>46077.53886574074</v>
+        <v>46077.57711805555</v>
       </c>
       <c r="O359" t="inlineStr">
         <is>
@@ -23523,7 +23518,7 @@
         <v>2</v>
       </c>
       <c r="N360" s="3" t="n">
-        <v>46077.54126157407</v>
+        <v>46077.58222222222</v>
       </c>
       <c r="O360" t="inlineStr">
         <is>
@@ -23587,7 +23582,7 @@
         <v>1</v>
       </c>
       <c r="N361" s="3" t="n">
-        <v>46077.54055555556</v>
+        <v>46077.57768518518</v>
       </c>
       <c r="O361" t="inlineStr">
         <is>
@@ -23648,7 +23643,7 @@
         </is>
       </c>
       <c r="N362" s="3" t="n">
-        <v>46077.53945601852</v>
+        <v>46077.57978009259</v>
       </c>
       <c r="O362" t="inlineStr">
         <is>
@@ -23836,7 +23831,7 @@
         <v>1</v>
       </c>
       <c r="N365" s="3" t="n">
-        <v>46077.53125</v>
+        <v>46077.65002314815</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
@@ -23902,7 +23897,7 @@
         </is>
       </c>
       <c r="N366" s="3" t="n">
-        <v>46077.54054398148</v>
+        <v>46077.61840277778</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -24028,7 +24023,7 @@
         </is>
       </c>
       <c r="N368" s="3" t="n">
-        <v>46077.53418981482</v>
+        <v>46077.64894675926</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -24047,6 +24042,11 @@
           <t>RH</t>
         </is>
       </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>10.69.3.13</t>
+        </is>
+      </c>
       <c r="D369" t="n">
         <v>2025</v>
       </c>
@@ -24089,7 +24089,7 @@
         </is>
       </c>
       <c r="N369" s="3" t="n">
-        <v>46077.53405092593</v>
+        <v>46077.65112268519</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
@@ -24158,7 +24158,7 @@
         <v>1</v>
       </c>
       <c r="N370" s="3" t="n">
-        <v>46077.56773148148</v>
+        <v>46077.64572916667</v>
       </c>
       <c r="O370" t="inlineStr">
         <is>
@@ -24227,7 +24227,7 @@
         <v>1</v>
       </c>
       <c r="N371" s="3" t="n">
-        <v>46077.5341087963</v>
+        <v>46077.61494212963</v>
       </c>
       <c r="O371" t="inlineStr">
         <is>
@@ -24431,7 +24431,7 @@
         <v>1</v>
       </c>
       <c r="N374" s="3" t="n">
-        <v>46077.55479166667</v>
+        <v>46077.63546296296</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24497,7 +24497,7 @@
         </is>
       </c>
       <c r="N375" s="3" t="n">
-        <v>46077.54384259259</v>
+        <v>46077.6228587963</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
@@ -24561,7 +24561,7 @@
         <v>1</v>
       </c>
       <c r="N376" s="3" t="n">
-        <v>46077.54415509259</v>
+        <v>46077.62104166667</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -24630,7 +24630,7 @@
         <v>2</v>
       </c>
       <c r="N377" s="3" t="n">
-        <v>46077.56071759259</v>
+        <v>46077.63424768519</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -24699,7 +24699,7 @@
         <v>2</v>
       </c>
       <c r="N378" s="3" t="n">
-        <v>46077.56997685185</v>
+        <v>46077.65004629629</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização automática 2026-02-24 17:52:06.165983
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>46077.63839120371</v>
+        <v>46077.71185185185</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>46077.62663194445</v>
+        <v>46077.70107638889</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
         <v>1</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>46077.63384259259</v>
+        <v>46077.70921296296</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>46077.63504629629</v>
+        <v>46077.71545138889</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -875,7 +875,7 @@
         <v>1</v>
       </c>
       <c r="N6" s="3" t="n">
-        <v>46064.4572800926</v>
+        <v>46077.73386574074</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -944,7 +944,7 @@
         <v>1</v>
       </c>
       <c r="N7" s="3" t="n">
-        <v>46064.42020833334</v>
+        <v>46077.72559027778</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -1072,7 +1072,7 @@
         <v>1</v>
       </c>
       <c r="N9" s="3" t="n">
-        <v>46066.60008101852</v>
+        <v>46077.73664351852</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -1131,7 +1131,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="3" t="n">
-        <v>46077.62392361111</v>
+        <v>46077.70212962963</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1259,7 +1259,7 @@
         <v>1</v>
       </c>
       <c r="N12" s="3" t="n">
-        <v>46064.45525462963</v>
+        <v>46077.6994675926</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1323,7 +1323,7 @@
         <v>1</v>
       </c>
       <c r="N13" s="3" t="n">
-        <v>46064.46146990741</v>
+        <v>46077.69547453704</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1387,7 +1387,7 @@
         <v>2</v>
       </c>
       <c r="N14" s="3" t="n">
-        <v>46064.45708333333</v>
+        <v>46077.69408564815</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1515,7 +1515,7 @@
         <v>2</v>
       </c>
       <c r="N16" s="3" t="n">
-        <v>46077.65178240741</v>
+        <v>46077.72754629629</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1643,7 +1643,7 @@
         <v>2</v>
       </c>
       <c r="N18" s="3" t="n">
-        <v>46066.59618055556</v>
+        <v>46077.69524305555</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1768,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="N20" s="3" t="n">
-        <v>46066.59634259259</v>
+        <v>46077.69560185185</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1832,7 +1832,7 @@
         <v>1</v>
       </c>
       <c r="N21" s="3" t="n">
-        <v>46064.47733796296</v>
+        <v>46077.69509259259</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -2009,7 +2009,7 @@
         <v>1</v>
       </c>
       <c r="N24" s="3" t="n">
-        <v>46058.21155092592</v>
+        <v>46077.73109953704</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2143,6 +2143,11 @@
           <t>AUDITORIO</t>
         </is>
       </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>10.69.3.151</t>
+        </is>
+      </c>
       <c r="D27" t="n">
         <v>2019</v>
       </c>
@@ -2183,7 +2188,7 @@
         <v>1</v>
       </c>
       <c r="N27" s="3" t="n">
-        <v>46064.45870370371</v>
+        <v>46077.73377314815</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2244,7 +2249,7 @@
         </is>
       </c>
       <c r="N28" s="3" t="n">
-        <v>46077.64833333333</v>
+        <v>46077.72322916667</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -6570,7 +6575,7 @@
         <v>1</v>
       </c>
       <c r="N95" s="3" t="n">
-        <v>46077.62827546296</v>
+        <v>46077.73479166667</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -6658,11 +6663,6 @@
           <t>COORDENACAO</t>
         </is>
       </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>10.69.3.93</t>
-        </is>
-      </c>
       <c r="D97" t="n">
         <v>2025</v>
       </c>
@@ -6708,7 +6708,7 @@
         <v>1</v>
       </c>
       <c r="N97" s="3" t="n">
-        <v>46077.64597222222</v>
+        <v>46077.68791666667</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -6772,7 +6772,7 @@
         <v>1</v>
       </c>
       <c r="N98" s="3" t="n">
-        <v>46077.62741898148</v>
+        <v>46077.70405092592</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -6841,7 +6841,7 @@
         <v>1</v>
       </c>
       <c r="N99" s="3" t="n">
-        <v>46077.64577546297</v>
+        <v>46077.72603009259</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -6910,7 +6910,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>46077.62858796296</v>
+        <v>46077.70415509259</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6979,7 +6979,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="3" t="n">
-        <v>46077.64050925926</v>
+        <v>46077.71961805555</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -7117,7 +7117,7 @@
         <v>2</v>
       </c>
       <c r="N103" s="3" t="n">
-        <v>46077.63486111111</v>
+        <v>46077.71810185185</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7377,7 +7377,7 @@
         <v>1</v>
       </c>
       <c r="N107" s="3" t="n">
-        <v>46077.6244212963</v>
+        <v>46077.66335648148</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -7515,7 +7515,7 @@
         <v>1</v>
       </c>
       <c r="N109" s="3" t="n">
-        <v>46077.63554398148</v>
+        <v>46077.71163194445</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7584,7 +7584,7 @@
         <v>2</v>
       </c>
       <c r="N110" s="3" t="n">
-        <v>46077.64055555555</v>
+        <v>46077.71523148148</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7653,7 +7653,7 @@
         <v>2</v>
       </c>
       <c r="N111" s="3" t="n">
-        <v>46077.65118055556</v>
+        <v>46077.7334837963</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
@@ -7722,7 +7722,7 @@
         <v>2</v>
       </c>
       <c r="N112" s="3" t="n">
-        <v>46077.61469907407</v>
+        <v>46077.69805555556</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7791,7 +7791,7 @@
         <v>1</v>
       </c>
       <c r="N113" s="3" t="n">
-        <v>46077.63082175926</v>
+        <v>46077.70722222222</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7860,7 +7860,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>46077.64034722222</v>
+        <v>46077.72015046296</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -7926,7 +7926,7 @@
         </is>
       </c>
       <c r="N115" s="3" t="n">
-        <v>46077.61847222222</v>
+        <v>46077.70039351852</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -8059,7 +8059,7 @@
         <v>1</v>
       </c>
       <c r="N117" s="3" t="n">
-        <v>46077.62097222222</v>
+        <v>46077.69564814815</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -8125,7 +8125,7 @@
         </is>
       </c>
       <c r="N118" s="3" t="n">
-        <v>46077.65268518519</v>
+        <v>46077.69180555556</v>
       </c>
       <c r="O118" t="inlineStr">
         <is>
@@ -8263,7 +8263,7 @@
         <v>1</v>
       </c>
       <c r="N120" s="3" t="n">
-        <v>46077.6215625</v>
+        <v>46077.70016203704</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -8332,7 +8332,7 @@
         <v>1</v>
       </c>
       <c r="N121" s="3" t="n">
-        <v>46077.62072916667</v>
+        <v>46077.72427083334</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -8398,7 +8398,7 @@
         </is>
       </c>
       <c r="N122" s="3" t="n">
-        <v>46077.63923611111</v>
+        <v>46077.71670138889</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -8467,7 +8467,7 @@
         <v>2</v>
       </c>
       <c r="N123" s="3" t="n">
-        <v>46077.6355787037</v>
+        <v>46077.70841435185</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -8536,7 +8536,7 @@
         <v>1</v>
       </c>
       <c r="N124" s="3" t="n">
-        <v>46077.63288194445</v>
+        <v>46077.70832175926</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -8605,7 +8605,7 @@
         <v>1</v>
       </c>
       <c r="N125" s="3" t="n">
-        <v>46077.63804398148</v>
+        <v>46077.71057870371</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -8674,7 +8674,7 @@
         <v>2</v>
       </c>
       <c r="N126" s="3" t="n">
-        <v>46077.62353009259</v>
+        <v>46077.73717592593</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -8743,7 +8743,7 @@
         <v>2</v>
       </c>
       <c r="N127" s="3" t="n">
-        <v>46077.63859953704</v>
+        <v>46077.7133912037</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -8812,7 +8812,7 @@
         <v>1</v>
       </c>
       <c r="N128" s="3" t="n">
-        <v>46077.64770833333</v>
+        <v>46077.68741898148</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -8881,7 +8881,7 @@
         <v>1</v>
       </c>
       <c r="N129" s="3" t="n">
-        <v>46077.63869212963</v>
+        <v>46077.71604166667</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -8950,7 +8950,7 @@
         <v>1</v>
       </c>
       <c r="N130" s="3" t="n">
-        <v>46077.6315625</v>
+        <v>46077.70789351852</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -9014,7 +9014,7 @@
         <v>1</v>
       </c>
       <c r="N131" s="3" t="n">
-        <v>46077.63515046296</v>
+        <v>46077.71408564815</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -9147,7 +9147,7 @@
         <v>1</v>
       </c>
       <c r="N133" s="3" t="n">
-        <v>46077.63475694445</v>
+        <v>46077.71635416667</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -9275,7 +9275,7 @@
         <v>1</v>
       </c>
       <c r="N135" s="3" t="n">
-        <v>46077.62508101852</v>
+        <v>46077.7375462963</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -9466,7 +9466,7 @@
         <v>1</v>
       </c>
       <c r="N138" s="3" t="n">
-        <v>46077.64489583333</v>
+        <v>46077.72376157407</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9530,7 +9530,7 @@
         <v>1</v>
       </c>
       <c r="N139" s="3" t="n">
-        <v>46077.62334490741</v>
+        <v>46077.70211805555</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9594,7 +9594,7 @@
         <v>1</v>
       </c>
       <c r="N140" s="3" t="n">
-        <v>46077.6225462963</v>
+        <v>46077.73208333334</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9658,7 +9658,7 @@
         <v>1</v>
       </c>
       <c r="N141" s="3" t="n">
-        <v>46077.64447916667</v>
+        <v>46077.70430555556</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9722,7 +9722,7 @@
         <v>1</v>
       </c>
       <c r="N142" s="3" t="n">
-        <v>46077.65336805556</v>
+        <v>46077.71456018519</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9786,7 +9786,7 @@
         <v>1</v>
       </c>
       <c r="N143" s="3" t="n">
-        <v>46077.65210648148</v>
+        <v>46077.73275462963</v>
       </c>
       <c r="O143" t="inlineStr">
         <is>
@@ -9850,7 +9850,7 @@
         <v>1</v>
       </c>
       <c r="N144" s="3" t="n">
-        <v>46077.61748842592</v>
+        <v>46077.72986111111</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9914,7 +9914,7 @@
         <v>1</v>
       </c>
       <c r="N145" s="3" t="n">
-        <v>46077.62471064815</v>
+        <v>46077.70570601852</v>
       </c>
       <c r="O145" t="inlineStr">
         <is>
@@ -9978,7 +9978,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="3" t="n">
-        <v>46077.62408564815</v>
+        <v>46077.7012962963</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10042,7 +10042,7 @@
         <v>1</v>
       </c>
       <c r="N147" s="3" t="n">
-        <v>46077.6524074074</v>
+        <v>46077.73097222222</v>
       </c>
       <c r="O147" t="inlineStr">
         <is>
@@ -10106,7 +10106,7 @@
         <v>1</v>
       </c>
       <c r="N148" s="3" t="n">
-        <v>46077.62709490741</v>
+        <v>46077.7078125</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10170,7 +10170,7 @@
         <v>1</v>
       </c>
       <c r="N149" s="3" t="n">
-        <v>46077.62493055555</v>
+        <v>46077.70630787037</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -10234,7 +10234,7 @@
         <v>1</v>
       </c>
       <c r="N150" s="3" t="n">
-        <v>46077.63912037037</v>
+        <v>46077.72081018519</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -10362,7 +10362,7 @@
         <v>1</v>
       </c>
       <c r="N152" s="3" t="n">
-        <v>46077.62432870371</v>
+        <v>46077.73574074074</v>
       </c>
       <c r="O152" t="inlineStr">
         <is>
@@ -10421,7 +10421,7 @@
         <v>1</v>
       </c>
       <c r="N153" s="3" t="n">
-        <v>46077.63391203704</v>
+        <v>46077.70797453704</v>
       </c>
       <c r="O153" t="inlineStr">
         <is>
@@ -10485,7 +10485,7 @@
         <v>1</v>
       </c>
       <c r="N154" s="3" t="n">
-        <v>46077.61899305556</v>
+        <v>46077.73232638889</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10549,7 +10549,7 @@
         <v>1</v>
       </c>
       <c r="N155" s="3" t="n">
-        <v>46077.63365740741</v>
+        <v>46077.71140046296</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10613,7 +10613,7 @@
         <v>1</v>
       </c>
       <c r="N156" s="3" t="n">
-        <v>46077.64038194445</v>
+        <v>46077.71466435185</v>
       </c>
       <c r="O156" t="inlineStr">
         <is>
@@ -10869,7 +10869,7 @@
         <v>1</v>
       </c>
       <c r="N160" s="3" t="n">
-        <v>46077.61825231482</v>
+        <v>46077.73239583334</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
@@ -10933,7 +10933,7 @@
         <v>1</v>
       </c>
       <c r="N161" s="3" t="n">
-        <v>46077.62640046296</v>
+        <v>46077.70966435185</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -10997,7 +10997,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="3" t="n">
-        <v>46077.64685185185</v>
+        <v>46077.72755787037</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11125,7 +11125,7 @@
         <v>2</v>
       </c>
       <c r="N164" s="3" t="n">
-        <v>46077.62945601852</v>
+        <v>46077.70850694444</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11253,7 +11253,7 @@
         <v>2</v>
       </c>
       <c r="N166" s="3" t="n">
-        <v>46077.62545138889</v>
+        <v>46077.70320601852</v>
       </c>
       <c r="O166" t="inlineStr">
         <is>
@@ -11445,7 +11445,7 @@
         <v>2</v>
       </c>
       <c r="N169" s="3" t="n">
-        <v>46077.63670138889</v>
+        <v>46077.71512731481</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -11637,7 +11637,7 @@
         <v>2</v>
       </c>
       <c r="N172" s="3" t="n">
-        <v>46077.64152777778</v>
+        <v>46077.72340277778</v>
       </c>
       <c r="O172" t="inlineStr">
         <is>
@@ -11701,7 +11701,7 @@
         <v>2</v>
       </c>
       <c r="N173" s="3" t="n">
-        <v>46077.63701388889</v>
+        <v>46077.71538194444</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -11829,7 +11829,7 @@
         <v>2</v>
       </c>
       <c r="N175" s="3" t="n">
-        <v>46077.64855324074</v>
+        <v>46077.72474537037</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -11957,7 +11957,7 @@
         <v>2</v>
       </c>
       <c r="N177" s="3" t="n">
-        <v>46077.65207175926</v>
+        <v>46077.69383101852</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
@@ -12021,7 +12021,7 @@
         <v>2</v>
       </c>
       <c r="N178" s="3" t="n">
-        <v>46077.62881944444</v>
+        <v>46077.70302083333</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12085,7 +12085,7 @@
         <v>1</v>
       </c>
       <c r="N179" s="3" t="n">
-        <v>46077.62793981482</v>
+        <v>46077.70721064815</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12149,7 +12149,7 @@
         <v>1</v>
       </c>
       <c r="N180" s="3" t="n">
-        <v>46077.62267361111</v>
+        <v>46077.69952546297</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12602,7 +12602,7 @@
         <v>1</v>
       </c>
       <c r="N187" s="3" t="n">
-        <v>46077.64548611111</v>
+        <v>46077.72331018518</v>
       </c>
       <c r="O187" t="inlineStr">
         <is>
@@ -12666,7 +12666,7 @@
         <v>1</v>
       </c>
       <c r="N188" s="3" t="n">
-        <v>46077.63094907408</v>
+        <v>46077.70809027777</v>
       </c>
       <c r="O188" t="inlineStr">
         <is>
@@ -12794,7 +12794,7 @@
         </is>
       </c>
       <c r="N190" s="3" t="n">
-        <v>46077.62240740741</v>
+        <v>46077.70061342593</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12858,7 +12858,7 @@
         <v>1</v>
       </c>
       <c r="N191" s="3" t="n">
-        <v>46077.63354166667</v>
+        <v>46077.71546296297</v>
       </c>
       <c r="O191" t="inlineStr">
         <is>
@@ -12922,7 +12922,7 @@
         <v>1</v>
       </c>
       <c r="N192" s="3" t="n">
-        <v>46077.65400462963</v>
+        <v>46077.73459490741</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -13047,7 +13047,7 @@
         <v>2</v>
       </c>
       <c r="N194" s="3" t="n">
-        <v>46077.61952546296</v>
+        <v>46077.7372337963</v>
       </c>
       <c r="O194" t="inlineStr">
         <is>
@@ -13111,7 +13111,7 @@
         <v>1</v>
       </c>
       <c r="N195" s="3" t="n">
-        <v>46077.63070601852</v>
+        <v>46077.71179398148</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13175,7 +13175,7 @@
         <v>1</v>
       </c>
       <c r="N196" s="3" t="n">
-        <v>46077.62728009259</v>
+        <v>46077.73609953704</v>
       </c>
       <c r="O196" t="inlineStr">
         <is>
@@ -13239,7 +13239,7 @@
         <v>1</v>
       </c>
       <c r="N197" s="3" t="n">
-        <v>46076.83055555556</v>
+        <v>46077.71123842592</v>
       </c>
       <c r="O197" t="inlineStr">
         <is>
@@ -13303,7 +13303,7 @@
         <v>1</v>
       </c>
       <c r="N198" s="3" t="n">
-        <v>46077.62471064815</v>
+        <v>46077.73679398148</v>
       </c>
       <c r="O198" t="inlineStr">
         <is>
@@ -13367,7 +13367,7 @@
         <v>1</v>
       </c>
       <c r="N199" s="3" t="n">
-        <v>46076.81893518518</v>
+        <v>46077.70880787037</v>
       </c>
       <c r="O199" t="inlineStr">
         <is>
@@ -13556,7 +13556,7 @@
         <v>1</v>
       </c>
       <c r="N202" s="3" t="n">
-        <v>46077.62212962963</v>
+        <v>46077.73496527778</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13620,7 +13620,7 @@
         <v>1</v>
       </c>
       <c r="N203" s="3" t="n">
-        <v>46077.63532407407</v>
+        <v>46077.71528935185</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13684,7 +13684,7 @@
         <v>1</v>
       </c>
       <c r="N204" s="3" t="n">
-        <v>46077.62125</v>
+        <v>46077.70165509259</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13748,7 +13748,7 @@
         <v>1</v>
       </c>
       <c r="N205" s="3" t="n">
-        <v>46077.62782407407</v>
+        <v>46077.70765046297</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13812,7 +13812,7 @@
         <v>1</v>
       </c>
       <c r="N206" s="3" t="n">
-        <v>46077.62460648148</v>
+        <v>46077.70174768518</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -13876,7 +13876,7 @@
         <v>1</v>
       </c>
       <c r="N207" s="3" t="n">
-        <v>46077.61884259259</v>
+        <v>46077.73275462963</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -14004,7 +14004,7 @@
         <v>1</v>
       </c>
       <c r="N209" s="3" t="n">
-        <v>46077.62618055556</v>
+        <v>46077.70469907407</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14068,7 +14068,7 @@
         <v>1</v>
       </c>
       <c r="N210" s="3" t="n">
-        <v>46077.64262731482</v>
+        <v>46077.72592592592</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14132,7 +14132,7 @@
         <v>1</v>
       </c>
       <c r="N211" s="3" t="n">
-        <v>46077.58377314815</v>
+        <v>46077.73409722222</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -14196,7 +14196,7 @@
         <v>1</v>
       </c>
       <c r="N212" s="3" t="n">
-        <v>46077.65006944445</v>
+        <v>46077.72342592593</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -14260,7 +14260,7 @@
         <v>1</v>
       </c>
       <c r="N213" s="3" t="n">
-        <v>46077.61665509259</v>
+        <v>46077.69707175926</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
@@ -14324,7 +14324,7 @@
         <v>1</v>
       </c>
       <c r="N214" s="3" t="n">
-        <v>46077.61806712963</v>
+        <v>46077.73109953704</v>
       </c>
       <c r="O214" t="inlineStr">
         <is>
@@ -14388,7 +14388,7 @@
         <v>1</v>
       </c>
       <c r="N215" s="3" t="n">
-        <v>46077.64884259259</v>
+        <v>46077.72137731482</v>
       </c>
       <c r="O215" t="inlineStr">
         <is>
@@ -14452,7 +14452,7 @@
         <v>1</v>
       </c>
       <c r="N216" s="3" t="n">
-        <v>46077.62361111111</v>
+        <v>46077.70396990741</v>
       </c>
       <c r="O216" t="inlineStr">
         <is>
@@ -14516,7 +14516,7 @@
         <v>1</v>
       </c>
       <c r="N217" s="3" t="n">
-        <v>46077.65446759259</v>
+        <v>46077.71175925926</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14580,7 +14580,7 @@
         <v>1</v>
       </c>
       <c r="N218" s="3" t="n">
-        <v>46077.64707175926</v>
+        <v>46077.72510416667</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14644,7 +14644,7 @@
         <v>1</v>
       </c>
       <c r="N219" s="3" t="n">
-        <v>46077.65460648148</v>
+        <v>46077.72831018519</v>
       </c>
       <c r="O219" t="inlineStr">
         <is>
@@ -14713,7 +14713,7 @@
         <v>1</v>
       </c>
       <c r="N220" s="3" t="n">
-        <v>46077.65157407407</v>
+        <v>46077.72895833333</v>
       </c>
       <c r="O220" t="inlineStr">
         <is>
@@ -14777,7 +14777,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="3" t="n">
-        <v>46077.64524305556</v>
+        <v>46077.72363425926</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14841,7 +14841,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="3" t="n">
-        <v>46077.6371412037</v>
+        <v>46077.71284722222</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -14905,7 +14905,7 @@
         <v>1</v>
       </c>
       <c r="N223" s="3" t="n">
-        <v>46077.61907407407</v>
+        <v>46077.73164351852</v>
       </c>
       <c r="O223" t="inlineStr">
         <is>
@@ -14969,7 +14969,7 @@
         <v>1</v>
       </c>
       <c r="N224" s="3" t="n">
-        <v>46077.65172453703</v>
+        <v>46077.73393518518</v>
       </c>
       <c r="O224" t="inlineStr">
         <is>
@@ -15033,7 +15033,7 @@
         <v>1</v>
       </c>
       <c r="N225" s="3" t="n">
-        <v>46077.64261574074</v>
+        <v>46077.72090277778</v>
       </c>
       <c r="O225" t="inlineStr">
         <is>
@@ -15097,7 +15097,7 @@
         <v>1</v>
       </c>
       <c r="N226" s="3" t="n">
-        <v>46077.62444444445</v>
+        <v>46077.73769675926</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15161,7 +15161,7 @@
         <v>1</v>
       </c>
       <c r="N227" s="3" t="n">
-        <v>46077.63923611111</v>
+        <v>46077.72225694444</v>
       </c>
       <c r="O227" t="inlineStr">
         <is>
@@ -15225,7 +15225,7 @@
         <v>1</v>
       </c>
       <c r="N228" s="3" t="n">
-        <v>46077.63497685185</v>
+        <v>46077.71354166666</v>
       </c>
       <c r="O228" t="inlineStr">
         <is>
@@ -15289,7 +15289,7 @@
         <v>1</v>
       </c>
       <c r="N229" s="3" t="n">
-        <v>46077.62744212963</v>
+        <v>46077.70449074074</v>
       </c>
       <c r="O229" t="inlineStr">
         <is>
@@ -15353,7 +15353,7 @@
         <v>1</v>
       </c>
       <c r="N230" s="3" t="n">
-        <v>46077.63831018518</v>
+        <v>46077.71423611111</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15417,7 +15417,7 @@
         <v>1</v>
       </c>
       <c r="N231" s="3" t="n">
-        <v>46077.64783564815</v>
+        <v>46077.72822916666</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15481,7 +15481,7 @@
         <v>1</v>
       </c>
       <c r="N232" s="3" t="n">
-        <v>46077.63295138889</v>
+        <v>46077.70789351852</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -15545,7 +15545,7 @@
         <v>1</v>
       </c>
       <c r="N233" s="3" t="n">
-        <v>46077.62726851852</v>
+        <v>46077.70168981481</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15609,7 +15609,7 @@
         <v>1</v>
       </c>
       <c r="N234" s="3" t="n">
-        <v>46077.64981481482</v>
+        <v>46077.72518518518</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -15673,7 +15673,7 @@
         <v>1</v>
       </c>
       <c r="N235" s="3" t="n">
-        <v>46077.64527777778</v>
+        <v>46077.71960648148</v>
       </c>
       <c r="O235" t="inlineStr">
         <is>
@@ -15737,7 +15737,7 @@
         <v>1</v>
       </c>
       <c r="N236" s="3" t="n">
-        <v>46077.64450231481</v>
+        <v>46077.71814814815</v>
       </c>
       <c r="O236" t="inlineStr">
         <is>
@@ -15801,7 +15801,7 @@
         <v>1</v>
       </c>
       <c r="N237" s="3" t="n">
-        <v>46077.64510416667</v>
+        <v>46077.72113425926</v>
       </c>
       <c r="O237" t="inlineStr">
         <is>
@@ -15865,7 +15865,7 @@
         <v>1</v>
       </c>
       <c r="N238" s="3" t="n">
-        <v>46077.64895833333</v>
+        <v>46077.73167824074</v>
       </c>
       <c r="O238" t="inlineStr">
         <is>
@@ -15929,7 +15929,7 @@
         <v>1</v>
       </c>
       <c r="N239" s="3" t="n">
-        <v>46077.64486111111</v>
+        <v>46077.70726851852</v>
       </c>
       <c r="O239" t="inlineStr">
         <is>
@@ -15993,7 +15993,7 @@
         <v>1</v>
       </c>
       <c r="N240" s="3" t="n">
-        <v>46077.64497685185</v>
+        <v>46077.7215162037</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16057,7 +16057,7 @@
         <v>1</v>
       </c>
       <c r="N241" s="3" t="n">
-        <v>46077.6447800926</v>
+        <v>46077.72079861111</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16121,7 +16121,7 @@
         <v>1</v>
       </c>
       <c r="N242" s="3" t="n">
-        <v>46077.61967592593</v>
+        <v>46077.73631944445</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16185,7 +16185,7 @@
         <v>1</v>
       </c>
       <c r="N243" s="3" t="n">
-        <v>46077.6455787037</v>
+        <v>46077.72568287037</v>
       </c>
       <c r="O243" t="inlineStr">
         <is>
@@ -16204,11 +16204,6 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
-      <c r="C244" t="inlineStr">
-        <is>
-          <t>10.69.5.112</t>
-        </is>
-      </c>
       <c r="D244" t="n">
         <v>2019</v>
       </c>
@@ -16249,7 +16244,7 @@
         <v>1</v>
       </c>
       <c r="N244" s="3" t="n">
-        <v>46077.62056712963</v>
+        <v>46077.65939814815</v>
       </c>
       <c r="O244" t="inlineStr">
         <is>
@@ -16313,7 +16308,7 @@
         <v>1</v>
       </c>
       <c r="N245" s="3" t="n">
-        <v>46077.64050925926</v>
+        <v>46077.72328703704</v>
       </c>
       <c r="O245" t="inlineStr">
         <is>
@@ -16377,7 +16372,7 @@
         <v>1</v>
       </c>
       <c r="N246" s="3" t="n">
-        <v>46077.65365740741</v>
+        <v>46077.73341435185</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16441,7 +16436,7 @@
         <v>1</v>
       </c>
       <c r="N247" s="3" t="n">
-        <v>46077.62946759259</v>
+        <v>46077.70711805556</v>
       </c>
       <c r="O247" t="inlineStr">
         <is>
@@ -16505,7 +16500,7 @@
         <v>1</v>
       </c>
       <c r="N248" s="3" t="n">
-        <v>46077.63165509259</v>
+        <v>46077.70364583333</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16569,7 +16564,7 @@
         <v>1</v>
       </c>
       <c r="N249" s="3" t="n">
-        <v>46076.64736111111</v>
+        <v>46077.72174768519</v>
       </c>
       <c r="O249" t="inlineStr">
         <is>
@@ -16628,7 +16623,7 @@
         <v>1</v>
       </c>
       <c r="N250" s="3" t="n">
-        <v>46077.62133101852</v>
+        <v>46077.69770833333</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16692,7 +16687,7 @@
         <v>1</v>
       </c>
       <c r="N251" s="3" t="n">
-        <v>46077.59622685185</v>
+        <v>46077.71799768518</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16756,7 +16751,7 @@
         <v>1</v>
       </c>
       <c r="N252" s="3" t="n">
-        <v>46077.65347222222</v>
+        <v>46077.72673611111</v>
       </c>
       <c r="O252" t="inlineStr">
         <is>
@@ -16820,7 +16815,7 @@
         <v>1</v>
       </c>
       <c r="N253" s="3" t="n">
-        <v>46077.62064814815</v>
+        <v>46077.70172453704</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16878,7 +16873,7 @@
         <v>1</v>
       </c>
       <c r="N254" s="3" t="n">
-        <v>46077.63607638889</v>
+        <v>46077.72497685185</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -16942,7 +16937,7 @@
         <v>1</v>
       </c>
       <c r="N255" s="3" t="n">
-        <v>46077.63594907407</v>
+        <v>46077.70706018519</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -17006,7 +17001,7 @@
         <v>1</v>
       </c>
       <c r="N256" s="3" t="n">
-        <v>46077.62634259259</v>
+        <v>46077.66888888889</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17070,7 +17065,7 @@
         <v>1</v>
       </c>
       <c r="N257" s="3" t="n">
-        <v>46077.63267361111</v>
+        <v>46077.70769675926</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17134,7 +17129,7 @@
         <v>1</v>
       </c>
       <c r="N258" s="3" t="n">
-        <v>46077.62508101852</v>
+        <v>46077.71174768519</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
@@ -17198,7 +17193,7 @@
         <v>1</v>
       </c>
       <c r="N259" s="3" t="n">
-        <v>46077.61796296296</v>
+        <v>46077.70586805556</v>
       </c>
       <c r="O259" t="inlineStr">
         <is>
@@ -17326,7 +17321,7 @@
         <v>1</v>
       </c>
       <c r="N261" s="3" t="n">
-        <v>46077.62353009259</v>
+        <v>46077.70289351852</v>
       </c>
       <c r="O261" t="inlineStr">
         <is>
@@ -17390,7 +17385,7 @@
         <v>1</v>
       </c>
       <c r="N262" s="3" t="n">
-        <v>46077.62891203703</v>
+        <v>46077.70795138889</v>
       </c>
       <c r="O262" t="inlineStr">
         <is>
@@ -17454,7 +17449,7 @@
         <v>1</v>
       </c>
       <c r="N263" s="3" t="n">
-        <v>46077.64537037037</v>
+        <v>46077.72064814815</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17518,7 +17513,7 @@
         <v>1</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>46077.64123842592</v>
+        <v>46077.71534722222</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17582,7 +17577,7 @@
         <v>1</v>
       </c>
       <c r="N265" s="3" t="n">
-        <v>46077.63707175926</v>
+        <v>46077.7147337963</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17710,7 +17705,7 @@
         <v>1</v>
       </c>
       <c r="N267" s="3" t="n">
-        <v>46077.62315972222</v>
+        <v>46077.7016087963</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17774,7 +17769,7 @@
         <v>1</v>
       </c>
       <c r="N268" s="3" t="n">
-        <v>46077.63834490741</v>
+        <v>46077.71954861111</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17838,7 +17833,7 @@
         <v>1</v>
       </c>
       <c r="N269" s="3" t="n">
-        <v>46077.62708333333</v>
+        <v>46077.7067824074</v>
       </c>
       <c r="O269" t="inlineStr">
         <is>
@@ -17899,7 +17894,7 @@
         </is>
       </c>
       <c r="N270" s="3" t="n">
-        <v>46077.64460648148</v>
+        <v>46077.72414351852</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -18091,7 +18086,7 @@
         <v>2</v>
       </c>
       <c r="N273" s="3" t="n">
-        <v>46077.63230324074</v>
+        <v>46077.7109837963</v>
       </c>
       <c r="O273" t="inlineStr">
         <is>
@@ -18411,7 +18406,7 @@
         <v>1</v>
       </c>
       <c r="N278" s="3" t="n">
-        <v>46077.64924768519</v>
+        <v>46077.72836805556</v>
       </c>
       <c r="O278" t="inlineStr">
         <is>
@@ -18539,7 +18534,7 @@
         <v>1</v>
       </c>
       <c r="N280" s="3" t="n">
-        <v>46077.65201388889</v>
+        <v>46077.72876157407</v>
       </c>
       <c r="O280" t="inlineStr">
         <is>
@@ -18662,7 +18657,7 @@
         <v>1</v>
       </c>
       <c r="N282" s="3" t="n">
-        <v>46077.63173611111</v>
+        <v>46077.70456018519</v>
       </c>
       <c r="O282" t="inlineStr">
         <is>
@@ -18726,7 +18721,7 @@
         <v>1</v>
       </c>
       <c r="N283" s="3" t="n">
-        <v>46077.62453703704</v>
+        <v>46077.70515046296</v>
       </c>
       <c r="O283" t="inlineStr">
         <is>
@@ -18790,7 +18785,7 @@
         <v>1</v>
       </c>
       <c r="N284" s="3" t="n">
-        <v>46077.65251157407</v>
+        <v>46077.73510416667</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18854,7 +18849,7 @@
         <v>1</v>
       </c>
       <c r="N285" s="3" t="n">
-        <v>46077.63390046296</v>
+        <v>46077.70840277777</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -18977,7 +18972,7 @@
         <v>1</v>
       </c>
       <c r="N287" s="3" t="n">
-        <v>46077.61728009259</v>
+        <v>46077.73431712963</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
@@ -19105,7 +19100,7 @@
         <v>1</v>
       </c>
       <c r="N289" s="3" t="n">
-        <v>46077.64225694445</v>
+        <v>46077.72077546296</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -19899,7 +19894,7 @@
         <v>1</v>
       </c>
       <c r="N302" s="3" t="n">
-        <v>46077.63256944445</v>
+        <v>46077.70734953704</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -21015,7 +21010,7 @@
         </is>
       </c>
       <c r="N320" s="3" t="n">
-        <v>46077.63829861111</v>
+        <v>46077.7153125</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21393,7 +21388,7 @@
         </is>
       </c>
       <c r="N326" s="3" t="n">
-        <v>46052.87260416667</v>
+        <v>46077.73675925926</v>
       </c>
       <c r="O326" t="inlineStr">
         <is>
@@ -21740,7 +21735,7 @@
         <v>1</v>
       </c>
       <c r="N332" s="3" t="n">
-        <v>46077.63261574074</v>
+        <v>46077.70997685185</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21804,7 +21799,7 @@
         <v>2</v>
       </c>
       <c r="N333" s="3" t="n">
-        <v>46077.62244212963</v>
+        <v>46077.7375462963</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21868,7 +21863,7 @@
         <v>2</v>
       </c>
       <c r="N334" s="3" t="n">
-        <v>46077.6459837963</v>
+        <v>46077.72782407407</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21932,7 +21927,7 @@
         <v>2</v>
       </c>
       <c r="N335" s="3" t="n">
-        <v>46077.65045138889</v>
+        <v>46077.72697916667</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -21996,7 +21991,7 @@
         <v>1</v>
       </c>
       <c r="N336" s="3" t="n">
-        <v>46077.64826388889</v>
+        <v>46077.6835300926</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22060,7 +22055,7 @@
         <v>1</v>
       </c>
       <c r="N337" s="3" t="n">
-        <v>46077.64509259259</v>
+        <v>46077.72237268519</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22124,7 +22119,7 @@
         <v>2</v>
       </c>
       <c r="N338" s="3" t="n">
-        <v>46077.64678240741</v>
+        <v>46077.73020833333</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -22446,7 +22441,7 @@
         </is>
       </c>
       <c r="N343" s="3" t="n">
-        <v>46077.6328587963</v>
+        <v>46077.7067824074</v>
       </c>
       <c r="O343" t="inlineStr">
         <is>
@@ -23831,7 +23826,7 @@
         <v>1</v>
       </c>
       <c r="N365" s="3" t="n">
-        <v>46077.65002314815</v>
+        <v>46077.68586805555</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
@@ -23897,7 +23892,7 @@
         </is>
       </c>
       <c r="N366" s="3" t="n">
-        <v>46077.61840277778</v>
+        <v>46077.73435185185</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -24023,7 +24018,7 @@
         </is>
       </c>
       <c r="N368" s="3" t="n">
-        <v>46077.64894675926</v>
+        <v>46077.72487268518</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -24089,7 +24084,7 @@
         </is>
       </c>
       <c r="N369" s="3" t="n">
-        <v>46077.65112268519</v>
+        <v>46077.72804398148</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
@@ -24158,7 +24153,7 @@
         <v>1</v>
       </c>
       <c r="N370" s="3" t="n">
-        <v>46077.64572916667</v>
+        <v>46077.71864583333</v>
       </c>
       <c r="O370" t="inlineStr">
         <is>
@@ -24227,7 +24222,7 @@
         <v>1</v>
       </c>
       <c r="N371" s="3" t="n">
-        <v>46077.61494212963</v>
+        <v>46077.69305555556</v>
       </c>
       <c r="O371" t="inlineStr">
         <is>
@@ -24431,7 +24426,7 @@
         <v>1</v>
       </c>
       <c r="N374" s="3" t="n">
-        <v>46077.63546296296</v>
+        <v>46077.7084837963</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24497,7 +24492,7 @@
         </is>
       </c>
       <c r="N375" s="3" t="n">
-        <v>46077.6228587963</v>
+        <v>46077.7372800926</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
@@ -24516,6 +24511,11 @@
           <t>COORDENACAO</t>
         </is>
       </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>10.69.3.72</t>
+        </is>
+      </c>
       <c r="D376" t="n">
         <v>2025</v>
       </c>
@@ -24561,7 +24561,7 @@
         <v>1</v>
       </c>
       <c r="N376" s="3" t="n">
-        <v>46077.62104166667</v>
+        <v>46077.73570601852</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -24630,7 +24630,7 @@
         <v>2</v>
       </c>
       <c r="N377" s="3" t="n">
-        <v>46077.63424768519</v>
+        <v>46077.70633101852</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -24699,7 +24699,7 @@
         <v>2</v>
       </c>
       <c r="N378" s="3" t="n">
-        <v>46077.65004629629</v>
+        <v>46077.72825231482</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização automática 2026-02-25 12:04:08.412204
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>46077.71185185185</v>
+        <v>46078.48479166667</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>46077.70107638889</v>
+        <v>46078.4733912037</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
         <v>1</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>46077.70921296296</v>
+        <v>46078.45667824074</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>46077.71545138889</v>
+        <v>46078.45774305556</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -875,7 +875,7 @@
         <v>1</v>
       </c>
       <c r="N6" s="3" t="n">
-        <v>46077.73386574074</v>
+        <v>46077.77353009259</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -944,7 +944,7 @@
         <v>1</v>
       </c>
       <c r="N7" s="3" t="n">
-        <v>46077.72559027778</v>
+        <v>46077.76526620371</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -1131,7 +1131,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="3" t="n">
-        <v>46077.70212962963</v>
+        <v>46078.47103009259</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -2009,7 +2009,7 @@
         <v>1</v>
       </c>
       <c r="N24" s="3" t="n">
-        <v>46077.73109953704</v>
+        <v>46078.20137731481</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2141,11 +2141,6 @@
       <c r="B27" t="inlineStr">
         <is>
           <t>AUDITORIO</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>10.69.3.151</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -6575,7 +6570,7 @@
         <v>1</v>
       </c>
       <c r="N95" s="3" t="n">
-        <v>46077.73479166667</v>
+        <v>46078.47793981482</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -6644,7 +6639,7 @@
         <v>1</v>
       </c>
       <c r="N96" s="3" t="n">
-        <v>46073.82103009259</v>
+        <v>46078.46424768519</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
@@ -6708,7 +6703,7 @@
         <v>1</v>
       </c>
       <c r="N97" s="3" t="n">
-        <v>46077.68791666667</v>
+        <v>46078.46658564815</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -6772,7 +6767,7 @@
         <v>1</v>
       </c>
       <c r="N98" s="3" t="n">
-        <v>46077.70405092592</v>
+        <v>46078.48465277778</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -6841,7 +6836,7 @@
         <v>1</v>
       </c>
       <c r="N99" s="3" t="n">
-        <v>46077.72603009259</v>
+        <v>46078.46572916667</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -6910,7 +6905,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>46077.70415509259</v>
+        <v>46078.48517361111</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6979,7 +6974,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="3" t="n">
-        <v>46077.71961805555</v>
+        <v>46078.46268518519</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -7117,7 +7112,7 @@
         <v>2</v>
       </c>
       <c r="N103" s="3" t="n">
-        <v>46077.71810185185</v>
+        <v>46078.46942129629</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7243,11 +7238,8 @@
           <t>HP ProBook 440 14 inch G9 Notebook PC</t>
         </is>
       </c>
-      <c r="M105" t="n">
-        <v>1</v>
-      </c>
       <c r="N105" s="3" t="n">
-        <v>46077.50876157408</v>
+        <v>46078.45886574074</v>
       </c>
       <c r="O105" t="inlineStr">
         <is>
@@ -7377,7 +7369,7 @@
         <v>1</v>
       </c>
       <c r="N107" s="3" t="n">
-        <v>46077.66335648148</v>
+        <v>46078.46722222222</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -7515,7 +7507,7 @@
         <v>1</v>
       </c>
       <c r="N109" s="3" t="n">
-        <v>46077.71163194445</v>
+        <v>46078.4555787037</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7584,7 +7576,7 @@
         <v>2</v>
       </c>
       <c r="N110" s="3" t="n">
-        <v>46077.71523148148</v>
+        <v>46078.46891203704</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7653,7 +7645,7 @@
         <v>2</v>
       </c>
       <c r="N111" s="3" t="n">
-        <v>46077.7334837963</v>
+        <v>46078.46814814815</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
@@ -7722,7 +7714,7 @@
         <v>2</v>
       </c>
       <c r="N112" s="3" t="n">
-        <v>46077.69805555556</v>
+        <v>46078.48305555555</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7791,7 +7783,7 @@
         <v>1</v>
       </c>
       <c r="N113" s="3" t="n">
-        <v>46077.70722222222</v>
+        <v>46078.47728009259</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7860,7 +7852,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>46077.72015046296</v>
+        <v>46078.4730787037</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -7926,7 +7918,7 @@
         </is>
       </c>
       <c r="N115" s="3" t="n">
-        <v>46077.70039351852</v>
+        <v>46078.48471064815</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -7995,7 +7987,7 @@
         <v>1</v>
       </c>
       <c r="N116" s="3" t="n">
-        <v>46076.57146990741</v>
+        <v>46078.48628472222</v>
       </c>
       <c r="O116" t="inlineStr">
         <is>
@@ -8014,6 +8006,11 @@
           <t>DP</t>
         </is>
       </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>10.69.3.23</t>
+        </is>
+      </c>
       <c r="D117" t="n">
         <v>2025</v>
       </c>
@@ -8059,7 +8056,7 @@
         <v>1</v>
       </c>
       <c r="N117" s="3" t="n">
-        <v>46077.69564814815</v>
+        <v>46078.48497685185</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -8125,7 +8122,7 @@
         </is>
       </c>
       <c r="N118" s="3" t="n">
-        <v>46077.69180555556</v>
+        <v>46078.46006944445</v>
       </c>
       <c r="O118" t="inlineStr">
         <is>
@@ -8263,7 +8260,7 @@
         <v>1</v>
       </c>
       <c r="N120" s="3" t="n">
-        <v>46077.70016203704</v>
+        <v>46078.46357638889</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -8332,7 +8329,7 @@
         <v>1</v>
       </c>
       <c r="N121" s="3" t="n">
-        <v>46077.72427083334</v>
+        <v>46078.46646990741</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -8398,7 +8395,7 @@
         </is>
       </c>
       <c r="N122" s="3" t="n">
-        <v>46077.71670138889</v>
+        <v>46078.48327546296</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -8467,7 +8464,7 @@
         <v>2</v>
       </c>
       <c r="N123" s="3" t="n">
-        <v>46077.70841435185</v>
+        <v>46078.47386574074</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -8536,7 +8533,7 @@
         <v>1</v>
       </c>
       <c r="N124" s="3" t="n">
-        <v>46077.70832175926</v>
+        <v>46078.47922453703</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -8605,7 +8602,7 @@
         <v>1</v>
       </c>
       <c r="N125" s="3" t="n">
-        <v>46077.71057870371</v>
+        <v>46078.45295138889</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -8674,7 +8671,7 @@
         <v>2</v>
       </c>
       <c r="N126" s="3" t="n">
-        <v>46077.73717592593</v>
+        <v>46078.46078703704</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -8743,7 +8740,7 @@
         <v>2</v>
       </c>
       <c r="N127" s="3" t="n">
-        <v>46077.7133912037</v>
+        <v>46078.46689814814</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -8812,7 +8809,7 @@
         <v>1</v>
       </c>
       <c r="N128" s="3" t="n">
-        <v>46077.68741898148</v>
+        <v>46078.47548611111</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -8881,7 +8878,7 @@
         <v>1</v>
       </c>
       <c r="N129" s="3" t="n">
-        <v>46077.71604166667</v>
+        <v>46078.48148148148</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -8950,7 +8947,7 @@
         <v>1</v>
       </c>
       <c r="N130" s="3" t="n">
-        <v>46077.70789351852</v>
+        <v>46078.45804398148</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -8969,6 +8966,11 @@
           <t>ADM/FIN</t>
         </is>
       </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>10.69.3.6</t>
+        </is>
+      </c>
       <c r="D131" t="n">
         <v>2025</v>
       </c>
@@ -9014,7 +9016,7 @@
         <v>1</v>
       </c>
       <c r="N131" s="3" t="n">
-        <v>46077.71408564815</v>
+        <v>46078.48592592592</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -9147,7 +9149,7 @@
         <v>1</v>
       </c>
       <c r="N133" s="3" t="n">
-        <v>46077.71635416667</v>
+        <v>46078.45733796297</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -9271,11 +9273,8 @@
           <t>HP Compaq Pro 4300 SFF Brazil PC</t>
         </is>
       </c>
-      <c r="M135" t="n">
-        <v>1</v>
-      </c>
       <c r="N135" s="3" t="n">
-        <v>46077.7375462963</v>
+        <v>46077.81891203704</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -9466,7 +9465,7 @@
         <v>1</v>
       </c>
       <c r="N138" s="3" t="n">
-        <v>46077.72376157407</v>
+        <v>46078.44731481482</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9530,7 +9529,7 @@
         <v>1</v>
       </c>
       <c r="N139" s="3" t="n">
-        <v>46077.70211805555</v>
+        <v>46078.46912037037</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9594,7 +9593,7 @@
         <v>1</v>
       </c>
       <c r="N140" s="3" t="n">
-        <v>46077.73208333334</v>
+        <v>46078.45165509259</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9655,10 +9654,10 @@
         </is>
       </c>
       <c r="M141" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N141" s="3" t="n">
-        <v>46077.70430555556</v>
+        <v>46078.46081018518</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9722,7 +9721,7 @@
         <v>1</v>
       </c>
       <c r="N142" s="3" t="n">
-        <v>46077.71456018519</v>
+        <v>46078.45163194444</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9786,7 +9785,7 @@
         <v>1</v>
       </c>
       <c r="N143" s="3" t="n">
-        <v>46077.73275462963</v>
+        <v>46078.47792824074</v>
       </c>
       <c r="O143" t="inlineStr">
         <is>
@@ -9850,7 +9849,7 @@
         <v>1</v>
       </c>
       <c r="N144" s="3" t="n">
-        <v>46077.72986111111</v>
+        <v>46078.45966435185</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9914,7 +9913,7 @@
         <v>1</v>
       </c>
       <c r="N145" s="3" t="n">
-        <v>46077.70570601852</v>
+        <v>46078.46798611111</v>
       </c>
       <c r="O145" t="inlineStr">
         <is>
@@ -9978,7 +9977,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="3" t="n">
-        <v>46077.7012962963</v>
+        <v>46078.48679398148</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10042,7 +10041,7 @@
         <v>1</v>
       </c>
       <c r="N147" s="3" t="n">
-        <v>46077.73097222222</v>
+        <v>46078.47673611111</v>
       </c>
       <c r="O147" t="inlineStr">
         <is>
@@ -10106,7 +10105,7 @@
         <v>1</v>
       </c>
       <c r="N148" s="3" t="n">
-        <v>46077.7078125</v>
+        <v>46078.45818287037</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10170,7 +10169,7 @@
         <v>1</v>
       </c>
       <c r="N149" s="3" t="n">
-        <v>46077.70630787037</v>
+        <v>46078.48717592593</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -10234,7 +10233,7 @@
         <v>1</v>
       </c>
       <c r="N150" s="3" t="n">
-        <v>46077.72081018519</v>
+        <v>46078.47556712963</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -10362,7 +10361,7 @@
         <v>1</v>
       </c>
       <c r="N152" s="3" t="n">
-        <v>46077.73574074074</v>
+        <v>46077.81385416666</v>
       </c>
       <c r="O152" t="inlineStr">
         <is>
@@ -10381,6 +10380,11 @@
           <t>OPERACAO 7.1</t>
         </is>
       </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>10.69.5.21</t>
+        </is>
+      </c>
       <c r="D153" t="n">
         <v>2018</v>
       </c>
@@ -10421,7 +10425,7 @@
         <v>1</v>
       </c>
       <c r="N153" s="3" t="n">
-        <v>46077.70797453704</v>
+        <v>46078.48524305555</v>
       </c>
       <c r="O153" t="inlineStr">
         <is>
@@ -10485,7 +10489,7 @@
         <v>1</v>
       </c>
       <c r="N154" s="3" t="n">
-        <v>46077.73232638889</v>
+        <v>46078.45193287037</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10549,7 +10553,7 @@
         <v>1</v>
       </c>
       <c r="N155" s="3" t="n">
-        <v>46077.71140046296</v>
+        <v>46078.44721064815</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10613,7 +10617,7 @@
         <v>1</v>
       </c>
       <c r="N156" s="3" t="n">
-        <v>46077.71466435185</v>
+        <v>46078.46853009259</v>
       </c>
       <c r="O156" t="inlineStr">
         <is>
@@ -10677,7 +10681,7 @@
         <v>1</v>
       </c>
       <c r="N157" s="3" t="n">
-        <v>46077.57313657407</v>
+        <v>46078.45967592593</v>
       </c>
       <c r="O157" t="inlineStr">
         <is>
@@ -10741,7 +10745,7 @@
         <v>1</v>
       </c>
       <c r="N158" s="3" t="n">
-        <v>46077.54832175926</v>
+        <v>46078.4849537037</v>
       </c>
       <c r="O158" t="inlineStr">
         <is>
@@ -10805,7 +10809,7 @@
         <v>1</v>
       </c>
       <c r="N159" s="3" t="n">
-        <v>46077.55333333334</v>
+        <v>46078.4753125</v>
       </c>
       <c r="O159" t="inlineStr">
         <is>
@@ -10869,7 +10873,7 @@
         <v>1</v>
       </c>
       <c r="N160" s="3" t="n">
-        <v>46077.73239583334</v>
+        <v>46078.45277777778</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
@@ -10933,7 +10937,7 @@
         <v>1</v>
       </c>
       <c r="N161" s="3" t="n">
-        <v>46077.70966435185</v>
+        <v>46078.45211805555</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -10997,7 +11001,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="3" t="n">
-        <v>46077.72755787037</v>
+        <v>46078.47810185186</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11125,7 +11129,7 @@
         <v>2</v>
       </c>
       <c r="N164" s="3" t="n">
-        <v>46077.70850694444</v>
+        <v>46078.47390046297</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11189,7 +11193,7 @@
         <v>2</v>
       </c>
       <c r="N165" s="3" t="n">
-        <v>46077.52436342592</v>
+        <v>46078.44908564815</v>
       </c>
       <c r="O165" t="inlineStr">
         <is>
@@ -11253,7 +11257,7 @@
         <v>2</v>
       </c>
       <c r="N166" s="3" t="n">
-        <v>46077.70320601852</v>
+        <v>46078.44902777778</v>
       </c>
       <c r="O166" t="inlineStr">
         <is>
@@ -11317,7 +11321,7 @@
         <v>2</v>
       </c>
       <c r="N167" s="3" t="n">
-        <v>46077.60215277778</v>
+        <v>46078.48438657408</v>
       </c>
       <c r="O167" t="inlineStr">
         <is>
@@ -11381,7 +11385,7 @@
         <v>2</v>
       </c>
       <c r="N168" s="3" t="n">
-        <v>46077.55825231481</v>
+        <v>46078.47186342593</v>
       </c>
       <c r="O168" t="inlineStr">
         <is>
@@ -11445,7 +11449,7 @@
         <v>2</v>
       </c>
       <c r="N169" s="3" t="n">
-        <v>46077.71512731481</v>
+        <v>46078.48221064815</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -11509,7 +11513,7 @@
         <v>2</v>
       </c>
       <c r="N170" s="3" t="n">
-        <v>46077.55481481482</v>
+        <v>46078.48496527778</v>
       </c>
       <c r="O170" t="inlineStr">
         <is>
@@ -11573,7 +11577,7 @@
         <v>1</v>
       </c>
       <c r="N171" s="3" t="n">
-        <v>46077.55986111111</v>
+        <v>46078.46061342592</v>
       </c>
       <c r="O171" t="inlineStr">
         <is>
@@ -11637,7 +11641,7 @@
         <v>2</v>
       </c>
       <c r="N172" s="3" t="n">
-        <v>46077.72340277778</v>
+        <v>46077.76346064815</v>
       </c>
       <c r="O172" t="inlineStr">
         <is>
@@ -11701,7 +11705,7 @@
         <v>2</v>
       </c>
       <c r="N173" s="3" t="n">
-        <v>46077.71538194444</v>
+        <v>46078.48421296296</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -11765,7 +11769,7 @@
         <v>2</v>
       </c>
       <c r="N174" s="3" t="n">
-        <v>46077.53944444445</v>
+        <v>46078.47538194444</v>
       </c>
       <c r="O174" t="inlineStr">
         <is>
@@ -11829,7 +11833,7 @@
         <v>2</v>
       </c>
       <c r="N175" s="3" t="n">
-        <v>46077.72474537037</v>
+        <v>46078.45765046297</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -11893,7 +11897,7 @@
         <v>2</v>
       </c>
       <c r="N176" s="3" t="n">
-        <v>46077.64177083333</v>
+        <v>46078.46560185185</v>
       </c>
       <c r="O176" t="inlineStr">
         <is>
@@ -11957,7 +11961,7 @@
         <v>2</v>
       </c>
       <c r="N177" s="3" t="n">
-        <v>46077.69383101852</v>
+        <v>46078.46690972222</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
@@ -12021,7 +12025,7 @@
         <v>2</v>
       </c>
       <c r="N178" s="3" t="n">
-        <v>46077.70302083333</v>
+        <v>46078.47993055556</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12085,7 +12089,7 @@
         <v>1</v>
       </c>
       <c r="N179" s="3" t="n">
-        <v>46077.70721064815</v>
+        <v>46078.47502314814</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12149,7 +12153,7 @@
         <v>1</v>
       </c>
       <c r="N180" s="3" t="n">
-        <v>46077.69952546297</v>
+        <v>46078.46925925926</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12213,7 +12217,7 @@
         <v>1</v>
       </c>
       <c r="N181" s="3" t="n">
-        <v>46076.85011574074</v>
+        <v>46078.48498842592</v>
       </c>
       <c r="O181" t="inlineStr">
         <is>
@@ -12602,7 +12606,7 @@
         <v>1</v>
       </c>
       <c r="N187" s="3" t="n">
-        <v>46077.72331018518</v>
+        <v>46078.46965277778</v>
       </c>
       <c r="O187" t="inlineStr">
         <is>
@@ -12666,7 +12670,7 @@
         <v>1</v>
       </c>
       <c r="N188" s="3" t="n">
-        <v>46077.70809027777</v>
+        <v>46078.48660879629</v>
       </c>
       <c r="O188" t="inlineStr">
         <is>
@@ -12794,7 +12798,7 @@
         </is>
       </c>
       <c r="N190" s="3" t="n">
-        <v>46077.70061342593</v>
+        <v>46078.46982638889</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12858,7 +12862,7 @@
         <v>1</v>
       </c>
       <c r="N191" s="3" t="n">
-        <v>46077.71546296297</v>
+        <v>46077.79695601852</v>
       </c>
       <c r="O191" t="inlineStr">
         <is>
@@ -12922,7 +12926,7 @@
         <v>1</v>
       </c>
       <c r="N192" s="3" t="n">
-        <v>46077.73459490741</v>
+        <v>46078.47851851852</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -13047,7 +13051,7 @@
         <v>2</v>
       </c>
       <c r="N194" s="3" t="n">
-        <v>46077.7372337963</v>
+        <v>46078.48105324074</v>
       </c>
       <c r="O194" t="inlineStr">
         <is>
@@ -13111,7 +13115,7 @@
         <v>1</v>
       </c>
       <c r="N195" s="3" t="n">
-        <v>46077.71179398148</v>
+        <v>46078.46210648148</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13175,7 +13179,7 @@
         <v>1</v>
       </c>
       <c r="N196" s="3" t="n">
-        <v>46077.73609953704</v>
+        <v>46077.81361111111</v>
       </c>
       <c r="O196" t="inlineStr">
         <is>
@@ -13239,7 +13243,7 @@
         <v>1</v>
       </c>
       <c r="N197" s="3" t="n">
-        <v>46077.71123842592</v>
+        <v>46077.8303125</v>
       </c>
       <c r="O197" t="inlineStr">
         <is>
@@ -13303,7 +13307,7 @@
         <v>1</v>
       </c>
       <c r="N198" s="3" t="n">
-        <v>46077.73679398148</v>
+        <v>46078.47444444444</v>
       </c>
       <c r="O198" t="inlineStr">
         <is>
@@ -13367,7 +13371,7 @@
         <v>1</v>
       </c>
       <c r="N199" s="3" t="n">
-        <v>46077.70880787037</v>
+        <v>46077.82847222222</v>
       </c>
       <c r="O199" t="inlineStr">
         <is>
@@ -13492,7 +13496,7 @@
         </is>
       </c>
       <c r="N201" s="3" t="n">
-        <v>46077.62520833333</v>
+        <v>46078.46471064815</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -13556,7 +13560,7 @@
         <v>1</v>
       </c>
       <c r="N202" s="3" t="n">
-        <v>46077.73496527778</v>
+        <v>46078.45842592593</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13620,7 +13624,7 @@
         <v>1</v>
       </c>
       <c r="N203" s="3" t="n">
-        <v>46077.71528935185</v>
+        <v>46078.45521990741</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13684,7 +13688,7 @@
         <v>1</v>
       </c>
       <c r="N204" s="3" t="n">
-        <v>46077.70165509259</v>
+        <v>46078.45334490741</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13748,7 +13752,7 @@
         <v>1</v>
       </c>
       <c r="N205" s="3" t="n">
-        <v>46077.70765046297</v>
+        <v>46078.4728587963</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13812,7 +13816,7 @@
         <v>1</v>
       </c>
       <c r="N206" s="3" t="n">
-        <v>46077.70174768518</v>
+        <v>46077.82380787037</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -13876,7 +13880,7 @@
         <v>1</v>
       </c>
       <c r="N207" s="3" t="n">
-        <v>46077.73275462963</v>
+        <v>46078.45667824074</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -13940,7 +13944,7 @@
         <v>1</v>
       </c>
       <c r="N208" s="3" t="n">
-        <v>46077.57952546296</v>
+        <v>46078.45357638889</v>
       </c>
       <c r="O208" t="inlineStr">
         <is>
@@ -14004,7 +14008,7 @@
         <v>1</v>
       </c>
       <c r="N209" s="3" t="n">
-        <v>46077.70469907407</v>
+        <v>46078.47603009259</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14068,7 +14072,7 @@
         <v>1</v>
       </c>
       <c r="N210" s="3" t="n">
-        <v>46077.72592592592</v>
+        <v>46078.48771990741</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14132,7 +14136,7 @@
         <v>1</v>
       </c>
       <c r="N211" s="3" t="n">
-        <v>46077.73409722222</v>
+        <v>46078.45149305555</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -14196,7 +14200,7 @@
         <v>1</v>
       </c>
       <c r="N212" s="3" t="n">
-        <v>46077.72342592593</v>
+        <v>46078.45365740741</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -14260,7 +14264,7 @@
         <v>1</v>
       </c>
       <c r="N213" s="3" t="n">
-        <v>46077.69707175926</v>
+        <v>46078.47652777778</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
@@ -14324,7 +14328,7 @@
         <v>1</v>
       </c>
       <c r="N214" s="3" t="n">
-        <v>46077.73109953704</v>
+        <v>46078.37199074074</v>
       </c>
       <c r="O214" t="inlineStr">
         <is>
@@ -14388,7 +14392,7 @@
         <v>1</v>
       </c>
       <c r="N215" s="3" t="n">
-        <v>46077.72137731482</v>
+        <v>46077.83409722222</v>
       </c>
       <c r="O215" t="inlineStr">
         <is>
@@ -14452,7 +14456,7 @@
         <v>1</v>
       </c>
       <c r="N216" s="3" t="n">
-        <v>46077.70396990741</v>
+        <v>46078.48261574074</v>
       </c>
       <c r="O216" t="inlineStr">
         <is>
@@ -14471,11 +14475,6 @@
           <t>OPERACAO 8.1</t>
         </is>
       </c>
-      <c r="C217" t="inlineStr">
-        <is>
-          <t>10.69.5.85</t>
-        </is>
-      </c>
       <c r="D217" t="n">
         <v>2017</v>
       </c>
@@ -14516,7 +14515,7 @@
         <v>1</v>
       </c>
       <c r="N217" s="3" t="n">
-        <v>46077.71175925926</v>
+        <v>46078.45222222222</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14580,7 +14579,7 @@
         <v>1</v>
       </c>
       <c r="N218" s="3" t="n">
-        <v>46077.72510416667</v>
+        <v>46078.48447916667</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14644,7 +14643,7 @@
         <v>1</v>
       </c>
       <c r="N219" s="3" t="n">
-        <v>46077.72831018519</v>
+        <v>46078.40295138889</v>
       </c>
       <c r="O219" t="inlineStr">
         <is>
@@ -14713,7 +14712,7 @@
         <v>1</v>
       </c>
       <c r="N220" s="3" t="n">
-        <v>46077.72895833333</v>
+        <v>46078.48685185185</v>
       </c>
       <c r="O220" t="inlineStr">
         <is>
@@ -14777,7 +14776,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="3" t="n">
-        <v>46077.72363425926</v>
+        <v>46078.45928240741</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14841,7 +14840,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="3" t="n">
-        <v>46077.71284722222</v>
+        <v>46078.466875</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -14905,7 +14904,7 @@
         <v>1</v>
       </c>
       <c r="N223" s="3" t="n">
-        <v>46077.73164351852</v>
+        <v>46078.45415509259</v>
       </c>
       <c r="O223" t="inlineStr">
         <is>
@@ -14969,7 +14968,7 @@
         <v>1</v>
       </c>
       <c r="N224" s="3" t="n">
-        <v>46077.73393518518</v>
+        <v>46078.47532407408</v>
       </c>
       <c r="O224" t="inlineStr">
         <is>
@@ -15033,7 +15032,7 @@
         <v>1</v>
       </c>
       <c r="N225" s="3" t="n">
-        <v>46077.72090277778</v>
+        <v>46078.47582175926</v>
       </c>
       <c r="O225" t="inlineStr">
         <is>
@@ -15097,7 +15096,7 @@
         <v>1</v>
       </c>
       <c r="N226" s="3" t="n">
-        <v>46077.73769675926</v>
+        <v>46078.48530092592</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15161,7 +15160,7 @@
         <v>1</v>
       </c>
       <c r="N227" s="3" t="n">
-        <v>46077.72225694444</v>
+        <v>46078.46837962963</v>
       </c>
       <c r="O227" t="inlineStr">
         <is>
@@ -15225,7 +15224,7 @@
         <v>1</v>
       </c>
       <c r="N228" s="3" t="n">
-        <v>46077.71354166666</v>
+        <v>46078.47028935186</v>
       </c>
       <c r="O228" t="inlineStr">
         <is>
@@ -15289,7 +15288,7 @@
         <v>1</v>
       </c>
       <c r="N229" s="3" t="n">
-        <v>46077.70449074074</v>
+        <v>46078.45387731482</v>
       </c>
       <c r="O229" t="inlineStr">
         <is>
@@ -15353,7 +15352,7 @@
         <v>1</v>
       </c>
       <c r="N230" s="3" t="n">
-        <v>46077.71423611111</v>
+        <v>46078.4618287037</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15417,7 +15416,7 @@
         <v>1</v>
       </c>
       <c r="N231" s="3" t="n">
-        <v>46077.72822916666</v>
+        <v>46078.48357638889</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15481,7 +15480,7 @@
         <v>1</v>
       </c>
       <c r="N232" s="3" t="n">
-        <v>46077.70789351852</v>
+        <v>46078.47865740741</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -15545,7 +15544,7 @@
         <v>1</v>
       </c>
       <c r="N233" s="3" t="n">
-        <v>46077.70168981481</v>
+        <v>46078.45724537037</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15609,7 +15608,7 @@
         <v>1</v>
       </c>
       <c r="N234" s="3" t="n">
-        <v>46077.72518518518</v>
+        <v>46078.44936342593</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -15673,7 +15672,7 @@
         <v>1</v>
       </c>
       <c r="N235" s="3" t="n">
-        <v>46077.71960648148</v>
+        <v>46078.4497337963</v>
       </c>
       <c r="O235" t="inlineStr">
         <is>
@@ -15737,7 +15736,7 @@
         <v>1</v>
       </c>
       <c r="N236" s="3" t="n">
-        <v>46077.71814814815</v>
+        <v>46078.48525462963</v>
       </c>
       <c r="O236" t="inlineStr">
         <is>
@@ -15801,7 +15800,7 @@
         <v>1</v>
       </c>
       <c r="N237" s="3" t="n">
-        <v>46077.72113425926</v>
+        <v>46077.79817129629</v>
       </c>
       <c r="O237" t="inlineStr">
         <is>
@@ -15865,7 +15864,7 @@
         <v>1</v>
       </c>
       <c r="N238" s="3" t="n">
-        <v>46077.73167824074</v>
+        <v>46078.48001157407</v>
       </c>
       <c r="O238" t="inlineStr">
         <is>
@@ -15929,7 +15928,7 @@
         <v>1</v>
       </c>
       <c r="N239" s="3" t="n">
-        <v>46077.70726851852</v>
+        <v>46078.48751157407</v>
       </c>
       <c r="O239" t="inlineStr">
         <is>
@@ -15993,7 +15992,7 @@
         <v>1</v>
       </c>
       <c r="N240" s="3" t="n">
-        <v>46077.7215162037</v>
+        <v>46078.4744212963</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16057,7 +16056,7 @@
         <v>1</v>
       </c>
       <c r="N241" s="3" t="n">
-        <v>46077.72079861111</v>
+        <v>46078.47614583333</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16121,7 +16120,7 @@
         <v>1</v>
       </c>
       <c r="N242" s="3" t="n">
-        <v>46077.73631944445</v>
+        <v>46078.47881944444</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16185,7 +16184,7 @@
         <v>1</v>
       </c>
       <c r="N243" s="3" t="n">
-        <v>46077.72568287037</v>
+        <v>46077.76497685185</v>
       </c>
       <c r="O243" t="inlineStr">
         <is>
@@ -16244,7 +16243,7 @@
         <v>1</v>
       </c>
       <c r="N244" s="3" t="n">
-        <v>46077.65939814815</v>
+        <v>46078.40516203704</v>
       </c>
       <c r="O244" t="inlineStr">
         <is>
@@ -16308,7 +16307,7 @@
         <v>1</v>
       </c>
       <c r="N245" s="3" t="n">
-        <v>46077.72328703704</v>
+        <v>46078.45295138889</v>
       </c>
       <c r="O245" t="inlineStr">
         <is>
@@ -16372,7 +16371,7 @@
         <v>1</v>
       </c>
       <c r="N246" s="3" t="n">
-        <v>46077.73341435185</v>
+        <v>46078.45226851852</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16436,7 +16435,7 @@
         <v>1</v>
       </c>
       <c r="N247" s="3" t="n">
-        <v>46077.70711805556</v>
+        <v>46078.47230324074</v>
       </c>
       <c r="O247" t="inlineStr">
         <is>
@@ -16500,7 +16499,7 @@
         <v>1</v>
       </c>
       <c r="N248" s="3" t="n">
-        <v>46077.70364583333</v>
+        <v>46078.45214120371</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16564,7 +16563,7 @@
         <v>1</v>
       </c>
       <c r="N249" s="3" t="n">
-        <v>46077.72174768519</v>
+        <v>46078.47575231481</v>
       </c>
       <c r="O249" t="inlineStr">
         <is>
@@ -16583,6 +16582,11 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>10.69.5.118</t>
+        </is>
+      </c>
       <c r="D250" t="n">
         <v>2017</v>
       </c>
@@ -16623,7 +16627,7 @@
         <v>1</v>
       </c>
       <c r="N250" s="3" t="n">
-        <v>46077.69770833333</v>
+        <v>46078.48413194445</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16687,7 +16691,7 @@
         <v>1</v>
       </c>
       <c r="N251" s="3" t="n">
-        <v>46077.71799768518</v>
+        <v>46078.48716435185</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16751,7 +16755,7 @@
         <v>1</v>
       </c>
       <c r="N252" s="3" t="n">
-        <v>46077.72673611111</v>
+        <v>46078.45513888889</v>
       </c>
       <c r="O252" t="inlineStr">
         <is>
@@ -16815,7 +16819,7 @@
         <v>1</v>
       </c>
       <c r="N253" s="3" t="n">
-        <v>46077.70172453704</v>
+        <v>46078.47984953703</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16873,7 +16877,7 @@
         <v>1</v>
       </c>
       <c r="N254" s="3" t="n">
-        <v>46077.72497685185</v>
+        <v>46078.45273148148</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -16937,7 +16941,7 @@
         <v>1</v>
       </c>
       <c r="N255" s="3" t="n">
-        <v>46077.70706018519</v>
+        <v>46078.48706018519</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -17001,7 +17005,7 @@
         <v>1</v>
       </c>
       <c r="N256" s="3" t="n">
-        <v>46077.66888888889</v>
+        <v>46078.4521875</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17065,7 +17069,7 @@
         <v>1</v>
       </c>
       <c r="N257" s="3" t="n">
-        <v>46077.70769675926</v>
+        <v>46078.44929398148</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17129,7 +17133,7 @@
         <v>1</v>
       </c>
       <c r="N258" s="3" t="n">
-        <v>46077.71174768519</v>
+        <v>46078.48373842592</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
@@ -17193,7 +17197,7 @@
         <v>1</v>
       </c>
       <c r="N259" s="3" t="n">
-        <v>46077.70586805556</v>
+        <v>46078.48795138889</v>
       </c>
       <c r="O259" t="inlineStr">
         <is>
@@ -17257,7 +17261,7 @@
         <v>1</v>
       </c>
       <c r="N260" s="3" t="n">
-        <v>46077.61910879629</v>
+        <v>46078.45258101852</v>
       </c>
       <c r="O260" t="inlineStr">
         <is>
@@ -17321,7 +17325,7 @@
         <v>1</v>
       </c>
       <c r="N261" s="3" t="n">
-        <v>46077.70289351852</v>
+        <v>46078.48232638889</v>
       </c>
       <c r="O261" t="inlineStr">
         <is>
@@ -17385,7 +17389,7 @@
         <v>1</v>
       </c>
       <c r="N262" s="3" t="n">
-        <v>46077.70795138889</v>
+        <v>46078.45458333333</v>
       </c>
       <c r="O262" t="inlineStr">
         <is>
@@ -17449,7 +17453,7 @@
         <v>1</v>
       </c>
       <c r="N263" s="3" t="n">
-        <v>46077.72064814815</v>
+        <v>46078.46046296296</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17513,7 +17517,7 @@
         <v>1</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>46077.71534722222</v>
+        <v>46078.45185185185</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17577,7 +17581,7 @@
         <v>1</v>
       </c>
       <c r="N265" s="3" t="n">
-        <v>46077.7147337963</v>
+        <v>46078.48126157407</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17641,7 +17645,7 @@
         <v>1</v>
       </c>
       <c r="N266" s="3" t="n">
-        <v>46077.63783564815</v>
+        <v>46078.46108796296</v>
       </c>
       <c r="O266" t="inlineStr">
         <is>
@@ -17705,7 +17709,7 @@
         <v>1</v>
       </c>
       <c r="N267" s="3" t="n">
-        <v>46077.7016087963</v>
+        <v>46078.45009259259</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17769,7 +17773,7 @@
         <v>1</v>
       </c>
       <c r="N268" s="3" t="n">
-        <v>46077.71954861111</v>
+        <v>46078.45643518519</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17833,7 +17837,7 @@
         <v>1</v>
       </c>
       <c r="N269" s="3" t="n">
-        <v>46077.7067824074</v>
+        <v>46078.4708912037</v>
       </c>
       <c r="O269" t="inlineStr">
         <is>
@@ -17894,7 +17898,7 @@
         </is>
       </c>
       <c r="N270" s="3" t="n">
-        <v>46077.72414351852</v>
+        <v>46078.47869212963</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -17958,7 +17962,7 @@
         <v>1</v>
       </c>
       <c r="N271" s="3" t="n">
-        <v>46077.32462962963</v>
+        <v>46078.12091435185</v>
       </c>
       <c r="O271" t="inlineStr">
         <is>
@@ -18022,7 +18026,7 @@
         <v>1</v>
       </c>
       <c r="N272" s="3" t="n">
-        <v>46077.64484953704</v>
+        <v>46078.45087962963</v>
       </c>
       <c r="O272" t="inlineStr">
         <is>
@@ -18086,7 +18090,7 @@
         <v>2</v>
       </c>
       <c r="N273" s="3" t="n">
-        <v>46077.7109837963</v>
+        <v>46078.41335648148</v>
       </c>
       <c r="O273" t="inlineStr">
         <is>
@@ -18406,7 +18410,7 @@
         <v>1</v>
       </c>
       <c r="N278" s="3" t="n">
-        <v>46077.72836805556</v>
+        <v>46078.45108796296</v>
       </c>
       <c r="O278" t="inlineStr">
         <is>
@@ -18470,7 +18474,7 @@
         <v>1</v>
       </c>
       <c r="N279" s="3" t="n">
-        <v>46077.62165509259</v>
+        <v>46078.47736111111</v>
       </c>
       <c r="O279" t="inlineStr">
         <is>
@@ -18534,7 +18538,7 @@
         <v>1</v>
       </c>
       <c r="N280" s="3" t="n">
-        <v>46077.72876157407</v>
+        <v>46078.45782407407</v>
       </c>
       <c r="O280" t="inlineStr">
         <is>
@@ -18598,7 +18602,7 @@
         <v>1</v>
       </c>
       <c r="N281" s="3" t="n">
-        <v>46077.54679398148</v>
+        <v>46078.4841087963</v>
       </c>
       <c r="O281" t="inlineStr">
         <is>
@@ -18657,7 +18661,7 @@
         <v>1</v>
       </c>
       <c r="N282" s="3" t="n">
-        <v>46077.70456018519</v>
+        <v>46078.47760416667</v>
       </c>
       <c r="O282" t="inlineStr">
         <is>
@@ -18721,7 +18725,7 @@
         <v>1</v>
       </c>
       <c r="N283" s="3" t="n">
-        <v>46077.70515046296</v>
+        <v>46078.4549537037</v>
       </c>
       <c r="O283" t="inlineStr">
         <is>
@@ -18785,7 +18789,7 @@
         <v>1</v>
       </c>
       <c r="N284" s="3" t="n">
-        <v>46077.73510416667</v>
+        <v>46078.47991898148</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18849,7 +18853,7 @@
         <v>1</v>
       </c>
       <c r="N285" s="3" t="n">
-        <v>46077.70840277777</v>
+        <v>46078.45111111111</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -18868,6 +18872,11 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>10.69.5.155</t>
+        </is>
+      </c>
       <c r="D286" t="n">
         <v>2019</v>
       </c>
@@ -18908,7 +18917,7 @@
         <v>1</v>
       </c>
       <c r="N286" s="3" t="n">
-        <v>46077.60193287037</v>
+        <v>46078.48677083333</v>
       </c>
       <c r="O286" t="inlineStr">
         <is>
@@ -18972,7 +18981,7 @@
         <v>1</v>
       </c>
       <c r="N287" s="3" t="n">
-        <v>46077.73431712963</v>
+        <v>46078.46034722222</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
@@ -19036,7 +19045,7 @@
         <v>1</v>
       </c>
       <c r="N288" s="3" t="n">
-        <v>46077.64530092593</v>
+        <v>46078.48518518519</v>
       </c>
       <c r="O288" t="inlineStr">
         <is>
@@ -19100,7 +19109,7 @@
         <v>1</v>
       </c>
       <c r="N289" s="3" t="n">
-        <v>46077.72077546296</v>
+        <v>46078.45756944444</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -19894,7 +19903,7 @@
         <v>1</v>
       </c>
       <c r="N302" s="3" t="n">
-        <v>46077.70734953704</v>
+        <v>46078.48150462963</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -20635,7 +20644,7 @@
         </is>
       </c>
       <c r="N314" s="3" t="n">
-        <v>46071.79034722222</v>
+        <v>46078.4800925926</v>
       </c>
       <c r="O314" t="inlineStr">
         <is>
@@ -21010,7 +21019,7 @@
         </is>
       </c>
       <c r="N320" s="3" t="n">
-        <v>46077.7153125</v>
+        <v>46078.46047453704</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21388,7 +21397,7 @@
         </is>
       </c>
       <c r="N326" s="3" t="n">
-        <v>46077.73675925926</v>
+        <v>46077.85212962963</v>
       </c>
       <c r="O326" t="inlineStr">
         <is>
@@ -21735,7 +21744,7 @@
         <v>1</v>
       </c>
       <c r="N332" s="3" t="n">
-        <v>46077.70997685185</v>
+        <v>46078.46850694445</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21799,7 +21808,7 @@
         <v>2</v>
       </c>
       <c r="N333" s="3" t="n">
-        <v>46077.7375462963</v>
+        <v>46078.46899305555</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21863,7 +21872,7 @@
         <v>2</v>
       </c>
       <c r="N334" s="3" t="n">
-        <v>46077.72782407407</v>
+        <v>46078.48003472222</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21927,7 +21936,7 @@
         <v>2</v>
       </c>
       <c r="N335" s="3" t="n">
-        <v>46077.72697916667</v>
+        <v>46078.47496527778</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -21991,7 +22000,7 @@
         <v>1</v>
       </c>
       <c r="N336" s="3" t="n">
-        <v>46077.6835300926</v>
+        <v>46078.47752314815</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22055,7 +22064,7 @@
         <v>1</v>
       </c>
       <c r="N337" s="3" t="n">
-        <v>46077.72237268519</v>
+        <v>46078.48417824074</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22119,7 +22128,7 @@
         <v>2</v>
       </c>
       <c r="N338" s="3" t="n">
-        <v>46077.73020833333</v>
+        <v>46078.485</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -22375,7 +22384,7 @@
         <v>2</v>
       </c>
       <c r="N342" s="3" t="n">
-        <v>46077.56387731482</v>
+        <v>46078.46246527778</v>
       </c>
       <c r="O342" t="inlineStr">
         <is>
@@ -22394,11 +22403,6 @@
           <t>OPERACAO 9.1</t>
         </is>
       </c>
-      <c r="C343" t="inlineStr">
-        <is>
-          <t>10.69.5.237</t>
-        </is>
-      </c>
       <c r="D343" t="n">
         <v>2017</v>
       </c>
@@ -22441,7 +22445,7 @@
         </is>
       </c>
       <c r="N343" s="3" t="n">
-        <v>46077.7067824074</v>
+        <v>46078.47210648148</v>
       </c>
       <c r="O343" t="inlineStr">
         <is>
@@ -22697,7 +22701,7 @@
         <v>1</v>
       </c>
       <c r="N347" s="3" t="n">
-        <v>46077.50989583333</v>
+        <v>46078.47096064815</v>
       </c>
       <c r="O347" t="inlineStr">
         <is>
@@ -22758,10 +22762,10 @@
         </is>
       </c>
       <c r="M348" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N348" s="3" t="n">
-        <v>46077.57815972222</v>
+        <v>46078.47572916667</v>
       </c>
       <c r="O348" t="inlineStr">
         <is>
@@ -22825,7 +22829,7 @@
         <v>1</v>
       </c>
       <c r="N349" s="3" t="n">
-        <v>46077.57738425926</v>
+        <v>46078.48490740741</v>
       </c>
       <c r="O349" t="inlineStr">
         <is>
@@ -22884,7 +22888,7 @@
         <v>1</v>
       </c>
       <c r="N350" s="3" t="n">
-        <v>46077.6040625</v>
+        <v>46078.46881944445</v>
       </c>
       <c r="O350" t="inlineStr">
         <is>
@@ -22948,7 +22952,7 @@
         <v>1</v>
       </c>
       <c r="N351" s="3" t="n">
-        <v>46077.58238425926</v>
+        <v>46078.40324074074</v>
       </c>
       <c r="O351" t="inlineStr">
         <is>
@@ -23073,7 +23077,7 @@
         </is>
       </c>
       <c r="N353" s="3" t="n">
-        <v>46077.57596064815</v>
+        <v>46078.48393518518</v>
       </c>
       <c r="O353" t="inlineStr">
         <is>
@@ -23134,7 +23138,7 @@
         </is>
       </c>
       <c r="N354" s="3" t="n">
-        <v>46077.57831018518</v>
+        <v>46078.40594907408</v>
       </c>
       <c r="O354" t="inlineStr">
         <is>
@@ -23198,7 +23202,7 @@
         <v>1</v>
       </c>
       <c r="N355" s="3" t="n">
-        <v>46077.57148148148</v>
+        <v>46078.47880787037</v>
       </c>
       <c r="O355" t="inlineStr">
         <is>
@@ -23262,7 +23266,7 @@
         <v>1</v>
       </c>
       <c r="N356" s="3" t="n">
-        <v>46077.57331018519</v>
+        <v>46078.48070601852</v>
       </c>
       <c r="O356" t="inlineStr">
         <is>
@@ -23326,7 +23330,7 @@
         <v>1</v>
       </c>
       <c r="N357" s="3" t="n">
-        <v>46077.57607638889</v>
+        <v>46078.48508101852</v>
       </c>
       <c r="O357" t="inlineStr">
         <is>
@@ -23449,7 +23453,7 @@
         <v>2</v>
       </c>
       <c r="N359" s="3" t="n">
-        <v>46077.57711805555</v>
+        <v>46078.47711805555</v>
       </c>
       <c r="O359" t="inlineStr">
         <is>
@@ -23513,7 +23517,7 @@
         <v>2</v>
       </c>
       <c r="N360" s="3" t="n">
-        <v>46077.58222222222</v>
+        <v>46078.48373842592</v>
       </c>
       <c r="O360" t="inlineStr">
         <is>
@@ -23577,7 +23581,7 @@
         <v>1</v>
       </c>
       <c r="N361" s="3" t="n">
-        <v>46077.57768518518</v>
+        <v>46078.48011574074</v>
       </c>
       <c r="O361" t="inlineStr">
         <is>
@@ -23638,7 +23642,7 @@
         </is>
       </c>
       <c r="N362" s="3" t="n">
-        <v>46077.57978009259</v>
+        <v>46078.48282407408</v>
       </c>
       <c r="O362" t="inlineStr">
         <is>
@@ -23826,7 +23830,7 @@
         <v>1</v>
       </c>
       <c r="N365" s="3" t="n">
-        <v>46077.68586805555</v>
+        <v>46078.48314814815</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
@@ -23892,7 +23896,7 @@
         </is>
       </c>
       <c r="N366" s="3" t="n">
-        <v>46077.73435185185</v>
+        <v>46078.47699074074</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -24018,7 +24022,7 @@
         </is>
       </c>
       <c r="N368" s="3" t="n">
-        <v>46077.72487268518</v>
+        <v>46078.4771412037</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -24037,11 +24041,6 @@
           <t>RH</t>
         </is>
       </c>
-      <c r="C369" t="inlineStr">
-        <is>
-          <t>10.69.3.13</t>
-        </is>
-      </c>
       <c r="D369" t="n">
         <v>2025</v>
       </c>
@@ -24084,7 +24083,7 @@
         </is>
       </c>
       <c r="N369" s="3" t="n">
-        <v>46077.72804398148</v>
+        <v>46078.4762962963</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
@@ -24153,7 +24152,7 @@
         <v>1</v>
       </c>
       <c r="N370" s="3" t="n">
-        <v>46077.71864583333</v>
+        <v>46078.45079861111</v>
       </c>
       <c r="O370" t="inlineStr">
         <is>
@@ -24222,7 +24221,7 @@
         <v>1</v>
       </c>
       <c r="N371" s="3" t="n">
-        <v>46077.69305555556</v>
+        <v>46078.44900462963</v>
       </c>
       <c r="O371" t="inlineStr">
         <is>
@@ -24356,8 +24355,11 @@
           <t>HP ProDesk 400 G5 SFF (Brazil)</t>
         </is>
       </c>
+      <c r="M373" t="n">
+        <v>1</v>
+      </c>
       <c r="N373" s="3" t="n">
-        <v>46073.62837962963</v>
+        <v>46078.44162037037</v>
       </c>
       <c r="O373" t="inlineStr">
         <is>
@@ -24426,7 +24428,7 @@
         <v>1</v>
       </c>
       <c r="N374" s="3" t="n">
-        <v>46077.7084837963</v>
+        <v>46078.47106481482</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24492,7 +24494,7 @@
         </is>
       </c>
       <c r="N375" s="3" t="n">
-        <v>46077.7372800926</v>
+        <v>46078.46810185185</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
@@ -24511,11 +24513,6 @@
           <t>COORDENACAO</t>
         </is>
       </c>
-      <c r="C376" t="inlineStr">
-        <is>
-          <t>10.69.3.72</t>
-        </is>
-      </c>
       <c r="D376" t="n">
         <v>2025</v>
       </c>
@@ -24561,7 +24558,7 @@
         <v>1</v>
       </c>
       <c r="N376" s="3" t="n">
-        <v>46077.73570601852</v>
+        <v>46078.47907407407</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -24630,7 +24627,7 @@
         <v>2</v>
       </c>
       <c r="N377" s="3" t="n">
-        <v>46077.70633101852</v>
+        <v>46078.47793981482</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -24699,7 +24696,7 @@
         <v>2</v>
       </c>
       <c r="N378" s="3" t="n">
-        <v>46077.72825231482</v>
+        <v>46078.48601851852</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização automática 2026-02-25 13:52:03.849473
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>46078.48479166667</v>
+        <v>46078.56585648148</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>46078.4733912037</v>
+        <v>46078.5516087963</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
         <v>1</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>46078.45667824074</v>
+        <v>46078.53431712963</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>46078.45774305556</v>
+        <v>46078.53530092593</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -875,7 +875,7 @@
         <v>1</v>
       </c>
       <c r="N6" s="3" t="n">
-        <v>46077.77353009259</v>
+        <v>46078.54894675926</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -944,7 +944,7 @@
         <v>1</v>
       </c>
       <c r="N7" s="3" t="n">
-        <v>46077.76526620371</v>
+        <v>46078.55216435185</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -1072,7 +1072,7 @@
         <v>1</v>
       </c>
       <c r="N9" s="3" t="n">
-        <v>46077.73664351852</v>
+        <v>46078.54554398148</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -1131,7 +1131,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="3" t="n">
-        <v>46078.47103009259</v>
+        <v>46078.54422453704</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1259,7 +1259,7 @@
         <v>1</v>
       </c>
       <c r="N12" s="3" t="n">
-        <v>46077.6994675926</v>
+        <v>46078.54601851852</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1323,7 +1323,7 @@
         <v>1</v>
       </c>
       <c r="N13" s="3" t="n">
-        <v>46077.69547453704</v>
+        <v>46078.54613425926</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1387,7 +1387,7 @@
         <v>2</v>
       </c>
       <c r="N14" s="3" t="n">
-        <v>46077.69408564815</v>
+        <v>46078.54605324074</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1451,7 +1451,7 @@
         <v>1</v>
       </c>
       <c r="N15" s="3" t="n">
-        <v>46077.39167824074</v>
+        <v>46078.54996527778</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1515,7 +1515,7 @@
         <v>2</v>
       </c>
       <c r="N16" s="3" t="n">
-        <v>46077.72754629629</v>
+        <v>46078.54274305556</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1643,7 +1643,7 @@
         <v>2</v>
       </c>
       <c r="N18" s="3" t="n">
-        <v>46077.69524305555</v>
+        <v>46078.53900462963</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1768,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="N20" s="3" t="n">
-        <v>46077.69560185185</v>
+        <v>46078.54314814815</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1832,7 +1832,7 @@
         <v>1</v>
       </c>
       <c r="N21" s="3" t="n">
-        <v>46077.69509259259</v>
+        <v>46078.54496527778</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -2009,7 +2009,7 @@
         <v>1</v>
       </c>
       <c r="N24" s="3" t="n">
-        <v>46078.20137731481</v>
+        <v>46078.53980324074</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2183,7 +2183,7 @@
         <v>1</v>
       </c>
       <c r="N27" s="3" t="n">
-        <v>46077.73377314815</v>
+        <v>46078.53818287037</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2244,7 +2244,7 @@
         </is>
       </c>
       <c r="N28" s="3" t="n">
-        <v>46077.72322916667</v>
+        <v>46078.53824074074</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -6570,7 +6570,7 @@
         <v>1</v>
       </c>
       <c r="N95" s="3" t="n">
-        <v>46078.47793981482</v>
+        <v>46078.55678240741</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -6639,7 +6639,7 @@
         <v>1</v>
       </c>
       <c r="N96" s="3" t="n">
-        <v>46078.46424768519</v>
+        <v>46078.53973379629</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
@@ -6703,7 +6703,7 @@
         <v>1</v>
       </c>
       <c r="N97" s="3" t="n">
-        <v>46078.46658564815</v>
+        <v>46078.54201388889</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -6767,7 +6767,7 @@
         <v>1</v>
       </c>
       <c r="N98" s="3" t="n">
-        <v>46078.48465277778</v>
+        <v>46078.56221064815</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -6836,7 +6836,7 @@
         <v>1</v>
       </c>
       <c r="N99" s="3" t="n">
-        <v>46078.46572916667</v>
+        <v>46078.54172453703</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -6905,7 +6905,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>46078.48517361111</v>
+        <v>46078.56525462963</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6974,7 +6974,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="3" t="n">
-        <v>46078.46268518519</v>
+        <v>46078.53958333333</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -7112,7 +7112,7 @@
         <v>2</v>
       </c>
       <c r="N103" s="3" t="n">
-        <v>46078.46942129629</v>
+        <v>46078.54878472222</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7238,8 +7238,11 @@
           <t>HP ProBook 440 14 inch G9 Notebook PC</t>
         </is>
       </c>
+      <c r="M105" t="n">
+        <v>1</v>
+      </c>
       <c r="N105" s="3" t="n">
-        <v>46078.45886574074</v>
+        <v>46078.56394675926</v>
       </c>
       <c r="O105" t="inlineStr">
         <is>
@@ -7369,7 +7372,7 @@
         <v>1</v>
       </c>
       <c r="N107" s="3" t="n">
-        <v>46078.46722222222</v>
+        <v>46078.55010416666</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -7507,7 +7510,7 @@
         <v>1</v>
       </c>
       <c r="N109" s="3" t="n">
-        <v>46078.4555787037</v>
+        <v>46078.5356712963</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7576,7 +7579,7 @@
         <v>2</v>
       </c>
       <c r="N110" s="3" t="n">
-        <v>46078.46891203704</v>
+        <v>46078.55113425926</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7645,7 +7648,7 @@
         <v>2</v>
       </c>
       <c r="N111" s="3" t="n">
-        <v>46078.46814814815</v>
+        <v>46078.54837962963</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
@@ -7714,7 +7717,7 @@
         <v>2</v>
       </c>
       <c r="N112" s="3" t="n">
-        <v>46078.48305555555</v>
+        <v>46078.566875</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7783,7 +7786,7 @@
         <v>1</v>
       </c>
       <c r="N113" s="3" t="n">
-        <v>46078.47728009259</v>
+        <v>46078.55446759259</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7852,7 +7855,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>46078.4730787037</v>
+        <v>46078.54967592593</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -7918,7 +7921,7 @@
         </is>
       </c>
       <c r="N115" s="3" t="n">
-        <v>46078.48471064815</v>
+        <v>46078.56825231481</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -7987,7 +7990,7 @@
         <v>1</v>
       </c>
       <c r="N116" s="3" t="n">
-        <v>46078.48628472222</v>
+        <v>46078.56302083333</v>
       </c>
       <c r="O116" t="inlineStr">
         <is>
@@ -8006,11 +8009,6 @@
           <t>DP</t>
         </is>
       </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>10.69.3.23</t>
-        </is>
-      </c>
       <c r="D117" t="n">
         <v>2025</v>
       </c>
@@ -8056,7 +8054,7 @@
         <v>1</v>
       </c>
       <c r="N117" s="3" t="n">
-        <v>46078.48497685185</v>
+        <v>46078.55758101852</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -8122,7 +8120,7 @@
         </is>
       </c>
       <c r="N118" s="3" t="n">
-        <v>46078.46006944445</v>
+        <v>46078.57021990741</v>
       </c>
       <c r="O118" t="inlineStr">
         <is>
@@ -8260,7 +8258,7 @@
         <v>1</v>
       </c>
       <c r="N120" s="3" t="n">
-        <v>46078.46357638889</v>
+        <v>46078.54679398148</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -8329,7 +8327,7 @@
         <v>1</v>
       </c>
       <c r="N121" s="3" t="n">
-        <v>46078.46646990741</v>
+        <v>46078.5425925926</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -8395,7 +8393,7 @@
         </is>
       </c>
       <c r="N122" s="3" t="n">
-        <v>46078.48327546296</v>
+        <v>46078.55806712963</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -8464,7 +8462,7 @@
         <v>2</v>
       </c>
       <c r="N123" s="3" t="n">
-        <v>46078.47386574074</v>
+        <v>46078.55454861111</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -8533,7 +8531,7 @@
         <v>1</v>
       </c>
       <c r="N124" s="3" t="n">
-        <v>46078.47922453703</v>
+        <v>46078.55518518519</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -8602,7 +8600,7 @@
         <v>1</v>
       </c>
       <c r="N125" s="3" t="n">
-        <v>46078.45295138889</v>
+        <v>46078.56849537037</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -8671,7 +8669,7 @@
         <v>2</v>
       </c>
       <c r="N126" s="3" t="n">
-        <v>46078.46078703704</v>
+        <v>46078.53763888889</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -8740,7 +8738,7 @@
         <v>2</v>
       </c>
       <c r="N127" s="3" t="n">
-        <v>46078.46689814814</v>
+        <v>46078.54917824074</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -8809,7 +8807,7 @@
         <v>1</v>
       </c>
       <c r="N128" s="3" t="n">
-        <v>46078.47548611111</v>
+        <v>46078.55079861111</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -8878,7 +8876,7 @@
         <v>1</v>
       </c>
       <c r="N129" s="3" t="n">
-        <v>46078.48148148148</v>
+        <v>46078.56065972222</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -8947,7 +8945,7 @@
         <v>1</v>
       </c>
       <c r="N130" s="3" t="n">
-        <v>46078.45804398148</v>
+        <v>46078.53596064815</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -9016,7 +9014,7 @@
         <v>1</v>
       </c>
       <c r="N131" s="3" t="n">
-        <v>46078.48592592592</v>
+        <v>46078.56835648148</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -9149,7 +9147,7 @@
         <v>1</v>
       </c>
       <c r="N133" s="3" t="n">
-        <v>46078.45733796297</v>
+        <v>46078.56908564815</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -9465,7 +9463,7 @@
         <v>1</v>
       </c>
       <c r="N138" s="3" t="n">
-        <v>46078.44731481482</v>
+        <v>46078.56310185185</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9529,7 +9527,7 @@
         <v>1</v>
       </c>
       <c r="N139" s="3" t="n">
-        <v>46078.46912037037</v>
+        <v>46078.54238425926</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9593,7 +9591,7 @@
         <v>1</v>
       </c>
       <c r="N140" s="3" t="n">
-        <v>46078.45165509259</v>
+        <v>46078.56890046296</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9654,10 +9652,10 @@
         </is>
       </c>
       <c r="M141" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N141" s="3" t="n">
-        <v>46078.46081018518</v>
+        <v>46078.54099537037</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9721,7 +9719,7 @@
         <v>1</v>
       </c>
       <c r="N142" s="3" t="n">
-        <v>46078.45163194444</v>
+        <v>46078.5663425926</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9785,7 +9783,7 @@
         <v>1</v>
       </c>
       <c r="N143" s="3" t="n">
-        <v>46078.47792824074</v>
+        <v>46078.54859953704</v>
       </c>
       <c r="O143" t="inlineStr">
         <is>
@@ -9849,7 +9847,7 @@
         <v>1</v>
       </c>
       <c r="N144" s="3" t="n">
-        <v>46078.45966435185</v>
+        <v>46078.53967592592</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9913,7 +9911,7 @@
         <v>1</v>
       </c>
       <c r="N145" s="3" t="n">
-        <v>46078.46798611111</v>
+        <v>46078.5425925926</v>
       </c>
       <c r="O145" t="inlineStr">
         <is>
@@ -9977,7 +9975,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="3" t="n">
-        <v>46078.48679398148</v>
+        <v>46078.56262731482</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10041,7 +10039,7 @@
         <v>1</v>
       </c>
       <c r="N147" s="3" t="n">
-        <v>46078.47673611111</v>
+        <v>46078.54922453704</v>
       </c>
       <c r="O147" t="inlineStr">
         <is>
@@ -10105,7 +10103,7 @@
         <v>1</v>
       </c>
       <c r="N148" s="3" t="n">
-        <v>46078.45818287037</v>
+        <v>46078.56696759259</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10169,7 +10167,7 @@
         <v>1</v>
       </c>
       <c r="N149" s="3" t="n">
-        <v>46078.48717592593</v>
+        <v>46078.56865740741</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -10233,7 +10231,7 @@
         <v>1</v>
       </c>
       <c r="N150" s="3" t="n">
-        <v>46078.47556712963</v>
+        <v>46078.55412037037</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -10425,7 +10423,7 @@
         <v>1</v>
       </c>
       <c r="N153" s="3" t="n">
-        <v>46078.48524305555</v>
+        <v>46078.56505787037</v>
       </c>
       <c r="O153" t="inlineStr">
         <is>
@@ -10489,7 +10487,7 @@
         <v>1</v>
       </c>
       <c r="N154" s="3" t="n">
-        <v>46078.45193287037</v>
+        <v>46078.56493055556</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10553,7 +10551,7 @@
         <v>1</v>
       </c>
       <c r="N155" s="3" t="n">
-        <v>46078.44721064815</v>
+        <v>46078.56486111111</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10617,7 +10615,7 @@
         <v>1</v>
       </c>
       <c r="N156" s="3" t="n">
-        <v>46078.46853009259</v>
+        <v>46078.54244212963</v>
       </c>
       <c r="O156" t="inlineStr">
         <is>
@@ -10681,7 +10679,7 @@
         <v>1</v>
       </c>
       <c r="N157" s="3" t="n">
-        <v>46078.45967592593</v>
+        <v>46078.53774305555</v>
       </c>
       <c r="O157" t="inlineStr">
         <is>
@@ -10745,7 +10743,7 @@
         <v>1</v>
       </c>
       <c r="N158" s="3" t="n">
-        <v>46078.4849537037</v>
+        <v>46078.56077546296</v>
       </c>
       <c r="O158" t="inlineStr">
         <is>
@@ -10809,7 +10807,7 @@
         <v>1</v>
       </c>
       <c r="N159" s="3" t="n">
-        <v>46078.4753125</v>
+        <v>46078.55532407408</v>
       </c>
       <c r="O159" t="inlineStr">
         <is>
@@ -10873,7 +10871,7 @@
         <v>1</v>
       </c>
       <c r="N160" s="3" t="n">
-        <v>46078.45277777778</v>
+        <v>46078.56958333333</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
@@ -10937,7 +10935,7 @@
         <v>1</v>
       </c>
       <c r="N161" s="3" t="n">
-        <v>46078.45211805555</v>
+        <v>46078.53363425926</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -11001,7 +10999,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="3" t="n">
-        <v>46078.47810185186</v>
+        <v>46078.55699074074</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11062,10 +11060,10 @@
         </is>
       </c>
       <c r="M163" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N163" s="3" t="n">
-        <v>46051.66149305556</v>
+        <v>46078.50972222222</v>
       </c>
       <c r="O163" t="inlineStr">
         <is>
@@ -11129,7 +11127,7 @@
         <v>2</v>
       </c>
       <c r="N164" s="3" t="n">
-        <v>46078.47390046297</v>
+        <v>46078.54511574074</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11193,7 +11191,7 @@
         <v>2</v>
       </c>
       <c r="N165" s="3" t="n">
-        <v>46078.44908564815</v>
+        <v>46078.5657175926</v>
       </c>
       <c r="O165" t="inlineStr">
         <is>
@@ -11257,7 +11255,7 @@
         <v>2</v>
       </c>
       <c r="N166" s="3" t="n">
-        <v>46078.44902777778</v>
+        <v>46078.56887731481</v>
       </c>
       <c r="O166" t="inlineStr">
         <is>
@@ -11321,7 +11319,7 @@
         <v>2</v>
       </c>
       <c r="N167" s="3" t="n">
-        <v>46078.48438657408</v>
+        <v>46078.56487268519</v>
       </c>
       <c r="O167" t="inlineStr">
         <is>
@@ -11385,7 +11383,7 @@
         <v>2</v>
       </c>
       <c r="N168" s="3" t="n">
-        <v>46078.47186342593</v>
+        <v>46078.54982638889</v>
       </c>
       <c r="O168" t="inlineStr">
         <is>
@@ -11449,7 +11447,7 @@
         <v>2</v>
       </c>
       <c r="N169" s="3" t="n">
-        <v>46078.48221064815</v>
+        <v>46078.56100694444</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -11513,7 +11511,7 @@
         <v>2</v>
       </c>
       <c r="N170" s="3" t="n">
-        <v>46078.48496527778</v>
+        <v>46078.56444444445</v>
       </c>
       <c r="O170" t="inlineStr">
         <is>
@@ -11577,7 +11575,7 @@
         <v>1</v>
       </c>
       <c r="N171" s="3" t="n">
-        <v>46078.46061342592</v>
+        <v>46078.53545138889</v>
       </c>
       <c r="O171" t="inlineStr">
         <is>
@@ -11641,7 +11639,7 @@
         <v>2</v>
       </c>
       <c r="N172" s="3" t="n">
-        <v>46077.76346064815</v>
+        <v>46078.54083333333</v>
       </c>
       <c r="O172" t="inlineStr">
         <is>
@@ -11705,7 +11703,7 @@
         <v>2</v>
       </c>
       <c r="N173" s="3" t="n">
-        <v>46078.48421296296</v>
+        <v>46078.56283564815</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -11769,7 +11767,7 @@
         <v>2</v>
       </c>
       <c r="N174" s="3" t="n">
-        <v>46078.47538194444</v>
+        <v>46078.55256944444</v>
       </c>
       <c r="O174" t="inlineStr">
         <is>
@@ -11833,7 +11831,7 @@
         <v>2</v>
       </c>
       <c r="N175" s="3" t="n">
-        <v>46078.45765046297</v>
+        <v>46078.53097222222</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -11897,7 +11895,7 @@
         <v>2</v>
       </c>
       <c r="N176" s="3" t="n">
-        <v>46078.46560185185</v>
+        <v>46078.54165509259</v>
       </c>
       <c r="O176" t="inlineStr">
         <is>
@@ -11961,7 +11959,7 @@
         <v>2</v>
       </c>
       <c r="N177" s="3" t="n">
-        <v>46078.46690972222</v>
+        <v>46078.54300925926</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
@@ -12025,7 +12023,7 @@
         <v>2</v>
       </c>
       <c r="N178" s="3" t="n">
-        <v>46078.47993055556</v>
+        <v>46078.56019675926</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12089,7 +12087,7 @@
         <v>1</v>
       </c>
       <c r="N179" s="3" t="n">
-        <v>46078.47502314814</v>
+        <v>46078.5508912037</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12153,7 +12151,7 @@
         <v>1</v>
       </c>
       <c r="N180" s="3" t="n">
-        <v>46078.46925925926</v>
+        <v>46078.54559027778</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12217,7 +12215,7 @@
         <v>1</v>
       </c>
       <c r="N181" s="3" t="n">
-        <v>46078.48498842592</v>
+        <v>46078.56280092592</v>
       </c>
       <c r="O181" t="inlineStr">
         <is>
@@ -12606,7 +12604,7 @@
         <v>1</v>
       </c>
       <c r="N187" s="3" t="n">
-        <v>46078.46965277778</v>
+        <v>46078.54868055556</v>
       </c>
       <c r="O187" t="inlineStr">
         <is>
@@ -12670,7 +12668,7 @@
         <v>1</v>
       </c>
       <c r="N188" s="3" t="n">
-        <v>46078.48660879629</v>
+        <v>46078.55351851852</v>
       </c>
       <c r="O188" t="inlineStr">
         <is>
@@ -12756,11 +12754,6 @@
           <t>OPERACAO 8.1</t>
         </is>
       </c>
-      <c r="C190" t="inlineStr">
-        <is>
-          <t>10.69.5.59</t>
-        </is>
-      </c>
       <c r="D190" t="n">
         <v>2015</v>
       </c>
@@ -12798,7 +12791,7 @@
         </is>
       </c>
       <c r="N190" s="3" t="n">
-        <v>46078.46982638889</v>
+        <v>46078.54487268518</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12926,7 +12919,7 @@
         <v>1</v>
       </c>
       <c r="N192" s="3" t="n">
-        <v>46078.47851851852</v>
+        <v>46078.55626157407</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -13051,7 +13044,7 @@
         <v>2</v>
       </c>
       <c r="N194" s="3" t="n">
-        <v>46078.48105324074</v>
+        <v>46078.5587037037</v>
       </c>
       <c r="O194" t="inlineStr">
         <is>
@@ -13115,7 +13108,7 @@
         <v>1</v>
       </c>
       <c r="N195" s="3" t="n">
-        <v>46078.46210648148</v>
+        <v>46078.54197916666</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13307,7 +13300,7 @@
         <v>1</v>
       </c>
       <c r="N198" s="3" t="n">
-        <v>46078.47444444444</v>
+        <v>46078.55230324074</v>
       </c>
       <c r="O198" t="inlineStr">
         <is>
@@ -13496,7 +13489,7 @@
         </is>
       </c>
       <c r="N201" s="3" t="n">
-        <v>46078.46471064815</v>
+        <v>46078.54787037037</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -13560,7 +13553,7 @@
         <v>1</v>
       </c>
       <c r="N202" s="3" t="n">
-        <v>46078.45842592593</v>
+        <v>46078.53300925926</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13624,7 +13617,7 @@
         <v>1</v>
       </c>
       <c r="N203" s="3" t="n">
-        <v>46078.45521990741</v>
+        <v>46078.5375462963</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13688,7 +13681,7 @@
         <v>1</v>
       </c>
       <c r="N204" s="3" t="n">
-        <v>46078.45334490741</v>
+        <v>46078.53262731482</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13752,7 +13745,7 @@
         <v>1</v>
       </c>
       <c r="N205" s="3" t="n">
-        <v>46078.4728587963</v>
+        <v>46078.55136574074</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13880,7 +13873,7 @@
         <v>1</v>
       </c>
       <c r="N207" s="3" t="n">
-        <v>46078.45667824074</v>
+        <v>46078.52907407407</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -13944,7 +13937,7 @@
         <v>1</v>
       </c>
       <c r="N208" s="3" t="n">
-        <v>46078.45357638889</v>
+        <v>46078.56446759259</v>
       </c>
       <c r="O208" t="inlineStr">
         <is>
@@ -14008,7 +14001,7 @@
         <v>1</v>
       </c>
       <c r="N209" s="3" t="n">
-        <v>46078.47603009259</v>
+        <v>46078.55226851852</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14072,7 +14065,7 @@
         <v>1</v>
       </c>
       <c r="N210" s="3" t="n">
-        <v>46078.48771990741</v>
+        <v>46078.5666550926</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14136,7 +14129,7 @@
         <v>1</v>
       </c>
       <c r="N211" s="3" t="n">
-        <v>46078.45149305555</v>
+        <v>46078.56876157408</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -14200,7 +14193,7 @@
         <v>1</v>
       </c>
       <c r="N212" s="3" t="n">
-        <v>46078.45365740741</v>
+        <v>46078.56939814815</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -14264,7 +14257,7 @@
         <v>1</v>
       </c>
       <c r="N213" s="3" t="n">
-        <v>46078.47652777778</v>
+        <v>46078.55322916667</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
@@ -14456,7 +14449,7 @@
         <v>1</v>
       </c>
       <c r="N216" s="3" t="n">
-        <v>46078.48261574074</v>
+        <v>46078.54422453704</v>
       </c>
       <c r="O216" t="inlineStr">
         <is>
@@ -14515,7 +14508,7 @@
         <v>1</v>
       </c>
       <c r="N217" s="3" t="n">
-        <v>46078.45222222222</v>
+        <v>46078.53479166667</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14579,7 +14572,7 @@
         <v>1</v>
       </c>
       <c r="N218" s="3" t="n">
-        <v>46078.48447916667</v>
+        <v>46078.55929398148</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14776,7 +14769,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="3" t="n">
-        <v>46078.45928240741</v>
+        <v>46078.53570601852</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14840,7 +14833,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="3" t="n">
-        <v>46078.466875</v>
+        <v>46078.5409375</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -14904,7 +14897,7 @@
         <v>1</v>
       </c>
       <c r="N223" s="3" t="n">
-        <v>46078.45415509259</v>
+        <v>46078.56770833334</v>
       </c>
       <c r="O223" t="inlineStr">
         <is>
@@ -14968,7 +14961,7 @@
         <v>1</v>
       </c>
       <c r="N224" s="3" t="n">
-        <v>46078.47532407408</v>
+        <v>46078.55299768518</v>
       </c>
       <c r="O224" t="inlineStr">
         <is>
@@ -15032,7 +15025,7 @@
         <v>1</v>
       </c>
       <c r="N225" s="3" t="n">
-        <v>46078.47582175926</v>
+        <v>46078.55334490741</v>
       </c>
       <c r="O225" t="inlineStr">
         <is>
@@ -15096,7 +15089,7 @@
         <v>1</v>
       </c>
       <c r="N226" s="3" t="n">
-        <v>46078.48530092592</v>
+        <v>46078.55998842593</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15160,7 +15153,7 @@
         <v>1</v>
       </c>
       <c r="N227" s="3" t="n">
-        <v>46078.46837962963</v>
+        <v>46078.54892361111</v>
       </c>
       <c r="O227" t="inlineStr">
         <is>
@@ -15224,7 +15217,7 @@
         <v>1</v>
       </c>
       <c r="N228" s="3" t="n">
-        <v>46078.47028935186</v>
+        <v>46078.54648148148</v>
       </c>
       <c r="O228" t="inlineStr">
         <is>
@@ -15288,7 +15281,7 @@
         <v>1</v>
       </c>
       <c r="N229" s="3" t="n">
-        <v>46078.45387731482</v>
+        <v>46078.53190972222</v>
       </c>
       <c r="O229" t="inlineStr">
         <is>
@@ -15352,7 +15345,7 @@
         <v>1</v>
       </c>
       <c r="N230" s="3" t="n">
-        <v>46078.4618287037</v>
+        <v>46078.54291666667</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15416,7 +15409,7 @@
         <v>1</v>
       </c>
       <c r="N231" s="3" t="n">
-        <v>46078.48357638889</v>
+        <v>46078.56234953704</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15480,7 +15473,7 @@
         <v>1</v>
       </c>
       <c r="N232" s="3" t="n">
-        <v>46078.47865740741</v>
+        <v>46078.5521875</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -15544,7 +15537,7 @@
         <v>1</v>
       </c>
       <c r="N233" s="3" t="n">
-        <v>46078.45724537037</v>
+        <v>46078.5418287037</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15608,7 +15601,7 @@
         <v>1</v>
       </c>
       <c r="N234" s="3" t="n">
-        <v>46078.44936342593</v>
+        <v>46078.56962962963</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -15672,7 +15665,7 @@
         <v>1</v>
       </c>
       <c r="N235" s="3" t="n">
-        <v>46078.4497337963</v>
+        <v>46078.56435185186</v>
       </c>
       <c r="O235" t="inlineStr">
         <is>
@@ -15736,7 +15729,7 @@
         <v>1</v>
       </c>
       <c r="N236" s="3" t="n">
-        <v>46078.48525462963</v>
+        <v>46078.56503472223</v>
       </c>
       <c r="O236" t="inlineStr">
         <is>
@@ -15864,7 +15857,7 @@
         <v>1</v>
       </c>
       <c r="N238" s="3" t="n">
-        <v>46078.48001157407</v>
+        <v>46078.55677083333</v>
       </c>
       <c r="O238" t="inlineStr">
         <is>
@@ -15928,7 +15921,7 @@
         <v>1</v>
       </c>
       <c r="N239" s="3" t="n">
-        <v>46078.48751157407</v>
+        <v>46078.5664699074</v>
       </c>
       <c r="O239" t="inlineStr">
         <is>
@@ -15992,7 +15985,7 @@
         <v>1</v>
       </c>
       <c r="N240" s="3" t="n">
-        <v>46078.4744212963</v>
+        <v>46078.55107638889</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16056,7 +16049,7 @@
         <v>1</v>
       </c>
       <c r="N241" s="3" t="n">
-        <v>46078.47614583333</v>
+        <v>46078.55320601852</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16120,7 +16113,7 @@
         <v>1</v>
       </c>
       <c r="N242" s="3" t="n">
-        <v>46078.47881944444</v>
+        <v>46078.55567129629</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16307,7 +16300,7 @@
         <v>1</v>
       </c>
       <c r="N245" s="3" t="n">
-        <v>46078.45295138889</v>
+        <v>46078.53224537037</v>
       </c>
       <c r="O245" t="inlineStr">
         <is>
@@ -16371,7 +16364,7 @@
         <v>1</v>
       </c>
       <c r="N246" s="3" t="n">
-        <v>46078.45226851852</v>
+        <v>46078.56759259259</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16435,7 +16428,7 @@
         <v>1</v>
       </c>
       <c r="N247" s="3" t="n">
-        <v>46078.47230324074</v>
+        <v>46078.55452546296</v>
       </c>
       <c r="O247" t="inlineStr">
         <is>
@@ -16499,7 +16492,7 @@
         <v>1</v>
       </c>
       <c r="N248" s="3" t="n">
-        <v>46078.45214120371</v>
+        <v>46078.56932870371</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16563,7 +16556,7 @@
         <v>1</v>
       </c>
       <c r="N249" s="3" t="n">
-        <v>46078.47575231481</v>
+        <v>46078.54880787037</v>
       </c>
       <c r="O249" t="inlineStr">
         <is>
@@ -16627,7 +16620,7 @@
         <v>1</v>
       </c>
       <c r="N250" s="3" t="n">
-        <v>46078.48413194445</v>
+        <v>46078.56059027778</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16691,7 +16684,7 @@
         <v>1</v>
       </c>
       <c r="N251" s="3" t="n">
-        <v>46078.48716435185</v>
+        <v>46078.56376157407</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16755,7 +16748,7 @@
         <v>1</v>
       </c>
       <c r="N252" s="3" t="n">
-        <v>46078.45513888889</v>
+        <v>46078.53275462963</v>
       </c>
       <c r="O252" t="inlineStr">
         <is>
@@ -16819,7 +16812,7 @@
         <v>1</v>
       </c>
       <c r="N253" s="3" t="n">
-        <v>46078.47984953703</v>
+        <v>46078.55461805555</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16877,7 +16870,7 @@
         <v>1</v>
       </c>
       <c r="N254" s="3" t="n">
-        <v>46078.45273148148</v>
+        <v>46078.56100694444</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -16941,7 +16934,7 @@
         <v>1</v>
       </c>
       <c r="N255" s="3" t="n">
-        <v>46078.48706018519</v>
+        <v>46078.56243055555</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -17005,7 +16998,7 @@
         <v>1</v>
       </c>
       <c r="N256" s="3" t="n">
-        <v>46078.4521875</v>
+        <v>46078.57001157408</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17069,7 +17062,7 @@
         <v>1</v>
       </c>
       <c r="N257" s="3" t="n">
-        <v>46078.44929398148</v>
+        <v>46078.56605324074</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17133,7 +17126,7 @@
         <v>1</v>
       </c>
       <c r="N258" s="3" t="n">
-        <v>46078.48373842592</v>
+        <v>46078.5575462963</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
@@ -17197,7 +17190,7 @@
         <v>1</v>
       </c>
       <c r="N259" s="3" t="n">
-        <v>46078.48795138889</v>
+        <v>46078.56502314815</v>
       </c>
       <c r="O259" t="inlineStr">
         <is>
@@ -17261,7 +17254,7 @@
         <v>1</v>
       </c>
       <c r="N260" s="3" t="n">
-        <v>46078.45258101852</v>
+        <v>46078.57061342592</v>
       </c>
       <c r="O260" t="inlineStr">
         <is>
@@ -17325,7 +17318,7 @@
         <v>1</v>
       </c>
       <c r="N261" s="3" t="n">
-        <v>46078.48232638889</v>
+        <v>46078.56122685185</v>
       </c>
       <c r="O261" t="inlineStr">
         <is>
@@ -17389,7 +17382,7 @@
         <v>1</v>
       </c>
       <c r="N262" s="3" t="n">
-        <v>46078.45458333333</v>
+        <v>46078.53269675926</v>
       </c>
       <c r="O262" t="inlineStr">
         <is>
@@ -17453,7 +17446,7 @@
         <v>1</v>
       </c>
       <c r="N263" s="3" t="n">
-        <v>46078.46046296296</v>
+        <v>46078.53876157408</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17517,7 +17510,7 @@
         <v>1</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>46078.45185185185</v>
+        <v>46078.5659375</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17581,7 +17574,7 @@
         <v>1</v>
       </c>
       <c r="N265" s="3" t="n">
-        <v>46078.48126157407</v>
+        <v>46078.55936342593</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17645,7 +17638,7 @@
         <v>1</v>
       </c>
       <c r="N266" s="3" t="n">
-        <v>46078.46108796296</v>
+        <v>46078.5350462963</v>
       </c>
       <c r="O266" t="inlineStr">
         <is>
@@ -17709,7 +17702,7 @@
         <v>1</v>
       </c>
       <c r="N267" s="3" t="n">
-        <v>46078.45009259259</v>
+        <v>46078.56815972222</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17773,7 +17766,7 @@
         <v>1</v>
       </c>
       <c r="N268" s="3" t="n">
-        <v>46078.45643518519</v>
+        <v>46078.53659722222</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17837,7 +17830,7 @@
         <v>1</v>
       </c>
       <c r="N269" s="3" t="n">
-        <v>46078.4708912037</v>
+        <v>46078.54856481482</v>
       </c>
       <c r="O269" t="inlineStr">
         <is>
@@ -17898,7 +17891,7 @@
         </is>
       </c>
       <c r="N270" s="3" t="n">
-        <v>46078.47869212963</v>
+        <v>46078.56079861111</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -18026,7 +18019,7 @@
         <v>1</v>
       </c>
       <c r="N272" s="3" t="n">
-        <v>46078.45087962963</v>
+        <v>46078.57111111111</v>
       </c>
       <c r="O272" t="inlineStr">
         <is>
@@ -18410,7 +18403,7 @@
         <v>1</v>
       </c>
       <c r="N278" s="3" t="n">
-        <v>46078.45108796296</v>
+        <v>46078.57021990741</v>
       </c>
       <c r="O278" t="inlineStr">
         <is>
@@ -18474,7 +18467,7 @@
         <v>1</v>
       </c>
       <c r="N279" s="3" t="n">
-        <v>46078.47736111111</v>
+        <v>46078.55523148148</v>
       </c>
       <c r="O279" t="inlineStr">
         <is>
@@ -18538,7 +18531,7 @@
         <v>1</v>
       </c>
       <c r="N280" s="3" t="n">
-        <v>46078.45782407407</v>
+        <v>46078.54112268519</v>
       </c>
       <c r="O280" t="inlineStr">
         <is>
@@ -18602,7 +18595,7 @@
         <v>1</v>
       </c>
       <c r="N281" s="3" t="n">
-        <v>46078.4841087963</v>
+        <v>46078.565625</v>
       </c>
       <c r="O281" t="inlineStr">
         <is>
@@ -18661,7 +18654,7 @@
         <v>1</v>
       </c>
       <c r="N282" s="3" t="n">
-        <v>46078.47760416667</v>
+        <v>46078.55240740741</v>
       </c>
       <c r="O282" t="inlineStr">
         <is>
@@ -18725,7 +18718,7 @@
         <v>1</v>
       </c>
       <c r="N283" s="3" t="n">
-        <v>46078.4549537037</v>
+        <v>46078.56862268518</v>
       </c>
       <c r="O283" t="inlineStr">
         <is>
@@ -18789,7 +18782,7 @@
         <v>1</v>
       </c>
       <c r="N284" s="3" t="n">
-        <v>46078.47991898148</v>
+        <v>46078.56114583334</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18853,7 +18846,7 @@
         <v>1</v>
       </c>
       <c r="N285" s="3" t="n">
-        <v>46078.45111111111</v>
+        <v>46078.56429398148</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -18917,7 +18910,7 @@
         <v>1</v>
       </c>
       <c r="N286" s="3" t="n">
-        <v>46078.48677083333</v>
+        <v>46078.56862268518</v>
       </c>
       <c r="O286" t="inlineStr">
         <is>
@@ -18981,7 +18974,7 @@
         <v>1</v>
       </c>
       <c r="N287" s="3" t="n">
-        <v>46078.46034722222</v>
+        <v>46078.56967592592</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
@@ -19045,7 +19038,7 @@
         <v>1</v>
       </c>
       <c r="N288" s="3" t="n">
-        <v>46078.48518518519</v>
+        <v>46078.56586805556</v>
       </c>
       <c r="O288" t="inlineStr">
         <is>
@@ -19109,7 +19102,7 @@
         <v>1</v>
       </c>
       <c r="N289" s="3" t="n">
-        <v>46078.45756944444</v>
+        <v>46078.53180555555</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -19903,7 +19896,7 @@
         <v>1</v>
       </c>
       <c r="N302" s="3" t="n">
-        <v>46078.48150462963</v>
+        <v>46078.55847222222</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -20644,7 +20637,7 @@
         </is>
       </c>
       <c r="N314" s="3" t="n">
-        <v>46078.4800925926</v>
+        <v>46078.55743055556</v>
       </c>
       <c r="O314" t="inlineStr">
         <is>
@@ -21019,7 +21012,7 @@
         </is>
       </c>
       <c r="N320" s="3" t="n">
-        <v>46078.46047453704</v>
+        <v>46078.53989583333</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21744,7 +21737,7 @@
         <v>1</v>
       </c>
       <c r="N332" s="3" t="n">
-        <v>46078.46850694445</v>
+        <v>46078.54989583333</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21808,7 +21801,7 @@
         <v>2</v>
       </c>
       <c r="N333" s="3" t="n">
-        <v>46078.46899305555</v>
+        <v>46078.5433912037</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21872,7 +21865,7 @@
         <v>2</v>
       </c>
       <c r="N334" s="3" t="n">
-        <v>46078.48003472222</v>
+        <v>46078.56039351852</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21936,7 +21929,7 @@
         <v>2</v>
       </c>
       <c r="N335" s="3" t="n">
-        <v>46078.47496527778</v>
+        <v>46078.55385416667</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -22000,7 +21993,7 @@
         <v>1</v>
       </c>
       <c r="N336" s="3" t="n">
-        <v>46078.47752314815</v>
+        <v>46078.55247685185</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22064,7 +22057,7 @@
         <v>1</v>
       </c>
       <c r="N337" s="3" t="n">
-        <v>46078.48417824074</v>
+        <v>46078.56362268519</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22128,7 +22121,7 @@
         <v>2</v>
       </c>
       <c r="N338" s="3" t="n">
-        <v>46078.485</v>
+        <v>46078.56516203703</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -22192,7 +22185,7 @@
         <v>2</v>
       </c>
       <c r="N339" s="3" t="n">
-        <v>46073.55048611111</v>
+        <v>46078.56081018518</v>
       </c>
       <c r="O339" t="inlineStr">
         <is>
@@ -22320,7 +22313,7 @@
         <v>2</v>
       </c>
       <c r="N341" s="3" t="n">
-        <v>46077.57143518519</v>
+        <v>46078.56283564815</v>
       </c>
       <c r="O341" t="inlineStr">
         <is>
@@ -22384,7 +22377,7 @@
         <v>2</v>
       </c>
       <c r="N342" s="3" t="n">
-        <v>46078.46246527778</v>
+        <v>46078.54081018519</v>
       </c>
       <c r="O342" t="inlineStr">
         <is>
@@ -22445,7 +22438,7 @@
         </is>
       </c>
       <c r="N343" s="3" t="n">
-        <v>46078.47210648148</v>
+        <v>46078.55253472222</v>
       </c>
       <c r="O343" t="inlineStr">
         <is>
@@ -22701,7 +22694,7 @@
         <v>1</v>
       </c>
       <c r="N347" s="3" t="n">
-        <v>46078.47096064815</v>
+        <v>46078.55133101852</v>
       </c>
       <c r="O347" t="inlineStr">
         <is>
@@ -22765,7 +22758,7 @@
         <v>1</v>
       </c>
       <c r="N348" s="3" t="n">
-        <v>46078.47572916667</v>
+        <v>46078.55825231481</v>
       </c>
       <c r="O348" t="inlineStr">
         <is>
@@ -22829,7 +22822,7 @@
         <v>1</v>
       </c>
       <c r="N349" s="3" t="n">
-        <v>46078.48490740741</v>
+        <v>46078.56190972222</v>
       </c>
       <c r="O349" t="inlineStr">
         <is>
@@ -22848,6 +22841,11 @@
           <t>OPERACAO 9.1</t>
         </is>
       </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>10.69.5.244</t>
+        </is>
+      </c>
       <c r="D350" t="n">
         <v>2014</v>
       </c>
@@ -22888,7 +22886,7 @@
         <v>1</v>
       </c>
       <c r="N350" s="3" t="n">
-        <v>46078.46881944445</v>
+        <v>46078.54770833333</v>
       </c>
       <c r="O350" t="inlineStr">
         <is>
@@ -23077,7 +23075,7 @@
         </is>
       </c>
       <c r="N353" s="3" t="n">
-        <v>46078.48393518518</v>
+        <v>46078.55489583333</v>
       </c>
       <c r="O353" t="inlineStr">
         <is>
@@ -23202,7 +23200,7 @@
         <v>1</v>
       </c>
       <c r="N355" s="3" t="n">
-        <v>46078.47880787037</v>
+        <v>46078.56057870371</v>
       </c>
       <c r="O355" t="inlineStr">
         <is>
@@ -23266,7 +23264,7 @@
         <v>1</v>
       </c>
       <c r="N356" s="3" t="n">
-        <v>46078.48070601852</v>
+        <v>46078.56122685185</v>
       </c>
       <c r="O356" t="inlineStr">
         <is>
@@ -23330,7 +23328,7 @@
         <v>1</v>
       </c>
       <c r="N357" s="3" t="n">
-        <v>46078.48508101852</v>
+        <v>46078.56133101852</v>
       </c>
       <c r="O357" t="inlineStr">
         <is>
@@ -23453,7 +23451,7 @@
         <v>2</v>
       </c>
       <c r="N359" s="3" t="n">
-        <v>46078.47711805555</v>
+        <v>46078.54993055556</v>
       </c>
       <c r="O359" t="inlineStr">
         <is>
@@ -23517,7 +23515,7 @@
         <v>2</v>
       </c>
       <c r="N360" s="3" t="n">
-        <v>46078.48373842592</v>
+        <v>46078.5678587963</v>
       </c>
       <c r="O360" t="inlineStr">
         <is>
@@ -23581,7 +23579,7 @@
         <v>1</v>
       </c>
       <c r="N361" s="3" t="n">
-        <v>46078.48011574074</v>
+        <v>46078.55652777778</v>
       </c>
       <c r="O361" t="inlineStr">
         <is>
@@ -23642,7 +23640,7 @@
         </is>
       </c>
       <c r="N362" s="3" t="n">
-        <v>46078.48282407408</v>
+        <v>46078.52708333333</v>
       </c>
       <c r="O362" t="inlineStr">
         <is>
@@ -23830,7 +23828,7 @@
         <v>1</v>
       </c>
       <c r="N365" s="3" t="n">
-        <v>46078.48314814815</v>
+        <v>46078.55903935185</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
@@ -23896,7 +23894,7 @@
         </is>
       </c>
       <c r="N366" s="3" t="n">
-        <v>46078.47699074074</v>
+        <v>46078.55025462963</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -24022,7 +24020,7 @@
         </is>
       </c>
       <c r="N368" s="3" t="n">
-        <v>46078.4771412037</v>
+        <v>46078.55609953704</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -24041,6 +24039,11 @@
           <t>RH</t>
         </is>
       </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>10.69.3.13</t>
+        </is>
+      </c>
       <c r="D369" t="n">
         <v>2025</v>
       </c>
@@ -24083,7 +24086,7 @@
         </is>
       </c>
       <c r="N369" s="3" t="n">
-        <v>46078.4762962963</v>
+        <v>46078.56673611111</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
@@ -24152,7 +24155,7 @@
         <v>1</v>
       </c>
       <c r="N370" s="3" t="n">
-        <v>46078.45079861111</v>
+        <v>46078.56127314815</v>
       </c>
       <c r="O370" t="inlineStr">
         <is>
@@ -24221,7 +24224,7 @@
         <v>1</v>
       </c>
       <c r="N371" s="3" t="n">
-        <v>46078.44900462963</v>
+        <v>46078.56458333333</v>
       </c>
       <c r="O371" t="inlineStr">
         <is>
@@ -24355,9 +24358,6 @@
           <t>HP ProDesk 400 G5 SFF (Brazil)</t>
         </is>
       </c>
-      <c r="M373" t="n">
-        <v>1</v>
-      </c>
       <c r="N373" s="3" t="n">
         <v>46078.44162037037</v>
       </c>
@@ -24428,7 +24428,7 @@
         <v>1</v>
       </c>
       <c r="N374" s="3" t="n">
-        <v>46078.47106481482</v>
+        <v>46078.54667824074</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24494,7 +24494,7 @@
         </is>
       </c>
       <c r="N375" s="3" t="n">
-        <v>46078.46810185185</v>
+        <v>46078.54888888889</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
@@ -24558,7 +24558,7 @@
         <v>1</v>
       </c>
       <c r="N376" s="3" t="n">
-        <v>46078.47907407407</v>
+        <v>46078.55358796296</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -24627,7 +24627,7 @@
         <v>2</v>
       </c>
       <c r="N377" s="3" t="n">
-        <v>46078.47793981482</v>
+        <v>46078.55849537037</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -24696,7 +24696,7 @@
         <v>2</v>
       </c>
       <c r="N378" s="3" t="n">
-        <v>46078.48601851852</v>
+        <v>46078.5684837963</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização automática 2026-02-25 15:52:03.858538
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>46078.56585648148</v>
+        <v>46078.64266203704</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>46078.5516087963</v>
+        <v>46078.63167824074</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
         <v>1</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>46078.53431712963</v>
+        <v>46078.61388888889</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>46078.53530092593</v>
+        <v>46078.64631944444</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -875,7 +875,7 @@
         <v>1</v>
       </c>
       <c r="N6" s="3" t="n">
-        <v>46078.54894675926</v>
+        <v>46078.58994212963</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -944,7 +944,7 @@
         <v>1</v>
       </c>
       <c r="N7" s="3" t="n">
-        <v>46078.55216435185</v>
+        <v>46078.6312962963</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -1072,7 +1072,7 @@
         <v>1</v>
       </c>
       <c r="N9" s="3" t="n">
-        <v>46078.54554398148</v>
+        <v>46078.62243055556</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -1259,7 +1259,7 @@
         <v>1</v>
       </c>
       <c r="N12" s="3" t="n">
-        <v>46078.54601851852</v>
+        <v>46078.6234837963</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1323,7 +1323,7 @@
         <v>1</v>
       </c>
       <c r="N13" s="3" t="n">
-        <v>46078.54613425926</v>
+        <v>46078.62032407407</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1387,7 +1387,7 @@
         <v>2</v>
       </c>
       <c r="N14" s="3" t="n">
-        <v>46078.54605324074</v>
+        <v>46078.62516203704</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1451,7 +1451,7 @@
         <v>1</v>
       </c>
       <c r="N15" s="3" t="n">
-        <v>46078.54996527778</v>
+        <v>46078.62567129629</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1515,7 +1515,7 @@
         <v>2</v>
       </c>
       <c r="N16" s="3" t="n">
-        <v>46078.54274305556</v>
+        <v>46078.62329861111</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1643,7 +1643,7 @@
         <v>2</v>
       </c>
       <c r="N18" s="3" t="n">
-        <v>46078.53900462963</v>
+        <v>46078.61817129629</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1768,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="N20" s="3" t="n">
-        <v>46078.54314814815</v>
+        <v>46078.62662037037</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1832,7 +1832,7 @@
         <v>1</v>
       </c>
       <c r="N21" s="3" t="n">
-        <v>46078.54496527778</v>
+        <v>46078.62983796297</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -1950,7 +1950,7 @@
         <v>1</v>
       </c>
       <c r="N23" s="3" t="n">
-        <v>46064.41899305556</v>
+        <v>46078.64517361111</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2009,7 +2009,7 @@
         <v>1</v>
       </c>
       <c r="N24" s="3" t="n">
-        <v>46078.53980324074</v>
+        <v>46078.62148148148</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2143,6 +2143,11 @@
           <t>AUDITORIO</t>
         </is>
       </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>10.69.3.151</t>
+        </is>
+      </c>
       <c r="D27" t="n">
         <v>2019</v>
       </c>
@@ -2183,7 +2188,7 @@
         <v>1</v>
       </c>
       <c r="N27" s="3" t="n">
-        <v>46078.53818287037</v>
+        <v>46078.65180555556</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2244,7 +2249,7 @@
         </is>
       </c>
       <c r="N28" s="3" t="n">
-        <v>46078.53824074074</v>
+        <v>46078.65396990741</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -6570,7 +6575,7 @@
         <v>1</v>
       </c>
       <c r="N95" s="3" t="n">
-        <v>46078.55678240741</v>
+        <v>46078.6343287037</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -6639,7 +6644,7 @@
         <v>1</v>
       </c>
       <c r="N96" s="3" t="n">
-        <v>46078.53973379629</v>
+        <v>46078.61712962963</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
@@ -6703,7 +6708,7 @@
         <v>1</v>
       </c>
       <c r="N97" s="3" t="n">
-        <v>46078.54201388889</v>
+        <v>46078.61734953704</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -6767,7 +6772,7 @@
         <v>1</v>
       </c>
       <c r="N98" s="3" t="n">
-        <v>46078.56221064815</v>
+        <v>46078.63829861111</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -6836,7 +6841,7 @@
         <v>1</v>
       </c>
       <c r="N99" s="3" t="n">
-        <v>46078.54172453703</v>
+        <v>46078.62019675926</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -6905,7 +6910,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>46078.56525462963</v>
+        <v>46078.63938657408</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6974,7 +6979,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="3" t="n">
-        <v>46078.53958333333</v>
+        <v>46078.63725694444</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -7112,7 +7117,7 @@
         <v>2</v>
       </c>
       <c r="N103" s="3" t="n">
-        <v>46078.54878472222</v>
+        <v>46078.63226851852</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7242,7 +7247,7 @@
         <v>1</v>
       </c>
       <c r="N105" s="3" t="n">
-        <v>46078.56394675926</v>
+        <v>46078.64126157408</v>
       </c>
       <c r="O105" t="inlineStr">
         <is>
@@ -7372,7 +7377,7 @@
         <v>1</v>
       </c>
       <c r="N107" s="3" t="n">
-        <v>46078.55010416666</v>
+        <v>46078.6299074074</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -7510,7 +7515,7 @@
         <v>1</v>
       </c>
       <c r="N109" s="3" t="n">
-        <v>46078.5356712963</v>
+        <v>46078.64701388889</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7579,7 +7584,7 @@
         <v>2</v>
       </c>
       <c r="N110" s="3" t="n">
-        <v>46078.55113425926</v>
+        <v>46078.62803240741</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7648,7 +7653,7 @@
         <v>2</v>
       </c>
       <c r="N111" s="3" t="n">
-        <v>46078.54837962963</v>
+        <v>46078.62600694445</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
@@ -7717,7 +7722,7 @@
         <v>2</v>
       </c>
       <c r="N112" s="3" t="n">
-        <v>46078.566875</v>
+        <v>46078.64269675926</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7786,7 +7791,7 @@
         <v>1</v>
       </c>
       <c r="N113" s="3" t="n">
-        <v>46078.55446759259</v>
+        <v>46078.63449074074</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7855,7 +7860,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>46078.54967592593</v>
+        <v>46078.62618055556</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -7921,7 +7926,7 @@
         </is>
       </c>
       <c r="N115" s="3" t="n">
-        <v>46078.56825231481</v>
+        <v>46078.64337962963</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -7990,7 +7995,7 @@
         <v>1</v>
       </c>
       <c r="N116" s="3" t="n">
-        <v>46078.56302083333</v>
+        <v>46078.63895833334</v>
       </c>
       <c r="O116" t="inlineStr">
         <is>
@@ -8054,7 +8059,7 @@
         <v>1</v>
       </c>
       <c r="N117" s="3" t="n">
-        <v>46078.55758101852</v>
+        <v>46078.63121527778</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -8120,7 +8125,7 @@
         </is>
       </c>
       <c r="N118" s="3" t="n">
-        <v>46078.57021990741</v>
+        <v>46078.64457175926</v>
       </c>
       <c r="O118" t="inlineStr">
         <is>
@@ -8258,7 +8263,7 @@
         <v>1</v>
       </c>
       <c r="N120" s="3" t="n">
-        <v>46078.54679398148</v>
+        <v>46078.62641203704</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -8327,7 +8332,7 @@
         <v>1</v>
       </c>
       <c r="N121" s="3" t="n">
-        <v>46078.5425925926</v>
+        <v>46078.62087962963</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -8393,7 +8398,7 @@
         </is>
       </c>
       <c r="N122" s="3" t="n">
-        <v>46078.55806712963</v>
+        <v>46078.65241898148</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -8462,7 +8467,7 @@
         <v>2</v>
       </c>
       <c r="N123" s="3" t="n">
-        <v>46078.55454861111</v>
+        <v>46078.63115740741</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -8531,7 +8536,7 @@
         <v>1</v>
       </c>
       <c r="N124" s="3" t="n">
-        <v>46078.55518518519</v>
+        <v>46078.63758101852</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -8600,7 +8605,7 @@
         <v>1</v>
       </c>
       <c r="N125" s="3" t="n">
-        <v>46078.56849537037</v>
+        <v>46078.65012731482</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -8669,7 +8674,7 @@
         <v>2</v>
       </c>
       <c r="N126" s="3" t="n">
-        <v>46078.53763888889</v>
+        <v>46078.65243055556</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -8738,7 +8743,7 @@
         <v>2</v>
       </c>
       <c r="N127" s="3" t="n">
-        <v>46078.54917824074</v>
+        <v>46078.63252314815</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -8807,7 +8812,7 @@
         <v>1</v>
       </c>
       <c r="N128" s="3" t="n">
-        <v>46078.55079861111</v>
+        <v>46078.62909722222</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -8876,7 +8881,7 @@
         <v>1</v>
       </c>
       <c r="N129" s="3" t="n">
-        <v>46078.56065972222</v>
+        <v>46078.63635416667</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -8945,7 +8950,7 @@
         <v>1</v>
       </c>
       <c r="N130" s="3" t="n">
-        <v>46078.53596064815</v>
+        <v>46078.65289351852</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -9014,7 +9019,7 @@
         <v>1</v>
       </c>
       <c r="N131" s="3" t="n">
-        <v>46078.56835648148</v>
+        <v>46078.64614583334</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -9147,7 +9152,7 @@
         <v>1</v>
       </c>
       <c r="N133" s="3" t="n">
-        <v>46078.56908564815</v>
+        <v>46078.64706018518</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -9211,7 +9216,7 @@
         <v>1</v>
       </c>
       <c r="N134" s="3" t="n">
-        <v>46076.87162037037</v>
+        <v>46078.65225694444</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -9271,8 +9276,11 @@
           <t>HP Compaq Pro 4300 SFF Brazil PC</t>
         </is>
       </c>
+      <c r="M135" t="n">
+        <v>1</v>
+      </c>
       <c r="N135" s="3" t="n">
-        <v>46077.81891203704</v>
+        <v>46078.62599537037</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -9463,7 +9471,7 @@
         <v>1</v>
       </c>
       <c r="N138" s="3" t="n">
-        <v>46078.56310185185</v>
+        <v>46078.64166666667</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9527,7 +9535,7 @@
         <v>1</v>
       </c>
       <c r="N139" s="3" t="n">
-        <v>46078.54238425926</v>
+        <v>46078.62056712963</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9591,7 +9599,7 @@
         <v>1</v>
       </c>
       <c r="N140" s="3" t="n">
-        <v>46078.56890046296</v>
+        <v>46078.64896990741</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9655,7 +9663,7 @@
         <v>1</v>
       </c>
       <c r="N141" s="3" t="n">
-        <v>46078.54099537037</v>
+        <v>46078.62148148148</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9719,7 +9727,7 @@
         <v>1</v>
       </c>
       <c r="N142" s="3" t="n">
-        <v>46078.5663425926</v>
+        <v>46078.6445949074</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9783,7 +9791,7 @@
         <v>1</v>
       </c>
       <c r="N143" s="3" t="n">
-        <v>46078.54859953704</v>
+        <v>46078.62886574074</v>
       </c>
       <c r="O143" t="inlineStr">
         <is>
@@ -9847,7 +9855,7 @@
         <v>1</v>
       </c>
       <c r="N144" s="3" t="n">
-        <v>46078.53967592592</v>
+        <v>46078.65446759259</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9911,7 +9919,7 @@
         <v>1</v>
       </c>
       <c r="N145" s="3" t="n">
-        <v>46078.5425925926</v>
+        <v>46078.62118055556</v>
       </c>
       <c r="O145" t="inlineStr">
         <is>
@@ -9975,7 +9983,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="3" t="n">
-        <v>46078.56262731482</v>
+        <v>46078.62097222222</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10103,7 +10111,7 @@
         <v>1</v>
       </c>
       <c r="N148" s="3" t="n">
-        <v>46078.56696759259</v>
+        <v>46078.6447800926</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10167,7 +10175,7 @@
         <v>1</v>
       </c>
       <c r="N149" s="3" t="n">
-        <v>46078.56865740741</v>
+        <v>46078.64045138889</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -10231,7 +10239,7 @@
         <v>1</v>
       </c>
       <c r="N150" s="3" t="n">
-        <v>46078.55412037037</v>
+        <v>46078.62663194445</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -10295,7 +10303,7 @@
         <v>1</v>
       </c>
       <c r="N151" s="3" t="n">
-        <v>46076.69913194444</v>
+        <v>46078.62715277778</v>
       </c>
       <c r="O151" t="inlineStr">
         <is>
@@ -10359,7 +10367,7 @@
         <v>1</v>
       </c>
       <c r="N152" s="3" t="n">
-        <v>46077.81385416666</v>
+        <v>46078.62174768518</v>
       </c>
       <c r="O152" t="inlineStr">
         <is>
@@ -10378,11 +10386,6 @@
           <t>OPERACAO 7.1</t>
         </is>
       </c>
-      <c r="C153" t="inlineStr">
-        <is>
-          <t>10.69.5.21</t>
-        </is>
-      </c>
       <c r="D153" t="n">
         <v>2018</v>
       </c>
@@ -10423,7 +10426,7 @@
         <v>1</v>
       </c>
       <c r="N153" s="3" t="n">
-        <v>46078.56505787037</v>
+        <v>46078.60457175926</v>
       </c>
       <c r="O153" t="inlineStr">
         <is>
@@ -10487,7 +10490,7 @@
         <v>1</v>
       </c>
       <c r="N154" s="3" t="n">
-        <v>46078.56493055556</v>
+        <v>46078.61708333333</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10551,7 +10554,7 @@
         <v>1</v>
       </c>
       <c r="N155" s="3" t="n">
-        <v>46078.56486111111</v>
+        <v>46078.64184027778</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10807,7 +10810,7 @@
         <v>1</v>
       </c>
       <c r="N159" s="3" t="n">
-        <v>46078.55532407408</v>
+        <v>46078.63446759259</v>
       </c>
       <c r="O159" t="inlineStr">
         <is>
@@ -10935,7 +10938,7 @@
         <v>1</v>
       </c>
       <c r="N161" s="3" t="n">
-        <v>46078.53363425926</v>
+        <v>46078.62905092593</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -10999,7 +11002,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="3" t="n">
-        <v>46078.55699074074</v>
+        <v>46078.63310185185</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11127,7 +11130,7 @@
         <v>2</v>
       </c>
       <c r="N164" s="3" t="n">
-        <v>46078.54511574074</v>
+        <v>46078.62606481482</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11191,7 +11194,7 @@
         <v>2</v>
       </c>
       <c r="N165" s="3" t="n">
-        <v>46078.5657175926</v>
+        <v>46078.64303240741</v>
       </c>
       <c r="O165" t="inlineStr">
         <is>
@@ -11255,7 +11258,7 @@
         <v>2</v>
       </c>
       <c r="N166" s="3" t="n">
-        <v>46078.56887731481</v>
+        <v>46078.60667824074</v>
       </c>
       <c r="O166" t="inlineStr">
         <is>
@@ -11319,7 +11322,7 @@
         <v>2</v>
       </c>
       <c r="N167" s="3" t="n">
-        <v>46078.56487268519</v>
+        <v>46078.605</v>
       </c>
       <c r="O167" t="inlineStr">
         <is>
@@ -11447,7 +11450,7 @@
         <v>2</v>
       </c>
       <c r="N169" s="3" t="n">
-        <v>46078.56100694444</v>
+        <v>46078.63847222222</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -11511,7 +11514,7 @@
         <v>2</v>
       </c>
       <c r="N170" s="3" t="n">
-        <v>46078.56444444445</v>
+        <v>46078.64467592593</v>
       </c>
       <c r="O170" t="inlineStr">
         <is>
@@ -11575,7 +11578,7 @@
         <v>1</v>
       </c>
       <c r="N171" s="3" t="n">
-        <v>46078.53545138889</v>
+        <v>46078.57716435185</v>
       </c>
       <c r="O171" t="inlineStr">
         <is>
@@ -11639,7 +11642,7 @@
         <v>2</v>
       </c>
       <c r="N172" s="3" t="n">
-        <v>46078.54083333333</v>
+        <v>46078.62841435185</v>
       </c>
       <c r="O172" t="inlineStr">
         <is>
@@ -11703,7 +11706,7 @@
         <v>2</v>
       </c>
       <c r="N173" s="3" t="n">
-        <v>46078.56283564815</v>
+        <v>46078.6427662037</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -11831,7 +11834,7 @@
         <v>2</v>
       </c>
       <c r="N175" s="3" t="n">
-        <v>46078.53097222222</v>
+        <v>46078.65278935185</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -11895,7 +11898,7 @@
         <v>2</v>
       </c>
       <c r="N176" s="3" t="n">
-        <v>46078.54165509259</v>
+        <v>46078.61819444445</v>
       </c>
       <c r="O176" t="inlineStr">
         <is>
@@ -11959,7 +11962,7 @@
         <v>2</v>
       </c>
       <c r="N177" s="3" t="n">
-        <v>46078.54300925926</v>
+        <v>46078.61791666667</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
@@ -12023,7 +12026,7 @@
         <v>2</v>
       </c>
       <c r="N178" s="3" t="n">
-        <v>46078.56019675926</v>
+        <v>46078.63988425926</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12087,7 +12090,7 @@
         <v>1</v>
       </c>
       <c r="N179" s="3" t="n">
-        <v>46078.5508912037</v>
+        <v>46078.63153935185</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12151,7 +12154,7 @@
         <v>1</v>
       </c>
       <c r="N180" s="3" t="n">
-        <v>46078.54559027778</v>
+        <v>46078.61775462963</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12215,7 +12218,7 @@
         <v>1</v>
       </c>
       <c r="N181" s="3" t="n">
-        <v>46078.56280092592</v>
+        <v>46078.63964120371</v>
       </c>
       <c r="O181" t="inlineStr">
         <is>
@@ -12604,7 +12607,7 @@
         <v>1</v>
       </c>
       <c r="N187" s="3" t="n">
-        <v>46078.54868055556</v>
+        <v>46078.63028935185</v>
       </c>
       <c r="O187" t="inlineStr">
         <is>
@@ -12754,6 +12757,11 @@
           <t>OPERACAO 8.1</t>
         </is>
       </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>10.69.5.59</t>
+        </is>
+      </c>
       <c r="D190" t="n">
         <v>2015</v>
       </c>
@@ -12791,7 +12799,7 @@
         </is>
       </c>
       <c r="N190" s="3" t="n">
-        <v>46078.54487268518</v>
+        <v>46078.62180555556</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12855,7 +12863,7 @@
         <v>1</v>
       </c>
       <c r="N191" s="3" t="n">
-        <v>46077.79695601852</v>
+        <v>46078.62324074074</v>
       </c>
       <c r="O191" t="inlineStr">
         <is>
@@ -12919,7 +12927,7 @@
         <v>1</v>
       </c>
       <c r="N192" s="3" t="n">
-        <v>46078.55626157407</v>
+        <v>46078.63185185185</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -13044,7 +13052,7 @@
         <v>2</v>
       </c>
       <c r="N194" s="3" t="n">
-        <v>46078.5587037037</v>
+        <v>46078.63803240741</v>
       </c>
       <c r="O194" t="inlineStr">
         <is>
@@ -13108,7 +13116,7 @@
         <v>1</v>
       </c>
       <c r="N195" s="3" t="n">
-        <v>46078.54197916666</v>
+        <v>46078.61908564815</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13172,7 +13180,7 @@
         <v>1</v>
       </c>
       <c r="N196" s="3" t="n">
-        <v>46077.81361111111</v>
+        <v>46078.65358796297</v>
       </c>
       <c r="O196" t="inlineStr">
         <is>
@@ -13236,7 +13244,7 @@
         <v>1</v>
       </c>
       <c r="N197" s="3" t="n">
-        <v>46077.8303125</v>
+        <v>46078.65353009259</v>
       </c>
       <c r="O197" t="inlineStr">
         <is>
@@ -13300,7 +13308,7 @@
         <v>1</v>
       </c>
       <c r="N198" s="3" t="n">
-        <v>46078.55230324074</v>
+        <v>46078.6300462963</v>
       </c>
       <c r="O198" t="inlineStr">
         <is>
@@ -13364,7 +13372,7 @@
         <v>1</v>
       </c>
       <c r="N199" s="3" t="n">
-        <v>46077.82847222222</v>
+        <v>46078.64041666667</v>
       </c>
       <c r="O199" t="inlineStr">
         <is>
@@ -13428,7 +13436,7 @@
         <v>1</v>
       </c>
       <c r="N200" s="3" t="n">
-        <v>46076.82861111111</v>
+        <v>46078.63975694445</v>
       </c>
       <c r="O200" t="inlineStr">
         <is>
@@ -13489,7 +13497,7 @@
         </is>
       </c>
       <c r="N201" s="3" t="n">
-        <v>46078.54787037037</v>
+        <v>46078.63099537037</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -13553,7 +13561,7 @@
         <v>1</v>
       </c>
       <c r="N202" s="3" t="n">
-        <v>46078.53300925926</v>
+        <v>46078.62569444445</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13617,7 +13625,7 @@
         <v>1</v>
       </c>
       <c r="N203" s="3" t="n">
-        <v>46078.5375462963</v>
+        <v>46078.62173611111</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13681,7 +13689,7 @@
         <v>1</v>
       </c>
       <c r="N204" s="3" t="n">
-        <v>46078.53262731482</v>
+        <v>46078.61515046296</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13745,7 +13753,7 @@
         <v>1</v>
       </c>
       <c r="N205" s="3" t="n">
-        <v>46078.55136574074</v>
+        <v>46078.63435185186</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13809,7 +13817,7 @@
         <v>1</v>
       </c>
       <c r="N206" s="3" t="n">
-        <v>46077.82380787037</v>
+        <v>46078.63149305555</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -13873,7 +13881,7 @@
         <v>1</v>
       </c>
       <c r="N207" s="3" t="n">
-        <v>46078.52907407407</v>
+        <v>46078.65363425926</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -13937,7 +13945,7 @@
         <v>1</v>
       </c>
       <c r="N208" s="3" t="n">
-        <v>46078.56446759259</v>
+        <v>46078.6445949074</v>
       </c>
       <c r="O208" t="inlineStr">
         <is>
@@ -14001,7 +14009,7 @@
         <v>1</v>
       </c>
       <c r="N209" s="3" t="n">
-        <v>46078.55226851852</v>
+        <v>46078.63021990741</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14065,7 +14073,7 @@
         <v>1</v>
       </c>
       <c r="N210" s="3" t="n">
-        <v>46078.5666550926</v>
+        <v>46078.6437962963</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14129,7 +14137,7 @@
         <v>1</v>
       </c>
       <c r="N211" s="3" t="n">
-        <v>46078.56876157408</v>
+        <v>46078.63957175926</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -14193,7 +14201,7 @@
         <v>1</v>
       </c>
       <c r="N212" s="3" t="n">
-        <v>46078.56939814815</v>
+        <v>46078.62751157407</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -14257,7 +14265,7 @@
         <v>1</v>
       </c>
       <c r="N213" s="3" t="n">
-        <v>46078.55322916667</v>
+        <v>46078.63978009259</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
@@ -14321,7 +14329,7 @@
         <v>1</v>
       </c>
       <c r="N214" s="3" t="n">
-        <v>46078.37199074074</v>
+        <v>46078.63913194444</v>
       </c>
       <c r="O214" t="inlineStr">
         <is>
@@ -14385,7 +14393,7 @@
         <v>1</v>
       </c>
       <c r="N215" s="3" t="n">
-        <v>46077.83409722222</v>
+        <v>46078.63936342593</v>
       </c>
       <c r="O215" t="inlineStr">
         <is>
@@ -14449,7 +14457,7 @@
         <v>1</v>
       </c>
       <c r="N216" s="3" t="n">
-        <v>46078.54422453704</v>
+        <v>46078.62537037037</v>
       </c>
       <c r="O216" t="inlineStr">
         <is>
@@ -14468,6 +14476,11 @@
           <t>OPERACAO 8.1</t>
         </is>
       </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>10.69.5.85</t>
+        </is>
+      </c>
       <c r="D217" t="n">
         <v>2017</v>
       </c>
@@ -14508,7 +14521,7 @@
         <v>1</v>
       </c>
       <c r="N217" s="3" t="n">
-        <v>46078.53479166667</v>
+        <v>46078.64325231482</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14572,7 +14585,7 @@
         <v>1</v>
       </c>
       <c r="N218" s="3" t="n">
-        <v>46078.55929398148</v>
+        <v>46078.63256944445</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14636,7 +14649,7 @@
         <v>1</v>
       </c>
       <c r="N219" s="3" t="n">
-        <v>46078.40295138889</v>
+        <v>46078.62384259259</v>
       </c>
       <c r="O219" t="inlineStr">
         <is>
@@ -14705,7 +14718,7 @@
         <v>1</v>
       </c>
       <c r="N220" s="3" t="n">
-        <v>46078.48685185185</v>
+        <v>46078.6437037037</v>
       </c>
       <c r="O220" t="inlineStr">
         <is>
@@ -14769,7 +14782,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="3" t="n">
-        <v>46078.53570601852</v>
+        <v>46078.62417824074</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14833,7 +14846,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="3" t="n">
-        <v>46078.5409375</v>
+        <v>46078.6206712963</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -14897,7 +14910,7 @@
         <v>1</v>
       </c>
       <c r="N223" s="3" t="n">
-        <v>46078.56770833334</v>
+        <v>46078.63645833333</v>
       </c>
       <c r="O223" t="inlineStr">
         <is>
@@ -14961,7 +14974,7 @@
         <v>1</v>
       </c>
       <c r="N224" s="3" t="n">
-        <v>46078.55299768518</v>
+        <v>46078.6459375</v>
       </c>
       <c r="O224" t="inlineStr">
         <is>
@@ -15025,7 +15038,7 @@
         <v>1</v>
       </c>
       <c r="N225" s="3" t="n">
-        <v>46078.55334490741</v>
+        <v>46078.63025462963</v>
       </c>
       <c r="O225" t="inlineStr">
         <is>
@@ -15089,7 +15102,7 @@
         <v>1</v>
       </c>
       <c r="N226" s="3" t="n">
-        <v>46078.55998842593</v>
+        <v>46078.65459490741</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15153,7 +15166,7 @@
         <v>1</v>
       </c>
       <c r="N227" s="3" t="n">
-        <v>46078.54892361111</v>
+        <v>46078.62581018519</v>
       </c>
       <c r="O227" t="inlineStr">
         <is>
@@ -15217,7 +15230,7 @@
         <v>1</v>
       </c>
       <c r="N228" s="3" t="n">
-        <v>46078.54648148148</v>
+        <v>46078.62380787037</v>
       </c>
       <c r="O228" t="inlineStr">
         <is>
@@ -15281,7 +15294,7 @@
         <v>1</v>
       </c>
       <c r="N229" s="3" t="n">
-        <v>46078.53190972222</v>
+        <v>46078.65040509259</v>
       </c>
       <c r="O229" t="inlineStr">
         <is>
@@ -15345,7 +15358,7 @@
         <v>1</v>
       </c>
       <c r="N230" s="3" t="n">
-        <v>46078.54291666667</v>
+        <v>46078.62075231481</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15409,7 +15422,7 @@
         <v>1</v>
       </c>
       <c r="N231" s="3" t="n">
-        <v>46078.56234953704</v>
+        <v>46078.6387962963</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15473,7 +15486,7 @@
         <v>1</v>
       </c>
       <c r="N232" s="3" t="n">
-        <v>46078.5521875</v>
+        <v>46078.63377314815</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -15537,7 +15550,7 @@
         <v>1</v>
       </c>
       <c r="N233" s="3" t="n">
-        <v>46078.5418287037</v>
+        <v>46078.62729166666</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15601,7 +15614,7 @@
         <v>1</v>
       </c>
       <c r="N234" s="3" t="n">
-        <v>46078.56962962963</v>
+        <v>46078.6286574074</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -15665,7 +15678,7 @@
         <v>1</v>
       </c>
       <c r="N235" s="3" t="n">
-        <v>46078.56435185186</v>
+        <v>46078.61899305556</v>
       </c>
       <c r="O235" t="inlineStr">
         <is>
@@ -15729,7 +15742,7 @@
         <v>1</v>
       </c>
       <c r="N236" s="3" t="n">
-        <v>46078.56503472223</v>
+        <v>46078.64453703703</v>
       </c>
       <c r="O236" t="inlineStr">
         <is>
@@ -15793,7 +15806,7 @@
         <v>1</v>
       </c>
       <c r="N237" s="3" t="n">
-        <v>46077.79817129629</v>
+        <v>46078.63938657408</v>
       </c>
       <c r="O237" t="inlineStr">
         <is>
@@ -15857,7 +15870,7 @@
         <v>1</v>
       </c>
       <c r="N238" s="3" t="n">
-        <v>46078.55677083333</v>
+        <v>46078.63561342593</v>
       </c>
       <c r="O238" t="inlineStr">
         <is>
@@ -15921,7 +15934,7 @@
         <v>1</v>
       </c>
       <c r="N239" s="3" t="n">
-        <v>46078.5664699074</v>
+        <v>46078.63952546296</v>
       </c>
       <c r="O239" t="inlineStr">
         <is>
@@ -15985,7 +15998,7 @@
         <v>1</v>
       </c>
       <c r="N240" s="3" t="n">
-        <v>46078.55107638889</v>
+        <v>46078.62743055556</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16049,7 +16062,7 @@
         <v>1</v>
       </c>
       <c r="N241" s="3" t="n">
-        <v>46078.55320601852</v>
+        <v>46078.63944444444</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16113,7 +16126,7 @@
         <v>1</v>
       </c>
       <c r="N242" s="3" t="n">
-        <v>46078.55567129629</v>
+        <v>46078.63113425926</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16177,7 +16190,7 @@
         <v>1</v>
       </c>
       <c r="N243" s="3" t="n">
-        <v>46077.76497685185</v>
+        <v>46078.63947916667</v>
       </c>
       <c r="O243" t="inlineStr">
         <is>
@@ -16236,7 +16249,7 @@
         <v>1</v>
       </c>
       <c r="N244" s="3" t="n">
-        <v>46078.40516203704</v>
+        <v>46078.63931712963</v>
       </c>
       <c r="O244" t="inlineStr">
         <is>
@@ -16300,7 +16313,7 @@
         <v>1</v>
       </c>
       <c r="N245" s="3" t="n">
-        <v>46078.53224537037</v>
+        <v>46078.64873842592</v>
       </c>
       <c r="O245" t="inlineStr">
         <is>
@@ -16364,7 +16377,7 @@
         <v>1</v>
       </c>
       <c r="N246" s="3" t="n">
-        <v>46078.56759259259</v>
+        <v>46078.64141203704</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16428,7 +16441,7 @@
         <v>1</v>
       </c>
       <c r="N247" s="3" t="n">
-        <v>46078.55452546296</v>
+        <v>46078.63472222222</v>
       </c>
       <c r="O247" t="inlineStr">
         <is>
@@ -16492,7 +16505,7 @@
         <v>1</v>
       </c>
       <c r="N248" s="3" t="n">
-        <v>46078.56932870371</v>
+        <v>46078.6328587963</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16556,7 +16569,7 @@
         <v>1</v>
       </c>
       <c r="N249" s="3" t="n">
-        <v>46078.54880787037</v>
+        <v>46078.62634259259</v>
       </c>
       <c r="O249" t="inlineStr">
         <is>
@@ -16620,7 +16633,7 @@
         <v>1</v>
       </c>
       <c r="N250" s="3" t="n">
-        <v>46078.56059027778</v>
+        <v>46078.64</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16684,7 +16697,7 @@
         <v>1</v>
       </c>
       <c r="N251" s="3" t="n">
-        <v>46078.56376157407</v>
+        <v>46078.64005787037</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16748,7 +16761,7 @@
         <v>1</v>
       </c>
       <c r="N252" s="3" t="n">
-        <v>46078.53275462963</v>
+        <v>46078.64967592592</v>
       </c>
       <c r="O252" t="inlineStr">
         <is>
@@ -16812,7 +16825,7 @@
         <v>1</v>
       </c>
       <c r="N253" s="3" t="n">
-        <v>46078.55461805555</v>
+        <v>46078.62550925926</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16870,7 +16883,7 @@
         <v>1</v>
       </c>
       <c r="N254" s="3" t="n">
-        <v>46078.56100694444</v>
+        <v>46078.63756944444</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -16934,7 +16947,7 @@
         <v>1</v>
       </c>
       <c r="N255" s="3" t="n">
-        <v>46078.56243055555</v>
+        <v>46078.63966435185</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -16998,7 +17011,7 @@
         <v>1</v>
       </c>
       <c r="N256" s="3" t="n">
-        <v>46078.57001157408</v>
+        <v>46078.6438425926</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17062,7 +17075,7 @@
         <v>1</v>
       </c>
       <c r="N257" s="3" t="n">
-        <v>46078.56605324074</v>
+        <v>46078.64716435185</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17126,7 +17139,7 @@
         <v>1</v>
       </c>
       <c r="N258" s="3" t="n">
-        <v>46078.5575462963</v>
+        <v>46078.63880787037</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
@@ -17190,7 +17203,7 @@
         <v>1</v>
       </c>
       <c r="N259" s="3" t="n">
-        <v>46078.56502314815</v>
+        <v>46078.64032407408</v>
       </c>
       <c r="O259" t="inlineStr">
         <is>
@@ -17254,7 +17267,7 @@
         <v>1</v>
       </c>
       <c r="N260" s="3" t="n">
-        <v>46078.57061342592</v>
+        <v>46078.613125</v>
       </c>
       <c r="O260" t="inlineStr">
         <is>
@@ -17318,7 +17331,7 @@
         <v>1</v>
       </c>
       <c r="N261" s="3" t="n">
-        <v>46078.56122685185</v>
+        <v>46078.64159722222</v>
       </c>
       <c r="O261" t="inlineStr">
         <is>
@@ -17382,7 +17395,7 @@
         <v>1</v>
       </c>
       <c r="N262" s="3" t="n">
-        <v>46078.53269675926</v>
+        <v>46078.62449074074</v>
       </c>
       <c r="O262" t="inlineStr">
         <is>
@@ -17446,7 +17459,7 @@
         <v>1</v>
       </c>
       <c r="N263" s="3" t="n">
-        <v>46078.53876157408</v>
+        <v>46078.61869212963</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17510,7 +17523,7 @@
         <v>1</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>46078.5659375</v>
+        <v>46078.64130787037</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17574,7 +17587,7 @@
         <v>1</v>
       </c>
       <c r="N265" s="3" t="n">
-        <v>46078.55936342593</v>
+        <v>46078.62777777778</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17638,7 +17651,7 @@
         <v>1</v>
       </c>
       <c r="N266" s="3" t="n">
-        <v>46078.5350462963</v>
+        <v>46078.57684027778</v>
       </c>
       <c r="O266" t="inlineStr">
         <is>
@@ -17702,7 +17715,7 @@
         <v>1</v>
       </c>
       <c r="N267" s="3" t="n">
-        <v>46078.56815972222</v>
+        <v>46078.64559027777</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17766,7 +17779,7 @@
         <v>1</v>
       </c>
       <c r="N268" s="3" t="n">
-        <v>46078.53659722222</v>
+        <v>46078.65158564815</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17830,7 +17843,7 @@
         <v>1</v>
       </c>
       <c r="N269" s="3" t="n">
-        <v>46078.54856481482</v>
+        <v>46078.62967592593</v>
       </c>
       <c r="O269" t="inlineStr">
         <is>
@@ -17891,7 +17904,7 @@
         </is>
       </c>
       <c r="N270" s="3" t="n">
-        <v>46078.56079861111</v>
+        <v>46078.63883101852</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -17955,7 +17968,7 @@
         <v>1</v>
       </c>
       <c r="N271" s="3" t="n">
-        <v>46078.12091435185</v>
+        <v>46078.62690972222</v>
       </c>
       <c r="O271" t="inlineStr">
         <is>
@@ -18019,7 +18032,7 @@
         <v>1</v>
       </c>
       <c r="N272" s="3" t="n">
-        <v>46078.57111111111</v>
+        <v>46078.62369212963</v>
       </c>
       <c r="O272" t="inlineStr">
         <is>
@@ -18403,7 +18416,7 @@
         <v>1</v>
       </c>
       <c r="N278" s="3" t="n">
-        <v>46078.57021990741</v>
+        <v>46078.63351851852</v>
       </c>
       <c r="O278" t="inlineStr">
         <is>
@@ -18467,7 +18480,7 @@
         <v>1</v>
       </c>
       <c r="N279" s="3" t="n">
-        <v>46078.55523148148</v>
+        <v>46078.64271990741</v>
       </c>
       <c r="O279" t="inlineStr">
         <is>
@@ -18531,7 +18544,7 @@
         <v>1</v>
       </c>
       <c r="N280" s="3" t="n">
-        <v>46078.54112268519</v>
+        <v>46078.57743055555</v>
       </c>
       <c r="O280" t="inlineStr">
         <is>
@@ -18718,7 +18731,7 @@
         <v>1</v>
       </c>
       <c r="N283" s="3" t="n">
-        <v>46078.56862268518</v>
+        <v>46078.65328703704</v>
       </c>
       <c r="O283" t="inlineStr">
         <is>
@@ -18782,7 +18795,7 @@
         <v>1</v>
       </c>
       <c r="N284" s="3" t="n">
-        <v>46078.56114583334</v>
+        <v>46078.63818287037</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18846,7 +18859,7 @@
         <v>1</v>
       </c>
       <c r="N285" s="3" t="n">
-        <v>46078.56429398148</v>
+        <v>46078.62998842593</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -18865,11 +18878,6 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
-      <c r="C286" t="inlineStr">
-        <is>
-          <t>10.69.5.155</t>
-        </is>
-      </c>
       <c r="D286" t="n">
         <v>2019</v>
       </c>
@@ -18974,7 +18982,7 @@
         <v>1</v>
       </c>
       <c r="N287" s="3" t="n">
-        <v>46078.56967592592</v>
+        <v>46078.64945601852</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
@@ -19038,7 +19046,7 @@
         <v>1</v>
       </c>
       <c r="N288" s="3" t="n">
-        <v>46078.56586805556</v>
+        <v>46078.62541666667</v>
       </c>
       <c r="O288" t="inlineStr">
         <is>
@@ -19102,7 +19110,7 @@
         <v>1</v>
       </c>
       <c r="N289" s="3" t="n">
-        <v>46078.53180555555</v>
+        <v>46078.64796296296</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -19896,7 +19904,7 @@
         <v>1</v>
       </c>
       <c r="N302" s="3" t="n">
-        <v>46078.55847222222</v>
+        <v>46078.63231481481</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -20637,7 +20645,7 @@
         </is>
       </c>
       <c r="N314" s="3" t="n">
-        <v>46078.55743055556</v>
+        <v>46078.62900462963</v>
       </c>
       <c r="O314" t="inlineStr">
         <is>
@@ -21012,7 +21020,7 @@
         </is>
       </c>
       <c r="N320" s="3" t="n">
-        <v>46078.53989583333</v>
+        <v>46078.61966435185</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21737,7 +21745,7 @@
         <v>1</v>
       </c>
       <c r="N332" s="3" t="n">
-        <v>46078.54989583333</v>
+        <v>46078.62871527778</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21801,7 +21809,7 @@
         <v>2</v>
       </c>
       <c r="N333" s="3" t="n">
-        <v>46078.5433912037</v>
+        <v>46078.62116898148</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21865,7 +21873,7 @@
         <v>2</v>
       </c>
       <c r="N334" s="3" t="n">
-        <v>46078.56039351852</v>
+        <v>46078.63637731481</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21929,7 +21937,7 @@
         <v>2</v>
       </c>
       <c r="N335" s="3" t="n">
-        <v>46078.55385416667</v>
+        <v>46078.63046296296</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -21993,7 +22001,7 @@
         <v>1</v>
       </c>
       <c r="N336" s="3" t="n">
-        <v>46078.55247685185</v>
+        <v>46078.63217592592</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22057,7 +22065,7 @@
         <v>1</v>
       </c>
       <c r="N337" s="3" t="n">
-        <v>46078.56362268519</v>
+        <v>46078.64321759259</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22121,7 +22129,7 @@
         <v>2</v>
       </c>
       <c r="N338" s="3" t="n">
-        <v>46078.56516203703</v>
+        <v>46078.64625</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -22185,7 +22193,7 @@
         <v>2</v>
       </c>
       <c r="N339" s="3" t="n">
-        <v>46078.56081018518</v>
+        <v>46078.63417824074</v>
       </c>
       <c r="O339" t="inlineStr">
         <is>
@@ -22377,7 +22385,7 @@
         <v>2</v>
       </c>
       <c r="N342" s="3" t="n">
-        <v>46078.54081018519</v>
+        <v>46078.57918981482</v>
       </c>
       <c r="O342" t="inlineStr">
         <is>
@@ -22438,7 +22446,7 @@
         </is>
       </c>
       <c r="N343" s="3" t="n">
-        <v>46078.55253472222</v>
+        <v>46078.63077546296</v>
       </c>
       <c r="O343" t="inlineStr">
         <is>
@@ -22694,7 +22702,7 @@
         <v>1</v>
       </c>
       <c r="N347" s="3" t="n">
-        <v>46078.55133101852</v>
+        <v>46078.58936342593</v>
       </c>
       <c r="O347" t="inlineStr">
         <is>
@@ -22758,7 +22766,7 @@
         <v>1</v>
       </c>
       <c r="N348" s="3" t="n">
-        <v>46078.55825231481</v>
+        <v>46078.60284722222</v>
       </c>
       <c r="O348" t="inlineStr">
         <is>
@@ -22822,7 +22830,7 @@
         <v>1</v>
       </c>
       <c r="N349" s="3" t="n">
-        <v>46078.56190972222</v>
+        <v>46078.59994212963</v>
       </c>
       <c r="O349" t="inlineStr">
         <is>
@@ -22841,11 +22849,6 @@
           <t>OPERACAO 9.1</t>
         </is>
       </c>
-      <c r="C350" t="inlineStr">
-        <is>
-          <t>10.69.5.244</t>
-        </is>
-      </c>
       <c r="D350" t="n">
         <v>2014</v>
       </c>
@@ -22886,7 +22889,7 @@
         <v>1</v>
       </c>
       <c r="N350" s="3" t="n">
-        <v>46078.54770833333</v>
+        <v>46078.5891087963</v>
       </c>
       <c r="O350" t="inlineStr">
         <is>
@@ -23075,7 +23078,7 @@
         </is>
       </c>
       <c r="N353" s="3" t="n">
-        <v>46078.55489583333</v>
+        <v>46078.59373842592</v>
       </c>
       <c r="O353" t="inlineStr">
         <is>
@@ -23200,7 +23203,7 @@
         <v>1</v>
       </c>
       <c r="N355" s="3" t="n">
-        <v>46078.56057870371</v>
+        <v>46078.59833333334</v>
       </c>
       <c r="O355" t="inlineStr">
         <is>
@@ -23451,7 +23454,7 @@
         <v>2</v>
       </c>
       <c r="N359" s="3" t="n">
-        <v>46078.54993055556</v>
+        <v>46078.59206018518</v>
       </c>
       <c r="O359" t="inlineStr">
         <is>
@@ -23579,7 +23582,7 @@
         <v>1</v>
       </c>
       <c r="N361" s="3" t="n">
-        <v>46078.55652777778</v>
+        <v>46078.59190972222</v>
       </c>
       <c r="O361" t="inlineStr">
         <is>
@@ -23640,7 +23643,7 @@
         </is>
       </c>
       <c r="N362" s="3" t="n">
-        <v>46078.52708333333</v>
+        <v>46078.57268518519</v>
       </c>
       <c r="O362" t="inlineStr">
         <is>
@@ -23828,7 +23831,7 @@
         <v>1</v>
       </c>
       <c r="N365" s="3" t="n">
-        <v>46078.55903935185</v>
+        <v>46078.63043981481</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
@@ -23894,7 +23897,7 @@
         </is>
       </c>
       <c r="N366" s="3" t="n">
-        <v>46078.55025462963</v>
+        <v>46078.63236111111</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -24020,7 +24023,7 @@
         </is>
       </c>
       <c r="N368" s="3" t="n">
-        <v>46078.55609953704</v>
+        <v>46078.6290162037</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -24086,7 +24089,7 @@
         </is>
       </c>
       <c r="N369" s="3" t="n">
-        <v>46078.56673611111</v>
+        <v>46078.6425</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
@@ -24155,7 +24158,7 @@
         <v>1</v>
       </c>
       <c r="N370" s="3" t="n">
-        <v>46078.56127314815</v>
+        <v>46078.63587962963</v>
       </c>
       <c r="O370" t="inlineStr">
         <is>
@@ -24224,7 +24227,7 @@
         <v>1</v>
       </c>
       <c r="N371" s="3" t="n">
-        <v>46078.56458333333</v>
+        <v>46078.64103009259</v>
       </c>
       <c r="O371" t="inlineStr">
         <is>
@@ -24359,7 +24362,7 @@
         </is>
       </c>
       <c r="N373" s="3" t="n">
-        <v>46078.44162037037</v>
+        <v>46078.57886574074</v>
       </c>
       <c r="O373" t="inlineStr">
         <is>
@@ -24428,7 +24431,7 @@
         <v>1</v>
       </c>
       <c r="N374" s="3" t="n">
-        <v>46078.54667824074</v>
+        <v>46078.62300925926</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24494,7 +24497,7 @@
         </is>
       </c>
       <c r="N375" s="3" t="n">
-        <v>46078.54888888889</v>
+        <v>46078.62302083334</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
@@ -24558,7 +24561,7 @@
         <v>1</v>
       </c>
       <c r="N376" s="3" t="n">
-        <v>46078.55358796296</v>
+        <v>46078.6282175926</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -24627,7 +24630,7 @@
         <v>2</v>
       </c>
       <c r="N377" s="3" t="n">
-        <v>46078.55849537037</v>
+        <v>46078.64170138889</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -24696,7 +24699,7 @@
         <v>2</v>
       </c>
       <c r="N378" s="3" t="n">
-        <v>46078.5684837963</v>
+        <v>46078.64489583333</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização automática 2026-02-25 17:52:03.571198
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>46078.64266203704</v>
+        <v>46078.71922453704</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>46078.63167824074</v>
+        <v>46078.71548611111</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
         <v>1</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>46078.61388888889</v>
+        <v>46078.69167824074</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>46078.64631944444</v>
+        <v>46078.72538194444</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -944,7 +944,7 @@
         <v>1</v>
       </c>
       <c r="N7" s="3" t="n">
-        <v>46078.6312962963</v>
+        <v>46078.70773148148</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -1072,7 +1072,7 @@
         <v>1</v>
       </c>
       <c r="N9" s="3" t="n">
-        <v>46078.62243055556</v>
+        <v>46078.72996527778</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -1323,7 +1323,7 @@
         <v>1</v>
       </c>
       <c r="N13" s="3" t="n">
-        <v>46078.62032407407</v>
+        <v>46078.7371875</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1387,7 +1387,7 @@
         <v>2</v>
       </c>
       <c r="N14" s="3" t="n">
-        <v>46078.62516203704</v>
+        <v>46078.73407407408</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1451,7 +1451,7 @@
         <v>1</v>
       </c>
       <c r="N15" s="3" t="n">
-        <v>46078.62567129629</v>
+        <v>46078.70284722222</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1515,7 +1515,7 @@
         <v>2</v>
       </c>
       <c r="N16" s="3" t="n">
-        <v>46078.62329861111</v>
+        <v>46078.73741898148</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1643,7 +1643,7 @@
         <v>2</v>
       </c>
       <c r="N18" s="3" t="n">
-        <v>46078.61817129629</v>
+        <v>46078.73734953703</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1768,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="N20" s="3" t="n">
-        <v>46078.62662037037</v>
+        <v>46078.70361111111</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1832,7 +1832,7 @@
         <v>1</v>
       </c>
       <c r="N21" s="3" t="n">
-        <v>46078.62983796297</v>
+        <v>46078.70927083334</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -1950,7 +1950,7 @@
         <v>1</v>
       </c>
       <c r="N23" s="3" t="n">
-        <v>46078.64517361111</v>
+        <v>46078.72707175926</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -1969,6 +1969,11 @@
           <t>AUDITORIO</t>
         </is>
       </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>10.69.3.150</t>
+        </is>
+      </c>
       <c r="D24" t="n">
         <v>2019</v>
       </c>
@@ -2009,7 +2014,7 @@
         <v>1</v>
       </c>
       <c r="N24" s="3" t="n">
-        <v>46078.62148148148</v>
+        <v>46078.73511574074</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2143,11 +2148,6 @@
           <t>AUDITORIO</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>10.69.3.151</t>
-        </is>
-      </c>
       <c r="D27" t="n">
         <v>2019</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>1</v>
       </c>
       <c r="N27" s="3" t="n">
-        <v>46078.65180555556</v>
+        <v>46078.72754629629</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2249,7 +2249,7 @@
         </is>
       </c>
       <c r="N28" s="3" t="n">
-        <v>46078.65396990741</v>
+        <v>46078.73241898148</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -6575,7 +6575,7 @@
         <v>1</v>
       </c>
       <c r="N95" s="3" t="n">
-        <v>46078.6343287037</v>
+        <v>46078.7060300926</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -6644,7 +6644,7 @@
         <v>1</v>
       </c>
       <c r="N96" s="3" t="n">
-        <v>46078.61712962963</v>
+        <v>46078.7325462963</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
@@ -6708,7 +6708,7 @@
         <v>1</v>
       </c>
       <c r="N97" s="3" t="n">
-        <v>46078.61734953704</v>
+        <v>46078.69038194444</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -6727,6 +6727,11 @@
           <t>COORDENACAO</t>
         </is>
       </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>10.69.3.94</t>
+        </is>
+      </c>
       <c r="D98" t="n">
         <v>2025</v>
       </c>
@@ -6772,7 +6777,7 @@
         <v>1</v>
       </c>
       <c r="N98" s="3" t="n">
-        <v>46078.63829861111</v>
+        <v>46078.71636574074</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -6841,7 +6846,7 @@
         <v>1</v>
       </c>
       <c r="N99" s="3" t="n">
-        <v>46078.62019675926</v>
+        <v>46078.70243055555</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -6910,7 +6915,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>46078.63938657408</v>
+        <v>46078.72143518519</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6979,7 +6984,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="3" t="n">
-        <v>46078.63725694444</v>
+        <v>46078.71096064815</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -7117,7 +7122,7 @@
         <v>2</v>
       </c>
       <c r="N103" s="3" t="n">
-        <v>46078.63226851852</v>
+        <v>46078.71195601852</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7247,7 +7252,7 @@
         <v>1</v>
       </c>
       <c r="N105" s="3" t="n">
-        <v>46078.64126157408</v>
+        <v>46078.67922453704</v>
       </c>
       <c r="O105" t="inlineStr">
         <is>
@@ -7377,7 +7382,7 @@
         <v>1</v>
       </c>
       <c r="N107" s="3" t="n">
-        <v>46078.6299074074</v>
+        <v>46078.66605324074</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -7515,7 +7520,7 @@
         <v>1</v>
       </c>
       <c r="N109" s="3" t="n">
-        <v>46078.64701388889</v>
+        <v>46078.72763888889</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7584,7 +7589,7 @@
         <v>2</v>
       </c>
       <c r="N110" s="3" t="n">
-        <v>46078.62803240741</v>
+        <v>46078.70770833334</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7653,7 +7658,7 @@
         <v>2</v>
       </c>
       <c r="N111" s="3" t="n">
-        <v>46078.62600694445</v>
+        <v>46078.70545138889</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
@@ -7722,7 +7727,7 @@
         <v>2</v>
       </c>
       <c r="N112" s="3" t="n">
-        <v>46078.64269675926</v>
+        <v>46078.71792824074</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7791,7 +7796,7 @@
         <v>1</v>
       </c>
       <c r="N113" s="3" t="n">
-        <v>46078.63449074074</v>
+        <v>46078.70827546297</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7860,7 +7865,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>46078.62618055556</v>
+        <v>46078.7075462963</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -7926,7 +7931,7 @@
         </is>
       </c>
       <c r="N115" s="3" t="n">
-        <v>46078.64337962963</v>
+        <v>46078.68179398148</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -7995,7 +8000,7 @@
         <v>1</v>
       </c>
       <c r="N116" s="3" t="n">
-        <v>46078.63895833334</v>
+        <v>46078.67899305555</v>
       </c>
       <c r="O116" t="inlineStr">
         <is>
@@ -8059,7 +8064,7 @@
         <v>1</v>
       </c>
       <c r="N117" s="3" t="n">
-        <v>46078.63121527778</v>
+        <v>46078.70715277778</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -8125,7 +8130,7 @@
         </is>
       </c>
       <c r="N118" s="3" t="n">
-        <v>46078.64457175926</v>
+        <v>46078.68390046297</v>
       </c>
       <c r="O118" t="inlineStr">
         <is>
@@ -8263,7 +8268,7 @@
         <v>1</v>
       </c>
       <c r="N120" s="3" t="n">
-        <v>46078.62641203704</v>
+        <v>46078.70737268519</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -8332,7 +8337,7 @@
         <v>1</v>
       </c>
       <c r="N121" s="3" t="n">
-        <v>46078.62087962963</v>
+        <v>46078.69997685185</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -8398,7 +8403,7 @@
         </is>
       </c>
       <c r="N122" s="3" t="n">
-        <v>46078.65241898148</v>
+        <v>46078.71435185185</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -8467,7 +8472,7 @@
         <v>2</v>
       </c>
       <c r="N123" s="3" t="n">
-        <v>46078.63115740741</v>
+        <v>46078.73043981481</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -8536,7 +8541,7 @@
         <v>1</v>
       </c>
       <c r="N124" s="3" t="n">
-        <v>46078.63758101852</v>
+        <v>46078.71516203704</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -8605,7 +8610,7 @@
         <v>1</v>
       </c>
       <c r="N125" s="3" t="n">
-        <v>46078.65012731482</v>
+        <v>46078.72989583333</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -8674,7 +8679,7 @@
         <v>2</v>
       </c>
       <c r="N126" s="3" t="n">
-        <v>46078.65243055556</v>
+        <v>46078.73196759259</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -8743,7 +8748,7 @@
         <v>2</v>
       </c>
       <c r="N127" s="3" t="n">
-        <v>46078.63252314815</v>
+        <v>46078.71207175926</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -8812,7 +8817,7 @@
         <v>1</v>
       </c>
       <c r="N128" s="3" t="n">
-        <v>46078.62909722222</v>
+        <v>46078.70385416667</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -8881,7 +8886,7 @@
         <v>1</v>
       </c>
       <c r="N129" s="3" t="n">
-        <v>46078.63635416667</v>
+        <v>46078.71693287037</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -8950,7 +8955,7 @@
         <v>1</v>
       </c>
       <c r="N130" s="3" t="n">
-        <v>46078.65289351852</v>
+        <v>46078.72685185185</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -8969,11 +8974,6 @@
           <t>ADM/FIN</t>
         </is>
       </c>
-      <c r="C131" t="inlineStr">
-        <is>
-          <t>10.69.3.6</t>
-        </is>
-      </c>
       <c r="D131" t="n">
         <v>2025</v>
       </c>
@@ -9019,7 +9019,7 @@
         <v>1</v>
       </c>
       <c r="N131" s="3" t="n">
-        <v>46078.64614583334</v>
+        <v>46078.68429398148</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -9152,7 +9152,7 @@
         <v>1</v>
       </c>
       <c r="N133" s="3" t="n">
-        <v>46078.64706018518</v>
+        <v>46078.7259837963</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -9216,7 +9216,7 @@
         <v>1</v>
       </c>
       <c r="N134" s="3" t="n">
-        <v>46078.65225694444</v>
+        <v>46078.73136574074</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -9280,7 +9280,7 @@
         <v>1</v>
       </c>
       <c r="N135" s="3" t="n">
-        <v>46078.62599537037</v>
+        <v>46078.70425925926</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -9471,7 +9471,7 @@
         <v>1</v>
       </c>
       <c r="N138" s="3" t="n">
-        <v>46078.64166666667</v>
+        <v>46078.71447916667</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9535,7 +9535,7 @@
         <v>1</v>
       </c>
       <c r="N139" s="3" t="n">
-        <v>46078.62056712963</v>
+        <v>46078.73390046296</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9599,7 +9599,7 @@
         <v>1</v>
       </c>
       <c r="N140" s="3" t="n">
-        <v>46078.64896990741</v>
+        <v>46078.72938657407</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9663,7 +9663,7 @@
         <v>1</v>
       </c>
       <c r="N141" s="3" t="n">
-        <v>46078.62148148148</v>
+        <v>46078.70391203704</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9727,7 +9727,7 @@
         <v>1</v>
       </c>
       <c r="N142" s="3" t="n">
-        <v>46078.6445949074</v>
+        <v>46078.72481481481</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9791,7 +9791,7 @@
         <v>1</v>
       </c>
       <c r="N143" s="3" t="n">
-        <v>46078.62886574074</v>
+        <v>46078.71155092592</v>
       </c>
       <c r="O143" t="inlineStr">
         <is>
@@ -9855,7 +9855,7 @@
         <v>1</v>
       </c>
       <c r="N144" s="3" t="n">
-        <v>46078.65446759259</v>
+        <v>46078.73494212963</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9919,7 +9919,7 @@
         <v>1</v>
       </c>
       <c r="N145" s="3" t="n">
-        <v>46078.62118055556</v>
+        <v>46078.7371875</v>
       </c>
       <c r="O145" t="inlineStr">
         <is>
@@ -9983,7 +9983,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="3" t="n">
-        <v>46078.62097222222</v>
+        <v>46078.70028935185</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10047,7 +10047,7 @@
         <v>1</v>
       </c>
       <c r="N147" s="3" t="n">
-        <v>46078.54922453704</v>
+        <v>46078.73190972222</v>
       </c>
       <c r="O147" t="inlineStr">
         <is>
@@ -10111,7 +10111,7 @@
         <v>1</v>
       </c>
       <c r="N148" s="3" t="n">
-        <v>46078.6447800926</v>
+        <v>46078.68680555555</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10175,7 +10175,7 @@
         <v>1</v>
       </c>
       <c r="N149" s="3" t="n">
-        <v>46078.64045138889</v>
+        <v>46078.71895833333</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -10239,7 +10239,7 @@
         <v>1</v>
       </c>
       <c r="N150" s="3" t="n">
-        <v>46078.62663194445</v>
+        <v>46078.70731481481</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -10303,7 +10303,7 @@
         <v>1</v>
       </c>
       <c r="N151" s="3" t="n">
-        <v>46078.62715277778</v>
+        <v>46078.70539351852</v>
       </c>
       <c r="O151" t="inlineStr">
         <is>
@@ -10367,7 +10367,7 @@
         <v>1</v>
       </c>
       <c r="N152" s="3" t="n">
-        <v>46078.62174768518</v>
+        <v>46078.72820601852</v>
       </c>
       <c r="O152" t="inlineStr">
         <is>
@@ -10490,7 +10490,7 @@
         <v>1</v>
       </c>
       <c r="N154" s="3" t="n">
-        <v>46078.61708333333</v>
+        <v>46078.7377662037</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10554,7 +10554,7 @@
         <v>1</v>
       </c>
       <c r="N155" s="3" t="n">
-        <v>46078.64184027778</v>
+        <v>46078.71418981482</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10810,7 +10810,7 @@
         <v>1</v>
       </c>
       <c r="N159" s="3" t="n">
-        <v>46078.63446759259</v>
+        <v>46078.71728009259</v>
       </c>
       <c r="O159" t="inlineStr">
         <is>
@@ -10938,7 +10938,7 @@
         <v>1</v>
       </c>
       <c r="N161" s="3" t="n">
-        <v>46078.62905092593</v>
+        <v>46078.70913194444</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -11002,7 +11002,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="3" t="n">
-        <v>46078.63310185185</v>
+        <v>46078.71184027778</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11130,7 +11130,7 @@
         <v>2</v>
       </c>
       <c r="N164" s="3" t="n">
-        <v>46078.62606481482</v>
+        <v>46078.70701388889</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11194,7 +11194,7 @@
         <v>2</v>
       </c>
       <c r="N165" s="3" t="n">
-        <v>46078.64303240741</v>
+        <v>46078.71900462963</v>
       </c>
       <c r="O165" t="inlineStr">
         <is>
@@ -11450,7 +11450,7 @@
         <v>2</v>
       </c>
       <c r="N169" s="3" t="n">
-        <v>46078.63847222222</v>
+        <v>46078.71163194445</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -11514,7 +11514,7 @@
         <v>2</v>
       </c>
       <c r="N170" s="3" t="n">
-        <v>46078.64467592593</v>
+        <v>46078.72520833334</v>
       </c>
       <c r="O170" t="inlineStr">
         <is>
@@ -11642,7 +11642,7 @@
         <v>2</v>
       </c>
       <c r="N172" s="3" t="n">
-        <v>46078.62841435185</v>
+        <v>46078.70452546296</v>
       </c>
       <c r="O172" t="inlineStr">
         <is>
@@ -11706,7 +11706,7 @@
         <v>2</v>
       </c>
       <c r="N173" s="3" t="n">
-        <v>46078.6427662037</v>
+        <v>46078.72114583333</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -11834,7 +11834,7 @@
         <v>2</v>
       </c>
       <c r="N175" s="3" t="n">
-        <v>46078.65278935185</v>
+        <v>46078.73321759259</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -11898,7 +11898,7 @@
         <v>2</v>
       </c>
       <c r="N176" s="3" t="n">
-        <v>46078.61819444445</v>
+        <v>46078.65570601852</v>
       </c>
       <c r="O176" t="inlineStr">
         <is>
@@ -11962,7 +11962,7 @@
         <v>2</v>
       </c>
       <c r="N177" s="3" t="n">
-        <v>46078.61791666667</v>
+        <v>46078.69855324074</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
@@ -12026,7 +12026,7 @@
         <v>2</v>
       </c>
       <c r="N178" s="3" t="n">
-        <v>46078.63988425926</v>
+        <v>46078.71924768519</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12090,7 +12090,7 @@
         <v>1</v>
       </c>
       <c r="N179" s="3" t="n">
-        <v>46078.63153935185</v>
+        <v>46078.70567129629</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12154,7 +12154,7 @@
         <v>1</v>
       </c>
       <c r="N180" s="3" t="n">
-        <v>46078.61775462963</v>
+        <v>46078.69734953704</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12218,7 +12218,7 @@
         <v>1</v>
       </c>
       <c r="N181" s="3" t="n">
-        <v>46078.63964120371</v>
+        <v>46078.7147337963</v>
       </c>
       <c r="O181" t="inlineStr">
         <is>
@@ -12607,7 +12607,7 @@
         <v>1</v>
       </c>
       <c r="N187" s="3" t="n">
-        <v>46078.63028935185</v>
+        <v>46078.7059837963</v>
       </c>
       <c r="O187" t="inlineStr">
         <is>
@@ -12799,7 +12799,7 @@
         </is>
       </c>
       <c r="N190" s="3" t="n">
-        <v>46078.62180555556</v>
+        <v>46078.69872685185</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12863,7 +12863,7 @@
         <v>1</v>
       </c>
       <c r="N191" s="3" t="n">
-        <v>46078.62324074074</v>
+        <v>46078.70435185185</v>
       </c>
       <c r="O191" t="inlineStr">
         <is>
@@ -12927,7 +12927,7 @@
         <v>1</v>
       </c>
       <c r="N192" s="3" t="n">
-        <v>46078.63185185185</v>
+        <v>46078.70978009259</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -13116,7 +13116,7 @@
         <v>1</v>
       </c>
       <c r="N195" s="3" t="n">
-        <v>46078.61908564815</v>
+        <v>46078.7358912037</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13372,7 +13372,7 @@
         <v>1</v>
       </c>
       <c r="N199" s="3" t="n">
-        <v>46078.64041666667</v>
+        <v>46078.71614583334</v>
       </c>
       <c r="O199" t="inlineStr">
         <is>
@@ -13436,7 +13436,7 @@
         <v>1</v>
       </c>
       <c r="N200" s="3" t="n">
-        <v>46078.63975694445</v>
+        <v>46078.71329861111</v>
       </c>
       <c r="O200" t="inlineStr">
         <is>
@@ -13497,7 +13497,7 @@
         </is>
       </c>
       <c r="N201" s="3" t="n">
-        <v>46078.63099537037</v>
+        <v>46078.70219907408</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -13561,7 +13561,7 @@
         <v>1</v>
       </c>
       <c r="N202" s="3" t="n">
-        <v>46078.62569444445</v>
+        <v>46078.70159722222</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13625,7 +13625,7 @@
         <v>1</v>
       </c>
       <c r="N203" s="3" t="n">
-        <v>46078.62173611111</v>
+        <v>46078.69952546297</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13689,7 +13689,7 @@
         <v>1</v>
       </c>
       <c r="N204" s="3" t="n">
-        <v>46078.61515046296</v>
+        <v>46078.73802083333</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13753,7 +13753,7 @@
         <v>1</v>
       </c>
       <c r="N205" s="3" t="n">
-        <v>46078.63435185186</v>
+        <v>46078.71168981482</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13817,7 +13817,7 @@
         <v>1</v>
       </c>
       <c r="N206" s="3" t="n">
-        <v>46078.63149305555</v>
+        <v>46078.70891203704</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -13881,7 +13881,7 @@
         <v>1</v>
       </c>
       <c r="N207" s="3" t="n">
-        <v>46078.65363425926</v>
+        <v>46078.73577546296</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -14009,7 +14009,7 @@
         <v>1</v>
       </c>
       <c r="N209" s="3" t="n">
-        <v>46078.63021990741</v>
+        <v>46078.70732638889</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14073,7 +14073,7 @@
         <v>1</v>
       </c>
       <c r="N210" s="3" t="n">
-        <v>46078.6437962963</v>
+        <v>46078.72394675926</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14137,7 +14137,7 @@
         <v>1</v>
       </c>
       <c r="N211" s="3" t="n">
-        <v>46078.63957175926</v>
+        <v>46078.71479166667</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -14201,7 +14201,7 @@
         <v>1</v>
       </c>
       <c r="N212" s="3" t="n">
-        <v>46078.62751157407</v>
+        <v>46078.70280092592</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -14265,7 +14265,7 @@
         <v>1</v>
       </c>
       <c r="N213" s="3" t="n">
-        <v>46078.63978009259</v>
+        <v>46078.71846064815</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
@@ -14329,7 +14329,7 @@
         <v>1</v>
       </c>
       <c r="N214" s="3" t="n">
-        <v>46078.63913194444</v>
+        <v>46078.71346064815</v>
       </c>
       <c r="O214" t="inlineStr">
         <is>
@@ -14393,7 +14393,7 @@
         <v>1</v>
       </c>
       <c r="N215" s="3" t="n">
-        <v>46078.63936342593</v>
+        <v>46078.71666666667</v>
       </c>
       <c r="O215" t="inlineStr">
         <is>
@@ -14457,7 +14457,7 @@
         <v>1</v>
       </c>
       <c r="N216" s="3" t="n">
-        <v>46078.62537037037</v>
+        <v>46078.70054398148</v>
       </c>
       <c r="O216" t="inlineStr">
         <is>
@@ -14521,7 +14521,7 @@
         <v>1</v>
       </c>
       <c r="N217" s="3" t="n">
-        <v>46078.64325231482</v>
+        <v>46078.72100694444</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14585,7 +14585,7 @@
         <v>1</v>
       </c>
       <c r="N218" s="3" t="n">
-        <v>46078.63256944445</v>
+        <v>46078.7077199074</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14649,7 +14649,7 @@
         <v>1</v>
       </c>
       <c r="N219" s="3" t="n">
-        <v>46078.62384259259</v>
+        <v>46078.70319444445</v>
       </c>
       <c r="O219" t="inlineStr">
         <is>
@@ -14718,7 +14718,7 @@
         <v>1</v>
       </c>
       <c r="N220" s="3" t="n">
-        <v>46078.6437037037</v>
+        <v>46078.71834490741</v>
       </c>
       <c r="O220" t="inlineStr">
         <is>
@@ -14782,7 +14782,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="3" t="n">
-        <v>46078.62417824074</v>
+        <v>46078.70407407408</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14846,7 +14846,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="3" t="n">
-        <v>46078.6206712963</v>
+        <v>46078.73457175926</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -14910,7 +14910,7 @@
         <v>1</v>
       </c>
       <c r="N223" s="3" t="n">
-        <v>46078.63645833333</v>
+        <v>46078.71403935185</v>
       </c>
       <c r="O223" t="inlineStr">
         <is>
@@ -14974,7 +14974,7 @@
         <v>1</v>
       </c>
       <c r="N224" s="3" t="n">
-        <v>46078.6459375</v>
+        <v>46078.72402777777</v>
       </c>
       <c r="O224" t="inlineStr">
         <is>
@@ -15038,7 +15038,7 @@
         <v>1</v>
       </c>
       <c r="N225" s="3" t="n">
-        <v>46078.63025462963</v>
+        <v>46078.70952546296</v>
       </c>
       <c r="O225" t="inlineStr">
         <is>
@@ -15102,7 +15102,7 @@
         <v>1</v>
       </c>
       <c r="N226" s="3" t="n">
-        <v>46078.65459490741</v>
+        <v>46078.73037037037</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15166,7 +15166,7 @@
         <v>1</v>
       </c>
       <c r="N227" s="3" t="n">
-        <v>46078.62581018519</v>
+        <v>46078.73547453704</v>
       </c>
       <c r="O227" t="inlineStr">
         <is>
@@ -15230,7 +15230,7 @@
         <v>1</v>
       </c>
       <c r="N228" s="3" t="n">
-        <v>46078.62380787037</v>
+        <v>46078.73762731482</v>
       </c>
       <c r="O228" t="inlineStr">
         <is>
@@ -15294,7 +15294,7 @@
         <v>1</v>
       </c>
       <c r="N229" s="3" t="n">
-        <v>46078.65040509259</v>
+        <v>46078.73215277777</v>
       </c>
       <c r="O229" t="inlineStr">
         <is>
@@ -15358,7 +15358,7 @@
         <v>1</v>
       </c>
       <c r="N230" s="3" t="n">
-        <v>46078.62075231481</v>
+        <v>46078.70083333334</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15422,7 +15422,7 @@
         <v>1</v>
       </c>
       <c r="N231" s="3" t="n">
-        <v>46078.6387962963</v>
+        <v>46078.7166087963</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15486,7 +15486,7 @@
         <v>1</v>
       </c>
       <c r="N232" s="3" t="n">
-        <v>46078.63377314815</v>
+        <v>46078.71194444445</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -15550,7 +15550,7 @@
         <v>1</v>
       </c>
       <c r="N233" s="3" t="n">
-        <v>46078.62729166666</v>
+        <v>46078.69993055556</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15614,7 +15614,7 @@
         <v>1</v>
       </c>
       <c r="N234" s="3" t="n">
-        <v>46078.6286574074</v>
+        <v>46078.70622685185</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -15678,7 +15678,7 @@
         <v>1</v>
       </c>
       <c r="N235" s="3" t="n">
-        <v>46078.61899305556</v>
+        <v>46078.73659722223</v>
       </c>
       <c r="O235" t="inlineStr">
         <is>
@@ -15742,7 +15742,7 @@
         <v>1</v>
       </c>
       <c r="N236" s="3" t="n">
-        <v>46078.64453703703</v>
+        <v>46078.72092592593</v>
       </c>
       <c r="O236" t="inlineStr">
         <is>
@@ -15806,7 +15806,7 @@
         <v>1</v>
       </c>
       <c r="N237" s="3" t="n">
-        <v>46078.63938657408</v>
+        <v>46078.71408564815</v>
       </c>
       <c r="O237" t="inlineStr">
         <is>
@@ -15870,7 +15870,7 @@
         <v>1</v>
       </c>
       <c r="N238" s="3" t="n">
-        <v>46078.63561342593</v>
+        <v>46078.71400462963</v>
       </c>
       <c r="O238" t="inlineStr">
         <is>
@@ -15934,7 +15934,7 @@
         <v>1</v>
       </c>
       <c r="N239" s="3" t="n">
-        <v>46078.63952546296</v>
+        <v>46078.71701388889</v>
       </c>
       <c r="O239" t="inlineStr">
         <is>
@@ -15998,7 +15998,7 @@
         <v>1</v>
       </c>
       <c r="N240" s="3" t="n">
-        <v>46078.62743055556</v>
+        <v>46078.70292824074</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16062,7 +16062,7 @@
         <v>1</v>
       </c>
       <c r="N241" s="3" t="n">
-        <v>46078.63944444444</v>
+        <v>46078.71195601852</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16126,7 +16126,7 @@
         <v>1</v>
       </c>
       <c r="N242" s="3" t="n">
-        <v>46078.63113425926</v>
+        <v>46078.71236111111</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16190,7 +16190,7 @@
         <v>1</v>
       </c>
       <c r="N243" s="3" t="n">
-        <v>46078.63947916667</v>
+        <v>46078.71484953703</v>
       </c>
       <c r="O243" t="inlineStr">
         <is>
@@ -16313,7 +16313,7 @@
         <v>1</v>
       </c>
       <c r="N245" s="3" t="n">
-        <v>46078.64873842592</v>
+        <v>46078.72578703704</v>
       </c>
       <c r="O245" t="inlineStr">
         <is>
@@ -16377,7 +16377,7 @@
         <v>1</v>
       </c>
       <c r="N246" s="3" t="n">
-        <v>46078.64141203704</v>
+        <v>46078.72346064815</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16441,7 +16441,7 @@
         <v>1</v>
       </c>
       <c r="N247" s="3" t="n">
-        <v>46078.63472222222</v>
+        <v>46078.70795138889</v>
       </c>
       <c r="O247" t="inlineStr">
         <is>
@@ -16505,7 +16505,7 @@
         <v>1</v>
       </c>
       <c r="N248" s="3" t="n">
-        <v>46078.6328587963</v>
+        <v>46078.71046296296</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16569,7 +16569,7 @@
         <v>1</v>
       </c>
       <c r="N249" s="3" t="n">
-        <v>46078.62634259259</v>
+        <v>46078.69980324074</v>
       </c>
       <c r="O249" t="inlineStr">
         <is>
@@ -16633,7 +16633,7 @@
         <v>1</v>
       </c>
       <c r="N250" s="3" t="n">
-        <v>46078.64</v>
+        <v>46078.71489583333</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16697,7 +16697,7 @@
         <v>1</v>
       </c>
       <c r="N251" s="3" t="n">
-        <v>46078.64005787037</v>
+        <v>46078.71981481482</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16761,7 +16761,7 @@
         <v>1</v>
       </c>
       <c r="N252" s="3" t="n">
-        <v>46078.64967592592</v>
+        <v>46078.72649305555</v>
       </c>
       <c r="O252" t="inlineStr">
         <is>
@@ -16825,7 +16825,7 @@
         <v>1</v>
       </c>
       <c r="N253" s="3" t="n">
-        <v>46078.62550925926</v>
+        <v>46078.7043287037</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16883,7 +16883,7 @@
         <v>1</v>
       </c>
       <c r="N254" s="3" t="n">
-        <v>46078.63756944444</v>
+        <v>46078.7346875</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -16947,7 +16947,7 @@
         <v>1</v>
       </c>
       <c r="N255" s="3" t="n">
-        <v>46078.63966435185</v>
+        <v>46078.73700231482</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -17011,7 +17011,7 @@
         <v>1</v>
       </c>
       <c r="N256" s="3" t="n">
-        <v>46078.6438425926</v>
+        <v>46078.72035879629</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17075,7 +17075,7 @@
         <v>1</v>
       </c>
       <c r="N257" s="3" t="n">
-        <v>46078.64716435185</v>
+        <v>46078.72258101852</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17139,7 +17139,7 @@
         <v>1</v>
       </c>
       <c r="N258" s="3" t="n">
-        <v>46078.63880787037</v>
+        <v>46078.7146875</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
@@ -17203,7 +17203,7 @@
         <v>1</v>
       </c>
       <c r="N259" s="3" t="n">
-        <v>46078.64032407408</v>
+        <v>46078.71515046297</v>
       </c>
       <c r="O259" t="inlineStr">
         <is>
@@ -17331,7 +17331,7 @@
         <v>1</v>
       </c>
       <c r="N261" s="3" t="n">
-        <v>46078.64159722222</v>
+        <v>46078.71563657407</v>
       </c>
       <c r="O261" t="inlineStr">
         <is>
@@ -17395,7 +17395,7 @@
         <v>1</v>
       </c>
       <c r="N262" s="3" t="n">
-        <v>46078.62449074074</v>
+        <v>46078.69908564815</v>
       </c>
       <c r="O262" t="inlineStr">
         <is>
@@ -17459,7 +17459,7 @@
         <v>1</v>
       </c>
       <c r="N263" s="3" t="n">
-        <v>46078.61869212963</v>
+        <v>46078.72571759259</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17523,7 +17523,7 @@
         <v>1</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>46078.64130787037</v>
+        <v>46078.72104166666</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17587,7 +17587,7 @@
         <v>1</v>
       </c>
       <c r="N265" s="3" t="n">
-        <v>46078.62777777778</v>
+        <v>46078.70638888889</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17715,7 +17715,7 @@
         <v>1</v>
       </c>
       <c r="N267" s="3" t="n">
-        <v>46078.64559027777</v>
+        <v>46078.72273148148</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17779,7 +17779,7 @@
         <v>1</v>
       </c>
       <c r="N268" s="3" t="n">
-        <v>46078.65158564815</v>
+        <v>46078.73215277777</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17843,7 +17843,7 @@
         <v>1</v>
       </c>
       <c r="N269" s="3" t="n">
-        <v>46078.62967592593</v>
+        <v>46078.70392361111</v>
       </c>
       <c r="O269" t="inlineStr">
         <is>
@@ -17904,7 +17904,7 @@
         </is>
       </c>
       <c r="N270" s="3" t="n">
-        <v>46078.63883101852</v>
+        <v>46078.71869212963</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -18416,7 +18416,7 @@
         <v>1</v>
       </c>
       <c r="N278" s="3" t="n">
-        <v>46078.63351851852</v>
+        <v>46078.70655092593</v>
       </c>
       <c r="O278" t="inlineStr">
         <is>
@@ -18480,7 +18480,7 @@
         <v>1</v>
       </c>
       <c r="N279" s="3" t="n">
-        <v>46078.64271990741</v>
+        <v>46078.69969907407</v>
       </c>
       <c r="O279" t="inlineStr">
         <is>
@@ -18731,7 +18731,7 @@
         <v>1</v>
       </c>
       <c r="N283" s="3" t="n">
-        <v>46078.65328703704</v>
+        <v>46078.73538194445</v>
       </c>
       <c r="O283" t="inlineStr">
         <is>
@@ -18795,7 +18795,7 @@
         <v>1</v>
       </c>
       <c r="N284" s="3" t="n">
-        <v>46078.63818287037</v>
+        <v>46078.71141203704</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18859,7 +18859,7 @@
         <v>1</v>
       </c>
       <c r="N285" s="3" t="n">
-        <v>46078.62998842593</v>
+        <v>46078.70327546296</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -18982,7 +18982,7 @@
         <v>1</v>
       </c>
       <c r="N287" s="3" t="n">
-        <v>46078.64945601852</v>
+        <v>46078.72793981482</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
@@ -19110,7 +19110,7 @@
         <v>1</v>
       </c>
       <c r="N289" s="3" t="n">
-        <v>46078.64796296296</v>
+        <v>46078.72037037037</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -19904,7 +19904,7 @@
         <v>1</v>
       </c>
       <c r="N302" s="3" t="n">
-        <v>46078.63231481481</v>
+        <v>46078.70657407407</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -20645,7 +20645,7 @@
         </is>
       </c>
       <c r="N314" s="3" t="n">
-        <v>46078.62900462963</v>
+        <v>46078.70356481482</v>
       </c>
       <c r="O314" t="inlineStr">
         <is>
@@ -21020,7 +21020,7 @@
         </is>
       </c>
       <c r="N320" s="3" t="n">
-        <v>46078.61966435185</v>
+        <v>46078.73123842593</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21745,7 +21745,7 @@
         <v>1</v>
       </c>
       <c r="N332" s="3" t="n">
-        <v>46078.62871527778</v>
+        <v>46078.70275462963</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21809,7 +21809,7 @@
         <v>2</v>
       </c>
       <c r="N333" s="3" t="n">
-        <v>46078.62116898148</v>
+        <v>46078.73445601852</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21873,7 +21873,7 @@
         <v>2</v>
       </c>
       <c r="N334" s="3" t="n">
-        <v>46078.63637731481</v>
+        <v>46078.71582175926</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21937,7 +21937,7 @@
         <v>2</v>
       </c>
       <c r="N335" s="3" t="n">
-        <v>46078.63046296296</v>
+        <v>46078.70298611111</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -22001,7 +22001,7 @@
         <v>1</v>
       </c>
       <c r="N336" s="3" t="n">
-        <v>46078.63217592592</v>
+        <v>46078.70303240741</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22065,7 +22065,7 @@
         <v>1</v>
       </c>
       <c r="N337" s="3" t="n">
-        <v>46078.64321759259</v>
+        <v>46078.7205787037</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22129,7 +22129,7 @@
         <v>2</v>
       </c>
       <c r="N338" s="3" t="n">
-        <v>46078.64625</v>
+        <v>46078.72797453704</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -22193,7 +22193,7 @@
         <v>2</v>
       </c>
       <c r="N339" s="3" t="n">
-        <v>46078.63417824074</v>
+        <v>46078.713125</v>
       </c>
       <c r="O339" t="inlineStr">
         <is>
@@ -22446,7 +22446,7 @@
         </is>
       </c>
       <c r="N343" s="3" t="n">
-        <v>46078.63077546296</v>
+        <v>46078.70171296296</v>
       </c>
       <c r="O343" t="inlineStr">
         <is>
@@ -23831,7 +23831,7 @@
         <v>1</v>
       </c>
       <c r="N365" s="3" t="n">
-        <v>46078.63043981481</v>
+        <v>46078.67153935185</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
@@ -23897,7 +23897,7 @@
         </is>
       </c>
       <c r="N366" s="3" t="n">
-        <v>46078.63236111111</v>
+        <v>46078.70841435185</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -24023,7 +24023,7 @@
         </is>
       </c>
       <c r="N368" s="3" t="n">
-        <v>46078.6290162037</v>
+        <v>46078.70872685185</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -24089,7 +24089,7 @@
         </is>
       </c>
       <c r="N369" s="3" t="n">
-        <v>46078.6425</v>
+        <v>46078.72190972222</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
@@ -24158,7 +24158,7 @@
         <v>1</v>
       </c>
       <c r="N370" s="3" t="n">
-        <v>46078.63587962963</v>
+        <v>46078.70878472222</v>
       </c>
       <c r="O370" t="inlineStr">
         <is>
@@ -24227,7 +24227,7 @@
         <v>1</v>
       </c>
       <c r="N371" s="3" t="n">
-        <v>46078.64103009259</v>
+        <v>46078.68076388889</v>
       </c>
       <c r="O371" t="inlineStr">
         <is>
@@ -24431,7 +24431,7 @@
         <v>1</v>
       </c>
       <c r="N374" s="3" t="n">
-        <v>46078.62300925926</v>
+        <v>46078.69993055556</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24497,7 +24497,7 @@
         </is>
       </c>
       <c r="N375" s="3" t="n">
-        <v>46078.62302083334</v>
+        <v>46078.70127314814</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
@@ -24561,7 +24561,7 @@
         <v>1</v>
       </c>
       <c r="N376" s="3" t="n">
-        <v>46078.6282175926</v>
+        <v>46078.70834490741</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -24630,7 +24630,7 @@
         <v>2</v>
       </c>
       <c r="N377" s="3" t="n">
-        <v>46078.64170138889</v>
+        <v>46078.72466435185</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -24699,7 +24699,7 @@
         <v>2</v>
       </c>
       <c r="N378" s="3" t="n">
-        <v>46078.64489583333</v>
+        <v>46078.72149305556</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização automática 2026-02-26 09:52:05.691068
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>46078.71922453704</v>
+        <v>46079.37276620371</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>46078.71548611111</v>
+        <v>46079.37380787037</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -739,10 +739,10 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>46078.69167824074</v>
+        <v>46079.39236111111</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>46078.72538194444</v>
+        <v>46079.375625</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -944,7 +944,7 @@
         <v>1</v>
       </c>
       <c r="N7" s="3" t="n">
-        <v>46078.70773148148</v>
+        <v>46078.89480324074</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -1643,7 +1643,7 @@
         <v>2</v>
       </c>
       <c r="N18" s="3" t="n">
-        <v>46078.73734953703</v>
+        <v>46079.40050925926</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1768,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="N20" s="3" t="n">
-        <v>46078.70361111111</v>
+        <v>46079.38277777778</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1969,11 +1969,6 @@
           <t>AUDITORIO</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>10.69.3.150</t>
-        </is>
-      </c>
       <c r="D24" t="n">
         <v>2019</v>
       </c>
@@ -2014,7 +2009,7 @@
         <v>1</v>
       </c>
       <c r="N24" s="3" t="n">
-        <v>46078.73511574074</v>
+        <v>46079.19900462963</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -6644,7 +6639,7 @@
         <v>1</v>
       </c>
       <c r="N96" s="3" t="n">
-        <v>46078.7325462963</v>
+        <v>46078.81081018518</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
@@ -6708,7 +6703,7 @@
         <v>1</v>
       </c>
       <c r="N97" s="3" t="n">
-        <v>46078.69038194444</v>
+        <v>46079.37601851852</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -6727,11 +6722,6 @@
           <t>COORDENACAO</t>
         </is>
       </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>10.69.3.94</t>
-        </is>
-      </c>
       <c r="D98" t="n">
         <v>2025</v>
       </c>
@@ -6777,7 +6767,7 @@
         <v>1</v>
       </c>
       <c r="N98" s="3" t="n">
-        <v>46078.71636574074</v>
+        <v>46079.38182870371</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -6846,7 +6836,7 @@
         <v>1</v>
       </c>
       <c r="N99" s="3" t="n">
-        <v>46078.70243055555</v>
+        <v>46079.38302083333</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -6915,7 +6905,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>46078.72143518519</v>
+        <v>46079.38922453704</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6984,7 +6974,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="3" t="n">
-        <v>46078.71096064815</v>
+        <v>46079.38803240741</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -7122,7 +7112,7 @@
         <v>2</v>
       </c>
       <c r="N103" s="3" t="n">
-        <v>46078.71195601852</v>
+        <v>46079.37818287037</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7382,7 +7372,7 @@
         <v>1</v>
       </c>
       <c r="N107" s="3" t="n">
-        <v>46078.66605324074</v>
+        <v>46079.37074074074</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -7520,7 +7510,7 @@
         <v>1</v>
       </c>
       <c r="N109" s="3" t="n">
-        <v>46078.72763888889</v>
+        <v>46079.39797453704</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7589,7 +7579,7 @@
         <v>2</v>
       </c>
       <c r="N110" s="3" t="n">
-        <v>46078.70770833334</v>
+        <v>46079.38300925926</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7658,7 +7648,7 @@
         <v>2</v>
       </c>
       <c r="N111" s="3" t="n">
-        <v>46078.70545138889</v>
+        <v>46079.36805555555</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
@@ -7727,7 +7717,7 @@
         <v>2</v>
       </c>
       <c r="N112" s="3" t="n">
-        <v>46078.71792824074</v>
+        <v>46079.37113425926</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7796,7 +7786,7 @@
         <v>1</v>
       </c>
       <c r="N113" s="3" t="n">
-        <v>46078.70827546297</v>
+        <v>46079.39659722222</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7865,7 +7855,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>46078.7075462963</v>
+        <v>46079.40396990741</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -7931,7 +7921,7 @@
         </is>
       </c>
       <c r="N115" s="3" t="n">
-        <v>46078.68179398148</v>
+        <v>46079.37898148148</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -8000,7 +7990,7 @@
         <v>1</v>
       </c>
       <c r="N116" s="3" t="n">
-        <v>46078.67899305555</v>
+        <v>46079.38185185185</v>
       </c>
       <c r="O116" t="inlineStr">
         <is>
@@ -8064,7 +8054,7 @@
         <v>1</v>
       </c>
       <c r="N117" s="3" t="n">
-        <v>46078.70715277778</v>
+        <v>46079.36695601852</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -8130,7 +8120,7 @@
         </is>
       </c>
       <c r="N118" s="3" t="n">
-        <v>46078.68390046297</v>
+        <v>46079.38075231481</v>
       </c>
       <c r="O118" t="inlineStr">
         <is>
@@ -8268,7 +8258,7 @@
         <v>1</v>
       </c>
       <c r="N120" s="3" t="n">
-        <v>46078.70737268519</v>
+        <v>46079.39700231481</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -8337,7 +8327,7 @@
         <v>1</v>
       </c>
       <c r="N121" s="3" t="n">
-        <v>46078.69997685185</v>
+        <v>46079.38952546296</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -8403,7 +8393,7 @@
         </is>
       </c>
       <c r="N122" s="3" t="n">
-        <v>46078.71435185185</v>
+        <v>46079.37047453703</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -8472,7 +8462,7 @@
         <v>2</v>
       </c>
       <c r="N123" s="3" t="n">
-        <v>46078.73043981481</v>
+        <v>46079.30954861111</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -8541,7 +8531,7 @@
         <v>1</v>
       </c>
       <c r="N124" s="3" t="n">
-        <v>46078.71516203704</v>
+        <v>46079.37851851852</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -8610,7 +8600,7 @@
         <v>1</v>
       </c>
       <c r="N125" s="3" t="n">
-        <v>46078.72989583333</v>
+        <v>46079.39939814815</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -8679,7 +8669,7 @@
         <v>2</v>
       </c>
       <c r="N126" s="3" t="n">
-        <v>46078.73196759259</v>
+        <v>46078.77155092593</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -8748,7 +8738,7 @@
         <v>2</v>
       </c>
       <c r="N127" s="3" t="n">
-        <v>46078.71207175926</v>
+        <v>46079.3693287037</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -8817,7 +8807,7 @@
         <v>1</v>
       </c>
       <c r="N128" s="3" t="n">
-        <v>46078.70385416667</v>
+        <v>46079.37707175926</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -8886,7 +8876,7 @@
         <v>1</v>
       </c>
       <c r="N129" s="3" t="n">
-        <v>46078.71693287037</v>
+        <v>46079.39829861111</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -8955,7 +8945,7 @@
         <v>1</v>
       </c>
       <c r="N130" s="3" t="n">
-        <v>46078.72685185185</v>
+        <v>46079.36809027778</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -8974,6 +8964,11 @@
           <t>ADM/FIN</t>
         </is>
       </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>10.69.3.6</t>
+        </is>
+      </c>
       <c r="D131" t="n">
         <v>2025</v>
       </c>
@@ -9019,7 +9014,7 @@
         <v>1</v>
       </c>
       <c r="N131" s="3" t="n">
-        <v>46078.68429398148</v>
+        <v>46079.38357638889</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -9152,7 +9147,7 @@
         <v>1</v>
       </c>
       <c r="N133" s="3" t="n">
-        <v>46078.7259837963</v>
+        <v>46078.80311342593</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -9216,7 +9211,7 @@
         <v>1</v>
       </c>
       <c r="N134" s="3" t="n">
-        <v>46078.73136574074</v>
+        <v>46078.84300925926</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -9280,7 +9275,7 @@
         <v>1</v>
       </c>
       <c r="N135" s="3" t="n">
-        <v>46078.70425925926</v>
+        <v>46078.81565972222</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -9471,7 +9466,7 @@
         <v>1</v>
       </c>
       <c r="N138" s="3" t="n">
-        <v>46078.71447916667</v>
+        <v>46079.37739583333</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9535,7 +9530,7 @@
         <v>1</v>
       </c>
       <c r="N139" s="3" t="n">
-        <v>46078.73390046296</v>
+        <v>46079.36962962963</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9599,7 +9594,7 @@
         <v>1</v>
       </c>
       <c r="N140" s="3" t="n">
-        <v>46078.72938657407</v>
+        <v>46079.38509259259</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9663,7 +9658,7 @@
         <v>1</v>
       </c>
       <c r="N141" s="3" t="n">
-        <v>46078.70391203704</v>
+        <v>46079.37163194444</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9727,7 +9722,7 @@
         <v>1</v>
       </c>
       <c r="N142" s="3" t="n">
-        <v>46078.72481481481</v>
+        <v>46079.39322916666</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9791,7 +9786,7 @@
         <v>1</v>
       </c>
       <c r="N143" s="3" t="n">
-        <v>46078.71155092592</v>
+        <v>46079.39385416666</v>
       </c>
       <c r="O143" t="inlineStr">
         <is>
@@ -9855,7 +9850,7 @@
         <v>1</v>
       </c>
       <c r="N144" s="3" t="n">
-        <v>46078.73494212963</v>
+        <v>46079.39171296296</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9919,7 +9914,7 @@
         <v>1</v>
       </c>
       <c r="N145" s="3" t="n">
-        <v>46078.7371875</v>
+        <v>46078.81521990741</v>
       </c>
       <c r="O145" t="inlineStr">
         <is>
@@ -9983,7 +9978,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="3" t="n">
-        <v>46078.70028935185</v>
+        <v>46079.3783912037</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10047,7 +10042,7 @@
         <v>1</v>
       </c>
       <c r="N147" s="3" t="n">
-        <v>46078.73190972222</v>
+        <v>46079.40283564815</v>
       </c>
       <c r="O147" t="inlineStr">
         <is>
@@ -10111,7 +10106,7 @@
         <v>1</v>
       </c>
       <c r="N148" s="3" t="n">
-        <v>46078.68680555555</v>
+        <v>46079.38275462963</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10175,7 +10170,7 @@
         <v>1</v>
       </c>
       <c r="N149" s="3" t="n">
-        <v>46078.71895833333</v>
+        <v>46079.37759259259</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -10239,7 +10234,7 @@
         <v>1</v>
       </c>
       <c r="N150" s="3" t="n">
-        <v>46078.70731481481</v>
+        <v>46079.39837962963</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -10303,7 +10298,7 @@
         <v>1</v>
       </c>
       <c r="N151" s="3" t="n">
-        <v>46078.70539351852</v>
+        <v>46078.82223379629</v>
       </c>
       <c r="O151" t="inlineStr">
         <is>
@@ -10367,7 +10362,7 @@
         <v>1</v>
       </c>
       <c r="N152" s="3" t="n">
-        <v>46078.72820601852</v>
+        <v>46079.38721064815</v>
       </c>
       <c r="O152" t="inlineStr">
         <is>
@@ -10386,6 +10381,11 @@
           <t>OPERACAO 7.1</t>
         </is>
       </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>10.69.5.21</t>
+        </is>
+      </c>
       <c r="D153" t="n">
         <v>2018</v>
       </c>
@@ -10426,7 +10426,7 @@
         <v>1</v>
       </c>
       <c r="N153" s="3" t="n">
-        <v>46078.60457175926</v>
+        <v>46079.3779050926</v>
       </c>
       <c r="O153" t="inlineStr">
         <is>
@@ -10490,7 +10490,7 @@
         <v>1</v>
       </c>
       <c r="N154" s="3" t="n">
-        <v>46078.7377662037</v>
+        <v>46079.36612268518</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10554,7 +10554,7 @@
         <v>1</v>
       </c>
       <c r="N155" s="3" t="n">
-        <v>46078.71418981482</v>
+        <v>46079.37496527778</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10618,7 +10618,7 @@
         <v>1</v>
       </c>
       <c r="N156" s="3" t="n">
-        <v>46078.54244212963</v>
+        <v>46079.39541666667</v>
       </c>
       <c r="O156" t="inlineStr">
         <is>
@@ -10682,7 +10682,7 @@
         <v>1</v>
       </c>
       <c r="N157" s="3" t="n">
-        <v>46078.53774305555</v>
+        <v>46079.37704861111</v>
       </c>
       <c r="O157" t="inlineStr">
         <is>
@@ -10746,7 +10746,7 @@
         <v>1</v>
       </c>
       <c r="N158" s="3" t="n">
-        <v>46078.56077546296</v>
+        <v>46079.37501157408</v>
       </c>
       <c r="O158" t="inlineStr">
         <is>
@@ -10810,7 +10810,7 @@
         <v>1</v>
       </c>
       <c r="N159" s="3" t="n">
-        <v>46078.71728009259</v>
+        <v>46079.3955787037</v>
       </c>
       <c r="O159" t="inlineStr">
         <is>
@@ -10874,7 +10874,7 @@
         <v>1</v>
       </c>
       <c r="N160" s="3" t="n">
-        <v>46078.56958333333</v>
+        <v>46079.37181712963</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
@@ -10938,7 +10938,7 @@
         <v>1</v>
       </c>
       <c r="N161" s="3" t="n">
-        <v>46078.70913194444</v>
+        <v>46079.37488425926</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -11002,7 +11002,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="3" t="n">
-        <v>46078.71184027778</v>
+        <v>46079.37144675926</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11130,7 +11130,7 @@
         <v>2</v>
       </c>
       <c r="N164" s="3" t="n">
-        <v>46078.70701388889</v>
+        <v>46079.40444444444</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11194,7 +11194,7 @@
         <v>2</v>
       </c>
       <c r="N165" s="3" t="n">
-        <v>46078.71900462963</v>
+        <v>46079.37037037037</v>
       </c>
       <c r="O165" t="inlineStr">
         <is>
@@ -11258,7 +11258,7 @@
         <v>2</v>
       </c>
       <c r="N166" s="3" t="n">
-        <v>46078.60667824074</v>
+        <v>46079.37417824074</v>
       </c>
       <c r="O166" t="inlineStr">
         <is>
@@ -11319,10 +11319,10 @@
         </is>
       </c>
       <c r="M167" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N167" s="3" t="n">
-        <v>46078.605</v>
+        <v>46079.36737268518</v>
       </c>
       <c r="O167" t="inlineStr">
         <is>
@@ -11386,7 +11386,7 @@
         <v>2</v>
       </c>
       <c r="N168" s="3" t="n">
-        <v>46078.54982638889</v>
+        <v>46079.37060185185</v>
       </c>
       <c r="O168" t="inlineStr">
         <is>
@@ -11450,7 +11450,7 @@
         <v>2</v>
       </c>
       <c r="N169" s="3" t="n">
-        <v>46078.71163194445</v>
+        <v>46079.37075231481</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -11514,7 +11514,7 @@
         <v>2</v>
       </c>
       <c r="N170" s="3" t="n">
-        <v>46078.72520833334</v>
+        <v>46079.39797453704</v>
       </c>
       <c r="O170" t="inlineStr">
         <is>
@@ -11578,7 +11578,7 @@
         <v>1</v>
       </c>
       <c r="N171" s="3" t="n">
-        <v>46078.57716435185</v>
+        <v>46079.36778935185</v>
       </c>
       <c r="O171" t="inlineStr">
         <is>
@@ -11642,7 +11642,7 @@
         <v>2</v>
       </c>
       <c r="N172" s="3" t="n">
-        <v>46078.70452546296</v>
+        <v>46078.77956018518</v>
       </c>
       <c r="O172" t="inlineStr">
         <is>
@@ -11703,10 +11703,10 @@
         </is>
       </c>
       <c r="M173" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N173" s="3" t="n">
-        <v>46078.72114583333</v>
+        <v>46079.38108796296</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -11770,7 +11770,7 @@
         <v>2</v>
       </c>
       <c r="N174" s="3" t="n">
-        <v>46078.55256944444</v>
+        <v>46079.40034722222</v>
       </c>
       <c r="O174" t="inlineStr">
         <is>
@@ -11834,7 +11834,7 @@
         <v>2</v>
       </c>
       <c r="N175" s="3" t="n">
-        <v>46078.73321759259</v>
+        <v>46079.3779050926</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -12026,7 +12026,7 @@
         <v>2</v>
       </c>
       <c r="N178" s="3" t="n">
-        <v>46078.71924768519</v>
+        <v>46079.399375</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12090,7 +12090,7 @@
         <v>1</v>
       </c>
       <c r="N179" s="3" t="n">
-        <v>46078.70567129629</v>
+        <v>46079.36613425926</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12154,7 +12154,7 @@
         <v>1</v>
       </c>
       <c r="N180" s="3" t="n">
-        <v>46078.69734953704</v>
+        <v>46079.37844907407</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12218,7 +12218,7 @@
         <v>1</v>
       </c>
       <c r="N181" s="3" t="n">
-        <v>46078.7147337963</v>
+        <v>46079.39989583333</v>
       </c>
       <c r="O181" t="inlineStr">
         <is>
@@ -12346,7 +12346,7 @@
         <v>1</v>
       </c>
       <c r="N183" s="3" t="n">
-        <v>46074.60883101852</v>
+        <v>46079.40079861111</v>
       </c>
       <c r="O183" t="inlineStr">
         <is>
@@ -12415,7 +12415,7 @@
         <v>2</v>
       </c>
       <c r="N184" s="3" t="n">
-        <v>46076.37796296296</v>
+        <v>46079.38961805555</v>
       </c>
       <c r="O184" t="inlineStr">
         <is>
@@ -12479,7 +12479,7 @@
         <v>1</v>
       </c>
       <c r="N185" s="3" t="n">
-        <v>46073.43803240741</v>
+        <v>46079.39871527778</v>
       </c>
       <c r="O185" t="inlineStr">
         <is>
@@ -12543,7 +12543,7 @@
         <v>1</v>
       </c>
       <c r="N186" s="3" t="n">
-        <v>46077.49327546296</v>
+        <v>46079.38248842592</v>
       </c>
       <c r="O186" t="inlineStr">
         <is>
@@ -12607,7 +12607,7 @@
         <v>1</v>
       </c>
       <c r="N187" s="3" t="n">
-        <v>46078.7059837963</v>
+        <v>46079.4033912037</v>
       </c>
       <c r="O187" t="inlineStr">
         <is>
@@ -12671,7 +12671,7 @@
         <v>1</v>
       </c>
       <c r="N188" s="3" t="n">
-        <v>46078.55351851852</v>
+        <v>46079.36717592592</v>
       </c>
       <c r="O188" t="inlineStr">
         <is>
@@ -12799,7 +12799,7 @@
         </is>
       </c>
       <c r="N190" s="3" t="n">
-        <v>46078.69872685185</v>
+        <v>46079.39745370371</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12863,7 +12863,7 @@
         <v>1</v>
       </c>
       <c r="N191" s="3" t="n">
-        <v>46078.70435185185</v>
+        <v>46078.82586805556</v>
       </c>
       <c r="O191" t="inlineStr">
         <is>
@@ -12927,7 +12927,7 @@
         <v>1</v>
       </c>
       <c r="N192" s="3" t="n">
-        <v>46078.70978009259</v>
+        <v>46079.39052083333</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -13052,7 +13052,7 @@
         <v>2</v>
       </c>
       <c r="N194" s="3" t="n">
-        <v>46078.63803240741</v>
+        <v>46079.38112268518</v>
       </c>
       <c r="O194" t="inlineStr">
         <is>
@@ -13116,7 +13116,7 @@
         <v>1</v>
       </c>
       <c r="N195" s="3" t="n">
-        <v>46078.7358912037</v>
+        <v>46079.40199074074</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13180,7 +13180,7 @@
         <v>1</v>
       </c>
       <c r="N196" s="3" t="n">
-        <v>46078.65358796297</v>
+        <v>46079.38256944445</v>
       </c>
       <c r="O196" t="inlineStr">
         <is>
@@ -13244,7 +13244,7 @@
         <v>1</v>
       </c>
       <c r="N197" s="3" t="n">
-        <v>46078.65353009259</v>
+        <v>46079.39512731481</v>
       </c>
       <c r="O197" t="inlineStr">
         <is>
@@ -13308,7 +13308,7 @@
         <v>1</v>
       </c>
       <c r="N198" s="3" t="n">
-        <v>46078.6300462963</v>
+        <v>46079.38622685185</v>
       </c>
       <c r="O198" t="inlineStr">
         <is>
@@ -13372,7 +13372,7 @@
         <v>1</v>
       </c>
       <c r="N199" s="3" t="n">
-        <v>46078.71614583334</v>
+        <v>46079.39532407407</v>
       </c>
       <c r="O199" t="inlineStr">
         <is>
@@ -13436,7 +13436,7 @@
         <v>1</v>
       </c>
       <c r="N200" s="3" t="n">
-        <v>46078.71329861111</v>
+        <v>46078.79266203703</v>
       </c>
       <c r="O200" t="inlineStr">
         <is>
@@ -13497,7 +13497,7 @@
         </is>
       </c>
       <c r="N201" s="3" t="n">
-        <v>46078.70219907408</v>
+        <v>46079.38711805556</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -13561,7 +13561,7 @@
         <v>1</v>
       </c>
       <c r="N202" s="3" t="n">
-        <v>46078.70159722222</v>
+        <v>46079.40178240741</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13625,7 +13625,7 @@
         <v>1</v>
       </c>
       <c r="N203" s="3" t="n">
-        <v>46078.69952546297</v>
+        <v>46079.39152777778</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13689,7 +13689,7 @@
         <v>1</v>
       </c>
       <c r="N204" s="3" t="n">
-        <v>46078.73802083333</v>
+        <v>46079.38211805555</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13753,7 +13753,7 @@
         <v>1</v>
       </c>
       <c r="N205" s="3" t="n">
-        <v>46078.71168981482</v>
+        <v>46079.3777662037</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13817,7 +13817,7 @@
         <v>1</v>
       </c>
       <c r="N206" s="3" t="n">
-        <v>46078.70891203704</v>
+        <v>46079.37552083333</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -13881,7 +13881,7 @@
         <v>1</v>
       </c>
       <c r="N207" s="3" t="n">
-        <v>46078.73577546296</v>
+        <v>46079.40247685185</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -13945,7 +13945,7 @@
         <v>1</v>
       </c>
       <c r="N208" s="3" t="n">
-        <v>46078.6445949074</v>
+        <v>46079.38053240741</v>
       </c>
       <c r="O208" t="inlineStr">
         <is>
@@ -14009,7 +14009,7 @@
         <v>1</v>
       </c>
       <c r="N209" s="3" t="n">
-        <v>46078.70732638889</v>
+        <v>46079.3696412037</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14073,7 +14073,7 @@
         <v>1</v>
       </c>
       <c r="N210" s="3" t="n">
-        <v>46078.72394675926</v>
+        <v>46079.37238425926</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14137,7 +14137,7 @@
         <v>1</v>
       </c>
       <c r="N211" s="3" t="n">
-        <v>46078.71479166667</v>
+        <v>46079.37491898148</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -14201,7 +14201,7 @@
         <v>1</v>
       </c>
       <c r="N212" s="3" t="n">
-        <v>46078.70280092592</v>
+        <v>46079.37373842593</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -14265,7 +14265,7 @@
         <v>1</v>
       </c>
       <c r="N213" s="3" t="n">
-        <v>46078.71846064815</v>
+        <v>46079.38690972222</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
@@ -14329,7 +14329,7 @@
         <v>1</v>
       </c>
       <c r="N214" s="3" t="n">
-        <v>46078.71346064815</v>
+        <v>46079.37537037037</v>
       </c>
       <c r="O214" t="inlineStr">
         <is>
@@ -14393,7 +14393,7 @@
         <v>1</v>
       </c>
       <c r="N215" s="3" t="n">
-        <v>46078.71666666667</v>
+        <v>46078.79136574074</v>
       </c>
       <c r="O215" t="inlineStr">
         <is>
@@ -14457,7 +14457,7 @@
         <v>1</v>
       </c>
       <c r="N216" s="3" t="n">
-        <v>46078.70054398148</v>
+        <v>46079.37575231482</v>
       </c>
       <c r="O216" t="inlineStr">
         <is>
@@ -14476,11 +14476,6 @@
           <t>OPERACAO 8.1</t>
         </is>
       </c>
-      <c r="C217" t="inlineStr">
-        <is>
-          <t>10.69.5.85</t>
-        </is>
-      </c>
       <c r="D217" t="n">
         <v>2017</v>
       </c>
@@ -14521,7 +14516,7 @@
         <v>1</v>
       </c>
       <c r="N217" s="3" t="n">
-        <v>46078.72100694444</v>
+        <v>46079.3704050926</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14585,7 +14580,7 @@
         <v>1</v>
       </c>
       <c r="N218" s="3" t="n">
-        <v>46078.7077199074</v>
+        <v>46079.37349537037</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14649,7 +14644,7 @@
         <v>1</v>
       </c>
       <c r="N219" s="3" t="n">
-        <v>46078.70319444445</v>
+        <v>46079.33395833334</v>
       </c>
       <c r="O219" t="inlineStr">
         <is>
@@ -14718,7 +14713,7 @@
         <v>1</v>
       </c>
       <c r="N220" s="3" t="n">
-        <v>46078.71834490741</v>
+        <v>46079.3708912037</v>
       </c>
       <c r="O220" t="inlineStr">
         <is>
@@ -14782,7 +14777,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="3" t="n">
-        <v>46078.70407407408</v>
+        <v>46079.37903935185</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14846,7 +14841,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="3" t="n">
-        <v>46078.73457175926</v>
+        <v>46079.39098379629</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -14910,7 +14905,7 @@
         <v>1</v>
       </c>
       <c r="N223" s="3" t="n">
-        <v>46078.71403935185</v>
+        <v>46079.401875</v>
       </c>
       <c r="O223" t="inlineStr">
         <is>
@@ -14974,7 +14969,7 @@
         <v>1</v>
       </c>
       <c r="N224" s="3" t="n">
-        <v>46078.72402777777</v>
+        <v>46078.80011574074</v>
       </c>
       <c r="O224" t="inlineStr">
         <is>
@@ -15038,7 +15033,7 @@
         <v>1</v>
       </c>
       <c r="N225" s="3" t="n">
-        <v>46078.70952546296</v>
+        <v>46078.82145833333</v>
       </c>
       <c r="O225" t="inlineStr">
         <is>
@@ -15102,7 +15097,7 @@
         <v>1</v>
       </c>
       <c r="N226" s="3" t="n">
-        <v>46078.73037037037</v>
+        <v>46079.36709490741</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15166,7 +15161,7 @@
         <v>1</v>
       </c>
       <c r="N227" s="3" t="n">
-        <v>46078.73547453704</v>
+        <v>46078.81472222223</v>
       </c>
       <c r="O227" t="inlineStr">
         <is>
@@ -15230,7 +15225,7 @@
         <v>1</v>
       </c>
       <c r="N228" s="3" t="n">
-        <v>46078.73762731482</v>
+        <v>46079.39921296296</v>
       </c>
       <c r="O228" t="inlineStr">
         <is>
@@ -15294,7 +15289,7 @@
         <v>1</v>
       </c>
       <c r="N229" s="3" t="n">
-        <v>46078.73215277777</v>
+        <v>46079.36696759259</v>
       </c>
       <c r="O229" t="inlineStr">
         <is>
@@ -15358,7 +15353,7 @@
         <v>1</v>
       </c>
       <c r="N230" s="3" t="n">
-        <v>46078.70083333334</v>
+        <v>46079.39349537037</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15422,7 +15417,7 @@
         <v>1</v>
       </c>
       <c r="N231" s="3" t="n">
-        <v>46078.7166087963</v>
+        <v>46079.39707175926</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15486,7 +15481,7 @@
         <v>1</v>
       </c>
       <c r="N232" s="3" t="n">
-        <v>46078.71194444445</v>
+        <v>46079.38729166667</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -15550,7 +15545,7 @@
         <v>1</v>
       </c>
       <c r="N233" s="3" t="n">
-        <v>46078.69993055556</v>
+        <v>46079.36534722222</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15614,7 +15609,7 @@
         <v>1</v>
       </c>
       <c r="N234" s="3" t="n">
-        <v>46078.70622685185</v>
+        <v>46079.38773148148</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -15678,7 +15673,7 @@
         <v>1</v>
       </c>
       <c r="N235" s="3" t="n">
-        <v>46078.73659722223</v>
+        <v>46079.38143518518</v>
       </c>
       <c r="O235" t="inlineStr">
         <is>
@@ -15742,7 +15737,7 @@
         <v>1</v>
       </c>
       <c r="N236" s="3" t="n">
-        <v>46078.72092592593</v>
+        <v>46079.39681712963</v>
       </c>
       <c r="O236" t="inlineStr">
         <is>
@@ -15806,7 +15801,7 @@
         <v>1</v>
       </c>
       <c r="N237" s="3" t="n">
-        <v>46078.71408564815</v>
+        <v>46079.36840277778</v>
       </c>
       <c r="O237" t="inlineStr">
         <is>
@@ -15870,7 +15865,7 @@
         <v>1</v>
       </c>
       <c r="N238" s="3" t="n">
-        <v>46078.71400462963</v>
+        <v>46079.37599537037</v>
       </c>
       <c r="O238" t="inlineStr">
         <is>
@@ -15934,7 +15929,7 @@
         <v>1</v>
       </c>
       <c r="N239" s="3" t="n">
-        <v>46078.71701388889</v>
+        <v>46079.37174768518</v>
       </c>
       <c r="O239" t="inlineStr">
         <is>
@@ -15998,7 +15993,7 @@
         <v>1</v>
       </c>
       <c r="N240" s="3" t="n">
-        <v>46078.70292824074</v>
+        <v>46079.38373842592</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16062,7 +16057,7 @@
         <v>1</v>
       </c>
       <c r="N241" s="3" t="n">
-        <v>46078.71195601852</v>
+        <v>46079.37689814815</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16126,7 +16121,7 @@
         <v>1</v>
       </c>
       <c r="N242" s="3" t="n">
-        <v>46078.71236111111</v>
+        <v>46079.39303240741</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16190,7 +16185,7 @@
         <v>1</v>
       </c>
       <c r="N243" s="3" t="n">
-        <v>46078.71484953703</v>
+        <v>46079.39375</v>
       </c>
       <c r="O243" t="inlineStr">
         <is>
@@ -16249,7 +16244,7 @@
         <v>1</v>
       </c>
       <c r="N244" s="3" t="n">
-        <v>46078.63931712963</v>
+        <v>46079.17092592592</v>
       </c>
       <c r="O244" t="inlineStr">
         <is>
@@ -16313,7 +16308,7 @@
         <v>1</v>
       </c>
       <c r="N245" s="3" t="n">
-        <v>46078.72578703704</v>
+        <v>46079.39539351852</v>
       </c>
       <c r="O245" t="inlineStr">
         <is>
@@ -16377,7 +16372,7 @@
         <v>1</v>
       </c>
       <c r="N246" s="3" t="n">
-        <v>46078.72346064815</v>
+        <v>46079.38834490741</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16441,7 +16436,7 @@
         <v>1</v>
       </c>
       <c r="N247" s="3" t="n">
-        <v>46078.70795138889</v>
+        <v>46079.39790509259</v>
       </c>
       <c r="O247" t="inlineStr">
         <is>
@@ -16505,7 +16500,7 @@
         <v>1</v>
       </c>
       <c r="N248" s="3" t="n">
-        <v>46078.71046296296</v>
+        <v>46079.39883101852</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16569,7 +16564,7 @@
         <v>1</v>
       </c>
       <c r="N249" s="3" t="n">
-        <v>46078.69980324074</v>
+        <v>46079.39144675926</v>
       </c>
       <c r="O249" t="inlineStr">
         <is>
@@ -16588,11 +16583,6 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
-      <c r="C250" t="inlineStr">
-        <is>
-          <t>10.69.5.118</t>
-        </is>
-      </c>
       <c r="D250" t="n">
         <v>2017</v>
       </c>
@@ -16633,7 +16623,7 @@
         <v>1</v>
       </c>
       <c r="N250" s="3" t="n">
-        <v>46078.71489583333</v>
+        <v>46079.37424768518</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16697,7 +16687,7 @@
         <v>1</v>
       </c>
       <c r="N251" s="3" t="n">
-        <v>46078.71981481482</v>
+        <v>46079.39520833334</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16761,7 +16751,7 @@
         <v>1</v>
       </c>
       <c r="N252" s="3" t="n">
-        <v>46078.72649305555</v>
+        <v>46079.4015625</v>
       </c>
       <c r="O252" t="inlineStr">
         <is>
@@ -16825,7 +16815,7 @@
         <v>1</v>
       </c>
       <c r="N253" s="3" t="n">
-        <v>46078.7043287037</v>
+        <v>46079.37753472223</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16883,7 +16873,7 @@
         <v>1</v>
       </c>
       <c r="N254" s="3" t="n">
-        <v>46078.7346875</v>
+        <v>46079.39758101852</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -16947,7 +16937,7 @@
         <v>1</v>
       </c>
       <c r="N255" s="3" t="n">
-        <v>46078.73700231482</v>
+        <v>46079.39728009259</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -17011,7 +17001,7 @@
         <v>1</v>
       </c>
       <c r="N256" s="3" t="n">
-        <v>46078.72035879629</v>
+        <v>46079.37936342593</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17075,7 +17065,7 @@
         <v>1</v>
       </c>
       <c r="N257" s="3" t="n">
-        <v>46078.72258101852</v>
+        <v>46079.38851851852</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17139,7 +17129,7 @@
         <v>1</v>
       </c>
       <c r="N258" s="3" t="n">
-        <v>46078.7146875</v>
+        <v>46079.37704861111</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
@@ -17203,7 +17193,7 @@
         <v>1</v>
       </c>
       <c r="N259" s="3" t="n">
-        <v>46078.71515046297</v>
+        <v>46079.35188657408</v>
       </c>
       <c r="O259" t="inlineStr">
         <is>
@@ -17267,7 +17257,7 @@
         <v>1</v>
       </c>
       <c r="N260" s="3" t="n">
-        <v>46078.613125</v>
+        <v>46079.3700925926</v>
       </c>
       <c r="O260" t="inlineStr">
         <is>
@@ -17331,7 +17321,7 @@
         <v>1</v>
       </c>
       <c r="N261" s="3" t="n">
-        <v>46078.71563657407</v>
+        <v>46079.40420138889</v>
       </c>
       <c r="O261" t="inlineStr">
         <is>
@@ -17395,7 +17385,7 @@
         <v>1</v>
       </c>
       <c r="N262" s="3" t="n">
-        <v>46078.69908564815</v>
+        <v>46079.39037037037</v>
       </c>
       <c r="O262" t="inlineStr">
         <is>
@@ -17459,7 +17449,7 @@
         <v>1</v>
       </c>
       <c r="N263" s="3" t="n">
-        <v>46078.72571759259</v>
+        <v>46079.39888888889</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17523,7 +17513,7 @@
         <v>1</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>46078.72104166666</v>
+        <v>46079.38222222222</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17587,7 +17577,7 @@
         <v>1</v>
       </c>
       <c r="N265" s="3" t="n">
-        <v>46078.70638888889</v>
+        <v>46079.36679398148</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17651,7 +17641,7 @@
         <v>1</v>
       </c>
       <c r="N266" s="3" t="n">
-        <v>46078.57684027778</v>
+        <v>46079.37402777778</v>
       </c>
       <c r="O266" t="inlineStr">
         <is>
@@ -17715,7 +17705,7 @@
         <v>1</v>
       </c>
       <c r="N267" s="3" t="n">
-        <v>46078.72273148148</v>
+        <v>46079.37193287037</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17779,7 +17769,7 @@
         <v>1</v>
       </c>
       <c r="N268" s="3" t="n">
-        <v>46078.73215277777</v>
+        <v>46079.37832175926</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17843,7 +17833,7 @@
         <v>1</v>
       </c>
       <c r="N269" s="3" t="n">
-        <v>46078.70392361111</v>
+        <v>46078.86444444444</v>
       </c>
       <c r="O269" t="inlineStr">
         <is>
@@ -17904,7 +17894,7 @@
         </is>
       </c>
       <c r="N270" s="3" t="n">
-        <v>46078.71869212963</v>
+        <v>46079.38876157408</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -17968,7 +17958,7 @@
         <v>1</v>
       </c>
       <c r="N271" s="3" t="n">
-        <v>46078.62690972222</v>
+        <v>46079.2383449074</v>
       </c>
       <c r="O271" t="inlineStr">
         <is>
@@ -18416,7 +18406,7 @@
         <v>1</v>
       </c>
       <c r="N278" s="3" t="n">
-        <v>46078.70655092593</v>
+        <v>46079.39979166666</v>
       </c>
       <c r="O278" t="inlineStr">
         <is>
@@ -18480,7 +18470,7 @@
         <v>1</v>
       </c>
       <c r="N279" s="3" t="n">
-        <v>46078.69969907407</v>
+        <v>46079.37945601852</v>
       </c>
       <c r="O279" t="inlineStr">
         <is>
@@ -18544,7 +18534,7 @@
         <v>1</v>
       </c>
       <c r="N280" s="3" t="n">
-        <v>46078.57743055555</v>
+        <v>46079.37284722222</v>
       </c>
       <c r="O280" t="inlineStr">
         <is>
@@ -18627,6 +18617,11 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>10.69.5.151</t>
+        </is>
+      </c>
       <c r="D282" t="n">
         <v>2017</v>
       </c>
@@ -18667,7 +18662,7 @@
         <v>1</v>
       </c>
       <c r="N282" s="3" t="n">
-        <v>46078.55240740741</v>
+        <v>46079.40283564815</v>
       </c>
       <c r="O282" t="inlineStr">
         <is>
@@ -18731,7 +18726,7 @@
         <v>1</v>
       </c>
       <c r="N283" s="3" t="n">
-        <v>46078.73538194445</v>
+        <v>46078.81083333334</v>
       </c>
       <c r="O283" t="inlineStr">
         <is>
@@ -18795,7 +18790,7 @@
         <v>1</v>
       </c>
       <c r="N284" s="3" t="n">
-        <v>46078.71141203704</v>
+        <v>46079.3706712963</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18859,7 +18854,7 @@
         <v>1</v>
       </c>
       <c r="N285" s="3" t="n">
-        <v>46078.70327546296</v>
+        <v>46079.38053240741</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -18878,6 +18873,11 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>10.69.5.155</t>
+        </is>
+      </c>
       <c r="D286" t="n">
         <v>2019</v>
       </c>
@@ -18918,7 +18918,7 @@
         <v>1</v>
       </c>
       <c r="N286" s="3" t="n">
-        <v>46078.56862268518</v>
+        <v>46079.39363425926</v>
       </c>
       <c r="O286" t="inlineStr">
         <is>
@@ -18982,7 +18982,7 @@
         <v>1</v>
       </c>
       <c r="N287" s="3" t="n">
-        <v>46078.72793981482</v>
+        <v>46079.37765046296</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
@@ -19046,7 +19046,7 @@
         <v>1</v>
       </c>
       <c r="N288" s="3" t="n">
-        <v>46078.62541666667</v>
+        <v>46079.3632175926</v>
       </c>
       <c r="O288" t="inlineStr">
         <is>
@@ -19110,7 +19110,7 @@
         <v>1</v>
       </c>
       <c r="N289" s="3" t="n">
-        <v>46078.72037037037</v>
+        <v>46079.39600694444</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -19904,7 +19904,7 @@
         <v>1</v>
       </c>
       <c r="N302" s="3" t="n">
-        <v>46078.70657407407</v>
+        <v>46079.39976851852</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -20645,7 +20645,7 @@
         </is>
       </c>
       <c r="N314" s="3" t="n">
-        <v>46078.70356481482</v>
+        <v>46079.04523148148</v>
       </c>
       <c r="O314" t="inlineStr">
         <is>
@@ -21020,7 +21020,7 @@
         </is>
       </c>
       <c r="N320" s="3" t="n">
-        <v>46078.73123842593</v>
+        <v>46079.38806712963</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21745,7 +21745,7 @@
         <v>1</v>
       </c>
       <c r="N332" s="3" t="n">
-        <v>46078.70275462963</v>
+        <v>46079.36636574074</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21809,7 +21809,7 @@
         <v>2</v>
       </c>
       <c r="N333" s="3" t="n">
-        <v>46078.73445601852</v>
+        <v>46079.39377314815</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21873,7 +21873,7 @@
         <v>2</v>
       </c>
       <c r="N334" s="3" t="n">
-        <v>46078.71582175926</v>
+        <v>46079.40150462963</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21937,7 +21937,7 @@
         <v>2</v>
       </c>
       <c r="N335" s="3" t="n">
-        <v>46078.70298611111</v>
+        <v>46079.39576388889</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -22001,7 +22001,7 @@
         <v>1</v>
       </c>
       <c r="N336" s="3" t="n">
-        <v>46078.70303240741</v>
+        <v>46079.3984375</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22065,7 +22065,7 @@
         <v>1</v>
       </c>
       <c r="N337" s="3" t="n">
-        <v>46078.7205787037</v>
+        <v>46079.38277777778</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22129,7 +22129,7 @@
         <v>2</v>
       </c>
       <c r="N338" s="3" t="n">
-        <v>46078.72797453704</v>
+        <v>46079.39449074074</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -22193,7 +22193,7 @@
         <v>2</v>
       </c>
       <c r="N339" s="3" t="n">
-        <v>46078.713125</v>
+        <v>46079.40258101852</v>
       </c>
       <c r="O339" t="inlineStr">
         <is>
@@ -22446,7 +22446,7 @@
         </is>
       </c>
       <c r="N343" s="3" t="n">
-        <v>46078.70171296296</v>
+        <v>46079.38466435186</v>
       </c>
       <c r="O343" t="inlineStr">
         <is>
@@ -23831,7 +23831,7 @@
         <v>1</v>
       </c>
       <c r="N365" s="3" t="n">
-        <v>46078.67153935185</v>
+        <v>46079.36765046296</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
@@ -23897,7 +23897,7 @@
         </is>
       </c>
       <c r="N366" s="3" t="n">
-        <v>46078.70841435185</v>
+        <v>46079.40423611111</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -24023,7 +24023,7 @@
         </is>
       </c>
       <c r="N368" s="3" t="n">
-        <v>46078.70872685185</v>
+        <v>46079.39657407408</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -24089,7 +24089,7 @@
         </is>
       </c>
       <c r="N369" s="3" t="n">
-        <v>46078.72190972222</v>
+        <v>46079.39780092592</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
@@ -24158,7 +24158,7 @@
         <v>1</v>
       </c>
       <c r="N370" s="3" t="n">
-        <v>46078.70878472222</v>
+        <v>46079.39724537037</v>
       </c>
       <c r="O370" t="inlineStr">
         <is>
@@ -24431,7 +24431,7 @@
         <v>1</v>
       </c>
       <c r="N374" s="3" t="n">
-        <v>46078.69993055556</v>
+        <v>46079.38832175926</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24497,7 +24497,7 @@
         </is>
       </c>
       <c r="N375" s="3" t="n">
-        <v>46078.70127314814</v>
+        <v>46079.38832175926</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
@@ -24561,7 +24561,7 @@
         <v>1</v>
       </c>
       <c r="N376" s="3" t="n">
-        <v>46078.70834490741</v>
+        <v>46079.37414351852</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -24630,7 +24630,7 @@
         <v>2</v>
       </c>
       <c r="N377" s="3" t="n">
-        <v>46078.72466435185</v>
+        <v>46079.40401620371</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -24699,7 +24699,7 @@
         <v>2</v>
       </c>
       <c r="N378" s="3" t="n">
-        <v>46078.72149305556</v>
+        <v>46079.38674768519</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização automática 2026-02-26 11:52:03.351771
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>46079.37276620371</v>
+        <v>46079.48491898148</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>46079.37380787037</v>
+        <v>46079.4525</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -739,10 +739,10 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>46079.39236111111</v>
+        <v>46079.4693287037</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>46079.375625</v>
+        <v>46079.45071759259</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -1259,7 +1259,7 @@
         <v>1</v>
       </c>
       <c r="N12" s="3" t="n">
-        <v>46078.6234837963</v>
+        <v>46079.45965277778</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1515,7 +1515,7 @@
         <v>2</v>
       </c>
       <c r="N16" s="3" t="n">
-        <v>46078.73741898148</v>
+        <v>46079.45452546296</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1579,7 +1579,7 @@
         <v>1</v>
       </c>
       <c r="N17" s="3" t="n">
-        <v>46072.59577546296</v>
+        <v>46079.47435185185</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1643,7 +1643,7 @@
         <v>2</v>
       </c>
       <c r="N18" s="3" t="n">
-        <v>46079.40050925926</v>
+        <v>46079.47866898148</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1768,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="N20" s="3" t="n">
-        <v>46079.38277777778</v>
+        <v>46079.45961805555</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1950,7 +1950,7 @@
         <v>1</v>
       </c>
       <c r="N23" s="3" t="n">
-        <v>46078.72707175926</v>
+        <v>46079.45313657408</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -6570,7 +6570,7 @@
         <v>1</v>
       </c>
       <c r="N95" s="3" t="n">
-        <v>46078.7060300926</v>
+        <v>46079.48383101852</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -6639,7 +6639,7 @@
         <v>1</v>
       </c>
       <c r="N96" s="3" t="n">
-        <v>46078.81081018518</v>
+        <v>46079.47336805556</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
@@ -6703,7 +6703,7 @@
         <v>1</v>
       </c>
       <c r="N97" s="3" t="n">
-        <v>46079.37601851852</v>
+        <v>46079.44966435185</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -6767,7 +6767,7 @@
         <v>1</v>
       </c>
       <c r="N98" s="3" t="n">
-        <v>46079.38182870371</v>
+        <v>46079.46195601852</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -6836,7 +6836,7 @@
         <v>1</v>
       </c>
       <c r="N99" s="3" t="n">
-        <v>46079.38302083333</v>
+        <v>46079.46267361111</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -6905,7 +6905,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>46079.38922453704</v>
+        <v>46079.46215277778</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6974,7 +6974,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="3" t="n">
-        <v>46079.38803240741</v>
+        <v>46079.46616898148</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -7112,7 +7112,7 @@
         <v>2</v>
       </c>
       <c r="N103" s="3" t="n">
-        <v>46079.37818287037</v>
+        <v>46079.45846064815</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7242,7 +7242,7 @@
         <v>1</v>
       </c>
       <c r="N105" s="3" t="n">
-        <v>46078.67922453704</v>
+        <v>46079.48565972222</v>
       </c>
       <c r="O105" t="inlineStr">
         <is>
@@ -7372,7 +7372,7 @@
         <v>1</v>
       </c>
       <c r="N107" s="3" t="n">
-        <v>46079.37074074074</v>
+        <v>46079.45363425926</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -7510,7 +7510,7 @@
         <v>1</v>
       </c>
       <c r="N109" s="3" t="n">
-        <v>46079.39797453704</v>
+        <v>46079.47922453703</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7579,7 +7579,7 @@
         <v>2</v>
       </c>
       <c r="N110" s="3" t="n">
-        <v>46079.38300925926</v>
+        <v>46079.46409722222</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7648,7 +7648,7 @@
         <v>2</v>
       </c>
       <c r="N111" s="3" t="n">
-        <v>46079.36805555555</v>
+        <v>46079.45648148148</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
@@ -7717,7 +7717,7 @@
         <v>2</v>
       </c>
       <c r="N112" s="3" t="n">
-        <v>46079.37113425926</v>
+        <v>46079.45326388889</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7786,7 +7786,7 @@
         <v>1</v>
       </c>
       <c r="N113" s="3" t="n">
-        <v>46079.39659722222</v>
+        <v>46079.47232638889</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7855,7 +7855,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>46079.40396990741</v>
+        <v>46079.48275462963</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -7921,7 +7921,7 @@
         </is>
       </c>
       <c r="N115" s="3" t="n">
-        <v>46079.37898148148</v>
+        <v>46079.45853009259</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -7990,7 +7990,7 @@
         <v>1</v>
       </c>
       <c r="N116" s="3" t="n">
-        <v>46079.38185185185</v>
+        <v>46079.45710648148</v>
       </c>
       <c r="O116" t="inlineStr">
         <is>
@@ -8054,7 +8054,7 @@
         <v>1</v>
       </c>
       <c r="N117" s="3" t="n">
-        <v>46079.36695601852</v>
+        <v>46079.44967592593</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -8120,7 +8120,7 @@
         </is>
       </c>
       <c r="N118" s="3" t="n">
-        <v>46079.38075231481</v>
+        <v>46079.45829861111</v>
       </c>
       <c r="O118" t="inlineStr">
         <is>
@@ -8258,7 +8258,7 @@
         <v>1</v>
       </c>
       <c r="N120" s="3" t="n">
-        <v>46079.39700231481</v>
+        <v>46079.47665509259</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -8327,7 +8327,7 @@
         <v>1</v>
       </c>
       <c r="N121" s="3" t="n">
-        <v>46079.38952546296</v>
+        <v>46079.47423611111</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -8393,7 +8393,7 @@
         </is>
       </c>
       <c r="N122" s="3" t="n">
-        <v>46079.37047453703</v>
+        <v>46079.48568287037</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -8462,7 +8462,7 @@
         <v>2</v>
       </c>
       <c r="N123" s="3" t="n">
-        <v>46079.30954861111</v>
+        <v>46079.46644675926</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -8531,7 +8531,7 @@
         <v>1</v>
       </c>
       <c r="N124" s="3" t="n">
-        <v>46079.37851851852</v>
+        <v>46079.45349537037</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -8600,7 +8600,7 @@
         <v>1</v>
       </c>
       <c r="N125" s="3" t="n">
-        <v>46079.39939814815</v>
+        <v>46079.48237268518</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -8669,7 +8669,7 @@
         <v>2</v>
       </c>
       <c r="N126" s="3" t="n">
-        <v>46078.77155092593</v>
+        <v>46079.48162037037</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -8738,7 +8738,7 @@
         <v>2</v>
       </c>
       <c r="N127" s="3" t="n">
-        <v>46079.3693287037</v>
+        <v>46079.48451388889</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -8807,7 +8807,7 @@
         <v>1</v>
       </c>
       <c r="N128" s="3" t="n">
-        <v>46079.37707175926</v>
+        <v>46079.45284722222</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -8876,7 +8876,7 @@
         <v>1</v>
       </c>
       <c r="N129" s="3" t="n">
-        <v>46079.39829861111</v>
+        <v>46079.4783912037</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -8945,7 +8945,7 @@
         <v>1</v>
       </c>
       <c r="N130" s="3" t="n">
-        <v>46079.36809027778</v>
+        <v>46079.47847222222</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -8964,11 +8964,6 @@
           <t>ADM/FIN</t>
         </is>
       </c>
-      <c r="C131" t="inlineStr">
-        <is>
-          <t>10.69.3.6</t>
-        </is>
-      </c>
       <c r="D131" t="n">
         <v>2025</v>
       </c>
@@ -9014,7 +9009,7 @@
         <v>1</v>
       </c>
       <c r="N131" s="3" t="n">
-        <v>46079.38357638889</v>
+        <v>46079.45976851852</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -9466,7 +9461,7 @@
         <v>1</v>
       </c>
       <c r="N138" s="3" t="n">
-        <v>46079.37739583333</v>
+        <v>46079.45554398148</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9530,7 +9525,7 @@
         <v>1</v>
       </c>
       <c r="N139" s="3" t="n">
-        <v>46079.36962962963</v>
+        <v>46079.4872337963</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9594,7 +9589,7 @@
         <v>1</v>
       </c>
       <c r="N140" s="3" t="n">
-        <v>46079.38509259259</v>
+        <v>46079.46677083334</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9658,7 +9653,7 @@
         <v>1</v>
       </c>
       <c r="N141" s="3" t="n">
-        <v>46079.37163194444</v>
+        <v>46079.4725</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9722,7 +9717,7 @@
         <v>1</v>
       </c>
       <c r="N142" s="3" t="n">
-        <v>46079.39322916666</v>
+        <v>46079.46787037037</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9786,7 +9781,7 @@
         <v>1</v>
       </c>
       <c r="N143" s="3" t="n">
-        <v>46079.39385416666</v>
+        <v>46079.47604166667</v>
       </c>
       <c r="O143" t="inlineStr">
         <is>
@@ -9850,7 +9845,7 @@
         <v>1</v>
       </c>
       <c r="N144" s="3" t="n">
-        <v>46079.39171296296</v>
+        <v>46079.46849537037</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9978,7 +9973,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="3" t="n">
-        <v>46079.3783912037</v>
+        <v>46079.45458333333</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10042,7 +10037,7 @@
         <v>1</v>
       </c>
       <c r="N147" s="3" t="n">
-        <v>46079.40283564815</v>
+        <v>46079.47811342592</v>
       </c>
       <c r="O147" t="inlineStr">
         <is>
@@ -10106,7 +10101,7 @@
         <v>1</v>
       </c>
       <c r="N148" s="3" t="n">
-        <v>46079.38275462963</v>
+        <v>46079.45717592593</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10170,7 +10165,7 @@
         <v>1</v>
       </c>
       <c r="N149" s="3" t="n">
-        <v>46079.37759259259</v>
+        <v>46079.44863425926</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -10234,7 +10229,7 @@
         <v>1</v>
       </c>
       <c r="N150" s="3" t="n">
-        <v>46079.39837962963</v>
+        <v>46079.4800925926</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -10298,7 +10293,7 @@
         <v>1</v>
       </c>
       <c r="N151" s="3" t="n">
-        <v>46078.82223379629</v>
+        <v>46079.45417824074</v>
       </c>
       <c r="O151" t="inlineStr">
         <is>
@@ -10362,7 +10357,7 @@
         <v>1</v>
       </c>
       <c r="N152" s="3" t="n">
-        <v>46079.38721064815</v>
+        <v>46079.46793981481</v>
       </c>
       <c r="O152" t="inlineStr">
         <is>
@@ -10426,7 +10421,7 @@
         <v>1</v>
       </c>
       <c r="N153" s="3" t="n">
-        <v>46079.3779050926</v>
+        <v>46079.4521875</v>
       </c>
       <c r="O153" t="inlineStr">
         <is>
@@ -10490,7 +10485,7 @@
         <v>1</v>
       </c>
       <c r="N154" s="3" t="n">
-        <v>46079.36612268518</v>
+        <v>46079.48783564815</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10554,7 +10549,7 @@
         <v>1</v>
       </c>
       <c r="N155" s="3" t="n">
-        <v>46079.37496527778</v>
+        <v>46079.48525462963</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10618,7 +10613,7 @@
         <v>1</v>
       </c>
       <c r="N156" s="3" t="n">
-        <v>46079.39541666667</v>
+        <v>46079.47872685185</v>
       </c>
       <c r="O156" t="inlineStr">
         <is>
@@ -10682,7 +10677,7 @@
         <v>1</v>
       </c>
       <c r="N157" s="3" t="n">
-        <v>46079.37704861111</v>
+        <v>46079.45737268519</v>
       </c>
       <c r="O157" t="inlineStr">
         <is>
@@ -10746,7 +10741,7 @@
         <v>1</v>
       </c>
       <c r="N158" s="3" t="n">
-        <v>46079.37501157408</v>
+        <v>46079.45199074074</v>
       </c>
       <c r="O158" t="inlineStr">
         <is>
@@ -10810,7 +10805,7 @@
         <v>1</v>
       </c>
       <c r="N159" s="3" t="n">
-        <v>46079.3955787037</v>
+        <v>46079.47627314815</v>
       </c>
       <c r="O159" t="inlineStr">
         <is>
@@ -10874,7 +10869,7 @@
         <v>1</v>
       </c>
       <c r="N160" s="3" t="n">
-        <v>46079.37181712963</v>
+        <v>46079.48569444445</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
@@ -10938,7 +10933,7 @@
         <v>1</v>
       </c>
       <c r="N161" s="3" t="n">
-        <v>46079.37488425926</v>
+        <v>46079.4875462963</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -11002,7 +10997,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="3" t="n">
-        <v>46079.37144675926</v>
+        <v>46079.48130787037</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11130,7 +11125,7 @@
         <v>2</v>
       </c>
       <c r="N164" s="3" t="n">
-        <v>46079.40444444444</v>
+        <v>46079.48048611111</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11194,7 +11189,7 @@
         <v>2</v>
       </c>
       <c r="N165" s="3" t="n">
-        <v>46079.37037037037</v>
+        <v>46079.48491898148</v>
       </c>
       <c r="O165" t="inlineStr">
         <is>
@@ -11258,7 +11253,7 @@
         <v>2</v>
       </c>
       <c r="N166" s="3" t="n">
-        <v>46079.37417824074</v>
+        <v>46079.45075231481</v>
       </c>
       <c r="O166" t="inlineStr">
         <is>
@@ -11319,10 +11314,10 @@
         </is>
       </c>
       <c r="M167" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N167" s="3" t="n">
-        <v>46079.36737268518</v>
+        <v>46079.48487268519</v>
       </c>
       <c r="O167" t="inlineStr">
         <is>
@@ -11386,7 +11381,7 @@
         <v>2</v>
       </c>
       <c r="N168" s="3" t="n">
-        <v>46079.37060185185</v>
+        <v>46079.45298611111</v>
       </c>
       <c r="O168" t="inlineStr">
         <is>
@@ -11450,7 +11445,7 @@
         <v>2</v>
       </c>
       <c r="N169" s="3" t="n">
-        <v>46079.37075231481</v>
+        <v>46079.48660879629</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -11514,7 +11509,7 @@
         <v>2</v>
       </c>
       <c r="N170" s="3" t="n">
-        <v>46079.39797453704</v>
+        <v>46079.47512731481</v>
       </c>
       <c r="O170" t="inlineStr">
         <is>
@@ -11575,10 +11570,10 @@
         </is>
       </c>
       <c r="M171" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N171" s="3" t="n">
-        <v>46079.36778935185</v>
+        <v>46079.48173611111</v>
       </c>
       <c r="O171" t="inlineStr">
         <is>
@@ -11642,7 +11637,7 @@
         <v>2</v>
       </c>
       <c r="N172" s="3" t="n">
-        <v>46078.77956018518</v>
+        <v>46079.46847222222</v>
       </c>
       <c r="O172" t="inlineStr">
         <is>
@@ -11706,7 +11701,7 @@
         <v>1</v>
       </c>
       <c r="N173" s="3" t="n">
-        <v>46079.38108796296</v>
+        <v>46079.45515046296</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -11770,7 +11765,7 @@
         <v>2</v>
       </c>
       <c r="N174" s="3" t="n">
-        <v>46079.40034722222</v>
+        <v>46079.47434027777</v>
       </c>
       <c r="O174" t="inlineStr">
         <is>
@@ -11834,7 +11829,7 @@
         <v>2</v>
       </c>
       <c r="N175" s="3" t="n">
-        <v>46079.3779050926</v>
+        <v>46079.45849537037</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -11898,7 +11893,7 @@
         <v>2</v>
       </c>
       <c r="N176" s="3" t="n">
-        <v>46078.65570601852</v>
+        <v>46079.47229166667</v>
       </c>
       <c r="O176" t="inlineStr">
         <is>
@@ -11962,7 +11957,7 @@
         <v>2</v>
       </c>
       <c r="N177" s="3" t="n">
-        <v>46078.69855324074</v>
+        <v>46079.46505787037</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
@@ -12026,7 +12021,7 @@
         <v>2</v>
       </c>
       <c r="N178" s="3" t="n">
-        <v>46079.399375</v>
+        <v>46079.47356481481</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12090,7 +12085,7 @@
         <v>1</v>
       </c>
       <c r="N179" s="3" t="n">
-        <v>46079.36613425926</v>
+        <v>46079.47994212963</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12154,7 +12149,7 @@
         <v>1</v>
       </c>
       <c r="N180" s="3" t="n">
-        <v>46079.37844907407</v>
+        <v>46079.45074074074</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12218,7 +12213,7 @@
         <v>1</v>
       </c>
       <c r="N181" s="3" t="n">
-        <v>46079.39989583333</v>
+        <v>46079.47958333333</v>
       </c>
       <c r="O181" t="inlineStr">
         <is>
@@ -12346,7 +12341,7 @@
         <v>1</v>
       </c>
       <c r="N183" s="3" t="n">
-        <v>46079.40079861111</v>
+        <v>46079.47413194444</v>
       </c>
       <c r="O183" t="inlineStr">
         <is>
@@ -12415,7 +12410,7 @@
         <v>2</v>
       </c>
       <c r="N184" s="3" t="n">
-        <v>46079.38961805555</v>
+        <v>46079.46527777778</v>
       </c>
       <c r="O184" t="inlineStr">
         <is>
@@ -12479,7 +12474,7 @@
         <v>1</v>
       </c>
       <c r="N185" s="3" t="n">
-        <v>46079.39871527778</v>
+        <v>46079.4756712963</v>
       </c>
       <c r="O185" t="inlineStr">
         <is>
@@ -12543,7 +12538,7 @@
         <v>1</v>
       </c>
       <c r="N186" s="3" t="n">
-        <v>46079.38248842592</v>
+        <v>46079.45516203704</v>
       </c>
       <c r="O186" t="inlineStr">
         <is>
@@ -12607,7 +12602,7 @@
         <v>1</v>
       </c>
       <c r="N187" s="3" t="n">
-        <v>46079.4033912037</v>
+        <v>46079.48561342592</v>
       </c>
       <c r="O187" t="inlineStr">
         <is>
@@ -12671,7 +12666,7 @@
         <v>1</v>
       </c>
       <c r="N188" s="3" t="n">
-        <v>46079.36717592592</v>
+        <v>46079.4828125</v>
       </c>
       <c r="O188" t="inlineStr">
         <is>
@@ -12799,7 +12794,7 @@
         </is>
       </c>
       <c r="N190" s="3" t="n">
-        <v>46079.39745370371</v>
+        <v>46079.47493055555</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12927,7 +12922,7 @@
         <v>1</v>
       </c>
       <c r="N192" s="3" t="n">
-        <v>46079.39052083333</v>
+        <v>46079.48621527778</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -13052,7 +13047,7 @@
         <v>2</v>
       </c>
       <c r="N194" s="3" t="n">
-        <v>46079.38112268518</v>
+        <v>46079.4570949074</v>
       </c>
       <c r="O194" t="inlineStr">
         <is>
@@ -13116,7 +13111,7 @@
         <v>1</v>
       </c>
       <c r="N195" s="3" t="n">
-        <v>46079.40199074074</v>
+        <v>46079.4800925926</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13180,7 +13175,7 @@
         <v>1</v>
       </c>
       <c r="N196" s="3" t="n">
-        <v>46079.38256944445</v>
+        <v>46079.45402777778</v>
       </c>
       <c r="O196" t="inlineStr">
         <is>
@@ -13244,7 +13239,7 @@
         <v>1</v>
       </c>
       <c r="N197" s="3" t="n">
-        <v>46079.39512731481</v>
+        <v>46079.47207175926</v>
       </c>
       <c r="O197" t="inlineStr">
         <is>
@@ -13308,7 +13303,7 @@
         <v>1</v>
       </c>
       <c r="N198" s="3" t="n">
-        <v>46079.38622685185</v>
+        <v>46079.47293981481</v>
       </c>
       <c r="O198" t="inlineStr">
         <is>
@@ -13372,7 +13367,7 @@
         <v>1</v>
       </c>
       <c r="N199" s="3" t="n">
-        <v>46079.39532407407</v>
+        <v>46079.47952546296</v>
       </c>
       <c r="O199" t="inlineStr">
         <is>
@@ -13497,7 +13492,7 @@
         </is>
       </c>
       <c r="N201" s="3" t="n">
-        <v>46079.38711805556</v>
+        <v>46079.47065972222</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -13561,7 +13556,7 @@
         <v>1</v>
       </c>
       <c r="N202" s="3" t="n">
-        <v>46079.40178240741</v>
+        <v>46079.47430555556</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13625,7 +13620,7 @@
         <v>1</v>
       </c>
       <c r="N203" s="3" t="n">
-        <v>46079.39152777778</v>
+        <v>46079.46493055556</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13689,7 +13684,7 @@
         <v>1</v>
       </c>
       <c r="N204" s="3" t="n">
-        <v>46079.38211805555</v>
+        <v>46079.46111111111</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13753,7 +13748,7 @@
         <v>1</v>
       </c>
       <c r="N205" s="3" t="n">
-        <v>46079.3777662037</v>
+        <v>46079.46158564815</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13817,7 +13812,7 @@
         <v>1</v>
       </c>
       <c r="N206" s="3" t="n">
-        <v>46079.37552083333</v>
+        <v>46079.45233796296</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -13881,7 +13876,7 @@
         <v>1</v>
       </c>
       <c r="N207" s="3" t="n">
-        <v>46079.40247685185</v>
+        <v>46079.47954861111</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -13945,7 +13940,7 @@
         <v>1</v>
       </c>
       <c r="N208" s="3" t="n">
-        <v>46079.38053240741</v>
+        <v>46079.46167824074</v>
       </c>
       <c r="O208" t="inlineStr">
         <is>
@@ -14009,7 +14004,7 @@
         <v>1</v>
       </c>
       <c r="N209" s="3" t="n">
-        <v>46079.3696412037</v>
+        <v>46079.48626157407</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14073,7 +14068,7 @@
         <v>1</v>
       </c>
       <c r="N210" s="3" t="n">
-        <v>46079.37238425926</v>
+        <v>46079.4540625</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14137,7 +14132,7 @@
         <v>1</v>
       </c>
       <c r="N211" s="3" t="n">
-        <v>46079.37491898148</v>
+        <v>46079.45359953704</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -14201,7 +14196,7 @@
         <v>1</v>
       </c>
       <c r="N212" s="3" t="n">
-        <v>46079.37373842593</v>
+        <v>46079.48752314815</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -14265,7 +14260,7 @@
         <v>1</v>
       </c>
       <c r="N213" s="3" t="n">
-        <v>46079.38690972222</v>
+        <v>46079.46826388889</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
@@ -14329,7 +14324,7 @@
         <v>1</v>
       </c>
       <c r="N214" s="3" t="n">
-        <v>46079.37537037037</v>
+        <v>46079.45596064815</v>
       </c>
       <c r="O214" t="inlineStr">
         <is>
@@ -14457,7 +14452,7 @@
         <v>1</v>
       </c>
       <c r="N216" s="3" t="n">
-        <v>46079.37575231482</v>
+        <v>46079.45358796296</v>
       </c>
       <c r="O216" t="inlineStr">
         <is>
@@ -14516,7 +14511,7 @@
         <v>1</v>
       </c>
       <c r="N217" s="3" t="n">
-        <v>46079.3704050926</v>
+        <v>46079.44787037037</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14580,7 +14575,7 @@
         <v>1</v>
       </c>
       <c r="N218" s="3" t="n">
-        <v>46079.37349537037</v>
+        <v>46079.48678240741</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14713,7 +14708,7 @@
         <v>1</v>
       </c>
       <c r="N220" s="3" t="n">
-        <v>46079.3708912037</v>
+        <v>46079.44871527778</v>
       </c>
       <c r="O220" t="inlineStr">
         <is>
@@ -14777,7 +14772,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="3" t="n">
-        <v>46079.37903935185</v>
+        <v>46079.45604166666</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14841,7 +14836,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="3" t="n">
-        <v>46079.39098379629</v>
+        <v>46079.46947916667</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -14905,7 +14900,7 @@
         <v>1</v>
       </c>
       <c r="N223" s="3" t="n">
-        <v>46079.401875</v>
+        <v>46079.48200231481</v>
       </c>
       <c r="O223" t="inlineStr">
         <is>
@@ -15097,7 +15092,7 @@
         <v>1</v>
       </c>
       <c r="N226" s="3" t="n">
-        <v>46079.36709490741</v>
+        <v>46079.48350694445</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15225,7 +15220,7 @@
         <v>1</v>
       </c>
       <c r="N228" s="3" t="n">
-        <v>46079.39921296296</v>
+        <v>46079.47607638889</v>
       </c>
       <c r="O228" t="inlineStr">
         <is>
@@ -15289,7 +15284,7 @@
         <v>1</v>
       </c>
       <c r="N229" s="3" t="n">
-        <v>46079.36696759259</v>
+        <v>46079.48219907407</v>
       </c>
       <c r="O229" t="inlineStr">
         <is>
@@ -15353,7 +15348,7 @@
         <v>1</v>
       </c>
       <c r="N230" s="3" t="n">
-        <v>46079.39349537037</v>
+        <v>46079.46508101852</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15417,7 +15412,7 @@
         <v>1</v>
       </c>
       <c r="N231" s="3" t="n">
-        <v>46079.39707175926</v>
+        <v>46079.4777662037</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15481,7 +15476,7 @@
         <v>1</v>
       </c>
       <c r="N232" s="3" t="n">
-        <v>46079.38729166667</v>
+        <v>46079.46740740741</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -15545,7 +15540,7 @@
         <v>1</v>
       </c>
       <c r="N233" s="3" t="n">
-        <v>46079.36534722222</v>
+        <v>46079.48690972223</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15609,7 +15604,7 @@
         <v>1</v>
       </c>
       <c r="N234" s="3" t="n">
-        <v>46079.38773148148</v>
+        <v>46079.46427083333</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -15673,7 +15668,7 @@
         <v>1</v>
       </c>
       <c r="N235" s="3" t="n">
-        <v>46079.38143518518</v>
+        <v>46079.46505787037</v>
       </c>
       <c r="O235" t="inlineStr">
         <is>
@@ -15737,7 +15732,7 @@
         <v>1</v>
       </c>
       <c r="N236" s="3" t="n">
-        <v>46079.39681712963</v>
+        <v>46079.46902777778</v>
       </c>
       <c r="O236" t="inlineStr">
         <is>
@@ -15865,7 +15860,7 @@
         <v>1</v>
       </c>
       <c r="N238" s="3" t="n">
-        <v>46079.37599537037</v>
+        <v>46079.45262731481</v>
       </c>
       <c r="O238" t="inlineStr">
         <is>
@@ -15993,7 +15988,7 @@
         <v>1</v>
       </c>
       <c r="N240" s="3" t="n">
-        <v>46079.38373842592</v>
+        <v>46079.45894675926</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16057,7 +16052,7 @@
         <v>1</v>
       </c>
       <c r="N241" s="3" t="n">
-        <v>46079.37689814815</v>
+        <v>46079.45638888889</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16121,7 +16116,7 @@
         <v>1</v>
       </c>
       <c r="N242" s="3" t="n">
-        <v>46079.39303240741</v>
+        <v>46079.46662037037</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16185,7 +16180,7 @@
         <v>1</v>
       </c>
       <c r="N243" s="3" t="n">
-        <v>46079.39375</v>
+        <v>46079.47277777778</v>
       </c>
       <c r="O243" t="inlineStr">
         <is>
@@ -16308,7 +16303,7 @@
         <v>1</v>
       </c>
       <c r="N245" s="3" t="n">
-        <v>46079.39539351852</v>
+        <v>46079.4766087963</v>
       </c>
       <c r="O245" t="inlineStr">
         <is>
@@ -16372,7 +16367,7 @@
         <v>1</v>
       </c>
       <c r="N246" s="3" t="n">
-        <v>46079.38834490741</v>
+        <v>46079.46990740741</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16436,7 +16431,7 @@
         <v>1</v>
       </c>
       <c r="N247" s="3" t="n">
-        <v>46079.39790509259</v>
+        <v>46079.47354166667</v>
       </c>
       <c r="O247" t="inlineStr">
         <is>
@@ -16500,7 +16495,7 @@
         <v>1</v>
       </c>
       <c r="N248" s="3" t="n">
-        <v>46079.39883101852</v>
+        <v>46079.47817129629</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16564,7 +16559,7 @@
         <v>1</v>
       </c>
       <c r="N249" s="3" t="n">
-        <v>46079.39144675926</v>
+        <v>46079.47188657407</v>
       </c>
       <c r="O249" t="inlineStr">
         <is>
@@ -16583,6 +16578,11 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>10.69.5.118</t>
+        </is>
+      </c>
       <c r="D250" t="n">
         <v>2017</v>
       </c>
@@ -16623,7 +16623,7 @@
         <v>1</v>
       </c>
       <c r="N250" s="3" t="n">
-        <v>46079.37424768518</v>
+        <v>46079.48670138889</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16687,7 +16687,7 @@
         <v>1</v>
       </c>
       <c r="N251" s="3" t="n">
-        <v>46079.39520833334</v>
+        <v>46079.47681712963</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16751,7 +16751,7 @@
         <v>1</v>
       </c>
       <c r="N252" s="3" t="n">
-        <v>46079.4015625</v>
+        <v>46079.4753125</v>
       </c>
       <c r="O252" t="inlineStr">
         <is>
@@ -16815,7 +16815,7 @@
         <v>1</v>
       </c>
       <c r="N253" s="3" t="n">
-        <v>46079.37753472223</v>
+        <v>46079.45710648148</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16873,7 +16873,7 @@
         <v>1</v>
       </c>
       <c r="N254" s="3" t="n">
-        <v>46079.39758101852</v>
+        <v>46079.47923611111</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -16937,7 +16937,7 @@
         <v>1</v>
       </c>
       <c r="N255" s="3" t="n">
-        <v>46079.39728009259</v>
+        <v>46079.47327546297</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -17001,7 +17001,7 @@
         <v>1</v>
       </c>
       <c r="N256" s="3" t="n">
-        <v>46079.37936342593</v>
+        <v>46079.4584375</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17065,7 +17065,7 @@
         <v>1</v>
       </c>
       <c r="N257" s="3" t="n">
-        <v>46079.38851851852</v>
+        <v>46079.4649537037</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17129,7 +17129,7 @@
         <v>1</v>
       </c>
       <c r="N258" s="3" t="n">
-        <v>46079.37704861111</v>
+        <v>46079.485</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
@@ -17257,7 +17257,7 @@
         <v>1</v>
       </c>
       <c r="N260" s="3" t="n">
-        <v>46079.3700925926</v>
+        <v>46079.48768518519</v>
       </c>
       <c r="O260" t="inlineStr">
         <is>
@@ -17321,7 +17321,7 @@
         <v>1</v>
       </c>
       <c r="N261" s="3" t="n">
-        <v>46079.40420138889</v>
+        <v>46079.4806712963</v>
       </c>
       <c r="O261" t="inlineStr">
         <is>
@@ -17385,7 +17385,7 @@
         <v>1</v>
       </c>
       <c r="N262" s="3" t="n">
-        <v>46079.39037037037</v>
+        <v>46079.46703703704</v>
       </c>
       <c r="O262" t="inlineStr">
         <is>
@@ -17449,7 +17449,7 @@
         <v>1</v>
       </c>
       <c r="N263" s="3" t="n">
-        <v>46079.39888888889</v>
+        <v>46079.47767361111</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17513,7 +17513,7 @@
         <v>1</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>46079.38222222222</v>
+        <v>46079.46248842592</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17577,7 +17577,7 @@
         <v>1</v>
       </c>
       <c r="N265" s="3" t="n">
-        <v>46079.36679398148</v>
+        <v>46079.44974537037</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17641,7 +17641,7 @@
         <v>1</v>
       </c>
       <c r="N266" s="3" t="n">
-        <v>46079.37402777778</v>
+        <v>46079.44974537037</v>
       </c>
       <c r="O266" t="inlineStr">
         <is>
@@ -17705,7 +17705,7 @@
         <v>1</v>
       </c>
       <c r="N267" s="3" t="n">
-        <v>46079.37193287037</v>
+        <v>46079.48478009259</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17769,7 +17769,7 @@
         <v>1</v>
       </c>
       <c r="N268" s="3" t="n">
-        <v>46079.37832175926</v>
+        <v>46079.45177083334</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17833,7 +17833,7 @@
         <v>1</v>
       </c>
       <c r="N269" s="3" t="n">
-        <v>46078.86444444444</v>
+        <v>46079.44898148148</v>
       </c>
       <c r="O269" t="inlineStr">
         <is>
@@ -17894,7 +17894,7 @@
         </is>
       </c>
       <c r="N270" s="3" t="n">
-        <v>46079.38876157408</v>
+        <v>46079.46638888889</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -18022,7 +18022,7 @@
         <v>1</v>
       </c>
       <c r="N272" s="3" t="n">
-        <v>46078.62369212963</v>
+        <v>46079.45494212963</v>
       </c>
       <c r="O272" t="inlineStr">
         <is>
@@ -18406,7 +18406,7 @@
         <v>1</v>
       </c>
       <c r="N278" s="3" t="n">
-        <v>46079.39979166666</v>
+        <v>46079.47587962963</v>
       </c>
       <c r="O278" t="inlineStr">
         <is>
@@ -18470,7 +18470,7 @@
         <v>1</v>
       </c>
       <c r="N279" s="3" t="n">
-        <v>46079.37945601852</v>
+        <v>46079.45444444445</v>
       </c>
       <c r="O279" t="inlineStr">
         <is>
@@ -18534,7 +18534,7 @@
         <v>1</v>
       </c>
       <c r="N280" s="3" t="n">
-        <v>46079.37284722222</v>
+        <v>46079.47704861111</v>
       </c>
       <c r="O280" t="inlineStr">
         <is>
@@ -18598,7 +18598,7 @@
         <v>1</v>
       </c>
       <c r="N281" s="3" t="n">
-        <v>46078.565625</v>
+        <v>46079.48320601852</v>
       </c>
       <c r="O281" t="inlineStr">
         <is>
@@ -18617,11 +18617,6 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
-      <c r="C282" t="inlineStr">
-        <is>
-          <t>10.69.5.151</t>
-        </is>
-      </c>
       <c r="D282" t="n">
         <v>2017</v>
       </c>
@@ -18662,7 +18657,7 @@
         <v>1</v>
       </c>
       <c r="N282" s="3" t="n">
-        <v>46079.40283564815</v>
+        <v>46079.48270833334</v>
       </c>
       <c r="O282" t="inlineStr">
         <is>
@@ -18726,7 +18721,7 @@
         <v>1</v>
       </c>
       <c r="N283" s="3" t="n">
-        <v>46078.81083333334</v>
+        <v>46079.44024305556</v>
       </c>
       <c r="O283" t="inlineStr">
         <is>
@@ -18790,7 +18785,7 @@
         <v>1</v>
       </c>
       <c r="N284" s="3" t="n">
-        <v>46079.3706712963</v>
+        <v>46079.48789351852</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18854,7 +18849,7 @@
         <v>1</v>
       </c>
       <c r="N285" s="3" t="n">
-        <v>46079.38053240741</v>
+        <v>46079.45896990741</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -18918,7 +18913,7 @@
         <v>1</v>
       </c>
       <c r="N286" s="3" t="n">
-        <v>46079.39363425926</v>
+        <v>46079.47096064815</v>
       </c>
       <c r="O286" t="inlineStr">
         <is>
@@ -18982,7 +18977,7 @@
         <v>1</v>
       </c>
       <c r="N287" s="3" t="n">
-        <v>46079.37765046296</v>
+        <v>46079.45738425926</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
@@ -19046,7 +19041,7 @@
         <v>1</v>
       </c>
       <c r="N288" s="3" t="n">
-        <v>46079.3632175926</v>
+        <v>46079.48334490741</v>
       </c>
       <c r="O288" t="inlineStr">
         <is>
@@ -19110,7 +19105,7 @@
         <v>1</v>
       </c>
       <c r="N289" s="3" t="n">
-        <v>46079.39600694444</v>
+        <v>46079.4777662037</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -19904,7 +19899,7 @@
         <v>1</v>
       </c>
       <c r="N302" s="3" t="n">
-        <v>46079.39976851852</v>
+        <v>46079.47530092593</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -21020,7 +21015,7 @@
         </is>
       </c>
       <c r="N320" s="3" t="n">
-        <v>46079.38806712963</v>
+        <v>46079.46159722222</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21745,7 +21740,7 @@
         <v>1</v>
       </c>
       <c r="N332" s="3" t="n">
-        <v>46079.36636574074</v>
+        <v>46079.48311342593</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21809,7 +21804,7 @@
         <v>2</v>
       </c>
       <c r="N333" s="3" t="n">
-        <v>46079.39377314815</v>
+        <v>46079.47231481481</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21873,7 +21868,7 @@
         <v>2</v>
       </c>
       <c r="N334" s="3" t="n">
-        <v>46079.40150462963</v>
+        <v>46079.47956018519</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21937,7 +21932,7 @@
         <v>2</v>
       </c>
       <c r="N335" s="3" t="n">
-        <v>46079.39576388889</v>
+        <v>46079.47697916667</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -22001,7 +21996,7 @@
         <v>1</v>
       </c>
       <c r="N336" s="3" t="n">
-        <v>46079.3984375</v>
+        <v>46079.47658564815</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22065,7 +22060,7 @@
         <v>1</v>
       </c>
       <c r="N337" s="3" t="n">
-        <v>46079.38277777778</v>
+        <v>46079.46079861111</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22129,7 +22124,7 @@
         <v>2</v>
       </c>
       <c r="N338" s="3" t="n">
-        <v>46079.39449074074</v>
+        <v>46079.47392361111</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -22193,7 +22188,7 @@
         <v>2</v>
       </c>
       <c r="N339" s="3" t="n">
-        <v>46079.40258101852</v>
+        <v>46079.47626157408</v>
       </c>
       <c r="O339" t="inlineStr">
         <is>
@@ -22385,7 +22380,7 @@
         <v>2</v>
       </c>
       <c r="N342" s="3" t="n">
-        <v>46078.57918981482</v>
+        <v>46079.46834490741</v>
       </c>
       <c r="O342" t="inlineStr">
         <is>
@@ -22446,7 +22441,7 @@
         </is>
       </c>
       <c r="N343" s="3" t="n">
-        <v>46079.38466435186</v>
+        <v>46079.42385416666</v>
       </c>
       <c r="O343" t="inlineStr">
         <is>
@@ -23831,7 +23826,7 @@
         <v>1</v>
       </c>
       <c r="N365" s="3" t="n">
-        <v>46079.36765046296</v>
+        <v>46079.48180555556</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
@@ -23897,7 +23892,7 @@
         </is>
       </c>
       <c r="N366" s="3" t="n">
-        <v>46079.40423611111</v>
+        <v>46079.48222222222</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -24023,7 +24018,7 @@
         </is>
       </c>
       <c r="N368" s="3" t="n">
-        <v>46079.39657407408</v>
+        <v>46079.47171296296</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -24089,7 +24084,7 @@
         </is>
       </c>
       <c r="N369" s="3" t="n">
-        <v>46079.39780092592</v>
+        <v>46079.47700231482</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
@@ -24158,7 +24153,7 @@
         <v>1</v>
       </c>
       <c r="N370" s="3" t="n">
-        <v>46079.39724537037</v>
+        <v>46079.46847222222</v>
       </c>
       <c r="O370" t="inlineStr">
         <is>
@@ -24431,7 +24426,7 @@
         <v>1</v>
       </c>
       <c r="N374" s="3" t="n">
-        <v>46079.38832175926</v>
+        <v>46079.46734953704</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24497,7 +24492,7 @@
         </is>
       </c>
       <c r="N375" s="3" t="n">
-        <v>46079.38832175926</v>
+        <v>46079.46820601852</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
@@ -24516,6 +24511,11 @@
           <t>COORDENACAO</t>
         </is>
       </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>10.69.3.72</t>
+        </is>
+      </c>
       <c r="D376" t="n">
         <v>2025</v>
       </c>
@@ -24561,7 +24561,7 @@
         <v>1</v>
       </c>
       <c r="N376" s="3" t="n">
-        <v>46079.37414351852</v>
+        <v>46079.48564814815</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -24630,7 +24630,7 @@
         <v>2</v>
       </c>
       <c r="N377" s="3" t="n">
-        <v>46079.40401620371</v>
+        <v>46079.48153935185</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -24699,7 +24699,7 @@
         <v>2</v>
       </c>
       <c r="N378" s="3" t="n">
-        <v>46079.38674768519</v>
+        <v>46079.46601851852</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização automática 2026-02-26 13:52:04.578302
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>46079.48491898148</v>
+        <v>46079.56414351852</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>46079.4525</v>
+        <v>46079.53265046296</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
         <v>1</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>46079.4693287037</v>
+        <v>46079.55021990741</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>46079.45071759259</v>
+        <v>46079.56971064815</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -1259,7 +1259,7 @@
         <v>1</v>
       </c>
       <c r="N12" s="3" t="n">
-        <v>46079.45965277778</v>
+        <v>46079.53686342593</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1515,7 +1515,7 @@
         <v>2</v>
       </c>
       <c r="N16" s="3" t="n">
-        <v>46079.45452546296</v>
+        <v>46079.53008101852</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1579,7 +1579,7 @@
         <v>1</v>
       </c>
       <c r="N17" s="3" t="n">
-        <v>46079.47435185185</v>
+        <v>46079.55170138889</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1643,7 +1643,7 @@
         <v>2</v>
       </c>
       <c r="N18" s="3" t="n">
-        <v>46079.47866898148</v>
+        <v>46079.55622685186</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1768,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="N20" s="3" t="n">
-        <v>46079.45961805555</v>
+        <v>46079.54232638889</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1950,7 +1950,7 @@
         <v>1</v>
       </c>
       <c r="N23" s="3" t="n">
-        <v>46079.45313657408</v>
+        <v>46079.49225694445</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2009,7 +2009,7 @@
         <v>1</v>
       </c>
       <c r="N24" s="3" t="n">
-        <v>46079.19900462963</v>
+        <v>46079.53746527778</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -6570,7 +6570,7 @@
         <v>1</v>
       </c>
       <c r="N95" s="3" t="n">
-        <v>46079.48383101852</v>
+        <v>46079.56140046296</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -6639,7 +6639,7 @@
         <v>1</v>
       </c>
       <c r="N96" s="3" t="n">
-        <v>46079.47336805556</v>
+        <v>46079.55541666667</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
@@ -6703,7 +6703,7 @@
         <v>1</v>
       </c>
       <c r="N97" s="3" t="n">
-        <v>46079.44966435185</v>
+        <v>46079.56730324074</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -6722,6 +6722,11 @@
           <t>COORDENACAO</t>
         </is>
       </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>10.69.3.94</t>
+        </is>
+      </c>
       <c r="D98" t="n">
         <v>2025</v>
       </c>
@@ -6767,7 +6772,7 @@
         <v>1</v>
       </c>
       <c r="N98" s="3" t="n">
-        <v>46079.46195601852</v>
+        <v>46079.56954861111</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -6836,7 +6841,7 @@
         <v>1</v>
       </c>
       <c r="N99" s="3" t="n">
-        <v>46079.46267361111</v>
+        <v>46079.54527777778</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -6905,7 +6910,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>46079.46215277778</v>
+        <v>46079.53658564815</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6974,7 +6979,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="3" t="n">
-        <v>46079.46616898148</v>
+        <v>46079.54232638889</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -7112,7 +7117,7 @@
         <v>2</v>
       </c>
       <c r="N103" s="3" t="n">
-        <v>46079.45846064815</v>
+        <v>46079.53436342593</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7242,7 +7247,7 @@
         <v>1</v>
       </c>
       <c r="N105" s="3" t="n">
-        <v>46079.48565972222</v>
+        <v>46079.52680555556</v>
       </c>
       <c r="O105" t="inlineStr">
         <is>
@@ -7372,7 +7377,7 @@
         <v>1</v>
       </c>
       <c r="N107" s="3" t="n">
-        <v>46079.45363425926</v>
+        <v>46079.53462962963</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -7510,7 +7515,7 @@
         <v>1</v>
       </c>
       <c r="N109" s="3" t="n">
-        <v>46079.47922453703</v>
+        <v>46079.55327546296</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7579,7 +7584,7 @@
         <v>2</v>
       </c>
       <c r="N110" s="3" t="n">
-        <v>46079.46409722222</v>
+        <v>46079.5433912037</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7648,7 +7653,7 @@
         <v>2</v>
       </c>
       <c r="N111" s="3" t="n">
-        <v>46079.45648148148</v>
+        <v>46079.53177083333</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
@@ -7717,7 +7722,7 @@
         <v>2</v>
       </c>
       <c r="N112" s="3" t="n">
-        <v>46079.45326388889</v>
+        <v>46079.57063657408</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7786,7 +7791,7 @@
         <v>1</v>
       </c>
       <c r="N113" s="3" t="n">
-        <v>46079.47232638889</v>
+        <v>46079.55090277778</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7855,7 +7860,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>46079.48275462963</v>
+        <v>46079.56619212963</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -7921,7 +7926,7 @@
         </is>
       </c>
       <c r="N115" s="3" t="n">
-        <v>46079.45853009259</v>
+        <v>46079.56819444444</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -7990,7 +7995,7 @@
         <v>1</v>
       </c>
       <c r="N116" s="3" t="n">
-        <v>46079.45710648148</v>
+        <v>46079.53865740741</v>
       </c>
       <c r="O116" t="inlineStr">
         <is>
@@ -8009,6 +8014,11 @@
           <t>DP</t>
         </is>
       </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>10.69.3.23</t>
+        </is>
+      </c>
       <c r="D117" t="n">
         <v>2025</v>
       </c>
@@ -8054,7 +8064,7 @@
         <v>1</v>
       </c>
       <c r="N117" s="3" t="n">
-        <v>46079.44967592593</v>
+        <v>46079.56611111111</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -8120,7 +8130,7 @@
         </is>
       </c>
       <c r="N118" s="3" t="n">
-        <v>46079.45829861111</v>
+        <v>46079.56975694445</v>
       </c>
       <c r="O118" t="inlineStr">
         <is>
@@ -8258,7 +8268,7 @@
         <v>1</v>
       </c>
       <c r="N120" s="3" t="n">
-        <v>46079.47665509259</v>
+        <v>46079.55517361111</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -8327,7 +8337,7 @@
         <v>1</v>
       </c>
       <c r="N121" s="3" t="n">
-        <v>46079.47423611111</v>
+        <v>46079.55118055556</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -8393,7 +8403,7 @@
         </is>
       </c>
       <c r="N122" s="3" t="n">
-        <v>46079.48568287037</v>
+        <v>46079.56135416667</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -8462,7 +8472,7 @@
         <v>2</v>
       </c>
       <c r="N123" s="3" t="n">
-        <v>46079.46644675926</v>
+        <v>46079.54084490741</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -8531,7 +8541,7 @@
         <v>1</v>
       </c>
       <c r="N124" s="3" t="n">
-        <v>46079.45349537037</v>
+        <v>46079.53310185186</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -8600,7 +8610,7 @@
         <v>1</v>
       </c>
       <c r="N125" s="3" t="n">
-        <v>46079.48237268518</v>
+        <v>46079.55939814815</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -8669,7 +8679,7 @@
         <v>2</v>
       </c>
       <c r="N126" s="3" t="n">
-        <v>46079.48162037037</v>
+        <v>46079.5637037037</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -8738,7 +8748,7 @@
         <v>2</v>
       </c>
       <c r="N127" s="3" t="n">
-        <v>46079.48451388889</v>
+        <v>46079.56527777778</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -8807,7 +8817,7 @@
         <v>1</v>
       </c>
       <c r="N128" s="3" t="n">
-        <v>46079.45284722222</v>
+        <v>46079.56128472222</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -8876,7 +8886,7 @@
         <v>1</v>
       </c>
       <c r="N129" s="3" t="n">
-        <v>46079.4783912037</v>
+        <v>46079.55975694444</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -8945,7 +8955,7 @@
         <v>1</v>
       </c>
       <c r="N130" s="3" t="n">
-        <v>46079.47847222222</v>
+        <v>46079.55263888889</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -9009,7 +9019,7 @@
         <v>1</v>
       </c>
       <c r="N131" s="3" t="n">
-        <v>46079.45976851852</v>
+        <v>46079.54010416667</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -9461,7 +9471,7 @@
         <v>1</v>
       </c>
       <c r="N138" s="3" t="n">
-        <v>46079.45554398148</v>
+        <v>46079.53417824074</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9525,7 +9535,7 @@
         <v>1</v>
       </c>
       <c r="N139" s="3" t="n">
-        <v>46079.4872337963</v>
+        <v>46079.56990740741</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9589,7 +9599,7 @@
         <v>1</v>
       </c>
       <c r="N140" s="3" t="n">
-        <v>46079.46677083334</v>
+        <v>46079.54722222222</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9653,7 +9663,7 @@
         <v>1</v>
       </c>
       <c r="N141" s="3" t="n">
-        <v>46079.4725</v>
+        <v>46079.54894675926</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9717,7 +9727,7 @@
         <v>1</v>
       </c>
       <c r="N142" s="3" t="n">
-        <v>46079.46787037037</v>
+        <v>46079.54814814815</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9781,7 +9791,7 @@
         <v>1</v>
       </c>
       <c r="N143" s="3" t="n">
-        <v>46079.47604166667</v>
+        <v>46079.55361111111</v>
       </c>
       <c r="O143" t="inlineStr">
         <is>
@@ -9845,7 +9855,7 @@
         <v>1</v>
       </c>
       <c r="N144" s="3" t="n">
-        <v>46079.46849537037</v>
+        <v>46079.54167824074</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9973,7 +9983,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="3" t="n">
-        <v>46079.45458333333</v>
+        <v>46079.53511574074</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10037,7 +10047,7 @@
         <v>1</v>
       </c>
       <c r="N147" s="3" t="n">
-        <v>46079.47811342592</v>
+        <v>46079.55849537037</v>
       </c>
       <c r="O147" t="inlineStr">
         <is>
@@ -10101,7 +10111,7 @@
         <v>1</v>
       </c>
       <c r="N148" s="3" t="n">
-        <v>46079.45717592593</v>
+        <v>46079.53626157407</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10165,7 +10175,7 @@
         <v>1</v>
       </c>
       <c r="N149" s="3" t="n">
-        <v>46079.44863425926</v>
+        <v>46079.56458333333</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -10229,7 +10239,7 @@
         <v>1</v>
       </c>
       <c r="N150" s="3" t="n">
-        <v>46079.4800925926</v>
+        <v>46079.55873842593</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -10293,7 +10303,7 @@
         <v>1</v>
       </c>
       <c r="N151" s="3" t="n">
-        <v>46079.45417824074</v>
+        <v>46079.53193287037</v>
       </c>
       <c r="O151" t="inlineStr">
         <is>
@@ -10357,7 +10367,7 @@
         <v>1</v>
       </c>
       <c r="N152" s="3" t="n">
-        <v>46079.46793981481</v>
+        <v>46079.54636574074</v>
       </c>
       <c r="O152" t="inlineStr">
         <is>
@@ -10421,7 +10431,7 @@
         <v>1</v>
       </c>
       <c r="N153" s="3" t="n">
-        <v>46079.4521875</v>
+        <v>46079.57071759259</v>
       </c>
       <c r="O153" t="inlineStr">
         <is>
@@ -10485,7 +10495,7 @@
         <v>1</v>
       </c>
       <c r="N154" s="3" t="n">
-        <v>46079.48783564815</v>
+        <v>46079.56189814815</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10549,7 +10559,7 @@
         <v>1</v>
       </c>
       <c r="N155" s="3" t="n">
-        <v>46079.48525462963</v>
+        <v>46079.55753472223</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10613,7 +10623,7 @@
         <v>1</v>
       </c>
       <c r="N156" s="3" t="n">
-        <v>46079.47872685185</v>
+        <v>46079.55498842592</v>
       </c>
       <c r="O156" t="inlineStr">
         <is>
@@ -10677,7 +10687,7 @@
         <v>1</v>
       </c>
       <c r="N157" s="3" t="n">
-        <v>46079.45737268519</v>
+        <v>46079.53510416667</v>
       </c>
       <c r="O157" t="inlineStr">
         <is>
@@ -10741,7 +10751,7 @@
         <v>1</v>
       </c>
       <c r="N158" s="3" t="n">
-        <v>46079.45199074074</v>
+        <v>46079.55101851852</v>
       </c>
       <c r="O158" t="inlineStr">
         <is>
@@ -10805,7 +10815,7 @@
         <v>1</v>
       </c>
       <c r="N159" s="3" t="n">
-        <v>46079.47627314815</v>
+        <v>46079.54811342592</v>
       </c>
       <c r="O159" t="inlineStr">
         <is>
@@ -10869,7 +10879,7 @@
         <v>1</v>
       </c>
       <c r="N160" s="3" t="n">
-        <v>46079.48569444445</v>
+        <v>46079.56278935185</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
@@ -10933,7 +10943,7 @@
         <v>1</v>
       </c>
       <c r="N161" s="3" t="n">
-        <v>46079.4875462963</v>
+        <v>46079.56318287037</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -10997,7 +11007,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="3" t="n">
-        <v>46079.48130787037</v>
+        <v>46079.56283564815</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11061,7 +11071,7 @@
         <v>2</v>
       </c>
       <c r="N163" s="3" t="n">
-        <v>46078.50972222222</v>
+        <v>46079.55581018519</v>
       </c>
       <c r="O163" t="inlineStr">
         <is>
@@ -11125,7 +11135,7 @@
         <v>2</v>
       </c>
       <c r="N164" s="3" t="n">
-        <v>46079.48048611111</v>
+        <v>46079.56171296296</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11189,7 +11199,7 @@
         <v>2</v>
       </c>
       <c r="N165" s="3" t="n">
-        <v>46079.48491898148</v>
+        <v>46079.56068287037</v>
       </c>
       <c r="O165" t="inlineStr">
         <is>
@@ -11253,7 +11263,7 @@
         <v>2</v>
       </c>
       <c r="N166" s="3" t="n">
-        <v>46079.45075231481</v>
+        <v>46079.57015046296</v>
       </c>
       <c r="O166" t="inlineStr">
         <is>
@@ -11317,7 +11327,7 @@
         <v>2</v>
       </c>
       <c r="N167" s="3" t="n">
-        <v>46079.48487268519</v>
+        <v>46079.56164351852</v>
       </c>
       <c r="O167" t="inlineStr">
         <is>
@@ -11381,7 +11391,7 @@
         <v>2</v>
       </c>
       <c r="N168" s="3" t="n">
-        <v>46079.45298611111</v>
+        <v>46079.56518518519</v>
       </c>
       <c r="O168" t="inlineStr">
         <is>
@@ -11445,7 +11455,7 @@
         <v>2</v>
       </c>
       <c r="N169" s="3" t="n">
-        <v>46079.48660879629</v>
+        <v>46079.55982638889</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -11509,7 +11519,7 @@
         <v>2</v>
       </c>
       <c r="N170" s="3" t="n">
-        <v>46079.47512731481</v>
+        <v>46079.54729166667</v>
       </c>
       <c r="O170" t="inlineStr">
         <is>
@@ -11570,10 +11580,10 @@
         </is>
       </c>
       <c r="M171" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N171" s="3" t="n">
-        <v>46079.48173611111</v>
+        <v>46079.55938657407</v>
       </c>
       <c r="O171" t="inlineStr">
         <is>
@@ -11637,7 +11647,7 @@
         <v>2</v>
       </c>
       <c r="N172" s="3" t="n">
-        <v>46079.46847222222</v>
+        <v>46079.54769675926</v>
       </c>
       <c r="O172" t="inlineStr">
         <is>
@@ -11698,10 +11708,10 @@
         </is>
       </c>
       <c r="M173" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N173" s="3" t="n">
-        <v>46079.45515046296</v>
+        <v>46079.56776620371</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -11765,7 +11775,7 @@
         <v>2</v>
       </c>
       <c r="N174" s="3" t="n">
-        <v>46079.47434027777</v>
+        <v>46079.55133101852</v>
       </c>
       <c r="O174" t="inlineStr">
         <is>
@@ -11829,7 +11839,7 @@
         <v>2</v>
       </c>
       <c r="N175" s="3" t="n">
-        <v>46079.45849537037</v>
+        <v>46079.53645833334</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -11893,7 +11903,7 @@
         <v>2</v>
       </c>
       <c r="N176" s="3" t="n">
-        <v>46079.47229166667</v>
+        <v>46079.5496875</v>
       </c>
       <c r="O176" t="inlineStr">
         <is>
@@ -11957,7 +11967,7 @@
         <v>2</v>
       </c>
       <c r="N177" s="3" t="n">
-        <v>46079.46505787037</v>
+        <v>46079.54571759259</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
@@ -12021,7 +12031,7 @@
         <v>2</v>
       </c>
       <c r="N178" s="3" t="n">
-        <v>46079.47356481481</v>
+        <v>46079.55065972222</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12085,7 +12095,7 @@
         <v>1</v>
       </c>
       <c r="N179" s="3" t="n">
-        <v>46079.47994212963</v>
+        <v>46079.55805555556</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12149,7 +12159,7 @@
         <v>1</v>
       </c>
       <c r="N180" s="3" t="n">
-        <v>46079.45074074074</v>
+        <v>46079.56868055555</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12213,7 +12223,7 @@
         <v>1</v>
       </c>
       <c r="N181" s="3" t="n">
-        <v>46079.47958333333</v>
+        <v>46079.55662037037</v>
       </c>
       <c r="O181" t="inlineStr">
         <is>
@@ -12341,7 +12351,7 @@
         <v>1</v>
       </c>
       <c r="N183" s="3" t="n">
-        <v>46079.47413194444</v>
+        <v>46079.55118055556</v>
       </c>
       <c r="O183" t="inlineStr">
         <is>
@@ -12410,7 +12420,7 @@
         <v>2</v>
       </c>
       <c r="N184" s="3" t="n">
-        <v>46079.46527777778</v>
+        <v>46079.54085648148</v>
       </c>
       <c r="O184" t="inlineStr">
         <is>
@@ -12474,7 +12484,7 @@
         <v>1</v>
       </c>
       <c r="N185" s="3" t="n">
-        <v>46079.4756712963</v>
+        <v>46079.55450231482</v>
       </c>
       <c r="O185" t="inlineStr">
         <is>
@@ -12538,7 +12548,7 @@
         <v>1</v>
       </c>
       <c r="N186" s="3" t="n">
-        <v>46079.45516203704</v>
+        <v>46079.56818287037</v>
       </c>
       <c r="O186" t="inlineStr">
         <is>
@@ -12602,7 +12612,7 @@
         <v>1</v>
       </c>
       <c r="N187" s="3" t="n">
-        <v>46079.48561342592</v>
+        <v>46079.5681712963</v>
       </c>
       <c r="O187" t="inlineStr">
         <is>
@@ -12666,7 +12676,7 @@
         <v>1</v>
       </c>
       <c r="N188" s="3" t="n">
-        <v>46079.4828125</v>
+        <v>46079.56212962963</v>
       </c>
       <c r="O188" t="inlineStr">
         <is>
@@ -12794,7 +12804,7 @@
         </is>
       </c>
       <c r="N190" s="3" t="n">
-        <v>46079.47493055555</v>
+        <v>46079.54884259259</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12922,7 +12932,7 @@
         <v>1</v>
       </c>
       <c r="N192" s="3" t="n">
-        <v>46079.48621527778</v>
+        <v>46079.56480324074</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -13047,7 +13057,7 @@
         <v>2</v>
       </c>
       <c r="N194" s="3" t="n">
-        <v>46079.4570949074</v>
+        <v>46079.5708912037</v>
       </c>
       <c r="O194" t="inlineStr">
         <is>
@@ -13111,7 +13121,7 @@
         <v>1</v>
       </c>
       <c r="N195" s="3" t="n">
-        <v>46079.4800925926</v>
+        <v>46079.56032407407</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13175,7 +13185,7 @@
         <v>1</v>
       </c>
       <c r="N196" s="3" t="n">
-        <v>46079.45402777778</v>
+        <v>46079.53146990741</v>
       </c>
       <c r="O196" t="inlineStr">
         <is>
@@ -13239,7 +13249,7 @@
         <v>1</v>
       </c>
       <c r="N197" s="3" t="n">
-        <v>46079.47207175926</v>
+        <v>46079.55083333333</v>
       </c>
       <c r="O197" t="inlineStr">
         <is>
@@ -13303,7 +13313,7 @@
         <v>1</v>
       </c>
       <c r="N198" s="3" t="n">
-        <v>46079.47293981481</v>
+        <v>46079.54706018518</v>
       </c>
       <c r="O198" t="inlineStr">
         <is>
@@ -13367,7 +13377,7 @@
         <v>1</v>
       </c>
       <c r="N199" s="3" t="n">
-        <v>46079.47952546296</v>
+        <v>46079.56296296296</v>
       </c>
       <c r="O199" t="inlineStr">
         <is>
@@ -13492,7 +13502,7 @@
         </is>
       </c>
       <c r="N201" s="3" t="n">
-        <v>46079.47065972222</v>
+        <v>46079.55339120371</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -13556,7 +13566,7 @@
         <v>1</v>
       </c>
       <c r="N202" s="3" t="n">
-        <v>46079.47430555556</v>
+        <v>46079.551875</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13620,7 +13630,7 @@
         <v>1</v>
       </c>
       <c r="N203" s="3" t="n">
-        <v>46079.46493055556</v>
+        <v>46079.53502314815</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13684,7 +13694,7 @@
         <v>1</v>
       </c>
       <c r="N204" s="3" t="n">
-        <v>46079.46111111111</v>
+        <v>46079.53776620371</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13748,7 +13758,7 @@
         <v>1</v>
       </c>
       <c r="N205" s="3" t="n">
-        <v>46079.46158564815</v>
+        <v>46079.535</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13812,7 +13822,7 @@
         <v>1</v>
       </c>
       <c r="N206" s="3" t="n">
-        <v>46079.45233796296</v>
+        <v>46079.56975694445</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -13876,7 +13886,7 @@
         <v>1</v>
       </c>
       <c r="N207" s="3" t="n">
-        <v>46079.47954861111</v>
+        <v>46079.55866898148</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -13940,7 +13950,7 @@
         <v>1</v>
       </c>
       <c r="N208" s="3" t="n">
-        <v>46079.46167824074</v>
+        <v>46079.54260416667</v>
       </c>
       <c r="O208" t="inlineStr">
         <is>
@@ -14004,7 +14014,7 @@
         <v>1</v>
       </c>
       <c r="N209" s="3" t="n">
-        <v>46079.48626157407</v>
+        <v>46079.56896990741</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14068,7 +14078,7 @@
         <v>1</v>
       </c>
       <c r="N210" s="3" t="n">
-        <v>46079.4540625</v>
+        <v>46079.56989583333</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14132,7 +14142,7 @@
         <v>1</v>
       </c>
       <c r="N211" s="3" t="n">
-        <v>46079.45359953704</v>
+        <v>46079.5616087963</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -14196,7 +14206,7 @@
         <v>1</v>
       </c>
       <c r="N212" s="3" t="n">
-        <v>46079.48752314815</v>
+        <v>46079.56719907407</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -14260,7 +14270,7 @@
         <v>1</v>
       </c>
       <c r="N213" s="3" t="n">
-        <v>46079.46826388889</v>
+        <v>46079.54940972223</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
@@ -14324,7 +14334,7 @@
         <v>1</v>
       </c>
       <c r="N214" s="3" t="n">
-        <v>46079.45596064815</v>
+        <v>46079.53744212963</v>
       </c>
       <c r="O214" t="inlineStr">
         <is>
@@ -14452,7 +14462,7 @@
         <v>1</v>
       </c>
       <c r="N216" s="3" t="n">
-        <v>46079.45358796296</v>
+        <v>46079.56653935185</v>
       </c>
       <c r="O216" t="inlineStr">
         <is>
@@ -14511,7 +14521,7 @@
         <v>1</v>
       </c>
       <c r="N217" s="3" t="n">
-        <v>46079.44787037037</v>
+        <v>46079.56327546296</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14575,7 +14585,7 @@
         <v>1</v>
       </c>
       <c r="N218" s="3" t="n">
-        <v>46079.48678240741</v>
+        <v>46079.56854166667</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14708,7 +14718,7 @@
         <v>1</v>
       </c>
       <c r="N220" s="3" t="n">
-        <v>46079.44871527778</v>
+        <v>46079.56922453704</v>
       </c>
       <c r="O220" t="inlineStr">
         <is>
@@ -14772,7 +14782,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="3" t="n">
-        <v>46079.45604166666</v>
+        <v>46079.5366087963</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14836,7 +14846,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="3" t="n">
-        <v>46079.46947916667</v>
+        <v>46079.54344907407</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -14900,7 +14910,7 @@
         <v>1</v>
       </c>
       <c r="N223" s="3" t="n">
-        <v>46079.48200231481</v>
+        <v>46079.56135416667</v>
       </c>
       <c r="O223" t="inlineStr">
         <is>
@@ -15092,7 +15102,7 @@
         <v>1</v>
       </c>
       <c r="N226" s="3" t="n">
-        <v>46079.48350694445</v>
+        <v>46079.55592592592</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15220,7 +15230,7 @@
         <v>1</v>
       </c>
       <c r="N228" s="3" t="n">
-        <v>46079.47607638889</v>
+        <v>46079.55600694445</v>
       </c>
       <c r="O228" t="inlineStr">
         <is>
@@ -15284,7 +15294,7 @@
         <v>1</v>
       </c>
       <c r="N229" s="3" t="n">
-        <v>46079.48219907407</v>
+        <v>46079.55915509259</v>
       </c>
       <c r="O229" t="inlineStr">
         <is>
@@ -15348,7 +15358,7 @@
         <v>1</v>
       </c>
       <c r="N230" s="3" t="n">
-        <v>46079.46508101852</v>
+        <v>46079.54101851852</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15412,7 +15422,7 @@
         <v>1</v>
       </c>
       <c r="N231" s="3" t="n">
-        <v>46079.4777662037</v>
+        <v>46079.55740740741</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15476,7 +15486,7 @@
         <v>1</v>
       </c>
       <c r="N232" s="3" t="n">
-        <v>46079.46740740741</v>
+        <v>46079.54314814815</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -15540,7 +15550,7 @@
         <v>1</v>
       </c>
       <c r="N233" s="3" t="n">
-        <v>46079.48690972223</v>
+        <v>46079.5633912037</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15604,7 +15614,7 @@
         <v>1</v>
       </c>
       <c r="N234" s="3" t="n">
-        <v>46079.46427083333</v>
+        <v>46079.54465277777</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -15668,7 +15678,7 @@
         <v>1</v>
       </c>
       <c r="N235" s="3" t="n">
-        <v>46079.46505787037</v>
+        <v>46079.54231481482</v>
       </c>
       <c r="O235" t="inlineStr">
         <is>
@@ -15732,7 +15742,7 @@
         <v>1</v>
       </c>
       <c r="N236" s="3" t="n">
-        <v>46079.46902777778</v>
+        <v>46079.54666666667</v>
       </c>
       <c r="O236" t="inlineStr">
         <is>
@@ -15860,7 +15870,7 @@
         <v>1</v>
       </c>
       <c r="N238" s="3" t="n">
-        <v>46079.45262731481</v>
+        <v>46079.56805555556</v>
       </c>
       <c r="O238" t="inlineStr">
         <is>
@@ -15988,7 +15998,7 @@
         <v>1</v>
       </c>
       <c r="N240" s="3" t="n">
-        <v>46079.45894675926</v>
+        <v>46079.53667824074</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16052,7 +16062,7 @@
         <v>1</v>
       </c>
       <c r="N241" s="3" t="n">
-        <v>46079.45638888889</v>
+        <v>46079.53385416666</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16116,7 +16126,7 @@
         <v>1</v>
       </c>
       <c r="N242" s="3" t="n">
-        <v>46079.46662037037</v>
+        <v>46079.54392361111</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16180,7 +16190,7 @@
         <v>1</v>
       </c>
       <c r="N243" s="3" t="n">
-        <v>46079.47277777778</v>
+        <v>46079.54930555556</v>
       </c>
       <c r="O243" t="inlineStr">
         <is>
@@ -16303,7 +16313,7 @@
         <v>1</v>
       </c>
       <c r="N245" s="3" t="n">
-        <v>46079.4766087963</v>
+        <v>46079.55</v>
       </c>
       <c r="O245" t="inlineStr">
         <is>
@@ -16367,7 +16377,7 @@
         <v>1</v>
       </c>
       <c r="N246" s="3" t="n">
-        <v>46079.46990740741</v>
+        <v>46079.54928240741</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16431,7 +16441,7 @@
         <v>1</v>
       </c>
       <c r="N247" s="3" t="n">
-        <v>46079.47354166667</v>
+        <v>46079.54763888889</v>
       </c>
       <c r="O247" t="inlineStr">
         <is>
@@ -16495,7 +16505,7 @@
         <v>1</v>
       </c>
       <c r="N248" s="3" t="n">
-        <v>46079.47817129629</v>
+        <v>46079.55756944444</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16559,7 +16569,7 @@
         <v>1</v>
       </c>
       <c r="N249" s="3" t="n">
-        <v>46079.47188657407</v>
+        <v>46079.54954861111</v>
       </c>
       <c r="O249" t="inlineStr">
         <is>
@@ -16623,7 +16633,7 @@
         <v>1</v>
       </c>
       <c r="N250" s="3" t="n">
-        <v>46079.48670138889</v>
+        <v>46079.56664351852</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16687,7 +16697,7 @@
         <v>1</v>
       </c>
       <c r="N251" s="3" t="n">
-        <v>46079.47681712963</v>
+        <v>46079.55637731482</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16751,7 +16761,7 @@
         <v>1</v>
       </c>
       <c r="N252" s="3" t="n">
-        <v>46079.4753125</v>
+        <v>46079.55366898148</v>
       </c>
       <c r="O252" t="inlineStr">
         <is>
@@ -16815,7 +16825,7 @@
         <v>1</v>
       </c>
       <c r="N253" s="3" t="n">
-        <v>46079.45710648148</v>
+        <v>46079.53563657407</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16873,7 +16883,7 @@
         <v>1</v>
       </c>
       <c r="N254" s="3" t="n">
-        <v>46079.47923611111</v>
+        <v>46079.55512731482</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -16937,7 +16947,7 @@
         <v>1</v>
       </c>
       <c r="N255" s="3" t="n">
-        <v>46079.47327546297</v>
+        <v>46079.55157407407</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -17001,7 +17011,7 @@
         <v>1</v>
       </c>
       <c r="N256" s="3" t="n">
-        <v>46079.4584375</v>
+        <v>46079.53554398148</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17065,7 +17075,7 @@
         <v>1</v>
       </c>
       <c r="N257" s="3" t="n">
-        <v>46079.4649537037</v>
+        <v>46079.54041666666</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17129,7 +17139,7 @@
         <v>1</v>
       </c>
       <c r="N258" s="3" t="n">
-        <v>46079.485</v>
+        <v>46079.56388888889</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
@@ -17257,7 +17267,7 @@
         <v>1</v>
       </c>
       <c r="N260" s="3" t="n">
-        <v>46079.48768518519</v>
+        <v>46079.56025462963</v>
       </c>
       <c r="O260" t="inlineStr">
         <is>
@@ -17321,7 +17331,7 @@
         <v>1</v>
       </c>
       <c r="N261" s="3" t="n">
-        <v>46079.4806712963</v>
+        <v>46079.52805555556</v>
       </c>
       <c r="O261" t="inlineStr">
         <is>
@@ -17385,7 +17395,7 @@
         <v>1</v>
       </c>
       <c r="N262" s="3" t="n">
-        <v>46079.46703703704</v>
+        <v>46079.5462962963</v>
       </c>
       <c r="O262" t="inlineStr">
         <is>
@@ -17449,7 +17459,7 @@
         <v>1</v>
       </c>
       <c r="N263" s="3" t="n">
-        <v>46079.47767361111</v>
+        <v>46079.55350694444</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17513,7 +17523,7 @@
         <v>1</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>46079.46248842592</v>
+        <v>46079.54574074074</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17577,7 +17587,7 @@
         <v>1</v>
       </c>
       <c r="N265" s="3" t="n">
-        <v>46079.44974537037</v>
+        <v>46079.56912037037</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17641,7 +17651,7 @@
         <v>1</v>
       </c>
       <c r="N266" s="3" t="n">
-        <v>46079.44974537037</v>
+        <v>46079.56784722222</v>
       </c>
       <c r="O266" t="inlineStr">
         <is>
@@ -17705,7 +17715,7 @@
         <v>1</v>
       </c>
       <c r="N267" s="3" t="n">
-        <v>46079.48478009259</v>
+        <v>46079.56126157408</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17769,7 +17779,7 @@
         <v>1</v>
       </c>
       <c r="N268" s="3" t="n">
-        <v>46079.45177083334</v>
+        <v>46079.57082175926</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17833,7 +17843,7 @@
         <v>1</v>
       </c>
       <c r="N269" s="3" t="n">
-        <v>46079.44898148148</v>
+        <v>46079.56170138889</v>
       </c>
       <c r="O269" t="inlineStr">
         <is>
@@ -17894,7 +17904,7 @@
         </is>
       </c>
       <c r="N270" s="3" t="n">
-        <v>46079.46638888889</v>
+        <v>46079.54480324074</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -18022,7 +18032,7 @@
         <v>1</v>
       </c>
       <c r="N272" s="3" t="n">
-        <v>46079.45494212963</v>
+        <v>46079.5667824074</v>
       </c>
       <c r="O272" t="inlineStr">
         <is>
@@ -18406,7 +18416,7 @@
         <v>1</v>
       </c>
       <c r="N278" s="3" t="n">
-        <v>46079.47587962963</v>
+        <v>46079.55091435185</v>
       </c>
       <c r="O278" t="inlineStr">
         <is>
@@ -18470,7 +18480,7 @@
         <v>1</v>
       </c>
       <c r="N279" s="3" t="n">
-        <v>46079.45444444445</v>
+        <v>46079.53002314815</v>
       </c>
       <c r="O279" t="inlineStr">
         <is>
@@ -18534,7 +18544,7 @@
         <v>1</v>
       </c>
       <c r="N280" s="3" t="n">
-        <v>46079.47704861111</v>
+        <v>46079.55402777778</v>
       </c>
       <c r="O280" t="inlineStr">
         <is>
@@ -18598,7 +18608,7 @@
         <v>1</v>
       </c>
       <c r="N281" s="3" t="n">
-        <v>46079.48320601852</v>
+        <v>46079.56378472222</v>
       </c>
       <c r="O281" t="inlineStr">
         <is>
@@ -18657,7 +18667,7 @@
         <v>1</v>
       </c>
       <c r="N282" s="3" t="n">
-        <v>46079.48270833334</v>
+        <v>46079.56299768519</v>
       </c>
       <c r="O282" t="inlineStr">
         <is>
@@ -18785,7 +18795,7 @@
         <v>1</v>
       </c>
       <c r="N284" s="3" t="n">
-        <v>46079.48789351852</v>
+        <v>46079.56722222222</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18849,7 +18859,7 @@
         <v>1</v>
       </c>
       <c r="N285" s="3" t="n">
-        <v>46079.45896990741</v>
+        <v>46079.54042824074</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -18913,7 +18923,7 @@
         <v>1</v>
       </c>
       <c r="N286" s="3" t="n">
-        <v>46079.47096064815</v>
+        <v>46079.5496875</v>
       </c>
       <c r="O286" t="inlineStr">
         <is>
@@ -18977,7 +18987,7 @@
         <v>1</v>
       </c>
       <c r="N287" s="3" t="n">
-        <v>46079.45738425926</v>
+        <v>46079.5349074074</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
@@ -19041,7 +19051,7 @@
         <v>1</v>
       </c>
       <c r="N288" s="3" t="n">
-        <v>46079.48334490741</v>
+        <v>46079.5597337963</v>
       </c>
       <c r="O288" t="inlineStr">
         <is>
@@ -19105,7 +19115,7 @@
         <v>1</v>
       </c>
       <c r="N289" s="3" t="n">
-        <v>46079.4777662037</v>
+        <v>46079.55629629629</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -19899,7 +19909,7 @@
         <v>1</v>
       </c>
       <c r="N302" s="3" t="n">
-        <v>46079.47530092593</v>
+        <v>46079.54892361111</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -21015,7 +21025,7 @@
         </is>
       </c>
       <c r="N320" s="3" t="n">
-        <v>46079.46159722222</v>
+        <v>46079.53766203704</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21740,7 +21750,7 @@
         <v>1</v>
       </c>
       <c r="N332" s="3" t="n">
-        <v>46079.48311342593</v>
+        <v>46079.56005787037</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21804,7 +21814,7 @@
         <v>2</v>
       </c>
       <c r="N333" s="3" t="n">
-        <v>46079.47231481481</v>
+        <v>46079.55247685185</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21868,7 +21878,7 @@
         <v>2</v>
       </c>
       <c r="N334" s="3" t="n">
-        <v>46079.47956018519</v>
+        <v>46079.55481481482</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21932,7 +21942,7 @@
         <v>2</v>
       </c>
       <c r="N335" s="3" t="n">
-        <v>46079.47697916667</v>
+        <v>46079.55064814815</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -21996,7 +22006,7 @@
         <v>1</v>
       </c>
       <c r="N336" s="3" t="n">
-        <v>46079.47658564815</v>
+        <v>46079.55734953703</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22060,7 +22070,7 @@
         <v>1</v>
       </c>
       <c r="N337" s="3" t="n">
-        <v>46079.46079861111</v>
+        <v>46079.5412037037</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22124,7 +22134,7 @@
         <v>2</v>
       </c>
       <c r="N338" s="3" t="n">
-        <v>46079.47392361111</v>
+        <v>46079.55175925926</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -22188,7 +22198,7 @@
         <v>2</v>
       </c>
       <c r="N339" s="3" t="n">
-        <v>46079.47626157408</v>
+        <v>46079.55762731482</v>
       </c>
       <c r="O339" t="inlineStr">
         <is>
@@ -22316,7 +22326,7 @@
         <v>2</v>
       </c>
       <c r="N341" s="3" t="n">
-        <v>46078.56283564815</v>
+        <v>46079.54128472223</v>
       </c>
       <c r="O341" t="inlineStr">
         <is>
@@ -22380,7 +22390,7 @@
         <v>2</v>
       </c>
       <c r="N342" s="3" t="n">
-        <v>46079.46834490741</v>
+        <v>46079.55180555556</v>
       </c>
       <c r="O342" t="inlineStr">
         <is>
@@ -23826,7 +23836,7 @@
         <v>1</v>
       </c>
       <c r="N365" s="3" t="n">
-        <v>46079.48180555556</v>
+        <v>46079.55438657408</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
@@ -23892,7 +23902,7 @@
         </is>
       </c>
       <c r="N366" s="3" t="n">
-        <v>46079.48222222222</v>
+        <v>46079.55908564815</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -24018,7 +24028,7 @@
         </is>
       </c>
       <c r="N368" s="3" t="n">
-        <v>46079.47171296296</v>
+        <v>46079.55396990741</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -24037,11 +24047,6 @@
           <t>RH</t>
         </is>
       </c>
-      <c r="C369" t="inlineStr">
-        <is>
-          <t>10.69.3.13</t>
-        </is>
-      </c>
       <c r="D369" t="n">
         <v>2025</v>
       </c>
@@ -24084,7 +24089,7 @@
         </is>
       </c>
       <c r="N369" s="3" t="n">
-        <v>46079.47700231482</v>
+        <v>46079.56550925926</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
@@ -24153,7 +24158,7 @@
         <v>1</v>
       </c>
       <c r="N370" s="3" t="n">
-        <v>46079.46847222222</v>
+        <v>46079.54859953704</v>
       </c>
       <c r="O370" t="inlineStr">
         <is>
@@ -24222,7 +24227,7 @@
         <v>1</v>
       </c>
       <c r="N371" s="3" t="n">
-        <v>46078.68076388889</v>
+        <v>46079.54758101852</v>
       </c>
       <c r="O371" t="inlineStr">
         <is>
@@ -24426,7 +24431,7 @@
         <v>1</v>
       </c>
       <c r="N374" s="3" t="n">
-        <v>46079.46734953704</v>
+        <v>46079.54868055556</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24492,7 +24497,7 @@
         </is>
       </c>
       <c r="N375" s="3" t="n">
-        <v>46079.46820601852</v>
+        <v>46079.54457175926</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
@@ -24511,11 +24516,6 @@
           <t>COORDENACAO</t>
         </is>
       </c>
-      <c r="C376" t="inlineStr">
-        <is>
-          <t>10.69.3.72</t>
-        </is>
-      </c>
       <c r="D376" t="n">
         <v>2025</v>
       </c>
@@ -24561,7 +24561,7 @@
         <v>1</v>
       </c>
       <c r="N376" s="3" t="n">
-        <v>46079.48564814815</v>
+        <v>46079.56269675926</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -24630,7 +24630,7 @@
         <v>2</v>
       </c>
       <c r="N377" s="3" t="n">
-        <v>46079.48153935185</v>
+        <v>46079.5584375</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -24699,7 +24699,7 @@
         <v>2</v>
       </c>
       <c r="N378" s="3" t="n">
-        <v>46079.46601851852</v>
+        <v>46079.54621527778</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização automática 2026-02-26 15:52:04.525605
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>46079.56414351852</v>
+        <v>46079.6430787037</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>46079.53265046296</v>
+        <v>46079.65287037037</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
         <v>1</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>46079.55021990741</v>
+        <v>46079.6328587963</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>46079.56971064815</v>
+        <v>46079.64631944444</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -1259,7 +1259,7 @@
         <v>1</v>
       </c>
       <c r="N12" s="3" t="n">
-        <v>46079.53686342593</v>
+        <v>46079.65438657408</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1515,7 +1515,7 @@
         <v>2</v>
       </c>
       <c r="N16" s="3" t="n">
-        <v>46079.53008101852</v>
+        <v>46079.65189814815</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1579,7 +1579,7 @@
         <v>1</v>
       </c>
       <c r="N17" s="3" t="n">
-        <v>46079.55170138889</v>
+        <v>46079.63244212963</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1643,7 +1643,7 @@
         <v>2</v>
       </c>
       <c r="N18" s="3" t="n">
-        <v>46079.55622685186</v>
+        <v>46079.63508101852</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1768,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="N20" s="3" t="n">
-        <v>46079.54232638889</v>
+        <v>46079.62445601852</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1969,6 +1969,11 @@
           <t>AUDITORIO</t>
         </is>
       </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>10.69.3.150</t>
+        </is>
+      </c>
       <c r="D24" t="n">
         <v>2019</v>
       </c>
@@ -2009,7 +2014,7 @@
         <v>1</v>
       </c>
       <c r="N24" s="3" t="n">
-        <v>46079.53746527778</v>
+        <v>46079.60684027777</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -6570,7 +6575,7 @@
         <v>1</v>
       </c>
       <c r="N95" s="3" t="n">
-        <v>46079.56140046296</v>
+        <v>46079.63451388889</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -6639,7 +6644,7 @@
         <v>1</v>
       </c>
       <c r="N96" s="3" t="n">
-        <v>46079.55541666667</v>
+        <v>46079.63488425926</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
@@ -6703,7 +6708,7 @@
         <v>1</v>
       </c>
       <c r="N97" s="3" t="n">
-        <v>46079.56730324074</v>
+        <v>46079.64471064815</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -6772,7 +6777,7 @@
         <v>1</v>
       </c>
       <c r="N98" s="3" t="n">
-        <v>46079.56954861111</v>
+        <v>46079.64555555556</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -6841,7 +6846,7 @@
         <v>1</v>
       </c>
       <c r="N99" s="3" t="n">
-        <v>46079.54527777778</v>
+        <v>46079.62204861111</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -6910,7 +6915,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>46079.53658564815</v>
+        <v>46079.65357638889</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6979,7 +6984,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="3" t="n">
-        <v>46079.54232638889</v>
+        <v>46079.62114583333</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -7048,7 +7053,7 @@
         <v>1</v>
       </c>
       <c r="N102" s="3" t="n">
-        <v>46065.69311342593</v>
+        <v>46079.62344907408</v>
       </c>
       <c r="O102" t="inlineStr">
         <is>
@@ -7117,7 +7122,7 @@
         <v>2</v>
       </c>
       <c r="N103" s="3" t="n">
-        <v>46079.53436342593</v>
+        <v>46079.65072916666</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7377,7 +7382,7 @@
         <v>1</v>
       </c>
       <c r="N107" s="3" t="n">
-        <v>46079.53462962963</v>
+        <v>46079.6159837963</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -7515,7 +7520,7 @@
         <v>1</v>
       </c>
       <c r="N109" s="3" t="n">
-        <v>46079.55327546296</v>
+        <v>46079.62739583333</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7584,7 +7589,7 @@
         <v>2</v>
       </c>
       <c r="N110" s="3" t="n">
-        <v>46079.5433912037</v>
+        <v>46079.62699074074</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7653,7 +7658,7 @@
         <v>2</v>
       </c>
       <c r="N111" s="3" t="n">
-        <v>46079.53177083333</v>
+        <v>46079.65428240741</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
@@ -7722,7 +7727,7 @@
         <v>2</v>
       </c>
       <c r="N112" s="3" t="n">
-        <v>46079.57063657408</v>
+        <v>46079.6530324074</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7791,7 +7796,7 @@
         <v>1</v>
       </c>
       <c r="N113" s="3" t="n">
-        <v>46079.55090277778</v>
+        <v>46079.62806712963</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7860,7 +7865,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>46079.56619212963</v>
+        <v>46079.64497685185</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -7926,7 +7931,7 @@
         </is>
       </c>
       <c r="N115" s="3" t="n">
-        <v>46079.56819444444</v>
+        <v>46079.64802083333</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -7995,7 +8000,7 @@
         <v>1</v>
       </c>
       <c r="N116" s="3" t="n">
-        <v>46079.53865740741</v>
+        <v>46079.64862268518</v>
       </c>
       <c r="O116" t="inlineStr">
         <is>
@@ -8064,7 +8069,7 @@
         <v>1</v>
       </c>
       <c r="N117" s="3" t="n">
-        <v>46079.56611111111</v>
+        <v>46079.64728009259</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -8130,7 +8135,7 @@
         </is>
       </c>
       <c r="N118" s="3" t="n">
-        <v>46079.56975694445</v>
+        <v>46079.64939814815</v>
       </c>
       <c r="O118" t="inlineStr">
         <is>
@@ -8268,7 +8273,7 @@
         <v>1</v>
       </c>
       <c r="N120" s="3" t="n">
-        <v>46079.55517361111</v>
+        <v>46079.63424768519</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -8337,7 +8342,7 @@
         <v>1</v>
       </c>
       <c r="N121" s="3" t="n">
-        <v>46079.55118055556</v>
+        <v>46079.64380787037</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -8403,7 +8408,7 @@
         </is>
       </c>
       <c r="N122" s="3" t="n">
-        <v>46079.56135416667</v>
+        <v>46079.63668981481</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -8472,7 +8477,7 @@
         <v>2</v>
       </c>
       <c r="N123" s="3" t="n">
-        <v>46079.54084490741</v>
+        <v>46079.6159375</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -8541,7 +8546,7 @@
         <v>1</v>
       </c>
       <c r="N124" s="3" t="n">
-        <v>46079.53310185186</v>
+        <v>46079.64834490741</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -8610,7 +8615,7 @@
         <v>1</v>
       </c>
       <c r="N125" s="3" t="n">
-        <v>46079.55939814815</v>
+        <v>46079.63854166667</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -8679,7 +8684,7 @@
         <v>2</v>
       </c>
       <c r="N126" s="3" t="n">
-        <v>46079.5637037037</v>
+        <v>46079.63790509259</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -8748,7 +8753,7 @@
         <v>2</v>
       </c>
       <c r="N127" s="3" t="n">
-        <v>46079.56527777778</v>
+        <v>46079.64895833333</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -8817,7 +8822,7 @@
         <v>1</v>
       </c>
       <c r="N128" s="3" t="n">
-        <v>46079.56128472222</v>
+        <v>46079.63752314815</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -8886,7 +8891,7 @@
         <v>1</v>
       </c>
       <c r="N129" s="3" t="n">
-        <v>46079.55975694444</v>
+        <v>46079.64192129629</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -8955,7 +8960,7 @@
         <v>1</v>
       </c>
       <c r="N130" s="3" t="n">
-        <v>46079.55263888889</v>
+        <v>46079.62581018519</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -9019,7 +9024,7 @@
         <v>1</v>
       </c>
       <c r="N131" s="3" t="n">
-        <v>46079.54010416667</v>
+        <v>46079.6200462963</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -9152,7 +9157,7 @@
         <v>1</v>
       </c>
       <c r="N133" s="3" t="n">
-        <v>46078.80311342593</v>
+        <v>46079.62319444444</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -9280,7 +9285,7 @@
         <v>1</v>
       </c>
       <c r="N135" s="3" t="n">
-        <v>46078.81565972222</v>
+        <v>46079.62197916667</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -9471,7 +9476,7 @@
         <v>1</v>
       </c>
       <c r="N138" s="3" t="n">
-        <v>46079.53417824074</v>
+        <v>46079.65167824074</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9535,7 +9540,7 @@
         <v>1</v>
       </c>
       <c r="N139" s="3" t="n">
-        <v>46079.56990740741</v>
+        <v>46079.62090277778</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9599,7 +9604,7 @@
         <v>1</v>
       </c>
       <c r="N140" s="3" t="n">
-        <v>46079.54722222222</v>
+        <v>46079.6281712963</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9663,7 +9668,7 @@
         <v>1</v>
       </c>
       <c r="N141" s="3" t="n">
-        <v>46079.54894675926</v>
+        <v>46079.62262731481</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9727,7 +9732,7 @@
         <v>1</v>
       </c>
       <c r="N142" s="3" t="n">
-        <v>46079.54814814815</v>
+        <v>46079.6265162037</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9791,7 +9796,7 @@
         <v>1</v>
       </c>
       <c r="N143" s="3" t="n">
-        <v>46079.55361111111</v>
+        <v>46079.63347222222</v>
       </c>
       <c r="O143" t="inlineStr">
         <is>
@@ -9855,7 +9860,7 @@
         <v>1</v>
       </c>
       <c r="N144" s="3" t="n">
-        <v>46079.54167824074</v>
+        <v>46079.62125</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9919,7 +9924,7 @@
         <v>1</v>
       </c>
       <c r="N145" s="3" t="n">
-        <v>46078.81521990741</v>
+        <v>46079.62268518518</v>
       </c>
       <c r="O145" t="inlineStr">
         <is>
@@ -9983,7 +9988,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="3" t="n">
-        <v>46079.53511574074</v>
+        <v>46079.62734953704</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10111,7 +10116,7 @@
         <v>1</v>
       </c>
       <c r="N148" s="3" t="n">
-        <v>46079.53626157407</v>
+        <v>46079.65043981482</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10175,7 +10180,7 @@
         <v>1</v>
       </c>
       <c r="N149" s="3" t="n">
-        <v>46079.56458333333</v>
+        <v>46079.64192129629</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -10239,7 +10244,7 @@
         <v>1</v>
       </c>
       <c r="N150" s="3" t="n">
-        <v>46079.55873842593</v>
+        <v>46079.63627314815</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -10303,7 +10308,7 @@
         <v>1</v>
       </c>
       <c r="N151" s="3" t="n">
-        <v>46079.53193287037</v>
+        <v>46079.65236111111</v>
       </c>
       <c r="O151" t="inlineStr">
         <is>
@@ -10367,7 +10372,7 @@
         <v>1</v>
       </c>
       <c r="N152" s="3" t="n">
-        <v>46079.54636574074</v>
+        <v>46079.62054398148</v>
       </c>
       <c r="O152" t="inlineStr">
         <is>
@@ -10431,7 +10436,7 @@
         <v>1</v>
       </c>
       <c r="N153" s="3" t="n">
-        <v>46079.57071759259</v>
+        <v>46079.64678240741</v>
       </c>
       <c r="O153" t="inlineStr">
         <is>
@@ -10495,7 +10500,7 @@
         <v>1</v>
       </c>
       <c r="N154" s="3" t="n">
-        <v>46079.56189814815</v>
+        <v>46079.62297453704</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10559,7 +10564,7 @@
         <v>1</v>
       </c>
       <c r="N155" s="3" t="n">
-        <v>46079.55753472223</v>
+        <v>46079.63564814815</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10623,7 +10628,7 @@
         <v>1</v>
       </c>
       <c r="N156" s="3" t="n">
-        <v>46079.55498842592</v>
+        <v>46079.62564814815</v>
       </c>
       <c r="O156" t="inlineStr">
         <is>
@@ -10687,7 +10692,7 @@
         <v>1</v>
       </c>
       <c r="N157" s="3" t="n">
-        <v>46079.53510416667</v>
+        <v>46079.57226851852</v>
       </c>
       <c r="O157" t="inlineStr">
         <is>
@@ -10751,7 +10756,7 @@
         <v>1</v>
       </c>
       <c r="N158" s="3" t="n">
-        <v>46079.55101851852</v>
+        <v>46079.62773148148</v>
       </c>
       <c r="O158" t="inlineStr">
         <is>
@@ -10815,7 +10820,7 @@
         <v>1</v>
       </c>
       <c r="N159" s="3" t="n">
-        <v>46079.54811342592</v>
+        <v>46079.62496527778</v>
       </c>
       <c r="O159" t="inlineStr">
         <is>
@@ -10879,7 +10884,7 @@
         <v>1</v>
       </c>
       <c r="N160" s="3" t="n">
-        <v>46079.56278935185</v>
+        <v>46079.64303240741</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
@@ -10943,7 +10948,7 @@
         <v>1</v>
       </c>
       <c r="N161" s="3" t="n">
-        <v>46079.56318287037</v>
+        <v>46079.61913194445</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -11007,7 +11012,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="3" t="n">
-        <v>46079.56283564815</v>
+        <v>46079.64402777778</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11135,7 +11140,7 @@
         <v>2</v>
       </c>
       <c r="N164" s="3" t="n">
-        <v>46079.56171296296</v>
+        <v>46079.63925925926</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11263,7 +11268,7 @@
         <v>2</v>
       </c>
       <c r="N166" s="3" t="n">
-        <v>46079.57015046296</v>
+        <v>46079.60831018518</v>
       </c>
       <c r="O166" t="inlineStr">
         <is>
@@ -11327,7 +11332,7 @@
         <v>2</v>
       </c>
       <c r="N167" s="3" t="n">
-        <v>46079.56164351852</v>
+        <v>46079.59871527777</v>
       </c>
       <c r="O167" t="inlineStr">
         <is>
@@ -11455,7 +11460,7 @@
         <v>2</v>
       </c>
       <c r="N169" s="3" t="n">
-        <v>46079.55982638889</v>
+        <v>46079.63814814815</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -11519,7 +11524,7 @@
         <v>2</v>
       </c>
       <c r="N170" s="3" t="n">
-        <v>46079.54729166667</v>
+        <v>46079.61899305556</v>
       </c>
       <c r="O170" t="inlineStr">
         <is>
@@ -11583,7 +11588,7 @@
         <v>1</v>
       </c>
       <c r="N171" s="3" t="n">
-        <v>46079.55938657407</v>
+        <v>46079.63297453704</v>
       </c>
       <c r="O171" t="inlineStr">
         <is>
@@ -11647,7 +11652,7 @@
         <v>2</v>
       </c>
       <c r="N172" s="3" t="n">
-        <v>46079.54769675926</v>
+        <v>46079.62644675926</v>
       </c>
       <c r="O172" t="inlineStr">
         <is>
@@ -11711,7 +11716,7 @@
         <v>2</v>
       </c>
       <c r="N173" s="3" t="n">
-        <v>46079.56776620371</v>
+        <v>46079.64613425926</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -11839,7 +11844,7 @@
         <v>2</v>
       </c>
       <c r="N175" s="3" t="n">
-        <v>46079.53645833334</v>
+        <v>46079.65361111111</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -11903,7 +11908,7 @@
         <v>2</v>
       </c>
       <c r="N176" s="3" t="n">
-        <v>46079.5496875</v>
+        <v>46079.62309027778</v>
       </c>
       <c r="O176" t="inlineStr">
         <is>
@@ -11967,7 +11972,7 @@
         <v>2</v>
       </c>
       <c r="N177" s="3" t="n">
-        <v>46079.54571759259</v>
+        <v>46079.62315972222</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
@@ -12031,7 +12036,7 @@
         <v>2</v>
       </c>
       <c r="N178" s="3" t="n">
-        <v>46079.55065972222</v>
+        <v>46079.62555555555</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12095,7 +12100,7 @@
         <v>1</v>
       </c>
       <c r="N179" s="3" t="n">
-        <v>46079.55805555556</v>
+        <v>46079.63232638889</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12159,7 +12164,7 @@
         <v>1</v>
       </c>
       <c r="N180" s="3" t="n">
-        <v>46079.56868055555</v>
+        <v>46079.62148148148</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12223,7 +12228,7 @@
         <v>1</v>
       </c>
       <c r="N181" s="3" t="n">
-        <v>46079.55662037037</v>
+        <v>46079.63746527778</v>
       </c>
       <c r="O181" t="inlineStr">
         <is>
@@ -12351,7 +12356,7 @@
         <v>1</v>
       </c>
       <c r="N183" s="3" t="n">
-        <v>46079.55118055556</v>
+        <v>46079.62239583334</v>
       </c>
       <c r="O183" t="inlineStr">
         <is>
@@ -12420,7 +12425,7 @@
         <v>2</v>
       </c>
       <c r="N184" s="3" t="n">
-        <v>46079.54085648148</v>
+        <v>46079.61998842593</v>
       </c>
       <c r="O184" t="inlineStr">
         <is>
@@ -12484,7 +12489,7 @@
         <v>1</v>
       </c>
       <c r="N185" s="3" t="n">
-        <v>46079.55450231482</v>
+        <v>46079.63212962963</v>
       </c>
       <c r="O185" t="inlineStr">
         <is>
@@ -12548,7 +12553,7 @@
         <v>1</v>
       </c>
       <c r="N186" s="3" t="n">
-        <v>46079.56818287037</v>
+        <v>46079.60418981482</v>
       </c>
       <c r="O186" t="inlineStr">
         <is>
@@ -12676,7 +12681,7 @@
         <v>1</v>
       </c>
       <c r="N188" s="3" t="n">
-        <v>46079.56212962963</v>
+        <v>46079.64160879629</v>
       </c>
       <c r="O188" t="inlineStr">
         <is>
@@ -12804,7 +12809,7 @@
         </is>
       </c>
       <c r="N190" s="3" t="n">
-        <v>46079.54884259259</v>
+        <v>46079.62539351852</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12868,7 +12873,7 @@
         <v>1</v>
       </c>
       <c r="N191" s="3" t="n">
-        <v>46078.82586805556</v>
+        <v>46079.63087962963</v>
       </c>
       <c r="O191" t="inlineStr">
         <is>
@@ -12932,7 +12937,7 @@
         <v>1</v>
       </c>
       <c r="N192" s="3" t="n">
-        <v>46079.56480324074</v>
+        <v>46079.64480324074</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -13057,7 +13062,7 @@
         <v>2</v>
       </c>
       <c r="N194" s="3" t="n">
-        <v>46079.5708912037</v>
+        <v>46079.58024305556</v>
       </c>
       <c r="O194" t="inlineStr">
         <is>
@@ -13121,7 +13126,7 @@
         <v>1</v>
       </c>
       <c r="N195" s="3" t="n">
-        <v>46079.56032407407</v>
+        <v>46079.64325231482</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13185,7 +13190,7 @@
         <v>1</v>
       </c>
       <c r="N196" s="3" t="n">
-        <v>46079.53146990741</v>
+        <v>46079.62775462963</v>
       </c>
       <c r="O196" t="inlineStr">
         <is>
@@ -13249,7 +13254,7 @@
         <v>1</v>
       </c>
       <c r="N197" s="3" t="n">
-        <v>46079.55083333333</v>
+        <v>46079.62679398148</v>
       </c>
       <c r="O197" t="inlineStr">
         <is>
@@ -13313,7 +13318,7 @@
         <v>1</v>
       </c>
       <c r="N198" s="3" t="n">
-        <v>46079.54706018518</v>
+        <v>46079.62819444444</v>
       </c>
       <c r="O198" t="inlineStr">
         <is>
@@ -13377,7 +13382,7 @@
         <v>1</v>
       </c>
       <c r="N199" s="3" t="n">
-        <v>46079.56296296296</v>
+        <v>46079.6365162037</v>
       </c>
       <c r="O199" t="inlineStr">
         <is>
@@ -13502,7 +13507,7 @@
         </is>
       </c>
       <c r="N201" s="3" t="n">
-        <v>46079.55339120371</v>
+        <v>46079.62903935185</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -13566,7 +13571,7 @@
         <v>1</v>
       </c>
       <c r="N202" s="3" t="n">
-        <v>46079.551875</v>
+        <v>46079.63363425926</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13630,7 +13635,7 @@
         <v>1</v>
       </c>
       <c r="N203" s="3" t="n">
-        <v>46079.53502314815</v>
+        <v>46079.6222337963</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13694,7 +13699,7 @@
         <v>1</v>
       </c>
       <c r="N204" s="3" t="n">
-        <v>46079.53776620371</v>
+        <v>46079.61575231481</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13758,7 +13763,7 @@
         <v>1</v>
       </c>
       <c r="N205" s="3" t="n">
-        <v>46079.535</v>
+        <v>46079.61527777778</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13822,7 +13827,7 @@
         <v>1</v>
       </c>
       <c r="N206" s="3" t="n">
-        <v>46079.56975694445</v>
+        <v>46079.64820601852</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -13886,7 +13891,7 @@
         <v>1</v>
       </c>
       <c r="N207" s="3" t="n">
-        <v>46079.55866898148</v>
+        <v>46079.63438657407</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -13950,7 +13955,7 @@
         <v>1</v>
       </c>
       <c r="N208" s="3" t="n">
-        <v>46079.54260416667</v>
+        <v>46079.57876157408</v>
       </c>
       <c r="O208" t="inlineStr">
         <is>
@@ -14014,7 +14019,7 @@
         <v>1</v>
       </c>
       <c r="N209" s="3" t="n">
-        <v>46079.56896990741</v>
+        <v>46079.62228009259</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14078,7 +14083,7 @@
         <v>1</v>
       </c>
       <c r="N210" s="3" t="n">
-        <v>46079.56989583333</v>
+        <v>46079.64651620371</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14142,7 +14147,7 @@
         <v>1</v>
       </c>
       <c r="N211" s="3" t="n">
-        <v>46079.5616087963</v>
+        <v>46079.62037037037</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -14334,7 +14339,7 @@
         <v>1</v>
       </c>
       <c r="N214" s="3" t="n">
-        <v>46079.53744212963</v>
+        <v>46079.64634259259</v>
       </c>
       <c r="O214" t="inlineStr">
         <is>
@@ -14462,7 +14467,7 @@
         <v>1</v>
       </c>
       <c r="N216" s="3" t="n">
-        <v>46079.56653935185</v>
+        <v>46079.64403935185</v>
       </c>
       <c r="O216" t="inlineStr">
         <is>
@@ -14521,7 +14526,7 @@
         <v>1</v>
       </c>
       <c r="N217" s="3" t="n">
-        <v>46079.56327546296</v>
+        <v>46079.62137731481</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14585,7 +14590,7 @@
         <v>1</v>
       </c>
       <c r="N218" s="3" t="n">
-        <v>46079.56854166667</v>
+        <v>46079.6440625</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14649,7 +14654,7 @@
         <v>1</v>
       </c>
       <c r="N219" s="3" t="n">
-        <v>46079.33395833334</v>
+        <v>46079.62420138889</v>
       </c>
       <c r="O219" t="inlineStr">
         <is>
@@ -14718,7 +14723,7 @@
         <v>1</v>
       </c>
       <c r="N220" s="3" t="n">
-        <v>46079.56922453704</v>
+        <v>46079.64703703704</v>
       </c>
       <c r="O220" t="inlineStr">
         <is>
@@ -14782,7 +14787,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="3" t="n">
-        <v>46079.5366087963</v>
+        <v>46079.65465277778</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14846,7 +14851,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="3" t="n">
-        <v>46079.54344907407</v>
+        <v>46079.65178240741</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -14910,7 +14915,7 @@
         <v>1</v>
       </c>
       <c r="N223" s="3" t="n">
-        <v>46079.56135416667</v>
+        <v>46079.64148148148</v>
       </c>
       <c r="O223" t="inlineStr">
         <is>
@@ -14974,7 +14979,7 @@
         <v>1</v>
       </c>
       <c r="N224" s="3" t="n">
-        <v>46078.80011574074</v>
+        <v>46079.64331018519</v>
       </c>
       <c r="O224" t="inlineStr">
         <is>
@@ -15038,7 +15043,7 @@
         <v>1</v>
       </c>
       <c r="N225" s="3" t="n">
-        <v>46078.82145833333</v>
+        <v>46079.63831018518</v>
       </c>
       <c r="O225" t="inlineStr">
         <is>
@@ -15102,7 +15107,7 @@
         <v>1</v>
       </c>
       <c r="N226" s="3" t="n">
-        <v>46079.55592592592</v>
+        <v>46079.63606481482</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15230,7 +15235,7 @@
         <v>1</v>
       </c>
       <c r="N228" s="3" t="n">
-        <v>46079.55600694445</v>
+        <v>46079.63410879629</v>
       </c>
       <c r="O228" t="inlineStr">
         <is>
@@ -15358,7 +15363,7 @@
         <v>1</v>
       </c>
       <c r="N230" s="3" t="n">
-        <v>46079.54101851852</v>
+        <v>46079.62208333334</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15422,7 +15427,7 @@
         <v>1</v>
       </c>
       <c r="N231" s="3" t="n">
-        <v>46079.55740740741</v>
+        <v>46079.63505787037</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15486,7 +15491,7 @@
         <v>1</v>
       </c>
       <c r="N232" s="3" t="n">
-        <v>46079.54314814815</v>
+        <v>46079.61938657407</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -15550,7 +15555,7 @@
         <v>1</v>
       </c>
       <c r="N233" s="3" t="n">
-        <v>46079.5633912037</v>
+        <v>46079.63806712963</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15614,7 +15619,7 @@
         <v>1</v>
       </c>
       <c r="N234" s="3" t="n">
-        <v>46079.54465277777</v>
+        <v>46079.61935185185</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -15678,7 +15683,7 @@
         <v>1</v>
       </c>
       <c r="N235" s="3" t="n">
-        <v>46079.54231481482</v>
+        <v>46079.62104166667</v>
       </c>
       <c r="O235" t="inlineStr">
         <is>
@@ -15870,7 +15875,7 @@
         <v>1</v>
       </c>
       <c r="N238" s="3" t="n">
-        <v>46079.56805555556</v>
+        <v>46079.63232638889</v>
       </c>
       <c r="O238" t="inlineStr">
         <is>
@@ -15934,7 +15939,7 @@
         <v>1</v>
       </c>
       <c r="N239" s="3" t="n">
-        <v>46079.37174768518</v>
+        <v>46079.58893518519</v>
       </c>
       <c r="O239" t="inlineStr">
         <is>
@@ -15998,7 +16003,7 @@
         <v>1</v>
       </c>
       <c r="N240" s="3" t="n">
-        <v>46079.53667824074</v>
+        <v>46079.62204861111</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16062,7 +16067,7 @@
         <v>1</v>
       </c>
       <c r="N241" s="3" t="n">
-        <v>46079.53385416666</v>
+        <v>46079.61740740741</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16126,7 +16131,7 @@
         <v>1</v>
       </c>
       <c r="N242" s="3" t="n">
-        <v>46079.54392361111</v>
+        <v>46079.62788194444</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16190,7 +16195,7 @@
         <v>1</v>
       </c>
       <c r="N243" s="3" t="n">
-        <v>46079.54930555556</v>
+        <v>46079.63395833333</v>
       </c>
       <c r="O243" t="inlineStr">
         <is>
@@ -16313,7 +16318,7 @@
         <v>1</v>
       </c>
       <c r="N245" s="3" t="n">
-        <v>46079.55</v>
+        <v>46079.62625</v>
       </c>
       <c r="O245" t="inlineStr">
         <is>
@@ -16377,7 +16382,7 @@
         <v>1</v>
       </c>
       <c r="N246" s="3" t="n">
-        <v>46079.54928240741</v>
+        <v>46079.63238425926</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16441,7 +16446,7 @@
         <v>1</v>
       </c>
       <c r="N247" s="3" t="n">
-        <v>46079.54763888889</v>
+        <v>46079.62234953704</v>
       </c>
       <c r="O247" t="inlineStr">
         <is>
@@ -16505,7 +16510,7 @@
         <v>1</v>
       </c>
       <c r="N248" s="3" t="n">
-        <v>46079.55756944444</v>
+        <v>46079.64152777778</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16569,7 +16574,7 @@
         <v>1</v>
       </c>
       <c r="N249" s="3" t="n">
-        <v>46079.54954861111</v>
+        <v>46079.6435300926</v>
       </c>
       <c r="O249" t="inlineStr">
         <is>
@@ -16633,7 +16638,7 @@
         <v>1</v>
       </c>
       <c r="N250" s="3" t="n">
-        <v>46079.56664351852</v>
+        <v>46079.64246527778</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16697,7 +16702,7 @@
         <v>1</v>
       </c>
       <c r="N251" s="3" t="n">
-        <v>46079.55637731482</v>
+        <v>46079.63626157407</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16761,7 +16766,7 @@
         <v>1</v>
       </c>
       <c r="N252" s="3" t="n">
-        <v>46079.55366898148</v>
+        <v>46079.63535879629</v>
       </c>
       <c r="O252" t="inlineStr">
         <is>
@@ -16825,7 +16830,7 @@
         <v>1</v>
       </c>
       <c r="N253" s="3" t="n">
-        <v>46079.53563657407</v>
+        <v>46079.6203125</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16883,7 +16888,7 @@
         <v>1</v>
       </c>
       <c r="N254" s="3" t="n">
-        <v>46079.55512731482</v>
+        <v>46079.63315972222</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -16947,7 +16952,7 @@
         <v>1</v>
       </c>
       <c r="N255" s="3" t="n">
-        <v>46079.55157407407</v>
+        <v>46079.58980324074</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -17011,7 +17016,7 @@
         <v>1</v>
       </c>
       <c r="N256" s="3" t="n">
-        <v>46079.53554398148</v>
+        <v>46079.65296296297</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17075,7 +17080,7 @@
         <v>1</v>
       </c>
       <c r="N257" s="3" t="n">
-        <v>46079.54041666666</v>
+        <v>46079.61744212963</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17139,7 +17144,7 @@
         <v>1</v>
       </c>
       <c r="N258" s="3" t="n">
-        <v>46079.56388888889</v>
+        <v>46079.64549768518</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
@@ -17203,7 +17208,7 @@
         <v>1</v>
       </c>
       <c r="N259" s="3" t="n">
-        <v>46079.35188657408</v>
+        <v>46079.64957175926</v>
       </c>
       <c r="O259" t="inlineStr">
         <is>
@@ -17267,7 +17272,7 @@
         <v>1</v>
       </c>
       <c r="N260" s="3" t="n">
-        <v>46079.56025462963</v>
+        <v>46079.60084490741</v>
       </c>
       <c r="O260" t="inlineStr">
         <is>
@@ -17331,7 +17336,7 @@
         <v>1</v>
       </c>
       <c r="N261" s="3" t="n">
-        <v>46079.52805555556</v>
+        <v>46079.63605324074</v>
       </c>
       <c r="O261" t="inlineStr">
         <is>
@@ -17395,7 +17400,7 @@
         <v>1</v>
       </c>
       <c r="N262" s="3" t="n">
-        <v>46079.5462962963</v>
+        <v>46079.63423611111</v>
       </c>
       <c r="O262" t="inlineStr">
         <is>
@@ -17459,7 +17464,7 @@
         <v>1</v>
       </c>
       <c r="N263" s="3" t="n">
-        <v>46079.55350694444</v>
+        <v>46079.62979166667</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17523,7 +17528,7 @@
         <v>1</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>46079.54574074074</v>
+        <v>46079.65428240741</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17587,7 +17592,7 @@
         <v>1</v>
       </c>
       <c r="N265" s="3" t="n">
-        <v>46079.56912037037</v>
+        <v>46079.62508101852</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17651,7 +17656,7 @@
         <v>1</v>
       </c>
       <c r="N266" s="3" t="n">
-        <v>46079.56784722222</v>
+        <v>46079.64818287037</v>
       </c>
       <c r="O266" t="inlineStr">
         <is>
@@ -17715,7 +17720,7 @@
         <v>1</v>
       </c>
       <c r="N267" s="3" t="n">
-        <v>46079.56126157408</v>
+        <v>46079.64049768518</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17779,7 +17784,7 @@
         <v>1</v>
       </c>
       <c r="N268" s="3" t="n">
-        <v>46079.57082175926</v>
+        <v>46079.64549768518</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17843,7 +17848,7 @@
         <v>1</v>
       </c>
       <c r="N269" s="3" t="n">
-        <v>46079.56170138889</v>
+        <v>46079.63863425926</v>
       </c>
       <c r="O269" t="inlineStr">
         <is>
@@ -17904,7 +17909,7 @@
         </is>
       </c>
       <c r="N270" s="3" t="n">
-        <v>46079.54480324074</v>
+        <v>46079.62311342593</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -18032,7 +18037,7 @@
         <v>1</v>
       </c>
       <c r="N272" s="3" t="n">
-        <v>46079.5667824074</v>
+        <v>46079.64212962963</v>
       </c>
       <c r="O272" t="inlineStr">
         <is>
@@ -18096,7 +18101,7 @@
         <v>2</v>
       </c>
       <c r="N273" s="3" t="n">
-        <v>46078.41335648148</v>
+        <v>46079.6253125</v>
       </c>
       <c r="O273" t="inlineStr">
         <is>
@@ -18480,7 +18485,7 @@
         <v>1</v>
       </c>
       <c r="N279" s="3" t="n">
-        <v>46079.53002314815</v>
+        <v>46079.6471875</v>
       </c>
       <c r="O279" t="inlineStr">
         <is>
@@ -18544,7 +18549,7 @@
         <v>1</v>
       </c>
       <c r="N280" s="3" t="n">
-        <v>46079.55402777778</v>
+        <v>46079.62320601852</v>
       </c>
       <c r="O280" t="inlineStr">
         <is>
@@ -18608,7 +18613,7 @@
         <v>1</v>
       </c>
       <c r="N281" s="3" t="n">
-        <v>46079.56378472222</v>
+        <v>46079.64037037037</v>
       </c>
       <c r="O281" t="inlineStr">
         <is>
@@ -18731,7 +18736,7 @@
         <v>1</v>
       </c>
       <c r="N283" s="3" t="n">
-        <v>46079.44024305556</v>
+        <v>46079.62425925926</v>
       </c>
       <c r="O283" t="inlineStr">
         <is>
@@ -18795,7 +18800,7 @@
         <v>1</v>
       </c>
       <c r="N284" s="3" t="n">
-        <v>46079.56722222222</v>
+        <v>46079.64435185185</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18859,7 +18864,7 @@
         <v>1</v>
       </c>
       <c r="N285" s="3" t="n">
-        <v>46079.54042824074</v>
+        <v>46079.64952546296</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -18878,11 +18883,6 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
-      <c r="C286" t="inlineStr">
-        <is>
-          <t>10.69.5.155</t>
-        </is>
-      </c>
       <c r="D286" t="n">
         <v>2019</v>
       </c>
@@ -18923,7 +18923,7 @@
         <v>1</v>
       </c>
       <c r="N286" s="3" t="n">
-        <v>46079.5496875</v>
+        <v>46079.58777777778</v>
       </c>
       <c r="O286" t="inlineStr">
         <is>
@@ -18987,7 +18987,7 @@
         <v>1</v>
       </c>
       <c r="N287" s="3" t="n">
-        <v>46079.5349074074</v>
+        <v>46079.65112268519</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
@@ -19115,7 +19115,7 @@
         <v>1</v>
       </c>
       <c r="N289" s="3" t="n">
-        <v>46079.55629629629</v>
+        <v>46079.63079861111</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -19909,7 +19909,7 @@
         <v>1</v>
       </c>
       <c r="N302" s="3" t="n">
-        <v>46079.54892361111</v>
+        <v>46079.62987268518</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -21025,7 +21025,7 @@
         </is>
       </c>
       <c r="N320" s="3" t="n">
-        <v>46079.53766203704</v>
+        <v>46079.6524074074</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21750,7 +21750,7 @@
         <v>1</v>
       </c>
       <c r="N332" s="3" t="n">
-        <v>46079.56005787037</v>
+        <v>46079.6378587963</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21814,7 +21814,7 @@
         <v>2</v>
       </c>
       <c r="N333" s="3" t="n">
-        <v>46079.55247685185</v>
+        <v>46079.62675925926</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21878,7 +21878,7 @@
         <v>2</v>
       </c>
       <c r="N334" s="3" t="n">
-        <v>46079.55481481482</v>
+        <v>46079.63233796296</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21942,7 +21942,7 @@
         <v>2</v>
       </c>
       <c r="N335" s="3" t="n">
-        <v>46079.55064814815</v>
+        <v>46079.62372685185</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -22006,7 +22006,7 @@
         <v>1</v>
       </c>
       <c r="N336" s="3" t="n">
-        <v>46079.55734953703</v>
+        <v>46079.63207175926</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22070,7 +22070,7 @@
         <v>1</v>
       </c>
       <c r="N337" s="3" t="n">
-        <v>46079.5412037037</v>
+        <v>46079.61945601852</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22134,7 +22134,7 @@
         <v>2</v>
       </c>
       <c r="N338" s="3" t="n">
-        <v>46079.55175925926</v>
+        <v>46079.62994212963</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -22198,7 +22198,7 @@
         <v>2</v>
       </c>
       <c r="N339" s="3" t="n">
-        <v>46079.55762731482</v>
+        <v>46079.63625</v>
       </c>
       <c r="O339" t="inlineStr">
         <is>
@@ -22326,7 +22326,7 @@
         <v>2</v>
       </c>
       <c r="N341" s="3" t="n">
-        <v>46079.54128472223</v>
+        <v>46079.5818287037</v>
       </c>
       <c r="O341" t="inlineStr">
         <is>
@@ -22707,7 +22707,7 @@
         <v>1</v>
       </c>
       <c r="N347" s="3" t="n">
-        <v>46078.58936342593</v>
+        <v>46079.62734953704</v>
       </c>
       <c r="O347" t="inlineStr">
         <is>
@@ -22771,7 +22771,7 @@
         <v>1</v>
       </c>
       <c r="N348" s="3" t="n">
-        <v>46078.60284722222</v>
+        <v>46079.62532407408</v>
       </c>
       <c r="O348" t="inlineStr">
         <is>
@@ -22835,7 +22835,7 @@
         <v>1</v>
       </c>
       <c r="N349" s="3" t="n">
-        <v>46078.59994212963</v>
+        <v>46079.62761574074</v>
       </c>
       <c r="O349" t="inlineStr">
         <is>
@@ -22958,7 +22958,7 @@
         <v>1</v>
       </c>
       <c r="N351" s="3" t="n">
-        <v>46078.40324074074</v>
+        <v>46079.63040509259</v>
       </c>
       <c r="O351" t="inlineStr">
         <is>
@@ -23083,7 +23083,7 @@
         </is>
       </c>
       <c r="N353" s="3" t="n">
-        <v>46078.59373842592</v>
+        <v>46079.62387731481</v>
       </c>
       <c r="O353" t="inlineStr">
         <is>
@@ -23144,7 +23144,7 @@
         </is>
       </c>
       <c r="N354" s="3" t="n">
-        <v>46078.40594907408</v>
+        <v>46079.62708333333</v>
       </c>
       <c r="O354" t="inlineStr">
         <is>
@@ -23208,7 +23208,7 @@
         <v>1</v>
       </c>
       <c r="N355" s="3" t="n">
-        <v>46078.59833333334</v>
+        <v>46079.6249537037</v>
       </c>
       <c r="O355" t="inlineStr">
         <is>
@@ -23272,7 +23272,7 @@
         <v>1</v>
       </c>
       <c r="N356" s="3" t="n">
-        <v>46078.56122685185</v>
+        <v>46079.62578703704</v>
       </c>
       <c r="O356" t="inlineStr">
         <is>
@@ -23336,7 +23336,7 @@
         <v>1</v>
       </c>
       <c r="N357" s="3" t="n">
-        <v>46078.56133101852</v>
+        <v>46079.6234837963</v>
       </c>
       <c r="O357" t="inlineStr">
         <is>
@@ -23395,7 +23395,7 @@
         <v>1</v>
       </c>
       <c r="N358" s="3" t="n">
-        <v>46072.40707175926</v>
+        <v>46079.62993055556</v>
       </c>
       <c r="O358" t="inlineStr">
         <is>
@@ -23459,7 +23459,7 @@
         <v>2</v>
       </c>
       <c r="N359" s="3" t="n">
-        <v>46078.59206018518</v>
+        <v>46079.6287037037</v>
       </c>
       <c r="O359" t="inlineStr">
         <is>
@@ -23523,7 +23523,7 @@
         <v>2</v>
       </c>
       <c r="N360" s="3" t="n">
-        <v>46078.5678587963</v>
+        <v>46079.63311342592</v>
       </c>
       <c r="O360" t="inlineStr">
         <is>
@@ -23836,7 +23836,7 @@
         <v>1</v>
       </c>
       <c r="N365" s="3" t="n">
-        <v>46079.55438657408</v>
+        <v>46079.62862268519</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
@@ -23902,7 +23902,7 @@
         </is>
       </c>
       <c r="N366" s="3" t="n">
-        <v>46079.55908564815</v>
+        <v>46079.64136574074</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -24028,7 +24028,7 @@
         </is>
       </c>
       <c r="N368" s="3" t="n">
-        <v>46079.55396990741</v>
+        <v>46079.6325462963</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -24089,7 +24089,7 @@
         </is>
       </c>
       <c r="N369" s="3" t="n">
-        <v>46079.56550925926</v>
+        <v>46079.64480324074</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
@@ -24158,7 +24158,7 @@
         <v>1</v>
       </c>
       <c r="N370" s="3" t="n">
-        <v>46079.54859953704</v>
+        <v>46079.62497685185</v>
       </c>
       <c r="O370" t="inlineStr">
         <is>
@@ -24227,7 +24227,7 @@
         <v>1</v>
       </c>
       <c r="N371" s="3" t="n">
-        <v>46079.54758101852</v>
+        <v>46079.6274537037</v>
       </c>
       <c r="O371" t="inlineStr">
         <is>
@@ -24431,7 +24431,7 @@
         <v>1</v>
       </c>
       <c r="N374" s="3" t="n">
-        <v>46079.54868055556</v>
+        <v>46079.63142361111</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24497,7 +24497,7 @@
         </is>
       </c>
       <c r="N375" s="3" t="n">
-        <v>46079.54457175926</v>
+        <v>46079.62508101852</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
@@ -24561,7 +24561,7 @@
         <v>1</v>
       </c>
       <c r="N376" s="3" t="n">
-        <v>46079.56269675926</v>
+        <v>46079.63615740741</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -24630,7 +24630,7 @@
         <v>2</v>
       </c>
       <c r="N377" s="3" t="n">
-        <v>46079.5584375</v>
+        <v>46079.63505787037</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -24699,7 +24699,7 @@
         <v>2</v>
       </c>
       <c r="N378" s="3" t="n">
-        <v>46079.54621527778</v>
+        <v>46079.62598379629</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização automática 2026-02-26 17:52:04.562168
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>46079.6430787037</v>
+        <v>46079.71989583333</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>46079.65287037037</v>
+        <v>46079.72850694445</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
         <v>1</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>46079.6328587963</v>
+        <v>46079.67033564814</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -1259,7 +1259,7 @@
         <v>1</v>
       </c>
       <c r="N12" s="3" t="n">
-        <v>46079.65438657408</v>
+        <v>46079.73184027777</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1515,7 +1515,7 @@
         <v>2</v>
       </c>
       <c r="N16" s="3" t="n">
-        <v>46079.65189814815</v>
+        <v>46079.72951388889</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1579,7 +1579,7 @@
         <v>1</v>
       </c>
       <c r="N17" s="3" t="n">
-        <v>46079.63244212963</v>
+        <v>46079.71280092592</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1643,7 +1643,7 @@
         <v>2</v>
       </c>
       <c r="N18" s="3" t="n">
-        <v>46079.63508101852</v>
+        <v>46079.71333333333</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1768,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="N20" s="3" t="n">
-        <v>46079.62445601852</v>
+        <v>46079.70195601852</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1910,6 +1910,11 @@
           <t>AUDITORIO</t>
         </is>
       </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>10.69.3.146</t>
+        </is>
+      </c>
       <c r="D23" t="n">
         <v>2018</v>
       </c>
@@ -1950,7 +1955,7 @@
         <v>1</v>
       </c>
       <c r="N23" s="3" t="n">
-        <v>46079.49225694445</v>
+        <v>46079.69763888889</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -1967,11 +1972,6 @@
       <c r="B24" t="inlineStr">
         <is>
           <t>AUDITORIO</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>10.69.3.150</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -6575,7 +6575,7 @@
         <v>1</v>
       </c>
       <c r="N95" s="3" t="n">
-        <v>46079.63451388889</v>
+        <v>46079.70763888889</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -6644,7 +6644,7 @@
         <v>1</v>
       </c>
       <c r="N96" s="3" t="n">
-        <v>46079.63488425926</v>
+        <v>46079.71269675926</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
@@ -6708,7 +6708,7 @@
         <v>1</v>
       </c>
       <c r="N97" s="3" t="n">
-        <v>46079.64471064815</v>
+        <v>46079.68333333333</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -6727,11 +6727,6 @@
           <t>COORDENACAO</t>
         </is>
       </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>10.69.3.94</t>
-        </is>
-      </c>
       <c r="D98" t="n">
         <v>2025</v>
       </c>
@@ -6777,7 +6772,7 @@
         <v>1</v>
       </c>
       <c r="N98" s="3" t="n">
-        <v>46079.64555555556</v>
+        <v>46079.6834837963</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -6846,7 +6841,7 @@
         <v>1</v>
       </c>
       <c r="N99" s="3" t="n">
-        <v>46079.62204861111</v>
+        <v>46079.70041666667</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -6915,7 +6910,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>46079.65357638889</v>
+        <v>46079.73715277778</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6984,7 +6979,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="3" t="n">
-        <v>46079.62114583333</v>
+        <v>46079.70375</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -7053,7 +7048,7 @@
         <v>1</v>
       </c>
       <c r="N102" s="3" t="n">
-        <v>46079.62344907408</v>
+        <v>46079.69769675926</v>
       </c>
       <c r="O102" t="inlineStr">
         <is>
@@ -7122,7 +7117,7 @@
         <v>2</v>
       </c>
       <c r="N103" s="3" t="n">
-        <v>46079.65072916666</v>
+        <v>46079.72861111111</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7382,7 +7377,7 @@
         <v>1</v>
       </c>
       <c r="N107" s="3" t="n">
-        <v>46079.6159837963</v>
+        <v>46079.65697916667</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -7520,7 +7515,7 @@
         <v>1</v>
       </c>
       <c r="N109" s="3" t="n">
-        <v>46079.62739583333</v>
+        <v>46079.70490740741</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7589,7 +7584,7 @@
         <v>2</v>
       </c>
       <c r="N110" s="3" t="n">
-        <v>46079.62699074074</v>
+        <v>46079.70668981481</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7658,7 +7653,7 @@
         <v>2</v>
       </c>
       <c r="N111" s="3" t="n">
-        <v>46079.65428240741</v>
+        <v>46079.73306712963</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
@@ -7727,7 +7722,7 @@
         <v>2</v>
       </c>
       <c r="N112" s="3" t="n">
-        <v>46079.6530324074</v>
+        <v>46079.73024305556</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7796,7 +7791,7 @@
         <v>1</v>
       </c>
       <c r="N113" s="3" t="n">
-        <v>46079.62806712963</v>
+        <v>46079.70835648148</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7865,7 +7860,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>46079.64497685185</v>
+        <v>46079.71826388889</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -7931,7 +7926,7 @@
         </is>
       </c>
       <c r="N115" s="3" t="n">
-        <v>46079.64802083333</v>
+        <v>46079.68575231481</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -8000,7 +7995,7 @@
         <v>1</v>
       </c>
       <c r="N116" s="3" t="n">
-        <v>46079.64862268518</v>
+        <v>46079.68635416667</v>
       </c>
       <c r="O116" t="inlineStr">
         <is>
@@ -8019,11 +8014,6 @@
           <t>DP</t>
         </is>
       </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>10.69.3.23</t>
-        </is>
-      </c>
       <c r="D117" t="n">
         <v>2025</v>
       </c>
@@ -8069,7 +8059,7 @@
         <v>1</v>
       </c>
       <c r="N117" s="3" t="n">
-        <v>46079.64728009259</v>
+        <v>46079.685625</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -8135,7 +8125,7 @@
         </is>
       </c>
       <c r="N118" s="3" t="n">
-        <v>46079.64939814815</v>
+        <v>46079.72672453704</v>
       </c>
       <c r="O118" t="inlineStr">
         <is>
@@ -8273,7 +8263,7 @@
         <v>1</v>
       </c>
       <c r="N120" s="3" t="n">
-        <v>46079.63424768519</v>
+        <v>46079.71542824074</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -8342,7 +8332,7 @@
         <v>1</v>
       </c>
       <c r="N121" s="3" t="n">
-        <v>46079.64380787037</v>
+        <v>46079.72481481481</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -8408,7 +8398,7 @@
         </is>
       </c>
       <c r="N122" s="3" t="n">
-        <v>46079.63668981481</v>
+        <v>46079.71303240741</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -8477,7 +8467,7 @@
         <v>2</v>
       </c>
       <c r="N123" s="3" t="n">
-        <v>46079.6159375</v>
+        <v>46079.71407407407</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -8546,7 +8536,7 @@
         <v>1</v>
       </c>
       <c r="N124" s="3" t="n">
-        <v>46079.64834490741</v>
+        <v>46079.73099537037</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -8615,7 +8605,7 @@
         <v>1</v>
       </c>
       <c r="N125" s="3" t="n">
-        <v>46079.63854166667</v>
+        <v>46079.71719907408</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -8684,7 +8674,7 @@
         <v>2</v>
       </c>
       <c r="N126" s="3" t="n">
-        <v>46079.63790509259</v>
+        <v>46079.71350694444</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -8753,7 +8743,7 @@
         <v>2</v>
       </c>
       <c r="N127" s="3" t="n">
-        <v>46079.64895833333</v>
+        <v>46079.72417824074</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -8822,7 +8812,7 @@
         <v>1</v>
       </c>
       <c r="N128" s="3" t="n">
-        <v>46079.63752314815</v>
+        <v>46079.67697916667</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -8891,7 +8881,7 @@
         <v>1</v>
       </c>
       <c r="N129" s="3" t="n">
-        <v>46079.64192129629</v>
+        <v>46079.68133101852</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -8960,7 +8950,7 @@
         <v>1</v>
       </c>
       <c r="N130" s="3" t="n">
-        <v>46079.62581018519</v>
+        <v>46079.70355324074</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -9024,7 +9014,7 @@
         <v>1</v>
       </c>
       <c r="N131" s="3" t="n">
-        <v>46079.6200462963</v>
+        <v>46079.69508101852</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -9157,7 +9147,7 @@
         <v>1</v>
       </c>
       <c r="N133" s="3" t="n">
-        <v>46079.62319444444</v>
+        <v>46079.70553240741</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -9285,7 +9275,7 @@
         <v>1</v>
       </c>
       <c r="N135" s="3" t="n">
-        <v>46079.62197916667</v>
+        <v>46079.69825231482</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -9476,7 +9466,7 @@
         <v>1</v>
       </c>
       <c r="N138" s="3" t="n">
-        <v>46079.65167824074</v>
+        <v>46079.7283912037</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9540,7 +9530,7 @@
         <v>1</v>
       </c>
       <c r="N139" s="3" t="n">
-        <v>46079.62090277778</v>
+        <v>46079.73611111111</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9604,7 +9594,7 @@
         <v>1</v>
       </c>
       <c r="N140" s="3" t="n">
-        <v>46079.6281712963</v>
+        <v>46079.7066087963</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9668,7 +9658,7 @@
         <v>1</v>
       </c>
       <c r="N141" s="3" t="n">
-        <v>46079.62262731481</v>
+        <v>46079.69827546296</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9732,7 +9722,7 @@
         <v>1</v>
       </c>
       <c r="N142" s="3" t="n">
-        <v>46079.6265162037</v>
+        <v>46079.70356481482</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9796,7 +9786,7 @@
         <v>1</v>
       </c>
       <c r="N143" s="3" t="n">
-        <v>46079.63347222222</v>
+        <v>46079.71569444444</v>
       </c>
       <c r="O143" t="inlineStr">
         <is>
@@ -9860,7 +9850,7 @@
         <v>1</v>
       </c>
       <c r="N144" s="3" t="n">
-        <v>46079.62125</v>
+        <v>46079.69655092592</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9924,7 +9914,7 @@
         <v>1</v>
       </c>
       <c r="N145" s="3" t="n">
-        <v>46079.62268518518</v>
+        <v>46079.70256944445</v>
       </c>
       <c r="O145" t="inlineStr">
         <is>
@@ -9988,7 +9978,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="3" t="n">
-        <v>46079.62734953704</v>
+        <v>46079.70131944444</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10052,7 +10042,7 @@
         <v>1</v>
       </c>
       <c r="N147" s="3" t="n">
-        <v>46079.55849537037</v>
+        <v>46079.71344907407</v>
       </c>
       <c r="O147" t="inlineStr">
         <is>
@@ -10116,7 +10106,7 @@
         <v>1</v>
       </c>
       <c r="N148" s="3" t="n">
-        <v>46079.65043981482</v>
+        <v>46079.72521990741</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10180,7 +10170,7 @@
         <v>1</v>
       </c>
       <c r="N149" s="3" t="n">
-        <v>46079.64192129629</v>
+        <v>46079.71798611111</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -10244,7 +10234,7 @@
         <v>1</v>
       </c>
       <c r="N150" s="3" t="n">
-        <v>46079.63627314815</v>
+        <v>46079.71336805556</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -10308,7 +10298,7 @@
         <v>1</v>
       </c>
       <c r="N151" s="3" t="n">
-        <v>46079.65236111111</v>
+        <v>46079.72495370371</v>
       </c>
       <c r="O151" t="inlineStr">
         <is>
@@ -10372,7 +10362,7 @@
         <v>1</v>
       </c>
       <c r="N152" s="3" t="n">
-        <v>46079.62054398148</v>
+        <v>46079.69537037037</v>
       </c>
       <c r="O152" t="inlineStr">
         <is>
@@ -10391,11 +10381,6 @@
           <t>OPERACAO 7.1</t>
         </is>
       </c>
-      <c r="C153" t="inlineStr">
-        <is>
-          <t>10.69.5.21</t>
-        </is>
-      </c>
       <c r="D153" t="n">
         <v>2018</v>
       </c>
@@ -10436,7 +10421,7 @@
         <v>1</v>
       </c>
       <c r="N153" s="3" t="n">
-        <v>46079.64678240741</v>
+        <v>46079.725</v>
       </c>
       <c r="O153" t="inlineStr">
         <is>
@@ -10500,7 +10485,7 @@
         <v>1</v>
       </c>
       <c r="N154" s="3" t="n">
-        <v>46079.62297453704</v>
+        <v>46079.70211805555</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10564,7 +10549,7 @@
         <v>1</v>
       </c>
       <c r="N155" s="3" t="n">
-        <v>46079.63564814815</v>
+        <v>46079.71293981482</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10628,7 +10613,7 @@
         <v>1</v>
       </c>
       <c r="N156" s="3" t="n">
-        <v>46079.62564814815</v>
+        <v>46079.73515046296</v>
       </c>
       <c r="O156" t="inlineStr">
         <is>
@@ -10756,7 +10741,7 @@
         <v>1</v>
       </c>
       <c r="N158" s="3" t="n">
-        <v>46079.62773148148</v>
+        <v>46079.70872685185</v>
       </c>
       <c r="O158" t="inlineStr">
         <is>
@@ -10820,7 +10805,7 @@
         <v>1</v>
       </c>
       <c r="N159" s="3" t="n">
-        <v>46079.62496527778</v>
+        <v>46079.73662037037</v>
       </c>
       <c r="O159" t="inlineStr">
         <is>
@@ -10884,7 +10869,7 @@
         <v>1</v>
       </c>
       <c r="N160" s="3" t="n">
-        <v>46079.64303240741</v>
+        <v>46079.7208912037</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
@@ -10948,7 +10933,7 @@
         <v>1</v>
       </c>
       <c r="N161" s="3" t="n">
-        <v>46079.61913194445</v>
+        <v>46079.73206018518</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -11012,7 +10997,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="3" t="n">
-        <v>46079.64402777778</v>
+        <v>46079.72184027778</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11140,7 +11125,7 @@
         <v>2</v>
       </c>
       <c r="N164" s="3" t="n">
-        <v>46079.63925925926</v>
+        <v>46079.7228125</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11460,7 +11445,7 @@
         <v>2</v>
       </c>
       <c r="N169" s="3" t="n">
-        <v>46079.63814814815</v>
+        <v>46079.71186342592</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -11524,7 +11509,7 @@
         <v>2</v>
       </c>
       <c r="N170" s="3" t="n">
-        <v>46079.61899305556</v>
+        <v>46079.69833333333</v>
       </c>
       <c r="O170" t="inlineStr">
         <is>
@@ -11588,7 +11573,7 @@
         <v>1</v>
       </c>
       <c r="N171" s="3" t="n">
-        <v>46079.63297453704</v>
+        <v>46079.71199074074</v>
       </c>
       <c r="O171" t="inlineStr">
         <is>
@@ -11652,7 +11637,7 @@
         <v>2</v>
       </c>
       <c r="N172" s="3" t="n">
-        <v>46079.62644675926</v>
+        <v>46079.70431712963</v>
       </c>
       <c r="O172" t="inlineStr">
         <is>
@@ -11716,7 +11701,7 @@
         <v>2</v>
       </c>
       <c r="N173" s="3" t="n">
-        <v>46079.64613425926</v>
+        <v>46079.72493055555</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -11844,7 +11829,7 @@
         <v>2</v>
       </c>
       <c r="N175" s="3" t="n">
-        <v>46079.65361111111</v>
+        <v>46079.73612268519</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -11908,7 +11893,7 @@
         <v>2</v>
       </c>
       <c r="N176" s="3" t="n">
-        <v>46079.62309027778</v>
+        <v>46079.70173611111</v>
       </c>
       <c r="O176" t="inlineStr">
         <is>
@@ -11972,7 +11957,7 @@
         <v>2</v>
       </c>
       <c r="N177" s="3" t="n">
-        <v>46079.62315972222</v>
+        <v>46079.70418981482</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
@@ -12036,7 +12021,7 @@
         <v>2</v>
       </c>
       <c r="N178" s="3" t="n">
-        <v>46079.62555555555</v>
+        <v>46079.70393518519</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12100,7 +12085,7 @@
         <v>1</v>
       </c>
       <c r="N179" s="3" t="n">
-        <v>46079.63232638889</v>
+        <v>46079.70834490741</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12164,7 +12149,7 @@
         <v>1</v>
       </c>
       <c r="N180" s="3" t="n">
-        <v>46079.62148148148</v>
+        <v>46079.73506944445</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12228,7 +12213,7 @@
         <v>1</v>
       </c>
       <c r="N181" s="3" t="n">
-        <v>46079.63746527778</v>
+        <v>46079.71427083333</v>
       </c>
       <c r="O181" t="inlineStr">
         <is>
@@ -12356,7 +12341,7 @@
         <v>1</v>
       </c>
       <c r="N183" s="3" t="n">
-        <v>46079.62239583334</v>
+        <v>46079.70050925926</v>
       </c>
       <c r="O183" t="inlineStr">
         <is>
@@ -12425,7 +12410,7 @@
         <v>2</v>
       </c>
       <c r="N184" s="3" t="n">
-        <v>46079.61998842593</v>
+        <v>46079.73400462963</v>
       </c>
       <c r="O184" t="inlineStr">
         <is>
@@ -12489,7 +12474,7 @@
         <v>1</v>
       </c>
       <c r="N185" s="3" t="n">
-        <v>46079.63212962963</v>
+        <v>46079.71046296296</v>
       </c>
       <c r="O185" t="inlineStr">
         <is>
@@ -12681,7 +12666,7 @@
         <v>1</v>
       </c>
       <c r="N188" s="3" t="n">
-        <v>46079.64160879629</v>
+        <v>46079.71652777777</v>
       </c>
       <c r="O188" t="inlineStr">
         <is>
@@ -12809,7 +12794,7 @@
         </is>
       </c>
       <c r="N190" s="3" t="n">
-        <v>46079.62539351852</v>
+        <v>46079.70427083333</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12873,7 +12858,7 @@
         <v>1</v>
       </c>
       <c r="N191" s="3" t="n">
-        <v>46079.63087962963</v>
+        <v>46079.71270833333</v>
       </c>
       <c r="O191" t="inlineStr">
         <is>
@@ -12937,7 +12922,7 @@
         <v>1</v>
       </c>
       <c r="N192" s="3" t="n">
-        <v>46079.64480324074</v>
+        <v>46079.72293981481</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -13126,7 +13111,7 @@
         <v>1</v>
       </c>
       <c r="N195" s="3" t="n">
-        <v>46079.64325231482</v>
+        <v>46079.71853009259</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13190,7 +13175,7 @@
         <v>1</v>
       </c>
       <c r="N196" s="3" t="n">
-        <v>46079.62775462963</v>
+        <v>46079.70417824074</v>
       </c>
       <c r="O196" t="inlineStr">
         <is>
@@ -13254,7 +13239,7 @@
         <v>1</v>
       </c>
       <c r="N197" s="3" t="n">
-        <v>46079.62679398148</v>
+        <v>46079.70305555555</v>
       </c>
       <c r="O197" t="inlineStr">
         <is>
@@ -13318,7 +13303,7 @@
         <v>1</v>
       </c>
       <c r="N198" s="3" t="n">
-        <v>46079.62819444444</v>
+        <v>46079.70875</v>
       </c>
       <c r="O198" t="inlineStr">
         <is>
@@ -13382,7 +13367,7 @@
         <v>1</v>
       </c>
       <c r="N199" s="3" t="n">
-        <v>46079.6365162037</v>
+        <v>46079.70972222222</v>
       </c>
       <c r="O199" t="inlineStr">
         <is>
@@ -13507,7 +13492,7 @@
         </is>
       </c>
       <c r="N201" s="3" t="n">
-        <v>46079.62903935185</v>
+        <v>46079.70369212963</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -13571,7 +13556,7 @@
         <v>1</v>
       </c>
       <c r="N202" s="3" t="n">
-        <v>46079.63363425926</v>
+        <v>46079.70829861111</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13635,7 +13620,7 @@
         <v>1</v>
       </c>
       <c r="N203" s="3" t="n">
-        <v>46079.6222337963</v>
+        <v>46079.70020833334</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13699,7 +13684,7 @@
         <v>1</v>
       </c>
       <c r="N204" s="3" t="n">
-        <v>46079.61575231481</v>
+        <v>46079.73258101852</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13763,7 +13748,7 @@
         <v>1</v>
       </c>
       <c r="N205" s="3" t="n">
-        <v>46079.61527777778</v>
+        <v>46079.73412037037</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13827,7 +13812,7 @@
         <v>1</v>
       </c>
       <c r="N206" s="3" t="n">
-        <v>46079.64820601852</v>
+        <v>46079.7271875</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -13891,7 +13876,7 @@
         <v>1</v>
       </c>
       <c r="N207" s="3" t="n">
-        <v>46079.63438657407</v>
+        <v>46079.71113425926</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -14019,7 +14004,7 @@
         <v>1</v>
       </c>
       <c r="N209" s="3" t="n">
-        <v>46079.62228009259</v>
+        <v>46079.69916666667</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14083,7 +14068,7 @@
         <v>1</v>
       </c>
       <c r="N210" s="3" t="n">
-        <v>46079.64651620371</v>
+        <v>46079.72460648148</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14147,7 +14132,7 @@
         <v>1</v>
       </c>
       <c r="N211" s="3" t="n">
-        <v>46079.62037037037</v>
+        <v>46079.65694444445</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -14211,7 +14196,7 @@
         <v>1</v>
       </c>
       <c r="N212" s="3" t="n">
-        <v>46079.56719907407</v>
+        <v>46079.7152199074</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -14275,7 +14260,7 @@
         <v>1</v>
       </c>
       <c r="N213" s="3" t="n">
-        <v>46079.54940972223</v>
+        <v>46079.71081018518</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
@@ -14339,7 +14324,7 @@
         <v>1</v>
       </c>
       <c r="N214" s="3" t="n">
-        <v>46079.64634259259</v>
+        <v>46079.7234375</v>
       </c>
       <c r="O214" t="inlineStr">
         <is>
@@ -14403,7 +14388,7 @@
         <v>1</v>
       </c>
       <c r="N215" s="3" t="n">
-        <v>46078.79136574074</v>
+        <v>46079.72015046296</v>
       </c>
       <c r="O215" t="inlineStr">
         <is>
@@ -14467,7 +14452,7 @@
         <v>1</v>
       </c>
       <c r="N216" s="3" t="n">
-        <v>46079.64403935185</v>
+        <v>46079.7246875</v>
       </c>
       <c r="O216" t="inlineStr">
         <is>
@@ -14486,6 +14471,11 @@
           <t>OPERACAO 8.1</t>
         </is>
       </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>10.69.5.85</t>
+        </is>
+      </c>
       <c r="D217" t="n">
         <v>2017</v>
       </c>
@@ -14526,7 +14516,7 @@
         <v>1</v>
       </c>
       <c r="N217" s="3" t="n">
-        <v>46079.62137731481</v>
+        <v>46079.73453703704</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14590,7 +14580,7 @@
         <v>1</v>
       </c>
       <c r="N218" s="3" t="n">
-        <v>46079.6440625</v>
+        <v>46079.72134259259</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14654,7 +14644,7 @@
         <v>1</v>
       </c>
       <c r="N219" s="3" t="n">
-        <v>46079.62420138889</v>
+        <v>46079.70515046296</v>
       </c>
       <c r="O219" t="inlineStr">
         <is>
@@ -14723,7 +14713,7 @@
         <v>1</v>
       </c>
       <c r="N220" s="3" t="n">
-        <v>46079.64703703704</v>
+        <v>46079.72834490741</v>
       </c>
       <c r="O220" t="inlineStr">
         <is>
@@ -14787,7 +14777,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="3" t="n">
-        <v>46079.65465277778</v>
+        <v>46079.72886574074</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14851,7 +14841,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="3" t="n">
-        <v>46079.65178240741</v>
+        <v>46079.72856481482</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -14915,7 +14905,7 @@
         <v>1</v>
       </c>
       <c r="N223" s="3" t="n">
-        <v>46079.64148148148</v>
+        <v>46079.71748842593</v>
       </c>
       <c r="O223" t="inlineStr">
         <is>
@@ -14979,7 +14969,7 @@
         <v>1</v>
       </c>
       <c r="N224" s="3" t="n">
-        <v>46079.64331018519</v>
+        <v>46079.71975694445</v>
       </c>
       <c r="O224" t="inlineStr">
         <is>
@@ -15043,7 +15033,7 @@
         <v>1</v>
       </c>
       <c r="N225" s="3" t="n">
-        <v>46079.63831018518</v>
+        <v>46079.7121875</v>
       </c>
       <c r="O225" t="inlineStr">
         <is>
@@ -15107,7 +15097,7 @@
         <v>1</v>
       </c>
       <c r="N226" s="3" t="n">
-        <v>46079.63606481482</v>
+        <v>46079.71391203703</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15171,7 +15161,7 @@
         <v>1</v>
       </c>
       <c r="N227" s="3" t="n">
-        <v>46078.81472222223</v>
+        <v>46079.70667824074</v>
       </c>
       <c r="O227" t="inlineStr">
         <is>
@@ -15235,7 +15225,7 @@
         <v>1</v>
       </c>
       <c r="N228" s="3" t="n">
-        <v>46079.63410879629</v>
+        <v>46079.71450231481</v>
       </c>
       <c r="O228" t="inlineStr">
         <is>
@@ -15299,7 +15289,7 @@
         <v>1</v>
       </c>
       <c r="N229" s="3" t="n">
-        <v>46079.55915509259</v>
+        <v>46079.70047453704</v>
       </c>
       <c r="O229" t="inlineStr">
         <is>
@@ -15363,7 +15353,7 @@
         <v>1</v>
       </c>
       <c r="N230" s="3" t="n">
-        <v>46079.62208333334</v>
+        <v>46079.70012731481</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15427,7 +15417,7 @@
         <v>1</v>
       </c>
       <c r="N231" s="3" t="n">
-        <v>46079.63505787037</v>
+        <v>46079.71428240741</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15491,7 +15481,7 @@
         <v>1</v>
       </c>
       <c r="N232" s="3" t="n">
-        <v>46079.61938657407</v>
+        <v>46079.73401620371</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -15555,7 +15545,7 @@
         <v>1</v>
       </c>
       <c r="N233" s="3" t="n">
-        <v>46079.63806712963</v>
+        <v>46079.71525462963</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15619,7 +15609,7 @@
         <v>1</v>
       </c>
       <c r="N234" s="3" t="n">
-        <v>46079.61935185185</v>
+        <v>46079.73405092592</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -15683,7 +15673,7 @@
         <v>1</v>
       </c>
       <c r="N235" s="3" t="n">
-        <v>46079.62104166667</v>
+        <v>46079.73681712963</v>
       </c>
       <c r="O235" t="inlineStr">
         <is>
@@ -15747,7 +15737,7 @@
         <v>1</v>
       </c>
       <c r="N236" s="3" t="n">
-        <v>46079.54666666667</v>
+        <v>46079.73403935185</v>
       </c>
       <c r="O236" t="inlineStr">
         <is>
@@ -15875,7 +15865,7 @@
         <v>1</v>
       </c>
       <c r="N238" s="3" t="n">
-        <v>46079.63232638889</v>
+        <v>46079.70431712963</v>
       </c>
       <c r="O238" t="inlineStr">
         <is>
@@ -16003,7 +15993,7 @@
         <v>1</v>
       </c>
       <c r="N240" s="3" t="n">
-        <v>46079.62204861111</v>
+        <v>46079.73664351852</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16067,7 +16057,7 @@
         <v>1</v>
       </c>
       <c r="N241" s="3" t="n">
-        <v>46079.61740740741</v>
+        <v>46079.73658564815</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16131,7 +16121,7 @@
         <v>1</v>
       </c>
       <c r="N242" s="3" t="n">
-        <v>46079.62788194444</v>
+        <v>46079.70179398148</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16195,7 +16185,7 @@
         <v>1</v>
       </c>
       <c r="N243" s="3" t="n">
-        <v>46079.63395833333</v>
+        <v>46079.71256944445</v>
       </c>
       <c r="O243" t="inlineStr">
         <is>
@@ -16318,7 +16308,7 @@
         <v>1</v>
       </c>
       <c r="N245" s="3" t="n">
-        <v>46079.62625</v>
+        <v>46079.7080787037</v>
       </c>
       <c r="O245" t="inlineStr">
         <is>
@@ -16382,7 +16372,7 @@
         <v>1</v>
       </c>
       <c r="N246" s="3" t="n">
-        <v>46079.63238425926</v>
+        <v>46079.70784722222</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16446,7 +16436,7 @@
         <v>1</v>
       </c>
       <c r="N247" s="3" t="n">
-        <v>46079.62234953704</v>
+        <v>46079.7375925926</v>
       </c>
       <c r="O247" t="inlineStr">
         <is>
@@ -16510,7 +16500,7 @@
         <v>1</v>
       </c>
       <c r="N248" s="3" t="n">
-        <v>46079.64152777778</v>
+        <v>46079.72039351852</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16574,7 +16564,7 @@
         <v>1</v>
       </c>
       <c r="N249" s="3" t="n">
-        <v>46079.6435300926</v>
+        <v>46079.71885416667</v>
       </c>
       <c r="O249" t="inlineStr">
         <is>
@@ -16638,7 +16628,7 @@
         <v>1</v>
       </c>
       <c r="N250" s="3" t="n">
-        <v>46079.64246527778</v>
+        <v>46079.72076388889</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16702,7 +16692,7 @@
         <v>1</v>
       </c>
       <c r="N251" s="3" t="n">
-        <v>46079.63626157407</v>
+        <v>46079.71620370371</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16766,7 +16756,7 @@
         <v>1</v>
       </c>
       <c r="N252" s="3" t="n">
-        <v>46079.63535879629</v>
+        <v>46079.70997685185</v>
       </c>
       <c r="O252" t="inlineStr">
         <is>
@@ -16830,7 +16820,7 @@
         <v>1</v>
       </c>
       <c r="N253" s="3" t="n">
-        <v>46079.6203125</v>
+        <v>46079.73636574074</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16888,7 +16878,7 @@
         <v>1</v>
       </c>
       <c r="N254" s="3" t="n">
-        <v>46079.63315972222</v>
+        <v>46079.71046296296</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -17016,7 +17006,7 @@
         <v>1</v>
       </c>
       <c r="N256" s="3" t="n">
-        <v>46079.65296296297</v>
+        <v>46079.73050925926</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17080,7 +17070,7 @@
         <v>1</v>
       </c>
       <c r="N257" s="3" t="n">
-        <v>46079.61744212963</v>
+        <v>46079.73525462963</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17144,7 +17134,7 @@
         <v>1</v>
       </c>
       <c r="N258" s="3" t="n">
-        <v>46079.64549768518</v>
+        <v>46079.72193287037</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
@@ -17208,7 +17198,7 @@
         <v>1</v>
       </c>
       <c r="N259" s="3" t="n">
-        <v>46079.64957175926</v>
+        <v>46079.72855324074</v>
       </c>
       <c r="O259" t="inlineStr">
         <is>
@@ -17336,7 +17326,7 @@
         <v>1</v>
       </c>
       <c r="N261" s="3" t="n">
-        <v>46079.63605324074</v>
+        <v>46079.73284722222</v>
       </c>
       <c r="O261" t="inlineStr">
         <is>
@@ -17400,7 +17390,7 @@
         <v>1</v>
       </c>
       <c r="N262" s="3" t="n">
-        <v>46079.63423611111</v>
+        <v>46079.70824074074</v>
       </c>
       <c r="O262" t="inlineStr">
         <is>
@@ -17464,7 +17454,7 @@
         <v>1</v>
       </c>
       <c r="N263" s="3" t="n">
-        <v>46079.62979166667</v>
+        <v>46079.70553240741</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17528,7 +17518,7 @@
         <v>1</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>46079.65428240741</v>
+        <v>46079.73064814815</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17592,7 +17582,7 @@
         <v>1</v>
       </c>
       <c r="N265" s="3" t="n">
-        <v>46079.62508101852</v>
+        <v>46079.70332175926</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17656,7 +17646,7 @@
         <v>1</v>
       </c>
       <c r="N266" s="3" t="n">
-        <v>46079.64818287037</v>
+        <v>46079.72761574074</v>
       </c>
       <c r="O266" t="inlineStr">
         <is>
@@ -17720,7 +17710,7 @@
         <v>1</v>
       </c>
       <c r="N267" s="3" t="n">
-        <v>46079.64049768518</v>
+        <v>46079.72100694444</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17784,7 +17774,7 @@
         <v>1</v>
       </c>
       <c r="N268" s="3" t="n">
-        <v>46079.64549768518</v>
+        <v>46079.72413194444</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17848,7 +17838,7 @@
         <v>1</v>
       </c>
       <c r="N269" s="3" t="n">
-        <v>46079.63863425926</v>
+        <v>46079.71319444444</v>
       </c>
       <c r="O269" t="inlineStr">
         <is>
@@ -17909,7 +17899,7 @@
         </is>
       </c>
       <c r="N270" s="3" t="n">
-        <v>46079.62311342593</v>
+        <v>46079.70202546296</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -18101,7 +18091,7 @@
         <v>2</v>
       </c>
       <c r="N273" s="3" t="n">
-        <v>46079.6253125</v>
+        <v>46079.66320601852</v>
       </c>
       <c r="O273" t="inlineStr">
         <is>
@@ -18485,7 +18475,7 @@
         <v>1</v>
       </c>
       <c r="N279" s="3" t="n">
-        <v>46079.6471875</v>
+        <v>46079.72244212963</v>
       </c>
       <c r="O279" t="inlineStr">
         <is>
@@ -18549,7 +18539,7 @@
         <v>1</v>
       </c>
       <c r="N280" s="3" t="n">
-        <v>46079.62320601852</v>
+        <v>46079.70355324074</v>
       </c>
       <c r="O280" t="inlineStr">
         <is>
@@ -18613,7 +18603,7 @@
         <v>1</v>
       </c>
       <c r="N281" s="3" t="n">
-        <v>46079.64037037037</v>
+        <v>46079.71649305556</v>
       </c>
       <c r="O281" t="inlineStr">
         <is>
@@ -18736,7 +18726,7 @@
         <v>1</v>
       </c>
       <c r="N283" s="3" t="n">
-        <v>46079.62425925926</v>
+        <v>46079.73575231482</v>
       </c>
       <c r="O283" t="inlineStr">
         <is>
@@ -18800,7 +18790,7 @@
         <v>1</v>
       </c>
       <c r="N284" s="3" t="n">
-        <v>46079.64435185185</v>
+        <v>46079.72288194444</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18864,7 +18854,7 @@
         <v>1</v>
       </c>
       <c r="N285" s="3" t="n">
-        <v>46079.64952546296</v>
+        <v>46079.72607638889</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -18987,7 +18977,7 @@
         <v>1</v>
       </c>
       <c r="N287" s="3" t="n">
-        <v>46079.65112268519</v>
+        <v>46079.72891203704</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
@@ -19115,7 +19105,7 @@
         <v>1</v>
       </c>
       <c r="N289" s="3" t="n">
-        <v>46079.63079861111</v>
+        <v>46079.70324074074</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -19909,7 +19899,7 @@
         <v>1</v>
       </c>
       <c r="N302" s="3" t="n">
-        <v>46079.62987268518</v>
+        <v>46079.70971064815</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -21025,7 +21015,7 @@
         </is>
       </c>
       <c r="N320" s="3" t="n">
-        <v>46079.6524074074</v>
+        <v>46079.72775462963</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21750,7 +21740,7 @@
         <v>1</v>
       </c>
       <c r="N332" s="3" t="n">
-        <v>46079.6378587963</v>
+        <v>46079.71637731481</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21814,7 +21804,7 @@
         <v>2</v>
       </c>
       <c r="N333" s="3" t="n">
-        <v>46079.62675925926</v>
+        <v>46079.70217592592</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21878,7 +21868,7 @@
         <v>2</v>
       </c>
       <c r="N334" s="3" t="n">
-        <v>46079.63233796296</v>
+        <v>46079.71271990741</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21942,7 +21932,7 @@
         <v>2</v>
       </c>
       <c r="N335" s="3" t="n">
-        <v>46079.62372685185</v>
+        <v>46079.69729166666</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -22006,7 +21996,7 @@
         <v>1</v>
       </c>
       <c r="N336" s="3" t="n">
-        <v>46079.63207175926</v>
+        <v>46079.66770833333</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22070,7 +22060,7 @@
         <v>1</v>
       </c>
       <c r="N337" s="3" t="n">
-        <v>46079.61945601852</v>
+        <v>46079.73407407408</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22134,7 +22124,7 @@
         <v>2</v>
       </c>
       <c r="N338" s="3" t="n">
-        <v>46079.62994212963</v>
+        <v>46079.70646990741</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -22198,7 +22188,7 @@
         <v>2</v>
       </c>
       <c r="N339" s="3" t="n">
-        <v>46079.63625</v>
+        <v>46079.71229166666</v>
       </c>
       <c r="O339" t="inlineStr">
         <is>
@@ -22771,7 +22761,7 @@
         <v>1</v>
       </c>
       <c r="N348" s="3" t="n">
-        <v>46079.62532407408</v>
+        <v>46079.6684837963</v>
       </c>
       <c r="O348" t="inlineStr">
         <is>
@@ -22894,7 +22884,7 @@
         <v>1</v>
       </c>
       <c r="N350" s="3" t="n">
-        <v>46078.5891087963</v>
+        <v>46079.69943287037</v>
       </c>
       <c r="O350" t="inlineStr">
         <is>
@@ -22958,7 +22948,7 @@
         <v>1</v>
       </c>
       <c r="N351" s="3" t="n">
-        <v>46079.63040509259</v>
+        <v>46079.71148148148</v>
       </c>
       <c r="O351" t="inlineStr">
         <is>
@@ -23083,7 +23073,7 @@
         </is>
       </c>
       <c r="N353" s="3" t="n">
-        <v>46079.62387731481</v>
+        <v>46079.65965277778</v>
       </c>
       <c r="O353" t="inlineStr">
         <is>
@@ -23144,7 +23134,7 @@
         </is>
       </c>
       <c r="N354" s="3" t="n">
-        <v>46079.62708333333</v>
+        <v>46079.6679050926</v>
       </c>
       <c r="O354" t="inlineStr">
         <is>
@@ -23208,7 +23198,7 @@
         <v>1</v>
       </c>
       <c r="N355" s="3" t="n">
-        <v>46079.6249537037</v>
+        <v>46079.66519675926</v>
       </c>
       <c r="O355" t="inlineStr">
         <is>
@@ -23272,7 +23262,7 @@
         <v>1</v>
       </c>
       <c r="N356" s="3" t="n">
-        <v>46079.62578703704</v>
+        <v>46079.6677662037</v>
       </c>
       <c r="O356" t="inlineStr">
         <is>
@@ -23336,7 +23326,7 @@
         <v>1</v>
       </c>
       <c r="N357" s="3" t="n">
-        <v>46079.6234837963</v>
+        <v>46079.66325231481</v>
       </c>
       <c r="O357" t="inlineStr">
         <is>
@@ -23395,7 +23385,7 @@
         <v>1</v>
       </c>
       <c r="N358" s="3" t="n">
-        <v>46079.62993055556</v>
+        <v>46079.67070601852</v>
       </c>
       <c r="O358" t="inlineStr">
         <is>
@@ -23459,7 +23449,7 @@
         <v>2</v>
       </c>
       <c r="N359" s="3" t="n">
-        <v>46079.6287037037</v>
+        <v>46079.66747685185</v>
       </c>
       <c r="O359" t="inlineStr">
         <is>
@@ -23523,7 +23513,7 @@
         <v>2</v>
       </c>
       <c r="N360" s="3" t="n">
-        <v>46079.63311342592</v>
+        <v>46079.67631944444</v>
       </c>
       <c r="O360" t="inlineStr">
         <is>
@@ -23836,7 +23826,7 @@
         <v>1</v>
       </c>
       <c r="N365" s="3" t="n">
-        <v>46079.62862268519</v>
+        <v>46079.70519675926</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
@@ -23902,7 +23892,7 @@
         </is>
       </c>
       <c r="N366" s="3" t="n">
-        <v>46079.64136574074</v>
+        <v>46079.71809027778</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -24028,7 +24018,7 @@
         </is>
       </c>
       <c r="N368" s="3" t="n">
-        <v>46079.6325462963</v>
+        <v>46079.7078587963</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -24047,6 +24037,11 @@
           <t>RH</t>
         </is>
       </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>10.69.3.13</t>
+        </is>
+      </c>
       <c r="D369" t="n">
         <v>2025</v>
       </c>
@@ -24089,7 +24084,7 @@
         </is>
       </c>
       <c r="N369" s="3" t="n">
-        <v>46079.64480324074</v>
+        <v>46079.71952546296</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
@@ -24158,7 +24153,7 @@
         <v>1</v>
       </c>
       <c r="N370" s="3" t="n">
-        <v>46079.62497685185</v>
+        <v>46079.70358796296</v>
       </c>
       <c r="O370" t="inlineStr">
         <is>
@@ -24227,7 +24222,7 @@
         <v>1</v>
       </c>
       <c r="N371" s="3" t="n">
-        <v>46079.6274537037</v>
+        <v>46079.70053240741</v>
       </c>
       <c r="O371" t="inlineStr">
         <is>
@@ -24431,7 +24426,7 @@
         <v>1</v>
       </c>
       <c r="N374" s="3" t="n">
-        <v>46079.63142361111</v>
+        <v>46079.70917824074</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24497,7 +24492,7 @@
         </is>
       </c>
       <c r="N375" s="3" t="n">
-        <v>46079.62508101852</v>
+        <v>46079.72599537037</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
@@ -24516,6 +24511,11 @@
           <t>COORDENACAO</t>
         </is>
       </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>10.69.3.72</t>
+        </is>
+      </c>
       <c r="D376" t="n">
         <v>2025</v>
       </c>
@@ -24561,7 +24561,7 @@
         <v>1</v>
       </c>
       <c r="N376" s="3" t="n">
-        <v>46079.63615740741</v>
+        <v>46079.71738425926</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -24630,7 +24630,7 @@
         <v>2</v>
       </c>
       <c r="N377" s="3" t="n">
-        <v>46079.63505787037</v>
+        <v>46079.71207175926</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -24699,7 +24699,7 @@
         <v>2</v>
       </c>
       <c r="N378" s="3" t="n">
-        <v>46079.62598379629</v>
+        <v>46079.70734953704</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização automática 2026-02-27 07:52:05.220270
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>46079.71989583333</v>
+        <v>46080.29556712963</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>46079.72850694445</v>
+        <v>46080.314375</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -1259,7 +1259,7 @@
         <v>1</v>
       </c>
       <c r="N12" s="3" t="n">
-        <v>46079.73184027777</v>
+        <v>46080.31922453704</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1515,7 +1515,7 @@
         <v>2</v>
       </c>
       <c r="N16" s="3" t="n">
-        <v>46079.72951388889</v>
+        <v>46080.30274305555</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1579,7 +1579,7 @@
         <v>1</v>
       </c>
       <c r="N17" s="3" t="n">
-        <v>46079.71280092592</v>
+        <v>46080.3121875</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1643,7 +1643,7 @@
         <v>2</v>
       </c>
       <c r="N18" s="3" t="n">
-        <v>46079.71333333333</v>
+        <v>46080.29148148148</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1768,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="N20" s="3" t="n">
-        <v>46079.70195601852</v>
+        <v>46080.31166666667</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1910,11 +1910,6 @@
           <t>AUDITORIO</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>10.69.3.146</t>
-        </is>
-      </c>
       <c r="D23" t="n">
         <v>2018</v>
       </c>
@@ -1955,7 +1950,7 @@
         <v>1</v>
       </c>
       <c r="N23" s="3" t="n">
-        <v>46079.69763888889</v>
+        <v>46080.10675925926</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -6575,7 +6570,7 @@
         <v>1</v>
       </c>
       <c r="N95" s="3" t="n">
-        <v>46079.70763888889</v>
+        <v>46079.82608796296</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -6644,7 +6639,7 @@
         <v>1</v>
       </c>
       <c r="N96" s="3" t="n">
-        <v>46079.71269675926</v>
+        <v>46079.82724537037</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
@@ -6910,7 +6905,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>46079.73715277778</v>
+        <v>46080.31297453704</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6979,7 +6974,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="3" t="n">
-        <v>46079.70375</v>
+        <v>46079.81753472222</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -7117,7 +7112,7 @@
         <v>2</v>
       </c>
       <c r="N103" s="3" t="n">
-        <v>46079.72861111111</v>
+        <v>46080.28097222222</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7515,7 +7510,7 @@
         <v>1</v>
       </c>
       <c r="N109" s="3" t="n">
-        <v>46079.70490740741</v>
+        <v>46080.29549768518</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7584,7 +7579,7 @@
         <v>2</v>
       </c>
       <c r="N110" s="3" t="n">
-        <v>46079.70668981481</v>
+        <v>46080.28954861111</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7653,7 +7648,7 @@
         <v>2</v>
       </c>
       <c r="N111" s="3" t="n">
-        <v>46079.73306712963</v>
+        <v>46080.31909722222</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
@@ -7722,7 +7717,7 @@
         <v>2</v>
       </c>
       <c r="N112" s="3" t="n">
-        <v>46079.73024305556</v>
+        <v>46080.31684027778</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7791,7 +7786,7 @@
         <v>1</v>
       </c>
       <c r="N113" s="3" t="n">
-        <v>46079.70835648148</v>
+        <v>46080.28915509259</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7860,7 +7855,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>46079.71826388889</v>
+        <v>46080.29603009259</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -8014,6 +8009,11 @@
           <t>DP</t>
         </is>
       </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>10.69.3.23</t>
+        </is>
+      </c>
       <c r="D117" t="n">
         <v>2025</v>
       </c>
@@ -8059,7 +8059,7 @@
         <v>1</v>
       </c>
       <c r="N117" s="3" t="n">
-        <v>46079.685625</v>
+        <v>46080.32011574074</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -8263,7 +8263,7 @@
         <v>1</v>
       </c>
       <c r="N120" s="3" t="n">
-        <v>46079.71542824074</v>
+        <v>46080.29375</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -8332,7 +8332,7 @@
         <v>1</v>
       </c>
       <c r="N121" s="3" t="n">
-        <v>46079.72481481481</v>
+        <v>46079.80608796296</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -8398,7 +8398,7 @@
         </is>
       </c>
       <c r="N122" s="3" t="n">
-        <v>46079.71303240741</v>
+        <v>46079.7866087963</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -8467,7 +8467,7 @@
         <v>2</v>
       </c>
       <c r="N123" s="3" t="n">
-        <v>46079.71407407407</v>
+        <v>46080.30180555556</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -8536,7 +8536,7 @@
         <v>1</v>
       </c>
       <c r="N124" s="3" t="n">
-        <v>46079.73099537037</v>
+        <v>46080.31997685185</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -8605,7 +8605,7 @@
         <v>1</v>
       </c>
       <c r="N125" s="3" t="n">
-        <v>46079.71719907408</v>
+        <v>46080.28650462963</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -8674,7 +8674,7 @@
         <v>2</v>
       </c>
       <c r="N126" s="3" t="n">
-        <v>46079.71350694444</v>
+        <v>46079.78649305556</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -8743,7 +8743,7 @@
         <v>2</v>
       </c>
       <c r="N127" s="3" t="n">
-        <v>46079.72417824074</v>
+        <v>46080.30769675926</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -8950,7 +8950,7 @@
         <v>1</v>
       </c>
       <c r="N130" s="3" t="n">
-        <v>46079.70355324074</v>
+        <v>46079.77684027778</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -8969,6 +8969,11 @@
           <t>ADM/FIN</t>
         </is>
       </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>10.69.3.6</t>
+        </is>
+      </c>
       <c r="D131" t="n">
         <v>2025</v>
       </c>
@@ -9014,7 +9019,7 @@
         <v>1</v>
       </c>
       <c r="N131" s="3" t="n">
-        <v>46079.69508101852</v>
+        <v>46080.31950231481</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -9147,7 +9152,7 @@
         <v>1</v>
       </c>
       <c r="N133" s="3" t="n">
-        <v>46079.70553240741</v>
+        <v>46079.81851851852</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -9275,7 +9280,7 @@
         <v>1</v>
       </c>
       <c r="N135" s="3" t="n">
-        <v>46079.69825231482</v>
+        <v>46079.80307870371</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -9466,7 +9471,7 @@
         <v>1</v>
       </c>
       <c r="N138" s="3" t="n">
-        <v>46079.7283912037</v>
+        <v>46079.81016203704</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9530,7 +9535,7 @@
         <v>1</v>
       </c>
       <c r="N139" s="3" t="n">
-        <v>46079.73611111111</v>
+        <v>46079.81265046296</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9594,7 +9599,7 @@
         <v>1</v>
       </c>
       <c r="N140" s="3" t="n">
-        <v>46079.7066087963</v>
+        <v>46079.82202546296</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9658,7 +9663,7 @@
         <v>1</v>
       </c>
       <c r="N141" s="3" t="n">
-        <v>46079.69827546296</v>
+        <v>46079.8047337963</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9722,7 +9727,7 @@
         <v>1</v>
       </c>
       <c r="N142" s="3" t="n">
-        <v>46079.70356481482</v>
+        <v>46079.82223379629</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9786,7 +9791,7 @@
         <v>1</v>
       </c>
       <c r="N143" s="3" t="n">
-        <v>46079.71569444444</v>
+        <v>46079.79195601852</v>
       </c>
       <c r="O143" t="inlineStr">
         <is>
@@ -9850,7 +9855,7 @@
         <v>1</v>
       </c>
       <c r="N144" s="3" t="n">
-        <v>46079.69655092592</v>
+        <v>46079.81663194444</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9914,7 +9919,7 @@
         <v>1</v>
       </c>
       <c r="N145" s="3" t="n">
-        <v>46079.70256944445</v>
+        <v>46079.8215625</v>
       </c>
       <c r="O145" t="inlineStr">
         <is>
@@ -9978,7 +9983,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="3" t="n">
-        <v>46079.70131944444</v>
+        <v>46079.8159375</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10042,7 +10047,7 @@
         <v>1</v>
       </c>
       <c r="N147" s="3" t="n">
-        <v>46079.71344907407</v>
+        <v>46079.7934837963</v>
       </c>
       <c r="O147" t="inlineStr">
         <is>
@@ -10106,7 +10111,7 @@
         <v>1</v>
       </c>
       <c r="N148" s="3" t="n">
-        <v>46079.72521990741</v>
+        <v>46079.80366898148</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10170,7 +10175,7 @@
         <v>1</v>
       </c>
       <c r="N149" s="3" t="n">
-        <v>46079.71798611111</v>
+        <v>46079.87311342593</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -10234,7 +10239,7 @@
         <v>1</v>
       </c>
       <c r="N150" s="3" t="n">
-        <v>46079.71336805556</v>
+        <v>46079.7537037037</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -10298,7 +10303,7 @@
         <v>1</v>
       </c>
       <c r="N151" s="3" t="n">
-        <v>46079.72495370371</v>
+        <v>46079.80550925926</v>
       </c>
       <c r="O151" t="inlineStr">
         <is>
@@ -10381,6 +10386,11 @@
           <t>OPERACAO 7.1</t>
         </is>
       </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>10.69.5.21</t>
+        </is>
+      </c>
       <c r="D153" t="n">
         <v>2018</v>
       </c>
@@ -10421,7 +10431,7 @@
         <v>1</v>
       </c>
       <c r="N153" s="3" t="n">
-        <v>46079.725</v>
+        <v>46079.87296296296</v>
       </c>
       <c r="O153" t="inlineStr">
         <is>
@@ -10485,7 +10495,7 @@
         <v>1</v>
       </c>
       <c r="N154" s="3" t="n">
-        <v>46079.70211805555</v>
+        <v>46080.31497685185</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10549,7 +10559,7 @@
         <v>1</v>
       </c>
       <c r="N155" s="3" t="n">
-        <v>46079.71293981482</v>
+        <v>46079.79131944444</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10613,7 +10623,7 @@
         <v>1</v>
       </c>
       <c r="N156" s="3" t="n">
-        <v>46079.73515046296</v>
+        <v>46079.81130787037</v>
       </c>
       <c r="O156" t="inlineStr">
         <is>
@@ -10741,7 +10751,7 @@
         <v>1</v>
       </c>
       <c r="N158" s="3" t="n">
-        <v>46079.70872685185</v>
+        <v>46080.3127662037</v>
       </c>
       <c r="O158" t="inlineStr">
         <is>
@@ -10805,7 +10815,7 @@
         <v>1</v>
       </c>
       <c r="N159" s="3" t="n">
-        <v>46079.73662037037</v>
+        <v>46080.31447916666</v>
       </c>
       <c r="O159" t="inlineStr">
         <is>
@@ -10869,7 +10879,7 @@
         <v>1</v>
       </c>
       <c r="N160" s="3" t="n">
-        <v>46079.7208912037</v>
+        <v>46079.79456018518</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
@@ -10933,7 +10943,7 @@
         <v>1</v>
       </c>
       <c r="N161" s="3" t="n">
-        <v>46079.73206018518</v>
+        <v>46079.80791666666</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -10997,7 +11007,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="3" t="n">
-        <v>46079.72184027778</v>
+        <v>46079.79564814815</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11122,10 +11132,10 @@
         </is>
       </c>
       <c r="M164" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N164" s="3" t="n">
-        <v>46079.7228125</v>
+        <v>46080.28221064815</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11381,7 +11391,7 @@
         <v>2</v>
       </c>
       <c r="N168" s="3" t="n">
-        <v>46079.56518518519</v>
+        <v>46080.31921296296</v>
       </c>
       <c r="O168" t="inlineStr">
         <is>
@@ -11445,7 +11455,7 @@
         <v>2</v>
       </c>
       <c r="N169" s="3" t="n">
-        <v>46079.71186342592</v>
+        <v>46079.74877314815</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -11509,7 +11519,7 @@
         <v>2</v>
       </c>
       <c r="N170" s="3" t="n">
-        <v>46079.69833333333</v>
+        <v>46080.30814814815</v>
       </c>
       <c r="O170" t="inlineStr">
         <is>
@@ -11573,7 +11583,7 @@
         <v>1</v>
       </c>
       <c r="N171" s="3" t="n">
-        <v>46079.71199074074</v>
+        <v>46080.28824074074</v>
       </c>
       <c r="O171" t="inlineStr">
         <is>
@@ -11637,7 +11647,7 @@
         <v>2</v>
       </c>
       <c r="N172" s="3" t="n">
-        <v>46079.70431712963</v>
+        <v>46079.8635300926</v>
       </c>
       <c r="O172" t="inlineStr">
         <is>
@@ -11698,10 +11708,10 @@
         </is>
       </c>
       <c r="M173" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N173" s="3" t="n">
-        <v>46079.72493055555</v>
+        <v>46080.30158564815</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -11829,7 +11839,7 @@
         <v>2</v>
       </c>
       <c r="N175" s="3" t="n">
-        <v>46079.73612268519</v>
+        <v>46080.30027777778</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -11893,7 +11903,7 @@
         <v>2</v>
       </c>
       <c r="N176" s="3" t="n">
-        <v>46079.70173611111</v>
+        <v>46080.29123842593</v>
       </c>
       <c r="O176" t="inlineStr">
         <is>
@@ -12021,7 +12031,7 @@
         <v>2</v>
       </c>
       <c r="N178" s="3" t="n">
-        <v>46079.70393518519</v>
+        <v>46080.3203587963</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12085,7 +12095,7 @@
         <v>1</v>
       </c>
       <c r="N179" s="3" t="n">
-        <v>46079.70834490741</v>
+        <v>46080.31607638889</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12149,7 +12159,7 @@
         <v>1</v>
       </c>
       <c r="N180" s="3" t="n">
-        <v>46079.73506944445</v>
+        <v>46080.31592592593</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12213,7 +12223,7 @@
         <v>1</v>
       </c>
       <c r="N181" s="3" t="n">
-        <v>46079.71427083333</v>
+        <v>46079.86542824074</v>
       </c>
       <c r="O181" t="inlineStr">
         <is>
@@ -12341,7 +12351,7 @@
         <v>1</v>
       </c>
       <c r="N183" s="3" t="n">
-        <v>46079.70050925926</v>
+        <v>46080.28488425926</v>
       </c>
       <c r="O183" t="inlineStr">
         <is>
@@ -12410,7 +12420,7 @@
         <v>2</v>
       </c>
       <c r="N184" s="3" t="n">
-        <v>46079.73400462963</v>
+        <v>46080.28256944445</v>
       </c>
       <c r="O184" t="inlineStr">
         <is>
@@ -12474,7 +12484,7 @@
         <v>1</v>
       </c>
       <c r="N185" s="3" t="n">
-        <v>46079.71046296296</v>
+        <v>46079.82648148148</v>
       </c>
       <c r="O185" t="inlineStr">
         <is>
@@ -12666,7 +12676,7 @@
         <v>1</v>
       </c>
       <c r="N188" s="3" t="n">
-        <v>46079.71652777777</v>
+        <v>46080.29646990741</v>
       </c>
       <c r="O188" t="inlineStr">
         <is>
@@ -12794,7 +12804,7 @@
         </is>
       </c>
       <c r="N190" s="3" t="n">
-        <v>46079.70427083333</v>
+        <v>46080.31819444444</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12858,7 +12868,7 @@
         <v>1</v>
       </c>
       <c r="N191" s="3" t="n">
-        <v>46079.71270833333</v>
+        <v>46079.794375</v>
       </c>
       <c r="O191" t="inlineStr">
         <is>
@@ -12922,7 +12932,7 @@
         <v>1</v>
       </c>
       <c r="N192" s="3" t="n">
-        <v>46079.72293981481</v>
+        <v>46079.79903935185</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -13047,7 +13057,7 @@
         <v>2</v>
       </c>
       <c r="N194" s="3" t="n">
-        <v>46079.58024305556</v>
+        <v>46079.9927662037</v>
       </c>
       <c r="O194" t="inlineStr">
         <is>
@@ -13111,7 +13121,7 @@
         <v>1</v>
       </c>
       <c r="N195" s="3" t="n">
-        <v>46079.71853009259</v>
+        <v>46079.83634259259</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13175,7 +13185,7 @@
         <v>1</v>
       </c>
       <c r="N196" s="3" t="n">
-        <v>46079.70417824074</v>
+        <v>46079.81520833333</v>
       </c>
       <c r="O196" t="inlineStr">
         <is>
@@ -13239,7 +13249,7 @@
         <v>1</v>
       </c>
       <c r="N197" s="3" t="n">
-        <v>46079.70305555555</v>
+        <v>46079.84797453704</v>
       </c>
       <c r="O197" t="inlineStr">
         <is>
@@ -13303,7 +13313,7 @@
         <v>1</v>
       </c>
       <c r="N198" s="3" t="n">
-        <v>46079.70875</v>
+        <v>46079.8665625</v>
       </c>
       <c r="O198" t="inlineStr">
         <is>
@@ -13367,7 +13377,7 @@
         <v>1</v>
       </c>
       <c r="N199" s="3" t="n">
-        <v>46079.70972222222</v>
+        <v>46080.28875</v>
       </c>
       <c r="O199" t="inlineStr">
         <is>
@@ -13492,7 +13502,7 @@
         </is>
       </c>
       <c r="N201" s="3" t="n">
-        <v>46079.70369212963</v>
+        <v>46079.81636574074</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -13556,7 +13566,7 @@
         <v>1</v>
       </c>
       <c r="N202" s="3" t="n">
-        <v>46079.70829861111</v>
+        <v>46079.81935185185</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13620,7 +13630,7 @@
         <v>1</v>
       </c>
       <c r="N203" s="3" t="n">
-        <v>46079.70020833334</v>
+        <v>46079.81766203704</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13684,7 +13694,7 @@
         <v>1</v>
       </c>
       <c r="N204" s="3" t="n">
-        <v>46079.73258101852</v>
+        <v>46079.81115740741</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13748,7 +13758,7 @@
         <v>1</v>
       </c>
       <c r="N205" s="3" t="n">
-        <v>46079.73412037037</v>
+        <v>46079.8190625</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13812,7 +13822,7 @@
         <v>1</v>
       </c>
       <c r="N206" s="3" t="n">
-        <v>46079.7271875</v>
+        <v>46079.8059375</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -13876,7 +13886,7 @@
         <v>1</v>
       </c>
       <c r="N207" s="3" t="n">
-        <v>46079.71113425926</v>
+        <v>46080.30528935185</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -14004,7 +14014,7 @@
         <v>1</v>
       </c>
       <c r="N209" s="3" t="n">
-        <v>46079.69916666667</v>
+        <v>46079.80993055556</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14068,7 +14078,7 @@
         <v>1</v>
       </c>
       <c r="N210" s="3" t="n">
-        <v>46079.72460648148</v>
+        <v>46079.84193287037</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14196,7 +14206,7 @@
         <v>1</v>
       </c>
       <c r="N212" s="3" t="n">
-        <v>46079.7152199074</v>
+        <v>46079.79335648148</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -14260,7 +14270,7 @@
         <v>1</v>
       </c>
       <c r="N213" s="3" t="n">
-        <v>46079.71081018518</v>
+        <v>46079.83048611111</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
@@ -14324,7 +14334,7 @@
         <v>1</v>
       </c>
       <c r="N214" s="3" t="n">
-        <v>46079.7234375</v>
+        <v>46079.80457175926</v>
       </c>
       <c r="O214" t="inlineStr">
         <is>
@@ -14388,7 +14398,7 @@
         <v>1</v>
       </c>
       <c r="N215" s="3" t="n">
-        <v>46079.72015046296</v>
+        <v>46079.80315972222</v>
       </c>
       <c r="O215" t="inlineStr">
         <is>
@@ -14452,7 +14462,7 @@
         <v>1</v>
       </c>
       <c r="N216" s="3" t="n">
-        <v>46079.7246875</v>
+        <v>46079.80461805555</v>
       </c>
       <c r="O216" t="inlineStr">
         <is>
@@ -14471,11 +14481,6 @@
           <t>OPERACAO 8.1</t>
         </is>
       </c>
-      <c r="C217" t="inlineStr">
-        <is>
-          <t>10.69.5.85</t>
-        </is>
-      </c>
       <c r="D217" t="n">
         <v>2017</v>
       </c>
@@ -14516,7 +14521,7 @@
         <v>1</v>
       </c>
       <c r="N217" s="3" t="n">
-        <v>46079.73453703704</v>
+        <v>46079.81326388889</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14580,7 +14585,7 @@
         <v>1</v>
       </c>
       <c r="N218" s="3" t="n">
-        <v>46079.72134259259</v>
+        <v>46080.29625</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14777,7 +14782,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="3" t="n">
-        <v>46079.72886574074</v>
+        <v>46079.81023148148</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14841,7 +14846,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="3" t="n">
-        <v>46079.72856481482</v>
+        <v>46079.80219907407</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -14905,7 +14910,7 @@
         <v>1</v>
       </c>
       <c r="N223" s="3" t="n">
-        <v>46079.71748842593</v>
+        <v>46079.79640046296</v>
       </c>
       <c r="O223" t="inlineStr">
         <is>
@@ -14969,7 +14974,7 @@
         <v>1</v>
       </c>
       <c r="N224" s="3" t="n">
-        <v>46079.71975694445</v>
+        <v>46079.82978009259</v>
       </c>
       <c r="O224" t="inlineStr">
         <is>
@@ -15033,7 +15038,7 @@
         <v>1</v>
       </c>
       <c r="N225" s="3" t="n">
-        <v>46079.7121875</v>
+        <v>46079.82745370371</v>
       </c>
       <c r="O225" t="inlineStr">
         <is>
@@ -15097,7 +15102,7 @@
         <v>1</v>
       </c>
       <c r="N226" s="3" t="n">
-        <v>46079.71391203703</v>
+        <v>46079.8284375</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15161,7 +15166,7 @@
         <v>1</v>
       </c>
       <c r="N227" s="3" t="n">
-        <v>46079.70667824074</v>
+        <v>46079.82400462963</v>
       </c>
       <c r="O227" t="inlineStr">
         <is>
@@ -15225,7 +15230,7 @@
         <v>1</v>
       </c>
       <c r="N228" s="3" t="n">
-        <v>46079.71450231481</v>
+        <v>46079.82949074074</v>
       </c>
       <c r="O228" t="inlineStr">
         <is>
@@ -15289,7 +15294,7 @@
         <v>1</v>
       </c>
       <c r="N229" s="3" t="n">
-        <v>46079.70047453704</v>
+        <v>46079.8172337963</v>
       </c>
       <c r="O229" t="inlineStr">
         <is>
@@ -15353,7 +15358,7 @@
         <v>1</v>
       </c>
       <c r="N230" s="3" t="n">
-        <v>46079.70012731481</v>
+        <v>46080.3202662037</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15417,7 +15422,7 @@
         <v>1</v>
       </c>
       <c r="N231" s="3" t="n">
-        <v>46079.71428240741</v>
+        <v>46079.79586805555</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15481,7 +15486,7 @@
         <v>1</v>
       </c>
       <c r="N232" s="3" t="n">
-        <v>46079.73401620371</v>
+        <v>46079.81185185185</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -15545,7 +15550,7 @@
         <v>1</v>
       </c>
       <c r="N233" s="3" t="n">
-        <v>46079.71525462963</v>
+        <v>46079.78872685185</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15609,7 +15614,7 @@
         <v>1</v>
       </c>
       <c r="N234" s="3" t="n">
-        <v>46079.73405092592</v>
+        <v>46079.81498842593</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -15673,7 +15678,7 @@
         <v>1</v>
       </c>
       <c r="N235" s="3" t="n">
-        <v>46079.73681712963</v>
+        <v>46079.81289351852</v>
       </c>
       <c r="O235" t="inlineStr">
         <is>
@@ -15737,7 +15742,7 @@
         <v>1</v>
       </c>
       <c r="N236" s="3" t="n">
-        <v>46079.73403935185</v>
+        <v>46079.80925925926</v>
       </c>
       <c r="O236" t="inlineStr">
         <is>
@@ -15865,7 +15870,7 @@
         <v>1</v>
       </c>
       <c r="N238" s="3" t="n">
-        <v>46079.70431712963</v>
+        <v>46079.82001157408</v>
       </c>
       <c r="O238" t="inlineStr">
         <is>
@@ -15993,7 +15998,7 @@
         <v>1</v>
       </c>
       <c r="N240" s="3" t="n">
-        <v>46079.73664351852</v>
+        <v>46079.81193287037</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16057,7 +16062,7 @@
         <v>1</v>
       </c>
       <c r="N241" s="3" t="n">
-        <v>46079.73658564815</v>
+        <v>46079.80981481481</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16121,7 +16126,7 @@
         <v>1</v>
       </c>
       <c r="N242" s="3" t="n">
-        <v>46079.70179398148</v>
+        <v>46079.81471064815</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16185,7 +16190,7 @@
         <v>1</v>
       </c>
       <c r="N243" s="3" t="n">
-        <v>46079.71256944445</v>
+        <v>46079.78887731482</v>
       </c>
       <c r="O243" t="inlineStr">
         <is>
@@ -16204,6 +16209,11 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>10.69.5.112</t>
+        </is>
+      </c>
       <c r="D244" t="n">
         <v>2019</v>
       </c>
@@ -16244,7 +16254,7 @@
         <v>1</v>
       </c>
       <c r="N244" s="3" t="n">
-        <v>46079.17092592592</v>
+        <v>46080.23087962963</v>
       </c>
       <c r="O244" t="inlineStr">
         <is>
@@ -16308,7 +16318,7 @@
         <v>1</v>
       </c>
       <c r="N245" s="3" t="n">
-        <v>46079.7080787037</v>
+        <v>46079.8245949074</v>
       </c>
       <c r="O245" t="inlineStr">
         <is>
@@ -16372,7 +16382,7 @@
         <v>1</v>
       </c>
       <c r="N246" s="3" t="n">
-        <v>46079.70784722222</v>
+        <v>46079.82884259259</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16436,7 +16446,7 @@
         <v>1</v>
       </c>
       <c r="N247" s="3" t="n">
-        <v>46079.7375925926</v>
+        <v>46079.81962962963</v>
       </c>
       <c r="O247" t="inlineStr">
         <is>
@@ -16500,7 +16510,7 @@
         <v>1</v>
       </c>
       <c r="N248" s="3" t="n">
-        <v>46079.72039351852</v>
+        <v>46079.79261574074</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16564,7 +16574,7 @@
         <v>1</v>
       </c>
       <c r="N249" s="3" t="n">
-        <v>46079.71885416667</v>
+        <v>46079.75825231482</v>
       </c>
       <c r="O249" t="inlineStr">
         <is>
@@ -16583,11 +16593,6 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
-      <c r="C250" t="inlineStr">
-        <is>
-          <t>10.69.5.118</t>
-        </is>
-      </c>
       <c r="D250" t="n">
         <v>2017</v>
       </c>
@@ -16628,7 +16633,7 @@
         <v>1</v>
       </c>
       <c r="N250" s="3" t="n">
-        <v>46079.72076388889</v>
+        <v>46080.30893518519</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16692,7 +16697,7 @@
         <v>1</v>
       </c>
       <c r="N251" s="3" t="n">
-        <v>46079.71620370371</v>
+        <v>46079.79591435185</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16756,7 +16761,7 @@
         <v>1</v>
       </c>
       <c r="N252" s="3" t="n">
-        <v>46079.70997685185</v>
+        <v>46079.78913194445</v>
       </c>
       <c r="O252" t="inlineStr">
         <is>
@@ -16820,7 +16825,7 @@
         <v>1</v>
       </c>
       <c r="N253" s="3" t="n">
-        <v>46079.73636574074</v>
+        <v>46079.81583333333</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16878,7 +16883,7 @@
         <v>1</v>
       </c>
       <c r="N254" s="3" t="n">
-        <v>46079.71046296296</v>
+        <v>46079.83004629629</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -16942,7 +16947,7 @@
         <v>1</v>
       </c>
       <c r="N255" s="3" t="n">
-        <v>46079.58980324074</v>
+        <v>46079.80324074074</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -17006,7 +17011,7 @@
         <v>1</v>
       </c>
       <c r="N256" s="3" t="n">
-        <v>46079.73050925926</v>
+        <v>46079.80778935185</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17070,7 +17075,7 @@
         <v>1</v>
       </c>
       <c r="N257" s="3" t="n">
-        <v>46079.73525462963</v>
+        <v>46079.81305555555</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17134,7 +17139,7 @@
         <v>1</v>
       </c>
       <c r="N258" s="3" t="n">
-        <v>46079.72193287037</v>
+        <v>46079.80392361111</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
@@ -17198,7 +17203,7 @@
         <v>1</v>
       </c>
       <c r="N259" s="3" t="n">
-        <v>46079.72855324074</v>
+        <v>46079.80809027778</v>
       </c>
       <c r="O259" t="inlineStr">
         <is>
@@ -17326,7 +17331,7 @@
         <v>1</v>
       </c>
       <c r="N261" s="3" t="n">
-        <v>46079.73284722222</v>
+        <v>46079.82717592592</v>
       </c>
       <c r="O261" t="inlineStr">
         <is>
@@ -17390,7 +17395,7 @@
         <v>1</v>
       </c>
       <c r="N262" s="3" t="n">
-        <v>46079.70824074074</v>
+        <v>46079.81940972222</v>
       </c>
       <c r="O262" t="inlineStr">
         <is>
@@ -17454,7 +17459,7 @@
         <v>1</v>
       </c>
       <c r="N263" s="3" t="n">
-        <v>46079.70553240741</v>
+        <v>46079.81905092593</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17518,7 +17523,7 @@
         <v>1</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>46079.73064814815</v>
+        <v>46079.81013888889</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17582,7 +17587,7 @@
         <v>1</v>
       </c>
       <c r="N265" s="3" t="n">
-        <v>46079.70332175926</v>
+        <v>46079.82109953704</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17646,7 +17651,7 @@
         <v>1</v>
       </c>
       <c r="N266" s="3" t="n">
-        <v>46079.72761574074</v>
+        <v>46079.84724537037</v>
       </c>
       <c r="O266" t="inlineStr">
         <is>
@@ -17710,7 +17715,7 @@
         <v>1</v>
       </c>
       <c r="N267" s="3" t="n">
-        <v>46079.72100694444</v>
+        <v>46079.79821759259</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17774,7 +17779,7 @@
         <v>1</v>
       </c>
       <c r="N268" s="3" t="n">
-        <v>46079.72413194444</v>
+        <v>46079.80445601852</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17838,7 +17843,7 @@
         <v>1</v>
       </c>
       <c r="N269" s="3" t="n">
-        <v>46079.71319444444</v>
+        <v>46079.86325231481</v>
       </c>
       <c r="O269" t="inlineStr">
         <is>
@@ -17899,7 +17904,7 @@
         </is>
       </c>
       <c r="N270" s="3" t="n">
-        <v>46079.70202546296</v>
+        <v>46080.30166666667</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -17963,7 +17968,7 @@
         <v>1</v>
       </c>
       <c r="N271" s="3" t="n">
-        <v>46079.2383449074</v>
+        <v>46080.08175925926</v>
       </c>
       <c r="O271" t="inlineStr">
         <is>
@@ -18411,7 +18416,7 @@
         <v>1</v>
       </c>
       <c r="N278" s="3" t="n">
-        <v>46079.55091435185</v>
+        <v>46080.31898148148</v>
       </c>
       <c r="O278" t="inlineStr">
         <is>
@@ -18475,7 +18480,7 @@
         <v>1</v>
       </c>
       <c r="N279" s="3" t="n">
-        <v>46079.72244212963</v>
+        <v>46080.3037962963</v>
       </c>
       <c r="O279" t="inlineStr">
         <is>
@@ -18539,7 +18544,7 @@
         <v>1</v>
       </c>
       <c r="N280" s="3" t="n">
-        <v>46079.70355324074</v>
+        <v>46079.8146412037</v>
       </c>
       <c r="O280" t="inlineStr">
         <is>
@@ -18603,7 +18608,7 @@
         <v>1</v>
       </c>
       <c r="N281" s="3" t="n">
-        <v>46079.71649305556</v>
+        <v>46079.87063657407</v>
       </c>
       <c r="O281" t="inlineStr">
         <is>
@@ -18622,6 +18627,11 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>10.69.5.151</t>
+        </is>
+      </c>
       <c r="D282" t="n">
         <v>2017</v>
       </c>
@@ -18662,7 +18672,7 @@
         <v>1</v>
       </c>
       <c r="N282" s="3" t="n">
-        <v>46079.56299768519</v>
+        <v>46080.31703703704</v>
       </c>
       <c r="O282" t="inlineStr">
         <is>
@@ -18726,7 +18736,7 @@
         <v>1</v>
       </c>
       <c r="N283" s="3" t="n">
-        <v>46079.73575231482</v>
+        <v>46079.81559027778</v>
       </c>
       <c r="O283" t="inlineStr">
         <is>
@@ -18790,7 +18800,7 @@
         <v>1</v>
       </c>
       <c r="N284" s="3" t="n">
-        <v>46079.72288194444</v>
+        <v>46079.80465277778</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18854,7 +18864,7 @@
         <v>1</v>
       </c>
       <c r="N285" s="3" t="n">
-        <v>46079.72607638889</v>
+        <v>46079.80431712963</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -18913,7 +18923,7 @@
         <v>1</v>
       </c>
       <c r="N286" s="3" t="n">
-        <v>46079.58777777778</v>
+        <v>46080.17166666667</v>
       </c>
       <c r="O286" t="inlineStr">
         <is>
@@ -18977,7 +18987,7 @@
         <v>1</v>
       </c>
       <c r="N287" s="3" t="n">
-        <v>46079.72891203704</v>
+        <v>46079.80842592593</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
@@ -19041,7 +19051,7 @@
         <v>1</v>
       </c>
       <c r="N288" s="3" t="n">
-        <v>46079.5597337963</v>
+        <v>46080.31662037037</v>
       </c>
       <c r="O288" t="inlineStr">
         <is>
@@ -19105,7 +19115,7 @@
         <v>1</v>
       </c>
       <c r="N289" s="3" t="n">
-        <v>46079.70324074074</v>
+        <v>46079.85931712963</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -19899,7 +19909,7 @@
         <v>1</v>
       </c>
       <c r="N302" s="3" t="n">
-        <v>46079.70971064815</v>
+        <v>46080.31326388889</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -21015,7 +21025,7 @@
         </is>
       </c>
       <c r="N320" s="3" t="n">
-        <v>46079.72775462963</v>
+        <v>46080.30824074074</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21740,7 +21750,7 @@
         <v>1</v>
       </c>
       <c r="N332" s="3" t="n">
-        <v>46079.71637731481</v>
+        <v>46079.7544212963</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21804,7 +21814,7 @@
         <v>2</v>
       </c>
       <c r="N333" s="3" t="n">
-        <v>46079.70217592592</v>
+        <v>46080.28355324074</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21868,7 +21878,7 @@
         <v>2</v>
       </c>
       <c r="N334" s="3" t="n">
-        <v>46079.71271990741</v>
+        <v>46080.28387731482</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21932,7 +21942,7 @@
         <v>2</v>
       </c>
       <c r="N335" s="3" t="n">
-        <v>46079.69729166666</v>
+        <v>46080.28358796296</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -21996,7 +22006,7 @@
         <v>1</v>
       </c>
       <c r="N336" s="3" t="n">
-        <v>46079.66770833333</v>
+        <v>46080.28539351852</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22060,7 +22070,7 @@
         <v>1</v>
       </c>
       <c r="N337" s="3" t="n">
-        <v>46079.73407407408</v>
+        <v>46080.28399305556</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22124,7 +22134,7 @@
         <v>2</v>
       </c>
       <c r="N338" s="3" t="n">
-        <v>46079.70646990741</v>
+        <v>46080.28365740741</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -22188,7 +22198,7 @@
         <v>2</v>
       </c>
       <c r="N339" s="3" t="n">
-        <v>46079.71229166666</v>
+        <v>46080.30105324074</v>
       </c>
       <c r="O339" t="inlineStr">
         <is>
@@ -22948,7 +22958,7 @@
         <v>1</v>
       </c>
       <c r="N351" s="3" t="n">
-        <v>46079.71148148148</v>
+        <v>46079.86789351852</v>
       </c>
       <c r="O351" t="inlineStr">
         <is>
@@ -23892,7 +23902,7 @@
         </is>
       </c>
       <c r="N366" s="3" t="n">
-        <v>46079.71809027778</v>
+        <v>46080.30050925926</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -24018,7 +24028,7 @@
         </is>
       </c>
       <c r="N368" s="3" t="n">
-        <v>46079.7078587963</v>
+        <v>46080.31581018519</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -24037,11 +24047,6 @@
           <t>RH</t>
         </is>
       </c>
-      <c r="C369" t="inlineStr">
-        <is>
-          <t>10.69.3.13</t>
-        </is>
-      </c>
       <c r="D369" t="n">
         <v>2025</v>
       </c>
@@ -24153,7 +24158,7 @@
         <v>1</v>
       </c>
       <c r="N370" s="3" t="n">
-        <v>46079.70358796296</v>
+        <v>46079.78256944445</v>
       </c>
       <c r="O370" t="inlineStr">
         <is>
@@ -24426,7 +24431,7 @@
         <v>1</v>
       </c>
       <c r="N374" s="3" t="n">
-        <v>46079.70917824074</v>
+        <v>46079.75130787037</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24511,11 +24516,6 @@
           <t>COORDENACAO</t>
         </is>
       </c>
-      <c r="C376" t="inlineStr">
-        <is>
-          <t>10.69.3.72</t>
-        </is>
-      </c>
       <c r="D376" t="n">
         <v>2025</v>
       </c>
@@ -24561,7 +24561,7 @@
         <v>1</v>
       </c>
       <c r="N376" s="3" t="n">
-        <v>46079.71738425926</v>
+        <v>46080.29885416666</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -24630,7 +24630,7 @@
         <v>2</v>
       </c>
       <c r="N377" s="3" t="n">
-        <v>46079.71207175926</v>
+        <v>46079.74957175926</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -24699,7 +24699,7 @@
         <v>2</v>
       </c>
       <c r="N378" s="3" t="n">
-        <v>46079.70734953704</v>
+        <v>46080.32064814815</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização automática 2026-02-27 09:52:09.991398
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>46080.29556712963</v>
+        <v>46080.36765046296</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>46080.314375</v>
+        <v>46080.39267361111</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
         <v>1</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>46079.67033564814</v>
+        <v>46080.37395833333</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>46079.64631944444</v>
+        <v>46080.38234953704</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -1259,7 +1259,7 @@
         <v>1</v>
       </c>
       <c r="N12" s="3" t="n">
-        <v>46080.31922453704</v>
+        <v>46080.40229166667</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1323,7 +1323,7 @@
         <v>1</v>
       </c>
       <c r="N13" s="3" t="n">
-        <v>46078.7371875</v>
+        <v>46080.39877314815</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1387,7 +1387,7 @@
         <v>2</v>
       </c>
       <c r="N14" s="3" t="n">
-        <v>46078.73407407408</v>
+        <v>46080.4034375</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1515,7 +1515,7 @@
         <v>2</v>
       </c>
       <c r="N16" s="3" t="n">
-        <v>46080.30274305555</v>
+        <v>46080.37883101852</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1579,7 +1579,7 @@
         <v>1</v>
       </c>
       <c r="N17" s="3" t="n">
-        <v>46080.3121875</v>
+        <v>46080.40078703704</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1643,7 +1643,7 @@
         <v>2</v>
       </c>
       <c r="N18" s="3" t="n">
-        <v>46080.29148148148</v>
+        <v>46080.40098379629</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1768,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="N20" s="3" t="n">
-        <v>46080.31166666667</v>
+        <v>46080.38796296297</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1950,7 +1950,7 @@
         <v>1</v>
       </c>
       <c r="N23" s="3" t="n">
-        <v>46080.10675925926</v>
+        <v>46080.38017361111</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2009,7 +2009,7 @@
         <v>1</v>
       </c>
       <c r="N24" s="3" t="n">
-        <v>46079.60684027777</v>
+        <v>46080.3716087963</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2065,7 +2065,7 @@
         </is>
       </c>
       <c r="N25" s="3" t="n">
-        <v>46063.72092592593</v>
+        <v>46080.39040509259</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -2143,6 +2143,11 @@
           <t>AUDITORIO</t>
         </is>
       </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>10.69.3.151</t>
+        </is>
+      </c>
       <c r="D27" t="n">
         <v>2019</v>
       </c>
@@ -2183,7 +2188,7 @@
         <v>1</v>
       </c>
       <c r="N27" s="3" t="n">
-        <v>46078.72754629629</v>
+        <v>46080.39244212963</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -6570,7 +6575,7 @@
         <v>1</v>
       </c>
       <c r="N95" s="3" t="n">
-        <v>46079.82608796296</v>
+        <v>46080.37099537037</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -6703,7 +6708,7 @@
         <v>1</v>
       </c>
       <c r="N97" s="3" t="n">
-        <v>46079.68333333333</v>
+        <v>46080.36945601852</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -6767,7 +6772,7 @@
         <v>1</v>
       </c>
       <c r="N98" s="3" t="n">
-        <v>46079.6834837963</v>
+        <v>46080.37287037037</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -6836,7 +6841,7 @@
         <v>1</v>
       </c>
       <c r="N99" s="3" t="n">
-        <v>46079.70041666667</v>
+        <v>46080.38021990741</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -6905,7 +6910,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>46080.31297453704</v>
+        <v>46080.39115740741</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6974,7 +6979,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="3" t="n">
-        <v>46079.81753472222</v>
+        <v>46080.37886574074</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -7112,7 +7117,7 @@
         <v>2</v>
       </c>
       <c r="N103" s="3" t="n">
-        <v>46080.28097222222</v>
+        <v>46080.39851851852</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7510,7 +7515,7 @@
         <v>1</v>
       </c>
       <c r="N109" s="3" t="n">
-        <v>46080.29549768518</v>
+        <v>46080.37085648148</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7579,7 +7584,7 @@
         <v>2</v>
       </c>
       <c r="N110" s="3" t="n">
-        <v>46080.28954861111</v>
+        <v>46080.365</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7648,7 +7653,7 @@
         <v>2</v>
       </c>
       <c r="N111" s="3" t="n">
-        <v>46080.31909722222</v>
+        <v>46080.40094907407</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
@@ -7717,7 +7722,7 @@
         <v>2</v>
       </c>
       <c r="N112" s="3" t="n">
-        <v>46080.31684027778</v>
+        <v>46080.39350694444</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7786,7 +7791,7 @@
         <v>1</v>
       </c>
       <c r="N113" s="3" t="n">
-        <v>46080.28915509259</v>
+        <v>46080.36824074074</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7855,7 +7860,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>46080.29603009259</v>
+        <v>46080.37372685185</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -7921,7 +7926,7 @@
         </is>
       </c>
       <c r="N115" s="3" t="n">
-        <v>46079.68575231481</v>
+        <v>46080.37569444445</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -7990,7 +7995,7 @@
         <v>1</v>
       </c>
       <c r="N116" s="3" t="n">
-        <v>46079.68635416667</v>
+        <v>46080.37627314815</v>
       </c>
       <c r="O116" t="inlineStr">
         <is>
@@ -8059,7 +8064,7 @@
         <v>1</v>
       </c>
       <c r="N117" s="3" t="n">
-        <v>46080.32011574074</v>
+        <v>46080.39326388889</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -8125,7 +8130,7 @@
         </is>
       </c>
       <c r="N118" s="3" t="n">
-        <v>46079.72672453704</v>
+        <v>46080.37770833333</v>
       </c>
       <c r="O118" t="inlineStr">
         <is>
@@ -8263,7 +8268,7 @@
         <v>1</v>
       </c>
       <c r="N120" s="3" t="n">
-        <v>46080.29375</v>
+        <v>46080.36945601852</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -8398,7 +8403,7 @@
         </is>
       </c>
       <c r="N122" s="3" t="n">
-        <v>46079.7866087963</v>
+        <v>46080.36865740741</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -8536,7 +8541,7 @@
         <v>1</v>
       </c>
       <c r="N124" s="3" t="n">
-        <v>46080.31997685185</v>
+        <v>46080.40225694444</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -8605,7 +8610,7 @@
         <v>1</v>
       </c>
       <c r="N125" s="3" t="n">
-        <v>46080.28650462963</v>
+        <v>46080.36364583333</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -8743,7 +8748,7 @@
         <v>2</v>
       </c>
       <c r="N127" s="3" t="n">
-        <v>46080.30769675926</v>
+        <v>46080.38659722222</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -8812,7 +8817,7 @@
         <v>1</v>
       </c>
       <c r="N128" s="3" t="n">
-        <v>46079.67697916667</v>
+        <v>46080.37311342593</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -8950,7 +8955,7 @@
         <v>1</v>
       </c>
       <c r="N130" s="3" t="n">
-        <v>46079.77684027778</v>
+        <v>46080.37387731481</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -9019,7 +9024,7 @@
         <v>1</v>
       </c>
       <c r="N131" s="3" t="n">
-        <v>46080.31950231481</v>
+        <v>46080.39912037037</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -9152,7 +9157,7 @@
         <v>1</v>
       </c>
       <c r="N133" s="3" t="n">
-        <v>46079.81851851852</v>
+        <v>46080.37106481481</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -9471,7 +9476,7 @@
         <v>1</v>
       </c>
       <c r="N138" s="3" t="n">
-        <v>46079.81016203704</v>
+        <v>46080.37650462963</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9535,7 +9540,7 @@
         <v>1</v>
       </c>
       <c r="N139" s="3" t="n">
-        <v>46079.81265046296</v>
+        <v>46080.37484953704</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9599,7 +9604,7 @@
         <v>1</v>
       </c>
       <c r="N140" s="3" t="n">
-        <v>46079.82202546296</v>
+        <v>46080.37309027778</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9663,7 +9668,7 @@
         <v>1</v>
       </c>
       <c r="N141" s="3" t="n">
-        <v>46079.8047337963</v>
+        <v>46080.37251157407</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9727,7 +9732,7 @@
         <v>1</v>
       </c>
       <c r="N142" s="3" t="n">
-        <v>46079.82223379629</v>
+        <v>46080.37215277777</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9855,7 +9860,7 @@
         <v>1</v>
       </c>
       <c r="N144" s="3" t="n">
-        <v>46079.81663194444</v>
+        <v>46080.3874074074</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9983,7 +9988,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="3" t="n">
-        <v>46079.8159375</v>
+        <v>46080.36858796296</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10047,7 +10052,7 @@
         <v>1</v>
       </c>
       <c r="N147" s="3" t="n">
-        <v>46079.7934837963</v>
+        <v>46080.40246527778</v>
       </c>
       <c r="O147" t="inlineStr">
         <is>
@@ -10111,7 +10116,7 @@
         <v>1</v>
       </c>
       <c r="N148" s="3" t="n">
-        <v>46079.80366898148</v>
+        <v>46080.37829861111</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10239,7 +10244,7 @@
         <v>1</v>
       </c>
       <c r="N150" s="3" t="n">
-        <v>46079.7537037037</v>
+        <v>46080.37076388889</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -10303,7 +10308,7 @@
         <v>1</v>
       </c>
       <c r="N151" s="3" t="n">
-        <v>46079.80550925926</v>
+        <v>46080.38425925926</v>
       </c>
       <c r="O151" t="inlineStr">
         <is>
@@ -10367,7 +10372,7 @@
         <v>1</v>
       </c>
       <c r="N152" s="3" t="n">
-        <v>46079.69537037037</v>
+        <v>46080.37346064814</v>
       </c>
       <c r="O152" t="inlineStr">
         <is>
@@ -10386,11 +10391,6 @@
           <t>OPERACAO 7.1</t>
         </is>
       </c>
-      <c r="C153" t="inlineStr">
-        <is>
-          <t>10.69.5.21</t>
-        </is>
-      </c>
       <c r="D153" t="n">
         <v>2018</v>
       </c>
@@ -10495,7 +10495,7 @@
         <v>1</v>
       </c>
       <c r="N154" s="3" t="n">
-        <v>46080.31497685185</v>
+        <v>46080.39429398148</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10559,7 +10559,7 @@
         <v>1</v>
       </c>
       <c r="N155" s="3" t="n">
-        <v>46079.79131944444</v>
+        <v>46080.37458333333</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10623,7 +10623,7 @@
         <v>1</v>
       </c>
       <c r="N156" s="3" t="n">
-        <v>46079.81130787037</v>
+        <v>46080.36940972223</v>
       </c>
       <c r="O156" t="inlineStr">
         <is>
@@ -10687,7 +10687,7 @@
         <v>1</v>
       </c>
       <c r="N157" s="3" t="n">
-        <v>46079.57226851852</v>
+        <v>46080.37290509259</v>
       </c>
       <c r="O157" t="inlineStr">
         <is>
@@ -10751,7 +10751,7 @@
         <v>1</v>
       </c>
       <c r="N158" s="3" t="n">
-        <v>46080.3127662037</v>
+        <v>46080.3871875</v>
       </c>
       <c r="O158" t="inlineStr">
         <is>
@@ -10815,7 +10815,7 @@
         <v>1</v>
       </c>
       <c r="N159" s="3" t="n">
-        <v>46080.31447916666</v>
+        <v>46080.38908564814</v>
       </c>
       <c r="O159" t="inlineStr">
         <is>
@@ -10879,7 +10879,7 @@
         <v>1</v>
       </c>
       <c r="N160" s="3" t="n">
-        <v>46079.79456018518</v>
+        <v>46080.36987268519</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
@@ -10943,7 +10943,7 @@
         <v>1</v>
       </c>
       <c r="N161" s="3" t="n">
-        <v>46079.80791666666</v>
+        <v>46080.37319444444</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -11007,7 +11007,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="3" t="n">
-        <v>46079.79564814815</v>
+        <v>46080.3959837963</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11132,10 +11132,10 @@
         </is>
       </c>
       <c r="M164" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N164" s="3" t="n">
-        <v>46080.28221064815</v>
+        <v>46080.36446759259</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11199,7 +11199,7 @@
         <v>2</v>
       </c>
       <c r="N165" s="3" t="n">
-        <v>46079.56068287037</v>
+        <v>46080.36883101852</v>
       </c>
       <c r="O165" t="inlineStr">
         <is>
@@ -11263,7 +11263,7 @@
         <v>2</v>
       </c>
       <c r="N166" s="3" t="n">
-        <v>46079.60831018518</v>
+        <v>46080.38336805555</v>
       </c>
       <c r="O166" t="inlineStr">
         <is>
@@ -11327,7 +11327,7 @@
         <v>2</v>
       </c>
       <c r="N167" s="3" t="n">
-        <v>46079.59871527777</v>
+        <v>46080.40265046297</v>
       </c>
       <c r="O167" t="inlineStr">
         <is>
@@ -11391,7 +11391,7 @@
         <v>2</v>
       </c>
       <c r="N168" s="3" t="n">
-        <v>46080.31921296296</v>
+        <v>46080.39711805555</v>
       </c>
       <c r="O168" t="inlineStr">
         <is>
@@ -11519,7 +11519,7 @@
         <v>2</v>
       </c>
       <c r="N170" s="3" t="n">
-        <v>46080.30814814815</v>
+        <v>46080.38101851852</v>
       </c>
       <c r="O170" t="inlineStr">
         <is>
@@ -11580,10 +11580,10 @@
         </is>
       </c>
       <c r="M171" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N171" s="3" t="n">
-        <v>46080.28824074074</v>
+        <v>46080.40368055556</v>
       </c>
       <c r="O171" t="inlineStr">
         <is>
@@ -11711,7 +11711,7 @@
         <v>1</v>
       </c>
       <c r="N173" s="3" t="n">
-        <v>46080.30158564815</v>
+        <v>46080.38402777778</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -11775,7 +11775,7 @@
         <v>2</v>
       </c>
       <c r="N174" s="3" t="n">
-        <v>46079.55133101852</v>
+        <v>46080.38055555556</v>
       </c>
       <c r="O174" t="inlineStr">
         <is>
@@ -11839,7 +11839,7 @@
         <v>2</v>
       </c>
       <c r="N175" s="3" t="n">
-        <v>46080.30027777778</v>
+        <v>46080.37818287037</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -11903,7 +11903,7 @@
         <v>2</v>
       </c>
       <c r="N176" s="3" t="n">
-        <v>46080.29123842593</v>
+        <v>46080.4025925926</v>
       </c>
       <c r="O176" t="inlineStr">
         <is>
@@ -12031,7 +12031,7 @@
         <v>2</v>
       </c>
       <c r="N178" s="3" t="n">
-        <v>46080.3203587963</v>
+        <v>46080.3987037037</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12095,7 +12095,7 @@
         <v>1</v>
       </c>
       <c r="N179" s="3" t="n">
-        <v>46080.31607638889</v>
+        <v>46080.39746527778</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12159,7 +12159,7 @@
         <v>1</v>
       </c>
       <c r="N180" s="3" t="n">
-        <v>46080.31592592593</v>
+        <v>46080.39327546296</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12351,7 +12351,7 @@
         <v>1</v>
       </c>
       <c r="N183" s="3" t="n">
-        <v>46080.28488425926</v>
+        <v>46080.39916666667</v>
       </c>
       <c r="O183" t="inlineStr">
         <is>
@@ -12420,7 +12420,7 @@
         <v>2</v>
       </c>
       <c r="N184" s="3" t="n">
-        <v>46080.28256944445</v>
+        <v>46080.39745370371</v>
       </c>
       <c r="O184" t="inlineStr">
         <is>
@@ -12548,7 +12548,7 @@
         <v>1</v>
       </c>
       <c r="N186" s="3" t="n">
-        <v>46079.60418981482</v>
+        <v>46080.36486111111</v>
       </c>
       <c r="O186" t="inlineStr">
         <is>
@@ -12612,7 +12612,7 @@
         <v>1</v>
       </c>
       <c r="N187" s="3" t="n">
-        <v>46079.5681712963</v>
+        <v>46080.3965625</v>
       </c>
       <c r="O187" t="inlineStr">
         <is>
@@ -12676,7 +12676,7 @@
         <v>1</v>
       </c>
       <c r="N188" s="3" t="n">
-        <v>46080.29646990741</v>
+        <v>46080.37136574074</v>
       </c>
       <c r="O188" t="inlineStr">
         <is>
@@ -12804,7 +12804,7 @@
         </is>
       </c>
       <c r="N190" s="3" t="n">
-        <v>46080.31819444444</v>
+        <v>46080.38706018519</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12932,7 +12932,7 @@
         <v>1</v>
       </c>
       <c r="N192" s="3" t="n">
-        <v>46079.79903935185</v>
+        <v>46080.39361111111</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -13057,7 +13057,7 @@
         <v>2</v>
       </c>
       <c r="N194" s="3" t="n">
-        <v>46079.9927662037</v>
+        <v>46080.3684375</v>
       </c>
       <c r="O194" t="inlineStr">
         <is>
@@ -13121,7 +13121,7 @@
         <v>1</v>
       </c>
       <c r="N195" s="3" t="n">
-        <v>46079.83634259259</v>
+        <v>46080.37892361111</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13185,7 +13185,7 @@
         <v>1</v>
       </c>
       <c r="N196" s="3" t="n">
-        <v>46079.81520833333</v>
+        <v>46080.38236111111</v>
       </c>
       <c r="O196" t="inlineStr">
         <is>
@@ -13313,7 +13313,7 @@
         <v>1</v>
       </c>
       <c r="N198" s="3" t="n">
-        <v>46079.8665625</v>
+        <v>46080.37958333334</v>
       </c>
       <c r="O198" t="inlineStr">
         <is>
@@ -13377,7 +13377,7 @@
         <v>1</v>
       </c>
       <c r="N199" s="3" t="n">
-        <v>46080.28875</v>
+        <v>46080.36868055556</v>
       </c>
       <c r="O199" t="inlineStr">
         <is>
@@ -13441,7 +13441,7 @@
         <v>1</v>
       </c>
       <c r="N200" s="3" t="n">
-        <v>46078.79266203703</v>
+        <v>46080.39163194445</v>
       </c>
       <c r="O200" t="inlineStr">
         <is>
@@ -13502,7 +13502,7 @@
         </is>
       </c>
       <c r="N201" s="3" t="n">
-        <v>46079.81636574074</v>
+        <v>46080.40106481482</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -13566,7 +13566,7 @@
         <v>1</v>
       </c>
       <c r="N202" s="3" t="n">
-        <v>46079.81935185185</v>
+        <v>46080.40204861111</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13630,7 +13630,7 @@
         <v>1</v>
       </c>
       <c r="N203" s="3" t="n">
-        <v>46079.81766203704</v>
+        <v>46080.3786574074</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13694,7 +13694,7 @@
         <v>1</v>
       </c>
       <c r="N204" s="3" t="n">
-        <v>46079.81115740741</v>
+        <v>46080.39340277778</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13758,7 +13758,7 @@
         <v>1</v>
       </c>
       <c r="N205" s="3" t="n">
-        <v>46079.8190625</v>
+        <v>46080.37083333333</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13822,7 +13822,7 @@
         <v>1</v>
       </c>
       <c r="N206" s="3" t="n">
-        <v>46079.8059375</v>
+        <v>46080.37386574074</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -13886,7 +13886,7 @@
         <v>1</v>
       </c>
       <c r="N207" s="3" t="n">
-        <v>46080.30528935185</v>
+        <v>46080.38532407407</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -13950,7 +13950,7 @@
         <v>1</v>
       </c>
       <c r="N208" s="3" t="n">
-        <v>46079.57876157408</v>
+        <v>46080.38958333333</v>
       </c>
       <c r="O208" t="inlineStr">
         <is>
@@ -14014,7 +14014,7 @@
         <v>1</v>
       </c>
       <c r="N209" s="3" t="n">
-        <v>46079.80993055556</v>
+        <v>46080.37030092593</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14078,7 +14078,7 @@
         <v>1</v>
       </c>
       <c r="N210" s="3" t="n">
-        <v>46079.84193287037</v>
+        <v>46080.36388888889</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14142,7 +14142,7 @@
         <v>1</v>
       </c>
       <c r="N211" s="3" t="n">
-        <v>46079.65694444445</v>
+        <v>46080.36549768518</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -14206,7 +14206,7 @@
         <v>1</v>
       </c>
       <c r="N212" s="3" t="n">
-        <v>46079.79335648148</v>
+        <v>46080.4030324074</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -14270,7 +14270,7 @@
         <v>1</v>
       </c>
       <c r="N213" s="3" t="n">
-        <v>46079.83048611111</v>
+        <v>46080.38321759259</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
@@ -14334,7 +14334,7 @@
         <v>1</v>
       </c>
       <c r="N214" s="3" t="n">
-        <v>46079.80457175926</v>
+        <v>46080.39730324074</v>
       </c>
       <c r="O214" t="inlineStr">
         <is>
@@ -14398,7 +14398,7 @@
         <v>1</v>
       </c>
       <c r="N215" s="3" t="n">
-        <v>46079.80315972222</v>
+        <v>46080.39803240741</v>
       </c>
       <c r="O215" t="inlineStr">
         <is>
@@ -14462,7 +14462,7 @@
         <v>1</v>
       </c>
       <c r="N216" s="3" t="n">
-        <v>46079.80461805555</v>
+        <v>46080.40012731482</v>
       </c>
       <c r="O216" t="inlineStr">
         <is>
@@ -14481,6 +14481,11 @@
           <t>OPERACAO 8.1</t>
         </is>
       </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>10.69.5.85</t>
+        </is>
+      </c>
       <c r="D217" t="n">
         <v>2017</v>
       </c>
@@ -14521,7 +14526,7 @@
         <v>1</v>
       </c>
       <c r="N217" s="3" t="n">
-        <v>46079.81326388889</v>
+        <v>46080.40179398148</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14585,7 +14590,7 @@
         <v>1</v>
       </c>
       <c r="N218" s="3" t="n">
-        <v>46080.29625</v>
+        <v>46080.37081018519</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14649,7 +14654,7 @@
         <v>1</v>
       </c>
       <c r="N219" s="3" t="n">
-        <v>46079.70515046296</v>
+        <v>46080.3232175926</v>
       </c>
       <c r="O219" t="inlineStr">
         <is>
@@ -14718,7 +14723,7 @@
         <v>1</v>
       </c>
       <c r="N220" s="3" t="n">
-        <v>46079.72834490741</v>
+        <v>46080.36267361111</v>
       </c>
       <c r="O220" t="inlineStr">
         <is>
@@ -14782,7 +14787,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="3" t="n">
-        <v>46079.81023148148</v>
+        <v>46080.37655092592</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14846,7 +14851,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="3" t="n">
-        <v>46079.80219907407</v>
+        <v>46080.38730324074</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -14910,7 +14915,7 @@
         <v>1</v>
       </c>
       <c r="N223" s="3" t="n">
-        <v>46079.79640046296</v>
+        <v>46080.37760416666</v>
       </c>
       <c r="O223" t="inlineStr">
         <is>
@@ -15102,7 +15107,7 @@
         <v>1</v>
       </c>
       <c r="N226" s="3" t="n">
-        <v>46079.8284375</v>
+        <v>46080.39855324074</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15166,7 +15171,7 @@
         <v>1</v>
       </c>
       <c r="N227" s="3" t="n">
-        <v>46079.82400462963</v>
+        <v>46080.39767361111</v>
       </c>
       <c r="O227" t="inlineStr">
         <is>
@@ -15230,7 +15235,7 @@
         <v>1</v>
       </c>
       <c r="N228" s="3" t="n">
-        <v>46079.82949074074</v>
+        <v>46080.38738425926</v>
       </c>
       <c r="O228" t="inlineStr">
         <is>
@@ -15294,7 +15299,7 @@
         <v>1</v>
       </c>
       <c r="N229" s="3" t="n">
-        <v>46079.8172337963</v>
+        <v>46080.40356481481</v>
       </c>
       <c r="O229" t="inlineStr">
         <is>
@@ -15358,7 +15363,7 @@
         <v>1</v>
       </c>
       <c r="N230" s="3" t="n">
-        <v>46080.3202662037</v>
+        <v>46080.39807870371</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15422,7 +15427,7 @@
         <v>1</v>
       </c>
       <c r="N231" s="3" t="n">
-        <v>46079.79586805555</v>
+        <v>46080.38127314814</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15486,7 +15491,7 @@
         <v>1</v>
       </c>
       <c r="N232" s="3" t="n">
-        <v>46079.81185185185</v>
+        <v>46080.37523148148</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -15550,7 +15555,7 @@
         <v>1</v>
       </c>
       <c r="N233" s="3" t="n">
-        <v>46079.78872685185</v>
+        <v>46080.37386574074</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15614,7 +15619,7 @@
         <v>1</v>
       </c>
       <c r="N234" s="3" t="n">
-        <v>46079.81498842593</v>
+        <v>46080.37746527778</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -15678,7 +15683,7 @@
         <v>1</v>
       </c>
       <c r="N235" s="3" t="n">
-        <v>46079.81289351852</v>
+        <v>46080.39731481481</v>
       </c>
       <c r="O235" t="inlineStr">
         <is>
@@ -15870,7 +15875,7 @@
         <v>1</v>
       </c>
       <c r="N238" s="3" t="n">
-        <v>46079.82001157408</v>
+        <v>46080.39987268519</v>
       </c>
       <c r="O238" t="inlineStr">
         <is>
@@ -15934,7 +15939,7 @@
         <v>1</v>
       </c>
       <c r="N239" s="3" t="n">
-        <v>46079.58893518519</v>
+        <v>46080.37438657408</v>
       </c>
       <c r="O239" t="inlineStr">
         <is>
@@ -15998,7 +16003,7 @@
         <v>1</v>
       </c>
       <c r="N240" s="3" t="n">
-        <v>46079.81193287037</v>
+        <v>46080.37405092592</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16062,7 +16067,7 @@
         <v>1</v>
       </c>
       <c r="N241" s="3" t="n">
-        <v>46079.80981481481</v>
+        <v>46080.38453703704</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16126,7 +16131,7 @@
         <v>1</v>
       </c>
       <c r="N242" s="3" t="n">
-        <v>46079.81471064815</v>
+        <v>46080.38105324074</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16209,11 +16214,6 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
-      <c r="C244" t="inlineStr">
-        <is>
-          <t>10.69.5.112</t>
-        </is>
-      </c>
       <c r="D244" t="n">
         <v>2019</v>
       </c>
@@ -16382,7 +16382,7 @@
         <v>1</v>
       </c>
       <c r="N246" s="3" t="n">
-        <v>46079.82884259259</v>
+        <v>46080.37559027778</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16446,7 +16446,7 @@
         <v>1</v>
       </c>
       <c r="N247" s="3" t="n">
-        <v>46079.81962962963</v>
+        <v>46080.37290509259</v>
       </c>
       <c r="O247" t="inlineStr">
         <is>
@@ -16510,7 +16510,7 @@
         <v>1</v>
       </c>
       <c r="N248" s="3" t="n">
-        <v>46079.79261574074</v>
+        <v>46080.39711805555</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16633,7 +16633,7 @@
         <v>1</v>
       </c>
       <c r="N250" s="3" t="n">
-        <v>46080.30893518519</v>
+        <v>46080.3866087963</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16697,7 +16697,7 @@
         <v>1</v>
       </c>
       <c r="N251" s="3" t="n">
-        <v>46079.79591435185</v>
+        <v>46080.37895833333</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16825,7 +16825,7 @@
         <v>1</v>
       </c>
       <c r="N253" s="3" t="n">
-        <v>46079.81583333333</v>
+        <v>46080.39982638889</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16883,7 +16883,7 @@
         <v>1</v>
       </c>
       <c r="N254" s="3" t="n">
-        <v>46079.83004629629</v>
+        <v>46080.37438657408</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -16947,7 +16947,7 @@
         <v>1</v>
       </c>
       <c r="N255" s="3" t="n">
-        <v>46079.80324074074</v>
+        <v>46080.39741898148</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -17011,7 +17011,7 @@
         <v>1</v>
       </c>
       <c r="N256" s="3" t="n">
-        <v>46079.80778935185</v>
+        <v>46080.3947337963</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17075,7 +17075,7 @@
         <v>1</v>
       </c>
       <c r="N257" s="3" t="n">
-        <v>46079.81305555555</v>
+        <v>46080.39664351852</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17139,7 +17139,7 @@
         <v>1</v>
       </c>
       <c r="N258" s="3" t="n">
-        <v>46079.80392361111</v>
+        <v>46080.38574074074</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
@@ -17203,7 +17203,7 @@
         <v>1</v>
       </c>
       <c r="N259" s="3" t="n">
-        <v>46079.80809027778</v>
+        <v>46080.32083333333</v>
       </c>
       <c r="O259" t="inlineStr">
         <is>
@@ -17267,7 +17267,7 @@
         <v>1</v>
       </c>
       <c r="N260" s="3" t="n">
-        <v>46079.60084490741</v>
+        <v>46080.36402777778</v>
       </c>
       <c r="O260" t="inlineStr">
         <is>
@@ -17331,7 +17331,7 @@
         <v>1</v>
       </c>
       <c r="N261" s="3" t="n">
-        <v>46079.82717592592</v>
+        <v>46080.36748842592</v>
       </c>
       <c r="O261" t="inlineStr">
         <is>
@@ -17395,7 +17395,7 @@
         <v>1</v>
       </c>
       <c r="N262" s="3" t="n">
-        <v>46079.81940972222</v>
+        <v>46080.36471064815</v>
       </c>
       <c r="O262" t="inlineStr">
         <is>
@@ -17459,7 +17459,7 @@
         <v>1</v>
       </c>
       <c r="N263" s="3" t="n">
-        <v>46079.81905092593</v>
+        <v>46080.37491898148</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17523,7 +17523,7 @@
         <v>1</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>46079.81013888889</v>
+        <v>46080.38934027778</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17587,7 +17587,7 @@
         <v>1</v>
       </c>
       <c r="N265" s="3" t="n">
-        <v>46079.82109953704</v>
+        <v>46080.37231481481</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17651,7 +17651,7 @@
         <v>1</v>
       </c>
       <c r="N266" s="3" t="n">
-        <v>46079.84724537037</v>
+        <v>46080.38167824074</v>
       </c>
       <c r="O266" t="inlineStr">
         <is>
@@ -17715,7 +17715,7 @@
         <v>1</v>
       </c>
       <c r="N267" s="3" t="n">
-        <v>46079.79821759259</v>
+        <v>46080.37428240741</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17779,7 +17779,7 @@
         <v>1</v>
       </c>
       <c r="N268" s="3" t="n">
-        <v>46079.80445601852</v>
+        <v>46080.37297453704</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17904,7 +17904,7 @@
         </is>
       </c>
       <c r="N270" s="3" t="n">
-        <v>46080.30166666667</v>
+        <v>46080.38266203704</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -18032,7 +18032,7 @@
         <v>1</v>
       </c>
       <c r="N272" s="3" t="n">
-        <v>46079.64212962963</v>
+        <v>46080.3781712963</v>
       </c>
       <c r="O272" t="inlineStr">
         <is>
@@ -18096,7 +18096,7 @@
         <v>2</v>
       </c>
       <c r="N273" s="3" t="n">
-        <v>46079.66320601852</v>
+        <v>46080.37763888889</v>
       </c>
       <c r="O273" t="inlineStr">
         <is>
@@ -18320,7 +18320,7 @@
       </c>
       <c r="F277" t="inlineStr">
         <is>
-          <t>Windows</t>
+          <t>Microsoft Windows 7 Professional</t>
         </is>
       </c>
       <c r="G277" t="inlineStr">
@@ -18352,7 +18352,7 @@
         <v>1</v>
       </c>
       <c r="N277" s="3" t="n">
-        <v>46076.46351851852</v>
+        <v>46080.40255787037</v>
       </c>
       <c r="O277" t="inlineStr">
         <is>
@@ -18416,7 +18416,7 @@
         <v>1</v>
       </c>
       <c r="N278" s="3" t="n">
-        <v>46080.31898148148</v>
+        <v>46080.40071759259</v>
       </c>
       <c r="O278" t="inlineStr">
         <is>
@@ -18480,7 +18480,7 @@
         <v>1</v>
       </c>
       <c r="N279" s="3" t="n">
-        <v>46080.3037962963</v>
+        <v>46080.38216435185</v>
       </c>
       <c r="O279" t="inlineStr">
         <is>
@@ -18544,7 +18544,7 @@
         <v>1</v>
       </c>
       <c r="N280" s="3" t="n">
-        <v>46079.8146412037</v>
+        <v>46080.3755787037</v>
       </c>
       <c r="O280" t="inlineStr">
         <is>
@@ -18608,7 +18608,7 @@
         <v>1</v>
       </c>
       <c r="N281" s="3" t="n">
-        <v>46079.87063657407</v>
+        <v>46080.36991898148</v>
       </c>
       <c r="O281" t="inlineStr">
         <is>
@@ -18672,7 +18672,7 @@
         <v>1</v>
       </c>
       <c r="N282" s="3" t="n">
-        <v>46080.31703703704</v>
+        <v>46080.39451388889</v>
       </c>
       <c r="O282" t="inlineStr">
         <is>
@@ -18736,7 +18736,7 @@
         <v>1</v>
       </c>
       <c r="N283" s="3" t="n">
-        <v>46079.81559027778</v>
+        <v>46080.3693287037</v>
       </c>
       <c r="O283" t="inlineStr">
         <is>
@@ -18800,7 +18800,7 @@
         <v>1</v>
       </c>
       <c r="N284" s="3" t="n">
-        <v>46079.80465277778</v>
+        <v>46080.38702546297</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18864,7 +18864,7 @@
         <v>1</v>
       </c>
       <c r="N285" s="3" t="n">
-        <v>46079.80431712963</v>
+        <v>46080.37729166666</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -18923,7 +18923,7 @@
         <v>1</v>
       </c>
       <c r="N286" s="3" t="n">
-        <v>46080.17166666667</v>
+        <v>46080.3784837963</v>
       </c>
       <c r="O286" t="inlineStr">
         <is>
@@ -18987,7 +18987,7 @@
         <v>1</v>
       </c>
       <c r="N287" s="3" t="n">
-        <v>46079.80842592593</v>
+        <v>46080.38151620371</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
@@ -19051,7 +19051,7 @@
         <v>1</v>
       </c>
       <c r="N288" s="3" t="n">
-        <v>46080.31662037037</v>
+        <v>46080.39306712963</v>
       </c>
       <c r="O288" t="inlineStr">
         <is>
@@ -19115,7 +19115,7 @@
         <v>1</v>
       </c>
       <c r="N289" s="3" t="n">
-        <v>46079.85931712963</v>
+        <v>46080.38306712963</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -19909,7 +19909,7 @@
         <v>1</v>
       </c>
       <c r="N302" s="3" t="n">
-        <v>46080.31326388889</v>
+        <v>46080.38935185185</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -21025,7 +21025,7 @@
         </is>
       </c>
       <c r="N320" s="3" t="n">
-        <v>46080.30824074074</v>
+        <v>46080.38905092593</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21750,7 +21750,7 @@
         <v>1</v>
       </c>
       <c r="N332" s="3" t="n">
-        <v>46079.7544212963</v>
+        <v>46080.37769675926</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21814,7 +21814,7 @@
         <v>2</v>
       </c>
       <c r="N333" s="3" t="n">
-        <v>46080.28355324074</v>
+        <v>46080.40077546296</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21878,7 +21878,7 @@
         <v>2</v>
       </c>
       <c r="N334" s="3" t="n">
-        <v>46080.28387731482</v>
+        <v>46080.40155092593</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21942,7 +21942,7 @@
         <v>2</v>
       </c>
       <c r="N335" s="3" t="n">
-        <v>46080.28358796296</v>
+        <v>46080.39936342592</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -22006,7 +22006,7 @@
         <v>1</v>
       </c>
       <c r="N336" s="3" t="n">
-        <v>46080.28539351852</v>
+        <v>46080.39951388889</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22070,7 +22070,7 @@
         <v>1</v>
       </c>
       <c r="N337" s="3" t="n">
-        <v>46080.28399305556</v>
+        <v>46080.4034837963</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22134,7 +22134,7 @@
         <v>2</v>
       </c>
       <c r="N338" s="3" t="n">
-        <v>46080.28365740741</v>
+        <v>46080.40048611111</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -22198,7 +22198,7 @@
         <v>2</v>
       </c>
       <c r="N339" s="3" t="n">
-        <v>46080.30105324074</v>
+        <v>46080.38011574074</v>
       </c>
       <c r="O339" t="inlineStr">
         <is>
@@ -23836,7 +23836,7 @@
         <v>1</v>
       </c>
       <c r="N365" s="3" t="n">
-        <v>46079.70519675926</v>
+        <v>46080.37835648148</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
@@ -23902,7 +23902,7 @@
         </is>
       </c>
       <c r="N366" s="3" t="n">
-        <v>46080.30050925926</v>
+        <v>46080.37943287037</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -24028,7 +24028,7 @@
         </is>
       </c>
       <c r="N368" s="3" t="n">
-        <v>46080.31581018519</v>
+        <v>46080.39349537037</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -24089,7 +24089,7 @@
         </is>
       </c>
       <c r="N369" s="3" t="n">
-        <v>46079.71952546296</v>
+        <v>46080.39113425926</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
@@ -24431,7 +24431,7 @@
         <v>1</v>
       </c>
       <c r="N374" s="3" t="n">
-        <v>46079.75130787037</v>
+        <v>46080.39359953703</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24497,7 +24497,7 @@
         </is>
       </c>
       <c r="N375" s="3" t="n">
-        <v>46079.72599537037</v>
+        <v>46080.37733796296</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
@@ -24561,7 +24561,7 @@
         <v>1</v>
       </c>
       <c r="N376" s="3" t="n">
-        <v>46080.29885416666</v>
+        <v>46080.37488425926</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -24630,7 +24630,7 @@
         <v>2</v>
       </c>
       <c r="N377" s="3" t="n">
-        <v>46079.74957175926</v>
+        <v>46080.3978587963</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -24699,7 +24699,7 @@
         <v>2</v>
       </c>
       <c r="N378" s="3" t="n">
-        <v>46080.32064814815</v>
+        <v>46080.39538194444</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização automática 2026-02-27 11:52:06.015515
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>46080.36765046296</v>
+        <v>46080.48038194444</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>46080.39267361111</v>
+        <v>46080.47114583333</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
         <v>1</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>46080.37395833333</v>
+        <v>46080.45179398148</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>46080.38234953704</v>
+        <v>46080.45825231481</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -875,7 +875,7 @@
         <v>1</v>
       </c>
       <c r="N6" s="3" t="n">
-        <v>46078.58994212963</v>
+        <v>46080.45040509259</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -944,7 +944,7 @@
         <v>1</v>
       </c>
       <c r="N7" s="3" t="n">
-        <v>46078.89480324074</v>
+        <v>46080.48715277778</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -1259,7 +1259,7 @@
         <v>1</v>
       </c>
       <c r="N12" s="3" t="n">
-        <v>46080.40229166667</v>
+        <v>46080.47465277778</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1323,7 +1323,7 @@
         <v>1</v>
       </c>
       <c r="N13" s="3" t="n">
-        <v>46080.39877314815</v>
+        <v>46080.47429398148</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1387,7 +1387,7 @@
         <v>2</v>
       </c>
       <c r="N14" s="3" t="n">
-        <v>46080.4034375</v>
+        <v>46080.48453703704</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1451,7 +1451,7 @@
         <v>1</v>
       </c>
       <c r="N15" s="3" t="n">
-        <v>46078.70284722222</v>
+        <v>46080.47511574074</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1515,7 +1515,7 @@
         <v>2</v>
       </c>
       <c r="N16" s="3" t="n">
-        <v>46080.37883101852</v>
+        <v>46080.45637731482</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1579,7 +1579,7 @@
         <v>1</v>
       </c>
       <c r="N17" s="3" t="n">
-        <v>46080.40078703704</v>
+        <v>46080.48695601852</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1643,7 +1643,7 @@
         <v>2</v>
       </c>
       <c r="N18" s="3" t="n">
-        <v>46080.40098379629</v>
+        <v>46080.47741898148</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1768,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="N20" s="3" t="n">
-        <v>46080.38796296297</v>
+        <v>46080.46861111111</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1832,7 +1832,7 @@
         <v>1</v>
       </c>
       <c r="N21" s="3" t="n">
-        <v>46078.70927083334</v>
+        <v>46080.42368055556</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -2009,7 +2009,7 @@
         <v>1</v>
       </c>
       <c r="N24" s="3" t="n">
-        <v>46080.3716087963</v>
+        <v>46080.4104050926</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2143,11 +2143,6 @@
           <t>AUDITORIO</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>10.69.3.151</t>
-        </is>
-      </c>
       <c r="D27" t="n">
         <v>2019</v>
       </c>
@@ -2188,7 +2183,7 @@
         <v>1</v>
       </c>
       <c r="N27" s="3" t="n">
-        <v>46080.39244212963</v>
+        <v>46080.44975694444</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -6575,7 +6570,7 @@
         <v>1</v>
       </c>
       <c r="N95" s="3" t="n">
-        <v>46080.37099537037</v>
+        <v>46080.48771990741</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -6644,7 +6639,7 @@
         <v>1</v>
       </c>
       <c r="N96" s="3" t="n">
-        <v>46079.82724537037</v>
+        <v>46080.47575231481</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
@@ -6663,6 +6658,11 @@
           <t>COORDENACAO</t>
         </is>
       </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>10.69.3.93</t>
+        </is>
+      </c>
       <c r="D97" t="n">
         <v>2025</v>
       </c>
@@ -6708,7 +6708,7 @@
         <v>1</v>
       </c>
       <c r="N97" s="3" t="n">
-        <v>46080.36945601852</v>
+        <v>46080.48465277778</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -6772,7 +6772,7 @@
         <v>1</v>
       </c>
       <c r="N98" s="3" t="n">
-        <v>46080.37287037037</v>
+        <v>46080.45106481481</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -6841,7 +6841,7 @@
         <v>1</v>
       </c>
       <c r="N99" s="3" t="n">
-        <v>46080.38021990741</v>
+        <v>46080.45789351852</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -6910,7 +6910,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>46080.39115740741</v>
+        <v>46080.46795138889</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6979,7 +6979,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="3" t="n">
-        <v>46080.37886574074</v>
+        <v>46080.4562037037</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -7117,7 +7117,7 @@
         <v>2</v>
       </c>
       <c r="N103" s="3" t="n">
-        <v>46080.39851851852</v>
+        <v>46080.473125</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7243,9 +7243,6 @@
           <t>HP ProBook 440 14 inch G9 Notebook PC</t>
         </is>
       </c>
-      <c r="M105" t="n">
-        <v>1</v>
-      </c>
       <c r="N105" s="3" t="n">
         <v>46079.52680555556</v>
       </c>
@@ -7515,7 +7512,7 @@
         <v>1</v>
       </c>
       <c r="N109" s="3" t="n">
-        <v>46080.37085648148</v>
+        <v>46080.45012731481</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7584,7 +7581,7 @@
         <v>2</v>
       </c>
       <c r="N110" s="3" t="n">
-        <v>46080.365</v>
+        <v>46080.48027777778</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7653,7 +7650,7 @@
         <v>2</v>
       </c>
       <c r="N111" s="3" t="n">
-        <v>46080.40094907407</v>
+        <v>46080.43893518519</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
@@ -7722,7 +7719,7 @@
         <v>2</v>
       </c>
       <c r="N112" s="3" t="n">
-        <v>46080.39350694444</v>
+        <v>46080.46828703704</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7791,7 +7788,7 @@
         <v>1</v>
       </c>
       <c r="N113" s="3" t="n">
-        <v>46080.36824074074</v>
+        <v>46080.48717592593</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7860,7 +7857,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>46080.37372685185</v>
+        <v>46080.45215277778</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -7926,7 +7923,7 @@
         </is>
       </c>
       <c r="N115" s="3" t="n">
-        <v>46080.37569444445</v>
+        <v>46080.4874537037</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -7995,7 +7992,7 @@
         <v>1</v>
       </c>
       <c r="N116" s="3" t="n">
-        <v>46080.37627314815</v>
+        <v>46080.48638888889</v>
       </c>
       <c r="O116" t="inlineStr">
         <is>
@@ -8064,7 +8061,7 @@
         <v>1</v>
       </c>
       <c r="N117" s="3" t="n">
-        <v>46080.39326388889</v>
+        <v>46080.47449074074</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -8130,7 +8127,7 @@
         </is>
       </c>
       <c r="N118" s="3" t="n">
-        <v>46080.37770833333</v>
+        <v>46080.4571875</v>
       </c>
       <c r="O118" t="inlineStr">
         <is>
@@ -8268,7 +8265,7 @@
         <v>1</v>
       </c>
       <c r="N120" s="3" t="n">
-        <v>46080.36945601852</v>
+        <v>46080.48518518519</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -8337,7 +8334,7 @@
         <v>1</v>
       </c>
       <c r="N121" s="3" t="n">
-        <v>46079.80608796296</v>
+        <v>46080.46542824074</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -8403,7 +8400,7 @@
         </is>
       </c>
       <c r="N122" s="3" t="n">
-        <v>46080.36865740741</v>
+        <v>46080.4846875</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -8472,7 +8469,7 @@
         <v>2</v>
       </c>
       <c r="N123" s="3" t="n">
-        <v>46080.30180555556</v>
+        <v>46080.45436342592</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -8541,7 +8538,7 @@
         <v>1</v>
       </c>
       <c r="N124" s="3" t="n">
-        <v>46080.40225694444</v>
+        <v>46080.48311342593</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -8679,7 +8676,7 @@
         <v>2</v>
       </c>
       <c r="N126" s="3" t="n">
-        <v>46079.78649305556</v>
+        <v>46080.47274305556</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -8748,7 +8745,7 @@
         <v>2</v>
       </c>
       <c r="N127" s="3" t="n">
-        <v>46080.38659722222</v>
+        <v>46080.46353009259</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -8817,7 +8814,7 @@
         <v>1</v>
       </c>
       <c r="N128" s="3" t="n">
-        <v>46080.37311342593</v>
+        <v>46080.45328703704</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -8886,7 +8883,7 @@
         <v>1</v>
       </c>
       <c r="N129" s="3" t="n">
-        <v>46079.68133101852</v>
+        <v>46080.46626157407</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -8955,7 +8952,7 @@
         <v>1</v>
       </c>
       <c r="N130" s="3" t="n">
-        <v>46080.37387731481</v>
+        <v>46080.45143518518</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -8974,11 +8971,6 @@
           <t>ADM/FIN</t>
         </is>
       </c>
-      <c r="C131" t="inlineStr">
-        <is>
-          <t>10.69.3.6</t>
-        </is>
-      </c>
       <c r="D131" t="n">
         <v>2025</v>
       </c>
@@ -9024,7 +9016,7 @@
         <v>1</v>
       </c>
       <c r="N131" s="3" t="n">
-        <v>46080.39912037037</v>
+        <v>46080.47667824074</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -9157,7 +9149,7 @@
         <v>1</v>
       </c>
       <c r="N133" s="3" t="n">
-        <v>46080.37106481481</v>
+        <v>46080.48716435185</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -9221,7 +9213,7 @@
         <v>1</v>
       </c>
       <c r="N134" s="3" t="n">
-        <v>46078.84300925926</v>
+        <v>46080.4570949074</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -9285,7 +9277,7 @@
         <v>1</v>
       </c>
       <c r="N135" s="3" t="n">
-        <v>46079.80307870371</v>
+        <v>46080.4569212963</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -9476,7 +9468,7 @@
         <v>1</v>
       </c>
       <c r="N138" s="3" t="n">
-        <v>46080.37650462963</v>
+        <v>46080.45041666667</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9540,7 +9532,7 @@
         <v>1</v>
       </c>
       <c r="N139" s="3" t="n">
-        <v>46080.37484953704</v>
+        <v>46080.45789351852</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9604,7 +9596,7 @@
         <v>1</v>
       </c>
       <c r="N140" s="3" t="n">
-        <v>46080.37309027778</v>
+        <v>46080.45467592592</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9668,7 +9660,7 @@
         <v>1</v>
       </c>
       <c r="N141" s="3" t="n">
-        <v>46080.37251157407</v>
+        <v>46080.48293981481</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9732,7 +9724,7 @@
         <v>1</v>
       </c>
       <c r="N142" s="3" t="n">
-        <v>46080.37215277777</v>
+        <v>46080.454375</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9860,7 +9852,7 @@
         <v>1</v>
       </c>
       <c r="N144" s="3" t="n">
-        <v>46080.3874074074</v>
+        <v>46080.45821759259</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9988,7 +9980,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="3" t="n">
-        <v>46080.36858796296</v>
+        <v>46080.45150462963</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10052,7 +10044,7 @@
         <v>1</v>
       </c>
       <c r="N147" s="3" t="n">
-        <v>46080.40246527778</v>
+        <v>46080.48042824074</v>
       </c>
       <c r="O147" t="inlineStr">
         <is>
@@ -10116,7 +10108,7 @@
         <v>1</v>
       </c>
       <c r="N148" s="3" t="n">
-        <v>46080.37829861111</v>
+        <v>46080.45887731481</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10180,7 +10172,7 @@
         <v>1</v>
       </c>
       <c r="N149" s="3" t="n">
-        <v>46079.87311342593</v>
+        <v>46080.47166666666</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -10244,7 +10236,7 @@
         <v>1</v>
       </c>
       <c r="N150" s="3" t="n">
-        <v>46080.37076388889</v>
+        <v>46080.45399305555</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -10308,7 +10300,7 @@
         <v>1</v>
       </c>
       <c r="N151" s="3" t="n">
-        <v>46080.38425925926</v>
+        <v>46080.45797453704</v>
       </c>
       <c r="O151" t="inlineStr">
         <is>
@@ -10372,7 +10364,7 @@
         <v>1</v>
       </c>
       <c r="N152" s="3" t="n">
-        <v>46080.37346064814</v>
+        <v>46080.45348379629</v>
       </c>
       <c r="O152" t="inlineStr">
         <is>
@@ -10495,7 +10487,7 @@
         <v>1</v>
       </c>
       <c r="N154" s="3" t="n">
-        <v>46080.39429398148</v>
+        <v>46080.46960648148</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10559,7 +10551,7 @@
         <v>1</v>
       </c>
       <c r="N155" s="3" t="n">
-        <v>46080.37458333333</v>
+        <v>46080.45189814815</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10623,7 +10615,7 @@
         <v>1</v>
       </c>
       <c r="N156" s="3" t="n">
-        <v>46080.36940972223</v>
+        <v>46080.48587962963</v>
       </c>
       <c r="O156" t="inlineStr">
         <is>
@@ -10687,7 +10679,7 @@
         <v>1</v>
       </c>
       <c r="N157" s="3" t="n">
-        <v>46080.37290509259</v>
+        <v>46080.45710648148</v>
       </c>
       <c r="O157" t="inlineStr">
         <is>
@@ -10751,7 +10743,7 @@
         <v>1</v>
       </c>
       <c r="N158" s="3" t="n">
-        <v>46080.3871875</v>
+        <v>46080.46634259259</v>
       </c>
       <c r="O158" t="inlineStr">
         <is>
@@ -10815,7 +10807,7 @@
         <v>1</v>
       </c>
       <c r="N159" s="3" t="n">
-        <v>46080.38908564814</v>
+        <v>46080.4621875</v>
       </c>
       <c r="O159" t="inlineStr">
         <is>
@@ -10879,7 +10871,7 @@
         <v>1</v>
       </c>
       <c r="N160" s="3" t="n">
-        <v>46080.36987268519</v>
+        <v>46080.48313657408</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
@@ -10943,7 +10935,7 @@
         <v>1</v>
       </c>
       <c r="N161" s="3" t="n">
-        <v>46080.37319444444</v>
+        <v>46080.45240740741</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -11007,7 +10999,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="3" t="n">
-        <v>46080.3959837963</v>
+        <v>46080.4729050926</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11135,7 +11127,7 @@
         <v>2</v>
       </c>
       <c r="N164" s="3" t="n">
-        <v>46080.36446759259</v>
+        <v>46080.48660879629</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11199,7 +11191,7 @@
         <v>2</v>
       </c>
       <c r="N165" s="3" t="n">
-        <v>46080.36883101852</v>
+        <v>46080.48392361111</v>
       </c>
       <c r="O165" t="inlineStr">
         <is>
@@ -11263,7 +11255,7 @@
         <v>2</v>
       </c>
       <c r="N166" s="3" t="n">
-        <v>46080.38336805555</v>
+        <v>46080.45648148148</v>
       </c>
       <c r="O166" t="inlineStr">
         <is>
@@ -11327,7 +11319,7 @@
         <v>2</v>
       </c>
       <c r="N167" s="3" t="n">
-        <v>46080.40265046297</v>
+        <v>46080.48092592593</v>
       </c>
       <c r="O167" t="inlineStr">
         <is>
@@ -11391,7 +11383,7 @@
         <v>2</v>
       </c>
       <c r="N168" s="3" t="n">
-        <v>46080.39711805555</v>
+        <v>46080.47665509259</v>
       </c>
       <c r="O168" t="inlineStr">
         <is>
@@ -11519,7 +11511,7 @@
         <v>2</v>
       </c>
       <c r="N170" s="3" t="n">
-        <v>46080.38101851852</v>
+        <v>46080.46075231482</v>
       </c>
       <c r="O170" t="inlineStr">
         <is>
@@ -11583,7 +11575,7 @@
         <v>2</v>
       </c>
       <c r="N171" s="3" t="n">
-        <v>46080.40368055556</v>
+        <v>46080.48310185185</v>
       </c>
       <c r="O171" t="inlineStr">
         <is>
@@ -11647,7 +11639,7 @@
         <v>2</v>
       </c>
       <c r="N172" s="3" t="n">
-        <v>46079.8635300926</v>
+        <v>46080.4549537037</v>
       </c>
       <c r="O172" t="inlineStr">
         <is>
@@ -11711,7 +11703,7 @@
         <v>1</v>
       </c>
       <c r="N173" s="3" t="n">
-        <v>46080.38402777778</v>
+        <v>46080.46209490741</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -11775,7 +11767,7 @@
         <v>2</v>
       </c>
       <c r="N174" s="3" t="n">
-        <v>46080.38055555556</v>
+        <v>46080.45770833334</v>
       </c>
       <c r="O174" t="inlineStr">
         <is>
@@ -11839,7 +11831,7 @@
         <v>2</v>
       </c>
       <c r="N175" s="3" t="n">
-        <v>46080.37818287037</v>
+        <v>46080.45481481482</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -11903,7 +11895,7 @@
         <v>2</v>
       </c>
       <c r="N176" s="3" t="n">
-        <v>46080.4025925926</v>
+        <v>46080.47548611111</v>
       </c>
       <c r="O176" t="inlineStr">
         <is>
@@ -11967,7 +11959,7 @@
         <v>2</v>
       </c>
       <c r="N177" s="3" t="n">
-        <v>46079.70418981482</v>
+        <v>46080.45980324074</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
@@ -12031,7 +12023,7 @@
         <v>2</v>
       </c>
       <c r="N178" s="3" t="n">
-        <v>46080.3987037037</v>
+        <v>46080.4775</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12095,7 +12087,7 @@
         <v>1</v>
       </c>
       <c r="N179" s="3" t="n">
-        <v>46080.39746527778</v>
+        <v>46080.47530092593</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12159,7 +12151,7 @@
         <v>1</v>
       </c>
       <c r="N180" s="3" t="n">
-        <v>46080.39327546296</v>
+        <v>46080.47428240741</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12351,7 +12343,7 @@
         <v>1</v>
       </c>
       <c r="N183" s="3" t="n">
-        <v>46080.39916666667</v>
+        <v>46080.48096064815</v>
       </c>
       <c r="O183" t="inlineStr">
         <is>
@@ -12420,7 +12412,7 @@
         <v>2</v>
       </c>
       <c r="N184" s="3" t="n">
-        <v>46080.39745370371</v>
+        <v>46080.47369212963</v>
       </c>
       <c r="O184" t="inlineStr">
         <is>
@@ -12548,7 +12540,7 @@
         <v>1</v>
       </c>
       <c r="N186" s="3" t="n">
-        <v>46080.36486111111</v>
+        <v>46080.48287037037</v>
       </c>
       <c r="O186" t="inlineStr">
         <is>
@@ -12612,7 +12604,7 @@
         <v>1</v>
       </c>
       <c r="N187" s="3" t="n">
-        <v>46080.3965625</v>
+        <v>46080.47230324074</v>
       </c>
       <c r="O187" t="inlineStr">
         <is>
@@ -12676,7 +12668,7 @@
         <v>1</v>
       </c>
       <c r="N188" s="3" t="n">
-        <v>46080.37136574074</v>
+        <v>46080.44773148148</v>
       </c>
       <c r="O188" t="inlineStr">
         <is>
@@ -12804,7 +12796,7 @@
         </is>
       </c>
       <c r="N190" s="3" t="n">
-        <v>46080.38706018519</v>
+        <v>46080.46491898148</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12932,7 +12924,7 @@
         <v>1</v>
       </c>
       <c r="N192" s="3" t="n">
-        <v>46080.39361111111</v>
+        <v>46080.47545138889</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -13057,7 +13049,7 @@
         <v>2</v>
       </c>
       <c r="N194" s="3" t="n">
-        <v>46080.3684375</v>
+        <v>46080.48358796296</v>
       </c>
       <c r="O194" t="inlineStr">
         <is>
@@ -13121,7 +13113,7 @@
         <v>1</v>
       </c>
       <c r="N195" s="3" t="n">
-        <v>46080.37892361111</v>
+        <v>46080.45819444444</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13185,7 +13177,7 @@
         <v>1</v>
       </c>
       <c r="N196" s="3" t="n">
-        <v>46080.38236111111</v>
+        <v>46080.46078703704</v>
       </c>
       <c r="O196" t="inlineStr">
         <is>
@@ -13313,7 +13305,7 @@
         <v>1</v>
       </c>
       <c r="N198" s="3" t="n">
-        <v>46080.37958333334</v>
+        <v>46080.45265046296</v>
       </c>
       <c r="O198" t="inlineStr">
         <is>
@@ -13377,7 +13369,7 @@
         <v>1</v>
       </c>
       <c r="N199" s="3" t="n">
-        <v>46080.36868055556</v>
+        <v>46080.48491898148</v>
       </c>
       <c r="O199" t="inlineStr">
         <is>
@@ -13441,7 +13433,7 @@
         <v>1</v>
       </c>
       <c r="N200" s="3" t="n">
-        <v>46080.39163194445</v>
+        <v>46080.46542824074</v>
       </c>
       <c r="O200" t="inlineStr">
         <is>
@@ -13502,7 +13494,7 @@
         </is>
       </c>
       <c r="N201" s="3" t="n">
-        <v>46080.40106481482</v>
+        <v>46080.47800925926</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -13566,7 +13558,7 @@
         <v>1</v>
       </c>
       <c r="N202" s="3" t="n">
-        <v>46080.40204861111</v>
+        <v>46080.48430555555</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13630,7 +13622,7 @@
         <v>1</v>
       </c>
       <c r="N203" s="3" t="n">
-        <v>46080.3786574074</v>
+        <v>46080.45458333333</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13694,7 +13686,7 @@
         <v>1</v>
       </c>
       <c r="N204" s="3" t="n">
-        <v>46080.39340277778</v>
+        <v>46080.46799768518</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13758,7 +13750,7 @@
         <v>1</v>
       </c>
       <c r="N205" s="3" t="n">
-        <v>46080.37083333333</v>
+        <v>46080.44791666666</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13822,7 +13814,7 @@
         <v>1</v>
       </c>
       <c r="N206" s="3" t="n">
-        <v>46080.37386574074</v>
+        <v>46080.45133101852</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -13886,7 +13878,7 @@
         <v>1</v>
       </c>
       <c r="N207" s="3" t="n">
-        <v>46080.38532407407</v>
+        <v>46080.46159722222</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -13950,7 +13942,7 @@
         <v>1</v>
       </c>
       <c r="N208" s="3" t="n">
-        <v>46080.38958333333</v>
+        <v>46080.46368055556</v>
       </c>
       <c r="O208" t="inlineStr">
         <is>
@@ -14014,7 +14006,7 @@
         <v>1</v>
       </c>
       <c r="N209" s="3" t="n">
-        <v>46080.37030092593</v>
+        <v>46080.47939814815</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14078,7 +14070,7 @@
         <v>1</v>
       </c>
       <c r="N210" s="3" t="n">
-        <v>46080.36388888889</v>
+        <v>46080.48724537037</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14142,7 +14134,7 @@
         <v>1</v>
       </c>
       <c r="N211" s="3" t="n">
-        <v>46080.36549768518</v>
+        <v>46080.48079861111</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -14206,7 +14198,7 @@
         <v>1</v>
       </c>
       <c r="N212" s="3" t="n">
-        <v>46080.4030324074</v>
+        <v>46080.48443287037</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -14270,7 +14262,7 @@
         <v>1</v>
       </c>
       <c r="N213" s="3" t="n">
-        <v>46080.38321759259</v>
+        <v>46080.46354166666</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
@@ -14334,7 +14326,7 @@
         <v>1</v>
       </c>
       <c r="N214" s="3" t="n">
-        <v>46080.39730324074</v>
+        <v>46080.47532407408</v>
       </c>
       <c r="O214" t="inlineStr">
         <is>
@@ -14398,7 +14390,7 @@
         <v>1</v>
       </c>
       <c r="N215" s="3" t="n">
-        <v>46080.39803240741</v>
+        <v>46080.47494212963</v>
       </c>
       <c r="O215" t="inlineStr">
         <is>
@@ -14462,7 +14454,7 @@
         <v>1</v>
       </c>
       <c r="N216" s="3" t="n">
-        <v>46080.40012731482</v>
+        <v>46080.47881944444</v>
       </c>
       <c r="O216" t="inlineStr">
         <is>
@@ -14526,7 +14518,7 @@
         <v>1</v>
       </c>
       <c r="N217" s="3" t="n">
-        <v>46080.40179398148</v>
+        <v>46080.47697916667</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14590,7 +14582,7 @@
         <v>1</v>
       </c>
       <c r="N218" s="3" t="n">
-        <v>46080.37081018519</v>
+        <v>46080.45056712963</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14723,7 +14715,7 @@
         <v>1</v>
       </c>
       <c r="N220" s="3" t="n">
-        <v>46080.36267361111</v>
+        <v>46080.40474537037</v>
       </c>
       <c r="O220" t="inlineStr">
         <is>
@@ -14787,7 +14779,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="3" t="n">
-        <v>46080.37655092592</v>
+        <v>46080.45899305555</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14851,7 +14843,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="3" t="n">
-        <v>46080.38730324074</v>
+        <v>46080.46358796296</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -14915,7 +14907,7 @@
         <v>1</v>
       </c>
       <c r="N223" s="3" t="n">
-        <v>46080.37760416666</v>
+        <v>46080.45162037037</v>
       </c>
       <c r="O223" t="inlineStr">
         <is>
@@ -15107,7 +15099,7 @@
         <v>1</v>
       </c>
       <c r="N226" s="3" t="n">
-        <v>46080.39855324074</v>
+        <v>46080.48328703704</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15171,7 +15163,7 @@
         <v>1</v>
       </c>
       <c r="N227" s="3" t="n">
-        <v>46080.39767361111</v>
+        <v>46080.48710648148</v>
       </c>
       <c r="O227" t="inlineStr">
         <is>
@@ -15235,7 +15227,7 @@
         <v>1</v>
       </c>
       <c r="N228" s="3" t="n">
-        <v>46080.38738425926</v>
+        <v>46080.46450231481</v>
       </c>
       <c r="O228" t="inlineStr">
         <is>
@@ -15299,7 +15291,7 @@
         <v>1</v>
       </c>
       <c r="N229" s="3" t="n">
-        <v>46080.40356481481</v>
+        <v>46080.47861111111</v>
       </c>
       <c r="O229" t="inlineStr">
         <is>
@@ -15363,7 +15355,7 @@
         <v>1</v>
       </c>
       <c r="N230" s="3" t="n">
-        <v>46080.39807870371</v>
+        <v>46080.47380787037</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15427,7 +15419,7 @@
         <v>1</v>
       </c>
       <c r="N231" s="3" t="n">
-        <v>46080.38127314814</v>
+        <v>46080.46395833333</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15491,7 +15483,7 @@
         <v>1</v>
       </c>
       <c r="N232" s="3" t="n">
-        <v>46080.37523148148</v>
+        <v>46080.4562037037</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -15555,7 +15547,7 @@
         <v>1</v>
       </c>
       <c r="N233" s="3" t="n">
-        <v>46080.37386574074</v>
+        <v>46080.45034722222</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15619,7 +15611,7 @@
         <v>1</v>
       </c>
       <c r="N234" s="3" t="n">
-        <v>46080.37746527778</v>
+        <v>46080.45418981482</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -15683,7 +15675,7 @@
         <v>1</v>
       </c>
       <c r="N235" s="3" t="n">
-        <v>46080.39731481481</v>
+        <v>46080.47844907407</v>
       </c>
       <c r="O235" t="inlineStr">
         <is>
@@ -15875,7 +15867,7 @@
         <v>1</v>
       </c>
       <c r="N238" s="3" t="n">
-        <v>46080.39987268519</v>
+        <v>46080.4740625</v>
       </c>
       <c r="O238" t="inlineStr">
         <is>
@@ -15939,7 +15931,7 @@
         <v>1</v>
       </c>
       <c r="N239" s="3" t="n">
-        <v>46080.37438657408</v>
+        <v>46080.45162037037</v>
       </c>
       <c r="O239" t="inlineStr">
         <is>
@@ -16003,7 +15995,7 @@
         <v>1</v>
       </c>
       <c r="N240" s="3" t="n">
-        <v>46080.37405092592</v>
+        <v>46080.45166666667</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16067,7 +16059,7 @@
         <v>1</v>
       </c>
       <c r="N241" s="3" t="n">
-        <v>46080.38453703704</v>
+        <v>46080.45829861111</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16131,7 +16123,7 @@
         <v>1</v>
       </c>
       <c r="N242" s="3" t="n">
-        <v>46080.38105324074</v>
+        <v>46080.4580324074</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16382,7 +16374,7 @@
         <v>1</v>
       </c>
       <c r="N246" s="3" t="n">
-        <v>46080.37559027778</v>
+        <v>46080.45684027778</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16446,7 +16438,7 @@
         <v>1</v>
       </c>
       <c r="N247" s="3" t="n">
-        <v>46080.37290509259</v>
+        <v>46080.45277777778</v>
       </c>
       <c r="O247" t="inlineStr">
         <is>
@@ -16510,7 +16502,7 @@
         <v>1</v>
       </c>
       <c r="N248" s="3" t="n">
-        <v>46080.39711805555</v>
+        <v>46080.47719907408</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16633,7 +16625,7 @@
         <v>1</v>
       </c>
       <c r="N250" s="3" t="n">
-        <v>46080.3866087963</v>
+        <v>46080.46539351852</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16697,7 +16689,7 @@
         <v>1</v>
       </c>
       <c r="N251" s="3" t="n">
-        <v>46080.37895833333</v>
+        <v>46080.45438657407</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16825,7 +16817,7 @@
         <v>1</v>
       </c>
       <c r="N253" s="3" t="n">
-        <v>46080.39982638889</v>
+        <v>46080.47783564815</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16883,7 +16875,7 @@
         <v>1</v>
       </c>
       <c r="N254" s="3" t="n">
-        <v>46080.37438657408</v>
+        <v>46080.44922453703</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -16947,7 +16939,7 @@
         <v>1</v>
       </c>
       <c r="N255" s="3" t="n">
-        <v>46080.39741898148</v>
+        <v>46080.47686342592</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -17011,7 +17003,7 @@
         <v>1</v>
       </c>
       <c r="N256" s="3" t="n">
-        <v>46080.3947337963</v>
+        <v>46080.47652777778</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17075,7 +17067,7 @@
         <v>1</v>
       </c>
       <c r="N257" s="3" t="n">
-        <v>46080.39664351852</v>
+        <v>46080.47431712963</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17139,7 +17131,7 @@
         <v>1</v>
       </c>
       <c r="N258" s="3" t="n">
-        <v>46080.38574074074</v>
+        <v>46080.46045138889</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
@@ -17267,7 +17259,7 @@
         <v>1</v>
       </c>
       <c r="N260" s="3" t="n">
-        <v>46080.36402777778</v>
+        <v>46080.48371527778</v>
       </c>
       <c r="O260" t="inlineStr">
         <is>
@@ -17331,7 +17323,7 @@
         <v>1</v>
       </c>
       <c r="N261" s="3" t="n">
-        <v>46080.36748842592</v>
+        <v>46080.48236111111</v>
       </c>
       <c r="O261" t="inlineStr">
         <is>
@@ -17395,7 +17387,7 @@
         <v>1</v>
       </c>
       <c r="N262" s="3" t="n">
-        <v>46080.36471064815</v>
+        <v>46080.48291666667</v>
       </c>
       <c r="O262" t="inlineStr">
         <is>
@@ -17459,7 +17451,7 @@
         <v>1</v>
       </c>
       <c r="N263" s="3" t="n">
-        <v>46080.37491898148</v>
+        <v>46080.4571412037</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17523,7 +17515,7 @@
         <v>1</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>46080.38934027778</v>
+        <v>46080.46570601852</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17587,7 +17579,7 @@
         <v>1</v>
       </c>
       <c r="N265" s="3" t="n">
-        <v>46080.37231481481</v>
+        <v>46080.45185185185</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17651,7 +17643,7 @@
         <v>1</v>
       </c>
       <c r="N266" s="3" t="n">
-        <v>46080.38167824074</v>
+        <v>46080.46283564815</v>
       </c>
       <c r="O266" t="inlineStr">
         <is>
@@ -17715,7 +17707,7 @@
         <v>1</v>
       </c>
       <c r="N267" s="3" t="n">
-        <v>46080.37428240741</v>
+        <v>46080.4521875</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17779,7 +17771,7 @@
         <v>1</v>
       </c>
       <c r="N268" s="3" t="n">
-        <v>46080.37297453704</v>
+        <v>46080.48538194445</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17843,7 +17835,7 @@
         <v>1</v>
       </c>
       <c r="N269" s="3" t="n">
-        <v>46079.86325231481</v>
+        <v>46080.45818287037</v>
       </c>
       <c r="O269" t="inlineStr">
         <is>
@@ -17904,7 +17896,7 @@
         </is>
       </c>
       <c r="N270" s="3" t="n">
-        <v>46080.38266203704</v>
+        <v>46080.46216435185</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -18032,7 +18024,7 @@
         <v>1</v>
       </c>
       <c r="N272" s="3" t="n">
-        <v>46080.3781712963</v>
+        <v>46080.45615740741</v>
       </c>
       <c r="O272" t="inlineStr">
         <is>
@@ -18096,7 +18088,7 @@
         <v>2</v>
       </c>
       <c r="N273" s="3" t="n">
-        <v>46080.37763888889</v>
+        <v>46080.45869212963</v>
       </c>
       <c r="O273" t="inlineStr">
         <is>
@@ -18416,7 +18408,7 @@
         <v>1</v>
       </c>
       <c r="N278" s="3" t="n">
-        <v>46080.40071759259</v>
+        <v>46080.47564814815</v>
       </c>
       <c r="O278" t="inlineStr">
         <is>
@@ -18480,7 +18472,7 @@
         <v>1</v>
       </c>
       <c r="N279" s="3" t="n">
-        <v>46080.38216435185</v>
+        <v>46080.46008101852</v>
       </c>
       <c r="O279" t="inlineStr">
         <is>
@@ -18544,7 +18536,7 @@
         <v>1</v>
       </c>
       <c r="N280" s="3" t="n">
-        <v>46080.3755787037</v>
+        <v>46080.45103009259</v>
       </c>
       <c r="O280" t="inlineStr">
         <is>
@@ -18608,7 +18600,7 @@
         <v>1</v>
       </c>
       <c r="N281" s="3" t="n">
-        <v>46080.36991898148</v>
+        <v>46080.48280092593</v>
       </c>
       <c r="O281" t="inlineStr">
         <is>
@@ -18672,7 +18664,7 @@
         <v>1</v>
       </c>
       <c r="N282" s="3" t="n">
-        <v>46080.39451388889</v>
+        <v>46080.47349537037</v>
       </c>
       <c r="O282" t="inlineStr">
         <is>
@@ -18736,7 +18728,7 @@
         <v>1</v>
       </c>
       <c r="N283" s="3" t="n">
-        <v>46080.3693287037</v>
+        <v>46080.45049768518</v>
       </c>
       <c r="O283" t="inlineStr">
         <is>
@@ -18800,7 +18792,7 @@
         <v>1</v>
       </c>
       <c r="N284" s="3" t="n">
-        <v>46080.38702546297</v>
+        <v>46080.47009259259</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18864,7 +18856,7 @@
         <v>1</v>
       </c>
       <c r="N285" s="3" t="n">
-        <v>46080.37729166666</v>
+        <v>46080.45846064815</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -18883,6 +18875,11 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>10.69.5.155</t>
+        </is>
+      </c>
       <c r="D286" t="n">
         <v>2019</v>
       </c>
@@ -18923,7 +18920,7 @@
         <v>1</v>
       </c>
       <c r="N286" s="3" t="n">
-        <v>46080.3784837963</v>
+        <v>46080.45284722222</v>
       </c>
       <c r="O286" t="inlineStr">
         <is>
@@ -18987,7 +18984,7 @@
         <v>1</v>
       </c>
       <c r="N287" s="3" t="n">
-        <v>46080.38151620371</v>
+        <v>46080.4609375</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
@@ -19051,7 +19048,7 @@
         <v>1</v>
       </c>
       <c r="N288" s="3" t="n">
-        <v>46080.39306712963</v>
+        <v>46080.46641203704</v>
       </c>
       <c r="O288" t="inlineStr">
         <is>
@@ -19115,7 +19112,7 @@
         <v>1</v>
       </c>
       <c r="N289" s="3" t="n">
-        <v>46080.38306712963</v>
+        <v>46080.45881944444</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -19909,7 +19906,7 @@
         <v>1</v>
       </c>
       <c r="N302" s="3" t="n">
-        <v>46080.38935185185</v>
+        <v>46080.46190972222</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -21025,7 +21022,7 @@
         </is>
       </c>
       <c r="N320" s="3" t="n">
-        <v>46080.38905092593</v>
+        <v>46080.46177083333</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21750,7 +21747,7 @@
         <v>1</v>
       </c>
       <c r="N332" s="3" t="n">
-        <v>46080.37769675926</v>
+        <v>46080.45699074074</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21814,7 +21811,7 @@
         <v>2</v>
       </c>
       <c r="N333" s="3" t="n">
-        <v>46080.40077546296</v>
+        <v>46080.4806712963</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21878,7 +21875,7 @@
         <v>2</v>
       </c>
       <c r="N334" s="3" t="n">
-        <v>46080.40155092593</v>
+        <v>46080.47775462963</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21942,7 +21939,7 @@
         <v>2</v>
       </c>
       <c r="N335" s="3" t="n">
-        <v>46080.39936342592</v>
+        <v>46080.4759837963</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -22006,7 +22003,7 @@
         <v>1</v>
       </c>
       <c r="N336" s="3" t="n">
-        <v>46080.39951388889</v>
+        <v>46080.47527777778</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22070,7 +22067,7 @@
         <v>1</v>
       </c>
       <c r="N337" s="3" t="n">
-        <v>46080.4034837963</v>
+        <v>46080.48038194444</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22134,7 +22131,7 @@
         <v>2</v>
       </c>
       <c r="N338" s="3" t="n">
-        <v>46080.40048611111</v>
+        <v>46080.48092592593</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -22198,7 +22195,7 @@
         <v>2</v>
       </c>
       <c r="N339" s="3" t="n">
-        <v>46080.38011574074</v>
+        <v>46080.45813657407</v>
       </c>
       <c r="O339" t="inlineStr">
         <is>
@@ -22390,7 +22387,7 @@
         <v>2</v>
       </c>
       <c r="N342" s="3" t="n">
-        <v>46079.55180555556</v>
+        <v>46080.46607638889</v>
       </c>
       <c r="O342" t="inlineStr">
         <is>
@@ -23836,7 +23833,7 @@
         <v>1</v>
       </c>
       <c r="N365" s="3" t="n">
-        <v>46080.37835648148</v>
+        <v>46080.45556712963</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
@@ -23902,7 +23899,7 @@
         </is>
       </c>
       <c r="N366" s="3" t="n">
-        <v>46080.37943287037</v>
+        <v>46080.46136574074</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -24028,7 +24025,7 @@
         </is>
       </c>
       <c r="N368" s="3" t="n">
-        <v>46080.39349537037</v>
+        <v>46080.46957175926</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -24089,7 +24086,7 @@
         </is>
       </c>
       <c r="N369" s="3" t="n">
-        <v>46080.39113425926</v>
+        <v>46080.46869212963</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
@@ -24361,8 +24358,11 @@
           <t>HP ProDesk 400 G5 SFF (Brazil)</t>
         </is>
       </c>
+      <c r="M373" t="n">
+        <v>1</v>
+      </c>
       <c r="N373" s="3" t="n">
-        <v>46078.57886574074</v>
+        <v>46080.48386574074</v>
       </c>
       <c r="O373" t="inlineStr">
         <is>
@@ -24431,7 +24431,7 @@
         <v>1</v>
       </c>
       <c r="N374" s="3" t="n">
-        <v>46080.39359953703</v>
+        <v>46080.47391203704</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24497,7 +24497,7 @@
         </is>
       </c>
       <c r="N375" s="3" t="n">
-        <v>46080.37733796296</v>
+        <v>46080.450625</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
@@ -24561,7 +24561,7 @@
         <v>1</v>
       </c>
       <c r="N376" s="3" t="n">
-        <v>46080.37488425926</v>
+        <v>46080.45059027777</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -24630,7 +24630,7 @@
         <v>2</v>
       </c>
       <c r="N377" s="3" t="n">
-        <v>46080.3978587963</v>
+        <v>46080.47788194445</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -24699,7 +24699,7 @@
         <v>2</v>
       </c>
       <c r="N378" s="3" t="n">
-        <v>46080.39538194444</v>
+        <v>46080.47616898148</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização automática 2026-02-27 13:52:07.938935
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>46080.48038194444</v>
+        <v>46080.55444444445</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>46080.47114583333</v>
+        <v>46080.54863425926</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
         <v>1</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>46080.45179398148</v>
+        <v>46080.53020833333</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>46080.45825231481</v>
+        <v>46080.53447916666</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -875,7 +875,7 @@
         <v>1</v>
       </c>
       <c r="N6" s="3" t="n">
-        <v>46080.45040509259</v>
+        <v>46080.48991898148</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -944,7 +944,7 @@
         <v>1</v>
       </c>
       <c r="N7" s="3" t="n">
-        <v>46080.48715277778</v>
+        <v>46080.56850694444</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -1259,7 +1259,7 @@
         <v>1</v>
       </c>
       <c r="N12" s="3" t="n">
-        <v>46080.47465277778</v>
+        <v>46080.55045138889</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1323,7 +1323,7 @@
         <v>1</v>
       </c>
       <c r="N13" s="3" t="n">
-        <v>46080.47429398148</v>
+        <v>46080.54997685185</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1387,7 +1387,7 @@
         <v>2</v>
       </c>
       <c r="N14" s="3" t="n">
-        <v>46080.48453703704</v>
+        <v>46080.55947916667</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1451,7 +1451,7 @@
         <v>1</v>
       </c>
       <c r="N15" s="3" t="n">
-        <v>46080.47511574074</v>
+        <v>46080.54986111111</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1515,7 +1515,7 @@
         <v>2</v>
       </c>
       <c r="N16" s="3" t="n">
-        <v>46080.45637731482</v>
+        <v>46080.53510416667</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1579,7 +1579,7 @@
         <v>1</v>
       </c>
       <c r="N17" s="3" t="n">
-        <v>46080.48695601852</v>
+        <v>46080.56532407407</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1643,7 +1643,7 @@
         <v>2</v>
       </c>
       <c r="N18" s="3" t="n">
-        <v>46080.47741898148</v>
+        <v>46080.55571759259</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1768,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="N20" s="3" t="n">
-        <v>46080.46861111111</v>
+        <v>46080.54733796296</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -2009,7 +2009,7 @@
         <v>1</v>
       </c>
       <c r="N24" s="3" t="n">
-        <v>46080.4104050926</v>
+        <v>46080.50407407407</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2183,7 +2183,7 @@
         <v>1</v>
       </c>
       <c r="N27" s="3" t="n">
-        <v>46080.44975694444</v>
+        <v>46080.50165509259</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -6570,7 +6570,7 @@
         <v>1</v>
       </c>
       <c r="N95" s="3" t="n">
-        <v>46080.48771990741</v>
+        <v>46080.56150462963</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -6639,7 +6639,7 @@
         <v>1</v>
       </c>
       <c r="N96" s="3" t="n">
-        <v>46080.47575231481</v>
+        <v>46080.55663194445</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
@@ -6658,11 +6658,6 @@
           <t>COORDENACAO</t>
         </is>
       </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>10.69.3.93</t>
-        </is>
-      </c>
       <c r="D97" t="n">
         <v>2025</v>
       </c>
@@ -6708,7 +6703,7 @@
         <v>1</v>
       </c>
       <c r="N97" s="3" t="n">
-        <v>46080.48465277778</v>
+        <v>46080.56026620371</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -6727,6 +6722,11 @@
           <t>COORDENACAO</t>
         </is>
       </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>10.69.3.94</t>
+        </is>
+      </c>
       <c r="D98" t="n">
         <v>2025</v>
       </c>
@@ -6772,7 +6772,7 @@
         <v>1</v>
       </c>
       <c r="N98" s="3" t="n">
-        <v>46080.45106481481</v>
+        <v>46080.57091435185</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -6841,7 +6841,7 @@
         <v>1</v>
       </c>
       <c r="N99" s="3" t="n">
-        <v>46080.45789351852</v>
+        <v>46080.56995370371</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -6910,7 +6910,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>46080.46795138889</v>
+        <v>46080.54212962963</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6979,7 +6979,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="3" t="n">
-        <v>46080.4562037037</v>
+        <v>46080.53892361111</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -7048,7 +7048,7 @@
         <v>1</v>
       </c>
       <c r="N102" s="3" t="n">
-        <v>46079.69769675926</v>
+        <v>46080.55222222222</v>
       </c>
       <c r="O102" t="inlineStr">
         <is>
@@ -7117,7 +7117,7 @@
         <v>2</v>
       </c>
       <c r="N103" s="3" t="n">
-        <v>46080.473125</v>
+        <v>46080.54775462963</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7512,7 +7512,7 @@
         <v>1</v>
       </c>
       <c r="N109" s="3" t="n">
-        <v>46080.45012731481</v>
+        <v>46080.56951388889</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7581,7 +7581,7 @@
         <v>2</v>
       </c>
       <c r="N110" s="3" t="n">
-        <v>46080.48027777778</v>
+        <v>46080.56189814815</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7719,7 +7719,7 @@
         <v>2</v>
       </c>
       <c r="N112" s="3" t="n">
-        <v>46080.46828703704</v>
+        <v>46080.54488425926</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7788,7 +7788,7 @@
         <v>1</v>
       </c>
       <c r="N113" s="3" t="n">
-        <v>46080.48717592593</v>
+        <v>46080.56380787037</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7857,7 +7857,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>46080.45215277778</v>
+        <v>46080.56927083333</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -7923,7 +7923,7 @@
         </is>
       </c>
       <c r="N115" s="3" t="n">
-        <v>46080.4874537037</v>
+        <v>46080.56152777778</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -7992,7 +7992,7 @@
         <v>1</v>
       </c>
       <c r="N116" s="3" t="n">
-        <v>46080.48638888889</v>
+        <v>46080.56825231481</v>
       </c>
       <c r="O116" t="inlineStr">
         <is>
@@ -8011,11 +8011,6 @@
           <t>DP</t>
         </is>
       </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>10.69.3.23</t>
-        </is>
-      </c>
       <c r="D117" t="n">
         <v>2025</v>
       </c>
@@ -8061,7 +8056,7 @@
         <v>1</v>
       </c>
       <c r="N117" s="3" t="n">
-        <v>46080.47449074074</v>
+        <v>46080.55467592592</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -8127,7 +8122,7 @@
         </is>
       </c>
       <c r="N118" s="3" t="n">
-        <v>46080.4571875</v>
+        <v>46080.53351851852</v>
       </c>
       <c r="O118" t="inlineStr">
         <is>
@@ -8265,7 +8260,7 @@
         <v>1</v>
       </c>
       <c r="N120" s="3" t="n">
-        <v>46080.48518518519</v>
+        <v>46080.56359953704</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -8334,7 +8329,7 @@
         <v>1</v>
       </c>
       <c r="N121" s="3" t="n">
-        <v>46080.46542824074</v>
+        <v>46080.5434375</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -8400,7 +8395,7 @@
         </is>
       </c>
       <c r="N122" s="3" t="n">
-        <v>46080.4846875</v>
+        <v>46080.56210648148</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -8469,7 +8464,7 @@
         <v>2</v>
       </c>
       <c r="N123" s="3" t="n">
-        <v>46080.45436342592</v>
+        <v>46080.56474537037</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -8538,7 +8533,7 @@
         <v>1</v>
       </c>
       <c r="N124" s="3" t="n">
-        <v>46080.48311342593</v>
+        <v>46080.56439814815</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -8676,7 +8671,7 @@
         <v>2</v>
       </c>
       <c r="N126" s="3" t="n">
-        <v>46080.47274305556</v>
+        <v>46080.54996527778</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -8745,7 +8740,7 @@
         <v>2</v>
       </c>
       <c r="N127" s="3" t="n">
-        <v>46080.46353009259</v>
+        <v>46080.54420138889</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -8814,7 +8809,7 @@
         <v>1</v>
       </c>
       <c r="N128" s="3" t="n">
-        <v>46080.45328703704</v>
+        <v>46080.56803240741</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -8883,7 +8878,7 @@
         <v>1</v>
       </c>
       <c r="N129" s="3" t="n">
-        <v>46080.46626157407</v>
+        <v>46080.54393518518</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -8952,7 +8947,7 @@
         <v>1</v>
       </c>
       <c r="N130" s="3" t="n">
-        <v>46080.45143518518</v>
+        <v>46080.53233796296</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -9016,7 +9011,7 @@
         <v>1</v>
       </c>
       <c r="N131" s="3" t="n">
-        <v>46080.47667824074</v>
+        <v>46080.55104166667</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -9149,7 +9144,7 @@
         <v>1</v>
       </c>
       <c r="N133" s="3" t="n">
-        <v>46080.48716435185</v>
+        <v>46080.56614583333</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -9213,7 +9208,7 @@
         <v>1</v>
       </c>
       <c r="N134" s="3" t="n">
-        <v>46080.4570949074</v>
+        <v>46080.53532407407</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -9277,7 +9272,7 @@
         <v>1</v>
       </c>
       <c r="N135" s="3" t="n">
-        <v>46080.4569212963</v>
+        <v>46080.53714120371</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -9468,7 +9463,7 @@
         <v>1</v>
       </c>
       <c r="N138" s="3" t="n">
-        <v>46080.45041666667</v>
+        <v>46080.5653125</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9532,7 +9527,7 @@
         <v>1</v>
       </c>
       <c r="N139" s="3" t="n">
-        <v>46080.45789351852</v>
+        <v>46080.53659722222</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9596,7 +9591,7 @@
         <v>1</v>
       </c>
       <c r="N140" s="3" t="n">
-        <v>46080.45467592592</v>
+        <v>46080.53516203703</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9660,7 +9655,7 @@
         <v>1</v>
       </c>
       <c r="N141" s="3" t="n">
-        <v>46080.48293981481</v>
+        <v>46080.56797453704</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9724,7 +9719,7 @@
         <v>1</v>
       </c>
       <c r="N142" s="3" t="n">
-        <v>46080.454375</v>
+        <v>46080.5315625</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9852,7 +9847,7 @@
         <v>1</v>
       </c>
       <c r="N144" s="3" t="n">
-        <v>46080.45821759259</v>
+        <v>46080.56961805555</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9980,7 +9975,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="3" t="n">
-        <v>46080.45150462963</v>
+        <v>46080.56328703704</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10044,7 +10039,7 @@
         <v>1</v>
       </c>
       <c r="N147" s="3" t="n">
-        <v>46080.48042824074</v>
+        <v>46080.55989583334</v>
       </c>
       <c r="O147" t="inlineStr">
         <is>
@@ -10108,7 +10103,7 @@
         <v>1</v>
       </c>
       <c r="N148" s="3" t="n">
-        <v>46080.45887731481</v>
+        <v>46080.5372337963</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10172,7 +10167,7 @@
         <v>1</v>
       </c>
       <c r="N149" s="3" t="n">
-        <v>46080.47166666666</v>
+        <v>46080.54928240741</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -10236,7 +10231,7 @@
         <v>1</v>
       </c>
       <c r="N150" s="3" t="n">
-        <v>46080.45399305555</v>
+        <v>46080.56776620371</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -10300,7 +10295,7 @@
         <v>1</v>
       </c>
       <c r="N151" s="3" t="n">
-        <v>46080.45797453704</v>
+        <v>46080.53873842592</v>
       </c>
       <c r="O151" t="inlineStr">
         <is>
@@ -10364,7 +10359,7 @@
         <v>1</v>
       </c>
       <c r="N152" s="3" t="n">
-        <v>46080.45348379629</v>
+        <v>46080.56958333333</v>
       </c>
       <c r="O152" t="inlineStr">
         <is>
@@ -10487,7 +10482,7 @@
         <v>1</v>
       </c>
       <c r="N154" s="3" t="n">
-        <v>46080.46960648148</v>
+        <v>46080.54640046296</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10551,7 +10546,7 @@
         <v>1</v>
       </c>
       <c r="N155" s="3" t="n">
-        <v>46080.45189814815</v>
+        <v>46080.57050925926</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10615,7 +10610,7 @@
         <v>1</v>
       </c>
       <c r="N156" s="3" t="n">
-        <v>46080.48587962963</v>
+        <v>46080.56537037037</v>
       </c>
       <c r="O156" t="inlineStr">
         <is>
@@ -10679,7 +10674,7 @@
         <v>1</v>
       </c>
       <c r="N157" s="3" t="n">
-        <v>46080.45710648148</v>
+        <v>46080.53200231482</v>
       </c>
       <c r="O157" t="inlineStr">
         <is>
@@ -10743,7 +10738,7 @@
         <v>1</v>
       </c>
       <c r="N158" s="3" t="n">
-        <v>46080.46634259259</v>
+        <v>46080.54263888889</v>
       </c>
       <c r="O158" t="inlineStr">
         <is>
@@ -10807,7 +10802,7 @@
         <v>1</v>
       </c>
       <c r="N159" s="3" t="n">
-        <v>46080.4621875</v>
+        <v>46080.53868055555</v>
       </c>
       <c r="O159" t="inlineStr">
         <is>
@@ -10871,7 +10866,7 @@
         <v>1</v>
       </c>
       <c r="N160" s="3" t="n">
-        <v>46080.48313657408</v>
+        <v>46080.55818287037</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
@@ -10935,7 +10930,7 @@
         <v>1</v>
       </c>
       <c r="N161" s="3" t="n">
-        <v>46080.45240740741</v>
+        <v>46080.5344675926</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -10999,7 +10994,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="3" t="n">
-        <v>46080.4729050926</v>
+        <v>46080.55130787037</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11127,7 +11122,7 @@
         <v>2</v>
       </c>
       <c r="N164" s="3" t="n">
-        <v>46080.48660879629</v>
+        <v>46080.56961805555</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11191,7 +11186,7 @@
         <v>2</v>
       </c>
       <c r="N165" s="3" t="n">
-        <v>46080.48392361111</v>
+        <v>46080.56491898148</v>
       </c>
       <c r="O165" t="inlineStr">
         <is>
@@ -11255,7 +11250,7 @@
         <v>2</v>
       </c>
       <c r="N166" s="3" t="n">
-        <v>46080.45648148148</v>
+        <v>46080.53633101852</v>
       </c>
       <c r="O166" t="inlineStr">
         <is>
@@ -11319,7 +11314,7 @@
         <v>2</v>
       </c>
       <c r="N167" s="3" t="n">
-        <v>46080.48092592593</v>
+        <v>46080.5565625</v>
       </c>
       <c r="O167" t="inlineStr">
         <is>
@@ -11383,7 +11378,7 @@
         <v>2</v>
       </c>
       <c r="N168" s="3" t="n">
-        <v>46080.47665509259</v>
+        <v>46080.55756944444</v>
       </c>
       <c r="O168" t="inlineStr">
         <is>
@@ -11447,7 +11442,7 @@
         <v>2</v>
       </c>
       <c r="N169" s="3" t="n">
-        <v>46079.74877314815</v>
+        <v>46080.54219907407</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -11511,7 +11506,7 @@
         <v>2</v>
       </c>
       <c r="N170" s="3" t="n">
-        <v>46080.46075231482</v>
+        <v>46080.56950231481</v>
       </c>
       <c r="O170" t="inlineStr">
         <is>
@@ -11575,7 +11570,7 @@
         <v>2</v>
       </c>
       <c r="N171" s="3" t="n">
-        <v>46080.48310185185</v>
+        <v>46080.56064814814</v>
       </c>
       <c r="O171" t="inlineStr">
         <is>
@@ -11639,7 +11634,7 @@
         <v>2</v>
       </c>
       <c r="N172" s="3" t="n">
-        <v>46080.4549537037</v>
+        <v>46080.56850694444</v>
       </c>
       <c r="O172" t="inlineStr">
         <is>
@@ -11703,7 +11698,7 @@
         <v>1</v>
       </c>
       <c r="N173" s="3" t="n">
-        <v>46080.46209490741</v>
+        <v>46080.57068287037</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -11767,7 +11762,7 @@
         <v>2</v>
       </c>
       <c r="N174" s="3" t="n">
-        <v>46080.45770833334</v>
+        <v>46080.53223379629</v>
       </c>
       <c r="O174" t="inlineStr">
         <is>
@@ -11831,7 +11826,7 @@
         <v>2</v>
       </c>
       <c r="N175" s="3" t="n">
-        <v>46080.45481481482</v>
+        <v>46080.56753472222</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -11895,7 +11890,7 @@
         <v>2</v>
       </c>
       <c r="N176" s="3" t="n">
-        <v>46080.47548611111</v>
+        <v>46080.54592592592</v>
       </c>
       <c r="O176" t="inlineStr">
         <is>
@@ -11959,7 +11954,7 @@
         <v>2</v>
       </c>
       <c r="N177" s="3" t="n">
-        <v>46080.45980324074</v>
+        <v>46080.5381712963</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
@@ -12023,7 +12018,7 @@
         <v>2</v>
       </c>
       <c r="N178" s="3" t="n">
-        <v>46080.4775</v>
+        <v>46080.55266203704</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12087,7 +12082,7 @@
         <v>1</v>
       </c>
       <c r="N179" s="3" t="n">
-        <v>46080.47530092593</v>
+        <v>46080.55313657408</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12151,7 +12146,7 @@
         <v>1</v>
       </c>
       <c r="N180" s="3" t="n">
-        <v>46080.47428240741</v>
+        <v>46080.5505324074</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12343,7 +12338,7 @@
         <v>1</v>
       </c>
       <c r="N183" s="3" t="n">
-        <v>46080.48096064815</v>
+        <v>46080.55359953704</v>
       </c>
       <c r="O183" t="inlineStr">
         <is>
@@ -12412,7 +12407,7 @@
         <v>2</v>
       </c>
       <c r="N184" s="3" t="n">
-        <v>46080.47369212963</v>
+        <v>46080.55438657408</v>
       </c>
       <c r="O184" t="inlineStr">
         <is>
@@ -12540,7 +12535,7 @@
         <v>1</v>
       </c>
       <c r="N186" s="3" t="n">
-        <v>46080.48287037037</v>
+        <v>46080.56283564815</v>
       </c>
       <c r="O186" t="inlineStr">
         <is>
@@ -12604,7 +12599,7 @@
         <v>1</v>
       </c>
       <c r="N187" s="3" t="n">
-        <v>46080.47230324074</v>
+        <v>46080.55517361111</v>
       </c>
       <c r="O187" t="inlineStr">
         <is>
@@ -12668,7 +12663,7 @@
         <v>1</v>
       </c>
       <c r="N188" s="3" t="n">
-        <v>46080.44773148148</v>
+        <v>46080.48842592593</v>
       </c>
       <c r="O188" t="inlineStr">
         <is>
@@ -12796,7 +12791,7 @@
         </is>
       </c>
       <c r="N190" s="3" t="n">
-        <v>46080.46491898148</v>
+        <v>46080.54241898148</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12924,7 +12919,7 @@
         <v>1</v>
       </c>
       <c r="N192" s="3" t="n">
-        <v>46080.47545138889</v>
+        <v>46080.5575462963</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -13049,7 +13044,7 @@
         <v>2</v>
       </c>
       <c r="N194" s="3" t="n">
-        <v>46080.48358796296</v>
+        <v>46080.55902777778</v>
       </c>
       <c r="O194" t="inlineStr">
         <is>
@@ -13113,7 +13108,7 @@
         <v>1</v>
       </c>
       <c r="N195" s="3" t="n">
-        <v>46080.45819444444</v>
+        <v>46080.54003472222</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13177,7 +13172,7 @@
         <v>1</v>
       </c>
       <c r="N196" s="3" t="n">
-        <v>46080.46078703704</v>
+        <v>46080.5384375</v>
       </c>
       <c r="O196" t="inlineStr">
         <is>
@@ -13305,7 +13300,7 @@
         <v>1</v>
       </c>
       <c r="N198" s="3" t="n">
-        <v>46080.45265046296</v>
+        <v>46080.53100694445</v>
       </c>
       <c r="O198" t="inlineStr">
         <is>
@@ -13369,7 +13364,7 @@
         <v>1</v>
       </c>
       <c r="N199" s="3" t="n">
-        <v>46080.48491898148</v>
+        <v>46080.56252314815</v>
       </c>
       <c r="O199" t="inlineStr">
         <is>
@@ -13433,7 +13428,7 @@
         <v>1</v>
       </c>
       <c r="N200" s="3" t="n">
-        <v>46080.46542824074</v>
+        <v>46080.54413194444</v>
       </c>
       <c r="O200" t="inlineStr">
         <is>
@@ -13494,7 +13489,7 @@
         </is>
       </c>
       <c r="N201" s="3" t="n">
-        <v>46080.47800925926</v>
+        <v>46080.55903935185</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -13558,7 +13553,7 @@
         <v>1</v>
       </c>
       <c r="N202" s="3" t="n">
-        <v>46080.48430555555</v>
+        <v>46080.5609375</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13622,7 +13617,7 @@
         <v>1</v>
       </c>
       <c r="N203" s="3" t="n">
-        <v>46080.45458333333</v>
+        <v>46080.56707175926</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13686,7 +13681,7 @@
         <v>1</v>
       </c>
       <c r="N204" s="3" t="n">
-        <v>46080.46799768518</v>
+        <v>46080.54509259259</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13750,7 +13745,7 @@
         <v>1</v>
       </c>
       <c r="N205" s="3" t="n">
-        <v>46080.44791666666</v>
+        <v>46080.56994212963</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13814,7 +13809,7 @@
         <v>1</v>
       </c>
       <c r="N206" s="3" t="n">
-        <v>46080.45133101852</v>
+        <v>46080.56957175926</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -13878,7 +13873,7 @@
         <v>1</v>
       </c>
       <c r="N207" s="3" t="n">
-        <v>46080.46159722222</v>
+        <v>46080.53872685185</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -13942,7 +13937,7 @@
         <v>1</v>
       </c>
       <c r="N208" s="3" t="n">
-        <v>46080.46368055556</v>
+        <v>46080.53621527777</v>
       </c>
       <c r="O208" t="inlineStr">
         <is>
@@ -14006,7 +14001,7 @@
         <v>1</v>
       </c>
       <c r="N209" s="3" t="n">
-        <v>46080.47939814815</v>
+        <v>46080.5510300926</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14070,7 +14065,7 @@
         <v>1</v>
       </c>
       <c r="N210" s="3" t="n">
-        <v>46080.48724537037</v>
+        <v>46080.56743055556</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14134,7 +14129,7 @@
         <v>1</v>
       </c>
       <c r="N211" s="3" t="n">
-        <v>46080.48079861111</v>
+        <v>46080.55789351852</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -14198,7 +14193,7 @@
         <v>1</v>
       </c>
       <c r="N212" s="3" t="n">
-        <v>46080.48443287037</v>
+        <v>46080.56390046296</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -14262,7 +14257,7 @@
         <v>1</v>
       </c>
       <c r="N213" s="3" t="n">
-        <v>46080.46354166666</v>
+        <v>46080.54304398148</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
@@ -14326,7 +14321,7 @@
         <v>1</v>
       </c>
       <c r="N214" s="3" t="n">
-        <v>46080.47532407408</v>
+        <v>46080.55319444444</v>
       </c>
       <c r="O214" t="inlineStr">
         <is>
@@ -14390,7 +14385,7 @@
         <v>1</v>
       </c>
       <c r="N215" s="3" t="n">
-        <v>46080.47494212963</v>
+        <v>46080.555625</v>
       </c>
       <c r="O215" t="inlineStr">
         <is>
@@ -14454,7 +14449,7 @@
         <v>1</v>
       </c>
       <c r="N216" s="3" t="n">
-        <v>46080.47881944444</v>
+        <v>46080.56047453704</v>
       </c>
       <c r="O216" t="inlineStr">
         <is>
@@ -14518,7 +14513,7 @@
         <v>1</v>
       </c>
       <c r="N217" s="3" t="n">
-        <v>46080.47697916667</v>
+        <v>46080.54903935185</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14582,7 +14577,7 @@
         <v>1</v>
       </c>
       <c r="N218" s="3" t="n">
-        <v>46080.45056712963</v>
+        <v>46080.5675462963</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14779,7 +14774,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="3" t="n">
-        <v>46080.45899305555</v>
+        <v>46080.53951388889</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14843,7 +14838,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="3" t="n">
-        <v>46080.46358796296</v>
+        <v>46080.54767361111</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -14907,7 +14902,7 @@
         <v>1</v>
       </c>
       <c r="N223" s="3" t="n">
-        <v>46080.45162037037</v>
+        <v>46080.56981481481</v>
       </c>
       <c r="O223" t="inlineStr">
         <is>
@@ -15099,7 +15094,7 @@
         <v>1</v>
       </c>
       <c r="N226" s="3" t="n">
-        <v>46080.48328703704</v>
+        <v>46080.56177083333</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15163,7 +15158,7 @@
         <v>1</v>
       </c>
       <c r="N227" s="3" t="n">
-        <v>46080.48710648148</v>
+        <v>46080.56414351852</v>
       </c>
       <c r="O227" t="inlineStr">
         <is>
@@ -15227,7 +15222,7 @@
         <v>1</v>
       </c>
       <c r="N228" s="3" t="n">
-        <v>46080.46450231481</v>
+        <v>46080.53840277778</v>
       </c>
       <c r="O228" t="inlineStr">
         <is>
@@ -15291,7 +15286,7 @@
         <v>1</v>
       </c>
       <c r="N229" s="3" t="n">
-        <v>46080.47861111111</v>
+        <v>46080.55005787037</v>
       </c>
       <c r="O229" t="inlineStr">
         <is>
@@ -15355,7 +15350,7 @@
         <v>1</v>
       </c>
       <c r="N230" s="3" t="n">
-        <v>46080.47380787037</v>
+        <v>46080.55082175926</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15419,7 +15414,7 @@
         <v>1</v>
       </c>
       <c r="N231" s="3" t="n">
-        <v>46080.46395833333</v>
+        <v>46080.53966435185</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15483,7 +15478,7 @@
         <v>1</v>
       </c>
       <c r="N232" s="3" t="n">
-        <v>46080.4562037037</v>
+        <v>46080.53744212963</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -15547,7 +15542,7 @@
         <v>1</v>
       </c>
       <c r="N233" s="3" t="n">
-        <v>46080.45034722222</v>
+        <v>46080.56686342593</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15611,7 +15606,7 @@
         <v>1</v>
       </c>
       <c r="N234" s="3" t="n">
-        <v>46080.45418981482</v>
+        <v>46080.56596064815</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -15675,7 +15670,7 @@
         <v>1</v>
       </c>
       <c r="N235" s="3" t="n">
-        <v>46080.47844907407</v>
+        <v>46080.55693287037</v>
       </c>
       <c r="O235" t="inlineStr">
         <is>
@@ -15867,7 +15862,7 @@
         <v>1</v>
       </c>
       <c r="N238" s="3" t="n">
-        <v>46080.4740625</v>
+        <v>46080.54597222222</v>
       </c>
       <c r="O238" t="inlineStr">
         <is>
@@ -15931,7 +15926,7 @@
         <v>1</v>
       </c>
       <c r="N239" s="3" t="n">
-        <v>46080.45162037037</v>
+        <v>46080.56372685185</v>
       </c>
       <c r="O239" t="inlineStr">
         <is>
@@ -15995,7 +15990,7 @@
         <v>1</v>
       </c>
       <c r="N240" s="3" t="n">
-        <v>46080.45166666667</v>
+        <v>46080.56627314815</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16059,7 +16054,7 @@
         <v>1</v>
       </c>
       <c r="N241" s="3" t="n">
-        <v>46080.45829861111</v>
+        <v>46080.57028935185</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16123,7 +16118,7 @@
         <v>1</v>
       </c>
       <c r="N242" s="3" t="n">
-        <v>46080.4580324074</v>
+        <v>46080.53491898148</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16374,7 +16369,7 @@
         <v>1</v>
       </c>
       <c r="N246" s="3" t="n">
-        <v>46080.45684027778</v>
+        <v>46080.53731481481</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16438,7 +16433,7 @@
         <v>1</v>
       </c>
       <c r="N247" s="3" t="n">
-        <v>46080.45277777778</v>
+        <v>46080.56631944444</v>
       </c>
       <c r="O247" t="inlineStr">
         <is>
@@ -16502,7 +16497,7 @@
         <v>1</v>
       </c>
       <c r="N248" s="3" t="n">
-        <v>46080.47719907408</v>
+        <v>46080.55763888889</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16625,7 +16620,7 @@
         <v>1</v>
       </c>
       <c r="N250" s="3" t="n">
-        <v>46080.46539351852</v>
+        <v>46080.53921296296</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16689,7 +16684,7 @@
         <v>1</v>
       </c>
       <c r="N251" s="3" t="n">
-        <v>46080.45438657407</v>
+        <v>46080.53762731481</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16817,7 +16812,7 @@
         <v>1</v>
       </c>
       <c r="N253" s="3" t="n">
-        <v>46080.47783564815</v>
+        <v>46080.55491898148</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16875,7 +16870,7 @@
         <v>1</v>
       </c>
       <c r="N254" s="3" t="n">
-        <v>46080.44922453703</v>
+        <v>46080.56361111111</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -16939,7 +16934,7 @@
         <v>1</v>
       </c>
       <c r="N255" s="3" t="n">
-        <v>46080.47686342592</v>
+        <v>46080.55412037037</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -17003,7 +16998,7 @@
         <v>1</v>
       </c>
       <c r="N256" s="3" t="n">
-        <v>46080.47652777778</v>
+        <v>46080.55171296297</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17067,7 +17062,7 @@
         <v>1</v>
       </c>
       <c r="N257" s="3" t="n">
-        <v>46080.47431712963</v>
+        <v>46080.55157407407</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17131,7 +17126,7 @@
         <v>1</v>
       </c>
       <c r="N258" s="3" t="n">
-        <v>46080.46045138889</v>
+        <v>46080.53712962963</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
@@ -17259,7 +17254,7 @@
         <v>1</v>
       </c>
       <c r="N260" s="3" t="n">
-        <v>46080.48371527778</v>
+        <v>46080.55952546297</v>
       </c>
       <c r="O260" t="inlineStr">
         <is>
@@ -17323,7 +17318,7 @@
         <v>1</v>
       </c>
       <c r="N261" s="3" t="n">
-        <v>46080.48236111111</v>
+        <v>46080.55782407407</v>
       </c>
       <c r="O261" t="inlineStr">
         <is>
@@ -17387,7 +17382,7 @@
         <v>1</v>
       </c>
       <c r="N262" s="3" t="n">
-        <v>46080.48291666667</v>
+        <v>46080.56418981482</v>
       </c>
       <c r="O262" t="inlineStr">
         <is>
@@ -17451,7 +17446,7 @@
         <v>1</v>
       </c>
       <c r="N263" s="3" t="n">
-        <v>46080.4571412037</v>
+        <v>46080.53746527778</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17515,7 +17510,7 @@
         <v>1</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>46080.46570601852</v>
+        <v>46080.54418981481</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17579,7 +17574,7 @@
         <v>1</v>
       </c>
       <c r="N265" s="3" t="n">
-        <v>46080.45185185185</v>
+        <v>46080.56488425926</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17643,7 +17638,7 @@
         <v>1</v>
       </c>
       <c r="N266" s="3" t="n">
-        <v>46080.46283564815</v>
+        <v>46080.54351851852</v>
       </c>
       <c r="O266" t="inlineStr">
         <is>
@@ -17707,7 +17702,7 @@
         <v>1</v>
       </c>
       <c r="N267" s="3" t="n">
-        <v>46080.4521875</v>
+        <v>46080.57068287037</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17771,7 +17766,7 @@
         <v>1</v>
       </c>
       <c r="N268" s="3" t="n">
-        <v>46080.48538194445</v>
+        <v>46080.56880787037</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17835,7 +17830,7 @@
         <v>1</v>
       </c>
       <c r="N269" s="3" t="n">
-        <v>46080.45818287037</v>
+        <v>46080.5344212963</v>
       </c>
       <c r="O269" t="inlineStr">
         <is>
@@ -17896,7 +17891,7 @@
         </is>
       </c>
       <c r="N270" s="3" t="n">
-        <v>46080.46216435185</v>
+        <v>46080.54138888889</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -18024,7 +18019,7 @@
         <v>1</v>
       </c>
       <c r="N272" s="3" t="n">
-        <v>46080.45615740741</v>
+        <v>46080.5358449074</v>
       </c>
       <c r="O272" t="inlineStr">
         <is>
@@ -18088,7 +18083,7 @@
         <v>2</v>
       </c>
       <c r="N273" s="3" t="n">
-        <v>46080.45869212963</v>
+        <v>46080.53863425926</v>
       </c>
       <c r="O273" t="inlineStr">
         <is>
@@ -18344,7 +18339,7 @@
         <v>1</v>
       </c>
       <c r="N277" s="3" t="n">
-        <v>46080.40255787037</v>
+        <v>46080.53513888889</v>
       </c>
       <c r="O277" t="inlineStr">
         <is>
@@ -18408,7 +18403,7 @@
         <v>1</v>
       </c>
       <c r="N278" s="3" t="n">
-        <v>46080.47564814815</v>
+        <v>46080.54747685185</v>
       </c>
       <c r="O278" t="inlineStr">
         <is>
@@ -18472,7 +18467,7 @@
         <v>1</v>
       </c>
       <c r="N279" s="3" t="n">
-        <v>46080.46008101852</v>
+        <v>46080.53621527777</v>
       </c>
       <c r="O279" t="inlineStr">
         <is>
@@ -18536,7 +18531,7 @@
         <v>1</v>
       </c>
       <c r="N280" s="3" t="n">
-        <v>46080.45103009259</v>
+        <v>46080.56951388889</v>
       </c>
       <c r="O280" t="inlineStr">
         <is>
@@ -18600,7 +18595,7 @@
         <v>1</v>
       </c>
       <c r="N281" s="3" t="n">
-        <v>46080.48280092593</v>
+        <v>46080.56284722222</v>
       </c>
       <c r="O281" t="inlineStr">
         <is>
@@ -18664,7 +18659,7 @@
         <v>1</v>
       </c>
       <c r="N282" s="3" t="n">
-        <v>46080.47349537037</v>
+        <v>46080.55122685185</v>
       </c>
       <c r="O282" t="inlineStr">
         <is>
@@ -18728,7 +18723,7 @@
         <v>1</v>
       </c>
       <c r="N283" s="3" t="n">
-        <v>46080.45049768518</v>
+        <v>46080.56560185185</v>
       </c>
       <c r="O283" t="inlineStr">
         <is>
@@ -18792,7 +18787,7 @@
         <v>1</v>
       </c>
       <c r="N284" s="3" t="n">
-        <v>46080.47009259259</v>
+        <v>46080.54980324074</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18856,7 +18851,7 @@
         <v>1</v>
       </c>
       <c r="N285" s="3" t="n">
-        <v>46080.45846064815</v>
+        <v>46080.53575231481</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -18920,7 +18915,7 @@
         <v>1</v>
       </c>
       <c r="N286" s="3" t="n">
-        <v>46080.45284722222</v>
+        <v>46080.56425925926</v>
       </c>
       <c r="O286" t="inlineStr">
         <is>
@@ -18984,7 +18979,7 @@
         <v>1</v>
       </c>
       <c r="N287" s="3" t="n">
-        <v>46080.4609375</v>
+        <v>46080.54148148148</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
@@ -19048,7 +19043,7 @@
         <v>1</v>
       </c>
       <c r="N288" s="3" t="n">
-        <v>46080.46641203704</v>
+        <v>46080.54546296296</v>
       </c>
       <c r="O288" t="inlineStr">
         <is>
@@ -19112,7 +19107,7 @@
         <v>1</v>
       </c>
       <c r="N289" s="3" t="n">
-        <v>46080.45881944444</v>
+        <v>46080.53413194444</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -19906,7 +19901,7 @@
         <v>1</v>
       </c>
       <c r="N302" s="3" t="n">
-        <v>46080.46190972222</v>
+        <v>46080.54085648148</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -21022,7 +21017,7 @@
         </is>
       </c>
       <c r="N320" s="3" t="n">
-        <v>46080.46177083333</v>
+        <v>46080.53795138889</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21747,7 +21742,7 @@
         <v>1</v>
       </c>
       <c r="N332" s="3" t="n">
-        <v>46080.45699074074</v>
+        <v>46080.565</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21811,7 +21806,7 @@
         <v>2</v>
       </c>
       <c r="N333" s="3" t="n">
-        <v>46080.4806712963</v>
+        <v>46080.56015046296</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21875,7 +21870,7 @@
         <v>2</v>
       </c>
       <c r="N334" s="3" t="n">
-        <v>46080.47775462963</v>
+        <v>46080.55841435185</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21939,7 +21934,7 @@
         <v>2</v>
       </c>
       <c r="N335" s="3" t="n">
-        <v>46080.4759837963</v>
+        <v>46080.55457175926</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -22003,7 +21998,7 @@
         <v>1</v>
       </c>
       <c r="N336" s="3" t="n">
-        <v>46080.47527777778</v>
+        <v>46080.55201388889</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22067,7 +22062,7 @@
         <v>1</v>
       </c>
       <c r="N337" s="3" t="n">
-        <v>46080.48038194444</v>
+        <v>46080.56247685185</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22131,7 +22126,7 @@
         <v>2</v>
       </c>
       <c r="N338" s="3" t="n">
-        <v>46080.48092592593</v>
+        <v>46080.56357638889</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -22195,7 +22190,7 @@
         <v>2</v>
       </c>
       <c r="N339" s="3" t="n">
-        <v>46080.45813657407</v>
+        <v>46080.53240740741</v>
       </c>
       <c r="O339" t="inlineStr">
         <is>
@@ -22323,7 +22318,7 @@
         <v>2</v>
       </c>
       <c r="N341" s="3" t="n">
-        <v>46079.5818287037</v>
+        <v>46080.54791666667</v>
       </c>
       <c r="O341" t="inlineStr">
         <is>
@@ -22387,7 +22382,7 @@
         <v>2</v>
       </c>
       <c r="N342" s="3" t="n">
-        <v>46080.46607638889</v>
+        <v>46080.54152777778</v>
       </c>
       <c r="O342" t="inlineStr">
         <is>
@@ -22704,7 +22699,7 @@
         <v>1</v>
       </c>
       <c r="N347" s="3" t="n">
-        <v>46079.62734953704</v>
+        <v>46080.52020833334</v>
       </c>
       <c r="O347" t="inlineStr">
         <is>
@@ -22768,7 +22763,7 @@
         <v>1</v>
       </c>
       <c r="N348" s="3" t="n">
-        <v>46079.6684837963</v>
+        <v>46080.55288194444</v>
       </c>
       <c r="O348" t="inlineStr">
         <is>
@@ -22832,7 +22827,7 @@
         <v>1</v>
       </c>
       <c r="N349" s="3" t="n">
-        <v>46079.62761574074</v>
+        <v>46080.55310185185</v>
       </c>
       <c r="O349" t="inlineStr">
         <is>
@@ -22891,7 +22886,7 @@
         <v>1</v>
       </c>
       <c r="N350" s="3" t="n">
-        <v>46079.69943287037</v>
+        <v>46080.53824074074</v>
       </c>
       <c r="O350" t="inlineStr">
         <is>
@@ -22955,7 +22950,7 @@
         <v>1</v>
       </c>
       <c r="N351" s="3" t="n">
-        <v>46079.86789351852</v>
+        <v>46080.54899305556</v>
       </c>
       <c r="O351" t="inlineStr">
         <is>
@@ -23019,7 +23014,7 @@
         <v>1</v>
       </c>
       <c r="N352" s="3" t="n">
-        <v>46077.58256944444</v>
+        <v>46080.55096064815</v>
       </c>
       <c r="O352" t="inlineStr">
         <is>
@@ -23080,7 +23075,7 @@
         </is>
       </c>
       <c r="N353" s="3" t="n">
-        <v>46079.65965277778</v>
+        <v>46080.55033564815</v>
       </c>
       <c r="O353" t="inlineStr">
         <is>
@@ -23141,7 +23136,7 @@
         </is>
       </c>
       <c r="N354" s="3" t="n">
-        <v>46079.6679050926</v>
+        <v>46080.51325231481</v>
       </c>
       <c r="O354" t="inlineStr">
         <is>
@@ -23205,7 +23200,7 @@
         <v>1</v>
       </c>
       <c r="N355" s="3" t="n">
-        <v>46079.66519675926</v>
+        <v>46080.54849537037</v>
       </c>
       <c r="O355" t="inlineStr">
         <is>
@@ -23269,7 +23264,7 @@
         <v>1</v>
       </c>
       <c r="N356" s="3" t="n">
-        <v>46079.6677662037</v>
+        <v>46080.55354166667</v>
       </c>
       <c r="O356" t="inlineStr">
         <is>
@@ -23333,7 +23328,7 @@
         <v>1</v>
       </c>
       <c r="N357" s="3" t="n">
-        <v>46079.66325231481</v>
+        <v>46080.55361111111</v>
       </c>
       <c r="O357" t="inlineStr">
         <is>
@@ -23392,7 +23387,7 @@
         <v>1</v>
       </c>
       <c r="N358" s="3" t="n">
-        <v>46079.67070601852</v>
+        <v>46080.55364583333</v>
       </c>
       <c r="O358" t="inlineStr">
         <is>
@@ -23456,7 +23451,7 @@
         <v>2</v>
       </c>
       <c r="N359" s="3" t="n">
-        <v>46079.66747685185</v>
+        <v>46080.55465277778</v>
       </c>
       <c r="O359" t="inlineStr">
         <is>
@@ -23520,7 +23515,7 @@
         <v>2</v>
       </c>
       <c r="N360" s="3" t="n">
-        <v>46079.67631944444</v>
+        <v>46080.55405092592</v>
       </c>
       <c r="O360" t="inlineStr">
         <is>
@@ -23833,7 +23828,7 @@
         <v>1</v>
       </c>
       <c r="N365" s="3" t="n">
-        <v>46080.45556712963</v>
+        <v>46080.56840277778</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
@@ -23899,7 +23894,7 @@
         </is>
       </c>
       <c r="N366" s="3" t="n">
-        <v>46080.46136574074</v>
+        <v>46080.53409722223</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -24025,7 +24020,7 @@
         </is>
       </c>
       <c r="N368" s="3" t="n">
-        <v>46080.46957175926</v>
+        <v>46080.54230324074</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -24044,6 +24039,11 @@
           <t>RH</t>
         </is>
       </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>10.69.3.13</t>
+        </is>
+      </c>
       <c r="D369" t="n">
         <v>2025</v>
       </c>
@@ -24086,7 +24086,7 @@
         </is>
       </c>
       <c r="N369" s="3" t="n">
-        <v>46080.46869212963</v>
+        <v>46080.56685185185</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
@@ -24431,7 +24431,7 @@
         <v>1</v>
       </c>
       <c r="N374" s="3" t="n">
-        <v>46080.47391203704</v>
+        <v>46080.55211805556</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24497,7 +24497,7 @@
         </is>
       </c>
       <c r="N375" s="3" t="n">
-        <v>46080.450625</v>
+        <v>46080.56451388889</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
@@ -24561,7 +24561,7 @@
         <v>1</v>
       </c>
       <c r="N376" s="3" t="n">
-        <v>46080.45059027777</v>
+        <v>46080.56719907407</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -24630,7 +24630,7 @@
         <v>2</v>
       </c>
       <c r="N377" s="3" t="n">
-        <v>46080.47788194445</v>
+        <v>46080.55475694445</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -24699,7 +24699,7 @@
         <v>2</v>
       </c>
       <c r="N378" s="3" t="n">
-        <v>46080.47616898148</v>
+        <v>46080.55615740741</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização automática 2026-02-27 15:52:05.422298
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>46080.55444444445</v>
+        <v>46080.62944444444</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>46080.54863425926</v>
+        <v>46080.62396990741</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -739,10 +739,10 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>46080.53020833333</v>
+        <v>46080.64891203704</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>46080.53447916666</v>
+        <v>46080.65253472222</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -944,7 +944,7 @@
         <v>1</v>
       </c>
       <c r="N7" s="3" t="n">
-        <v>46080.56850694444</v>
+        <v>46080.64746527778</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -1259,7 +1259,7 @@
         <v>1</v>
       </c>
       <c r="N12" s="3" t="n">
-        <v>46080.55045138889</v>
+        <v>46080.62701388889</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1323,7 +1323,7 @@
         <v>1</v>
       </c>
       <c r="N13" s="3" t="n">
-        <v>46080.54997685185</v>
+        <v>46080.62956018518</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1387,7 +1387,7 @@
         <v>2</v>
       </c>
       <c r="N14" s="3" t="n">
-        <v>46080.55947916667</v>
+        <v>46080.6306712963</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1451,7 +1451,7 @@
         <v>1</v>
       </c>
       <c r="N15" s="3" t="n">
-        <v>46080.54986111111</v>
+        <v>46080.62552083333</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1515,7 +1515,7 @@
         <v>2</v>
       </c>
       <c r="N16" s="3" t="n">
-        <v>46080.53510416667</v>
+        <v>46080.65090277778</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1579,7 +1579,7 @@
         <v>1</v>
       </c>
       <c r="N17" s="3" t="n">
-        <v>46080.56532407407</v>
+        <v>46080.61520833334</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1643,7 +1643,7 @@
         <v>2</v>
       </c>
       <c r="N18" s="3" t="n">
-        <v>46080.55571759259</v>
+        <v>46080.63137731481</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1768,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="N20" s="3" t="n">
-        <v>46080.54733796296</v>
+        <v>46080.62667824074</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1910,6 +1910,11 @@
           <t>AUDITORIO</t>
         </is>
       </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>10.69.3.146</t>
+        </is>
+      </c>
       <c r="D23" t="n">
         <v>2018</v>
       </c>
@@ -1950,7 +1955,7 @@
         <v>1</v>
       </c>
       <c r="N23" s="3" t="n">
-        <v>46080.38017361111</v>
+        <v>46080.61047453704</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -6570,7 +6575,7 @@
         <v>1</v>
       </c>
       <c r="N95" s="3" t="n">
-        <v>46080.56150462963</v>
+        <v>46080.63277777778</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -6639,7 +6644,7 @@
         <v>1</v>
       </c>
       <c r="N96" s="3" t="n">
-        <v>46080.55663194445</v>
+        <v>46080.63701388889</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
@@ -6703,7 +6708,7 @@
         <v>1</v>
       </c>
       <c r="N97" s="3" t="n">
-        <v>46080.56026620371</v>
+        <v>46080.63965277778</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -6772,7 +6777,7 @@
         <v>1</v>
       </c>
       <c r="N98" s="3" t="n">
-        <v>46080.57091435185</v>
+        <v>46080.65280092593</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -6841,7 +6846,7 @@
         <v>1</v>
       </c>
       <c r="N99" s="3" t="n">
-        <v>46080.56995370371</v>
+        <v>46080.65282407407</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -6910,7 +6915,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>46080.54212962963</v>
+        <v>46080.62483796296</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6979,7 +6984,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="3" t="n">
-        <v>46080.53892361111</v>
+        <v>46080.65049768519</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -7048,7 +7053,7 @@
         <v>1</v>
       </c>
       <c r="N102" s="3" t="n">
-        <v>46080.55222222222</v>
+        <v>46080.63371527778</v>
       </c>
       <c r="O102" t="inlineStr">
         <is>
@@ -7117,7 +7122,7 @@
         <v>2</v>
       </c>
       <c r="N103" s="3" t="n">
-        <v>46080.54775462963</v>
+        <v>46080.62516203704</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7512,7 +7517,7 @@
         <v>1</v>
       </c>
       <c r="N109" s="3" t="n">
-        <v>46080.56951388889</v>
+        <v>46080.64436342593</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7581,7 +7586,7 @@
         <v>2</v>
       </c>
       <c r="N110" s="3" t="n">
-        <v>46080.56189814815</v>
+        <v>46080.64480324074</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7719,7 +7724,7 @@
         <v>2</v>
       </c>
       <c r="N112" s="3" t="n">
-        <v>46080.54488425926</v>
+        <v>46080.62628472222</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7788,7 +7793,7 @@
         <v>1</v>
       </c>
       <c r="N113" s="3" t="n">
-        <v>46080.56380787037</v>
+        <v>46080.63946759259</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7857,7 +7862,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>46080.56927083333</v>
+        <v>46080.646875</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -7923,7 +7928,7 @@
         </is>
       </c>
       <c r="N115" s="3" t="n">
-        <v>46080.56152777778</v>
+        <v>46080.63893518518</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -7992,7 +7997,7 @@
         <v>1</v>
       </c>
       <c r="N116" s="3" t="n">
-        <v>46080.56825231481</v>
+        <v>46080.64761574074</v>
       </c>
       <c r="O116" t="inlineStr">
         <is>
@@ -8056,7 +8061,7 @@
         <v>1</v>
       </c>
       <c r="N117" s="3" t="n">
-        <v>46080.55467592592</v>
+        <v>46080.63133101852</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -8122,7 +8127,7 @@
         </is>
       </c>
       <c r="N118" s="3" t="n">
-        <v>46080.53351851852</v>
+        <v>46080.65119212963</v>
       </c>
       <c r="O118" t="inlineStr">
         <is>
@@ -8260,7 +8265,7 @@
         <v>1</v>
       </c>
       <c r="N120" s="3" t="n">
-        <v>46080.56359953704</v>
+        <v>46080.64048611111</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -8329,7 +8334,7 @@
         <v>1</v>
       </c>
       <c r="N121" s="3" t="n">
-        <v>46080.5434375</v>
+        <v>46080.63362268519</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -8395,7 +8400,7 @@
         </is>
       </c>
       <c r="N122" s="3" t="n">
-        <v>46080.56210648148</v>
+        <v>46080.63844907407</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -8464,7 +8469,7 @@
         <v>2</v>
       </c>
       <c r="N123" s="3" t="n">
-        <v>46080.56474537037</v>
+        <v>46080.64402777778</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -8533,7 +8538,7 @@
         <v>1</v>
       </c>
       <c r="N124" s="3" t="n">
-        <v>46080.56439814815</v>
+        <v>46080.6445949074</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -8671,7 +8676,7 @@
         <v>2</v>
       </c>
       <c r="N126" s="3" t="n">
-        <v>46080.54996527778</v>
+        <v>46080.62743055556</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -8740,7 +8745,7 @@
         <v>2</v>
       </c>
       <c r="N127" s="3" t="n">
-        <v>46080.54420138889</v>
+        <v>46080.62059027778</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -8809,7 +8814,7 @@
         <v>1</v>
       </c>
       <c r="N128" s="3" t="n">
-        <v>46080.56803240741</v>
+        <v>46080.6449074074</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -8878,7 +8883,7 @@
         <v>1</v>
       </c>
       <c r="N129" s="3" t="n">
-        <v>46080.54393518518</v>
+        <v>46080.62761574074</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -8947,7 +8952,7 @@
         <v>1</v>
       </c>
       <c r="N130" s="3" t="n">
-        <v>46080.53233796296</v>
+        <v>46080.65162037037</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -9011,7 +9016,7 @@
         <v>1</v>
       </c>
       <c r="N131" s="3" t="n">
-        <v>46080.55104166667</v>
+        <v>46080.62782407407</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -9208,7 +9213,7 @@
         <v>1</v>
       </c>
       <c r="N134" s="3" t="n">
-        <v>46080.53532407407</v>
+        <v>46080.5740625</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -9272,7 +9277,7 @@
         <v>1</v>
       </c>
       <c r="N135" s="3" t="n">
-        <v>46080.53714120371</v>
+        <v>46080.6172337963</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -9463,7 +9468,7 @@
         <v>1</v>
       </c>
       <c r="N138" s="3" t="n">
-        <v>46080.5653125</v>
+        <v>46080.63853009259</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9527,7 +9532,7 @@
         <v>1</v>
       </c>
       <c r="N139" s="3" t="n">
-        <v>46080.53659722222</v>
+        <v>46080.63141203704</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9591,7 +9596,7 @@
         <v>1</v>
       </c>
       <c r="N140" s="3" t="n">
-        <v>46080.53516203703</v>
+        <v>46080.65231481481</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9655,7 +9660,7 @@
         <v>1</v>
       </c>
       <c r="N141" s="3" t="n">
-        <v>46080.56797453704</v>
+        <v>46080.64844907408</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9719,7 +9724,7 @@
         <v>1</v>
       </c>
       <c r="N142" s="3" t="n">
-        <v>46080.5315625</v>
+        <v>46080.65237268519</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9847,7 +9852,7 @@
         <v>1</v>
       </c>
       <c r="N144" s="3" t="n">
-        <v>46080.56961805555</v>
+        <v>46080.65091435185</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9911,7 +9916,7 @@
         <v>1</v>
       </c>
       <c r="N145" s="3" t="n">
-        <v>46079.8215625</v>
+        <v>46080.61993055556</v>
       </c>
       <c r="O145" t="inlineStr">
         <is>
@@ -9975,7 +9980,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="3" t="n">
-        <v>46080.56328703704</v>
+        <v>46080.61956018519</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10039,7 +10044,7 @@
         <v>1</v>
       </c>
       <c r="N147" s="3" t="n">
-        <v>46080.55989583334</v>
+        <v>46080.60875</v>
       </c>
       <c r="O147" t="inlineStr">
         <is>
@@ -10103,7 +10108,7 @@
         <v>1</v>
       </c>
       <c r="N148" s="3" t="n">
-        <v>46080.5372337963</v>
+        <v>46080.65302083334</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10167,7 +10172,7 @@
         <v>1</v>
       </c>
       <c r="N149" s="3" t="n">
-        <v>46080.54928240741</v>
+        <v>46080.62432870371</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -10231,7 +10236,7 @@
         <v>1</v>
       </c>
       <c r="N150" s="3" t="n">
-        <v>46080.56776620371</v>
+        <v>46080.64971064815</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -10295,7 +10300,7 @@
         <v>1</v>
       </c>
       <c r="N151" s="3" t="n">
-        <v>46080.53873842592</v>
+        <v>46080.65299768518</v>
       </c>
       <c r="O151" t="inlineStr">
         <is>
@@ -10359,7 +10364,7 @@
         <v>1</v>
       </c>
       <c r="N152" s="3" t="n">
-        <v>46080.56958333333</v>
+        <v>46080.6196875</v>
       </c>
       <c r="O152" t="inlineStr">
         <is>
@@ -10482,7 +10487,7 @@
         <v>1</v>
       </c>
       <c r="N154" s="3" t="n">
-        <v>46080.54640046296</v>
+        <v>46080.62075231481</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10546,7 +10551,7 @@
         <v>1</v>
       </c>
       <c r="N155" s="3" t="n">
-        <v>46080.57050925926</v>
+        <v>46080.65188657407</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10610,7 +10615,7 @@
         <v>1</v>
       </c>
       <c r="N156" s="3" t="n">
-        <v>46080.56537037037</v>
+        <v>46080.62487268518</v>
       </c>
       <c r="O156" t="inlineStr">
         <is>
@@ -10674,7 +10679,7 @@
         <v>1</v>
       </c>
       <c r="N157" s="3" t="n">
-        <v>46080.53200231482</v>
+        <v>46080.5724537037</v>
       </c>
       <c r="O157" t="inlineStr">
         <is>
@@ -10738,7 +10743,7 @@
         <v>1</v>
       </c>
       <c r="N158" s="3" t="n">
-        <v>46080.54263888889</v>
+        <v>46080.61611111111</v>
       </c>
       <c r="O158" t="inlineStr">
         <is>
@@ -10802,7 +10807,7 @@
         <v>1</v>
       </c>
       <c r="N159" s="3" t="n">
-        <v>46080.53868055555</v>
+        <v>46080.61833333333</v>
       </c>
       <c r="O159" t="inlineStr">
         <is>
@@ -10866,7 +10871,7 @@
         <v>1</v>
       </c>
       <c r="N160" s="3" t="n">
-        <v>46080.55818287037</v>
+        <v>46080.63131944444</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
@@ -10930,7 +10935,7 @@
         <v>1</v>
       </c>
       <c r="N161" s="3" t="n">
-        <v>46080.5344675926</v>
+        <v>46080.62393518518</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -10994,7 +10999,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="3" t="n">
-        <v>46080.55130787037</v>
+        <v>46080.63324074074</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11122,7 +11127,7 @@
         <v>2</v>
       </c>
       <c r="N164" s="3" t="n">
-        <v>46080.56961805555</v>
+        <v>46080.64672453704</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11250,7 +11255,7 @@
         <v>2</v>
       </c>
       <c r="N166" s="3" t="n">
-        <v>46080.53633101852</v>
+        <v>46080.61219907407</v>
       </c>
       <c r="O166" t="inlineStr">
         <is>
@@ -11314,7 +11319,7 @@
         <v>2</v>
       </c>
       <c r="N167" s="3" t="n">
-        <v>46080.5565625</v>
+        <v>46080.59599537037</v>
       </c>
       <c r="O167" t="inlineStr">
         <is>
@@ -11442,7 +11447,7 @@
         <v>2</v>
       </c>
       <c r="N169" s="3" t="n">
-        <v>46080.54219907407</v>
+        <v>46080.62070601852</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -11506,7 +11511,7 @@
         <v>2</v>
       </c>
       <c r="N170" s="3" t="n">
-        <v>46080.56950231481</v>
+        <v>46080.64862268518</v>
       </c>
       <c r="O170" t="inlineStr">
         <is>
@@ -11567,7 +11572,7 @@
         </is>
       </c>
       <c r="M171" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N171" s="3" t="n">
         <v>46080.56064814814</v>
@@ -11634,7 +11639,7 @@
         <v>2</v>
       </c>
       <c r="N172" s="3" t="n">
-        <v>46080.56850694444</v>
+        <v>46080.64740740741</v>
       </c>
       <c r="O172" t="inlineStr">
         <is>
@@ -11698,7 +11703,7 @@
         <v>1</v>
       </c>
       <c r="N173" s="3" t="n">
-        <v>46080.57068287037</v>
+        <v>46080.65034722222</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -11762,7 +11767,7 @@
         <v>2</v>
       </c>
       <c r="N174" s="3" t="n">
-        <v>46080.53223379629</v>
+        <v>46080.57200231482</v>
       </c>
       <c r="O174" t="inlineStr">
         <is>
@@ -11826,7 +11831,7 @@
         <v>2</v>
       </c>
       <c r="N175" s="3" t="n">
-        <v>46080.56753472222</v>
+        <v>46080.64421296296</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -11890,7 +11895,7 @@
         <v>2</v>
       </c>
       <c r="N176" s="3" t="n">
-        <v>46080.54592592592</v>
+        <v>46080.62340277778</v>
       </c>
       <c r="O176" t="inlineStr">
         <is>
@@ -11954,7 +11959,7 @@
         <v>2</v>
       </c>
       <c r="N177" s="3" t="n">
-        <v>46080.5381712963</v>
+        <v>46080.62196759259</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
@@ -12018,7 +12023,7 @@
         <v>2</v>
       </c>
       <c r="N178" s="3" t="n">
-        <v>46080.55266203704</v>
+        <v>46080.62789351852</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12082,7 +12087,7 @@
         <v>1</v>
       </c>
       <c r="N179" s="3" t="n">
-        <v>46080.55313657408</v>
+        <v>46080.63086805555</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12146,7 +12151,7 @@
         <v>1</v>
       </c>
       <c r="N180" s="3" t="n">
-        <v>46080.5505324074</v>
+        <v>46080.62075231481</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12338,7 +12343,7 @@
         <v>1</v>
       </c>
       <c r="N183" s="3" t="n">
-        <v>46080.55359953704</v>
+        <v>46080.62266203704</v>
       </c>
       <c r="O183" t="inlineStr">
         <is>
@@ -12407,7 +12412,7 @@
         <v>2</v>
       </c>
       <c r="N184" s="3" t="n">
-        <v>46080.55438657408</v>
+        <v>46080.63200231481</v>
       </c>
       <c r="O184" t="inlineStr">
         <is>
@@ -12535,7 +12540,7 @@
         <v>1</v>
       </c>
       <c r="N186" s="3" t="n">
-        <v>46080.56283564815</v>
+        <v>46080.60023148148</v>
       </c>
       <c r="O186" t="inlineStr">
         <is>
@@ -12599,7 +12604,7 @@
         <v>1</v>
       </c>
       <c r="N187" s="3" t="n">
-        <v>46080.55517361111</v>
+        <v>46080.63108796296</v>
       </c>
       <c r="O187" t="inlineStr">
         <is>
@@ -12749,11 +12754,6 @@
           <t>OPERACAO 8.1</t>
         </is>
       </c>
-      <c r="C190" t="inlineStr">
-        <is>
-          <t>10.69.5.59</t>
-        </is>
-      </c>
       <c r="D190" t="n">
         <v>2015</v>
       </c>
@@ -12791,7 +12791,7 @@
         </is>
       </c>
       <c r="N190" s="3" t="n">
-        <v>46080.54241898148</v>
+        <v>46080.63501157407</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12855,7 +12855,7 @@
         <v>1</v>
       </c>
       <c r="N191" s="3" t="n">
-        <v>46079.794375</v>
+        <v>46080.63179398148</v>
       </c>
       <c r="O191" t="inlineStr">
         <is>
@@ -12919,7 +12919,7 @@
         <v>1</v>
       </c>
       <c r="N192" s="3" t="n">
-        <v>46080.5575462963</v>
+        <v>46080.63790509259</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -13108,7 +13108,7 @@
         <v>1</v>
       </c>
       <c r="N195" s="3" t="n">
-        <v>46080.54003472222</v>
+        <v>46080.61961805556</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13172,7 +13172,7 @@
         <v>1</v>
       </c>
       <c r="N196" s="3" t="n">
-        <v>46080.5384375</v>
+        <v>46080.57857638889</v>
       </c>
       <c r="O196" t="inlineStr">
         <is>
@@ -13300,7 +13300,7 @@
         <v>1</v>
       </c>
       <c r="N198" s="3" t="n">
-        <v>46080.53100694445</v>
+        <v>46080.65349537037</v>
       </c>
       <c r="O198" t="inlineStr">
         <is>
@@ -13364,7 +13364,7 @@
         <v>1</v>
       </c>
       <c r="N199" s="3" t="n">
-        <v>46080.56252314815</v>
+        <v>46080.64201388889</v>
       </c>
       <c r="O199" t="inlineStr">
         <is>
@@ -13428,7 +13428,7 @@
         <v>1</v>
       </c>
       <c r="N200" s="3" t="n">
-        <v>46080.54413194444</v>
+        <v>46080.61910879629</v>
       </c>
       <c r="O200" t="inlineStr">
         <is>
@@ -13489,7 +13489,7 @@
         </is>
       </c>
       <c r="N201" s="3" t="n">
-        <v>46080.55903935185</v>
+        <v>46080.63416666666</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -13553,7 +13553,7 @@
         <v>1</v>
       </c>
       <c r="N202" s="3" t="n">
-        <v>46080.5609375</v>
+        <v>46080.6408912037</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13617,7 +13617,7 @@
         <v>1</v>
       </c>
       <c r="N203" s="3" t="n">
-        <v>46080.56707175926</v>
+        <v>46080.61767361111</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13681,7 +13681,7 @@
         <v>1</v>
       </c>
       <c r="N204" s="3" t="n">
-        <v>46080.54509259259</v>
+        <v>46080.6215625</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13745,7 +13745,7 @@
         <v>1</v>
       </c>
       <c r="N205" s="3" t="n">
-        <v>46080.56994212963</v>
+        <v>46080.64327546296</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13809,7 +13809,7 @@
         <v>1</v>
       </c>
       <c r="N206" s="3" t="n">
-        <v>46080.56957175926</v>
+        <v>46080.65179398148</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -13873,7 +13873,7 @@
         <v>1</v>
       </c>
       <c r="N207" s="3" t="n">
-        <v>46080.53872685185</v>
+        <v>46080.6159375</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -13937,7 +13937,7 @@
         <v>1</v>
       </c>
       <c r="N208" s="3" t="n">
-        <v>46080.53621527777</v>
+        <v>46080.57481481481</v>
       </c>
       <c r="O208" t="inlineStr">
         <is>
@@ -14001,7 +14001,7 @@
         <v>1</v>
       </c>
       <c r="N209" s="3" t="n">
-        <v>46080.5510300926</v>
+        <v>46080.62675925926</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14065,7 +14065,7 @@
         <v>1</v>
       </c>
       <c r="N210" s="3" t="n">
-        <v>46080.56743055556</v>
+        <v>46080.64144675926</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14129,7 +14129,7 @@
         <v>1</v>
       </c>
       <c r="N211" s="3" t="n">
-        <v>46080.55789351852</v>
+        <v>46080.62349537037</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -14193,7 +14193,7 @@
         <v>1</v>
       </c>
       <c r="N212" s="3" t="n">
-        <v>46080.56390046296</v>
+        <v>46080.63898148148</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -14321,7 +14321,7 @@
         <v>1</v>
       </c>
       <c r="N214" s="3" t="n">
-        <v>46080.55319444444</v>
+        <v>46080.63309027778</v>
       </c>
       <c r="O214" t="inlineStr">
         <is>
@@ -14385,7 +14385,7 @@
         <v>1</v>
       </c>
       <c r="N215" s="3" t="n">
-        <v>46080.555625</v>
+        <v>46080.63670138889</v>
       </c>
       <c r="O215" t="inlineStr">
         <is>
@@ -14449,7 +14449,7 @@
         <v>1</v>
       </c>
       <c r="N216" s="3" t="n">
-        <v>46080.56047453704</v>
+        <v>46080.63435185186</v>
       </c>
       <c r="O216" t="inlineStr">
         <is>
@@ -14513,7 +14513,7 @@
         <v>1</v>
       </c>
       <c r="N217" s="3" t="n">
-        <v>46080.54903935185</v>
+        <v>46080.62259259259</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14577,7 +14577,7 @@
         <v>1</v>
       </c>
       <c r="N218" s="3" t="n">
-        <v>46080.5675462963</v>
+        <v>46080.64501157407</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14641,7 +14641,7 @@
         <v>1</v>
       </c>
       <c r="N219" s="3" t="n">
-        <v>46080.3232175926</v>
+        <v>46080.61856481482</v>
       </c>
       <c r="O219" t="inlineStr">
         <is>
@@ -14774,7 +14774,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="3" t="n">
-        <v>46080.53951388889</v>
+        <v>46080.62303240741</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14838,7 +14838,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="3" t="n">
-        <v>46080.54767361111</v>
+        <v>46080.62339120371</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -14902,7 +14902,7 @@
         <v>1</v>
       </c>
       <c r="N223" s="3" t="n">
-        <v>46080.56981481481</v>
+        <v>46080.65202546296</v>
       </c>
       <c r="O223" t="inlineStr">
         <is>
@@ -14966,7 +14966,7 @@
         <v>1</v>
       </c>
       <c r="N224" s="3" t="n">
-        <v>46079.82978009259</v>
+        <v>46080.64589120371</v>
       </c>
       <c r="O224" t="inlineStr">
         <is>
@@ -15094,7 +15094,7 @@
         <v>1</v>
       </c>
       <c r="N226" s="3" t="n">
-        <v>46080.56177083333</v>
+        <v>46080.63903935185</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15158,7 +15158,7 @@
         <v>1</v>
       </c>
       <c r="N227" s="3" t="n">
-        <v>46080.56414351852</v>
+        <v>46080.63994212963</v>
       </c>
       <c r="O227" t="inlineStr">
         <is>
@@ -15222,7 +15222,7 @@
         <v>1</v>
       </c>
       <c r="N228" s="3" t="n">
-        <v>46080.53840277778</v>
+        <v>46080.61568287037</v>
       </c>
       <c r="O228" t="inlineStr">
         <is>
@@ -15350,7 +15350,7 @@
         <v>1</v>
       </c>
       <c r="N230" s="3" t="n">
-        <v>46080.55082175926</v>
+        <v>46080.62736111111</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15414,7 +15414,7 @@
         <v>1</v>
       </c>
       <c r="N231" s="3" t="n">
-        <v>46080.53966435185</v>
+        <v>46080.61688657408</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15478,7 +15478,7 @@
         <v>1</v>
       </c>
       <c r="N232" s="3" t="n">
-        <v>46080.53744212963</v>
+        <v>46080.65204861111</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -15542,7 +15542,7 @@
         <v>1</v>
       </c>
       <c r="N233" s="3" t="n">
-        <v>46080.56686342593</v>
+        <v>46080.64737268518</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15670,7 +15670,7 @@
         <v>1</v>
       </c>
       <c r="N235" s="3" t="n">
-        <v>46080.55693287037</v>
+        <v>46080.63100694444</v>
       </c>
       <c r="O235" t="inlineStr">
         <is>
@@ -15862,7 +15862,7 @@
         <v>1</v>
       </c>
       <c r="N238" s="3" t="n">
-        <v>46080.54597222222</v>
+        <v>46080.62494212963</v>
       </c>
       <c r="O238" t="inlineStr">
         <is>
@@ -15926,7 +15926,7 @@
         <v>1</v>
       </c>
       <c r="N239" s="3" t="n">
-        <v>46080.56372685185</v>
+        <v>46080.64140046296</v>
       </c>
       <c r="O239" t="inlineStr">
         <is>
@@ -15990,7 +15990,7 @@
         <v>1</v>
       </c>
       <c r="N240" s="3" t="n">
-        <v>46080.56627314815</v>
+        <v>46080.63086805555</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16054,7 +16054,7 @@
         <v>1</v>
       </c>
       <c r="N241" s="3" t="n">
-        <v>46080.57028935185</v>
+        <v>46080.60583333333</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16118,7 +16118,7 @@
         <v>1</v>
       </c>
       <c r="N242" s="3" t="n">
-        <v>46080.53491898148</v>
+        <v>46080.61520833334</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16305,7 +16305,7 @@
         <v>1</v>
       </c>
       <c r="N245" s="3" t="n">
-        <v>46079.8245949074</v>
+        <v>46080.62653935186</v>
       </c>
       <c r="O245" t="inlineStr">
         <is>
@@ -16369,7 +16369,7 @@
         <v>1</v>
       </c>
       <c r="N246" s="3" t="n">
-        <v>46080.53731481481</v>
+        <v>46080.61601851852</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16433,7 +16433,7 @@
         <v>1</v>
       </c>
       <c r="N247" s="3" t="n">
-        <v>46080.56631944444</v>
+        <v>46080.62762731482</v>
       </c>
       <c r="O247" t="inlineStr">
         <is>
@@ -16497,7 +16497,7 @@
         <v>1</v>
       </c>
       <c r="N248" s="3" t="n">
-        <v>46080.55763888889</v>
+        <v>46080.63480324074</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16620,7 +16620,7 @@
         <v>1</v>
       </c>
       <c r="N250" s="3" t="n">
-        <v>46080.53921296296</v>
+        <v>46080.62015046296</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16684,7 +16684,7 @@
         <v>1</v>
       </c>
       <c r="N251" s="3" t="n">
-        <v>46080.53762731481</v>
+        <v>46080.61557870371</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16748,7 +16748,7 @@
         <v>1</v>
       </c>
       <c r="N252" s="3" t="n">
-        <v>46079.78913194445</v>
+        <v>46080.6252662037</v>
       </c>
       <c r="O252" t="inlineStr">
         <is>
@@ -16812,7 +16812,7 @@
         <v>1</v>
       </c>
       <c r="N253" s="3" t="n">
-        <v>46080.55491898148</v>
+        <v>46080.62340277778</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16870,7 +16870,7 @@
         <v>1</v>
       </c>
       <c r="N254" s="3" t="n">
-        <v>46080.56361111111</v>
+        <v>46080.63398148148</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -16934,7 +16934,7 @@
         <v>1</v>
       </c>
       <c r="N255" s="3" t="n">
-        <v>46080.55412037037</v>
+        <v>46080.62864583333</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -16998,7 +16998,7 @@
         <v>1</v>
       </c>
       <c r="N256" s="3" t="n">
-        <v>46080.55171296297</v>
+        <v>46080.63064814815</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17062,7 +17062,7 @@
         <v>1</v>
       </c>
       <c r="N257" s="3" t="n">
-        <v>46080.55157407407</v>
+        <v>46080.63596064815</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17126,7 +17126,7 @@
         <v>1</v>
       </c>
       <c r="N258" s="3" t="n">
-        <v>46080.53712962963</v>
+        <v>46080.62800925926</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
@@ -17190,7 +17190,7 @@
         <v>1</v>
       </c>
       <c r="N259" s="3" t="n">
-        <v>46080.32083333333</v>
+        <v>46080.62923611111</v>
       </c>
       <c r="O259" t="inlineStr">
         <is>
@@ -17254,7 +17254,7 @@
         <v>1</v>
       </c>
       <c r="N260" s="3" t="n">
-        <v>46080.55952546297</v>
+        <v>46080.60126157408</v>
       </c>
       <c r="O260" t="inlineStr">
         <is>
@@ -17318,7 +17318,7 @@
         <v>1</v>
       </c>
       <c r="N261" s="3" t="n">
-        <v>46080.55782407407</v>
+        <v>46080.63490740741</v>
       </c>
       <c r="O261" t="inlineStr">
         <is>
@@ -17382,7 +17382,7 @@
         <v>1</v>
       </c>
       <c r="N262" s="3" t="n">
-        <v>46080.56418981482</v>
+        <v>46080.62202546297</v>
       </c>
       <c r="O262" t="inlineStr">
         <is>
@@ -17446,7 +17446,7 @@
         <v>1</v>
       </c>
       <c r="N263" s="3" t="n">
-        <v>46080.53746527778</v>
+        <v>46080.65016203704</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17510,7 +17510,7 @@
         <v>1</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>46080.54418981481</v>
+        <v>46080.62268518518</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17574,7 +17574,7 @@
         <v>1</v>
       </c>
       <c r="N265" s="3" t="n">
-        <v>46080.56488425926</v>
+        <v>46080.63731481481</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17638,7 +17638,7 @@
         <v>1</v>
       </c>
       <c r="N266" s="3" t="n">
-        <v>46080.54351851852</v>
+        <v>46080.62184027778</v>
       </c>
       <c r="O266" t="inlineStr">
         <is>
@@ -17702,7 +17702,7 @@
         <v>1</v>
       </c>
       <c r="N267" s="3" t="n">
-        <v>46080.57068287037</v>
+        <v>46080.65155092593</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17766,7 +17766,7 @@
         <v>1</v>
       </c>
       <c r="N268" s="3" t="n">
-        <v>46080.56880787037</v>
+        <v>46080.64229166666</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17830,7 +17830,7 @@
         <v>1</v>
       </c>
       <c r="N269" s="3" t="n">
-        <v>46080.5344212963</v>
+        <v>46080.65320601852</v>
       </c>
       <c r="O269" t="inlineStr">
         <is>
@@ -17891,7 +17891,7 @@
         </is>
       </c>
       <c r="N270" s="3" t="n">
-        <v>46080.54138888889</v>
+        <v>46080.62010416666</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -18019,7 +18019,7 @@
         <v>1</v>
       </c>
       <c r="N272" s="3" t="n">
-        <v>46080.5358449074</v>
+        <v>46080.62271990741</v>
       </c>
       <c r="O272" t="inlineStr">
         <is>
@@ -18083,7 +18083,7 @@
         <v>2</v>
       </c>
       <c r="N273" s="3" t="n">
-        <v>46080.53863425926</v>
+        <v>46080.6541087963</v>
       </c>
       <c r="O273" t="inlineStr">
         <is>
@@ -18659,7 +18659,7 @@
         <v>1</v>
       </c>
       <c r="N282" s="3" t="n">
-        <v>46080.55122685185</v>
+        <v>46080.62888888889</v>
       </c>
       <c r="O282" t="inlineStr">
         <is>
@@ -18787,7 +18787,7 @@
         <v>1</v>
       </c>
       <c r="N284" s="3" t="n">
-        <v>46080.54980324074</v>
+        <v>46080.62822916666</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18851,7 +18851,7 @@
         <v>1</v>
       </c>
       <c r="N285" s="3" t="n">
-        <v>46080.53575231481</v>
+        <v>46080.61467592593</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -18870,11 +18870,6 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
-      <c r="C286" t="inlineStr">
-        <is>
-          <t>10.69.5.155</t>
-        </is>
-      </c>
       <c r="D286" t="n">
         <v>2019</v>
       </c>
@@ -18915,7 +18910,7 @@
         <v>1</v>
       </c>
       <c r="N286" s="3" t="n">
-        <v>46080.56425925926</v>
+        <v>46080.59967592593</v>
       </c>
       <c r="O286" t="inlineStr">
         <is>
@@ -18979,7 +18974,7 @@
         <v>1</v>
       </c>
       <c r="N287" s="3" t="n">
-        <v>46080.54148148148</v>
+        <v>46080.57688657408</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
@@ -19107,7 +19102,7 @@
         <v>1</v>
       </c>
       <c r="N289" s="3" t="n">
-        <v>46080.53413194444</v>
+        <v>46080.57341435185</v>
       </c>
       <c r="O289" t="inlineStr">
         <is>
@@ -19901,7 +19896,7 @@
         <v>1</v>
       </c>
       <c r="N302" s="3" t="n">
-        <v>46080.54085648148</v>
+        <v>46080.65412037037</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -21017,7 +21012,7 @@
         </is>
       </c>
       <c r="N320" s="3" t="n">
-        <v>46080.53795138889</v>
+        <v>46080.65309027778</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21742,7 +21737,7 @@
         <v>1</v>
       </c>
       <c r="N332" s="3" t="n">
-        <v>46080.565</v>
+        <v>46080.64280092593</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21806,7 +21801,7 @@
         <v>2</v>
       </c>
       <c r="N333" s="3" t="n">
-        <v>46080.56015046296</v>
+        <v>46080.6371412037</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21870,7 +21865,7 @@
         <v>2</v>
       </c>
       <c r="N334" s="3" t="n">
-        <v>46080.55841435185</v>
+        <v>46080.63818287037</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21934,7 +21929,7 @@
         <v>2</v>
       </c>
       <c r="N335" s="3" t="n">
-        <v>46080.55457175926</v>
+        <v>46080.62885416667</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -21998,7 +21993,7 @@
         <v>1</v>
       </c>
       <c r="N336" s="3" t="n">
-        <v>46080.55201388889</v>
+        <v>46080.62769675926</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22062,7 +22057,7 @@
         <v>1</v>
       </c>
       <c r="N337" s="3" t="n">
-        <v>46080.56247685185</v>
+        <v>46080.63943287037</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22126,7 +22121,7 @@
         <v>2</v>
       </c>
       <c r="N338" s="3" t="n">
-        <v>46080.56357638889</v>
+        <v>46080.6374537037</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -22190,7 +22185,7 @@
         <v>2</v>
       </c>
       <c r="N339" s="3" t="n">
-        <v>46080.53240740741</v>
+        <v>46080.65016203704</v>
       </c>
       <c r="O339" t="inlineStr">
         <is>
@@ -22382,7 +22377,7 @@
         <v>2</v>
       </c>
       <c r="N342" s="3" t="n">
-        <v>46080.54152777778</v>
+        <v>46080.58256944444</v>
       </c>
       <c r="O342" t="inlineStr">
         <is>
@@ -22699,7 +22694,7 @@
         <v>1</v>
       </c>
       <c r="N347" s="3" t="n">
-        <v>46080.52020833334</v>
+        <v>46080.63840277777</v>
       </c>
       <c r="O347" t="inlineStr">
         <is>
@@ -22763,7 +22758,7 @@
         <v>1</v>
       </c>
       <c r="N348" s="3" t="n">
-        <v>46080.55288194444</v>
+        <v>46080.63027777777</v>
       </c>
       <c r="O348" t="inlineStr">
         <is>
@@ -22827,7 +22822,7 @@
         <v>1</v>
       </c>
       <c r="N349" s="3" t="n">
-        <v>46080.55310185185</v>
+        <v>46080.63084490741</v>
       </c>
       <c r="O349" t="inlineStr">
         <is>
@@ -22846,6 +22841,11 @@
           <t>OPERACAO 9.1</t>
         </is>
       </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>10.69.5.244</t>
+        </is>
+      </c>
       <c r="D350" t="n">
         <v>2014</v>
       </c>
@@ -22886,7 +22886,7 @@
         <v>1</v>
       </c>
       <c r="N350" s="3" t="n">
-        <v>46080.53824074074</v>
+        <v>46080.65211805556</v>
       </c>
       <c r="O350" t="inlineStr">
         <is>
@@ -22950,7 +22950,7 @@
         <v>1</v>
       </c>
       <c r="N351" s="3" t="n">
-        <v>46080.54899305556</v>
+        <v>46080.62912037037</v>
       </c>
       <c r="O351" t="inlineStr">
         <is>
@@ -23014,7 +23014,7 @@
         <v>1</v>
       </c>
       <c r="N352" s="3" t="n">
-        <v>46080.55096064815</v>
+        <v>46080.62783564815</v>
       </c>
       <c r="O352" t="inlineStr">
         <is>
@@ -23075,7 +23075,7 @@
         </is>
       </c>
       <c r="N353" s="3" t="n">
-        <v>46080.55033564815</v>
+        <v>46080.62822916666</v>
       </c>
       <c r="O353" t="inlineStr">
         <is>
@@ -23200,7 +23200,7 @@
         <v>1</v>
       </c>
       <c r="N355" s="3" t="n">
-        <v>46080.54849537037</v>
+        <v>46080.6255787037</v>
       </c>
       <c r="O355" t="inlineStr">
         <is>
@@ -23264,7 +23264,7 @@
         <v>1</v>
       </c>
       <c r="N356" s="3" t="n">
-        <v>46080.55354166667</v>
+        <v>46080.63412037037</v>
       </c>
       <c r="O356" t="inlineStr">
         <is>
@@ -23328,7 +23328,7 @@
         <v>1</v>
       </c>
       <c r="N357" s="3" t="n">
-        <v>46080.55361111111</v>
+        <v>46080.63456018519</v>
       </c>
       <c r="O357" t="inlineStr">
         <is>
@@ -23451,7 +23451,7 @@
         <v>2</v>
       </c>
       <c r="N359" s="3" t="n">
-        <v>46080.55465277778</v>
+        <v>46080.6303587963</v>
       </c>
       <c r="O359" t="inlineStr">
         <is>
@@ -23515,7 +23515,7 @@
         <v>2</v>
       </c>
       <c r="N360" s="3" t="n">
-        <v>46080.55405092592</v>
+        <v>46080.63105324074</v>
       </c>
       <c r="O360" t="inlineStr">
         <is>
@@ -23828,7 +23828,7 @@
         <v>1</v>
       </c>
       <c r="N365" s="3" t="n">
-        <v>46080.56840277778</v>
+        <v>46080.64300925926</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
@@ -23894,7 +23894,7 @@
         </is>
       </c>
       <c r="N366" s="3" t="n">
-        <v>46080.53409722223</v>
+        <v>46080.65256944444</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -24020,7 +24020,7 @@
         </is>
       </c>
       <c r="N368" s="3" t="n">
-        <v>46080.54230324074</v>
+        <v>46080.62314814814</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -24086,7 +24086,7 @@
         </is>
       </c>
       <c r="N369" s="3" t="n">
-        <v>46080.56685185185</v>
+        <v>46080.64634259259</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
@@ -24431,7 +24431,7 @@
         <v>1</v>
       </c>
       <c r="N374" s="3" t="n">
-        <v>46080.55211805556</v>
+        <v>46080.628125</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24497,7 +24497,7 @@
         </is>
       </c>
       <c r="N375" s="3" t="n">
-        <v>46080.56451388889</v>
+        <v>46080.64086805555</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
@@ -24561,7 +24561,7 @@
         <v>1</v>
       </c>
       <c r="N376" s="3" t="n">
-        <v>46080.56719907407</v>
+        <v>46080.64790509259</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -24630,7 +24630,7 @@
         <v>2</v>
       </c>
       <c r="N377" s="3" t="n">
-        <v>46080.55475694445</v>
+        <v>46080.63305555555</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -24699,7 +24699,7 @@
         <v>2</v>
       </c>
       <c r="N378" s="3" t="n">
-        <v>46080.55615740741</v>
+        <v>46080.6312962963</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização automática 2026-02-27 17:52:04.255022
</commit_message>
<xml_diff>
--- a/Computadores.xlsx
+++ b/Computadores.xlsx
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>46080.62944444444</v>
+        <v>46080.70622685185</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>46080.62396990741</v>
+        <v>46080.73770833333</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
         <v>2</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>46080.64891203704</v>
+        <v>46080.68978009259</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>46080.65253472222</v>
+        <v>46080.72899305556</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -944,7 +944,7 @@
         <v>1</v>
       </c>
       <c r="N7" s="3" t="n">
-        <v>46080.64746527778</v>
+        <v>46080.72792824074</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -1259,7 +1259,7 @@
         <v>1</v>
       </c>
       <c r="N12" s="3" t="n">
-        <v>46080.62701388889</v>
+        <v>46080.7062037037</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1323,7 +1323,7 @@
         <v>1</v>
       </c>
       <c r="N13" s="3" t="n">
-        <v>46080.62956018518</v>
+        <v>46080.70592592593</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1387,7 +1387,7 @@
         <v>2</v>
       </c>
       <c r="N14" s="3" t="n">
-        <v>46080.6306712963</v>
+        <v>46080.7094212963</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1451,7 +1451,7 @@
         <v>1</v>
       </c>
       <c r="N15" s="3" t="n">
-        <v>46080.62552083333</v>
+        <v>46080.70561342593</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1515,7 +1515,7 @@
         <v>2</v>
       </c>
       <c r="N16" s="3" t="n">
-        <v>46080.65090277778</v>
+        <v>46080.73059027778</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1579,7 +1579,7 @@
         <v>1</v>
       </c>
       <c r="N17" s="3" t="n">
-        <v>46080.61520833334</v>
+        <v>46080.65475694444</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1643,7 +1643,7 @@
         <v>2</v>
       </c>
       <c r="N18" s="3" t="n">
-        <v>46080.63137731481</v>
+        <v>46080.71113425926</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1768,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="N20" s="3" t="n">
-        <v>46080.62667824074</v>
+        <v>46080.70501157407</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -6575,7 +6575,7 @@
         <v>1</v>
       </c>
       <c r="N95" s="3" t="n">
-        <v>46080.63277777778</v>
+        <v>46080.67180555555</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -6644,7 +6644,7 @@
         <v>1</v>
       </c>
       <c r="N96" s="3" t="n">
-        <v>46080.63701388889</v>
+        <v>46080.71556712963</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
@@ -6708,7 +6708,7 @@
         <v>1</v>
       </c>
       <c r="N97" s="3" t="n">
-        <v>46080.63965277778</v>
+        <v>46080.71765046296</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -6727,11 +6727,6 @@
           <t>COORDENACAO</t>
         </is>
       </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>10.69.3.94</t>
-        </is>
-      </c>
       <c r="D98" t="n">
         <v>2025</v>
       </c>
@@ -6777,7 +6772,7 @@
         <v>1</v>
       </c>
       <c r="N98" s="3" t="n">
-        <v>46080.65280092593</v>
+        <v>46080.68881944445</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -6846,7 +6841,7 @@
         <v>1</v>
       </c>
       <c r="N99" s="3" t="n">
-        <v>46080.65282407407</v>
+        <v>46080.7337962963</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -6915,7 +6910,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>46080.62483796296</v>
+        <v>46080.70234953704</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -6984,7 +6979,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="3" t="n">
-        <v>46080.65049768519</v>
+        <v>46080.7233449074</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -7053,7 +7048,7 @@
         <v>1</v>
       </c>
       <c r="N102" s="3" t="n">
-        <v>46080.63371527778</v>
+        <v>46080.71074074074</v>
       </c>
       <c r="O102" t="inlineStr">
         <is>
@@ -7122,7 +7117,7 @@
         <v>2</v>
       </c>
       <c r="N103" s="3" t="n">
-        <v>46080.62516203704</v>
+        <v>46080.70444444445</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
@@ -7517,7 +7512,7 @@
         <v>1</v>
       </c>
       <c r="N109" s="3" t="n">
-        <v>46080.64436342593</v>
+        <v>46080.72489583334</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -7586,7 +7581,7 @@
         <v>2</v>
       </c>
       <c r="N110" s="3" t="n">
-        <v>46080.64480324074</v>
+        <v>46080.72483796296</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -7655,7 +7650,7 @@
         <v>2</v>
       </c>
       <c r="N111" s="3" t="n">
-        <v>46080.43893518519</v>
+        <v>46080.71645833334</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
@@ -7724,7 +7719,7 @@
         <v>2</v>
       </c>
       <c r="N112" s="3" t="n">
-        <v>46080.62628472222</v>
+        <v>46080.70658564815</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -7793,7 +7788,7 @@
         <v>1</v>
       </c>
       <c r="N113" s="3" t="n">
-        <v>46080.63946759259</v>
+        <v>46080.72392361111</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -7862,7 +7857,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>46080.646875</v>
+        <v>46080.72119212963</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -7928,7 +7923,7 @@
         </is>
       </c>
       <c r="N115" s="3" t="n">
-        <v>46080.63893518518</v>
+        <v>46080.68064814815</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -7997,7 +7992,7 @@
         <v>1</v>
       </c>
       <c r="N116" s="3" t="n">
-        <v>46080.64761574074</v>
+        <v>46080.68903935186</v>
       </c>
       <c r="O116" t="inlineStr">
         <is>
@@ -8061,7 +8056,7 @@
         <v>1</v>
       </c>
       <c r="N117" s="3" t="n">
-        <v>46080.63133101852</v>
+        <v>46080.70883101852</v>
       </c>
       <c r="O117" t="inlineStr">
         <is>
@@ -8127,7 +8122,7 @@
         </is>
       </c>
       <c r="N118" s="3" t="n">
-        <v>46080.65119212963</v>
+        <v>46080.69048611111</v>
       </c>
       <c r="O118" t="inlineStr">
         <is>
@@ -8265,7 +8260,7 @@
         <v>1</v>
       </c>
       <c r="N120" s="3" t="n">
-        <v>46080.64048611111</v>
+        <v>46080.71517361111</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -8334,7 +8329,7 @@
         <v>1</v>
       </c>
       <c r="N121" s="3" t="n">
-        <v>46080.63362268519</v>
+        <v>46080.71342592593</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -8400,7 +8395,7 @@
         </is>
       </c>
       <c r="N122" s="3" t="n">
-        <v>46080.63844907407</v>
+        <v>46080.715</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -8469,7 +8464,7 @@
         <v>2</v>
       </c>
       <c r="N123" s="3" t="n">
-        <v>46080.64402777778</v>
+        <v>46080.72591435185</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -8538,7 +8533,7 @@
         <v>1</v>
       </c>
       <c r="N124" s="3" t="n">
-        <v>46080.6445949074</v>
+        <v>46080.72495370371</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -8607,7 +8602,7 @@
         <v>1</v>
       </c>
       <c r="N125" s="3" t="n">
-        <v>46080.36364583333</v>
+        <v>46080.73165509259</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -8676,7 +8671,7 @@
         <v>2</v>
       </c>
       <c r="N126" s="3" t="n">
-        <v>46080.62743055556</v>
+        <v>46080.70289351852</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -8745,7 +8740,7 @@
         <v>2</v>
       </c>
       <c r="N127" s="3" t="n">
-        <v>46080.62059027778</v>
+        <v>46080.73563657407</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -8814,7 +8809,7 @@
         <v>1</v>
       </c>
       <c r="N128" s="3" t="n">
-        <v>46080.6449074074</v>
+        <v>46080.6821412037</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -8883,7 +8878,7 @@
         <v>1</v>
       </c>
       <c r="N129" s="3" t="n">
-        <v>46080.62761574074</v>
+        <v>46080.70576388889</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -9016,7 +9011,7 @@
         <v>1</v>
       </c>
       <c r="N131" s="3" t="n">
-        <v>46080.62782407407</v>
+        <v>46080.66407407408</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -9277,7 +9272,7 @@
         <v>1</v>
       </c>
       <c r="N135" s="3" t="n">
-        <v>46080.6172337963</v>
+        <v>46080.73708333333</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -9468,7 +9463,7 @@
         <v>1</v>
       </c>
       <c r="N138" s="3" t="n">
-        <v>46080.63853009259</v>
+        <v>46080.7143287037</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -9532,7 +9527,7 @@
         <v>1</v>
       </c>
       <c r="N139" s="3" t="n">
-        <v>46080.63141203704</v>
+        <v>46080.70793981481</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -9596,7 +9591,7 @@
         <v>1</v>
       </c>
       <c r="N140" s="3" t="n">
-        <v>46080.65231481481</v>
+        <v>46080.73418981482</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -9660,7 +9655,7 @@
         <v>1</v>
       </c>
       <c r="N141" s="3" t="n">
-        <v>46080.64844907408</v>
+        <v>46080.72565972222</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -9724,7 +9719,7 @@
         <v>1</v>
       </c>
       <c r="N142" s="3" t="n">
-        <v>46080.65237268519</v>
+        <v>46080.73232638889</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -9852,7 +9847,7 @@
         <v>1</v>
       </c>
       <c r="N144" s="3" t="n">
-        <v>46080.65091435185</v>
+        <v>46080.72837962963</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -9916,7 +9911,7 @@
         <v>1</v>
       </c>
       <c r="N145" s="3" t="n">
-        <v>46080.61993055556</v>
+        <v>46080.73259259259</v>
       </c>
       <c r="O145" t="inlineStr">
         <is>
@@ -9980,7 +9975,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="3" t="n">
-        <v>46080.61956018519</v>
+        <v>46080.70055555556</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -10044,7 +10039,7 @@
         <v>1</v>
       </c>
       <c r="N147" s="3" t="n">
-        <v>46080.60875</v>
+        <v>46080.72015046296</v>
       </c>
       <c r="O147" t="inlineStr">
         <is>
@@ -10108,7 +10103,7 @@
         <v>1</v>
       </c>
       <c r="N148" s="3" t="n">
-        <v>46080.65302083334</v>
+        <v>46080.72857638889</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -10172,7 +10167,7 @@
         <v>1</v>
       </c>
       <c r="N149" s="3" t="n">
-        <v>46080.62432870371</v>
+        <v>46080.70193287037</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -10236,7 +10231,7 @@
         <v>1</v>
       </c>
       <c r="N150" s="3" t="n">
-        <v>46080.64971064815</v>
+        <v>46080.73216435185</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -10300,7 +10295,7 @@
         <v>1</v>
       </c>
       <c r="N151" s="3" t="n">
-        <v>46080.65299768518</v>
+        <v>46080.73047453703</v>
       </c>
       <c r="O151" t="inlineStr">
         <is>
@@ -10364,7 +10359,7 @@
         <v>1</v>
       </c>
       <c r="N152" s="3" t="n">
-        <v>46080.6196875</v>
+        <v>46080.73289351852</v>
       </c>
       <c r="O152" t="inlineStr">
         <is>
@@ -10487,7 +10482,7 @@
         <v>1</v>
       </c>
       <c r="N154" s="3" t="n">
-        <v>46080.62075231481</v>
+        <v>46080.73444444445</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
@@ -10551,7 +10546,7 @@
         <v>1</v>
       </c>
       <c r="N155" s="3" t="n">
-        <v>46080.65188657407</v>
+        <v>46080.73128472222</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -10615,7 +10610,7 @@
         <v>1</v>
       </c>
       <c r="N156" s="3" t="n">
-        <v>46080.62487268518</v>
+        <v>46080.69834490741</v>
       </c>
       <c r="O156" t="inlineStr">
         <is>
@@ -10743,7 +10738,7 @@
         <v>1</v>
       </c>
       <c r="N158" s="3" t="n">
-        <v>46080.61611111111</v>
+        <v>46080.73016203703</v>
       </c>
       <c r="O158" t="inlineStr">
         <is>
@@ -10807,7 +10802,7 @@
         <v>1</v>
       </c>
       <c r="N159" s="3" t="n">
-        <v>46080.61833333333</v>
+        <v>46080.70040509259</v>
       </c>
       <c r="O159" t="inlineStr">
         <is>
@@ -10871,7 +10866,7 @@
         <v>1</v>
       </c>
       <c r="N160" s="3" t="n">
-        <v>46080.63131944444</v>
+        <v>46080.70798611111</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
@@ -10935,7 +10930,7 @@
         <v>1</v>
       </c>
       <c r="N161" s="3" t="n">
-        <v>46080.62393518518</v>
+        <v>46080.73342592592</v>
       </c>
       <c r="O161" t="inlineStr">
         <is>
@@ -10999,7 +10994,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="3" t="n">
-        <v>46080.63324074074</v>
+        <v>46080.70929398148</v>
       </c>
       <c r="O162" t="inlineStr">
         <is>
@@ -11127,7 +11122,7 @@
         <v>2</v>
       </c>
       <c r="N164" s="3" t="n">
-        <v>46080.64672453704</v>
+        <v>46080.71997685185</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
@@ -11447,7 +11442,7 @@
         <v>2</v>
       </c>
       <c r="N169" s="3" t="n">
-        <v>46080.62070601852</v>
+        <v>46080.70202546296</v>
       </c>
       <c r="O169" t="inlineStr">
         <is>
@@ -11511,7 +11506,7 @@
         <v>2</v>
       </c>
       <c r="N170" s="3" t="n">
-        <v>46080.64862268518</v>
+        <v>46080.72527777778</v>
       </c>
       <c r="O170" t="inlineStr">
         <is>
@@ -11703,7 +11698,7 @@
         <v>1</v>
       </c>
       <c r="N173" s="3" t="n">
-        <v>46080.65034722222</v>
+        <v>46080.7253125</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -11831,7 +11826,7 @@
         <v>2</v>
       </c>
       <c r="N175" s="3" t="n">
-        <v>46080.64421296296</v>
+        <v>46080.72491898148</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
@@ -11895,7 +11890,7 @@
         <v>2</v>
       </c>
       <c r="N176" s="3" t="n">
-        <v>46080.62340277778</v>
+        <v>46080.70550925926</v>
       </c>
       <c r="O176" t="inlineStr">
         <is>
@@ -11959,7 +11954,7 @@
         <v>2</v>
       </c>
       <c r="N177" s="3" t="n">
-        <v>46080.62196759259</v>
+        <v>46080.69650462963</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
@@ -12023,7 +12018,7 @@
         <v>2</v>
       </c>
       <c r="N178" s="3" t="n">
-        <v>46080.62789351852</v>
+        <v>46080.70347222222</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -12087,7 +12082,7 @@
         <v>1</v>
       </c>
       <c r="N179" s="3" t="n">
-        <v>46080.63086805555</v>
+        <v>46080.70797453704</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -12151,7 +12146,7 @@
         <v>1</v>
       </c>
       <c r="N180" s="3" t="n">
-        <v>46080.62075231481</v>
+        <v>46080.73609953704</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -12343,7 +12338,7 @@
         <v>1</v>
       </c>
       <c r="N183" s="3" t="n">
-        <v>46080.62266203704</v>
+        <v>46080.69935185185</v>
       </c>
       <c r="O183" t="inlineStr">
         <is>
@@ -12412,7 +12407,7 @@
         <v>2</v>
       </c>
       <c r="N184" s="3" t="n">
-        <v>46080.63200231481</v>
+        <v>46080.70799768518</v>
       </c>
       <c r="O184" t="inlineStr">
         <is>
@@ -12604,7 +12599,7 @@
         <v>1</v>
       </c>
       <c r="N187" s="3" t="n">
-        <v>46080.63108796296</v>
+        <v>46080.7100462963</v>
       </c>
       <c r="O187" t="inlineStr">
         <is>
@@ -12791,7 +12786,7 @@
         </is>
       </c>
       <c r="N190" s="3" t="n">
-        <v>46080.63501157407</v>
+        <v>46080.71196759259</v>
       </c>
       <c r="O190" t="inlineStr">
         <is>
@@ -12855,7 +12850,7 @@
         <v>1</v>
       </c>
       <c r="N191" s="3" t="n">
-        <v>46080.63179398148</v>
+        <v>46080.7084837963</v>
       </c>
       <c r="O191" t="inlineStr">
         <is>
@@ -12919,7 +12914,7 @@
         <v>1</v>
       </c>
       <c r="N192" s="3" t="n">
-        <v>46080.63790509259</v>
+        <v>46080.71560185185</v>
       </c>
       <c r="O192" t="inlineStr">
         <is>
@@ -13108,7 +13103,7 @@
         <v>1</v>
       </c>
       <c r="N195" s="3" t="n">
-        <v>46080.61961805556</v>
+        <v>46080.70313657408</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
@@ -13172,7 +13167,7 @@
         <v>1</v>
       </c>
       <c r="N196" s="3" t="n">
-        <v>46080.57857638889</v>
+        <v>46080.70790509259</v>
       </c>
       <c r="O196" t="inlineStr">
         <is>
@@ -13236,7 +13231,7 @@
         <v>1</v>
       </c>
       <c r="N197" s="3" t="n">
-        <v>46079.84797453704</v>
+        <v>46080.70378472222</v>
       </c>
       <c r="O197" t="inlineStr">
         <is>
@@ -13300,7 +13295,7 @@
         <v>1</v>
       </c>
       <c r="N198" s="3" t="n">
-        <v>46080.65349537037</v>
+        <v>46080.73332175926</v>
       </c>
       <c r="O198" t="inlineStr">
         <is>
@@ -13364,7 +13359,7 @@
         <v>1</v>
       </c>
       <c r="N199" s="3" t="n">
-        <v>46080.64201388889</v>
+        <v>46080.72146990741</v>
       </c>
       <c r="O199" t="inlineStr">
         <is>
@@ -13428,7 +13423,7 @@
         <v>1</v>
       </c>
       <c r="N200" s="3" t="n">
-        <v>46080.61910879629</v>
+        <v>46080.73277777778</v>
       </c>
       <c r="O200" t="inlineStr">
         <is>
@@ -13489,7 +13484,7 @@
         </is>
       </c>
       <c r="N201" s="3" t="n">
-        <v>46080.63416666666</v>
+        <v>46080.71288194445</v>
       </c>
       <c r="O201" t="inlineStr">
         <is>
@@ -13553,7 +13548,7 @@
         <v>1</v>
       </c>
       <c r="N202" s="3" t="n">
-        <v>46080.6408912037</v>
+        <v>46080.71694444444</v>
       </c>
       <c r="O202" t="inlineStr">
         <is>
@@ -13617,7 +13612,7 @@
         <v>1</v>
       </c>
       <c r="N203" s="3" t="n">
-        <v>46080.61767361111</v>
+        <v>46080.73456018518</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
@@ -13681,7 +13676,7 @@
         <v>1</v>
       </c>
       <c r="N204" s="3" t="n">
-        <v>46080.6215625</v>
+        <v>46080.73109953704</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
@@ -13745,7 +13740,7 @@
         <v>1</v>
       </c>
       <c r="N205" s="3" t="n">
-        <v>46080.64327546296</v>
+        <v>46080.72067129629</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
@@ -13809,7 +13804,7 @@
         <v>1</v>
       </c>
       <c r="N206" s="3" t="n">
-        <v>46080.65179398148</v>
+        <v>46080.73501157408</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -13873,7 +13868,7 @@
         <v>1</v>
       </c>
       <c r="N207" s="3" t="n">
-        <v>46080.6159375</v>
+        <v>46080.73173611111</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
@@ -14001,7 +13996,7 @@
         <v>1</v>
       </c>
       <c r="N209" s="3" t="n">
-        <v>46080.62675925926</v>
+        <v>46080.70480324074</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
@@ -14065,7 +14060,7 @@
         <v>1</v>
       </c>
       <c r="N210" s="3" t="n">
-        <v>46080.64144675926</v>
+        <v>46080.72105324074</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
@@ -14129,7 +14124,7 @@
         <v>1</v>
       </c>
       <c r="N211" s="3" t="n">
-        <v>46080.62349537037</v>
+        <v>46080.70155092593</v>
       </c>
       <c r="O211" t="inlineStr">
         <is>
@@ -14193,7 +14188,7 @@
         <v>1</v>
       </c>
       <c r="N212" s="3" t="n">
-        <v>46080.63898148148</v>
+        <v>46080.71762731481</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
@@ -14257,7 +14252,7 @@
         <v>1</v>
       </c>
       <c r="N213" s="3" t="n">
-        <v>46080.54304398148</v>
+        <v>46080.7065625</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
@@ -14321,7 +14316,7 @@
         <v>1</v>
       </c>
       <c r="N214" s="3" t="n">
-        <v>46080.63309027778</v>
+        <v>46080.71466435185</v>
       </c>
       <c r="O214" t="inlineStr">
         <is>
@@ -14385,7 +14380,7 @@
         <v>1</v>
       </c>
       <c r="N215" s="3" t="n">
-        <v>46080.63670138889</v>
+        <v>46080.71866898148</v>
       </c>
       <c r="O215" t="inlineStr">
         <is>
@@ -14449,7 +14444,7 @@
         <v>1</v>
       </c>
       <c r="N216" s="3" t="n">
-        <v>46080.63435185186</v>
+        <v>46080.71372685185</v>
       </c>
       <c r="O216" t="inlineStr">
         <is>
@@ -14513,7 +14508,7 @@
         <v>1</v>
       </c>
       <c r="N217" s="3" t="n">
-        <v>46080.62259259259</v>
+        <v>46080.7375</v>
       </c>
       <c r="O217" t="inlineStr">
         <is>
@@ -14577,7 +14572,7 @@
         <v>1</v>
       </c>
       <c r="N218" s="3" t="n">
-        <v>46080.64501157407</v>
+        <v>46080.72359953704</v>
       </c>
       <c r="O218" t="inlineStr">
         <is>
@@ -14641,7 +14636,7 @@
         <v>1</v>
       </c>
       <c r="N219" s="3" t="n">
-        <v>46080.61856481482</v>
+        <v>46080.73417824074</v>
       </c>
       <c r="O219" t="inlineStr">
         <is>
@@ -14710,7 +14705,7 @@
         <v>1</v>
       </c>
       <c r="N220" s="3" t="n">
-        <v>46080.40474537037</v>
+        <v>46080.71976851852</v>
       </c>
       <c r="O220" t="inlineStr">
         <is>
@@ -14774,7 +14769,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="3" t="n">
-        <v>46080.62303240741</v>
+        <v>46080.70052083334</v>
       </c>
       <c r="O221" t="inlineStr">
         <is>
@@ -14838,7 +14833,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="3" t="n">
-        <v>46080.62339120371</v>
+        <v>46080.73560185185</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
@@ -14902,7 +14897,7 @@
         <v>1</v>
       </c>
       <c r="N223" s="3" t="n">
-        <v>46080.65202546296</v>
+        <v>46080.7293287037</v>
       </c>
       <c r="O223" t="inlineStr">
         <is>
@@ -14966,7 +14961,7 @@
         <v>1</v>
       </c>
       <c r="N224" s="3" t="n">
-        <v>46080.64589120371</v>
+        <v>46080.71967592592</v>
       </c>
       <c r="O224" t="inlineStr">
         <is>
@@ -15094,7 +15089,7 @@
         <v>1</v>
       </c>
       <c r="N226" s="3" t="n">
-        <v>46080.63903935185</v>
+        <v>46080.71939814815</v>
       </c>
       <c r="O226" t="inlineStr">
         <is>
@@ -15158,7 +15153,7 @@
         <v>1</v>
       </c>
       <c r="N227" s="3" t="n">
-        <v>46080.63994212963</v>
+        <v>46080.71240740741</v>
       </c>
       <c r="O227" t="inlineStr">
         <is>
@@ -15222,7 +15217,7 @@
         <v>1</v>
       </c>
       <c r="N228" s="3" t="n">
-        <v>46080.61568287037</v>
+        <v>46080.73627314815</v>
       </c>
       <c r="O228" t="inlineStr">
         <is>
@@ -15350,7 +15345,7 @@
         <v>1</v>
       </c>
       <c r="N230" s="3" t="n">
-        <v>46080.62736111111</v>
+        <v>46080.70516203704</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -15414,7 +15409,7 @@
         <v>1</v>
       </c>
       <c r="N231" s="3" t="n">
-        <v>46080.61688657408</v>
+        <v>46080.73565972222</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -15478,7 +15473,7 @@
         <v>1</v>
       </c>
       <c r="N232" s="3" t="n">
-        <v>46080.65204861111</v>
+        <v>46080.73290509259</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -15542,7 +15537,7 @@
         <v>1</v>
       </c>
       <c r="N233" s="3" t="n">
-        <v>46080.64737268518</v>
+        <v>46080.72672453704</v>
       </c>
       <c r="O233" t="inlineStr">
         <is>
@@ -15606,7 +15601,7 @@
         <v>1</v>
       </c>
       <c r="N234" s="3" t="n">
-        <v>46080.56596064815</v>
+        <v>46080.70543981482</v>
       </c>
       <c r="O234" t="inlineStr">
         <is>
@@ -15670,7 +15665,7 @@
         <v>1</v>
       </c>
       <c r="N235" s="3" t="n">
-        <v>46080.63100694444</v>
+        <v>46080.70927083334</v>
       </c>
       <c r="O235" t="inlineStr">
         <is>
@@ -15734,7 +15729,7 @@
         <v>1</v>
       </c>
       <c r="N236" s="3" t="n">
-        <v>46079.80925925926</v>
+        <v>46080.70577546296</v>
       </c>
       <c r="O236" t="inlineStr">
         <is>
@@ -15862,7 +15857,7 @@
         <v>1</v>
       </c>
       <c r="N238" s="3" t="n">
-        <v>46080.62494212963</v>
+        <v>46080.70150462963</v>
       </c>
       <c r="O238" t="inlineStr">
         <is>
@@ -15926,7 +15921,7 @@
         <v>1</v>
       </c>
       <c r="N239" s="3" t="n">
-        <v>46080.64140046296</v>
+        <v>46080.72047453704</v>
       </c>
       <c r="O239" t="inlineStr">
         <is>
@@ -15990,7 +15985,7 @@
         <v>1</v>
       </c>
       <c r="N240" s="3" t="n">
-        <v>46080.63086805555</v>
+        <v>46080.7078125</v>
       </c>
       <c r="O240" t="inlineStr">
         <is>
@@ -16054,7 +16049,7 @@
         <v>1</v>
       </c>
       <c r="N241" s="3" t="n">
-        <v>46080.60583333333</v>
+        <v>46080.70758101852</v>
       </c>
       <c r="O241" t="inlineStr">
         <is>
@@ -16118,7 +16113,7 @@
         <v>1</v>
       </c>
       <c r="N242" s="3" t="n">
-        <v>46080.61520833334</v>
+        <v>46080.73600694445</v>
       </c>
       <c r="O242" t="inlineStr">
         <is>
@@ -16182,7 +16177,7 @@
         <v>1</v>
       </c>
       <c r="N243" s="3" t="n">
-        <v>46079.78887731482</v>
+        <v>46080.67122685185</v>
       </c>
       <c r="O243" t="inlineStr">
         <is>
@@ -16305,7 +16300,7 @@
         <v>1</v>
       </c>
       <c r="N245" s="3" t="n">
-        <v>46080.62653935186</v>
+        <v>46080.70635416666</v>
       </c>
       <c r="O245" t="inlineStr">
         <is>
@@ -16369,7 +16364,7 @@
         <v>1</v>
       </c>
       <c r="N246" s="3" t="n">
-        <v>46080.61601851852</v>
+        <v>46080.73402777778</v>
       </c>
       <c r="O246" t="inlineStr">
         <is>
@@ -16433,7 +16428,7 @@
         <v>1</v>
       </c>
       <c r="N247" s="3" t="n">
-        <v>46080.62762731482</v>
+        <v>46080.709375</v>
       </c>
       <c r="O247" t="inlineStr">
         <is>
@@ -16497,7 +16492,7 @@
         <v>1</v>
       </c>
       <c r="N248" s="3" t="n">
-        <v>46080.63480324074</v>
+        <v>46080.70929398148</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
@@ -16580,6 +16575,11 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>10.69.5.118</t>
+        </is>
+      </c>
       <c r="D250" t="n">
         <v>2017</v>
       </c>
@@ -16620,7 +16620,7 @@
         <v>1</v>
       </c>
       <c r="N250" s="3" t="n">
-        <v>46080.62015046296</v>
+        <v>46080.73658564815</v>
       </c>
       <c r="O250" t="inlineStr">
         <is>
@@ -16684,7 +16684,7 @@
         <v>1</v>
       </c>
       <c r="N251" s="3" t="n">
-        <v>46080.61557870371</v>
+        <v>46080.71563657407</v>
       </c>
       <c r="O251" t="inlineStr">
         <is>
@@ -16748,7 +16748,7 @@
         <v>1</v>
       </c>
       <c r="N252" s="3" t="n">
-        <v>46080.6252662037</v>
+        <v>46080.7049537037</v>
       </c>
       <c r="O252" t="inlineStr">
         <is>
@@ -16812,7 +16812,7 @@
         <v>1</v>
       </c>
       <c r="N253" s="3" t="n">
-        <v>46080.62340277778</v>
+        <v>46080.6999074074</v>
       </c>
       <c r="O253" t="inlineStr">
         <is>
@@ -16870,7 +16870,7 @@
         <v>1</v>
       </c>
       <c r="N254" s="3" t="n">
-        <v>46080.63398148148</v>
+        <v>46080.70893518518</v>
       </c>
       <c r="O254" t="inlineStr">
         <is>
@@ -16934,7 +16934,7 @@
         <v>1</v>
       </c>
       <c r="N255" s="3" t="n">
-        <v>46080.62864583333</v>
+        <v>46080.71915509259</v>
       </c>
       <c r="O255" t="inlineStr">
         <is>
@@ -16998,7 +16998,7 @@
         <v>1</v>
       </c>
       <c r="N256" s="3" t="n">
-        <v>46080.63064814815</v>
+        <v>46080.71219907407</v>
       </c>
       <c r="O256" t="inlineStr">
         <is>
@@ -17062,7 +17062,7 @@
         <v>1</v>
       </c>
       <c r="N257" s="3" t="n">
-        <v>46080.63596064815</v>
+        <v>46080.71725694444</v>
       </c>
       <c r="O257" t="inlineStr">
         <is>
@@ -17126,7 +17126,7 @@
         <v>1</v>
       </c>
       <c r="N258" s="3" t="n">
-        <v>46080.62800925926</v>
+        <v>46080.71673611111</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
@@ -17190,7 +17190,7 @@
         <v>1</v>
       </c>
       <c r="N259" s="3" t="n">
-        <v>46080.62923611111</v>
+        <v>46080.70047453704</v>
       </c>
       <c r="O259" t="inlineStr">
         <is>
@@ -17318,7 +17318,7 @@
         <v>1</v>
       </c>
       <c r="N261" s="3" t="n">
-        <v>46080.63490740741</v>
+        <v>46080.71167824074</v>
       </c>
       <c r="O261" t="inlineStr">
         <is>
@@ -17382,7 +17382,7 @@
         <v>1</v>
       </c>
       <c r="N262" s="3" t="n">
-        <v>46080.62202546297</v>
+        <v>46080.73739583333</v>
       </c>
       <c r="O262" t="inlineStr">
         <is>
@@ -17446,7 +17446,7 @@
         <v>1</v>
       </c>
       <c r="N263" s="3" t="n">
-        <v>46080.65016203704</v>
+        <v>46080.72732638889</v>
       </c>
       <c r="O263" t="inlineStr">
         <is>
@@ -17510,7 +17510,7 @@
         <v>1</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>46080.62268518518</v>
+        <v>46080.70329861111</v>
       </c>
       <c r="O264" t="inlineStr">
         <is>
@@ -17574,7 +17574,7 @@
         <v>1</v>
       </c>
       <c r="N265" s="3" t="n">
-        <v>46080.63731481481</v>
+        <v>46080.7137037037</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -17638,7 +17638,7 @@
         <v>1</v>
       </c>
       <c r="N266" s="3" t="n">
-        <v>46080.62184027778</v>
+        <v>46080.7033912037</v>
       </c>
       <c r="O266" t="inlineStr">
         <is>
@@ -17702,7 +17702,7 @@
         <v>1</v>
       </c>
       <c r="N267" s="3" t="n">
-        <v>46080.65155092593</v>
+        <v>46080.73524305555</v>
       </c>
       <c r="O267" t="inlineStr">
         <is>
@@ -17766,7 +17766,7 @@
         <v>1</v>
       </c>
       <c r="N268" s="3" t="n">
-        <v>46080.64229166666</v>
+        <v>46080.71549768518</v>
       </c>
       <c r="O268" t="inlineStr">
         <is>
@@ -17830,7 +17830,7 @@
         <v>1</v>
       </c>
       <c r="N269" s="3" t="n">
-        <v>46080.65320601852</v>
+        <v>46080.72547453704</v>
       </c>
       <c r="O269" t="inlineStr">
         <is>
@@ -17891,7 +17891,7 @@
         </is>
       </c>
       <c r="N270" s="3" t="n">
-        <v>46080.62010416666</v>
+        <v>46080.70121527778</v>
       </c>
       <c r="O270" t="inlineStr">
         <is>
@@ -18019,7 +18019,7 @@
         <v>1</v>
       </c>
       <c r="N272" s="3" t="n">
-        <v>46080.62271990741</v>
+        <v>46080.65876157407</v>
       </c>
       <c r="O272" t="inlineStr">
         <is>
@@ -18339,7 +18339,7 @@
         <v>1</v>
       </c>
       <c r="N277" s="3" t="n">
-        <v>46080.53513888889</v>
+        <v>46080.70896990741</v>
       </c>
       <c r="O277" t="inlineStr">
         <is>
@@ -18614,11 +18614,6 @@
           <t>OPERACAO 8.2</t>
         </is>
       </c>
-      <c r="C282" t="inlineStr">
-        <is>
-          <t>10.69.5.151</t>
-        </is>
-      </c>
       <c r="D282" t="n">
         <v>2017</v>
       </c>
@@ -18659,7 +18654,7 @@
         <v>1</v>
       </c>
       <c r="N282" s="3" t="n">
-        <v>46080.62888888889</v>
+        <v>46080.70571759259</v>
       </c>
       <c r="O282" t="inlineStr">
         <is>
@@ -18787,7 +18782,7 @@
         <v>1</v>
       </c>
       <c r="N284" s="3" t="n">
-        <v>46080.62822916666</v>
+        <v>46080.70614583333</v>
       </c>
       <c r="O284" t="inlineStr">
         <is>
@@ -18851,7 +18846,7 @@
         <v>1</v>
       </c>
       <c r="N285" s="3" t="n">
-        <v>46080.61467592593</v>
+        <v>46080.73055555556</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
@@ -19896,7 +19891,7 @@
         <v>1</v>
       </c>
       <c r="N302" s="3" t="n">
-        <v>46080.65412037037</v>
+        <v>46080.73355324074</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -21012,7 +21007,7 @@
         </is>
       </c>
       <c r="N320" s="3" t="n">
-        <v>46080.65309027778</v>
+        <v>46080.72577546296</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -21737,7 +21732,7 @@
         <v>1</v>
       </c>
       <c r="N332" s="3" t="n">
-        <v>46080.64280092593</v>
+        <v>46080.71975694445</v>
       </c>
       <c r="O332" t="inlineStr">
         <is>
@@ -21801,7 +21796,7 @@
         <v>2</v>
       </c>
       <c r="N333" s="3" t="n">
-        <v>46080.6371412037</v>
+        <v>46080.71267361111</v>
       </c>
       <c r="O333" t="inlineStr">
         <is>
@@ -21865,7 +21860,7 @@
         <v>2</v>
       </c>
       <c r="N334" s="3" t="n">
-        <v>46080.63818287037</v>
+        <v>46080.71724537037</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
@@ -21929,7 +21924,7 @@
         <v>2</v>
       </c>
       <c r="N335" s="3" t="n">
-        <v>46080.62885416667</v>
+        <v>46080.70806712963</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
@@ -21993,7 +21988,7 @@
         <v>1</v>
       </c>
       <c r="N336" s="3" t="n">
-        <v>46080.62769675926</v>
+        <v>46080.70563657407</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
@@ -22057,7 +22052,7 @@
         <v>1</v>
       </c>
       <c r="N337" s="3" t="n">
-        <v>46080.63943287037</v>
+        <v>46080.71649305556</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
@@ -22121,7 +22116,7 @@
         <v>2</v>
       </c>
       <c r="N338" s="3" t="n">
-        <v>46080.6374537037</v>
+        <v>46080.71361111111</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -22185,7 +22180,7 @@
         <v>2</v>
       </c>
       <c r="N339" s="3" t="n">
-        <v>46080.65016203704</v>
+        <v>46080.73273148148</v>
       </c>
       <c r="O339" t="inlineStr">
         <is>
@@ -22758,7 +22753,7 @@
         <v>1</v>
       </c>
       <c r="N348" s="3" t="n">
-        <v>46080.63027777777</v>
+        <v>46080.70405092592</v>
       </c>
       <c r="O348" t="inlineStr">
         <is>
@@ -22822,7 +22817,7 @@
         <v>1</v>
       </c>
       <c r="N349" s="3" t="n">
-        <v>46080.63084490741</v>
+        <v>46080.71203703704</v>
       </c>
       <c r="O349" t="inlineStr">
         <is>
@@ -22886,7 +22881,7 @@
         <v>1</v>
       </c>
       <c r="N350" s="3" t="n">
-        <v>46080.65211805556</v>
+        <v>46080.72943287037</v>
       </c>
       <c r="O350" t="inlineStr">
         <is>
@@ -22950,7 +22945,7 @@
         <v>1</v>
       </c>
       <c r="N351" s="3" t="n">
-        <v>46080.62912037037</v>
+        <v>46080.70388888889</v>
       </c>
       <c r="O351" t="inlineStr">
         <is>
@@ -23014,7 +23009,7 @@
         <v>1</v>
       </c>
       <c r="N352" s="3" t="n">
-        <v>46080.62783564815</v>
+        <v>46080.70270833333</v>
       </c>
       <c r="O352" t="inlineStr">
         <is>
@@ -23075,7 +23070,7 @@
         </is>
       </c>
       <c r="N353" s="3" t="n">
-        <v>46080.62822916666</v>
+        <v>46080.70700231481</v>
       </c>
       <c r="O353" t="inlineStr">
         <is>
@@ -23200,7 +23195,7 @@
         <v>1</v>
       </c>
       <c r="N355" s="3" t="n">
-        <v>46080.6255787037</v>
+        <v>46080.70574074074</v>
       </c>
       <c r="O355" t="inlineStr">
         <is>
@@ -23264,7 +23259,7 @@
         <v>1</v>
       </c>
       <c r="N356" s="3" t="n">
-        <v>46080.63412037037</v>
+        <v>46080.7109375</v>
       </c>
       <c r="O356" t="inlineStr">
         <is>
@@ -23328,7 +23323,7 @@
         <v>1</v>
       </c>
       <c r="N357" s="3" t="n">
-        <v>46080.63456018519</v>
+        <v>46080.70726851852</v>
       </c>
       <c r="O357" t="inlineStr">
         <is>
@@ -23451,7 +23446,7 @@
         <v>2</v>
       </c>
       <c r="N359" s="3" t="n">
-        <v>46080.6303587963</v>
+        <v>46080.7069675926</v>
       </c>
       <c r="O359" t="inlineStr">
         <is>
@@ -23515,7 +23510,7 @@
         <v>2</v>
       </c>
       <c r="N360" s="3" t="n">
-        <v>46080.63105324074</v>
+        <v>46080.70782407407</v>
       </c>
       <c r="O360" t="inlineStr">
         <is>
@@ -23828,7 +23823,7 @@
         <v>1</v>
       </c>
       <c r="N365" s="3" t="n">
-        <v>46080.64300925926</v>
+        <v>46080.68246527778</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
@@ -23894,7 +23889,7 @@
         </is>
       </c>
       <c r="N366" s="3" t="n">
-        <v>46080.65256944444</v>
+        <v>46080.72945601852</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -24020,7 +24015,7 @@
         </is>
       </c>
       <c r="N368" s="3" t="n">
-        <v>46080.62314814814</v>
+        <v>46080.73319444444</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -24086,7 +24081,7 @@
         </is>
       </c>
       <c r="N369" s="3" t="n">
-        <v>46080.64634259259</v>
+        <v>46080.72767361111</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
@@ -24431,7 +24426,7 @@
         <v>1</v>
       </c>
       <c r="N374" s="3" t="n">
-        <v>46080.628125</v>
+        <v>46080.70642361111</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -24497,7 +24492,7 @@
         </is>
       </c>
       <c r="N375" s="3" t="n">
-        <v>46080.64086805555</v>
+        <v>46080.72482638889</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
@@ -24516,6 +24511,11 @@
           <t>COORDENACAO</t>
         </is>
       </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>10.69.3.72</t>
+        </is>
+      </c>
       <c r="D376" t="n">
         <v>2025</v>
       </c>
@@ -24561,7 +24561,7 @@
         <v>1</v>
       </c>
       <c r="N376" s="3" t="n">
-        <v>46080.64790509259</v>
+        <v>46080.72820601852</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -24630,7 +24630,7 @@
         <v>2</v>
       </c>
       <c r="N377" s="3" t="n">
-        <v>46080.63305555555</v>
+        <v>46080.71266203704</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
@@ -24699,7 +24699,7 @@
         <v>2</v>
       </c>
       <c r="N378" s="3" t="n">
-        <v>46080.6312962963</v>
+        <v>46080.70809027777</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>

</xml_diff>